<commit_message>
CI: Auto Update Data
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -767,7 +767,7 @@
       </c>
       <c r="T2" s="14" t="inlineStr">
         <is>
-          <t>maa://22742 (91.47)</t>
+          <t>maa://22742 (91.51)</t>
         </is>
       </c>
       <c r="U2" s="11" t="n"/>
@@ -897,7 +897,7 @@
       </c>
       <c r="T3" s="14" t="inlineStr">
         <is>
-          <t>maa://24617 (90.91), maa://45854 (85.11)</t>
+          <t>maa://24617 (90.98), maa://45854 (84.21)</t>
         </is>
       </c>
       <c r="U3" s="11" t="n"/>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="AF7" s="14" t="inlineStr">
         <is>
-          <t>maa://45272 (97.06)</t>
+          <t>maa://45272 (97.14)</t>
         </is>
       </c>
       <c r="AG7" s="27" t="n"/>
@@ -1478,7 +1478,7 @@
     <row r="8">
       <c r="A8" s="10" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.12 13:21:11</t>
+          <t>更新日期：2025.06.13 13:21:05</t>
         </is>
       </c>
       <c r="B8" s="11" t="inlineStr">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="AB11" s="14" t="inlineStr">
         <is>
-          <t>maa://29912 (97.8), maa://22516 (87.36)</t>
+          <t>maa://29912 (97.85), maa://22516 (87.36)</t>
         </is>
       </c>
       <c r="AC11" s="11" t="n"/>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="AF12" s="14" t="inlineStr">
         <is>
-          <t>*maa://28932 (79.1), *maa://20106 (64.29), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (79.21), *maa://20106 (64.29), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="27" t="n"/>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>maa://24999 (92.71), maa://36673 (91.95), maa://25001 (86.49)</t>
+          <t>maa://24999 (92.74), maa://36673 (91.95), maa://25001 (86.49)</t>
         </is>
       </c>
       <c r="E13" s="11" t="n"/>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="H13" s="14" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.84), **maa://22728 (46.94)</t>
+          <t>*maa://21248 (73.93), **maa://22728 (46.94)</t>
         </is>
       </c>
       <c r="I13" s="11" t="n"/>
@@ -2305,7 +2305,7 @@
       </c>
       <c r="L14" s="14" t="inlineStr">
         <is>
-          <t>maa://39841 (94.34), maa://26245 (96.7), maa://21288 (96.3), maa://36682 (95.92)</t>
+          <t>maa://39841 (94.38), maa://26245 (96.7), maa://21288 (96.3), maa://36682 (95.92)</t>
         </is>
       </c>
       <c r="M14" s="11" t="n"/>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="D15" s="14" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.93), maa://22734 (84.55), *maa://30808 (64.79), *maa://36048 (69.64), maa://45058 (84.21)</t>
+          <t>*maa://22743 (78.93), maa://22734 (84.55), *maa://30808 (65.28), *maa://36048 (69.64), maa://45058 (85.0)</t>
         </is>
       </c>
       <c r="E15" s="11" t="n"/>
@@ -2515,7 +2515,7 @@
       </c>
       <c r="AF15" s="14" t="inlineStr">
         <is>
-          <t>maa://21364 (81.3), maa://36666 (81.99), *maa://22766 (68.55)</t>
+          <t>maa://21364 (81.3), maa://36666 (82.1), *maa://22766 (68.55)</t>
         </is>
       </c>
       <c r="AG15" s="27" t="n"/>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="H17" s="14" t="inlineStr">
         <is>
-          <t>maa://22430 (89.67), maa://39599 (86.59)</t>
+          <t>maa://22430 (89.67), maa://39599 (86.75)</t>
         </is>
       </c>
       <c r="I17" s="11" t="n"/>
@@ -2873,7 +2873,7 @@
       </c>
       <c r="X18" s="14" t="inlineStr">
         <is>
-          <t>maa://21917 (97.12), maa://22741 (87.5)</t>
+          <t>maa://21917 (97.14), maa://22741 (87.5)</t>
         </is>
       </c>
       <c r="Y18" s="11" t="n"/>
@@ -3019,7 +3019,7 @@
       </c>
       <c r="AB19" s="14" t="inlineStr">
         <is>
-          <t>*maa://30709 (68.6), *maa://36668 (57.32)</t>
+          <t>*maa://30709 (68.66), *maa://36668 (57.32)</t>
         </is>
       </c>
       <c r="AC19" s="11" t="n"/>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="H20" s="14" t="inlineStr">
         <is>
-          <t>maa://22864 (90.81)</t>
+          <t>maa://22864 (90.86)</t>
         </is>
       </c>
       <c r="I20" s="11" t="n"/>
@@ -3085,7 +3085,7 @@
       </c>
       <c r="L20" s="14" t="inlineStr">
         <is>
-          <t>maa://41331 (86.4)</t>
+          <t>maa://41331 (86.11)</t>
         </is>
       </c>
       <c r="M20" s="11" t="n"/>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="X20" s="14" t="inlineStr">
         <is>
-          <t>maa://50085 (87.77), maa://49976 (86.59), maa://56241 (88.89)</t>
+          <t>maa://50085 (87.94), maa://49976 (86.59), maa://56241 (88.89)</t>
         </is>
       </c>
       <c r="Y20" s="11" t="n"/>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="AB21" s="14" t="inlineStr">
         <is>
-          <t>maa://21443 (82.77), ***maa://23820 (30.0), **maa://52223 (40.62)</t>
+          <t>maa://21443 (82.81), ***maa://23820 (30.0), **maa://52223 (40.62)</t>
         </is>
       </c>
       <c r="AC21" s="11" t="n"/>
@@ -3425,7 +3425,7 @@
       </c>
       <c r="AF22" s="14" t="inlineStr">
         <is>
-          <t>maa://29658 (94.44)</t>
+          <t>maa://29658 (94.55)</t>
         </is>
       </c>
       <c r="AG22" s="27" t="n"/>
@@ -3475,7 +3475,7 @@
       </c>
       <c r="L23" s="14" t="inlineStr">
         <is>
-          <t>maa://39756 (95.77), maa://39875 (94.81)</t>
+          <t>maa://39756 (95.77), maa://39875 (94.87)</t>
         </is>
       </c>
       <c r="M23" s="11" t="n"/>
@@ -3573,7 +3573,7 @@
       </c>
       <c r="D24" s="14" t="inlineStr">
         <is>
-          <t>*maa://24368 (79.18), *maa://46650 (61.29)</t>
+          <t>*maa://24368 (79.23), *maa://46650 (61.29)</t>
         </is>
       </c>
       <c r="E24" s="11" t="n"/>
@@ -3653,7 +3653,7 @@
       </c>
       <c r="X24" s="14" t="inlineStr">
         <is>
-          <t>maa://29988 (85.15), maa://23504 (93.68), *maa://25141 (77.37), *maa://36663 (78.0), maa://52227 (100.0)</t>
+          <t>maa://29988 (85.2), maa://23504 (93.68), *maa://25141 (77.37), *maa://36663 (78.0), maa://52227 (100.0)</t>
         </is>
       </c>
       <c r="Y24" s="11" t="n"/>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="AF24" s="14" t="inlineStr">
         <is>
-          <t>maa://22523 (81.74), *maa://36672 (75.38), maa://29910 (93.75), maa://45831 (85.71)</t>
+          <t>maa://22523 (81.74), *maa://36672 (75.38), maa://29910 (93.75), maa://45831 (86.67)</t>
         </is>
       </c>
       <c r="AG24" s="27" t="n"/>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="H25" s="14" t="inlineStr">
         <is>
-          <t>*maa://29063 (72.82), *maa://25311 (74.11), ***maa://22725 (4.76), *maa://45047 (73.33)</t>
+          <t>*maa://29063 (72.96), *maa://25311 (74.11), ***maa://22725 (4.76), *maa://45047 (73.33)</t>
         </is>
       </c>
       <c r="I25" s="11" t="n"/>
@@ -3799,7 +3799,7 @@
       </c>
       <c r="AB25" s="14" t="inlineStr">
         <is>
-          <t>maa://31215 (89.44), *maa://24516 (79.57), maa://26001 (84.75)</t>
+          <t>maa://31215 (89.51), *maa://24516 (79.57), maa://26001 (84.75)</t>
         </is>
       </c>
       <c r="AC25" s="11" t="n"/>
@@ -3815,7 +3815,7 @@
       </c>
       <c r="AF25" s="14" t="inlineStr">
         <is>
-          <t>maa://20108 (95.89), maa://24621 (97.16), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (80.0)</t>
+          <t>maa://20108 (95.89), maa://24621 (97.18), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (80.0)</t>
         </is>
       </c>
       <c r="AG25" s="27" t="n"/>
@@ -3929,7 +3929,7 @@
       </c>
       <c r="AB26" s="14" t="inlineStr">
         <is>
-          <t>maa://42235 (96.03)</t>
+          <t>maa://42235 (96.05)</t>
         </is>
       </c>
       <c r="AC26" s="11" t="n"/>
@@ -4335,7 +4335,7 @@
       </c>
       <c r="AF29" s="14" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.17), maa://42865 (80.18), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (69.17), maa://42865 (80.36), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="27" t="n"/>
@@ -4937,7 +4937,7 @@
       </c>
       <c r="T34" s="14" t="inlineStr">
         <is>
-          <t>maa://24526 (92.36)</t>
+          <t>maa://24526 (92.39)</t>
         </is>
       </c>
       <c r="U34" s="11" t="n"/>
@@ -5035,7 +5035,7 @@
       </c>
       <c r="L35" s="14" t="inlineStr">
         <is>
-          <t>maa://41296 (97.36)</t>
+          <t>maa://41296 (97.37)</t>
         </is>
       </c>
       <c r="M35" s="11" t="n"/>
@@ -5497,7 +5497,7 @@
       </c>
       <c r="P39" s="14" t="inlineStr">
         <is>
-          <t>maa://24709 (91.95), maa://47093 (100.0)</t>
+          <t>maa://24709 (92.0), maa://47093 (100.0)</t>
         </is>
       </c>
       <c r="Q39" s="11" t="n"/>
@@ -5513,7 +5513,7 @@
       </c>
       <c r="T39" s="14" t="inlineStr">
         <is>
-          <t>maa://47079 (95.96), *maa://45788 (73.11), maa://45790 (82.76)</t>
+          <t>maa://47079 (96.0), *maa://45788 (72.5), maa://45790 (82.76)</t>
         </is>
       </c>
       <c r="U39" s="11" t="n"/>
@@ -5922,7 +5922,7 @@
       </c>
       <c r="H44" s="14" t="inlineStr">
         <is>
-          <t>maa://29768 (97.95), maa://27728 (96.19)</t>
+          <t>maa://29768 (97.97), maa://27728 (96.19)</t>
         </is>
       </c>
       <c r="I44" s="11" t="n"/>
@@ -6023,7 +6023,7 @@
       </c>
       <c r="T45" s="14" t="inlineStr">
         <is>
-          <t>**maa://39364 (44.07)</t>
+          <t>**maa://39364 (45.0)</t>
         </is>
       </c>
       <c r="U45" s="11" t="n"/>
@@ -6060,7 +6060,7 @@
       </c>
       <c r="H46" s="14" t="inlineStr">
         <is>
-          <t>maa://35931 (92.65), maa://43901 (94.74)</t>
+          <t>maa://35931 (92.67), maa://43901 (94.74)</t>
         </is>
       </c>
       <c r="I46" s="11" t="n"/>
@@ -6404,7 +6404,7 @@
       </c>
       <c r="P52" s="14" t="inlineStr">
         <is>
-          <t>maa://59378 (100.0), maa://59394 (100.0)</t>
+          <t>maa://59378 (96.77), maa://59394 (100.0)</t>
         </is>
       </c>
       <c r="Q52" s="11" t="n"/>
@@ -6594,7 +6594,7 @@
       </c>
       <c r="H59" s="14" t="inlineStr">
         <is>
-          <t>maa://31270 (94.67), maa://27746 (82.91)</t>
+          <t>maa://31270 (94.74), maa://27746 (82.91)</t>
         </is>
       </c>
       <c r="I59" s="11" t="n"/>
@@ -6666,7 +6666,7 @@
       </c>
       <c r="H63" s="14" t="inlineStr">
         <is>
-          <t>maa://59534 (97.37), maa://59413 (100.0)</t>
+          <t>maa://59534 (97.44), maa://59413 (100.0)</t>
         </is>
       </c>
       <c r="I63" s="11" t="n"/>
@@ -6968,7 +6968,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A1" s="13" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.12 13:21:11</t>
+          <t>更新日期：2025.06.13 13:21:05</t>
         </is>
       </c>
       <c r="E1" s="16" t="inlineStr">
@@ -8480,7 +8480,7 @@
       </c>
       <c r="D29" s="20" t="inlineStr">
         <is>
-          <t>maa://20863 (89.03), maa://20832 (99.07), maa://20727 (100.0)</t>
+          <t>maa://20863 (89.08), maa://20832 (99.07), maa://20727 (100.0)</t>
         </is>
       </c>
       <c r="E29" s="21" t="inlineStr">
@@ -8642,7 +8642,7 @@
       </c>
       <c r="D32" s="20" t="inlineStr">
         <is>
-          <t>maa://36644 (88.36), maa://36866 (96.15), maa://45572 (91.67), maa://27794 (100.0), maa://20960 (100.0), maa://20843 (100.0), **maa://24483 (50.0), maa://20862 (83.33), *maa://20893 (77.78)</t>
+          <t>maa://36644 (88.42), maa://36866 (96.15), maa://45572 (91.67), maa://27794 (100.0), maa://20960 (100.0), maa://20843 (100.0), **maa://24483 (50.0), maa://20862 (83.33), *maa://20893 (77.78)</t>
         </is>
       </c>
       <c r="E32" s="21" t="inlineStr">
@@ -8750,7 +8750,7 @@
       </c>
       <c r="D34" s="20" t="inlineStr">
         <is>
-          <t>maa://20916 (82.35), maa://52658 (83.33)</t>
+          <t>maa://20916 (82.86), maa://52658 (85.71)</t>
         </is>
       </c>
       <c r="E34" s="21" t="inlineStr">
@@ -9938,7 +9938,7 @@
       </c>
       <c r="D56" s="20" t="inlineStr">
         <is>
-          <t>maa://44235 (98.19), maa://45604 (100.0), maa://20961 (100.0), maa://44220 (100.0), maa://20910 (100.0)</t>
+          <t>maa://44235 (98.2), maa://45604 (100.0), maa://20961 (100.0), maa://44220 (100.0), maa://20910 (100.0)</t>
         </is>
       </c>
       <c r="E56" s="21" t="inlineStr">
@@ -10748,7 +10748,7 @@
       </c>
       <c r="D71" s="20" t="inlineStr">
         <is>
-          <t>maa://20943 (99.37), maa://30673 (100.0), maa://30672 (100.0), maa://20856 (100.0)</t>
+          <t>maa://20943 (99.38), maa://30673 (100.0), maa://30672 (100.0), maa://20856 (100.0)</t>
         </is>
       </c>
       <c r="E71" s="21" t="inlineStr">
@@ -13448,7 +13448,7 @@
       </c>
       <c r="D121" s="20" t="inlineStr">
         <is>
-          <t>maa://20869 (100.0), maa://44690 (94.12)</t>
+          <t>maa://20869 (100.0), maa://44690 (94.44)</t>
         </is>
       </c>
       <c r="E121" s="21" t="inlineStr">
@@ -14960,7 +14960,7 @@
       </c>
       <c r="D149" s="20" t="inlineStr">
         <is>
-          <t>maa://36641 (98.44), maa://40957 (93.32), maa://36865 (96.3), maa://44635 (87.74), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
+          <t>maa://36641 (98.44), maa://40957 (93.36), maa://36865 (96.32), maa://44635 (87.74), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
         </is>
       </c>
       <c r="E149" s="21" t="inlineStr">
@@ -17552,7 +17552,7 @@
       </c>
       <c r="D197" s="20" t="inlineStr">
         <is>
-          <t>maa://44224 (90.19), maa://35854 (85.06), maa://50388 (97.83), maa://25760 (86.84), ***maa://43911 (14.29), *maa://20872 (52.0), maa://51066 (100.0)</t>
+          <t>maa://44224 (90.19), maa://35854 (85.06), maa://50388 (97.84), maa://25760 (86.84), ***maa://43911 (13.64), *maa://20872 (52.0), maa://51066 (100.0)</t>
         </is>
       </c>
       <c r="E197" s="21" t="inlineStr">
@@ -19874,7 +19874,7 @@
       </c>
       <c r="D240" s="20" t="inlineStr">
         <is>
-          <t>*maa://30667 (78.63), maa://30666 (83.41), **maa://30739 (43.24), *maa://30723 (56.45), maa://39588 (88.46)</t>
+          <t>*maa://30667 (78.63), maa://30666 (83.41), **maa://30739 (43.24), *maa://30723 (56.45), maa://39588 (88.68)</t>
         </is>
       </c>
       <c r="E240" s="21" t="inlineStr">
@@ -25868,7 +25868,7 @@
       </c>
       <c r="D351" s="17" t="inlineStr">
         <is>
-          <t>maa://36868 (100.0), maa://35996 (97.56), **maa://39217 (41.18), maa://47349 (93.75)</t>
+          <t>maa://36868 (100.0), maa://35996 (97.59), **maa://39217 (41.18), maa://47349 (93.75)</t>
         </is>
       </c>
       <c r="E351" s="17" t="inlineStr">
@@ -26408,7 +26408,7 @@
       </c>
       <c r="D361" s="17" t="inlineStr">
         <is>
-          <t>maa://40957 (93.32), maa://44635 (87.74), maa://48026 (96.39), maa://41035 (92.42), maa://44660 (92.31), maa://41128 (83.78)</t>
+          <t>maa://40957 (93.36), maa://44635 (87.74), maa://48026 (96.39), maa://41035 (92.42), maa://44660 (92.31), maa://41128 (83.78)</t>
         </is>
       </c>
       <c r="E361" s="17" t="inlineStr">
@@ -26840,7 +26840,7 @@
       </c>
       <c r="D369" s="17" t="inlineStr">
         <is>
-          <t>maa://41110 (98.29), maa://45605 (100.0)</t>
+          <t>maa://41110 (98.31), maa://45605 (100.0)</t>
         </is>
       </c>
       <c r="E369" s="17" t="inlineStr">
@@ -27272,7 +27272,7 @@
       </c>
       <c r="D377" s="17" t="inlineStr">
         <is>
-          <t>maa://42970 (83.86), maa://44745 (98.15), **maa://49516 (42.11), *maa://45952 (80.0), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
+          <t>maa://42970 (83.86), maa://44745 (98.17), **maa://49516 (42.11), *maa://45952 (80.0), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E377" s="17" t="inlineStr">
@@ -28028,7 +28028,7 @@
       </c>
       <c r="D391" s="17" t="inlineStr">
         <is>
-          <t>maa://51872 (96.62), maa://51876 (98.75), maa://51873 (100.0)</t>
+          <t>maa://51872 (96.63), maa://51876 (98.75), maa://51873 (100.0)</t>
         </is>
       </c>
       <c r="E391" s="17" t="inlineStr">
@@ -28082,7 +28082,7 @@
       </c>
       <c r="D392" s="17" t="inlineStr">
         <is>
-          <t>maa://59493 (95.59), maa://59603 (100.0)</t>
+          <t>maa://59493 (95.83), maa://59603 (100.0)</t>
         </is>
       </c>
       <c r="E392" s="17" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#196)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -767,7 +767,7 @@
       </c>
       <c r="T2" s="14" t="inlineStr">
         <is>
-          <t>maa://22742 (91.47)</t>
+          <t>maa://22742 (91.51)</t>
         </is>
       </c>
       <c r="U2" s="11" t="n"/>
@@ -897,7 +897,7 @@
       </c>
       <c r="T3" s="14" t="inlineStr">
         <is>
-          <t>maa://24617 (90.91), maa://45854 (85.11)</t>
+          <t>maa://24617 (90.98), maa://45854 (84.21)</t>
         </is>
       </c>
       <c r="U3" s="11" t="n"/>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="AF7" s="14" t="inlineStr">
         <is>
-          <t>maa://45272 (97.06)</t>
+          <t>maa://45272 (97.14)</t>
         </is>
       </c>
       <c r="AG7" s="27" t="n"/>
@@ -1478,7 +1478,7 @@
     <row r="8">
       <c r="A8" s="10" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.12 13:21:11</t>
+          <t>更新日期：2025.06.13 13:21:05</t>
         </is>
       </c>
       <c r="B8" s="11" t="inlineStr">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="AB11" s="14" t="inlineStr">
         <is>
-          <t>maa://29912 (97.8), maa://22516 (87.36)</t>
+          <t>maa://29912 (97.85), maa://22516 (87.36)</t>
         </is>
       </c>
       <c r="AC11" s="11" t="n"/>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="AF12" s="14" t="inlineStr">
         <is>
-          <t>*maa://28932 (79.1), *maa://20106 (64.29), *maa://22769 (64.29)</t>
+          <t>*maa://28932 (79.21), *maa://20106 (64.29), *maa://22769 (64.29)</t>
         </is>
       </c>
       <c r="AG12" s="27" t="n"/>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>maa://24999 (92.71), maa://36673 (91.95), maa://25001 (86.49)</t>
+          <t>maa://24999 (92.74), maa://36673 (91.95), maa://25001 (86.49)</t>
         </is>
       </c>
       <c r="E13" s="11" t="n"/>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="H13" s="14" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.84), **maa://22728 (46.94)</t>
+          <t>*maa://21248 (73.93), **maa://22728 (46.94)</t>
         </is>
       </c>
       <c r="I13" s="11" t="n"/>
@@ -2305,7 +2305,7 @@
       </c>
       <c r="L14" s="14" t="inlineStr">
         <is>
-          <t>maa://39841 (94.34), maa://26245 (96.7), maa://21288 (96.3), maa://36682 (95.92)</t>
+          <t>maa://39841 (94.38), maa://26245 (96.7), maa://21288 (96.3), maa://36682 (95.92)</t>
         </is>
       </c>
       <c r="M14" s="11" t="n"/>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="D15" s="14" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.93), maa://22734 (84.55), *maa://30808 (64.79), *maa://36048 (69.64), maa://45058 (84.21)</t>
+          <t>*maa://22743 (78.93), maa://22734 (84.55), *maa://30808 (65.28), *maa://36048 (69.64), maa://45058 (85.0)</t>
         </is>
       </c>
       <c r="E15" s="11" t="n"/>
@@ -2515,7 +2515,7 @@
       </c>
       <c r="AF15" s="14" t="inlineStr">
         <is>
-          <t>maa://21364 (81.3), maa://36666 (81.99), *maa://22766 (68.55)</t>
+          <t>maa://21364 (81.3), maa://36666 (82.1), *maa://22766 (68.55)</t>
         </is>
       </c>
       <c r="AG15" s="27" t="n"/>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="H17" s="14" t="inlineStr">
         <is>
-          <t>maa://22430 (89.67), maa://39599 (86.59)</t>
+          <t>maa://22430 (89.67), maa://39599 (86.75)</t>
         </is>
       </c>
       <c r="I17" s="11" t="n"/>
@@ -2873,7 +2873,7 @@
       </c>
       <c r="X18" s="14" t="inlineStr">
         <is>
-          <t>maa://21917 (97.12), maa://22741 (87.5)</t>
+          <t>maa://21917 (97.14), maa://22741 (87.5)</t>
         </is>
       </c>
       <c r="Y18" s="11" t="n"/>
@@ -3019,7 +3019,7 @@
       </c>
       <c r="AB19" s="14" t="inlineStr">
         <is>
-          <t>*maa://30709 (68.6), *maa://36668 (57.32)</t>
+          <t>*maa://30709 (68.66), *maa://36668 (57.32)</t>
         </is>
       </c>
       <c r="AC19" s="11" t="n"/>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="H20" s="14" t="inlineStr">
         <is>
-          <t>maa://22864 (90.81)</t>
+          <t>maa://22864 (90.86)</t>
         </is>
       </c>
       <c r="I20" s="11" t="n"/>
@@ -3085,7 +3085,7 @@
       </c>
       <c r="L20" s="14" t="inlineStr">
         <is>
-          <t>maa://41331 (86.4)</t>
+          <t>maa://41331 (86.11)</t>
         </is>
       </c>
       <c r="M20" s="11" t="n"/>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="X20" s="14" t="inlineStr">
         <is>
-          <t>maa://50085 (87.77), maa://49976 (86.59), maa://56241 (88.89)</t>
+          <t>maa://50085 (87.94), maa://49976 (86.59), maa://56241 (88.89)</t>
         </is>
       </c>
       <c r="Y20" s="11" t="n"/>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="AB21" s="14" t="inlineStr">
         <is>
-          <t>maa://21443 (82.77), ***maa://23820 (30.0), **maa://52223 (40.62)</t>
+          <t>maa://21443 (82.81), ***maa://23820 (30.0), **maa://52223 (40.62)</t>
         </is>
       </c>
       <c r="AC21" s="11" t="n"/>
@@ -3425,7 +3425,7 @@
       </c>
       <c r="AF22" s="14" t="inlineStr">
         <is>
-          <t>maa://29658 (94.44)</t>
+          <t>maa://29658 (94.55)</t>
         </is>
       </c>
       <c r="AG22" s="27" t="n"/>
@@ -3475,7 +3475,7 @@
       </c>
       <c r="L23" s="14" t="inlineStr">
         <is>
-          <t>maa://39756 (95.77), maa://39875 (94.81)</t>
+          <t>maa://39756 (95.77), maa://39875 (94.87)</t>
         </is>
       </c>
       <c r="M23" s="11" t="n"/>
@@ -3573,7 +3573,7 @@
       </c>
       <c r="D24" s="14" t="inlineStr">
         <is>
-          <t>*maa://24368 (79.18), *maa://46650 (61.29)</t>
+          <t>*maa://24368 (79.23), *maa://46650 (61.29)</t>
         </is>
       </c>
       <c r="E24" s="11" t="n"/>
@@ -3653,7 +3653,7 @@
       </c>
       <c r="X24" s="14" t="inlineStr">
         <is>
-          <t>maa://29988 (85.15), maa://23504 (93.68), *maa://25141 (77.37), *maa://36663 (78.0), maa://52227 (100.0)</t>
+          <t>maa://29988 (85.2), maa://23504 (93.68), *maa://25141 (77.37), *maa://36663 (78.0), maa://52227 (100.0)</t>
         </is>
       </c>
       <c r="Y24" s="11" t="n"/>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="AF24" s="14" t="inlineStr">
         <is>
-          <t>maa://22523 (81.74), *maa://36672 (75.38), maa://29910 (93.75), maa://45831 (85.71)</t>
+          <t>maa://22523 (81.74), *maa://36672 (75.38), maa://29910 (93.75), maa://45831 (86.67)</t>
         </is>
       </c>
       <c r="AG24" s="27" t="n"/>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="H25" s="14" t="inlineStr">
         <is>
-          <t>*maa://29063 (72.82), *maa://25311 (74.11), ***maa://22725 (4.76), *maa://45047 (73.33)</t>
+          <t>*maa://29063 (72.96), *maa://25311 (74.11), ***maa://22725 (4.76), *maa://45047 (73.33)</t>
         </is>
       </c>
       <c r="I25" s="11" t="n"/>
@@ -3799,7 +3799,7 @@
       </c>
       <c r="AB25" s="14" t="inlineStr">
         <is>
-          <t>maa://31215 (89.44), *maa://24516 (79.57), maa://26001 (84.75)</t>
+          <t>maa://31215 (89.51), *maa://24516 (79.57), maa://26001 (84.75)</t>
         </is>
       </c>
       <c r="AC25" s="11" t="n"/>
@@ -3815,7 +3815,7 @@
       </c>
       <c r="AF25" s="14" t="inlineStr">
         <is>
-          <t>maa://20108 (95.89), maa://24621 (97.16), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (80.0)</t>
+          <t>maa://20108 (95.89), maa://24621 (97.18), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (80.0)</t>
         </is>
       </c>
       <c r="AG25" s="27" t="n"/>
@@ -3929,7 +3929,7 @@
       </c>
       <c r="AB26" s="14" t="inlineStr">
         <is>
-          <t>maa://42235 (96.03)</t>
+          <t>maa://42235 (96.05)</t>
         </is>
       </c>
       <c r="AC26" s="11" t="n"/>
@@ -4335,7 +4335,7 @@
       </c>
       <c r="AF29" s="14" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.17), maa://42865 (80.18), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (69.17), maa://42865 (80.36), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="27" t="n"/>
@@ -4937,7 +4937,7 @@
       </c>
       <c r="T34" s="14" t="inlineStr">
         <is>
-          <t>maa://24526 (92.36)</t>
+          <t>maa://24526 (92.39)</t>
         </is>
       </c>
       <c r="U34" s="11" t="n"/>
@@ -5035,7 +5035,7 @@
       </c>
       <c r="L35" s="14" t="inlineStr">
         <is>
-          <t>maa://41296 (97.36)</t>
+          <t>maa://41296 (97.37)</t>
         </is>
       </c>
       <c r="M35" s="11" t="n"/>
@@ -5497,7 +5497,7 @@
       </c>
       <c r="P39" s="14" t="inlineStr">
         <is>
-          <t>maa://24709 (91.95), maa://47093 (100.0)</t>
+          <t>maa://24709 (92.0), maa://47093 (100.0)</t>
         </is>
       </c>
       <c r="Q39" s="11" t="n"/>
@@ -5513,7 +5513,7 @@
       </c>
       <c r="T39" s="14" t="inlineStr">
         <is>
-          <t>maa://47079 (95.96), *maa://45788 (73.11), maa://45790 (82.76)</t>
+          <t>maa://47079 (96.0), *maa://45788 (72.5), maa://45790 (82.76)</t>
         </is>
       </c>
       <c r="U39" s="11" t="n"/>
@@ -5922,7 +5922,7 @@
       </c>
       <c r="H44" s="14" t="inlineStr">
         <is>
-          <t>maa://29768 (97.95), maa://27728 (96.19)</t>
+          <t>maa://29768 (97.97), maa://27728 (96.19)</t>
         </is>
       </c>
       <c r="I44" s="11" t="n"/>
@@ -6023,7 +6023,7 @@
       </c>
       <c r="T45" s="14" t="inlineStr">
         <is>
-          <t>**maa://39364 (44.07)</t>
+          <t>**maa://39364 (45.0)</t>
         </is>
       </c>
       <c r="U45" s="11" t="n"/>
@@ -6060,7 +6060,7 @@
       </c>
       <c r="H46" s="14" t="inlineStr">
         <is>
-          <t>maa://35931 (92.65), maa://43901 (94.74)</t>
+          <t>maa://35931 (92.67), maa://43901 (94.74)</t>
         </is>
       </c>
       <c r="I46" s="11" t="n"/>
@@ -6404,7 +6404,7 @@
       </c>
       <c r="P52" s="14" t="inlineStr">
         <is>
-          <t>maa://59378 (100.0), maa://59394 (100.0)</t>
+          <t>maa://59378 (96.77), maa://59394 (100.0)</t>
         </is>
       </c>
       <c r="Q52" s="11" t="n"/>
@@ -6594,7 +6594,7 @@
       </c>
       <c r="H59" s="14" t="inlineStr">
         <is>
-          <t>maa://31270 (94.67), maa://27746 (82.91)</t>
+          <t>maa://31270 (94.74), maa://27746 (82.91)</t>
         </is>
       </c>
       <c r="I59" s="11" t="n"/>
@@ -6666,7 +6666,7 @@
       </c>
       <c r="H63" s="14" t="inlineStr">
         <is>
-          <t>maa://59534 (97.37), maa://59413 (100.0)</t>
+          <t>maa://59534 (97.44), maa://59413 (100.0)</t>
         </is>
       </c>
       <c r="I63" s="11" t="n"/>
@@ -6968,7 +6968,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A1" s="13" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.12 13:21:11</t>
+          <t>更新日期：2025.06.13 13:21:05</t>
         </is>
       </c>
       <c r="E1" s="16" t="inlineStr">
@@ -8480,7 +8480,7 @@
       </c>
       <c r="D29" s="20" t="inlineStr">
         <is>
-          <t>maa://20863 (89.03), maa://20832 (99.07), maa://20727 (100.0)</t>
+          <t>maa://20863 (89.08), maa://20832 (99.07), maa://20727 (100.0)</t>
         </is>
       </c>
       <c r="E29" s="21" t="inlineStr">
@@ -8642,7 +8642,7 @@
       </c>
       <c r="D32" s="20" t="inlineStr">
         <is>
-          <t>maa://36644 (88.36), maa://36866 (96.15), maa://45572 (91.67), maa://27794 (100.0), maa://20960 (100.0), maa://20843 (100.0), **maa://24483 (50.0), maa://20862 (83.33), *maa://20893 (77.78)</t>
+          <t>maa://36644 (88.42), maa://36866 (96.15), maa://45572 (91.67), maa://27794 (100.0), maa://20960 (100.0), maa://20843 (100.0), **maa://24483 (50.0), maa://20862 (83.33), *maa://20893 (77.78)</t>
         </is>
       </c>
       <c r="E32" s="21" t="inlineStr">
@@ -8750,7 +8750,7 @@
       </c>
       <c r="D34" s="20" t="inlineStr">
         <is>
-          <t>maa://20916 (82.35), maa://52658 (83.33)</t>
+          <t>maa://20916 (82.86), maa://52658 (85.71)</t>
         </is>
       </c>
       <c r="E34" s="21" t="inlineStr">
@@ -9938,7 +9938,7 @@
       </c>
       <c r="D56" s="20" t="inlineStr">
         <is>
-          <t>maa://44235 (98.19), maa://45604 (100.0), maa://20961 (100.0), maa://44220 (100.0), maa://20910 (100.0)</t>
+          <t>maa://44235 (98.2), maa://45604 (100.0), maa://20961 (100.0), maa://44220 (100.0), maa://20910 (100.0)</t>
         </is>
       </c>
       <c r="E56" s="21" t="inlineStr">
@@ -10748,7 +10748,7 @@
       </c>
       <c r="D71" s="20" t="inlineStr">
         <is>
-          <t>maa://20943 (99.37), maa://30673 (100.0), maa://30672 (100.0), maa://20856 (100.0)</t>
+          <t>maa://20943 (99.38), maa://30673 (100.0), maa://30672 (100.0), maa://20856 (100.0)</t>
         </is>
       </c>
       <c r="E71" s="21" t="inlineStr">
@@ -13448,7 +13448,7 @@
       </c>
       <c r="D121" s="20" t="inlineStr">
         <is>
-          <t>maa://20869 (100.0), maa://44690 (94.12)</t>
+          <t>maa://20869 (100.0), maa://44690 (94.44)</t>
         </is>
       </c>
       <c r="E121" s="21" t="inlineStr">
@@ -14960,7 +14960,7 @@
       </c>
       <c r="D149" s="20" t="inlineStr">
         <is>
-          <t>maa://36641 (98.44), maa://40957 (93.32), maa://36865 (96.3), maa://44635 (87.74), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
+          <t>maa://36641 (98.44), maa://40957 (93.36), maa://36865 (96.32), maa://44635 (87.74), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
         </is>
       </c>
       <c r="E149" s="21" t="inlineStr">
@@ -17552,7 +17552,7 @@
       </c>
       <c r="D197" s="20" t="inlineStr">
         <is>
-          <t>maa://44224 (90.19), maa://35854 (85.06), maa://50388 (97.83), maa://25760 (86.84), ***maa://43911 (14.29), *maa://20872 (52.0), maa://51066 (100.0)</t>
+          <t>maa://44224 (90.19), maa://35854 (85.06), maa://50388 (97.84), maa://25760 (86.84), ***maa://43911 (13.64), *maa://20872 (52.0), maa://51066 (100.0)</t>
         </is>
       </c>
       <c r="E197" s="21" t="inlineStr">
@@ -19874,7 +19874,7 @@
       </c>
       <c r="D240" s="20" t="inlineStr">
         <is>
-          <t>*maa://30667 (78.63), maa://30666 (83.41), **maa://30739 (43.24), *maa://30723 (56.45), maa://39588 (88.46)</t>
+          <t>*maa://30667 (78.63), maa://30666 (83.41), **maa://30739 (43.24), *maa://30723 (56.45), maa://39588 (88.68)</t>
         </is>
       </c>
       <c r="E240" s="21" t="inlineStr">
@@ -25868,7 +25868,7 @@
       </c>
       <c r="D351" s="17" t="inlineStr">
         <is>
-          <t>maa://36868 (100.0), maa://35996 (97.56), **maa://39217 (41.18), maa://47349 (93.75)</t>
+          <t>maa://36868 (100.0), maa://35996 (97.59), **maa://39217 (41.18), maa://47349 (93.75)</t>
         </is>
       </c>
       <c r="E351" s="17" t="inlineStr">
@@ -26408,7 +26408,7 @@
       </c>
       <c r="D361" s="17" t="inlineStr">
         <is>
-          <t>maa://40957 (93.32), maa://44635 (87.74), maa://48026 (96.39), maa://41035 (92.42), maa://44660 (92.31), maa://41128 (83.78)</t>
+          <t>maa://40957 (93.36), maa://44635 (87.74), maa://48026 (96.39), maa://41035 (92.42), maa://44660 (92.31), maa://41128 (83.78)</t>
         </is>
       </c>
       <c r="E361" s="17" t="inlineStr">
@@ -26840,7 +26840,7 @@
       </c>
       <c r="D369" s="17" t="inlineStr">
         <is>
-          <t>maa://41110 (98.29), maa://45605 (100.0)</t>
+          <t>maa://41110 (98.31), maa://45605 (100.0)</t>
         </is>
       </c>
       <c r="E369" s="17" t="inlineStr">
@@ -27272,7 +27272,7 @@
       </c>
       <c r="D377" s="17" t="inlineStr">
         <is>
-          <t>maa://42970 (83.86), maa://44745 (98.15), **maa://49516 (42.11), *maa://45952 (80.0), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
+          <t>maa://42970 (83.86), maa://44745 (98.17), **maa://49516 (42.11), *maa://45952 (80.0), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E377" s="17" t="inlineStr">
@@ -28028,7 +28028,7 @@
       </c>
       <c r="D391" s="17" t="inlineStr">
         <is>
-          <t>maa://51872 (96.62), maa://51876 (98.75), maa://51873 (100.0)</t>
+          <t>maa://51872 (96.63), maa://51876 (98.75), maa://51873 (100.0)</t>
         </is>
       </c>
       <c r="E391" s="17" t="inlineStr">
@@ -28082,7 +28082,7 @@
       </c>
       <c r="D392" s="17" t="inlineStr">
         <is>
-          <t>maa://59493 (95.59), maa://59603 (100.0)</t>
+          <t>maa://59493 (95.83), maa://59603 (100.0)</t>
         </is>
       </c>
       <c r="E392" s="17" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#197)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -897,7 +897,7 @@
       </c>
       <c r="T3" s="14" t="inlineStr">
         <is>
-          <t>maa://24617 (90.98), maa://45854 (84.21)</t>
+          <t>maa://24617 (91.04), maa://45854 (84.38)</t>
         </is>
       </c>
       <c r="U3" s="11" t="n"/>
@@ -1478,7 +1478,7 @@
     <row r="8">
       <c r="A8" s="10" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.13 13:21:05</t>
+          <t>更新日期：2025.06.14 13:21:08</t>
         </is>
       </c>
       <c r="B8" s="11" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="X8" s="14" t="inlineStr">
         <is>
-          <t>maa://21411 (96.07)</t>
+          <t>maa://21411 (96.09)</t>
         </is>
       </c>
       <c r="Y8" s="11" t="n"/>
@@ -1735,7 +1735,7 @@
       </c>
       <c r="AF9" s="14" t="inlineStr">
         <is>
-          <t>maa://26206 (89.2), *maa://22865 (53.57)</t>
+          <t>maa://26206 (89.27), *maa://22865 (53.57)</t>
         </is>
       </c>
       <c r="AG9" s="27" t="n"/>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="D10" s="14" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.72), ***maa://39951 (11.84), ***maa://34206 (22.22), *maa://45271 (60.26), ***maa://39243 (25.0), **maa://54000 (33.33)</t>
+          <t>***maa://25695 (18.72), ***maa://39951 (11.84), ***maa://34206 (22.22), *maa://45271 (60.76), ***maa://39243 (25.0), **maa://54000 (33.33)</t>
         </is>
       </c>
       <c r="E10" s="11" t="n"/>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="X10" s="14" t="inlineStr">
         <is>
-          <t>maa://22301 (97.9), maa://45828 (93.48), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.91), maa://45828 (93.48), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="11" t="n"/>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="T11" s="14" t="inlineStr">
         <is>
-          <t>maa://22747 (90.96), maa://22501 (98.23), maa://45521 (91.67)</t>
+          <t>maa://22747 (90.45), maa://22501 (98.25), maa://45521 (91.67)</t>
         </is>
       </c>
       <c r="U11" s="11" t="n"/>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="H13" s="14" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.93), **maa://22728 (46.94)</t>
+          <t>*maa://21248 (74.02), **maa://22728 (46.94)</t>
         </is>
       </c>
       <c r="I13" s="11" t="n"/>
@@ -2305,7 +2305,7 @@
       </c>
       <c r="L14" s="14" t="inlineStr">
         <is>
-          <t>maa://39841 (94.38), maa://26245 (96.7), maa://21288 (96.3), maa://36682 (95.92)</t>
+          <t>maa://39841 (94.41), maa://26245 (96.72), maa://21288 (96.3), maa://36682 (95.92)</t>
         </is>
       </c>
       <c r="M14" s="11" t="n"/>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="D15" s="14" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.93), maa://22734 (84.55), *maa://30808 (65.28), *maa://36048 (69.64), maa://45058 (85.0)</t>
+          <t>*maa://22743 (79.01), maa://22734 (84.55), *maa://30808 (65.28), *maa://36048 (69.64), maa://45058 (85.0)</t>
         </is>
       </c>
       <c r="E15" s="11" t="n"/>
@@ -2809,7 +2809,7 @@
       </c>
       <c r="H18" s="14" t="inlineStr">
         <is>
-          <t>maa://24421 (87.19)</t>
+          <t>maa://24421 (86.88)</t>
         </is>
       </c>
       <c r="I18" s="11" t="n"/>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="T19" s="14" t="inlineStr">
         <is>
-          <t>maa://24386 (98.66)</t>
+          <t>maa://24386 (98.67)</t>
         </is>
       </c>
       <c r="U19" s="11" t="n"/>
@@ -3085,7 +3085,7 @@
       </c>
       <c r="L20" s="14" t="inlineStr">
         <is>
-          <t>maa://41331 (86.11)</t>
+          <t>maa://41331 (86.17)</t>
         </is>
       </c>
       <c r="M20" s="11" t="n"/>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="X20" s="14" t="inlineStr">
         <is>
-          <t>maa://50085 (87.94), maa://49976 (86.59), maa://56241 (88.89)</t>
+          <t>maa://50085 (88.03), maa://49976 (86.59), maa://56241 (88.89)</t>
         </is>
       </c>
       <c r="Y20" s="11" t="n"/>
@@ -3295,7 +3295,7 @@
       </c>
       <c r="AF21" s="14" t="inlineStr">
         <is>
-          <t>maa://22524 (88.76), maa://22432 (83.21)</t>
+          <t>maa://22524 (88.8), maa://22432 (83.21)</t>
         </is>
       </c>
       <c r="AG21" s="27" t="n"/>
@@ -3393,7 +3393,7 @@
       </c>
       <c r="X22" s="14" t="inlineStr">
         <is>
-          <t>maa://21282 (98.72), *maa://37649 (73.17)</t>
+          <t>maa://21282 (98.72), *maa://37649 (73.81)</t>
         </is>
       </c>
       <c r="Y22" s="11" t="n"/>
@@ -3523,7 +3523,7 @@
       </c>
       <c r="X23" s="14" t="inlineStr">
         <is>
-          <t>*maa://28503 (65.26)</t>
+          <t>*maa://28503 (64.58)</t>
         </is>
       </c>
       <c r="Y23" s="11" t="n"/>
@@ -3573,7 +3573,7 @@
       </c>
       <c r="D24" s="14" t="inlineStr">
         <is>
-          <t>*maa://24368 (79.23), *maa://46650 (61.29)</t>
+          <t>*maa://24368 (79.23), *maa://46650 (59.38)</t>
         </is>
       </c>
       <c r="E24" s="11" t="n"/>
@@ -3653,7 +3653,7 @@
       </c>
       <c r="X24" s="14" t="inlineStr">
         <is>
-          <t>maa://29988 (85.2), maa://23504 (93.68), *maa://25141 (77.37), *maa://36663 (78.0), maa://52227 (100.0)</t>
+          <t>maa://29988 (84.92), maa://23504 (93.7), *maa://25141 (77.37), *maa://36663 (78.0), maa://52227 (100.0)</t>
         </is>
       </c>
       <c r="Y24" s="11" t="n"/>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="AF24" s="14" t="inlineStr">
         <is>
-          <t>maa://22523 (81.74), *maa://36672 (75.38), maa://29910 (93.75), maa://45831 (86.67)</t>
+          <t>maa://22523 (81.74), *maa://36672 (75.76), maa://29910 (93.75), maa://45831 (86.67)</t>
         </is>
       </c>
       <c r="AG24" s="27" t="n"/>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="D28" s="14" t="inlineStr">
         <is>
-          <t>maa://24465 (90.66), maa://25725 (82.83)</t>
+          <t>maa://24465 (90.67), maa://25725 (82.83)</t>
         </is>
       </c>
       <c r="E28" s="11" t="n"/>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="H32" s="14" t="inlineStr">
         <is>
-          <t>maa://21895 (97.62), maa://36667 (97.32), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.63), maa://36667 (97.32), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="11" t="n"/>
@@ -4791,7 +4791,7 @@
       </c>
       <c r="P33" s="14" t="inlineStr">
         <is>
-          <t>maa://21956 (81.48), *maa://22730 (71.88)</t>
+          <t>maa://21956 (81.6), *maa://22730 (71.88)</t>
         </is>
       </c>
       <c r="Q33" s="11" t="n"/>
@@ -5279,7 +5279,7 @@
       </c>
       <c r="L37" s="14" t="inlineStr">
         <is>
-          <t>maa://45718 (98.45), maa://47069 (81.82), maa://56336 (87.5), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.46), maa://47069 (81.82), maa://56336 (87.5), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="11" t="n"/>
@@ -5444,7 +5444,7 @@
       </c>
       <c r="AF38" s="14" t="inlineStr">
         <is>
-          <t>maa://36697 (89.27)</t>
+          <t>maa://36697 (89.31)</t>
         </is>
       </c>
       <c r="AG38" s="27" t="n"/>
@@ -5917,12 +5917,12 @@
       </c>
       <c r="G44" s="11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H44" s="14" t="inlineStr">
         <is>
-          <t>maa://29768 (97.97), maa://27728 (96.19)</t>
+          <t>maa://29768 (97.97), maa://27728 (96.19), maa://56386 (100.0)</t>
         </is>
       </c>
       <c r="I44" s="11" t="n"/>
@@ -6404,7 +6404,7 @@
       </c>
       <c r="P52" s="14" t="inlineStr">
         <is>
-          <t>maa://59378 (96.77), maa://59394 (100.0)</t>
+          <t>maa://59378 (96.88), maa://59394 (91.67)</t>
         </is>
       </c>
       <c r="Q52" s="11" t="n"/>
@@ -6666,7 +6666,7 @@
       </c>
       <c r="H63" s="14" t="inlineStr">
         <is>
-          <t>maa://59534 (97.44), maa://59413 (100.0)</t>
+          <t>maa://59534 (97.5), maa://59413 (100.0)</t>
         </is>
       </c>
       <c r="I63" s="11" t="n"/>
@@ -6968,7 +6968,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A1" s="13" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.13 13:21:05</t>
+          <t>更新日期：2025.06.14 13:21:08</t>
         </is>
       </c>
       <c r="E1" s="16" t="inlineStr">
@@ -8480,7 +8480,7 @@
       </c>
       <c r="D29" s="20" t="inlineStr">
         <is>
-          <t>maa://20863 (89.08), maa://20832 (99.07), maa://20727 (100.0)</t>
+          <t>maa://20863 (89.12), maa://20832 (99.07), maa://20727 (100.0)</t>
         </is>
       </c>
       <c r="E29" s="21" t="inlineStr">
@@ -8750,7 +8750,7 @@
       </c>
       <c r="D34" s="20" t="inlineStr">
         <is>
-          <t>maa://20916 (82.86), maa://52658 (85.71)</t>
+          <t>maa://20916 (82.86), maa://52658 (87.5)</t>
         </is>
       </c>
       <c r="E34" s="21" t="inlineStr">
@@ -9938,7 +9938,7 @@
       </c>
       <c r="D56" s="20" t="inlineStr">
         <is>
-          <t>maa://44235 (98.2), maa://45604 (100.0), maa://20961 (100.0), maa://44220 (100.0), maa://20910 (100.0)</t>
+          <t>maa://44235 (98.21), maa://45604 (100.0), maa://20961 (100.0), maa://44220 (100.0), maa://20910 (100.0)</t>
         </is>
       </c>
       <c r="E56" s="21" t="inlineStr">
@@ -12152,7 +12152,7 @@
       </c>
       <c r="D97" s="20" t="inlineStr">
         <is>
-          <t>maa://20991 (100.0), maa://51015 (83.33)</t>
+          <t>maa://20991 (100.0), maa://51015 (85.71)</t>
         </is>
       </c>
       <c r="E97" s="21" t="inlineStr">
@@ -12746,7 +12746,7 @@
       </c>
       <c r="D108" s="20" t="inlineStr">
         <is>
-          <t>maa://25018 (96.61), maa://51881 (99.16), maa://25776 (92.11), maa://28361 (97.37), maa://25772 (94.12), maa://56588 (93.75), maa://32653 (85.71), maa://45194 (87.5), maa://25161 (81.25)</t>
+          <t>maa://25018 (96.63), maa://51881 (99.16), maa://25776 (92.11), maa://28361 (97.37), maa://25772 (94.12), maa://56588 (94.12), maa://45194 (87.5), maa://32653 (85.71), maa://25161 (81.25)</t>
         </is>
       </c>
       <c r="E108" s="21" t="inlineStr">
@@ -13448,7 +13448,7 @@
       </c>
       <c r="D121" s="20" t="inlineStr">
         <is>
-          <t>maa://20869 (100.0), maa://44690 (94.44)</t>
+          <t>maa://20869 (100.0), maa://44690 (94.74)</t>
         </is>
       </c>
       <c r="E121" s="21" t="inlineStr">
@@ -15014,7 +15014,7 @@
       </c>
       <c r="D150" s="20" t="inlineStr">
         <is>
-          <t>maa://51549 (97.44), maa://51923 (95.45)</t>
+          <t>maa://51549 (95.12), maa://51923 (95.65)</t>
         </is>
       </c>
       <c r="E150" s="21" t="inlineStr">
@@ -15500,7 +15500,7 @@
       </c>
       <c r="D159" s="20" t="inlineStr">
         <is>
-          <t>maa://44232 (98.55), maa://45603 (90.32), maa://44305 (100.0)</t>
+          <t>maa://44232 (98.56), maa://45603 (90.62), maa://44305 (100.0)</t>
         </is>
       </c>
       <c r="E159" s="21" t="inlineStr">
@@ -17552,7 +17552,7 @@
       </c>
       <c r="D197" s="20" t="inlineStr">
         <is>
-          <t>maa://44224 (90.19), maa://35854 (85.06), maa://50388 (97.84), maa://25760 (86.84), ***maa://43911 (13.64), *maa://20872 (52.0), maa://51066 (100.0)</t>
+          <t>maa://44224 (90.25), maa://35854 (85.23), maa://50388 (97.84), maa://25760 (86.84), ***maa://43911 (13.64), *maa://20872 (52.0), maa://51066 (100.0)</t>
         </is>
       </c>
       <c r="E197" s="21" t="inlineStr">
@@ -18308,7 +18308,7 @@
       </c>
       <c r="D211" s="20" t="inlineStr">
         <is>
-          <t>maa://20956 (95.77), *maa://20830 (80.0), maa://44703 (90.91)</t>
+          <t>maa://20956 (95.81), *maa://20830 (80.0), maa://44703 (91.67)</t>
         </is>
       </c>
       <c r="E211" s="21" t="inlineStr">
@@ -20360,7 +20360,7 @@
       </c>
       <c r="D249" s="20" t="inlineStr">
         <is>
-          <t>maa://42287 (90.24), maa://45570 (97.87), maa://42225 (100.0)</t>
+          <t>maa://42287 (90.48), maa://45570 (97.87), maa://42225 (100.0)</t>
         </is>
       </c>
       <c r="E249" s="21" t="inlineStr">
@@ -21602,7 +21602,7 @@
       </c>
       <c r="D272" s="20" t="inlineStr">
         <is>
-          <t>maa://51881 (99.16), maa://51630 (96.59), maa://56588 (93.75), *maa://55171 (55.0), maa://51893 (88.89)</t>
+          <t>maa://51881 (99.16), maa://51630 (96.59), maa://56588 (94.12), *maa://55171 (57.14), maa://51893 (88.89)</t>
         </is>
       </c>
       <c r="E272" s="21" t="inlineStr">
@@ -23276,7 +23276,7 @@
       </c>
       <c r="D303" s="20" t="inlineStr">
         <is>
-          <t>maa://50280 (97.46), maa://49642 (96.88), maa://49660 (92.86), *maa://50517 (80.0)</t>
+          <t>maa://50280 (97.52), maa://49642 (96.88), maa://49660 (92.86), *maa://50517 (80.0)</t>
         </is>
       </c>
       <c r="E303" s="21" t="inlineStr">
@@ -25058,7 +25058,7 @@
       </c>
       <c r="D336" s="22" t="inlineStr">
         <is>
-          <t>maa://30671 (81.58), maa://30669 (99.21), maa://37275 (82.93), *maa://32410 (66.67), maa://41605 (100.0)</t>
+          <t>maa://30671 (81.58), maa://30669 (99.22), maa://37275 (82.93), *maa://32410 (66.67), maa://41605 (100.0)</t>
         </is>
       </c>
       <c r="E336" s="22" t="inlineStr">
@@ -25868,7 +25868,7 @@
       </c>
       <c r="D351" s="17" t="inlineStr">
         <is>
-          <t>maa://36868 (100.0), maa://35996 (97.59), **maa://39217 (41.18), maa://47349 (93.75)</t>
+          <t>maa://36868 (100.0), maa://35996 (97.62), **maa://39217 (41.18), maa://47349 (93.94)</t>
         </is>
       </c>
       <c r="E351" s="17" t="inlineStr">
@@ -26084,7 +26084,7 @@
       </c>
       <c r="D355" s="17" t="inlineStr">
         <is>
-          <t>maa://49648 (95.45), *maa://49662 (71.43)</t>
+          <t>maa://49648 (95.56), *maa://49662 (71.43)</t>
         </is>
       </c>
       <c r="E355" s="17" t="inlineStr">
@@ -26840,7 +26840,7 @@
       </c>
       <c r="D369" s="17" t="inlineStr">
         <is>
-          <t>maa://41110 (98.31), maa://45605 (100.0)</t>
+          <t>maa://41110 (98.32), maa://45605 (100.0)</t>
         </is>
       </c>
       <c r="E369" s="17" t="inlineStr">
@@ -28028,7 +28028,7 @@
       </c>
       <c r="D391" s="17" t="inlineStr">
         <is>
-          <t>maa://51872 (96.63), maa://51876 (98.75), maa://51873 (100.0)</t>
+          <t>maa://51872 (96.65), maa://51876 (98.77), maa://51873 (100.0)</t>
         </is>
       </c>
       <c r="E391" s="17" t="inlineStr">
@@ -28082,7 +28082,7 @@
       </c>
       <c r="D392" s="17" t="inlineStr">
         <is>
-          <t>maa://59493 (95.83), maa://59603 (100.0)</t>
+          <t>maa://59493 (96.3), maa://59603 (100.0)</t>
         </is>
       </c>
       <c r="E392" s="17" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#198)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -703,7 +703,7 @@
       </c>
       <c r="D2" s="14" t="inlineStr">
         <is>
-          <t>maa://25390 (95.47), maa://24702 (94.84), maa://36681 (86.42)</t>
+          <t>maa://25390 (95.48), maa://24702 (94.84), maa://36681 (86.42)</t>
         </is>
       </c>
       <c r="E2" s="11" t="n"/>
@@ -730,12 +730,12 @@
       </c>
       <c r="K2" s="11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="L2" s="14" t="inlineStr">
         <is>
-          <t>maa://39402 (94.87), *maa://30515 (70.37), *maa://34787 (73.91)</t>
+          <t>maa://39402 (94.87), *maa://34787 (73.91)</t>
         </is>
       </c>
       <c r="M2" s="11" t="n"/>
@@ -767,7 +767,7 @@
       </c>
       <c r="T2" s="14" t="inlineStr">
         <is>
-          <t>maa://22742 (91.51)</t>
+          <t>maa://22742 (91.55)</t>
         </is>
       </c>
       <c r="U2" s="11" t="n"/>
@@ -833,7 +833,7 @@
       </c>
       <c r="D3" s="14" t="inlineStr">
         <is>
-          <t>maa://40192 (96.23), maa://36987 (96.23), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.26), maa://36987 (96.3), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="11" t="n"/>
@@ -849,7 +849,7 @@
       </c>
       <c r="H3" s="14" t="inlineStr">
         <is>
-          <t>maa://21247 (98.46)</t>
+          <t>maa://21247 (98.47)</t>
         </is>
       </c>
       <c r="I3" s="11" t="n"/>
@@ -865,7 +865,7 @@
       </c>
       <c r="L3" s="14" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.95), maa://20276 (88.63), *maa://22749 (77.78)</t>
+          <t>*maa://22880 (66.24), maa://20276 (88.63), *maa://22749 (77.78)</t>
         </is>
       </c>
       <c r="M3" s="11" t="n"/>
@@ -929,7 +929,7 @@
       </c>
       <c r="AB3" s="14" t="inlineStr">
         <is>
-          <t>maa://24390 (95.6), maa://52241 (100.0)</t>
+          <t>maa://24390 (95.7), maa://52241 (100.0)</t>
         </is>
       </c>
       <c r="AC3" s="11" t="n"/>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="T4" s="14" t="inlineStr">
         <is>
-          <t>maa://32509 (93.98), maa://27295 (88.3), maa://22754 (89.19), *maa://31008 (79.55)</t>
+          <t>maa://32509 (93.98), maa://27295 (88.42), maa://22754 (89.19), *maa://31008 (79.55)</t>
         </is>
       </c>
       <c r="U4" s="11" t="n"/>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="X4" s="14" t="inlineStr">
         <is>
-          <t>maa://43217 (93.8)</t>
+          <t>maa://43217 (93.85)</t>
         </is>
       </c>
       <c r="Y4" s="11" t="n"/>
@@ -1098,7 +1098,7 @@
       </c>
       <c r="D5" s="14" t="inlineStr">
         <is>
-          <t>maa://21245 (84.56), maa://22744 (82.14), maa://54105 (100.0)</t>
+          <t>maa://21245 (84.62), maa://22744 (82.14), maa://54105 (100.0)</t>
         </is>
       </c>
       <c r="E5" s="11" t="n"/>
@@ -1260,7 +1260,7 @@
       </c>
       <c r="L6" s="14" t="inlineStr">
         <is>
-          <t>maa://24839 (98.83)</t>
+          <t>maa://24839 (98.84)</t>
         </is>
       </c>
       <c r="M6" s="11" t="n"/>
@@ -1308,7 +1308,7 @@
       </c>
       <c r="X6" s="14" t="inlineStr">
         <is>
-          <t>maa://52754 (82.35)</t>
+          <t>maa://52754 (83.33)</t>
         </is>
       </c>
       <c r="Y6" s="11" t="n"/>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="AF6" s="14" t="inlineStr">
         <is>
-          <t>*maa://33152 (63.93), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (64.52), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="27" t="n"/>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="L7" s="14" t="inlineStr">
         <is>
-          <t>maa://28624 (93.84), maa://24957 (97.78)</t>
+          <t>maa://28624 (93.88), maa://24957 (97.78)</t>
         </is>
       </c>
       <c r="M7" s="11" t="n"/>
@@ -1422,7 +1422,7 @@
       </c>
       <c r="T7" s="14" t="inlineStr">
         <is>
-          <t>maa://21291 (86.67)</t>
+          <t>maa://21291 (87.1)</t>
         </is>
       </c>
       <c r="U7" s="11" t="n"/>
@@ -1478,7 +1478,7 @@
     <row r="8">
       <c r="A8" s="10" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.14 13:21:08</t>
+          <t>更新日期：2025.06.17 13:22:20</t>
         </is>
       </c>
       <c r="B8" s="11" t="inlineStr">
@@ -1509,7 +1509,7 @@
       </c>
       <c r="H8" s="14" t="inlineStr">
         <is>
-          <t>*maa://24371 (55.13)</t>
+          <t>*maa://24371 (55.7)</t>
         </is>
       </c>
       <c r="I8" s="11" t="n"/>
@@ -1623,7 +1623,7 @@
       </c>
       <c r="D9" s="14" t="inlineStr">
         <is>
-          <t>maa://22765 (90.1), *maa://21915 (71.88)</t>
+          <t>maa://22765 (90.2), *maa://21915 (71.88)</t>
         </is>
       </c>
       <c r="E9" s="11" t="n"/>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="L9" s="14" t="inlineStr">
         <is>
-          <t>maa://22762 (92.93), maa://39552 (83.33)</t>
+          <t>maa://22762 (93.07), maa://39552 (83.33)</t>
         </is>
       </c>
       <c r="M9" s="11" t="n"/>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="P9" s="14" t="inlineStr">
         <is>
-          <t>maa://22736 (83.33)</t>
+          <t>maa://22736 (83.48)</t>
         </is>
       </c>
       <c r="Q9" s="11" t="n"/>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="T9" s="14" t="inlineStr">
         <is>
-          <t>maa://26222 (98.33)</t>
+          <t>maa://26222 (98.36)</t>
         </is>
       </c>
       <c r="U9" s="11" t="n"/>
@@ -1719,7 +1719,7 @@
       </c>
       <c r="AB9" s="14" t="inlineStr">
         <is>
-          <t>maa://28711 (87.32), maa://40166 (93.88)</t>
+          <t>maa://28711 (87.41), maa://40166 (93.88)</t>
         </is>
       </c>
       <c r="AC9" s="11" t="n"/>
@@ -1735,7 +1735,7 @@
       </c>
       <c r="AF9" s="14" t="inlineStr">
         <is>
-          <t>maa://26206 (89.27), *maa://22865 (53.57)</t>
+          <t>maa://26206 (89.33), *maa://22865 (53.57)</t>
         </is>
       </c>
       <c r="AG9" s="27" t="n"/>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="D10" s="14" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.72), ***maa://39951 (11.84), ***maa://34206 (22.22), *maa://45271 (60.76), ***maa://39243 (25.0), **maa://54000 (33.33)</t>
+          <t>***maa://25695 (18.63), ***maa://39951 (11.84), ***maa://34206 (22.22), *maa://45271 (62.2), ***maa://39243 (25.0), **maa://54000 (33.33)</t>
         </is>
       </c>
       <c r="E10" s="11" t="n"/>
@@ -1801,7 +1801,7 @@
       </c>
       <c r="P10" s="14" t="inlineStr">
         <is>
-          <t>maa://28977 (87.63), maa://36669 (81.48), *maa://23264 (61.4)</t>
+          <t>maa://28977 (87.63), *maa://36669 (80.0), *maa://23264 (62.07)</t>
         </is>
       </c>
       <c r="Q10" s="11" t="n"/>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="T10" s="14" t="inlineStr">
         <is>
-          <t>maa://27395 (96.75), maa://22755 (89.15)</t>
+          <t>maa://27395 (96.77), maa://22755 (89.15)</t>
         </is>
       </c>
       <c r="U10" s="11" t="n"/>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="X10" s="14" t="inlineStr">
         <is>
-          <t>maa://22301 (97.91), maa://45828 (93.48), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.93), maa://45828 (93.48), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="11" t="n"/>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="AF10" s="14" t="inlineStr">
         <is>
-          <t>*maa://25021 (54.21), *maa://22733 (64.29), **maa://22761 (50.0)</t>
+          <t>*maa://25021 (53.7), *maa://22733 (64.29), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="27" t="n"/>
@@ -2093,7 +2093,7 @@
       </c>
       <c r="X12" s="14" t="inlineStr">
         <is>
-          <t>maa://22753 (91.94), *maa://21485 (75.84), maa://37962 (92.65)</t>
+          <t>maa://22753 (91.98), *maa://21485 (76.0), maa://37962 (92.75)</t>
         </is>
       </c>
       <c r="Y12" s="11" t="n"/>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="AB12" s="14" t="inlineStr">
         <is>
-          <t>maa://23669 (95.67), maa://36677 (95.35), maa://39872 (93.1)</t>
+          <t>maa://23669 (95.68), maa://36677 (95.35), maa://39872 (93.1)</t>
         </is>
       </c>
       <c r="AC12" s="11" t="n"/>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>maa://24999 (92.74), maa://36673 (91.95), maa://25001 (86.49)</t>
+          <t>maa://24999 (92.76), maa://36673 (91.95), maa://25001 (86.49)</t>
         </is>
       </c>
       <c r="E13" s="11" t="n"/>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="H13" s="14" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.02), **maa://22728 (46.94)</t>
+          <t>*maa://21248 (74.11), **maa://22728 (46.94)</t>
         </is>
       </c>
       <c r="I13" s="11" t="n"/>
@@ -2273,7 +2273,7 @@
       </c>
       <c r="D14" s="14" t="inlineStr">
         <is>
-          <t>maa://30764 (89.86)</t>
+          <t>maa://30764 (90.0)</t>
         </is>
       </c>
       <c r="E14" s="11" t="n"/>
@@ -2305,7 +2305,7 @@
       </c>
       <c r="L14" s="14" t="inlineStr">
         <is>
-          <t>maa://39841 (94.41), maa://26245 (96.72), maa://21288 (96.3), maa://36682 (95.92)</t>
+          <t>maa://39841 (94.44), maa://26245 (96.72), maa://21288 (96.3), maa://36682 (95.92)</t>
         </is>
       </c>
       <c r="M14" s="11" t="n"/>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="P14" s="14" t="inlineStr">
         <is>
-          <t>maa://23250 (98.87), maa://20107 (87.1), maa://22772 (100.0)</t>
+          <t>maa://23250 (98.88), maa://20107 (87.1), maa://22772 (100.0)</t>
         </is>
       </c>
       <c r="Q14" s="11" t="n"/>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="T14" s="14" t="inlineStr">
         <is>
-          <t>maa://22521 (94.87), maa://42751 (100.0)</t>
+          <t>maa://22521 (94.92), maa://42751 (100.0)</t>
         </is>
       </c>
       <c r="U14" s="11" t="n"/>
@@ -2353,7 +2353,7 @@
       </c>
       <c r="X14" s="14" t="inlineStr">
         <is>
-          <t>maa://37468 (92.0)</t>
+          <t>maa://37468 (92.31)</t>
         </is>
       </c>
       <c r="Y14" s="11" t="n"/>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="H15" s="14" t="inlineStr">
         <is>
-          <t>maa://24304 (87.06), maa://21478 (90.0)</t>
+          <t>maa://24304 (87.16), maa://21478 (90.0)</t>
         </is>
       </c>
       <c r="I15" s="11" t="n"/>
@@ -2451,7 +2451,7 @@
       </c>
       <c r="P15" s="14" t="inlineStr">
         <is>
-          <t>maa://24762 (91.35), *maa://22727 (70.0)</t>
+          <t>maa://24762 (91.4), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="11" t="n"/>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="T15" s="14" t="inlineStr">
         <is>
-          <t>maa://23892 (96.63)</t>
+          <t>maa://23892 (96.67)</t>
         </is>
       </c>
       <c r="U15" s="11" t="n"/>
@@ -2515,7 +2515,7 @@
       </c>
       <c r="AF15" s="14" t="inlineStr">
         <is>
-          <t>maa://21364 (81.3), maa://36666 (82.1), *maa://22766 (68.55)</t>
+          <t>maa://21364 (81.35), maa://36666 (82.1), *maa://22766 (68.55)</t>
         </is>
       </c>
       <c r="AG15" s="27" t="n"/>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="T16" s="14" t="inlineStr">
         <is>
-          <t>maa://22729 (94.48), *maa://28648 (73.75), maa://36674 (80.33)</t>
+          <t>maa://22729 (94.48), *maa://28648 (73.75), maa://36674 (80.65)</t>
         </is>
       </c>
       <c r="U16" s="11" t="n"/>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="H17" s="14" t="inlineStr">
         <is>
-          <t>maa://22430 (89.67), maa://39599 (86.75)</t>
+          <t>maa://22430 (89.72), maa://39599 (86.9)</t>
         </is>
       </c>
       <c r="I17" s="11" t="n"/>
@@ -2775,7 +2775,7 @@
       </c>
       <c r="AF17" s="14" t="inlineStr">
         <is>
-          <t>maa://50136 (95.45)</t>
+          <t>maa://50136 (96.0)</t>
         </is>
       </c>
       <c r="AG17" s="27" t="n"/>
@@ -2793,7 +2793,7 @@
       </c>
       <c r="D18" s="14" t="inlineStr">
         <is>
-          <t>maa://24570 (97.07)</t>
+          <t>maa://24570 (97.08)</t>
         </is>
       </c>
       <c r="E18" s="11" t="n"/>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="L18" s="14" t="inlineStr">
         <is>
-          <t>maa://22466 (92.12), maa://52226 (95.65)</t>
+          <t>maa://22466 (92.16), maa://52226 (95.65)</t>
         </is>
       </c>
       <c r="M18" s="11" t="n"/>
@@ -2889,7 +2889,7 @@
       </c>
       <c r="AB18" s="14" t="inlineStr">
         <is>
-          <t>maa://24393 (98.18)</t>
+          <t>maa://24393 (98.21)</t>
         </is>
       </c>
       <c r="AC18" s="11" t="n"/>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="T19" s="14" t="inlineStr">
         <is>
-          <t>maa://24386 (98.67)</t>
+          <t>maa://24386 (98.68)</t>
         </is>
       </c>
       <c r="U19" s="11" t="n"/>
@@ -3019,7 +3019,7 @@
       </c>
       <c r="AB19" s="14" t="inlineStr">
         <is>
-          <t>*maa://30709 (68.66), *maa://36668 (57.32)</t>
+          <t>*maa://30709 (68.85), *maa://36668 (57.32)</t>
         </is>
       </c>
       <c r="AC19" s="11" t="n"/>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="H20" s="14" t="inlineStr">
         <is>
-          <t>maa://22864 (90.86)</t>
+          <t>maa://22864 (90.37)</t>
         </is>
       </c>
       <c r="I20" s="11" t="n"/>
@@ -3085,7 +3085,7 @@
       </c>
       <c r="L20" s="14" t="inlineStr">
         <is>
-          <t>maa://41331 (86.17)</t>
+          <t>maa://41331 (86.27)</t>
         </is>
       </c>
       <c r="M20" s="11" t="n"/>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="P20" s="14" t="inlineStr">
         <is>
-          <t>maa://37442 (96.15)</t>
+          <t>maa://37442 (96.23)</t>
         </is>
       </c>
       <c r="Q20" s="11" t="n"/>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="X20" s="14" t="inlineStr">
         <is>
-          <t>maa://50085 (88.03), maa://49976 (86.59), maa://56241 (88.89)</t>
+          <t>maa://50085 (88.51), maa://49976 (86.59), maa://56241 (88.89)</t>
         </is>
       </c>
       <c r="Y20" s="11" t="n"/>
@@ -3183,7 +3183,7 @@
       </c>
       <c r="D21" s="14" t="inlineStr">
         <is>
-          <t>maa://21261 (98.0)</t>
+          <t>maa://21261 (98.08)</t>
         </is>
       </c>
       <c r="E21" s="11" t="n"/>
@@ -3199,7 +3199,7 @@
       </c>
       <c r="H21" s="14" t="inlineStr">
         <is>
-          <t>maa://24372 (97.17)</t>
+          <t>maa://24372 (97.2)</t>
         </is>
       </c>
       <c r="I21" s="11" t="n"/>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="P21" s="14" t="inlineStr">
         <is>
-          <t>maa://24381 (81.82)</t>
+          <t>maa://24381 (82.61)</t>
         </is>
       </c>
       <c r="Q21" s="11" t="n"/>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="AB21" s="14" t="inlineStr">
         <is>
-          <t>maa://21443 (82.81), ***maa://23820 (30.0), **maa://52223 (40.62)</t>
+          <t>maa://21443 (82.81), ***maa://23820 (30.0), **maa://52223 (39.39)</t>
         </is>
       </c>
       <c r="AC21" s="11" t="n"/>
@@ -3393,7 +3393,7 @@
       </c>
       <c r="X22" s="14" t="inlineStr">
         <is>
-          <t>maa://21282 (98.72), *maa://37649 (73.81)</t>
+          <t>maa://21282 (98.73), *maa://37649 (73.81)</t>
         </is>
       </c>
       <c r="Y22" s="11" t="n"/>
@@ -3443,7 +3443,7 @@
       </c>
       <c r="D23" s="14" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.75), **maa://41753 (50.0)</t>
+          <t>***maa://28036 (28.4), **maa://41753 (50.0)</t>
         </is>
       </c>
       <c r="E23" s="11" t="n"/>
@@ -3475,7 +3475,7 @@
       </c>
       <c r="L23" s="14" t="inlineStr">
         <is>
-          <t>maa://39756 (95.77), maa://39875 (94.87)</t>
+          <t>maa://39756 (95.78), maa://39875 (94.87)</t>
         </is>
       </c>
       <c r="M23" s="11" t="n"/>
@@ -3491,7 +3491,7 @@
       </c>
       <c r="P23" s="14" t="inlineStr">
         <is>
-          <t>maa://30587 (92.09), *maa://29748 (76.3), *maa://37566 (78.26)</t>
+          <t>maa://30587 (92.13), *maa://29748 (76.3), *maa://37566 (78.72)</t>
         </is>
       </c>
       <c r="Q23" s="11" t="n"/>
@@ -3507,7 +3507,7 @@
       </c>
       <c r="T23" s="14" t="inlineStr">
         <is>
-          <t>maa://31212 (89.47), maa://24387 (82.93)</t>
+          <t>maa://31212 (89.74), maa://24387 (82.93)</t>
         </is>
       </c>
       <c r="U23" s="11" t="n"/>
@@ -3653,7 +3653,7 @@
       </c>
       <c r="X24" s="14" t="inlineStr">
         <is>
-          <t>maa://29988 (84.92), maa://23504 (93.7), *maa://25141 (77.37), *maa://36663 (78.0), maa://52227 (100.0)</t>
+          <t>maa://29988 (84.92), maa://23504 (93.71), *maa://25141 (77.37), *maa://36663 (78.0), maa://52227 (100.0)</t>
         </is>
       </c>
       <c r="Y24" s="11" t="n"/>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="AF24" s="14" t="inlineStr">
         <is>
-          <t>maa://22523 (81.74), *maa://36672 (75.76), maa://29910 (93.75), maa://45831 (86.67)</t>
+          <t>maa://22523 (81.74), *maa://36672 (74.63), maa://29910 (93.85), maa://45831 (87.5)</t>
         </is>
       </c>
       <c r="AG24" s="27" t="n"/>
@@ -3703,7 +3703,7 @@
       </c>
       <c r="D25" s="14" t="inlineStr">
         <is>
-          <t>maa://29753 (95.47)</t>
+          <t>maa://29753 (95.48)</t>
         </is>
       </c>
       <c r="E25" s="11" t="n"/>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="P25" s="14" t="inlineStr">
         <is>
-          <t>maa://24382 (94.29)</t>
+          <t>maa://24382 (94.44)</t>
         </is>
       </c>
       <c r="Q25" s="11" t="n"/>
@@ -3799,7 +3799,7 @@
       </c>
       <c r="AB25" s="14" t="inlineStr">
         <is>
-          <t>maa://31215 (89.51), *maa://24516 (79.57), maa://26001 (84.75)</t>
+          <t>maa://31215 (89.66), *maa://24516 (79.57), maa://26001 (84.75)</t>
         </is>
       </c>
       <c r="AC25" s="11" t="n"/>
@@ -3815,7 +3815,7 @@
       </c>
       <c r="AF25" s="14" t="inlineStr">
         <is>
-          <t>maa://20108 (95.89), maa://24621 (97.18), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (80.0)</t>
+          <t>maa://20108 (95.92), maa://24621 (97.18), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (80.0)</t>
         </is>
       </c>
       <c r="AG25" s="27" t="n"/>
@@ -3913,7 +3913,7 @@
       </c>
       <c r="X26" s="14" t="inlineStr">
         <is>
-          <t>maa://24389 (96.88)</t>
+          <t>maa://24389 (96.97)</t>
         </is>
       </c>
       <c r="Y26" s="11" t="n"/>
@@ -3929,7 +3929,7 @@
       </c>
       <c r="AB26" s="14" t="inlineStr">
         <is>
-          <t>maa://42235 (96.05)</t>
+          <t>maa://42235 (96.1)</t>
         </is>
       </c>
       <c r="AC26" s="11" t="n"/>
@@ -3945,7 +3945,7 @@
       </c>
       <c r="AF26" s="14" t="inlineStr">
         <is>
-          <t>*maa://30511 (75.0), *maa://29760 (52.94)</t>
+          <t>*maa://30511 (75.47), *maa://29760 (52.94)</t>
         </is>
       </c>
       <c r="AG26" s="27" t="n"/>
@@ -3979,7 +3979,7 @@
       </c>
       <c r="H27" s="14" t="inlineStr">
         <is>
-          <t>*maa://39601 (79.17), maa://34494 (97.3)</t>
+          <t>maa://39601 (80.77), maa://34494 (97.3)</t>
         </is>
       </c>
       <c r="I27" s="11" t="n"/>
@@ -4075,7 +4075,7 @@
       </c>
       <c r="AF27" s="14" t="inlineStr">
         <is>
-          <t>maa://24023 (96.15)</t>
+          <t>maa://24023 (96.2)</t>
         </is>
       </c>
       <c r="AG27" s="27" t="n"/>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="D28" s="14" t="inlineStr">
         <is>
-          <t>maa://24465 (90.67), maa://25725 (82.83)</t>
+          <t>maa://24465 (90.68), maa://25725 (82.83)</t>
         </is>
       </c>
       <c r="E28" s="11" t="n"/>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="T28" s="14" t="inlineStr">
         <is>
-          <t>maa://23263 (95.45)</t>
+          <t>maa://23263 (95.5)</t>
         </is>
       </c>
       <c r="U28" s="11" t="n"/>
@@ -4173,7 +4173,7 @@
       </c>
       <c r="X28" s="14" t="inlineStr">
         <is>
-          <t>maa://39929 (91.97), maa://41749 (92.25)</t>
+          <t>maa://39929 (91.98), maa://41749 (92.31)</t>
         </is>
       </c>
       <c r="Y28" s="11" t="n"/>
@@ -4205,7 +4205,7 @@
       </c>
       <c r="AF28" s="14" t="inlineStr">
         <is>
-          <t>maa://36660 (92.54)</t>
+          <t>maa://36660 (92.58)</t>
         </is>
       </c>
       <c r="AG28" s="27" t="n"/>
@@ -4255,7 +4255,7 @@
       </c>
       <c r="L29" s="14" t="inlineStr">
         <is>
-          <t>maa://28432 (94.05), maa://31400 (98.89), maa://28440 (83.94), *maa://28650 (71.43)</t>
+          <t>maa://28432 (94.05), maa://31400 (98.89), maa://28440 (84.17), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="11" t="n"/>
@@ -4335,7 +4335,7 @@
       </c>
       <c r="AF29" s="14" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.17), maa://42865 (80.36), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (69.17), maa://42865 (80.53), ***maa://34960 (8.33)</t>
         </is>
       </c>
       <c r="AG29" s="27" t="n"/>
@@ -4353,7 +4353,7 @@
       </c>
       <c r="D30" s="14" t="inlineStr">
         <is>
-          <t>maa://45792 (89.66)</t>
+          <t>maa://45792 (90.0)</t>
         </is>
       </c>
       <c r="E30" s="11" t="n"/>
@@ -4417,7 +4417,7 @@
       </c>
       <c r="T30" s="14" t="inlineStr">
         <is>
-          <t>*maa://32940 (72.73), maa://24388 (94.74)</t>
+          <t>*maa://32940 (72.73), maa://24388 (95.0)</t>
         </is>
       </c>
       <c r="U30" s="11" t="n"/>
@@ -4449,7 +4449,7 @@
       </c>
       <c r="AB30" s="14" t="inlineStr">
         <is>
-          <t>maa://42979 (97.08), maa://45822 (100.0), maa://45045 (83.33)</t>
+          <t>maa://42979 (97.1), maa://45822 (100.0), maa://45045 (83.33)</t>
         </is>
       </c>
       <c r="AC30" s="11" t="n"/>
@@ -4515,7 +4515,7 @@
       </c>
       <c r="L31" s="14" t="inlineStr">
         <is>
-          <t>maa://35926 (93.75), maa://36258 (87.88), *maa://43904 (73.33)</t>
+          <t>maa://35926 (93.75), maa://36258 (87.95), *maa://43904 (73.33)</t>
         </is>
       </c>
       <c r="M31" s="11" t="n"/>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="H32" s="14" t="inlineStr">
         <is>
-          <t>maa://21895 (97.63), maa://36667 (97.32), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.64), maa://36667 (97.32), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="11" t="n"/>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="T32" s="14" t="inlineStr">
         <is>
-          <t>maa://42859 (96.98), maa://41108 (86.27), maa://41238 (97.99), maa://45523 (100.0)</t>
+          <t>maa://42859 (97.01), maa://41108 (86.27), maa://41238 (98.01), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="11" t="n"/>
@@ -4921,7 +4921,7 @@
       </c>
       <c r="P34" s="14" t="inlineStr">
         <is>
-          <t>maa://48817 (96.88), maa://56235 (100.0)</t>
+          <t>maa://48817 (96.92), maa://56235 (100.0)</t>
         </is>
       </c>
       <c r="Q34" s="11" t="n"/>
@@ -4937,7 +4937,7 @@
       </c>
       <c r="T34" s="14" t="inlineStr">
         <is>
-          <t>maa://24526 (92.39)</t>
+          <t>maa://24526 (92.42)</t>
         </is>
       </c>
       <c r="U34" s="11" t="n"/>
@@ -5035,7 +5035,7 @@
       </c>
       <c r="L35" s="14" t="inlineStr">
         <is>
-          <t>maa://41296 (97.37)</t>
+          <t>maa://41296 (97.38)</t>
         </is>
       </c>
       <c r="M35" s="11" t="n"/>
@@ -5149,7 +5149,7 @@
       </c>
       <c r="H36" s="14" t="inlineStr">
         <is>
-          <t>maa://24375 (90.7)</t>
+          <t>maa://24375 (90.91)</t>
         </is>
       </c>
       <c r="I36" s="11" t="n"/>
@@ -5279,7 +5279,7 @@
       </c>
       <c r="L37" s="14" t="inlineStr">
         <is>
-          <t>maa://45718 (98.46), maa://47069 (81.82), maa://56336 (87.5), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.46), maa://47069 (81.82), maa://56336 (88.89), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="11" t="n"/>
@@ -5444,7 +5444,7 @@
       </c>
       <c r="AF38" s="14" t="inlineStr">
         <is>
-          <t>maa://36697 (89.31)</t>
+          <t>maa://36697 (89.1)</t>
         </is>
       </c>
       <c r="AG38" s="27" t="n"/>
@@ -5465,7 +5465,7 @@
       </c>
       <c r="H39" s="14" t="inlineStr">
         <is>
-          <t>maa://36670 (89.57), maa://25199 (85.22), maa://30434 (93.13), *maa://45059 (79.41)</t>
+          <t>maa://36670 (89.66), maa://25199 (85.34), maa://30434 (93.18), *maa://45059 (79.41)</t>
         </is>
       </c>
       <c r="I39" s="11" t="n"/>
@@ -5513,7 +5513,7 @@
       </c>
       <c r="T39" s="14" t="inlineStr">
         <is>
-          <t>maa://47079 (96.0), *maa://45788 (72.5), maa://45790 (82.76)</t>
+          <t>maa://47079 (95.05), *maa://45788 (72.5), maa://45790 (82.76)</t>
         </is>
       </c>
       <c r="U39" s="11" t="n"/>
@@ -5667,7 +5667,7 @@
       </c>
       <c r="H41" s="14" t="inlineStr">
         <is>
-          <t>maa://24466 (93.88)</t>
+          <t>maa://24466 (94.0)</t>
         </is>
       </c>
       <c r="I41" s="11" t="n"/>
@@ -5991,7 +5991,7 @@
       </c>
       <c r="H45" s="14" t="inlineStr">
         <is>
-          <t>maa://21229 (84.42), maa://30807 (93.51), maa://42459 (89.47)</t>
+          <t>maa://21229 (84.42), maa://30807 (93.51), maa://42459 (87.18)</t>
         </is>
       </c>
       <c r="I45" s="11" t="n"/>
@@ -6007,7 +6007,7 @@
       </c>
       <c r="P45" s="14" t="inlineStr">
         <is>
-          <t>*maa://36237 (76.19)</t>
+          <t>*maa://36237 (77.27)</t>
         </is>
       </c>
       <c r="Q45" s="11" t="n"/>
@@ -6023,7 +6023,7 @@
       </c>
       <c r="T45" s="14" t="inlineStr">
         <is>
-          <t>**maa://39364 (45.0)</t>
+          <t>**maa://39364 (44.26)</t>
         </is>
       </c>
       <c r="U45" s="11" t="n"/>
@@ -6060,7 +6060,7 @@
       </c>
       <c r="H46" s="14" t="inlineStr">
         <is>
-          <t>maa://35931 (92.67), maa://43901 (94.74)</t>
+          <t>maa://35931 (92.71), maa://43901 (94.74)</t>
         </is>
       </c>
       <c r="I46" s="11" t="n"/>
@@ -6404,7 +6404,7 @@
       </c>
       <c r="P52" s="14" t="inlineStr">
         <is>
-          <t>maa://59378 (96.88), maa://59394 (91.67)</t>
+          <t>maa://59378 (96.88), maa://59394 (93.75)</t>
         </is>
       </c>
       <c r="Q52" s="11" t="n"/>
@@ -6438,7 +6438,7 @@
       </c>
       <c r="H53" s="14" t="inlineStr">
         <is>
-          <t>maa://32534 (95.13)</t>
+          <t>maa://32534 (95.16)</t>
         </is>
       </c>
       <c r="I53" s="11" t="n"/>
@@ -6594,7 +6594,7 @@
       </c>
       <c r="H59" s="14" t="inlineStr">
         <is>
-          <t>maa://31270 (94.74), maa://27746 (82.91)</t>
+          <t>maa://31270 (94.77), maa://27746 (82.91)</t>
         </is>
       </c>
       <c r="I59" s="11" t="n"/>
@@ -6612,7 +6612,7 @@
       </c>
       <c r="H60" s="14" t="inlineStr">
         <is>
-          <t>*maa://40438 (74.68)</t>
+          <t>*maa://40438 (75.0)</t>
         </is>
       </c>
       <c r="I60" s="11" t="n"/>
@@ -6661,12 +6661,12 @@
       </c>
       <c r="G63" s="11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H63" s="14" t="inlineStr">
         <is>
-          <t>maa://59534 (97.5), maa://59413 (100.0)</t>
+          <t>maa://59534 (97.73), maa://59693 (100.0), maa://59413 (100.0)</t>
         </is>
       </c>
       <c r="I63" s="11" t="n"/>
@@ -6968,7 +6968,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A1" s="13" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.14 13:21:08</t>
+          <t>更新日期：2025.06.17 13:22:20</t>
         </is>
       </c>
       <c r="E1" s="16" t="inlineStr">
@@ -8156,7 +8156,7 @@
       </c>
       <c r="D23" s="20" t="inlineStr">
         <is>
-          <t>maa://20876 (96.77)</t>
+          <t>maa://20876 (96.88)</t>
         </is>
       </c>
       <c r="E23" s="21" t="inlineStr">
@@ -8480,7 +8480,7 @@
       </c>
       <c r="D29" s="20" t="inlineStr">
         <is>
-          <t>maa://20863 (89.12), maa://20832 (99.07), maa://20727 (100.0)</t>
+          <t>maa://20863 (89.17), maa://20832 (99.08), maa://20727 (100.0)</t>
         </is>
       </c>
       <c r="E29" s="21" t="inlineStr">
@@ -8642,7 +8642,7 @@
       </c>
       <c r="D32" s="20" t="inlineStr">
         <is>
-          <t>maa://36644 (88.42), maa://36866 (96.15), maa://45572 (91.67), maa://27794 (100.0), maa://20960 (100.0), maa://20843 (100.0), **maa://24483 (50.0), maa://20862 (83.33), *maa://20893 (77.78)</t>
+          <t>maa://36644 (88.42), maa://36866 (96.23), maa://45572 (91.67), maa://27794 (100.0), maa://20960 (100.0), maa://20843 (100.0), **maa://24483 (50.0), maa://20862 (83.33), *maa://20893 (77.78)</t>
         </is>
       </c>
       <c r="E32" s="21" t="inlineStr">
@@ -8750,7 +8750,7 @@
       </c>
       <c r="D34" s="20" t="inlineStr">
         <is>
-          <t>maa://20916 (82.86), maa://52658 (87.5)</t>
+          <t>maa://20916 (82.86), maa://52658 (88.89)</t>
         </is>
       </c>
       <c r="E34" s="21" t="inlineStr">
@@ -9128,7 +9128,7 @@
       </c>
       <c r="D41" s="20" t="inlineStr">
         <is>
-          <t>maa://20892 (80.22)</t>
+          <t>maa://20892 (80.43)</t>
         </is>
       </c>
       <c r="E41" s="21" t="inlineStr">
@@ -10424,7 +10424,7 @@
       </c>
       <c r="D65" s="20" t="inlineStr">
         <is>
-          <t>maa://28567 (96.88), **maa://20947 (44.12), maa://30525 (100.0), maa://38735 (100.0), *maa://28188 (70.0), maa://30524 (100.0)</t>
+          <t>maa://28567 (96.92), **maa://20947 (44.12), maa://30525 (100.0), maa://38735 (100.0), *maa://28188 (70.0), maa://30524 (100.0)</t>
         </is>
       </c>
       <c r="E65" s="21" t="inlineStr">
@@ -10586,7 +10586,7 @@
       </c>
       <c r="D68" s="20" t="inlineStr">
         <is>
-          <t>maa://20976 (97.82), maa://20815 (100.0)</t>
+          <t>maa://20976 (97.83), maa://20815 (100.0)</t>
         </is>
       </c>
       <c r="E68" s="21" t="inlineStr">
@@ -11666,7 +11666,7 @@
       </c>
       <c r="D88" s="20" t="inlineStr">
         <is>
-          <t>maa://24472 (88.29), *maa://35841 (62.5)</t>
+          <t>maa://24472 (88.41), *maa://35841 (64.71)</t>
         </is>
       </c>
       <c r="E88" s="21" t="inlineStr">
@@ -12152,7 +12152,7 @@
       </c>
       <c r="D97" s="20" t="inlineStr">
         <is>
-          <t>maa://20991 (100.0), maa://51015 (85.71)</t>
+          <t>maa://20991 (100.0), maa://51015 (86.36)</t>
         </is>
       </c>
       <c r="E97" s="21" t="inlineStr">
@@ -12260,7 +12260,7 @@
       </c>
       <c r="D99" s="20" t="inlineStr">
         <is>
-          <t>maa://20929 (94.74)</t>
+          <t>maa://20929 (95.0)</t>
         </is>
       </c>
       <c r="E99" s="21" t="inlineStr">
@@ -12476,7 +12476,7 @@
       </c>
       <c r="D103" s="20" t="inlineStr">
         <is>
-          <t>*maa://29094 (70.45), maa://28904 (88.57), **maa://20931 (44.83)</t>
+          <t>*maa://29094 (71.11), maa://28904 (88.57), **maa://20931 (44.83)</t>
         </is>
       </c>
       <c r="E103" s="21" t="inlineStr">
@@ -12746,7 +12746,7 @@
       </c>
       <c r="D108" s="20" t="inlineStr">
         <is>
-          <t>maa://25018 (96.63), maa://51881 (99.16), maa://25776 (92.11), maa://28361 (97.37), maa://25772 (94.12), maa://56588 (94.12), maa://45194 (87.5), maa://32653 (85.71), maa://25161 (81.25)</t>
+          <t>maa://25018 (96.66), maa://51881 (99.18), maa://25776 (92.11), maa://28361 (97.37), maa://25772 (94.12), maa://56588 (94.44), maa://45194 (87.5), maa://32653 (85.71), maa://25161 (81.25)</t>
         </is>
       </c>
       <c r="E108" s="21" t="inlineStr">
@@ -13016,7 +13016,7 @@
       </c>
       <c r="D113" s="20" t="inlineStr">
         <is>
-          <t>maa://29037 (98.46)</t>
+          <t>maa://29037 (98.48)</t>
         </is>
       </c>
       <c r="E113" s="21" t="inlineStr">
@@ -13448,7 +13448,7 @@
       </c>
       <c r="D121" s="20" t="inlineStr">
         <is>
-          <t>maa://20869 (100.0), maa://44690 (94.74)</t>
+          <t>maa://20869 (100.0), maa://44690 (95.0)</t>
         </is>
       </c>
       <c r="E121" s="21" t="inlineStr">
@@ -13502,7 +13502,7 @@
       </c>
       <c r="D122" s="20" t="inlineStr">
         <is>
-          <t>maa://29650 (98.31), maa://45570 (97.87)</t>
+          <t>maa://29650 (98.31), maa://45570 (97.92)</t>
         </is>
       </c>
       <c r="E122" s="21" t="inlineStr">
@@ -14420,7 +14420,7 @@
       </c>
       <c r="D139" s="20" t="inlineStr">
         <is>
-          <t>**maa://30679 (50.0), maa://45258 (92.86)</t>
+          <t>**maa://30679 (50.0), maa://45258 (93.33)</t>
         </is>
       </c>
       <c r="E139" s="21" t="inlineStr">
@@ -14582,7 +14582,7 @@
       </c>
       <c r="D142" s="20" t="inlineStr">
         <is>
-          <t>maa://28484 (97.08), **maa://23736 (43.28), maa://31185 (83.33), maa://30306 (100.0)</t>
+          <t>maa://28484 (97.1), **maa://23736 (43.28), maa://31185 (85.71), maa://30306 (100.0)</t>
         </is>
       </c>
       <c r="E142" s="21" t="inlineStr">
@@ -14636,7 +14636,7 @@
       </c>
       <c r="D143" s="20" t="inlineStr">
         <is>
-          <t>maa://30670 (96.6), maa://31470 (96.67), *maa://45066 (66.67), **maa://30867 (40.0)</t>
+          <t>maa://30670 (96.64), maa://31470 (96.67), *maa://45066 (66.67), **maa://30867 (40.0)</t>
         </is>
       </c>
       <c r="E143" s="21" t="inlineStr">
@@ -14960,7 +14960,7 @@
       </c>
       <c r="D149" s="20" t="inlineStr">
         <is>
-          <t>maa://36641 (98.44), maa://40957 (93.36), maa://36865 (96.32), maa://44635 (87.74), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
+          <t>maa://36641 (98.44), maa://40957 (93.39), maa://36865 (96.34), maa://44635 (87.74), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
         </is>
       </c>
       <c r="E149" s="21" t="inlineStr">
@@ -15014,7 +15014,7 @@
       </c>
       <c r="D150" s="20" t="inlineStr">
         <is>
-          <t>maa://51549 (95.12), maa://51923 (95.65)</t>
+          <t>maa://51549 (95.24), maa://51923 (95.65)</t>
         </is>
       </c>
       <c r="E150" s="21" t="inlineStr">
@@ -15500,7 +15500,7 @@
       </c>
       <c r="D159" s="20" t="inlineStr">
         <is>
-          <t>maa://44232 (98.56), maa://45603 (90.62), maa://44305 (100.0)</t>
+          <t>maa://44232 (98.57), maa://45603 (90.62), maa://44305 (100.0)</t>
         </is>
       </c>
       <c r="E159" s="21" t="inlineStr">
@@ -15932,7 +15932,7 @@
       </c>
       <c r="D167" s="20" t="inlineStr">
         <is>
-          <t>maa://29633 (92.28), maa://29627 (92.69), maa://29659 (85.29), maa://49074 (97.56), **maa://30679 (50.0), maa://29861 (100.0), maa://42343 (100.0)</t>
+          <t>maa://29633 (92.31), maa://29627 (92.69), maa://29659 (85.29), maa://49074 (97.62), **maa://30679 (50.0), maa://29861 (100.0), maa://42343 (100.0)</t>
         </is>
       </c>
       <c r="E167" s="21" t="inlineStr">
@@ -15986,7 +15986,7 @@
       </c>
       <c r="D168" s="20" t="inlineStr">
         <is>
-          <t>maa://49867 (90.0), maa://49655 (96.3)</t>
+          <t>maa://49867 (90.32), maa://49655 (96.3)</t>
         </is>
       </c>
       <c r="E168" s="21" t="inlineStr">
@@ -17552,7 +17552,7 @@
       </c>
       <c r="D197" s="20" t="inlineStr">
         <is>
-          <t>maa://44224 (90.25), maa://35854 (85.23), maa://50388 (97.84), maa://25760 (86.84), ***maa://43911 (13.64), *maa://20872 (52.0), maa://51066 (100.0)</t>
+          <t>maa://44224 (90.25), maa://35854 (85.39), maa://50388 (97.84), maa://25760 (86.84), ***maa://43911 (13.64), *maa://20872 (52.0), maa://51066 (100.0)</t>
         </is>
       </c>
       <c r="E197" s="21" t="inlineStr">
@@ -17768,7 +17768,7 @@
       </c>
       <c r="D201" s="20" t="inlineStr">
         <is>
-          <t>maa://42223 (99.59), maa://49077 (94.29), maa://42292 (97.22), maa://42402 (100.0)</t>
+          <t>maa://42223 (99.6), maa://49077 (94.29), maa://42292 (97.22), maa://42402 (100.0)</t>
         </is>
       </c>
       <c r="E201" s="21" t="inlineStr">
@@ -18897,12 +18897,12 @@
       </c>
       <c r="C222" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D222" s="20" t="inlineStr">
         <is>
-          <t>maa://39695 (100.0)</t>
+          <t>maa://39695 (100.0), **maa://39911 (33.33)</t>
         </is>
       </c>
       <c r="E222" s="21" t="inlineStr">
@@ -19172,7 +19172,7 @@
       </c>
       <c r="D227" s="20" t="inlineStr">
         <is>
-          <t>maa://20987 (93.55), *maa://35801 (77.78)</t>
+          <t>maa://20987 (93.62), *maa://35801 (77.78)</t>
         </is>
       </c>
       <c r="E227" s="21" t="inlineStr">
@@ -19658,7 +19658,7 @@
       </c>
       <c r="D236" s="20" t="inlineStr">
         <is>
-          <t>maa://20917 (98.28)</t>
+          <t>maa://20917 (98.31)</t>
         </is>
       </c>
       <c r="E236" s="21" t="inlineStr">
@@ -19874,7 +19874,7 @@
       </c>
       <c r="D240" s="20" t="inlineStr">
         <is>
-          <t>*maa://30667 (78.63), maa://30666 (83.41), **maa://30739 (43.24), *maa://30723 (56.45), maa://39588 (88.68)</t>
+          <t>*maa://30667 (78.68), maa://30666 (83.41), **maa://30739 (43.24), *maa://30723 (56.45), maa://39588 (88.89)</t>
         </is>
       </c>
       <c r="E240" s="21" t="inlineStr">
@@ -20360,7 +20360,7 @@
       </c>
       <c r="D249" s="20" t="inlineStr">
         <is>
-          <t>maa://42287 (90.48), maa://45570 (97.87), maa://42225 (100.0)</t>
+          <t>maa://42287 (90.7), maa://45570 (97.92), maa://42225 (100.0)</t>
         </is>
       </c>
       <c r="E249" s="21" t="inlineStr">
@@ -21332,7 +21332,7 @@
       </c>
       <c r="D267" s="20" t="inlineStr">
         <is>
-          <t>maa://49643 (86.36)</t>
+          <t>maa://49643 (86.96)</t>
         </is>
       </c>
       <c r="E267" s="21" t="inlineStr">
@@ -21602,7 +21602,7 @@
       </c>
       <c r="D272" s="20" t="inlineStr">
         <is>
-          <t>maa://51881 (99.16), maa://51630 (96.59), maa://56588 (94.12), *maa://55171 (57.14), maa://51893 (88.89)</t>
+          <t>maa://51881 (99.18), maa://51630 (96.59), maa://56588 (94.44), *maa://55171 (57.14), maa://51893 (88.89)</t>
         </is>
       </c>
       <c r="E272" s="21" t="inlineStr">
@@ -22142,7 +22142,7 @@
       </c>
       <c r="D282" s="20" t="inlineStr">
         <is>
-          <t>*maa://39165 (66.67)</t>
+          <t>*maa://39165 (70.0)</t>
         </is>
       </c>
       <c r="E282" s="21" t="inlineStr">
@@ -22520,7 +22520,7 @@
       </c>
       <c r="D289" s="20" t="inlineStr">
         <is>
-          <t>maa://30710 (97.87), maa://36845 (95.59), maa://31558 (97.06), **maa://39217 (41.18), maa://30668 (86.67)</t>
+          <t>maa://30710 (97.87), maa://36845 (95.62), maa://31558 (97.14), **maa://39217 (41.18), maa://30668 (86.67)</t>
         </is>
       </c>
       <c r="E289" s="21" t="inlineStr">
@@ -22682,7 +22682,7 @@
       </c>
       <c r="D292" s="20" t="inlineStr">
         <is>
-          <t>maa://25774 (97.1), maa://28133 (92.86), maa://22469 (92.86), **maa://39217 (41.18), **maa://31349 (50.0)</t>
+          <t>maa://25774 (97.14), maa://28133 (92.86), maa://22469 (92.86), **maa://39217 (41.18), **maa://31349 (50.0)</t>
         </is>
       </c>
       <c r="E292" s="21" t="inlineStr">
@@ -23276,7 +23276,7 @@
       </c>
       <c r="D303" s="20" t="inlineStr">
         <is>
-          <t>maa://50280 (97.52), maa://49642 (96.88), maa://49660 (92.86), *maa://50517 (80.0)</t>
+          <t>maa://50280 (97.56), maa://49642 (96.88), maa://49660 (92.86), *maa://50517 (80.0)</t>
         </is>
       </c>
       <c r="E303" s="21" t="inlineStr">
@@ -23546,7 +23546,7 @@
       </c>
       <c r="D308" s="20" t="inlineStr">
         <is>
-          <t>maa://36005 (91.67)</t>
+          <t>maa://36005 (92.31)</t>
         </is>
       </c>
       <c r="E308" s="21" t="inlineStr">
@@ -24248,7 +24248,7 @@
       </c>
       <c r="D321" s="20" t="inlineStr">
         <is>
-          <t>maa://39692 (99.61), maa://39810 (86.36)</t>
+          <t>maa://39692 (99.62), maa://39810 (86.36)</t>
         </is>
       </c>
       <c r="E321" s="21" t="inlineStr">
@@ -24734,7 +24734,7 @@
       </c>
       <c r="D330" s="20" t="inlineStr">
         <is>
-          <t>maa://34205 (87.5), **maa://39541 (50.0)</t>
+          <t>maa://34205 (87.5), *maa://39541 (66.67)</t>
         </is>
       </c>
       <c r="E330" s="21" t="inlineStr">
@@ -24842,7 +24842,7 @@
       </c>
       <c r="D332" s="22" t="inlineStr">
         <is>
-          <t>maa://44234 (99.03)</t>
+          <t>maa://44234 (99.04)</t>
         </is>
       </c>
       <c r="E332" s="22" t="inlineStr">
@@ -24896,7 +24896,7 @@
       </c>
       <c r="D333" s="22" t="inlineStr">
         <is>
-          <t>maa://42968 (99.18), maa://49245 (100.0)</t>
+          <t>maa://42968 (99.19), maa://49245 (100.0)</t>
         </is>
       </c>
       <c r="E333" s="22" t="inlineStr">
@@ -25058,7 +25058,7 @@
       </c>
       <c r="D336" s="22" t="inlineStr">
         <is>
-          <t>maa://30671 (81.58), maa://30669 (99.22), maa://37275 (82.93), *maa://32410 (66.67), maa://41605 (100.0)</t>
+          <t>maa://30671 (81.58), maa://30669 (99.23), maa://37275 (82.93), *maa://32410 (66.67), maa://41605 (100.0)</t>
         </is>
       </c>
       <c r="E336" s="22" t="inlineStr">
@@ -25112,7 +25112,7 @@
       </c>
       <c r="D337" s="22" t="inlineStr">
         <is>
-          <t>maa://38295 (94.57), maa://49332 (100.0)</t>
+          <t>maa://38295 (94.62), maa://49332 (100.0)</t>
         </is>
       </c>
       <c r="E337" s="22" t="inlineStr">
@@ -25652,7 +25652,7 @@
       </c>
       <c r="D347" s="17" t="inlineStr">
         <is>
-          <t>maa://34865 (97.81), maa://34717 (94.03), *maa://45066 (66.67)</t>
+          <t>maa://34865 (97.82), maa://34717 (94.03), *maa://45066 (66.67)</t>
         </is>
       </c>
       <c r="E347" s="17" t="inlineStr">
@@ -25868,7 +25868,7 @@
       </c>
       <c r="D351" s="17" t="inlineStr">
         <is>
-          <t>maa://36868 (100.0), maa://35996 (97.62), **maa://39217 (41.18), maa://47349 (93.94)</t>
+          <t>maa://36868 (100.0), maa://35996 (97.67), **maa://39217 (41.18), maa://47349 (94.12)</t>
         </is>
       </c>
       <c r="E351" s="17" t="inlineStr">
@@ -26030,7 +26030,7 @@
       </c>
       <c r="D354" s="17" t="inlineStr">
         <is>
-          <t>maa://42299 (97.56), maa://42224 (81.25)</t>
+          <t>maa://42299 (97.62), maa://42224 (81.25)</t>
         </is>
       </c>
       <c r="E354" s="17" t="inlineStr">
@@ -26138,7 +26138,7 @@
       </c>
       <c r="D356" s="17" t="inlineStr">
         <is>
-          <t>maa://36646 (98.79), maa://36845 (95.59), **maa://39217 (41.18), maa://51007 (98.15)</t>
+          <t>maa://36646 (98.8), maa://36845 (95.62), **maa://39217 (41.18), maa://51007 (98.18)</t>
         </is>
       </c>
       <c r="E356" s="17" t="inlineStr">
@@ -26408,7 +26408,7 @@
       </c>
       <c r="D361" s="17" t="inlineStr">
         <is>
-          <t>maa://40957 (93.36), maa://44635 (87.74), maa://48026 (96.39), maa://41035 (92.42), maa://44660 (92.31), maa://41128 (83.78)</t>
+          <t>maa://40957 (93.39), maa://44635 (87.74), maa://48026 (96.43), maa://41035 (92.42), maa://44660 (92.31), maa://41128 (83.78)</t>
         </is>
       </c>
       <c r="E361" s="17" t="inlineStr">
@@ -26732,7 +26732,7 @@
       </c>
       <c r="D367" s="17" t="inlineStr">
         <is>
-          <t>maa://42333 (100.0), maa://41977 (100.0), maa://50518 (100.0)</t>
+          <t>maa://42333 (100.0), maa://50518 (100.0), maa://41977 (100.0)</t>
         </is>
       </c>
       <c r="E367" s="17" t="inlineStr">
@@ -26840,7 +26840,7 @@
       </c>
       <c r="D369" s="17" t="inlineStr">
         <is>
-          <t>maa://41110 (98.32), maa://45605 (100.0)</t>
+          <t>maa://41110 (98.35), maa://45605 (100.0)</t>
         </is>
       </c>
       <c r="E369" s="17" t="inlineStr">
@@ -27002,7 +27002,7 @@
       </c>
       <c r="D372" s="17" t="inlineStr">
         <is>
-          <t>maa://44233 (92.16), maa://45570 (97.87)</t>
+          <t>maa://44233 (92.16), maa://45570 (97.92)</t>
         </is>
       </c>
       <c r="E372" s="17" t="inlineStr">
@@ -27164,7 +27164,7 @@
       </c>
       <c r="D375" s="17" t="inlineStr">
         <is>
-          <t>*maa://53307 (69.23)</t>
+          <t>*maa://53307 (64.29)</t>
         </is>
       </c>
       <c r="E375" s="17" t="inlineStr">
@@ -27272,7 +27272,7 @@
       </c>
       <c r="D377" s="17" t="inlineStr">
         <is>
-          <t>maa://42970 (83.86), maa://44745 (98.17), **maa://49516 (42.11), *maa://45952 (80.0), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
+          <t>maa://42970 (83.59), maa://44745 (98.2), **maa://49516 (42.11), *maa://45952 (80.0), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E377" s="17" t="inlineStr">
@@ -28028,7 +28028,7 @@
       </c>
       <c r="D391" s="17" t="inlineStr">
         <is>
-          <t>maa://51872 (96.65), maa://51876 (98.77), maa://51873 (100.0)</t>
+          <t>maa://51872 (96.72), maa://51876 (98.78), maa://51873 (100.0)</t>
         </is>
       </c>
       <c r="E391" s="17" t="inlineStr">
@@ -28082,7 +28082,7 @@
       </c>
       <c r="D392" s="17" t="inlineStr">
         <is>
-          <t>maa://59493 (96.3), maa://59603 (100.0)</t>
+          <t>maa://59493 (96.97), maa://59603 (100.0)</t>
         </is>
       </c>
       <c r="E392" s="17" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#199)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -767,7 +767,7 @@
       </c>
       <c r="T2" s="14" t="inlineStr">
         <is>
-          <t>maa://22742 (91.55)</t>
+          <t>maa://22742 (91.63)</t>
         </is>
       </c>
       <c r="U2" s="11" t="n"/>
@@ -799,7 +799,7 @@
       </c>
       <c r="AB2" s="14" t="inlineStr">
         <is>
-          <t>maa://21246 (91.48), maa://36684 (93.17)</t>
+          <t>maa://21246 (91.48), maa://36684 (93.21)</t>
         </is>
       </c>
       <c r="AC2" s="11" t="n"/>
@@ -833,7 +833,7 @@
       </c>
       <c r="D3" s="14" t="inlineStr">
         <is>
-          <t>maa://40192 (96.26), maa://36987 (96.3), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.3), maa://36987 (96.3), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="11" t="n"/>
@@ -865,7 +865,7 @@
       </c>
       <c r="L3" s="14" t="inlineStr">
         <is>
-          <t>*maa://22880 (66.24), maa://20276 (88.63), *maa://22749 (77.78)</t>
+          <t>*maa://22880 (66.38), maa://20276 (88.63), *maa://22749 (77.78)</t>
         </is>
       </c>
       <c r="M3" s="11" t="n"/>
@@ -881,7 +881,7 @@
       </c>
       <c r="P3" s="14" t="inlineStr">
         <is>
-          <t>maa://21249 (94.72), maa://26254 (97.22)</t>
+          <t>maa://21249 (94.74), maa://26254 (97.22)</t>
         </is>
       </c>
       <c r="Q3" s="11" t="n"/>
@@ -897,7 +897,7 @@
       </c>
       <c r="T3" s="14" t="inlineStr">
         <is>
-          <t>maa://24617 (91.04), maa://45854 (84.38)</t>
+          <t>maa://24617 (91.11), maa://45854 (84.54)</t>
         </is>
       </c>
       <c r="U3" s="11" t="n"/>
@@ -963,7 +963,7 @@
       </c>
       <c r="D4" s="14" t="inlineStr">
         <is>
-          <t>maa://24632 (93.63), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.66), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="11" t="n"/>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="P4" s="14" t="inlineStr">
         <is>
-          <t>maa://49983 (96.1), maa://50121 (94.87)</t>
+          <t>maa://49983 (96.1), maa://50121 (95.0)</t>
         </is>
       </c>
       <c r="Q4" s="11" t="n"/>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="T4" s="14" t="inlineStr">
         <is>
-          <t>maa://32509 (93.98), maa://27295 (88.42), maa://22754 (89.19), *maa://31008 (79.55)</t>
+          <t>maa://32509 (94.03), maa://27295 (88.42), maa://22754 (89.19), *maa://31008 (79.55)</t>
         </is>
       </c>
       <c r="U4" s="11" t="n"/>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="X4" s="14" t="inlineStr">
         <is>
-          <t>maa://43217 (93.85)</t>
+          <t>maa://43217 (93.94)</t>
         </is>
       </c>
       <c r="Y4" s="11" t="n"/>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="AF6" s="14" t="inlineStr">
         <is>
-          <t>*maa://33152 (64.52), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (65.08), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="27" t="n"/>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="L7" s="14" t="inlineStr">
         <is>
-          <t>maa://28624 (93.88), maa://24957 (97.78)</t>
+          <t>maa://28624 (93.96), maa://24957 (97.78)</t>
         </is>
       </c>
       <c r="M7" s="11" t="n"/>
@@ -1478,7 +1478,7 @@
     <row r="8">
       <c r="A8" s="10" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.17 13:22:20</t>
+          <t>更新日期：2025.06.18 13:21:34</t>
         </is>
       </c>
       <c r="B8" s="11" t="inlineStr">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="P8" s="14" t="inlineStr">
         <is>
-          <t>maa://32931 (83.8), maa://23252 (91.67), maa://37496 (97.44)</t>
+          <t>maa://32931 (83.92), maa://23252 (91.67), maa://37496 (97.44)</t>
         </is>
       </c>
       <c r="Q8" s="11" t="n"/>
@@ -1623,7 +1623,7 @@
       </c>
       <c r="D9" s="14" t="inlineStr">
         <is>
-          <t>maa://22765 (90.2), *maa://21915 (71.88)</t>
+          <t>maa://22765 (90.38), *maa://21915 (71.88)</t>
         </is>
       </c>
       <c r="E9" s="11" t="n"/>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="D10" s="14" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.63), ***maa://39951 (11.84), ***maa://34206 (22.22), *maa://45271 (62.2), ***maa://39243 (25.0), **maa://54000 (33.33)</t>
+          <t>***maa://25695 (18.54), ***maa://39951 (11.69), ***maa://34206 (22.22), *maa://45271 (62.2), ***maa://39243 (25.0), **maa://54000 (33.33)</t>
         </is>
       </c>
       <c r="E10" s="11" t="n"/>
@@ -1801,7 +1801,7 @@
       </c>
       <c r="P10" s="14" t="inlineStr">
         <is>
-          <t>maa://28977 (87.63), *maa://36669 (80.0), *maa://23264 (62.07)</t>
+          <t>maa://28977 (87.63), maa://36669 (80.36), *maa://23264 (62.07)</t>
         </is>
       </c>
       <c r="Q10" s="11" t="n"/>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="T10" s="14" t="inlineStr">
         <is>
-          <t>maa://27395 (96.77), maa://22755 (89.15)</t>
+          <t>maa://27395 (96.77), maa://22755 (89.23)</t>
         </is>
       </c>
       <c r="U10" s="11" t="n"/>
@@ -1963,7 +1963,7 @@
       </c>
       <c r="X11" s="14" t="inlineStr">
         <is>
-          <t>maa://36713 (98.16)</t>
+          <t>maa://36713 (98.17)</t>
         </is>
       </c>
       <c r="Y11" s="11" t="n"/>
@@ -2093,7 +2093,7 @@
       </c>
       <c r="X12" s="14" t="inlineStr">
         <is>
-          <t>maa://22753 (91.98), *maa://21485 (76.0), maa://37962 (92.75)</t>
+          <t>maa://22753 (91.98), *maa://21485 (76.0), maa://37962 (92.96)</t>
         </is>
       </c>
       <c r="Y12" s="11" t="n"/>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="AB12" s="14" t="inlineStr">
         <is>
-          <t>maa://23669 (95.68), maa://36677 (95.35), maa://39872 (93.1)</t>
+          <t>maa://23669 (95.68), maa://36677 (95.4), maa://39872 (93.1)</t>
         </is>
       </c>
       <c r="AC12" s="11" t="n"/>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>maa://24999 (92.76), maa://36673 (91.95), maa://25001 (86.49)</t>
+          <t>maa://24999 (92.76), maa://36673 (92.05), maa://25001 (86.49)</t>
         </is>
       </c>
       <c r="E13" s="11" t="n"/>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="P13" s="14" t="inlineStr">
         <is>
-          <t>maa://22676 (93.66), *maa://22583 (78.05), maa://48321 (92.31)</t>
+          <t>maa://22676 (93.66), *maa://22583 (78.05), maa://48321 (85.71)</t>
         </is>
       </c>
       <c r="Q13" s="11" t="n"/>
@@ -2223,7 +2223,7 @@
       </c>
       <c r="X13" s="14" t="inlineStr">
         <is>
-          <t>maa://34957 (83.78), **maa://22768 (50.0)</t>
+          <t>maa://34957 (83.93), **maa://22768 (50.0)</t>
         </is>
       </c>
       <c r="Y13" s="11" t="n"/>
@@ -2250,12 +2250,12 @@
       </c>
       <c r="AE13" s="11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF13" s="14" t="inlineStr">
         <is>
-          <t>**maa://22737 (38.61), maa://39883 (87.3), **maa://39885 (50.0)</t>
+          <t>maa://39883 (87.3), **maa://39885 (50.0)</t>
         </is>
       </c>
       <c r="AG13" s="27" t="n"/>
@@ -2305,7 +2305,7 @@
       </c>
       <c r="L14" s="14" t="inlineStr">
         <is>
-          <t>maa://39841 (94.44), maa://26245 (96.72), maa://21288 (96.3), maa://36682 (95.92)</t>
+          <t>maa://39841 (94.48), maa://26245 (96.72), maa://21288 (96.3), maa://36682 (95.92)</t>
         </is>
       </c>
       <c r="M14" s="11" t="n"/>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="H15" s="14" t="inlineStr">
         <is>
-          <t>maa://24304 (87.16), maa://21478 (90.0)</t>
+          <t>maa://24304 (87.21), maa://21478 (90.0)</t>
         </is>
       </c>
       <c r="I15" s="11" t="n"/>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="T16" s="14" t="inlineStr">
         <is>
-          <t>maa://22729 (94.48), *maa://28648 (73.75), maa://36674 (80.65)</t>
+          <t>maa://22729 (94.51), *maa://28648 (73.75), maa://36674 (80.65)</t>
         </is>
       </c>
       <c r="U16" s="11" t="n"/>
@@ -2809,7 +2809,7 @@
       </c>
       <c r="H18" s="14" t="inlineStr">
         <is>
-          <t>maa://24421 (86.88)</t>
+          <t>maa://24421 (86.93)</t>
         </is>
       </c>
       <c r="I18" s="11" t="n"/>
@@ -3019,7 +3019,7 @@
       </c>
       <c r="AB19" s="14" t="inlineStr">
         <is>
-          <t>*maa://30709 (68.85), *maa://36668 (57.32)</t>
+          <t>*maa://30709 (68.85), *maa://36668 (57.83)</t>
         </is>
       </c>
       <c r="AC19" s="11" t="n"/>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="H20" s="14" t="inlineStr">
         <is>
-          <t>maa://22864 (90.37)</t>
+          <t>maa://22864 (90.43)</t>
         </is>
       </c>
       <c r="I20" s="11" t="n"/>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="X20" s="14" t="inlineStr">
         <is>
-          <t>maa://50085 (88.51), maa://49976 (86.59), maa://56241 (88.89)</t>
+          <t>maa://50085 (88.59), maa://49976 (86.59), maa://56241 (88.89)</t>
         </is>
       </c>
       <c r="Y20" s="11" t="n"/>
@@ -3274,12 +3274,12 @@
       </c>
       <c r="AA21" s="11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AB21" s="14" t="inlineStr">
         <is>
-          <t>maa://21443 (82.81), ***maa://23820 (30.0), **maa://52223 (39.39)</t>
+          <t>maa://21443 (82.85)</t>
         </is>
       </c>
       <c r="AC21" s="11" t="n"/>
@@ -3295,7 +3295,7 @@
       </c>
       <c r="AF21" s="14" t="inlineStr">
         <is>
-          <t>maa://22524 (88.8), maa://22432 (83.21)</t>
+          <t>maa://22524 (88.84), maa://22432 (83.33)</t>
         </is>
       </c>
       <c r="AG21" s="27" t="n"/>
@@ -3329,7 +3329,7 @@
       </c>
       <c r="H22" s="14" t="inlineStr">
         <is>
-          <t>maa://25236 (96.23)</t>
+          <t>maa://25236 (96.26)</t>
         </is>
       </c>
       <c r="I22" s="11" t="n"/>
@@ -3393,7 +3393,7 @@
       </c>
       <c r="X22" s="14" t="inlineStr">
         <is>
-          <t>maa://21282 (98.73), *maa://37649 (73.81)</t>
+          <t>maa://21282 (98.73), *maa://37649 (74.42)</t>
         </is>
       </c>
       <c r="Y22" s="11" t="n"/>
@@ -3475,7 +3475,7 @@
       </c>
       <c r="L23" s="14" t="inlineStr">
         <is>
-          <t>maa://39756 (95.78), maa://39875 (94.87)</t>
+          <t>maa://39756 (95.78), maa://39875 (94.94)</t>
         </is>
       </c>
       <c r="M23" s="11" t="n"/>
@@ -3653,7 +3653,7 @@
       </c>
       <c r="X24" s="14" t="inlineStr">
         <is>
-          <t>maa://29988 (84.92), maa://23504 (93.71), *maa://25141 (77.37), *maa://36663 (78.0), maa://52227 (100.0)</t>
+          <t>maa://29988 (84.92), maa://23504 (93.72), *maa://25141 (77.37), *maa://36663 (78.0), maa://52227 (100.0)</t>
         </is>
       </c>
       <c r="Y24" s="11" t="n"/>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="AB24" s="14" t="inlineStr">
         <is>
-          <t>maa://39349 (87.5)</t>
+          <t>maa://39349 (88.89)</t>
         </is>
       </c>
       <c r="AC24" s="11" t="n"/>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="AF24" s="14" t="inlineStr">
         <is>
-          <t>maa://22523 (81.74), *maa://36672 (74.63), maa://29910 (93.85), maa://45831 (87.5)</t>
+          <t>maa://22523 (81.74), *maa://36672 (75.0), maa://29910 (93.85), maa://45831 (87.5)</t>
         </is>
       </c>
       <c r="AG24" s="27" t="n"/>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="H25" s="14" t="inlineStr">
         <is>
-          <t>*maa://29063 (72.96), *maa://25311 (74.11), ***maa://22725 (4.76), *maa://45047 (73.33)</t>
+          <t>*maa://29063 (72.59), *maa://25311 (74.11), ***maa://22725 (4.76), *maa://45047 (73.33)</t>
         </is>
       </c>
       <c r="I25" s="11" t="n"/>
@@ -3799,7 +3799,7 @@
       </c>
       <c r="AB25" s="14" t="inlineStr">
         <is>
-          <t>maa://31215 (89.66), *maa://24516 (79.57), maa://26001 (84.75)</t>
+          <t>maa://31215 (89.73), *maa://24516 (79.57), maa://26001 (84.75)</t>
         </is>
       </c>
       <c r="AC25" s="11" t="n"/>
@@ -3929,7 +3929,7 @@
       </c>
       <c r="AB26" s="14" t="inlineStr">
         <is>
-          <t>maa://42235 (96.1)</t>
+          <t>maa://42235 (96.13)</t>
         </is>
       </c>
       <c r="AC26" s="11" t="n"/>
@@ -4255,7 +4255,7 @@
       </c>
       <c r="L29" s="14" t="inlineStr">
         <is>
-          <t>maa://28432 (94.05), maa://31400 (98.89), maa://28440 (84.17), *maa://28650 (71.43)</t>
+          <t>maa://28432 (94.07), maa://31400 (98.89), maa://28440 (84.17), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="11" t="n"/>
@@ -4330,12 +4330,12 @@
       </c>
       <c r="AE29" s="11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF29" s="14" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.17), maa://42865 (80.53), ***maa://34960 (8.33)</t>
+          <t>*maa://24080 (69.17), maa://42865 (80.7)</t>
         </is>
       </c>
       <c r="AG29" s="27" t="n"/>
@@ -4449,7 +4449,7 @@
       </c>
       <c r="AB30" s="14" t="inlineStr">
         <is>
-          <t>maa://42979 (97.1), maa://45822 (100.0), maa://45045 (83.33)</t>
+          <t>maa://42979 (97.12), maa://45822 (100.0), maa://45045 (83.33)</t>
         </is>
       </c>
       <c r="AC30" s="11" t="n"/>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="H32" s="14" t="inlineStr">
         <is>
-          <t>maa://21895 (97.64), maa://36667 (97.32), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.65), maa://36667 (97.32), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="11" t="n"/>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="T32" s="14" t="inlineStr">
         <is>
-          <t>maa://42859 (97.01), maa://41108 (86.27), maa://41238 (98.01), maa://45523 (100.0)</t>
+          <t>maa://42859 (97.03), maa://41108 (86.27), maa://41238 (98.01), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="11" t="n"/>
@@ -4725,7 +4725,7 @@
       </c>
       <c r="AF32" s="14" t="inlineStr">
         <is>
-          <t>maa://42408 (88.24)</t>
+          <t>maa://42408 (88.89)</t>
         </is>
       </c>
       <c r="AG32" s="27" t="n"/>
@@ -4791,7 +4791,7 @@
       </c>
       <c r="P33" s="14" t="inlineStr">
         <is>
-          <t>maa://21956 (81.6), *maa://22730 (71.88)</t>
+          <t>maa://21956 (81.71), *maa://22730 (71.88)</t>
         </is>
       </c>
       <c r="Q33" s="11" t="n"/>
@@ -5035,7 +5035,7 @@
       </c>
       <c r="L35" s="14" t="inlineStr">
         <is>
-          <t>maa://41296 (97.38)</t>
+          <t>maa://41296 (97.39)</t>
         </is>
       </c>
       <c r="M35" s="11" t="n"/>
@@ -5279,7 +5279,7 @@
       </c>
       <c r="L37" s="14" t="inlineStr">
         <is>
-          <t>maa://45718 (98.46), maa://47069 (81.82), maa://56336 (88.89), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.46), maa://47069 (81.82), maa://56336 (90.0), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="11" t="n"/>
@@ -5311,7 +5311,7 @@
       </c>
       <c r="T37" s="14" t="inlineStr">
         <is>
-          <t>**maa://39354 (41.67)</t>
+          <t>**maa://39354 (38.46)</t>
         </is>
       </c>
       <c r="U37" s="11" t="n"/>
@@ -5444,7 +5444,7 @@
       </c>
       <c r="AF38" s="14" t="inlineStr">
         <is>
-          <t>maa://36697 (89.1)</t>
+          <t>maa://36697 (89.13)</t>
         </is>
       </c>
       <c r="AG38" s="27" t="n"/>
@@ -5513,7 +5513,7 @@
       </c>
       <c r="T39" s="14" t="inlineStr">
         <is>
-          <t>maa://47079 (95.05), *maa://45788 (72.5), maa://45790 (82.76)</t>
+          <t>maa://47079 (95.05), *maa://45788 (71.9), maa://45790 (82.76)</t>
         </is>
       </c>
       <c r="U39" s="11" t="n"/>
@@ -5598,7 +5598,7 @@
       </c>
       <c r="P40" s="14" t="inlineStr">
         <is>
-          <t>maa://23278 (95.27), maa://21386 (95.83), maa://36664 (90.0), maa://45550 (87.5)</t>
+          <t>maa://23278 (95.27), maa://21386 (95.83), maa://36664 (90.16), maa://45550 (87.5)</t>
         </is>
       </c>
       <c r="Q40" s="11" t="n"/>
@@ -5694,12 +5694,12 @@
       </c>
       <c r="O41" s="11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P41" s="14" t="inlineStr">
         <is>
-          <t>**maa://35616 (40.54), maa://43177 (87.88)</t>
+          <t>maa://43177 (87.88)</t>
         </is>
       </c>
       <c r="Q41" s="11" t="n"/>
@@ -5922,7 +5922,7 @@
       </c>
       <c r="H44" s="14" t="inlineStr">
         <is>
-          <t>maa://29768 (97.97), maa://27728 (96.19), maa://56386 (100.0)</t>
+          <t>maa://29768 (97.64), maa://27728 (96.19), maa://56386 (100.0)</t>
         </is>
       </c>
       <c r="I44" s="11" t="n"/>
@@ -5991,7 +5991,7 @@
       </c>
       <c r="H45" s="14" t="inlineStr">
         <is>
-          <t>maa://21229 (84.42), maa://30807 (93.51), maa://42459 (87.18)</t>
+          <t>maa://21229 (84.42), maa://30807 (93.51), maa://42459 (87.5)</t>
         </is>
       </c>
       <c r="I45" s="11" t="n"/>
@@ -6060,7 +6060,7 @@
       </c>
       <c r="H46" s="14" t="inlineStr">
         <is>
-          <t>maa://35931 (92.71), maa://43901 (94.74)</t>
+          <t>maa://35931 (92.71), maa://43901 (94.83)</t>
         </is>
       </c>
       <c r="I46" s="11" t="n"/>
@@ -6251,7 +6251,7 @@
       </c>
       <c r="P49" s="14" t="inlineStr">
         <is>
-          <t>*maa://39643 (55.32)</t>
+          <t>*maa://39643 (56.25)</t>
         </is>
       </c>
       <c r="Q49" s="11" t="n"/>
@@ -6404,7 +6404,7 @@
       </c>
       <c r="P52" s="14" t="inlineStr">
         <is>
-          <t>maa://59378 (96.88), maa://59394 (93.75)</t>
+          <t>maa://59378 (96.88), maa://59394 (94.12)</t>
         </is>
       </c>
       <c r="Q52" s="11" t="n"/>
@@ -6438,7 +6438,7 @@
       </c>
       <c r="H53" s="14" t="inlineStr">
         <is>
-          <t>maa://32534 (95.16)</t>
+          <t>maa://32534 (95.17)</t>
         </is>
       </c>
       <c r="I53" s="11" t="n"/>
@@ -6522,7 +6522,7 @@
       </c>
       <c r="H55" s="14" t="inlineStr">
         <is>
-          <t>maa://32532 (93.39)</t>
+          <t>maa://32532 (93.42)</t>
         </is>
       </c>
       <c r="I55" s="11" t="n"/>
@@ -6968,7 +6968,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A1" s="13" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.17 13:22:20</t>
+          <t>更新日期：2025.06.18 13:21:34</t>
         </is>
       </c>
       <c r="E1" s="16" t="inlineStr">
@@ -8912,7 +8912,7 @@
       </c>
       <c r="D37" s="20" t="inlineStr">
         <is>
-          <t>maa://27376 (91.49), maa://42635 (95.56), *maa://20838 (52.63)</t>
+          <t>maa://27376 (91.49), maa://42635 (95.65), *maa://20838 (52.63)</t>
         </is>
       </c>
       <c r="E37" s="21" t="inlineStr">
@@ -9182,7 +9182,7 @@
       </c>
       <c r="D42" s="20" t="inlineStr">
         <is>
-          <t>maa://20918 (95.24), maa://34883 (93.75), maa://20824 (100.0)</t>
+          <t>maa://20918 (95.45), maa://34883 (93.75), maa://20824 (100.0)</t>
         </is>
       </c>
       <c r="E42" s="21" t="inlineStr">
@@ -9938,7 +9938,7 @@
       </c>
       <c r="D56" s="20" t="inlineStr">
         <is>
-          <t>maa://44235 (98.21), maa://45604 (100.0), maa://20961 (100.0), maa://44220 (100.0), maa://20910 (100.0)</t>
+          <t>maa://44235 (98.22), maa://45604 (100.0), maa://20961 (100.0), maa://44220 (100.0), maa://20910 (100.0)</t>
         </is>
       </c>
       <c r="E56" s="21" t="inlineStr">
@@ -10802,7 +10802,7 @@
       </c>
       <c r="D72" s="20" t="inlineStr">
         <is>
-          <t>maa://36643 (98.24), maa://36864 (98.0), maa://39140 (100.0)</t>
+          <t>maa://36643 (98.25), maa://36864 (98.0), maa://39140 (100.0)</t>
         </is>
       </c>
       <c r="E72" s="21" t="inlineStr">
@@ -12746,7 +12746,7 @@
       </c>
       <c r="D108" s="20" t="inlineStr">
         <is>
-          <t>maa://25018 (96.66), maa://51881 (99.18), maa://25776 (92.11), maa://28361 (97.37), maa://25772 (94.12), maa://56588 (94.44), maa://45194 (87.5), maa://32653 (85.71), maa://25161 (81.25)</t>
+          <t>maa://25018 (96.66), maa://51881 (99.19), maa://25776 (92.11), maa://28361 (97.37), maa://25772 (94.12), maa://56588 (94.44), maa://45194 (87.5), maa://32653 (85.71), maa://25161 (81.25)</t>
         </is>
       </c>
       <c r="E108" s="21" t="inlineStr">
@@ -13502,7 +13502,7 @@
       </c>
       <c r="D122" s="20" t="inlineStr">
         <is>
-          <t>maa://29650 (98.31), maa://45570 (97.92)</t>
+          <t>maa://29650 (98.31), maa://45570 (98.0)</t>
         </is>
       </c>
       <c r="E122" s="21" t="inlineStr">
@@ -17552,7 +17552,7 @@
       </c>
       <c r="D197" s="20" t="inlineStr">
         <is>
-          <t>maa://44224 (90.25), maa://35854 (85.39), maa://50388 (97.84), maa://25760 (86.84), ***maa://43911 (13.64), *maa://20872 (52.0), maa://51066 (100.0)</t>
+          <t>maa://44224 (90.25), maa://35854 (85.56), maa://50388 (97.86), maa://25760 (86.84), ***maa://43911 (13.64), *maa://20872 (52.0), maa://51066 (100.0)</t>
         </is>
       </c>
       <c r="E197" s="21" t="inlineStr">
@@ -18254,7 +18254,7 @@
       </c>
       <c r="D210" s="20" t="inlineStr">
         <is>
-          <t>maa://28133 (92.86), **maa://39217 (41.18), maa://25369 (94.29)</t>
+          <t>maa://28133 (92.98), **maa://39217 (41.18), maa://25369 (94.29)</t>
         </is>
       </c>
       <c r="E210" s="21" t="inlineStr">
@@ -18740,7 +18740,7 @@
       </c>
       <c r="D219" s="20" t="inlineStr">
         <is>
-          <t>**maa://26496 (33.33), **maa://20995 (50.0)</t>
+          <t>***maa://26496 (30.0), *maa://20995 (54.55)</t>
         </is>
       </c>
       <c r="E219" s="21" t="inlineStr">
@@ -20090,7 +20090,7 @@
       </c>
       <c r="D244" s="20" t="inlineStr">
         <is>
-          <t>maa://20867 (93.33), maa://38485 (95.65), *maa://32202 (80.0)</t>
+          <t>maa://20867 (93.33), maa://38485 (95.83), *maa://32202 (80.0)</t>
         </is>
       </c>
       <c r="E244" s="21" t="inlineStr">
@@ -20360,7 +20360,7 @@
       </c>
       <c r="D249" s="20" t="inlineStr">
         <is>
-          <t>maa://42287 (90.7), maa://45570 (97.92), maa://42225 (100.0)</t>
+          <t>maa://42287 (90.8), maa://45570 (98.0), maa://42225 (100.0)</t>
         </is>
       </c>
       <c r="E249" s="21" t="inlineStr">
@@ -20468,7 +20468,7 @@
       </c>
       <c r="D251" s="20" t="inlineStr">
         <is>
-          <t>maa://20923 (92.31)</t>
+          <t>maa://20923 (92.59)</t>
         </is>
       </c>
       <c r="E251" s="21" t="inlineStr">
@@ -21602,7 +21602,7 @@
       </c>
       <c r="D272" s="20" t="inlineStr">
         <is>
-          <t>maa://51881 (99.18), maa://51630 (96.59), maa://56588 (94.44), *maa://55171 (57.14), maa://51893 (88.89)</t>
+          <t>maa://51881 (99.19), maa://51630 (96.59), maa://56588 (94.44), *maa://55171 (57.14), maa://51893 (88.89)</t>
         </is>
       </c>
       <c r="E272" s="21" t="inlineStr">
@@ -21872,7 +21872,7 @@
       </c>
       <c r="D277" s="20" t="inlineStr">
         <is>
-          <t>maa://28133 (92.86), maa://33394 (100.0)</t>
+          <t>maa://28133 (92.98), maa://33394 (100.0)</t>
         </is>
       </c>
       <c r="E277" s="21" t="inlineStr">
@@ -22682,7 +22682,7 @@
       </c>
       <c r="D292" s="20" t="inlineStr">
         <is>
-          <t>maa://25774 (97.14), maa://28133 (92.86), maa://22469 (92.86), **maa://39217 (41.18), **maa://31349 (50.0)</t>
+          <t>maa://25774 (97.14), maa://28133 (92.98), maa://22469 (92.86), **maa://39217 (41.18), **maa://31349 (50.0)</t>
         </is>
       </c>
       <c r="E292" s="21" t="inlineStr">
@@ -23276,7 +23276,7 @@
       </c>
       <c r="D303" s="20" t="inlineStr">
         <is>
-          <t>maa://50280 (97.56), maa://49642 (96.88), maa://49660 (92.86), *maa://50517 (80.0)</t>
+          <t>maa://50280 (97.58), maa://49642 (96.88), maa://49660 (92.86), *maa://50517 (80.0)</t>
         </is>
       </c>
       <c r="E303" s="21" t="inlineStr">
@@ -24410,7 +24410,7 @@
       </c>
       <c r="D324" s="20" t="inlineStr">
         <is>
-          <t>maa://34867 (97.87), maa://34715 (100.0)</t>
+          <t>maa://34867 (97.96), maa://34715 (100.0)</t>
         </is>
       </c>
       <c r="E324" s="21" t="inlineStr">
@@ -24626,7 +24626,7 @@
       </c>
       <c r="D328" s="20" t="inlineStr">
         <is>
-          <t>maa://40956 (93.51)</t>
+          <t>maa://40956 (93.59)</t>
         </is>
       </c>
       <c r="E328" s="21" t="inlineStr">
@@ -24842,7 +24842,7 @@
       </c>
       <c r="D332" s="22" t="inlineStr">
         <is>
-          <t>maa://44234 (99.04)</t>
+          <t>maa://44234 (99.05)</t>
         </is>
       </c>
       <c r="E332" s="22" t="inlineStr">
@@ -25058,7 +25058,7 @@
       </c>
       <c r="D336" s="22" t="inlineStr">
         <is>
-          <t>maa://30671 (81.58), maa://30669 (99.23), maa://37275 (82.93), *maa://32410 (66.67), maa://41605 (100.0)</t>
+          <t>maa://30671 (81.15), maa://30669 (99.23), maa://37275 (82.93), *maa://32410 (66.67), maa://41605 (100.0)</t>
         </is>
       </c>
       <c r="E336" s="22" t="inlineStr">
@@ -26246,7 +26246,7 @@
       </c>
       <c r="D358" s="17" t="inlineStr">
         <is>
-          <t>maa://42635 (95.56), maa://50629 (100.0), maa://48859 (100.0)</t>
+          <t>maa://42635 (95.65), maa://50629 (100.0), maa://48859 (100.0)</t>
         </is>
       </c>
       <c r="E358" s="17" t="inlineStr">
@@ -26408,7 +26408,7 @@
       </c>
       <c r="D361" s="17" t="inlineStr">
         <is>
-          <t>maa://40957 (93.39), maa://44635 (87.74), maa://48026 (96.43), maa://41035 (92.42), maa://44660 (92.31), maa://41128 (83.78)</t>
+          <t>maa://40957 (93.39), maa://44635 (87.74), maa://48026 (96.47), maa://41035 (92.42), maa://44660 (92.31), maa://41128 (83.78)</t>
         </is>
       </c>
       <c r="E361" s="17" t="inlineStr">
@@ -26840,7 +26840,7 @@
       </c>
       <c r="D369" s="17" t="inlineStr">
         <is>
-          <t>maa://41110 (98.35), maa://45605 (100.0)</t>
+          <t>maa://41110 (98.36), maa://45605 (100.0)</t>
         </is>
       </c>
       <c r="E369" s="17" t="inlineStr">
@@ -27002,7 +27002,7 @@
       </c>
       <c r="D372" s="17" t="inlineStr">
         <is>
-          <t>maa://44233 (92.16), maa://45570 (97.92)</t>
+          <t>maa://44233 (92.31), maa://45570 (98.0)</t>
         </is>
       </c>
       <c r="E372" s="17" t="inlineStr">
@@ -27272,7 +27272,7 @@
       </c>
       <c r="D377" s="17" t="inlineStr">
         <is>
-          <t>maa://42970 (83.59), maa://44745 (98.2), **maa://49516 (42.11), *maa://45952 (80.0), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
+          <t>maa://42970 (83.59), maa://44745 (98.21), **maa://49516 (42.11), *maa://45952 (80.0), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E377" s="17" t="inlineStr">
@@ -28028,7 +28028,7 @@
       </c>
       <c r="D391" s="17" t="inlineStr">
         <is>
-          <t>maa://51872 (96.72), maa://51876 (98.78), maa://51873 (100.0)</t>
+          <t>maa://51872 (96.73), maa://51876 (98.78), maa://51873 (100.0)</t>
         </is>
       </c>
       <c r="E391" s="17" t="inlineStr">
@@ -28082,7 +28082,7 @@
       </c>
       <c r="D392" s="17" t="inlineStr">
         <is>
-          <t>maa://59493 (96.97), maa://59603 (100.0)</t>
+          <t>maa://59493 (97.12), maa://59603 (100.0)</t>
         </is>
       </c>
       <c r="E392" s="17" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#200)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -735,7 +735,7 @@
       </c>
       <c r="L2" s="14" t="inlineStr">
         <is>
-          <t>maa://39402 (94.87), *maa://34787 (73.91)</t>
+          <t>maa://39402 (94.92), *maa://34787 (73.91)</t>
         </is>
       </c>
       <c r="M2" s="11" t="n"/>
@@ -767,7 +767,7 @@
       </c>
       <c r="T2" s="14" t="inlineStr">
         <is>
-          <t>maa://22742 (91.63)</t>
+          <t>maa://22742 (91.67)</t>
         </is>
       </c>
       <c r="U2" s="11" t="n"/>
@@ -881,7 +881,7 @@
       </c>
       <c r="P3" s="14" t="inlineStr">
         <is>
-          <t>maa://21249 (94.74), maa://26254 (97.22)</t>
+          <t>maa://21249 (94.76), maa://26254 (97.22)</t>
         </is>
       </c>
       <c r="Q3" s="11" t="n"/>
@@ -897,7 +897,7 @@
       </c>
       <c r="T3" s="14" t="inlineStr">
         <is>
-          <t>maa://24617 (91.11), maa://45854 (84.54)</t>
+          <t>maa://24617 (91.18), maa://45854 (83.67)</t>
         </is>
       </c>
       <c r="U3" s="11" t="n"/>
@@ -913,7 +913,7 @@
       </c>
       <c r="X3" s="14" t="inlineStr">
         <is>
-          <t>maa://27396 (84.03), maa://27484 (96.32), maa://27480 (84.62)</t>
+          <t>maa://27396 (84.03), maa://27484 (96.35), maa://27480 (84.62)</t>
         </is>
       </c>
       <c r="Y3" s="11" t="n"/>
@@ -1098,7 +1098,7 @@
       </c>
       <c r="D5" s="14" t="inlineStr">
         <is>
-          <t>maa://21245 (84.62), maa://22744 (82.14), maa://54105 (100.0)</t>
+          <t>maa://21245 (84.67), maa://22744 (82.14), maa://54105 (100.0)</t>
         </is>
       </c>
       <c r="E5" s="11" t="n"/>
@@ -1478,7 +1478,7 @@
     <row r="8">
       <c r="A8" s="10" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.18 13:21:34</t>
+          <t>更新日期：2025.06.19 13:20:55</t>
         </is>
       </c>
       <c r="B8" s="11" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="X8" s="14" t="inlineStr">
         <is>
-          <t>maa://21411 (96.09)</t>
+          <t>maa://21411 (95.87)</t>
         </is>
       </c>
       <c r="Y8" s="11" t="n"/>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="T10" s="14" t="inlineStr">
         <is>
-          <t>maa://27395 (96.77), maa://22755 (89.23)</t>
+          <t>maa://27395 (96.79), maa://22755 (89.23)</t>
         </is>
       </c>
       <c r="U10" s="11" t="n"/>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="H15" s="14" t="inlineStr">
         <is>
-          <t>maa://24304 (87.21), maa://21478 (90.0)</t>
+          <t>maa://24304 (87.26), maa://21478 (90.0)</t>
         </is>
       </c>
       <c r="I15" s="11" t="n"/>
@@ -2451,7 +2451,7 @@
       </c>
       <c r="P15" s="14" t="inlineStr">
         <is>
-          <t>maa://24762 (91.4), *maa://22727 (70.0)</t>
+          <t>maa://24762 (91.44), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="11" t="n"/>
@@ -2515,7 +2515,7 @@
       </c>
       <c r="AF15" s="14" t="inlineStr">
         <is>
-          <t>maa://21364 (81.35), maa://36666 (82.1), *maa://22766 (68.55)</t>
+          <t>maa://21364 (81.35), maa://36666 (82.21), *maa://22766 (68.55)</t>
         </is>
       </c>
       <c r="AG15" s="27" t="n"/>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="T16" s="14" t="inlineStr">
         <is>
-          <t>maa://22729 (94.51), *maa://28648 (73.75), maa://36674 (80.65)</t>
+          <t>maa://22729 (94.51), *maa://28648 (74.07), maa://36674 (80.65)</t>
         </is>
       </c>
       <c r="U16" s="11" t="n"/>
@@ -2793,7 +2793,7 @@
       </c>
       <c r="D18" s="14" t="inlineStr">
         <is>
-          <t>maa://24570 (97.08)</t>
+          <t>maa://24570 (97.09)</t>
         </is>
       </c>
       <c r="E18" s="11" t="n"/>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="L18" s="14" t="inlineStr">
         <is>
-          <t>maa://22466 (92.16), maa://52226 (95.65)</t>
+          <t>maa://22466 (92.16), maa://52226 (95.83)</t>
         </is>
       </c>
       <c r="M18" s="11" t="n"/>
@@ -3019,7 +3019,7 @@
       </c>
       <c r="AB19" s="14" t="inlineStr">
         <is>
-          <t>*maa://30709 (68.85), *maa://36668 (57.83)</t>
+          <t>*maa://30709 (68.98), *maa://36668 (57.83)</t>
         </is>
       </c>
       <c r="AC19" s="11" t="n"/>
@@ -3329,7 +3329,7 @@
       </c>
       <c r="H22" s="14" t="inlineStr">
         <is>
-          <t>maa://25236 (96.26)</t>
+          <t>maa://25236 (96.3)</t>
         </is>
       </c>
       <c r="I22" s="11" t="n"/>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="L22" s="14" t="inlineStr">
         <is>
-          <t>*maa://27127 (78.2), *maa://22751 (70.67)</t>
+          <t>*maa://27127 (77.61), *maa://22751 (70.67)</t>
         </is>
       </c>
       <c r="M22" s="11" t="n"/>
@@ -3799,7 +3799,7 @@
       </c>
       <c r="AB25" s="14" t="inlineStr">
         <is>
-          <t>maa://31215 (89.73), *maa://24516 (79.57), maa://26001 (84.75)</t>
+          <t>maa://31215 (89.8), *maa://24516 (79.57), maa://26001 (84.75)</t>
         </is>
       </c>
       <c r="AC25" s="11" t="n"/>
@@ -3815,7 +3815,7 @@
       </c>
       <c r="AF25" s="14" t="inlineStr">
         <is>
-          <t>maa://20108 (95.92), maa://24621 (97.18), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (80.0)</t>
+          <t>maa://20108 (95.95), maa://24621 (97.18), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (80.0)</t>
         </is>
       </c>
       <c r="AG25" s="27" t="n"/>
@@ -4027,7 +4027,7 @@
       </c>
       <c r="T27" s="14" t="inlineStr">
         <is>
-          <t>*maa://30624 (77.33)</t>
+          <t>*maa://30624 (77.63)</t>
         </is>
       </c>
       <c r="U27" s="11" t="n"/>
@@ -4205,7 +4205,7 @@
       </c>
       <c r="AF28" s="14" t="inlineStr">
         <is>
-          <t>maa://36660 (92.58)</t>
+          <t>maa://36660 (92.59)</t>
         </is>
       </c>
       <c r="AG28" s="27" t="n"/>
@@ -4515,7 +4515,7 @@
       </c>
       <c r="L31" s="14" t="inlineStr">
         <is>
-          <t>maa://35926 (93.75), maa://36258 (87.95), *maa://43904 (73.33)</t>
+          <t>maa://35926 (93.77), maa://36258 (88.1), *maa://43904 (73.33)</t>
         </is>
       </c>
       <c r="M31" s="11" t="n"/>
@@ -5035,7 +5035,7 @@
       </c>
       <c r="L35" s="14" t="inlineStr">
         <is>
-          <t>maa://41296 (97.39)</t>
+          <t>maa://41296 (97.41)</t>
         </is>
       </c>
       <c r="M35" s="11" t="n"/>
@@ -5115,7 +5115,7 @@
       </c>
       <c r="AF35" s="14" t="inlineStr">
         <is>
-          <t>maa://39479 (91.67)</t>
+          <t>maa://39479 (92.0)</t>
         </is>
       </c>
       <c r="AG35" s="27" t="n"/>
@@ -5444,7 +5444,7 @@
       </c>
       <c r="AF38" s="14" t="inlineStr">
         <is>
-          <t>maa://36697 (89.13)</t>
+          <t>maa://36697 (89.16)</t>
         </is>
       </c>
       <c r="AG38" s="27" t="n"/>
@@ -6023,7 +6023,7 @@
       </c>
       <c r="T45" s="14" t="inlineStr">
         <is>
-          <t>**maa://39364 (44.26)</t>
+          <t>**maa://39364 (43.55)</t>
         </is>
       </c>
       <c r="U45" s="11" t="n"/>
@@ -6060,7 +6060,7 @@
       </c>
       <c r="H46" s="14" t="inlineStr">
         <is>
-          <t>maa://35931 (92.71), maa://43901 (94.83)</t>
+          <t>maa://35931 (92.75), maa://43901 (94.83)</t>
         </is>
       </c>
       <c r="I46" s="11" t="n"/>
@@ -6404,7 +6404,7 @@
       </c>
       <c r="P52" s="14" t="inlineStr">
         <is>
-          <t>maa://59378 (96.88), maa://59394 (94.12)</t>
+          <t>maa://59378 (96.97), maa://59394 (94.74)</t>
         </is>
       </c>
       <c r="Q52" s="11" t="n"/>
@@ -6438,7 +6438,7 @@
       </c>
       <c r="H53" s="14" t="inlineStr">
         <is>
-          <t>maa://32534 (95.17)</t>
+          <t>maa://32534 (95.18)</t>
         </is>
       </c>
       <c r="I53" s="11" t="n"/>
@@ -6522,7 +6522,7 @@
       </c>
       <c r="H55" s="14" t="inlineStr">
         <is>
-          <t>maa://32532 (93.42)</t>
+          <t>maa://32532 (93.44)</t>
         </is>
       </c>
       <c r="I55" s="11" t="n"/>
@@ -6968,7 +6968,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A1" s="13" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.18 13:21:34</t>
+          <t>更新日期：2025.06.19 13:20:55</t>
         </is>
       </c>
       <c r="E1" s="16" t="inlineStr">
@@ -10208,7 +10208,7 @@
       </c>
       <c r="D61" s="20" t="inlineStr">
         <is>
-          <t>maa://20841 (100.0), maa://24093 (100.0), maa://31559 (94.29), maa://20924 (95.24), maa://25777 (100.0), maa://20631 (100.0), maa://28241 (100.0)</t>
+          <t>maa://20841 (100.0), maa://24093 (100.0), maa://31559 (94.44), maa://20924 (95.24), maa://25777 (100.0), maa://20631 (100.0), maa://28241 (100.0)</t>
         </is>
       </c>
       <c r="E61" s="21" t="inlineStr">
@@ -10748,7 +10748,7 @@
       </c>
       <c r="D71" s="20" t="inlineStr">
         <is>
-          <t>maa://20943 (99.38), maa://30673 (100.0), maa://30672 (100.0), maa://20856 (100.0)</t>
+          <t>maa://20943 (99.39), maa://30673 (100.0), maa://30672 (100.0), maa://20856 (100.0)</t>
         </is>
       </c>
       <c r="E71" s="21" t="inlineStr">
@@ -13448,7 +13448,7 @@
       </c>
       <c r="D121" s="20" t="inlineStr">
         <is>
-          <t>maa://20869 (100.0), maa://44690 (95.0)</t>
+          <t>maa://20869 (100.0), maa://44690 (95.45)</t>
         </is>
       </c>
       <c r="E121" s="21" t="inlineStr">
@@ -14960,7 +14960,7 @@
       </c>
       <c r="D149" s="20" t="inlineStr">
         <is>
-          <t>maa://36641 (98.44), maa://40957 (93.39), maa://36865 (96.34), maa://44635 (87.74), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
+          <t>maa://36641 (98.44), maa://40957 (93.44), maa://36865 (96.34), maa://44635 (87.74), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
         </is>
       </c>
       <c r="E149" s="21" t="inlineStr">
@@ -17552,7 +17552,7 @@
       </c>
       <c r="D197" s="20" t="inlineStr">
         <is>
-          <t>maa://44224 (90.25), maa://35854 (85.56), maa://50388 (97.86), maa://25760 (86.84), ***maa://43911 (13.64), *maa://20872 (52.0), maa://51066 (100.0)</t>
+          <t>maa://44224 (90.27), maa://35854 (85.56), maa://50388 (97.87), maa://25760 (86.84), ***maa://43911 (13.64), *maa://20872 (52.0), maa://51066 (100.0)</t>
         </is>
       </c>
       <c r="E197" s="21" t="inlineStr">
@@ -18254,7 +18254,7 @@
       </c>
       <c r="D210" s="20" t="inlineStr">
         <is>
-          <t>maa://28133 (92.98), **maa://39217 (41.18), maa://25369 (94.29)</t>
+          <t>maa://28133 (92.98), **maa://39217 (41.18), maa://25369 (94.44)</t>
         </is>
       </c>
       <c r="E210" s="21" t="inlineStr">
@@ -18308,7 +18308,7 @@
       </c>
       <c r="D211" s="20" t="inlineStr">
         <is>
-          <t>maa://20956 (95.81), *maa://20830 (80.0), maa://44703 (91.67)</t>
+          <t>maa://20956 (95.83), *maa://20830 (80.0), maa://44703 (91.67)</t>
         </is>
       </c>
       <c r="E211" s="21" t="inlineStr">
@@ -20090,7 +20090,7 @@
       </c>
       <c r="D244" s="20" t="inlineStr">
         <is>
-          <t>maa://20867 (93.33), maa://38485 (95.83), *maa://32202 (80.0)</t>
+          <t>maa://20867 (93.33), maa://38485 (96.0), *maa://32202 (80.0)</t>
         </is>
       </c>
       <c r="E244" s="21" t="inlineStr">
@@ -20522,7 +20522,7 @@
       </c>
       <c r="D252" s="20" t="inlineStr">
         <is>
-          <t>maa://24093 (100.0), maa://31559 (94.29), maa://20924 (95.24), **maa://49440 (50.0)</t>
+          <t>maa://24093 (100.0), maa://31559 (94.44), maa://20924 (95.24), **maa://49440 (50.0)</t>
         </is>
       </c>
       <c r="E252" s="21" t="inlineStr">
@@ -21386,7 +21386,7 @@
       </c>
       <c r="D268" s="20" t="inlineStr">
         <is>
-          <t>maa://48265 (82.35)</t>
+          <t>*maa://48265 (77.78)</t>
         </is>
       </c>
       <c r="E268" s="21" t="inlineStr">
@@ -21440,7 +21440,7 @@
       </c>
       <c r="D269" s="20" t="inlineStr">
         <is>
-          <t>*maa://20825 (71.43), *maa://21445 (72.22), *maa://35726 (63.64), ***maa://20891 (30.0)</t>
+          <t>*maa://20825 (72.41), *maa://21445 (72.22), *maa://35726 (63.64), ***maa://20891 (30.0)</t>
         </is>
       </c>
       <c r="E269" s="21" t="inlineStr">
@@ -24410,7 +24410,7 @@
       </c>
       <c r="D324" s="20" t="inlineStr">
         <is>
-          <t>maa://34867 (97.96), maa://34715 (100.0)</t>
+          <t>maa://34867 (98.0), maa://34715 (100.0)</t>
         </is>
       </c>
       <c r="E324" s="21" t="inlineStr">
@@ -25868,7 +25868,7 @@
       </c>
       <c r="D351" s="17" t="inlineStr">
         <is>
-          <t>maa://36868 (100.0), maa://35996 (97.67), **maa://39217 (41.18), maa://47349 (94.12)</t>
+          <t>maa://36868 (100.0), maa://35996 (97.67), **maa://39217 (41.18), maa://47349 (94.29)</t>
         </is>
       </c>
       <c r="E351" s="17" t="inlineStr">
@@ -25922,7 +25922,7 @@
       </c>
       <c r="D352" s="17" t="inlineStr">
         <is>
-          <t>maa://49696 (99.55), maa://49695 (100.0), maa://49758 (98.44), *maa://52357 (71.43), *maa://59402 (66.67)</t>
+          <t>maa://49696 (99.55), maa://49695 (100.0), maa://49758 (98.44), *maa://59402 (70.0), *maa://52357 (71.43)</t>
         </is>
       </c>
       <c r="E352" s="17" t="inlineStr">
@@ -26192,7 +26192,7 @@
       </c>
       <c r="D357" s="17" t="inlineStr">
         <is>
-          <t>maa://36645 (98.36), maa://36841 (92.65), maa://37484 (94.23), maa://37858 (93.33), maa://40489 (100.0), *maa://56268 (60.0)</t>
+          <t>maa://36645 (98.37), maa://36841 (92.65), maa://37484 (94.23), maa://37858 (93.33), maa://40489 (100.0), *maa://56268 (60.0)</t>
         </is>
       </c>
       <c r="E357" s="17" t="inlineStr">
@@ -26408,7 +26408,7 @@
       </c>
       <c r="D361" s="17" t="inlineStr">
         <is>
-          <t>maa://40957 (93.39), maa://44635 (87.74), maa://48026 (96.47), maa://41035 (92.42), maa://44660 (92.31), maa://41128 (83.78)</t>
+          <t>maa://40957 (93.44), maa://44635 (87.74), maa://48026 (96.47), maa://41035 (92.42), maa://44660 (92.31), maa://41128 (83.78)</t>
         </is>
       </c>
       <c r="E361" s="17" t="inlineStr">
@@ -27272,7 +27272,7 @@
       </c>
       <c r="D377" s="17" t="inlineStr">
         <is>
-          <t>maa://42970 (83.59), maa://44745 (98.21), **maa://49516 (42.11), *maa://45952 (80.0), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
+          <t>maa://42970 (83.27), maa://44745 (98.21), **maa://49516 (40.0), *maa://45952 (80.0), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E377" s="17" t="inlineStr">
@@ -28028,7 +28028,7 @@
       </c>
       <c r="D391" s="17" t="inlineStr">
         <is>
-          <t>maa://51872 (96.73), maa://51876 (98.78), maa://51873 (100.0)</t>
+          <t>maa://51872 (96.73), maa://51876 (98.8), maa://51873 (100.0)</t>
         </is>
       </c>
       <c r="E391" s="17" t="inlineStr">
@@ -28082,7 +28082,7 @@
       </c>
       <c r="D392" s="17" t="inlineStr">
         <is>
-          <t>maa://59493 (97.12), maa://59603 (100.0)</t>
+          <t>maa://59493 (97.2), maa://59603 (100.0)</t>
         </is>
       </c>
       <c r="E392" s="17" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#201)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -730,12 +730,12 @@
       </c>
       <c r="K2" s="11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="L2" s="14" t="inlineStr">
         <is>
-          <t>maa://39402 (94.92), *maa://34787 (73.91)</t>
+          <t>maa://39402 (94.96), *maa://34787 (73.91), *maa://58660 (80.0)</t>
         </is>
       </c>
       <c r="M2" s="11" t="n"/>
@@ -767,7 +767,7 @@
       </c>
       <c r="T2" s="14" t="inlineStr">
         <is>
-          <t>maa://22742 (91.67)</t>
+          <t>maa://22742 (91.71)</t>
         </is>
       </c>
       <c r="U2" s="11" t="n"/>
@@ -833,7 +833,7 @@
       </c>
       <c r="D3" s="14" t="inlineStr">
         <is>
-          <t>maa://40192 (96.3), maa://36987 (96.3), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.4), maa://36987 (96.3), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="11" t="n"/>
@@ -849,7 +849,7 @@
       </c>
       <c r="H3" s="14" t="inlineStr">
         <is>
-          <t>maa://21247 (98.47)</t>
+          <t>maa://21247 (98.48)</t>
         </is>
       </c>
       <c r="I3" s="11" t="n"/>
@@ -881,7 +881,7 @@
       </c>
       <c r="P3" s="14" t="inlineStr">
         <is>
-          <t>maa://21249 (94.76), maa://26254 (97.22)</t>
+          <t>maa://21249 (94.77), maa://26254 (97.22)</t>
         </is>
       </c>
       <c r="Q3" s="11" t="n"/>
@@ -897,7 +897,7 @@
       </c>
       <c r="T3" s="14" t="inlineStr">
         <is>
-          <t>maa://24617 (91.18), maa://45854 (83.67)</t>
+          <t>maa://24617 (91.18), maa://45854 (83.84)</t>
         </is>
       </c>
       <c r="U3" s="11" t="n"/>
@@ -963,7 +963,7 @@
       </c>
       <c r="D4" s="14" t="inlineStr">
         <is>
-          <t>maa://24632 (93.66), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.69), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="11" t="n"/>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="P4" s="14" t="inlineStr">
         <is>
-          <t>maa://49983 (96.1), maa://50121 (95.0)</t>
+          <t>maa://49983 (96.1), maa://50121 (95.12)</t>
         </is>
       </c>
       <c r="Q4" s="11" t="n"/>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="X4" s="14" t="inlineStr">
         <is>
-          <t>maa://43217 (93.94)</t>
+          <t>maa://43217 (93.98)</t>
         </is>
       </c>
       <c r="Y4" s="11" t="n"/>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="AB4" s="14" t="inlineStr">
         <is>
-          <t>*maa://32658 (76.92)</t>
+          <t>*maa://32658 (77.78)</t>
         </is>
       </c>
       <c r="AC4" s="11" t="n"/>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="D6" s="14" t="inlineStr">
         <is>
-          <t>maa://42407 (95.06)</t>
+          <t>maa://42407 (92.77)</t>
         </is>
       </c>
       <c r="E6" s="11" t="n"/>
@@ -1478,7 +1478,7 @@
     <row r="8">
       <c r="A8" s="10" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.19 13:20:55</t>
+          <t>更新日期：2025.06.21 13:21:26</t>
         </is>
       </c>
       <c r="B8" s="11" t="inlineStr">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="P8" s="14" t="inlineStr">
         <is>
-          <t>maa://32931 (83.92), maa://23252 (91.67), maa://37496 (97.44)</t>
+          <t>maa://32931 (83.92), maa://23252 (91.67), maa://37496 (97.5)</t>
         </is>
       </c>
       <c r="Q8" s="11" t="n"/>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="X8" s="14" t="inlineStr">
         <is>
-          <t>maa://21411 (95.87)</t>
+          <t>maa://21411 (95.89)</t>
         </is>
       </c>
       <c r="Y8" s="11" t="n"/>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="L9" s="14" t="inlineStr">
         <is>
-          <t>maa://22762 (93.07), maa://39552 (83.33)</t>
+          <t>maa://22762 (93.14), maa://39552 (83.33)</t>
         </is>
       </c>
       <c r="M9" s="11" t="n"/>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="T10" s="14" t="inlineStr">
         <is>
-          <t>maa://27395 (96.79), maa://22755 (89.23)</t>
+          <t>maa://27395 (96.8), maa://22755 (89.23)</t>
         </is>
       </c>
       <c r="U10" s="11" t="n"/>
@@ -2223,7 +2223,7 @@
       </c>
       <c r="X13" s="14" t="inlineStr">
         <is>
-          <t>maa://34957 (83.93), **maa://22768 (50.0)</t>
+          <t>maa://34957 (84.07), **maa://22768 (50.0)</t>
         </is>
       </c>
       <c r="Y13" s="11" t="n"/>
@@ -2305,7 +2305,7 @@
       </c>
       <c r="L14" s="14" t="inlineStr">
         <is>
-          <t>maa://39841 (94.48), maa://26245 (96.72), maa://21288 (96.3), maa://36682 (95.92)</t>
+          <t>maa://39841 (94.51), maa://26245 (96.74), maa://21288 (96.3), maa://36682 (96.0)</t>
         </is>
       </c>
       <c r="M14" s="11" t="n"/>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="P14" s="14" t="inlineStr">
         <is>
-          <t>maa://23250 (98.88), maa://20107 (87.1), maa://22772 (100.0)</t>
+          <t>maa://23250 (98.89), maa://20107 (87.1), maa://22772 (100.0)</t>
         </is>
       </c>
       <c r="Q14" s="11" t="n"/>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="D15" s="14" t="inlineStr">
         <is>
-          <t>*maa://22743 (79.01), maa://22734 (84.55), *maa://30808 (65.28), *maa://36048 (69.64), maa://45058 (85.0)</t>
+          <t>*maa://22743 (78.69), maa://22734 (84.55), *maa://30808 (65.28), *maa://36048 (69.64), maa://45058 (85.0)</t>
         </is>
       </c>
       <c r="E15" s="11" t="n"/>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="H15" s="14" t="inlineStr">
         <is>
-          <t>maa://24304 (87.26), maa://21478 (90.0)</t>
+          <t>maa://24304 (87.36), maa://21478 (90.0)</t>
         </is>
       </c>
       <c r="I15" s="11" t="n"/>
@@ -2515,7 +2515,7 @@
       </c>
       <c r="AF15" s="14" t="inlineStr">
         <is>
-          <t>maa://21364 (81.35), maa://36666 (82.21), *maa://22766 (68.55)</t>
+          <t>maa://21364 (81.4), maa://36666 (82.21), *maa://22766 (68.55)</t>
         </is>
       </c>
       <c r="AG15" s="27" t="n"/>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="AB16" s="14" t="inlineStr">
         <is>
-          <t>maa://26228 (95.61)</t>
+          <t>maa://26228 (95.65)</t>
         </is>
       </c>
       <c r="AC16" s="11" t="n"/>
@@ -2727,7 +2727,7 @@
       </c>
       <c r="T17" s="14" t="inlineStr">
         <is>
-          <t>*maa://42324 (58.0)</t>
+          <t>*maa://42324 (58.82)</t>
         </is>
       </c>
       <c r="U17" s="11" t="n"/>
@@ -2793,7 +2793,7 @@
       </c>
       <c r="D18" s="14" t="inlineStr">
         <is>
-          <t>maa://24570 (97.09)</t>
+          <t>maa://24570 (97.1)</t>
         </is>
       </c>
       <c r="E18" s="11" t="n"/>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="L18" s="14" t="inlineStr">
         <is>
-          <t>maa://22466 (92.16), maa://52226 (95.83)</t>
+          <t>maa://22466 (92.2), maa://52226 (95.83)</t>
         </is>
       </c>
       <c r="M18" s="11" t="n"/>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="D20" s="14" t="inlineStr">
         <is>
-          <t>maa://21432 (90.73), maa://25198 (93.89), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.78), maa://25198 (93.89), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="11" t="n"/>
@@ -3085,7 +3085,7 @@
       </c>
       <c r="L20" s="14" t="inlineStr">
         <is>
-          <t>maa://41331 (86.27)</t>
+          <t>maa://41331 (86.33)</t>
         </is>
       </c>
       <c r="M20" s="11" t="n"/>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="X20" s="14" t="inlineStr">
         <is>
-          <t>maa://50085 (88.59), maa://49976 (86.59), maa://56241 (88.89)</t>
+          <t>maa://50085 (88.59), maa://49976 (86.75), maa://56241 (88.89)</t>
         </is>
       </c>
       <c r="Y20" s="11" t="n"/>
@@ -3295,7 +3295,7 @@
       </c>
       <c r="AF21" s="14" t="inlineStr">
         <is>
-          <t>maa://22524 (88.84), maa://22432 (83.33)</t>
+          <t>maa://22524 (88.49), maa://22432 (83.33)</t>
         </is>
       </c>
       <c r="AG21" s="27" t="n"/>
@@ -3475,7 +3475,7 @@
       </c>
       <c r="L23" s="14" t="inlineStr">
         <is>
-          <t>maa://39756 (95.78), maa://39875 (94.94)</t>
+          <t>maa://39756 (95.8), maa://39875 (94.94)</t>
         </is>
       </c>
       <c r="M23" s="11" t="n"/>
@@ -3523,7 +3523,7 @@
       </c>
       <c r="X23" s="14" t="inlineStr">
         <is>
-          <t>*maa://28503 (64.58)</t>
+          <t>*maa://28503 (63.92)</t>
         </is>
       </c>
       <c r="Y23" s="11" t="n"/>
@@ -3573,7 +3573,7 @@
       </c>
       <c r="D24" s="14" t="inlineStr">
         <is>
-          <t>*maa://24368 (79.23), *maa://46650 (59.38)</t>
+          <t>*maa://24368 (79.33), *maa://46650 (59.38)</t>
         </is>
       </c>
       <c r="E24" s="11" t="n"/>
@@ -3653,7 +3653,7 @@
       </c>
       <c r="X24" s="14" t="inlineStr">
         <is>
-          <t>maa://29988 (84.92), maa://23504 (93.72), *maa://25141 (77.37), *maa://36663 (78.0), maa://52227 (100.0)</t>
+          <t>maa://29988 (84.97), maa://23504 (93.74), *maa://25141 (77.37), *maa://36663 (78.0), maa://52227 (100.0)</t>
         </is>
       </c>
       <c r="Y24" s="11" t="n"/>
@@ -4205,7 +4205,7 @@
       </c>
       <c r="AF28" s="14" t="inlineStr">
         <is>
-          <t>maa://36660 (92.59)</t>
+          <t>maa://36660 (92.61)</t>
         </is>
       </c>
       <c r="AG28" s="27" t="n"/>
@@ -4223,7 +4223,7 @@
       </c>
       <c r="D29" s="14" t="inlineStr">
         <is>
-          <t>maa://31694 (98.36)</t>
+          <t>maa://31694 (98.39)</t>
         </is>
       </c>
       <c r="E29" s="11" t="n"/>
@@ -4255,7 +4255,7 @@
       </c>
       <c r="L29" s="14" t="inlineStr">
         <is>
-          <t>maa://28432 (94.07), maa://31400 (98.89), maa://28440 (84.17), *maa://28650 (71.43)</t>
+          <t>maa://28432 (94.07), maa://31400 (98.9), maa://28440 (84.4), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="11" t="n"/>
@@ -4335,7 +4335,7 @@
       </c>
       <c r="AF29" s="14" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.17), maa://42865 (80.7)</t>
+          <t>*maa://24080 (69.17), maa://42865 (81.03)</t>
         </is>
       </c>
       <c r="AG29" s="27" t="n"/>
@@ -4449,7 +4449,7 @@
       </c>
       <c r="AB30" s="14" t="inlineStr">
         <is>
-          <t>maa://42979 (97.12), maa://45822 (100.0), maa://45045 (83.33)</t>
+          <t>maa://42979 (97.13), maa://45822 (100.0), maa://45045 (83.33)</t>
         </is>
       </c>
       <c r="AC30" s="11" t="n"/>
@@ -4515,7 +4515,7 @@
       </c>
       <c r="L31" s="14" t="inlineStr">
         <is>
-          <t>maa://35926 (93.77), maa://36258 (88.1), *maa://43904 (73.33)</t>
+          <t>maa://35926 (93.79), maa://36258 (88.17), *maa://43904 (73.33)</t>
         </is>
       </c>
       <c r="M31" s="11" t="n"/>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="H32" s="14" t="inlineStr">
         <is>
-          <t>maa://21895 (97.65), maa://36667 (97.32), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.67), maa://36667 (97.32), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="11" t="n"/>
@@ -4645,7 +4645,7 @@
       </c>
       <c r="L32" s="14" t="inlineStr">
         <is>
-          <t>maa://28065 (96.0)</t>
+          <t>maa://28065 (96.08)</t>
         </is>
       </c>
       <c r="M32" s="11" t="n"/>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="T32" s="14" t="inlineStr">
         <is>
-          <t>maa://42859 (97.03), maa://41108 (86.27), maa://41238 (98.01), maa://45523 (100.0)</t>
+          <t>maa://42859 (97.03), maa://41108 (86.27), maa://41238 (98.03), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="11" t="n"/>
@@ -5035,7 +5035,7 @@
       </c>
       <c r="L35" s="14" t="inlineStr">
         <is>
-          <t>maa://41296 (97.41)</t>
+          <t>maa://41296 (97.42)</t>
         </is>
       </c>
       <c r="M35" s="11" t="n"/>
@@ -5444,7 +5444,7 @@
       </c>
       <c r="AF38" s="14" t="inlineStr">
         <is>
-          <t>maa://36697 (89.16)</t>
+          <t>maa://36697 (89.2)</t>
         </is>
       </c>
       <c r="AG38" s="27" t="n"/>
@@ -5465,7 +5465,7 @@
       </c>
       <c r="H39" s="14" t="inlineStr">
         <is>
-          <t>maa://36670 (89.66), maa://25199 (85.34), maa://30434 (93.18), *maa://45059 (79.41)</t>
+          <t>maa://36670 (89.66), maa://25199 (85.34), maa://30434 (93.23), *maa://45059 (79.41)</t>
         </is>
       </c>
       <c r="I39" s="11" t="n"/>
@@ -5922,7 +5922,7 @@
       </c>
       <c r="H44" s="14" t="inlineStr">
         <is>
-          <t>maa://29768 (97.64), maa://27728 (96.19), maa://56386 (100.0)</t>
+          <t>maa://29768 (97.66), maa://27728 (96.19), maa://56386 (100.0)</t>
         </is>
       </c>
       <c r="I44" s="11" t="n"/>
@@ -6060,7 +6060,7 @@
       </c>
       <c r="H46" s="14" t="inlineStr">
         <is>
-          <t>maa://35931 (92.75), maa://43901 (94.83)</t>
+          <t>maa://35931 (92.76), maa://43901 (94.83)</t>
         </is>
       </c>
       <c r="I46" s="11" t="n"/>
@@ -6404,7 +6404,7 @@
       </c>
       <c r="P52" s="14" t="inlineStr">
         <is>
-          <t>maa://59378 (96.97), maa://59394 (94.74)</t>
+          <t>maa://59378 (97.14), maa://59394 (95.45)</t>
         </is>
       </c>
       <c r="Q52" s="11" t="n"/>
@@ -6438,7 +6438,7 @@
       </c>
       <c r="H53" s="14" t="inlineStr">
         <is>
-          <t>maa://32534 (95.18)</t>
+          <t>maa://32534 (95.19)</t>
         </is>
       </c>
       <c r="I53" s="11" t="n"/>
@@ -6522,7 +6522,7 @@
       </c>
       <c r="H55" s="14" t="inlineStr">
         <is>
-          <t>maa://32532 (93.44)</t>
+          <t>maa://32532 (93.49)</t>
         </is>
       </c>
       <c r="I55" s="11" t="n"/>
@@ -6576,7 +6576,7 @@
       </c>
       <c r="H58" s="14" t="inlineStr">
         <is>
-          <t>*maa://37964 (56.14)</t>
+          <t>*maa://37964 (55.17)</t>
         </is>
       </c>
       <c r="I58" s="11" t="n"/>
@@ -6666,7 +6666,7 @@
       </c>
       <c r="H63" s="14" t="inlineStr">
         <is>
-          <t>maa://59534 (97.73), maa://59693 (100.0), maa://59413 (100.0)</t>
+          <t>maa://59534 (97.83), maa://59693 (100.0), maa://59413 (100.0)</t>
         </is>
       </c>
       <c r="I63" s="11" t="n"/>
@@ -6968,7 +6968,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A1" s="13" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.19 13:20:55</t>
+          <t>更新日期：2025.06.21 13:21:26</t>
         </is>
       </c>
       <c r="E1" s="16" t="inlineStr">
@@ -8696,7 +8696,7 @@
       </c>
       <c r="D33" s="20" t="inlineStr">
         <is>
-          <t>maa://30500 (98.88), *maa://27290 (70.59), ***maa://42154 (8.33)</t>
+          <t>maa://30500 (98.89), *maa://27290 (70.59), ***maa://42154 (8.33)</t>
         </is>
       </c>
       <c r="E33" s="21" t="inlineStr">
@@ -9020,7 +9020,7 @@
       </c>
       <c r="D39" s="20" t="inlineStr">
         <is>
-          <t>*maa://29012 (80.0), maa://20928 (100.0)</t>
+          <t>maa://29012 (83.33), maa://20928 (100.0)</t>
         </is>
       </c>
       <c r="E39" s="21" t="inlineStr">
@@ -9236,7 +9236,7 @@
       </c>
       <c r="D43" s="20" t="inlineStr">
         <is>
-          <t>maa://20889 (90.91)</t>
+          <t>maa://20889 (91.67)</t>
         </is>
       </c>
       <c r="E43" s="21" t="inlineStr">
@@ -9398,7 +9398,7 @@
       </c>
       <c r="D46" s="20" t="inlineStr">
         <is>
-          <t>maa://39025 (85.71)</t>
+          <t>maa://39025 (87.5)</t>
         </is>
       </c>
       <c r="E46" s="21" t="inlineStr">
@@ -9776,7 +9776,7 @@
       </c>
       <c r="D53" s="20" t="inlineStr">
         <is>
-          <t>maa://20953 (95.83), maa://31173 (96.15)</t>
+          <t>maa://20953 (96.0), maa://31173 (96.3)</t>
         </is>
       </c>
       <c r="E53" s="21" t="inlineStr">
@@ -10208,7 +10208,7 @@
       </c>
       <c r="D61" s="20" t="inlineStr">
         <is>
-          <t>maa://20841 (100.0), maa://24093 (100.0), maa://31559 (94.44), maa://20924 (95.24), maa://25777 (100.0), maa://20631 (100.0), maa://28241 (100.0)</t>
+          <t>maa://20841 (100.0), maa://24093 (100.0), maa://31559 (94.59), maa://20924 (95.24), maa://25777 (100.0), maa://20631 (100.0), maa://28241 (100.0)</t>
         </is>
       </c>
       <c r="E61" s="21" t="inlineStr">
@@ -10316,7 +10316,7 @@
       </c>
       <c r="D63" s="20" t="inlineStr">
         <is>
-          <t>*maa://20845 (68.0), maa://38727 (87.5)</t>
+          <t>*maa://20845 (68.0), maa://38727 (88.89)</t>
         </is>
       </c>
       <c r="E63" s="21" t="inlineStr">
@@ -10640,7 +10640,7 @@
       </c>
       <c r="D69" s="20" t="inlineStr">
         <is>
-          <t>maa://20974 (96.43), maa://29079 (80.95), maa://29096 (95.65), maa://29087 (100.0), *maa://20823 (80.0), maa://20855 (93.33), maa://20904 (100.0)</t>
+          <t>maa://20974 (96.43), maa://29079 (80.95), maa://29096 (95.65), maa://29087 (100.0), *maa://20823 (80.0), maa://20855 (93.75), maa://20904 (100.0)</t>
         </is>
       </c>
       <c r="E69" s="21" t="inlineStr">
@@ -12476,7 +12476,7 @@
       </c>
       <c r="D103" s="20" t="inlineStr">
         <is>
-          <t>*maa://29094 (71.11), maa://28904 (88.57), **maa://20931 (44.83)</t>
+          <t>*maa://29094 (71.74), maa://28904 (88.57), **maa://20931 (44.83)</t>
         </is>
       </c>
       <c r="E103" s="21" t="inlineStr">
@@ -12746,7 +12746,7 @@
       </c>
       <c r="D108" s="20" t="inlineStr">
         <is>
-          <t>maa://25018 (96.66), maa://51881 (99.19), maa://25776 (92.11), maa://28361 (97.37), maa://25772 (94.12), maa://56588 (94.44), maa://45194 (87.5), maa://32653 (85.71), maa://25161 (81.25)</t>
+          <t>maa://25018 (96.66), maa://51881 (99.2), maa://25776 (92.11), maa://28361 (97.44), maa://25772 (94.12), maa://56588 (94.44), maa://45194 (87.5), maa://32653 (85.71), maa://25161 (81.25)</t>
         </is>
       </c>
       <c r="E108" s="21" t="inlineStr">
@@ -12908,7 +12908,7 @@
       </c>
       <c r="D111" s="20" t="inlineStr">
         <is>
-          <t>*maa://28554 (79.17)</t>
+          <t>*maa://28554 (80.0)</t>
         </is>
       </c>
       <c r="E111" s="21" t="inlineStr">
@@ -13934,7 +13934,7 @@
       </c>
       <c r="D130" s="20" t="inlineStr">
         <is>
-          <t>maa://21422 (99.09)</t>
+          <t>maa://21422 (99.1)</t>
         </is>
       </c>
       <c r="E130" s="21" t="inlineStr">
@@ -14096,7 +14096,7 @@
       </c>
       <c r="D133" s="20" t="inlineStr">
         <is>
-          <t>maa://29023 (100.0), maa://39515 (90.91)</t>
+          <t>maa://29023 (100.0), maa://39515 (91.67)</t>
         </is>
       </c>
       <c r="E133" s="21" t="inlineStr">
@@ -14906,7 +14906,7 @@
       </c>
       <c r="D148" s="20" t="inlineStr">
         <is>
-          <t>maa://28828 (88.24), maa://20846 (95.83), **maa://47286 (50.0)</t>
+          <t>maa://28828 (88.24), maa://20846 (95.83), *maa://47286 (66.67)</t>
         </is>
       </c>
       <c r="E148" s="21" t="inlineStr">
@@ -14960,7 +14960,7 @@
       </c>
       <c r="D149" s="20" t="inlineStr">
         <is>
-          <t>maa://36641 (98.44), maa://40957 (93.44), maa://36865 (96.34), maa://44635 (87.74), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
+          <t>maa://36641 (98.44), maa://40957 (93.6), maa://36865 (96.34), maa://44635 (87.85), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
         </is>
       </c>
       <c r="E149" s="21" t="inlineStr">
@@ -15500,7 +15500,7 @@
       </c>
       <c r="D159" s="20" t="inlineStr">
         <is>
-          <t>maa://44232 (98.57), maa://45603 (90.62), maa://44305 (100.0)</t>
+          <t>maa://44232 (98.58), maa://45603 (90.62), maa://44305 (100.0)</t>
         </is>
       </c>
       <c r="E159" s="21" t="inlineStr">
@@ -15608,7 +15608,7 @@
       </c>
       <c r="D161" s="20" t="inlineStr">
         <is>
-          <t>maa://20855 (93.33)</t>
+          <t>maa://20855 (93.75)</t>
         </is>
       </c>
       <c r="E161" s="21" t="inlineStr">
@@ -15986,7 +15986,7 @@
       </c>
       <c r="D168" s="20" t="inlineStr">
         <is>
-          <t>maa://49867 (90.32), maa://49655 (96.3)</t>
+          <t>maa://49867 (90.62), maa://49655 (96.3)</t>
         </is>
       </c>
       <c r="E168" s="21" t="inlineStr">
@@ -16580,7 +16580,7 @@
       </c>
       <c r="D179" s="20" t="inlineStr">
         <is>
-          <t>maa://20911 (95.65), *maa://29012 (80.0)</t>
+          <t>maa://20911 (95.65), maa://29012 (83.33)</t>
         </is>
       </c>
       <c r="E179" s="21" t="inlineStr">
@@ -17552,7 +17552,7 @@
       </c>
       <c r="D197" s="20" t="inlineStr">
         <is>
-          <t>maa://44224 (90.27), maa://35854 (85.56), maa://50388 (97.87), maa://25760 (86.84), ***maa://43911 (13.64), *maa://20872 (52.0), maa://51066 (100.0)</t>
+          <t>maa://44224 (90.27), maa://35854 (85.71), maa://50388 (97.89), maa://25760 (86.84), ***maa://43911 (13.04), *maa://20872 (52.0), maa://51066 (100.0)</t>
         </is>
       </c>
       <c r="E197" s="21" t="inlineStr">
@@ -17768,7 +17768,7 @@
       </c>
       <c r="D201" s="20" t="inlineStr">
         <is>
-          <t>maa://42223 (99.6), maa://49077 (94.29), maa://42292 (97.22), maa://42402 (100.0)</t>
+          <t>maa://42223 (99.6), maa://49077 (94.44), maa://42292 (97.22), maa://42402 (100.0)</t>
         </is>
       </c>
       <c r="E201" s="21" t="inlineStr">
@@ -18362,7 +18362,7 @@
       </c>
       <c r="D212" s="20" t="inlineStr">
         <is>
-          <t>*maa://20955 (79.49)</t>
+          <t>*maa://20955 (80.0)</t>
         </is>
       </c>
       <c r="E212" s="21" t="inlineStr">
@@ -18416,7 +18416,7 @@
       </c>
       <c r="D213" s="20" t="inlineStr">
         <is>
-          <t>maa://39238 (99.49)</t>
+          <t>maa://39238 (99.5)</t>
         </is>
       </c>
       <c r="E213" s="21" t="inlineStr">
@@ -19172,7 +19172,7 @@
       </c>
       <c r="D227" s="20" t="inlineStr">
         <is>
-          <t>maa://20987 (93.62), *maa://35801 (77.78)</t>
+          <t>maa://20987 (93.68), *maa://35801 (77.78)</t>
         </is>
       </c>
       <c r="E227" s="21" t="inlineStr">
@@ -19226,7 +19226,7 @@
       </c>
       <c r="D228" s="20" t="inlineStr">
         <is>
-          <t>*maa://29644 (73.91), maa://39159 (96.55), ***maa://30061 (30.0)</t>
+          <t>*maa://29644 (74.47), maa://39159 (96.55), ***maa://30061 (30.0)</t>
         </is>
       </c>
       <c r="E228" s="21" t="inlineStr">
@@ -19442,7 +19442,7 @@
       </c>
       <c r="D232" s="20" t="inlineStr">
         <is>
-          <t>*maa://48263 (77.78)</t>
+          <t>*maa://48263 (73.68)</t>
         </is>
       </c>
       <c r="E232" s="21" t="inlineStr">
@@ -19874,7 +19874,7 @@
       </c>
       <c r="D240" s="20" t="inlineStr">
         <is>
-          <t>*maa://30667 (78.68), maa://30666 (83.41), **maa://30739 (43.24), *maa://30723 (56.45), maa://39588 (88.89)</t>
+          <t>*maa://30667 (78.68), maa://30666 (83.48), **maa://30739 (43.24), *maa://30723 (56.45), maa://39588 (88.89)</t>
         </is>
       </c>
       <c r="E240" s="21" t="inlineStr">
@@ -20306,7 +20306,7 @@
       </c>
       <c r="D248" s="20" t="inlineStr">
         <is>
-          <t>maa://28923 (92.19), maa://28906 (98.28), ***maa://28825 (11.54)</t>
+          <t>maa://28923 (92.23), maa://28906 (98.28), ***maa://28825 (11.54)</t>
         </is>
       </c>
       <c r="E248" s="21" t="inlineStr">
@@ -20522,7 +20522,7 @@
       </c>
       <c r="D252" s="20" t="inlineStr">
         <is>
-          <t>maa://24093 (100.0), maa://31559 (94.44), maa://20924 (95.24), **maa://49440 (50.0)</t>
+          <t>maa://24093 (100.0), maa://31559 (94.59), maa://20924 (95.24), **maa://49440 (50.0)</t>
         </is>
       </c>
       <c r="E252" s="21" t="inlineStr">
@@ -21602,7 +21602,7 @@
       </c>
       <c r="D272" s="20" t="inlineStr">
         <is>
-          <t>maa://51881 (99.19), maa://51630 (96.59), maa://56588 (94.44), *maa://55171 (57.14), maa://51893 (88.89)</t>
+          <t>maa://51881 (99.2), maa://51630 (96.59), maa://56588 (94.44), *maa://55171 (57.14), maa://51893 (88.89)</t>
         </is>
       </c>
       <c r="E272" s="21" t="inlineStr">
@@ -22358,7 +22358,7 @@
       </c>
       <c r="D286" s="20" t="inlineStr">
         <is>
-          <t>maa://20899 (89.41), maa://46332 (94.74), ***maa://44744 (25.0)</t>
+          <t>maa://20899 (89.41), maa://46332 (95.0), ***maa://44744 (25.0)</t>
         </is>
       </c>
       <c r="E286" s="21" t="inlineStr">
@@ -22520,7 +22520,7 @@
       </c>
       <c r="D289" s="20" t="inlineStr">
         <is>
-          <t>maa://30710 (97.87), maa://36845 (95.62), maa://31558 (97.14), **maa://39217 (41.18), maa://30668 (86.67)</t>
+          <t>maa://30710 (97.87), maa://36845 (95.65), maa://31558 (97.14), **maa://39217 (41.18), maa://30668 (86.67)</t>
         </is>
       </c>
       <c r="E289" s="21" t="inlineStr">
@@ -22790,7 +22790,7 @@
       </c>
       <c r="D294" s="20" t="inlineStr">
         <is>
-          <t>maa://32414 (98.78), maa://32505 (100.0), maa://39155 (97.44)</t>
+          <t>maa://32414 (98.79), maa://32505 (100.0), maa://39155 (97.44)</t>
         </is>
       </c>
       <c r="E294" s="21" t="inlineStr">
@@ -23276,7 +23276,7 @@
       </c>
       <c r="D303" s="20" t="inlineStr">
         <is>
-          <t>maa://50280 (97.58), maa://49642 (96.88), maa://49660 (92.86), *maa://50517 (80.0)</t>
+          <t>maa://50280 (97.61), maa://49642 (96.88), maa://49660 (92.86), *maa://50517 (80.0)</t>
         </is>
       </c>
       <c r="E303" s="21" t="inlineStr">
@@ -24626,7 +24626,7 @@
       </c>
       <c r="D328" s="20" t="inlineStr">
         <is>
-          <t>maa://40956 (93.59)</t>
+          <t>maa://40956 (93.67)</t>
         </is>
       </c>
       <c r="E328" s="21" t="inlineStr">
@@ -24842,7 +24842,7 @@
       </c>
       <c r="D332" s="22" t="inlineStr">
         <is>
-          <t>maa://44234 (99.05)</t>
+          <t>maa://44234 (99.06)</t>
         </is>
       </c>
       <c r="E332" s="22" t="inlineStr">
@@ -24950,7 +24950,7 @@
       </c>
       <c r="D334" s="22" t="inlineStr">
         <is>
-          <t>*maa://40162 (66.67)</t>
+          <t>*maa://40162 (71.43)</t>
         </is>
       </c>
       <c r="E334" s="22" t="inlineStr">
@@ -25868,7 +25868,7 @@
       </c>
       <c r="D351" s="17" t="inlineStr">
         <is>
-          <t>maa://36868 (100.0), maa://35996 (97.67), **maa://39217 (41.18), maa://47349 (94.29)</t>
+          <t>maa://36868 (100.0), maa://35996 (97.7), **maa://39217 (41.18), maa://47349 (94.29)</t>
         </is>
       </c>
       <c r="E351" s="17" t="inlineStr">
@@ -25922,7 +25922,7 @@
       </c>
       <c r="D352" s="17" t="inlineStr">
         <is>
-          <t>maa://49696 (99.55), maa://49695 (100.0), maa://49758 (98.44), *maa://59402 (70.0), *maa://52357 (71.43)</t>
+          <t>maa://49696 (99.55), maa://49695 (100.0), maa://49758 (98.44), *maa://59402 (66.67), *maa://52357 (75.0)</t>
         </is>
       </c>
       <c r="E352" s="17" t="inlineStr">
@@ -26138,7 +26138,7 @@
       </c>
       <c r="D356" s="17" t="inlineStr">
         <is>
-          <t>maa://36646 (98.8), maa://36845 (95.62), **maa://39217 (41.18), maa://51007 (98.18)</t>
+          <t>maa://36646 (98.8), maa://36845 (95.65), **maa://39217 (41.18), maa://51007 (98.18)</t>
         </is>
       </c>
       <c r="E356" s="17" t="inlineStr">
@@ -26403,12 +26403,12 @@
       </c>
       <c r="C361" s="19" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D361" s="17" t="inlineStr">
         <is>
-          <t>maa://40957 (93.44), maa://44635 (87.74), maa://48026 (96.47), maa://41035 (92.42), maa://44660 (92.31), maa://41128 (83.78)</t>
+          <t>maa://40957 (93.6), maa://44635 (87.85), maa://48026 (95.65), maa://41035 (92.42), maa://44660 (92.31), maa://41128 (83.78), maa://60251 (100.0)</t>
         </is>
       </c>
       <c r="E361" s="17" t="inlineStr">
@@ -27272,7 +27272,7 @@
       </c>
       <c r="D377" s="17" t="inlineStr">
         <is>
-          <t>maa://42970 (83.27), maa://44745 (98.21), **maa://49516 (40.0), *maa://45952 (80.0), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
+          <t>maa://42970 (83.33), maa://44745 (98.23), **maa://49516 (40.0), *maa://45952 (80.0), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E377" s="17" t="inlineStr">
@@ -27974,7 +27974,7 @@
       </c>
       <c r="D390" s="17" t="inlineStr">
         <is>
-          <t>maa://51880 (99.22), maa://51878 (100.0), maa://56651 (100.0)</t>
+          <t>maa://51880 (99.23), maa://51878 (100.0), maa://56651 (100.0)</t>
         </is>
       </c>
       <c r="E390" s="17" t="inlineStr">
@@ -28028,7 +28028,7 @@
       </c>
       <c r="D391" s="17" t="inlineStr">
         <is>
-          <t>maa://51872 (96.73), maa://51876 (98.8), maa://51873 (100.0)</t>
+          <t>maa://51872 (96.75), maa://51876 (98.81), maa://51873 (100.0)</t>
         </is>
       </c>
       <c r="E391" s="17" t="inlineStr">
@@ -28077,12 +28077,12 @@
       </c>
       <c r="C392" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D392" s="17" t="inlineStr">
         <is>
-          <t>maa://59493 (97.2), maa://59603 (100.0)</t>
+          <t>maa://59493 (96.49), maa://59603 (100.0), maa://60449 (100.0)</t>
         </is>
       </c>
       <c r="E392" s="17" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#202)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -87,7 +87,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -167,6 +167,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -703,7 +706,7 @@
       </c>
       <c r="D2" s="14" t="inlineStr">
         <is>
-          <t>maa://25390 (95.48), maa://24702 (94.84), maa://36681 (86.42)</t>
+          <t>maa://25390 (95.52), maa://24702 (94.87), maa://36681 (86.42)</t>
         </is>
       </c>
       <c r="E2" s="11" t="n"/>
@@ -735,7 +738,7 @@
       </c>
       <c r="L2" s="14" t="inlineStr">
         <is>
-          <t>maa://39402 (94.96), *maa://34787 (73.91), *maa://58660 (80.0)</t>
+          <t>maa://39402 (95.0), *maa://34787 (73.91), maa://58660 (83.33)</t>
         </is>
       </c>
       <c r="M2" s="11" t="n"/>
@@ -767,7 +770,7 @@
       </c>
       <c r="T2" s="14" t="inlineStr">
         <is>
-          <t>maa://22742 (91.71)</t>
+          <t>maa://22742 (91.74)</t>
         </is>
       </c>
       <c r="U2" s="11" t="n"/>
@@ -799,7 +802,7 @@
       </c>
       <c r="AB2" s="14" t="inlineStr">
         <is>
-          <t>maa://21246 (91.48), maa://36684 (93.21)</t>
+          <t>maa://21246 (91.48), maa://36684 (93.25)</t>
         </is>
       </c>
       <c r="AC2" s="11" t="n"/>
@@ -815,7 +818,7 @@
       </c>
       <c r="AF2" s="14" t="inlineStr">
         <is>
-          <t>maa://25251 (91.91), maa://59087 (100.0)</t>
+          <t>maa://25251 (91.91), maa://59087 (92.31)</t>
         </is>
       </c>
       <c r="AG2" s="27" t="n"/>
@@ -865,7 +868,7 @@
       </c>
       <c r="L3" s="14" t="inlineStr">
         <is>
-          <t>*maa://22880 (66.38), maa://20276 (88.63), *maa://22749 (77.78)</t>
+          <t>*maa://22880 (66.1), maa://20276 (88.68), *maa://22749 (77.78)</t>
         </is>
       </c>
       <c r="M3" s="11" t="n"/>
@@ -881,7 +884,7 @@
       </c>
       <c r="P3" s="14" t="inlineStr">
         <is>
-          <t>maa://21249 (94.77), maa://26254 (97.22)</t>
+          <t>maa://21249 (94.77), maa://26254 (97.3)</t>
         </is>
       </c>
       <c r="Q3" s="11" t="n"/>
@@ -892,12 +895,12 @@
       </c>
       <c r="S3" s="11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="T3" s="14" t="inlineStr">
         <is>
-          <t>maa://24617 (91.18), maa://45854 (83.84)</t>
+          <t>maa://24617 (91.18), maa://45854 (83.0), maa://60545 (100.0)</t>
         </is>
       </c>
       <c r="U3" s="11" t="n"/>
@@ -929,7 +932,7 @@
       </c>
       <c r="AB3" s="14" t="inlineStr">
         <is>
-          <t>maa://24390 (95.7), maa://52241 (100.0)</t>
+          <t>maa://24390 (95.7), maa://52241 (91.67)</t>
         </is>
       </c>
       <c r="AC3" s="11" t="n"/>
@@ -1011,7 +1014,7 @@
       </c>
       <c r="P4" s="14" t="inlineStr">
         <is>
-          <t>maa://49983 (96.1), maa://50121 (95.12)</t>
+          <t>maa://49983 (96.2), maa://50121 (95.12)</t>
         </is>
       </c>
       <c r="Q4" s="11" t="n"/>
@@ -1027,7 +1030,7 @@
       </c>
       <c r="T4" s="14" t="inlineStr">
         <is>
-          <t>maa://32509 (94.03), maa://27295 (88.42), maa://22754 (89.19), *maa://31008 (79.55)</t>
+          <t>maa://32509 (94.03), maa://27295 (88.54), maa://22754 (89.19), *maa://31008 (79.55)</t>
         </is>
       </c>
       <c r="U4" s="11" t="n"/>
@@ -1043,7 +1046,7 @@
       </c>
       <c r="X4" s="14" t="inlineStr">
         <is>
-          <t>maa://43217 (93.98)</t>
+          <t>maa://43217 (94.03)</t>
         </is>
       </c>
       <c r="Y4" s="11" t="n"/>
@@ -1098,7 +1101,7 @@
       </c>
       <c r="D5" s="14" t="inlineStr">
         <is>
-          <t>maa://21245 (84.67), maa://22744 (82.14), maa://54105 (100.0)</t>
+          <t>maa://21245 (84.43), maa://22744 (82.14), maa://54105 (100.0)</t>
         </is>
       </c>
       <c r="E5" s="11" t="n"/>
@@ -1390,7 +1393,7 @@
       </c>
       <c r="L7" s="14" t="inlineStr">
         <is>
-          <t>maa://28624 (93.96), maa://24957 (97.78)</t>
+          <t>maa://28624 (94.04), maa://24957 (97.78)</t>
         </is>
       </c>
       <c r="M7" s="11" t="n"/>
@@ -1438,7 +1441,7 @@
       </c>
       <c r="X7" s="14" t="inlineStr">
         <is>
-          <t>maa://22399 (96.2), *maa://22758 (77.5)</t>
+          <t>maa://22399 (96.22), *maa://22758 (77.5)</t>
         </is>
       </c>
       <c r="Y7" s="11" t="n"/>
@@ -1478,7 +1481,7 @@
     <row r="8">
       <c r="A8" s="10" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.21 13:21:26</t>
+          <t>更新日期：2025.06.23 13:23:39</t>
         </is>
       </c>
       <c r="B8" s="11" t="inlineStr">
@@ -1541,7 +1544,7 @@
       </c>
       <c r="P8" s="14" t="inlineStr">
         <is>
-          <t>maa://32931 (83.92), maa://23252 (91.67), maa://37496 (97.5)</t>
+          <t>maa://32931 (83.92), maa://23252 (91.67), maa://37496 (97.56)</t>
         </is>
       </c>
       <c r="Q8" s="11" t="n"/>
@@ -1573,7 +1576,7 @@
       </c>
       <c r="X8" s="14" t="inlineStr">
         <is>
-          <t>maa://21411 (95.89)</t>
+          <t>maa://21411 (95.69)</t>
         </is>
       </c>
       <c r="Y8" s="11" t="n"/>
@@ -1719,7 +1722,7 @@
       </c>
       <c r="AB9" s="14" t="inlineStr">
         <is>
-          <t>maa://28711 (87.41), maa://40166 (93.88)</t>
+          <t>maa://28711 (87.5), maa://40166 (93.88)</t>
         </is>
       </c>
       <c r="AC9" s="11" t="n"/>
@@ -1735,7 +1738,7 @@
       </c>
       <c r="AF9" s="14" t="inlineStr">
         <is>
-          <t>maa://26206 (89.33), *maa://22865 (53.57)</t>
+          <t>maa://26206 (89.33), *maa://22865 (52.63)</t>
         </is>
       </c>
       <c r="AG9" s="27" t="n"/>
@@ -1753,7 +1756,7 @@
       </c>
       <c r="D10" s="14" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.54), ***maa://39951 (11.69), ***maa://34206 (22.22), *maa://45271 (62.2), ***maa://39243 (25.0), **maa://54000 (33.33)</t>
+          <t>***maa://25695 (18.54), ***maa://39951 (11.69), ***maa://34206 (22.22), *maa://45271 (62.2), ***maa://39243 (25.0), **maa://54000 (50.0)</t>
         </is>
       </c>
       <c r="E10" s="11" t="n"/>
@@ -1817,7 +1820,7 @@
       </c>
       <c r="T10" s="14" t="inlineStr">
         <is>
-          <t>maa://27395 (96.8), maa://22755 (89.23)</t>
+          <t>maa://27395 (96.81), maa://22755 (89.31)</t>
         </is>
       </c>
       <c r="U10" s="11" t="n"/>
@@ -1833,7 +1836,7 @@
       </c>
       <c r="X10" s="14" t="inlineStr">
         <is>
-          <t>maa://22301 (97.93), maa://45828 (93.48), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.93), maa://45828 (93.75), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="11" t="n"/>
@@ -1883,7 +1886,7 @@
       </c>
       <c r="D11" s="14" t="inlineStr">
         <is>
-          <t>maa://36707 (99.39)</t>
+          <t>maa://36707 (99.4)</t>
         </is>
       </c>
       <c r="E11" s="11" t="n"/>
@@ -1947,7 +1950,7 @@
       </c>
       <c r="T11" s="14" t="inlineStr">
         <is>
-          <t>maa://22747 (90.45), maa://22501 (98.25), maa://45521 (91.67)</t>
+          <t>maa://22747 (90.45), maa://22501 (98.26), maa://45521 (91.67)</t>
         </is>
       </c>
       <c r="U11" s="11" t="n"/>
@@ -1979,7 +1982,7 @@
       </c>
       <c r="AB11" s="14" t="inlineStr">
         <is>
-          <t>maa://29912 (97.85), maa://22516 (87.36)</t>
+          <t>maa://29912 (97.87), maa://22516 (87.36)</t>
         </is>
       </c>
       <c r="AC11" s="11" t="n"/>
@@ -2093,7 +2096,7 @@
       </c>
       <c r="X12" s="14" t="inlineStr">
         <is>
-          <t>maa://22753 (91.98), *maa://21485 (76.0), maa://37962 (92.96)</t>
+          <t>maa://22753 (92.02), *maa://21485 (76.0), maa://37962 (92.96)</t>
         </is>
       </c>
       <c r="Y12" s="11" t="n"/>
@@ -2109,7 +2112,7 @@
       </c>
       <c r="AB12" s="14" t="inlineStr">
         <is>
-          <t>maa://23669 (95.68), maa://36677 (95.4), maa://39872 (93.1)</t>
+          <t>maa://23669 (95.68), maa://36677 (95.45), maa://39872 (93.1)</t>
         </is>
       </c>
       <c r="AC12" s="11" t="n"/>
@@ -2159,7 +2162,7 @@
       </c>
       <c r="H13" s="14" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.11), **maa://22728 (46.94)</t>
+          <t>*maa://21248 (74.2), **maa://22728 (46.94)</t>
         </is>
       </c>
       <c r="I13" s="11" t="n"/>
@@ -2223,7 +2226,7 @@
       </c>
       <c r="X13" s="14" t="inlineStr">
         <is>
-          <t>maa://34957 (84.07), **maa://22768 (50.0)</t>
+          <t>maa://34957 (84.21), **maa://22768 (50.0)</t>
         </is>
       </c>
       <c r="Y13" s="11" t="n"/>
@@ -2305,7 +2308,7 @@
       </c>
       <c r="L14" s="14" t="inlineStr">
         <is>
-          <t>maa://39841 (94.51), maa://26245 (96.74), maa://21288 (96.3), maa://36682 (96.0)</t>
+          <t>maa://39841 (94.51), maa://26245 (96.74), maa://21288 (96.3), maa://36682 (96.08)</t>
         </is>
       </c>
       <c r="M14" s="11" t="n"/>
@@ -2337,7 +2340,7 @@
       </c>
       <c r="T14" s="14" t="inlineStr">
         <is>
-          <t>maa://22521 (94.92), maa://42751 (100.0)</t>
+          <t>maa://22521 (94.92), maa://42751 (96.0)</t>
         </is>
       </c>
       <c r="U14" s="11" t="n"/>
@@ -2369,7 +2372,7 @@
       </c>
       <c r="AB14" s="14" t="inlineStr">
         <is>
-          <t>maa://22764 (96.43)</t>
+          <t>maa://22764 (96.47)</t>
         </is>
       </c>
       <c r="AC14" s="11" t="n"/>
@@ -2403,7 +2406,7 @@
       </c>
       <c r="D15" s="14" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.69), maa://22734 (84.55), *maa://30808 (65.28), *maa://36048 (69.64), maa://45058 (85.0)</t>
+          <t>*maa://22743 (78.78), maa://22734 (84.55), *maa://30808 (64.38), *maa://36048 (69.91), maa://45058 (85.0)</t>
         </is>
       </c>
       <c r="E15" s="11" t="n"/>
@@ -2451,7 +2454,7 @@
       </c>
       <c r="P15" s="14" t="inlineStr">
         <is>
-          <t>maa://24762 (91.44), *maa://22727 (70.0)</t>
+          <t>maa://24762 (91.53), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="11" t="n"/>
@@ -2515,7 +2518,7 @@
       </c>
       <c r="AF15" s="14" t="inlineStr">
         <is>
-          <t>maa://21364 (81.4), maa://36666 (82.21), *maa://22766 (68.55)</t>
+          <t>maa://21364 (81.45), maa://36666 (82.21), *maa://22766 (68.55)</t>
         </is>
       </c>
       <c r="AG15" s="27" t="n"/>
@@ -2533,7 +2536,7 @@
       </c>
       <c r="D16" s="14" t="inlineStr">
         <is>
-          <t>maa://21441 (96.54), maa://37650 (96.49), maa://36679 (94.55)</t>
+          <t>maa://21441 (96.54), maa://37650 (96.55), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="11" t="n"/>
@@ -2597,7 +2600,7 @@
       </c>
       <c r="T16" s="14" t="inlineStr">
         <is>
-          <t>maa://22729 (94.51), *maa://28648 (74.07), maa://36674 (80.65)</t>
+          <t>maa://22729 (94.54), *maa://28648 (74.39), maa://36674 (80.65)</t>
         </is>
       </c>
       <c r="U16" s="11" t="n"/>
@@ -2679,7 +2682,7 @@
       </c>
       <c r="H17" s="14" t="inlineStr">
         <is>
-          <t>maa://22430 (89.72), maa://39599 (86.9)</t>
+          <t>maa://22430 (89.77), maa://39599 (86.9)</t>
         </is>
       </c>
       <c r="I17" s="11" t="n"/>
@@ -2711,7 +2714,7 @@
       </c>
       <c r="P17" s="14" t="inlineStr">
         <is>
-          <t>maa://23890 (81.08), maa://56238 (100.0)</t>
+          <t>maa://23890 (81.25), maa://56238 (100.0)</t>
         </is>
       </c>
       <c r="Q17" s="11" t="n"/>
@@ -2793,7 +2796,7 @@
       </c>
       <c r="D18" s="14" t="inlineStr">
         <is>
-          <t>maa://24570 (97.1)</t>
+          <t>maa://24570 (97.11)</t>
         </is>
       </c>
       <c r="E18" s="11" t="n"/>
@@ -2809,7 +2812,7 @@
       </c>
       <c r="H18" s="14" t="inlineStr">
         <is>
-          <t>maa://24421 (86.93)</t>
+          <t>maa://24421 (86.97)</t>
         </is>
       </c>
       <c r="I18" s="11" t="n"/>
@@ -2825,7 +2828,7 @@
       </c>
       <c r="L18" s="14" t="inlineStr">
         <is>
-          <t>maa://22466 (92.2), maa://52226 (95.83)</t>
+          <t>maa://22466 (92.23), maa://52226 (95.83)</t>
         </is>
       </c>
       <c r="M18" s="11" t="n"/>
@@ -2889,7 +2892,7 @@
       </c>
       <c r="AB18" s="14" t="inlineStr">
         <is>
-          <t>maa://24393 (98.21)</t>
+          <t>maa://24393 (98.25)</t>
         </is>
       </c>
       <c r="AC18" s="11" t="n"/>
@@ -2905,7 +2908,7 @@
       </c>
       <c r="AF18" s="14" t="inlineStr">
         <is>
-          <t>*maa://24313 (59.88), **maa://29784 (50.0), maa://47854 (81.25)</t>
+          <t>*maa://24313 (60.12), **maa://29784 (50.0), maa://47854 (82.35)</t>
         </is>
       </c>
       <c r="AG18" s="27" t="n"/>
@@ -3053,7 +3056,7 @@
       </c>
       <c r="D20" s="14" t="inlineStr">
         <is>
-          <t>maa://21432 (90.78), maa://25198 (93.89), maa://36680 (91.18)</t>
+          <t>maa://21432 (90.82), maa://25198 (93.94), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="11" t="n"/>
@@ -3069,7 +3072,7 @@
       </c>
       <c r="H20" s="14" t="inlineStr">
         <is>
-          <t>maa://22864 (90.43)</t>
+          <t>maa://22864 (90.48)</t>
         </is>
       </c>
       <c r="I20" s="11" t="n"/>
@@ -3133,7 +3136,7 @@
       </c>
       <c r="X20" s="14" t="inlineStr">
         <is>
-          <t>maa://50085 (88.59), maa://49976 (86.75), maa://56241 (88.89)</t>
+          <t>maa://50085 (88.74), maa://49976 (86.75), maa://56241 (88.89)</t>
         </is>
       </c>
       <c r="Y20" s="11" t="n"/>
@@ -3279,7 +3282,7 @@
       </c>
       <c r="AB21" s="14" t="inlineStr">
         <is>
-          <t>maa://21443 (82.85)</t>
+          <t>maa://21443 (82.93)</t>
         </is>
       </c>
       <c r="AC21" s="11" t="n"/>
@@ -3295,7 +3298,7 @@
       </c>
       <c r="AF21" s="14" t="inlineStr">
         <is>
-          <t>maa://22524 (88.49), maa://22432 (83.33)</t>
+          <t>maa://22524 (88.14), maa://22432 (83.58)</t>
         </is>
       </c>
       <c r="AG21" s="27" t="n"/>
@@ -3329,7 +3332,7 @@
       </c>
       <c r="H22" s="14" t="inlineStr">
         <is>
-          <t>maa://25236 (96.3)</t>
+          <t>maa://25236 (96.33)</t>
         </is>
       </c>
       <c r="I22" s="11" t="n"/>
@@ -3345,7 +3348,7 @@
       </c>
       <c r="L22" s="14" t="inlineStr">
         <is>
-          <t>*maa://27127 (77.61), *maa://22751 (70.67)</t>
+          <t>*maa://27127 (77.78), *maa://22751 (70.67)</t>
         </is>
       </c>
       <c r="M22" s="11" t="n"/>
@@ -3443,7 +3446,7 @@
       </c>
       <c r="D23" s="14" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.4), **maa://41753 (50.0)</t>
+          <t>***maa://28036 (28.4), **maa://41753 (48.28)</t>
         </is>
       </c>
       <c r="E23" s="11" t="n"/>
@@ -3475,7 +3478,7 @@
       </c>
       <c r="L23" s="14" t="inlineStr">
         <is>
-          <t>maa://39756 (95.8), maa://39875 (94.94)</t>
+          <t>maa://39756 (95.63), maa://39875 (93.75)</t>
         </is>
       </c>
       <c r="M23" s="11" t="n"/>
@@ -3523,7 +3526,7 @@
       </c>
       <c r="X23" s="14" t="inlineStr">
         <is>
-          <t>*maa://28503 (63.92)</t>
+          <t>*maa://28503 (63.64)</t>
         </is>
       </c>
       <c r="Y23" s="11" t="n"/>
@@ -3653,7 +3656,7 @@
       </c>
       <c r="X24" s="14" t="inlineStr">
         <is>
-          <t>maa://29988 (84.97), maa://23504 (93.74), *maa://25141 (77.37), *maa://36663 (78.0), maa://52227 (100.0)</t>
+          <t>maa://29988 (84.97), maa://23504 (93.75), *maa://25141 (77.37), *maa://36663 (78.0), maa://52227 (95.24)</t>
         </is>
       </c>
       <c r="Y24" s="11" t="n"/>
@@ -3767,7 +3770,7 @@
       </c>
       <c r="T25" s="14" t="inlineStr">
         <is>
-          <t>maa://20109 (92.63), maa://22545 (100.0), *maa://42915 (75.0)</t>
+          <t>maa://20109 (92.67), maa://22545 (100.0), *maa://42915 (75.0)</t>
         </is>
       </c>
       <c r="U25" s="11" t="n"/>
@@ -3799,7 +3802,7 @@
       </c>
       <c r="AB25" s="14" t="inlineStr">
         <is>
-          <t>maa://31215 (89.8), *maa://24516 (79.57), maa://26001 (84.75)</t>
+          <t>maa://31215 (89.86), *maa://24516 (79.57), maa://26001 (84.75)</t>
         </is>
       </c>
       <c r="AC25" s="11" t="n"/>
@@ -3815,7 +3818,7 @@
       </c>
       <c r="AF25" s="14" t="inlineStr">
         <is>
-          <t>maa://20108 (95.95), maa://24621 (97.18), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (80.0)</t>
+          <t>maa://20108 (95.95), maa://24621 (97.2), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (80.0)</t>
         </is>
       </c>
       <c r="AG25" s="27" t="n"/>
@@ -3929,7 +3932,7 @@
       </c>
       <c r="AB26" s="14" t="inlineStr">
         <is>
-          <t>maa://42235 (96.13)</t>
+          <t>maa://42235 (96.15)</t>
         </is>
       </c>
       <c r="AC26" s="11" t="n"/>
@@ -3945,7 +3948,7 @@
       </c>
       <c r="AF26" s="14" t="inlineStr">
         <is>
-          <t>*maa://30511 (75.47), *maa://29760 (52.94)</t>
+          <t>*maa://30511 (74.07), **maa://29760 (50.0)</t>
         </is>
       </c>
       <c r="AG26" s="27" t="n"/>
@@ -4075,7 +4078,7 @@
       </c>
       <c r="AF27" s="14" t="inlineStr">
         <is>
-          <t>maa://24023 (96.2)</t>
+          <t>maa://24023 (96.25)</t>
         </is>
       </c>
       <c r="AG27" s="27" t="n"/>
@@ -4093,7 +4096,7 @@
       </c>
       <c r="D28" s="14" t="inlineStr">
         <is>
-          <t>maa://24465 (90.68), maa://25725 (82.83)</t>
+          <t>maa://24465 (90.71), maa://25725 (82.83)</t>
         </is>
       </c>
       <c r="E28" s="11" t="n"/>
@@ -4173,7 +4176,7 @@
       </c>
       <c r="X28" s="14" t="inlineStr">
         <is>
-          <t>maa://39929 (91.98), maa://41749 (92.31)</t>
+          <t>maa://39929 (92.0), maa://41749 (92.36)</t>
         </is>
       </c>
       <c r="Y28" s="11" t="n"/>
@@ -4205,7 +4208,7 @@
       </c>
       <c r="AF28" s="14" t="inlineStr">
         <is>
-          <t>maa://36660 (92.61)</t>
+          <t>maa://36660 (92.64)</t>
         </is>
       </c>
       <c r="AG28" s="27" t="n"/>
@@ -4223,7 +4226,7 @@
       </c>
       <c r="D29" s="14" t="inlineStr">
         <is>
-          <t>maa://31694 (98.39)</t>
+          <t>maa://31694 (98.41)</t>
         </is>
       </c>
       <c r="E29" s="11" t="n"/>
@@ -4255,7 +4258,7 @@
       </c>
       <c r="L29" s="14" t="inlineStr">
         <is>
-          <t>maa://28432 (94.07), maa://31400 (98.9), maa://28440 (84.4), *maa://28650 (71.43)</t>
+          <t>maa://28432 (94.12), maa://31400 (98.9), maa://28440 (84.51), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="11" t="n"/>
@@ -4449,7 +4452,7 @@
       </c>
       <c r="AB30" s="14" t="inlineStr">
         <is>
-          <t>maa://42979 (97.13), maa://45822 (100.0), maa://45045 (83.33)</t>
+          <t>maa://42979 (97.15), maa://45822 (100.0), maa://45045 (83.33)</t>
         </is>
       </c>
       <c r="AC30" s="11" t="n"/>
@@ -4515,7 +4518,7 @@
       </c>
       <c r="L31" s="14" t="inlineStr">
         <is>
-          <t>maa://35926 (93.79), maa://36258 (88.17), *maa://43904 (73.33)</t>
+          <t>maa://35926 (93.79), maa://36258 (88.24), *maa://43904 (73.33)</t>
         </is>
       </c>
       <c r="M31" s="11" t="n"/>
@@ -4629,7 +4632,7 @@
       </c>
       <c r="H32" s="14" t="inlineStr">
         <is>
-          <t>maa://21895 (97.67), maa://36667 (97.32), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.67), maa://36667 (97.35), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="11" t="n"/>
@@ -4677,7 +4680,7 @@
       </c>
       <c r="T32" s="14" t="inlineStr">
         <is>
-          <t>maa://42859 (97.03), maa://41108 (86.27), maa://41238 (98.03), maa://45523 (100.0)</t>
+          <t>maa://42859 (97.06), maa://41108 (86.27), maa://41238 (98.04), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="11" t="n"/>
@@ -4791,7 +4794,7 @@
       </c>
       <c r="P33" s="14" t="inlineStr">
         <is>
-          <t>maa://21956 (81.71), *maa://22730 (71.88)</t>
+          <t>maa://21956 (81.33), *maa://22730 (71.88)</t>
         </is>
       </c>
       <c r="Q33" s="11" t="n"/>
@@ -4921,7 +4924,7 @@
       </c>
       <c r="P34" s="14" t="inlineStr">
         <is>
-          <t>maa://48817 (96.92), maa://56235 (100.0)</t>
+          <t>maa://48817 (97.01), maa://56235 (100.0)</t>
         </is>
       </c>
       <c r="Q34" s="11" t="n"/>
@@ -4937,7 +4940,7 @@
       </c>
       <c r="T34" s="14" t="inlineStr">
         <is>
-          <t>maa://24526 (92.42)</t>
+          <t>maa://24526 (92.45)</t>
         </is>
       </c>
       <c r="U34" s="11" t="n"/>
@@ -5035,7 +5038,7 @@
       </c>
       <c r="L35" s="14" t="inlineStr">
         <is>
-          <t>maa://41296 (97.42)</t>
+          <t>maa://41296 (97.44)</t>
         </is>
       </c>
       <c r="M35" s="11" t="n"/>
@@ -5279,7 +5282,7 @@
       </c>
       <c r="L37" s="14" t="inlineStr">
         <is>
-          <t>maa://45718 (98.46), maa://47069 (81.82), maa://56336 (90.0), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.48), maa://47069 (81.82), maa://56336 (90.0), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="11" t="n"/>
@@ -5295,7 +5298,7 @@
       </c>
       <c r="P37" s="14" t="inlineStr">
         <is>
-          <t>maa://21280 (89.66), *maa://21239 (71.43)</t>
+          <t>maa://21280 (89.7), *maa://21239 (71.43)</t>
         </is>
       </c>
       <c r="Q37" s="11" t="n"/>
@@ -5444,7 +5447,7 @@
       </c>
       <c r="AF38" s="14" t="inlineStr">
         <is>
-          <t>maa://36697 (89.2)</t>
+          <t>maa://36697 (89.23)</t>
         </is>
       </c>
       <c r="AG38" s="27" t="n"/>
@@ -5465,7 +5468,7 @@
       </c>
       <c r="H39" s="14" t="inlineStr">
         <is>
-          <t>maa://36670 (89.66), maa://25199 (85.34), maa://30434 (93.23), *maa://45059 (79.41)</t>
+          <t>maa://36670 (88.89), maa://25199 (85.47), maa://30434 (93.38), *maa://45059 (77.14)</t>
         </is>
       </c>
       <c r="I39" s="11" t="n"/>
@@ -5513,7 +5516,7 @@
       </c>
       <c r="T39" s="14" t="inlineStr">
         <is>
-          <t>maa://47079 (95.05), *maa://45788 (71.9), maa://45790 (82.76)</t>
+          <t>maa://47079 (95.15), *maa://45788 (71.9), maa://45790 (82.76)</t>
         </is>
       </c>
       <c r="U39" s="11" t="n"/>
@@ -5837,7 +5840,7 @@
       </c>
       <c r="H43" s="14" t="inlineStr">
         <is>
-          <t>maa://22525 (84.24), maa://21284 (87.27)</t>
+          <t>maa://22525 (83.83), maa://21284 (87.27)</t>
         </is>
       </c>
       <c r="I43" s="11" t="n"/>
@@ -5991,7 +5994,7 @@
       </c>
       <c r="H45" s="14" t="inlineStr">
         <is>
-          <t>maa://21229 (84.42), maa://30807 (93.51), maa://42459 (87.5)</t>
+          <t>maa://21229 (84.58), maa://30807 (93.51), maa://42459 (87.8)</t>
         </is>
       </c>
       <c r="I45" s="11" t="n"/>
@@ -6023,7 +6026,7 @@
       </c>
       <c r="T45" s="14" t="inlineStr">
         <is>
-          <t>**maa://39364 (43.55)</t>
+          <t>**maa://39364 (42.86)</t>
         </is>
       </c>
       <c r="U45" s="11" t="n"/>
@@ -6060,7 +6063,7 @@
       </c>
       <c r="H46" s="14" t="inlineStr">
         <is>
-          <t>maa://35931 (92.76), maa://43901 (94.83)</t>
+          <t>maa://35931 (92.54), maa://43901 (95.0)</t>
         </is>
       </c>
       <c r="I46" s="11" t="n"/>
@@ -6129,7 +6132,7 @@
       </c>
       <c r="H47" s="14" t="inlineStr">
         <is>
-          <t>maa://27410 (96.88), maa://29661 (97.65), maa://28038 (84.62), maa://56236 (100.0)</t>
+          <t>maa://27410 (96.89), maa://29661 (97.65), maa://28038 (84.62), maa://56236 (100.0)</t>
         </is>
       </c>
       <c r="I47" s="11" t="n"/>
@@ -6404,7 +6407,7 @@
       </c>
       <c r="P52" s="14" t="inlineStr">
         <is>
-          <t>maa://59378 (97.14), maa://59394 (95.45)</t>
+          <t>maa://59378 (97.37), maa://59394 (96.15)</t>
         </is>
       </c>
       <c r="Q52" s="11" t="n"/>
@@ -6438,7 +6441,7 @@
       </c>
       <c r="H53" s="14" t="inlineStr">
         <is>
-          <t>maa://32534 (95.19)</t>
+          <t>maa://32534 (95.2)</t>
         </is>
       </c>
       <c r="I53" s="11" t="n"/>
@@ -6522,7 +6525,7 @@
       </c>
       <c r="H55" s="14" t="inlineStr">
         <is>
-          <t>maa://32532 (93.49)</t>
+          <t>maa://32532 (93.52)</t>
         </is>
       </c>
       <c r="I55" s="11" t="n"/>
@@ -6594,7 +6597,7 @@
       </c>
       <c r="H59" s="14" t="inlineStr">
         <is>
-          <t>maa://31270 (94.77), maa://27746 (82.91)</t>
+          <t>maa://31270 (94.81), maa://27746 (82.91)</t>
         </is>
       </c>
       <c r="I59" s="11" t="n"/>
@@ -6612,7 +6615,7 @@
       </c>
       <c r="H60" s="14" t="inlineStr">
         <is>
-          <t>*maa://40438 (75.0)</t>
+          <t>*maa://40438 (75.31)</t>
         </is>
       </c>
       <c r="I60" s="11" t="n"/>
@@ -6661,12 +6664,12 @@
       </c>
       <c r="G63" s="11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H63" s="14" t="inlineStr">
         <is>
-          <t>maa://59534 (97.83), maa://59693 (100.0), maa://59413 (100.0)</t>
+          <t>maa://59534 (98.11), maa://59413 (100.0)</t>
         </is>
       </c>
       <c r="I63" s="11" t="n"/>
@@ -6922,7 +6925,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF392"/>
+  <dimension ref="A1:AF394"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -6968,7 +6971,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A1" s="13" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.21 13:21:26</t>
+          <t>更新日期：2025.06.23 13:23:39</t>
         </is>
       </c>
       <c r="E1" s="16" t="inlineStr">
@@ -8642,7 +8645,7 @@
       </c>
       <c r="D32" s="20" t="inlineStr">
         <is>
-          <t>maa://36644 (88.42), maa://36866 (96.23), maa://45572 (91.67), maa://27794 (100.0), maa://20960 (100.0), maa://20843 (100.0), **maa://24483 (50.0), maa://20862 (83.33), *maa://20893 (77.78)</t>
+          <t>maa://36644 (88.48), maa://36866 (96.23), maa://45572 (91.67), maa://27794 (100.0), maa://20960 (100.0), maa://20843 (100.0), **maa://24483 (50.0), maa://20862 (83.33), *maa://20893 (77.78)</t>
         </is>
       </c>
       <c r="E32" s="21" t="inlineStr">
@@ -9938,7 +9941,7 @@
       </c>
       <c r="D56" s="20" t="inlineStr">
         <is>
-          <t>maa://44235 (98.22), maa://45604 (100.0), maa://20961 (100.0), maa://44220 (100.0), maa://20910 (100.0)</t>
+          <t>maa://44235 (98.24), maa://45604 (100.0), maa://20961 (100.0), maa://44220 (100.0), maa://20910 (100.0)</t>
         </is>
       </c>
       <c r="E56" s="21" t="inlineStr">
@@ -10802,7 +10805,7 @@
       </c>
       <c r="D72" s="20" t="inlineStr">
         <is>
-          <t>maa://36643 (98.25), maa://36864 (98.0), maa://39140 (100.0)</t>
+          <t>maa://36643 (98.26), maa://36864 (98.0), maa://39140 (100.0)</t>
         </is>
       </c>
       <c r="E72" s="21" t="inlineStr">
@@ -12746,7 +12749,7 @@
       </c>
       <c r="D108" s="20" t="inlineStr">
         <is>
-          <t>maa://25018 (96.66), maa://51881 (99.2), maa://25776 (92.11), maa://28361 (97.44), maa://25772 (94.12), maa://56588 (94.44), maa://45194 (87.5), maa://32653 (85.71), maa://25161 (81.25)</t>
+          <t>maa://25018 (96.66), maa://51881 (99.2), maa://25776 (92.11), maa://28361 (95.0), maa://25772 (94.12), maa://56588 (94.74), maa://45194 (82.35), maa://32653 (85.71), maa://25161 (81.25)</t>
         </is>
       </c>
       <c r="E108" s="21" t="inlineStr">
@@ -13178,7 +13181,7 @@
       </c>
       <c r="D116" s="20" t="inlineStr">
         <is>
-          <t>maa://29659 (85.29), maa://29031 (89.19)</t>
+          <t>maa://29659 (85.71), maa://29031 (89.19)</t>
         </is>
       </c>
       <c r="E116" s="21" t="inlineStr">
@@ -13502,7 +13505,7 @@
       </c>
       <c r="D122" s="20" t="inlineStr">
         <is>
-          <t>maa://29650 (98.31), maa://45570 (98.0)</t>
+          <t>maa://29650 (98.31), maa://45570 (98.04)</t>
         </is>
       </c>
       <c r="E122" s="21" t="inlineStr">
@@ -14420,7 +14423,7 @@
       </c>
       <c r="D139" s="20" t="inlineStr">
         <is>
-          <t>**maa://30679 (50.0), maa://45258 (93.33)</t>
+          <t>**maa://30679 (50.0), maa://45258 (93.75)</t>
         </is>
       </c>
       <c r="E139" s="21" t="inlineStr">
@@ -14582,7 +14585,7 @@
       </c>
       <c r="D142" s="20" t="inlineStr">
         <is>
-          <t>maa://28484 (97.1), **maa://23736 (43.28), maa://31185 (85.71), maa://30306 (100.0)</t>
+          <t>maa://28484 (97.14), **maa://23736 (44.12), maa://31185 (85.71), maa://30306 (100.0)</t>
         </is>
       </c>
       <c r="E142" s="21" t="inlineStr">
@@ -14690,7 +14693,7 @@
       </c>
       <c r="D144" s="20" t="inlineStr">
         <is>
-          <t>maa://20971 (90.0)</t>
+          <t>maa://20971 (90.91)</t>
         </is>
       </c>
       <c r="E144" s="21" t="inlineStr">
@@ -14960,7 +14963,7 @@
       </c>
       <c r="D149" s="20" t="inlineStr">
         <is>
-          <t>maa://36641 (98.44), maa://40957 (93.6), maa://36865 (96.34), maa://44635 (87.85), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
+          <t>maa://36641 (98.44), maa://40957 (93.72), maa://36865 (96.34), maa://44635 (87.85), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
         </is>
       </c>
       <c r="E149" s="21" t="inlineStr">
@@ -15932,7 +15935,7 @@
       </c>
       <c r="D167" s="20" t="inlineStr">
         <is>
-          <t>maa://29633 (92.31), maa://29627 (92.69), maa://29659 (85.29), maa://49074 (97.62), **maa://30679 (50.0), maa://29861 (100.0), maa://42343 (100.0)</t>
+          <t>maa://29633 (92.31), maa://29627 (92.69), maa://29659 (85.71), maa://49074 (97.67), **maa://30679 (50.0), maa://29861 (100.0), maa://42343 (100.0)</t>
         </is>
       </c>
       <c r="E167" s="21" t="inlineStr">
@@ -16256,7 +16259,7 @@
       </c>
       <c r="D173" s="20" t="inlineStr">
         <is>
-          <t>*maa://20905 (78.95), maa://52268 (100.0)</t>
+          <t>*maa://20905 (80.0), maa://52268 (100.0)</t>
         </is>
       </c>
       <c r="E173" s="21" t="inlineStr">
@@ -17552,7 +17555,7 @@
       </c>
       <c r="D197" s="20" t="inlineStr">
         <is>
-          <t>maa://44224 (90.27), maa://35854 (85.71), maa://50388 (97.89), maa://25760 (86.84), ***maa://43911 (13.04), *maa://20872 (52.0), maa://51066 (100.0)</t>
+          <t>maa://44224 (90.3), maa://35854 (85.87), maa://50388 (97.9), maa://25760 (86.96), ***maa://43911 (13.04), *maa://20872 (52.0), maa://51066 (100.0)</t>
         </is>
       </c>
       <c r="E197" s="21" t="inlineStr">
@@ -19442,7 +19445,7 @@
       </c>
       <c r="D232" s="20" t="inlineStr">
         <is>
-          <t>*maa://48263 (73.68)</t>
+          <t>*maa://48263 (75.0)</t>
         </is>
       </c>
       <c r="E232" s="21" t="inlineStr">
@@ -19874,7 +19877,7 @@
       </c>
       <c r="D240" s="20" t="inlineStr">
         <is>
-          <t>*maa://30667 (78.68), maa://30666 (83.48), **maa://30739 (43.24), *maa://30723 (56.45), maa://39588 (88.89)</t>
+          <t>*maa://30667 (78.68), maa://30666 (83.48), **maa://30739 (43.24), *maa://30723 (56.45), maa://39588 (89.09)</t>
         </is>
       </c>
       <c r="E240" s="21" t="inlineStr">
@@ -20252,7 +20255,7 @@
       </c>
       <c r="D247" s="20" t="inlineStr">
         <is>
-          <t>maa://30674 (88.89)</t>
+          <t>maa://30674 (90.0)</t>
         </is>
       </c>
       <c r="E247" s="21" t="inlineStr">
@@ -20306,7 +20309,7 @@
       </c>
       <c r="D248" s="20" t="inlineStr">
         <is>
-          <t>maa://28923 (92.23), maa://28906 (98.28), ***maa://28825 (11.54)</t>
+          <t>maa://28923 (92.27), maa://28906 (98.28), ***maa://28825 (11.54)</t>
         </is>
       </c>
       <c r="E248" s="21" t="inlineStr">
@@ -20360,7 +20363,7 @@
       </c>
       <c r="D249" s="20" t="inlineStr">
         <is>
-          <t>maa://42287 (90.8), maa://45570 (98.0), maa://42225 (100.0)</t>
+          <t>maa://42287 (90.8), maa://45570 (98.04), maa://42225 (100.0)</t>
         </is>
       </c>
       <c r="E249" s="21" t="inlineStr">
@@ -20468,7 +20471,7 @@
       </c>
       <c r="D251" s="20" t="inlineStr">
         <is>
-          <t>maa://20923 (92.59)</t>
+          <t>maa://20923 (92.86)</t>
         </is>
       </c>
       <c r="E251" s="21" t="inlineStr">
@@ -21386,7 +21389,7 @@
       </c>
       <c r="D268" s="20" t="inlineStr">
         <is>
-          <t>*maa://48265 (77.78)</t>
+          <t>*maa://48265 (78.95)</t>
         </is>
       </c>
       <c r="E268" s="21" t="inlineStr">
@@ -21602,7 +21605,7 @@
       </c>
       <c r="D272" s="20" t="inlineStr">
         <is>
-          <t>maa://51881 (99.2), maa://51630 (96.59), maa://56588 (94.44), *maa://55171 (57.14), maa://51893 (88.89)</t>
+          <t>maa://51881 (99.2), maa://51630 (96.59), maa://56588 (94.74), *maa://55171 (57.14), maa://51893 (88.89)</t>
         </is>
       </c>
       <c r="E272" s="21" t="inlineStr">
@@ -22520,7 +22523,7 @@
       </c>
       <c r="D289" s="20" t="inlineStr">
         <is>
-          <t>maa://30710 (97.87), maa://36845 (95.65), maa://31558 (97.14), **maa://39217 (41.18), maa://30668 (86.67)</t>
+          <t>maa://30710 (97.89), maa://36845 (95.65), maa://31558 (97.14), **maa://39217 (41.18), maa://30668 (86.67)</t>
         </is>
       </c>
       <c r="E289" s="21" t="inlineStr">
@@ -23276,7 +23279,7 @@
       </c>
       <c r="D303" s="20" t="inlineStr">
         <is>
-          <t>maa://50280 (97.61), maa://49642 (96.88), maa://49660 (92.86), *maa://50517 (80.0)</t>
+          <t>maa://50280 (97.62), maa://49642 (96.94), maa://49660 (92.86), *maa://50517 (80.0)</t>
         </is>
       </c>
       <c r="E303" s="21" t="inlineStr">
@@ -23816,7 +23819,7 @@
       </c>
       <c r="D313" s="20" t="inlineStr">
         <is>
-          <t>maa://25775 (93.75), *maa://25393 (73.33)</t>
+          <t>maa://25775 (93.83), *maa://25393 (73.33)</t>
         </is>
       </c>
       <c r="E313" s="21" t="inlineStr">
@@ -24626,7 +24629,7 @@
       </c>
       <c r="D328" s="20" t="inlineStr">
         <is>
-          <t>maa://40956 (93.67)</t>
+          <t>maa://40956 (92.86)</t>
         </is>
       </c>
       <c r="E328" s="21" t="inlineStr">
@@ -25922,7 +25925,7 @@
       </c>
       <c r="D352" s="17" t="inlineStr">
         <is>
-          <t>maa://49696 (99.55), maa://49695 (100.0), maa://49758 (98.44), *maa://59402 (66.67), *maa://52357 (75.0)</t>
+          <t>maa://49696 (99.55), maa://49695 (100.0), maa://49758 (98.44), *maa://59402 (61.54), *maa://52357 (75.0)</t>
         </is>
       </c>
       <c r="E352" s="17" t="inlineStr">
@@ -26084,7 +26087,7 @@
       </c>
       <c r="D355" s="17" t="inlineStr">
         <is>
-          <t>maa://49648 (95.56), *maa://49662 (71.43)</t>
+          <t>maa://49648 (95.74), *maa://49662 (73.33)</t>
         </is>
       </c>
       <c r="E355" s="17" t="inlineStr">
@@ -26408,7 +26411,7 @@
       </c>
       <c r="D361" s="17" t="inlineStr">
         <is>
-          <t>maa://40957 (93.6), maa://44635 (87.85), maa://48026 (95.65), maa://41035 (92.42), maa://44660 (92.31), maa://41128 (83.78), maa://60251 (100.0)</t>
+          <t>maa://40957 (93.72), maa://44635 (87.85), maa://48026 (94.74), maa://41035 (92.54), maa://44660 (92.31), maa://41128 (83.78), maa://60251 (100.0)</t>
         </is>
       </c>
       <c r="E361" s="17" t="inlineStr">
@@ -27002,7 +27005,7 @@
       </c>
       <c r="D372" s="17" t="inlineStr">
         <is>
-          <t>maa://44233 (92.31), maa://45570 (98.0)</t>
+          <t>maa://44233 (92.31), maa://45570 (98.04)</t>
         </is>
       </c>
       <c r="E372" s="17" t="inlineStr">
@@ -27365,12 +27368,12 @@
     <row r="379" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A379" s="19" t="inlineStr">
         <is>
-          <t>特克诺</t>
+          <t>瑰盐</t>
         </is>
       </c>
       <c r="B379" s="19" t="inlineStr">
         <is>
-          <t>DH-6</t>
+          <t>4-6</t>
         </is>
       </c>
       <c r="C379" s="19" t="inlineStr">
@@ -27380,12 +27383,12 @@
       </c>
       <c r="D379" s="17" t="inlineStr">
         <is>
-          <t>maa://59690 (100.0)</t>
+          <t>maa://44389 (100.0)</t>
         </is>
       </c>
       <c r="E379" s="17" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战特克诺并上场，且每次战斗至少释放1次“恣意挥洒”&gt; 3星通关插曲DH-6，必须编入非助战特克诺并上场，其他成员仅可编入7名干员</t>
+          <t>&gt; 战斗中非助战瑰盐累计使用绝妙的长效药呀8次&gt; 3星通关主题曲4-6；必须编入非助战瑰盐并上场，且至少使用1次绝妙的长效药呀</t>
         </is>
       </c>
       <c r="F379" s="11" t="n"/>
@@ -27419,12 +27422,12 @@
     <row r="380" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A380" s="19" t="inlineStr">
         <is>
-          <t>引星棘刺</t>
+          <t>特克诺</t>
         </is>
       </c>
       <c r="B380" s="19" t="inlineStr">
         <is>
-          <t>OF-7</t>
+          <t>DH-6</t>
         </is>
       </c>
       <c r="C380" s="19" t="inlineStr">
@@ -27434,12 +27437,12 @@
       </c>
       <c r="D380" s="17" t="inlineStr">
         <is>
-          <t>maa://48113 (100.0)</t>
+          <t>maa://59690 (100.0)</t>
         </is>
       </c>
       <c r="E380" s="17" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战引星棘刺累计使用20次解构涌潮&gt; 3星通关别传OF-7；必须编入非助战引星棘刺并上场，其他成员仅可编入4名干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战特克诺并上场，且每次战斗至少释放1次“恣意挥洒”&gt; 3星通关插曲DH-6，必须编入非助战特克诺并上场，其他成员仅可编入7名干员</t>
         </is>
       </c>
       <c r="F380" s="11" t="n"/>
@@ -27473,12 +27476,12 @@
     <row r="381" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A381" s="19" t="inlineStr">
         <is>
-          <t>行箸</t>
+          <t>特克诺</t>
         </is>
       </c>
       <c r="B381" s="19" t="inlineStr">
         <is>
-          <t>3-2</t>
+          <t>DH-6</t>
         </is>
       </c>
       <c r="C381" s="19" t="inlineStr">
@@ -27488,12 +27491,12 @@
       </c>
       <c r="D381" s="17" t="inlineStr">
         <is>
-          <t>maa://45807 (100.0)</t>
+          <t>maa://59690 (100.0)</t>
         </is>
       </c>
       <c r="E381" s="17" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战行箸累计使用8次食不厌精&gt; 3星通关主题曲3-2；必须编入非助战行箸并上场，且所有干员不能被击倒</t>
+          <t>&gt; 完成5次战斗；必须编入非助战特克诺并上场，且每次战斗至少释放1次“恣意挥洒”&gt; 3星通关插曲DH-6，必须编入非助战特克诺并上场，其他成员仅可编入7名干员</t>
         </is>
       </c>
       <c r="F381" s="11" t="n"/>
@@ -27527,12 +27530,12 @@
     <row r="382" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A382" s="19" t="inlineStr">
         <is>
-          <t>寻澜</t>
+          <t>引星棘刺</t>
         </is>
       </c>
       <c r="B382" s="19" t="inlineStr">
         <is>
-          <t>3-5</t>
+          <t>OF-7</t>
         </is>
       </c>
       <c r="C382" s="19" t="inlineStr">
@@ -27542,12 +27545,12 @@
       </c>
       <c r="D382" s="17" t="inlineStr">
         <is>
-          <t>maa://50552 (100.0)</t>
+          <t>maa://48113 (100.0)</t>
         </is>
       </c>
       <c r="E382" s="17" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战寻澜并上场，且使用寻澜歼灭至少3个敌人&gt; 3星通关主题曲3-5；必须编入非助战寻澜并上场，且至少使用2次洞悉</t>
+          <t>&gt; 战斗中非助战引星棘刺累计使用20次解构涌潮&gt; 3星通关别传OF-7；必须编入非助战引星棘刺并上场，其他成员仅可编入4名干员</t>
         </is>
       </c>
       <c r="F382" s="11" t="n"/>
@@ -27581,27 +27584,27 @@
     <row r="383" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A383" s="19" t="inlineStr">
         <is>
-          <t>诺威尔</t>
+          <t>行箸</t>
         </is>
       </c>
       <c r="B383" s="19" t="inlineStr">
         <is>
-          <t>5-7</t>
+          <t>3-2</t>
         </is>
       </c>
       <c r="C383" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D383" s="17" t="inlineStr">
         <is>
-          <t>*maa://47175 (66.67), maa://47174 (100.0)</t>
+          <t>maa://45807 (100.0)</t>
         </is>
       </c>
       <c r="E383" s="17" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战诺威尔并上场，且每次战斗至少释放1次生命不息&gt; 3星通关主题曲5-7；必须编入非助战诺威尔并上场，且队伍中不能有其他医疗干员</t>
+          <t>&gt; 使用非助战行箸累计使用8次食不厌精&gt; 3星通关主题曲3-2；必须编入非助战行箸并上场，且所有干员不能被击倒</t>
         </is>
       </c>
       <c r="F383" s="11" t="n"/>
@@ -27635,12 +27638,12 @@
     <row r="384" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A384" s="19" t="inlineStr">
         <is>
-          <t>隐德来希</t>
+          <t>寻澜</t>
         </is>
       </c>
       <c r="B384" s="19" t="inlineStr">
         <is>
-          <t>10-12</t>
+          <t>3-5</t>
         </is>
       </c>
       <c r="C384" s="19" t="inlineStr">
@@ -27650,12 +27653,12 @@
       </c>
       <c r="D384" s="17" t="inlineStr">
         <is>
-          <t>maa://47023 (87.1)</t>
+          <t>maa://50552 (100.0)</t>
         </is>
       </c>
       <c r="E384" s="17" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战隐德来希累计造成100000点伤害&gt; 3星通关主题曲10-12标准实战环境；必须编入非助战隐德来希并上场，且隐德来希至少使用3次灵与欲的惜别</t>
+          <t>&gt; 完成5次战斗；必须编入非助战寻澜并上场，且使用寻澜歼灭至少3个敌人&gt; 3星通关主题曲3-5；必须编入非助战寻澜并上场，且至少使用2次洞悉</t>
         </is>
       </c>
       <c r="F384" s="11" t="n"/>
@@ -27689,27 +27692,27 @@
     <row r="385" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A385" s="19" t="inlineStr">
         <is>
-          <t>钼铅</t>
+          <t>诺威尔</t>
         </is>
       </c>
       <c r="B385" s="19" t="inlineStr">
         <is>
-          <t>9-6</t>
+          <t>5-7</t>
         </is>
       </c>
       <c r="C385" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D385" s="17" t="inlineStr">
         <is>
-          <t>maa://48618 (100.0)</t>
+          <t>*maa://47175 (66.67), maa://47174 (100.0)</t>
         </is>
       </c>
       <c r="E385" s="17" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战钼铅累计部署矿石“杀手”30个&gt; 3星通关主题曲9-6标准实战环境；必须编入非助战钼铅并上场，且使用钼铅至少击败1名深池重甲卫士</t>
+          <t>&gt; 完成5次战斗；必须编入非助战诺威尔并上场，且每次战斗至少释放1次生命不息&gt; 3星通关主题曲5-7；必须编入非助战诺威尔并上场，且队伍中不能有其他医疗干员</t>
         </is>
       </c>
       <c r="F385" s="11" t="n"/>
@@ -27743,27 +27746,27 @@
     <row r="386" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A386" s="19" t="inlineStr">
         <is>
-          <t>死芒</t>
+          <t>隐德来希</t>
         </is>
       </c>
       <c r="B386" s="19" t="inlineStr">
         <is>
-          <t>4-8</t>
+          <t>10-12</t>
         </is>
       </c>
       <c r="C386" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D386" s="17" t="inlineStr">
         <is>
-          <t>maa://59533 (100.0), maa://59577 (100.0)</t>
+          <t>maa://47023 (87.1)</t>
         </is>
       </c>
       <c r="E386" s="17" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战死芒并上场，且每次战斗至少释放2次“冠死以冕”&gt; 3星通关主题曲4-8，必须编入非助战死芒并上场，其他成员仅可编入辅助干员</t>
+          <t>&gt; 使用非助战隐德来希累计造成100000点伤害&gt; 3星通关主题曲10-12标准实战环境；必须编入非助战隐德来希并上场，且隐德来希至少使用3次灵与欲的惜别</t>
         </is>
       </c>
       <c r="F386" s="11" t="n"/>
@@ -27797,27 +27800,27 @@
     <row r="387" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A387" s="19" t="inlineStr">
         <is>
-          <t>骋风</t>
+          <t>钼铅</t>
         </is>
       </c>
       <c r="B387" s="19" t="inlineStr">
         <is>
-          <t>SN-2</t>
+          <t>9-6</t>
         </is>
       </c>
       <c r="C387" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D387" s="17" t="inlineStr">
         <is>
-          <t>maa://51907 (100.0), maa://51908 (100.0)</t>
+          <t>maa://48618 (100.0)</t>
         </is>
       </c>
       <c r="E387" s="17" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战骋风并上场，且每次战斗至少释放1次招无虚发&gt; 3星通关插曲SN-2；必须编入非助战骋风并上场，且使用2次招无虚发</t>
+          <t>&gt; 战斗中非助战钼铅累计部署矿石“杀手”30个&gt; 3星通关主题曲9-6标准实战环境；必须编入非助战钼铅并上场，且使用钼铅至少击败1名深池重甲卫士</t>
         </is>
       </c>
       <c r="F387" s="11" t="n"/>
@@ -27851,27 +27854,27 @@
     <row r="388" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A388" s="19" t="inlineStr">
         <is>
-          <t>阿兰娜</t>
+          <t>死芒</t>
         </is>
       </c>
       <c r="B388" s="19" t="inlineStr">
         <is>
-          <t>7-14</t>
+          <t>4-8</t>
         </is>
       </c>
       <c r="C388" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D388" s="17" t="inlineStr">
         <is>
-          <t>maa://59691 (100.0)</t>
+          <t>maa://59533 (100.0), maa://59577 (100.0)</t>
         </is>
       </c>
       <c r="E388" s="17" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战阿兰娜累计部署15个“支援装置”&gt; 3星通关主题曲7-14；必须编入非助战阿兰娜并上场，且至少使用2次“万斤顶”</t>
+          <t>&gt; 完成5次战斗；必须编入非助战死芒并上场，且每次战斗至少释放2次“冠死以冕”&gt; 3星通关主题曲4-8，必须编入非助战死芒并上场，其他成员仅可编入辅助干员</t>
         </is>
       </c>
       <c r="F388" s="11" t="n"/>
@@ -27905,12 +27908,12 @@
     <row r="389" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A389" s="19" t="inlineStr">
         <is>
-          <t>信仰搅拌机</t>
+          <t>骋风</t>
         </is>
       </c>
       <c r="B389" s="19" t="inlineStr">
         <is>
-          <t>14-5</t>
+          <t>SN-2</t>
         </is>
       </c>
       <c r="C389" s="19" t="inlineStr">
@@ -27920,12 +27923,12 @@
       </c>
       <c r="D389" s="17" t="inlineStr">
         <is>
-          <t>maa://51898 (100.0), maa://57241 (100.0)</t>
+          <t>maa://51907 (100.0), maa://51908 (100.0)</t>
         </is>
       </c>
       <c r="E389" s="17" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战信仰搅拌机并上场，且每次战斗至少释放1次退休前布道&gt; 3星通关主题曲14-5标准实战环境；必须编入非助战信仰搅拌机并上场，且使用信仰搅拌机歼灭至少10名敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战骋风并上场，且每次战斗至少释放1次招无虚发&gt; 3星通关插曲SN-2；必须编入非助战骋风并上场，且使用2次招无虚发</t>
         </is>
       </c>
       <c r="F389" s="11" t="n"/>
@@ -27959,27 +27962,27 @@
     <row r="390" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A390" s="19" t="inlineStr">
         <is>
-          <t>蕾缪安</t>
+          <t>阿兰娜</t>
         </is>
       </c>
       <c r="B390" s="19" t="inlineStr">
         <is>
-          <t>13-13</t>
+          <t>7-14</t>
         </is>
       </c>
       <c r="C390" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D390" s="17" t="inlineStr">
         <is>
-          <t>maa://51880 (99.23), maa://51878 (100.0), maa://56651 (100.0)</t>
+          <t>maa://59691 (100.0)</t>
         </is>
       </c>
       <c r="E390" s="17" t="inlineStr">
         <is>
-          <t>&gt; 由非助战蕾缪安累计造成30歼灭数&gt; 3星通关主题曲13-13标准实战环境；必须编入非助战蕾缪安并上场，且蕾缪安歼灭至少2个萨卡兹骸骨鞭笞者</t>
+          <t>&gt; 使用非助战阿兰娜累计部署15个“支援装置”&gt; 3星通关主题曲7-14；必须编入非助战阿兰娜并上场，且至少使用2次“万斤顶”</t>
         </is>
       </c>
       <c r="F390" s="11" t="n"/>
@@ -28013,27 +28016,27 @@
     <row r="391" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A391" s="19" t="inlineStr">
         <is>
-          <t>新约能天使</t>
+          <t>信仰搅拌机</t>
         </is>
       </c>
       <c r="B391" s="19" t="inlineStr">
         <is>
-          <t>GA-EX-5</t>
+          <t>14-5</t>
         </is>
       </c>
       <c r="C391" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D391" s="17" t="inlineStr">
         <is>
-          <t>maa://51872 (96.75), maa://51876 (98.81), maa://51873 (100.0)</t>
+          <t>maa://51898 (100.0), maa://57241 (100.0)</t>
         </is>
       </c>
       <c r="E391" s="17" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战新约能天使累计使用开火成瘾症8次&gt; 3星通关插曲GA-EX-5；必须编入非助战新约能天使并上场，且使用2次开火成瘾症</t>
+          <t>&gt; 完成5次战斗；必须编入非助战信仰搅拌机并上场，且每次战斗至少释放1次退休前布道&gt; 3星通关主题曲14-5标准实战环境；必须编入非助战信仰搅拌机并上场，且使用信仰搅拌机歼灭至少10名敌人</t>
         </is>
       </c>
       <c r="F391" s="11" t="n"/>
@@ -28067,12 +28070,12 @@
     <row r="392" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A392" s="19" t="inlineStr">
         <is>
-          <t>酒神</t>
+          <t>蕾缪安</t>
         </is>
       </c>
       <c r="B392" s="19" t="inlineStr">
         <is>
-          <t>9-6</t>
+          <t>13-13</t>
         </is>
       </c>
       <c r="C392" s="19" t="inlineStr">
@@ -28082,12 +28085,12 @@
       </c>
       <c r="D392" s="17" t="inlineStr">
         <is>
-          <t>maa://59493 (96.49), maa://59603 (100.0), maa://60449 (100.0)</t>
+          <t>maa://51880 (99.23), maa://51878 (100.0), maa://56651 (100.0)</t>
         </is>
       </c>
       <c r="E392" s="17" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战酒神累计造成60000点神经损伤&gt; 3星通关主题曲9-6标准实战环境，必须编入非助战酒神并上场，且酒神使用至少2次“空剧场”</t>
+          <t>&gt; 由非助战蕾缪安累计造成30歼灭数&gt; 3星通关主题曲13-13标准实战环境；必须编入非助战蕾缪安并上场，且蕾缪安歼灭至少2个萨卡兹骸骨鞭笞者</t>
         </is>
       </c>
       <c r="F392" s="11" t="n"/>
@@ -28118,6 +28121,60 @@
       <c r="AE392" s="11" t="n"/>
       <c r="AF392" s="14" t="n"/>
     </row>
+    <row r="393">
+      <c r="A393" s="28" t="inlineStr">
+        <is>
+          <t>新约能天使</t>
+        </is>
+      </c>
+      <c r="B393" s="28" t="inlineStr">
+        <is>
+          <t>GA-EX-5</t>
+        </is>
+      </c>
+      <c r="C393" s="28" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D393" t="inlineStr">
+        <is>
+          <t>maa://51872 (96.79), maa://51876 (98.81), maa://51873 (100.0)</t>
+        </is>
+      </c>
+      <c r="E393" t="inlineStr">
+        <is>
+          <t>&gt; 战斗中非助战新约能天使累计使用开火成瘾症8次&gt; 3星通关插曲GA-EX-5；必须编入非助战新约能天使并上场，且使用2次开火成瘾症</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="28" t="inlineStr">
+        <is>
+          <t>酒神</t>
+        </is>
+      </c>
+      <c r="B394" s="28" t="inlineStr">
+        <is>
+          <t>9-6</t>
+        </is>
+      </c>
+      <c r="C394" s="28" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D394" t="inlineStr">
+        <is>
+          <t>maa://59493 (96.52), maa://59603 (100.0), maa://60449 (100.0)</t>
+        </is>
+      </c>
+      <c r="E394" t="inlineStr">
+        <is>
+          <t>&gt; 使用非助战酒神累计造成60000点神经损伤&gt; 3星通关主题曲9-6标准实战环境，必须编入非助战酒神并上场，且酒神使用至少2次“空剧场”</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>

<commit_message>
CI: Auto Update Data (#203)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -868,7 +868,7 @@
       </c>
       <c r="L3" s="14" t="inlineStr">
         <is>
-          <t>*maa://22880 (66.1), maa://20276 (88.68), *maa://22749 (77.78)</t>
+          <t>*maa://22880 (66.1), maa://20276 (88.68), *maa://22749 (78.95)</t>
         </is>
       </c>
       <c r="M3" s="11" t="n"/>
@@ -884,7 +884,7 @@
       </c>
       <c r="P3" s="14" t="inlineStr">
         <is>
-          <t>maa://21249 (94.77), maa://26254 (97.3)</t>
+          <t>maa://21249 (94.79), maa://26254 (97.3)</t>
         </is>
       </c>
       <c r="Q3" s="11" t="n"/>
@@ -932,7 +932,7 @@
       </c>
       <c r="AB3" s="14" t="inlineStr">
         <is>
-          <t>maa://24390 (95.7), maa://52241 (91.67)</t>
+          <t>maa://24390 (95.74), maa://52241 (92.31)</t>
         </is>
       </c>
       <c r="AC3" s="11" t="n"/>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="L5" s="14" t="inlineStr">
         <is>
-          <t>*maa://22757 (79.55)</t>
+          <t>*maa://22757 (80.0)</t>
         </is>
       </c>
       <c r="M5" s="11" t="n"/>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="X6" s="14" t="inlineStr">
         <is>
-          <t>maa://52754 (83.33)</t>
+          <t>maa://52754 (84.21)</t>
         </is>
       </c>
       <c r="Y6" s="11" t="n"/>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="T7" s="14" t="inlineStr">
         <is>
-          <t>maa://21291 (87.1)</t>
+          <t>maa://21291 (87.3)</t>
         </is>
       </c>
       <c r="U7" s="11" t="n"/>
@@ -1481,7 +1481,7 @@
     <row r="8">
       <c r="A8" s="10" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.23 13:23:39</t>
+          <t>更新日期：2025.06.24 13:22:20</t>
         </is>
       </c>
       <c r="B8" s="11" t="inlineStr">
@@ -1756,7 +1756,7 @@
       </c>
       <c r="D10" s="14" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.54), ***maa://39951 (11.69), ***maa://34206 (22.22), *maa://45271 (62.2), ***maa://39243 (25.0), **maa://54000 (50.0)</t>
+          <t>***maa://25695 (18.45), ***maa://39951 (11.69), ***maa://34206 (22.22), *maa://45271 (62.2), ***maa://39243 (25.0), **maa://54000 (50.0)</t>
         </is>
       </c>
       <c r="E10" s="11" t="n"/>
@@ -2112,7 +2112,7 @@
       </c>
       <c r="AB12" s="14" t="inlineStr">
         <is>
-          <t>maa://23669 (95.68), maa://36677 (95.45), maa://39872 (93.1)</t>
+          <t>maa://23669 (95.68), maa://36677 (95.51), maa://39872 (93.1)</t>
         </is>
       </c>
       <c r="AC12" s="11" t="n"/>
@@ -2146,7 +2146,7 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>maa://24999 (92.76), maa://36673 (92.05), maa://25001 (86.49)</t>
+          <t>maa://24999 (92.77), maa://36673 (92.05), maa://25001 (86.49)</t>
         </is>
       </c>
       <c r="E13" s="11" t="n"/>
@@ -2422,7 +2422,7 @@
       </c>
       <c r="H15" s="14" t="inlineStr">
         <is>
-          <t>maa://24304 (87.36), maa://21478 (90.0)</t>
+          <t>maa://24304 (87.36), maa://21478 (90.24)</t>
         </is>
       </c>
       <c r="I15" s="11" t="n"/>
@@ -2812,7 +2812,7 @@
       </c>
       <c r="H18" s="14" t="inlineStr">
         <is>
-          <t>maa://24421 (86.97)</t>
+          <t>maa://24421 (87.02)</t>
         </is>
       </c>
       <c r="I18" s="11" t="n"/>
@@ -3396,7 +3396,7 @@
       </c>
       <c r="X22" s="14" t="inlineStr">
         <is>
-          <t>maa://21282 (98.73), *maa://37649 (74.42)</t>
+          <t>maa://21282 (98.73), *maa://37649 (75.0)</t>
         </is>
       </c>
       <c r="Y22" s="11" t="n"/>
@@ -3932,7 +3932,7 @@
       </c>
       <c r="AB26" s="14" t="inlineStr">
         <is>
-          <t>maa://42235 (96.15)</t>
+          <t>maa://42235 (96.18)</t>
         </is>
       </c>
       <c r="AC26" s="11" t="n"/>
@@ -4632,7 +4632,7 @@
       </c>
       <c r="H32" s="14" t="inlineStr">
         <is>
-          <t>maa://21895 (97.67), maa://36667 (97.35), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.67), maa://36667 (97.37), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="11" t="n"/>
@@ -5200,7 +5200,7 @@
       </c>
       <c r="T36" s="14" t="inlineStr">
         <is>
-          <t>maa://27613 (99.13)</t>
+          <t>maa://27613 (99.14)</t>
         </is>
       </c>
       <c r="U36" s="11" t="n"/>
@@ -6407,7 +6407,7 @@
       </c>
       <c r="P52" s="14" t="inlineStr">
         <is>
-          <t>maa://59378 (97.37), maa://59394 (96.15)</t>
+          <t>maa://59378 (97.5), maa://59394 (96.3)</t>
         </is>
       </c>
       <c r="Q52" s="11" t="n"/>
@@ -6669,7 +6669,7 @@
       </c>
       <c r="H63" s="14" t="inlineStr">
         <is>
-          <t>maa://59534 (98.11), maa://59413 (100.0)</t>
+          <t>maa://59534 (98.21), maa://59413 (100.0)</t>
         </is>
       </c>
       <c r="I63" s="11" t="n"/>
@@ -6971,7 +6971,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A1" s="13" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.23 13:23:39</t>
+          <t>更新日期：2025.06.24 13:22:20</t>
         </is>
       </c>
       <c r="E1" s="16" t="inlineStr">
@@ -14909,7 +14909,7 @@
       </c>
       <c r="D148" s="20" t="inlineStr">
         <is>
-          <t>maa://28828 (88.24), maa://20846 (95.83), *maa://47286 (66.67)</t>
+          <t>maa://28828 (88.24), maa://20846 (95.83), *maa://47286 (75.0)</t>
         </is>
       </c>
       <c r="E148" s="21" t="inlineStr">
@@ -14963,7 +14963,7 @@
       </c>
       <c r="D149" s="20" t="inlineStr">
         <is>
-          <t>maa://36641 (98.44), maa://40957 (93.72), maa://36865 (96.34), maa://44635 (87.85), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
+          <t>maa://36641 (98.44), maa://40957 (93.76), maa://36865 (96.34), maa://44635 (87.85), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
         </is>
       </c>
       <c r="E149" s="21" t="inlineStr">
@@ -15017,7 +15017,7 @@
       </c>
       <c r="D150" s="20" t="inlineStr">
         <is>
-          <t>maa://51549 (95.24), maa://51923 (95.65)</t>
+          <t>maa://51549 (95.24), maa://51923 (95.83)</t>
         </is>
       </c>
       <c r="E150" s="21" t="inlineStr">
@@ -15935,7 +15935,7 @@
       </c>
       <c r="D167" s="20" t="inlineStr">
         <is>
-          <t>maa://29633 (92.31), maa://29627 (92.69), maa://29659 (85.71), maa://49074 (97.67), **maa://30679 (50.0), maa://29861 (100.0), maa://42343 (100.0)</t>
+          <t>maa://29633 (92.31), maa://29627 (92.69), maa://29659 (85.71), maa://49074 (97.73), **maa://30679 (50.0), maa://29861 (100.0), maa://42343 (100.0)</t>
         </is>
       </c>
       <c r="E167" s="21" t="inlineStr">
@@ -17555,7 +17555,7 @@
       </c>
       <c r="D197" s="20" t="inlineStr">
         <is>
-          <t>maa://44224 (90.3), maa://35854 (85.87), maa://50388 (97.9), maa://25760 (86.96), ***maa://43911 (13.04), *maa://20872 (52.0), maa://51066 (100.0)</t>
+          <t>maa://44224 (90.3), maa://35854 (85.87), maa://50388 (97.92), maa://25760 (86.96), ***maa://43911 (13.04), *maa://20872 (52.0), maa://51066 (100.0)</t>
         </is>
       </c>
       <c r="E197" s="21" t="inlineStr">
@@ -18311,7 +18311,7 @@
       </c>
       <c r="D211" s="20" t="inlineStr">
         <is>
-          <t>maa://20956 (95.83), *maa://20830 (80.0), maa://44703 (91.67)</t>
+          <t>maa://20956 (95.85), *maa://20830 (80.0), maa://44703 (91.67)</t>
         </is>
       </c>
       <c r="E211" s="21" t="inlineStr">
@@ -18905,7 +18905,7 @@
       </c>
       <c r="D222" s="20" t="inlineStr">
         <is>
-          <t>maa://39695 (100.0), **maa://39911 (33.33)</t>
+          <t>maa://39695 (100.0), ***maa://39911 (25.0)</t>
         </is>
       </c>
       <c r="E222" s="21" t="inlineStr">
@@ -19175,7 +19175,7 @@
       </c>
       <c r="D227" s="20" t="inlineStr">
         <is>
-          <t>maa://20987 (93.68), *maa://35801 (77.78)</t>
+          <t>maa://20987 (93.75), *maa://35801 (77.78)</t>
         </is>
       </c>
       <c r="E227" s="21" t="inlineStr">
@@ -19877,7 +19877,7 @@
       </c>
       <c r="D240" s="20" t="inlineStr">
         <is>
-          <t>*maa://30667 (78.68), maa://30666 (83.48), **maa://30739 (43.24), *maa://30723 (56.45), maa://39588 (89.09)</t>
+          <t>*maa://30667 (78.68), maa://30666 (83.55), **maa://30739 (43.24), *maa://30723 (56.45), maa://39588 (89.09)</t>
         </is>
       </c>
       <c r="E240" s="21" t="inlineStr">
@@ -20466,12 +20466,12 @@
       </c>
       <c r="C251" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D251" s="20" t="inlineStr">
         <is>
-          <t>maa://20923 (92.86)</t>
+          <t>maa://20923 (92.86), maa://60577 (100.0)</t>
         </is>
       </c>
       <c r="E251" s="21" t="inlineStr">
@@ -26195,7 +26195,7 @@
       </c>
       <c r="D357" s="17" t="inlineStr">
         <is>
-          <t>maa://36645 (98.37), maa://36841 (92.65), maa://37484 (94.23), maa://37858 (93.33), maa://40489 (100.0), *maa://56268 (60.0)</t>
+          <t>maa://36645 (98.38), maa://36841 (92.65), maa://37484 (94.23), maa://37858 (93.33), maa://40489 (100.0), *maa://56268 (60.0)</t>
         </is>
       </c>
       <c r="E357" s="17" t="inlineStr">
@@ -26411,7 +26411,7 @@
       </c>
       <c r="D361" s="17" t="inlineStr">
         <is>
-          <t>maa://40957 (93.72), maa://44635 (87.85), maa://48026 (94.74), maa://41035 (92.54), maa://44660 (92.31), maa://41128 (83.78), maa://60251 (100.0)</t>
+          <t>maa://40957 (93.76), maa://44635 (87.85), maa://48026 (94.74), maa://41035 (92.54), maa://44660 (92.31), maa://41128 (83.78), maa://60251 (100.0)</t>
         </is>
       </c>
       <c r="E361" s="17" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#204)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -868,7 +868,7 @@
       </c>
       <c r="L3" s="14" t="inlineStr">
         <is>
-          <t>*maa://22880 (66.1), maa://20276 (88.68), *maa://22749 (78.95)</t>
+          <t>*maa://22880 (66.24), maa://20276 (88.68), *maa://22749 (78.95)</t>
         </is>
       </c>
       <c r="M3" s="11" t="n"/>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="P4" s="14" t="inlineStr">
         <is>
-          <t>maa://49983 (96.2), maa://50121 (95.12)</t>
+          <t>maa://49983 (96.25), maa://50121 (95.12)</t>
         </is>
       </c>
       <c r="Q4" s="11" t="n"/>
@@ -1327,7 +1327,7 @@
       </c>
       <c r="AB6" s="14" t="inlineStr">
         <is>
-          <t>maa://22739 (91.94)</t>
+          <t>maa://22739 (92.06)</t>
         </is>
       </c>
       <c r="AC6" s="11" t="n"/>
@@ -1481,7 +1481,7 @@
     <row r="8">
       <c r="A8" s="10" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.24 13:22:20</t>
+          <t>更新日期：2025.06.25 13:22:19</t>
         </is>
       </c>
       <c r="B8" s="11" t="inlineStr">
@@ -1592,7 +1592,7 @@
       </c>
       <c r="AB8" s="14" t="inlineStr">
         <is>
-          <t>maa://25389 (90.48)</t>
+          <t>maa://25389 (88.37)</t>
         </is>
       </c>
       <c r="AC8" s="11" t="n"/>
@@ -1966,7 +1966,7 @@
       </c>
       <c r="X11" s="14" t="inlineStr">
         <is>
-          <t>maa://36713 (98.17)</t>
+          <t>maa://36713 (98.18)</t>
         </is>
       </c>
       <c r="Y11" s="11" t="n"/>
@@ -2146,7 +2146,7 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>maa://24999 (92.77), maa://36673 (92.05), maa://25001 (86.49)</t>
+          <t>maa://24999 (92.78), maa://36673 (92.05), maa://25001 (86.49)</t>
         </is>
       </c>
       <c r="E13" s="11" t="n"/>
@@ -2828,7 +2828,7 @@
       </c>
       <c r="L18" s="14" t="inlineStr">
         <is>
-          <t>maa://22466 (92.23), maa://52226 (95.83)</t>
+          <t>maa://22466 (92.27), maa://52226 (95.83)</t>
         </is>
       </c>
       <c r="M18" s="11" t="n"/>
@@ -3298,7 +3298,7 @@
       </c>
       <c r="AF21" s="14" t="inlineStr">
         <is>
-          <t>maa://22524 (88.14), maa://22432 (83.58)</t>
+          <t>maa://22524 (88.14), maa://22432 (82.96)</t>
         </is>
       </c>
       <c r="AG21" s="27" t="n"/>
@@ -3396,7 +3396,7 @@
       </c>
       <c r="X22" s="14" t="inlineStr">
         <is>
-          <t>maa://21282 (98.73), *maa://37649 (75.0)</t>
+          <t>maa://21282 (98.74), *maa://37649 (73.33)</t>
         </is>
       </c>
       <c r="Y22" s="11" t="n"/>
@@ -3526,7 +3526,7 @@
       </c>
       <c r="X23" s="14" t="inlineStr">
         <is>
-          <t>*maa://28503 (63.64)</t>
+          <t>*maa://28503 (63.0)</t>
         </is>
       </c>
       <c r="Y23" s="11" t="n"/>
@@ -3656,7 +3656,7 @@
       </c>
       <c r="X24" s="14" t="inlineStr">
         <is>
-          <t>maa://29988 (84.97), maa://23504 (93.75), *maa://25141 (77.37), *maa://36663 (78.0), maa://52227 (95.24)</t>
+          <t>maa://29988 (84.97), maa://23504 (93.76), *maa://25141 (77.37), *maa://36663 (78.0), maa://52227 (95.24)</t>
         </is>
       </c>
       <c r="Y24" s="11" t="n"/>
@@ -3770,7 +3770,7 @@
       </c>
       <c r="T25" s="14" t="inlineStr">
         <is>
-          <t>maa://20109 (92.67), maa://22545 (100.0), *maa://42915 (75.0)</t>
+          <t>maa://20109 (92.71), maa://22545 (100.0), *maa://42915 (75.0)</t>
         </is>
       </c>
       <c r="U25" s="11" t="n"/>
@@ -4436,7 +4436,7 @@
       </c>
       <c r="X30" s="14" t="inlineStr">
         <is>
-          <t>maa://39477 (92.0)</t>
+          <t>maa://39477 (92.31)</t>
         </is>
       </c>
       <c r="Y30" s="11" t="n"/>
@@ -5468,7 +5468,7 @@
       </c>
       <c r="H39" s="14" t="inlineStr">
         <is>
-          <t>maa://36670 (88.89), maa://25199 (85.47), maa://30434 (93.38), *maa://45059 (77.14)</t>
+          <t>maa://36670 (88.89), maa://25199 (85.47), maa://30434 (93.43), *maa://45059 (77.14)</t>
         </is>
       </c>
       <c r="I39" s="11" t="n"/>
@@ -5702,7 +5702,7 @@
       </c>
       <c r="P41" s="14" t="inlineStr">
         <is>
-          <t>maa://43177 (87.88)</t>
+          <t>maa://43177 (88.24)</t>
         </is>
       </c>
       <c r="Q41" s="11" t="n"/>
@@ -6407,7 +6407,7 @@
       </c>
       <c r="P52" s="14" t="inlineStr">
         <is>
-          <t>maa://59378 (97.5), maa://59394 (96.3)</t>
+          <t>maa://59378 (97.56), maa://59394 (96.3)</t>
         </is>
       </c>
       <c r="Q52" s="11" t="n"/>
@@ -6597,7 +6597,7 @@
       </c>
       <c r="H59" s="14" t="inlineStr">
         <is>
-          <t>maa://31270 (94.81), maa://27746 (82.91)</t>
+          <t>maa://31270 (94.84), maa://27746 (82.91)</t>
         </is>
       </c>
       <c r="I59" s="11" t="n"/>
@@ -6669,7 +6669,7 @@
       </c>
       <c r="H63" s="14" t="inlineStr">
         <is>
-          <t>maa://59534 (98.21), maa://59413 (100.0)</t>
+          <t>maa://59534 (98.28), maa://59413 (100.0)</t>
         </is>
       </c>
       <c r="I63" s="11" t="n"/>
@@ -6971,7 +6971,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A1" s="13" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.24 13:22:20</t>
+          <t>更新日期：2025.06.25 13:22:19</t>
         </is>
       </c>
       <c r="E1" s="16" t="inlineStr">
@@ -8483,7 +8483,7 @@
       </c>
       <c r="D29" s="20" t="inlineStr">
         <is>
-          <t>maa://20863 (89.17), maa://20832 (99.08), maa://20727 (100.0)</t>
+          <t>maa://20863 (88.8), maa://20832 (99.08), maa://20727 (100.0)</t>
         </is>
       </c>
       <c r="E29" s="21" t="inlineStr">
@@ -10103,7 +10103,7 @@
       </c>
       <c r="D59" s="20" t="inlineStr">
         <is>
-          <t>maa://27970 (98.61), maa://41118 (85.71)</t>
+          <t>maa://27970 (98.63), maa://41118 (85.71)</t>
         </is>
       </c>
       <c r="E59" s="21" t="inlineStr">
@@ -10157,7 +10157,7 @@
       </c>
       <c r="D60" s="20" t="inlineStr">
         <is>
-          <t>maa://38298 (87.5)</t>
+          <t>maa://38298 (87.62)</t>
         </is>
       </c>
       <c r="E60" s="21" t="inlineStr">
@@ -14639,7 +14639,7 @@
       </c>
       <c r="D143" s="20" t="inlineStr">
         <is>
-          <t>maa://30670 (96.64), maa://31470 (96.67), *maa://45066 (66.67), **maa://30867 (40.0)</t>
+          <t>maa://30670 (96.67), maa://31470 (96.67), *maa://45066 (66.67), **maa://30867 (40.0)</t>
         </is>
       </c>
       <c r="E143" s="21" t="inlineStr">
@@ -14963,7 +14963,7 @@
       </c>
       <c r="D149" s="20" t="inlineStr">
         <is>
-          <t>maa://36641 (98.44), maa://40957 (93.76), maa://36865 (96.34), maa://44635 (87.85), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
+          <t>maa://36641 (98.44), maa://40957 (93.79), maa://36865 (96.34), maa://44635 (88.07), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
         </is>
       </c>
       <c r="E149" s="21" t="inlineStr">
@@ -16367,7 +16367,7 @@
       </c>
       <c r="D175" s="20" t="inlineStr">
         <is>
-          <t>maa://32418 (99.68), maa://51440 (100.0)</t>
+          <t>maa://32418 (99.69), maa://51440 (100.0)</t>
         </is>
       </c>
       <c r="E175" s="21" t="inlineStr">
@@ -17555,7 +17555,7 @@
       </c>
       <c r="D197" s="20" t="inlineStr">
         <is>
-          <t>maa://44224 (90.3), maa://35854 (85.87), maa://50388 (97.92), maa://25760 (86.96), ***maa://43911 (13.04), *maa://20872 (52.0), maa://51066 (100.0)</t>
+          <t>maa://44224 (90.32), maa://35854 (86.02), maa://50388 (97.92), maa://25760 (86.96), ***maa://43911 (13.04), *maa://20872 (52.0), maa://51066 (100.0)</t>
         </is>
       </c>
       <c r="E197" s="21" t="inlineStr">
@@ -19391,7 +19391,7 @@
       </c>
       <c r="D231" s="20" t="inlineStr">
         <is>
-          <t>maa://29058 (96.05), maa://39140 (100.0), maa://38723 (100.0)</t>
+          <t>maa://29058 (96.1), maa://39140 (100.0), maa://38723 (100.0)</t>
         </is>
       </c>
       <c r="E231" s="21" t="inlineStr">
@@ -19445,7 +19445,7 @@
       </c>
       <c r="D232" s="20" t="inlineStr">
         <is>
-          <t>*maa://48263 (75.0)</t>
+          <t>*maa://48263 (76.19)</t>
         </is>
       </c>
       <c r="E232" s="21" t="inlineStr">
@@ -21497,7 +21497,7 @@
       </c>
       <c r="D270" s="20" t="inlineStr">
         <is>
-          <t>maa://25769 (97.42)</t>
+          <t>maa://25769 (97.44)</t>
         </is>
       </c>
       <c r="E270" s="21" t="inlineStr">
@@ -22361,7 +22361,7 @@
       </c>
       <c r="D286" s="20" t="inlineStr">
         <is>
-          <t>maa://20899 (89.41), maa://46332 (95.0), ***maa://44744 (25.0)</t>
+          <t>maa://20899 (89.41), maa://46332 (95.24), ***maa://44744 (25.0)</t>
         </is>
       </c>
       <c r="E286" s="21" t="inlineStr">
@@ -22523,7 +22523,7 @@
       </c>
       <c r="D289" s="20" t="inlineStr">
         <is>
-          <t>maa://30710 (97.89), maa://36845 (95.65), maa://31558 (97.14), **maa://39217 (41.18), maa://30668 (86.67)</t>
+          <t>maa://30710 (97.89), maa://36845 (95.68), maa://31558 (97.14), **maa://39217 (41.18), maa://30668 (86.67)</t>
         </is>
       </c>
       <c r="E289" s="21" t="inlineStr">
@@ -26141,7 +26141,7 @@
       </c>
       <c r="D356" s="17" t="inlineStr">
         <is>
-          <t>maa://36646 (98.8), maa://36845 (95.65), **maa://39217 (41.18), maa://51007 (98.18)</t>
+          <t>maa://36646 (98.8), maa://36845 (95.68), **maa://39217 (41.18), maa://51007 (98.18)</t>
         </is>
       </c>
       <c r="E356" s="17" t="inlineStr">
@@ -26411,7 +26411,7 @@
       </c>
       <c r="D361" s="17" t="inlineStr">
         <is>
-          <t>maa://40957 (93.76), maa://44635 (87.85), maa://48026 (94.74), maa://41035 (92.54), maa://44660 (92.31), maa://41128 (83.78), maa://60251 (100.0)</t>
+          <t>maa://40957 (93.79), maa://44635 (88.07), maa://48026 (94.85), maa://41035 (92.65), maa://44660 (92.31), maa://41128 (83.78), maa://60251 (85.71)</t>
         </is>
       </c>
       <c r="E361" s="17" t="inlineStr">
@@ -27275,7 +27275,7 @@
       </c>
       <c r="D377" s="17" t="inlineStr">
         <is>
-          <t>maa://42970 (83.33), maa://44745 (98.23), **maa://49516 (40.0), *maa://45952 (80.0), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
+          <t>maa://42970 (83.33), maa://44745 (98.25), **maa://49516 (38.1), *maa://45952 (80.0), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E377" s="17" t="inlineStr">
@@ -28139,7 +28139,7 @@
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>maa://51872 (96.79), maa://51876 (98.81), maa://51873 (100.0)</t>
+          <t>maa://51872 (96.82), maa://51876 (98.82), maa://51873 (100.0)</t>
         </is>
       </c>
       <c r="E393" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#205)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -802,7 +802,7 @@
       </c>
       <c r="AB2" s="14" t="inlineStr">
         <is>
-          <t>maa://21246 (91.48), maa://36684 (93.25)</t>
+          <t>maa://21246 (91.48), maa://36684 (93.29)</t>
         </is>
       </c>
       <c r="AC2" s="11" t="n"/>
@@ -836,7 +836,7 @@
       </c>
       <c r="D3" s="14" t="inlineStr">
         <is>
-          <t>maa://40192 (96.4), maa://36987 (96.3), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.43), maa://36987 (96.3), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="11" t="n"/>
@@ -868,7 +868,7 @@
       </c>
       <c r="L3" s="14" t="inlineStr">
         <is>
-          <t>*maa://22880 (66.24), maa://20276 (88.68), *maa://22749 (78.95)</t>
+          <t>*maa://22880 (66.39), maa://20276 (88.68), *maa://22749 (78.95)</t>
         </is>
       </c>
       <c r="M3" s="11" t="n"/>
@@ -884,7 +884,7 @@
       </c>
       <c r="P3" s="14" t="inlineStr">
         <is>
-          <t>maa://21249 (94.79), maa://26254 (97.3)</t>
+          <t>maa://21249 (94.81), maa://26254 (97.3)</t>
         </is>
       </c>
       <c r="Q3" s="11" t="n"/>
@@ -966,7 +966,7 @@
       </c>
       <c r="D4" s="14" t="inlineStr">
         <is>
-          <t>maa://24632 (93.69), maa://22499 (86.67), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.72), maa://22499 (86.67), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="11" t="n"/>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="P4" s="14" t="inlineStr">
         <is>
-          <t>maa://49983 (96.25), maa://50121 (95.12)</t>
+          <t>maa://49983 (96.43), maa://50121 (95.12)</t>
         </is>
       </c>
       <c r="Q4" s="11" t="n"/>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="T4" s="14" t="inlineStr">
         <is>
-          <t>maa://32509 (94.03), maa://27295 (88.54), maa://22754 (89.19), *maa://31008 (79.55)</t>
+          <t>maa://32509 (94.03), maa://27295 (88.66), maa://22754 (89.19), *maa://31008 (79.55)</t>
         </is>
       </c>
       <c r="U4" s="11" t="n"/>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="X4" s="14" t="inlineStr">
         <is>
-          <t>maa://43217 (94.03)</t>
+          <t>maa://43217 (94.07)</t>
         </is>
       </c>
       <c r="Y4" s="11" t="n"/>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="D5" s="14" t="inlineStr">
         <is>
-          <t>maa://21245 (84.43), maa://22744 (82.14), maa://54105 (100.0)</t>
+          <t>maa://21245 (84.14), maa://22744 (82.14), maa://54105 (100.0)</t>
         </is>
       </c>
       <c r="E5" s="11" t="n"/>
@@ -1295,7 +1295,7 @@
       </c>
       <c r="T6" s="14" t="inlineStr">
         <is>
-          <t>maa://37411 (90.91)</t>
+          <t>maa://37411 (86.96)</t>
         </is>
       </c>
       <c r="U6" s="11" t="n"/>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="AF6" s="14" t="inlineStr">
         <is>
-          <t>*maa://33152 (65.08), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (64.06), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="27" t="n"/>
@@ -1393,7 +1393,7 @@
       </c>
       <c r="L7" s="14" t="inlineStr">
         <is>
-          <t>maa://28624 (94.04), maa://24957 (97.78)</t>
+          <t>maa://28624 (94.04), maa://24957 (97.83)</t>
         </is>
       </c>
       <c r="M7" s="11" t="n"/>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="X7" s="14" t="inlineStr">
         <is>
-          <t>maa://22399 (96.22), *maa://22758 (77.5)</t>
+          <t>maa://22399 (95.7), *maa://22758 (77.78)</t>
         </is>
       </c>
       <c r="Y7" s="11" t="n"/>
@@ -1481,7 +1481,7 @@
     <row r="8">
       <c r="A8" s="10" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.25 13:22:19</t>
+          <t>更新日期：2025.06.27 13:21:40</t>
         </is>
       </c>
       <c r="B8" s="11" t="inlineStr">
@@ -1722,7 +1722,7 @@
       </c>
       <c r="AB9" s="14" t="inlineStr">
         <is>
-          <t>maa://28711 (87.5), maa://40166 (93.88)</t>
+          <t>maa://28711 (87.5), maa://40166 (93.75)</t>
         </is>
       </c>
       <c r="AC9" s="11" t="n"/>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="P10" s="14" t="inlineStr">
         <is>
-          <t>maa://28977 (87.63), maa://36669 (80.36), *maa://23264 (62.07)</t>
+          <t>maa://28977 (87.63), *maa://36669 (78.95), *maa://23264 (62.07)</t>
         </is>
       </c>
       <c r="Q10" s="11" t="n"/>
@@ -1868,7 +1868,7 @@
       </c>
       <c r="AF10" s="14" t="inlineStr">
         <is>
-          <t>*maa://25021 (53.7), *maa://22733 (64.29), **maa://22761 (50.0)</t>
+          <t>*maa://25021 (53.21), *maa://22733 (64.29), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="27" t="n"/>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="T11" s="14" t="inlineStr">
         <is>
-          <t>maa://22747 (90.45), maa://22501 (98.26), maa://45521 (91.67)</t>
+          <t>maa://22747 (90.45), maa://22501 (98.26), maa://45521 (91.89)</t>
         </is>
       </c>
       <c r="U11" s="11" t="n"/>
@@ -2096,7 +2096,7 @@
       </c>
       <c r="X12" s="14" t="inlineStr">
         <is>
-          <t>maa://22753 (92.02), *maa://21485 (76.0), maa://37962 (92.96)</t>
+          <t>maa://22753 (92.02), maa://37962 (92.96), *maa://21485 (76.0)</t>
         </is>
       </c>
       <c r="Y12" s="11" t="n"/>
@@ -2226,7 +2226,7 @@
       </c>
       <c r="X13" s="14" t="inlineStr">
         <is>
-          <t>maa://34957 (84.21), **maa://22768 (50.0)</t>
+          <t>maa://34957 (84.35), **maa://22768 (50.0)</t>
         </is>
       </c>
       <c r="Y13" s="11" t="n"/>
@@ -2308,7 +2308,7 @@
       </c>
       <c r="L14" s="14" t="inlineStr">
         <is>
-          <t>maa://39841 (94.51), maa://26245 (96.74), maa://21288 (96.3), maa://36682 (96.08)</t>
+          <t>maa://39841 (94.58), maa://26245 (96.74), maa://21288 (96.3), maa://36682 (96.08)</t>
         </is>
       </c>
       <c r="M14" s="11" t="n"/>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="D15" s="14" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.78), maa://22734 (84.55), *maa://30808 (64.38), *maa://36048 (69.91), maa://45058 (85.0)</t>
+          <t>*maa://22743 (78.78), maa://22734 (84.55), *maa://30808 (64.38), *maa://36048 (70.43), maa://45058 (85.71)</t>
         </is>
       </c>
       <c r="E15" s="11" t="n"/>
@@ -2422,7 +2422,7 @@
       </c>
       <c r="H15" s="14" t="inlineStr">
         <is>
-          <t>maa://24304 (87.36), maa://21478 (90.24)</t>
+          <t>maa://24304 (87.4), maa://21478 (90.24)</t>
         </is>
       </c>
       <c r="I15" s="11" t="n"/>
@@ -2454,7 +2454,7 @@
       </c>
       <c r="P15" s="14" t="inlineStr">
         <is>
-          <t>maa://24762 (91.53), *maa://22727 (70.0)</t>
+          <t>maa://24762 (91.05), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="11" t="n"/>
@@ -2518,7 +2518,7 @@
       </c>
       <c r="AF15" s="14" t="inlineStr">
         <is>
-          <t>maa://21364 (81.45), maa://36666 (82.21), *maa://22766 (68.55)</t>
+          <t>maa://21364 (81.45), maa://36666 (82.32), *maa://22766 (68.55)</t>
         </is>
       </c>
       <c r="AG15" s="27" t="n"/>
@@ -2600,7 +2600,7 @@
       </c>
       <c r="T16" s="14" t="inlineStr">
         <is>
-          <t>maa://22729 (94.54), *maa://28648 (74.39), maa://36674 (80.65)</t>
+          <t>maa://22729 (94.54), *maa://28648 (74.39), *maa://36674 (79.37)</t>
         </is>
       </c>
       <c r="U16" s="11" t="n"/>
@@ -2632,7 +2632,7 @@
       </c>
       <c r="AB16" s="14" t="inlineStr">
         <is>
-          <t>maa://26228 (95.65)</t>
+          <t>maa://26228 (95.69)</t>
         </is>
       </c>
       <c r="AC16" s="11" t="n"/>
@@ -2796,7 +2796,7 @@
       </c>
       <c r="D18" s="14" t="inlineStr">
         <is>
-          <t>maa://24570 (97.11)</t>
+          <t>maa://24570 (97.12)</t>
         </is>
       </c>
       <c r="E18" s="11" t="n"/>
@@ -2812,7 +2812,7 @@
       </c>
       <c r="H18" s="14" t="inlineStr">
         <is>
-          <t>maa://24421 (87.02)</t>
+          <t>maa://24421 (87.06)</t>
         </is>
       </c>
       <c r="I18" s="11" t="n"/>
@@ -2876,7 +2876,7 @@
       </c>
       <c r="X18" s="14" t="inlineStr">
         <is>
-          <t>maa://21917 (97.14), maa://22741 (87.5)</t>
+          <t>maa://21917 (97.17), maa://22741 (87.5)</t>
         </is>
       </c>
       <c r="Y18" s="11" t="n"/>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="AF18" s="14" t="inlineStr">
         <is>
-          <t>*maa://24313 (60.12), **maa://29784 (50.0), maa://47854 (82.35)</t>
+          <t>*maa://24313 (60.12), **maa://29784 (50.0), maa://47854 (83.33)</t>
         </is>
       </c>
       <c r="AG18" s="27" t="n"/>
@@ -3136,7 +3136,7 @@
       </c>
       <c r="X20" s="14" t="inlineStr">
         <is>
-          <t>maa://50085 (88.74), maa://49976 (86.75), maa://56241 (88.89)</t>
+          <t>maa://50085 (88.96), maa://49976 (86.75), maa://56241 (88.89)</t>
         </is>
       </c>
       <c r="Y20" s="11" t="n"/>
@@ -3186,7 +3186,7 @@
       </c>
       <c r="D21" s="14" t="inlineStr">
         <is>
-          <t>maa://21261 (98.08)</t>
+          <t>maa://21261 (98.11)</t>
         </is>
       </c>
       <c r="E21" s="11" t="n"/>
@@ -3282,7 +3282,7 @@
       </c>
       <c r="AB21" s="14" t="inlineStr">
         <is>
-          <t>maa://21443 (82.93)</t>
+          <t>maa://21443 (82.97)</t>
         </is>
       </c>
       <c r="AC21" s="11" t="n"/>
@@ -3446,7 +3446,7 @@
       </c>
       <c r="D23" s="14" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.4), **maa://41753 (48.28)</t>
+          <t>***maa://28036 (28.05), **maa://41753 (46.67)</t>
         </is>
       </c>
       <c r="E23" s="11" t="n"/>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="L23" s="14" t="inlineStr">
         <is>
-          <t>maa://39756 (95.63), maa://39875 (93.75)</t>
+          <t>maa://39756 (95.63), maa://39875 (93.83)</t>
         </is>
       </c>
       <c r="M23" s="11" t="n"/>
@@ -3542,7 +3542,7 @@
       </c>
       <c r="AB23" s="14" t="inlineStr">
         <is>
-          <t>maa://29652 (97.96)</t>
+          <t>maa://29652 (98.0)</t>
         </is>
       </c>
       <c r="AC23" s="11" t="n"/>
@@ -3802,7 +3802,7 @@
       </c>
       <c r="AB25" s="14" t="inlineStr">
         <is>
-          <t>maa://31215 (89.86), *maa://24516 (79.57), maa://26001 (84.75)</t>
+          <t>maa://31215 (89.93), *maa://24516 (79.57), maa://26001 (84.75)</t>
         </is>
       </c>
       <c r="AC25" s="11" t="n"/>
@@ -4176,7 +4176,7 @@
       </c>
       <c r="X28" s="14" t="inlineStr">
         <is>
-          <t>maa://39929 (92.0), maa://41749 (92.36)</t>
+          <t>maa://39929 (92.02), maa://41749 (92.41)</t>
         </is>
       </c>
       <c r="Y28" s="11" t="n"/>
@@ -4242,7 +4242,7 @@
       </c>
       <c r="H29" s="14" t="inlineStr">
         <is>
-          <t>*maa://25175 (58.21)</t>
+          <t>*maa://25175 (57.35)</t>
         </is>
       </c>
       <c r="I29" s="11" t="n"/>
@@ -4518,7 +4518,7 @@
       </c>
       <c r="L31" s="14" t="inlineStr">
         <is>
-          <t>maa://35926 (93.79), maa://36258 (88.24), *maa://43904 (73.33)</t>
+          <t>maa://35926 (93.79), maa://36258 (88.3), *maa://43904 (73.33)</t>
         </is>
       </c>
       <c r="M31" s="11" t="n"/>
@@ -4680,7 +4680,7 @@
       </c>
       <c r="T32" s="14" t="inlineStr">
         <is>
-          <t>maa://42859 (97.06), maa://41108 (86.27), maa://41238 (98.04), maa://45523 (100.0)</t>
+          <t>maa://42859 (97.07), maa://41108 (86.27), maa://41238 (98.05), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="11" t="n"/>
@@ -4924,7 +4924,7 @@
       </c>
       <c r="P34" s="14" t="inlineStr">
         <is>
-          <t>maa://48817 (97.01), maa://56235 (100.0)</t>
+          <t>maa://48817 (97.06), maa://56235 (100.0)</t>
         </is>
       </c>
       <c r="Q34" s="11" t="n"/>
@@ -5500,7 +5500,7 @@
       </c>
       <c r="P39" s="14" t="inlineStr">
         <is>
-          <t>maa://24709 (92.0), maa://47093 (100.0)</t>
+          <t>maa://24709 (92.05), maa://47093 (100.0)</t>
         </is>
       </c>
       <c r="Q39" s="11" t="n"/>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="H43" s="14" t="inlineStr">
         <is>
-          <t>maa://22525 (83.83), maa://21284 (87.27)</t>
+          <t>maa://22525 (82.94), maa://21284 (87.27)</t>
         </is>
       </c>
       <c r="I43" s="11" t="n"/>
@@ -6407,7 +6407,7 @@
       </c>
       <c r="P52" s="14" t="inlineStr">
         <is>
-          <t>maa://59378 (97.56), maa://59394 (96.3)</t>
+          <t>maa://59378 (97.78), maa://59394 (96.3)</t>
         </is>
       </c>
       <c r="Q52" s="11" t="n"/>
@@ -6441,7 +6441,7 @@
       </c>
       <c r="H53" s="14" t="inlineStr">
         <is>
-          <t>maa://32534 (95.2)</t>
+          <t>maa://32534 (95.23)</t>
         </is>
       </c>
       <c r="I53" s="11" t="n"/>
@@ -6579,7 +6579,7 @@
       </c>
       <c r="H58" s="14" t="inlineStr">
         <is>
-          <t>*maa://37964 (55.17)</t>
+          <t>*maa://37964 (55.93)</t>
         </is>
       </c>
       <c r="I58" s="11" t="n"/>
@@ -6615,7 +6615,7 @@
       </c>
       <c r="H60" s="14" t="inlineStr">
         <is>
-          <t>*maa://40438 (75.31)</t>
+          <t>*maa://40438 (75.61)</t>
         </is>
       </c>
       <c r="I60" s="11" t="n"/>
@@ -6669,7 +6669,7 @@
       </c>
       <c r="H63" s="14" t="inlineStr">
         <is>
-          <t>maa://59534 (98.28), maa://59413 (100.0)</t>
+          <t>maa://59534 (98.39), maa://59413 (100.0)</t>
         </is>
       </c>
       <c r="I63" s="11" t="n"/>
@@ -6971,7 +6971,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A1" s="13" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.25 13:22:19</t>
+          <t>更新日期：2025.06.27 13:21:40</t>
         </is>
       </c>
       <c r="E1" s="16" t="inlineStr">
@@ -8483,7 +8483,7 @@
       </c>
       <c r="D29" s="20" t="inlineStr">
         <is>
-          <t>maa://20863 (88.8), maa://20832 (99.08), maa://20727 (100.0)</t>
+          <t>maa://20863 (88.84), maa://20832 (99.08), maa://20727 (100.0)</t>
         </is>
       </c>
       <c r="E29" s="21" t="inlineStr">
@@ -8645,7 +8645,7 @@
       </c>
       <c r="D32" s="20" t="inlineStr">
         <is>
-          <t>maa://36644 (88.48), maa://36866 (96.23), maa://45572 (91.67), maa://27794 (100.0), maa://20960 (100.0), maa://20843 (100.0), **maa://24483 (50.0), maa://20862 (83.33), *maa://20893 (77.78)</t>
+          <t>maa://36644 (88.54), maa://36866 (96.23), maa://45572 (91.67), maa://27794 (100.0), maa://20960 (100.0), maa://20843 (100.0), **maa://24483 (50.0), maa://20862 (83.33), *maa://20893 (77.78)</t>
         </is>
       </c>
       <c r="E32" s="21" t="inlineStr">
@@ -8699,7 +8699,7 @@
       </c>
       <c r="D33" s="20" t="inlineStr">
         <is>
-          <t>maa://30500 (98.89), *maa://27290 (70.59), ***maa://42154 (8.33)</t>
+          <t>maa://30500 (98.89), *maa://27290 (72.22), ***maa://42154 (8.33)</t>
         </is>
       </c>
       <c r="E33" s="21" t="inlineStr">
@@ -9941,7 +9941,7 @@
       </c>
       <c r="D56" s="20" t="inlineStr">
         <is>
-          <t>maa://44235 (98.24), maa://45604 (100.0), maa://20961 (100.0), maa://44220 (100.0), maa://20910 (100.0)</t>
+          <t>maa://44235 (98.25), maa://45604 (100.0), maa://20961 (100.0), maa://44220 (100.0), maa://20910 (100.0)</t>
         </is>
       </c>
       <c r="E56" s="21" t="inlineStr">
@@ -10211,7 +10211,7 @@
       </c>
       <c r="D61" s="20" t="inlineStr">
         <is>
-          <t>maa://20841 (100.0), maa://24093 (100.0), maa://31559 (94.59), maa://20924 (95.24), maa://25777 (100.0), maa://20631 (100.0), maa://28241 (100.0)</t>
+          <t>maa://20841 (100.0), maa://24093 (100.0), maa://31559 (94.74), maa://20924 (95.24), maa://25777 (100.0), maa://20631 (100.0), maa://28241 (100.0)</t>
         </is>
       </c>
       <c r="E61" s="21" t="inlineStr">
@@ -12749,7 +12749,7 @@
       </c>
       <c r="D108" s="20" t="inlineStr">
         <is>
-          <t>maa://25018 (96.66), maa://51881 (99.2), maa://25776 (92.11), maa://28361 (95.0), maa://25772 (94.12), maa://56588 (94.74), maa://45194 (82.35), maa://32653 (85.71), maa://25161 (81.25)</t>
+          <t>maa://25018 (96.66), maa://51881 (99.21), maa://25776 (92.11), maa://28361 (95.0), maa://25772 (94.12), maa://56588 (94.74), maa://45194 (82.35), maa://32653 (85.71), maa://25161 (81.25)</t>
         </is>
       </c>
       <c r="E108" s="21" t="inlineStr">
@@ -13019,7 +13019,7 @@
       </c>
       <c r="D113" s="20" t="inlineStr">
         <is>
-          <t>maa://29037 (98.48)</t>
+          <t>maa://29037 (98.51)</t>
         </is>
       </c>
       <c r="E113" s="21" t="inlineStr">
@@ -14963,7 +14963,7 @@
       </c>
       <c r="D149" s="20" t="inlineStr">
         <is>
-          <t>maa://36641 (98.44), maa://40957 (93.79), maa://36865 (96.34), maa://44635 (88.07), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
+          <t>maa://36641 (98.44), maa://40957 (93.87), maa://36865 (95.76), maa://44635 (88.07), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
         </is>
       </c>
       <c r="E149" s="21" t="inlineStr">
@@ -15498,12 +15498,12 @@
       </c>
       <c r="C159" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D159" s="20" t="inlineStr">
         <is>
-          <t>maa://44232 (98.58), maa://45603 (90.62), maa://44305 (100.0)</t>
+          <t>maa://44232 (98.59), maa://45603 (90.62)</t>
         </is>
       </c>
       <c r="E159" s="21" t="inlineStr">
@@ -15881,7 +15881,7 @@
       </c>
       <c r="D166" s="20" t="inlineStr">
         <is>
-          <t>maa://20975 (90.91), maa://30806 (100.0), *maa://47950 (75.0)</t>
+          <t>maa://20975 (90.91), maa://30806 (100.0), *maa://47950 (80.0)</t>
         </is>
       </c>
       <c r="E166" s="21" t="inlineStr">
@@ -15935,7 +15935,7 @@
       </c>
       <c r="D167" s="20" t="inlineStr">
         <is>
-          <t>maa://29633 (92.31), maa://29627 (92.69), maa://29659 (85.71), maa://49074 (97.73), **maa://30679 (50.0), maa://29861 (100.0), maa://42343 (100.0)</t>
+          <t>maa://29633 (92.31), maa://29627 (92.69), maa://29659 (85.71), maa://49074 (97.78), **maa://30679 (50.0), maa://29861 (100.0), maa://42343 (100.0)</t>
         </is>
       </c>
       <c r="E167" s="21" t="inlineStr">
@@ -16475,7 +16475,7 @@
       </c>
       <c r="D177" s="20" t="inlineStr">
         <is>
-          <t>maa://20842 (92.86)</t>
+          <t>maa://20842 (93.33)</t>
         </is>
       </c>
       <c r="E177" s="21" t="inlineStr">
@@ -17555,7 +17555,7 @@
       </c>
       <c r="D197" s="20" t="inlineStr">
         <is>
-          <t>maa://44224 (90.32), maa://35854 (86.02), maa://50388 (97.92), maa://25760 (86.96), ***maa://43911 (13.04), *maa://20872 (52.0), maa://51066 (100.0)</t>
+          <t>maa://44224 (90.32), maa://35854 (85.42), maa://50388 (97.93), maa://25760 (86.96), ***maa://43911 (13.04), *maa://20872 (52.0), maa://51066 (100.0)</t>
         </is>
       </c>
       <c r="E197" s="21" t="inlineStr">
@@ -18311,7 +18311,7 @@
       </c>
       <c r="D211" s="20" t="inlineStr">
         <is>
-          <t>maa://20956 (95.85), *maa://20830 (80.0), maa://44703 (91.67)</t>
+          <t>maa://20956 (95.9), *maa://20830 (80.0), maa://44703 (91.67)</t>
         </is>
       </c>
       <c r="E211" s="21" t="inlineStr">
@@ -19391,7 +19391,7 @@
       </c>
       <c r="D231" s="20" t="inlineStr">
         <is>
-          <t>maa://29058 (96.1), maa://39140 (100.0), maa://38723 (100.0)</t>
+          <t>maa://29058 (96.15), maa://39140 (100.0), maa://38723 (100.0)</t>
         </is>
       </c>
       <c r="E231" s="21" t="inlineStr">
@@ -20525,7 +20525,7 @@
       </c>
       <c r="D252" s="20" t="inlineStr">
         <is>
-          <t>maa://24093 (100.0), maa://31559 (94.59), maa://20924 (95.24), **maa://49440 (50.0)</t>
+          <t>maa://24093 (100.0), maa://31559 (94.74), maa://20924 (95.24), **maa://49440 (50.0)</t>
         </is>
       </c>
       <c r="E252" s="21" t="inlineStr">
@@ -21497,7 +21497,7 @@
       </c>
       <c r="D270" s="20" t="inlineStr">
         <is>
-          <t>maa://25769 (97.44)</t>
+          <t>maa://25769 (97.45)</t>
         </is>
       </c>
       <c r="E270" s="21" t="inlineStr">
@@ -21605,7 +21605,7 @@
       </c>
       <c r="D272" s="20" t="inlineStr">
         <is>
-          <t>maa://51881 (99.2), maa://51630 (96.59), maa://56588 (94.74), *maa://55171 (57.14), maa://51893 (88.89)</t>
+          <t>maa://51881 (99.21), maa://51630 (96.59), maa://56588 (94.74), *maa://55171 (57.14), maa://51893 (88.89)</t>
         </is>
       </c>
       <c r="E272" s="21" t="inlineStr">
@@ -23549,7 +23549,7 @@
       </c>
       <c r="D308" s="20" t="inlineStr">
         <is>
-          <t>maa://36005 (92.31)</t>
+          <t>maa://36005 (92.86)</t>
         </is>
       </c>
       <c r="E308" s="21" t="inlineStr">
@@ -26411,7 +26411,7 @@
       </c>
       <c r="D361" s="17" t="inlineStr">
         <is>
-          <t>maa://40957 (93.79), maa://44635 (88.07), maa://48026 (94.85), maa://41035 (92.65), maa://44660 (92.31), maa://41128 (83.78), maa://60251 (85.71)</t>
+          <t>maa://40957 (93.87), maa://44635 (88.07), maa://48026 (95.0), maa://41035 (92.65), maa://44660 (92.31), maa://41128 (83.78), *maa://60251 (75.0)</t>
         </is>
       </c>
       <c r="E361" s="17" t="inlineStr">
@@ -27113,7 +27113,7 @@
       </c>
       <c r="D374" s="17" t="inlineStr">
         <is>
-          <t>maa://43872 (90.91)</t>
+          <t>maa://43872 (91.67)</t>
         </is>
       </c>
       <c r="E374" s="17" t="inlineStr">
@@ -27275,7 +27275,7 @@
       </c>
       <c r="D377" s="17" t="inlineStr">
         <is>
-          <t>maa://42970 (83.33), maa://44745 (98.25), **maa://49516 (38.1), *maa://45952 (80.0), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
+          <t>maa://42970 (83.14), maa://44745 (98.33), **maa://49516 (38.1), *maa://45952 (80.0), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E377" s="17" t="inlineStr">
@@ -28085,7 +28085,7 @@
       </c>
       <c r="D392" s="17" t="inlineStr">
         <is>
-          <t>maa://51880 (99.23), maa://51878 (100.0), maa://56651 (100.0)</t>
+          <t>maa://51880 (99.09), maa://51878 (100.0), maa://56651 (100.0)</t>
         </is>
       </c>
       <c r="E392" s="17" t="inlineStr">
@@ -28139,7 +28139,7 @@
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>maa://51872 (96.82), maa://51876 (98.82), maa://51873 (100.0)</t>
+          <t>maa://51872 (96.86), maa://51876 (98.85), maa://51873 (100.0)</t>
         </is>
       </c>
       <c r="E393" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#207)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -706,7 +706,7 @@
       </c>
       <c r="D2" s="14" t="inlineStr">
         <is>
-          <t>maa://25390 (95.52), maa://24702 (94.87), maa://36681 (86.42)</t>
+          <t>maa://25390 (95.54), maa://24702 (94.87), maa://36681 (86.42)</t>
         </is>
       </c>
       <c r="E2" s="11" t="n"/>
@@ -738,7 +738,7 @@
       </c>
       <c r="L2" s="14" t="inlineStr">
         <is>
-          <t>maa://39402 (95.0), *maa://34787 (73.91), maa://58660 (83.33)</t>
+          <t>maa://39402 (95.04), *maa://34787 (73.91), maa://58660 (83.33)</t>
         </is>
       </c>
       <c r="M2" s="11" t="n"/>
@@ -802,7 +802,7 @@
       </c>
       <c r="AB2" s="14" t="inlineStr">
         <is>
-          <t>maa://21246 (91.48), maa://36684 (93.29)</t>
+          <t>maa://21246 (91.48), maa://36684 (93.33)</t>
         </is>
       </c>
       <c r="AC2" s="11" t="n"/>
@@ -818,7 +818,7 @@
       </c>
       <c r="AF2" s="14" t="inlineStr">
         <is>
-          <t>maa://25251 (91.91), maa://59087 (92.31)</t>
+          <t>maa://25251 (91.91), maa://59087 (92.86)</t>
         </is>
       </c>
       <c r="AG2" s="27" t="n"/>
@@ -852,7 +852,7 @@
       </c>
       <c r="H3" s="14" t="inlineStr">
         <is>
-          <t>maa://21247 (98.48)</t>
+          <t>maa://21247 (98.49)</t>
         </is>
       </c>
       <c r="I3" s="11" t="n"/>
@@ -932,7 +932,7 @@
       </c>
       <c r="AB3" s="14" t="inlineStr">
         <is>
-          <t>maa://24390 (95.74), maa://52241 (92.31)</t>
+          <t>maa://24390 (95.74), maa://52241 (92.86)</t>
         </is>
       </c>
       <c r="AC3" s="11" t="n"/>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="P4" s="14" t="inlineStr">
         <is>
-          <t>maa://49983 (96.43), maa://50121 (95.12)</t>
+          <t>maa://49983 (96.51), maa://50121 (95.12)</t>
         </is>
       </c>
       <c r="Q4" s="11" t="n"/>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="AF4" s="14" t="inlineStr">
         <is>
-          <t>*maa://30062 (66.07), *maa://39394 (66.67), ***maa://26209 (13.04)</t>
+          <t>*maa://30062 (66.07), *maa://39394 (67.74), ***maa://26209 (13.04)</t>
         </is>
       </c>
       <c r="AG4" s="27" t="n"/>
@@ -1263,7 +1263,7 @@
       </c>
       <c r="L6" s="14" t="inlineStr">
         <is>
-          <t>maa://24839 (98.84)</t>
+          <t>maa://24839 (98.85)</t>
         </is>
       </c>
       <c r="M6" s="11" t="n"/>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="X6" s="14" t="inlineStr">
         <is>
-          <t>maa://52754 (84.21)</t>
+          <t>maa://52754 (85.0)</t>
         </is>
       </c>
       <c r="Y6" s="11" t="n"/>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="X7" s="14" t="inlineStr">
         <is>
-          <t>maa://22399 (95.7), *maa://22758 (77.78)</t>
+          <t>maa://22399 (95.72), *maa://22758 (77.78)</t>
         </is>
       </c>
       <c r="Y7" s="11" t="n"/>
@@ -1473,7 +1473,7 @@
       </c>
       <c r="AF7" s="14" t="inlineStr">
         <is>
-          <t>maa://45272 (97.14)</t>
+          <t>maa://45272 (97.22)</t>
         </is>
       </c>
       <c r="AG7" s="27" t="n"/>
@@ -1481,7 +1481,7 @@
     <row r="8">
       <c r="A8" s="10" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.27 13:21:40</t>
+          <t>更新日期：2025.06.29 13:23:12</t>
         </is>
       </c>
       <c r="B8" s="11" t="inlineStr">
@@ -2146,7 +2146,7 @@
       </c>
       <c r="D13" s="14" t="inlineStr">
         <is>
-          <t>maa://24999 (92.78), maa://36673 (92.05), maa://25001 (86.49)</t>
+          <t>maa://24999 (92.79), maa://36673 (92.13), maa://25001 (86.49)</t>
         </is>
       </c>
       <c r="E13" s="11" t="n"/>
@@ -2194,7 +2194,7 @@
       </c>
       <c r="P13" s="14" t="inlineStr">
         <is>
-          <t>maa://22676 (93.66), *maa://22583 (78.05), maa://48321 (85.71)</t>
+          <t>maa://22676 (93.66), *maa://22583 (78.31), maa://48321 (85.71)</t>
         </is>
       </c>
       <c r="Q13" s="11" t="n"/>
@@ -2308,7 +2308,7 @@
       </c>
       <c r="L14" s="14" t="inlineStr">
         <is>
-          <t>maa://39841 (94.58), maa://26245 (96.74), maa://21288 (96.3), maa://36682 (96.08)</t>
+          <t>maa://39841 (94.58), maa://26245 (96.74), maa://21288 (96.3), maa://36682 (96.15)</t>
         </is>
       </c>
       <c r="M14" s="11" t="n"/>
@@ -2422,7 +2422,7 @@
       </c>
       <c r="H15" s="14" t="inlineStr">
         <is>
-          <t>maa://24304 (87.4), maa://21478 (90.24)</t>
+          <t>maa://24304 (87.45), maa://21478 (90.24)</t>
         </is>
       </c>
       <c r="I15" s="11" t="n"/>
@@ -2486,7 +2486,7 @@
       </c>
       <c r="X15" s="14" t="inlineStr">
         <is>
-          <t>*maa://38786 (70.0), maa://56102 (100.0)</t>
+          <t>*maa://38786 (72.73), maa://56102 (100.0)</t>
         </is>
       </c>
       <c r="Y15" s="11" t="n"/>
@@ -2600,7 +2600,7 @@
       </c>
       <c r="T16" s="14" t="inlineStr">
         <is>
-          <t>maa://22729 (94.54), *maa://28648 (74.39), *maa://36674 (79.37)</t>
+          <t>maa://22729 (94.57), *maa://28648 (74.39), *maa://36674 (79.37)</t>
         </is>
       </c>
       <c r="U16" s="11" t="n"/>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="AF18" s="14" t="inlineStr">
         <is>
-          <t>*maa://24313 (60.12), **maa://29784 (50.0), maa://47854 (83.33)</t>
+          <t>*maa://24313 (60.12), **maa://29784 (50.0), *maa://47854 (78.95)</t>
         </is>
       </c>
       <c r="AG18" s="27" t="n"/>
@@ -3298,7 +3298,7 @@
       </c>
       <c r="AF21" s="14" t="inlineStr">
         <is>
-          <t>maa://22524 (88.14), maa://22432 (82.96)</t>
+          <t>maa://22524 (88.14), maa://22432 (82.61)</t>
         </is>
       </c>
       <c r="AG21" s="27" t="n"/>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="L23" s="14" t="inlineStr">
         <is>
-          <t>maa://39756 (95.63), maa://39875 (93.83)</t>
+          <t>maa://39756 (95.65), maa://39875 (93.83)</t>
         </is>
       </c>
       <c r="M23" s="11" t="n"/>
@@ -3494,7 +3494,7 @@
       </c>
       <c r="P23" s="14" t="inlineStr">
         <is>
-          <t>maa://30587 (92.13), *maa://29748 (76.3), *maa://37566 (78.72)</t>
+          <t>maa://30587 (92.17), *maa://29748 (76.3), *maa://37566 (78.72)</t>
         </is>
       </c>
       <c r="Q23" s="11" t="n"/>
@@ -3688,7 +3688,7 @@
       </c>
       <c r="AF24" s="14" t="inlineStr">
         <is>
-          <t>maa://22523 (81.74), *maa://36672 (75.0), maa://29910 (93.85), maa://45831 (87.5)</t>
+          <t>maa://22523 (81.74), *maa://36672 (73.91), maa://29910 (93.85), maa://45831 (87.5)</t>
         </is>
       </c>
       <c r="AG24" s="27" t="n"/>
@@ -3706,7 +3706,7 @@
       </c>
       <c r="D25" s="14" t="inlineStr">
         <is>
-          <t>maa://29753 (95.48)</t>
+          <t>maa://29753 (95.5)</t>
         </is>
       </c>
       <c r="E25" s="11" t="n"/>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="X25" s="14" t="inlineStr">
         <is>
-          <t>maa://29890 (83.33)</t>
+          <t>maa://29890 (81.97)</t>
         </is>
       </c>
       <c r="Y25" s="11" t="n"/>
@@ -3932,7 +3932,7 @@
       </c>
       <c r="AB26" s="14" t="inlineStr">
         <is>
-          <t>maa://42235 (96.18)</t>
+          <t>maa://42235 (96.2)</t>
         </is>
       </c>
       <c r="AC26" s="11" t="n"/>
@@ -4030,7 +4030,7 @@
       </c>
       <c r="T27" s="14" t="inlineStr">
         <is>
-          <t>*maa://30624 (77.63)</t>
+          <t>*maa://30624 (77.92)</t>
         </is>
       </c>
       <c r="U27" s="11" t="n"/>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="D28" s="14" t="inlineStr">
         <is>
-          <t>maa://24465 (90.71), maa://25725 (82.83)</t>
+          <t>maa://24465 (90.72), maa://25725 (82.83)</t>
         </is>
       </c>
       <c r="E28" s="11" t="n"/>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="L29" s="14" t="inlineStr">
         <is>
-          <t>maa://28432 (94.12), maa://31400 (98.9), maa://28440 (84.51), *maa://28650 (71.43)</t>
+          <t>maa://28432 (94.15), maa://31400 (98.9), maa://28440 (84.62), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="11" t="n"/>
@@ -4452,7 +4452,7 @@
       </c>
       <c r="AB30" s="14" t="inlineStr">
         <is>
-          <t>maa://42979 (97.15), maa://45822 (100.0), maa://45045 (83.33)</t>
+          <t>maa://42979 (97.18), maa://45822 (100.0), maa://45045 (83.33)</t>
         </is>
       </c>
       <c r="AC30" s="11" t="n"/>
@@ -4582,7 +4582,7 @@
       </c>
       <c r="AB31" s="14" t="inlineStr">
         <is>
-          <t>***maa://51420 (16.67)</t>
+          <t>***maa://51420 (14.29)</t>
         </is>
       </c>
       <c r="AC31" s="11" t="n"/>
@@ -4632,7 +4632,7 @@
       </c>
       <c r="H32" s="14" t="inlineStr">
         <is>
-          <t>maa://21895 (97.67), maa://36667 (97.37), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.68), maa://36667 (97.39), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="11" t="n"/>
@@ -4680,7 +4680,7 @@
       </c>
       <c r="T32" s="14" t="inlineStr">
         <is>
-          <t>maa://42859 (97.07), maa://41108 (86.27), maa://41238 (98.05), maa://45523 (100.0)</t>
+          <t>maa://42859 (97.1), maa://41108 (86.27), maa://41238 (98.05), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="11" t="n"/>
@@ -4940,7 +4940,7 @@
       </c>
       <c r="T34" s="14" t="inlineStr">
         <is>
-          <t>maa://24526 (92.45)</t>
+          <t>maa://24526 (92.47)</t>
         </is>
       </c>
       <c r="U34" s="11" t="n"/>
@@ -5282,7 +5282,7 @@
       </c>
       <c r="L37" s="14" t="inlineStr">
         <is>
-          <t>maa://45718 (98.48), maa://47069 (81.82), maa://56336 (90.0), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.5), maa://47069 (81.82), maa://56336 (90.0), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="11" t="n"/>
@@ -5447,7 +5447,7 @@
       </c>
       <c r="AF38" s="14" t="inlineStr">
         <is>
-          <t>maa://36697 (89.23)</t>
+          <t>maa://36697 (89.26)</t>
         </is>
       </c>
       <c r="AG38" s="27" t="n"/>
@@ -5463,12 +5463,12 @@
       </c>
       <c r="G39" s="11" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H39" s="14" t="inlineStr">
         <is>
-          <t>maa://36670 (88.89), maa://25199 (85.47), maa://30434 (93.43), *maa://45059 (77.14)</t>
+          <t>maa://36670 (88.89), maa://25199 (85.47), maa://30434 (93.43), *maa://45059 (77.14), *maa://44165 (75.0)</t>
         </is>
       </c>
       <c r="I39" s="11" t="n"/>
@@ -6407,7 +6407,7 @@
       </c>
       <c r="P52" s="14" t="inlineStr">
         <is>
-          <t>maa://59378 (97.78), maa://59394 (96.3)</t>
+          <t>maa://59378 (97.78), maa://59394 (96.43)</t>
         </is>
       </c>
       <c r="Q52" s="11" t="n"/>
@@ -6651,7 +6651,7 @@
       </c>
       <c r="H62" s="14" t="inlineStr">
         <is>
-          <t>maa://42981 (96.67), maa://43903 (100.0), maa://56228 (100.0)</t>
+          <t>maa://42981 (96.72), maa://43903 (100.0), maa://56228 (100.0)</t>
         </is>
       </c>
       <c r="I62" s="11" t="n"/>
@@ -6669,7 +6669,7 @@
       </c>
       <c r="H63" s="14" t="inlineStr">
         <is>
-          <t>maa://59534 (98.39), maa://59413 (100.0)</t>
+          <t>maa://59534 (98.46), maa://59413 (100.0)</t>
         </is>
       </c>
       <c r="I63" s="11" t="n"/>
@@ -6971,7 +6971,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="17">
       <c r="A1" s="13" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.27 13:21:40</t>
+          <t>更新日期：2025.06.29 13:23:12</t>
         </is>
       </c>
       <c r="E1" s="16" t="inlineStr">
@@ -8645,7 +8645,7 @@
       </c>
       <c r="D32" s="20" t="inlineStr">
         <is>
-          <t>maa://36644 (88.54), maa://36866 (96.23), maa://45572 (91.67), maa://27794 (100.0), maa://20960 (100.0), maa://20843 (100.0), **maa://24483 (50.0), maa://20862 (83.33), *maa://20893 (77.78)</t>
+          <t>maa://36644 (88.08), maa://36866 (96.23), maa://45572 (91.67), maa://27794 (100.0), maa://20960 (100.0), maa://20843 (100.0), **maa://24483 (50.0), maa://20862 (83.33), *maa://20893 (77.78)</t>
         </is>
       </c>
       <c r="E32" s="21" t="inlineStr">
@@ -9779,7 +9779,7 @@
       </c>
       <c r="D53" s="20" t="inlineStr">
         <is>
-          <t>maa://20953 (96.0), maa://31173 (96.3)</t>
+          <t>maa://20953 (96.0), maa://31173 (96.43)</t>
         </is>
       </c>
       <c r="E53" s="21" t="inlineStr">
@@ -10643,7 +10643,7 @@
       </c>
       <c r="D69" s="20" t="inlineStr">
         <is>
-          <t>maa://20974 (96.43), maa://29079 (80.95), maa://29096 (95.65), maa://29087 (100.0), *maa://20823 (80.0), maa://20855 (93.75), maa://20904 (100.0)</t>
+          <t>maa://20974 (96.47), maa://29079 (80.95), maa://29096 (95.65), maa://29087 (100.0), *maa://20823 (80.0), maa://20855 (93.75), maa://20904 (100.0)</t>
         </is>
       </c>
       <c r="E69" s="21" t="inlineStr">
@@ -11669,7 +11669,7 @@
       </c>
       <c r="D88" s="20" t="inlineStr">
         <is>
-          <t>maa://24472 (88.41), *maa://35841 (64.71)</t>
+          <t>maa://24472 (88.46), *maa://35841 (64.71)</t>
         </is>
       </c>
       <c r="E88" s="21" t="inlineStr">
@@ -12533,7 +12533,7 @@
       </c>
       <c r="D104" s="20" t="inlineStr">
         <is>
-          <t>*maa://20966 (80.0)</t>
+          <t>maa://20966 (83.33)</t>
         </is>
       </c>
       <c r="E104" s="21" t="inlineStr">
@@ -12744,12 +12744,12 @@
       </c>
       <c r="C108" s="19" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D108" s="20" t="inlineStr">
         <is>
-          <t>maa://25018 (96.66), maa://51881 (99.21), maa://25776 (92.11), maa://28361 (95.0), maa://25772 (94.12), maa://56588 (94.74), maa://45194 (82.35), maa://32653 (85.71), maa://25161 (81.25)</t>
+          <t>maa://25018 (96.68), maa://51881 (99.21), maa://25776 (92.11), maa://28361 (95.0), maa://25772 (94.12), maa://56588 (94.74), maa://45194 (82.35), maa://32653 (85.71), maa://25161 (81.25), maa://60902 (100.0)</t>
         </is>
       </c>
       <c r="E108" s="21" t="inlineStr">
@@ -13127,7 +13127,7 @@
       </c>
       <c r="D115" s="20" t="inlineStr">
         <is>
-          <t>maa://20908 (98.04), maa://35723 (95.92), *maa://23346 (77.78), maa://38822 (100.0), maa://58659 (100.0)</t>
+          <t>maa://20908 (98.05), maa://35723 (95.92), *maa://23346 (77.78), maa://38822 (100.0), maa://58659 (100.0)</t>
         </is>
       </c>
       <c r="E115" s="21" t="inlineStr">
@@ -13235,7 +13235,7 @@
       </c>
       <c r="D117" s="20" t="inlineStr">
         <is>
-          <t>maa://31560 (87.5), maa://20940 (100.0)</t>
+          <t>maa://31560 (88.89), maa://20940 (100.0)</t>
         </is>
       </c>
       <c r="E117" s="21" t="inlineStr">
@@ -13343,7 +13343,7 @@
       </c>
       <c r="D119" s="20" t="inlineStr">
         <is>
-          <t>maa://31560 (87.5), maa://20851 (100.0)</t>
+          <t>maa://31560 (88.89), maa://20851 (100.0)</t>
         </is>
       </c>
       <c r="E119" s="21" t="inlineStr">
@@ -13505,7 +13505,7 @@
       </c>
       <c r="D122" s="20" t="inlineStr">
         <is>
-          <t>maa://29650 (98.31), maa://45570 (98.04)</t>
+          <t>maa://29650 (98.31), maa://45570 (96.23)</t>
         </is>
       </c>
       <c r="E122" s="21" t="inlineStr">
@@ -13937,7 +13937,7 @@
       </c>
       <c r="D130" s="20" t="inlineStr">
         <is>
-          <t>maa://21422 (99.1)</t>
+          <t>maa://21422 (99.11)</t>
         </is>
       </c>
       <c r="E130" s="21" t="inlineStr">
@@ -14963,7 +14963,7 @@
       </c>
       <c r="D149" s="20" t="inlineStr">
         <is>
-          <t>maa://36641 (98.44), maa://40957 (93.87), maa://36865 (95.76), maa://44635 (88.07), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
+          <t>maa://36641 (98.44), maa://40957 (93.99), maa://36865 (95.76), maa://44635 (88.07), maa://44660 (92.31), maa://41128 (83.78), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
         </is>
       </c>
       <c r="E149" s="21" t="inlineStr">
@@ -15881,7 +15881,7 @@
       </c>
       <c r="D166" s="20" t="inlineStr">
         <is>
-          <t>maa://20975 (90.91), maa://30806 (100.0), *maa://47950 (80.0)</t>
+          <t>maa://20975 (90.91), *maa://47950 (80.0), maa://30806 (100.0)</t>
         </is>
       </c>
       <c r="E166" s="21" t="inlineStr">
@@ -15935,7 +15935,7 @@
       </c>
       <c r="D167" s="20" t="inlineStr">
         <is>
-          <t>maa://29633 (92.31), maa://29627 (92.69), maa://29659 (85.71), maa://49074 (97.78), **maa://30679 (50.0), maa://29861 (100.0), maa://42343 (100.0)</t>
+          <t>maa://29633 (92.31), maa://29627 (92.69), maa://29659 (85.71), maa://49074 (97.83), **maa://30679 (50.0), maa://29861 (100.0), maa://42343 (100.0)</t>
         </is>
       </c>
       <c r="E167" s="21" t="inlineStr">
@@ -15989,7 +15989,7 @@
       </c>
       <c r="D168" s="20" t="inlineStr">
         <is>
-          <t>maa://49867 (90.62), maa://49655 (96.3)</t>
+          <t>maa://49867 (90.91), maa://49655 (96.3)</t>
         </is>
       </c>
       <c r="E168" s="21" t="inlineStr">
@@ -16745,7 +16745,7 @@
       </c>
       <c r="D182" s="20" t="inlineStr">
         <is>
-          <t>maa://31560 (87.5), *maa://20968 (66.67)</t>
+          <t>maa://31560 (88.89), *maa://20968 (66.67)</t>
         </is>
       </c>
       <c r="E182" s="21" t="inlineStr">
@@ -17555,7 +17555,7 @@
       </c>
       <c r="D197" s="20" t="inlineStr">
         <is>
-          <t>maa://44224 (90.32), maa://35854 (85.42), maa://50388 (97.93), maa://25760 (86.96), ***maa://43911 (13.04), *maa://20872 (52.0), maa://51066 (100.0)</t>
+          <t>maa://44224 (90.13), maa://35854 (85.42), maa://50388 (97.93), maa://25760 (86.96), ***maa://43911 (13.04), *maa://20872 (52.0), maa://51066 (100.0)</t>
         </is>
       </c>
       <c r="E197" s="21" t="inlineStr">
@@ -17609,7 +17609,7 @@
       </c>
       <c r="D198" s="20" t="inlineStr">
         <is>
-          <t>maa://39156 (93.98), *maa://39550 (57.89), *maa://53417 (66.67)</t>
+          <t>maa://39156 (93.98), *maa://39550 (57.89), *maa://53417 (71.43)</t>
         </is>
       </c>
       <c r="E198" s="21" t="inlineStr">
@@ -18311,7 +18311,7 @@
       </c>
       <c r="D211" s="20" t="inlineStr">
         <is>
-          <t>maa://20956 (95.9), *maa://20830 (80.0), maa://44703 (91.67)</t>
+          <t>maa://20956 (95.94), *maa://20830 (80.0), maa://44703 (91.67)</t>
         </is>
       </c>
       <c r="E211" s="21" t="inlineStr">
@@ -20309,7 +20309,7 @@
       </c>
       <c r="D248" s="20" t="inlineStr">
         <is>
-          <t>maa://28923 (92.27), maa://28906 (98.28), ***maa://28825 (11.54)</t>
+          <t>maa://28923 (92.35), maa://28906 (98.28), ***maa://28825 (11.54)</t>
         </is>
       </c>
       <c r="E248" s="21" t="inlineStr">
@@ -20363,7 +20363,7 @@
       </c>
       <c r="D249" s="20" t="inlineStr">
         <is>
-          <t>maa://42287 (90.8), maa://45570 (98.04), maa://42225 (100.0)</t>
+          <t>maa://42287 (91.01), maa://45570 (96.23), maa://42225 (100.0)</t>
         </is>
       </c>
       <c r="E249" s="21" t="inlineStr">
@@ -20687,7 +20687,7 @@
       </c>
       <c r="D255" s="20" t="inlineStr">
         <is>
-          <t>maa://20877 (98.67), *maa://45067 (75.0), maa://20836 (100.0), maa://20632 (100.0)</t>
+          <t>maa://20877 (98.68), *maa://45067 (75.0), maa://20836 (100.0), maa://20632 (100.0)</t>
         </is>
       </c>
       <c r="E255" s="21" t="inlineStr">
@@ -20903,7 +20903,7 @@
       </c>
       <c r="D259" s="20" t="inlineStr">
         <is>
-          <t>maa://31560 (87.5), maa://20884 (96.0)</t>
+          <t>maa://31560 (88.89), maa://20884 (96.0)</t>
         </is>
       </c>
       <c r="E259" s="21" t="inlineStr">
@@ -21600,12 +21600,12 @@
       </c>
       <c r="C272" s="19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D272" s="20" t="inlineStr">
         <is>
-          <t>maa://51881 (99.21), maa://51630 (96.59), maa://56588 (94.74), *maa://55171 (57.14), maa://51893 (88.89)</t>
+          <t>maa://51881 (99.21), maa://51630 (96.59), maa://56588 (94.74), *maa://55171 (57.14), maa://51893 (88.89), maa://60902 (100.0)</t>
         </is>
       </c>
       <c r="E272" s="21" t="inlineStr">
@@ -22361,7 +22361,7 @@
       </c>
       <c r="D286" s="20" t="inlineStr">
         <is>
-          <t>maa://20899 (89.41), maa://46332 (95.24), ***maa://44744 (25.0)</t>
+          <t>maa://20899 (89.47), maa://46332 (95.24), ***maa://44744 (25.0)</t>
         </is>
       </c>
       <c r="E286" s="21" t="inlineStr">
@@ -23063,7 +23063,7 @@
       </c>
       <c r="D299" s="20" t="inlineStr">
         <is>
-          <t>maa://29005 (98.7), maa://31560 (87.5)</t>
+          <t>maa://29005 (98.7), maa://31560 (88.89)</t>
         </is>
       </c>
       <c r="E299" s="21" t="inlineStr">
@@ -23279,7 +23279,7 @@
       </c>
       <c r="D303" s="20" t="inlineStr">
         <is>
-          <t>maa://50280 (97.62), maa://49642 (96.94), maa://49660 (92.86), *maa://50517 (80.0)</t>
+          <t>maa://50280 (97.64), maa://49642 (96.94), maa://49660 (93.1), *maa://50517 (80.0)</t>
         </is>
       </c>
       <c r="E303" s="21" t="inlineStr">
@@ -23819,7 +23819,7 @@
       </c>
       <c r="D313" s="20" t="inlineStr">
         <is>
-          <t>maa://25775 (93.83), *maa://25393 (73.33)</t>
+          <t>maa://25775 (93.98), *maa://25393 (73.33)</t>
         </is>
       </c>
       <c r="E313" s="21" t="inlineStr">
@@ -24521,7 +24521,7 @@
       </c>
       <c r="D326" s="20" t="inlineStr">
         <is>
-          <t>maa://42316 (100.0)</t>
+          <t>maa://42316 (88.89)</t>
         </is>
       </c>
       <c r="E326" s="21" t="inlineStr">
@@ -24629,7 +24629,7 @@
       </c>
       <c r="D328" s="20" t="inlineStr">
         <is>
-          <t>maa://40956 (92.86)</t>
+          <t>maa://40956 (93.02)</t>
         </is>
       </c>
       <c r="E328" s="21" t="inlineStr">
@@ -24845,7 +24845,7 @@
       </c>
       <c r="D332" s="22" t="inlineStr">
         <is>
-          <t>maa://44234 (99.06)</t>
+          <t>maa://44234 (99.07)</t>
         </is>
       </c>
       <c r="E332" s="22" t="inlineStr">
@@ -25925,7 +25925,7 @@
       </c>
       <c r="D352" s="17" t="inlineStr">
         <is>
-          <t>maa://49696 (99.55), maa://49695 (100.0), maa://49758 (98.44), *maa://59402 (61.54), *maa://52357 (75.0)</t>
+          <t>maa://49696 (99.55), maa://49695 (100.0), maa://49758 (98.44), *maa://59402 (64.29), *maa://52357 (75.0)</t>
         </is>
       </c>
       <c r="E352" s="17" t="inlineStr">
@@ -26195,7 +26195,7 @@
       </c>
       <c r="D357" s="17" t="inlineStr">
         <is>
-          <t>maa://36645 (98.38), maa://36841 (92.65), maa://37484 (94.23), maa://37858 (93.33), maa://40489 (100.0), *maa://56268 (60.0)</t>
+          <t>maa://36645 (98.38), maa://36841 (92.65), maa://37484 (94.23), maa://37858 (93.33), *maa://56268 (60.0), maa://40489 (100.0)</t>
         </is>
       </c>
       <c r="E357" s="17" t="inlineStr">
@@ -26411,7 +26411,7 @@
       </c>
       <c r="D361" s="17" t="inlineStr">
         <is>
-          <t>maa://40957 (93.87), maa://44635 (88.07), maa://48026 (95.0), maa://41035 (92.65), maa://44660 (92.31), maa://41128 (83.78), *maa://60251 (75.0)</t>
+          <t>maa://40957 (93.99), maa://44635 (88.07), maa://48026 (95.19), maa://41035 (92.65), maa://44660 (92.31), maa://41128 (83.78), *maa://60251 (75.0)</t>
         </is>
       </c>
       <c r="E361" s="17" t="inlineStr">
@@ -27005,7 +27005,7 @@
       </c>
       <c r="D372" s="17" t="inlineStr">
         <is>
-          <t>maa://44233 (92.31), maa://45570 (98.04)</t>
+          <t>maa://44233 (90.57), maa://45570 (96.23)</t>
         </is>
       </c>
       <c r="E372" s="17" t="inlineStr">
@@ -27275,7 +27275,7 @@
       </c>
       <c r="D377" s="17" t="inlineStr">
         <is>
-          <t>maa://42970 (83.14), maa://44745 (98.33), **maa://49516 (38.1), *maa://45952 (80.0), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
+          <t>maa://42970 (82.82), maa://44745 (98.44), **maa://49516 (38.1), *maa://45952 (72.73), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E377" s="17" t="inlineStr">
@@ -28139,7 +28139,7 @@
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>maa://51872 (96.86), maa://51876 (98.85), maa://51873 (100.0)</t>
+          <t>maa://51872 (96.69), maa://51876 (98.86), maa://51873 (100.0)</t>
         </is>
       </c>
       <c r="E393" t="inlineStr">
@@ -28166,7 +28166,7 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>maa://59493 (96.52), maa://59603 (100.0), maa://60449 (100.0)</t>
+          <t>maa://59493 (96.55), maa://59603 (100.0), maa://60449 (100.0)</t>
         </is>
       </c>
       <c r="E394" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#209)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -705,7 +705,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (95.65), maa://24702 (94.87), maa://36681 (86.42)</t>
+          <t>maa://25390 (95.69), maa://24702 (94.87), maa://36681 (86.42)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -769,7 +769,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (91.59)</t>
+          <t>maa://22742 (91.63)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -835,7 +835,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (95.8), maa://36987 (96.3), maa://39849 (88.89)</t>
+          <t>maa://40192 (95.83), maa://36987 (96.3), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -878,12 +878,12 @@
       </c>
       <c r="O3" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (94.86), maa://26254 (97.44)</t>
+          <t>maa://21249 (94.9), maa://26254 (97.44), *maa://22738 (75.0)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -899,7 +899,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://45854 (81.55), maa://24617 (91.18)</t>
+          <t>maa://45854 (81.73), maa://24617 (91.18)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -931,7 +931,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://24390 (95.79), maa://52241 (93.33)</t>
+          <t>maa://24390 (95.79), maa://52241 (93.75)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (96.84), maa://50121 (95.35)</t>
+          <t>maa://49983 (96.88), maa://50121 (95.35)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1148,7 +1148,7 @@
       </c>
       <c r="P5" s="8" t="inlineStr">
         <is>
-          <t>maa://21919 (97.14), *maa://21281 (80.0)</t>
+          <t>maa://21919 (97.18), *maa://21281 (80.0)</t>
         </is>
       </c>
       <c r="Q5" s="19" t="n"/>
@@ -1392,7 +1392,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (94.27), maa://24957 (97.83)</t>
+          <t>maa://28624 (94.3), maa://24957 (97.83)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="P7" s="8" t="inlineStr">
         <is>
-          <t>maa://22750 (91.53)</t>
+          <t>maa://22750 (91.67)</t>
         </is>
       </c>
       <c r="Q7" s="19" t="n"/>
@@ -1480,7 +1480,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.07.11 13:25:31</t>
+          <t>更新日期：2025.07.12 13:21:48</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (95.3)</t>
+          <t>maa://21411 (95.31)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>*maa://24479 (76.77), *maa://21990 (51.85)</t>
+          <t>*maa://24479 (77.0), *maa://21990 (51.85)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1755,7 +1755,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.45), ***maa://39951 (11.54), ***maa://34206 (22.22), *maa://45271 (61.45), ***maa://39243 (25.0), **maa://54000 (50.0)</t>
+          <t>***maa://25695 (18.45), ***maa://39951 (11.54), ***maa://34206 (22.22), *maa://45271 (61.9), ***maa://39243 (25.0), **maa://54000 (50.0)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1867,7 +1867,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>*maa://25021 (53.15), *maa://22733 (65.91), **maa://22761 (50.0)</t>
+          <t>*maa://25021 (53.15), *maa://22733 (66.67), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1997,7 +1997,7 @@
       </c>
       <c r="AF11" s="8" t="inlineStr">
         <is>
-          <t>maa://31203 (96.77)</t>
+          <t>maa://31203 (96.88)</t>
         </is>
       </c>
       <c r="AG11" s="16" t="n"/>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (92.87), maa://36673 (92.22), maa://25001 (86.49)</t>
+          <t>maa://24999 (92.88), maa://36673 (92.22), maa://25001 (86.49)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2161,7 +2161,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.2), **maa://22728 (46.94)</t>
+          <t>*maa://21248 (73.94), **maa://22728 (46.94)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2193,7 +2193,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (93.75), *maa://22583 (78.57), maa://48321 (85.71)</t>
+          <t>maa://22676 (93.79), *maa://22583 (78.57), maa://48321 (85.71)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2225,7 +2225,7 @@
       </c>
       <c r="X13" s="8" t="inlineStr">
         <is>
-          <t>maa://34957 (84.62)</t>
+          <t>maa://34957 (84.75)</t>
         </is>
       </c>
       <c r="Y13" s="19" t="n"/>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (87.5), **maa://39885 (50.0)</t>
+          <t>maa://39883 (87.69), **maa://39885 (50.0)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (94.77), maa://26245 (96.83), maa://21288 (96.3), maa://36682 (96.23)</t>
+          <t>maa://39841 (94.8), maa://26245 (96.83), maa://21288 (96.3), maa://36682 (96.3)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2405,7 +2405,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.54), maa://22734 (84.55), *maa://30808 (64.38), *maa://36048 (70.09), maa://45058 (86.36)</t>
+          <t>*maa://22743 (78.54), maa://22734 (84.55), *maa://30808 (64.38), *maa://36048 (69.49), maa://45058 (86.36)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2517,7 +2517,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://21364 (81.65), maa://36666 (81.82), *maa://22766 (68.8)</t>
+          <t>maa://21364 (81.89), maa://36666 (81.82), *maa://22766 (68.8)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2535,7 +2535,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://21441 (96.54), maa://37650 (96.77), maa://36679 (94.55)</t>
+          <t>maa://21441 (96.54), maa://37650 (96.88), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2647,7 +2647,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>*maa://23911 (70.16), maa://27755 (94.06)</t>
+          <t>*maa://23911 (70.16), maa://27755 (94.12)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="T18" s="8" t="inlineStr">
         <is>
-          <t>maa://24385 (97.44)</t>
+          <t>maa://24385 (97.5)</t>
         </is>
       </c>
       <c r="U18" s="19" t="n"/>
@@ -3135,7 +3135,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (89.41), maa://49976 (87.06), maa://56241 (90.0)</t>
+          <t>maa://50085 (89.47), maa://49976 (87.06), maa://56241 (90.0)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3201,7 +3201,7 @@
       </c>
       <c r="H21" s="8" t="inlineStr">
         <is>
-          <t>maa://24372 (97.22)</t>
+          <t>maa://24372 (97.25)</t>
         </is>
       </c>
       <c r="I21" s="19" t="n"/>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22524 (87.21), maa://22432 (83.33)</t>
+          <t>maa://22524 (87.21), maa://22432 (83.56)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3395,7 +3395,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://21282 (98.76), *maa://37649 (73.47)</t>
+          <t>maa://21282 (98.76), *maa://37649 (72.55)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (95.73), maa://39875 (93.9)</t>
+          <t>maa://39756 (95.74), maa://39875 (93.9)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (95.58)</t>
+          <t>maa://29753 (95.6)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3721,7 +3721,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>*maa://29063 (72.14), *maa://25311 (74.34), ***maa://22725 (4.76), *maa://45047 (73.33)</t>
+          <t>*maa://29063 (72.14), *maa://25311 (74.56), ***maa://22725 (4.76), *maa://45047 (73.33)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -4175,7 +4175,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (92.11), maa://41749 (91.95)</t>
+          <t>maa://39929 (92.14), maa://41749 (91.95)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (92.45)</t>
+          <t>maa://36660 (92.24)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4225,7 +4225,7 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>maa://31694 (98.41)</t>
+          <t>maa://31694 (98.44)</t>
         </is>
       </c>
       <c r="E29" s="19" t="n"/>
@@ -4517,7 +4517,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (93.81), maa://36258 (88.37), *maa://43904 (73.33)</t>
+          <t>maa://35926 (93.53), maa://36258 (88.37), *maa://43904 (73.33)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4581,7 +4581,7 @@
       </c>
       <c r="AB31" s="8" t="inlineStr">
         <is>
-          <t>***maa://51420 (16.67)</t>
+          <t>***maa://51420 (15.38)</t>
         </is>
       </c>
       <c r="AC31" s="19" t="n"/>
@@ -5151,7 +5151,7 @@
       </c>
       <c r="H36" s="8" t="inlineStr">
         <is>
-          <t>maa://24375 (90.91)</t>
+          <t>maa://24375 (91.11)</t>
         </is>
       </c>
       <c r="I36" s="19" t="n"/>
@@ -5297,7 +5297,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (98.56), maa://47069 (81.82), maa://56336 (90.0), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.57), maa://47069 (81.82), maa://56336 (90.0), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5515,7 +5515,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://24709 (91.57), maa://47093 (100.0)</t>
+          <t>maa://24709 (91.62), maa://47093 (100.0)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -6041,7 +6041,7 @@
       </c>
       <c r="T45" s="8" t="inlineStr">
         <is>
-          <t>**maa://39364 (43.94)</t>
+          <t>**maa://39364 (44.78)</t>
         </is>
       </c>
       <c r="U45" s="19" t="n"/>
@@ -6078,7 +6078,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (92.09), maa://43901 (93.65)</t>
+          <t>maa://35931 (91.86), maa://43901 (92.31)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6322,7 +6322,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>*maa://62852 (75.0)</t>
+          <t>*maa://62852 (66.67)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6422,7 +6422,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (97.73), maa://59378 (94.64)</t>
+          <t>maa://59394 (97.78), maa://59378 (94.64)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6456,7 +6456,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (95.26)</t>
+          <t>maa://32534 (95.27)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -7006,7 +7006,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.07.11 13:25:31</t>
+          <t>更新日期：2025.07.12 13:21:48</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8194,7 +8194,7 @@
       </c>
       <c r="D23" s="13" t="inlineStr">
         <is>
-          <t>maa://20876 (97.22)</t>
+          <t>maa://20876 (94.59)</t>
         </is>
       </c>
       <c r="E23" s="14" t="inlineStr">
@@ -8950,7 +8950,7 @@
       </c>
       <c r="D37" s="13" t="inlineStr">
         <is>
-          <t>maa://27376 (92.0), maa://42635 (95.65), *maa://20838 (55.0)</t>
+          <t>maa://27376 (92.45), maa://42635 (95.65), *maa://20838 (55.0)</t>
         </is>
       </c>
       <c r="E37" s="14" t="inlineStr">
@@ -9166,7 +9166,7 @@
       </c>
       <c r="D41" s="13" t="inlineStr">
         <is>
-          <t>maa://20892 (80.65)</t>
+          <t>maa://20892 (80.85)</t>
         </is>
       </c>
       <c r="E41" s="14" t="inlineStr">
@@ -9814,7 +9814,7 @@
       </c>
       <c r="D53" s="13" t="inlineStr">
         <is>
-          <t>maa://20953 (96.15), maa://31173 (96.55)</t>
+          <t>maa://20953 (96.15), maa://31173 (96.67)</t>
         </is>
       </c>
       <c r="E53" s="14" t="inlineStr">
@@ -10300,7 +10300,7 @@
       </c>
       <c r="D62" s="13" t="inlineStr">
         <is>
-          <t>maa://20844 (96.97)</t>
+          <t>maa://20844 (97.06)</t>
         </is>
       </c>
       <c r="E62" s="14" t="inlineStr">
@@ -10354,7 +10354,7 @@
       </c>
       <c r="D63" s="13" t="inlineStr">
         <is>
-          <t>*maa://20845 (68.0), maa://38727 (88.89)</t>
+          <t>*maa://20845 (68.0), maa://38727 (90.0)</t>
         </is>
       </c>
       <c r="E63" s="14" t="inlineStr">
@@ -10462,7 +10462,7 @@
       </c>
       <c r="D65" s="13" t="inlineStr">
         <is>
-          <t>maa://28567 (96.92), **maa://20947 (44.12), maa://30525 (100.0), maa://38735 (100.0), *maa://28188 (70.0), maa://30524 (100.0)</t>
+          <t>maa://28567 (97.01), **maa://20947 (44.12), maa://30525 (100.0), maa://38735 (100.0), *maa://28188 (70.0), maa://30524 (100.0)</t>
         </is>
       </c>
       <c r="E65" s="14" t="inlineStr">
@@ -10678,7 +10678,7 @@
       </c>
       <c r="D69" s="13" t="inlineStr">
         <is>
-          <t>maa://20974 (96.51), maa://29079 (80.95), maa://29096 (95.65), maa://29087 (100.0), *maa://20823 (80.0), maa://20855 (93.75), maa://20904 (100.0)</t>
+          <t>maa://20974 (96.55), maa://29079 (80.95), maa://29096 (95.65), maa://29087 (100.0), *maa://20823 (80.0), maa://20855 (93.75), maa://20904 (100.0)</t>
         </is>
       </c>
       <c r="E69" s="14" t="inlineStr">
@@ -13972,7 +13972,7 @@
       </c>
       <c r="D130" s="13" t="inlineStr">
         <is>
-          <t>maa://21422 (99.12)</t>
+          <t>maa://21422 (99.13)</t>
         </is>
       </c>
       <c r="E130" s="14" t="inlineStr">
@@ -14404,7 +14404,7 @@
       </c>
       <c r="D138" s="13" t="inlineStr">
         <is>
-          <t>maa://29025 (82.14), **maa://21000 (45.16)</t>
+          <t>maa://29025 (82.76), **maa://21000 (45.16)</t>
         </is>
       </c>
       <c r="E138" s="14" t="inlineStr">
@@ -14620,7 +14620,7 @@
       </c>
       <c r="D142" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (97.22), **maa://23736 (44.12), maa://31185 (85.71), maa://30306 (100.0)</t>
+          <t>maa://28484 (97.22), **maa://23736 (44.93), maa://31185 (85.71), maa://30306 (100.0)</t>
         </is>
       </c>
       <c r="E142" s="14" t="inlineStr">
@@ -14728,7 +14728,7 @@
       </c>
       <c r="D144" s="13" t="inlineStr">
         <is>
-          <t>maa://20971 (92.31)</t>
+          <t>maa://20971 (92.86)</t>
         </is>
       </c>
       <c r="E144" s="14" t="inlineStr">
@@ -14998,7 +14998,7 @@
       </c>
       <c r="D149" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.08), maa://36641 (98.45), maa://36865 (95.81), maa://44635 (88.07), maa://44660 (92.31), maa://41128 (84.21), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
+          <t>maa://40957 (94.12), maa://36641 (98.45), maa://36865 (95.81), maa://44635 (88.07), maa://44660 (92.31), maa://41128 (84.21), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
         </is>
       </c>
       <c r="E149" s="14" t="inlineStr">
@@ -15970,7 +15970,7 @@
       </c>
       <c r="D167" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (92.31), maa://29627 (92.73), maa://29659 (86.11), maa://49074 (97.83), **maa://30679 (50.0), maa://29861 (100.0), maa://42343 (100.0)</t>
+          <t>maa://29633 (92.31), maa://29627 (92.73), maa://29659 (86.11), maa://49074 (97.87), **maa://30679 (50.0), maa://29861 (100.0), maa://42343 (100.0)</t>
         </is>
       </c>
       <c r="E167" s="14" t="inlineStr">
@@ -16024,7 +16024,7 @@
       </c>
       <c r="D168" s="13" t="inlineStr">
         <is>
-          <t>maa://49867 (91.67), maa://49655 (96.3)</t>
+          <t>maa://49867 (91.89), maa://49655 (96.3)</t>
         </is>
       </c>
       <c r="E168" s="14" t="inlineStr">
@@ -17590,7 +17590,7 @@
       </c>
       <c r="D197" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.16), maa://35854 (85.86), maa://50388 (98.01), maa://25760 (86.96), ***maa://43911 (13.04), *maa://20872 (52.0), maa://51066 (100.0)</t>
+          <t>maa://44224 (90.18), maa://35854 (85.86), maa://50388 (98.01), maa://25760 (86.96), ***maa://43911 (12.5), *maa://20872 (52.0), maa://51066 (100.0)</t>
         </is>
       </c>
       <c r="E197" s="14" t="inlineStr">
@@ -17914,7 +17914,7 @@
       </c>
       <c r="D203" s="13" t="inlineStr">
         <is>
-          <t>maa://20854 (92.31)</t>
+          <t>maa://20854 (92.86)</t>
         </is>
       </c>
       <c r="E203" s="14" t="inlineStr">
@@ -18454,7 +18454,7 @@
       </c>
       <c r="D213" s="13" t="inlineStr">
         <is>
-          <t>maa://39238 (99.51)</t>
+          <t>maa://39238 (99.52)</t>
         </is>
       </c>
       <c r="E213" s="14" t="inlineStr">
@@ -19426,7 +19426,7 @@
       </c>
       <c r="D231" s="13" t="inlineStr">
         <is>
-          <t>maa://29058 (96.15), maa://39140 (100.0), maa://38723 (100.0)</t>
+          <t>maa://29058 (96.2), maa://39140 (100.0), maa://38723 (100.0)</t>
         </is>
       </c>
       <c r="E231" s="14" t="inlineStr">
@@ -19480,7 +19480,7 @@
       </c>
       <c r="D232" s="13" t="inlineStr">
         <is>
-          <t>*maa://48263 (76.0)</t>
+          <t>*maa://48263 (76.92)</t>
         </is>
       </c>
       <c r="E232" s="14" t="inlineStr">
@@ -21316,7 +21316,7 @@
       </c>
       <c r="D266" s="13" t="inlineStr">
         <is>
-          <t>maa://22467 (95.74)</t>
+          <t>maa://22467 (95.83)</t>
         </is>
       </c>
       <c r="E266" s="14" t="inlineStr">
@@ -21478,7 +21478,7 @@
       </c>
       <c r="D269" s="13" t="inlineStr">
         <is>
-          <t>maa://48265 (82.61)</t>
+          <t>maa://48265 (83.33)</t>
         </is>
       </c>
       <c r="E269" s="14" t="inlineStr">
@@ -21640,7 +21640,7 @@
       </c>
       <c r="D272" s="26" t="inlineStr">
         <is>
-          <t>**maa://62757 (40.0)</t>
+          <t>**maa://62757 (37.5)</t>
         </is>
       </c>
       <c r="E272" s="27" t="inlineStr">
@@ -23422,7 +23422,7 @@
       </c>
       <c r="D305" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (97.37), maa://49642 (97.0), maa://49660 (90.32), *maa://50517 (80.0)</t>
+          <t>maa://50280 (97.39), maa://49642 (97.0), maa://49660 (90.32), *maa://50517 (80.0)</t>
         </is>
       </c>
       <c r="E305" s="14" t="inlineStr">
@@ -23746,7 +23746,7 @@
       </c>
       <c r="D311" s="13" t="inlineStr">
         <is>
-          <t>maa://35859 (97.73)</t>
+          <t>maa://35859 (97.75)</t>
         </is>
       </c>
       <c r="E311" s="14" t="inlineStr">
@@ -23800,7 +23800,7 @@
       </c>
       <c r="D312" s="13" t="inlineStr">
         <is>
-          <t>maa://53348 (95.0)</t>
+          <t>maa://53348 (95.24)</t>
         </is>
       </c>
       <c r="E312" s="14" t="inlineStr">
@@ -25312,7 +25312,7 @@
       </c>
       <c r="D340" s="22" t="inlineStr">
         <is>
-          <t>maa://38295 (94.74), maa://49332 (100.0)</t>
+          <t>maa://38295 (94.85), maa://49332 (100.0)</t>
         </is>
       </c>
       <c r="E340" s="22" t="inlineStr">
@@ -26068,7 +26068,7 @@
       </c>
       <c r="D354" s="22" t="inlineStr">
         <is>
-          <t>maa://36868 (100.0), maa://35996 (97.7), **maa://39217 (41.18), maa://47349 (95.0)</t>
+          <t>maa://36868 (99.72), maa://35996 (97.73), **maa://39217 (41.18), maa://47349 (95.12)</t>
         </is>
       </c>
       <c r="E354" s="22" t="inlineStr">
@@ -26608,7 +26608,7 @@
       </c>
       <c r="D364" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (94.08), maa://44635 (88.07), maa://48026 (94.59), maa://41035 (93.06), maa://44660 (92.31), maa://41128 (84.21), *maa://60251 (72.73)</t>
+          <t>maa://40957 (94.12), maa://44635 (88.07), maa://48026 (94.59), maa://41035 (93.06), maa://44660 (92.31), maa://41128 (84.21), *maa://60251 (66.67)</t>
         </is>
       </c>
       <c r="E364" s="22" t="inlineStr">
@@ -27418,7 +27418,7 @@
       </c>
       <c r="D379" s="22" t="inlineStr">
         <is>
-          <t>maa://43875 (98.18)</t>
+          <t>maa://43875 (98.21)</t>
         </is>
       </c>
       <c r="E379" s="22" t="inlineStr">
@@ -27472,7 +27472,7 @@
       </c>
       <c r="D380" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (82.58), maa://44745 (97.33), **maa://49516 (34.78), *maa://45952 (72.73), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
+          <t>maa://42970 (82.58), maa://44745 (97.35), **maa://49516 (34.78), *maa://45952 (72.73), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E380" s="22" t="inlineStr">
@@ -27565,12 +27565,12 @@
     <row r="382" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A382" s="12" t="inlineStr">
         <is>
-          <t>瑰盐</t>
+          <t>特克诺</t>
         </is>
       </c>
       <c r="B382" s="11" t="inlineStr">
         <is>
-          <t>4-6</t>
+          <t>DH-6</t>
         </is>
       </c>
       <c r="C382" s="12" t="inlineStr">
@@ -27580,12 +27580,12 @@
       </c>
       <c r="D382" s="22" t="inlineStr">
         <is>
-          <t>maa://44389 (100.0)</t>
+          <t>maa://59690 (100.0)</t>
         </is>
       </c>
       <c r="E382" s="22" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战瑰盐累计使用绝妙的长效药呀8次&gt; 3星通关主题曲4-6；必须编入非助战瑰盐并上场，且至少使用1次绝妙的长效药呀</t>
+          <t>&gt; 完成5次战斗；必须编入非助战特克诺并上场，且每次战斗至少释放1次“恣意挥洒”&gt; 3星通关插曲DH-6，必须编入非助战特克诺并上场，其他成员仅可编入7名干员</t>
         </is>
       </c>
       <c r="F382" s="19" t="n"/>
@@ -27619,12 +27619,12 @@
     <row r="383" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A383" s="12" t="inlineStr">
         <is>
-          <t>特克诺</t>
+          <t>引星棘刺</t>
         </is>
       </c>
       <c r="B383" s="11" t="inlineStr">
         <is>
-          <t>DH-6</t>
+          <t>OF-7</t>
         </is>
       </c>
       <c r="C383" s="12" t="inlineStr">
@@ -27634,12 +27634,12 @@
       </c>
       <c r="D383" s="22" t="inlineStr">
         <is>
-          <t>maa://59690 (100.0)</t>
+          <t>maa://48113 (100.0)</t>
         </is>
       </c>
       <c r="E383" s="22" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战特克诺并上场，且每次战斗至少释放1次“恣意挥洒”&gt; 3星通关插曲DH-6，必须编入非助战特克诺并上场，其他成员仅可编入7名干员</t>
+          <t>&gt; 战斗中非助战引星棘刺累计使用20次解构涌潮&gt; 3星通关别传OF-7；必须编入非助战引星棘刺并上场，其他成员仅可编入4名干员</t>
         </is>
       </c>
       <c r="F383" s="19" t="n"/>
@@ -27673,12 +27673,12 @@
     <row r="384" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A384" s="12" t="inlineStr">
         <is>
-          <t>引星棘刺</t>
+          <t>行箸</t>
         </is>
       </c>
       <c r="B384" s="11" t="inlineStr">
         <is>
-          <t>OF-7</t>
+          <t>3-2</t>
         </is>
       </c>
       <c r="C384" s="12" t="inlineStr">
@@ -27688,12 +27688,12 @@
       </c>
       <c r="D384" s="22" t="inlineStr">
         <is>
-          <t>maa://48113 (100.0)</t>
+          <t>maa://45807 (100.0)</t>
         </is>
       </c>
       <c r="E384" s="22" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战引星棘刺累计使用20次解构涌潮&gt; 3星通关别传OF-7；必须编入非助战引星棘刺并上场，其他成员仅可编入4名干员</t>
+          <t>&gt; 使用非助战行箸累计使用8次食不厌精&gt; 3星通关主题曲3-2；必须编入非助战行箸并上场，且所有干员不能被击倒</t>
         </is>
       </c>
       <c r="F384" s="19" t="n"/>
@@ -27727,12 +27727,12 @@
     <row r="385" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A385" s="12" t="inlineStr">
         <is>
-          <t>行箸</t>
+          <t>寻澜</t>
         </is>
       </c>
       <c r="B385" s="11" t="inlineStr">
         <is>
-          <t>3-2</t>
+          <t>3-5</t>
         </is>
       </c>
       <c r="C385" s="12" t="inlineStr">
@@ -27742,12 +27742,12 @@
       </c>
       <c r="D385" s="22" t="inlineStr">
         <is>
-          <t>maa://45807 (100.0)</t>
+          <t>maa://50552 (100.0)</t>
         </is>
       </c>
       <c r="E385" s="22" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战行箸累计使用8次食不厌精&gt; 3星通关主题曲3-2；必须编入非助战行箸并上场，且所有干员不能被击倒</t>
+          <t>&gt; 完成5次战斗；必须编入非助战寻澜并上场，且使用寻澜歼灭至少3个敌人&gt; 3星通关主题曲3-5；必须编入非助战寻澜并上场，且至少使用2次洞悉</t>
         </is>
       </c>
       <c r="F385" s="19" t="n"/>
@@ -27781,27 +27781,27 @@
     <row r="386" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A386" s="12" t="inlineStr">
         <is>
-          <t>寻澜</t>
+          <t>诺威尔</t>
         </is>
       </c>
       <c r="B386" s="11" t="inlineStr">
         <is>
-          <t>3-5</t>
+          <t>5-7</t>
         </is>
       </c>
       <c r="C386" s="12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D386" s="22" t="inlineStr">
         <is>
-          <t>maa://50552 (100.0)</t>
+          <t>*maa://47175 (66.67), maa://47174 (100.0)</t>
         </is>
       </c>
       <c r="E386" s="22" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战寻澜并上场，且使用寻澜歼灭至少3个敌人&gt; 3星通关主题曲3-5；必须编入非助战寻澜并上场，且至少使用2次洞悉</t>
+          <t>&gt; 完成5次战斗；必须编入非助战诺威尔并上场，且每次战斗至少释放1次生命不息&gt; 3星通关主题曲5-7；必须编入非助战诺威尔并上场，且队伍中不能有其他医疗干员</t>
         </is>
       </c>
       <c r="F386" s="19" t="n"/>
@@ -27835,27 +27835,27 @@
     <row r="387" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A387" s="12" t="inlineStr">
         <is>
-          <t>诺威尔</t>
+          <t>隐德来希</t>
         </is>
       </c>
       <c r="B387" s="11" t="inlineStr">
         <is>
-          <t>5-7</t>
+          <t>10-12</t>
         </is>
       </c>
       <c r="C387" s="12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D387" s="22" t="inlineStr">
         <is>
-          <t>*maa://47175 (66.67), maa://47174 (100.0)</t>
+          <t>maa://47023 (88.24)</t>
         </is>
       </c>
       <c r="E387" s="22" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战诺威尔并上场，且每次战斗至少释放1次生命不息&gt; 3星通关主题曲5-7；必须编入非助战诺威尔并上场，且队伍中不能有其他医疗干员</t>
+          <t>&gt; 使用非助战隐德来希累计造成100000点伤害&gt; 3星通关主题曲10-12标准实战环境；必须编入非助战隐德来希并上场，且隐德来希至少使用3次灵与欲的惜别</t>
         </is>
       </c>
       <c r="F387" s="19" t="n"/>
@@ -27889,12 +27889,12 @@
     <row r="388" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A388" s="12" t="inlineStr">
         <is>
-          <t>隐德来希</t>
+          <t>钼铅</t>
         </is>
       </c>
       <c r="B388" s="11" t="inlineStr">
         <is>
-          <t>10-12</t>
+          <t>9-6</t>
         </is>
       </c>
       <c r="C388" s="12" t="inlineStr">
@@ -27904,12 +27904,12 @@
       </c>
       <c r="D388" s="22" t="inlineStr">
         <is>
-          <t>maa://47023 (88.24)</t>
+          <t>**maa://48618 (50.0)</t>
         </is>
       </c>
       <c r="E388" s="22" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战隐德来希累计造成100000点伤害&gt; 3星通关主题曲10-12标准实战环境；必须编入非助战隐德来希并上场，且隐德来希至少使用3次灵与欲的惜别</t>
+          <t>&gt; 战斗中非助战钼铅累计部署矿石“杀手”30个&gt; 3星通关主题曲9-6标准实战环境；必须编入非助战钼铅并上场，且使用钼铅至少击败1名深池重甲卫士</t>
         </is>
       </c>
       <c r="F388" s="19" t="n"/>
@@ -27943,27 +27943,27 @@
     <row r="389" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A389" s="12" t="inlineStr">
         <is>
-          <t>钼铅</t>
+          <t>死芒</t>
         </is>
       </c>
       <c r="B389" s="11" t="inlineStr">
         <is>
-          <t>9-6</t>
+          <t>4-8</t>
         </is>
       </c>
       <c r="C389" s="12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D389" s="22" t="inlineStr">
         <is>
-          <t>**maa://48618 (50.0)</t>
+          <t>maa://59533 (100.0), maa://59577 (100.0)</t>
         </is>
       </c>
       <c r="E389" s="22" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战钼铅累计部署矿石“杀手”30个&gt; 3星通关主题曲9-6标准实战环境；必须编入非助战钼铅并上场，且使用钼铅至少击败1名深池重甲卫士</t>
+          <t>&gt; 完成5次战斗；必须编入非助战死芒并上场，且每次战斗至少释放2次“冠死以冕”&gt; 3星通关主题曲4-8，必须编入非助战死芒并上场，其他成员仅可编入辅助干员</t>
         </is>
       </c>
       <c r="F389" s="19" t="n"/>
@@ -27997,12 +27997,12 @@
     <row r="390" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A390" s="12" t="inlineStr">
         <is>
-          <t>死芒</t>
+          <t>骋风</t>
         </is>
       </c>
       <c r="B390" s="11" t="inlineStr">
         <is>
-          <t>4-8</t>
+          <t>SN-2</t>
         </is>
       </c>
       <c r="C390" s="12" t="inlineStr">
@@ -28012,12 +28012,12 @@
       </c>
       <c r="D390" s="22" t="inlineStr">
         <is>
-          <t>maa://59533 (100.0), maa://59577 (100.0)</t>
+          <t>maa://51907 (100.0), maa://51908 (100.0)</t>
         </is>
       </c>
       <c r="E390" s="22" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战死芒并上场，且每次战斗至少释放2次“冠死以冕”&gt; 3星通关主题曲4-8，必须编入非助战死芒并上场，其他成员仅可编入辅助干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战骋风并上场，且每次战斗至少释放1次招无虚发&gt; 3星通关插曲SN-2；必须编入非助战骋风并上场，且使用2次招无虚发</t>
         </is>
       </c>
       <c r="F390" s="19" t="n"/>
@@ -28051,27 +28051,27 @@
     <row r="391" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A391" s="12" t="inlineStr">
         <is>
-          <t>骋风</t>
+          <t>阿兰娜</t>
         </is>
       </c>
       <c r="B391" s="11" t="inlineStr">
         <is>
-          <t>SN-2</t>
+          <t>7-14</t>
         </is>
       </c>
       <c r="C391" s="12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D391" s="22" t="inlineStr">
         <is>
-          <t>maa://51907 (100.0), maa://51908 (100.0)</t>
+          <t>**maa://59691 (50.0)</t>
         </is>
       </c>
       <c r="E391" s="22" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战骋风并上场，且每次战斗至少释放1次招无虚发&gt; 3星通关插曲SN-2；必须编入非助战骋风并上场，且使用2次招无虚发</t>
+          <t>&gt; 使用非助战阿兰娜累计部署15个“支援装置”&gt; 3星通关主题曲7-14；必须编入非助战阿兰娜并上场，且至少使用2次“万斤顶”</t>
         </is>
       </c>
       <c r="F391" s="19" t="n"/>
@@ -28105,27 +28105,27 @@
     <row r="392" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A392" s="12" t="inlineStr">
         <is>
-          <t>阿兰娜</t>
+          <t>信仰搅拌机</t>
         </is>
       </c>
       <c r="B392" s="11" t="inlineStr">
         <is>
-          <t>7-14</t>
+          <t>14-5</t>
         </is>
       </c>
       <c r="C392" s="12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D392" s="22" t="inlineStr">
         <is>
-          <t>**maa://59691 (50.0)</t>
+          <t>maa://51898 (100.0), maa://57241 (100.0)</t>
         </is>
       </c>
       <c r="E392" s="22" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战阿兰娜累计部署15个“支援装置”&gt; 3星通关主题曲7-14；必须编入非助战阿兰娜并上场，且至少使用2次“万斤顶”</t>
+          <t>&gt; 完成5次战斗；必须编入非助战信仰搅拌机并上场，且每次战斗至少释放1次退休前布道&gt; 3星通关主题曲14-5标准实战环境；必须编入非助战信仰搅拌机并上场，且使用信仰搅拌机歼灭至少10名敌人</t>
         </is>
       </c>
       <c r="F392" s="19" t="n"/>
@@ -28159,135 +28159,135 @@
     <row r="393">
       <c r="A393" s="17" t="inlineStr">
         <is>
-          <t>信仰搅拌机</t>
+          <t>蕾缪安</t>
         </is>
       </c>
       <c r="B393" s="23" t="inlineStr">
         <is>
-          <t>14-5</t>
+          <t>13-13</t>
         </is>
       </c>
       <c r="C393" s="17" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>maa://51898 (100.0), maa://57241 (100.0)</t>
+          <t>maa://51880 (99.14), maa://56651 (100.0), maa://51878 (100.0)</t>
         </is>
       </c>
       <c r="E393" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战信仰搅拌机并上场，且每次战斗至少释放1次退休前布道&gt; 3星通关主题曲14-5标准实战环境；必须编入非助战信仰搅拌机并上场，且使用信仰搅拌机歼灭至少10名敌人</t>
+          <t>&gt; 由非助战蕾缪安累计造成30歼灭数&gt; 3星通关主题曲13-13标准实战环境；必须编入非助战蕾缪安并上场，且蕾缪安歼灭至少2个萨卡兹骸骨鞭笞者</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="17" t="inlineStr">
         <is>
-          <t>蕾缪安</t>
+          <t>新约能天使</t>
         </is>
       </c>
       <c r="B394" s="23" t="inlineStr">
         <is>
-          <t>13-13</t>
+          <t>GA-EX-5</t>
         </is>
       </c>
       <c r="C394" s="17" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>maa://51880 (99.14), maa://56651 (100.0), maa://51878 (100.0)</t>
+          <t>maa://51872 (96.78), maa://51876 (98.92), maa://51873 (100.0), maa://62047 (90.91)</t>
         </is>
       </c>
       <c r="E394" t="inlineStr">
         <is>
-          <t>&gt; 由非助战蕾缪安累计造成30歼灭数&gt; 3星通关主题曲13-13标准实战环境；必须编入非助战蕾缪安并上场，且蕾缪安歼灭至少2个萨卡兹骸骨鞭笞者</t>
+          <t>&gt; 战斗中非助战新约能天使累计使用开火成瘾症8次&gt; 3星通关插曲GA-EX-5；必须编入非助战新约能天使并上场，且使用2次开火成瘾症</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="17" t="inlineStr">
         <is>
-          <t>新约能天使</t>
+          <t>酒神</t>
         </is>
       </c>
       <c r="B395" s="17" t="inlineStr">
         <is>
-          <t>GA-EX-5</t>
+          <t>9-6</t>
         </is>
       </c>
       <c r="C395" s="17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D395" t="inlineStr">
         <is>
-          <t>maa://51872 (96.77), maa://51876 (98.92), maa://51873 (100.0), maa://62047 (90.91)</t>
+          <t>maa://59493 (96.64), maa://60449 (98.04), maa://59603 (100.0)</t>
         </is>
       </c>
       <c r="E395" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战新约能天使累计使用开火成瘾症8次&gt; 3星通关插曲GA-EX-5；必须编入非助战新约能天使并上场，且使用2次开火成瘾症</t>
+          <t>&gt; 使用非助战酒神累计造成60000点神经损伤&gt; 3星通关主题曲9-6标准实战环境，必须编入非助战酒神并上场，且酒神使用至少2次“空剧场”</t>
         </is>
       </c>
     </row>
     <row r="396">
-      <c r="A396" s="17" t="inlineStr">
-        <is>
-          <t>酒神</t>
-        </is>
-      </c>
-      <c r="B396" s="17" t="inlineStr">
-        <is>
-          <t>9-6</t>
-        </is>
-      </c>
-      <c r="C396" s="17" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D396" t="inlineStr">
-        <is>
-          <t>maa://59493 (96.61), maa://60449 (97.96), maa://59603 (100.0)</t>
-        </is>
-      </c>
-      <c r="E396" t="inlineStr">
-        <is>
-          <t>&gt; 使用非助战酒神累计造成60000点神经损伤&gt; 3星通关主题曲9-6标准实战环境，必须编入非助战酒神并上场，且酒神使用至少2次“空剧场”</t>
+      <c r="A396" s="28" t="inlineStr">
+        <is>
+          <t>录武官</t>
+        </is>
+      </c>
+      <c r="B396" s="28" t="inlineStr">
+        <is>
+          <t>HS-5</t>
+        </is>
+      </c>
+      <c r="C396" s="28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D396" s="29" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E396" s="29" t="inlineStr">
+        <is>
+          <t>&gt; 战斗中非助战录武官累计使用“一点关窍”6次&gt; 3星通关插曲HS-5，必须编入非助战录武官并上场，且不编入其他医疗干员</t>
         </is>
       </c>
     </row>
     <row r="397">
-      <c r="A397" s="28" t="inlineStr">
-        <is>
-          <t>录武官</t>
-        </is>
-      </c>
-      <c r="B397" s="28" t="inlineStr">
-        <is>
-          <t>HS-5</t>
-        </is>
-      </c>
-      <c r="C397" s="28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D397" s="29" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E397" s="29" t="inlineStr">
-        <is>
-          <t>&gt; 战斗中非助战录武官累计使用“一点关窍”6次&gt; 3星通关插曲HS-5，必须编入非助战录武官并上场，且不编入其他医疗干员</t>
+      <c r="A397" s="17" t="inlineStr">
+        <is>
+          <t>司霆惊蛰</t>
+        </is>
+      </c>
+      <c r="B397" s="17" t="inlineStr">
+        <is>
+          <t>DV-7</t>
+        </is>
+      </c>
+      <c r="C397" s="17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>maa://62756 (90.0)</t>
+        </is>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>&gt; 由非助战司霆惊蛰累计造成120000点伤害&gt; 3星通关插曲DV-7；必须编入非助战司霆惊蛰并上场，且使用1次“天地通明”</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#210)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -737,7 +737,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://39402 (95.12), *maa://34787 (73.91), maa://58660 (90.0)</t>
+          <t>maa://39402 (95.12), *maa://34787 (73.91), maa://58660 (92.31)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -817,7 +817,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://25251 (91.91), maa://59087 (95.24)</t>
+          <t>maa://25251 (91.91), maa://59087 (95.45)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -867,7 +867,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>*maa://22880 (65.98), maa://20276 (87.96), *maa://22749 (78.95)</t>
+          <t>*maa://22880 (66.12), maa://20276 (87.96), *maa://22749 (78.95)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (96.88), maa://50121 (95.35)</t>
+          <t>maa://49983 (95.88), maa://50121 (95.35)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="X4" s="8" t="inlineStr">
         <is>
-          <t>maa://43217 (93.88)</t>
+          <t>maa://43217 (93.29)</t>
         </is>
       </c>
       <c r="Y4" s="19" t="n"/>
@@ -1100,7 +1100,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (84.25), maa://22744 (82.14), maa://54105 (100.0)</t>
+          <t>maa://21245 (83.96), maa://22744 (82.14), maa://54105 (94.74)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="X6" s="8" t="inlineStr">
         <is>
-          <t>maa://52754 (88.0)</t>
+          <t>maa://52754 (88.46)</t>
         </is>
       </c>
       <c r="Y6" s="19" t="n"/>
@@ -1392,7 +1392,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (94.3), maa://24957 (97.83)</t>
+          <t>maa://28624 (94.34), maa://24957 (97.83)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1480,7 +1480,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.07.12 13:21:48</t>
+          <t>更新日期：2025.07.13 13:23:12</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1755,7 +1755,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.45), ***maa://39951 (11.54), ***maa://34206 (22.22), *maa://45271 (61.9), ***maa://39243 (25.0), **maa://54000 (50.0)</t>
+          <t>***maa://25695 (18.45), ***maa://39951 (11.39), ***maa://34206 (22.22), *maa://45271 (61.9), ***maa://39243 (25.0), **maa://54000 (50.0)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="D11" s="8" t="inlineStr">
         <is>
-          <t>maa://36707 (99.4)</t>
+          <t>maa://36707 (99.41)</t>
         </is>
       </c>
       <c r="E11" s="19" t="n"/>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (90.0), maa://22501 (98.26), maa://45521 (91.89)</t>
+          <t>maa://22747 (90.0), maa://22501 (98.28), maa://45521 (91.89)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://22753 (92.06), maa://37962 (91.89), *maa://21485 (76.16)</t>
+          <t>maa://22753 (92.09), maa://37962 (91.89), *maa://21485 (76.16)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2275,7 +2275,7 @@
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>maa://30764 (90.14)</t>
+          <t>maa://30764 (90.28)</t>
         </is>
       </c>
       <c r="E14" s="19" t="n"/>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (94.8), maa://26245 (96.83), maa://21288 (96.3), maa://36682 (96.3)</t>
+          <t>maa://39841 (94.83), maa://26245 (96.83), maa://21288 (96.3), maa://36682 (96.3)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2405,7 +2405,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.54), maa://22734 (84.55), *maa://30808 (64.38), *maa://36048 (69.49), maa://45058 (86.36)</t>
+          <t>*maa://22743 (78.54), maa://22734 (84.55), *maa://30808 (64.38), *maa://36048 (69.75), maa://45058 (86.36)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2827,7 +2827,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://22466 (92.27), maa://52226 (96.0)</t>
+          <t>maa://22466 (92.27), maa://52226 (96.15)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>*maa://30709 (69.17), *maa://36668 (57.83)</t>
+          <t>*maa://30709 (69.23), *maa://36668 (57.83)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3135,7 +3135,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (89.47), maa://49976 (87.06), maa://56241 (90.0)</t>
+          <t>maa://50085 (89.53), maa://49976 (87.06), maa://56241 (90.0)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3265,7 +3265,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://20110 (87.14), maa://34946 (93.44)</t>
+          <t>maa://20110 (87.14), maa://34946 (93.55)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3493,7 +3493,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (91.86), *maa://29748 (76.3), *maa://37566 (79.17)</t>
+          <t>maa://30587 (91.89), *maa://29748 (76.3), *maa://37566 (79.17)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3525,7 +3525,7 @@
       </c>
       <c r="X23" s="8" t="inlineStr">
         <is>
-          <t>*maa://28503 (63.11)</t>
+          <t>*maa://28503 (62.5)</t>
         </is>
       </c>
       <c r="Y23" s="19" t="n"/>
@@ -3541,7 +3541,7 @@
       </c>
       <c r="AB23" s="8" t="inlineStr">
         <is>
-          <t>maa://29652 (98.04)</t>
+          <t>maa://29652 (96.15)</t>
         </is>
       </c>
       <c r="AC23" s="19" t="n"/>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (84.98), maa://23504 (93.8), *maa://25141 (77.37), *maa://36663 (78.22), maa://52227 (95.65)</t>
+          <t>maa://29988 (84.98), maa://23504 (93.8), *maa://25141 (77.37), *maa://36663 (78.43), maa://52227 (95.65)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3801,7 +3801,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (89.93), *maa://24516 (79.57), maa://26001 (84.75)</t>
+          <t>maa://31215 (89.4), *maa://24516 (79.57), maa://26001 (84.75)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -4095,7 +4095,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (90.79), maa://25725 (83.0)</t>
+          <t>maa://24465 (90.8), maa://25725 (83.0)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4175,7 +4175,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (92.14), maa://41749 (91.95)</t>
+          <t>maa://39929 (92.16), maa://41749 (91.95)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (92.24)</t>
+          <t>maa://36660 (92.27)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4679,7 +4679,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (97.16), maa://41108 (86.27), maa://41238 (98.11), maa://45523 (100.0)</t>
+          <t>maa://42859 (97.17), maa://41108 (86.27), maa://41238 (98.11), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4761,7 +4761,7 @@
       </c>
       <c r="H33" s="8" t="inlineStr">
         <is>
-          <t>**maa://39351 (42.86)</t>
+          <t>**maa://39351 (37.5)</t>
         </is>
       </c>
       <c r="I33" s="19" t="n"/>
@@ -5069,7 +5069,7 @@
       </c>
       <c r="T35" s="8" t="inlineStr">
         <is>
-          <t>maa://24842 (94.92)</t>
+          <t>maa://24842 (95.0)</t>
         </is>
       </c>
       <c r="U35" s="19" t="n"/>
@@ -5414,7 +5414,7 @@
       </c>
       <c r="P38" s="8" t="inlineStr">
         <is>
-          <t>*maa://24383 (70.8)</t>
+          <t>*maa://24383 (70.18)</t>
         </is>
       </c>
       <c r="Q38" s="19" t="n"/>
@@ -5531,7 +5531,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (94.55), *maa://45788 (70.73), maa://45790 (81.25)</t>
+          <t>maa://47079 (94.64), *maa://45788 (70.73), maa://45790 (81.25)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5558,12 +5558,12 @@
       </c>
       <c r="AE39" s="19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF39" s="8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>**maa://62953 (50.0)</t>
         </is>
       </c>
       <c r="AG39" s="16" t="n"/>
@@ -5685,7 +5685,7 @@
       </c>
       <c r="H41" s="8" t="inlineStr">
         <is>
-          <t>maa://24466 (94.0)</t>
+          <t>maa://24466 (92.16)</t>
         </is>
       </c>
       <c r="I41" s="19" t="n"/>
@@ -5855,7 +5855,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>maa://22525 (81.14), maa://21284 (88.14)</t>
+          <t>maa://22525 (80.68), maa://21284 (88.14)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -6322,7 +6322,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>*maa://62852 (66.67)</t>
+          <t>*maa://62852 (77.78)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6422,7 +6422,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (97.78), maa://59378 (94.64)</t>
+          <t>maa://59394 (97.83), maa://59378 (94.74)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6456,7 +6456,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (95.27)</t>
+          <t>maa://32534 (95.28)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -6612,7 +6612,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (94.94), maa://27746 (83.05)</t>
+          <t>maa://31270 (94.94), maa://27746 (83.19)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -7006,7 +7006,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.07.12 13:21:48</t>
+          <t>更新日期：2025.07.13 13:23:12</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8518,7 +8518,7 @@
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>maa://20863 (89.02), maa://20832 (99.11), maa://20727 (100.0)</t>
+          <t>maa://20863 (89.02), maa://20832 (99.12), maa://20727 (100.0)</t>
         </is>
       </c>
       <c r="E29" s="14" t="inlineStr">
@@ -9436,7 +9436,7 @@
       </c>
       <c r="D46" s="13" t="inlineStr">
         <is>
-          <t>maa://39025 (87.5)</t>
+          <t>*maa://39025 (77.78)</t>
         </is>
       </c>
       <c r="E46" s="14" t="inlineStr">
@@ -10624,7 +10624,7 @@
       </c>
       <c r="D68" s="13" t="inlineStr">
         <is>
-          <t>maa://20976 (97.84), maa://20815 (100.0)</t>
+          <t>maa://20976 (97.85), maa://20815 (100.0)</t>
         </is>
       </c>
       <c r="E68" s="14" t="inlineStr">
@@ -11704,7 +11704,7 @@
       </c>
       <c r="D88" s="13" t="inlineStr">
         <is>
-          <t>maa://24472 (88.52), *maa://35841 (61.11)</t>
+          <t>maa://24472 (88.63), *maa://35841 (61.11)</t>
         </is>
       </c>
       <c r="E88" s="14" t="inlineStr">
@@ -12136,7 +12136,7 @@
       </c>
       <c r="D96" s="13" t="inlineStr">
         <is>
-          <t>*maa://20926 (77.78)</t>
+          <t>*maa://20926 (80.0)</t>
         </is>
       </c>
       <c r="E96" s="14" t="inlineStr">
@@ -12784,7 +12784,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://25018 (96.71), maa://51881 (99.23), maa://25776 (92.11), maa://28361 (95.12), maa://25772 (94.12), maa://56588 (95.0), maa://45194 (82.35), maa://32653 (85.71), maa://25161 (81.25), ***maa://60902 (28.57)</t>
+          <t>maa://25018 (96.72), maa://51881 (99.24), maa://25776 (92.11), maa://28361 (95.12), maa://25772 (94.12), maa://56588 (95.0), maa://45194 (82.35), maa://25161 (81.25), maa://32653 (85.71), ***maa://60902 (28.57)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13486,7 +13486,7 @@
       </c>
       <c r="D121" s="13" t="inlineStr">
         <is>
-          <t>maa://20869 (100.0), maa://44690 (95.65)</t>
+          <t>maa://20869 (100.0), maa://44690 (95.83)</t>
         </is>
       </c>
       <c r="E121" s="14" t="inlineStr">
@@ -14998,7 +14998,7 @@
       </c>
       <c r="D149" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.12), maa://36641 (98.45), maa://36865 (95.81), maa://44635 (88.07), maa://44660 (92.31), maa://41128 (84.21), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
+          <t>maa://40957 (94.14), maa://36641 (98.45), maa://36865 (95.81), maa://44635 (88.07), maa://44660 (92.31), maa://41128 (84.21), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
         </is>
       </c>
       <c r="E149" s="14" t="inlineStr">
@@ -17590,7 +17590,7 @@
       </c>
       <c r="D197" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.18), maa://35854 (85.86), maa://50388 (98.01), maa://25760 (86.96), ***maa://43911 (12.5), *maa://20872 (52.0), maa://51066 (100.0)</t>
+          <t>maa://44224 (90.2), maa://35854 (86.0), maa://50388 (98.03), maa://25760 (86.96), ***maa://43911 (12.5), *maa://20872 (52.0), maa://51066 (100.0)</t>
         </is>
       </c>
       <c r="E197" s="14" t="inlineStr">
@@ -18292,7 +18292,7 @@
       </c>
       <c r="D210" s="13" t="inlineStr">
         <is>
-          <t>maa://28133 (93.1), **maa://39217 (41.18), maa://25369 (94.59)</t>
+          <t>maa://28133 (93.1), **maa://39217 (41.18), maa://25369 (94.74)</t>
         </is>
       </c>
       <c r="E210" s="14" t="inlineStr">
@@ -19210,7 +19210,7 @@
       </c>
       <c r="D227" s="13" t="inlineStr">
         <is>
-          <t>maa://20987 (93.81), *maa://35801 (77.78)</t>
+          <t>maa://20987 (93.88), *maa://35801 (77.78)</t>
         </is>
       </c>
       <c r="E227" s="14" t="inlineStr">
@@ -19912,7 +19912,7 @@
       </c>
       <c r="D240" s="13" t="inlineStr">
         <is>
-          <t>*maa://30667 (78.72), maa://30666 (83.55), **maa://30739 (43.24), *maa://30723 (56.45), maa://39588 (89.09)</t>
+          <t>*maa://30667 (78.77), maa://30666 (83.55), **maa://30739 (43.24), *maa://30723 (56.45), maa://39588 (89.09)</t>
         </is>
       </c>
       <c r="E240" s="14" t="inlineStr">
@@ -21424,7 +21424,7 @@
       </c>
       <c r="D268" s="13" t="inlineStr">
         <is>
-          <t>maa://49643 (88.46)</t>
+          <t>maa://49643 (88.89)</t>
         </is>
       </c>
       <c r="E268" s="14" t="inlineStr">
@@ -21640,7 +21640,7 @@
       </c>
       <c r="D272" s="26" t="inlineStr">
         <is>
-          <t>**maa://62757 (37.5)</t>
+          <t>***maa://62757 (30.0)</t>
         </is>
       </c>
       <c r="E272" s="27" t="inlineStr">
@@ -21748,7 +21748,7 @@
       </c>
       <c r="D274" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (99.23), maa://51630 (96.63), maa://56588 (95.0), *maa://55171 (57.14), maa://51893 (88.89), ***maa://60902 (28.57)</t>
+          <t>maa://51881 (99.24), maa://51630 (96.63), maa://56588 (95.0), *maa://55171 (57.14), maa://51893 (88.89), ***maa://60902 (28.57)</t>
         </is>
       </c>
       <c r="E274" s="14" t="inlineStr">
@@ -23422,7 +23422,7 @@
       </c>
       <c r="D305" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (97.39), maa://49642 (97.0), maa://49660 (90.32), *maa://50517 (80.0)</t>
+          <t>maa://50280 (97.4), maa://49642 (97.0), maa://49660 (90.32), *maa://50517 (80.0)</t>
         </is>
       </c>
       <c r="E305" s="14" t="inlineStr">
@@ -24124,7 +24124,7 @@
       </c>
       <c r="D318" s="13" t="inlineStr">
         <is>
-          <t>**maa://62755 (50.0)</t>
+          <t>*maa://62755 (60.0)</t>
         </is>
       </c>
       <c r="E318" s="14" t="inlineStr">
@@ -26122,7 +26122,7 @@
       </c>
       <c r="D355" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.56), maa://49695 (100.0), maa://49758 (98.46), *maa://59402 (60.87), *maa://52357 (76.92)</t>
+          <t>maa://49696 (99.56), maa://49695 (100.0), maa://49758 (98.46), *maa://59402 (60.87), *maa://52357 (71.43)</t>
         </is>
       </c>
       <c r="E355" s="22" t="inlineStr">
@@ -26230,7 +26230,7 @@
       </c>
       <c r="D357" s="22" t="inlineStr">
         <is>
-          <t>maa://42299 (97.62), maa://42224 (81.25)</t>
+          <t>maa://42299 (97.67), maa://42224 (82.35)</t>
         </is>
       </c>
       <c r="E357" s="22" t="inlineStr">
@@ -26608,7 +26608,7 @@
       </c>
       <c r="D364" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (94.12), maa://44635 (88.07), maa://48026 (94.59), maa://41035 (93.06), maa://44660 (92.31), maa://41128 (84.21), *maa://60251 (66.67)</t>
+          <t>maa://40957 (94.14), maa://44635 (88.07), maa://48026 (94.59), maa://41035 (93.06), maa://44660 (92.31), maa://41128 (84.21), *maa://60251 (66.67)</t>
         </is>
       </c>
       <c r="E364" s="22" t="inlineStr">
@@ -27472,7 +27472,7 @@
       </c>
       <c r="D380" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (82.58), maa://44745 (97.35), **maa://49516 (34.78), *maa://45952 (72.73), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
+          <t>maa://42970 (82.64), maa://44745 (97.37), **maa://49516 (34.78), *maa://45952 (72.73), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E380" s="22" t="inlineStr">
@@ -28201,7 +28201,7 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>maa://51872 (96.78), maa://51876 (98.92), maa://51873 (100.0), maa://62047 (90.91)</t>
+          <t>maa://51872 (96.8), maa://51876 (98.92), maa://51873 (100.0), maa://62047 (90.91)</t>
         </is>
       </c>
       <c r="E394" t="inlineStr">
@@ -28228,7 +28228,7 @@
       </c>
       <c r="D395" t="inlineStr">
         <is>
-          <t>maa://59493 (96.64), maa://60449 (98.04), maa://59603 (100.0)</t>
+          <t>maa://59493 (96.64), maa://60449 (98.11), maa://59603 (83.33)</t>
         </is>
       </c>
       <c r="E395" t="inlineStr">
@@ -28282,7 +28282,7 @@
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>maa://62756 (90.0)</t>
+          <t>maa://62756 (89.74)</t>
         </is>
       </c>
       <c r="E397" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#211)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -705,7 +705,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (95.69), maa://24702 (94.87), maa://36681 (86.42)</t>
+          <t>maa://25390 (95.69), maa://24702 (94.89), maa://36681 (86.42)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -737,7 +737,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://39402 (95.12), *maa://34787 (73.91), maa://58660 (92.31)</t>
+          <t>maa://39402 (95.12), *maa://34787 (74.19), maa://58660 (92.86)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -769,7 +769,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (91.63)</t>
+          <t>maa://22742 (91.67)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -835,7 +835,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (95.83), maa://36987 (96.3), maa://39849 (88.89)</t>
+          <t>maa://40192 (95.9), maa://36987 (96.3), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -883,7 +883,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (94.9), maa://26254 (97.44), *maa://22738 (75.0)</t>
+          <t>maa://21249 (94.92), maa://26254 (97.44), *maa://22738 (75.0)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -899,7 +899,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://45854 (81.73), maa://24617 (91.18)</t>
+          <t>maa://45854 (81.9), maa://24617 (91.18)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -915,7 +915,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (84.08), maa://27484 (96.55), maa://27480 (85.0)</t>
+          <t>maa://27396 (83.84), maa://27484 (96.58), maa://27480 (85.0)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (95.88), maa://50121 (95.35)</t>
+          <t>maa://49983 (95.92), maa://50121 (95.35)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="X4" s="8" t="inlineStr">
         <is>
-          <t>maa://43217 (93.29)</t>
+          <t>maa://43217 (93.33)</t>
         </is>
       </c>
       <c r="Y4" s="19" t="n"/>
@@ -1100,7 +1100,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (83.96), maa://22744 (82.14), maa://54105 (94.74)</t>
+          <t>maa://21245 (83.67), maa://22744 (82.14), maa://54105 (90.0)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1480,7 +1480,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.07.13 13:23:12</t>
+          <t>更新日期：2025.07.15 13:26:28</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (87.59), maa://40166 (91.84)</t>
+          <t>maa://28711 (87.67), maa://40166 (91.84)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (89.5), *maa://22865 (53.45)</t>
+          <t>maa://26206 (89.01), *maa://22865 (53.45)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (90.0), maa://22501 (98.28), maa://45521 (91.89)</t>
+          <t>maa://22747 (90.0), maa://22501 (98.29), maa://45521 (91.89)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="X11" s="8" t="inlineStr">
         <is>
-          <t>maa://36713 (98.2)</t>
+          <t>maa://36713 (98.21)</t>
         </is>
       </c>
       <c r="Y11" s="19" t="n"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://22753 (92.09), maa://37962 (91.89), *maa://21485 (76.16)</t>
+          <t>maa://22753 (92.13), maa://37962 (90.67), *maa://21485 (76.16)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (92.88), maa://36673 (92.22), maa://25001 (86.49)</t>
+          <t>maa://24999 (92.89), maa://36673 (92.22), maa://25001 (86.49)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (94.83), maa://26245 (96.83), maa://21288 (96.3), maa://36682 (96.3)</t>
+          <t>maa://39841 (94.86), maa://26245 (96.83), maa://21288 (96.3), maa://36682 (96.3)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2405,7 +2405,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.54), maa://22734 (84.55), *maa://30808 (64.38), *maa://36048 (69.75), maa://45058 (86.36)</t>
+          <t>*maa://22743 (78.63), maa://22734 (84.55), *maa://30808 (64.38), *maa://36048 (69.42), maa://45058 (86.36)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2421,7 +2421,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (86.99), maa://21478 (90.24)</t>
+          <t>maa://24304 (87.04), maa://21478 (90.24)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2517,7 +2517,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://21364 (81.89), maa://36666 (81.82), *maa://22766 (68.8)</t>
+          <t>maa://21364 (81.89), maa://36666 (81.93), *maa://22766 (68.8)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2599,7 +2599,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://22729 (94.59), *maa://28648 (75.0), *maa://36674 (79.69)</t>
+          <t>maa://22729 (94.59), *maa://28648 (75.29), *maa://36674 (79.69)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -3087,7 +3087,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (86.15)</t>
+          <t>maa://41331 (86.21)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22524 (87.21), maa://22432 (83.56)</t>
+          <t>maa://22524 (87.21), maa://22432 (83.67)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3347,7 +3347,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>*maa://27127 (77.37), *maa://22751 (70.67)</t>
+          <t>*maa://27127 (77.54), *maa://22751 (70.67)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (95.74), maa://39875 (93.9)</t>
+          <t>maa://39756 (95.76), maa://39875 (93.9)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (84.98), maa://23504 (93.8), *maa://25141 (77.37), *maa://36663 (78.43), maa://52227 (95.65)</t>
+          <t>maa://29988 (84.98), maa://23504 (93.83), *maa://25141 (77.37), *maa://36663 (78.43), maa://52227 (95.65)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3687,7 +3687,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://22523 (81.74), *maa://36672 (73.91), maa://29910 (93.85), maa://45831 (88.89)</t>
+          <t>maa://22523 (81.74), *maa://36672 (72.86), maa://29910 (93.85), maa://45831 (88.89)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3931,7 +3931,7 @@
       </c>
       <c r="AB26" s="8" t="inlineStr">
         <is>
-          <t>maa://42235 (96.27)</t>
+          <t>maa://42235 (96.3)</t>
         </is>
       </c>
       <c r="AC26" s="19" t="n"/>
@@ -4095,7 +4095,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (90.8), maa://25725 (83.0)</t>
+          <t>maa://24465 (90.81), maa://25725 (83.0)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4175,7 +4175,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (92.16), maa://41749 (91.95)</t>
+          <t>maa://39929 (92.17), maa://41749 (92.0)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4225,7 +4225,7 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>maa://31694 (98.44)</t>
+          <t>maa://31694 (98.46)</t>
         </is>
       </c>
       <c r="E29" s="19" t="n"/>
@@ -4337,7 +4337,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.25), maa://42865 (81.36)</t>
+          <t>*maa://24080 (69.25), maa://42865 (81.67)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4517,7 +4517,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (93.53), maa://36258 (88.37), *maa://43904 (73.33)</t>
+          <t>maa://35926 (93.55), maa://36258 (88.44), *maa://43904 (73.33)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4679,7 +4679,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (97.17), maa://41108 (86.27), maa://41238 (98.11), maa://45523 (100.0)</t>
+          <t>maa://42859 (97.18), maa://41108 (86.27), maa://41238 (98.14), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4923,7 +4923,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (97.37), maa://56235 (100.0)</t>
+          <t>maa://48817 (97.4), maa://56235 (100.0)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
-          <t>maa://41296 (97.47)</t>
+          <t>maa://41296 (97.49)</t>
         </is>
       </c>
       <c r="M35" s="19" t="n"/>
@@ -5297,7 +5297,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (98.57), maa://47069 (81.82), maa://56336 (90.0), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.58), maa://47069 (81.82), maa://56336 (90.0), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5313,7 +5313,7 @@
       </c>
       <c r="P37" s="8" t="inlineStr">
         <is>
-          <t>maa://21280 (89.74), *maa://21239 (71.43)</t>
+          <t>maa://21280 (89.79), *maa://21239 (71.43)</t>
         </is>
       </c>
       <c r="Q37" s="19" t="n"/>
@@ -5462,7 +5462,7 @@
       </c>
       <c r="AF38" s="8" t="inlineStr">
         <is>
-          <t>maa://36697 (89.58)</t>
+          <t>maa://36697 (89.64)</t>
         </is>
       </c>
       <c r="AG38" s="16" t="n"/>
@@ -5483,7 +5483,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://36670 (88.52), maa://25199 (85.47), maa://30434 (93.53), *maa://45059 (75.0), *maa://44165 (75.0)</t>
+          <t>maa://36670 (87.8), maa://25199 (85.47), maa://30434 (93.62), *maa://45059 (75.0), *maa://44165 (75.0)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5515,7 +5515,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://24709 (91.62), maa://47093 (100.0)</t>
+          <t>maa://24709 (91.67), maa://47093 (100.0)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5563,7 +5563,7 @@
       </c>
       <c r="AF39" s="8" t="inlineStr">
         <is>
-          <t>**maa://62953 (50.0)</t>
+          <t>*maa://62953 (62.5)</t>
         </is>
       </c>
       <c r="AG39" s="16" t="n"/>
@@ -6078,7 +6078,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (91.86), maa://43901 (92.31)</t>
+          <t>maa://35931 (91.88), maa://43901 (92.31)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6147,7 +6147,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (96.92), maa://29661 (97.66), maa://28038 (84.62), maa://56236 (100.0)</t>
+          <t>maa://27410 (96.92), maa://29661 (97.67), maa://28038 (84.62), maa://56236 (100.0)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6322,7 +6322,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>*maa://62852 (77.78)</t>
+          <t>*maa://62852 (63.64)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6422,7 +6422,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (97.83), maa://59378 (94.74)</t>
+          <t>maa://59394 (97.87), maa://59378 (94.74)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6456,7 +6456,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (95.28)</t>
+          <t>maa://32534 (95.31)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -6540,7 +6540,7 @@
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>maa://32532 (93.57)</t>
+          <t>maa://32532 (93.59)</t>
         </is>
       </c>
       <c r="I55" s="19" t="n"/>
@@ -6684,7 +6684,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (97.85), maa://59413 (100.0)</t>
+          <t>maa://59534 (97.89), maa://59413 (100.0)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7006,7 +7006,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.07.13 13:23:12</t>
+          <t>更新日期：2025.07.15 13:26:28</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8135,12 +8135,12 @@
       </c>
       <c r="C22" s="12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D22" s="13" t="inlineStr">
         <is>
-          <t>maa://20948 (88.89), maa://30844 (100.0)</t>
+          <t>maa://20948 (88.89), maa://30844 (100.0), maa://58691 (100.0)</t>
         </is>
       </c>
       <c r="E22" s="14" t="inlineStr">
@@ -8680,7 +8680,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (87.88), maa://36866 (96.49), maa://45572 (93.33), maa://27794 (100.0), maa://20960 (100.0), maa://20843 (100.0), **maa://24483 (50.0), maa://20862 (83.33), *maa://20893 (77.78), maa://62759 (100.0)</t>
+          <t>maa://36644 (87.94), maa://36866 (96.49), maa://45572 (93.33), maa://27794 (100.0), maa://20960 (100.0), maa://20843 (100.0), **maa://24483 (50.0), maa://20862 (83.33), maa://62759 (100.0), *maa://20893 (77.78)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -9976,7 +9976,7 @@
       </c>
       <c r="D56" s="13" t="inlineStr">
         <is>
-          <t>maa://44235 (98.26), maa://45604 (100.0), maa://20961 (100.0), maa://44220 (100.0), maa://20910 (100.0)</t>
+          <t>maa://44235 (98.27), maa://45604 (100.0), maa://20961 (100.0), maa://44220 (100.0), maa://20910 (100.0)</t>
         </is>
       </c>
       <c r="E56" s="14" t="inlineStr">
@@ -10192,7 +10192,7 @@
       </c>
       <c r="D60" s="13" t="inlineStr">
         <is>
-          <t>maa://38298 (87.74)</t>
+          <t>maa://38298 (87.85)</t>
         </is>
       </c>
       <c r="E60" s="14" t="inlineStr">
@@ -12784,7 +12784,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://25018 (96.72), maa://51881 (99.24), maa://25776 (92.11), maa://28361 (95.12), maa://25772 (94.12), maa://56588 (95.0), maa://45194 (82.35), maa://25161 (81.25), maa://32653 (85.71), ***maa://60902 (28.57)</t>
+          <t>maa://25018 (96.73), maa://51881 (99.24), maa://25776 (92.11), maa://28361 (95.24), maa://25772 (94.12), maa://56588 (95.0), maa://45194 (82.35), maa://25161 (81.25), maa://32653 (85.71), ***maa://60902 (28.57)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -12946,7 +12946,7 @@
       </c>
       <c r="D111" s="13" t="inlineStr">
         <is>
-          <t>*maa://28554 (80.0)</t>
+          <t>maa://28554 (80.77)</t>
         </is>
       </c>
       <c r="E111" s="14" t="inlineStr">
@@ -13054,7 +13054,7 @@
       </c>
       <c r="D113" s="13" t="inlineStr">
         <is>
-          <t>maa://29037 (98.51)</t>
+          <t>maa://29037 (97.06)</t>
         </is>
       </c>
       <c r="E113" s="14" t="inlineStr">
@@ -13486,7 +13486,7 @@
       </c>
       <c r="D121" s="13" t="inlineStr">
         <is>
-          <t>maa://20869 (100.0), maa://44690 (95.83)</t>
+          <t>maa://20869 (100.0), maa://44690 (96.0)</t>
         </is>
       </c>
       <c r="E121" s="14" t="inlineStr">
@@ -14674,7 +14674,7 @@
       </c>
       <c r="D143" s="13" t="inlineStr">
         <is>
-          <t>maa://30670 (96.73), maa://31470 (96.67), *maa://45066 (71.43), **maa://30867 (40.0)</t>
+          <t>maa://30670 (96.75), maa://31470 (96.67), *maa://45066 (71.43), **maa://30867 (40.0)</t>
         </is>
       </c>
       <c r="E143" s="14" t="inlineStr">
@@ -14998,7 +14998,7 @@
       </c>
       <c r="D149" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.14), maa://36641 (98.45), maa://36865 (95.81), maa://44635 (88.07), maa://44660 (92.31), maa://41128 (84.21), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
+          <t>maa://40957 (94.19), maa://36641 (98.45), maa://36865 (95.81), maa://44635 (88.07), maa://44660 (92.31), maa://41128 (84.21), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
         </is>
       </c>
       <c r="E149" s="14" t="inlineStr">
@@ -15970,7 +15970,7 @@
       </c>
       <c r="D167" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (92.31), maa://29627 (92.73), maa://29659 (86.11), maa://49074 (97.87), **maa://30679 (50.0), maa://29861 (100.0), maa://42343 (100.0)</t>
+          <t>maa://29633 (92.31), maa://29627 (92.73), maa://29659 (86.11), maa://49074 (95.92), **maa://30679 (50.0), maa://29861 (100.0), maa://42343 (100.0)</t>
         </is>
       </c>
       <c r="E167" s="14" t="inlineStr">
@@ -16456,7 +16456,7 @@
       </c>
       <c r="D176" s="13" t="inlineStr">
         <is>
-          <t>maa://37690 (88.89)</t>
+          <t>maa://37690 (90.0)</t>
         </is>
       </c>
       <c r="E176" s="14" t="inlineStr">
@@ -17590,7 +17590,7 @@
       </c>
       <c r="D197" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.2), maa://35854 (86.0), maa://50388 (98.03), maa://25760 (86.96), ***maa://43911 (12.5), *maa://20872 (52.0), maa://51066 (100.0)</t>
+          <t>maa://44224 (90.22), maa://35854 (86.14), maa://50388 (98.03), maa://25760 (86.96), ***maa://43911 (12.5), *maa://20872 (52.0), maa://51066 (100.0)</t>
         </is>
       </c>
       <c r="E197" s="14" t="inlineStr">
@@ -19912,7 +19912,7 @@
       </c>
       <c r="D240" s="13" t="inlineStr">
         <is>
-          <t>*maa://30667 (78.77), maa://30666 (83.55), **maa://30739 (43.24), *maa://30723 (56.45), maa://39588 (89.09)</t>
+          <t>*maa://30667 (78.81), maa://30666 (83.55), **maa://30739 (43.24), *maa://30723 (56.45), maa://39588 (89.09)</t>
         </is>
       </c>
       <c r="E240" s="14" t="inlineStr">
@@ -20398,7 +20398,7 @@
       </c>
       <c r="D249" s="13" t="inlineStr">
         <is>
-          <t>maa://28923 (91.46), maa://28906 (98.28), ***maa://28825 (11.54)</t>
+          <t>maa://28923 (91.5), maa://28906 (98.28), ***maa://28825 (11.54)</t>
         </is>
       </c>
       <c r="E249" s="14" t="inlineStr">
@@ -20830,7 +20830,7 @@
       </c>
       <c r="D257" s="13" t="inlineStr">
         <is>
-          <t>maa://20879 (87.21), maa://20834 (92.86)</t>
+          <t>maa://20879 (87.36), maa://20834 (92.86)</t>
         </is>
       </c>
       <c r="E257" s="14" t="inlineStr">
@@ -21316,7 +21316,7 @@
       </c>
       <c r="D266" s="13" t="inlineStr">
         <is>
-          <t>maa://22467 (95.83)</t>
+          <t>maa://22467 (95.92)</t>
         </is>
       </c>
       <c r="E266" s="14" t="inlineStr">
@@ -21640,7 +21640,7 @@
       </c>
       <c r="D272" s="26" t="inlineStr">
         <is>
-          <t>***maa://62757 (30.0)</t>
+          <t>**maa://62757 (36.36)</t>
         </is>
       </c>
       <c r="E272" s="27" t="inlineStr">
@@ -21748,7 +21748,7 @@
       </c>
       <c r="D274" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (99.24), maa://51630 (96.63), maa://56588 (95.0), *maa://55171 (57.14), maa://51893 (88.89), ***maa://60902 (28.57)</t>
+          <t>maa://51881 (99.24), maa://51630 (96.67), maa://56588 (95.0), *maa://55171 (57.14), maa://51893 (88.89), ***maa://60902 (28.57)</t>
         </is>
       </c>
       <c r="E274" s="14" t="inlineStr">
@@ -22504,7 +22504,7 @@
       </c>
       <c r="D288" s="13" t="inlineStr">
         <is>
-          <t>maa://20899 (89.66), maa://46332 (95.45), ***maa://44744 (25.0)</t>
+          <t>maa://20899 (89.71), maa://46332 (95.45), ***maa://44744 (25.0)</t>
         </is>
       </c>
       <c r="E288" s="14" t="inlineStr">
@@ -22828,7 +22828,7 @@
       </c>
       <c r="D294" s="13" t="inlineStr">
         <is>
-          <t>maa://25774 (97.14), maa://28133 (93.1), maa://22469 (92.86), **maa://39217 (41.18), **maa://31349 (50.0)</t>
+          <t>maa://25774 (97.18), maa://28133 (93.1), maa://22469 (92.86), **maa://39217 (41.18), **maa://31349 (50.0)</t>
         </is>
       </c>
       <c r="E294" s="14" t="inlineStr">
@@ -23422,7 +23422,7 @@
       </c>
       <c r="D305" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (97.4), maa://49642 (97.0), maa://49660 (90.32), *maa://50517 (80.0)</t>
+          <t>maa://50280 (97.44), maa://49642 (97.0), maa://49660 (90.32), *maa://50517 (80.0)</t>
         </is>
       </c>
       <c r="E305" s="14" t="inlineStr">
@@ -23746,7 +23746,7 @@
       </c>
       <c r="D311" s="13" t="inlineStr">
         <is>
-          <t>maa://35859 (97.75)</t>
+          <t>maa://35859 (97.78)</t>
         </is>
       </c>
       <c r="E311" s="14" t="inlineStr">
@@ -24124,7 +24124,7 @@
       </c>
       <c r="D318" s="13" t="inlineStr">
         <is>
-          <t>*maa://62755 (60.0)</t>
+          <t>**maa://62755 (50.0)</t>
         </is>
       </c>
       <c r="E318" s="14" t="inlineStr">
@@ -24934,7 +24934,7 @@
       </c>
       <c r="D333" s="15" t="inlineStr">
         <is>
-          <t>maa://34205 (88.89), *maa://39541 (75.0)</t>
+          <t>maa://34205 (90.0), *maa://39541 (75.0)</t>
         </is>
       </c>
       <c r="E333" s="15" t="inlineStr">
@@ -25852,7 +25852,7 @@
       </c>
       <c r="D350" s="22" t="inlineStr">
         <is>
-          <t>maa://34865 (97.84), maa://34717 (94.12), *maa://45066 (71.43)</t>
+          <t>maa://34865 (97.86), maa://34717 (94.12), *maa://45066 (71.43)</t>
         </is>
       </c>
       <c r="E350" s="22" t="inlineStr">
@@ -26608,7 +26608,7 @@
       </c>
       <c r="D364" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (94.14), maa://44635 (88.07), maa://48026 (94.59), maa://41035 (93.06), maa://44660 (92.31), maa://41128 (84.21), *maa://60251 (66.67)</t>
+          <t>maa://40957 (94.19), maa://44635 (88.07), maa://48026 (94.59), maa://41035 (93.06), maa://44660 (92.31), maa://41128 (84.21), *maa://60251 (66.67)</t>
         </is>
       </c>
       <c r="E364" s="22" t="inlineStr">
@@ -27472,7 +27472,7 @@
       </c>
       <c r="D380" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (82.64), maa://44745 (97.37), **maa://49516 (34.78), *maa://45952 (72.73), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
+          <t>maa://42970 (82.71), maa://44745 (97.39), **maa://49516 (34.78), *maa://45952 (72.73), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E380" s="22" t="inlineStr">
@@ -28201,7 +28201,7 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>maa://51872 (96.8), maa://51876 (98.92), maa://51873 (100.0), maa://62047 (90.91)</t>
+          <t>maa://51872 (96.62), maa://51876 (98.92), maa://51873 (100.0), maa://62047 (90.91)</t>
         </is>
       </c>
       <c r="E394" t="inlineStr">
@@ -28228,7 +28228,7 @@
       </c>
       <c r="D395" t="inlineStr">
         <is>
-          <t>maa://59493 (96.64), maa://60449 (98.11), maa://59603 (83.33)</t>
+          <t>maa://59493 (96.69), maa://60449 (98.15), *maa://59603 (77.78)</t>
         </is>
       </c>
       <c r="E395" t="inlineStr">
@@ -28282,7 +28282,7 @@
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>maa://62756 (89.74)</t>
+          <t>maa://62756 (91.3)</t>
         </is>
       </c>
       <c r="E397" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#212)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -705,7 +705,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (95.69), maa://24702 (94.89), maa://36681 (86.42)</t>
+          <t>maa://25390 (95.7), maa://24702 (94.89), maa://36681 (86.59)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -801,7 +801,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://21246 (91.53), maa://36684 (93.68)</t>
+          <t>maa://21246 (91.53), maa://36684 (93.75)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -817,7 +817,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://25251 (91.91), maa://59087 (95.45)</t>
+          <t>maa://25251 (91.91), maa://59087 (95.65)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -835,7 +835,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (95.9), maa://36987 (96.3), maa://39849 (88.89)</t>
+          <t>maa://40192 (95.97), maa://36987 (96.3), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -867,7 +867,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>*maa://22880 (66.12), maa://20276 (87.96), *maa://22749 (78.95)</t>
+          <t>*maa://22880 (66.4), maa://20276 (87.96), *maa://22749 (78.95)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -883,7 +883,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (94.92), maa://26254 (97.44), *maa://22738 (75.0)</t>
+          <t>maa://21249 (94.95), maa://26254 (97.44), *maa://22738 (75.0)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -915,7 +915,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (83.84), maa://27484 (96.58), maa://27480 (85.0)</t>
+          <t>maa://27396 (83.93), maa://27484 (96.58), maa://27480 (85.0)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (95.92), maa://50121 (95.35)</t>
+          <t>maa://49983 (95.96), maa://50121 (95.35)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://32509 (94.07), maa://27295 (88.12), maa://22754 (89.19), *maa://31008 (79.55)</t>
+          <t>maa://32509 (94.07), maa://27295 (87.25), maa://22754 (89.19), *maa://31008 (79.55)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="X4" s="8" t="inlineStr">
         <is>
-          <t>maa://43217 (93.33)</t>
+          <t>maa://43217 (93.42)</t>
         </is>
       </c>
       <c r="Y4" s="19" t="n"/>
@@ -1100,7 +1100,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (83.67), maa://22744 (82.14), maa://54105 (90.0)</t>
+          <t>maa://21245 (83.67), maa://22744 (82.14), maa://54105 (90.48)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>maa://21955 (94.0)</t>
+          <t>maa://21955 (94.12)</t>
         </is>
       </c>
       <c r="E7" s="19" t="n"/>
@@ -1392,7 +1392,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (94.34), maa://24957 (97.83)</t>
+          <t>maa://28624 (94.38), maa://24957 (97.83)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1472,7 +1472,7 @@
       </c>
       <c r="AF7" s="8" t="inlineStr">
         <is>
-          <t>maa://45272 (97.3)</t>
+          <t>maa://45272 (97.37)</t>
         </is>
       </c>
       <c r="AG7" s="16" t="n"/>
@@ -1480,7 +1480,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.07.15 13:26:28</t>
+          <t>更新日期：2025.07.16 13:27:18</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (95.31)</t>
+          <t>maa://21411 (95.33)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="AB8" s="8" t="inlineStr">
         <is>
-          <t>maa://25389 (89.13)</t>
+          <t>maa://25389 (89.36)</t>
         </is>
       </c>
       <c r="AC8" s="19" t="n"/>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>*maa://24479 (77.0), *maa://21990 (51.85)</t>
+          <t>*maa://24479 (77.23), *maa://21990 (51.85)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (89.01), *maa://22865 (53.45)</t>
+          <t>maa://26206 (89.13), *maa://22865 (53.45)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1755,7 +1755,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.45), ***maa://39951 (11.39), ***maa://34206 (22.22), *maa://45271 (61.9), ***maa://39243 (25.0), **maa://54000 (50.0)</t>
+          <t>***maa://25695 (18.84), ***maa://39951 (11.39), ***maa://34206 (22.22), *maa://45271 (61.18), ***maa://39243 (25.0), **maa://54000 (50.0)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -2095,7 +2095,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://22753 (92.13), maa://37962 (90.67), *maa://21485 (76.16)</t>
+          <t>maa://22753 (92.17), maa://37962 (90.67), *maa://21485 (76.16)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2193,7 +2193,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (93.79), *maa://22583 (78.57), maa://48321 (85.71)</t>
+          <t>maa://22676 (93.84), *maa://22583 (78.57), maa://48321 (85.71)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (94.86), maa://26245 (96.83), maa://21288 (96.3), maa://36682 (96.3)</t>
+          <t>maa://39841 (94.89), maa://26245 (96.83), maa://21288 (96.3), maa://36682 (96.3)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2405,7 +2405,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.63), maa://22734 (84.55), *maa://30808 (64.38), *maa://36048 (69.42), maa://45058 (86.36)</t>
+          <t>*maa://22743 (78.63), maa://22734 (84.55), *maa://30808 (63.51), *maa://36048 (69.42), maa://45058 (82.61)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2421,7 +2421,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (87.04), maa://21478 (90.24)</t>
+          <t>maa://24304 (87.08), maa://21478 (90.24)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2681,7 +2681,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://22430 (89.77), maa://39599 (87.21)</t>
+          <t>maa://22430 (89.4), maa://39599 (87.21)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2875,7 +2875,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (97.27), maa://22741 (87.5)</t>
+          <t>maa://21917 (97.3), maa://22741 (87.5)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2989,7 +2989,7 @@
       </c>
       <c r="T19" s="8" t="inlineStr">
         <is>
-          <t>maa://24386 (98.71)</t>
+          <t>maa://24386 (98.73)</t>
         </is>
       </c>
       <c r="U19" s="19" t="n"/>
@@ -3087,7 +3087,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (86.21)</t>
+          <t>maa://41331 (86.26)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3135,7 +3135,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (89.53), maa://49976 (87.06), maa://56241 (90.0)</t>
+          <t>maa://50085 (89.53), maa://49976 (87.21), maa://56241 (90.0)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3281,7 +3281,7 @@
       </c>
       <c r="AB21" s="8" t="inlineStr">
         <is>
-          <t>maa://21443 (83.14)</t>
+          <t>maa://21443 (83.18)</t>
         </is>
       </c>
       <c r="AC21" s="19" t="n"/>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22524 (87.21), maa://22432 (83.67)</t>
+          <t>maa://22524 (87.26), maa://22432 (83.67)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3411,7 +3411,7 @@
       </c>
       <c r="AB22" s="8" t="inlineStr">
         <is>
-          <t>maa://23656 (100.0)</t>
+          <t>maa://23656 (98.72)</t>
         </is>
       </c>
       <c r="AC22" s="19" t="n"/>
@@ -3687,7 +3687,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://22523 (81.74), *maa://36672 (72.86), maa://29910 (93.85), maa://45831 (88.89)</t>
+          <t>maa://22523 (81.36), *maa://36672 (72.86), maa://29910 (93.85), maa://45831 (88.89)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3801,7 +3801,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (89.4), *maa://24516 (79.57), maa://26001 (84.75)</t>
+          <t>maa://31215 (89.47), *maa://24516 (79.57), maa://26001 (84.75)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3997,7 +3997,7 @@
       </c>
       <c r="L27" s="8" t="inlineStr">
         <is>
-          <t>maa://28071 (91.3)</t>
+          <t>maa://28071 (91.67)</t>
         </is>
       </c>
       <c r="M27" s="19" t="n"/>
@@ -4095,7 +4095,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (90.81), maa://25725 (83.0)</t>
+          <t>maa://24465 (90.82), maa://25725 (83.0)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4631,7 +4631,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://21895 (97.71), maa://36667 (97.44), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.72), maa://36667 (97.44), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4679,7 +4679,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (97.18), maa://41108 (86.27), maa://41238 (98.14), maa://45523 (100.0)</t>
+          <t>maa://42859 (97.2), maa://41108 (86.27), maa://41238 (98.14), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -5297,7 +5297,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (98.58), maa://47069 (81.82), maa://56336 (90.0), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.59), maa://47069 (81.82), maa://56336 (90.0), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5483,7 +5483,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://36670 (87.8), maa://25199 (85.47), maa://30434 (93.62), *maa://45059 (75.0), *maa://44165 (75.0)</t>
+          <t>maa://36670 (87.8), maa://25199 (85.47), maa://30434 (93.66), *maa://45059 (75.0), *maa://44165 (75.0)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5563,7 +5563,7 @@
       </c>
       <c r="AF39" s="8" t="inlineStr">
         <is>
-          <t>*maa://62953 (62.5)</t>
+          <t>*maa://62953 (78.57)</t>
         </is>
       </c>
       <c r="AG39" s="16" t="n"/>
@@ -5737,6 +5737,22 @@
         </is>
       </c>
       <c r="U41" s="19" t="n"/>
+      <c r="Z41" s="16" t="inlineStr">
+        <is>
+          <t>电弧</t>
+        </is>
+      </c>
+      <c r="AA41" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB41" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC41" s="16" t="n"/>
       <c r="AD41" s="19" t="inlineStr">
         <is>
           <t>裁度</t>
@@ -5855,7 +5871,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>maa://22525 (80.68), maa://21284 (88.14)</t>
+          <t>maa://22525 (80.23), maa://21284 (88.14)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -6322,7 +6338,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>*maa://62852 (63.64)</t>
+          <t>*maa://62852 (68.0)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6456,7 +6472,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (95.31)</t>
+          <t>maa://32534 (95.32)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -7006,7 +7022,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.07.15 13:26:28</t>
+          <t>更新日期：2025.07.16 13:27:18</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8194,7 +8210,7 @@
       </c>
       <c r="D23" s="13" t="inlineStr">
         <is>
-          <t>maa://20876 (94.59)</t>
+          <t>maa://20876 (94.74)</t>
         </is>
       </c>
       <c r="E23" s="14" t="inlineStr">
@@ -8680,7 +8696,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (87.94), maa://36866 (96.49), maa://45572 (93.33), maa://27794 (100.0), maa://20960 (100.0), maa://20843 (100.0), **maa://24483 (50.0), maa://20862 (83.33), maa://62759 (100.0), *maa://20893 (77.78)</t>
+          <t>maa://36644 (87.94), maa://36866 (96.49), maa://45572 (93.33), maa://27794 (100.0), maa://20960 (100.0), maa://20843 (100.0), **maa://24483 (50.0), maa://62759 (100.0), maa://20862 (83.33), *maa://20893 (77.78)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -8734,7 +8750,7 @@
       </c>
       <c r="D33" s="13" t="inlineStr">
         <is>
-          <t>maa://30500 (98.92), *maa://27290 (72.22), ***maa://42154 (8.33)</t>
+          <t>maa://30500 (98.94), *maa://27290 (72.22), ***maa://42154 (8.33)</t>
         </is>
       </c>
       <c r="E33" s="14" t="inlineStr">
@@ -8950,7 +8966,7 @@
       </c>
       <c r="D37" s="13" t="inlineStr">
         <is>
-          <t>maa://27376 (92.45), maa://42635 (95.65), *maa://20838 (55.0)</t>
+          <t>maa://27376 (92.86), maa://42635 (95.65), *maa://20838 (55.0)</t>
         </is>
       </c>
       <c r="E37" s="14" t="inlineStr">
@@ -10840,7 +10856,7 @@
       </c>
       <c r="D72" s="13" t="inlineStr">
         <is>
-          <t>maa://36643 (98.27), maa://36864 (98.0), maa://39140 (100.0)</t>
+          <t>maa://36643 (98.27), maa://36864 (98.02), maa://39140 (100.0)</t>
         </is>
       </c>
       <c r="E72" s="14" t="inlineStr">
@@ -12190,7 +12206,7 @@
       </c>
       <c r="D97" s="13" t="inlineStr">
         <is>
-          <t>maa://20991 (100.0), maa://51015 (88.46)</t>
+          <t>maa://20991 (100.0), maa://51015 (88.89)</t>
         </is>
       </c>
       <c r="E97" s="14" t="inlineStr">
@@ -12779,12 +12795,12 @@
       </c>
       <c r="C108" s="12" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://25018 (96.73), maa://51881 (99.24), maa://25776 (92.11), maa://28361 (95.24), maa://25772 (94.12), maa://56588 (95.0), maa://45194 (82.35), maa://25161 (81.25), maa://32653 (85.71), ***maa://60902 (28.57)</t>
+          <t>maa://25018 (96.73), maa://51881 (99.24), maa://25776 (92.11), maa://28361 (95.24), maa://25772 (94.12), maa://56588 (95.0), maa://45194 (82.35), maa://25161 (81.25), maa://32653 (85.71), ***maa://60902 (28.57), maa://61839 (100.0)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13810,7 +13826,7 @@
       </c>
       <c r="D127" s="13" t="inlineStr">
         <is>
-          <t>maa://20914 (100.0), *maa://31937 (75.0), maa://20829 (100.0)</t>
+          <t>maa://20914 (100.0), *maa://31937 (80.0), maa://20829 (100.0)</t>
         </is>
       </c>
       <c r="E127" s="14" t="inlineStr">
@@ -13864,7 +13880,7 @@
       </c>
       <c r="D128" s="13" t="inlineStr">
         <is>
-          <t>maa://37484 (94.23), maa://24611 (90.62)</t>
+          <t>maa://37484 (94.23), maa://24611 (90.91)</t>
         </is>
       </c>
       <c r="E128" s="14" t="inlineStr">
@@ -14998,7 +15014,7 @@
       </c>
       <c r="D149" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.19), maa://36641 (98.45), maa://36865 (95.81), maa://44635 (88.07), maa://44660 (92.31), maa://41128 (84.21), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
+          <t>maa://40957 (94.22), maa://36641 (98.45), maa://36865 (95.81), maa://44635 (88.07), maa://44660 (92.31), maa://41128 (84.21), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
         </is>
       </c>
       <c r="E149" s="14" t="inlineStr">
@@ -17590,7 +17606,7 @@
       </c>
       <c r="D197" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.22), maa://35854 (86.14), maa://50388 (98.03), maa://25760 (86.96), ***maa://43911 (12.5), *maa://20872 (52.0), maa://51066 (100.0)</t>
+          <t>maa://44224 (90.26), maa://35854 (86.14), maa://50388 (98.03), maa://25760 (86.96), ***maa://43911 (12.5), *maa://20872 (52.0), maa://51066 (100.0)</t>
         </is>
       </c>
       <c r="E197" s="14" t="inlineStr">
@@ -19804,7 +19820,7 @@
       </c>
       <c r="D238" s="13" t="inlineStr">
         <is>
-          <t>maa://20922 (94.2), *maa://32623 (75.0), maa://34242 (85.71)</t>
+          <t>maa://20922 (94.2), *maa://32623 (76.19), maa://34242 (85.71)</t>
         </is>
       </c>
       <c r="E238" s="14" t="inlineStr">
@@ -19961,12 +19977,12 @@
       </c>
       <c r="C241" s="12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D241" s="13" t="inlineStr">
         <is>
-          <t>maa://62759 (100.0)</t>
+          <t>maa://62759 (100.0), maa://62764 (100.0)</t>
         </is>
       </c>
       <c r="E241" s="14" t="inlineStr">
@@ -20776,7 +20792,7 @@
       </c>
       <c r="D256" s="13" t="inlineStr">
         <is>
-          <t>maa://20877 (98.7), *maa://45067 (75.0), maa://20836 (100.0), maa://20632 (100.0)</t>
+          <t>maa://20877 (98.72), *maa://45067 (75.0), maa://20836 (100.0), maa://20632 (100.0)</t>
         </is>
       </c>
       <c r="E256" s="14" t="inlineStr">
@@ -20830,7 +20846,7 @@
       </c>
       <c r="D257" s="13" t="inlineStr">
         <is>
-          <t>maa://20879 (87.36), maa://20834 (92.86)</t>
+          <t>maa://20879 (87.5), maa://20834 (92.86)</t>
         </is>
       </c>
       <c r="E257" s="14" t="inlineStr">
@@ -21640,7 +21656,7 @@
       </c>
       <c r="D272" s="26" t="inlineStr">
         <is>
-          <t>**maa://62757 (36.36)</t>
+          <t>**maa://62757 (38.46)</t>
         </is>
       </c>
       <c r="E272" s="27" t="inlineStr">
@@ -22504,7 +22520,7 @@
       </c>
       <c r="D288" s="13" t="inlineStr">
         <is>
-          <t>maa://20899 (89.71), maa://46332 (95.45), ***maa://44744 (25.0)</t>
+          <t>maa://20899 (89.71), maa://46332 (95.65), ***maa://44744 (25.0)</t>
         </is>
       </c>
       <c r="E288" s="14" t="inlineStr">
@@ -23422,7 +23438,7 @@
       </c>
       <c r="D305" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (97.44), maa://49642 (97.0), maa://49660 (90.32), *maa://50517 (80.0)</t>
+          <t>maa://50280 (97.47), maa://49642 (97.0), maa://49660 (90.32), *maa://50517 (80.0)</t>
         </is>
       </c>
       <c r="E305" s="14" t="inlineStr">
@@ -24119,12 +24135,12 @@
       </c>
       <c r="C318" s="12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D318" s="13" t="inlineStr">
         <is>
-          <t>**maa://62755 (50.0)</t>
+          <t>maa://62761 (100.0), **maa://62755 (50.0)</t>
         </is>
       </c>
       <c r="E318" s="14" t="inlineStr">
@@ -25042,7 +25058,7 @@
       </c>
       <c r="D335" s="15" t="inlineStr">
         <is>
-          <t>maa://44234 (99.11)</t>
+          <t>maa://44234 (99.12)</t>
         </is>
       </c>
       <c r="E335" s="15" t="inlineStr">
@@ -25312,7 +25328,7 @@
       </c>
       <c r="D340" s="22" t="inlineStr">
         <is>
-          <t>maa://38295 (94.85), maa://49332 (100.0)</t>
+          <t>maa://38295 (94.9), maa://49332 (100.0)</t>
         </is>
       </c>
       <c r="E340" s="22" t="inlineStr">
@@ -25474,7 +25490,7 @@
       </c>
       <c r="D343" s="22" t="inlineStr">
         <is>
-          <t>maa://32416 (91.53)</t>
+          <t>maa://32416 (91.67)</t>
         </is>
       </c>
       <c r="E343" s="22" t="inlineStr">
@@ -25577,12 +25593,12 @@
       </c>
       <c r="C345" s="12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D345" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (97.89), maa://32415 (96.79), maa://34677 (100.0), maa://32892 (100.0), maa://32653 (85.71)</t>
+          <t>maa://32647 (97.89), maa://32415 (96.79), maa://34677 (100.0), maa://32892 (100.0), maa://32653 (85.71), maa://61839 (100.0)</t>
         </is>
       </c>
       <c r="E345" s="22" t="inlineStr">
@@ -26122,7 +26138,7 @@
       </c>
       <c r="D355" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.56), maa://49695 (100.0), maa://49758 (98.46), *maa://59402 (60.87), *maa://52357 (71.43)</t>
+          <t>maa://49696 (99.56), maa://49695 (100.0), maa://49758 (98.48), *maa://59402 (58.33), *maa://52357 (71.43)</t>
         </is>
       </c>
       <c r="E355" s="22" t="inlineStr">
@@ -26392,7 +26408,7 @@
       </c>
       <c r="D360" s="22" t="inlineStr">
         <is>
-          <t>maa://36645 (98.38), maa://36841 (92.65), maa://37484 (94.23), maa://37858 (93.33), *maa://56268 (60.0), maa://40489 (100.0)</t>
+          <t>maa://36645 (98.38), maa://36841 (92.65), maa://37484 (94.23), maa://37858 (93.55), *maa://56268 (60.0), maa://40489 (100.0)</t>
         </is>
       </c>
       <c r="E360" s="22" t="inlineStr">
@@ -26608,7 +26624,7 @@
       </c>
       <c r="D364" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (94.19), maa://44635 (88.07), maa://48026 (94.59), maa://41035 (93.06), maa://44660 (92.31), maa://41128 (84.21), *maa://60251 (66.67)</t>
+          <t>maa://40957 (94.22), maa://44635 (88.07), maa://48026 (93.75), maa://41035 (93.06), maa://44660 (92.31), maa://41128 (84.21), *maa://60251 (66.67)</t>
         </is>
       </c>
       <c r="E364" s="22" t="inlineStr">
@@ -28201,7 +28217,7 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>maa://51872 (96.62), maa://51876 (98.92), maa://51873 (100.0), maa://62047 (90.91)</t>
+          <t>maa://51872 (96.64), maa://51876 (98.92), maa://51873 (100.0), maa://62047 (91.67)</t>
         </is>
       </c>
       <c r="E394" t="inlineStr">
@@ -28223,12 +28239,12 @@
       </c>
       <c r="C395" s="17" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D395" t="inlineStr">
         <is>
-          <t>maa://59493 (96.69), maa://60449 (98.15), *maa://59603 (77.78)</t>
+          <t>maa://59493 (96.72), maa://60449 (98.25)</t>
         </is>
       </c>
       <c r="E395" t="inlineStr">
@@ -28282,7 +28298,7 @@
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>maa://62756 (91.3)</t>
+          <t>maa://62756 (92.59)</t>
         </is>
       </c>
       <c r="E397" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#214)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -706,7 +706,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (95.74), maa://24702 (94.9), maa://36681 (86.59)</t>
+          <t>maa://25390 (95.76), maa://24702 (94.9), maa://36681 (86.59)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -770,7 +770,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (91.67)</t>
+          <t>maa://22742 (91.27)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -836,7 +836,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (96.03), maa://36987 (96.3), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.06), maa://36987 (96.3), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://32509 (94.16), maa://27295 (87.38), maa://22754 (89.19), *maa://31008 (79.55)</t>
+          <t>maa://32509 (94.2), maa://27295 (87.38), maa://22754 (89.19), *maa://31008 (79.55)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="T7" s="8" t="inlineStr">
         <is>
-          <t>maa://21291 (88.06)</t>
+          <t>maa://21291 (88.24)</t>
         </is>
       </c>
       <c r="U7" s="19" t="n"/>
@@ -1481,7 +1481,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.07.23 13:29:43</t>
+          <t>更新日期：2025.07.25 13:29:06</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1512,7 +1512,7 @@
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
-          <t>*maa://24371 (57.32)</t>
+          <t>*maa://24371 (57.83)</t>
         </is>
       </c>
       <c r="I8" s="19" t="n"/>
@@ -1576,7 +1576,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (95.13)</t>
+          <t>maa://21411 (95.18)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1738,7 +1738,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (89.3), *maa://22865 (53.45)</t>
+          <t>maa://26206 (89.42), *maa://22865 (53.45)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1756,7 +1756,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.84), ***maa://39951 (11.39), ***maa://34206 (22.22), *maa://45271 (61.18), ***maa://39243 (25.0), **maa://54000 (50.0)</t>
+          <t>***maa://25695 (18.84), ***maa://39951 (11.25), ***maa://34206 (22.22), *maa://45271 (60.47), ***maa://39243 (25.0), **maa://54000 (50.0)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1836,7 +1836,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://22301 (97.96), maa://45828 (94.23), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.97), maa://45828 (94.23), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -2096,7 +2096,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://22753 (92.2), maa://37962 (90.67), *maa://21485 (76.16)</t>
+          <t>maa://22753 (92.24), maa://37962 (90.67), *maa://21485 (76.32)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2146,7 +2146,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (92.93), maa://36673 (92.39), maa://25001 (86.49)</t>
+          <t>maa://24999 (92.94), maa://36673 (92.39), maa://25001 (86.49)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2162,7 +2162,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.96), **maa://22728 (46.94)</t>
+          <t>*maa://21248 (74.05), **maa://22728 (46.94)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2226,7 +2226,7 @@
       </c>
       <c r="X13" s="8" t="inlineStr">
         <is>
-          <t>maa://34957 (85.12)</t>
+          <t>maa://34957 (85.25)</t>
         </is>
       </c>
       <c r="Y13" s="19" t="n"/>
@@ -2308,7 +2308,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (94.92), maa://26245 (96.84), maa://21288 (96.3), maa://36682 (96.3)</t>
+          <t>maa://39841 (94.38), maa://26245 (96.84), maa://21288 (96.3), maa://36682 (94.55)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.71), maa://22734 (84.55), *maa://30808 (63.51), *maa://36048 (70.87), maa://45058 (82.61)</t>
+          <t>*maa://22743 (78.8), maa://22734 (84.55), *maa://30808 (63.51), *maa://36048 (71.32), maa://45058 (82.61)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2518,7 +2518,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://21364 (81.98), maa://36666 (81.93), *maa://22766 (68.8)</t>
+          <t>maa://21364 (82.03), maa://36666 (81.93), *maa://22766 (68.8)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2616,7 +2616,7 @@
       </c>
       <c r="X16" s="8" t="inlineStr">
         <is>
-          <t>maa://28501 (98.39), maa://28051 (96.0)</t>
+          <t>maa://28501 (98.4), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="19" t="n"/>
@@ -2828,7 +2828,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://22466 (92.31), maa://52226 (96.43)</t>
+          <t>maa://22466 (92.38), maa://52226 (96.43)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -3056,7 +3056,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://21432 (90.95), maa://25198 (93.94), maa://36680 (91.18)</t>
+          <t>maa://21432 (91.0), maa://25198 (93.94), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3088,7 +3088,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (86.47)</t>
+          <t>maa://41331 (86.52)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3136,7 +3136,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (89.33), maa://49976 (87.36), maa://56241 (90.0)</t>
+          <t>maa://50085 (89.39), maa://49976 (87.36), maa://56241 (90.0)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3282,7 +3282,7 @@
       </c>
       <c r="AB21" s="8" t="inlineStr">
         <is>
-          <t>maa://21443 (83.22)</t>
+          <t>maa://21443 (83.25)</t>
         </is>
       </c>
       <c r="AC21" s="19" t="n"/>
@@ -3298,7 +3298,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22524 (86.92), maa://22432 (84.11)</t>
+          <t>maa://22524 (86.97), maa://22432 (84.11)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (95.82), maa://39875 (93.9)</t>
+          <t>maa://39756 (95.84), maa://39875 (93.9)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3576,7 +3576,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>*maa://24368 (79.67), *maa://46650 (62.86)</t>
+          <t>*maa://24368 (79.67), *maa://46650 (63.89)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3656,7 +3656,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (85.03), maa://23504 (93.87), *maa://25141 (77.37), *maa://36663 (78.43), maa://52227 (95.65)</t>
+          <t>maa://29988 (85.03), maa://23504 (93.88), *maa://25141 (77.37), *maa://36663 (78.43), maa://52227 (95.65)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3688,7 +3688,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://22523 (81.36), *maa://36672 (72.86), maa://29910 (93.85), maa://45831 (88.89)</t>
+          <t>maa://22523 (81.36), *maa://36672 (72.22), maa://29910 (93.85), maa://45831 (88.89)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -4176,7 +4176,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (92.25), maa://41749 (92.11)</t>
+          <t>maa://39929 (92.25), maa://41749 (92.21)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4208,7 +4208,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (92.33)</t>
+          <t>maa://36660 (92.34)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4242,7 +4242,7 @@
       </c>
       <c r="H29" s="8" t="inlineStr">
         <is>
-          <t>*maa://25175 (56.34)</t>
+          <t>*maa://25175 (55.56)</t>
         </is>
       </c>
       <c r="I29" s="19" t="n"/>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (94.18), maa://31400 (98.91), maa://28440 (85.03), *maa://28650 (71.43)</t>
+          <t>maa://28432 (94.18), maa://31400 (98.91), maa://28440 (85.14), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4452,7 +4452,7 @@
       </c>
       <c r="AB30" s="8" t="inlineStr">
         <is>
-          <t>maa://42979 (97.25), maa://45822 (100.0), maa://45045 (83.33)</t>
+          <t>maa://42979 (97.27), maa://45822 (100.0), maa://45045 (83.33)</t>
         </is>
       </c>
       <c r="AC30" s="19" t="n"/>
@@ -4680,7 +4680,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (97.25), maa://41108 (86.27), maa://41238 (98.24), maa://45523 (100.0)</t>
+          <t>maa://42859 (97.25), maa://41108 (86.27), maa://41238 (98.26), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -5038,7 +5038,7 @@
       </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
-          <t>maa://41296 (97.5)</t>
+          <t>maa://41296 (97.51)</t>
         </is>
       </c>
       <c r="M35" s="19" t="n"/>
@@ -5463,7 +5463,7 @@
       </c>
       <c r="AF38" s="8" t="inlineStr">
         <is>
-          <t>maa://36697 (89.94)</t>
+          <t>maa://36697 (89.97)</t>
         </is>
       </c>
       <c r="AG38" s="16" t="n"/>
@@ -5564,7 +5564,7 @@
       </c>
       <c r="AF39" s="8" t="inlineStr">
         <is>
-          <t>maa://62953 (93.62)</t>
+          <t>maa://62953 (94.0)</t>
         </is>
       </c>
       <c r="AG39" s="16" t="n"/>
@@ -5617,7 +5617,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (95.32), maa://21386 (95.83), maa://36664 (88.71), maa://45550 (87.5)</t>
+          <t>maa://23278 (95.34), maa://21386 (95.83), maa://36664 (88.71), maa://45550 (87.5)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5957,7 +5957,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (97.69), maa://27728 (96.19), maa://56386 (100.0)</t>
+          <t>maa://29768 (97.7), maa://27728 (96.19), maa://56386 (100.0)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6095,7 +6095,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (92.0), maa://43901 (92.31)</t>
+          <t>maa://35931 (92.02), maa://43901 (92.31)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6164,7 +6164,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (96.94), maa://29661 (97.69), maa://28038 (84.62), maa://56236 (100.0)</t>
+          <t>maa://27410 (96.96), maa://29661 (97.69), maa://28038 (84.62), maa://56236 (100.0)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6339,7 +6339,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>*maa://62852 (70.59)</t>
+          <t>*maa://62852 (69.64)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6439,7 +6439,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (98.04), maa://59378 (95.24)</t>
+          <t>maa://59394 (98.08), maa://59378 (95.24)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6473,7 +6473,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (95.38)</t>
+          <t>maa://32534 (95.39)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -6557,7 +6557,7 @@
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>maa://32532 (93.62)</t>
+          <t>maa://32532 (93.64)</t>
         </is>
       </c>
       <c r="I55" s="19" t="n"/>
@@ -6701,7 +6701,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (97.98), maa://59413 (100.0)</t>
+          <t>maa://59534 (98.0), maa://59413 (100.0)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7023,7 +7023,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.07.23 13:29:43</t>
+          <t>更新日期：2025.07.25 13:29:06</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -7887,7 +7887,7 @@
       </c>
       <c r="D17" s="13" t="inlineStr">
         <is>
-          <t>*maa://20848 (80.0)</t>
+          <t>maa://20848 (83.33)</t>
         </is>
       </c>
       <c r="E17" s="14" t="inlineStr">
@@ -8211,7 +8211,7 @@
       </c>
       <c r="D23" s="13" t="inlineStr">
         <is>
-          <t>maa://20876 (95.45)</t>
+          <t>maa://20876 (95.56)</t>
         </is>
       </c>
       <c r="E23" s="14" t="inlineStr">
@@ -8967,7 +8967,7 @@
       </c>
       <c r="D37" s="13" t="inlineStr">
         <is>
-          <t>maa://27376 (92.86), maa://42635 (95.74), *maa://20838 (55.0)</t>
+          <t>maa://27376 (92.86), maa://42635 (95.83), *maa://20838 (55.0)</t>
         </is>
       </c>
       <c r="E37" s="14" t="inlineStr">
@@ -9183,7 +9183,7 @@
       </c>
       <c r="D41" s="13" t="inlineStr">
         <is>
-          <t>maa://20892 (80.85)</t>
+          <t>maa://20892 (81.25)</t>
         </is>
       </c>
       <c r="E41" s="14" t="inlineStr">
@@ -10641,7 +10641,7 @@
       </c>
       <c r="D68" s="13" t="inlineStr">
         <is>
-          <t>maa://20976 (97.88), maa://20815 (100.0)</t>
+          <t>maa://20976 (97.9), maa://20815 (100.0)</t>
         </is>
       </c>
       <c r="E68" s="14" t="inlineStr">
@@ -10749,7 +10749,7 @@
       </c>
       <c r="D70" s="13" t="inlineStr">
         <is>
-          <t>maa://20944 (95.83), maa://35393 (100.0)</t>
+          <t>maa://20944 (95.92), maa://35393 (100.0)</t>
         </is>
       </c>
       <c r="E70" s="14" t="inlineStr">
@@ -10857,7 +10857,7 @@
       </c>
       <c r="D72" s="13" t="inlineStr">
         <is>
-          <t>maa://36643 (98.29), maa://36864 (98.02), maa://39140 (100.0)</t>
+          <t>maa://36643 (98.3), maa://36864 (98.02), maa://39140 (100.0)</t>
         </is>
       </c>
       <c r="E72" s="14" t="inlineStr">
@@ -12477,7 +12477,7 @@
       </c>
       <c r="D102" s="13" t="inlineStr">
         <is>
-          <t>maa://40517 (96.3), *maa://39240 (60.0)</t>
+          <t>maa://40517 (92.86), *maa://39240 (56.25)</t>
         </is>
       </c>
       <c r="E102" s="14" t="inlineStr">
@@ -12796,12 +12796,12 @@
       </c>
       <c r="C108" s="12" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://25018 (96.73), maa://51881 (99.25), maa://25776 (92.11), maa://28361 (95.24), maa://25772 (94.12), maa://56588 (95.0), maa://45194 (82.35), maa://25161 (82.35), maa://32653 (85.71), ***maa://60902 (25.0), maa://61839 (100.0)</t>
+          <t>maa://25018 (96.73), maa://51881 (99.25), maa://25776 (92.11), maa://28361 (95.24), maa://25772 (94.12), maa://56588 (95.24), maa://45194 (82.35), maa://25161 (82.35), maa://32653 (85.71), ***maa://60902 (25.0), maa://61275 (100.0), maa://61839 (100.0)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13071,7 +13071,7 @@
       </c>
       <c r="D113" s="13" t="inlineStr">
         <is>
-          <t>maa://29037 (97.1)</t>
+          <t>maa://29037 (97.14)</t>
         </is>
       </c>
       <c r="E113" s="14" t="inlineStr">
@@ -13287,7 +13287,7 @@
       </c>
       <c r="D117" s="13" t="inlineStr">
         <is>
-          <t>maa://31560 (92.31), maa://20940 (90.91)</t>
+          <t>maa://31560 (92.31), maa://20940 (83.33)</t>
         </is>
       </c>
       <c r="E117" s="14" t="inlineStr">
@@ -13989,7 +13989,7 @@
       </c>
       <c r="D130" s="13" t="inlineStr">
         <is>
-          <t>maa://21422 (99.15)</t>
+          <t>maa://21422 (99.16)</t>
         </is>
       </c>
       <c r="E130" s="14" t="inlineStr">
@@ -14961,7 +14961,7 @@
       </c>
       <c r="D148" s="13" t="inlineStr">
         <is>
-          <t>maa://51549 (95.83), maa://51923 (95.83)</t>
+          <t>maa://51549 (95.92), maa://51923 (95.83)</t>
         </is>
       </c>
       <c r="E148" s="14" t="inlineStr">
@@ -16257,7 +16257,7 @@
       </c>
       <c r="D172" s="13" t="inlineStr">
         <is>
-          <t>maa://37690 (91.67)</t>
+          <t>maa://37690 (92.31)</t>
         </is>
       </c>
       <c r="E172" s="14" t="inlineStr">
@@ -17445,7 +17445,7 @@
       </c>
       <c r="D194" s="13" t="inlineStr">
         <is>
-          <t>maa://39156 (93.98), *maa://39550 (57.89), *maa://53417 (71.43)</t>
+          <t>maa://39156 (93.98), *maa://39550 (55.0), *maa://53417 (71.43)</t>
         </is>
       </c>
       <c r="E194" s="14" t="inlineStr">
@@ -18039,7 +18039,7 @@
       </c>
       <c r="D205" s="13" t="inlineStr">
         <is>
-          <t>maa://20956 (96.0), *maa://20830 (80.0), maa://44703 (91.67)</t>
+          <t>maa://20956 (96.02), *maa://20830 (80.0), maa://44703 (91.67)</t>
         </is>
       </c>
       <c r="E205" s="14" t="inlineStr">
@@ -18957,7 +18957,7 @@
       </c>
       <c r="D222" s="13" t="inlineStr">
         <is>
-          <t>*maa://29644 (74.0), maa://39159 (96.77), ***maa://30061 (27.27)</t>
+          <t>*maa://29644 (72.55), maa://39159 (96.77), ***maa://30061 (27.27)</t>
         </is>
       </c>
       <c r="E222" s="14" t="inlineStr">
@@ -20145,7 +20145,7 @@
       </c>
       <c r="D244" s="13" t="inlineStr">
         <is>
-          <t>maa://42287 (90.72), maa://45570 (96.49), maa://42225 (100.0), maa://60678 (100.0)</t>
+          <t>maa://42287 (89.8), maa://45570 (96.49), maa://42225 (100.0), maa://60678 (100.0)</t>
         </is>
       </c>
       <c r="E244" s="14" t="inlineStr">
@@ -20361,7 +20361,7 @@
       </c>
       <c r="D248" s="13" t="inlineStr">
         <is>
-          <t>maa://40958 (89.29), *maa://45067 (75.0)</t>
+          <t>maa://40958 (89.66), *maa://45067 (75.0)</t>
         </is>
       </c>
       <c r="E248" s="14" t="inlineStr">
@@ -20523,7 +20523,7 @@
       </c>
       <c r="D251" s="13" t="inlineStr">
         <is>
-          <t>maa://20879 (86.67), maa://20834 (92.86)</t>
+          <t>maa://20879 (85.71), maa://20834 (92.86)</t>
         </is>
       </c>
       <c r="E251" s="14" t="inlineStr">
@@ -21009,7 +21009,7 @@
       </c>
       <c r="D260" s="13" t="inlineStr">
         <is>
-          <t>maa://49643 (90.91)</t>
+          <t>maa://49643 (91.43)</t>
         </is>
       </c>
       <c r="E260" s="14" t="inlineStr">
@@ -21333,7 +21333,7 @@
       </c>
       <c r="D266" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (99.25), maa://51630 (96.7), maa://56588 (95.0), *maa://55171 (57.14), maa://51893 (88.89), ***maa://60902 (25.0)</t>
+          <t>maa://51881 (99.25), maa://51630 (96.7), maa://56588 (95.24), *maa://55171 (57.14), maa://51893 (88.89), ***maa://60902 (25.0)</t>
         </is>
       </c>
       <c r="E266" s="14" t="inlineStr">
@@ -23007,7 +23007,7 @@
       </c>
       <c r="D297" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (97.53), maa://49642 (97.0), maa://49660 (90.32), *maa://50517 (80.0)</t>
+          <t>maa://50280 (97.55), maa://49642 (97.0), maa://49660 (90.32), *maa://50517 (80.0)</t>
         </is>
       </c>
       <c r="E297" s="14" t="inlineStr">
@@ -23547,7 +23547,7 @@
       </c>
       <c r="D307" s="13" t="inlineStr">
         <is>
-          <t>maa://25775 (93.18), *maa://25393 (73.33)</t>
+          <t>maa://25775 (92.13), *maa://25393 (75.0)</t>
         </is>
       </c>
       <c r="E307" s="14" t="inlineStr">
@@ -24411,7 +24411,7 @@
       </c>
       <c r="D323" s="13" t="inlineStr">
         <is>
-          <t>maa://40956 (93.55)</t>
+          <t>maa://40956 (93.62)</t>
         </is>
       </c>
       <c r="E323" s="14" t="inlineStr">
@@ -24843,7 +24843,7 @@
       </c>
       <c r="D331" s="15" t="inlineStr">
         <is>
-          <t>maa://38295 (94.95), maa://49332 (100.0)</t>
+          <t>maa://38295 (95.0), maa://49332 (100.0)</t>
         </is>
       </c>
       <c r="E331" s="15" t="inlineStr">
@@ -25005,7 +25005,7 @@
       </c>
       <c r="D334" s="15" t="inlineStr">
         <is>
-          <t>maa://32416 (91.94)</t>
+          <t>maa://32416 (92.06)</t>
         </is>
       </c>
       <c r="E334" s="15" t="inlineStr">
@@ -25108,12 +25108,12 @@
       </c>
       <c r="C336" s="12" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D336" s="15" t="inlineStr">
         <is>
-          <t>maa://32647 (97.89), maa://32415 (96.82), maa://34677 (100.0), maa://32892 (100.0), maa://32653 (85.71), maa://61839 (100.0)</t>
+          <t>maa://32647 (97.89), maa://32415 (96.82), maa://34677 (100.0), maa://32892 (100.0), maa://32653 (85.71), maa://61275 (100.0), maa://61839 (100.0)</t>
         </is>
       </c>
       <c r="E336" s="15" t="inlineStr">
@@ -25383,7 +25383,7 @@
       </c>
       <c r="D341" s="22" t="inlineStr">
         <is>
-          <t>maa://34865 (97.88), maa://34717 (94.12), *maa://45066 (71.43)</t>
+          <t>maa://34865 (97.88), maa://34717 (94.2), *maa://45066 (71.43)</t>
         </is>
       </c>
       <c r="E341" s="22" t="inlineStr">
@@ -25599,7 +25599,7 @@
       </c>
       <c r="D345" s="22" t="inlineStr">
         <is>
-          <t>maa://36868 (99.72), maa://35996 (97.73), **maa://39217 (41.18), maa://47349 (95.56)</t>
+          <t>maa://36868 (99.72), maa://35996 (97.73), **maa://39217 (41.18), maa://47349 (95.65)</t>
         </is>
       </c>
       <c r="E345" s="22" t="inlineStr">
@@ -25977,7 +25977,7 @@
       </c>
       <c r="D352" s="22" t="inlineStr">
         <is>
-          <t>maa://42635 (95.74), maa://50629 (100.0), maa://48859 (100.0)</t>
+          <t>maa://42635 (95.83), maa://50629 (100.0), maa://48859 (100.0)</t>
         </is>
       </c>
       <c r="E352" s="22" t="inlineStr">
@@ -26355,7 +26355,7 @@
       </c>
       <c r="D359" s="22" t="inlineStr">
         <is>
-          <t>maa://45798 (98.48)</t>
+          <t>maa://45798 (98.51)</t>
         </is>
       </c>
       <c r="E359" s="22" t="inlineStr">
@@ -26895,7 +26895,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (82.71), maa://44745 (97.5), **maa://49516 (37.5), *maa://45952 (72.73), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
+          <t>maa://42970 (82.71), maa://44745 (97.53), **maa://49516 (37.5), *maa://45952 (72.73), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -27651,7 +27651,7 @@
       </c>
       <c r="D383" s="22" t="inlineStr">
         <is>
-          <t>maa://51872 (96.34), maa://51876 (98.95), maa://51873 (100.0), maa://62047 (92.86), maa://63228 (85.71)</t>
+          <t>maa://51872 (96.36), maa://51876 (98.95), maa://51873 (100.0), maa://62047 (93.33), maa://63228 (88.89)</t>
         </is>
       </c>
       <c r="E383" s="22" t="inlineStr">
@@ -27705,7 +27705,7 @@
       </c>
       <c r="D384" s="22" t="inlineStr">
         <is>
-          <t>maa://59493 (96.75), maa://60449 (98.0)</t>
+          <t>maa://59493 (96.77), maa://60449 (98.08)</t>
         </is>
       </c>
       <c r="E384" s="22" t="inlineStr">
@@ -27813,7 +27813,7 @@
       </c>
       <c r="D386" s="22" t="inlineStr">
         <is>
-          <t>maa://62756 (94.0)</t>
+          <t>maa://62756 (94.12)</t>
         </is>
       </c>
       <c r="E386" s="22" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#216)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -706,7 +706,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (95.77), maa://24702 (94.92), maa://36681 (86.59)</t>
+          <t>maa://25390 (95.79), maa://24702 (94.92), maa://36681 (86.59)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -738,7 +738,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://39402 (95.16), *maa://34787 (74.47), maa://58660 (94.12)</t>
+          <t>maa://39402 (94.4), *maa://34787 (74.47), maa://58660 (94.44)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -770,7 +770,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (91.3)</t>
+          <t>maa://22742 (91.34)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -802,7 +802,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://21246 (91.56), maa://36684 (93.92)</t>
+          <t>maa://21246 (91.56), maa://36684 (93.96)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -818,7 +818,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://25251 (91.91), maa://59087 (93.33)</t>
+          <t>maa://25251 (92.03), maa://59087 (93.33)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -836,7 +836,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (96.06), maa://36987 (96.3), maa://39849 (88.89)</t>
+          <t>maa://40192 (96.15), maa://36987 (96.3), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -868,7 +868,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>*maa://22880 (66.4), maa://20276 (88.29), *maa://22749 (80.0)</t>
+          <t>*maa://22880 (66.53), maa://20276 (88.34), *maa://22749 (80.0)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -884,7 +884,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (95.03), maa://26254 (97.44), *maa://22738 (75.0)</t>
+          <t>maa://21249 (95.07), maa://26254 (97.44), *maa://22738 (75.0)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -900,7 +900,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://45854 (82.57), maa://24617 (91.18), *maa://60545 (75.0)</t>
+          <t>maa://45854 (82.57), maa://24617 (91.18), *maa://60545 (80.0)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -966,7 +966,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (93.43), maa://22499 (88.24), maa://22746 (100.0)</t>
+          <t>maa://24632 (93.46), maa://22499 (88.24), maa://22746 (100.0)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (95.19), maa://50121 (95.65)</t>
+          <t>maa://49983 (94.34), maa://50121 (95.74)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://32509 (94.2), maa://27295 (87.62), maa://22754 (89.19), *maa://31008 (79.55)</t>
+          <t>maa://32509 (94.2), maa://27295 (87.74), maa://22754 (89.19), *maa://31008 (79.55)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="X4" s="8" t="inlineStr">
         <is>
-          <t>maa://43217 (92.99)</t>
+          <t>maa://43217 (93.04)</t>
         </is>
       </c>
       <c r="Y4" s="19" t="n"/>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="D6" s="8" t="inlineStr">
         <is>
-          <t>maa://42407 (92.94)</t>
+          <t>maa://42407 (93.02)</t>
         </is>
       </c>
       <c r="E6" s="19" t="n"/>
@@ -1263,7 +1263,7 @@
       </c>
       <c r="L6" s="8" t="inlineStr">
         <is>
-          <t>maa://24839 (98.88)</t>
+          <t>maa://24839 (98.89)</t>
         </is>
       </c>
       <c r="M6" s="19" t="n"/>
@@ -1393,7 +1393,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (94.67), maa://24957 (97.83)</t>
+          <t>maa://28624 (94.71), maa://24957 (97.83)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1481,7 +1481,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.07.27 13:27:11</t>
+          <t>更新日期：2025.07.29 13:34:35</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>*maa://21476 (76.67), *maa://39431 (61.11), **maa://37551 (50.0)</t>
+          <t>*maa://21476 (77.05), *maa://39431 (61.11), **maa://37551 (50.0)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1576,7 +1576,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (95.18)</t>
+          <t>maa://21411 (95.22)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://26223 (98.16), maa://52237 (100.0)</t>
+          <t>maa://26223 (98.17), maa://52237 (100.0)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1738,7 +1738,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (89.47), *maa://22865 (53.45)</t>
+          <t>maa://26206 (89.53), *maa://22865 (53.45)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1756,7 +1756,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>***maa://25695 (18.75), ***maa://39951 (11.11), ***maa://34206 (22.22), *maa://45271 (60.47), ***maa://39243 (25.0), **maa://54000 (50.0)</t>
+          <t>***maa://25695 (19.05), ***maa://39951 (11.11), ***maa://34206 (22.22), *maa://45271 (60.47), ***maa://39243 (25.0), **maa://54000 (50.0)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1815,12 +1815,12 @@
       </c>
       <c r="S10" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (96.9), maa://22755 (88.72)</t>
+          <t>maa://27395 (96.91), maa://22755 (88.72), maa://63521 (100.0)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1836,7 +1836,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://22301 (97.98), maa://45828 (94.34), maa://22726 (100.0)</t>
+          <t>maa://22301 (97.98), maa://45828 (94.55), maa://22726 (100.0)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1868,7 +1868,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>*maa://25021 (53.15), *maa://22733 (66.67), **maa://22761 (50.0)</t>
+          <t>*maa://25021 (53.15), *maa://22733 (67.39), **maa://22761 (50.0)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1918,7 +1918,7 @@
       </c>
       <c r="L11" s="8" t="inlineStr">
         <is>
-          <t>maa://21287 (88.62)</t>
+          <t>maa://21287 (88.71)</t>
         </is>
       </c>
       <c r="M11" s="19" t="n"/>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (89.5), maa://22501 (98.36), maa://45521 (92.31)</t>
+          <t>maa://22747 (89.5), maa://22501 (98.36), maa://45521 (92.5)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1966,7 +1966,7 @@
       </c>
       <c r="X11" s="8" t="inlineStr">
         <is>
-          <t>maa://36713 (98.21)</t>
+          <t>maa://36713 (98.22)</t>
         </is>
       </c>
       <c r="Y11" s="19" t="n"/>
@@ -2096,7 +2096,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://22753 (92.24), maa://37962 (90.79), *maa://21485 (76.32)</t>
+          <t>maa://22753 (92.24), maa://37962 (91.25), *maa://21485 (76.32)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2112,7 +2112,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://23669 (95.71), maa://36677 (95.74), maa://39872 (93.55)</t>
+          <t>maa://23669 (95.71), maa://36677 (95.79), maa://39872 (93.55)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>*maa://28932 (78.89), *maa://20106 (64.29), *maa://22769 (62.07)</t>
+          <t>*maa://28932 (79.01), *maa://20106 (64.29), *maa://22769 (62.07)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2146,7 +2146,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (92.96), maa://36673 (92.39), maa://25001 (86.67)</t>
+          <t>maa://24999 (92.99), maa://36673 (92.47), maa://25001 (86.67)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2162,7 +2162,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.14), **maa://22728 (46.94)</t>
+          <t>*maa://21248 (74.49), **maa://22728 (46.94)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2194,7 +2194,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (93.96), *maa://22583 (78.82), *maa://48321 (80.0)</t>
+          <t>maa://22676 (93.96), *maa://22583 (79.07), *maa://48321 (80.0)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2308,7 +2308,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (94.38), maa://26245 (96.84), maa://21288 (96.32), maa://36682 (94.55)</t>
+          <t>maa://39841 (94.38), maa://26245 (96.86), maa://21288 (96.32), maa://36682 (94.55)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2340,7 +2340,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://22521 (95.0), maa://42751 (96.15)</t>
+          <t>maa://22521 (95.08), maa://42751 (96.15)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>*maa://22743 (78.49), maa://22734 (84.55), *maa://30808 (63.51), *maa://36048 (71.32), maa://45058 (82.61)</t>
+          <t>*maa://22743 (78.57), maa://22734 (84.55), *maa://30808 (64.0), *maa://36048 (71.76), maa://45058 (82.61)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2422,7 +2422,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (87.27), maa://21478 (90.24)</t>
+          <t>maa://24304 (87.0), maa://21478 (90.24)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2454,7 +2454,7 @@
       </c>
       <c r="P15" s="8" t="inlineStr">
         <is>
-          <t>maa://24762 (91.1), *maa://22727 (70.0)</t>
+          <t>maa://24762 (91.15), *maa://22727 (70.0)</t>
         </is>
       </c>
       <c r="Q15" s="19" t="n"/>
@@ -2536,7 +2536,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://21441 (96.55), maa://37650 (96.92), maa://36679 (94.55)</t>
+          <t>maa://21441 (96.55), maa://37650 (96.97), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2616,7 +2616,7 @@
       </c>
       <c r="X16" s="8" t="inlineStr">
         <is>
-          <t>maa://28501 (98.43), maa://28051 (96.0)</t>
+          <t>maa://28501 (98.44), maa://28051 (96.0)</t>
         </is>
       </c>
       <c r="Y16" s="19" t="n"/>
@@ -2632,7 +2632,7 @@
       </c>
       <c r="AB16" s="8" t="inlineStr">
         <is>
-          <t>maa://26228 (95.73)</t>
+          <t>maa://26228 (95.76)</t>
         </is>
       </c>
       <c r="AC16" s="19" t="n"/>
@@ -2648,7 +2648,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>*maa://23911 (70.4), maa://27755 (94.12)</t>
+          <t>*maa://23911 (70.63), maa://27755 (94.12)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2682,7 +2682,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://22430 (89.59), maa://39599 (87.64)</t>
+          <t>maa://22430 (89.59), maa://39599 (87.78)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2796,7 +2796,7 @@
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>maa://24570 (97.23)</t>
+          <t>maa://24570 (97.26)</t>
         </is>
       </c>
       <c r="E18" s="19" t="n"/>
@@ -2828,7 +2828,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://22466 (92.38), maa://52226 (96.43)</t>
+          <t>maa://22466 (92.38), maa://52226 (96.67)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -3056,7 +3056,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://21432 (91.0), maa://25198 (93.94), maa://36680 (91.18)</t>
+          <t>maa://21432 (91.04), maa://25198 (93.98), maa://36680 (91.18)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3072,7 +3072,7 @@
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>maa://22864 (90.58)</t>
+          <t>maa://22864 (90.67)</t>
         </is>
       </c>
       <c r="I20" s="19" t="n"/>
@@ -3088,7 +3088,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (86.57)</t>
+          <t>maa://41331 (86.62)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3136,7 +3136,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (89.5), maa://49976 (87.78), maa://56241 (90.0)</t>
+          <t>maa://50085 (89.62), maa://49976 (87.78), maa://56241 (90.0)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3298,7 +3298,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22524 (86.97), maa://22432 (84.11)</t>
+          <t>maa://22524 (87.02), maa://22432 (84.21)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3332,7 +3332,7 @@
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>maa://25236 (96.4)</t>
+          <t>maa://25236 (96.43)</t>
         </is>
       </c>
       <c r="I22" s="19" t="n"/>
@@ -3348,7 +3348,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>*maa://27127 (77.7), *maa://22751 (70.67)</t>
+          <t>*maa://27127 (77.14), *maa://22751 (71.05)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3391,12 +3391,12 @@
       </c>
       <c r="W22" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://21282 (98.77)</t>
+          <t>maa://21282 (98.78), *maa://37649 (70.37)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3446,7 +3446,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>***maa://28036 (28.05), **maa://41753 (48.39)</t>
+          <t>***maa://28036 (27.71), **maa://41753 (46.88)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (95.86), maa://39875 (93.9)</t>
+          <t>maa://39756 (95.71), maa://39875 (93.98)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3494,7 +3494,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (91.89), *maa://29748 (76.3), *maa://37566 (79.17)</t>
+          <t>maa://30587 (91.93), *maa://29748 (76.47), *maa://37566 (79.17)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3576,7 +3576,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>*maa://24368 (79.67), *maa://46650 (63.89)</t>
+          <t>*maa://24368 (79.67), *maa://46650 (65.79)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3656,7 +3656,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (85.03), maa://23504 (93.91), *maa://25141 (77.37), *maa://36663 (78.43), maa://52227 (95.83)</t>
+          <t>maa://29988 (85.17), maa://23504 (93.91), *maa://25141 (77.37), *maa://36663 (78.43), maa://52227 (95.83)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3688,7 +3688,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://22523 (81.36), *maa://36672 (72.22), maa://29910 (93.85), maa://45831 (89.47)</t>
+          <t>maa://22523 (81.36), *maa://36672 (72.22), maa://29910 (93.85), maa://45831 (90.0)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3706,7 +3706,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (95.6), maa://63016 (100.0)</t>
+          <t>maa://29753 (95.61), maa://63016 (100.0)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3722,7 +3722,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>*maa://29063 (71.57), *maa://25311 (74.78), ***maa://22725 (4.76), *maa://45047 (73.33)</t>
+          <t>*maa://29063 (71.22), *maa://25311 (74.78), ***maa://22725 (4.76), *maa://45047 (73.33)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3802,7 +3802,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (89.68), *maa://24516 (79.57), maa://26001 (84.75)</t>
+          <t>maa://31215 (89.1), *maa://24516 (79.57), maa://26001 (84.75)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3818,7 +3818,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (96.0), maa://24621 (97.24), maa://36676 (97.06), maa://22771 (85.71), *maa://37772 (80.0)</t>
+          <t>maa://20108 (96.0), maa://24621 (97.24), maa://36676 (97.14), maa://22771 (85.71), *maa://37772 (80.0)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3932,7 +3932,7 @@
       </c>
       <c r="AB26" s="8" t="inlineStr">
         <is>
-          <t>maa://42235 (96.34)</t>
+          <t>maa://42235 (96.36)</t>
         </is>
       </c>
       <c r="AC26" s="19" t="n"/>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (90.84), maa://25725 (82.18)</t>
+          <t>maa://24465 (90.85), maa://25725 (82.35)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4176,7 +4176,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (92.28), maa://41749 (92.21)</t>
+          <t>maa://39929 (92.28), maa://41749 (92.31)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (94.18), maa://31400 (98.91), maa://28440 (85.23), *maa://28650 (71.43)</t>
+          <t>maa://28432 (94.2), maa://31400 (98.91), maa://28440 (85.23), *maa://28650 (71.43)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4338,7 +4338,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>*maa://24080 (69.25), maa://42865 (80.33)</t>
+          <t>*maa://24080 (69.33), maa://42865 (80.33)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4404,7 +4404,7 @@
       </c>
       <c r="P30" s="8" t="inlineStr">
         <is>
-          <t>maa://21442 (98.85)</t>
+          <t>maa://21442 (98.86)</t>
         </is>
       </c>
       <c r="Q30" s="19" t="n"/>
@@ -4632,7 +4632,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://21895 (97.74), maa://36667 (97.5), maa://22760 (100.0)</t>
+          <t>maa://21895 (97.74), maa://36667 (97.52), maa://22760 (100.0)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4680,7 +4680,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (97.29), maa://41108 (86.27), maa://41238 (98.26), maa://45523 (100.0)</t>
+          <t>maa://42859 (97.31), maa://41108 (86.27), maa://41238 (98.28), maa://45523 (100.0)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -5038,7 +5038,7 @@
       </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
-          <t>maa://41296 (97.54)</t>
+          <t>maa://41296 (97.55)</t>
         </is>
       </c>
       <c r="M35" s="19" t="n"/>
@@ -5298,7 +5298,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (98.61), maa://47069 (81.82), maa://56336 (81.82), maa://45789 (100.0)</t>
+          <t>maa://45718 (98.61), maa://47069 (81.82), maa://56336 (85.71), maa://45789 (100.0)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5314,7 +5314,7 @@
       </c>
       <c r="P37" s="8" t="inlineStr">
         <is>
-          <t>maa://21280 (89.83), *maa://21239 (71.43)</t>
+          <t>maa://21280 (89.87), *maa://21239 (71.43)</t>
         </is>
       </c>
       <c r="Q37" s="19" t="n"/>
@@ -5463,7 +5463,7 @@
       </c>
       <c r="AF38" s="8" t="inlineStr">
         <is>
-          <t>maa://36697 (89.97)</t>
+          <t>maa://36697 (89.77)</t>
         </is>
       </c>
       <c r="AG38" s="16" t="n"/>
@@ -5532,7 +5532,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (93.1), *maa://45788 (70.63), maa://45790 (81.25)</t>
+          <t>maa://47079 (90.76), *maa://45788 (70.54), maa://45790 (81.25)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5564,7 +5564,7 @@
       </c>
       <c r="AF39" s="8" t="inlineStr">
         <is>
-          <t>maa://62953 (92.73)</t>
+          <t>maa://62953 (91.23)</t>
         </is>
       </c>
       <c r="AG39" s="16" t="n"/>
@@ -5872,7 +5872,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>maa://22525 (80.34), maa://21284 (88.33)</t>
+          <t>maa://22525 (80.34), maa://21284 (88.52)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -6339,7 +6339,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>*maa://62852 (70.69)</t>
+          <t>*maa://62852 (68.85)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6439,7 +6439,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (98.18), maa://59378 (95.31)</t>
+          <t>maa://59394 (98.28), maa://59378 (95.31)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6557,7 +6557,7 @@
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>maa://32532 (93.64)</t>
+          <t>maa://32532 (93.42)</t>
         </is>
       </c>
       <c r="I55" s="19" t="n"/>
@@ -6629,7 +6629,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (95.0), maa://27746 (83.19)</t>
+          <t>maa://31270 (95.03), maa://27746 (83.19)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -6701,7 +6701,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (98.08), maa://59413 (100.0)</t>
+          <t>maa://59534 (98.1), maa://59413 (100.0)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7023,7 +7023,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.07.27 13:27:11</t>
+          <t>更新日期：2025.07.29 13:34:35</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8049,7 +8049,7 @@
       </c>
       <c r="D20" s="13" t="inlineStr">
         <is>
-          <t>maa://20865 (91.67), maa://20826 (85.71)</t>
+          <t>maa://20865 (92.31), maa://20826 (85.71)</t>
         </is>
       </c>
       <c r="E20" s="14" t="inlineStr">
@@ -8152,12 +8152,12 @@
       </c>
       <c r="C22" s="12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D22" s="13" t="inlineStr">
         <is>
-          <t>maa://20948 (88.89), maa://30844 (100.0), maa://58691 (100.0)</t>
+          <t>maa://20948 (88.89), maa://30844 (100.0), maa://58691 (100.0), maa://63387 (100.0)</t>
         </is>
       </c>
       <c r="E22" s="14" t="inlineStr">
@@ -8535,7 +8535,7 @@
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>maa://20863 (89.07), maa://20832 (99.12), maa://20727 (100.0)</t>
+          <t>maa://20863 (89.24), maa://20832 (99.13), maa://20727 (100.0)</t>
         </is>
       </c>
       <c r="E29" s="14" t="inlineStr">
@@ -9939,7 +9939,7 @@
       </c>
       <c r="D55" s="13" t="inlineStr">
         <is>
-          <t>maa://20932 (96.3), maa://42415 (100.0), maa://40838 (100.0)</t>
+          <t>maa://20932 (96.34), maa://42415 (100.0), maa://40838 (100.0)</t>
         </is>
       </c>
       <c r="E55" s="14" t="inlineStr">
@@ -9993,7 +9993,7 @@
       </c>
       <c r="D56" s="13" t="inlineStr">
         <is>
-          <t>maa://44235 (98.29), maa://45604 (100.0), maa://20961 (100.0), maa://44220 (100.0), maa://20910 (100.0)</t>
+          <t>maa://44235 (98.31), maa://45604 (100.0), maa://20961 (100.0), maa://44220 (100.0), maa://20910 (100.0)</t>
         </is>
       </c>
       <c r="E56" s="14" t="inlineStr">
@@ -10155,7 +10155,7 @@
       </c>
       <c r="D59" s="13" t="inlineStr">
         <is>
-          <t>maa://27970 (98.65), maa://41118 (85.71)</t>
+          <t>maa://27970 (98.72), maa://41118 (85.71)</t>
         </is>
       </c>
       <c r="E59" s="14" t="inlineStr">
@@ -10209,7 +10209,7 @@
       </c>
       <c r="D60" s="13" t="inlineStr">
         <is>
-          <t>maa://38298 (88.07)</t>
+          <t>maa://38298 (88.18)</t>
         </is>
       </c>
       <c r="E60" s="14" t="inlineStr">
@@ -10263,7 +10263,7 @@
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (100.0), maa://24093 (100.0), maa://31559 (94.74), maa://20924 (95.24), maa://25777 (100.0), maa://20631 (100.0), maa://28241 (100.0)</t>
+          <t>maa://20841 (100.0), maa://24093 (100.0), maa://31559 (94.87), maa://20924 (95.24), maa://25777 (100.0), maa://20631 (100.0), maa://28241 (100.0)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -10425,7 +10425,7 @@
       </c>
       <c r="D64" s="13" t="inlineStr">
         <is>
-          <t>maa://28187 (97.67), maa://33504 (100.0), maa://45144 (100.0), maa://43531 (100.0)</t>
+          <t>maa://28187 (97.67), maa://45144 (100.0), maa://33504 (100.0), maa://43531 (100.0)</t>
         </is>
       </c>
       <c r="E64" s="14" t="inlineStr">
@@ -10641,7 +10641,7 @@
       </c>
       <c r="D68" s="13" t="inlineStr">
         <is>
-          <t>maa://20976 (97.9), maa://20815 (100.0)</t>
+          <t>maa://20976 (97.91), maa://20815 (100.0)</t>
         </is>
       </c>
       <c r="E68" s="14" t="inlineStr">
@@ -10803,7 +10803,7 @@
       </c>
       <c r="D71" s="13" t="inlineStr">
         <is>
-          <t>maa://20943 (99.4), maa://30673 (100.0), maa://30672 (100.0), maa://20856 (100.0)</t>
+          <t>maa://20943 (99.41), maa://30673 (100.0), maa://30672 (100.0), maa://20856 (100.0)</t>
         </is>
       </c>
       <c r="E71" s="14" t="inlineStr">
@@ -10857,7 +10857,7 @@
       </c>
       <c r="D72" s="13" t="inlineStr">
         <is>
-          <t>maa://36643 (98.3), maa://36864 (98.04), maa://39140 (100.0)</t>
+          <t>maa://36643 (98.31), maa://36864 (98.04), maa://39140 (100.0)</t>
         </is>
       </c>
       <c r="E72" s="14" t="inlineStr">
@@ -11721,7 +11721,7 @@
       </c>
       <c r="D88" s="13" t="inlineStr">
         <is>
-          <t>maa://24472 (88.32), *maa://35841 (63.16)</t>
+          <t>maa://24472 (88.37), *maa://35841 (63.16)</t>
         </is>
       </c>
       <c r="E88" s="14" t="inlineStr">
@@ -12153,7 +12153,7 @@
       </c>
       <c r="D96" s="13" t="inlineStr">
         <is>
-          <t>maa://20926 (81.82)</t>
+          <t>maa://20926 (83.33)</t>
         </is>
       </c>
       <c r="E96" s="14" t="inlineStr">
@@ -12207,7 +12207,7 @@
       </c>
       <c r="D97" s="13" t="inlineStr">
         <is>
-          <t>maa://20991 (100.0), maa://51015 (87.88)</t>
+          <t>maa://20991 (100.0), maa://51015 (85.29)</t>
         </is>
       </c>
       <c r="E97" s="14" t="inlineStr">
@@ -12801,7 +12801,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://25018 (96.73), maa://51881 (99.26), maa://25776 (92.11), maa://28361 (95.24), maa://25772 (94.12), maa://56588 (95.24), maa://45194 (82.35), maa://32653 (85.71), maa://25161 (82.35), ***maa://60902 (25.0), maa://61275 (100.0), maa://61839 (100.0)</t>
+          <t>maa://25018 (96.73), maa://51881 (99.26), maa://25776 (92.11), maa://28361 (95.24), maa://25772 (94.12), maa://56588 (95.24), maa://45194 (82.35), maa://25161 (82.35), maa://32653 (85.71), ***maa://60902 (25.0), maa://61275 (100.0), maa://61839 (100.0)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13017,7 +13017,7 @@
       </c>
       <c r="D112" s="13" t="inlineStr">
         <is>
-          <t>maa://20933 (85.0), maa://20822 (100.0)</t>
+          <t>maa://20933 (85.19), maa://20822 (100.0)</t>
         </is>
       </c>
       <c r="E112" s="14" t="inlineStr">
@@ -13179,7 +13179,7 @@
       </c>
       <c r="D115" s="13" t="inlineStr">
         <is>
-          <t>maa://20908 (98.07), maa://35723 (96.0), *maa://23346 (77.78), maa://38822 (100.0), maa://58659 (100.0)</t>
+          <t>maa://20908 (98.08), maa://35723 (96.0), *maa://23346 (77.78), maa://38822 (100.0), maa://58659 (100.0)</t>
         </is>
       </c>
       <c r="E115" s="14" t="inlineStr">
@@ -13341,7 +13341,7 @@
       </c>
       <c r="D118" s="13" t="inlineStr">
         <is>
-          <t>maa://20986 (93.75)</t>
+          <t>maa://20986 (94.12)</t>
         </is>
       </c>
       <c r="E118" s="14" t="inlineStr">
@@ -14475,7 +14475,7 @@
       </c>
       <c r="D139" s="13" t="inlineStr">
         <is>
-          <t>**maa://30679 (50.0), maa://45258 (94.12)</t>
+          <t>**maa://30679 (50.0), maa://45258 (88.89)</t>
         </is>
       </c>
       <c r="E139" s="14" t="inlineStr">
@@ -14691,7 +14691,7 @@
       </c>
       <c r="D143" s="13" t="inlineStr">
         <is>
-          <t>maa://30670 (96.75), maa://31470 (96.67), *maa://45066 (71.43), **maa://30867 (40.0), maa://61380 (100.0)</t>
+          <t>maa://30670 (96.77), maa://31470 (96.67), *maa://45066 (71.43), **maa://30867 (40.0), maa://61380 (100.0)</t>
         </is>
       </c>
       <c r="E143" s="14" t="inlineStr">
@@ -15015,7 +15015,7 @@
       </c>
       <c r="D149" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.25), maa://36641 (98.45), maa://36865 (95.81), maa://44635 (88.07), maa://44660 (92.5), maa://41128 (84.21), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
+          <t>maa://40957 (94.27), maa://36641 (98.45), maa://36865 (95.81), maa://44635 (88.07), maa://44660 (92.5), maa://41128 (84.21), maa://42918 (100.0), maa://44119 (97.44), maa://46108 (100.0), maa://37300 (100.0), maa://42917 (100.0)</t>
         </is>
       </c>
       <c r="E149" s="14" t="inlineStr">
@@ -15987,7 +15987,7 @@
       </c>
       <c r="D167" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (92.0), maa://29627 (92.76), maa://29659 (86.11), maa://49074 (96.08), **maa://30679 (50.0), maa://29861 (100.0), maa://42343 (100.0)</t>
+          <t>maa://29633 (92.0), maa://29627 (92.79), maa://29659 (86.11), maa://49074 (96.15), **maa://30679 (50.0), maa://29861 (100.0), maa://42343 (100.0)</t>
         </is>
       </c>
       <c r="E167" s="14" t="inlineStr">
@@ -17715,7 +17715,7 @@
       </c>
       <c r="D199" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (84.88), *maa://28190 (62.86), maa://22894 (91.43), *maa://20906 (72.22), **maa://20907 (35.48)</t>
+          <t>maa://27823 (85.06), *maa://28190 (62.86), maa://22894 (91.43), *maa://20906 (72.22), **maa://20907 (35.48)</t>
         </is>
       </c>
       <c r="E199" s="14" t="inlineStr">
@@ -17769,7 +17769,7 @@
       </c>
       <c r="D200" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (84.88), *maa://28190 (62.86), maa://22894 (91.43), *maa://20906 (72.22), **maa://20907 (35.48)</t>
+          <t>maa://27823 (85.06), *maa://28190 (62.86), maa://22894 (91.43), *maa://20906 (72.22), **maa://20907 (35.48)</t>
         </is>
       </c>
       <c r="E200" s="14" t="inlineStr">
@@ -17823,7 +17823,7 @@
       </c>
       <c r="D201" s="13" t="inlineStr">
         <is>
-          <t>maa://42223 (99.61), maa://49077 (93.18), maa://42292 (97.22), maa://42402 (100.0)</t>
+          <t>maa://42223 (99.61), maa://49077 (93.33), maa://42292 (97.22), maa://42402 (100.0)</t>
         </is>
       </c>
       <c r="E201" s="14" t="inlineStr">
@@ -18309,7 +18309,7 @@
       </c>
       <c r="D210" s="13" t="inlineStr">
         <is>
-          <t>maa://28133 (93.1), **maa://39217 (41.18), maa://25369 (94.87)</t>
+          <t>maa://28133 (93.1), **maa://39217 (41.18), maa://25369 (95.0)</t>
         </is>
       </c>
       <c r="E210" s="14" t="inlineStr">
@@ -19821,7 +19821,7 @@
       </c>
       <c r="D238" s="13" t="inlineStr">
         <is>
-          <t>maa://20922 (94.2), *maa://32623 (76.19), maa://34242 (85.71)</t>
+          <t>maa://20922 (94.29), *maa://32623 (76.19), maa://34242 (85.71)</t>
         </is>
       </c>
       <c r="E238" s="14" t="inlineStr">
@@ -20577,7 +20577,7 @@
       </c>
       <c r="D252" s="13" t="inlineStr">
         <is>
-          <t>maa://20923 (92.86), *maa://60577 (66.67)</t>
+          <t>maa://20923 (92.86), *maa://60577 (75.0)</t>
         </is>
       </c>
       <c r="E252" s="14" t="inlineStr">
@@ -20631,7 +20631,7 @@
       </c>
       <c r="D253" s="13" t="inlineStr">
         <is>
-          <t>maa://24093 (100.0), maa://31559 (94.74), maa://20924 (95.24), **maa://49440 (50.0)</t>
+          <t>maa://24093 (100.0), maa://31559 (94.87), maa://20924 (95.24), **maa://49440 (42.86)</t>
         </is>
       </c>
       <c r="E253" s="14" t="inlineStr">
@@ -22521,7 +22521,7 @@
       </c>
       <c r="D288" s="13" t="inlineStr">
         <is>
-          <t>maa://20899 (89.77), maa://46332 (96.0), ***maa://44744 (25.0)</t>
+          <t>maa://20899 (89.77), maa://46332 (96.15), ***maa://44744 (25.0)</t>
         </is>
       </c>
       <c r="E288" s="14" t="inlineStr">
@@ -23439,7 +23439,7 @@
       </c>
       <c r="D305" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (97.56), maa://49642 (97.0), maa://49660 (90.32), *maa://50517 (80.0)</t>
+          <t>maa://50280 (97.63), maa://49642 (97.03), maa://49660 (90.91), *maa://50517 (80.0)</t>
         </is>
       </c>
       <c r="E305" s="14" t="inlineStr">
@@ -23979,7 +23979,7 @@
       </c>
       <c r="D315" s="13" t="inlineStr">
         <is>
-          <t>maa://25775 (92.13), *maa://25393 (75.0)</t>
+          <t>maa://25775 (92.22), *maa://25393 (75.0)</t>
         </is>
       </c>
       <c r="E315" s="14" t="inlineStr">
@@ -24141,7 +24141,7 @@
       </c>
       <c r="D318" s="13" t="inlineStr">
         <is>
-          <t>maa://62761 (83.33), **maa://62755 (44.44)</t>
+          <t>maa://62761 (85.71), **maa://62755 (44.44)</t>
         </is>
       </c>
       <c r="E318" s="14" t="inlineStr">
@@ -25329,7 +25329,7 @@
       </c>
       <c r="D340" s="22" t="inlineStr">
         <is>
-          <t>maa://38295 (95.05), maa://49332 (100.0)</t>
+          <t>maa://38295 (95.1), maa://49332 (100.0)</t>
         </is>
       </c>
       <c r="E340" s="22" t="inlineStr">
@@ -26085,7 +26085,7 @@
       </c>
       <c r="D354" s="22" t="inlineStr">
         <is>
-          <t>maa://36868 (99.72), maa://35996 (97.73), **maa://39217 (41.18), maa://47349 (95.65)</t>
+          <t>maa://36868 (99.72), maa://35996 (97.75), **maa://39217 (41.18), maa://47349 (95.74)</t>
         </is>
       </c>
       <c r="E354" s="22" t="inlineStr">
@@ -26139,7 +26139,7 @@
       </c>
       <c r="D355" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.56), maa://49695 (100.0), maa://49758 (98.51), *maa://59402 (60.0), *maa://52357 (73.33), **maa://63091 (50.0)</t>
+          <t>maa://49696 (99.57), maa://49695 (100.0), maa://49758 (98.51), *maa://59402 (60.0), *maa://52357 (73.33), **maa://63091 (50.0)</t>
         </is>
       </c>
       <c r="E355" s="22" t="inlineStr">
@@ -26625,7 +26625,7 @@
       </c>
       <c r="D364" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (94.25), maa://44635 (88.07), maa://48026 (93.86), maa://41035 (93.15), maa://44660 (92.5), maa://41128 (84.21), *maa://60251 (69.23)</t>
+          <t>maa://40957 (94.27), maa://44635 (88.07), maa://48026 (93.86), maa://41035 (93.15), maa://44660 (92.5), maa://41128 (84.21), *maa://60251 (69.23)</t>
         </is>
       </c>
       <c r="E364" s="22" t="inlineStr">
@@ -27057,7 +27057,7 @@
       </c>
       <c r="D372" s="22" t="inlineStr">
         <is>
-          <t>maa://41110 (98.4), maa://45605 (100.0)</t>
+          <t>maa://41110 (98.43), maa://45605 (88.89)</t>
         </is>
       </c>
       <c r="E372" s="22" t="inlineStr">
@@ -27489,7 +27489,7 @@
       </c>
       <c r="D380" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (82.71), maa://44745 (97.56), **maa://49516 (37.5), *maa://45952 (72.73), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
+          <t>maa://42970 (82.71), maa://44745 (97.59), **maa://49516 (37.5), *maa://45952 (72.73), ***maa://46851 (14.29), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E380" s="22" t="inlineStr">
@@ -28191,7 +28191,7 @@
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>maa://51880 (99.15), maa://56651 (100.0), maa://51878 (100.0)</t>
+          <t>maa://51880 (99.16), maa://56651 (100.0), maa://51878 (100.0)</t>
         </is>
       </c>
       <c r="E393" t="inlineStr">
@@ -28218,7 +28218,7 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>maa://51872 (96.37), maa://51876 (98.96), maa://51873 (100.0), maa://63228 (90.91), maa://62047 (93.75)</t>
+          <t>maa://51872 (96.38), maa://51876 (98.96), maa://51873 (100.0), maa://63228 (92.86), maa://62047 (93.75)</t>
         </is>
       </c>
       <c r="E394" t="inlineStr">
@@ -28245,7 +28245,7 @@
       </c>
       <c r="D395" t="inlineStr">
         <is>
-          <t>maa://59493 (96.77), maa://60449 (98.18)</t>
+          <t>maa://59493 (96.77), maa://60449 (98.21)</t>
         </is>
       </c>
       <c r="E395" t="inlineStr">
@@ -28299,7 +28299,7 @@
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>maa://62756 (94.17)</t>
+          <t>maa://62756 (94.39)</t>
         </is>
       </c>
       <c r="E397" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#217)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -1481,7 +1481,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.07.29 23:24:36</t>
+          <t>更新日期：2025.07.30 14:18:05</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1868,7 +1868,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>maa://25021 (84.62), maa://22733 (100.00), ***maa://22761 (17.31)</t>
+          <t>maa://25021 (82.69), maa://22733 (100.00), ***maa://22761 (17.31)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -5298,7 +5298,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (100.00), *maa://47069 (63.54), *maa://56336 (62.50), *maa://45789 (67.71)</t>
+          <t>maa://45718 (100.00), *maa://47069 (62.89), *maa://56336 (61.86), *maa://45789 (67.01)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -6593,7 +6593,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://25176 (100.00), *maa://56237 (54.84)</t>
+          <t>maa://25176 (100.00), *maa://56237 (61.29)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -7023,7 +7023,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.07.29 23:24:36</t>
+          <t>更新日期：2025.07.30 14:18:05</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8427,7 +8427,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (70.37), *maa://28758 (64.20), maa://29036 (100.00), *maa://42172 (51.85), maa://30285 (80.25)</t>
+          <t>*maa://20849 (70.37), *maa://28758 (64.20), maa://29036 (100.00), *maa://42172 (51.85), maa://30285 (83.95)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8697,7 +8697,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (94.32), maa://36866 (100.00), *maa://45572 (79.55), *maa://27794 (64.77), maa://62759 (86.36), *maa://20960 (79.55), **maa://20843 (50.00), ***maa://24483 (10.23), **maa://20862 (50.00), *maa://20893 (62.50)</t>
+          <t>maa://36644 (94.32), maa://36866 (100.00), *maa://45572 (79.55), *maa://27794 (64.77), maa://62759 (87.50), *maa://20960 (79.55), **maa://20843 (50.00), ***maa://24483 (10.23), **maa://20862 (50.00), *maa://20893 (62.50)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -13287,7 +13287,7 @@
       </c>
       <c r="D117" s="13" t="inlineStr">
         <is>
-          <t>maa://31560 (100.00), maa://20940 (82.09)</t>
+          <t>maa://31560 (100.00), maa://20940 (86.57)</t>
         </is>
       </c>
       <c r="E117" s="14" t="inlineStr">
@@ -16041,7 +16041,7 @@
       </c>
       <c r="D168" s="13" t="inlineStr">
         <is>
-          <t>maa://49867 (97.59), maa://49655 (100.00)</t>
+          <t>maa://49867 (96.43), maa://49655 (100.00)</t>
         </is>
       </c>
       <c r="E168" s="14" t="inlineStr">
@@ -17607,7 +17607,7 @@
       </c>
       <c r="D197" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (92.55), maa://35854 (82.98), maa://50388 (100.00), maa://25760 (85.11), ***maa://43911 (4.26), **maa://20872 (35.11), *maa://51066 (69.15), *maa://63024 (74.47)</t>
+          <t>maa://44224 (92.55), maa://35854 (82.98), maa://50388 (100.00), maa://25760 (85.11), ***maa://43911 (4.26), **maa://20872 (35.11), *maa://51066 (69.15), *maa://63024 (76.60)</t>
         </is>
       </c>
       <c r="E197" s="14" t="inlineStr">
@@ -19983,7 +19983,7 @@
       </c>
       <c r="D241" s="13" t="inlineStr">
         <is>
-          <t>maa://62759 (100.00), **maa://62764 (44.74)</t>
+          <t>maa://62759 (100.00), **maa://62764 (44.16)</t>
         </is>
       </c>
       <c r="E241" s="14" t="inlineStr">
@@ -28245,7 +28245,7 @@
       </c>
       <c r="D395" t="inlineStr">
         <is>
-          <t>maa://59493 (97.87), maa://60449 (100.00)</t>
+          <t>maa://60449 (100.00), maa://59493 (97.87)</t>
         </is>
       </c>
       <c r="E395" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#220)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -712,7 +712,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (100.00), maa://24702 (98.92), maa://36681 (81.72)</t>
+          <t>maa://25390 (100.00), maa://24702 (98.92), maa://36681 (82.80)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://39402 (100.00), *maa://34787 (71.91), maa://58660 (92.13)</t>
+          <t>maa://39402 (100.00), *maa://34787 (73.86), maa://58660 (94.32)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://21246 (97.78), maa://36684 (100.00)</t>
+          <t>maa://21246 (98.88), maa://36684 (100.00)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://25251 (100.00), maa://59087 (93.02)</t>
+          <t>maa://25251 (100.00), maa://59087 (94.19)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>*maa://22880 (72.62), maa://20276 (100.00), *maa://22749 (71.43)</t>
+          <t>*maa://22880 (71.43), maa://20276 (100.00), *maa://22749 (72.62)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://45854 (88.24), maa://24617 (100.00), *maa://60545 (67.06)</t>
+          <t>maa://45854 (87.06), maa://24617 (100.00), *maa://60545 (71.76)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://24390 (100.00), maa://52241 (84.44)</t>
+          <t>maa://24390 (100.00), maa://52241 (87.78)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (100.00), *maa://22499 (73.33), *maa://22746 (67.78)</t>
+          <t>maa://24632 (100.00), *maa://22499 (74.44), *maa://22746 (67.78)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (100.00), maa://50121 (98.86)</t>
+          <t>maa://49983 (100.00), maa://50121 (94.38)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://32509 (100.00), maa://27295 (89.89), maa://22754 (89.89), *maa://31008 (73.03)</t>
+          <t>maa://32509 (100.00), maa://27295 (91.01), maa://22754 (89.89), *maa://31008 (73.03)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>maa://30062 (100.00), maa://39394 (96.23), ***maa://26209 (9.43)</t>
+          <t>maa://30062 (100.00), maa://39394 (96.15), ***maa://26209 (9.62)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (100.00), maa://54105 (94.94), maa://22744 (81.01)</t>
+          <t>maa://21245 (100.00), maa://54105 (97.47), maa://22744 (81.01)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="P5" s="8" t="inlineStr">
         <is>
-          <t>maa://21919 (100.00), *maa://21281 (61.11)</t>
+          <t>maa://21919 (100.00), *maa://21281 (60.44)</t>
         </is>
       </c>
       <c r="Q5" s="19" t="n"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="AF6" s="8" t="inlineStr">
         <is>
-          <t>maa://33152 (100.00), ***maa://22770 (25.00)</t>
+          <t>maa://33152 (100.00), ***maa://22770 (24.53)</t>
         </is>
       </c>
       <c r="AG6" s="16" t="n"/>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (100.00), *maa://22758 (75.82)</t>
+          <t>maa://22399 (100.00), *maa://22758 (75.00)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.04 13:44:54</t>
+          <t>更新日期：2025.08.08 13:32:35</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (86.36), maa://23252 (94.32), maa://37496 (100.00)</t>
+          <t>maa://32931 (87.50), maa://23252 (94.32), maa://37496 (100.00)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>maa://22765 (100.00), *maa://21915 (66.27)</t>
+          <t>maa://22765 (100.00), *maa://21915 (67.47)</t>
         </is>
       </c>
       <c r="E9" s="19" t="n"/>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (100.00), *maa://39552 (72.09)</t>
+          <t>maa://22762 (100.00), *maa://39552 (74.42)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://26223 (100.00), maa://52237 (86.32)</t>
+          <t>maa://26223 (100.00), maa://52237 (81.05)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (100.00), maa://40166 (96.34)</t>
+          <t>maa://28711 (100.00), maa://40166 (97.56)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (100.00), **maa://22865 (48.81)</t>
+          <t>maa://26206 (100.00), **maa://22865 (47.06)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>***maa://25695 (28.00), ***maa://39951 (14.00), maa://45271 (100.00), ***maa://34206 (22.00), ***maa://39243 (14.00), ***maa://54000 (30.00)</t>
+          <t>***maa://25695 (27.45), ***maa://39951 (11.76), maa://45271 (100.00), ***maa://34206 (21.57), ***maa://39243 (13.73), **maa://54000 (45.10)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (100.00), maa://36669 (82.50), *maa://23264 (61.25)</t>
+          <t>maa://28977 (100.00), maa://36669 (83.95), *maa://23264 (60.49)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (100.00), maa://22755 (87.23), *maa://63521 (55.32)</t>
+          <t>maa://27395 (100.00), maa://22755 (87.23), **maa://63521 (50.00)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://22301 (100.00), maa://45828 (89.47), maa://22726 (82.11)</t>
+          <t>maa://22301 (100.00), maa://45828 (90.53), maa://22726 (82.11)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>maa://25021 (88.00), maa://22733 (100.00), ***maa://22761 (18.00)</t>
+          <t>maa://25021 (84.62), maa://22733 (100.00), ***maa://22761 (17.31)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (89.36), maa://22501 (100.00), maa://45521 (87.23)</t>
+          <t>maa://22747 (90.43), maa://22501 (100.00), maa://45521 (88.30)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (100.00), **maa://54294 (39.53)</t>
+          <t>maa://21867 (100.00), *maa://54294 (66.28)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (100.00), maa://64046 (83.95)</t>
+          <t>maa://63896 (98.84), maa://64046 (100.00)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://22753 (100.00), maa://37962 (95.45), *maa://21485 (78.41)</t>
+          <t>maa://22753 (100.00), maa://37962 (94.32), *maa://21485 (77.27)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (100.00), maa://36673 (93.41), maa://25001 (84.62)</t>
+          <t>maa://24999 (100.00), maa://36673 (94.51), maa://25001 (84.62)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>maa://21248 (100.00), **maa://22728 (49.28)</t>
+          <t>maa://21248 (100.00), *maa://22728 (50.72)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (100.00), *maa://22583 (77.53), *maa://48321 (57.30)</t>
+          <t>maa://22676 (100.00), *maa://22583 (78.65), *maa://48321 (59.55)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (96.77), maa://26245 (100.00), maa://21288 (98.92), maa://36682 (91.40)</t>
+          <t>maa://39841 (96.77), maa://26245 (100.00), maa://21288 (98.92), maa://36682 (92.47)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (94.81), maa://22734 (100.00), *maa://30808 (68.83), maa://36048 (84.42), maa://45058 (83.12)</t>
+          <t>maa://22743 (94.81), maa://22734 (100.00), *maa://30808 (67.53), maa://36048 (84.42), maa://45058 (83.12)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="P15" s="8" t="inlineStr">
         <is>
-          <t>maa://24762 (100.00), **maa://22727 (46.51)</t>
+          <t>maa://24762 (100.00), **maa://22727 (45.98)</t>
         </is>
       </c>
       <c r="Q15" s="19" t="n"/>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://21364 (100.00), maa://36666 (97.44), *maa://22766 (76.92)</t>
+          <t>maa://21364 (100.00), maa://36666 (97.44), *maa://22766 (78.21)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>*maa://23911 (70.45), maa://27755 (100.00)</t>
+          <t>*maa://23911 (71.59), maa://27755 (100.00)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://22430 (100.00), maa://39599 (94.12)</t>
+          <t>maa://22430 (100.00), maa://39599 (95.29)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://22466 (100.00), maa://52226 (97.73)</t>
+          <t>maa://22466 (100.00), maa://52226 (98.86)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), *maa://54153 (76.60), *maa://24380 (69.15)</t>
+          <t>maa://24379 (100.00), maa://54153 (80.85), *maa://24380 (69.15)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (100.00), *maa://22741 (57.61)</t>
+          <t>maa://21917 (100.00), *maa://22741 (61.54)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://24313 (92.98), *maa://29784 (57.89), maa://47854 (100.00)</t>
+          <t>maa://24313 (92.98), maa://47854 (100.00), *maa://29784 (57.89)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (100.00), *maa://36668 (73.85)</t>
+          <t>maa://30709 (100.00), *maa://36668 (74.24)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://21432 (97.75), maa://25198 (100.00), maa://36680 (86.52)</t>
+          <t>maa://21432 (97.75), maa://25198 (100.00), maa://36680 (87.64)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (100.00), maa://49976 (94.12), *maa://56241 (76.47)</t>
+          <t>maa://50085 (100.00), maa://49976 (94.12), *maa://56241 (78.82)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3299,12 +3299,12 @@
       </c>
       <c r="AE21" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22524 (100.00), maa://22432 (97.50)</t>
+          <t>maa://22524 (100.00), maa://22432 (98.75), *maa://64221 (55.00)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>maa://27127 (100.00), maa://22751 (85.71)</t>
+          <t>maa://27127 (100.00), maa://22751 (88.24)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://21282 (100.00), *maa://37649 (59.79)</t>
+          <t>maa://21282 (100.00), *maa://37649 (61.86)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>*maa://28036 (64.52), maa://41753 (100.00)</t>
+          <t>*maa://28036 (66.67), maa://41753 (100.00)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (100.00), *maa://46650 (61.84)</t>
+          <t>maa://24368 (100.00), *maa://46650 (68.42)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (89.01), maa://23504 (100.00), *maa://25141 (76.92), *maa://36663 (75.82), maa://52227 (91.21)</t>
+          <t>maa://29988 (89.01), maa://23504 (100.00), *maa://25141 (76.92), *maa://36663 (75.82), maa://52227 (92.31)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3689,12 +3689,12 @@
       </c>
       <c r="AE24" s="19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://22523 (87.21), *maa://36672 (69.77), maa://29910 (100.00), maa://45831 (83.72)</t>
+          <t>maa://22523 (87.21), *maa://36672 (69.77), maa://29910 (100.00), maa://45831 (84.88), *maa://64165 (59.30)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (100.00), **maa://63016 (47.31)</t>
+          <t>maa://29753 (100.00), *maa://63016 (61.29)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>maa://29063 (95.45), maa://25311 (100.00), ***maa://22725 (3.03), *maa://45047 (72.73)</t>
+          <t>maa://29063 (95.45), maa://25311 (100.00), ***maa://22725 (3.03), maa://45047 (80.30)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://41802 (100.00), *maa://56374 (63.75)</t>
+          <t>maa://41802 (100.00), *maa://56374 (71.25)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>*maa://39601 (73.56), maa://34494 (100.00)</t>
+          <t>*maa://39601 (75.00), maa://34494 (100.00)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (100.00), maa://41749 (96.67)</t>
+          <t>maa://39929 (100.00), maa://41749 (97.78)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4357,12 +4357,12 @@
       </c>
       <c r="C30" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (100.00)</t>
+          <t>maa://45792 (100.00), ***maa://64191 (27.27)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4697,10 +4697,14 @@
       </c>
       <c r="W32" s="19" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="X32" s="8" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="X32" s="8" t="inlineStr">
+        <is>
+          <t>maa://64104 (100.00)</t>
+        </is>
+      </c>
       <c r="Y32" s="19" t="n"/>
       <c r="Z32" s="19" t="inlineStr">
         <is>
@@ -4796,7 +4800,7 @@
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (100.00), *maa://22730 (74.67)</t>
+          <t>maa://21956 (100.00), *maa://22730 (73.68)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4926,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (100.00), *maa://56235 (56.04)</t>
+          <t>maa://48817 (100.00), *maa://56235 (55.43)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -4969,12 +4973,12 @@
       </c>
       <c r="AA34" s="19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AB34" s="8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>maa://64329 (100.00)</t>
         </is>
       </c>
       <c r="AC34" s="19" t="n"/>
@@ -5229,10 +5233,14 @@
       </c>
       <c r="AA36" s="19" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AB36" s="19" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AB36" s="19" t="inlineStr">
+        <is>
+          <t>maa://64106 (100.00)</t>
+        </is>
+      </c>
       <c r="AC36" s="19" t="n"/>
       <c r="AD36" s="19" t="inlineStr">
         <is>
@@ -5495,7 +5503,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://36670 (91.01), maa://25199 (87.64), maa://30434 (100.00), *maa://45059 (69.66), **maa://44165 (33.71)</t>
+          <t>maa://36670 (91.11), maa://25199 (86.67), maa://30434 (100.00), *maa://45059 (68.89), **maa://44165 (42.22)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5527,7 +5535,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://24709 (97.75), maa://47093 (100.00)</t>
+          <t>maa://24709 (96.67), maa://47093 (100.00)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5538,12 +5546,12 @@
       </c>
       <c r="S39" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (100.00), *maa://45790 (71.76)</t>
+          <t>maa://47079 (100.00), *maa://45788 (71.43), *maa://45790 (76.19)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5628,7 +5636,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (100.00), maa://21386 (98.92), maa://36664 (84.95), *maa://45550 (56.99)</t>
+          <t>maa://23278 (100.00), maa://21386 (100.00), maa://36664 (85.87), **maa://45550 (48.91)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5671,10 +5679,14 @@
       </c>
       <c r="AE40" s="19" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AF40" s="19" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF40" s="19" t="inlineStr">
+        <is>
+          <t>maa://64205 (100.00)</t>
+        </is>
+      </c>
       <c r="AG40" s="16" t="n"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -5895,7 +5907,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>maa://22525 (93.59), maa://21284 (100.00)</t>
+          <t>maa://22525 (91.14), maa://21284 (100.00)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -5943,7 +5955,7 @@
       </c>
       <c r="T43" s="8" t="inlineStr">
         <is>
-          <t>maa://43198 (100.00), *maa://46286 (52.38)</t>
+          <t>maa://43198 (100.00), *maa://46286 (51.76)</t>
         </is>
       </c>
       <c r="U43" s="19" t="n"/>
@@ -5980,7 +5992,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (100.00), maa://27728 (95.79), *maa://56386 (68.42)</t>
+          <t>maa://29768 (100.00), maa://27728 (95.79), *maa://56386 (71.58)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6065,7 +6077,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://21229 (91.86), maa://30807 (100.00), maa://42459 (88.37)</t>
+          <t>maa://21229 (90.80), maa://30807 (100.00), maa://42459 (88.51)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6478,7 +6490,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (100.00), maa://59378 (91.30)</t>
+          <t>maa://59394 (100.00), maa://59378 (92.39)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6738,7 +6750,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (100.00), maa://43903 (89.89), **maa://56228 (49.44)</t>
+          <t>maa://42981 (100.00), maa://43903 (89.89), *maa://56228 (57.30)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6756,7 +6768,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (100.00), **maa://59413 (46.81)</t>
+          <t>maa://59534 (100.00), *maa://59413 (53.68)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7078,7 +7090,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.04 13:44:54</t>
+          <t>更新日期：2025.08.08 13:32:35</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -7888,7 +7900,7 @@
       </c>
       <c r="D16" s="13" t="inlineStr">
         <is>
-          <t>maa://20919 (100.00), **maa://31611 (46.74)</t>
+          <t>maa://20919 (100.00), *maa://31611 (51.09)</t>
         </is>
       </c>
       <c r="E16" s="14" t="inlineStr">
@@ -8266,7 +8278,7 @@
       </c>
       <c r="D23" s="13" t="inlineStr">
         <is>
-          <t>maa://20876 (100.00), ***maa://63498 (24.42)</t>
+          <t>maa://20876 (100.00), **maa://63498 (39.53)</t>
         </is>
       </c>
       <c r="E23" s="14" t="inlineStr">
@@ -8752,7 +8764,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (94.32), maa://36866 (100.00), *maa://45572 (79.55), *maa://27794 (64.77), maa://62759 (88.64), *maa://20960 (79.55), **maa://20843 (50.00), ***maa://24483 (10.23), **maa://20862 (50.00), *maa://20893 (62.50)</t>
+          <t>maa://36644 (93.26), maa://36866 (100.00), *maa://45572 (78.65), maa://62759 (87.64), *maa://27794 (64.04), *maa://20960 (78.65), **maa://20843 (49.44), ***maa://24483 (10.11), **maa://20862 (49.44), *maa://20893 (61.80)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -9292,7 +9304,7 @@
       </c>
       <c r="D42" s="13" t="inlineStr">
         <is>
-          <t>maa://20918 (100.00), maa://34883 (90.00), maa://20824 (96.25)</t>
+          <t>maa://34883 (90.00), maa://20918 (100.00), maa://20824 (96.25)</t>
         </is>
       </c>
       <c r="E42" s="14" t="inlineStr">
@@ -9886,7 +9898,7 @@
       </c>
       <c r="D53" s="13" t="inlineStr">
         <is>
-          <t>maa://20953 (97.62), maa://31173 (100.00)</t>
+          <t>maa://20953 (98.81), maa://31173 (100.00)</t>
         </is>
       </c>
       <c r="E53" s="14" t="inlineStr">
@@ -10318,7 +10330,7 @@
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (100.00), maa://24093 (100.00), maa://31559 (87.37), maa://20924 (81.05), **maa://25777 (35.79), *maa://20631 (60.00), **maa://28241 (46.32)</t>
+          <t>maa://20841 (100.00), maa://24093 (100.00), maa://31559 (87.37), maa://20924 (81.05), *maa://25777 (53.68), *maa://20631 (60.00), **maa://28241 (46.32)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -15070,7 +15082,7 @@
       </c>
       <c r="D149" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.85), maa://36641 (100.00), maa://36865 (94.85), maa://44635 (83.51), maa://44660 (82.47), *maa://41128 (72.16), maa://42918 (92.78), maa://44119 (89.69), maa://46108 (87.63), *maa://37300 (58.76), **maa://42917 (35.05)</t>
+          <t>maa://40957 (94.85), maa://36641 (100.00), maa://36865 (94.85), maa://44635 (83.51), maa://44660 (82.47), *maa://41128 (72.16), maa://42918 (92.78), maa://44119 (89.69), maa://46108 (88.66), *maa://37300 (58.76), **maa://42917 (35.05)</t>
         </is>
       </c>
       <c r="E149" s="14" t="inlineStr">
@@ -16042,7 +16054,7 @@
       </c>
       <c r="D167" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (100.00), maa://29627 (100.00), *maa://29659 (79.78), maa://49074 (97.75), **maa://30679 (34.83), maa://29861 (87.64), *maa://42343 (78.65)</t>
+          <t>maa://29633 (100.00), maa://29627 (100.00), *maa://29659 (79.78), maa://49074 (98.88), **maa://30679 (34.83), maa://29861 (87.64), *maa://42343 (78.65)</t>
         </is>
       </c>
       <c r="E167" s="14" t="inlineStr">
@@ -16415,12 +16427,12 @@
       </c>
       <c r="C174" s="12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D174" s="13" t="inlineStr">
         <is>
-          <t>maa://59681 (100.00)</t>
+          <t>maa://59681 (100.00), **maa://64200 (36.17)</t>
         </is>
       </c>
       <c r="E174" s="14" t="inlineStr">
@@ -16474,7 +16486,7 @@
       </c>
       <c r="D175" s="13" t="inlineStr">
         <is>
-          <t>maa://32418 (100.00), maa://51440 (89.90), *maa://63320 (65.66)</t>
+          <t>maa://32418 (100.00), maa://51440 (89.90), *maa://63320 (68.69)</t>
         </is>
       </c>
       <c r="E175" s="14" t="inlineStr">
@@ -17662,7 +17674,7 @@
       </c>
       <c r="D197" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (92.55), maa://35854 (81.91), maa://50388 (100.00), maa://25760 (85.11), ***maa://43911 (4.26), **maa://20872 (35.11), *maa://51066 (69.15), *maa://63024 (78.72)</t>
+          <t>maa://44224 (92.55), maa://35854 (81.91), maa://50388 (100.00), maa://25760 (85.11), ***maa://43911 (4.26), **maa://20872 (35.11), *maa://51066 (69.15), maa://63024 (80.85)</t>
         </is>
       </c>
       <c r="E197" s="14" t="inlineStr">
@@ -23548,7 +23560,7 @@
       </c>
       <c r="D306" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (100.00), maa://49642 (96.84), maa://49660 (81.05), **maa://50517 (40.00)</t>
+          <t>maa://50280 (100.00), maa://49642 (96.84), maa://49660 (82.11), **maa://50517 (40.00)</t>
         </is>
       </c>
       <c r="E306" s="14" t="inlineStr">
@@ -24574,7 +24586,7 @@
       </c>
       <c r="D325" s="13" t="inlineStr">
         <is>
-          <t>maa://39692 (100.00), *maa://39810 (68.69)</t>
+          <t>maa://39692 (100.00), *maa://39810 (69.70)</t>
         </is>
       </c>
       <c r="E325" s="14" t="inlineStr">
@@ -26950,7 +26962,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://63883 (100.00), *maa://64045 (61.76), *maa://64041 (61.76)</t>
+          <t>maa://63883 (100.00), **maa://64045 (47.73), **maa://64041 (47.73)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -28354,7 +28366,7 @@
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>maa://51898 (100.00), *maa://57241 (71.76)</t>
+          <t>maa://51898 (100.00), *maa://57241 (76.47)</t>
         </is>
       </c>
       <c r="E397" t="inlineStr">
@@ -28408,7 +28420,7 @@
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>maa://51872 (100.00), maa://51876 (100.00), *maa://63228 (76.60), maa://51873 (97.87), *maa://62047 (70.21)</t>
+          <t>maa://51872 (100.00), maa://51876 (100.00), *maa://63228 (75.53), maa://51873 (97.87), *maa://62047 (73.40)</t>
         </is>
       </c>
       <c r="E399" t="inlineStr">
@@ -28462,7 +28474,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>maa://60449 (100.00), maa://59493 (97.87)</t>
+          <t>maa://60449 (100.00), maa://59493 (96.84)</t>
         </is>
       </c>
       <c r="E401" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#221)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -842,7 +842,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (100.00), maa://36987 (94.57), *maa://39849 (60.87)</t>
+          <t>maa://40192 (100.00), maa://36987 (96.70), *maa://39849 (61.54)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>*maa://22880 (71.43), maa://20276 (100.00), *maa://22749 (72.62)</t>
+          <t>*maa://22880 (72.62), maa://20276 (100.00), *maa://22749 (72.62)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://45854 (87.06), maa://24617 (100.00), *maa://60545 (71.76)</t>
+          <t>maa://45854 (85.88), maa://24617 (100.00), *maa://60545 (71.76)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (86.02), maa://27484 (100.00), *maa://27480 (77.42)</t>
+          <t>maa://27396 (86.02), maa://27484 (100.00), *maa://27480 (78.49)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (100.00), maa://54105 (97.47), maa://22744 (81.01)</t>
+          <t>maa://21245 (100.00), maa://54105 (100.00), maa://22744 (81.01)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="AB5" s="8" t="inlineStr">
         <is>
-          <t>maa://29863 (100.00), ***maa://22752 (6.25), **maa://26013 (35.42)</t>
+          <t>maa://29863 (100.00), ***maa://22752 (6.12), **maa://26013 (34.69)</t>
         </is>
       </c>
       <c r="AC5" s="19" t="n"/>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (100.00), maa://24957 (94.51)</t>
+          <t>maa://28624 (100.00), maa://24957 (95.60)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.08 13:32:35</t>
+          <t>更新日期：2025.08.10 13:33:24</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1664,7 +1664,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (100.00), *maa://39552 (74.42)</t>
+          <t>maa://22762 (100.00), *maa://39552 (75.58)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://26223 (100.00), maa://52237 (81.05)</t>
+          <t>maa://26223 (100.00), maa://52237 (82.11)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (100.00), **maa://22865 (47.06)</t>
+          <t>maa://26206 (100.00), **maa://22865 (45.88)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>***maa://25695 (27.45), ***maa://39951 (11.76), maa://45271 (100.00), ***maa://34206 (21.57), ***maa://39243 (13.73), **maa://54000 (45.10)</t>
+          <t>***maa://25695 (26.92), ***maa://39951 (11.54), maa://45271 (100.00), ***maa://34206 (21.15), ***maa://39243 (13.46), **maa://54000 (44.23)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1821,12 +1821,12 @@
       </c>
       <c r="S10" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (100.00), maa://22755 (87.23), **maa://63521 (50.00)</t>
+          <t>maa://27395 (100.00), maa://22755 (87.23)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://22301 (100.00), maa://45828 (90.53), maa://22726 (82.11)</t>
+          <t>maa://22301 (100.00), maa://45828 (91.58), maa://22726 (82.11)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (100.00), *maa://54294 (66.28)</t>
+          <t>maa://21867 (100.00), *maa://54294 (75.58)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (98.84), maa://64046 (100.00)</t>
+          <t>maa://63896 (94.38), maa://64046 (100.00)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://23669 (100.00), maa://36677 (96.77), maa://39872 (86.02)</t>
+          <t>maa://23669 (100.00), maa://36677 (96.77), maa://39872 (87.10)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (100.00), *maa://22583 (78.65), *maa://48321 (59.55)</t>
+          <t>maa://22676 (100.00), *maa://22583 (77.78), *maa://48321 (58.89)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (94.81), maa://22734 (100.00), *maa://30808 (67.53), maa://36048 (84.42), maa://45058 (83.12)</t>
+          <t>maa://22743 (96.10), maa://22734 (100.00), *maa://30808 (67.53), maa://36048 (84.42), maa://45058 (84.42)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>*maa://23911 (71.59), maa://27755 (100.00)</t>
+          <t>*maa://23911 (70.45), maa://27755 (100.00)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -3039,12 +3039,12 @@
       </c>
       <c r="AE19" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF19" s="8" t="inlineStr">
         <is>
-          <t>maa://52239 (83.02)</t>
+          <t>maa://21663 (100.00), *maa://52239 (56.60)</t>
         </is>
       </c>
       <c r="AG19" s="16" t="n"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://21432 (97.75), maa://25198 (100.00), maa://36680 (87.64)</t>
+          <t>maa://21432 (98.86), maa://25198 (100.00), maa://36680 (88.64)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (100.00), maa://49976 (94.12), *maa://56241 (78.82)</t>
+          <t>maa://50085 (100.00), maa://49976 (94.12), *maa://56241 (70.59)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://20110 (90.59), maa://34946 (100.00)</t>
+          <t>maa://34946 (100.00), maa://20110 (90.59)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22524 (100.00), maa://22432 (98.75), *maa://64221 (55.00)</t>
+          <t>maa://22524 (100.00), maa://22432 (97.50), **maa://64221 (37.50)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (100.00), *maa://46650 (68.42)</t>
+          <t>maa://24368 (100.00), *maa://46650 (69.74)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>maa://29063 (95.45), maa://25311 (100.00), ***maa://22725 (3.03), maa://45047 (80.30)</t>
+          <t>maa://29063 (96.92), maa://25311 (100.00), ***maa://22725 (3.08), maa://45047 (81.54)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="AF26" s="8" t="inlineStr">
         <is>
-          <t>maa://30511 (100.00), **maa://29760 (46.77)</t>
+          <t>maa://30511 (100.00), **maa://29760 (47.54)</t>
         </is>
       </c>
       <c r="AG26" s="16" t="n"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (100.00), maa://36258 (91.21), *maa://43904 (52.75)</t>
+          <t>maa://35926 (100.00), maa://36258 (92.22), *maa://43904 (53.33)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="P37" s="8" t="inlineStr">
         <is>
-          <t>maa://21280 (100.00), *maa://21239 (52.94)</t>
+          <t>maa://21280 (100.00), *maa://21239 (52.33)</t>
         </is>
       </c>
       <c r="Q37" s="19" t="n"/>
@@ -5546,12 +5546,12 @@
       </c>
       <c r="S39" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (100.00), *maa://45788 (71.43), *maa://45790 (76.19)</t>
+          <t>maa://47079 (100.00), *maa://45790 (76.19)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5636,7 +5636,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (100.00), maa://21386 (100.00), maa://36664 (85.87), **maa://45550 (48.91)</t>
+          <t>maa://23278 (100.00), maa://21386 (100.00), maa://36664 (83.70), **maa://45550 (48.91)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>maa://22525 (91.14), maa://21284 (100.00)</t>
+          <t>maa://22525 (90.00), maa://21284 (100.00)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -6490,7 +6490,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (100.00), maa://59378 (92.39)</t>
+          <t>maa://59394 (100.00), maa://59378 (92.47)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -7090,7 +7090,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.08 13:32:35</t>
+          <t>更新日期：2025.08.10 13:33:24</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8494,7 +8494,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (70.37), *maa://28758 (65.43), maa://29036 (100.00), *maa://42172 (54.32), maa://30285 (83.95)</t>
+          <t>*maa://20849 (69.51), *maa://28758 (64.63), maa://29036 (100.00), *maa://42172 (53.66), maa://30285 (82.93)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8764,7 +8764,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (93.26), maa://36866 (100.00), *maa://45572 (78.65), maa://62759 (87.64), *maa://27794 (64.04), *maa://20960 (78.65), **maa://20843 (49.44), ***maa://24483 (10.11), **maa://20862 (49.44), *maa://20893 (61.80)</t>
+          <t>maa://36644 (93.26), maa://36866 (100.00), *maa://45572 (71.91), maa://62759 (89.89), *maa://27794 (64.04), *maa://20960 (78.65), **maa://20843 (49.44), ***maa://24483 (10.11), **maa://20862 (49.44), *maa://20893 (61.80)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -10330,7 +10330,7 @@
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (100.00), maa://24093 (100.00), maa://31559 (87.37), maa://20924 (81.05), *maa://25777 (53.68), *maa://20631 (60.00), **maa://28241 (46.32)</t>
+          <t>maa://20841 (100.00), maa://24093 (100.00), maa://31559 (88.42), maa://20924 (81.05), *maa://25777 (53.68), *maa://20631 (60.00), **maa://28241 (46.32)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -10870,7 +10870,7 @@
       </c>
       <c r="D71" s="13" t="inlineStr">
         <is>
-          <t>maa://20943 (100.00), *maa://30673 (73.47), *maa://30672 (66.33), maa://20856 (82.65), ***maa://63790 (21.43)</t>
+          <t>maa://20943 (100.00), *maa://30673 (73.47), *maa://30672 (66.33), maa://20856 (82.65), **maa://63790 (44.90)</t>
         </is>
       </c>
       <c r="E71" s="14" t="inlineStr">
@@ -11518,7 +11518,7 @@
       </c>
       <c r="D83" s="13" t="inlineStr">
         <is>
-          <t>maa://45572 (100.00), maa://27794 (81.43), maa://20960 (100.00)</t>
+          <t>maa://45572 (91.43), maa://27794 (81.43), maa://20960 (100.00)</t>
         </is>
       </c>
       <c r="E83" s="14" t="inlineStr">
@@ -12490,7 +12490,7 @@
       </c>
       <c r="D101" s="13" t="inlineStr">
         <is>
-          <t>maa://45572 (100.00), maa://27794 (81.43), *maa://20893 (78.57)</t>
+          <t>maa://45572 (100.00), maa://27794 (89.06), maa://20893 (85.94)</t>
         </is>
       </c>
       <c r="E101" s="14" t="inlineStr">
@@ -12760,7 +12760,7 @@
       </c>
       <c r="D106" s="13" t="inlineStr">
         <is>
-          <t>maa://45572 (100.00), maa://27794 (81.43), *maa://20843 (62.86), ***maa://24483 (12.86)</t>
+          <t>maa://45572 (100.00), maa://27794 (89.06), *maa://20843 (68.75), ***maa://24483 (14.06)</t>
         </is>
       </c>
       <c r="E106" s="14" t="inlineStr">
@@ -12868,7 +12868,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://25018 (96.94), maa://25776 (85.71), maa://28361 (85.71), maa://25772 (85.71), *maa://56588 (78.57), *maa://45194 (62.24), *maa://25161 (62.24), *maa://32653 (63.27), ***maa://60902 (7.14), **maa://61839 (34.69), **maa://61275 (34.69)</t>
+          <t>maa://51881 (100.00), maa://25018 (96.94), maa://25776 (85.71), maa://28361 (85.71), maa://25772 (85.71), *maa://56588 (79.59), *maa://45194 (63.27), *maa://25161 (62.24), *maa://32653 (63.27), ***maa://60902 (7.14), **maa://61839 (44.90), **maa://61275 (34.69)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -14704,7 +14704,7 @@
       </c>
       <c r="D142" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (100.00), **maa://23736 (36.56), *maa://31185 (52.69), *maa://30306 (54.84)</t>
+          <t>maa://28484 (100.00), **maa://23736 (35.48), *maa://31185 (56.99), *maa://30306 (54.84)</t>
         </is>
       </c>
       <c r="E142" s="14" t="inlineStr">
@@ -15077,12 +15077,12 @@
       </c>
       <c r="C149" s="12" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="D149" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.85), maa://36641 (100.00), maa://36865 (94.85), maa://44635 (83.51), maa://44660 (82.47), *maa://41128 (72.16), maa://42918 (92.78), maa://44119 (89.69), maa://46108 (88.66), *maa://37300 (58.76), **maa://42917 (35.05)</t>
+          <t>maa://40957 (94.85), maa://36641 (100.00), maa://36865 (94.85), maa://44635 (83.51), maa://44660 (82.47), *maa://41128 (72.16), maa://42918 (92.78), maa://44119 (89.69), maa://46108 (88.66), *maa://37300 (58.76), **maa://42917 (35.05), **maa://64408 (45.36)</t>
         </is>
       </c>
       <c r="E149" s="14" t="inlineStr">
@@ -16486,7 +16486,7 @@
       </c>
       <c r="D175" s="13" t="inlineStr">
         <is>
-          <t>maa://32418 (100.00), maa://51440 (89.90), *maa://63320 (68.69)</t>
+          <t>maa://32418 (100.00), maa://51440 (89.90), *maa://63320 (74.75)</t>
         </is>
       </c>
       <c r="E175" s="14" t="inlineStr">
@@ -17674,7 +17674,7 @@
       </c>
       <c r="D197" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (92.55), maa://35854 (81.91), maa://50388 (100.00), maa://25760 (85.11), ***maa://43911 (4.26), **maa://20872 (35.11), *maa://51066 (69.15), maa://63024 (80.85)</t>
+          <t>maa://44224 (91.58), maa://35854 (82.11), maa://50388 (100.00), maa://25760 (84.21), ***maa://43911 (4.21), **maa://20872 (34.74), *maa://51066 (68.42), maa://63024 (81.05)</t>
         </is>
       </c>
       <c r="E197" s="14" t="inlineStr">
@@ -17890,7 +17890,7 @@
       </c>
       <c r="D201" s="13" t="inlineStr">
         <is>
-          <t>maa://42223 (100.00), maa://49077 (83.67), maa://42292 (87.76), *maa://42402 (69.39)</t>
+          <t>maa://42223 (100.00), maa://49077 (84.69), maa://42292 (87.76), *maa://42402 (69.39)</t>
         </is>
       </c>
       <c r="E201" s="14" t="inlineStr">
@@ -18376,7 +18376,7 @@
       </c>
       <c r="D210" s="13" t="inlineStr">
         <is>
-          <t>maa://28133 (100.00), ***maa://39217 (26.19), maa://25369 (100.00)</t>
+          <t>maa://28133 (100.00), ***maa://39217 (23.81), maa://25369 (100.00)</t>
         </is>
       </c>
       <c r="E210" s="14" t="inlineStr">
@@ -20045,12 +20045,12 @@
       </c>
       <c r="C241" s="12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D241" s="13" t="inlineStr">
         <is>
-          <t>maa://30667 (96.15), maa://30666 (100.00), **maa://30739 (35.90), *maa://30723 (56.41), maa://39588 (98.72)</t>
+          <t>maa://30667 (96.15), maa://30666 (100.00), **maa://30739 (35.90), *maa://30723 (56.41), maa://39588 (98.72), ***maa://64079 (26.92)</t>
         </is>
       </c>
       <c r="E241" s="14" t="inlineStr">
@@ -20104,7 +20104,7 @@
       </c>
       <c r="D242" s="13" t="inlineStr">
         <is>
-          <t>maa://62759 (100.00), **maa://62764 (43.59)</t>
+          <t>maa://62759 (100.00), **maa://62764 (42.50)</t>
         </is>
       </c>
       <c r="E242" s="14" t="inlineStr">
@@ -20752,7 +20752,7 @@
       </c>
       <c r="D254" s="13" t="inlineStr">
         <is>
-          <t>maa://24093 (100.00), maa://31559 (87.37), maa://20924 (81.05), ***maa://49440 (16.84)</t>
+          <t>maa://24093 (100.00), maa://31559 (88.42), maa://20924 (81.05), ***maa://49440 (16.84)</t>
         </is>
       </c>
       <c r="E254" s="14" t="inlineStr">
@@ -21886,7 +21886,7 @@
       </c>
       <c r="D275" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://51630 (92.86), *maa://56588 (78.57), **maa://55171 (37.76), *maa://51893 (57.14), ***maa://60902 (7.14)</t>
+          <t>maa://51881 (100.00), maa://51630 (92.86), *maa://56588 (79.59), **maa://55171 (37.76), *maa://51893 (57.14), ***maa://60902 (7.14)</t>
         </is>
       </c>
       <c r="E275" s="14" t="inlineStr">
@@ -22804,7 +22804,7 @@
       </c>
       <c r="D292" s="13" t="inlineStr">
         <is>
-          <t>maa://30710 (100.00), maa://36845 (96.81), maa://31558 (90.43), ***maa://39217 (23.40), *maa://30668 (74.47)</t>
+          <t>maa://30710 (100.00), maa://36845 (96.81), maa://31558 (90.43), ***maa://39217 (21.28), *maa://30668 (74.47)</t>
         </is>
       </c>
       <c r="E292" s="14" t="inlineStr">
@@ -22966,7 +22966,7 @@
       </c>
       <c r="D295" s="13" t="inlineStr">
         <is>
-          <t>maa://25774 (100.00), maa://28133 (93.33), maa://22469 (92.22), ***maa://39217 (24.44), ***maa://31349 (27.78)</t>
+          <t>maa://25774 (100.00), maa://28133 (93.33), maa://22469 (92.22), ***maa://39217 (22.22), ***maa://31349 (27.78)</t>
         </is>
       </c>
       <c r="E295" s="14" t="inlineStr">
@@ -25828,7 +25828,7 @@
       </c>
       <c r="D348" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (100.00), maa://32415 (95.88), maa://34677 (95.88), maa://32892 (87.63), *maa://32653 (63.92), **maa://61839 (35.05), **maa://61275 (35.05)</t>
+          <t>maa://32647 (100.00), maa://32415 (95.88), maa://34677 (95.88), maa://32892 (87.63), *maa://32653 (63.92), **maa://61839 (45.36), **maa://61275 (35.05)</t>
         </is>
       </c>
       <c r="E348" s="22" t="inlineStr">
@@ -26314,7 +26314,7 @@
       </c>
       <c r="D357" s="22" t="inlineStr">
         <is>
-          <t>maa://36868 (100.00), maa://35996 (93.88), ***maa://39217 (22.45), maa://47349 (88.78)</t>
+          <t>maa://36868 (100.00), maa://35996 (92.93), ***maa://39217 (20.20), maa://47349 (87.88)</t>
         </is>
       </c>
       <c r="E357" s="22" t="inlineStr">
@@ -26476,7 +26476,7 @@
       </c>
       <c r="D360" s="22" t="inlineStr">
         <is>
-          <t>maa://42299 (100.00), *maa://42224 (69.32)</t>
+          <t>maa://42299 (100.00), *maa://42224 (70.45)</t>
         </is>
       </c>
       <c r="E360" s="22" t="inlineStr">
@@ -26584,7 +26584,7 @@
       </c>
       <c r="D362" s="22" t="inlineStr">
         <is>
-          <t>maa://36646 (100.00), maa://36845 (92.86), ***maa://39217 (22.45), maa://51007 (92.86)</t>
+          <t>maa://36646 (100.00), maa://36845 (92.86), ***maa://39217 (20.41), maa://51007 (92.86)</t>
         </is>
       </c>
       <c r="E362" s="22" t="inlineStr">
@@ -26854,7 +26854,7 @@
       </c>
       <c r="D367" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (100.00), maa://44635 (88.04), maa://48026 (95.65), maa://41035 (92.39), maa://44660 (86.96), *maa://41128 (76.09), **maa://60251 (45.65)</t>
+          <t>maa://40957 (100.00), maa://44635 (88.04), maa://48026 (95.65), maa://41035 (92.39), maa://44660 (86.96), *maa://41128 (76.09), **maa://60251 (48.91)</t>
         </is>
       </c>
       <c r="E367" s="22" t="inlineStr">
@@ -26962,7 +26962,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://63883 (100.00), **maa://64045 (47.73), **maa://64041 (47.73)</t>
+          <t>maa://63883 (100.00), *maa://64045 (66.67), ***maa://64041 (17.65)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -28393,7 +28393,7 @@
       </c>
       <c r="D398" t="inlineStr">
         <is>
-          <t>maa://51880 (100.00), maa://56651 (93.88), maa://51878 (90.82)</t>
+          <t>maa://51880 (100.00), maa://56651 (93.88), maa://51878 (91.84)</t>
         </is>
       </c>
       <c r="E398" t="inlineStr">
@@ -28420,7 +28420,7 @@
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>maa://51872 (100.00), maa://51876 (100.00), *maa://63228 (75.53), maa://51873 (97.87), *maa://62047 (73.40)</t>
+          <t>maa://51872 (100.00), maa://51876 (100.00), *maa://63228 (71.28), maa://51873 (97.87), *maa://62047 (73.40)</t>
         </is>
       </c>
       <c r="E399" t="inlineStr">
@@ -28474,7 +28474,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>maa://60449 (100.00), maa://59493 (96.84)</t>
+          <t>maa://60449 (100.00), maa://59493 (95.83)</t>
         </is>
       </c>
       <c r="E401" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#222)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://39402 (100.00), *maa://34787 (73.86), maa://58660 (94.32)</t>
+          <t>maa://39402 (100.00), *maa://34787 (73.86), maa://58660 (95.45)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://25251 (100.00), maa://59087 (94.19)</t>
+          <t>maa://25251 (100.00), maa://59087 (95.35)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://24390 (100.00), maa://52241 (87.78)</t>
+          <t>maa://24390 (100.00), maa://52241 (88.89)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (100.00), maa://30381 (89.16)</t>
+          <t>maa://31836 (100.00), maa://30381 (88.10)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.10 13:33:24</t>
+          <t>更新日期：2025.08.11 13:31:21</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://26223 (100.00), maa://52237 (82.11)</t>
+          <t>maa://26223 (100.00), maa://52237 (83.16)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1821,12 +1821,12 @@
       </c>
       <c r="S10" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (100.00), maa://22755 (87.23)</t>
+          <t>maa://27395 (100.00), maa://22755 (87.23), **maa://63521 (47.87)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (94.38), maa://64046 (100.00)</t>
+          <t>maa://63896 (93.33), maa://64046 (100.00)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>maa://21248 (100.00), *maa://22728 (50.72)</t>
+          <t>maa://21248 (100.00), **maa://22728 (49.28)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), maa://54153 (80.85), *maa://24380 (69.15)</t>
+          <t>maa://24379 (100.00), maa://54153 (81.91), *maa://24380 (69.15)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://24313 (92.98), maa://47854 (100.00), *maa://29784 (57.89)</t>
+          <t>maa://24313 (96.36), maa://47854 (100.00), *maa://29784 (60.00)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (100.00), maa://49976 (94.12), *maa://56241 (70.59)</t>
+          <t>maa://50085 (100.00), maa://49976 (93.02), *maa://56241 (69.77)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22524 (100.00), maa://22432 (97.50), **maa://64221 (37.50)</t>
+          <t>maa://22524 (100.00), maa://22432 (97.50), ***maa://64221 (28.75)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://22523 (87.21), *maa://36672 (69.77), maa://29910 (100.00), maa://45831 (84.88), *maa://64165 (59.30)</t>
+          <t>maa://22523 (87.21), *maa://36672 (69.77), maa://29910 (100.00), maa://45831 (84.88), *maa://64165 (66.28)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://41802 (100.00), *maa://56374 (71.25)</t>
+          <t>maa://41802 (100.00), *maa://56374 (76.25)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="P26" s="8" t="inlineStr">
         <is>
-          <t>maa://39870 (100.00), maa://56625 (82.61)</t>
+          <t>maa://39870 (100.00), maa://56625 (88.41)</t>
         </is>
       </c>
       <c r="Q26" s="19" t="n"/>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://24709 (96.67), maa://47093 (100.00)</t>
+          <t>maa://24709 (100.00), maa://47093 (98.85)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5679,12 +5679,12 @@
       </c>
       <c r="AE40" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://64205 (100.00)</t>
+          <t>maa://64107 (84.31), maa://64205 (100.00)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -6660,7 +6660,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://25176 (100.00), *maa://56237 (69.89)</t>
+          <t>maa://25176 (100.00), *maa://56237 (73.12)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6768,7 +6768,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (100.00), *maa://59413 (53.68)</t>
+          <t>maa://59534 (100.00), *maa://59413 (60.00)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7090,7 +7090,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.10 13:33:24</t>
+          <t>更新日期：2025.08.11 13:31:21</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8494,7 +8494,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (69.51), *maa://28758 (64.63), maa://29036 (100.00), *maa://42172 (53.66), maa://30285 (82.93)</t>
+          <t>*maa://20849 (69.51), *maa://28758 (65.85), maa://29036 (100.00), *maa://42172 (57.32), maa://30285 (82.93)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8764,7 +8764,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (93.26), maa://36866 (100.00), *maa://45572 (71.91), maa://62759 (89.89), *maa://27794 (64.04), *maa://20960 (78.65), **maa://20843 (49.44), ***maa://24483 (10.11), **maa://20862 (49.44), *maa://20893 (61.80)</t>
+          <t>maa://36644 (93.26), maa://36866 (100.00), *maa://45572 (71.91), maa://62759 (91.01), *maa://27794 (64.04), *maa://20960 (78.65), **maa://20843 (49.44), ***maa://24483 (10.11), **maa://20862 (49.44), *maa://20893 (61.80)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -9034,7 +9034,7 @@
       </c>
       <c r="D37" s="13" t="inlineStr">
         <is>
-          <t>maa://27376 (96.51), maa://42635 (100.00), **maa://20838 (39.53)</t>
+          <t>maa://42635 (100.00), maa://27376 (98.81), **maa://20838 (40.48)</t>
         </is>
       </c>
       <c r="E37" s="14" t="inlineStr">
@@ -9898,7 +9898,7 @@
       </c>
       <c r="D53" s="13" t="inlineStr">
         <is>
-          <t>maa://20953 (98.81), maa://31173 (100.00)</t>
+          <t>maa://20953 (100.00), maa://31173 (100.00)</t>
         </is>
       </c>
       <c r="E53" s="14" t="inlineStr">
@@ -10006,7 +10006,7 @@
       </c>
       <c r="D55" s="13" t="inlineStr">
         <is>
-          <t>maa://20932 (100.00), maa://42415 (92.47), *maa://40838 (79.57)</t>
+          <t>maa://20932 (100.00), maa://42415 (93.55), *maa://40838 (79.57)</t>
         </is>
       </c>
       <c r="E55" s="14" t="inlineStr">
@@ -10330,7 +10330,7 @@
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (100.00), maa://24093 (100.00), maa://31559 (88.42), maa://20924 (81.05), *maa://25777 (53.68), *maa://20631 (60.00), **maa://28241 (46.32)</t>
+          <t>maa://20841 (100.00), maa://24093 (100.00), maa://31559 (88.42), maa://20924 (81.05), *maa://25777 (60.00), *maa://20631 (60.00), **maa://28241 (46.32)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -10546,7 +10546,7 @@
       </c>
       <c r="D65" s="13" t="inlineStr">
         <is>
-          <t>maa://28567 (95.74), **maa://20947 (30.85), maa://30525 (88.30), maa://38735 (100.00), **maa://28188 (42.55), **maa://30524 (36.17)</t>
+          <t>maa://28567 (96.81), **maa://20947 (31.91), maa://30525 (88.30), maa://38735 (100.00), **maa://28188 (42.55), **maa://30524 (36.17)</t>
         </is>
       </c>
       <c r="E65" s="14" t="inlineStr">
@@ -10870,7 +10870,7 @@
       </c>
       <c r="D71" s="13" t="inlineStr">
         <is>
-          <t>maa://20943 (100.00), *maa://30673 (73.47), *maa://30672 (66.33), maa://20856 (82.65), **maa://63790 (44.90)</t>
+          <t>maa://20943 (100.00), *maa://30673 (73.47), *maa://30672 (66.33), maa://20856 (82.65), *maa://63790 (58.16)</t>
         </is>
       </c>
       <c r="E71" s="14" t="inlineStr">
@@ -11788,7 +11788,7 @@
       </c>
       <c r="D88" s="13" t="inlineStr">
         <is>
-          <t>maa://24472 (100.00), **maa://35841 (48.81)</t>
+          <t>maa://24472 (100.00), **maa://35841 (48.24)</t>
         </is>
       </c>
       <c r="E88" s="14" t="inlineStr">
@@ -12868,7 +12868,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://25018 (96.94), maa://25776 (85.71), maa://28361 (85.71), maa://25772 (85.71), *maa://56588 (79.59), *maa://45194 (63.27), *maa://25161 (62.24), *maa://32653 (63.27), ***maa://60902 (7.14), **maa://61839 (44.90), **maa://61275 (34.69)</t>
+          <t>maa://51881 (100.00), maa://25018 (96.94), maa://25776 (85.71), maa://28361 (85.71), maa://25772 (85.71), *maa://56588 (79.59), *maa://45194 (63.27), *maa://25161 (62.24), *maa://32653 (63.27), ***maa://60902 (12.24), *maa://61839 (52.04), **maa://61275 (34.69)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13246,7 +13246,7 @@
       </c>
       <c r="D115" s="13" t="inlineStr">
         <is>
-          <t>maa://20908 (100.00), maa://35723 (90.62), **maa://23346 (46.88), maa://38822 (92.71), *maa://58659 (63.54)</t>
+          <t>maa://20908 (100.00), maa://35723 (90.62), **maa://23346 (46.88), maa://38822 (92.71), *maa://58659 (67.71)</t>
         </is>
       </c>
       <c r="E115" s="14" t="inlineStr">
@@ -15136,7 +15136,7 @@
       </c>
       <c r="D150" s="13" t="inlineStr">
         <is>
-          <t>maa://51549 (100.00), maa://51923 (91.95)</t>
+          <t>maa://51549 (100.00), maa://51923 (90.91)</t>
         </is>
       </c>
       <c r="E150" s="14" t="inlineStr">
@@ -16432,7 +16432,7 @@
       </c>
       <c r="D174" s="13" t="inlineStr">
         <is>
-          <t>maa://59681 (100.00), **maa://64200 (36.17)</t>
+          <t>maa://59681 (100.00), **maa://64200 (46.81)</t>
         </is>
       </c>
       <c r="E174" s="14" t="inlineStr">
@@ -16486,7 +16486,7 @@
       </c>
       <c r="D175" s="13" t="inlineStr">
         <is>
-          <t>maa://32418 (100.00), maa://51440 (89.90), *maa://63320 (74.75)</t>
+          <t>maa://32418 (100.00), maa://51440 (89.90), *maa://63320 (76.77)</t>
         </is>
       </c>
       <c r="E175" s="14" t="inlineStr">
@@ -16702,7 +16702,7 @@
       </c>
       <c r="D179" s="13" t="inlineStr">
         <is>
-          <t>maa://20911 (100.00), *maa://29012 (62.03)</t>
+          <t>maa://20911 (100.00), *maa://29012 (61.25)</t>
         </is>
       </c>
       <c r="E179" s="14" t="inlineStr">
@@ -17723,12 +17723,12 @@
       </c>
       <c r="C198" s="12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D198" s="13" t="inlineStr">
         <is>
-          <t>maa://39156 (100.00), **maa://39550 (39.08), **maa://53417 (41.38)</t>
+          <t>maa://39156 (100.00), **maa://39550 (39.08), **maa://53417 (41.38), ***maa://63806 (24.14)</t>
         </is>
       </c>
       <c r="E198" s="14" t="inlineStr">
@@ -20050,7 +20050,7 @@
       </c>
       <c r="D241" s="13" t="inlineStr">
         <is>
-          <t>maa://30667 (96.15), maa://30666 (100.00), **maa://30739 (35.90), *maa://30723 (56.41), maa://39588 (98.72), ***maa://64079 (26.92)</t>
+          <t>maa://30667 (96.15), maa://30666 (100.00), **maa://30739 (35.90), *maa://30723 (57.69), maa://39588 (98.72), *maa://64079 (57.69)</t>
         </is>
       </c>
       <c r="E241" s="14" t="inlineStr">
@@ -20104,7 +20104,7 @@
       </c>
       <c r="D242" s="13" t="inlineStr">
         <is>
-          <t>maa://62759 (100.00), **maa://62764 (42.50)</t>
+          <t>maa://62759 (100.00), **maa://62764 (41.98)</t>
         </is>
       </c>
       <c r="E242" s="14" t="inlineStr">
@@ -20590,7 +20590,7 @@
       </c>
       <c r="D251" s="13" t="inlineStr">
         <is>
-          <t>maa://42287 (93.18), maa://45570 (100.00), maa://42225 (86.36), ***maa://60678 (23.86)</t>
+          <t>maa://42287 (94.32), maa://45570 (100.00), maa://42225 (87.50), *maa://60678 (57.95)</t>
         </is>
       </c>
       <c r="E251" s="14" t="inlineStr">
@@ -21886,7 +21886,7 @@
       </c>
       <c r="D275" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://51630 (92.86), *maa://56588 (79.59), **maa://55171 (37.76), *maa://51893 (57.14), ***maa://60902 (7.14)</t>
+          <t>maa://51881 (100.00), maa://51630 (91.84), *maa://56588 (79.59), **maa://55171 (37.76), *maa://51893 (57.14), ***maa://60902 (12.24)</t>
         </is>
       </c>
       <c r="E275" s="14" t="inlineStr">
@@ -24586,7 +24586,7 @@
       </c>
       <c r="D325" s="13" t="inlineStr">
         <is>
-          <t>maa://39692 (100.00), *maa://39810 (69.70)</t>
+          <t>maa://39692 (100.00), *maa://39810 (70.71)</t>
         </is>
       </c>
       <c r="E325" s="14" t="inlineStr">
@@ -25828,7 +25828,7 @@
       </c>
       <c r="D348" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (100.00), maa://32415 (95.88), maa://34677 (95.88), maa://32892 (87.63), *maa://32653 (63.92), **maa://61839 (45.36), **maa://61275 (35.05)</t>
+          <t>maa://32647 (100.00), maa://32415 (95.88), maa://34677 (95.88), maa://32892 (87.63), *maa://32653 (63.92), *maa://61839 (52.58), **maa://61275 (35.05)</t>
         </is>
       </c>
       <c r="E348" s="22" t="inlineStr">
@@ -26530,7 +26530,7 @@
       </c>
       <c r="D361" s="22" t="inlineStr">
         <is>
-          <t>maa://49648 (100.00), *maa://49662 (63.22)</t>
+          <t>maa://49648 (100.00), *maa://49662 (65.48)</t>
         </is>
       </c>
       <c r="E361" s="22" t="inlineStr">
@@ -26692,7 +26692,7 @@
       </c>
       <c r="D364" s="22" t="inlineStr">
         <is>
-          <t>maa://42635 (100.00), *maa://50629 (51.16), **maa://48859 (39.53)</t>
+          <t>maa://42635 (100.00), *maa://50629 (52.38), **maa://48859 (40.48)</t>
         </is>
       </c>
       <c r="E364" s="22" t="inlineStr">
@@ -26854,7 +26854,7 @@
       </c>
       <c r="D367" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (100.00), maa://44635 (88.04), maa://48026 (95.65), maa://41035 (92.39), maa://44660 (86.96), *maa://41128 (76.09), **maa://60251 (48.91)</t>
+          <t>maa://40957 (100.00), maa://44635 (88.04), maa://48026 (95.65), maa://41035 (92.39), maa://44660 (86.96), *maa://41128 (76.09), *maa://60251 (52.17)</t>
         </is>
       </c>
       <c r="E367" s="22" t="inlineStr">
@@ -27340,7 +27340,7 @@
       </c>
       <c r="D376" s="22" t="inlineStr">
         <is>
-          <t>maa://41110 (100.00), *maa://45605 (59.57)</t>
+          <t>maa://41110 (100.00), *maa://45605 (58.95)</t>
         </is>
       </c>
       <c r="E376" s="22" t="inlineStr">
@@ -27772,7 +27772,7 @@
       </c>
       <c r="D384" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (82.98), maa://44745 (100.00), ***maa://49516 (22.34), **maa://45952 (41.49), ***maa://46851 (3.19), **maa://44896 (47.87)</t>
+          <t>maa://42970 (81.91), maa://44745 (100.00), ***maa://49516 (22.34), **maa://45952 (41.49), ***maa://46851 (3.19), **maa://44896 (47.87)</t>
         </is>
       </c>
       <c r="E384" s="22" t="inlineStr">
@@ -28420,7 +28420,7 @@
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>maa://51872 (100.00), maa://51876 (100.00), *maa://63228 (71.28), maa://51873 (97.87), *maa://62047 (73.40)</t>
+          <t>maa://51872 (100.00), maa://51876 (100.00), *maa://63228 (72.34), maa://51873 (97.87), *maa://62047 (74.47)</t>
         </is>
       </c>
       <c r="E399" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#223)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -1084,7 +1084,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>maa://30062 (100.00), maa://39394 (96.15), ***maa://26209 (9.62)</t>
+          <t>maa://30062 (100.00), maa://39394 (98.08), ***maa://26209 (9.62)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.11 13:31:21</t>
+          <t>更新日期：2025.08.12 13:22:39</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1810,7 +1810,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (100.00), maa://36669 (83.95), *maa://23264 (60.49)</t>
+          <t>maa://28977 (100.00), maa://36669 (85.00), *maa://23264 (61.25)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (93.33), maa://64046 (100.00)</t>
+          <t>maa://63896 (92.31), maa://64046 (100.00)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://22753 (100.00), maa://37962 (94.32), *maa://21485 (77.27)</t>
+          <t>maa://22753 (100.00), maa://37962 (94.32), *maa://21485 (78.41)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (96.10), maa://22734 (100.00), *maa://30808 (67.53), maa://36048 (84.42), maa://45058 (84.42)</t>
+          <t>maa://22743 (96.10), maa://22734 (100.00), *maa://30808 (66.23), maa://36048 (84.42), maa://45058 (81.82)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://22466 (100.00), maa://52226 (98.86)</t>
+          <t>maa://22466 (100.00), maa://52226 (100.00)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), maa://54153 (81.91), *maa://24380 (69.15)</t>
+          <t>maa://24379 (100.00), maa://54153 (82.98), *maa://24380 (69.15)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://24313 (96.36), maa://47854 (100.00), *maa://29784 (60.00)</t>
+          <t>maa://24313 (92.98), maa://47854 (100.00), *maa://29784 (57.89)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (100.00), maa://49976 (93.02), *maa://56241 (69.77)</t>
+          <t>maa://50085 (100.00), maa://49976 (93.02), *maa://56241 (72.09)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22524 (100.00), maa://22432 (97.50), ***maa://64221 (28.75)</t>
+          <t>maa://22524 (100.00), maa://22432 (97.50), **maa://64221 (37.50)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (100.00), maa://36258 (92.22), *maa://43904 (53.33)</t>
+          <t>maa://35926 (100.00), maa://36258 (92.22), *maa://43904 (56.67)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (100.00), *maa://47069 (62.89), *maa://56336 (60.82), *maa://45789 (67.01)</t>
+          <t>maa://45718 (100.00), *maa://47069 (62.89), *maa://56336 (62.89), *maa://45789 (67.01)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://64107 (84.31), maa://64205 (100.00)</t>
+          <t>*maa://64107 (75.44), maa://64205 (100.00)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>maa://22525 (90.00), maa://21284 (100.00)</t>
+          <t>maa://22525 (88.75), maa://21284 (100.00)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -5992,7 +5992,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (100.00), maa://27728 (95.79), *maa://56386 (71.58)</t>
+          <t>maa://29768 (100.00), maa://27728 (95.79), *maa://56386 (73.68)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -7090,7 +7090,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.11 13:31:21</t>
+          <t>更新日期：2025.08.12 13:22:39</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8278,7 +8278,7 @@
       </c>
       <c r="D23" s="13" t="inlineStr">
         <is>
-          <t>maa://20876 (100.00), **maa://63498 (39.53)</t>
+          <t>maa://20876 (100.00), *maa://63498 (51.16)</t>
         </is>
       </c>
       <c r="E23" s="14" t="inlineStr">
@@ -8494,7 +8494,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (69.51), *maa://28758 (65.85), maa://29036 (100.00), *maa://42172 (57.32), maa://30285 (82.93)</t>
+          <t>*maa://20849 (69.51), *maa://28758 (67.07), maa://29036 (100.00), *maa://42172 (59.76), maa://30285 (82.93)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8764,7 +8764,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (93.26), maa://36866 (100.00), *maa://45572 (71.91), maa://62759 (91.01), *maa://27794 (64.04), *maa://20960 (78.65), **maa://20843 (49.44), ***maa://24483 (10.11), **maa://20862 (49.44), *maa://20893 (61.80)</t>
+          <t>maa://36644 (94.38), maa://36866 (100.00), *maa://45572 (71.91), maa://62759 (91.01), *maa://27794 (64.04), *maa://20960 (78.65), **maa://20843 (49.44), ***maa://24483 (10.11), **maa://20862 (49.44), *maa://20893 (61.80)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -9034,7 +9034,7 @@
       </c>
       <c r="D37" s="13" t="inlineStr">
         <is>
-          <t>maa://42635 (100.00), maa://27376 (98.81), **maa://20838 (40.48)</t>
+          <t>maa://27376 (98.81), maa://42635 (100.00), **maa://20838 (40.48)</t>
         </is>
       </c>
       <c r="E37" s="14" t="inlineStr">
@@ -9898,7 +9898,7 @@
       </c>
       <c r="D53" s="13" t="inlineStr">
         <is>
-          <t>maa://20953 (100.00), maa://31173 (100.00)</t>
+          <t>maa://20953 (100.00), maa://31173 (95.24)</t>
         </is>
       </c>
       <c r="E53" s="14" t="inlineStr">
@@ -10870,7 +10870,7 @@
       </c>
       <c r="D71" s="13" t="inlineStr">
         <is>
-          <t>maa://20943 (100.00), *maa://30673 (73.47), *maa://30672 (66.33), maa://20856 (82.65), *maa://63790 (58.16)</t>
+          <t>maa://20943 (100.00), *maa://30673 (73.47), *maa://30672 (66.33), maa://20856 (82.65), *maa://63790 (66.33)</t>
         </is>
       </c>
       <c r="E71" s="14" t="inlineStr">
@@ -12868,7 +12868,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://25018 (96.94), maa://25776 (85.71), maa://28361 (85.71), maa://25772 (85.71), *maa://56588 (79.59), *maa://45194 (63.27), *maa://25161 (62.24), *maa://32653 (63.27), ***maa://60902 (12.24), *maa://61839 (52.04), **maa://61275 (34.69)</t>
+          <t>maa://51881 (100.00), maa://25018 (96.94), maa://25776 (85.71), maa://28361 (85.71), maa://25772 (85.71), *maa://56588 (79.59), *maa://45194 (65.31), *maa://25161 (62.24), *maa://32653 (63.27), ***maa://60902 (12.24), *maa://61839 (52.04), **maa://61275 (34.69)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -16108,7 +16108,7 @@
       </c>
       <c r="D168" s="13" t="inlineStr">
         <is>
-          <t>maa://49867 (94.05), maa://49655 (100.00)</t>
+          <t>maa://49867 (92.94), maa://49655 (100.00)</t>
         </is>
       </c>
       <c r="E168" s="14" t="inlineStr">
@@ -16486,7 +16486,7 @@
       </c>
       <c r="D175" s="13" t="inlineStr">
         <is>
-          <t>maa://32418 (100.00), maa://51440 (89.90), *maa://63320 (76.77)</t>
+          <t>maa://32418 (100.00), maa://51440 (89.90), maa://63320 (82.83)</t>
         </is>
       </c>
       <c r="E175" s="14" t="inlineStr">
@@ -19564,7 +19564,7 @@
       </c>
       <c r="D232" s="13" t="inlineStr">
         <is>
-          <t>maa://29058 (96.74), maa://39140 (100.00), *maa://38723 (73.91)</t>
+          <t>maa://29058 (97.83), maa://39140 (100.00), *maa://38723 (73.91)</t>
         </is>
       </c>
       <c r="E232" s="14" t="inlineStr">
@@ -20050,7 +20050,7 @@
       </c>
       <c r="D241" s="13" t="inlineStr">
         <is>
-          <t>maa://30667 (96.15), maa://30666 (100.00), **maa://30739 (35.90), *maa://30723 (57.69), maa://39588 (98.72), *maa://64079 (57.69)</t>
+          <t>maa://30667 (96.15), maa://30666 (100.00), **maa://30739 (35.90), *maa://30723 (57.69), maa://39588 (98.72), *maa://64079 (62.82)</t>
         </is>
       </c>
       <c r="E241" s="14" t="inlineStr">
@@ -20590,7 +20590,7 @@
       </c>
       <c r="D251" s="13" t="inlineStr">
         <is>
-          <t>maa://42287 (94.32), maa://45570 (100.00), maa://42225 (87.50), *maa://60678 (57.95)</t>
+          <t>maa://42287 (95.45), maa://45570 (100.00), maa://42225 (87.50), *maa://60678 (64.77)</t>
         </is>
       </c>
       <c r="E251" s="14" t="inlineStr">
@@ -21886,7 +21886,7 @@
       </c>
       <c r="D275" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://51630 (91.84), *maa://56588 (79.59), **maa://55171 (37.76), *maa://51893 (57.14), ***maa://60902 (12.24)</t>
+          <t>maa://51881 (100.00), maa://51630 (91.84), *maa://56588 (79.59), **maa://55171 (37.76), *maa://51893 (61.22), ***maa://60902 (12.24)</t>
         </is>
       </c>
       <c r="E275" s="14" t="inlineStr">
@@ -26314,7 +26314,7 @@
       </c>
       <c r="D357" s="22" t="inlineStr">
         <is>
-          <t>maa://36868 (100.00), maa://35996 (92.93), ***maa://39217 (20.20), maa://47349 (87.88)</t>
+          <t>maa://36868 (100.00), maa://35996 (93.88), ***maa://39217 (20.41), maa://47349 (88.78)</t>
         </is>
       </c>
       <c r="E357" s="22" t="inlineStr">
@@ -26530,7 +26530,7 @@
       </c>
       <c r="D361" s="22" t="inlineStr">
         <is>
-          <t>maa://49648 (100.00), *maa://49662 (65.48)</t>
+          <t>maa://49648 (100.00), *maa://49662 (64.71)</t>
         </is>
       </c>
       <c r="E361" s="22" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#224)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://39402 (100.00), *maa://34787 (73.86), maa://58660 (95.45)</t>
+          <t>maa://39402 (100.00), *maa://34787 (73.86), maa://58660 (96.59)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://21246 (98.88), maa://36684 (100.00)</t>
+          <t>maa://21246 (97.78), maa://36684 (100.00)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://45854 (85.88), maa://24617 (100.00), *maa://60545 (71.76)</t>
+          <t>maa://45854 (85.88), maa://24617 (100.00), *maa://60545 (75.29)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (100.00), maa://50121 (94.38)</t>
+          <t>maa://49983 (100.00), maa://50121 (95.51)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>maa://30062 (100.00), maa://39394 (98.08), ***maa://26209 (9.62)</t>
+          <t>maa://30062 (100.00), maa://39394 (96.08), ***maa://26209 (9.80)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>maa://22763 (100.00)</t>
+          <t>**maa://64972 (42.00)</t>
         </is>
       </c>
       <c r="I7" s="19" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.12 13:22:39</t>
+          <t>更新日期：2025.08.13 13:25:33</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>maa://21248 (100.00), **maa://22728 (49.28)</t>
+          <t>maa://21248 (100.00), **maa://22728 (47.83)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (96.77), maa://26245 (100.00), maa://21288 (98.92), maa://36682 (92.47)</t>
+          <t>maa://39841 (97.85), maa://26245 (100.00), maa://21288 (98.92), maa://36682 (92.47)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (96.10), maa://22734 (100.00), *maa://30808 (66.23), maa://36048 (84.42), maa://45058 (81.82)</t>
+          <t>maa://22743 (96.10), maa://22734 (100.00), *maa://30808 (66.23), maa://36048 (84.42), maa://45058 (83.12)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://24313 (92.98), maa://47854 (100.00), *maa://29784 (57.89)</t>
+          <t>maa://24313 (91.38), maa://47854 (100.00), *maa://29784 (56.90)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (100.00), *maa://36668 (74.24)</t>
+          <t>maa://30709 (100.00), *maa://36668 (75.76)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (100.00), maa://49976 (93.02), *maa://56241 (72.09)</t>
+          <t>maa://50085 (100.00), maa://49976 (94.12), *maa://56241 (75.29)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22524 (100.00), maa://22432 (97.50), **maa://64221 (37.50)</t>
+          <t>maa://22524 (100.00), maa://22432 (97.50), **maa://64221 (31.25)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -4259,12 +4259,12 @@
       </c>
       <c r="K29" s="19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (96.81), maa://31400 (100.00), maa://28440 (84.04), **maa://28650 (38.30)</t>
+          <t>maa://28432 (96.81), maa://31400 (100.00), maa://28440 (84.04)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -5679,12 +5679,12 @@
       </c>
       <c r="AE40" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>*maa://64107 (75.44), maa://64205 (100.00)</t>
+          <t>maa://64205 (100.00)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -6215,7 +6215,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (100.00), maa://29661 (98.95), *maa://28038 (61.05), *maa://56236 (60.00)</t>
+          <t>maa://27410 (100.00), maa://29661 (98.95), *maa://28038 (61.05), *maa://56236 (64.21)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6660,7 +6660,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://25176 (100.00), *maa://56237 (73.12)</t>
+          <t>maa://25176 (100.00), *maa://56237 (75.27)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6768,7 +6768,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (100.00), *maa://59413 (60.00)</t>
+          <t>maa://59534 (100.00), *maa://59413 (64.21)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7090,7 +7090,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.12 13:22:39</t>
+          <t>更新日期：2025.08.13 13:25:33</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8278,7 +8278,7 @@
       </c>
       <c r="D23" s="13" t="inlineStr">
         <is>
-          <t>maa://20876 (100.00), *maa://63498 (51.16)</t>
+          <t>maa://20876 (100.00), *maa://63498 (59.30)</t>
         </is>
       </c>
       <c r="E23" s="14" t="inlineStr">
@@ -8494,7 +8494,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (69.51), *maa://28758 (67.07), maa://29036 (100.00), *maa://42172 (59.76), maa://30285 (82.93)</t>
+          <t>*maa://20849 (68.67), *maa://28758 (66.27), maa://29036 (100.00), *maa://42172 (59.04), maa://30285 (81.93)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8764,7 +8764,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (94.38), maa://36866 (100.00), *maa://45572 (71.91), maa://62759 (91.01), *maa://27794 (64.04), *maa://20960 (78.65), **maa://20843 (49.44), ***maa://24483 (10.11), **maa://20862 (49.44), *maa://20893 (61.80)</t>
+          <t>maa://36644 (94.38), maa://36866 (100.00), *maa://45572 (71.91), maa://62759 (92.13), *maa://27794 (64.04), *maa://20960 (78.65), **maa://20843 (49.44), ***maa://24483 (10.11), **maa://20862 (49.44), *maa://20893 (61.80)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -9898,7 +9898,7 @@
       </c>
       <c r="D53" s="13" t="inlineStr">
         <is>
-          <t>maa://20953 (100.00), maa://31173 (95.24)</t>
+          <t>maa://20953 (100.00), maa://31173 (96.43)</t>
         </is>
       </c>
       <c r="E53" s="14" t="inlineStr">
@@ -10330,7 +10330,7 @@
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (100.00), maa://24093 (100.00), maa://31559 (88.42), maa://20924 (81.05), *maa://25777 (60.00), *maa://20631 (60.00), **maa://28241 (46.32)</t>
+          <t>maa://20841 (100.00), maa://24093 (100.00), maa://31559 (89.47), maa://20924 (81.05), *maa://25777 (60.00), *maa://20631 (60.00), **maa://28241 (46.32)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -10600,7 +10600,7 @@
       </c>
       <c r="D66" s="13" t="inlineStr">
         <is>
-          <t>maa://20993 (100.00), maa://45606 (90.53), **maa://20914 (46.32), maa://20829 (81.05), maa://20900 (85.26), **maa://40159 (46.32)</t>
+          <t>maa://20993 (100.00), maa://45606 (91.58), **maa://20914 (46.32), maa://20829 (81.05), maa://20900 (85.26), **maa://40159 (46.32)</t>
         </is>
       </c>
       <c r="E66" s="14" t="inlineStr">
@@ -10870,7 +10870,7 @@
       </c>
       <c r="D71" s="13" t="inlineStr">
         <is>
-          <t>maa://20943 (100.00), *maa://30673 (73.47), *maa://30672 (66.33), maa://20856 (82.65), *maa://63790 (66.33)</t>
+          <t>maa://20943 (100.00), *maa://30673 (73.47), *maa://30672 (66.33), maa://20856 (82.65), *maa://63790 (69.39)</t>
         </is>
       </c>
       <c r="E71" s="14" t="inlineStr">
@@ -12274,7 +12274,7 @@
       </c>
       <c r="D97" s="13" t="inlineStr">
         <is>
-          <t>maa://20991 (100.00), *maa://51015 (73.20)</t>
+          <t>maa://20991 (100.00), *maa://51015 (74.23)</t>
         </is>
       </c>
       <c r="E97" s="14" t="inlineStr">
@@ -12868,7 +12868,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://25018 (96.94), maa://25776 (85.71), maa://28361 (85.71), maa://25772 (85.71), *maa://56588 (79.59), *maa://45194 (65.31), *maa://25161 (62.24), *maa://32653 (63.27), ***maa://60902 (12.24), *maa://61839 (52.04), **maa://61275 (34.69)</t>
+          <t>maa://51881 (100.00), maa://25018 (97.94), maa://25776 (86.60), maa://28361 (86.60), maa://25772 (86.60), maa://56588 (80.41), *maa://45194 (65.98), *maa://25161 (62.89), *maa://32653 (63.92), ***maa://60902 (12.37), *maa://61839 (52.58), **maa://61275 (35.05)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13084,7 +13084,7 @@
       </c>
       <c r="D112" s="13" t="inlineStr">
         <is>
-          <t>maa://20933 (100.00), maa://20822 (89.47)</t>
+          <t>maa://20933 (100.00), maa://20822 (88.31)</t>
         </is>
       </c>
       <c r="E112" s="14" t="inlineStr">
@@ -13354,7 +13354,7 @@
       </c>
       <c r="D117" s="13" t="inlineStr">
         <is>
-          <t>maa://31560 (100.00), maa://20940 (86.57)</t>
+          <t>maa://31560 (100.00), maa://20940 (89.55)</t>
         </is>
       </c>
       <c r="E117" s="14" t="inlineStr">
@@ -15082,7 +15082,7 @@
       </c>
       <c r="D149" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.85), maa://36641 (100.00), maa://36865 (94.85), maa://44635 (83.51), maa://44660 (82.47), *maa://41128 (72.16), maa://42918 (92.78), maa://44119 (89.69), maa://46108 (88.66), *maa://37300 (58.76), **maa://42917 (35.05), **maa://64408 (45.36)</t>
+          <t>maa://40957 (94.85), maa://36641 (100.00), maa://36865 (94.85), maa://44635 (83.51), maa://44660 (82.47), *maa://41128 (72.16), maa://42918 (92.78), maa://44119 (89.69), maa://46108 (88.66), *maa://37300 (58.76), **maa://42917 (35.05), *maa://64408 (58.76)</t>
         </is>
       </c>
       <c r="E149" s="14" t="inlineStr">
@@ -16432,7 +16432,7 @@
       </c>
       <c r="D174" s="13" t="inlineStr">
         <is>
-          <t>maa://59681 (100.00), **maa://64200 (46.81)</t>
+          <t>maa://59681 (100.00), *maa://64200 (60.64)</t>
         </is>
       </c>
       <c r="E174" s="14" t="inlineStr">
@@ -16486,7 +16486,7 @@
       </c>
       <c r="D175" s="13" t="inlineStr">
         <is>
-          <t>maa://32418 (100.00), maa://51440 (89.90), maa://63320 (82.83)</t>
+          <t>maa://32418 (100.00), maa://51440 (89.90), maa://63320 (84.85)</t>
         </is>
       </c>
       <c r="E175" s="14" t="inlineStr">
@@ -17674,7 +17674,7 @@
       </c>
       <c r="D197" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (91.58), maa://35854 (82.11), maa://50388 (100.00), maa://25760 (84.21), ***maa://43911 (4.21), **maa://20872 (34.74), *maa://51066 (68.42), maa://63024 (81.05)</t>
+          <t>maa://44224 (91.58), maa://35854 (82.11), maa://50388 (100.00), maa://25760 (84.21), ***maa://43911 (4.21), **maa://20872 (34.74), *maa://51066 (68.42), maa://63024 (82.11)</t>
         </is>
       </c>
       <c r="E197" s="14" t="inlineStr">
@@ -17728,7 +17728,7 @@
       </c>
       <c r="D198" s="13" t="inlineStr">
         <is>
-          <t>maa://39156 (100.00), **maa://39550 (39.08), **maa://53417 (41.38), ***maa://63806 (24.14)</t>
+          <t>maa://39156 (100.00), **maa://39550 (39.08), **maa://53417 (47.13), ***maa://63806 (24.14)</t>
         </is>
       </c>
       <c r="E198" s="14" t="inlineStr">
@@ -20050,7 +20050,7 @@
       </c>
       <c r="D241" s="13" t="inlineStr">
         <is>
-          <t>maa://30667 (96.15), maa://30666 (100.00), **maa://30739 (35.90), *maa://30723 (57.69), maa://39588 (98.72), *maa://64079 (62.82)</t>
+          <t>maa://30667 (96.15), maa://30666 (100.00), **maa://30739 (35.90), *maa://30723 (57.69), maa://39588 (98.72), *maa://64079 (66.67)</t>
         </is>
       </c>
       <c r="E241" s="14" t="inlineStr">
@@ -20104,7 +20104,7 @@
       </c>
       <c r="D242" s="13" t="inlineStr">
         <is>
-          <t>maa://62759 (100.00), **maa://62764 (41.98)</t>
+          <t>maa://62759 (100.00), **maa://62764 (41.46)</t>
         </is>
       </c>
       <c r="E242" s="14" t="inlineStr">
@@ -20590,7 +20590,7 @@
       </c>
       <c r="D251" s="13" t="inlineStr">
         <is>
-          <t>maa://42287 (95.45), maa://45570 (100.00), maa://42225 (87.50), *maa://60678 (64.77)</t>
+          <t>maa://42287 (95.45), maa://45570 (100.00), maa://42225 (87.50), *maa://60678 (69.32)</t>
         </is>
       </c>
       <c r="E251" s="14" t="inlineStr">
@@ -20752,7 +20752,7 @@
       </c>
       <c r="D254" s="13" t="inlineStr">
         <is>
-          <t>maa://24093 (100.00), maa://31559 (88.42), maa://20924 (81.05), ***maa://49440 (16.84)</t>
+          <t>maa://24093 (100.00), maa://31559 (89.47), maa://20924 (81.05), ***maa://49440 (16.84)</t>
         </is>
       </c>
       <c r="E254" s="14" t="inlineStr">
@@ -21886,7 +21886,7 @@
       </c>
       <c r="D275" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://51630 (91.84), *maa://56588 (79.59), **maa://55171 (37.76), *maa://51893 (61.22), ***maa://60902 (12.24)</t>
+          <t>maa://51881 (100.00), maa://51630 (92.78), maa://56588 (80.41), **maa://55171 (38.14), *maa://51893 (61.86), ***maa://60902 (12.37)</t>
         </is>
       </c>
       <c r="E275" s="14" t="inlineStr">
@@ -25828,7 +25828,7 @@
       </c>
       <c r="D348" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (100.00), maa://32415 (95.88), maa://34677 (95.88), maa://32892 (87.63), *maa://32653 (63.92), *maa://61839 (52.58), **maa://61275 (35.05)</t>
+          <t>maa://32647 (100.00), maa://32415 (96.88), maa://34677 (96.88), maa://32892 (88.54), *maa://32653 (64.58), *maa://61839 (53.12), **maa://61275 (35.42)</t>
         </is>
       </c>
       <c r="E348" s="22" t="inlineStr">
@@ -26368,7 +26368,7 @@
       </c>
       <c r="D358" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.00), maa://49695 (100.00), maa://49758 (92.00), **maa://59402 (39.00), **maa://52357 (48.00), ***maa://63091 (6.00)</t>
+          <t>maa://49696 (99.00), maa://49695 (100.00), maa://49758 (92.00), **maa://59402 (39.00), **maa://52357 (48.00), ***maa://63091 (23.00)</t>
         </is>
       </c>
       <c r="E358" s="22" t="inlineStr">
@@ -26530,7 +26530,7 @@
       </c>
       <c r="D361" s="22" t="inlineStr">
         <is>
-          <t>maa://49648 (100.00), *maa://49662 (64.71)</t>
+          <t>maa://49648 (100.00), *maa://49662 (66.28)</t>
         </is>
       </c>
       <c r="E361" s="22" t="inlineStr">
@@ -26962,7 +26962,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://63883 (100.00), *maa://64045 (66.67), ***maa://64041 (17.65)</t>
+          <t>maa://63883 (100.00), *maa://64045 (66.67), **maa://64041 (41.18)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -27772,7 +27772,7 @@
       </c>
       <c r="D384" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (81.91), maa://44745 (100.00), ***maa://49516 (22.34), **maa://45952 (41.49), ***maa://46851 (3.19), **maa://44896 (47.87)</t>
+          <t>maa://42970 (81.91), maa://44745 (100.00), ***maa://49516 (24.47), **maa://45952 (41.49), ***maa://46851 (3.19), **maa://44896 (47.87)</t>
         </is>
       </c>
       <c r="E384" s="22" t="inlineStr">
@@ -28420,7 +28420,7 @@
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>maa://51872 (100.00), maa://51876 (100.00), *maa://63228 (72.34), maa://51873 (97.87), *maa://62047 (74.47)</t>
+          <t>maa://51872 (100.00), maa://51876 (98.95), *maa://63228 (71.58), maa://51873 (96.84), *maa://62047 (74.74)</t>
         </is>
       </c>
       <c r="E399" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#225)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://39402 (100.00), *maa://34787 (73.86), maa://58660 (96.59)</t>
+          <t>maa://39402 (100.00), *maa://34787 (73.86), maa://58660 (88.64)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://21246 (97.78), maa://36684 (100.00)</t>
+          <t>maa://21246 (98.88), maa://36684 (100.00)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://25251 (100.00), maa://59087 (95.35)</t>
+          <t>maa://25251 (100.00), maa://59087 (96.51)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (100.00), *maa://22499 (74.44), *maa://22746 (67.78)</t>
+          <t>maa://24632 (100.00), *maa://22499 (75.28), *maa://22746 (68.54)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (100.00), maa://50121 (95.51)</t>
+          <t>maa://49983 (100.00), maa://50121 (96.59)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>maa://30062 (100.00), maa://39394 (96.08), ***maa://26209 (9.80)</t>
+          <t>maa://30062 (100.00), maa://39394 (100.00), ***maa://26209 (9.80)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (100.00), maa://54105 (100.00), maa://22744 (81.01)</t>
+          <t>maa://21245 (98.75), maa://54105 (100.00), *maa://22744 (80.00)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (100.00), maa://30381 (88.10)</t>
+          <t>maa://31836 (100.00), maa://30381 (89.29)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.13 13:25:33</t>
+          <t>更新日期：2025.08.16 13:20:53</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1614,7 +1614,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>maa://24479 (100.00), **maa://21990 (49.25)</t>
+          <t>maa://24479 (100.00), **maa://21990 (48.53)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://26223 (100.00), maa://52237 (83.16)</t>
+          <t>maa://26223 (100.00), maa://52237 (84.21)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>***maa://25695 (26.92), ***maa://39951 (11.54), maa://45271 (100.00), ***maa://34206 (21.15), ***maa://39243 (13.46), **maa://54000 (44.23)</t>
+          <t>***maa://25695 (26.42), ***maa://39951 (11.32), maa://45271 (100.00), ***maa://34206 (20.75), ***maa://39243 (13.21), **maa://54000 (43.40)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (100.00), maa://36669 (85.00), *maa://23264 (61.25)</t>
+          <t>maa://28977 (100.00), maa://36669 (81.25), *maa://23264 (61.25)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (100.00), maa://22755 (87.23), **maa://63521 (47.87)</t>
+          <t>maa://27395 (100.00), maa://22755 (87.23), *maa://63521 (51.06)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>maa://25021 (84.62), maa://22733 (100.00), ***maa://22761 (17.31)</t>
+          <t>maa://25021 (84.31), maa://22733 (100.00), ***maa://22761 (17.65)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (100.00), *maa://54294 (75.58)</t>
+          <t>maa://21867 (100.00), maa://54294 (83.72)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (92.31), maa://64046 (100.00)</t>
+          <t>maa://63896 (88.89), maa://64046 (100.00)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://22753 (100.00), maa://37962 (94.32), *maa://21485 (78.41)</t>
+          <t>maa://22753 (100.00), maa://37962 (93.18), *maa://21485 (78.41)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://23669 (100.00), maa://36677 (96.77), maa://39872 (87.10)</t>
+          <t>maa://23669 (100.00), maa://36677 (95.70), maa://39872 (88.17)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (100.00), *maa://22583 (77.78), *maa://48321 (58.89)</t>
+          <t>maa://22676 (100.00), *maa://22583 (77.78), *maa://48321 (61.11)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (97.85), maa://26245 (100.00), maa://21288 (98.92), maa://36682 (92.47)</t>
+          <t>maa://39841 (96.77), maa://26245 (100.00), maa://21288 (98.92), maa://36682 (92.47)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://22521 (100.00), maa://42751 (92.22)</t>
+          <t>maa://22521 (100.00), maa://42751 (93.26)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://21364 (100.00), maa://36666 (97.44), *maa://22766 (78.21)</t>
+          <t>maa://21364 (100.00), maa://36666 (98.72), *maa://22766 (78.21)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://22729 (100.00), *maa://28648 (72.53), *maa://36674 (76.92)</t>
+          <t>maa://22729 (100.00), *maa://28648 (73.33), *maa://36674 (77.78)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2672,7 +2672,7 @@
       </c>
       <c r="D17" s="8" t="inlineStr">
         <is>
-          <t>maa://21624 (100.00), **maa://56358 (47.22)</t>
+          <t>maa://21624 (100.00), **maa://56358 (46.58)</t>
         </is>
       </c>
       <c r="E17" s="19" t="n"/>
@@ -2715,12 +2715,12 @@
       </c>
       <c r="O17" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (100.00), maa://56238 (83.56)</t>
+          <t>maa://23890 (100.00), *maa://24940 (67.12), *maa://56238 (72.60)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://22466 (100.00), maa://52226 (100.00)</t>
+          <t>maa://22466 (98.88), maa://52226 (100.00)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), maa://54153 (82.98), *maa://24380 (69.15)</t>
+          <t>maa://24379 (100.00), maa://54153 (85.11), *maa://24380 (69.15)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (100.00), *maa://22741 (61.54)</t>
+          <t>maa://21917 (100.00), *maa://22741 (60.87)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://24313 (91.38), maa://47854 (100.00), *maa://29784 (56.90)</t>
+          <t>maa://24313 (89.83), maa://47854 (100.00), *maa://29784 (55.93)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (100.00), maa://49976 (94.12), *maa://56241 (75.29)</t>
+          <t>maa://50085 (100.00), maa://49976 (95.29), *maa://56241 (78.82)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (100.00), maa://20110 (90.59)</t>
+          <t>maa://34946 (100.00), maa://20110 (89.41)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22524 (100.00), maa://22432 (97.50), **maa://64221 (31.25)</t>
+          <t>maa://22524 (100.00), maa://22432 (97.50), **maa://64221 (38.75)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://21282 (100.00), *maa://37649 (61.86)</t>
+          <t>maa://21282 (100.00), *maa://37649 (62.89)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (89.01), maa://23504 (100.00), *maa://25141 (76.92), *maa://36663 (75.82), maa://52227 (92.31)</t>
+          <t>maa://29988 (89.01), maa://23504 (100.00), *maa://36663 (75.82), *maa://25141 (76.92), maa://52227 (92.31)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://22523 (87.21), *maa://36672 (69.77), maa://29910 (100.00), maa://45831 (84.88), *maa://64165 (66.28)</t>
+          <t>maa://22523 (87.21), *maa://36672 (69.77), maa://29910 (100.00), maa://45831 (84.88), *maa://64165 (70.93)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>maa://29063 (96.92), maa://25311 (100.00), ***maa://22725 (3.08), maa://45047 (81.54)</t>
+          <t>maa://29063 (95.38), maa://25311 (100.00), ***maa://22725 (3.08), maa://45047 (81.54)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (100.00), maa://24516 (85.54), maa://26001 (87.95)</t>
+          <t>maa://31215 (100.00), maa://24516 (84.52), maa://26001 (86.90)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://41802 (100.00), *maa://56374 (76.25)</t>
+          <t>maa://41802 (100.00), maa://56374 (81.25)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="AF26" s="8" t="inlineStr">
         <is>
-          <t>maa://30511 (100.00), **maa://29760 (47.54)</t>
+          <t>maa://30511 (100.00), **maa://29760 (48.33)</t>
         </is>
       </c>
       <c r="AG26" s="16" t="n"/>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (96.81), maa://31400 (100.00), maa://28440 (84.04)</t>
+          <t>maa://28432 (97.87), maa://31400 (100.00), maa://28440 (84.04)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (100.00), ***maa://64191 (27.27)</t>
+          <t>maa://45792 (100.00), **maa://64191 (44.16)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://21895 (100.00), maa://36667 (97.89), **maa://22760 (35.79)</t>
+          <t>maa://21895 (100.00), maa://36667 (98.95), **maa://22760 (35.79)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (100.00), *maa://56235 (55.43)</t>
+          <t>maa://48817 (100.00), *maa://56235 (61.96)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (100.00), *maa://47069 (62.89), *maa://56336 (62.89), *maa://45789 (67.01)</t>
+          <t>maa://45718 (100.00), *maa://47069 (59.79), *maa://56336 (63.92), *maa://45789 (67.01)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5418,7 +5418,7 @@
       </c>
       <c r="L38" s="8" t="inlineStr">
         <is>
-          <t>maa://39384 (100.00), *maa://49735 (61.29)</t>
+          <t>maa://39384 (100.00), *maa://49735 (64.89)</t>
         </is>
       </c>
       <c r="M38" s="19" t="n"/>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://24709 (100.00), maa://47093 (98.85)</t>
+          <t>maa://24709 (100.00), maa://47093 (95.40)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5546,12 +5546,12 @@
       </c>
       <c r="S39" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (100.00), *maa://45790 (76.19)</t>
+          <t>maa://47079 (100.00), *maa://45788 (72.84), *maa://45790 (79.01)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5679,12 +5679,12 @@
       </c>
       <c r="AE40" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://64205 (100.00)</t>
+          <t>*maa://64107 (65.28), maa://64205 (100.00), **maa://65283 (47.22)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -6490,7 +6490,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (100.00), maa://59378 (92.47)</t>
+          <t>maa://59394 (100.00), maa://59378 (91.49)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6763,12 +6763,12 @@
       </c>
       <c r="G63" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (100.00), *maa://59413 (64.21)</t>
+          <t>maa://59534 (100.00), **maa://59693 (43.62), *maa://59413 (69.15)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7090,7 +7090,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.13 13:25:33</t>
+          <t>更新日期：2025.08.16 13:20:53</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8278,7 +8278,7 @@
       </c>
       <c r="D23" s="13" t="inlineStr">
         <is>
-          <t>maa://20876 (100.00), *maa://63498 (59.30)</t>
+          <t>maa://20876 (100.00), *maa://63498 (58.62)</t>
         </is>
       </c>
       <c r="E23" s="14" t="inlineStr">
@@ -8494,7 +8494,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (68.67), *maa://28758 (66.27), maa://29036 (100.00), *maa://42172 (59.04), maa://30285 (81.93)</t>
+          <t>*maa://20849 (69.88), *maa://28758 (67.47), maa://29036 (100.00), *maa://42172 (59.04), maa://30285 (81.93)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8602,7 +8602,7 @@
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>maa://20863 (89.47), maa://20832 (100.00), *maa://20727 (75.79)</t>
+          <t>maa://20863 (90.53), maa://20832 (100.00), *maa://20727 (75.79)</t>
         </is>
       </c>
       <c r="E29" s="14" t="inlineStr">
@@ -10870,7 +10870,7 @@
       </c>
       <c r="D71" s="13" t="inlineStr">
         <is>
-          <t>maa://20943 (100.00), *maa://30673 (73.47), *maa://30672 (66.33), maa://20856 (82.65), *maa://63790 (69.39)</t>
+          <t>maa://20943 (100.00), *maa://30673 (73.47), *maa://30672 (66.33), maa://63790 (83.67), maa://20856 (82.65)</t>
         </is>
       </c>
       <c r="E71" s="14" t="inlineStr">
@@ -12598,7 +12598,7 @@
       </c>
       <c r="D103" s="13" t="inlineStr">
         <is>
-          <t>*maa://29094 (79.73), maa://28904 (100.00), **maa://20931 (37.84)</t>
+          <t>maa://29094 (80.26), maa://28904 (100.00), **maa://20931 (39.47)</t>
         </is>
       </c>
       <c r="E103" s="14" t="inlineStr">
@@ -12868,7 +12868,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://25018 (97.94), maa://25776 (86.60), maa://28361 (86.60), maa://25772 (86.60), maa://56588 (80.41), *maa://45194 (65.98), *maa://25161 (62.89), *maa://32653 (63.92), ***maa://60902 (12.37), *maa://61839 (52.58), **maa://61275 (35.05)</t>
+          <t>maa://51881 (100.00), maa://25018 (97.94), maa://25776 (86.60), maa://28361 (86.60), maa://25772 (86.60), maa://56588 (82.47), *maa://45194 (67.01), *maa://25161 (62.89), *maa://32653 (63.92), ***maa://60902 (11.34), *maa://61839 (52.58), **maa://61275 (45.36)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13246,7 +13246,7 @@
       </c>
       <c r="D115" s="13" t="inlineStr">
         <is>
-          <t>maa://20908 (100.00), maa://35723 (90.62), **maa://23346 (46.88), maa://38822 (92.71), *maa://58659 (67.71)</t>
+          <t>maa://20908 (100.00), maa://35723 (90.62), **maa://23346 (46.88), maa://38822 (92.71), *maa://58659 (70.83)</t>
         </is>
       </c>
       <c r="E115" s="14" t="inlineStr">
@@ -13300,7 +13300,7 @@
       </c>
       <c r="D116" s="13" t="inlineStr">
         <is>
-          <t>maa://29659 (95.95), maa://29031 (100.00)</t>
+          <t>maa://29659 (97.30), maa://29031 (100.00)</t>
         </is>
       </c>
       <c r="E116" s="14" t="inlineStr">
@@ -13354,7 +13354,7 @@
       </c>
       <c r="D117" s="13" t="inlineStr">
         <is>
-          <t>maa://31560 (100.00), maa://20940 (89.55)</t>
+          <t>maa://31560 (100.00), maa://20940 (92.54)</t>
         </is>
       </c>
       <c r="E117" s="14" t="inlineStr">
@@ -14704,7 +14704,7 @@
       </c>
       <c r="D142" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (100.00), **maa://23736 (35.48), *maa://31185 (56.99), *maa://30306 (54.84)</t>
+          <t>maa://28484 (100.00), **maa://23736 (35.11), *maa://31185 (56.38), *maa://30306 (54.26)</t>
         </is>
       </c>
       <c r="E142" s="14" t="inlineStr">
@@ -14758,7 +14758,7 @@
       </c>
       <c r="D143" s="13" t="inlineStr">
         <is>
-          <t>maa://30670 (100.00), maa://31470 (89.25), **maa://45066 (38.71), ***maa://30867 (12.90), ***maa://61380 (22.58)</t>
+          <t>maa://30670 (100.00), maa://31470 (89.25), **maa://45066 (38.71), **maa://61380 (36.56), ***maa://30867 (12.90)</t>
         </is>
       </c>
       <c r="E143" s="14" t="inlineStr">
@@ -15082,7 +15082,7 @@
       </c>
       <c r="D149" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.85), maa://36641 (100.00), maa://36865 (94.85), maa://44635 (83.51), maa://44660 (82.47), *maa://41128 (72.16), maa://42918 (92.78), maa://44119 (89.69), maa://46108 (88.66), *maa://37300 (58.76), **maa://42917 (35.05), *maa://64408 (58.76)</t>
+          <t>maa://40957 (94.85), maa://36641 (100.00), maa://36865 (93.81), maa://44635 (83.51), maa://44660 (82.47), *maa://41128 (72.16), maa://42918 (92.78), maa://44119 (89.69), maa://46108 (88.66), *maa://37300 (58.76), **maa://42917 (35.05), *maa://64408 (62.89)</t>
         </is>
       </c>
       <c r="E149" s="14" t="inlineStr">
@@ -16000,7 +16000,7 @@
       </c>
       <c r="D166" s="13" t="inlineStr">
         <is>
-          <t>maa://20975 (100.00), *maa://47950 (61.29), maa://30806 (91.94)</t>
+          <t>maa://20975 (100.00), *maa://47950 (70.97), maa://30806 (91.94)</t>
         </is>
       </c>
       <c r="E166" s="14" t="inlineStr">
@@ -16054,7 +16054,7 @@
       </c>
       <c r="D167" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (100.00), maa://29627 (100.00), *maa://29659 (79.78), maa://49074 (98.88), **maa://30679 (34.83), maa://29861 (87.64), *maa://42343 (78.65)</t>
+          <t>maa://29633 (100.00), maa://29627 (100.00), maa://29659 (80.90), maa://49074 (98.88), **maa://30679 (34.83), maa://29861 (87.64), *maa://42343 (78.65)</t>
         </is>
       </c>
       <c r="E167" s="14" t="inlineStr">
@@ -16486,7 +16486,7 @@
       </c>
       <c r="D175" s="13" t="inlineStr">
         <is>
-          <t>maa://32418 (100.00), maa://51440 (89.90), maa://63320 (84.85)</t>
+          <t>maa://32418 (100.00), maa://51440 (89.90), maa://63320 (86.87)</t>
         </is>
       </c>
       <c r="E175" s="14" t="inlineStr">
@@ -17674,7 +17674,7 @@
       </c>
       <c r="D197" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (91.58), maa://35854 (82.11), maa://50388 (100.00), maa://25760 (84.21), ***maa://43911 (4.21), **maa://20872 (34.74), *maa://51066 (68.42), maa://63024 (82.11)</t>
+          <t>maa://44224 (92.63), maa://35854 (83.16), maa://50388 (100.00), maa://25760 (83.16), ***maa://43911 (4.21), **maa://20872 (34.74), *maa://51066 (68.42), maa://63024 (86.32)</t>
         </is>
       </c>
       <c r="E197" s="14" t="inlineStr">
@@ -17728,7 +17728,7 @@
       </c>
       <c r="D198" s="13" t="inlineStr">
         <is>
-          <t>maa://39156 (100.00), **maa://39550 (39.08), **maa://53417 (47.13), ***maa://63806 (24.14)</t>
+          <t>maa://39156 (100.00), **maa://39550 (39.08), **maa://53417 (47.13), **maa://63806 (39.08)</t>
         </is>
       </c>
       <c r="E198" s="14" t="inlineStr">
@@ -20590,7 +20590,7 @@
       </c>
       <c r="D251" s="13" t="inlineStr">
         <is>
-          <t>maa://42287 (95.45), maa://45570 (100.00), maa://42225 (87.50), *maa://60678 (69.32)</t>
+          <t>maa://42287 (96.59), maa://45570 (100.00), *maa://60678 (77.27), maa://42225 (87.50)</t>
         </is>
       </c>
       <c r="E251" s="14" t="inlineStr">
@@ -20968,7 +20968,7 @@
       </c>
       <c r="D258" s="13" t="inlineStr">
         <is>
-          <t>maa://20879 (100.00), maa://20834 (89.61)</t>
+          <t>maa://20879 (100.00), maa://20834 (88.46)</t>
         </is>
       </c>
       <c r="E258" s="14" t="inlineStr">
@@ -21886,7 +21886,7 @@
       </c>
       <c r="D275" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://51630 (92.78), maa://56588 (80.41), **maa://55171 (38.14), *maa://51893 (61.86), ***maa://60902 (12.37)</t>
+          <t>maa://51881 (100.00), maa://51630 (92.78), maa://56588 (82.47), **maa://55171 (40.21), *maa://51893 (61.86), ***maa://60902 (11.34)</t>
         </is>
       </c>
       <c r="E275" s="14" t="inlineStr">
@@ -23128,7 +23128,7 @@
       </c>
       <c r="D298" s="13" t="inlineStr">
         <is>
-          <t>maa://45799 (100.00), maa://57199 (90.43)</t>
+          <t>maa://45799 (100.00), maa://57199 (91.49)</t>
         </is>
       </c>
       <c r="E298" s="14" t="inlineStr">
@@ -23560,7 +23560,7 @@
       </c>
       <c r="D306" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (100.00), maa://49642 (96.84), maa://49660 (82.11), **maa://50517 (40.00)</t>
+          <t>maa://50280 (100.00), maa://49642 (95.83), maa://49660 (83.33), **maa://50517 (39.58)</t>
         </is>
       </c>
       <c r="E306" s="14" t="inlineStr">
@@ -24262,7 +24262,7 @@
       </c>
       <c r="D319" s="13" t="inlineStr">
         <is>
-          <t>**maa://62755 (50.00), maa://62761 (100.00)</t>
+          <t>**maa://62755 (46.67), maa://62761 (100.00)</t>
         </is>
       </c>
       <c r="E319" s="14" t="inlineStr">
@@ -24586,7 +24586,7 @@
       </c>
       <c r="D325" s="13" t="inlineStr">
         <is>
-          <t>maa://39692 (100.00), *maa://39810 (70.71)</t>
+          <t>maa://39692 (100.00), *maa://39810 (71.72)</t>
         </is>
       </c>
       <c r="E325" s="14" t="inlineStr">
@@ -25828,7 +25828,7 @@
       </c>
       <c r="D348" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (100.00), maa://32415 (96.88), maa://34677 (96.88), maa://32892 (88.54), *maa://32653 (64.58), *maa://61839 (53.12), **maa://61275 (35.42)</t>
+          <t>maa://32647 (100.00), maa://32415 (96.88), maa://34677 (96.88), maa://32892 (88.54), *maa://32653 (64.58), *maa://61839 (53.12), **maa://61275 (45.83)</t>
         </is>
       </c>
       <c r="E348" s="22" t="inlineStr">
@@ -26368,7 +26368,7 @@
       </c>
       <c r="D358" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.00), maa://49695 (100.00), maa://49758 (92.00), **maa://59402 (39.00), **maa://52357 (48.00), ***maa://63091 (23.00)</t>
+          <t>maa://49696 (99.00), maa://49695 (100.00), maa://49758 (92.00), **maa://59402 (39.00), **maa://52357 (48.00), ***maa://63091 (19.00)</t>
         </is>
       </c>
       <c r="E358" s="22" t="inlineStr">
@@ -26530,7 +26530,7 @@
       </c>
       <c r="D361" s="22" t="inlineStr">
         <is>
-          <t>maa://49648 (100.00), *maa://49662 (66.28)</t>
+          <t>maa://49648 (100.00), *maa://49662 (72.41)</t>
         </is>
       </c>
       <c r="E361" s="22" t="inlineStr">
@@ -26854,7 +26854,7 @@
       </c>
       <c r="D367" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (100.00), maa://44635 (88.04), maa://48026 (95.65), maa://41035 (92.39), maa://44660 (86.96), *maa://41128 (76.09), *maa://60251 (52.17)</t>
+          <t>maa://40957 (100.00), maa://48026 (95.65), maa://44635 (88.04), maa://41035 (92.39), maa://44660 (86.96), *maa://41128 (76.09), *maa://60251 (55.43)</t>
         </is>
       </c>
       <c r="E367" s="22" t="inlineStr">
@@ -26962,7 +26962,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://63883 (100.00), *maa://64045 (66.67), **maa://64041 (41.18)</t>
+          <t>maa://63883 (100.00), *maa://64045 (75.00), **maa://64041 (30.88)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -27232,7 +27232,7 @@
       </c>
       <c r="D374" s="22" t="inlineStr">
         <is>
-          <t>maa://42333 (100.00), *maa://50518 (57.30), *maa://41977 (57.30)</t>
+          <t>maa://42333 (100.00), *maa://50518 (56.67), *maa://41977 (56.67)</t>
         </is>
       </c>
       <c r="E374" s="22" t="inlineStr">
@@ -27772,7 +27772,7 @@
       </c>
       <c r="D384" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (81.91), maa://44745 (100.00), ***maa://49516 (24.47), **maa://45952 (41.49), ***maa://46851 (3.19), **maa://44896 (47.87)</t>
+          <t>maa://42970 (81.91), maa://44745 (100.00), ***maa://49516 (24.47), **maa://45952 (38.30), ***maa://46851 (3.19), **maa://44896 (47.87)</t>
         </is>
       </c>
       <c r="E384" s="22" t="inlineStr">
@@ -28285,7 +28285,7 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>maa://59533 (100.00), *maa://59577 (77.27)</t>
+          <t>maa://59533 (100.00), *maa://59577 (80.00)</t>
         </is>
       </c>
       <c r="E394" t="inlineStr">
@@ -28420,7 +28420,7 @@
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>maa://51872 (100.00), maa://51876 (98.95), *maa://63228 (71.58), maa://51873 (96.84), *maa://62047 (74.74)</t>
+          <t>maa://51872 (100.00), maa://51876 (98.95), *maa://63228 (73.68), maa://51873 (96.84), *maa://62047 (74.74)</t>
         </is>
       </c>
       <c r="E399" t="inlineStr">
@@ -28474,7 +28474,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>maa://60449 (100.00), maa://59493 (95.83)</t>
+          <t>maa://60449 (100.00), maa://59493 (94.85)</t>
         </is>
       </c>
       <c r="E401" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#226)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://45854 (85.88), maa://24617 (100.00), *maa://60545 (75.29)</t>
+          <t>maa://45854 (85.88), maa://24617 (100.00), *maa://60545 (76.47)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (100.00), maa://50121 (96.59)</t>
+          <t>maa://49983 (100.00), maa://50121 (97.73)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.16 13:20:53</t>
+          <t>更新日期：2025.08.17 13:21:11</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (100.00), maa://22755 (87.23), *maa://63521 (51.06)</t>
+          <t>maa://27395 (100.00), maa://22755 (87.23), *maa://63521 (54.26)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (88.89), maa://64046 (100.00)</t>
+          <t>maa://63896 (90.00), maa://64046 (100.00)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://21441 (100.00), maa://37650 (96.77), maa://36679 (91.40)</t>
+          <t>maa://21441 (100.00), maa://37650 (97.85), maa://36679 (91.40)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (100.00), maa://49976 (95.29), *maa://56241 (78.82)</t>
+          <t>maa://50085 (100.00), maa://49976 (95.29), *maa://56241 (75.29)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (100.00), *maa://46650 (69.74)</t>
+          <t>maa://24368 (100.00), *maa://46650 (71.05)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (100.00), *maa://63016 (61.29)</t>
+          <t>maa://29753 (100.00), *maa://63016 (65.59)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (100.00), maa://36258 (92.22), *maa://43904 (56.67)</t>
+          <t>maa://35926 (100.00), maa://36258 (93.33), *maa://43904 (56.67)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (100.00), *maa://47069 (59.79), *maa://56336 (63.92), *maa://45789 (67.01)</t>
+          <t>maa://45718 (100.00), *maa://47069 (59.79), *maa://56336 (65.98), *maa://45789 (67.01)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (100.00), *maa://45788 (72.84), *maa://45790 (79.01)</t>
+          <t>maa://47079 (100.00), *maa://45788 (71.60), *maa://45790 (79.01)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5992,7 +5992,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (100.00), maa://27728 (95.79), *maa://56386 (73.68)</t>
+          <t>maa://29768 (100.00), maa://27728 (95.79), *maa://56386 (75.79)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6215,7 +6215,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (100.00), maa://29661 (98.95), *maa://28038 (61.05), *maa://56236 (64.21)</t>
+          <t>maa://27410 (100.00), maa://29661 (98.95), *maa://28038 (61.05), *maa://56236 (68.42)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6750,7 +6750,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (100.00), maa://43903 (89.89), *maa://56228 (57.30)</t>
+          <t>maa://42981 (100.00), maa://43903 (89.89), *maa://56228 (64.04)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6768,7 +6768,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (100.00), **maa://59693 (43.62), *maa://59413 (69.15)</t>
+          <t>maa://59534 (100.00), **maa://59693 (47.87), *maa://59413 (69.15)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7090,7 +7090,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.16 13:20:53</t>
+          <t>更新日期：2025.08.17 13:21:11</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8489,12 +8489,12 @@
       </c>
       <c r="C27" s="12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (69.88), *maa://28758 (67.47), maa://29036 (100.00), *maa://42172 (59.04), maa://30285 (81.93)</t>
+          <t>*maa://20849 (71.08), *maa://28758 (67.47), maa://29036 (100.00), *maa://42172 (55.42), maa://30285 (81.93), ***maa://65357 (25.30)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -10757,12 +10757,12 @@
       </c>
       <c r="C69" s="12" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D69" s="13" t="inlineStr">
         <is>
-          <t>maa://20974 (100.00), *maa://29079 (73.63), maa://29096 (86.81), maa://29087 (92.31), **maa://20823 (41.76), maa://20855 (80.22), maa://20904 (84.62)</t>
+          <t>maa://20974 (100.00), *maa://29079 (73.63), maa://29096 (86.81), maa://29087 (92.31), **maa://20823 (41.76), maa://20855 (80.22), maa://20904 (84.62), ***maa://63722 (23.08)</t>
         </is>
       </c>
       <c r="E69" s="14" t="inlineStr">
@@ -11788,7 +11788,7 @@
       </c>
       <c r="D88" s="13" t="inlineStr">
         <is>
-          <t>maa://24472 (100.00), **maa://35841 (48.24)</t>
+          <t>maa://24472 (100.00), **maa://35841 (47.67)</t>
         </is>
       </c>
       <c r="E88" s="14" t="inlineStr">
@@ -12868,7 +12868,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://25018 (97.94), maa://25776 (86.60), maa://28361 (86.60), maa://25772 (86.60), maa://56588 (82.47), *maa://45194 (67.01), *maa://25161 (62.89), *maa://32653 (63.92), ***maa://60902 (11.34), *maa://61839 (52.58), **maa://61275 (45.36)</t>
+          <t>maa://51881 (100.00), maa://25018 (97.94), maa://25776 (86.60), maa://28361 (86.60), maa://25772 (86.60), maa://56588 (83.51), *maa://45194 (67.01), *maa://25161 (62.89), *maa://32653 (63.92), ***maa://60902 (11.34), *maa://61839 (58.76), **maa://61275 (45.36)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13570,7 +13570,7 @@
       </c>
       <c r="D121" s="13" t="inlineStr">
         <is>
-          <t>maa://20869 (100.00), maa://44690 (81.44)</t>
+          <t>maa://20869 (100.00), maa://44690 (82.47)</t>
         </is>
       </c>
       <c r="E121" s="14" t="inlineStr">
@@ -14542,7 +14542,7 @@
       </c>
       <c r="D139" s="13" t="inlineStr">
         <is>
-          <t>**maa://30679 (44.93), maa://45258 (100.00)</t>
+          <t>maa://45258 (100.00), **maa://30679 (44.93)</t>
         </is>
       </c>
       <c r="E139" s="14" t="inlineStr">
@@ -15082,7 +15082,7 @@
       </c>
       <c r="D149" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.85), maa://36641 (100.00), maa://36865 (93.81), maa://44635 (83.51), maa://44660 (82.47), *maa://41128 (72.16), maa://42918 (92.78), maa://44119 (89.69), maa://46108 (88.66), *maa://37300 (58.76), **maa://42917 (35.05), *maa://64408 (62.89)</t>
+          <t>maa://40957 (95.88), maa://36641 (100.00), maa://36865 (93.81), maa://44635 (83.51), maa://44660 (82.47), *maa://41128 (72.16), maa://42918 (92.78), maa://44119 (89.69), maa://46108 (89.69), *maa://37300 (58.76), **maa://42917 (35.05), *maa://64408 (62.89)</t>
         </is>
       </c>
       <c r="E149" s="14" t="inlineStr">
@@ -17674,7 +17674,7 @@
       </c>
       <c r="D197" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (92.63), maa://35854 (83.16), maa://50388 (100.00), maa://25760 (83.16), ***maa://43911 (4.21), **maa://20872 (34.74), *maa://51066 (68.42), maa://63024 (86.32)</t>
+          <t>maa://44224 (91.58), maa://35854 (83.16), maa://50388 (100.00), maa://25760 (83.16), ***maa://43911 (4.21), **maa://20872 (34.74), *maa://51066 (68.42), maa://63024 (86.32)</t>
         </is>
       </c>
       <c r="E197" s="14" t="inlineStr">
@@ -19348,7 +19348,7 @@
       </c>
       <c r="D228" s="13" t="inlineStr">
         <is>
-          <t>maa://20987 (100.00), *maa://35801 (51.72)</t>
+          <t>maa://20987 (100.00), *maa://35801 (51.14)</t>
         </is>
       </c>
       <c r="E228" s="14" t="inlineStr">
@@ -20050,7 +20050,7 @@
       </c>
       <c r="D241" s="13" t="inlineStr">
         <is>
-          <t>maa://30667 (96.15), maa://30666 (100.00), **maa://30739 (35.90), *maa://30723 (57.69), maa://39588 (98.72), *maa://64079 (66.67)</t>
+          <t>maa://30667 (96.15), maa://30666 (100.00), **maa://30739 (35.90), *maa://30723 (57.69), maa://39588 (98.72), *maa://64079 (70.51)</t>
         </is>
       </c>
       <c r="E241" s="14" t="inlineStr">
@@ -20590,7 +20590,7 @@
       </c>
       <c r="D251" s="13" t="inlineStr">
         <is>
-          <t>maa://42287 (96.59), maa://45570 (100.00), *maa://60678 (77.27), maa://42225 (87.50)</t>
+          <t>maa://42287 (96.59), maa://45570 (100.00), *maa://60678 (79.55), maa://42225 (87.50)</t>
         </is>
       </c>
       <c r="E251" s="14" t="inlineStr">
@@ -20968,7 +20968,7 @@
       </c>
       <c r="D258" s="13" t="inlineStr">
         <is>
-          <t>maa://20879 (100.00), maa://20834 (88.46)</t>
+          <t>maa://20879 (100.00), maa://20834 (89.61)</t>
         </is>
       </c>
       <c r="E258" s="14" t="inlineStr">
@@ -21886,7 +21886,7 @@
       </c>
       <c r="D275" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://51630 (92.78), maa://56588 (82.47), **maa://55171 (40.21), *maa://51893 (61.86), ***maa://60902 (11.34)</t>
+          <t>maa://51881 (100.00), maa://51630 (92.78), maa://56588 (83.51), **maa://55171 (40.21), *maa://51893 (61.86), ***maa://60902 (11.34)</t>
         </is>
       </c>
       <c r="E275" s="14" t="inlineStr">
@@ -23560,7 +23560,7 @@
       </c>
       <c r="D306" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (100.00), maa://49642 (95.83), maa://49660 (83.33), **maa://50517 (39.58)</t>
+          <t>maa://50280 (100.00), maa://49642 (95.83), maa://49660 (84.38), **maa://50517 (45.83)</t>
         </is>
       </c>
       <c r="E306" s="14" t="inlineStr">
@@ -24586,7 +24586,7 @@
       </c>
       <c r="D325" s="13" t="inlineStr">
         <is>
-          <t>maa://39692 (100.00), *maa://39810 (71.72)</t>
+          <t>maa://39692 (100.00), *maa://39810 (72.73)</t>
         </is>
       </c>
       <c r="E325" s="14" t="inlineStr">
@@ -25828,7 +25828,7 @@
       </c>
       <c r="D348" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (100.00), maa://32415 (96.88), maa://34677 (96.88), maa://32892 (88.54), *maa://32653 (64.58), *maa://61839 (53.12), **maa://61275 (45.83)</t>
+          <t>maa://32647 (100.00), maa://32415 (96.88), maa://34677 (96.88), maa://32892 (88.54), *maa://32653 (64.58), *maa://61839 (59.38), **maa://61275 (45.83)</t>
         </is>
       </c>
       <c r="E348" s="22" t="inlineStr">
@@ -26530,7 +26530,7 @@
       </c>
       <c r="D361" s="22" t="inlineStr">
         <is>
-          <t>maa://49648 (100.00), *maa://49662 (72.41)</t>
+          <t>maa://49648 (100.00), *maa://49662 (73.56)</t>
         </is>
       </c>
       <c r="E361" s="22" t="inlineStr">
@@ -26854,7 +26854,7 @@
       </c>
       <c r="D367" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (100.00), maa://48026 (95.65), maa://44635 (88.04), maa://41035 (92.39), maa://44660 (86.96), *maa://41128 (76.09), *maa://60251 (55.43)</t>
+          <t>maa://40957 (100.00), maa://48026 (95.70), maa://44635 (87.10), maa://41035 (91.40), maa://44660 (86.02), *maa://60251 (54.84), *maa://41128 (75.27)</t>
         </is>
       </c>
       <c r="E367" s="22" t="inlineStr">
@@ -26962,7 +26962,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://63883 (100.00), *maa://64045 (75.00), **maa://64041 (30.88)</t>
+          <t>maa://63883 (100.00), maa://64045 (87.14), ***maa://64041 (30.00)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -27772,7 +27772,7 @@
       </c>
       <c r="D384" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (81.91), maa://44745 (100.00), ***maa://49516 (24.47), **maa://45952 (38.30), ***maa://46851 (3.19), **maa://44896 (47.87)</t>
+          <t>maa://42970 (81.91), maa://44745 (100.00), ***maa://49516 (27.66), **maa://45952 (38.30), ***maa://46851 (2.13), **maa://44896 (47.87)</t>
         </is>
       </c>
       <c r="E384" s="22" t="inlineStr">
@@ -28285,7 +28285,7 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>maa://59533 (100.00), *maa://59577 (80.00)</t>
+          <t>maa://59533 (100.00), *maa://59577 (79.12)</t>
         </is>
       </c>
       <c r="E394" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#227)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://39402 (100.00), *maa://34787 (73.86), maa://58660 (88.64)</t>
+          <t>maa://39402 (100.00), *maa://34787 (73.86), maa://58660 (89.77)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (100.00), maa://50121 (97.73)</t>
+          <t>maa://49983 (100.00), maa://50121 (96.63)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (98.75), maa://54105 (100.00), *maa://22744 (80.00)</t>
+          <t>maa://21245 (100.00), maa://54105 (97.47), maa://22744 (81.01)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.17 13:21:11</t>
+          <t>更新日期：2025.08.18 13:25:38</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (100.00), maa://40166 (97.56)</t>
+          <t>maa://28711 (100.00), maa://40166 (98.78)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (100.00), maa://22755 (87.23), *maa://63521 (54.26)</t>
+          <t>maa://27395 (100.00), maa://22755 (87.23), **maa://63521 (50.00)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (90.43), maa://22501 (100.00), maa://45521 (88.30)</t>
+          <t>maa://22747 (89.47), maa://22501 (100.00), maa://45521 (87.37)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (90.00), maa://64046 (100.00)</t>
+          <t>maa://63896 (90.11), maa://64046 (100.00)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://22753 (100.00), maa://37962 (93.18), *maa://21485 (78.41)</t>
+          <t>maa://22753 (100.00), maa://37962 (94.32), *maa://21485 (78.41)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://22430 (100.00), maa://39599 (95.29)</t>
+          <t>maa://22430 (100.00), maa://39599 (96.47)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (100.00), *maa://29748 (77.27), *maa://37566 (75.00)</t>
+          <t>maa://30587 (100.00), *maa://29748 (77.27), *maa://37566 (76.14)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (100.00), *maa://63016 (65.59)</t>
+          <t>maa://29753 (100.00), *maa://63016 (73.12)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://24080 (90.14), maa://42865 (100.00), ***maa://34960 (2.82)</t>
+          <t>maa://24080 (88.89), maa://42865 (100.00), ***maa://34960 (2.78)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (100.00), maa://36258 (93.33), *maa://43904 (56.67)</t>
+          <t>maa://35926 (100.00), maa://36258 (92.31), *maa://43904 (56.04)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (100.00), *maa://56235 (61.96)</t>
+          <t>maa://48817 (100.00), *maa://56235 (66.30)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (100.00), *maa://47069 (59.79), *maa://56336 (65.98), *maa://45789 (67.01)</t>
+          <t>maa://45718 (100.00), *maa://47069 (59.79), *maa://56336 (69.07), *maa://45789 (67.01)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5636,7 +5636,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (100.00), maa://21386 (100.00), maa://36664 (83.70), **maa://45550 (48.91)</t>
+          <t>maa://23278 (100.00), maa://21386 (98.92), maa://36664 (83.87), **maa://45550 (48.39)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>*maa://64107 (65.28), maa://64205 (100.00), **maa://65283 (47.22)</t>
+          <t>*maa://64107 (66.67), maa://64205 (100.00), **maa://65283 (47.22)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -6077,7 +6077,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://21229 (90.80), maa://30807 (100.00), maa://42459 (88.51)</t>
+          <t>maa://21229 (90.80), maa://30807 (100.00), maa://42459 (89.66)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6146,7 +6146,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (100.00), maa://43901 (94.38)</t>
+          <t>maa://35931 (100.00), maa://43901 (95.51)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6215,7 +6215,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (100.00), maa://29661 (98.95), *maa://28038 (61.05), *maa://56236 (68.42)</t>
+          <t>maa://27410 (100.00), maa://29661 (98.95), *maa://28038 (61.05), *maa://56236 (73.68)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6485,12 +6485,12 @@
       </c>
       <c r="O52" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (100.00), maa://59378 (91.49)</t>
+          <t>maa://59394 (100.00), maa://59378 (91.49), ***maa://65511 (22.34)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6768,7 +6768,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (100.00), **maa://59693 (47.87), *maa://59413 (69.15)</t>
+          <t>maa://59534 (100.00), *maa://59693 (52.13), *maa://59413 (69.15)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7090,7 +7090,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.17 13:21:11</t>
+          <t>更新日期：2025.08.18 13:25:38</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8494,7 +8494,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (71.08), *maa://28758 (67.47), maa://29036 (100.00), *maa://42172 (55.42), maa://30285 (81.93), ***maa://65357 (25.30)</t>
+          <t>*maa://20849 (71.08), *maa://28758 (67.47), maa://29036 (100.00), *maa://42172 (55.42), maa://30285 (81.93), *maa://65357 (61.45)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8764,7 +8764,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (94.38), maa://36866 (100.00), *maa://45572 (71.91), maa://62759 (92.13), *maa://27794 (64.04), *maa://20960 (78.65), **maa://20843 (49.44), ***maa://24483 (10.11), **maa://20862 (49.44), *maa://20893 (61.80)</t>
+          <t>maa://36644 (94.38), maa://36866 (100.00), maa://62759 (92.13), *maa://45572 (71.91), *maa://27794 (64.04), *maa://20960 (78.65), **maa://20843 (49.44), ***maa://24483 (10.11), **maa://20862 (49.44), *maa://20893 (61.80)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -9898,7 +9898,7 @@
       </c>
       <c r="D53" s="13" t="inlineStr">
         <is>
-          <t>maa://20953 (100.00), maa://31173 (96.43)</t>
+          <t>maa://20953 (100.00), maa://31173 (95.29)</t>
         </is>
       </c>
       <c r="E53" s="14" t="inlineStr">
@@ -10487,12 +10487,12 @@
       </c>
       <c r="C64" s="12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D64" s="13" t="inlineStr">
         <is>
-          <t>maa://28187 (92.63), maa://45144 (100.00), maa://33504 (94.74), **maa://43531 (35.79)</t>
+          <t>maa://28187 (92.63), maa://45144 (100.00), maa://33504 (94.74), **maa://43531 (35.79), ***maa://65290 (22.11)</t>
         </is>
       </c>
       <c r="E64" s="14" t="inlineStr">
@@ -10870,7 +10870,7 @@
       </c>
       <c r="D71" s="13" t="inlineStr">
         <is>
-          <t>maa://20943 (100.00), *maa://30673 (73.47), *maa://30672 (66.33), maa://63790 (83.67), maa://20856 (82.65)</t>
+          <t>maa://20943 (100.00), *maa://30673 (73.47), *maa://30672 (66.33), maa://63790 (86.73), maa://20856 (82.65)</t>
         </is>
       </c>
       <c r="E71" s="14" t="inlineStr">
@@ -11788,7 +11788,7 @@
       </c>
       <c r="D88" s="13" t="inlineStr">
         <is>
-          <t>maa://24472 (100.00), **maa://35841 (47.67)</t>
+          <t>maa://24472 (100.00), **maa://35841 (50.00)</t>
         </is>
       </c>
       <c r="E88" s="14" t="inlineStr">
@@ -12274,7 +12274,7 @@
       </c>
       <c r="D97" s="13" t="inlineStr">
         <is>
-          <t>maa://20991 (100.00), *maa://51015 (74.23)</t>
+          <t>maa://20991 (100.00), *maa://51015 (75.26)</t>
         </is>
       </c>
       <c r="E97" s="14" t="inlineStr">
@@ -12598,7 +12598,7 @@
       </c>
       <c r="D103" s="13" t="inlineStr">
         <is>
-          <t>maa://29094 (80.26), maa://28904 (100.00), **maa://20931 (39.47)</t>
+          <t>maa://29094 (81.58), maa://28904 (100.00), **maa://20931 (39.47)</t>
         </is>
       </c>
       <c r="E103" s="14" t="inlineStr">
@@ -12868,7 +12868,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://25018 (97.94), maa://25776 (86.60), maa://28361 (86.60), maa://25772 (86.60), maa://56588 (83.51), *maa://45194 (67.01), *maa://25161 (62.89), *maa://32653 (63.92), ***maa://60902 (11.34), *maa://61839 (58.76), **maa://61275 (45.36)</t>
+          <t>maa://51881 (100.00), maa://25018 (97.94), maa://25776 (86.60), maa://28361 (86.60), maa://25772 (86.60), maa://56588 (83.51), *maa://45194 (67.01), *maa://25161 (62.89), *maa://32653 (63.92), ***maa://60902 (11.34), *maa://61839 (62.89), **maa://61275 (45.36)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13300,7 +13300,7 @@
       </c>
       <c r="D116" s="13" t="inlineStr">
         <is>
-          <t>maa://29659 (97.30), maa://29031 (100.00)</t>
+          <t>maa://29659 (96.00), maa://29031 (100.00)</t>
         </is>
       </c>
       <c r="E116" s="14" t="inlineStr">
@@ -13354,7 +13354,7 @@
       </c>
       <c r="D117" s="13" t="inlineStr">
         <is>
-          <t>maa://31560 (100.00), maa://20940 (92.54)</t>
+          <t>maa://31560 (100.00), maa://20940 (89.86)</t>
         </is>
       </c>
       <c r="E117" s="14" t="inlineStr">
@@ -13462,7 +13462,7 @@
       </c>
       <c r="D119" s="13" t="inlineStr">
         <is>
-          <t>maa://31560 (100.00), *maa://20851 (65.67)</t>
+          <t>maa://31560 (100.00), *maa://20851 (63.77)</t>
         </is>
       </c>
       <c r="E119" s="14" t="inlineStr">
@@ -14704,7 +14704,7 @@
       </c>
       <c r="D142" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (100.00), **maa://23736 (35.11), *maa://31185 (56.38), *maa://30306 (54.26)</t>
+          <t>maa://28484 (100.00), **maa://23736 (35.11), *maa://31185 (63.83), *maa://30306 (54.26)</t>
         </is>
       </c>
       <c r="E142" s="14" t="inlineStr">
@@ -14758,7 +14758,7 @@
       </c>
       <c r="D143" s="13" t="inlineStr">
         <is>
-          <t>maa://30670 (100.00), maa://31470 (89.25), **maa://45066 (38.71), **maa://61380 (36.56), ***maa://30867 (12.90)</t>
+          <t>maa://30670 (100.00), maa://31470 (89.25), **maa://45066 (38.71), **maa://61380 (47.31), ***maa://30867 (12.90)</t>
         </is>
       </c>
       <c r="E143" s="14" t="inlineStr">
@@ -16054,7 +16054,7 @@
       </c>
       <c r="D167" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (100.00), maa://29627 (100.00), maa://29659 (80.90), maa://49074 (98.88), **maa://30679 (34.83), maa://29861 (87.64), *maa://42343 (78.65)</t>
+          <t>maa://29633 (100.00), maa://29627 (100.00), maa://29659 (80.90), maa://49074 (100.00), **maa://30679 (34.83), maa://29861 (87.64), *maa://42343 (78.65)</t>
         </is>
       </c>
       <c r="E167" s="14" t="inlineStr">
@@ -16108,7 +16108,7 @@
       </c>
       <c r="D168" s="13" t="inlineStr">
         <is>
-          <t>maa://49867 (92.94), maa://49655 (100.00)</t>
+          <t>maa://49867 (95.35), maa://49655 (100.00)</t>
         </is>
       </c>
       <c r="E168" s="14" t="inlineStr">
@@ -16486,7 +16486,7 @@
       </c>
       <c r="D175" s="13" t="inlineStr">
         <is>
-          <t>maa://32418 (100.00), maa://51440 (89.90), maa://63320 (86.87)</t>
+          <t>maa://32418 (100.00), maa://51440 (89.90), maa://63320 (87.88)</t>
         </is>
       </c>
       <c r="E175" s="14" t="inlineStr">
@@ -16864,7 +16864,7 @@
       </c>
       <c r="D182" s="13" t="inlineStr">
         <is>
-          <t>maa://31560 (100.00), **maa://20968 (31.34)</t>
+          <t>maa://31560 (100.00), **maa://20968 (30.43)</t>
         </is>
       </c>
       <c r="E182" s="14" t="inlineStr">
@@ -17674,7 +17674,7 @@
       </c>
       <c r="D197" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (91.58), maa://35854 (83.16), maa://50388 (100.00), maa://25760 (83.16), ***maa://43911 (4.21), **maa://20872 (34.74), *maa://51066 (68.42), maa://63024 (86.32)</t>
+          <t>maa://44224 (91.58), maa://35854 (83.16), maa://50388 (100.00), maa://25760 (83.16), ***maa://43911 (4.21), **maa://20872 (34.74), *maa://51066 (68.42), maa://63024 (87.37)</t>
         </is>
       </c>
       <c r="E197" s="14" t="inlineStr">
@@ -20050,7 +20050,7 @@
       </c>
       <c r="D241" s="13" t="inlineStr">
         <is>
-          <t>maa://30667 (96.15), maa://30666 (100.00), **maa://30739 (35.90), *maa://30723 (57.69), maa://39588 (98.72), *maa://64079 (70.51)</t>
+          <t>maa://30667 (96.15), maa://30666 (100.00), **maa://30739 (35.90), *maa://30723 (57.69), maa://39588 (98.72), *maa://64079 (79.49)</t>
         </is>
       </c>
       <c r="E241" s="14" t="inlineStr">
@@ -20590,7 +20590,7 @@
       </c>
       <c r="D251" s="13" t="inlineStr">
         <is>
-          <t>maa://42287 (96.59), maa://45570 (100.00), *maa://60678 (79.55), maa://42225 (87.50)</t>
+          <t>maa://42287 (96.59), maa://45570 (100.00), maa://60678 (81.82), maa://42225 (87.50)</t>
         </is>
       </c>
       <c r="E251" s="14" t="inlineStr">
@@ -21130,7 +21130,7 @@
       </c>
       <c r="D261" s="13" t="inlineStr">
         <is>
-          <t>maa://31560 (81.71), maa://20884 (100.00)</t>
+          <t>maa://31560 (84.15), maa://20884 (100.00)</t>
         </is>
       </c>
       <c r="E261" s="14" t="inlineStr">
@@ -23344,7 +23344,7 @@
       </c>
       <c r="D302" s="13" t="inlineStr">
         <is>
-          <t>maa://29005 (100.00), *maa://31560 (72.04)</t>
+          <t>maa://29005 (100.00), *maa://31560 (74.19)</t>
         </is>
       </c>
       <c r="E302" s="14" t="inlineStr">
@@ -23560,7 +23560,7 @@
       </c>
       <c r="D306" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (100.00), maa://49642 (95.83), maa://49660 (84.38), **maa://50517 (45.83)</t>
+          <t>maa://50280 (100.00), maa://49642 (95.83), maa://49660 (84.38), *maa://50517 (51.04)</t>
         </is>
       </c>
       <c r="E306" s="14" t="inlineStr">
@@ -25828,7 +25828,7 @@
       </c>
       <c r="D348" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (100.00), maa://32415 (96.88), maa://34677 (96.88), maa://32892 (88.54), *maa://32653 (64.58), *maa://61839 (59.38), **maa://61275 (45.83)</t>
+          <t>maa://32647 (100.00), maa://32415 (96.88), maa://34677 (96.88), maa://32892 (88.54), *maa://32653 (64.58), *maa://61839 (63.54), **maa://61275 (45.83)</t>
         </is>
       </c>
       <c r="E348" s="22" t="inlineStr">
@@ -26368,7 +26368,7 @@
       </c>
       <c r="D358" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.00), maa://49695 (100.00), maa://49758 (92.00), **maa://59402 (39.00), **maa://52357 (48.00), ***maa://63091 (19.00)</t>
+          <t>maa://49696 (99.00), maa://49695 (100.00), maa://49758 (92.00), **maa://59402 (39.00), **maa://52357 (48.00), ***maa://63091 (25.00)</t>
         </is>
       </c>
       <c r="E358" s="22" t="inlineStr">
@@ -26530,7 +26530,7 @@
       </c>
       <c r="D361" s="22" t="inlineStr">
         <is>
-          <t>maa://49648 (100.00), *maa://49662 (73.56)</t>
+          <t>maa://49648 (100.00), *maa://49662 (73.86)</t>
         </is>
       </c>
       <c r="E361" s="22" t="inlineStr">
@@ -26962,7 +26962,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://63883 (100.00), maa://64045 (87.14), ***maa://64041 (30.00)</t>
+          <t>maa://63883 (100.00), maa://64045 (90.28), ***maa://64041 (29.17)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -27772,7 +27772,7 @@
       </c>
       <c r="D384" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (81.91), maa://44745 (100.00), ***maa://49516 (27.66), **maa://45952 (38.30), ***maa://46851 (2.13), **maa://44896 (47.87)</t>
+          <t>maa://42970 (81.91), maa://44745 (100.00), ***maa://49516 (26.60), **maa://45952 (38.30), ***maa://46851 (2.13), **maa://44896 (47.87)</t>
         </is>
       </c>
       <c r="E384" s="22" t="inlineStr">
@@ -28420,7 +28420,7 @@
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>maa://51872 (100.00), maa://51876 (98.95), *maa://63228 (73.68), maa://51873 (96.84), *maa://62047 (74.74)</t>
+          <t>maa://51872 (100.00), maa://51876 (98.95), *maa://63228 (74.74), maa://51873 (96.84), *maa://62047 (74.74)</t>
         </is>
       </c>
       <c r="E399" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#228)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://25251 (100.00), maa://59087 (96.51)</t>
+          <t>maa://25251 (100.00), maa://59087 (97.67)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://45854 (85.88), maa://24617 (100.00), *maa://60545 (76.47)</t>
+          <t>maa://45854 (85.88), maa://24617 (100.00), maa://60545 (82.35)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://24390 (100.00), maa://52241 (88.89)</t>
+          <t>maa://24390 (100.00), maa://52241 (91.11)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://32509 (100.00), maa://27295 (91.01), maa://22754 (89.89), *maa://31008 (73.03)</t>
+          <t>maa://32509 (100.00), maa://27295 (92.13), maa://22754 (89.89), *maa://31008 (73.03)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>maa://30062 (100.00), maa://39394 (100.00), ***maa://26209 (9.80)</t>
+          <t>maa://30062 (96.23), maa://39394 (100.00), ***maa://26209 (9.43)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (100.00), maa://54105 (97.47), maa://22744 (81.01)</t>
+          <t>maa://21245 (100.00), maa://54105 (98.73), maa://22744 (81.01)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.18 13:25:38</t>
+          <t>更新日期：2025.08.22 13:21:00</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (100.00), *maa://39431 (60.00), **maa://37551 (33.85)</t>
+          <t>maa://21476 (100.00), *maa://39431 (54.55), **maa://37551 (33.33)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (87.50), maa://23252 (94.32), maa://37496 (100.00)</t>
+          <t>maa://32931 (86.52), maa://23252 (93.26), maa://37496 (100.00)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://26223 (100.00), maa://52237 (84.21)</t>
+          <t>maa://26223 (100.00), maa://52237 (85.26)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (100.00), maa://40166 (98.78)</t>
+          <t>maa://28711 (100.00), maa://40166 (97.56)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (100.00), maa://22755 (87.23), **maa://63521 (50.00)</t>
+          <t>maa://27395 (100.00), maa://22755 (87.23), *maa://63521 (51.06)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>maa://25021 (84.31), maa://22733 (100.00), ***maa://22761 (17.65)</t>
+          <t>maa://25021 (82.69), maa://22733 (100.00), ***maa://22761 (17.31)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (89.47), maa://22501 (100.00), maa://45521 (87.37)</t>
+          <t>maa://22747 (89.47), maa://22501 (100.00), maa://45521 (88.42)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (90.11), maa://64046 (100.00)</t>
+          <t>maa://63896 (93.26), maa://64046 (100.00)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://23669 (100.00), maa://36677 (95.70), maa://39872 (88.17)</t>
+          <t>maa://23669 (100.00), maa://36677 (96.74), maa://39872 (89.13)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (100.00), *maa://22583 (77.78), *maa://48321 (61.11)</t>
+          <t>maa://22676 (100.00), *maa://22583 (78.89), *maa://48321 (61.11)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://22521 (100.00), maa://42751 (93.26)</t>
+          <t>maa://22521 (100.00), maa://42751 (94.38)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (96.10), maa://22734 (100.00), *maa://30808 (66.23), maa://36048 (84.42), maa://45058 (83.12)</t>
+          <t>maa://22743 (96.10), maa://22734 (100.00), *maa://30808 (66.23), maa://36048 (84.42), maa://45058 (84.42)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2492,7 +2492,7 @@
       </c>
       <c r="X15" s="8" t="inlineStr">
         <is>
-          <t>maa://38786 (84.31), maa://56102 (100.00)</t>
+          <t>maa://38786 (92.16), maa://56102 (100.00)</t>
         </is>
       </c>
       <c r="Y15" s="19" t="n"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://22729 (100.00), *maa://28648 (73.33), *maa://36674 (77.78)</t>
+          <t>maa://22729 (100.00), *maa://28648 (73.33), *maa://36674 (78.89)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://22466 (98.88), maa://52226 (100.00)</t>
+          <t>maa://22466 (97.78), maa://52226 (100.00)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), maa://54153 (85.11), *maa://24380 (69.15)</t>
+          <t>maa://24379 (100.00), maa://54153 (86.17), *maa://24380 (69.15)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://24313 (89.83), maa://47854 (100.00), *maa://29784 (55.93)</t>
+          <t>maa://24313 (88.33), maa://47854 (100.00), *maa://29784 (55.00)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -3007,12 +3007,12 @@
       </c>
       <c r="W19" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="X19" s="8" t="inlineStr">
         <is>
-          <t>maa://31386 (100.00)</t>
+          <t>maa://31386 (100.00), **maa://58490 (35.29)</t>
         </is>
       </c>
       <c r="Y19" s="19" t="n"/>
@@ -3044,7 +3044,7 @@
       </c>
       <c r="AF19" s="8" t="inlineStr">
         <is>
-          <t>maa://21663 (100.00), *maa://52239 (56.60)</t>
+          <t>maa://21663 (100.00), *maa://52239 (71.70)</t>
         </is>
       </c>
       <c r="AG19" s="16" t="n"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://21432 (98.86), maa://25198 (100.00), maa://36680 (88.64)</t>
+          <t>maa://21432 (97.75), maa://25198 (100.00), maa://36680 (87.64)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (100.00), maa://49976 (95.29), *maa://56241 (75.29)</t>
+          <t>maa://50085 (100.00), maa://49976 (95.29), *maa://56241 (76.47)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (100.00), maa://20110 (89.41)</t>
+          <t>maa://34946 (100.00), maa://20110 (88.37)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22524 (100.00), maa://22432 (97.50), **maa://64221 (38.75)</t>
+          <t>maa://22524 (100.00), maa://22432 (98.75), **maa://64221 (50.00)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://21282 (100.00), *maa://37649 (62.89)</t>
+          <t>maa://21282 (100.00), *maa://37649 (63.92)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (100.00), *maa://46650 (71.05)</t>
+          <t>maa://24368 (100.00), *maa://46650 (72.37)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://22523 (87.21), *maa://36672 (69.77), maa://29910 (100.00), maa://45831 (84.88), *maa://64165 (70.93)</t>
+          <t>maa://22523 (87.21), *maa://36672 (69.77), maa://29910 (100.00), maa://45831 (84.88), maa://64165 (81.40)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (100.00), *maa://63016 (73.12)</t>
+          <t>maa://29753 (100.00), *maa://63016 (75.27)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>maa://29063 (95.38), maa://25311 (100.00), ***maa://22725 (3.08), maa://45047 (81.54)</t>
+          <t>maa://29063 (93.94), maa://25311 (100.00), ***maa://22725 (3.03), maa://45047 (80.30)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://41802 (100.00), maa://56374 (81.25)</t>
+          <t>maa://41802 (100.00), maa://56374 (80.25)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="P26" s="8" t="inlineStr">
         <is>
-          <t>maa://39870 (100.00), maa://56625 (88.41)</t>
+          <t>maa://39870 (100.00), maa://56625 (94.20)</t>
         </is>
       </c>
       <c r="Q26" s="19" t="n"/>
@@ -4209,12 +4209,12 @@
       </c>
       <c r="AE28" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (100.00)</t>
+          <t>maa://36660 (100.00), ***maa://65700 (23.33)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (100.00), **maa://64191 (44.16)</t>
+          <t>maa://45792 (100.00), *maa://64191 (57.14)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://21895 (100.00), maa://36667 (98.95), **maa://22760 (35.79)</t>
+          <t>maa://36667 (98.95), maa://21895 (100.00), **maa://22760 (35.79)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (100.00), *maa://56235 (66.30)</t>
+          <t>maa://48817 (100.00), *maa://56235 (70.65)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (100.00), *maa://47069 (59.79), *maa://56336 (69.07), *maa://45789 (67.01)</t>
+          <t>maa://45718 (100.00), *maa://47069 (59.79), *maa://56336 (68.04), *maa://45789 (67.01)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5636,7 +5636,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (100.00), maa://21386 (98.92), maa://36664 (83.87), **maa://45550 (48.39)</t>
+          <t>maa://23278 (100.00), maa://21386 (98.92), maa://36664 (83.87), *maa://45550 (52.69)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5679,12 +5679,12 @@
       </c>
       <c r="AE40" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>*maa://64107 (66.67), maa://64205 (100.00), **maa://65283 (47.22)</t>
+          <t>maa://64205 (100.00), *maa://65283 (71.25)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>maa://22525 (88.75), maa://21284 (100.00)</t>
+          <t>maa://22525 (86.42), maa://21284 (100.00)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -5992,7 +5992,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (100.00), maa://27728 (95.79), *maa://56386 (75.79)</t>
+          <t>maa://29768 (100.00), maa://27728 (95.79), *maa://56386 (77.89)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6215,7 +6215,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (100.00), maa://29661 (98.95), *maa://28038 (61.05), *maa://56236 (73.68)</t>
+          <t>maa://27410 (100.00), maa://29661 (98.95), *maa://28038 (61.05), *maa://56236 (75.79)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6490,7 +6490,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (100.00), maa://59378 (91.49), ***maa://65511 (22.34)</t>
+          <t>maa://59394 (100.00), maa://59378 (91.49), **maa://65511 (46.81)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6660,7 +6660,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://25176 (100.00), *maa://56237 (75.27)</t>
+          <t>maa://25176 (100.00), *maa://56237 (77.42)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6750,7 +6750,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (100.00), maa://43903 (89.89), *maa://56228 (64.04)</t>
+          <t>maa://42981 (100.00), maa://43903 (89.89), *maa://56228 (73.03)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6768,7 +6768,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (100.00), *maa://59693 (52.13), *maa://59413 (69.15)</t>
+          <t>maa://59534 (100.00), *maa://59693 (61.70), *maa://59413 (72.34)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7090,7 +7090,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.18 13:25:38</t>
+          <t>更新日期：2025.08.22 13:21:00</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8278,7 +8278,7 @@
       </c>
       <c r="D23" s="13" t="inlineStr">
         <is>
-          <t>maa://20876 (100.00), *maa://63498 (58.62)</t>
+          <t>maa://20876 (100.00), *maa://63498 (65.52)</t>
         </is>
       </c>
       <c r="E23" s="14" t="inlineStr">
@@ -8494,7 +8494,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (71.08), *maa://28758 (67.47), maa://29036 (100.00), *maa://42172 (55.42), maa://30285 (81.93), *maa://65357 (61.45)</t>
+          <t>*maa://20849 (72.29), *maa://28758 (67.47), maa://29036 (100.00), *maa://42172 (55.42), maa://30285 (81.93), *maa://65357 (78.31)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8764,7 +8764,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (94.38), maa://36866 (100.00), maa://62759 (92.13), *maa://45572 (71.91), *maa://27794 (64.04), *maa://20960 (78.65), **maa://20843 (49.44), ***maa://24483 (10.11), **maa://20862 (49.44), *maa://20893 (61.80)</t>
+          <t>maa://36644 (95.51), maa://36866 (100.00), maa://62759 (96.63), *maa://45572 (74.16), *maa://27794 (64.04), *maa://20960 (78.65), **maa://20843 (49.44), ***maa://24483 (10.11), **maa://20862 (49.44), *maa://20893 (61.80)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -10222,7 +10222,7 @@
       </c>
       <c r="D59" s="13" t="inlineStr">
         <is>
-          <t>maa://27970 (100.00), *maa://41118 (52.69)</t>
+          <t>maa://27970 (100.00), *maa://41118 (56.38)</t>
         </is>
       </c>
       <c r="E59" s="14" t="inlineStr">
@@ -10330,7 +10330,7 @@
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (100.00), maa://24093 (100.00), maa://31559 (89.47), maa://20924 (81.05), *maa://25777 (60.00), *maa://20631 (60.00), **maa://28241 (46.32)</t>
+          <t>maa://20841 (100.00), maa://24093 (100.00), maa://31559 (89.47), maa://20924 (81.05), *maa://25777 (64.21), *maa://20631 (60.00), **maa://28241 (46.32)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -10762,7 +10762,7 @@
       </c>
       <c r="D69" s="13" t="inlineStr">
         <is>
-          <t>maa://20974 (100.00), *maa://29079 (73.63), maa://29096 (86.81), maa://29087 (92.31), **maa://20823 (41.76), maa://20855 (80.22), maa://20904 (84.62), ***maa://63722 (23.08)</t>
+          <t>maa://20974 (100.00), *maa://29079 (73.63), maa://29096 (86.81), maa://29087 (92.31), **maa://20823 (48.35), maa://20855 (80.22), maa://20904 (84.62), **maa://63722 (48.35)</t>
         </is>
       </c>
       <c r="E69" s="14" t="inlineStr">
@@ -10870,7 +10870,7 @@
       </c>
       <c r="D71" s="13" t="inlineStr">
         <is>
-          <t>maa://20943 (100.00), *maa://30673 (73.47), *maa://30672 (66.33), maa://63790 (86.73), maa://20856 (82.65)</t>
+          <t>maa://20943 (100.00), *maa://30673 (73.47), maa://63790 (89.80), *maa://30672 (66.33), maa://20856 (82.65)</t>
         </is>
       </c>
       <c r="E71" s="14" t="inlineStr">
@@ -11518,7 +11518,7 @@
       </c>
       <c r="D83" s="13" t="inlineStr">
         <is>
-          <t>maa://45572 (91.43), maa://27794 (81.43), maa://20960 (100.00)</t>
+          <t>maa://45572 (94.29), maa://27794 (81.43), maa://20960 (100.00)</t>
         </is>
       </c>
       <c r="E83" s="14" t="inlineStr">
@@ -11734,7 +11734,7 @@
       </c>
       <c r="D87" s="13" t="inlineStr">
         <is>
-          <t>maa://20886 (100.00), ***maa://60772 (26.25)</t>
+          <t>maa://20886 (100.00), ***maa://60772 (25.93)</t>
         </is>
       </c>
       <c r="E87" s="14" t="inlineStr">
@@ -12490,7 +12490,7 @@
       </c>
       <c r="D101" s="13" t="inlineStr">
         <is>
-          <t>maa://45572 (100.00), maa://27794 (89.06), maa://20893 (85.94)</t>
+          <t>maa://45572 (100.00), maa://27794 (86.36), maa://20893 (83.33)</t>
         </is>
       </c>
       <c r="E101" s="14" t="inlineStr">
@@ -12598,7 +12598,7 @@
       </c>
       <c r="D103" s="13" t="inlineStr">
         <is>
-          <t>maa://29094 (81.58), maa://28904 (100.00), **maa://20931 (39.47)</t>
+          <t>maa://29094 (80.52), maa://28904 (100.00), **maa://20931 (38.96)</t>
         </is>
       </c>
       <c r="E103" s="14" t="inlineStr">
@@ -12760,7 +12760,7 @@
       </c>
       <c r="D106" s="13" t="inlineStr">
         <is>
-          <t>maa://45572 (100.00), maa://27794 (89.06), *maa://20843 (68.75), ***maa://24483 (14.06)</t>
+          <t>maa://45572 (100.00), maa://27794 (86.36), *maa://20843 (66.67), ***maa://24483 (13.64)</t>
         </is>
       </c>
       <c r="E106" s="14" t="inlineStr">
@@ -12868,7 +12868,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://25018 (97.94), maa://25776 (86.60), maa://28361 (86.60), maa://25772 (86.60), maa://56588 (83.51), *maa://45194 (67.01), *maa://25161 (62.89), *maa://32653 (63.92), ***maa://60902 (11.34), *maa://61839 (62.89), **maa://61275 (45.36)</t>
+          <t>maa://51881 (100.00), maa://25018 (96.94), maa://25776 (85.71), maa://28361 (85.71), maa://25772 (85.71), maa://56588 (83.67), *maa://45194 (66.33), *maa://25161 (62.24), *maa://32653 (63.27), ***maa://60902 (15.31), *maa://61839 (66.33), *maa://61275 (52.04)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13300,7 +13300,7 @@
       </c>
       <c r="D116" s="13" t="inlineStr">
         <is>
-          <t>maa://29659 (96.00), maa://29031 (100.00)</t>
+          <t>maa://29659 (96.05), maa://29031 (100.00)</t>
         </is>
       </c>
       <c r="E116" s="14" t="inlineStr">
@@ -13570,7 +13570,7 @@
       </c>
       <c r="D121" s="13" t="inlineStr">
         <is>
-          <t>maa://20869 (100.00), maa://44690 (82.47)</t>
+          <t>maa://20869 (100.00), maa://44690 (83.51)</t>
         </is>
       </c>
       <c r="E121" s="14" t="inlineStr">
@@ -14704,7 +14704,7 @@
       </c>
       <c r="D142" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (100.00), **maa://23736 (35.11), *maa://31185 (63.83), *maa://30306 (54.26)</t>
+          <t>maa://28484 (100.00), **maa://23736 (40.43), *maa://31185 (63.83), *maa://30306 (54.26)</t>
         </is>
       </c>
       <c r="E142" s="14" t="inlineStr">
@@ -14758,7 +14758,7 @@
       </c>
       <c r="D143" s="13" t="inlineStr">
         <is>
-          <t>maa://30670 (100.00), maa://31470 (89.25), **maa://45066 (38.71), **maa://61380 (47.31), ***maa://30867 (12.90)</t>
+          <t>maa://30670 (100.00), maa://31470 (89.25), **maa://45066 (38.71), *maa://61380 (61.29), ***maa://30867 (12.90)</t>
         </is>
       </c>
       <c r="E143" s="14" t="inlineStr">
@@ -15082,7 +15082,7 @@
       </c>
       <c r="D149" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (95.88), maa://36641 (100.00), maa://36865 (93.81), maa://44635 (83.51), maa://44660 (82.47), *maa://41128 (72.16), maa://42918 (92.78), maa://44119 (89.69), maa://46108 (89.69), *maa://37300 (58.76), **maa://42917 (35.05), *maa://64408 (62.89)</t>
+          <t>maa://40957 (95.88), maa://36641 (100.00), maa://36865 (93.81), maa://44635 (83.51), maa://44660 (83.51), *maa://41128 (72.16), maa://42918 (92.78), maa://44119 (89.69), maa://46108 (89.69), *maa://37300 (58.76), *maa://64408 (70.10), **maa://42917 (35.05)</t>
         </is>
       </c>
       <c r="E149" s="14" t="inlineStr">
@@ -15136,7 +15136,7 @@
       </c>
       <c r="D150" s="13" t="inlineStr">
         <is>
-          <t>maa://51549 (100.00), maa://51923 (90.91)</t>
+          <t>maa://51549 (100.00), maa://51923 (92.05)</t>
         </is>
       </c>
       <c r="E150" s="14" t="inlineStr">
@@ -15617,12 +15617,12 @@
       </c>
       <c r="C159" s="12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D159" s="13" t="inlineStr">
         <is>
-          <t>maa://44232 (100.00), *maa://45603 (78.35)</t>
+          <t>maa://44232 (100.00), *maa://45603 (78.35), ***maa://63114 (9.28)</t>
         </is>
       </c>
       <c r="E159" s="14" t="inlineStr">
@@ -16000,7 +16000,7 @@
       </c>
       <c r="D166" s="13" t="inlineStr">
         <is>
-          <t>maa://20975 (100.00), *maa://47950 (70.97), maa://30806 (91.94)</t>
+          <t>maa://20975 (100.00), *maa://47950 (79.03), maa://30806 (91.94)</t>
         </is>
       </c>
       <c r="E166" s="14" t="inlineStr">
@@ -16054,7 +16054,7 @@
       </c>
       <c r="D167" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (100.00), maa://29627 (100.00), maa://29659 (80.90), maa://49074 (100.00), **maa://30679 (34.83), maa://29861 (87.64), *maa://42343 (78.65)</t>
+          <t>maa://29633 (100.00), maa://29627 (100.00), maa://29659 (82.02), maa://49074 (100.00), **maa://30679 (34.83), maa://29861 (87.64), *maa://42343 (78.65)</t>
         </is>
       </c>
       <c r="E167" s="14" t="inlineStr">
@@ -16108,7 +16108,7 @@
       </c>
       <c r="D168" s="13" t="inlineStr">
         <is>
-          <t>maa://49867 (95.35), maa://49655 (100.00)</t>
+          <t>maa://49867 (97.70), maa://49655 (100.00)</t>
         </is>
       </c>
       <c r="E168" s="14" t="inlineStr">
@@ -16432,7 +16432,7 @@
       </c>
       <c r="D174" s="13" t="inlineStr">
         <is>
-          <t>maa://59681 (100.00), *maa://64200 (60.64)</t>
+          <t>maa://59681 (100.00), *maa://64200 (74.47)</t>
         </is>
       </c>
       <c r="E174" s="14" t="inlineStr">
@@ -17080,7 +17080,7 @@
       </c>
       <c r="D186" s="13" t="inlineStr">
         <is>
-          <t>maa://20969 (86.25), maa://41303 (100.00)</t>
+          <t>maa://20969 (85.19), maa://41303 (100.00)</t>
         </is>
       </c>
       <c r="E186" s="14" t="inlineStr">
@@ -17674,7 +17674,7 @@
       </c>
       <c r="D197" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (91.58), maa://35854 (83.16), maa://50388 (100.00), maa://25760 (83.16), ***maa://43911 (4.21), **maa://20872 (34.74), *maa://51066 (68.42), maa://63024 (87.37)</t>
+          <t>maa://44224 (92.63), maa://35854 (82.11), maa://50388 (100.00), maa://25760 (83.16), ***maa://43911 (4.21), **maa://20872 (34.74), *maa://51066 (68.42), maa://63024 (82.11)</t>
         </is>
       </c>
       <c r="E197" s="14" t="inlineStr">
@@ -17728,7 +17728,7 @@
       </c>
       <c r="D198" s="13" t="inlineStr">
         <is>
-          <t>maa://39156 (100.00), **maa://39550 (39.08), **maa://53417 (47.13), **maa://63806 (39.08)</t>
+          <t>maa://39156 (100.00), **maa://39550 (39.08), **maa://53417 (47.13), *maa://63806 (65.52)</t>
         </is>
       </c>
       <c r="E198" s="14" t="inlineStr">
@@ -17782,7 +17782,7 @@
       </c>
       <c r="D199" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (97.44), *maa://28190 (58.97), maa://22894 (100.00), *maa://20906 (62.82), ***maa://20907 (26.92)</t>
+          <t>maa://27823 (98.72), *maa://28190 (58.97), maa://22894 (100.00), *maa://20906 (62.82), ***maa://20907 (26.92)</t>
         </is>
       </c>
       <c r="E199" s="14" t="inlineStr">
@@ -17836,7 +17836,7 @@
       </c>
       <c r="D200" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (97.44), *maa://28190 (58.97), maa://22894 (100.00), *maa://20906 (62.82), ***maa://20907 (26.92)</t>
+          <t>maa://27823 (98.72), *maa://28190 (58.97), maa://22894 (100.00), *maa://20906 (62.82), ***maa://20907 (26.92)</t>
         </is>
       </c>
       <c r="E200" s="14" t="inlineStr">
@@ -19402,7 +19402,7 @@
       </c>
       <c r="D229" s="13" t="inlineStr">
         <is>
-          <t>*maa://29644 (70.24), maa://39159 (100.00), ***maa://30061 (11.90)</t>
+          <t>*maa://29644 (71.43), maa://39159 (100.00), ***maa://30061 (11.90)</t>
         </is>
       </c>
       <c r="E229" s="14" t="inlineStr">
@@ -20050,7 +20050,7 @@
       </c>
       <c r="D241" s="13" t="inlineStr">
         <is>
-          <t>maa://30667 (96.15), maa://30666 (100.00), **maa://30739 (35.90), *maa://30723 (57.69), maa://39588 (98.72), *maa://64079 (79.49)</t>
+          <t>maa://30667 (94.94), maa://30666 (100.00), **maa://30739 (35.44), *maa://30723 (56.96), maa://39588 (97.47), maa://64079 (84.81)</t>
         </is>
       </c>
       <c r="E241" s="14" t="inlineStr">
@@ -20104,7 +20104,7 @@
       </c>
       <c r="D242" s="13" t="inlineStr">
         <is>
-          <t>maa://62759 (100.00), **maa://62764 (41.46)</t>
+          <t>maa://62759 (100.00), ***maa://62764 (24.42)</t>
         </is>
       </c>
       <c r="E242" s="14" t="inlineStr">
@@ -20531,12 +20531,12 @@
       </c>
       <c r="C250" s="12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D250" s="13" t="inlineStr">
         <is>
-          <t>maa://28923 (95.60), maa://28906 (100.00), ***maa://28825 (4.40)</t>
+          <t>maa://28923 (95.60), maa://28906 (100.00), ***maa://28825 (4.40), ***maa://65613 (23.08)</t>
         </is>
       </c>
       <c r="E250" s="14" t="inlineStr">
@@ -20590,7 +20590,7 @@
       </c>
       <c r="D251" s="13" t="inlineStr">
         <is>
-          <t>maa://42287 (96.59), maa://45570 (100.00), maa://60678 (81.82), maa://42225 (87.50)</t>
+          <t>maa://42287 (96.59), maa://45570 (100.00), *maa://60678 (76.14), maa://42225 (88.64)</t>
         </is>
       </c>
       <c r="E251" s="14" t="inlineStr">
@@ -20806,7 +20806,7 @@
       </c>
       <c r="D255" s="13" t="inlineStr">
         <is>
-          <t>maa://40958 (100.00), *maa://45067 (55.41)</t>
+          <t>maa://40958 (100.00), *maa://45067 (54.67)</t>
         </is>
       </c>
       <c r="E255" s="14" t="inlineStr">
@@ -21886,7 +21886,7 @@
       </c>
       <c r="D275" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://51630 (92.78), maa://56588 (83.51), **maa://55171 (40.21), *maa://51893 (61.86), ***maa://60902 (11.34)</t>
+          <t>maa://51881 (100.00), maa://51630 (91.84), maa://56588 (83.67), **maa://55171 (41.84), *maa://51893 (61.22), ***maa://60902 (15.31)</t>
         </is>
       </c>
       <c r="E275" s="14" t="inlineStr">
@@ -23074,7 +23074,7 @@
       </c>
       <c r="D297" s="13" t="inlineStr">
         <is>
-          <t>maa://32414 (100.00), *maa://32505 (67.01), maa://39155 (89.69)</t>
+          <t>maa://32414 (100.00), maa://39155 (89.69), *maa://32505 (67.01)</t>
         </is>
       </c>
       <c r="E297" s="14" t="inlineStr">
@@ -23560,7 +23560,7 @@
       </c>
       <c r="D306" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (100.00), maa://49642 (95.83), maa://49660 (84.38), *maa://50517 (51.04)</t>
+          <t>maa://50280 (100.00), maa://49642 (95.88), maa://49660 (84.54), *maa://50517 (50.52)</t>
         </is>
       </c>
       <c r="E306" s="14" t="inlineStr">
@@ -24262,7 +24262,7 @@
       </c>
       <c r="D319" s="13" t="inlineStr">
         <is>
-          <t>**maa://62755 (46.67), maa://62761 (100.00)</t>
+          <t>*maa://62755 (65.00), maa://62761 (100.00)</t>
         </is>
       </c>
       <c r="E319" s="14" t="inlineStr">
@@ -24586,7 +24586,7 @@
       </c>
       <c r="D325" s="13" t="inlineStr">
         <is>
-          <t>maa://39692 (100.00), *maa://39810 (72.73)</t>
+          <t>maa://39692 (100.00), *maa://39810 (74.75)</t>
         </is>
       </c>
       <c r="E325" s="14" t="inlineStr">
@@ -24910,7 +24910,7 @@
       </c>
       <c r="D331" s="15" t="inlineStr">
         <is>
-          <t>maa://30680 (100.00), ***maa://41360 (25.61)</t>
+          <t>maa://30680 (100.00), ***maa://41360 (25.30)</t>
         </is>
       </c>
       <c r="E331" s="15" t="inlineStr">
@@ -25288,7 +25288,7 @@
       </c>
       <c r="D338" s="22" t="inlineStr">
         <is>
-          <t>maa://42968 (100.00), maa://49245 (92.86)</t>
+          <t>maa://42968 (100.00), maa://49245 (93.88)</t>
         </is>
       </c>
       <c r="E338" s="22" t="inlineStr">
@@ -25828,7 +25828,7 @@
       </c>
       <c r="D348" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (100.00), maa://32415 (96.88), maa://34677 (96.88), maa://32892 (88.54), *maa://32653 (64.58), *maa://61839 (63.54), **maa://61275 (45.83)</t>
+          <t>maa://32647 (100.00), maa://32415 (96.88), maa://34677 (96.88), maa://32892 (88.54), *maa://32653 (64.58), *maa://61839 (67.71), *maa://61275 (53.12)</t>
         </is>
       </c>
       <c r="E348" s="22" t="inlineStr">
@@ -26314,7 +26314,7 @@
       </c>
       <c r="D357" s="22" t="inlineStr">
         <is>
-          <t>maa://36868 (100.00), maa://35996 (93.88), ***maa://39217 (20.41), maa://47349 (88.78)</t>
+          <t>maa://36868 (100.00), maa://35996 (94.90), ***maa://39217 (20.41), maa://47349 (89.80)</t>
         </is>
       </c>
       <c r="E357" s="22" t="inlineStr">
@@ -26530,7 +26530,7 @@
       </c>
       <c r="D361" s="22" t="inlineStr">
         <is>
-          <t>maa://49648 (100.00), *maa://49662 (73.86)</t>
+          <t>maa://49648 (100.00), *maa://49662 (71.91)</t>
         </is>
       </c>
       <c r="E361" s="22" t="inlineStr">
@@ -26854,7 +26854,7 @@
       </c>
       <c r="D367" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (100.00), maa://48026 (95.70), maa://44635 (87.10), maa://41035 (91.40), maa://44660 (86.02), *maa://60251 (54.84), *maa://41128 (75.27)</t>
+          <t>maa://40957 (100.00), maa://48026 (95.70), maa://44635 (87.10), maa://41035 (91.40), maa://44660 (87.10), *maa://60251 (56.99), *maa://41128 (75.27)</t>
         </is>
       </c>
       <c r="E367" s="22" t="inlineStr">
@@ -26962,7 +26962,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://63883 (100.00), maa://64045 (90.28), ***maa://64041 (29.17)</t>
+          <t>maa://63883 (100.00), maa://64045 (84.42), **maa://64041 (38.96)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -27772,7 +27772,7 @@
       </c>
       <c r="D384" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (81.91), maa://44745 (100.00), ***maa://49516 (26.60), **maa://45952 (38.30), ***maa://46851 (2.13), **maa://44896 (47.87)</t>
+          <t>maa://42970 (81.05), maa://44745 (100.00), ***maa://49516 (26.32), **maa://45952 (37.89), ***maa://46851 (2.11), **maa://44896 (47.37)</t>
         </is>
       </c>
       <c r="E384" s="22" t="inlineStr">
@@ -28091,12 +28091,12 @@
       </c>
       <c r="C390" s="12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D390" s="22" t="inlineStr">
         <is>
-          <t>maa://63890 (100.00)</t>
+          <t>maa://63890 (100.00), ***maa://64043 (25.61)</t>
         </is>
       </c>
       <c r="E390" s="22" t="inlineStr">
@@ -28393,7 +28393,7 @@
       </c>
       <c r="D398" t="inlineStr">
         <is>
-          <t>maa://51880 (100.00), maa://56651 (93.88), maa://51878 (91.84)</t>
+          <t>maa://51880 (100.00), maa://56651 (94.90), maa://51878 (92.86)</t>
         </is>
       </c>
       <c r="E398" t="inlineStr">
@@ -28420,7 +28420,7 @@
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>maa://51872 (100.00), maa://51876 (98.95), *maa://63228 (74.74), maa://51873 (96.84), *maa://62047 (74.74)</t>
+          <t>maa://51872 (100.00), maa://51876 (100.00), *maa://63228 (76.84), maa://51873 (96.84), *maa://62047 (75.79)</t>
         </is>
       </c>
       <c r="E399" t="inlineStr">
@@ -28577,12 +28577,12 @@
       </c>
       <c r="C405" s="17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>maa://64040 (100.00)</t>
+          <t>maa://64040 (100.00), ***maa://65803 (21.65)</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#229)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://39402 (100.00), *maa://34787 (73.86), maa://58660 (89.77)</t>
+          <t>maa://39402 (100.00), *maa://34787 (74.71), maa://58660 (91.95)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://21246 (98.88), maa://36684 (100.00)</t>
+          <t>maa://36684 (100.00), maa://21246 (100.00)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://25251 (100.00), maa://59087 (97.67)</t>
+          <t>maa://25251 (100.00), maa://59087 (96.51)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -842,7 +842,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (100.00), maa://36987 (96.70), *maa://39849 (61.54)</t>
+          <t>maa://40192 (100.00), maa://36987 (95.65), *maa://39849 (60.87)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>*maa://22880 (72.62), maa://20276 (100.00), *maa://22749 (72.62)</t>
+          <t>*maa://22880 (72.62), maa://20276 (100.00), *maa://22749 (75.00)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -890,7 +890,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (100.00), maa://26254 (94.57), **maa://22738 (32.61)</t>
+          <t>maa://21249 (100.00), maa://26254 (95.65), **maa://22738 (32.61)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://45854 (85.88), maa://24617 (100.00), maa://60545 (82.35)</t>
+          <t>maa://45854 (85.88), maa://24617 (100.00), maa://60545 (85.88)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (86.02), maa://27484 (100.00), *maa://27480 (78.49)</t>
+          <t>maa://27396 (86.02), maa://27484 (100.00), *maa://27480 (77.42)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://24390 (100.00), maa://52241 (91.11)</t>
+          <t>maa://24390 (100.00), maa://52241 (92.22)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (100.00), maa://50121 (96.63)</t>
+          <t>maa://49983 (100.00), maa://50121 (95.56)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://32509 (100.00), maa://27295 (92.13), maa://22754 (89.89), *maa://31008 (73.03)</t>
+          <t>maa://32509 (100.00), maa://27295 (91.11), maa://22754 (88.89), *maa://31008 (72.22)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>maa://30062 (96.23), maa://39394 (100.00), ***maa://26209 (9.43)</t>
+          <t>maa://39394 (100.00), maa://30062 (94.34), ***maa://26209 (9.43)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (100.00), maa://54105 (98.73), maa://22744 (81.01)</t>
+          <t>maa://21245 (100.00), maa://54105 (98.73), *maa://22744 (78.48)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (100.00), maa://30381 (89.29)</t>
+          <t>maa://31836 (100.00), maa://30381 (88.24)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>**maa://64972 (42.00)</t>
+          <t>*maa://64972 (69.39)</t>
         </is>
       </c>
       <c r="I7" s="19" t="n"/>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (100.00), *maa://22758 (75.00)</t>
+          <t>maa://22399 (100.00), *maa://22758 (76.92)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.22 13:21:00</t>
+          <t>更新日期：2025.08.30 13:19:59</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (100.00), *maa://39431 (54.55), **maa://37551 (33.33)</t>
+          <t>maa://21476 (100.00), *maa://39431 (51.52), **maa://37551 (33.33)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (86.52), maa://23252 (93.26), maa://37496 (100.00)</t>
+          <t>maa://32931 (87.64), maa://23252 (93.26), maa://37496 (100.00)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (100.00), *maa://39552 (75.58)</t>
+          <t>maa://22762 (100.00), *maa://39552 (70.93)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1675,12 +1675,12 @@
       </c>
       <c r="O9" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="P9" s="8" t="inlineStr">
         <is>
-          <t>maa://22736 (100.00)</t>
+          <t>maa://22736 (100.00), ***maa://64516 (27.63)</t>
         </is>
       </c>
       <c r="Q9" s="19" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://26223 (100.00), maa://52237 (85.26)</t>
+          <t>maa://26223 (100.00), maa://52237 (86.32)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (100.00), **maa://22865 (45.88)</t>
+          <t>maa://26206 (100.00), **maa://22865 (45.24)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>***maa://25695 (26.42), ***maa://39951 (11.32), maa://45271 (100.00), ***maa://34206 (20.75), ***maa://39243 (13.21), **maa://54000 (43.40)</t>
+          <t>***maa://25695 (26.92), ***maa://39951 (11.54), maa://45271 (100.00), ***maa://34206 (21.15), ***maa://39243 (13.46), **maa://54000 (44.23)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (100.00), maa://22755 (87.23), *maa://63521 (51.06)</t>
+          <t>maa://27395 (100.00), maa://22755 (88.30), *maa://63521 (51.06)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://22301 (100.00), maa://45828 (91.58), maa://22726 (82.11)</t>
+          <t>maa://45828 (90.53), maa://22301 (100.00), maa://22726 (82.11)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>maa://25021 (82.69), maa://22733 (100.00), ***maa://22761 (17.31)</t>
+          <t>maa://25021 (82.69), maa://22733 (100.00), ***maa://22761 (11.54)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1951,12 +1951,12 @@
       </c>
       <c r="S11" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (89.47), maa://22501 (100.00), maa://45521 (88.42)</t>
+          <t>maa://22747 (89.47), maa://22501 (100.00), maa://45521 (88.42), **maa://64808 (46.32)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>maa://30766 (100.00), *maa://36678 (70.27)</t>
+          <t>maa://30766 (100.00), *maa://36678 (74.32)</t>
         </is>
       </c>
       <c r="E12" s="19" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (100.00), maa://54294 (83.72)</t>
+          <t>maa://21867 (100.00), maa://54294 (86.05)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (93.26), maa://64046 (100.00)</t>
+          <t>maa://63896 (90.00), maa://64046 (100.00)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://22753 (100.00), maa://37962 (94.32), *maa://21485 (78.41)</t>
+          <t>maa://22753 (100.00), maa://37962 (95.45), *maa://21485 (78.41)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://23669 (100.00), maa://36677 (96.74), maa://39872 (89.13)</t>
+          <t>maa://23669 (100.00), maa://36677 (95.65), maa://39872 (89.13)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>maa://28932 (100.00), *maa://20106 (75.34), *maa://22769 (60.27)</t>
+          <t>maa://28932 (100.00), *maa://20106 (76.39), *maa://22769 (61.11)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>maa://21248 (100.00), **maa://22728 (47.83)</t>
+          <t>maa://21248 (100.00), **maa://66545 (50.00)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (100.00), *maa://22583 (78.89), *maa://48321 (61.11)</t>
+          <t>maa://22676 (100.00), *maa://22583 (78.89), *maa://48321 (56.67)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2259,12 +2259,12 @@
       </c>
       <c r="AE13" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (100.00)</t>
+          <t>maa://39883 (100.00), **maa://39885 (45.68)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (96.77), maa://26245 (100.00), maa://21288 (98.92), maa://36682 (92.47)</t>
+          <t>maa://39841 (96.77), maa://26245 (100.00), maa://21288 (98.92), maa://36682 (90.32)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://22521 (100.00), maa://42751 (94.38)</t>
+          <t>maa://22521 (100.00), maa://42751 (91.01)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (96.10), maa://22734 (100.00), *maa://30808 (66.23), maa://36048 (84.42), maa://45058 (84.42)</t>
+          <t>maa://22743 (96.10), maa://22734 (100.00), *maa://30808 (64.94), maa://36048 (84.42), maa://45058 (87.01)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (100.00), maa://21478 (92.77)</t>
+          <t>maa://24304 (100.00), maa://21478 (91.67)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://21364 (100.00), maa://36666 (98.72), *maa://22766 (78.21)</t>
+          <t>maa://21364 (100.00), maa://36666 (100.00), *maa://22766 (78.21)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://21441 (100.00), maa://37650 (97.85), maa://36679 (91.40)</t>
+          <t>maa://37650 (97.85), maa://21441 (100.00), maa://36679 (91.40)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://22729 (100.00), *maa://28648 (73.33), *maa://36674 (78.89)</t>
+          <t>maa://22729 (100.00), *maa://28648 (74.44), *maa://36674 (78.89)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>*maa://23911 (70.45), maa://27755 (100.00)</t>
+          <t>*maa://23911 (71.59), maa://27755 (100.00)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://22430 (100.00), maa://39599 (96.47)</t>
+          <t>maa://39599 (95.29), maa://22430 (100.00)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), maa://54153 (86.17), *maa://24380 (69.15)</t>
+          <t>maa://24379 (100.00), maa://54153 (86.32), *maa://24380 (68.42)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://24313 (88.33), maa://47854 (100.00), *maa://29784 (55.00)</t>
+          <t>maa://24313 (89.83), maa://47854 (100.00), *maa://29784 (54.24)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://21432 (97.75), maa://25198 (100.00), maa://36680 (87.64)</t>
+          <t>maa://21432 (98.86), maa://25198 (100.00), maa://36680 (88.64)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (100.00), maa://49976 (95.29), *maa://56241 (76.47)</t>
+          <t>maa://50085 (100.00), maa://49976 (94.12), maa://56241 (82.35)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22524 (100.00), maa://22432 (98.75), **maa://64221 (50.00)</t>
+          <t>maa://22524 (100.00), maa://22432 (100.00), *maa://64221 (56.96)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (100.00), *maa://29748 (77.27), *maa://37566 (76.14)</t>
+          <t>maa://30587 (100.00), *maa://29748 (78.41), *maa://37566 (76.14)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (100.00), *maa://46650 (72.37)</t>
+          <t>maa://24368 (100.00), *maa://46650 (71.05)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (89.01), maa://23504 (100.00), *maa://36663 (75.82), *maa://25141 (76.92), maa://52227 (92.31)</t>
+          <t>maa://29988 (89.01), maa://23504 (100.00), *maa://25141 (76.92), *maa://36663 (75.82), maa://52227 (85.71)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://22523 (87.21), *maa://36672 (69.77), maa://29910 (100.00), maa://45831 (84.88), maa://64165 (81.40)</t>
+          <t>maa://22523 (87.21), *maa://36672 (68.60), maa://29910 (100.00), maa://45831 (86.05), maa://64165 (88.37)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (100.00), *maa://63016 (75.27)</t>
+          <t>maa://29753 (100.00), *maa://63016 (77.42)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3771,12 +3771,12 @@
       </c>
       <c r="S25" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="T25" s="8" t="inlineStr">
         <is>
-          <t>maa://20109 (90.72), maa://22545 (100.00), **maa://42915 (30.93)</t>
+          <t>maa://20109 (90.72), maa://22545 (100.00)</t>
         </is>
       </c>
       <c r="U25" s="19" t="n"/>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (100.00), maa://24516 (84.52), maa://26001 (86.90)</t>
+          <t>maa://31215 (100.00), maa://24516 (83.53), maa://26001 (85.88)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (98.92), maa://24621 (100.00), maa://36676 (91.40), *maa://22771 (64.52), **maa://37772 (40.86)</t>
+          <t>maa://20108 (98.92), maa://24621 (100.00), maa://36676 (91.40), *maa://22771 (66.67), **maa://37772 (40.86)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://41802 (100.00), maa://56374 (80.25)</t>
+          <t>maa://41802 (100.00), maa://56374 (86.42)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="P26" s="8" t="inlineStr">
         <is>
-          <t>maa://39870 (100.00), maa://56625 (94.20)</t>
+          <t>maa://39870 (91.18), maa://56625 (100.00)</t>
         </is>
       </c>
       <c r="Q26" s="19" t="n"/>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>*maa://39601 (75.00), maa://34494 (100.00)</t>
+          <t>*maa://39601 (76.14), maa://34494 (100.00)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4102,7 +4102,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (100.00), maa://25725 (83.15)</t>
+          <t>maa://24465 (100.00), maa://25725 (82.02)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (100.00), ***maa://65700 (23.33)</t>
+          <t>maa://36660 (100.00), *maa://65700 (54.44)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://24080 (88.89), maa://42865 (100.00), ***maa://34960 (2.78)</t>
+          <t>maa://24080 (90.14), maa://42865 (100.00), ***maa://34960 (2.82)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (100.00), *maa://64191 (57.14)</t>
+          <t>maa://45792 (100.00), *maa://64191 (66.23)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4421,12 +4421,12 @@
       </c>
       <c r="S30" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="T30" s="8" t="inlineStr">
         <is>
-          <t>*maa://32940 (55.84), maa://24388 (100.00)</t>
+          <t>maa://24388 (100.00)</t>
         </is>
       </c>
       <c r="U30" s="19" t="n"/>
@@ -4665,12 +4665,12 @@
       </c>
       <c r="O32" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="P32" s="8" t="inlineStr">
         <is>
-          <t>maa://26203 (100.00)</t>
+          <t>maa://26203 (100.00), ***maa://56429 (24.42)</t>
         </is>
       </c>
       <c r="Q32" s="19" t="n"/>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (98.95), *maa://41108 (77.89), maa://41238 (100.00), maa://45523 (98.95)</t>
+          <t>maa://42859 (100.00), *maa://41108 (77.89), maa://41238 (100.00), maa://45523 (98.95)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (100.00), *maa://56235 (70.65)</t>
+          <t>maa://48817 (100.00), *maa://56235 (75.27)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (100.00), *maa://47069 (59.79), *maa://56336 (68.04), *maa://45789 (67.01)</t>
+          <t>maa://45718 (100.00), *maa://56336 (69.07), *maa://47069 (59.79), *maa://45789 (67.01)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5418,7 +5418,7 @@
       </c>
       <c r="L38" s="8" t="inlineStr">
         <is>
-          <t>maa://39384 (100.00), *maa://49735 (64.89)</t>
+          <t>maa://39384 (100.00), *maa://49735 (69.15)</t>
         </is>
       </c>
       <c r="M38" s="19" t="n"/>
@@ -5503,7 +5503,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://36670 (91.11), maa://25199 (86.67), maa://30434 (100.00), *maa://45059 (68.89), **maa://44165 (42.22)</t>
+          <t>maa://36670 (88.89), maa://25199 (86.67), maa://30434 (100.00), *maa://45059 (67.78), **maa://44165 (42.22)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://24709 (100.00), maa://47093 (95.40)</t>
+          <t>maa://24709 (100.00), maa://47093 (94.25)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (100.00), *maa://45788 (71.60), *maa://45790 (79.01)</t>
+          <t>maa://47079 (100.00), *maa://45788 (70.73), *maa://45790 (78.05)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5679,12 +5679,12 @@
       </c>
       <c r="AE40" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://64205 (100.00), *maa://65283 (71.25)</t>
+          <t>*maa://64107 (62.96), maa://64205 (100.00), maa://65283 (86.42)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>maa://22525 (86.42), maa://21284 (100.00)</t>
+          <t>maa://22525 (85.19), maa://21284 (100.00)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -5955,7 +5955,7 @@
       </c>
       <c r="T43" s="8" t="inlineStr">
         <is>
-          <t>maa://43198 (100.00), *maa://46286 (51.76)</t>
+          <t>maa://43198 (100.00), *maa://46286 (60.00)</t>
         </is>
       </c>
       <c r="U43" s="19" t="n"/>
@@ -5992,7 +5992,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (100.00), maa://27728 (95.79), *maa://56386 (77.89)</t>
+          <t>maa://29768 (100.00), maa://27728 (95.79), maa://56386 (82.11)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6146,7 +6146,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (100.00), maa://43901 (95.51)</t>
+          <t>maa://35931 (100.00), maa://43901 (94.38)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6215,7 +6215,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (100.00), maa://29661 (98.95), *maa://28038 (61.05), *maa://56236 (75.79)</t>
+          <t>maa://27410 (100.00), maa://29661 (98.95), *maa://56236 (73.68), *maa://28038 (61.05)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6490,7 +6490,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (100.00), maa://59378 (91.49), **maa://65511 (46.81)</t>
+          <t>maa://59394 (100.00), maa://59378 (90.53), *maa://65511 (71.58)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6660,7 +6660,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://25176 (100.00), *maa://56237 (77.42)</t>
+          <t>maa://25176 (100.00), maa://56237 (81.72)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6750,7 +6750,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (100.00), maa://43903 (89.89), *maa://56228 (73.03)</t>
+          <t>maa://42981 (100.00), maa://43903 (89.89), *maa://56228 (76.40)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6768,7 +6768,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (100.00), *maa://59693 (61.70), *maa://59413 (72.34)</t>
+          <t>maa://59534 (100.00), *maa://59693 (60.64), *maa://59413 (74.47)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7090,7 +7090,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.22 13:21:00</t>
+          <t>更新日期：2025.08.30 13:19:59</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -7900,7 +7900,7 @@
       </c>
       <c r="D16" s="13" t="inlineStr">
         <is>
-          <t>maa://20919 (100.00), *maa://31611 (51.09)</t>
+          <t>maa://20919 (100.00), *maa://31611 (52.22)</t>
         </is>
       </c>
       <c r="E16" s="14" t="inlineStr">
@@ -8494,7 +8494,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (72.29), *maa://28758 (67.47), maa://29036 (100.00), *maa://42172 (55.42), maa://30285 (81.93), *maa://65357 (78.31)</t>
+          <t>*maa://20849 (72.29), *maa://28758 (67.47), maa://29036 (100.00), *maa://42172 (55.42), *maa://65357 (74.70), maa://30285 (81.93)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8602,7 +8602,7 @@
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>maa://20863 (90.53), maa://20832 (100.00), *maa://20727 (75.79)</t>
+          <t>maa://20863 (89.58), maa://20832 (100.00), *maa://20727 (75.00)</t>
         </is>
       </c>
       <c r="E29" s="14" t="inlineStr">
@@ -8764,7 +8764,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (95.51), maa://36866 (100.00), maa://62759 (96.63), *maa://45572 (74.16), *maa://27794 (64.04), *maa://20960 (78.65), **maa://20843 (49.44), ***maa://24483 (10.11), **maa://20862 (49.44), *maa://20893 (61.80)</t>
+          <t>maa://36644 (95.51), maa://36866 (100.00), maa://62759 (98.88), *maa://45572 (74.16), *maa://27794 (64.04), *maa://20960 (78.65), **maa://20843 (49.44), ***maa://24483 (10.11), **maa://20862 (49.44), *maa://20893 (61.80)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -8872,7 +8872,7 @@
       </c>
       <c r="D34" s="13" t="inlineStr">
         <is>
-          <t>maa://20916 (100.00), maa://52658 (92.54)</t>
+          <t>maa://20916 (97.10), maa://52658 (100.00)</t>
         </is>
       </c>
       <c r="E34" s="14" t="inlineStr">
@@ -9034,7 +9034,7 @@
       </c>
       <c r="D37" s="13" t="inlineStr">
         <is>
-          <t>maa://27376 (98.81), maa://42635 (100.00), **maa://20838 (40.48)</t>
+          <t>maa://27376 (100.00), maa://42635 (100.00), **maa://20838 (40.48)</t>
         </is>
       </c>
       <c r="E37" s="14" t="inlineStr">
@@ -10006,7 +10006,7 @@
       </c>
       <c r="D55" s="13" t="inlineStr">
         <is>
-          <t>maa://20932 (100.00), maa://42415 (93.55), *maa://40838 (79.57)</t>
+          <t>maa://20932 (100.00), maa://42415 (94.57), maa://40838 (82.61)</t>
         </is>
       </c>
       <c r="E55" s="14" t="inlineStr">
@@ -10330,7 +10330,7 @@
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (100.00), maa://24093 (100.00), maa://31559 (89.47), maa://20924 (81.05), *maa://25777 (64.21), *maa://20631 (60.00), **maa://28241 (46.32)</t>
+          <t>maa://20841 (100.00), maa://31559 (89.47), maa://24093 (100.00), maa://20924 (81.05), *maa://25777 (64.21), *maa://20631 (64.21), **maa://28241 (46.32)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -10487,12 +10487,12 @@
       </c>
       <c r="C64" s="12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D64" s="13" t="inlineStr">
         <is>
-          <t>maa://28187 (92.63), maa://45144 (100.00), maa://33504 (94.74), **maa://43531 (35.79), ***maa://65290 (22.11)</t>
+          <t>maa://28187 (92.63), maa://45144 (100.00), maa://33504 (94.74), **maa://43531 (35.79)</t>
         </is>
       </c>
       <c r="E64" s="14" t="inlineStr">
@@ -10546,7 +10546,7 @@
       </c>
       <c r="D65" s="13" t="inlineStr">
         <is>
-          <t>maa://28567 (96.81), **maa://20947 (31.91), maa://30525 (88.30), maa://38735 (100.00), **maa://28188 (42.55), **maa://30524 (36.17)</t>
+          <t>maa://28567 (96.81), **maa://20947 (31.91), maa://30525 (89.36), maa://38735 (100.00), **maa://28188 (42.55), **maa://30524 (36.17)</t>
         </is>
       </c>
       <c r="E65" s="14" t="inlineStr">
@@ -10600,7 +10600,7 @@
       </c>
       <c r="D66" s="13" t="inlineStr">
         <is>
-          <t>maa://20993 (100.00), maa://45606 (91.58), **maa://20914 (46.32), maa://20829 (81.05), maa://20900 (85.26), **maa://40159 (46.32)</t>
+          <t>maa://20993 (100.00), maa://45606 (92.63), **maa://20914 (46.32), maa://20829 (81.05), maa://20900 (85.26), **maa://40159 (46.32)</t>
         </is>
       </c>
       <c r="E66" s="14" t="inlineStr">
@@ -10708,7 +10708,7 @@
       </c>
       <c r="D68" s="13" t="inlineStr">
         <is>
-          <t>maa://20976 (100.00), maa://20815 (84.21)</t>
+          <t>maa://20976 (100.00), maa://20815 (83.33)</t>
         </is>
       </c>
       <c r="E68" s="14" t="inlineStr">
@@ -10762,7 +10762,7 @@
       </c>
       <c r="D69" s="13" t="inlineStr">
         <is>
-          <t>maa://20974 (100.00), *maa://29079 (73.63), maa://29096 (86.81), maa://29087 (92.31), **maa://20823 (48.35), maa://20855 (80.22), maa://20904 (84.62), **maa://63722 (48.35)</t>
+          <t>maa://20974 (100.00), *maa://29079 (73.63), maa://29096 (86.81), maa://29087 (92.31), *maa://20823 (53.85), maa://20855 (80.22), maa://20904 (84.62), **maa://63722 (48.35)</t>
         </is>
       </c>
       <c r="E69" s="14" t="inlineStr">
@@ -10816,7 +10816,7 @@
       </c>
       <c r="D70" s="13" t="inlineStr">
         <is>
-          <t>maa://20944 (93.48), maa://35393 (100.00)</t>
+          <t>maa://20944 (94.57), maa://35393 (100.00)</t>
         </is>
       </c>
       <c r="E70" s="14" t="inlineStr">
@@ -10865,12 +10865,12 @@
       </c>
       <c r="C71" s="12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D71" s="13" t="inlineStr">
         <is>
-          <t>maa://20943 (100.00), *maa://30673 (73.47), maa://63790 (89.80), *maa://30672 (66.33), maa://20856 (82.65)</t>
+          <t>maa://20943 (100.00), *maa://30673 (73.47), *maa://30672 (66.33), maa://20856 (82.65)</t>
         </is>
       </c>
       <c r="E71" s="14" t="inlineStr">
@@ -11410,7 +11410,7 @@
       </c>
       <c r="D81" s="13" t="inlineStr">
         <is>
-          <t>maa://30525 (95.40), maa://20859 (100.00), **maa://28188 (45.98), **maa://30524 (39.08)</t>
+          <t>maa://30525 (96.55), maa://20859 (100.00), **maa://28188 (45.98), **maa://30524 (39.08)</t>
         </is>
       </c>
       <c r="E81" s="14" t="inlineStr">
@@ -11788,7 +11788,7 @@
       </c>
       <c r="D88" s="13" t="inlineStr">
         <is>
-          <t>maa://24472 (100.00), **maa://35841 (50.00)</t>
+          <t>maa://24472 (100.00), *maa://35841 (51.72)</t>
         </is>
       </c>
       <c r="E88" s="14" t="inlineStr">
@@ -12274,7 +12274,7 @@
       </c>
       <c r="D97" s="13" t="inlineStr">
         <is>
-          <t>maa://20991 (100.00), *maa://51015 (75.26)</t>
+          <t>maa://20991 (100.00), *maa://51015 (77.32)</t>
         </is>
       </c>
       <c r="E97" s="14" t="inlineStr">
@@ -12598,7 +12598,7 @@
       </c>
       <c r="D103" s="13" t="inlineStr">
         <is>
-          <t>maa://29094 (80.52), maa://28904 (100.00), **maa://20931 (38.96)</t>
+          <t>maa://29094 (86.49), maa://28904 (100.00), **maa://20931 (39.19)</t>
         </is>
       </c>
       <c r="E103" s="14" t="inlineStr">
@@ -12868,7 +12868,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://25018 (96.94), maa://25776 (85.71), maa://28361 (85.71), maa://25772 (85.71), maa://56588 (83.67), *maa://45194 (66.33), *maa://25161 (62.24), *maa://32653 (63.27), ***maa://60902 (15.31), *maa://61839 (66.33), *maa://61275 (52.04)</t>
+          <t>maa://51881 (100.00), maa://25018 (96.94), maa://25776 (85.71), maa://28361 (86.73), maa://25772 (85.71), maa://56588 (84.69), *maa://45194 (66.33), *maa://25161 (62.24), *maa://32653 (63.27), *maa://61839 (73.47), ***maa://60902 (19.39), *maa://61275 (52.04)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13084,7 +13084,7 @@
       </c>
       <c r="D112" s="13" t="inlineStr">
         <is>
-          <t>maa://20933 (100.00), maa://20822 (88.31)</t>
+          <t>maa://20933 (100.00), maa://20822 (87.18)</t>
         </is>
       </c>
       <c r="E112" s="14" t="inlineStr">
@@ -13300,7 +13300,7 @@
       </c>
       <c r="D116" s="13" t="inlineStr">
         <is>
-          <t>maa://29659 (96.05), maa://29031 (100.00)</t>
+          <t>maa://29659 (97.37), maa://29031 (100.00)</t>
         </is>
       </c>
       <c r="E116" s="14" t="inlineStr">
@@ -13570,7 +13570,7 @@
       </c>
       <c r="D121" s="13" t="inlineStr">
         <is>
-          <t>maa://20869 (100.00), maa://44690 (83.51)</t>
+          <t>maa://20869 (100.00), maa://44690 (85.57)</t>
         </is>
       </c>
       <c r="E121" s="14" t="inlineStr">
@@ -13624,7 +13624,7 @@
       </c>
       <c r="D122" s="13" t="inlineStr">
         <is>
-          <t>maa://29650 (100.00), maa://45570 (95.65)</t>
+          <t>maa://29650 (100.00), maa://45570 (96.74)</t>
         </is>
       </c>
       <c r="E122" s="14" t="inlineStr">
@@ -14542,7 +14542,7 @@
       </c>
       <c r="D139" s="13" t="inlineStr">
         <is>
-          <t>maa://45258 (100.00), **maa://30679 (44.93)</t>
+          <t>maa://45258 (100.00), **maa://30679 (44.29)</t>
         </is>
       </c>
       <c r="E139" s="14" t="inlineStr">
@@ -14704,7 +14704,7 @@
       </c>
       <c r="D142" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (100.00), **maa://23736 (40.43), *maa://31185 (63.83), *maa://30306 (54.26)</t>
+          <t>maa://28484 (100.00), **maa://23736 (43.62), *maa://31185 (65.96), *maa://30306 (54.26)</t>
         </is>
       </c>
       <c r="E142" s="14" t="inlineStr">
@@ -14758,7 +14758,7 @@
       </c>
       <c r="D143" s="13" t="inlineStr">
         <is>
-          <t>maa://30670 (100.00), maa://31470 (89.25), **maa://45066 (38.71), *maa://61380 (61.29), ***maa://30867 (12.90)</t>
+          <t>maa://30670 (100.00), maa://31470 (84.95), **maa://45066 (38.71), *maa://61380 (75.27), ***maa://30867 (12.90)</t>
         </is>
       </c>
       <c r="E143" s="14" t="inlineStr">
@@ -15136,7 +15136,7 @@
       </c>
       <c r="D150" s="13" t="inlineStr">
         <is>
-          <t>maa://51549 (100.00), maa://51923 (92.05)</t>
+          <t>maa://51549 (100.00), maa://51923 (92.13)</t>
         </is>
       </c>
       <c r="E150" s="14" t="inlineStr">
@@ -15617,12 +15617,12 @@
       </c>
       <c r="C159" s="12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D159" s="13" t="inlineStr">
         <is>
-          <t>maa://44232 (100.00), *maa://45603 (78.35), ***maa://63114 (9.28)</t>
+          <t>maa://44232 (100.00), *maa://45603 (78.35), ***maa://63114 (21.65), ***maa://65963 (9.28)</t>
         </is>
       </c>
       <c r="E159" s="14" t="inlineStr">
@@ -16054,7 +16054,7 @@
       </c>
       <c r="D167" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (100.00), maa://29627 (100.00), maa://29659 (82.02), maa://49074 (100.00), **maa://30679 (34.83), maa://29861 (87.64), *maa://42343 (78.65)</t>
+          <t>maa://29633 (98.89), maa://29627 (98.89), maa://29659 (82.22), maa://49074 (100.00), **maa://30679 (34.44), maa://29861 (86.67), *maa://42343 (77.78)</t>
         </is>
       </c>
       <c r="E167" s="14" t="inlineStr">
@@ -16108,7 +16108,7 @@
       </c>
       <c r="D168" s="13" t="inlineStr">
         <is>
-          <t>maa://49867 (97.70), maa://49655 (100.00)</t>
+          <t>maa://49867 (97.73), maa://49655 (100.00)</t>
         </is>
       </c>
       <c r="E168" s="14" t="inlineStr">
@@ -16432,7 +16432,7 @@
       </c>
       <c r="D174" s="13" t="inlineStr">
         <is>
-          <t>maa://59681 (100.00), *maa://64200 (74.47)</t>
+          <t>maa://59681 (100.00), maa://64200 (82.98)</t>
         </is>
       </c>
       <c r="E174" s="14" t="inlineStr">
@@ -16486,7 +16486,7 @@
       </c>
       <c r="D175" s="13" t="inlineStr">
         <is>
-          <t>maa://32418 (100.00), maa://51440 (89.90), maa://63320 (87.88)</t>
+          <t>maa://32418 (100.00), maa://51440 (89.90), maa://63320 (88.89)</t>
         </is>
       </c>
       <c r="E175" s="14" t="inlineStr">
@@ -17674,7 +17674,7 @@
       </c>
       <c r="D197" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (92.63), maa://35854 (82.11), maa://50388 (100.00), maa://25760 (83.16), ***maa://43911 (4.21), **maa://20872 (34.74), *maa://51066 (68.42), maa://63024 (82.11)</t>
+          <t>maa://44224 (92.63), maa://35854 (83.16), maa://50388 (100.00), maa://25760 (83.16), ***maa://43911 (4.21), **maa://20872 (34.74), *maa://51066 (55.79), maa://63024 (86.32)</t>
         </is>
       </c>
       <c r="E197" s="14" t="inlineStr">
@@ -17728,7 +17728,7 @@
       </c>
       <c r="D198" s="13" t="inlineStr">
         <is>
-          <t>maa://39156 (100.00), **maa://39550 (39.08), **maa://53417 (47.13), *maa://63806 (65.52)</t>
+          <t>maa://39156 (100.00), **maa://39550 (39.08), **maa://53417 (47.13), *maa://63806 (56.32)</t>
         </is>
       </c>
       <c r="E198" s="14" t="inlineStr">
@@ -17890,7 +17890,7 @@
       </c>
       <c r="D201" s="13" t="inlineStr">
         <is>
-          <t>maa://42223 (100.00), maa://49077 (84.69), maa://42292 (87.76), *maa://42402 (69.39)</t>
+          <t>maa://42223 (100.00), maa://49077 (85.71), maa://42292 (87.76), *maa://42402 (69.39)</t>
         </is>
       </c>
       <c r="E201" s="14" t="inlineStr">
@@ -18430,7 +18430,7 @@
       </c>
       <c r="D211" s="13" t="inlineStr">
         <is>
-          <t>maa://20956 (100.00), *maa://20830 (63.04), *maa://44703 (70.65)</t>
+          <t>maa://20956 (100.00), *maa://20830 (62.37), *maa://44703 (72.04)</t>
         </is>
       </c>
       <c r="E211" s="14" t="inlineStr">
@@ -18754,7 +18754,7 @@
       </c>
       <c r="D217" s="13" t="inlineStr">
         <is>
-          <t>maa://24636 (100.00), maa://25778 (86.02)</t>
+          <t>maa://24636 (100.00), maa://25778 (85.11)</t>
         </is>
       </c>
       <c r="E217" s="14" t="inlineStr">
@@ -18970,7 +18970,7 @@
       </c>
       <c r="D221" s="13" t="inlineStr">
         <is>
-          <t>maa://26499 (100.00), ***maa://20998 (2.86)</t>
+          <t>maa://26499 (100.00), ***maa://20998 (2.78)</t>
         </is>
       </c>
       <c r="E221" s="14" t="inlineStr">
@@ -19942,7 +19942,7 @@
       </c>
       <c r="D239" s="13" t="inlineStr">
         <is>
-          <t>maa://20922 (100.00), *maa://32623 (63.95), *maa://34242 (56.98)</t>
+          <t>maa://20922 (100.00), *maa://32623 (66.28), *maa://34242 (56.98)</t>
         </is>
       </c>
       <c r="E239" s="14" t="inlineStr">
@@ -20045,12 +20045,12 @@
       </c>
       <c r="C241" s="12" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D241" s="13" t="inlineStr">
         <is>
-          <t>maa://30667 (94.94), maa://30666 (100.00), **maa://30739 (35.44), *maa://30723 (56.96), maa://39588 (97.47), maa://64079 (84.81)</t>
+          <t>maa://30667 (94.94), maa://30666 (100.00), **maa://30739 (35.44), *maa://30723 (56.96), maa://39588 (97.47), maa://64079 (86.08), **maa://65726 (43.04)</t>
         </is>
       </c>
       <c r="E241" s="14" t="inlineStr">
@@ -20104,7 +20104,7 @@
       </c>
       <c r="D242" s="13" t="inlineStr">
         <is>
-          <t>maa://62759 (100.00), ***maa://62764 (24.42)</t>
+          <t>maa://62759 (100.00), ***maa://62764 (23.86)</t>
         </is>
       </c>
       <c r="E242" s="14" t="inlineStr">
@@ -20590,7 +20590,7 @@
       </c>
       <c r="D251" s="13" t="inlineStr">
         <is>
-          <t>maa://42287 (96.59), maa://45570 (100.00), *maa://60678 (76.14), maa://42225 (88.64)</t>
+          <t>maa://42287 (95.51), maa://45570 (100.00), *maa://60678 (75.28), maa://42225 (87.64)</t>
         </is>
       </c>
       <c r="E251" s="14" t="inlineStr">
@@ -20752,7 +20752,7 @@
       </c>
       <c r="D254" s="13" t="inlineStr">
         <is>
-          <t>maa://24093 (100.00), maa://31559 (89.47), maa://20924 (81.05), ***maa://49440 (16.84)</t>
+          <t>maa://31559 (89.47), maa://24093 (100.00), maa://20924 (81.05), ***maa://49440 (16.84)</t>
         </is>
       </c>
       <c r="E254" s="14" t="inlineStr">
@@ -21886,7 +21886,7 @@
       </c>
       <c r="D275" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://51630 (91.84), maa://56588 (83.67), **maa://55171 (41.84), *maa://51893 (61.22), ***maa://60902 (15.31)</t>
+          <t>maa://51881 (100.00), maa://51630 (92.86), maa://56588 (84.69), **maa://55171 (41.84), *maa://51893 (61.22), ***maa://60902 (19.39)</t>
         </is>
       </c>
       <c r="E275" s="14" t="inlineStr">
@@ -22480,7 +22480,7 @@
       </c>
       <c r="D286" s="13" t="inlineStr">
         <is>
-          <t>maa://48267 (100.00), maa://48266 (93.85)</t>
+          <t>maa://48267 (100.00), maa://48266 (89.71)</t>
         </is>
       </c>
       <c r="E286" s="14" t="inlineStr">
@@ -22642,7 +22642,7 @@
       </c>
       <c r="D289" s="13" t="inlineStr">
         <is>
-          <t>maa://20899 (100.00), maa://46332 (96.43), ***maa://44744 (5.95)</t>
+          <t>maa://20899 (100.00), maa://46332 (95.29), ***maa://44744 (5.88)</t>
         </is>
       </c>
       <c r="E289" s="14" t="inlineStr">
@@ -23074,7 +23074,7 @@
       </c>
       <c r="D297" s="13" t="inlineStr">
         <is>
-          <t>maa://32414 (100.00), maa://39155 (89.69), *maa://32505 (67.01)</t>
+          <t>maa://32414 (100.00), *maa://32505 (67.01), maa://39155 (89.69)</t>
         </is>
       </c>
       <c r="E297" s="14" t="inlineStr">
@@ -23128,7 +23128,7 @@
       </c>
       <c r="D298" s="13" t="inlineStr">
         <is>
-          <t>maa://45799 (100.00), maa://57199 (91.49)</t>
+          <t>maa://45799 (100.00), maa://57199 (92.55)</t>
         </is>
       </c>
       <c r="E298" s="14" t="inlineStr">
@@ -23560,7 +23560,7 @@
       </c>
       <c r="D306" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (100.00), maa://49642 (95.88), maa://49660 (84.54), *maa://50517 (50.52)</t>
+          <t>maa://50280 (100.00), maa://49642 (95.88), maa://49660 (85.57), *maa://50517 (50.52)</t>
         </is>
       </c>
       <c r="E306" s="14" t="inlineStr">
@@ -24262,7 +24262,7 @@
       </c>
       <c r="D319" s="13" t="inlineStr">
         <is>
-          <t>*maa://62755 (65.00), maa://62761 (100.00)</t>
+          <t>*maa://62755 (70.00), maa://62761 (100.00)</t>
         </is>
       </c>
       <c r="E319" s="14" t="inlineStr">
@@ -25450,7 +25450,7 @@
       </c>
       <c r="D341" s="22" t="inlineStr">
         <is>
-          <t>*maa://30671 (78.12), maa://30669 (100.00), *maa://37275 (71.88), **maa://32410 (37.50), *maa://41605 (67.71)</t>
+          <t>*maa://30671 (78.12), maa://30669 (100.00), *maa://37275 (69.79), **maa://32410 (37.50), *maa://41605 (67.71)</t>
         </is>
       </c>
       <c r="E341" s="22" t="inlineStr">
@@ -25828,7 +25828,7 @@
       </c>
       <c r="D348" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (100.00), maa://32415 (96.88), maa://34677 (96.88), maa://32892 (88.54), *maa://32653 (64.58), *maa://61839 (67.71), *maa://61275 (53.12)</t>
+          <t>maa://32647 (100.00), maa://32415 (90.62), maa://34677 (96.88), maa://32892 (88.54), *maa://32653 (64.58), *maa://61839 (75.00), *maa://61275 (53.12)</t>
         </is>
       </c>
       <c r="E348" s="22" t="inlineStr">
@@ -26314,7 +26314,7 @@
       </c>
       <c r="D357" s="22" t="inlineStr">
         <is>
-          <t>maa://36868 (100.00), maa://35996 (94.90), ***maa://39217 (20.41), maa://47349 (89.80)</t>
+          <t>maa://36868 (100.00), maa://35996 (94.90), ***maa://39217 (20.41), maa://47349 (91.84)</t>
         </is>
       </c>
       <c r="E357" s="22" t="inlineStr">
@@ -26368,7 +26368,7 @@
       </c>
       <c r="D358" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.00), maa://49695 (100.00), maa://49758 (92.00), **maa://59402 (39.00), **maa://52357 (48.00), ***maa://63091 (25.00)</t>
+          <t>maa://49696 (99.00), maa://49695 (100.00), maa://49758 (92.00), **maa://59402 (41.00), **maa://52357 (48.00), ***maa://63091 (25.00)</t>
         </is>
       </c>
       <c r="E358" s="22" t="inlineStr">
@@ -26530,7 +26530,7 @@
       </c>
       <c r="D361" s="22" t="inlineStr">
         <is>
-          <t>maa://49648 (100.00), *maa://49662 (71.91)</t>
+          <t>maa://49648 (100.00), *maa://49662 (74.16)</t>
         </is>
       </c>
       <c r="E361" s="22" t="inlineStr">
@@ -26692,7 +26692,7 @@
       </c>
       <c r="D364" s="22" t="inlineStr">
         <is>
-          <t>maa://42635 (100.00), *maa://50629 (52.38), **maa://48859 (40.48)</t>
+          <t>maa://42635 (100.00), **maa://50629 (35.71), **maa://48859 (40.48)</t>
         </is>
       </c>
       <c r="E364" s="22" t="inlineStr">
@@ -26854,7 +26854,7 @@
       </c>
       <c r="D367" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (100.00), maa://48026 (95.70), maa://44635 (87.10), maa://41035 (91.40), maa://44660 (87.10), *maa://60251 (56.99), *maa://41128 (75.27)</t>
+          <t>maa://40957 (100.00), maa://48026 (95.70), maa://44635 (87.10), maa://41035 (92.47), maa://44660 (87.10), *maa://60251 (56.99), *maa://41128 (75.27)</t>
         </is>
       </c>
       <c r="E367" s="22" t="inlineStr">
@@ -26962,7 +26962,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://63883 (100.00), maa://64045 (84.42), **maa://64041 (38.96)</t>
+          <t>maa://63883 (100.00), maa://64045 (82.76), **maa://64041 (34.48)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -27502,7 +27502,7 @@
       </c>
       <c r="D379" s="22" t="inlineStr">
         <is>
-          <t>maa://44233 (92.05), maa://45570 (100.00)</t>
+          <t>maa://44233 (92.13), maa://45570 (100.00)</t>
         </is>
       </c>
       <c r="E379" s="22" t="inlineStr">
@@ -27772,7 +27772,7 @@
       </c>
       <c r="D384" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (81.05), maa://44745 (100.00), ***maa://49516 (26.32), **maa://45952 (37.89), ***maa://46851 (2.11), **maa://44896 (47.37)</t>
+          <t>*maa://42970 (80.00), maa://44745 (100.00), ***maa://49516 (26.32), **maa://45952 (34.74), ***maa://46851 (2.11), **maa://44896 (47.37)</t>
         </is>
       </c>
       <c r="E384" s="22" t="inlineStr">
@@ -28096,7 +28096,7 @@
       </c>
       <c r="D390" s="22" t="inlineStr">
         <is>
-          <t>maa://63890 (100.00), ***maa://64043 (25.61)</t>
+          <t>maa://63890 (100.00), ***maa://64043 (24.14)</t>
         </is>
       </c>
       <c r="E390" s="22" t="inlineStr">
@@ -28366,7 +28366,7 @@
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>maa://51898 (100.00), *maa://57241 (76.47)</t>
+          <t>maa://51898 (100.00), *maa://57241 (80.00)</t>
         </is>
       </c>
       <c r="E397" t="inlineStr">
@@ -28420,7 +28420,7 @@
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>maa://51872 (100.00), maa://51876 (100.00), *maa://63228 (76.84), maa://51873 (96.84), *maa://62047 (75.79)</t>
+          <t>maa://51872 (100.00), maa://51876 (100.00), *maa://63228 (74.74), maa://51873 (97.89), *maa://62047 (76.84)</t>
         </is>
       </c>
       <c r="E399" t="inlineStr">
@@ -28577,12 +28577,12 @@
       </c>
       <c r="C405" s="17" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>maa://64040 (100.00), ***maa://65803 (21.65)</t>
+          <t>maa://64040 (100.00), ***maa://66377 (21.65), ***maa://66376 (21.65)</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#230)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -771,12 +771,12 @@
       </c>
       <c r="S2" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (100.00)</t>
+          <t>maa://22742 (100.00), ***maa://66635 (23.86)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://25251 (100.00), maa://59087 (96.51)</t>
+          <t>maa://59087 (93.10), maa://25251 (100.00)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>*maa://22880 (72.62), maa://20276 (100.00), *maa://22749 (75.00)</t>
+          <t>*maa://22880 (73.81), maa://20276 (100.00), *maa://22749 (75.00)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://45854 (85.88), maa://24617 (100.00), maa://60545 (85.88)</t>
+          <t>maa://45854 (85.88), maa://24617 (100.00), maa://60545 (82.35)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (100.00), maa://50121 (95.56)</t>
+          <t>maa://49983 (100.00), maa://50121 (97.75)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://32509 (100.00), maa://27295 (91.11), maa://22754 (88.89), *maa://31008 (72.22)</t>
+          <t>maa://32509 (100.00), maa://27295 (92.22), maa://22754 (88.89), *maa://31008 (72.22)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>maa://39394 (100.00), maa://30062 (94.34), ***maa://26209 (9.43)</t>
+          <t>maa://39394 (100.00), maa://30062 (98.04), ***maa://26209 (9.80)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="P5" s="8" t="inlineStr">
         <is>
-          <t>maa://21919 (100.00), *maa://21281 (60.44)</t>
+          <t>maa://21919 (100.00), *maa://21281 (59.78)</t>
         </is>
       </c>
       <c r="Q5" s="19" t="n"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>*maa://64972 (69.39)</t>
+          <t>maa://64972 (89.80)</t>
         </is>
       </c>
       <c r="I7" s="19" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.30 13:19:59</t>
+          <t>更新日期：2025.08.31 13:19:07</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (87.64), maa://23252 (93.26), maa://37496 (100.00)</t>
+          <t>maa://32931 (86.52), maa://23252 (93.26), maa://37496 (100.00)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>maa://24479 (100.00), **maa://21990 (48.53)</t>
+          <t>maa://24479 (100.00), **maa://21990 (47.83)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://26223 (100.00), maa://52237 (86.32)</t>
+          <t>maa://26223 (100.00), maa://52237 (87.37)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (100.00), maa://40166 (97.56)</t>
+          <t>maa://28711 (100.00), maa://40166 (96.39)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (100.00), **maa://22865 (45.24)</t>
+          <t>maa://26206 (100.00), **maa://22865 (44.71)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>***maa://25695 (26.92), ***maa://39951 (11.54), maa://45271 (100.00), ***maa://34206 (21.15), ***maa://39243 (13.46), **maa://54000 (44.23)</t>
+          <t>***maa://25695 (26.92), ***maa://39951 (11.54), maa://45271 (100.00), ***maa://34206 (21.15), ***maa://39243 (13.46), *maa://54000 (69.23)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1821,12 +1821,12 @@
       </c>
       <c r="S10" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (100.00), maa://22755 (88.30), *maa://63521 (51.06)</t>
+          <t>maa://27395 (100.00), maa://22755 (88.30)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (89.47), maa://22501 (100.00), maa://45521 (88.42), **maa://64808 (46.32)</t>
+          <t>maa://22747 (89.47), maa://22501 (100.00), maa://45521 (89.47), *maa://64808 (64.21)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="AB11" s="8" t="inlineStr">
         <is>
-          <t>maa://29912 (100.00), maa://22516 (84.95)</t>
+          <t>maa://29912 (100.00), maa://22516 (84.04)</t>
         </is>
       </c>
       <c r="AC11" s="19" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (100.00), maa://54294 (86.05)</t>
+          <t>maa://21867 (100.00), *maa://54294 (77.91)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (90.00), maa://64046 (100.00)</t>
+          <t>maa://63896 (88.76), maa://64046 (100.00)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://22753 (100.00), maa://37962 (95.45), *maa://21485 (78.41)</t>
+          <t>maa://22753 (100.00), maa://37962 (95.45), *maa://21485 (77.27)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://23669 (100.00), maa://36677 (95.65), maa://39872 (89.13)</t>
+          <t>maa://36677 (95.65), maa://23669 (100.00), maa://39872 (89.13)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>maa://28932 (100.00), *maa://20106 (76.39), *maa://22769 (61.11)</t>
+          <t>maa://28932 (100.00), *maa://20106 (75.34), *maa://22769 (60.27)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (100.00), maa://36673 (94.51), maa://25001 (84.62)</t>
+          <t>maa://24999 (100.00), maa://36673 (95.60), maa://25001 (84.62)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>maa://21248 (100.00), **maa://66545 (50.00)</t>
+          <t>maa://21248 (100.00), *maa://66545 (64.71)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (100.00), *maa://22583 (78.89), *maa://48321 (56.67)</t>
+          <t>maa://22676 (100.00), *maa://22583 (78.89), *maa://48321 (58.89)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (100.00), **maa://39885 (45.68)</t>
+          <t>maa://39883 (100.00), **maa://39885 (44.44)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://22521 (100.00), maa://42751 (91.01)</t>
+          <t>maa://22521 (100.00), maa://42751 (92.13)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (96.10), maa://22734 (100.00), *maa://30808 (64.94), maa://36048 (84.42), maa://45058 (87.01)</t>
+          <t>maa://22743 (96.10), maa://22734 (100.00), *maa://30808 (66.23), maa://36048 (85.71), maa://45058 (90.91)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://22729 (100.00), *maa://28648 (74.44), *maa://36674 (78.89)</t>
+          <t>maa://22729 (100.00), *maa://36674 (80.00), *maa://28648 (75.56)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>*maa://23911 (71.59), maa://27755 (100.00)</t>
+          <t>*maa://23911 (72.73), maa://27755 (100.00)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://39599 (95.29), maa://22430 (100.00)</t>
+          <t>maa://39599 (95.35), maa://22430 (100.00)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (100.00), *maa://24940 (67.12), *maa://56238 (72.60)</t>
+          <t>maa://23890 (100.00), *maa://24940 (67.12), *maa://56238 (76.71)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://22466 (97.78), maa://52226 (100.00)</t>
+          <t>maa://52226 (100.00), maa://22466 (96.70)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), maa://54153 (86.32), *maa://24380 (68.42)</t>
+          <t>maa://24379 (100.00), maa://54153 (88.42), *maa://24380 (68.42)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://24313 (89.83), maa://47854 (100.00), *maa://29784 (54.24)</t>
+          <t>maa://47854 (100.00), maa://24313 (89.83), *maa://29784 (54.24)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -3007,12 +3007,12 @@
       </c>
       <c r="W19" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X19" s="8" t="inlineStr">
         <is>
-          <t>maa://31386 (100.00), **maa://58490 (35.29)</t>
+          <t>maa://31386 (100.00)</t>
         </is>
       </c>
       <c r="Y19" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (100.00), maa://49976 (94.12), maa://56241 (82.35)</t>
+          <t>maa://50085 (100.00), maa://49976 (93.02), maa://56241 (81.40)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (100.00), maa://20110 (88.37)</t>
+          <t>maa://34946 (100.00), maa://20110 (87.36)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22524 (100.00), maa://22432 (100.00), *maa://64221 (56.96)</t>
+          <t>maa://22524 (100.00), maa://22432 (100.00), *maa://64221 (60.26)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>maa://27127 (100.00), maa://22751 (88.24)</t>
+          <t>maa://22751 (89.55), maa://27127 (100.00)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://21282 (100.00), *maa://37649 (63.92)</t>
+          <t>*maa://37649 (64.95), maa://21282 (100.00)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>*maa://28036 (66.67), maa://41753 (100.00)</t>
+          <t>*maa://28036 (68.97), maa://41753 (100.00)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (100.00), maa://39875 (92.55)</t>
+          <t>maa://39756 (100.00), maa://39875 (93.62)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (100.00), *maa://29748 (78.41), *maa://37566 (76.14)</t>
+          <t>maa://30587 (100.00), *maa://29748 (78.41), *maa://37566 (73.86)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (89.01), maa://23504 (100.00), *maa://25141 (76.92), *maa://36663 (75.82), maa://52227 (85.71)</t>
+          <t>maa://29988 (90.11), maa://23504 (100.00), *maa://25141 (76.92), *maa://36663 (76.92), maa://52227 (86.81)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://22523 (87.21), *maa://36672 (68.60), maa://29910 (100.00), maa://45831 (86.05), maa://64165 (88.37)</t>
+          <t>maa://22523 (87.21), *maa://36672 (68.60), maa://29910 (100.00), maa://45831 (88.37), maa://64165 (81.40)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (100.00), *maa://63016 (77.42)</t>
+          <t>maa://29753 (100.00), *maa://63016 (79.57)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>maa://29063 (93.94), maa://25311 (100.00), ***maa://22725 (3.03), maa://45047 (80.30)</t>
+          <t>maa://29063 (95.38), maa://25311 (100.00), ***maa://22725 (3.08), maa://45047 (81.54)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://41802 (100.00), maa://56374 (86.42)</t>
+          <t>maa://41802 (100.00), maa://56374 (85.37)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="P26" s="8" t="inlineStr">
         <is>
-          <t>maa://39870 (91.18), maa://56625 (100.00)</t>
+          <t>maa://56625 (100.00), maa://39870 (88.57)</t>
         </is>
       </c>
       <c r="Q26" s="19" t="n"/>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="AF26" s="8" t="inlineStr">
         <is>
-          <t>maa://30511 (100.00), **maa://29760 (48.33)</t>
+          <t>maa://30511 (100.00), **maa://29760 (45.00)</t>
         </is>
       </c>
       <c r="AG26" s="16" t="n"/>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (100.00), maa://41749 (97.78)</t>
+          <t>maa://39929 (100.00), maa://41749 (98.89)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (100.00), *maa://65700 (54.44)</t>
+          <t>maa://36660 (100.00), *maa://65700 (68.89)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://24080 (90.14), maa://42865 (100.00), ***maa://34960 (2.82)</t>
+          <t>maa://24080 (88.89), maa://42865 (100.00), ***maa://34960 (2.78)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (100.00), maa://36258 (92.31), *maa://43904 (56.04)</t>
+          <t>maa://35926 (100.00), maa://36258 (91.21), *maa://43904 (58.24)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4556,7 +4556,7 @@
       </c>
       <c r="T31" s="8" t="inlineStr">
         <is>
-          <t>maa://30711 (100.00), **maa://30768 (48.89)</t>
+          <t>maa://30711 (100.00), **maa://30768 (50.00)</t>
         </is>
       </c>
       <c r="U31" s="19" t="n"/>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (100.00), *maa://41108 (77.89), maa://41238 (100.00), maa://45523 (98.95)</t>
+          <t>maa://42859 (98.96), *maa://41108 (77.08), maa://41238 (100.00), maa://45523 (97.92)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (100.00), *maa://22730 (73.68)</t>
+          <t>maa://21956 (100.00), *maa://22730 (72.73)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (100.00), *maa://56235 (75.27)</t>
+          <t>maa://48817 (100.00), *maa://56235 (77.42)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (100.00), *maa://56336 (69.07), *maa://47069 (59.79), *maa://45789 (67.01)</t>
+          <t>maa://45718 (100.00), *maa://56336 (74.23), *maa://47069 (59.79), *maa://45789 (67.01)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://24709 (100.00), maa://47093 (94.25)</t>
+          <t>maa://24709 (100.00), maa://47093 (93.18)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (100.00), *maa://45788 (70.73), *maa://45790 (78.05)</t>
+          <t>maa://47079 (100.00), *maa://45788 (72.50), maa://45790 (81.25)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5636,7 +5636,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (100.00), maa://21386 (98.92), maa://36664 (83.87), *maa://45550 (52.69)</t>
+          <t>maa://23278 (100.00), maa://21386 (100.00), maa://36664 (84.78), *maa://45550 (53.26)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5679,12 +5679,12 @@
       </c>
       <c r="AE40" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>*maa://64107 (62.96), maa://64205 (100.00), maa://65283 (86.42)</t>
+          <t>maa://64205 (100.00), *maa://65283 (73.17)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>maa://22525 (85.19), maa://21284 (100.00)</t>
+          <t>maa://22525 (83.95), maa://21284 (100.00)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -5992,7 +5992,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (100.00), maa://27728 (95.79), maa://56386 (82.11)</t>
+          <t>maa://29768 (100.00), maa://27728 (94.79), maa://56386 (87.50)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6146,7 +6146,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (100.00), maa://43901 (94.38)</t>
+          <t>maa://35931 (100.00), maa://43901 (96.59)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6215,7 +6215,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (100.00), maa://29661 (98.95), *maa://56236 (73.68), *maa://28038 (61.05)</t>
+          <t>maa://27410 (100.00), maa://29661 (98.95), maa://56236 (82.11), *maa://28038 (61.05)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6490,7 +6490,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (100.00), maa://59378 (90.53), *maa://65511 (71.58)</t>
+          <t>maa://59394 (100.00), maa://59378 (92.47), maa://65511 (81.72)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6750,7 +6750,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (100.00), maa://43903 (89.89), *maa://56228 (76.40)</t>
+          <t>maa://42981 (100.00), maa://56228 (85.39), maa://43903 (91.01)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6763,12 +6763,12 @@
       </c>
       <c r="G63" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (100.00), *maa://59693 (60.64), *maa://59413 (74.47)</t>
+          <t>maa://59534 (100.00), maa://59413 (80.85)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7090,7 +7090,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.30 13:19:59</t>
+          <t>更新日期：2025.08.31 13:19:07</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8494,7 +8494,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (72.29), *maa://28758 (67.47), maa://29036 (100.00), *maa://42172 (55.42), *maa://65357 (74.70), maa://30285 (81.93)</t>
+          <t>*maa://20849 (72.29), *maa://28758 (67.47), maa://29036 (100.00), *maa://42172 (55.42), *maa://65357 (78.31), maa://30285 (81.93)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -9682,7 +9682,7 @@
       </c>
       <c r="D49" s="13" t="inlineStr">
         <is>
-          <t>maa://32845 (100.00), *maa://20982 (52.63)</t>
+          <t>maa://32845 (100.00), *maa://20982 (51.72)</t>
         </is>
       </c>
       <c r="E49" s="14" t="inlineStr">
@@ -10708,7 +10708,7 @@
       </c>
       <c r="D68" s="13" t="inlineStr">
         <is>
-          <t>maa://20976 (100.00), maa://20815 (83.33)</t>
+          <t>maa://20976 (100.00), maa://20815 (84.21)</t>
         </is>
       </c>
       <c r="E68" s="14" t="inlineStr">
@@ -10762,7 +10762,7 @@
       </c>
       <c r="D69" s="13" t="inlineStr">
         <is>
-          <t>maa://20974 (100.00), *maa://29079 (73.63), maa://29096 (86.81), maa://29087 (92.31), *maa://20823 (53.85), maa://20855 (80.22), maa://20904 (84.62), **maa://63722 (48.35)</t>
+          <t>maa://20974 (100.00), *maa://29079 (73.63), maa://29096 (86.81), maa://29087 (92.31), **maa://20823 (45.05), maa://20855 (80.22), maa://20904 (84.62), **maa://63722 (48.35)</t>
         </is>
       </c>
       <c r="E69" s="14" t="inlineStr">
@@ -10919,12 +10919,12 @@
       </c>
       <c r="C72" s="12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D72" s="13" t="inlineStr">
         <is>
-          <t>maa://36643 (100.00), maa://36864 (95.88), maa://39140 (94.85)</t>
+          <t>maa://36643 (100.00), maa://36864 (95.88), maa://39140 (94.85), **maa://66335 (35.05)</t>
         </is>
       </c>
       <c r="E72" s="14" t="inlineStr">
@@ -12598,7 +12598,7 @@
       </c>
       <c r="D103" s="13" t="inlineStr">
         <is>
-          <t>maa://29094 (86.49), maa://28904 (100.00), **maa://20931 (39.19)</t>
+          <t>maa://29094 (84.00), maa://28904 (100.00), **maa://20931 (41.33)</t>
         </is>
       </c>
       <c r="E103" s="14" t="inlineStr">
@@ -12868,7 +12868,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://25018 (96.94), maa://25776 (85.71), maa://28361 (86.73), maa://25772 (85.71), maa://56588 (84.69), *maa://45194 (66.33), *maa://25161 (62.24), *maa://32653 (63.27), *maa://61839 (73.47), ***maa://60902 (19.39), *maa://61275 (52.04)</t>
+          <t>maa://51881 (100.00), maa://25018 (96.94), maa://25776 (85.71), maa://28361 (86.73), maa://25772 (85.71), maa://56588 (84.69), *maa://45194 (66.33), *maa://32653 (63.27), *maa://25161 (62.24), *maa://61839 (73.47), ***maa://60902 (19.39), *maa://61275 (52.04)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -15082,7 +15082,7 @@
       </c>
       <c r="D149" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (95.88), maa://36641 (100.00), maa://36865 (93.81), maa://44635 (83.51), maa://44660 (83.51), *maa://41128 (72.16), maa://42918 (92.78), maa://44119 (89.69), maa://46108 (89.69), *maa://37300 (58.76), *maa://64408 (70.10), **maa://42917 (35.05)</t>
+          <t>maa://40957 (95.88), maa://36641 (100.00), maa://36865 (93.81), maa://44635 (83.51), maa://44660 (83.51), *maa://41128 (72.16), maa://42918 (92.78), maa://46108 (89.69), maa://44119 (89.69), *maa://37300 (58.76), *maa://64408 (72.16), **maa://42917 (35.05)</t>
         </is>
       </c>
       <c r="E149" s="14" t="inlineStr">
@@ -15622,7 +15622,7 @@
       </c>
       <c r="D159" s="13" t="inlineStr">
         <is>
-          <t>maa://44232 (100.00), *maa://45603 (78.35), ***maa://63114 (21.65), ***maa://65963 (9.28)</t>
+          <t>maa://44232 (100.00), *maa://45603 (78.35), ***maa://63114 (21.65), ***maa://65963 (21.65)</t>
         </is>
       </c>
       <c r="E159" s="14" t="inlineStr">
@@ -15838,7 +15838,7 @@
       </c>
       <c r="D163" s="13" t="inlineStr">
         <is>
-          <t>*maa://32845 (64.04), maa://29054 (100.00)</t>
+          <t>*maa://32845 (65.17), maa://29054 (100.00)</t>
         </is>
       </c>
       <c r="E163" s="14" t="inlineStr">
@@ -16108,7 +16108,7 @@
       </c>
       <c r="D168" s="13" t="inlineStr">
         <is>
-          <t>maa://49867 (97.73), maa://49655 (100.00)</t>
+          <t>maa://49867 (98.86), maa://49655 (100.00)</t>
         </is>
       </c>
       <c r="E168" s="14" t="inlineStr">
@@ -16432,7 +16432,7 @@
       </c>
       <c r="D174" s="13" t="inlineStr">
         <is>
-          <t>maa://59681 (100.00), maa://64200 (82.98)</t>
+          <t>maa://59681 (100.00), maa://64200 (85.11)</t>
         </is>
       </c>
       <c r="E174" s="14" t="inlineStr">
@@ -16486,7 +16486,7 @@
       </c>
       <c r="D175" s="13" t="inlineStr">
         <is>
-          <t>maa://32418 (100.00), maa://51440 (89.90), maa://63320 (88.89)</t>
+          <t>maa://32418 (100.00), maa://51440 (89.90), maa://63320 (89.90)</t>
         </is>
       </c>
       <c r="E175" s="14" t="inlineStr">
@@ -17782,7 +17782,7 @@
       </c>
       <c r="D199" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (98.72), *maa://28190 (58.97), maa://22894 (100.00), *maa://20906 (62.82), ***maa://20907 (26.92)</t>
+          <t>maa://27823 (98.72), *maa://28190 (58.97), maa://22894 (100.00), *maa://20906 (62.82), ***maa://20907 (25.64)</t>
         </is>
       </c>
       <c r="E199" s="14" t="inlineStr">
@@ -17836,7 +17836,7 @@
       </c>
       <c r="D200" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (98.72), *maa://28190 (58.97), maa://22894 (100.00), *maa://20906 (62.82), ***maa://20907 (26.92)</t>
+          <t>maa://27823 (98.72), *maa://28190 (58.97), maa://22894 (100.00), *maa://20906 (62.82), ***maa://20907 (25.64)</t>
         </is>
       </c>
       <c r="E200" s="14" t="inlineStr">
@@ -20968,7 +20968,7 @@
       </c>
       <c r="D258" s="13" t="inlineStr">
         <is>
-          <t>maa://20879 (100.00), maa://20834 (89.61)</t>
+          <t>maa://20879 (100.00), maa://20834 (88.46)</t>
         </is>
       </c>
       <c r="E258" s="14" t="inlineStr">
@@ -25828,7 +25828,7 @@
       </c>
       <c r="D348" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (100.00), maa://32415 (90.62), maa://34677 (96.88), maa://32892 (88.54), *maa://32653 (64.58), *maa://61839 (75.00), *maa://61275 (53.12)</t>
+          <t>maa://32647 (100.00), maa://32415 (85.42), maa://34677 (96.88), maa://32892 (88.54), *maa://32653 (64.58), *maa://61839 (75.00), *maa://61275 (53.12)</t>
         </is>
       </c>
       <c r="E348" s="22" t="inlineStr">
@@ -28582,7 +28582,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>maa://64040 (100.00), ***maa://66377 (21.65), ***maa://66376 (21.65)</t>
+          <t>maa://64040 (100.00), *maa://66377 (53.12), ***maa://66376 (21.88)</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#231)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://39402 (100.00), *maa://34787 (74.71), maa://58660 (91.95)</t>
+          <t>maa://39402 (100.00), maa://58660 (94.25), *maa://34787 (74.71)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -776,7 +776,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (100.00), ***maa://66635 (23.86)</t>
+          <t>maa://22742 (100.00), *maa://66635 (64.77)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://59087 (93.10), maa://25251 (100.00)</t>
+          <t>maa://59087 (87.36), maa://25251 (100.00)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>*maa://22880 (73.81), maa://20276 (100.00), *maa://22749 (75.00)</t>
+          <t>*maa://22880 (75.00), maa://20276 (100.00), *maa://22749 (75.00)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://45854 (85.88), maa://24617 (100.00), maa://60545 (82.35)</t>
+          <t>maa://45854 (85.88), *maa://60545 (78.82), maa://24617 (100.00)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://24390 (100.00), maa://52241 (92.22)</t>
+          <t>maa://52241 (95.56), maa://24390 (100.00)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (100.00), *maa://22499 (75.28), *maa://22746 (68.54)</t>
+          <t>maa://24632 (100.00), *maa://22499 (76.14), *maa://22746 (69.32)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (100.00), maa://50121 (97.75)</t>
+          <t>maa://49983 (100.00), maa://50121 (98.86)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://32509 (100.00), maa://27295 (92.22), maa://22754 (88.89), *maa://31008 (72.22)</t>
+          <t>maa://32509 (100.00), maa://27295 (92.22), maa://22754 (87.78), *maa://31008 (72.22)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>maa://39394 (100.00), maa://30062 (98.04), ***maa://26209 (9.80)</t>
+          <t>maa://39394 (100.00), maa://30062 (100.00), ***maa://26209 (10.00)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (100.00), maa://54105 (98.73), *maa://22744 (78.48)</t>
+          <t>maa://21245 (100.00), maa://54105 (100.00), *maa://22744 (78.48)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="AB5" s="8" t="inlineStr">
         <is>
-          <t>maa://29863 (100.00), ***maa://22752 (6.12), **maa://26013 (34.69)</t>
+          <t>maa://29863 (100.00), ***maa://22752 (6.25), **maa://26013 (31.25)</t>
         </is>
       </c>
       <c r="AC5" s="19" t="n"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="AF6" s="8" t="inlineStr">
         <is>
-          <t>maa://33152 (100.00), ***maa://22770 (24.53)</t>
+          <t>maa://33152 (100.00), ***maa://22770 (24.07)</t>
         </is>
       </c>
       <c r="AG6" s="16" t="n"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>maa://64972 (89.80)</t>
+          <t>maa://64972 (100.00)</t>
         </is>
       </c>
       <c r="I7" s="19" t="n"/>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (100.00), *maa://22758 (76.92)</t>
+          <t>maa://22399 (100.00), *maa://22758 (78.02)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.31 13:19:07</t>
+          <t>更新日期：2025.09.02 13:21:02</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (100.00), *maa://39431 (51.52), **maa://37551 (33.33)</t>
+          <t>maa://21476 (100.00), *maa://39431 (53.12), **maa://37551 (34.38)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (86.52), maa://23252 (93.26), maa://37496 (100.00)</t>
+          <t>maa://32931 (85.39), maa://23252 (93.26), maa://37496 (100.00)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>maa://24479 (100.00), **maa://21990 (47.83)</t>
+          <t>maa://24479 (100.00), **maa://21990 (48.53)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (100.00), *maa://39552 (70.93)</t>
+          <t>maa://22762 (100.00), *maa://39552 (63.22)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1680,7 +1680,7 @@
       </c>
       <c r="P9" s="8" t="inlineStr">
         <is>
-          <t>maa://22736 (100.00), ***maa://64516 (27.63)</t>
+          <t>maa://22736 (100.00), *maa://64516 (75.00)</t>
         </is>
       </c>
       <c r="Q9" s="19" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://26223 (100.00), maa://52237 (87.37)</t>
+          <t>maa://52237 (90.53), maa://26223 (100.00)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (100.00), maa://40166 (96.39)</t>
+          <t>maa://28711 (100.00), maa://40166 (95.18)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1739,12 +1739,12 @@
       </c>
       <c r="AE9" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (100.00), **maa://22865 (44.71)</t>
+          <t>maa://26206 (100.00)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>***maa://25695 (26.92), ***maa://39951 (11.54), maa://45271 (100.00), ***maa://34206 (21.15), ***maa://39243 (13.46), *maa://54000 (69.23)</t>
+          <t>***maa://25695 (25.49), ***maa://39951 (11.76), maa://45271 (100.00), ***maa://34206 (21.57), maa://54000 (88.24), ***maa://39243 (13.73)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (100.00), maa://36669 (81.25), *maa://23264 (61.25)</t>
+          <t>maa://28977 (100.00), maa://36669 (83.12), *maa://23264 (63.64)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://45828 (90.53), maa://22301 (100.00), maa://22726 (82.11)</t>
+          <t>maa://45828 (91.58), maa://22301 (100.00), maa://22726 (82.11)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>maa://25021 (82.69), maa://22733 (100.00), ***maa://22761 (11.54)</t>
+          <t>maa://25021 (84.31), maa://22733 (100.00), ***maa://22761 (11.76)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (89.47), maa://22501 (100.00), maa://45521 (89.47), *maa://64808 (64.21)</t>
+          <t>maa://22747 (90.53), maa://22501 (100.00), maa://45521 (89.47), *maa://64808 (75.79)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="AB11" s="8" t="inlineStr">
         <is>
-          <t>maa://29912 (100.00), maa://22516 (84.04)</t>
+          <t>maa://29912 (100.00), maa://22516 (82.98)</t>
         </is>
       </c>
       <c r="AC11" s="19" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (100.00), *maa://54294 (77.91)</t>
+          <t>maa://21867 (100.00), *maa://54294 (76.74)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (88.76), maa://64046 (100.00)</t>
+          <t>maa://63896 (88.89), maa://64046 (100.00)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://22753 (100.00), maa://37962 (95.45), *maa://21485 (77.27)</t>
+          <t>*maa://21485 (77.27), maa://37962 (95.45), maa://22753 (100.00)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://36677 (95.65), maa://23669 (100.00), maa://39872 (89.13)</t>
+          <t>maa://36677 (96.74), maa://23669 (100.00), maa://39872 (89.13)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>maa://21248 (100.00), *maa://66545 (64.71)</t>
+          <t>maa://21248 (100.00), maa://66545 (86.57)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (100.00), *maa://22583 (78.89), *maa://48321 (58.89)</t>
+          <t>maa://22676 (100.00), *maa://48321 (60.00), *maa://22583 (78.89)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2259,12 +2259,12 @@
       </c>
       <c r="AE13" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (100.00), **maa://39885 (44.44)</t>
+          <t>maa://39883 (100.00)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (96.77), maa://26245 (100.00), maa://21288 (98.92), maa://36682 (90.32)</t>
+          <t>maa://39841 (95.70), maa://26245 (100.00), maa://21288 (98.92), maa://36682 (90.32)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://22521 (100.00), maa://42751 (92.13)</t>
+          <t>maa://22521 (100.00), maa://42751 (88.76)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (96.10), maa://22734 (100.00), *maa://30808 (66.23), maa://36048 (85.71), maa://45058 (90.91)</t>
+          <t>maa://22743 (94.81), maa://22734 (100.00), *maa://30808 (67.53), maa://45058 (90.91), maa://36048 (85.71)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://21364 (100.00), maa://36666 (100.00), *maa://22766 (78.21)</t>
+          <t>maa://36666 (100.00), maa://21364 (100.00), *maa://22766 (78.21)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://37650 (97.85), maa://21441 (100.00), maa://36679 (91.40)</t>
+          <t>maa://37650 (96.77), maa://21441 (100.00), maa://36679 (91.40)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>*maa://23911 (72.73), maa://27755 (100.00)</t>
+          <t>*maa://23911 (74.71), maa://27755 (100.00)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2672,7 +2672,7 @@
       </c>
       <c r="D17" s="8" t="inlineStr">
         <is>
-          <t>maa://21624 (100.00), **maa://56358 (46.58)</t>
+          <t>maa://21624 (100.00), *maa://56358 (69.86)</t>
         </is>
       </c>
       <c r="E17" s="19" t="n"/>
@@ -2715,12 +2715,12 @@
       </c>
       <c r="O17" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (100.00), *maa://24940 (67.12), *maa://56238 (76.71)</t>
+          <t>maa://23890 (100.00), maa://56238 (84.93)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://52226 (100.00), maa://22466 (96.70)</t>
+          <t>maa://52226 (100.00), maa://22466 (97.78)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), maa://54153 (88.42), *maa://24380 (68.42)</t>
+          <t>maa://24379 (100.00), maa://54153 (90.53), *maa://24380 (68.42)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://47854 (100.00), maa://24313 (89.83), *maa://29784 (54.24)</t>
+          <t>maa://47854 (100.00), maa://24313 (88.33), *maa://29784 (53.33)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -2946,11 +2946,7 @@
           <t>0</t>
         </is>
       </c>
-      <c r="H19" s="8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="H19" s="8" t="inlineStr"/>
       <c r="I19" s="19" t="n"/>
       <c r="J19" s="19" t="inlineStr">
         <is>
@@ -3028,7 +3024,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (100.00), *maa://36668 (75.76)</t>
+          <t>maa://30709 (100.00), *maa://36668 (74.63)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3044,7 +3040,7 @@
       </c>
       <c r="AF19" s="8" t="inlineStr">
         <is>
-          <t>maa://21663 (100.00), *maa://52239 (71.70)</t>
+          <t>maa://21663 (100.00), **maa://52239 (47.17)</t>
         </is>
       </c>
       <c r="AG19" s="16" t="n"/>
@@ -3062,7 +3058,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://21432 (98.86), maa://25198 (100.00), maa://36680 (88.64)</t>
+          <t>maa://21432 (97.75), maa://25198 (100.00), maa://36680 (89.89)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3142,7 +3138,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (100.00), maa://49976 (93.02), maa://56241 (81.40)</t>
+          <t>maa://50085 (100.00), maa://56241 (86.05), maa://49976 (93.02)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3304,7 +3300,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22524 (100.00), maa://22432 (100.00), *maa://64221 (60.26)</t>
+          <t>maa://22524 (98.73), maa://22432 (100.00), *maa://64221 (77.22)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3349,12 +3345,12 @@
       </c>
       <c r="K22" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>maa://22751 (89.55), maa://27127 (100.00)</t>
+          <t>maa://27127 (100.00), maa://22751 (88.24), **maa://66865 (30.88)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3402,7 +3398,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>*maa://37649 (64.95), maa://21282 (100.00)</t>
+          <t>*maa://37649 (65.98), maa://21282 (100.00)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3452,7 +3448,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>*maa://28036 (68.97), maa://41753 (100.00)</t>
+          <t>*maa://28036 (72.41), maa://41753 (100.00)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3500,7 +3496,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (100.00), *maa://29748 (78.41), *maa://37566 (73.86)</t>
+          <t>maa://30587 (100.00), *maa://29748 (77.53), *maa://37566 (73.03)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3516,7 +3512,7 @@
       </c>
       <c r="T23" s="8" t="inlineStr">
         <is>
-          <t>maa://31212 (100.00), maa://24387 (90.79)</t>
+          <t>maa://31212 (100.00), maa://24387 (93.24)</t>
         </is>
       </c>
       <c r="U23" s="19" t="n"/>
@@ -3582,7 +3578,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (100.00), *maa://46650 (71.05)</t>
+          <t>maa://24368 (100.00), *maa://46650 (73.68)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3662,7 +3658,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (90.11), maa://23504 (100.00), *maa://25141 (76.92), *maa://36663 (76.92), maa://52227 (86.81)</t>
+          <t>maa://29988 (90.11), maa://23504 (100.00), *maa://25141 (76.92), *maa://36663 (76.92), maa://52227 (85.71)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3694,7 +3690,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://22523 (87.21), *maa://36672 (68.60), maa://29910 (100.00), maa://45831 (88.37), maa://64165 (81.40)</t>
+          <t>maa://22523 (87.21), *maa://36672 (68.60), maa://64165 (91.86), maa://29910 (100.00), maa://45831 (89.53)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3728,7 +3724,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>maa://29063 (95.38), maa://25311 (100.00), ***maa://22725 (3.08), maa://45047 (81.54)</t>
+          <t>maa://29063 (95.31), maa://25311 (100.00), ***maa://22725 (3.12), *maa://45047 (79.69)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3808,7 +3804,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (100.00), maa://24516 (83.53), maa://26001 (85.88)</t>
+          <t>maa://31215 (100.00), maa://24516 (84.52), maa://26001 (85.71)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3824,7 +3820,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (98.92), maa://24621 (100.00), maa://36676 (91.40), *maa://22771 (66.67), **maa://37772 (40.86)</t>
+          <t>maa://20108 (97.87), maa://24621 (100.00), maa://36676 (91.49), *maa://22771 (65.96), **maa://37772 (40.43)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3842,7 +3838,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://41802 (100.00), maa://56374 (85.37)</t>
+          <t>maa://56374 (89.16), maa://41802 (100.00)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3890,7 +3886,7 @@
       </c>
       <c r="P26" s="8" t="inlineStr">
         <is>
-          <t>maa://56625 (100.00), maa://39870 (88.57)</t>
+          <t>maa://39870 (91.43), maa://56625 (100.00)</t>
         </is>
       </c>
       <c r="Q26" s="19" t="n"/>
@@ -3954,7 +3950,7 @@
       </c>
       <c r="AF26" s="8" t="inlineStr">
         <is>
-          <t>maa://30511 (100.00), **maa://29760 (45.00)</t>
+          <t>maa://30511 (100.00), **maa://29760 (44.83)</t>
         </is>
       </c>
       <c r="AG26" s="16" t="n"/>
@@ -3988,7 +3984,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>*maa://39601 (76.14), maa://34494 (100.00)</t>
+          <t>*maa://39601 (75.00), maa://34494 (100.00)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4182,7 +4178,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (100.00), maa://41749 (98.89)</t>
+          <t>maa://39929 (100.00), maa://41749 (97.78)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4214,7 +4210,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (100.00), *maa://65700 (68.89)</t>
+          <t>maa://36660 (100.00), *maa://65700 (59.55)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4264,7 +4260,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (97.87), maa://31400 (100.00), maa://28440 (84.04)</t>
+          <t>maa://28432 (97.85), maa://31400 (100.00), maa://28440 (84.95)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4362,7 +4358,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (100.00), *maa://64191 (66.23)</t>
+          <t>maa://45792 (100.00), maa://64191 (84.42)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4405,12 +4401,12 @@
       </c>
       <c r="O30" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="P30" s="8" t="inlineStr">
         <is>
-          <t>maa://21442 (100.00)</t>
+          <t>maa://21442 (100.00), **maa://66611 (35.05)</t>
         </is>
       </c>
       <c r="Q30" s="19" t="n"/>
@@ -4524,7 +4520,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (100.00), maa://36258 (91.21), *maa://43904 (58.24)</t>
+          <t>maa://35926 (100.00), maa://36258 (92.31), *maa://43904 (60.44)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4670,7 +4666,7 @@
       </c>
       <c r="P32" s="8" t="inlineStr">
         <is>
-          <t>maa://26203 (100.00), ***maa://56429 (24.42)</t>
+          <t>maa://26203 (100.00), **maa://56429 (39.53)</t>
         </is>
       </c>
       <c r="Q32" s="19" t="n"/>
@@ -4686,7 +4682,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (98.96), *maa://41108 (77.08), maa://41238 (100.00), maa://45523 (97.92)</t>
+          <t>maa://42859 (98.96), *maa://41108 (78.12), maa://41238 (100.00), maa://45523 (97.92)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4800,7 +4796,7 @@
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (100.00), *maa://22730 (72.73)</t>
+          <t>maa://21956 (100.00), *maa://22730 (70.13)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4893,12 +4889,12 @@
       </c>
       <c r="G34" s="19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H34" s="8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>maa://66817 (100.00)</t>
         </is>
       </c>
       <c r="I34" s="19" t="n"/>
@@ -4930,7 +4926,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (100.00), *maa://56235 (77.42)</t>
+          <t>maa://48817 (100.00), maa://56235 (82.80)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -5304,7 +5300,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (100.00), *maa://56336 (74.23), *maa://47069 (59.79), *maa://45789 (67.01)</t>
+          <t>maa://45718 (100.00), maa://56336 (80.41), *maa://47069 (61.86), *maa://45789 (67.01)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5503,7 +5499,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://36670 (88.89), maa://25199 (86.67), maa://30434 (100.00), *maa://45059 (67.78), **maa://44165 (42.22)</t>
+          <t>maa://36670 (87.78), maa://25199 (86.67), maa://30434 (100.00), *maa://45059 (67.78), **maa://44165 (42.22)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5535,7 +5531,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://24709 (100.00), maa://47093 (93.18)</t>
+          <t>maa://24709 (100.00), maa://47093 (89.77)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5684,7 +5680,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://64205 (100.00), *maa://65283 (73.17)</t>
+          <t>*maa://65283 (78.82), maa://64205 (100.00)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5748,12 +5744,12 @@
       </c>
       <c r="S41" s="19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="T41" s="8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>maa://66727 (100.00), maa://66675 (100.00)</t>
         </is>
       </c>
       <c r="U41" s="19" t="n"/>
@@ -5907,7 +5903,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>maa://22525 (83.95), maa://21284 (100.00)</t>
+          <t>*maa://22525 (79.27), maa://21284 (100.00)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -5992,7 +5988,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (100.00), maa://27728 (94.79), maa://56386 (87.50)</t>
+          <t>maa://29768 (100.00), maa://27728 (94.79), maa://56386 (80.21)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6077,7 +6073,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://21229 (90.80), maa://30807 (100.00), maa://42459 (89.66)</t>
+          <t>maa://21229 (90.80), maa://30807 (100.00), maa://42459 (86.21)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6146,7 +6142,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (100.00), maa://43901 (96.59)</t>
+          <t>maa://35931 (100.00), maa://43901 (95.45)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6215,7 +6211,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (100.00), maa://29661 (98.95), maa://56236 (82.11), *maa://28038 (61.05)</t>
+          <t>maa://27410 (100.00), maa://29661 (98.95), maa://56236 (86.32), *maa://28038 (61.05)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6490,7 +6486,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (100.00), maa://59378 (92.47), maa://65511 (81.72)</t>
+          <t>maa://59394 (100.00), maa://59378 (95.56), maa://65511 (86.67)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6660,7 +6656,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://25176 (100.00), maa://56237 (81.72)</t>
+          <t>maa://25176 (100.00), *maa://56237 (75.27)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6696,7 +6692,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (100.00), maa://27746 (83.52)</t>
+          <t>maa://31270 (100.00), maa://27746 (82.61)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -6750,7 +6746,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (100.00), maa://56228 (85.39), maa://43903 (91.01)</t>
+          <t>maa://42981 (100.00), maa://43903 (90.00), maa://56228 (88.89)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6768,7 +6764,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (100.00), maa://59413 (80.85)</t>
+          <t>maa://59534 (100.00), maa://59413 (85.11)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7090,7 +7086,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.08.31 13:19:07</t>
+          <t>更新日期：2025.09.02 13:21:02</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8494,7 +8490,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (72.29), *maa://28758 (67.47), maa://29036 (100.00), *maa://42172 (55.42), *maa://65357 (78.31), maa://30285 (81.93)</t>
+          <t>*maa://20849 (72.29), *maa://28758 (67.47), maa://29036 (100.00), *maa://42172 (57.83), maa://65357 (80.72), maa://30285 (81.93)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8764,7 +8760,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (95.51), maa://36866 (100.00), maa://62759 (98.88), *maa://45572 (74.16), *maa://27794 (64.04), *maa://20960 (78.65), **maa://20843 (49.44), ***maa://24483 (10.11), **maa://20862 (49.44), *maa://20893 (61.80)</t>
+          <t>maa://36644 (95.51), maa://36866 (100.00), maa://62759 (100.00), *maa://45572 (74.16), *maa://27794 (64.04), *maa://20960 (78.65), **maa://20843 (49.44), ***maa://24483 (10.11), **maa://20862 (49.44), *maa://20893 (61.80)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -10492,7 +10488,7 @@
       </c>
       <c r="D64" s="13" t="inlineStr">
         <is>
-          <t>maa://28187 (92.63), maa://45144 (100.00), maa://33504 (94.74), **maa://43531 (35.79)</t>
+          <t>maa://28187 (91.67), maa://45144 (100.00), maa://33504 (93.75), **maa://43531 (35.42)</t>
         </is>
       </c>
       <c r="E64" s="14" t="inlineStr">
@@ -12544,7 +12540,7 @@
       </c>
       <c r="D102" s="13" t="inlineStr">
         <is>
-          <t>maa://40517 (100.00), **maa://39240 (42.86)</t>
+          <t>maa://40517 (100.00), **maa://39240 (44.59)</t>
         </is>
       </c>
       <c r="E102" s="14" t="inlineStr">
@@ -12598,7 +12594,7 @@
       </c>
       <c r="D103" s="13" t="inlineStr">
         <is>
-          <t>maa://29094 (84.00), maa://28904 (100.00), **maa://20931 (41.33)</t>
+          <t>maa://29094 (85.33), maa://28904 (100.00), **maa://20931 (44.00)</t>
         </is>
       </c>
       <c r="E103" s="14" t="inlineStr">
@@ -13300,7 +13296,7 @@
       </c>
       <c r="D116" s="13" t="inlineStr">
         <is>
-          <t>maa://29659 (97.37), maa://29031 (100.00)</t>
+          <t>maa://29659 (96.10), maa://29031 (100.00)</t>
         </is>
       </c>
       <c r="E116" s="14" t="inlineStr">
@@ -13570,7 +13566,7 @@
       </c>
       <c r="D121" s="13" t="inlineStr">
         <is>
-          <t>maa://20869 (100.00), maa://44690 (85.57)</t>
+          <t>maa://20869 (100.00), maa://44690 (87.63)</t>
         </is>
       </c>
       <c r="E121" s="14" t="inlineStr">
@@ -14488,7 +14484,7 @@
       </c>
       <c r="D138" s="13" t="inlineStr">
         <is>
-          <t>maa://29025 (100.00), **maa://21000 (44.62)</t>
+          <t>maa://29025 (100.00), **maa://21000 (43.94)</t>
         </is>
       </c>
       <c r="E138" s="14" t="inlineStr">
@@ -14542,7 +14538,7 @@
       </c>
       <c r="D139" s="13" t="inlineStr">
         <is>
-          <t>maa://45258 (100.00), **maa://30679 (44.29)</t>
+          <t>maa://45258 (100.00), **maa://30679 (43.66)</t>
         </is>
       </c>
       <c r="E139" s="14" t="inlineStr">
@@ -14758,7 +14754,7 @@
       </c>
       <c r="D143" s="13" t="inlineStr">
         <is>
-          <t>maa://30670 (100.00), maa://31470 (84.95), **maa://45066 (38.71), *maa://61380 (75.27), ***maa://30867 (12.90)</t>
+          <t>maa://30670 (100.00), maa://31470 (86.02), **maa://45066 (38.71), *maa://61380 (77.42), ***maa://30867 (12.90)</t>
         </is>
       </c>
       <c r="E143" s="14" t="inlineStr">
@@ -16432,7 +16428,7 @@
       </c>
       <c r="D174" s="13" t="inlineStr">
         <is>
-          <t>maa://59681 (100.00), maa://64200 (85.11)</t>
+          <t>maa://59681 (100.00), maa://64200 (86.17)</t>
         </is>
       </c>
       <c r="E174" s="14" t="inlineStr">
@@ -17674,7 +17670,7 @@
       </c>
       <c r="D197" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (92.63), maa://35854 (83.16), maa://50388 (100.00), maa://25760 (83.16), ***maa://43911 (4.21), **maa://20872 (34.74), *maa://51066 (55.79), maa://63024 (86.32)</t>
+          <t>maa://44224 (92.63), maa://35854 (81.05), maa://50388 (100.00), maa://25760 (83.16), ***maa://43911 (4.21), **maa://20872 (34.74), *maa://51066 (55.79), maa://63024 (82.11)</t>
         </is>
       </c>
       <c r="E197" s="14" t="inlineStr">
@@ -20050,7 +20046,7 @@
       </c>
       <c r="D241" s="13" t="inlineStr">
         <is>
-          <t>maa://30667 (94.94), maa://30666 (100.00), **maa://30739 (35.44), *maa://30723 (56.96), maa://39588 (97.47), maa://64079 (86.08), **maa://65726 (43.04)</t>
+          <t>maa://30667 (94.94), maa://30666 (100.00), **maa://30739 (35.44), *maa://30723 (56.96), maa://39588 (97.47), maa://64079 (87.34), **maa://65726 (43.04)</t>
         </is>
       </c>
       <c r="E241" s="14" t="inlineStr">
@@ -20104,7 +20100,7 @@
       </c>
       <c r="D242" s="13" t="inlineStr">
         <is>
-          <t>maa://62759 (100.00), ***maa://62764 (23.86)</t>
+          <t>maa://62759 (100.00), ***maa://62764 (23.60)</t>
         </is>
       </c>
       <c r="E242" s="14" t="inlineStr">
@@ -21670,7 +21666,7 @@
       </c>
       <c r="D271" s="13" t="inlineStr">
         <is>
-          <t>maa://20825 (100.00), maa://21445 (90.74), *maa://35726 (66.67), ***maa://20891 (20.37)</t>
+          <t>maa://20825 (100.00), maa://21445 (87.50), *maa://35726 (64.29), ***maa://20891 (19.64)</t>
         </is>
       </c>
       <c r="E271" s="14" t="inlineStr">
@@ -24262,7 +24258,7 @@
       </c>
       <c r="D319" s="13" t="inlineStr">
         <is>
-          <t>*maa://62755 (70.00), maa://62761 (100.00)</t>
+          <t>*maa://62755 (73.33), maa://62761 (100.00)</t>
         </is>
       </c>
       <c r="E319" s="14" t="inlineStr">
@@ -24478,7 +24474,7 @@
       </c>
       <c r="D323" s="13" t="inlineStr">
         <is>
-          <t>maa://25773 (100.00), **maa://26088 (41.86)</t>
+          <t>maa://25773 (100.00), **maa://26088 (47.67)</t>
         </is>
       </c>
       <c r="E323" s="14" t="inlineStr">
@@ -26692,7 +26688,7 @@
       </c>
       <c r="D364" s="22" t="inlineStr">
         <is>
-          <t>maa://42635 (100.00), **maa://50629 (35.71), **maa://48859 (40.48)</t>
+          <t>maa://42635 (100.00), **maa://50629 (45.24), **maa://48859 (40.48)</t>
         </is>
       </c>
       <c r="E364" s="22" t="inlineStr">
@@ -26962,7 +26958,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://63883 (100.00), maa://64045 (82.76), **maa://64041 (34.48)</t>
+          <t>maa://63883 (100.00), maa://64045 (81.82), **maa://64041 (34.09)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -28366,7 +28362,7 @@
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>maa://51898 (100.00), *maa://57241 (80.00)</t>
+          <t>maa://51898 (100.00), maa://57241 (82.35)</t>
         </is>
       </c>
       <c r="E397" t="inlineStr">
@@ -28393,7 +28389,7 @@
       </c>
       <c r="D398" t="inlineStr">
         <is>
-          <t>maa://51880 (100.00), maa://56651 (94.90), maa://51878 (92.86)</t>
+          <t>maa://51880 (100.00), maa://56651 (95.92), maa://51878 (92.86)</t>
         </is>
       </c>
       <c r="E398" t="inlineStr">
@@ -28582,7 +28578,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>maa://64040 (100.00), *maa://66377 (53.12), ***maa://66376 (21.88)</t>
+          <t>maa://64040 (100.00), *maa://66377 (67.71), ***maa://66376 (9.38)</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#232)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://39402 (100.00), maa://58660 (94.25), *maa://34787 (74.71)</t>
+          <t>maa://39402 (100.00), maa://58660 (94.19), *maa://34787 (75.58)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -776,7 +776,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (100.00), *maa://66635 (64.77)</t>
+          <t>maa://22742 (100.00), maa://66635 (86.36)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://59087 (87.36), maa://25251 (100.00)</t>
+          <t>maa://59087 (88.51), maa://25251 (100.00)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -842,7 +842,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (100.00), maa://36987 (95.65), *maa://39849 (60.87)</t>
+          <t>maa://40192 (100.00), maa://36987 (94.62), *maa://39849 (60.22)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (100.00), *maa://22499 (76.14), *maa://22746 (69.32)</t>
+          <t>maa://24632 (100.00), *maa://22499 (75.28), *maa://22746 (68.54)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (100.00), maa://50121 (98.86)</t>
+          <t>maa://49983 (100.00), maa://50121 (97.75)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://32509 (100.00), maa://27295 (92.22), maa://22754 (87.78), *maa://31008 (72.22)</t>
+          <t>maa://32509 (100.00), maa://27295 (93.33), maa://22754 (87.78), *maa://31008 (72.22)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (100.00), maa://54105 (100.00), *maa://22744 (78.48)</t>
+          <t>maa://21245 (100.00), maa://54105 (96.25), *maa://22744 (77.50)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.02 13:21:02</t>
+          <t>更新日期：2025.09.03 13:18:59</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (85.39), maa://23252 (93.26), maa://37496 (100.00)</t>
+          <t>maa://32931 (83.33), maa://23252 (92.22), maa://37496 (100.00)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (100.00), *maa://39552 (63.22)</t>
+          <t>maa://22762 (100.00), *maa://39552 (65.52)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://52237 (90.53), maa://26223 (100.00)</t>
+          <t>maa://52237 (91.58), maa://26223 (100.00)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (100.00), maa://40166 (95.18)</t>
+          <t>maa://28711 (100.00), maa://40166 (94.05)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1739,12 +1739,12 @@
       </c>
       <c r="AE9" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (100.00)</t>
+          <t>maa://26206 (100.00), ***maa://66916 (24.71)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>***maa://25695 (25.49), ***maa://39951 (11.76), maa://45271 (100.00), ***maa://34206 (21.57), maa://54000 (88.24), ***maa://39243 (13.73)</t>
+          <t>***maa://25695 (25.00), ***maa://39951 (11.54), maa://45271 (100.00), ***maa://34206 (19.23), maa://54000 (86.54), ***maa://39243 (13.46)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (100.00), maa://36669 (83.12), *maa://23264 (63.64)</t>
+          <t>maa://28977 (100.00), maa://36669 (82.67), *maa://23264 (65.33)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://45828 (91.58), maa://22301 (100.00), maa://22726 (82.11)</t>
+          <t>maa://45828 (90.53), maa://22301 (100.00), maa://22726 (82.11)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (90.53), maa://22501 (100.00), maa://45521 (89.47), *maa://64808 (75.79)</t>
+          <t>maa://22747 (91.49), maa://22501 (100.00), maa://45521 (90.43), maa://64808 (81.91)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (100.00), *maa://54294 (76.74)</t>
+          <t>maa://21867 (100.00), *maa://54294 (74.42)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://36677 (96.74), maa://23669 (100.00), maa://39872 (89.13)</t>
+          <t>maa://36677 (96.74), maa://23669 (100.00), maa://39872 (90.22)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>maa://21248 (100.00), maa://66545 (86.57)</t>
+          <t>maa://21248 (100.00), maa://66545 (92.54)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (100.00), *maa://48321 (60.00), *maa://22583 (78.89)</t>
+          <t>maa://22676 (100.00), *maa://48321 (64.44), *maa://22583 (78.89)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://22521 (100.00), maa://42751 (88.76)</t>
+          <t>maa://22521 (100.00), maa://42751 (87.78)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (94.81), maa://22734 (100.00), *maa://30808 (67.53), maa://45058 (90.91), maa://36048 (85.71)</t>
+          <t>maa://22743 (94.81), maa://45058 (92.21), maa://22734 (100.00), *maa://30808 (67.53), maa://36048 (84.42)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://36666 (100.00), maa://21364 (100.00), *maa://22766 (78.21)</t>
+          <t>maa://36666 (100.00), maa://21364 (98.73), *maa://22766 (77.22)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2715,12 +2715,12 @@
       </c>
       <c r="O17" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (100.00), maa://56238 (84.93)</t>
+          <t>maa://23890 (100.00), *maa://56238 (75.34), *maa://24940 (67.12)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2955,12 +2955,12 @@
       </c>
       <c r="K19" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="L19" s="8" t="inlineStr">
         <is>
-          <t>maa://39347 (100.00)</t>
+          <t>maa://39347 (100.00), ***maa://56392 (27.63)</t>
         </is>
       </c>
       <c r="M19" s="19" t="n"/>
@@ -3024,7 +3024,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (100.00), *maa://36668 (74.63)</t>
+          <t>maa://30709 (100.00), *maa://36668 (76.12)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3300,7 +3300,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22524 (98.73), maa://22432 (100.00), *maa://64221 (77.22)</t>
+          <t>maa://22524 (98.73), maa://22432 (100.00), maa://64221 (83.54)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3350,7 +3350,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>maa://27127 (100.00), maa://22751 (88.24), **maa://66865 (30.88)</t>
+          <t>maa://27127 (100.00), maa://22751 (89.55), *maa://66865 (50.75)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3496,7 +3496,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (100.00), *maa://29748 (77.53), *maa://37566 (73.03)</t>
+          <t>maa://30587 (100.00), *maa://29748 (77.53), *maa://37566 (74.16)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3512,7 +3512,7 @@
       </c>
       <c r="T23" s="8" t="inlineStr">
         <is>
-          <t>maa://31212 (100.00), maa://24387 (93.24)</t>
+          <t>maa://31212 (100.00), maa://24387 (92.00)</t>
         </is>
       </c>
       <c r="U23" s="19" t="n"/>
@@ -3578,7 +3578,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (100.00), *maa://46650 (73.68)</t>
+          <t>maa://24368 (100.00), *maa://46650 (72.37)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3690,7 +3690,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://22523 (87.21), *maa://36672 (68.60), maa://64165 (91.86), maa://29910 (100.00), maa://45831 (89.53)</t>
+          <t>maa://22523 (87.21), maa://64165 (88.37), *maa://36672 (68.60), maa://29910 (100.00), maa://45831 (89.53)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3724,7 +3724,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>maa://29063 (95.31), maa://25311 (100.00), ***maa://22725 (3.12), *maa://45047 (79.69)</t>
+          <t>maa://29063 (95.31), maa://25311 (100.00), *maa://45047 (79.69), ***maa://22725 (3.12)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3804,7 +3804,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (100.00), maa://24516 (84.52), maa://26001 (85.71)</t>
+          <t>maa://31215 (100.00), maa://24516 (85.54), maa://26001 (86.75)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3820,7 +3820,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (97.87), maa://24621 (100.00), maa://36676 (91.49), *maa://22771 (65.96), **maa://37772 (40.43)</t>
+          <t>maa://20108 (98.92), maa://24621 (100.00), maa://36676 (93.55), *maa://22771 (66.67), **maa://37772 (40.86)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://56374 (89.16), maa://41802 (100.00)</t>
+          <t>maa://56374 (91.57), maa://41802 (100.00)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3984,7 +3984,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>*maa://39601 (75.00), maa://34494 (100.00)</t>
+          <t>*maa://39601 (73.86), maa://34494 (100.00)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4098,7 +4098,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (100.00), maa://25725 (82.02)</t>
+          <t>maa://24465 (100.00), maa://25725 (83.15)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4210,7 +4210,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (100.00), *maa://65700 (59.55)</t>
+          <t>maa://36660 (100.00), *maa://65700 (65.17)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4260,7 +4260,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (97.85), maa://31400 (100.00), maa://28440 (84.95)</t>
+          <t>maa://28432 (98.92), maa://31400 (100.00), maa://28440 (84.95)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4340,7 +4340,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://24080 (88.89), maa://42865 (100.00), ***maa://34960 (2.78)</t>
+          <t>maa://24080 (87.67), maa://42865 (100.00), ***maa://34960 (2.74)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4358,7 +4358,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (100.00), maa://64191 (84.42)</t>
+          <t>maa://45792 (100.00), maa://64191 (88.31)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4454,7 +4454,7 @@
       </c>
       <c r="AB30" s="8" t="inlineStr">
         <is>
-          <t>maa://42979 (100.00), maa://45822 (89.47), **maa://45045 (46.32)</t>
+          <t>maa://42979 (100.00), maa://45822 (89.47), *maa://45045 (51.58)</t>
         </is>
       </c>
       <c r="AC30" s="19" t="n"/>
@@ -4520,7 +4520,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (100.00), maa://36258 (92.31), *maa://43904 (60.44)</t>
+          <t>maa://35926 (100.00), maa://36258 (92.31), *maa://43904 (62.64)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4552,7 +4552,7 @@
       </c>
       <c r="T31" s="8" t="inlineStr">
         <is>
-          <t>maa://30711 (100.00), **maa://30768 (50.00)</t>
+          <t>maa://30711 (100.00), **maa://30768 (49.44)</t>
         </is>
       </c>
       <c r="U31" s="19" t="n"/>
@@ -4926,7 +4926,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (100.00), maa://56235 (82.80)</t>
+          <t>maa://48817 (100.00), maa://56235 (86.02)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -5300,7 +5300,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (100.00), maa://56336 (80.41), *maa://47069 (61.86), *maa://45789 (67.01)</t>
+          <t>maa://45718 (100.00), *maa://56336 (79.38), *maa://47069 (61.86), *maa://45789 (67.01)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5499,7 +5499,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://36670 (87.78), maa://25199 (86.67), maa://30434 (100.00), *maa://45059 (67.78), **maa://44165 (42.22)</t>
+          <t>maa://36670 (87.78), maa://25199 (86.67), maa://30434 (100.00), *maa://45059 (66.67), **maa://44165 (42.22)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5547,7 +5547,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (100.00), *maa://45788 (72.50), maa://45790 (81.25)</t>
+          <t>maa://47079 (100.00), *maa://45788 (72.15), maa://45790 (82.28)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5680,7 +5680,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>*maa://65283 (78.82), maa://64205 (100.00)</t>
+          <t>maa://65283 (83.72), maa://64205 (100.00)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5749,7 +5749,7 @@
       </c>
       <c r="T41" s="8" t="inlineStr">
         <is>
-          <t>maa://66727 (100.00), maa://66675 (100.00)</t>
+          <t>maa://66727 (100.00), maa://66675 (86.27)</t>
         </is>
       </c>
       <c r="U41" s="19" t="n"/>
@@ -5988,7 +5988,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (100.00), maa://27728 (94.79), maa://56386 (80.21)</t>
+          <t>maa://29768 (100.00), maa://27728 (94.79), maa://56386 (82.29)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6073,7 +6073,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://21229 (90.80), maa://30807 (100.00), maa://42459 (86.21)</t>
+          <t>maa://21229 (90.80), maa://42459 (86.21), maa://30807 (100.00)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6486,7 +6486,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (100.00), maa://59378 (95.56), maa://65511 (86.67)</t>
+          <t>maa://59394 (100.00), maa://59378 (95.56), maa://65511 (91.11)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6656,7 +6656,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://25176 (100.00), *maa://56237 (75.27)</t>
+          <t>maa://25176 (100.00), *maa://56237 (77.42)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6759,12 +6759,12 @@
       </c>
       <c r="G63" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (100.00), maa://59413 (85.11)</t>
+          <t>maa://59534 (100.00), *maa://59693 (55.32), *maa://59413 (76.60)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7086,7 +7086,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.02 13:21:02</t>
+          <t>更新日期：2025.09.03 13:18:59</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8490,7 +8490,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (72.29), *maa://28758 (67.47), maa://29036 (100.00), *maa://42172 (57.83), maa://65357 (80.72), maa://30285 (81.93)</t>
+          <t>*maa://20849 (72.29), *maa://28758 (67.47), maa://29036 (100.00), *maa://42172 (57.83), maa://65357 (86.75), maa://30285 (81.93)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -10434,7 +10434,7 @@
       </c>
       <c r="D63" s="13" t="inlineStr">
         <is>
-          <t>maa://20845 (80.65), maa://38727 (100.00)</t>
+          <t>*maa://20845 (76.92), maa://38727 (100.00)</t>
         </is>
       </c>
       <c r="E63" s="14" t="inlineStr">
@@ -10542,7 +10542,7 @@
       </c>
       <c r="D65" s="13" t="inlineStr">
         <is>
-          <t>maa://28567 (96.81), **maa://20947 (31.91), maa://30525 (89.36), maa://38735 (100.00), **maa://28188 (42.55), **maa://30524 (36.17)</t>
+          <t>maa://28567 (96.81), **maa://20947 (31.91), maa://30525 (89.36), maa://38735 (100.00), **maa://28188 (42.55), **maa://30524 (46.81)</t>
         </is>
       </c>
       <c r="E65" s="14" t="inlineStr">
@@ -10920,7 +10920,7 @@
       </c>
       <c r="D72" s="13" t="inlineStr">
         <is>
-          <t>maa://36643 (100.00), maa://36864 (95.88), maa://39140 (94.85), **maa://66335 (35.05)</t>
+          <t>maa://36643 (100.00), maa://36864 (95.88), maa://39140 (94.85), **maa://66335 (45.36)</t>
         </is>
       </c>
       <c r="E72" s="14" t="inlineStr">
@@ -11406,7 +11406,7 @@
       </c>
       <c r="D81" s="13" t="inlineStr">
         <is>
-          <t>maa://30525 (96.55), maa://20859 (100.00), **maa://28188 (45.98), **maa://30524 (39.08)</t>
+          <t>maa://30525 (96.55), maa://20859 (100.00), **maa://28188 (45.98), *maa://30524 (50.57)</t>
         </is>
       </c>
       <c r="E81" s="14" t="inlineStr">
@@ -12594,7 +12594,7 @@
       </c>
       <c r="D103" s="13" t="inlineStr">
         <is>
-          <t>maa://29094 (85.33), maa://28904 (100.00), **maa://20931 (44.00)</t>
+          <t>maa://29094 (84.21), maa://28904 (100.00), **maa://20931 (43.42)</t>
         </is>
       </c>
       <c r="E103" s="14" t="inlineStr">
@@ -12864,7 +12864,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://25018 (96.94), maa://25776 (85.71), maa://28361 (86.73), maa://25772 (85.71), maa://56588 (84.69), *maa://45194 (66.33), *maa://32653 (63.27), *maa://25161 (62.24), *maa://61839 (73.47), ***maa://60902 (19.39), *maa://61275 (52.04)</t>
+          <t>maa://51881 (100.00), maa://25018 (96.94), maa://25776 (85.71), maa://28361 (86.73), maa://25772 (85.71), maa://56588 (84.69), *maa://45194 (66.33), *maa://32653 (58.16), *maa://25161 (62.24), *maa://61839 (75.51), ***maa://60902 (19.39), *maa://61275 (52.04)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -16428,7 +16428,7 @@
       </c>
       <c r="D174" s="13" t="inlineStr">
         <is>
-          <t>maa://59681 (100.00), maa://64200 (86.17)</t>
+          <t>maa://59681 (100.00), maa://64200 (87.23)</t>
         </is>
       </c>
       <c r="E174" s="14" t="inlineStr">
@@ -23070,7 +23070,7 @@
       </c>
       <c r="D297" s="13" t="inlineStr">
         <is>
-          <t>maa://32414 (100.00), *maa://32505 (67.01), maa://39155 (89.69)</t>
+          <t>maa://32414 (100.00), maa://39155 (89.69), *maa://32505 (67.01)</t>
         </is>
       </c>
       <c r="E297" s="14" t="inlineStr">
@@ -25824,7 +25824,7 @@
       </c>
       <c r="D348" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (100.00), maa://32415 (85.42), maa://34677 (96.88), maa://32892 (88.54), *maa://32653 (64.58), *maa://61839 (75.00), *maa://61275 (53.12)</t>
+          <t>maa://32647 (100.00), maa://32415 (85.42), maa://34677 (96.88), maa://32892 (88.54), *maa://32653 (59.38), *maa://61839 (77.08), *maa://61275 (53.12)</t>
         </is>
       </c>
       <c r="E348" s="22" t="inlineStr">
@@ -28416,7 +28416,7 @@
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>maa://51872 (100.00), maa://51876 (100.00), *maa://63228 (74.74), maa://51873 (97.89), *maa://62047 (76.84)</t>
+          <t>maa://51872 (100.00), maa://51876 (100.00), *maa://63228 (74.74), maa://51873 (97.89), *maa://62047 (77.89)</t>
         </is>
       </c>
       <c r="E399" t="inlineStr">
@@ -28578,7 +28578,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>maa://64040 (100.00), *maa://66377 (67.71), ***maa://66376 (9.38)</t>
+          <t>maa://64040 (100.00), *maa://66377 (70.83), ***maa://66376 (6.25)</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#234)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -712,7 +712,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (100.00), maa://24702 (97.87), maa://36681 (81.91)</t>
+          <t>maa://25390 (100.00), maa://24702 (95.83), maa://36681 (80.21)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://39402 (91.58), maa://58660 (100.00), *maa://34787 (68.42)</t>
+          <t>maa://39402 (91.67), maa://58660 (100.00), *maa://34787 (67.71)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -776,7 +776,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (95.83), maa://66635 (100.00)</t>
+          <t>maa://22742 (95.92), maa://66635 (100.00)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://36684 (100.00), maa://21246 (93.62)</t>
+          <t>maa://36684 (100.00), maa://21246 (91.67)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://59087 (100.00), maa://25251 (97.75)</t>
+          <t>maa://59087 (100.00), maa://25251 (93.55)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -842,7 +842,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (100.00), maa://36987 (91.75), *maa://39849 (57.73)</t>
+          <t>maa://40192 (100.00), maa://36987 (90.82), *maa://39849 (57.14)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>maa://22880 (88.51), maa://20276 (100.00), *maa://22749 (72.41)</t>
+          <t>maa://22880 (92.13), maa://20276 (100.00), *maa://22749 (70.79)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -890,7 +890,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (100.00), maa://26254 (93.68), **maa://22738 (31.58)</t>
+          <t>maa://21249 (100.00), maa://26254 (93.75), **maa://22738 (31.25)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://45854 (80.43), maa://60545 (100.00), maa://24617 (92.39)</t>
+          <t>*maa://45854 (78.12), maa://60545 (100.00), maa://24617 (88.54)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (85.57), maa://27484 (100.00), *maa://27480 (75.26)</t>
+          <t>maa://27396 (87.63), maa://27484 (100.00), *maa://27480 (75.26)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://52241 (100.00), maa://24390 (96.81)</t>
+          <t>maa://52241 (100.00), maa://24390 (94.79)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (100.00), *maa://22499 (71.28), *maa://22746 (69.15)</t>
+          <t>maa://24632 (100.00), *maa://22499 (70.53), *maa://22746 (68.42)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (100.00), maa://50121 (91.67)</t>
+          <t>maa://49983 (100.00), maa://50121 (91.75)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://32509 (97.83), maa://27295 (100.00), maa://31008 (84.78), maa://22754 (85.87)</t>
+          <t>maa://27295 (100.00), maa://32509 (95.79), maa://31008 (90.53), maa://22754 (83.16)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (88.17), maa://54105 (100.00), *maa://22744 (66.67)</t>
+          <t>maa://21245 (89.47), maa://54105 (100.00), *maa://22744 (65.26)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (100.00), maa://30381 (84.44)</t>
+          <t>maa://31836 (100.00), maa://30381 (81.72)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="AF6" s="8" t="inlineStr">
         <is>
-          <t>maa://33152 (100.00), ***maa://22770 (21.31)</t>
+          <t>maa://33152 (100.00), ***maa://22770 (20.00)</t>
         </is>
       </c>
       <c r="AG6" s="16" t="n"/>
@@ -1378,12 +1378,12 @@
       </c>
       <c r="G7" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>maa://64972 (100.00)</t>
+          <t>*maa://22763 (78.38), maa://64972 (100.00)</t>
         </is>
       </c>
       <c r="I7" s="19" t="n"/>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (100.00), maa://24957 (91.58)</t>
+          <t>maa://28624 (100.00), maa://24957 (87.63)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (100.00), *maa://22758 (76.34)</t>
+          <t>maa://22399 (100.00), *maa://22758 (76.60)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.06 13:18:41</t>
+          <t>更新日期：2025.09.08 13:20:19</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (100.00), **maa://39431 (46.58), **maa://37551 (30.14)</t>
+          <t>maa://21476 (100.00), **maa://39431 (40.51), ***maa://37551 (27.85)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (88.89), maa://23252 (92.22), maa://37496 (100.00)</t>
+          <t>maa://32931 (93.41), maa://23252 (91.21), maa://37496 (100.00)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1577,12 +1577,12 @@
       </c>
       <c r="W8" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (100.00)</t>
+          <t>maa://21411 (100.00), *maa://67587 (74.47)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>maa://24479 (100.00), **maa://21990 (46.48)</t>
+          <t>maa://24479 (100.00), **maa://21990 (45.33)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>maa://22765 (100.00), *maa://21915 (69.77)</t>
+          <t>maa://22765 (100.00), *maa://21915 (70.45)</t>
         </is>
       </c>
       <c r="E9" s="19" t="n"/>
@@ -1643,12 +1643,12 @@
       </c>
       <c r="G9" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H9" s="8" t="inlineStr">
         <is>
-          <t>maa://56348 (100.00)</t>
+          <t>*maa://47450 (69.23), maa://56348 (100.00)</t>
         </is>
       </c>
       <c r="I9" s="19" t="n"/>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (100.00), *maa://39552 (75.00)</t>
+          <t>maa://22762 (100.00), *maa://39552 (78.89)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1680,7 +1680,7 @@
       </c>
       <c r="P9" s="8" t="inlineStr">
         <is>
-          <t>maa://22736 (82.61), maa://64516 (100.00)</t>
+          <t>maa://64516 (100.00), *maa://22736 (80.00)</t>
         </is>
       </c>
       <c r="Q9" s="19" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://52237 (100.00), maa://26223 (100.00)</t>
+          <t>maa://52237 (100.00), maa://26223 (97.94)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (100.00), maa://40166 (96.55)</t>
+          <t>maa://28711 (100.00), maa://40166 (97.78)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (98.85), maa://66916 (100.00)</t>
+          <t>maa://26206 (91.49), maa://66916 (100.00)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (100.00), *maa://36669 (77.50), *maa://23264 (65.00)</t>
+          <t>maa://28977 (100.00), *maa://36669 (75.00), *maa://23264 (61.90)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (100.00), maa://22755 (86.60), *maa://63521 (77.32)</t>
+          <t>maa://27395 (100.00), maa://22755 (86.73), maa://63521 (89.80)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://45828 (98.95), maa://22301 (100.00), maa://22726 (82.11)</t>
+          <t>maa://45828 (100.00), maa://22301 (97.94), maa://22726 (80.41)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>maa://25021 (81.48), maa://22733 (100.00), ***maa://22761 (11.11)</t>
+          <t>*maa://25021 (80.00), maa://22733 (100.00), ***maa://22761 (10.91)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (89.69), maa://22501 (100.00), maa://64808 (96.91), maa://45521 (87.63)</t>
+          <t>maa://22747 (89.80), maa://22501 (100.00), maa://64808 (97.96), maa://45521 (86.73)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="AB11" s="8" t="inlineStr">
         <is>
-          <t>maa://29912 (100.00), maa://22516 (80.41)</t>
+          <t>maa://29912 (100.00), *maa://22516 (79.59)</t>
         </is>
       </c>
       <c r="AC11" s="19" t="n"/>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>maa://36678 (100.00), maa://30766 (98.70)</t>
+          <t>maa://36678 (100.00), maa://30766 (90.48)</t>
         </is>
       </c>
       <c r="E12" s="19" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (100.00), maa://54294 (89.66)</t>
+          <t>maa://21867 (100.00), maa://54294 (98.86)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (100.00), maa://64046 (100.00)</t>
+          <t>maa://63896 (100.00), maa://64046 (98.96)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>*maa://21485 (77.42), maa://37962 (100.00), maa://22753 (94.62)</t>
+          <t>*maa://21485 (77.08), maa://37962 (100.00), maa://22753 (92.71)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://36677 (100.00), maa://23669 (97.87), maa://39872 (93.62)</t>
+          <t>maa://36677 (100.00), maa://23669 (95.88), maa://39872 (92.78)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2129,12 +2129,12 @@
       </c>
       <c r="AE12" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>maa://28932 (100.00), *maa://20106 (65.48), *maa://22769 (52.38)</t>
+          <t>maa://28932 (100.00)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (100.00), maa://36673 (93.55), maa://25001 (83.87)</t>
+          <t>maa://24999 (100.00), maa://36673 (92.55), maa://25001 (84.04)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.12), maa://66545 (100.00)</t>
+          <t>*maa://21248 (72.63), maa://66545 (100.00)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2195,12 +2195,12 @@
       </c>
       <c r="O13" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://48321 (100.00), maa://22676 (100.00), *maa://22583 (80.00)</t>
+          <t>maa://22676 (100.00), maa://22583 (81.52)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2259,12 +2259,12 @@
       </c>
       <c r="AE13" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (100.00), **maa://39885 (42.86)</t>
+          <t>maa://39883 (100.00)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (100.00), maa://26245 (97.92), maa://21288 (95.83), maa://36682 (91.67)</t>
+          <t>maa://39841 (100.00), maa://26245 (96.91), maa://21288 (94.85), maa://36682 (95.88)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2330,7 +2330,7 @@
       </c>
       <c r="P14" s="8" t="inlineStr">
         <is>
-          <t>maa://23250 (100.00), *maa://20107 (73.47), *maa://22772 (58.16)</t>
+          <t>maa://23250 (100.00), *maa://20107 (72.73), *maa://22772 (57.58)</t>
         </is>
       </c>
       <c r="Q14" s="19" t="n"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://42751 (100.00), maa://22521 (98.90)</t>
+          <t>maa://42751 (100.00), maa://22521 (95.79)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (84.78), maa://45058 (100.00), maa://22734 (83.70), *maa://36048 (72.83)</t>
+          <t>maa://22743 (84.21), maa://45058 (100.00), maa://22734 (81.05), *maa://36048 (70.53)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (100.00), maa://21478 (84.62)</t>
+          <t>maa://24304 (100.00), maa://21478 (82.80)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="P15" s="8" t="inlineStr">
         <is>
-          <t>maa://24762 (100.00), **maa://22727 (43.48)</t>
+          <t>maa://24762 (100.00), **maa://22727 (42.55)</t>
         </is>
       </c>
       <c r="Q15" s="19" t="n"/>
@@ -2492,7 +2492,7 @@
       </c>
       <c r="X15" s="8" t="inlineStr">
         <is>
-          <t>maa://38786 (100.00), maa://56102 (86.44)</t>
+          <t>maa://38786 (100.00), maa://56102 (82.61)</t>
         </is>
       </c>
       <c r="Y15" s="19" t="n"/>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://36666 (100.00), maa://21364 (89.77)</t>
+          <t>maa://36666 (100.00), maa://21364 (85.87)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://37650 (100.00), maa://21441 (96.88), maa://36679 (88.54)</t>
+          <t>maa://37650 (100.00), maa://21441 (94.90), maa://36679 (86.73)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://22729 (100.00), maa://36674 (98.90), *maa://28648 (74.73)</t>
+          <t>maa://36674 (100.00), maa://22729 (97.87), *maa://28648 (72.34)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2622,7 +2622,7 @@
       </c>
       <c r="X16" s="8" t="inlineStr">
         <is>
-          <t>maa://28501 (100.00), maa://28051 (85.42)</t>
+          <t>maa://28501 (100.00), maa://28051 (86.60)</t>
         </is>
       </c>
       <c r="Y16" s="19" t="n"/>
@@ -2649,12 +2649,12 @@
       </c>
       <c r="AE16" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>maa://23911 (88.51), maa://27755 (100.00)</t>
+          <t>maa://23911 (95.40), maa://27755 (100.00), *maa://67613 (50.57)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2672,7 +2672,7 @@
       </c>
       <c r="D17" s="8" t="inlineStr">
         <is>
-          <t>maa://21624 (100.00), *maa://56358 (68.00)</t>
+          <t>maa://21624 (100.00), *maa://56358 (75.00)</t>
         </is>
       </c>
       <c r="E17" s="19" t="n"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://39599 (100.00), maa://22430 (93.48)</t>
+          <t>maa://39599 (100.00), maa://22430 (90.53)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (89.16), maa://56238 (100.00)</t>
+          <t>maa://23890 (84.09), maa://56238 (100.00)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://52226 (100.00), maa://22466 (91.75)</t>
+          <t>maa://52226 (100.00), maa://22466 (90.82)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), maa://54153 (100.00), *maa://24380 (67.71)</t>
+          <t>maa://24379 (100.00), maa://54153 (100.00), *maa://24380 (67.01)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (100.00), *maa://22741 (59.57)</t>
+          <t>maa://21917 (100.00), *maa://22741 (65.26)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://47854 (100.00), *maa://24313 (70.67)</t>
+          <t>maa://47854 (100.00), *maa://24313 (67.50)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="L19" s="8" t="inlineStr">
         <is>
-          <t>maa://39347 (100.00), ***maa://56392 (26.25)</t>
+          <t>maa://39347 (100.00), *maa://56392 (51.76)</t>
         </is>
       </c>
       <c r="M19" s="19" t="n"/>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="X19" s="8" t="inlineStr">
         <is>
-          <t>maa://31386 (100.00), *maa://58490 (54.65)</t>
+          <t>maa://31386 (100.00), *maa://58490 (59.77)</t>
         </is>
       </c>
       <c r="Y19" s="19" t="n"/>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (100.00), *maa://36668 (76.71)</t>
+          <t>maa://30709 (100.00), *maa://36668 (75.32)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3044,7 +3044,7 @@
       </c>
       <c r="AF19" s="8" t="inlineStr">
         <is>
-          <t>maa://21663 (100.00), *maa://52239 (77.78)</t>
+          <t>maa://21663 (90.00), maa://52239 (100.00)</t>
         </is>
       </c>
       <c r="AG19" s="16" t="n"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://25198 (96.88), maa://36680 (100.00), maa://21432 (90.62)</t>
+          <t>maa://25198 (98.96), maa://36680 (100.00), maa://21432 (90.62)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (95.79), maa://56241 (100.00), maa://49976 (84.21)</t>
+          <t>maa://50085 (94.85), maa://56241 (100.00), maa://49976 (83.51)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (100.00), maa://20110 (84.62)</t>
+          <t>maa://34946 (100.00), maa://20110 (82.80)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="AB21" s="8" t="inlineStr">
         <is>
-          <t>maa://21443 (100.00), *maa://52223 (61.73)</t>
+          <t>maa://21443 (100.00), maa://52223 (82.72)</t>
         </is>
       </c>
       <c r="AC21" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22432 (93.33), maa://22524 (86.67), maa://64221 (100.00)</t>
+          <t>maa://22432 (93.62), maa://22524 (82.98), maa://64221 (100.00)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>*maa://27127 (74.74), *maa://22751 (64.21), maa://66865 (100.00)</t>
+          <t>*maa://27127 (76.84), *maa://22751 (64.21), maa://66865 (100.00)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://37649 (82.47), maa://21282 (100.00)</t>
+          <t>maa://37649 (89.69), maa://21282 (100.00)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>*maa://28036 (52.50), maa://41753 (100.00)</t>
+          <t>**maa://28036 (48.84), maa://41753 (100.00)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (100.00), maa://39875 (92.71)</t>
+          <t>maa://39756 (100.00), maa://39875 (91.75)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (100.00), *maa://29748 (79.12), *maa://37566 (74.73)</t>
+          <t>maa://30587 (100.00), *maa://29748 (79.57), *maa://37566 (70.97)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="T23" s="8" t="inlineStr">
         <is>
-          <t>maa://31212 (100.00), maa://24387 (84.15), *maa://67084 (53.66)</t>
+          <t>maa://31212 (100.00), maa://24387 (81.40), *maa://67084 (66.28)</t>
         </is>
       </c>
       <c r="U23" s="19" t="n"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (100.00), maa://46650 (97.44)</t>
+          <t>maa://24368 (98.77), maa://46650 (100.00)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (97.80), maa://23504 (100.00), *maa://25141 (78.02), *maa://36663 (76.92), maa://52227 (100.00)</t>
+          <t>maa://29988 (97.87), maa://23504 (97.87), *maa://25141 (75.53), *maa://36663 (74.47), maa://52227 (100.00)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>*maa://22523 (78.95), maa://64165 (100.00), maa://29910 (90.53), maa://45831 (81.05)</t>
+          <t>maa://64165 (100.00), *maa://22523 (77.32), maa://29910 (88.66), maa://45831 (80.41)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (100.00), maa://63016 (98.92)</t>
+          <t>maa://29753 (98.95), maa://63016 (100.00)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>maa://29063 (97.01), maa://25311 (94.03), maa://45047 (100.00)</t>
+          <t>maa://29063 (95.77), maa://25311 (88.73), maa://45047 (100.00)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="T25" s="8" t="inlineStr">
         <is>
-          <t>maa://20109 (90.91), maa://22545 (100.00)</t>
+          <t>maa://20109 (92.93), maa://22545 (100.00)</t>
         </is>
       </c>
       <c r="U25" s="19" t="n"/>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (100.00), maa://24516 (80.68), maa://26001 (81.82)</t>
+          <t>maa://31215 (100.00), *maa://24516 (79.78), maa://26001 (80.90)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (95.88), maa://36676 (100.00), maa://24621 (95.88), *maa://22771 (65.98), **maa://37772 (39.18)</t>
+          <t>maa://20108 (95.92), maa://36676 (100.00), maa://24621 (94.90), *maa://22771 (65.31), **maa://37772 (44.90)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://56374 (100.00), maa://41802 (94.38)</t>
+          <t>maa://56374 (100.00), maa://41802 (92.39)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3858,7 +3858,7 @@
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
-          <t>maa://56240 (96.47), maa://24913 (100.00)</t>
+          <t>maa://56240 (100.00), maa://24913 (97.70)</t>
         </is>
       </c>
       <c r="I26" s="19" t="n"/>
@@ -3869,12 +3869,12 @@
       </c>
       <c r="K26" s="19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L26" s="8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>maa://67563 (100.00)</t>
         </is>
       </c>
       <c r="M26" s="19" t="n"/>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="P26" s="8" t="inlineStr">
         <is>
-          <t>maa://39870 (83.91), maa://56625 (100.00)</t>
+          <t>maa://39870 (86.81), maa://56625 (100.00)</t>
         </is>
       </c>
       <c r="Q26" s="19" t="n"/>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="AF26" s="8" t="inlineStr">
         <is>
-          <t>maa://30511 (100.00), **maa://29760 (44.83)</t>
+          <t>maa://30511 (100.00), **maa://29760 (47.46)</t>
         </is>
       </c>
       <c r="AG26" s="16" t="n"/>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>*maa://39601 (79.12), maa://34494 (100.00)</t>
+          <t>maa://39601 (84.78), maa://34494 (100.00)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4102,7 +4102,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (100.00), maa://25725 (81.52)</t>
+          <t>maa://24465 (100.00), maa://25725 (81.72)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4166,7 +4166,7 @@
       </c>
       <c r="T28" s="8" t="inlineStr">
         <is>
-          <t>maa://29765 (86.81), maa://23263 (100.00)</t>
+          <t>maa://29765 (94.51), maa://23263 (100.00)</t>
         </is>
       </c>
       <c r="U28" s="19" t="n"/>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (100.00), maa://41749 (98.92)</t>
+          <t>maa://39929 (100.00), maa://41749 (98.95)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (97.83), maa://65700 (100.00)</t>
+          <t>maa://36660 (94.79), maa://65700 (100.00)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (98.95), maa://31400 (100.00), maa://28440 (84.21)</t>
+          <t>maa://28432 (100.00), maa://31400 (100.00), maa://28440 (84.21)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://42865 (100.00), *maa://24080 (78.05)</t>
+          <t>maa://42865 (100.00), *maa://24080 (74.42)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (100.00), maa://64191 (98.78)</t>
+          <t>maa://45792 (95.45), maa://64191 (100.00)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4410,7 +4410,7 @@
       </c>
       <c r="P30" s="8" t="inlineStr">
         <is>
-          <t>maa://21442 (100.00), maa://66611 (86.73)</t>
+          <t>maa://21442 (100.00), maa://66611 (91.84)</t>
         </is>
       </c>
       <c r="Q30" s="19" t="n"/>
@@ -4426,7 +4426,7 @@
       </c>
       <c r="T30" s="8" t="inlineStr">
         <is>
-          <t>*maa://32940 (58.44), maa://24388 (100.00)</t>
+          <t>*maa://32940 (67.09), maa://24388 (100.00)</t>
         </is>
       </c>
       <c r="U30" s="19" t="n"/>
@@ -4458,7 +4458,7 @@
       </c>
       <c r="AB30" s="8" t="inlineStr">
         <is>
-          <t>maa://42979 (100.00), maa://45822 (91.84), **maa://45045 (50.00)</t>
+          <t>maa://42979 (100.00), maa://45822 (91.92), **maa://45045 (49.49)</t>
         </is>
       </c>
       <c r="AC30" s="19" t="n"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (100.00), maa://36258 (91.49), *maa://43904 (72.34)</t>
+          <t>maa://35926 (100.00), maa://36258 (91.67), *maa://43904 (72.92)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4556,7 +4556,7 @@
       </c>
       <c r="T31" s="8" t="inlineStr">
         <is>
-          <t>maa://30711 (100.00), *maa://30768 (56.67)</t>
+          <t>maa://30711 (100.00), *maa://30768 (56.04)</t>
         </is>
       </c>
       <c r="U31" s="19" t="n"/>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://36667 (100.00), maa://21895 (96.94), **maa://22760 (34.69)</t>
+          <t>maa://36667 (100.00), maa://21895 (96.97), **maa://22760 (44.44)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4670,7 +4670,7 @@
       </c>
       <c r="P32" s="8" t="inlineStr">
         <is>
-          <t>maa://26203 (100.00), *maa://56429 (66.28)</t>
+          <t>maa://26203 (100.00), *maa://56429 (75.58)</t>
         </is>
       </c>
       <c r="Q32" s="19" t="n"/>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (100.00), *maa://41108 (77.55), maa://41238 (97.96), maa://45523 (95.92)</t>
+          <t>maa://42859 (100.00), *maa://41108 (77.55), maa://41238 (96.94), maa://45523 (95.92)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (100.00), *maa://22730 (64.29)</t>
+          <t>maa://21956 (100.00), *maa://22730 (61.36)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (97.94), maa://56235 (100.00)</t>
+          <t>maa://48817 (97.96), maa://56235 (100.00)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (100.00), maa://56336 (98.98), *maa://47069 (69.39), *maa://45789 (73.47)</t>
+          <t>maa://45718 (100.00), maa://56336 (100.00), *maa://47069 (71.43), *maa://45789 (73.47)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5418,7 +5418,7 @@
       </c>
       <c r="L38" s="8" t="inlineStr">
         <is>
-          <t>maa://39384 (100.00), *maa://49735 (71.58)</t>
+          <t>maa://39384 (100.00), *maa://49735 (70.83)</t>
         </is>
       </c>
       <c r="M38" s="19" t="n"/>
@@ -5498,12 +5498,12 @@
       </c>
       <c r="G39" s="19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://36670 (97.78), maa://25199 (86.67), maa://30434 (100.00), *maa://45059 (66.67), **maa://44165 (42.22)</t>
+          <t>maa://25199 (85.71), maa://30434 (100.00), *maa://45059 (75.82), **maa://44165 (41.76)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://24709 (97.80), maa://47093 (100.00)</t>
+          <t>maa://47093 (100.00), maa://24709 (94.68)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (100.00), *maa://45790 (79.55)</t>
+          <t>maa://47079 (100.00), maa://45790 (81.32)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5636,7 +5636,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (100.00), maa://21386 (97.87), maa://36664 (82.98), *maa://45550 (52.13)</t>
+          <t>maa://23278 (100.00), maa://21386 (95.83), maa://36664 (83.33), *maa://45550 (51.04)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://65283 (100.00), maa://64205 (95.40)</t>
+          <t>maa://65283 (100.00), maa://64205 (91.21)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5753,7 +5753,7 @@
       </c>
       <c r="T41" s="8" t="inlineStr">
         <is>
-          <t>maa://66727 (100.00), *maa://66675 (62.86)</t>
+          <t>maa://66727 (100.00), *maa://66675 (53.66)</t>
         </is>
       </c>
       <c r="U41" s="19" t="n"/>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>*maa://22525 (73.86), maa://21284 (100.00)</t>
+          <t>*maa://22525 (70.65), maa://21284 (100.00)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -5955,7 +5955,7 @@
       </c>
       <c r="T43" s="8" t="inlineStr">
         <is>
-          <t>maa://43198 (100.00), *maa://46286 (57.95)</t>
+          <t>maa://43198 (100.00), *maa://46286 (72.22)</t>
         </is>
       </c>
       <c r="U43" s="19" t="n"/>
@@ -6008,7 +6008,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (100.00), maa://56386 (100.00), maa://27728 (94.79)</t>
+          <t>maa://29768 (97.96), maa://56386 (100.00), maa://27728 (92.86)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://42459 (100.00), maa://21229 (84.95), maa://30807 (94.62)</t>
+          <t>maa://42459 (100.00), maa://21229 (83.16), maa://30807 (92.63)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6231,7 +6231,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (96.94), maa://29661 (95.92), maa://56236 (100.00), *maa://28038 (59.18)</t>
+          <t>maa://27410 (95.96), maa://29661 (94.95), maa://56236 (100.00), *maa://28038 (58.59)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6538,7 +6538,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (100.00), maa://59378 (88.66), maa://65511 (96.91)</t>
+          <t>maa://59394 (100.00), maa://59378 (87.76), maa://65511 (97.96)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6708,7 +6708,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://25176 (100.00), maa://56237 (95.70)</t>
+          <t>maa://25176 (100.00), maa://56237 (100.00)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6744,7 +6744,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (100.00), maa://27746 (83.16)</t>
+          <t>maa://31270 (100.00), maa://27746 (85.42)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -6798,7 +6798,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (98.90), maa://43903 (94.51), maa://56228 (100.00)</t>
+          <t>maa://42981 (96.81), maa://43903 (94.68), maa://56228 (100.00)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6816,7 +6816,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (100.00), *maa://59693 (56.70), maa://59413 (84.54)</t>
+          <t>maa://59534 (100.00), *maa://59693 (59.18), maa://59413 (89.80)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7174,7 +7174,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.06 13:18:41</t>
+          <t>更新日期：2025.09.08 13:20:19</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8578,7 +8578,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (72.29), *maa://28758 (67.47), maa://29036 (100.00), *maa://42172 (60.24), maa://65357 (86.75), maa://30285 (81.93)</t>
+          <t>*maa://20849 (72.29), *maa://28758 (67.47), maa://29036 (100.00), *maa://42172 (60.24), maa://65357 (89.16), maa://30285 (81.93)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -10414,7 +10414,7 @@
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (100.00), maa://31559 (86.32), maa://24093 (100.00), maa://20924 (81.05), *maa://25777 (64.21), *maa://20631 (64.21), **maa://28241 (46.32)</t>
+          <t>maa://20841 (100.00), maa://31559 (85.42), maa://24093 (98.96), maa://20924 (80.21), *maa://25777 (63.54), *maa://20631 (63.54), **maa://28241 (45.83)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -10684,7 +10684,7 @@
       </c>
       <c r="D66" s="13" t="inlineStr">
         <is>
-          <t>maa://20993 (100.00), maa://45606 (92.63), **maa://20914 (46.32), maa://20829 (81.05), maa://20900 (85.26), **maa://40159 (46.32)</t>
+          <t>maa://20993 (100.00), maa://45606 (93.68), **maa://20914 (46.32), maa://20829 (81.05), maa://20900 (85.26), **maa://40159 (46.32)</t>
         </is>
       </c>
       <c r="E66" s="14" t="inlineStr">
@@ -10900,7 +10900,7 @@
       </c>
       <c r="D70" s="13" t="inlineStr">
         <is>
-          <t>maa://20944 (94.57), maa://35393 (100.00)</t>
+          <t>maa://20944 (93.55), maa://35393 (100.00)</t>
         </is>
       </c>
       <c r="E70" s="14" t="inlineStr">
@@ -11008,7 +11008,7 @@
       </c>
       <c r="D72" s="13" t="inlineStr">
         <is>
-          <t>maa://36643 (100.00), maa://36864 (95.88), maa://39140 (94.85), *maa://66335 (58.76)</t>
+          <t>maa://36643 (100.00), maa://36864 (95.88), maa://39140 (94.85), *maa://66335 (62.89)</t>
         </is>
       </c>
       <c r="E72" s="14" t="inlineStr">
@@ -13006,7 +13006,7 @@
       </c>
       <c r="D109" s="13" t="inlineStr">
         <is>
-          <t>maa://36646 (100.00), maa://25774 (90.82), maa://35996 (94.90), maa://22469 (84.69), *maa://30668 (71.43), *maa://67286 (58.16)</t>
+          <t>maa://36646 (100.00), maa://25774 (90.82), maa://35996 (94.90), maa://22469 (84.69), *maa://30668 (71.43), *maa://67286 (62.24)</t>
         </is>
       </c>
       <c r="E109" s="14" t="inlineStr">
@@ -14842,7 +14842,7 @@
       </c>
       <c r="D143" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (100.00), **maa://23736 (44.68), *maa://31185 (65.96), *maa://30306 (54.26)</t>
+          <t>maa://28484 (100.00), **maa://23736 (44.68), *maa://31185 (69.15), *maa://30306 (54.26)</t>
         </is>
       </c>
       <c r="E143" s="14" t="inlineStr">
@@ -14896,7 +14896,7 @@
       </c>
       <c r="D144" s="13" t="inlineStr">
         <is>
-          <t>maa://30670 (100.00), maa://31470 (87.10), **maa://45066 (38.71), *maa://61380 (77.42), ***maa://30867 (12.90)</t>
+          <t>maa://30670 (100.00), maa://31470 (87.10), **maa://45066 (38.71), *maa://61380 (79.57), ***maa://30867 (12.90)</t>
         </is>
       </c>
       <c r="E144" s="14" t="inlineStr">
@@ -15220,7 +15220,7 @@
       </c>
       <c r="D150" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (95.88), maa://36641 (100.00), maa://36865 (93.81), maa://44635 (83.51), maa://44660 (83.51), *maa://41128 (72.16), maa://42918 (92.78), maa://46108 (89.69), maa://44119 (89.69), *maa://37300 (58.76), *maa://64408 (72.16), **maa://42917 (35.05)</t>
+          <t>maa://40957 (95.88), maa://36641 (100.00), maa://36865 (93.81), maa://44635 (83.51), maa://44660 (83.51), *maa://41128 (72.16), maa://42918 (92.78), maa://46108 (89.69), maa://44119 (89.69), *maa://37300 (58.76), *maa://64408 (74.23), **maa://42917 (35.05)</t>
         </is>
       </c>
       <c r="E150" s="14" t="inlineStr">
@@ -15760,7 +15760,7 @@
       </c>
       <c r="D160" s="13" t="inlineStr">
         <is>
-          <t>maa://44232 (100.00), *maa://45603 (78.35), ***maa://63114 (21.65), ***maa://65963 (21.65)</t>
+          <t>maa://44232 (100.00), *maa://45603 (78.35), ***maa://63114 (21.65), **maa://65963 (30.93)</t>
         </is>
       </c>
       <c r="E160" s="14" t="inlineStr">
@@ -16192,7 +16192,7 @@
       </c>
       <c r="D168" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (98.89), maa://29627 (98.89), maa://29659 (82.22), maa://49074 (100.00), **maa://30679 (34.44), maa://29861 (86.67), *maa://42343 (77.78)</t>
+          <t>maa://29633 (100.00), maa://29627 (100.00), maa://29659 (83.15), maa://49074 (98.88), **maa://30679 (34.83), maa://29861 (87.64), *maa://42343 (78.65)</t>
         </is>
       </c>
       <c r="E168" s="14" t="inlineStr">
@@ -17812,7 +17812,7 @@
       </c>
       <c r="D198" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (92.63), maa://35854 (81.05), maa://50388 (100.00), maa://25760 (83.16), ***maa://43911 (4.21), **maa://20872 (34.74), *maa://51066 (55.79), maa://63024 (83.16)</t>
+          <t>maa://44224 (92.63), maa://35854 (81.05), maa://50388 (100.00), maa://25760 (83.16), ***maa://43911 (4.21), **maa://20872 (34.74), *maa://51066 (55.79), maa://63024 (84.21)</t>
         </is>
       </c>
       <c r="E198" s="14" t="inlineStr">
@@ -17866,7 +17866,7 @@
       </c>
       <c r="D199" s="13" t="inlineStr">
         <is>
-          <t>maa://39156 (100.00), **maa://39550 (39.08), **maa://53417 (47.13), *maa://63806 (56.32)</t>
+          <t>maa://39156 (100.00), **maa://39550 (39.08), **maa://53417 (47.13), *maa://63806 (60.92)</t>
         </is>
       </c>
       <c r="E199" s="14" t="inlineStr">
@@ -17920,7 +17920,7 @@
       </c>
       <c r="D200" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (98.72), *maa://28190 (58.97), maa://22894 (100.00), *maa://20906 (62.82), ***maa://20907 (25.64)</t>
+          <t>maa://27823 (100.00), *maa://28190 (58.97), maa://22894 (100.00), *maa://20906 (62.82), ***maa://20907 (25.64)</t>
         </is>
       </c>
       <c r="E200" s="14" t="inlineStr">
@@ -17974,7 +17974,7 @@
       </c>
       <c r="D201" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (98.72), *maa://28190 (58.97), maa://22894 (100.00), *maa://20906 (62.82), ***maa://20907 (25.64)</t>
+          <t>maa://27823 (100.00), *maa://28190 (58.97), maa://22894 (100.00), *maa://20906 (62.82), ***maa://20907 (25.64)</t>
         </is>
       </c>
       <c r="E201" s="14" t="inlineStr">
@@ -20188,7 +20188,7 @@
       </c>
       <c r="D242" s="13" t="inlineStr">
         <is>
-          <t>maa://30667 (94.94), maa://30666 (100.00), **maa://30739 (35.44), *maa://30723 (56.96), maa://39588 (97.47), maa://64079 (87.34), *maa://65726 (55.70)</t>
+          <t>maa://30667 (94.94), maa://30666 (100.00), **maa://30739 (35.44), *maa://30723 (56.96), maa://39588 (97.47), maa://64079 (88.61), *maa://65726 (64.56)</t>
         </is>
       </c>
       <c r="E242" s="14" t="inlineStr">
@@ -22024,7 +22024,7 @@
       </c>
       <c r="D276" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (100.00), maa://51630 (92.86), maa://56588 (84.69), **maa://55171 (41.84), *maa://51893 (61.22), ***maa://60902 (19.39), **maa://66758 (30.61)</t>
+          <t>maa://51881 (100.00), maa://51630 (92.86), maa://56588 (84.69), **maa://55171 (41.84), *maa://51893 (61.22), ***maa://60902 (19.39), **maa://66758 (41.84)</t>
         </is>
       </c>
       <c r="E276" s="14" t="inlineStr">
@@ -26560,7 +26560,7 @@
       </c>
       <c r="D360" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.00), maa://49695 (100.00), maa://49758 (92.00), **maa://59402 (41.00), **maa://52357 (48.00), ***maa://63091 (25.00)</t>
+          <t>maa://49696 (99.00), maa://49695 (100.00), maa://49758 (93.00), **maa://59402 (41.00), **maa://52357 (48.00), **maa://63091 (31.00)</t>
         </is>
       </c>
       <c r="E360" s="22" t="inlineStr">
@@ -26884,7 +26884,7 @@
       </c>
       <c r="D366" s="22" t="inlineStr">
         <is>
-          <t>maa://42635 (100.00), **maa://50629 (45.24), **maa://48859 (40.48)</t>
+          <t>maa://42635 (100.00), *maa://50629 (52.38), **maa://48859 (40.48)</t>
         </is>
       </c>
       <c r="E366" s="22" t="inlineStr">
@@ -27046,7 +27046,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (100.00), maa://48026 (95.70), maa://44635 (87.10), maa://41035 (92.47), maa://44660 (87.10), *maa://60251 (56.99), *maa://41128 (75.27)</t>
+          <t>maa://40957 (100.00), maa://48026 (95.70), maa://44635 (87.10), maa://41035 (92.47), *maa://60251 (56.99), maa://44660 (87.10), *maa://41128 (75.27)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -28558,7 +28558,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>maa://51872 (100.00), maa://51876 (100.00), *maa://63228 (75.79), maa://51873 (97.89), *maa://62047 (78.95)</t>
+          <t>maa://51872 (100.00), maa://51876 (100.00), *maa://63228 (76.84), maa://51873 (97.89), *maa://62047 (78.95)</t>
         </is>
       </c>
       <c r="E401" t="inlineStr">
@@ -28715,12 +28715,12 @@
       </c>
       <c r="C407" s="17" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>maa://64040 (100.00), *maa://66377 (62.50), ***maa://66376 (6.25)</t>
+          <t>maa://64040 (98.97), maa://52505 (100.00), *maa://66377 (67.01), ***maa://66376 (6.19)</t>
         </is>
       </c>
       <c r="E407" t="inlineStr">
@@ -28801,7 +28801,7 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>maa://67089 (100.00), ***maa://67271 (14.75)</t>
+          <t>maa://67089 (100.00), *maa://67271 (64.47)</t>
         </is>
       </c>
       <c r="E410" t="inlineStr">
@@ -28855,7 +28855,7 @@
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>maa://67087 (100.00), maa://67268 (82.43), *maa://67269 (77.03)</t>
+          <t>maa://67087 (100.00), maa://67268 (97.50), maa://67269 (81.25)</t>
         </is>
       </c>
       <c r="E412" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#235)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -712,7 +712,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (97.26), maa://24702 (95.02), maa://36681 (86.21)</t>
+          <t>maa://25390 (97.50), maa://24702 (95.02), maa://36681 (86.21)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://39402 (92.99), maa://58660 (98.16), *maa://34787 (74.49)</t>
+          <t>maa://58660 (98.03), maa://39402 (93.37), *maa://34787 (74.49)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -776,7 +776,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (96.09), maa://66635 (99.64)</t>
+          <t>maa://22742 (96.20), maa://66635 (99.68)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://36684 (97.34), maa://21246 (91.29)</t>
+          <t>maa://36684 (97.55), maa://21246 (91.29)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://59087 (95.81), maa://25251 (92.20)</t>
+          <t>maa://59087 (95.87), maa://25251 (92.20)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -842,7 +842,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (99.14), maa://36987 (96.92), maa://39849 (88.89)</t>
+          <t>maa://40192 (99.23), maa://36987 (96.97), maa://39849 (88.89)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -858,7 +858,7 @@
       </c>
       <c r="H3" s="8" t="inlineStr">
         <is>
-          <t>maa://21247 (99.17)</t>
+          <t>maa://21247 (99.24)</t>
         </is>
       </c>
       <c r="I3" s="19" t="n"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>maa://22880 (85.76), maa://20276 (92.49), maa://22749 (82.61)</t>
+          <t>maa://22880 (86.37), maa://20276 (92.86), maa://22749 (82.61)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -890,7 +890,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (97.79), maa://26254 (98.00), *maa://22738 (75.00)</t>
+          <t>maa://21249 (97.86), maa://26254 (98.04), *maa://22738 (80.00)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://45854 (82.76), maa://60545 (97.72), maa://24617 (91.18)</t>
+          <t>maa://45854 (83.33), maa://60545 (97.93), maa://24617 (91.18)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (88.77), maa://27484 (98.89), maa://27480 (85.71)</t>
+          <t>maa://27396 (89.29), maa://27484 (98.96), maa://27480 (84.31)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://52241 (98.94), maa://24390 (96.49)</t>
+          <t>maa://52241 (99.02), maa://24390 (96.55)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -954,7 +954,7 @@
       </c>
       <c r="AF3" s="8" t="inlineStr">
         <is>
-          <t>maa://21289 (89.47)</t>
+          <t>maa://21289 (90.12)</t>
         </is>
       </c>
       <c r="AG3" s="16" t="n"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (97.00), maa://22499 (88.89), maa://22746 (100.00)</t>
+          <t>maa://24632 (97.22), maa://22499 (88.89), maa://22746 (100.00)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (98.56), maa://50121 (95.60)</t>
+          <t>maa://49983 (98.68), maa://50121 (95.70)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://27295 (96.95), maa://32509 (95.18), maa://31008 (92.86), maa://22754 (88.00)</t>
+          <t>maa://27295 (97.18), maa://32509 (95.27), maa://31008 (93.53), maa://22754 (88.00)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="X4" s="8" t="inlineStr">
         <is>
-          <t>maa://43217 (98.32)</t>
+          <t>maa://43217 (98.46)</t>
         </is>
       </c>
       <c r="Y4" s="19" t="n"/>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>*maa://39394 (60.00), *maa://30062 (63.33), ***maa://26209 (13.04)</t>
+          <t>*maa://39394 (60.00), *maa://30062 (62.30), ***maa://26209 (13.04)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (88.82), maa://54105 (97.59), *maa://22744 (79.31)</t>
+          <t>maa://21245 (89.41), maa://54105 (97.76), *maa://22744 (79.31)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="L5" s="8" t="inlineStr">
         <is>
-          <t>maa://22757 (88.24)</t>
+          <t>maa://22757 (88.51)</t>
         </is>
       </c>
       <c r="M5" s="19" t="n"/>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="P5" s="8" t="inlineStr">
         <is>
-          <t>maa://21919 (98.71), maa://21281 (81.25)</t>
+          <t>maa://21919 (98.78), maa://21281 (81.25)</t>
         </is>
       </c>
       <c r="Q5" s="19" t="n"/>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="AB5" s="8" t="inlineStr">
         <is>
-          <t>*maa://29863 (63.04), ***maa://22752 (12.50), **maa://26013 (36.36)</t>
+          <t>*maa://29863 (63.83), ***maa://22752 (12.50), **maa://26013 (33.33)</t>
         </is>
       </c>
       <c r="AC5" s="19" t="n"/>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="D6" s="8" t="inlineStr">
         <is>
-          <t>maa://42407 (96.18)</t>
+          <t>maa://42407 (96.34)</t>
         </is>
       </c>
       <c r="E6" s="19" t="n"/>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="H6" s="8" t="inlineStr">
         <is>
-          <t>maa://24370 (96.74)</t>
+          <t>maa://24370 (96.77)</t>
         </is>
       </c>
       <c r="I6" s="19" t="n"/>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="L6" s="8" t="inlineStr">
         <is>
-          <t>maa://24839 (99.16)</t>
+          <t>maa://24839 (99.19)</t>
         </is>
       </c>
       <c r="M6" s="19" t="n"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (98.20), maa://30381 (95.00)</t>
+          <t>maa://31836 (98.31), maa://30381 (95.00)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="T6" s="8" t="inlineStr">
         <is>
-          <t>*maa://37411 (80.00)</t>
+          <t>*maa://37411 (77.78)</t>
         </is>
       </c>
       <c r="U6" s="19" t="n"/>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="X6" s="8" t="inlineStr">
         <is>
-          <t>maa://52754 (95.00)</t>
+          <t>maa://52754 (95.45)</t>
         </is>
       </c>
       <c r="Y6" s="19" t="n"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="AB6" s="8" t="inlineStr">
         <is>
-          <t>maa://22739 (91.14)</t>
+          <t>maa://22739 (91.36)</t>
         </is>
       </c>
       <c r="AC6" s="19" t="n"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="AF6" s="8" t="inlineStr">
         <is>
-          <t>*maa://33152 (75.45), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (75.68), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="16" t="n"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>maa://21955 (97.35)</t>
+          <t>maa://21955 (97.60)</t>
         </is>
       </c>
       <c r="E7" s="19" t="n"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>*maa://22763 (71.70), maa://64972 (100.00)</t>
+          <t>*maa://22763 (72.22), maa://64972 (92.86)</t>
         </is>
       </c>
       <c r="I7" s="19" t="n"/>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (98.18), maa://24957 (94.34)</t>
+          <t>maa://28624 (98.17), maa://24957 (94.34)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="P7" s="8" t="inlineStr">
         <is>
-          <t>maa://22750 (95.50)</t>
+          <t>maa://22750 (95.80)</t>
         </is>
       </c>
       <c r="Q7" s="19" t="n"/>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="T7" s="8" t="inlineStr">
         <is>
-          <t>maa://21291 (91.38)</t>
+          <t>maa://21291 (92.00)</t>
         </is>
       </c>
       <c r="U7" s="19" t="n"/>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (96.77), maa://22758 (80.85)</t>
+          <t>maa://22399 (96.66), maa://22758 (80.85)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="AF7" s="8" t="inlineStr">
         <is>
-          <t>maa://45272 (98.82)</t>
+          <t>maa://45272 (98.88)</t>
         </is>
       </c>
       <c r="AG7" s="16" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.08 23:48:05</t>
+          <t>更新日期：2025.09.10 13:19:23</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (86.73), *maa://39431 (52.38), **maa://37551 (50.00)</t>
+          <t>maa://21476 (87.70), *maa://39431 (52.38), **maa://37551 (50.00)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
-          <t>*maa://24371 (72.03)</t>
+          <t>*maa://24371 (72.79)</t>
         </is>
       </c>
       <c r="I8" s="19" t="n"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (89.34), maa://23252 (91.67), maa://37496 (98.21)</t>
+          <t>maa://32931 (89.88), maa://23252 (91.67), maa://37496 (98.21)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (95.83), maa://67587 (100.00)</t>
+          <t>maa://21411 (95.93), maa://67587 (97.62)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="AB8" s="8" t="inlineStr">
         <is>
-          <t>maa://25389 (93.02)</t>
+          <t>maa://25389 (93.33)</t>
         </is>
       </c>
       <c r="AC8" s="19" t="n"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>maa://24479 (82.00), *maa://21990 (51.72)</t>
+          <t>maa://24479 (82.05), *maa://21990 (51.72)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>maa://22765 (93.41), *maa://21915 (78.05)</t>
+          <t>maa://22765 (93.78), *maa://21915 (78.05)</t>
         </is>
       </c>
       <c r="E9" s="19" t="n"/>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="H9" s="8" t="inlineStr">
         <is>
-          <t>*maa://47450 (73.33), maa://56348 (92.31)</t>
+          <t>*maa://47450 (70.59), maa://56348 (92.31)</t>
         </is>
       </c>
       <c r="I9" s="19" t="n"/>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (94.97), maa://39552 (85.37)</t>
+          <t>maa://22762 (95.15), maa://39552 (85.71)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="T9" s="8" t="inlineStr">
         <is>
-          <t>maa://26222 (99.20)</t>
+          <t>maa://26222 (99.27)</t>
         </is>
       </c>
       <c r="U9" s="19" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://52237 (99.53), maa://26223 (98.28)</t>
+          <t>maa://52237 (99.57), maa://26223 (98.29)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (93.50), maa://40166 (92.99)</t>
+          <t>maa://28711 (93.38), maa://40166 (93.49)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (90.65), maa://66916 (97.73)</t>
+          <t>maa://26206 (90.73), maa://66916 (97.96)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>maa://54000 (95.00)</t>
+          <t>maa://54000 (94.03)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (89.34), *maa://36669 (74.32), *maa://23264 (64.52)</t>
+          <t>maa://28977 (89.86), *maa://36669 (74.32), *maa://23264 (64.52)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (98.81), maa://22755 (90.85), maa://63521 (93.29)</t>
+          <t>maa://27395 (98.89), maa://22755 (90.91), maa://63521 (93.33)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://45828 (98.64), maa://22301 (97.63), maa://22726 (100.00)</t>
+          <t>maa://45828 (98.77), maa://22301 (97.63), maa://22726 (100.00)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>*maa://25021 (53.24), *maa://22733 (67.80), **maa://22761 (33.33)</t>
+          <t>*maa://25021 (53.90), *maa://22733 (68.33), **maa://22761 (33.33)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="D11" s="8" t="inlineStr">
         <is>
-          <t>maa://36707 (99.67)</t>
+          <t>maa://36707 (99.69)</t>
         </is>
       </c>
       <c r="E11" s="19" t="n"/>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="L11" s="8" t="inlineStr">
         <is>
-          <t>maa://21287 (92.11)</t>
+          <t>maa://21287 (91.88)</t>
         </is>
       </c>
       <c r="M11" s="19" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (91.92), maa://22501 (99.28), maa://64808 (100.00), maa://45521 (94.74)</t>
+          <t>maa://22747 (92.34), maa://22501 (99.34), maa://64808 (100.00), maa://45521 (94.74)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="AB11" s="8" t="inlineStr">
         <is>
-          <t>maa://29912 (99.51), maa://22516 (86.52)</t>
+          <t>maa://29912 (99.56), maa://22516 (86.52)</t>
         </is>
       </c>
       <c r="AC11" s="19" t="n"/>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="AF11" s="8" t="inlineStr">
         <is>
-          <t>maa://31203 (98.15)</t>
+          <t>maa://31203 (98.18)</t>
         </is>
       </c>
       <c r="AG11" s="16" t="n"/>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>maa://36678 (95.24), maa://30766 (90.91)</t>
+          <t>maa://36678 (95.35), maa://30766 (90.91)</t>
         </is>
       </c>
       <c r="E12" s="19" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (92.54), maa://54294 (94.62)</t>
+          <t>maa://21867 (92.61), maa://54294 (95.05)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (97.02), maa://64046 (97.93)</t>
+          <t>maa://63896 (97.04), maa://64046 (98.03)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="P12" s="8" t="inlineStr">
         <is>
-          <t>maa://57541 (95.65)</t>
+          <t>maa://57541 (91.67)</t>
         </is>
       </c>
       <c r="Q12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>*maa://21485 (79.51), maa://37962 (97.91), maa://22753 (92.67)</t>
+          <t>maa://37962 (98.12), *maa://21485 (79.33), maa://22753 (92.67)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://36677 (98.50), maa://23669 (95.37), maa://39872 (97.37)</t>
+          <t>maa://36677 (98.60), maa://23669 (95.37), maa://39872 (97.53)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>maa://28932 (91.62)</t>
+          <t>maa://28932 (92.21)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (95.51), maa://36673 (93.22), maa://25001 (87.80)</t>
+          <t>maa://24999 (95.77), maa://36673 (93.33), maa://25001 (87.80)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.42), maa://66545 (98.52)</t>
+          <t>*maa://21248 (72.90), maa://66545 (98.64)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (95.83), maa://22583 (83.19)</t>
+          <t>maa://22676 (96.17), maa://22583 (83.76)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="X13" s="8" t="inlineStr">
         <is>
-          <t>maa://34957 (92.81)</t>
+          <t>maa://34957 (93.23)</t>
         </is>
       </c>
       <c r="Y13" s="19" t="n"/>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (91.35)</t>
+          <t>maa://39883 (91.80)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2282,7 +2282,7 @@
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>maa://30764 (93.27)</t>
+          <t>maa://30764 (93.69)</t>
         </is>
       </c>
       <c r="E14" s="19" t="n"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (98.30), maa://26245 (96.98), maa://21288 (96.38), maa://36682 (97.35)</t>
+          <t>maa://39841 (98.42), maa://26245 (97.00), maa://36682 (97.56), maa://21288 (96.38)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2330,7 +2330,7 @@
       </c>
       <c r="P14" s="8" t="inlineStr">
         <is>
-          <t>maa://23250 (99.58), maa://20107 (87.50), maa://22772 (100.00)</t>
+          <t>maa://23250 (99.60), maa://20107 (87.50), maa://22772 (100.00)</t>
         </is>
       </c>
       <c r="Q14" s="19" t="n"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://42751 (98.29), maa://22521 (95.15)</t>
+          <t>maa://42751 (98.39), maa://22521 (95.48)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="X14" s="8" t="inlineStr">
         <is>
-          <t>maa://37468 (96.97)</t>
+          <t>maa://37468 (97.18)</t>
         </is>
       </c>
       <c r="Y14" s="19" t="n"/>
@@ -2378,7 +2378,7 @@
       </c>
       <c r="AB14" s="8" t="inlineStr">
         <is>
-          <t>maa://22764 (98.46)</t>
+          <t>maa://22764 (98.53)</t>
         </is>
       </c>
       <c r="AC14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (84.09), maa://45058 (97.69), maa://22734 (84.50), *maa://36048 (74.10)</t>
+          <t>maa://22743 (84.11), maa://45058 (97.88), maa://22734 (84.50), *maa://36048 (74.10)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (95.20), maa://21478 (90.24)</t>
+          <t>maa://24304 (95.41), maa://21478 (90.24)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="L15" s="8" t="inlineStr">
         <is>
-          <t>*maa://21334 (65.31)</t>
+          <t>*maa://21334 (66.67)</t>
         </is>
       </c>
       <c r="M15" s="19" t="n"/>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="P15" s="8" t="inlineStr">
         <is>
-          <t>maa://24762 (96.30), *maa://22727 (70.00)</t>
+          <t>maa://24762 (96.67), *maa://22727 (70.00)</t>
         </is>
       </c>
       <c r="Q15" s="19" t="n"/>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="T15" s="8" t="inlineStr">
         <is>
-          <t>maa://23892 (96.97)</t>
+          <t>maa://23892 (97.10)</t>
         </is>
       </c>
       <c r="U15" s="19" t="n"/>
@@ -2492,7 +2492,7 @@
       </c>
       <c r="X15" s="8" t="inlineStr">
         <is>
-          <t>maa://38786 (88.00), maa://56102 (100.00)</t>
+          <t>maa://38786 (88.89), maa://56102 (100.00)</t>
         </is>
       </c>
       <c r="Y15" s="19" t="n"/>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://36666 (94.75), maa://21364 (83.01)</t>
+          <t>maa://36666 (95.06), maa://21364 (83.01)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://37650 (99.55), maa://21441 (96.62), maa://36679 (94.55)</t>
+          <t>maa://37650 (99.60), maa://21441 (96.62), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2590,7 +2590,7 @@
       </c>
       <c r="P16" s="8" t="inlineStr">
         <is>
-          <t>maa://28504 (95.15)</t>
+          <t>maa://28504 (95.19)</t>
         </is>
       </c>
       <c r="Q16" s="19" t="n"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://36674 (96.57), maa://22729 (95.52), *maa://28648 (77.42)</t>
+          <t>maa://36674 (96.86), maa://22729 (95.59), *maa://28648 (77.42)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2622,7 +2622,7 @@
       </c>
       <c r="X16" s="8" t="inlineStr">
         <is>
-          <t>maa://28501 (98.95), maa://28051 (96.77)</t>
+          <t>maa://28501 (98.99), maa://28051 (96.88)</t>
         </is>
       </c>
       <c r="Y16" s="19" t="n"/>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="AB16" s="8" t="inlineStr">
         <is>
-          <t>maa://26228 (97.53)</t>
+          <t>maa://26228 (97.23)</t>
         </is>
       </c>
       <c r="AC16" s="19" t="n"/>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>maa://23911 (88.09), maa://27755 (93.64), maa://67613 (100.00)</t>
+          <t>maa://23911 (88.48), maa://27755 (93.64), maa://67613 (100.00)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://39599 (96.58), maa://22430 (90.13)</t>
+          <t>maa://39599 (96.87), maa://22430 (90.17)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="L17" s="8" t="inlineStr">
         <is>
-          <t>maa://21679 (84.62)</t>
+          <t>maa://21679 (86.36)</t>
         </is>
       </c>
       <c r="M17" s="19" t="n"/>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (82.20), maa://56238 (96.88)</t>
+          <t>maa://23890 (82.20), maa://56238 (97.18)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="AF17" s="8" t="inlineStr">
         <is>
-          <t>maa://50136 (98.44)</t>
+          <t>maa://50136 (98.48)</t>
         </is>
       </c>
       <c r="AG17" s="16" t="n"/>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>maa://24570 (97.83)</t>
+          <t>maa://24570 (97.91)</t>
         </is>
       </c>
       <c r="E18" s="19" t="n"/>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="H18" s="8" t="inlineStr">
         <is>
-          <t>maa://24421 (93.46)</t>
+          <t>maa://24421 (93.84)</t>
         </is>
       </c>
       <c r="I18" s="19" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://52226 (99.36), maa://22466 (92.79)</t>
+          <t>maa://52226 (99.43), maa://22466 (92.79)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), maa://54153 (99.41), maa://24380 (100.00)</t>
+          <t>maa://24379 (100.00), maa://54153 (99.46), maa://24380 (100.00)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2866,7 +2866,7 @@
       </c>
       <c r="T18" s="8" t="inlineStr">
         <is>
-          <t>maa://24385 (98.21)</t>
+          <t>maa://24385 (98.28)</t>
         </is>
       </c>
       <c r="U18" s="19" t="n"/>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (98.14), maa://22741 (90.91)</t>
+          <t>maa://21917 (98.25), maa://22741 (91.67)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="AB18" s="8" t="inlineStr">
         <is>
-          <t>maa://24393 (98.52)</t>
+          <t>maa://24393 (98.64)</t>
         </is>
       </c>
       <c r="AC18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://47854 (89.02), *maa://24313 (61.02)</t>
+          <t>maa://47854 (89.89), *maa://24313 (61.24)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -2932,7 +2932,7 @@
       </c>
       <c r="D19" s="8" t="inlineStr">
         <is>
-          <t>maa://62850 (99.10)</t>
+          <t>maa://62850 (99.28)</t>
         </is>
       </c>
       <c r="E19" s="19" t="n"/>
@@ -2948,7 +2948,7 @@
       </c>
       <c r="H19" s="8" t="inlineStr">
         <is>
-          <t>maa://66740 (88.89)</t>
+          <t>maa://66740 (90.00)</t>
         </is>
       </c>
       <c r="I19" s="19" t="n"/>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="L19" s="8" t="inlineStr">
         <is>
-          <t>maa://39347 (97.06), maa://56392 (100.00)</t>
+          <t>maa://39347 (97.22), maa://56392 (100.00)</t>
         </is>
       </c>
       <c r="M19" s="19" t="n"/>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="T19" s="8" t="inlineStr">
         <is>
-          <t>maa://24386 (99.48)</t>
+          <t>maa://24386 (99.52)</t>
         </is>
       </c>
       <c r="U19" s="19" t="n"/>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (81.06), *maa://36668 (67.29)</t>
+          <t>maa://30709 (81.74), *maa://36668 (67.29)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3044,7 +3044,7 @@
       </c>
       <c r="AF19" s="8" t="inlineStr">
         <is>
-          <t>*maa://21663 (64.71), maa://52239 (80.95)</t>
+          <t>*maa://21663 (64.71), maa://52239 (82.61)</t>
         </is>
       </c>
       <c r="AG19" s="16" t="n"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://25198 (97.22), maa://36680 (98.37), maa://21432 (91.30)</t>
+          <t>maa://25198 (97.42), maa://36680 (98.48), maa://21432 (91.34)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3078,7 +3078,7 @@
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>maa://22864 (94.03)</t>
+          <t>maa://22864 (94.24)</t>
         </is>
       </c>
       <c r="I20" s="19" t="n"/>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (93.35)</t>
+          <t>maa://41331 (93.71)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="P20" s="8" t="inlineStr">
         <is>
-          <t>maa://37442 (97.80)</t>
+          <t>maa://37442 (97.92)</t>
         </is>
       </c>
       <c r="Q20" s="19" t="n"/>
@@ -3126,7 +3126,7 @@
       </c>
       <c r="T20" s="8" t="inlineStr">
         <is>
-          <t>maa://29113 (91.80)</t>
+          <t>maa://29113 (92.19)</t>
         </is>
       </c>
       <c r="U20" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (94.88), maa://56241 (97.97), maa://49976 (88.24)</t>
+          <t>maa://50085 (94.89), maa://56241 (98.17), maa://49976 (88.24)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>maa://21261 (98.78)</t>
+          <t>maa://21261 (98.82)</t>
         </is>
       </c>
       <c r="E21" s="19" t="n"/>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="H21" s="8" t="inlineStr">
         <is>
-          <t>maa://24372 (98.34)</t>
+          <t>maa://24372 (98.42)</t>
         </is>
       </c>
       <c r="I21" s="19" t="n"/>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="L21" s="8" t="inlineStr">
         <is>
-          <t>maa://31731 (97.75)</t>
+          <t>maa://31731 (97.83)</t>
         </is>
       </c>
       <c r="M21" s="19" t="n"/>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (97.42), maa://20110 (86.67)</t>
+          <t>maa://34946 (97.53), maa://20110 (86.67)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="AB21" s="8" t="inlineStr">
         <is>
-          <t>maa://21443 (85.09), *maa://52223 (74.81)</t>
+          <t>maa://21443 (85.22), *maa://52223 (76.06)</t>
         </is>
       </c>
       <c r="AC21" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22432 (91.62), maa://22524 (82.67), maa://64221 (97.22)</t>
+          <t>maa://22432 (91.82), maa://22524 (82.37), maa://64221 (97.11)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>maa://25236 (98.61)</t>
+          <t>maa://25236 (98.71)</t>
         </is>
       </c>
       <c r="I22" s="19" t="n"/>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>*maa://27127 (79.58), *maa://22751 (70.93), maa://66865 (98.78)</t>
+          <t>*maa://27127 (80.00), *maa://22751 (70.93), maa://66865 (98.91)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://37649 (91.43), maa://21282 (98.87)</t>
+          <t>maa://37649 (91.95), maa://21282 (98.87)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="AB22" s="8" t="inlineStr">
         <is>
-          <t>maa://23656 (99.33)</t>
+          <t>maa://23656 (99.34)</t>
         </is>
       </c>
       <c r="AC22" s="19" t="n"/>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="AF22" s="8" t="inlineStr">
         <is>
-          <t>maa://29658 (96.25)</t>
+          <t>maa://29658 (96.39)</t>
         </is>
       </c>
       <c r="AG22" s="16" t="n"/>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>***maa://28036 (29.21), *maa://41753 (58.49)</t>
+          <t>***maa://28036 (29.21), *maa://41753 (59.26)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (98.03), maa://39875 (95.24)</t>
+          <t>maa://39756 (98.16), maa://39875 (95.28)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (95.72), maa://29748 (81.14), *maa://37566 (78.95)</t>
+          <t>maa://30587 (96.00), maa://29748 (81.36), *maa://37566 (78.95)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="T23" s="8" t="inlineStr">
         <is>
-          <t>maa://31212 (93.83), maa://24387 (83.72), maa://67084 (100.00)</t>
+          <t>maa://31212 (93.83), maa://24387 (84.09), maa://67084 (83.33)</t>
         </is>
       </c>
       <c r="U23" s="19" t="n"/>
@@ -3564,7 +3564,7 @@
       </c>
       <c r="AF23" s="8" t="inlineStr">
         <is>
-          <t>maa://31489 (97.06)</t>
+          <t>maa://31489 (97.30)</t>
         </is>
       </c>
       <c r="AG23" s="16" t="n"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (83.27), maa://46650 (86.55)</t>
+          <t>maa://24368 (83.36), maa://46650 (87.35)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (94.44), maa://23504 (93.96), *maa://25141 (78.47), *maa://36663 (79.25), maa://52227 (97.73)</t>
+          <t>maa://29988 (94.74), maa://23504 (93.98), *maa://25141 (78.47), *maa://36663 (79.25), maa://52227 (97.94)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="AB24" s="8" t="inlineStr">
         <is>
-          <t>maa://39349 (96.15)</t>
+          <t>maa://39349 (96.55)</t>
         </is>
       </c>
       <c r="AC24" s="19" t="n"/>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://64165 (98.69), maa://22523 (80.09), maa://29910 (94.20), maa://45831 (93.10)</t>
+          <t>maa://64165 (98.80), maa://22523 (80.09), maa://29910 (94.20), maa://45831 (93.33)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (96.11), maa://63016 (98.47)</t>
+          <t>maa://29753 (96.14), maa://63016 (98.66)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.26), *maa://25311 (71.53), maa://45047 (83.64)</t>
+          <t>*maa://29063 (73.45), *maa://25311 (71.01), maa://45047 (84.75)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3744,7 +3744,7 @@
       </c>
       <c r="L25" s="8" t="inlineStr">
         <is>
-          <t>maa://24378 (92.75)</t>
+          <t>maa://24378 (92.86)</t>
         </is>
       </c>
       <c r="M25" s="19" t="n"/>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="T25" s="8" t="inlineStr">
         <is>
-          <t>maa://20109 (95.24), maa://22545 (100.00)</t>
+          <t>maa://20109 (95.53), maa://22545 (100.00)</t>
         </is>
       </c>
       <c r="U25" s="19" t="n"/>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="X25" s="8" t="inlineStr">
         <is>
-          <t>maa://29890 (88.78)</t>
+          <t>maa://29890 (89.11)</t>
         </is>
       </c>
       <c r="Y25" s="19" t="n"/>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (92.70), *maa://24516 (79.59), maa://26001 (83.33)</t>
+          <t>maa://31215 (92.28), *maa://24516 (79.59), maa://26001 (83.33)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (97.48), maa://36676 (99.74), maa://24621 (96.82), maa://22771 (87.50), maa://37772 (83.33)</t>
+          <t>maa://20108 (97.56), maa://36676 (99.76), maa://24621 (96.82), maa://22771 (87.50), maa://37772 (83.33)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://56374 (100.00), maa://41802 (95.35)</t>
+          <t>maa://56374 (100.00), maa://41802 (95.45)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3858,7 +3858,7 @@
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
-          <t>maa://56240 (93.97), maa://24913 (91.89)</t>
+          <t>maa://56240 (94.57), maa://24913 (91.89)</t>
         </is>
       </c>
       <c r="I26" s="19" t="n"/>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="AB26" s="8" t="inlineStr">
         <is>
-          <t>maa://42235 (97.83)</t>
+          <t>maa://42235 (97.95)</t>
         </is>
       </c>
       <c r="AC26" s="19" t="n"/>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="AF26" s="8" t="inlineStr">
         <is>
-          <t>*maa://30511 (70.83), **maa://29760 (47.62)</t>
+          <t>*maa://30511 (71.62), **maa://29760 (47.62)</t>
         </is>
       </c>
       <c r="AG26" s="16" t="n"/>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>maa://39601 (88.24), maa://34494 (98.57)</t>
+          <t>maa://39601 (88.89), maa://34494 (98.65)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4004,7 +4004,7 @@
       </c>
       <c r="L27" s="8" t="inlineStr">
         <is>
-          <t>maa://28071 (86.05)</t>
+          <t>maa://28071 (86.96)</t>
         </is>
       </c>
       <c r="M27" s="19" t="n"/>
@@ -4020,7 +4020,7 @@
       </c>
       <c r="P27" s="8" t="inlineStr">
         <is>
-          <t>maa://56400 (87.50)</t>
+          <t>maa://56400 (88.89)</t>
         </is>
       </c>
       <c r="Q27" s="19" t="n"/>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="T27" s="8" t="inlineStr">
         <is>
-          <t>maa://30624 (86.76)</t>
+          <t>maa://30624 (87.76)</t>
         </is>
       </c>
       <c r="U27" s="19" t="n"/>
@@ -4084,7 +4084,7 @@
       </c>
       <c r="AF27" s="8" t="inlineStr">
         <is>
-          <t>maa://24023 (97.22)</t>
+          <t>maa://24023 (97.25)</t>
         </is>
       </c>
       <c r="AG27" s="16" t="n"/>
@@ -4102,7 +4102,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (94.62), maa://25725 (84.03)</t>
+          <t>maa://24465 (94.88), maa://25725 (84.43)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="L28" s="8" t="inlineStr">
         <is>
-          <t>maa://30770 (87.84)</t>
+          <t>maa://30770 (88.16)</t>
         </is>
       </c>
       <c r="M28" s="19" t="n"/>
@@ -4166,7 +4166,7 @@
       </c>
       <c r="T28" s="8" t="inlineStr">
         <is>
-          <t>maa://29765 (90.09), maa://23263 (96.00)</t>
+          <t>maa://29765 (90.62), maa://23263 (96.00)</t>
         </is>
       </c>
       <c r="U28" s="19" t="n"/>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (96.24), maa://41749 (96.73)</t>
+          <t>maa://39929 (96.41), maa://41749 (96.96)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (93.15), maa://65700 (97.98)</t>
+          <t>maa://36660 (93.26), maa://65700 (97.94)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4232,7 +4232,7 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>maa://31694 (99.11)</t>
+          <t>maa://31694 (99.15)</t>
         </is>
       </c>
       <c r="E29" s="19" t="n"/>
@@ -4248,7 +4248,7 @@
       </c>
       <c r="H29" s="8" t="inlineStr">
         <is>
-          <t>**maa://25175 (49.51)</t>
+          <t>**maa://25175 (50.00)</t>
         </is>
       </c>
       <c r="I29" s="19" t="n"/>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (96.88), maa://31400 (98.16), maa://28440 (86.08)</t>
+          <t>maa://28432 (97.07), maa://31400 (98.22), maa://28440 (86.08)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4280,7 +4280,7 @@
       </c>
       <c r="P29" s="8" t="inlineStr">
         <is>
-          <t>maa://54169 (97.26)</t>
+          <t>maa://54169 (97.44)</t>
         </is>
       </c>
       <c r="Q29" s="19" t="n"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://42865 (89.40), *maa://24080 (68.86)</t>
+          <t>maa://42865 (90.00), *maa://24080 (68.86)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="L30" s="8" t="inlineStr">
         <is>
-          <t>maa://30442 (96.94)</t>
+          <t>maa://30442 (97.03)</t>
         </is>
       </c>
       <c r="M30" s="19" t="n"/>
@@ -4410,7 +4410,7 @@
       </c>
       <c r="P30" s="8" t="inlineStr">
         <is>
-          <t>maa://21442 (99.43), maa://66611 (100.00)</t>
+          <t>maa://21442 (99.47), maa://66611 (100.00)</t>
         </is>
       </c>
       <c r="Q30" s="19" t="n"/>
@@ -4426,7 +4426,7 @@
       </c>
       <c r="T30" s="8" t="inlineStr">
         <is>
-          <t>*maa://32940 (76.47), maa://24388 (95.65)</t>
+          <t>*maa://32940 (77.78), maa://24388 (95.65)</t>
         </is>
       </c>
       <c r="U30" s="19" t="n"/>
@@ -4442,7 +4442,7 @@
       </c>
       <c r="X30" s="8" t="inlineStr">
         <is>
-          <t>maa://39477 (94.87)</t>
+          <t>maa://39477 (95.00)</t>
         </is>
       </c>
       <c r="Y30" s="19" t="n"/>
@@ -4458,7 +4458,7 @@
       </c>
       <c r="AB30" s="8" t="inlineStr">
         <is>
-          <t>maa://42979 (99.32), maa://45822 (100.00), maa://45045 (85.71)</t>
+          <t>maa://42979 (99.38), maa://45822 (100.00), maa://45045 (87.50)</t>
         </is>
       </c>
       <c r="AC30" s="19" t="n"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (97.10), maa://36258 (91.97), maa://43904 (86.67)</t>
+          <t>maa://35926 (97.33), maa://36258 (92.20), maa://43904 (86.67)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4556,7 +4556,7 @@
       </c>
       <c r="T31" s="8" t="inlineStr">
         <is>
-          <t>maa://30711 (96.67), maa://30768 (100.00)</t>
+          <t>maa://30711 (96.74), maa://30768 (100.00)</t>
         </is>
       </c>
       <c r="U31" s="19" t="n"/>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://36667 (99.53), maa://21895 (97.91), maa://22760 (100.00)</t>
+          <t>maa://36667 (99.57), maa://21895 (97.91), maa://22760 (100.00)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4654,7 +4654,7 @@
       </c>
       <c r="L32" s="8" t="inlineStr">
         <is>
-          <t>maa://28065 (96.15)</t>
+          <t>maa://28065 (96.34)</t>
         </is>
       </c>
       <c r="M32" s="19" t="n"/>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (99.09), maa://41108 (87.50), maa://41238 (98.07), maa://45523 (100.00)</t>
+          <t>maa://42859 (99.07), maa://41108 (87.50), maa://41238 (98.07), maa://45523 (100.00)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="X32" s="8" t="inlineStr">
         <is>
-          <t>maa://64104 (96.20)</t>
+          <t>maa://64104 (96.25)</t>
         </is>
       </c>
       <c r="Y32" s="19" t="n"/>
@@ -4734,7 +4734,7 @@
       </c>
       <c r="AF32" s="8" t="inlineStr">
         <is>
-          <t>maa://42408 (92.86)</t>
+          <t>maa://42408 (93.33)</t>
         </is>
       </c>
       <c r="AG32" s="16" t="n"/>
@@ -4747,12 +4747,12 @@
       </c>
       <c r="C33" s="19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D33" s="8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>maa://67752 (100.00)</t>
         </is>
       </c>
       <c r="E33" s="19" t="n"/>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (91.55), *maa://22730 (70.59)</t>
+          <t>maa://21956 (91.95), *maa://22730 (70.59)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (98.86), maa://56235 (100.00)</t>
+          <t>maa://48817 (98.91), maa://56235 (100.00)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="T34" s="8" t="inlineStr">
         <is>
-          <t>maa://24526 (95.94)</t>
+          <t>maa://24526 (96.13)</t>
         </is>
       </c>
       <c r="U34" s="19" t="n"/>
@@ -4994,7 +4994,7 @@
       </c>
       <c r="AF34" s="8" t="inlineStr">
         <is>
-          <t>maa://32650 (84.62)</t>
+          <t>maa://32650 (85.37)</t>
         </is>
       </c>
       <c r="AG34" s="16" t="n"/>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
-          <t>maa://41296 (98.97)</t>
+          <t>maa://41296 (99.02)</t>
         </is>
       </c>
       <c r="M35" s="19" t="n"/>
@@ -5124,7 +5124,7 @@
       </c>
       <c r="AF35" s="8" t="inlineStr">
         <is>
-          <t>maa://39479 (95.00)</t>
+          <t>maa://39479 (95.35)</t>
         </is>
       </c>
       <c r="AG35" s="16" t="n"/>
@@ -5206,7 +5206,7 @@
       </c>
       <c r="T36" s="8" t="inlineStr">
         <is>
-          <t>maa://27613 (99.43)</t>
+          <t>maa://27613 (99.44)</t>
         </is>
       </c>
       <c r="U36" s="19" t="n"/>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="H37" s="8" t="inlineStr">
         <is>
-          <t>*maa://24374 (56.90)</t>
+          <t>*maa://24374 (55.93)</t>
         </is>
       </c>
       <c r="I37" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (99.20), maa://56336 (98.88), maa://47069 (85.71), maa://45789 (100.00)</t>
+          <t>maa://45718 (99.23), maa://56336 (98.99), maa://47069 (85.71), maa://45789 (100.00)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="P37" s="8" t="inlineStr">
         <is>
-          <t>maa://21280 (96.36)</t>
+          <t>maa://21280 (96.63)</t>
         </is>
       </c>
       <c r="Q37" s="19" t="n"/>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="P38" s="8" t="inlineStr">
         <is>
-          <t>*maa://24383 (77.78)</t>
+          <t>*maa://24383 (78.06)</t>
         </is>
       </c>
       <c r="Q38" s="19" t="n"/>
@@ -5482,7 +5482,7 @@
       </c>
       <c r="AF38" s="8" t="inlineStr">
         <is>
-          <t>maa://36697 (94.59)</t>
+          <t>maa://36697 (94.88)</t>
         </is>
       </c>
       <c r="AG38" s="16" t="n"/>
@@ -5503,7 +5503,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://25199 (84.92), maa://30434 (94.94), maa://45059 (81.43), *maa://44165 (80.00)</t>
+          <t>maa://25199 (84.92), maa://30434 (94.94), maa://45059 (83.12), maa://44165 (83.33)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://47093 (97.47), maa://24709 (93.18)</t>
+          <t>maa://47093 (97.33), maa://24709 (93.30)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (94.09), maa://45790 (86.21)</t>
+          <t>maa://47079 (94.14), maa://45790 (86.67)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5583,7 +5583,7 @@
       </c>
       <c r="AF39" s="8" t="inlineStr">
         <is>
-          <t>maa://62953 (96.25)</t>
+          <t>maa://62953 (96.55)</t>
         </is>
       </c>
       <c r="AG39" s="16" t="n"/>
@@ -5636,7 +5636,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (97.45), maa://21386 (95.90), maa://36664 (89.19), *maa://45550 (80.00)</t>
+          <t>maa://23278 (97.61), maa://21386 (95.90), maa://36664 (89.33), *maa://45550 (80.00)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://65283 (96.33), maa://64205 (96.55)</t>
+          <t>maa://65283 (96.58), maa://64205 (96.55)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5705,7 +5705,7 @@
       </c>
       <c r="H41" s="8" t="inlineStr">
         <is>
-          <t>maa://24466 (92.06)</t>
+          <t>maa://24466 (92.19)</t>
         </is>
       </c>
       <c r="I41" s="19" t="n"/>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="P41" s="8" t="inlineStr">
         <is>
-          <t>maa://43177 (93.98)</t>
+          <t>maa://43177 (94.05)</t>
         </is>
       </c>
       <c r="Q41" s="19" t="n"/>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>*maa://22525 (71.49), maa://21284 (96.20)</t>
+          <t>*maa://22525 (71.62), maa://21284 (96.50)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -6008,7 +6008,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (98.02), maa://56386 (99.45), maa://27728 (96.33)</t>
+          <t>maa://29768 (98.04), maa://56386 (99.49), maa://27728 (96.33)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6056,7 +6056,7 @@
       </c>
       <c r="T44" s="8" t="inlineStr">
         <is>
-          <t>maa://39366 (92.65)</t>
+          <t>maa://39366 (92.96)</t>
         </is>
       </c>
       <c r="U44" s="19" t="n"/>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://42459 (97.94), maa://21229 (84.86), maa://30807 (94.51)</t>
+          <t>maa://42459 (98.09), maa://21229 (84.93), maa://30807 (94.51)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6125,7 +6125,7 @@
       </c>
       <c r="T45" s="8" t="inlineStr">
         <is>
-          <t>*maa://39364 (60.48)</t>
+          <t>*maa://39364 (61.24)</t>
         </is>
       </c>
       <c r="U45" s="19" t="n"/>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (93.95), maa://43901 (96.04)</t>
+          <t>maa://35931 (94.29), maa://43901 (96.23)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6231,7 +6231,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (97.27), maa://29661 (97.55), maa://56236 (99.80), maa://28038 (84.62)</t>
+          <t>maa://27410 (97.31), maa://29661 (97.56), maa://56236 (99.65), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6263,7 +6263,7 @@
       </c>
       <c r="T47" s="8" t="inlineStr">
         <is>
-          <t>maa://67476 (99.27)</t>
+          <t>maa://67476 (99.40)</t>
         </is>
       </c>
       <c r="U47" s="19" t="n"/>
@@ -6401,7 +6401,7 @@
       </c>
       <c r="T49" s="19" t="inlineStr">
         <is>
-          <t>maa://67231 (99.09)</t>
+          <t>maa://67231 (99.21)</t>
         </is>
       </c>
       <c r="U49" s="19" t="n"/>
@@ -6438,7 +6438,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>maa://62852 (90.77)</t>
+          <t>maa://62852 (91.37)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6472,7 +6472,7 @@
       </c>
       <c r="H51" s="8" t="inlineStr">
         <is>
-          <t>maa://30769 (86.96)</t>
+          <t>maa://30769 (87.50)</t>
         </is>
       </c>
       <c r="I51" s="19" t="n"/>
@@ -6522,7 +6522,7 @@
       </c>
       <c r="H52" s="8" t="inlineStr">
         <is>
-          <t>maa://24376 (98.65)</t>
+          <t>maa://24376 (98.80)</t>
         </is>
       </c>
       <c r="I52" s="19" t="n"/>
@@ -6538,7 +6538,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (99.01), maa://59378 (93.75), maa://65511 (100.00)</t>
+          <t>maa://59394 (98.99), maa://59378 (93.75), maa://65511 (100.00)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6572,7 +6572,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (97.06)</t>
+          <t>maa://32534 (97.19)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -6656,7 +6656,7 @@
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>maa://32532 (96.82)</t>
+          <t>maa://32532 (97.04)</t>
         </is>
       </c>
       <c r="I55" s="19" t="n"/>
@@ -6708,7 +6708,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://25176 (98.75), maa://56237 (98.80)</t>
+          <t>maa://25176 (98.75), maa://56237 (98.91)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6726,7 +6726,7 @@
       </c>
       <c r="H58" s="8" t="inlineStr">
         <is>
-          <t>*maa://37964 (61.70)</t>
+          <t>*maa://37964 (64.00)</t>
         </is>
       </c>
       <c r="I58" s="19" t="n"/>
@@ -6744,7 +6744,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (97.78), maa://27746 (87.88)</t>
+          <t>maa://31270 (97.92), maa://27746 (88.24)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -6762,7 +6762,7 @@
       </c>
       <c r="H60" s="8" t="inlineStr">
         <is>
-          <t>maa://40438 (88.46)</t>
+          <t>maa://40438 (89.06)</t>
         </is>
       </c>
       <c r="I60" s="19" t="n"/>
@@ -6798,7 +6798,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (97.26), maa://43903 (100.00), maa://56228 (98.88)</t>
+          <t>maa://42981 (97.30), maa://43903 (100.00), maa://56228 (99.01)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6816,7 +6816,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (99.18), *maa://59693 (73.81), maa://59413 (95.65)</t>
+          <t>maa://59534 (99.12), *maa://59693 (73.81), maa://59413 (95.74)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7027,12 +7027,12 @@
       </c>
       <c r="G75" s="19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H75" s="19" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>maa://67748 (100.00)</t>
         </is>
       </c>
       <c r="I75" s="19" t="n"/>
@@ -7174,7 +7174,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.08 23:48:05</t>
+          <t>更新日期：2025.09.10 13:19:23</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8578,7 +8578,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (73.21), *maa://28758 (71.11), maa://29036 (96.55), *maa://42172 (71.43), maa://65357 (94.74), maa://30285 (100.00)</t>
+          <t>*maa://20849 (73.21), *maa://28758 (71.11), maa://29036 (96.55), *maa://42172 (71.43), maa://65357 (95.00), maa://30285 (100.00)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8686,7 +8686,7 @@
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>maa://20863 (90.31), maa://20832 (99.20), maa://20727 (100.00)</t>
+          <t>maa://20863 (90.34), maa://20832 (99.20), maa://20727 (100.00)</t>
         </is>
       </c>
       <c r="E29" s="14" t="inlineStr">
@@ -10252,7 +10252,7 @@
       </c>
       <c r="D58" s="13" t="inlineStr">
         <is>
-          <t>maa://28900 (96.94), maa://30126 (100.00)</t>
+          <t>maa://28900 (96.97), maa://30126 (100.00)</t>
         </is>
       </c>
       <c r="E58" s="14" t="inlineStr">
@@ -10792,7 +10792,7 @@
       </c>
       <c r="D68" s="13" t="inlineStr">
         <is>
-          <t>maa://20976 (97.70), maa://20815 (100.00)</t>
+          <t>maa://20976 (97.71), maa://20815 (100.00)</t>
         </is>
       </c>
       <c r="E68" s="14" t="inlineStr">
@@ -13708,7 +13708,7 @@
       </c>
       <c r="D122" s="13" t="inlineStr">
         <is>
-          <t>maa://20869 (100.00), maa://44690 (95.65)</t>
+          <t>maa://20869 (100.00), maa://44690 (95.74)</t>
         </is>
       </c>
       <c r="E122" s="14" t="inlineStr">
@@ -15220,7 +15220,7 @@
       </c>
       <c r="D150" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.77), maa://36641 (98.48), maa://36865 (95.40), maa://44635 (88.07), maa://44660 (92.68), maa://41128 (84.21), maa://42918 (100.00), maa://46108 (100.00), maa://44119 (97.44), maa://37300 (100.00), maa://64408 (100.00), maa://42917 (100.00)</t>
+          <t>maa://40957 (94.78), maa://36641 (98.48), maa://36865 (95.40), maa://44635 (88.07), maa://44660 (92.68), maa://41128 (84.21), maa://42918 (100.00), maa://46108 (100.00), maa://44119 (97.44), maa://37300 (100.00), maa://64408 (100.00), maa://42917 (100.00)</t>
         </is>
       </c>
       <c r="E150" s="14" t="inlineStr">
@@ -16246,7 +16246,7 @@
       </c>
       <c r="D169" s="13" t="inlineStr">
         <is>
-          <t>maa://49867 (94.67), maa://49655 (97.73)</t>
+          <t>maa://49867 (94.81), maa://49655 (97.73)</t>
         </is>
       </c>
       <c r="E169" s="14" t="inlineStr">
@@ -17812,7 +17812,7 @@
       </c>
       <c r="D198" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.31), maa://35854 (84.75), maa://50388 (98.22), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (93.94)</t>
+          <t>maa://44224 (90.33), maa://35854 (84.75), maa://50388 (98.22), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (93.94)</t>
         </is>
       </c>
       <c r="E198" s="14" t="inlineStr">
@@ -24724,7 +24724,7 @@
       </c>
       <c r="D326" s="13" t="inlineStr">
         <is>
-          <t>maa://39692 (99.52), maa://39810 (89.66)</t>
+          <t>maa://39692 (99.53), maa://39810 (89.66)</t>
         </is>
       </c>
       <c r="E326" s="14" t="inlineStr">
@@ -26020,7 +26020,7 @@
       </c>
       <c r="D350" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (97.86), maa://32415 (86.15), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
+          <t>maa://32647 (97.72), maa://32415 (86.15), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E350" s="22" t="inlineStr">
@@ -26560,7 +26560,7 @@
       </c>
       <c r="D360" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.58), maa://49695 (100.00), maa://49758 (98.61), *maa://59402 (58.62), *maa://52357 (73.33), *maa://63091 (62.50)</t>
+          <t>maa://49696 (99.58), maa://49695 (100.00), maa://49758 (98.63), *maa://59402 (58.62), *maa://52357 (73.33), *maa://63091 (62.50)</t>
         </is>
       </c>
       <c r="E360" s="22" t="inlineStr">
@@ -27046,7 +27046,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (94.77), maa://48026 (94.62), maa://44635 (88.07), maa://41035 (93.51), *maa://60251 (76.47), maa://44660 (92.68), maa://41128 (84.21)</t>
+          <t>maa://40957 (94.78), maa://48026 (94.62), maa://44635 (88.07), maa://41035 (93.51), *maa://60251 (76.47), maa://44660 (92.68), maa://41128 (84.21)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -28720,7 +28720,7 @@
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>maa://64040 (98.95), maa://52505 (99.07), maa://66377 (91.67), **maa://66376 (33.33)</t>
+          <t>maa://64040 (98.95), maa://52505 (99.08), maa://66377 (91.67), **maa://66376 (33.33)</t>
         </is>
       </c>
       <c r="E407" t="inlineStr">
@@ -28747,7 +28747,7 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>*maa://67090 (66.67)</t>
+          <t>*maa://67090 (71.43)</t>
         </is>
       </c>
       <c r="E408" t="inlineStr">
@@ -28828,7 +28828,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>maa://67088 (91.67)</t>
+          <t>maa://67088 (92.86)</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
@@ -28850,12 +28850,12 @@
       </c>
       <c r="C412" s="17" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>maa://67087 (91.49), maa://67268 (100.00), maa://67269 (100.00)</t>
+          <t>maa://67087 (92.00), maa://67268 (96.30), maa://67269 (100.00), maa://67648 (100.00)</t>
         </is>
       </c>
       <c r="E412" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#236)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -712,7 +712,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (97.50), maa://24702 (95.02), maa://36681 (86.21)</t>
+          <t>maa://25390 (97.92), maa://24702 (95.02), maa://36681 (86.21)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://58660 (98.03), maa://39402 (93.37), *maa://34787 (74.49)</t>
+          <t>maa://58660 (98.51), maa://39402 (94.39), *maa://34787 (74.75)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -776,7 +776,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (96.20), maa://66635 (99.68)</t>
+          <t>maa://22742 (96.93), maa://66635 (99.77)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://36684 (97.55), maa://21246 (91.29)</t>
+          <t>maa://36684 (98.01), maa://21246 (91.29)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://59087 (95.87), maa://25251 (92.20)</t>
+          <t>maa://59087 (97.00), maa://25251 (92.25)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -842,7 +842,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (99.23), maa://36987 (96.97), maa://39849 (88.89)</t>
+          <t>maa://40192 (99.41), maa://36987 (97.06), maa://39849 (90.00)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>maa://22880 (86.37), maa://20276 (92.86), maa://22749 (82.61)</t>
+          <t>maa://22880 (88.76), maa://20276 (93.58), maa://22749 (84.00)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -890,7 +890,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (97.86), maa://26254 (98.04), *maa://22738 (80.00)</t>
+          <t>maa://21249 (98.17), maa://26254 (98.08), *maa://22738 (80.00)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://45854 (83.33), maa://60545 (97.93), maa://24617 (91.18)</t>
+          <t>maa://45854 (85.71), maa://60545 (98.33), maa://24617 (91.18)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (89.29), maa://27484 (98.96), maa://27480 (84.31)</t>
+          <t>maa://27396 (90.75), maa://27484 (99.17), maa://27480 (84.91)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://52241 (99.02), maa://24390 (96.55)</t>
+          <t>maa://52241 (99.26), maa://24390 (96.72)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -954,7 +954,7 @@
       </c>
       <c r="AF3" s="8" t="inlineStr">
         <is>
-          <t>maa://21289 (90.12)</t>
+          <t>maa://21289 (90.43)</t>
         </is>
       </c>
       <c r="AG3" s="16" t="n"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (97.22), maa://22499 (88.89), maa://22746 (100.00)</t>
+          <t>maa://24632 (97.67), maa://22499 (88.89), maa://22746 (100.00)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (98.68), maa://50121 (95.70)</t>
+          <t>maa://49983 (98.94), maa://50121 (96.19)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://27295 (97.18), maa://32509 (95.27), maa://31008 (93.53), maa://22754 (88.00)</t>
+          <t>maa://27295 (97.31), maa://32509 (95.63), maa://31008 (94.48), maa://22754 (88.00)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="X4" s="8" t="inlineStr">
         <is>
-          <t>maa://43217 (98.46)</t>
+          <t>maa://43217 (98.71)</t>
         </is>
       </c>
       <c r="Y4" s="19" t="n"/>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="AB4" s="8" t="inlineStr">
         <is>
-          <t>*maa://32658 (79.07)</t>
+          <t>maa://32658 (80.43)</t>
         </is>
       </c>
       <c r="AC4" s="19" t="n"/>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>*maa://39394 (60.00), *maa://30062 (62.30), ***maa://26209 (13.04)</t>
+          <t>*maa://39394 (58.70), *maa://30062 (62.30), ***maa://26209 (13.04)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (89.41), maa://54105 (97.76), *maa://22744 (79.31)</t>
+          <t>maa://21245 (90.53), maa://54105 (98.26), *maa://22744 (80.00)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="L5" s="8" t="inlineStr">
         <is>
-          <t>maa://22757 (88.51)</t>
+          <t>maa://22757 (89.90)</t>
         </is>
       </c>
       <c r="M5" s="19" t="n"/>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="P5" s="8" t="inlineStr">
         <is>
-          <t>maa://21919 (98.78), maa://21281 (81.25)</t>
+          <t>maa://21919 (98.97), maa://21281 (81.25)</t>
         </is>
       </c>
       <c r="Q5" s="19" t="n"/>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="X5" s="8" t="inlineStr">
         <is>
-          <t>maa://21290 (100.00)</t>
+          <t>maa://21290 (99.12)</t>
         </is>
       </c>
       <c r="Y5" s="19" t="n"/>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="AB5" s="8" t="inlineStr">
         <is>
-          <t>*maa://29863 (63.83), ***maa://22752 (12.50), **maa://26013 (33.33)</t>
+          <t>*maa://29863 (62.50), ***maa://22752 (12.50), **maa://26013 (33.33)</t>
         </is>
       </c>
       <c r="AC5" s="19" t="n"/>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="D6" s="8" t="inlineStr">
         <is>
-          <t>maa://42407 (96.34)</t>
+          <t>maa://42407 (96.98)</t>
         </is>
       </c>
       <c r="E6" s="19" t="n"/>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="H6" s="8" t="inlineStr">
         <is>
-          <t>maa://24370 (96.77)</t>
+          <t>maa://24370 (97.12)</t>
         </is>
       </c>
       <c r="I6" s="19" t="n"/>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="L6" s="8" t="inlineStr">
         <is>
-          <t>maa://24839 (99.19)</t>
+          <t>maa://24839 (99.31)</t>
         </is>
       </c>
       <c r="M6" s="19" t="n"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (98.31), maa://30381 (95.00)</t>
+          <t>maa://31836 (98.55), maa://30381 (95.00)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="X6" s="8" t="inlineStr">
         <is>
-          <t>maa://52754 (95.45)</t>
+          <t>maa://52754 (95.49)</t>
         </is>
       </c>
       <c r="Y6" s="19" t="n"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="AB6" s="8" t="inlineStr">
         <is>
-          <t>maa://22739 (91.36)</t>
+          <t>maa://22739 (90.59)</t>
         </is>
       </c>
       <c r="AC6" s="19" t="n"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="AF6" s="8" t="inlineStr">
         <is>
-          <t>*maa://33152 (75.68), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (77.87), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="16" t="n"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>maa://21955 (97.60)</t>
+          <t>maa://21955 (97.89)</t>
         </is>
       </c>
       <c r="E7" s="19" t="n"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>*maa://22763 (72.22), maa://64972 (92.86)</t>
+          <t>*maa://22763 (73.21), maa://64972 (94.44)</t>
         </is>
       </c>
       <c r="I7" s="19" t="n"/>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (98.17), maa://24957 (94.34)</t>
+          <t>maa://28624 (98.42), maa://24957 (94.34)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="P7" s="8" t="inlineStr">
         <is>
-          <t>maa://22750 (95.80)</t>
+          <t>maa://22750 (96.35)</t>
         </is>
       </c>
       <c r="Q7" s="19" t="n"/>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="T7" s="8" t="inlineStr">
         <is>
-          <t>maa://21291 (92.00)</t>
+          <t>maa://21291 (93.06)</t>
         </is>
       </c>
       <c r="U7" s="19" t="n"/>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (96.66), maa://22758 (80.85)</t>
+          <t>maa://22399 (96.86), maa://22758 (81.44)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="AF7" s="8" t="inlineStr">
         <is>
-          <t>maa://45272 (98.88)</t>
+          <t>maa://45272 (99.25)</t>
         </is>
       </c>
       <c r="AG7" s="16" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.10 13:19:23</t>
+          <t>更新日期：2025.09.15 13:24:29</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (87.70), *maa://39431 (52.38), **maa://37551 (50.00)</t>
+          <t>maa://21476 (89.66), *maa://39431 (58.33), **maa://37551 (50.00)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
-          <t>*maa://24371 (72.79)</t>
+          <t>*maa://24371 (76.61)</t>
         </is>
       </c>
       <c r="I8" s="19" t="n"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (89.88), maa://23252 (91.67), maa://37496 (98.21)</t>
+          <t>maa://32931 (91.12), maa://23252 (91.67), maa://37496 (98.25)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (95.93), maa://67587 (97.62)</t>
+          <t>maa://21411 (96.12), maa://67587 (97.89)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="AB8" s="8" t="inlineStr">
         <is>
-          <t>maa://25389 (93.33)</t>
+          <t>maa://25389 (93.94)</t>
         </is>
       </c>
       <c r="AC8" s="19" t="n"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>maa://24479 (82.05), *maa://21990 (51.72)</t>
+          <t>maa://24479 (83.33), *maa://21990 (51.72)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>maa://22765 (93.78), *maa://21915 (78.05)</t>
+          <t>maa://22765 (94.96), *maa://21915 (78.57)</t>
         </is>
       </c>
       <c r="E9" s="19" t="n"/>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="H9" s="8" t="inlineStr">
         <is>
-          <t>*maa://47450 (70.59), maa://56348 (92.31)</t>
+          <t>*maa://47450 (75.00), maa://56348 (93.75)</t>
         </is>
       </c>
       <c r="I9" s="19" t="n"/>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (95.15), maa://39552 (85.71)</t>
+          <t>maa://22762 (95.68), maa://39552 (86.36)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1680,7 +1680,7 @@
       </c>
       <c r="P9" s="8" t="inlineStr">
         <is>
-          <t>maa://64516 (100.00), maa://22736 (83.74)</t>
+          <t>maa://64516 (100.00), maa://22736 (83.06)</t>
         </is>
       </c>
       <c r="Q9" s="19" t="n"/>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="T9" s="8" t="inlineStr">
         <is>
-          <t>maa://26222 (99.27)</t>
+          <t>maa://26222 (99.37)</t>
         </is>
       </c>
       <c r="U9" s="19" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://52237 (99.57), maa://26223 (98.29)</t>
+          <t>maa://52237 (99.69), maa://26223 (98.30)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (93.38), maa://40166 (93.49)</t>
+          <t>maa://28711 (94.35), maa://40166 (94.47)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (90.73), maa://66916 (97.96)</t>
+          <t>maa://26206 (90.94), maa://66916 (97.36)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>maa://54000 (94.03)</t>
+          <t>maa://54000 (92.00)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="H10" s="8" t="inlineStr">
         <is>
-          <t>maa://32651 (97.06)</t>
+          <t>maa://32651 (95.00)</t>
         </is>
       </c>
       <c r="I10" s="19" t="n"/>
@@ -1794,7 +1794,7 @@
       </c>
       <c r="L10" s="8" t="inlineStr">
         <is>
-          <t>**maa://24395 (40.00)</t>
+          <t>**maa://24395 (41.30)</t>
         </is>
       </c>
       <c r="M10" s="19" t="n"/>
@@ -1805,12 +1805,12 @@
       </c>
       <c r="O10" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (89.86), *maa://36669 (74.32), *maa://23264 (64.52)</t>
+          <t>maa://28977 (91.10), *maa://36669 (73.33)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (98.89), maa://22755 (90.91), maa://63521 (93.33)</t>
+          <t>maa://27395 (99.09), maa://22755 (91.18), maa://63521 (93.93)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://45828 (98.77), maa://22301 (97.63), maa://22726 (100.00)</t>
+          <t>maa://45828 (98.96), maa://22301 (97.63), maa://22726 (100.00)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>*maa://25021 (53.90), *maa://22733 (68.33), **maa://22761 (33.33)</t>
+          <t>*maa://25021 (55.10), *maa://22733 (67.21), **maa://22761 (33.33)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="L11" s="8" t="inlineStr">
         <is>
-          <t>maa://21287 (91.88)</t>
+          <t>maa://21287 (92.95)</t>
         </is>
       </c>
       <c r="M11" s="19" t="n"/>
@@ -1940,7 +1940,7 @@
       </c>
       <c r="P11" s="8" t="inlineStr">
         <is>
-          <t>maa://45557 (93.55)</t>
+          <t>maa://45557 (95.35)</t>
         </is>
       </c>
       <c r="Q11" s="19" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (92.34), maa://22501 (99.34), maa://64808 (100.00), maa://45521 (94.74)</t>
+          <t>maa://22747 (92.63), maa://22501 (99.45), maa://64808 (100.00), maa://45521 (94.92)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="X11" s="8" t="inlineStr">
         <is>
-          <t>maa://36713 (98.95)</t>
+          <t>maa://36713 (99.13)</t>
         </is>
       </c>
       <c r="Y11" s="19" t="n"/>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="AB11" s="8" t="inlineStr">
         <is>
-          <t>maa://29912 (99.56), maa://22516 (86.52)</t>
+          <t>maa://29912 (99.65), maa://22516 (86.52)</t>
         </is>
       </c>
       <c r="AC11" s="19" t="n"/>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="AF11" s="8" t="inlineStr">
         <is>
-          <t>maa://31203 (98.18)</t>
+          <t>maa://31203 (98.36)</t>
         </is>
       </c>
       <c r="AG11" s="16" t="n"/>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>maa://36678 (95.35), maa://30766 (90.91)</t>
+          <t>maa://36678 (96.23), maa://30766 (91.18)</t>
         </is>
       </c>
       <c r="E12" s="19" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (92.61), maa://54294 (95.05)</t>
+          <t>maa://21867 (93.17), maa://54294 (95.74)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (97.04), maa://64046 (98.03)</t>
+          <t>maa://63896 (97.69), maa://64046 (98.36)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="P12" s="8" t="inlineStr">
         <is>
-          <t>maa://57541 (91.67)</t>
+          <t>maa://57541 (90.32)</t>
         </is>
       </c>
       <c r="Q12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://37962 (98.12), *maa://21485 (79.33), maa://22753 (92.67)</t>
+          <t>maa://37962 (98.52), maa://21485 (80.80), maa://22753 (92.70)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://36677 (98.60), maa://23669 (95.37), maa://39872 (97.53)</t>
+          <t>maa://36677 (98.94), maa://23669 (95.38), maa://39872 (97.75)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>maa://28932 (92.21)</t>
+          <t>maa://28932 (93.56)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (95.77), maa://36673 (93.33), maa://25001 (87.80)</t>
+          <t>maa://24999 (96.24), maa://36673 (93.60), maa://25001 (88.37)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (72.90), maa://66545 (98.64)</t>
+          <t>*maa://21248 (73.09), maa://66545 (98.83)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (96.17), maa://22583 (83.76)</t>
+          <t>maa://22676 (97.08), maa://22583 (86.43)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="X13" s="8" t="inlineStr">
         <is>
-          <t>maa://34957 (93.23)</t>
+          <t>maa://34957 (93.90)</t>
         </is>
       </c>
       <c r="Y13" s="19" t="n"/>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (91.80)</t>
+          <t>maa://39883 (93.09)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2282,7 +2282,7 @@
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>maa://30764 (93.69)</t>
+          <t>maa://30764 (94.62)</t>
         </is>
       </c>
       <c r="E14" s="19" t="n"/>
@@ -2298,7 +2298,7 @@
       </c>
       <c r="H14" s="8" t="inlineStr">
         <is>
-          <t>*maa://32656 (62.50)</t>
+          <t>*maa://32656 (55.56)</t>
         </is>
       </c>
       <c r="I14" s="19" t="n"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (98.42), maa://26245 (97.00), maa://36682 (97.56), maa://21288 (96.38)</t>
+          <t>maa://39841 (98.75), maa://26245 (97.00), maa://36682 (98.14), maa://21288 (96.38)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2330,7 +2330,7 @@
       </c>
       <c r="P14" s="8" t="inlineStr">
         <is>
-          <t>maa://23250 (99.60), maa://20107 (87.50), maa://22772 (100.00)</t>
+          <t>maa://23250 (99.56), maa://20107 (87.50), maa://22772 (100.00)</t>
         </is>
       </c>
       <c r="Q14" s="19" t="n"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://42751 (98.39), maa://22521 (95.48)</t>
+          <t>maa://42751 (98.68), maa://22521 (95.36)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="X14" s="8" t="inlineStr">
         <is>
-          <t>maa://37468 (97.18)</t>
+          <t>maa://37468 (97.59)</t>
         </is>
       </c>
       <c r="Y14" s="19" t="n"/>
@@ -2378,7 +2378,7 @@
       </c>
       <c r="AB14" s="8" t="inlineStr">
         <is>
-          <t>maa://22764 (98.53)</t>
+          <t>maa://22764 (98.73)</t>
         </is>
       </c>
       <c r="AC14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (84.11), maa://45058 (97.88), maa://22734 (84.50), *maa://36048 (74.10)</t>
+          <t>maa://22743 (84.85), maa://45058 (98.14), maa://22734 (84.85), *maa://36048 (73.53)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (95.41), maa://21478 (90.24)</t>
+          <t>maa://24304 (96.22), maa://21478 (90.48)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="P15" s="8" t="inlineStr">
         <is>
-          <t>maa://24762 (96.67), *maa://22727 (70.00)</t>
+          <t>maa://24762 (97.30), *maa://22727 (70.00)</t>
         </is>
       </c>
       <c r="Q15" s="19" t="n"/>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="T15" s="8" t="inlineStr">
         <is>
-          <t>maa://23892 (97.10)</t>
+          <t>maa://23892 (97.37)</t>
         </is>
       </c>
       <c r="U15" s="19" t="n"/>
@@ -2492,7 +2492,7 @@
       </c>
       <c r="X15" s="8" t="inlineStr">
         <is>
-          <t>maa://38786 (88.89), maa://56102 (100.00)</t>
+          <t>maa://38786 (90.91), maa://56102 (100.00)</t>
         </is>
       </c>
       <c r="Y15" s="19" t="n"/>
@@ -2519,12 +2519,12 @@
       </c>
       <c r="AE15" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://36666 (95.06), maa://21364 (83.01)</t>
+          <t>maa://36666 (95.85), maa://21364 (83.33), *maa://22766 (70.50)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://37650 (99.60), maa://21441 (96.62), maa://36679 (94.55)</t>
+          <t>maa://37650 (99.69), maa://21441 (96.62), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2590,7 +2590,7 @@
       </c>
       <c r="P16" s="8" t="inlineStr">
         <is>
-          <t>maa://28504 (95.19)</t>
+          <t>maa://28504 (95.65)</t>
         </is>
       </c>
       <c r="Q16" s="19" t="n"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://36674 (96.86), maa://22729 (95.59), *maa://28648 (77.42)</t>
+          <t>maa://36674 (97.56), maa://22729 (95.90), *maa://28648 (77.89)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2622,7 +2622,7 @@
       </c>
       <c r="X16" s="8" t="inlineStr">
         <is>
-          <t>maa://28501 (98.99), maa://28051 (96.88)</t>
+          <t>maa://28501 (99.16), maa://28051 (96.88)</t>
         </is>
       </c>
       <c r="Y16" s="19" t="n"/>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="AB16" s="8" t="inlineStr">
         <is>
-          <t>maa://26228 (97.23)</t>
+          <t>maa://26228 (97.54)</t>
         </is>
       </c>
       <c r="AC16" s="19" t="n"/>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>maa://23911 (88.48), maa://27755 (93.64), maa://67613 (100.00)</t>
+          <t>maa://23911 (89.70), maa://27755 (93.69), maa://67613 (98.94)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://39599 (96.87), maa://22430 (90.17)</t>
+          <t>maa://39599 (97.79), maa://22430 (90.17)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="L17" s="8" t="inlineStr">
         <is>
-          <t>maa://21679 (86.36)</t>
+          <t>maa://21679 (86.96)</t>
         </is>
       </c>
       <c r="M17" s="19" t="n"/>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (82.20), maa://56238 (97.18)</t>
+          <t>maa://23890 (82.50), maa://56238 (98.02)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="T17" s="8" t="inlineStr">
         <is>
-          <t>*maa://42324 (66.23)</t>
+          <t>*maa://42324 (67.90)</t>
         </is>
       </c>
       <c r="U17" s="19" t="n"/>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="AF17" s="8" t="inlineStr">
         <is>
-          <t>maa://50136 (98.48)</t>
+          <t>maa://50136 (98.78)</t>
         </is>
       </c>
       <c r="AG17" s="16" t="n"/>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>maa://24570 (97.91)</t>
+          <t>maa://24570 (98.12)</t>
         </is>
       </c>
       <c r="E18" s="19" t="n"/>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="H18" s="8" t="inlineStr">
         <is>
-          <t>maa://24421 (93.84)</t>
+          <t>maa://24421 (94.59)</t>
         </is>
       </c>
       <c r="I18" s="19" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://52226 (99.43), maa://22466 (92.79)</t>
+          <t>maa://52226 (99.62), maa://22466 (92.79)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), maa://54153 (99.46), maa://24380 (100.00)</t>
+          <t>maa://24379 (100.00), maa://54153 (99.57), maa://24380 (100.00)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2866,7 +2866,7 @@
       </c>
       <c r="T18" s="8" t="inlineStr">
         <is>
-          <t>maa://24385 (98.28)</t>
+          <t>maa://24385 (98.39)</t>
         </is>
       </c>
       <c r="U18" s="19" t="n"/>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (98.25), maa://22741 (91.67)</t>
+          <t>maa://21917 (98.48), maa://22741 (91.67)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="AB18" s="8" t="inlineStr">
         <is>
-          <t>maa://24393 (98.64)</t>
+          <t>maa://24393 (98.83)</t>
         </is>
       </c>
       <c r="AC18" s="19" t="n"/>
@@ -2909,12 +2909,12 @@
       </c>
       <c r="AE18" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://47854 (89.89), *maa://24313 (61.24)</t>
+          <t>maa://47854 (91.89)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -2948,7 +2948,7 @@
       </c>
       <c r="H19" s="8" t="inlineStr">
         <is>
-          <t>maa://66740 (90.00)</t>
+          <t>maa://66740 (91.67)</t>
         </is>
       </c>
       <c r="I19" s="19" t="n"/>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="L19" s="8" t="inlineStr">
         <is>
-          <t>maa://39347 (97.22), maa://56392 (100.00)</t>
+          <t>maa://39347 (97.73), maa://56392 (100.00)</t>
         </is>
       </c>
       <c r="M19" s="19" t="n"/>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="T19" s="8" t="inlineStr">
         <is>
-          <t>maa://24386 (99.52)</t>
+          <t>maa://24386 (99.60)</t>
         </is>
       </c>
       <c r="U19" s="19" t="n"/>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="X19" s="8" t="inlineStr">
         <is>
-          <t>maa://31386 (100.00), *maa://58490 (78.57)</t>
+          <t>maa://31386 (100.00), maa://58490 (83.33)</t>
         </is>
       </c>
       <c r="Y19" s="19" t="n"/>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (81.74), *maa://36668 (67.29)</t>
+          <t>maa://30709 (83.84), *maa://36668 (68.75)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3044,7 +3044,7 @@
       </c>
       <c r="AF19" s="8" t="inlineStr">
         <is>
-          <t>*maa://21663 (64.71), maa://52239 (82.61)</t>
+          <t>*maa://21663 (64.71), maa://52239 (84.62)</t>
         </is>
       </c>
       <c r="AG19" s="16" t="n"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://25198 (97.42), maa://36680 (98.48), maa://21432 (91.34)</t>
+          <t>maa://25198 (97.66), maa://36680 (98.83), maa://21432 (91.34)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3078,7 +3078,7 @@
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>maa://22864 (94.24)</t>
+          <t>maa://22864 (95.29)</t>
         </is>
       </c>
       <c r="I20" s="19" t="n"/>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (93.71)</t>
+          <t>maa://41331 (94.61)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="P20" s="8" t="inlineStr">
         <is>
-          <t>maa://37442 (97.92)</t>
+          <t>maa://37442 (98.26)</t>
         </is>
       </c>
       <c r="Q20" s="19" t="n"/>
@@ -3126,7 +3126,7 @@
       </c>
       <c r="T20" s="8" t="inlineStr">
         <is>
-          <t>maa://29113 (92.19)</t>
+          <t>maa://29113 (92.75)</t>
         </is>
       </c>
       <c r="U20" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (94.89), maa://56241 (98.17), maa://49976 (88.24)</t>
+          <t>maa://50085 (95.77), maa://56241 (98.24), maa://49976 (88.35)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>maa://21261 (98.82)</t>
+          <t>maa://21261 (98.92)</t>
         </is>
       </c>
       <c r="E21" s="19" t="n"/>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="H21" s="8" t="inlineStr">
         <is>
-          <t>maa://24372 (98.42)</t>
+          <t>maa://24372 (98.67)</t>
         </is>
       </c>
       <c r="I21" s="19" t="n"/>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="L21" s="8" t="inlineStr">
         <is>
-          <t>maa://31731 (97.83)</t>
+          <t>maa://31731 (96.08)</t>
         </is>
       </c>
       <c r="M21" s="19" t="n"/>
@@ -3240,7 +3240,7 @@
       </c>
       <c r="P21" s="8" t="inlineStr">
         <is>
-          <t>maa://24381 (86.21)</t>
+          <t>maa://24381 (86.67)</t>
         </is>
       </c>
       <c r="Q21" s="19" t="n"/>
@@ -3256,7 +3256,7 @@
       </c>
       <c r="T21" s="8" t="inlineStr">
         <is>
-          <t>maa://21993 (87.50)</t>
+          <t>maa://21993 (88.89)</t>
         </is>
       </c>
       <c r="U21" s="19" t="n"/>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (97.53), maa://20110 (86.67)</t>
+          <t>maa://34946 (98.01), maa://20110 (87.01)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="AB21" s="8" t="inlineStr">
         <is>
-          <t>maa://21443 (85.22), *maa://52223 (76.06)</t>
+          <t>maa://21443 (85.74), *maa://52223 (79.67)</t>
         </is>
       </c>
       <c r="AC21" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22432 (91.82), maa://22524 (82.37), maa://64221 (97.11)</t>
+          <t>maa://22432 (93.11), maa://22524 (82.69), maa://64221 (97.51)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>maa://25236 (98.71)</t>
+          <t>maa://25236 (99.00)</t>
         </is>
       </c>
       <c r="I22" s="19" t="n"/>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>*maa://27127 (80.00), *maa://22751 (70.93), maa://66865 (98.91)</t>
+          <t>maa://27127 (81.34), *maa://22751 (70.93), maa://66865 (99.27)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3386,7 +3386,7 @@
       </c>
       <c r="T22" s="8" t="inlineStr">
         <is>
-          <t>maa://38495 (85.71)</t>
+          <t>maa://38495 (82.05)</t>
         </is>
       </c>
       <c r="U22" s="19" t="n"/>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://37649 (91.95), maa://21282 (98.87)</t>
+          <t>maa://37649 (93.23), maa://21282 (98.88)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="AB22" s="8" t="inlineStr">
         <is>
-          <t>maa://23656 (99.34)</t>
+          <t>maa://23656 (99.43)</t>
         </is>
       </c>
       <c r="AC22" s="19" t="n"/>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="AF22" s="8" t="inlineStr">
         <is>
-          <t>maa://29658 (96.39)</t>
+          <t>maa://29658 (96.67)</t>
         </is>
       </c>
       <c r="AG22" s="16" t="n"/>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>***maa://28036 (29.21), *maa://41753 (59.26)</t>
+          <t>***maa://28036 (29.21), *maa://41753 (61.02)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (98.16), maa://39875 (95.28)</t>
+          <t>maa://39756 (98.47), maa://39875 (95.50)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (96.00), maa://29748 (81.36), *maa://37566 (78.95)</t>
+          <t>maa://30587 (96.72), maa://29748 (81.62), maa://37566 (80.33)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="T23" s="8" t="inlineStr">
         <is>
-          <t>maa://31212 (93.83), maa://24387 (84.09), maa://67084 (83.33)</t>
+          <t>maa://31212 (94.85), maa://24387 (84.09), maa://67084 (85.71)</t>
         </is>
       </c>
       <c r="U23" s="19" t="n"/>
@@ -3532,7 +3532,7 @@
       </c>
       <c r="X23" s="8" t="inlineStr">
         <is>
-          <t>*maa://28503 (59.15)</t>
+          <t>*maa://28503 (60.00)</t>
         </is>
       </c>
       <c r="Y23" s="19" t="n"/>
@@ -3548,7 +3548,7 @@
       </c>
       <c r="AB23" s="8" t="inlineStr">
         <is>
-          <t>maa://29652 (95.83)</t>
+          <t>maa://29652 (96.10)</t>
         </is>
       </c>
       <c r="AC23" s="19" t="n"/>
@@ -3564,7 +3564,7 @@
       </c>
       <c r="AF23" s="8" t="inlineStr">
         <is>
-          <t>maa://31489 (97.30)</t>
+          <t>maa://31489 (97.92)</t>
         </is>
       </c>
       <c r="AG23" s="16" t="n"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (83.36), maa://46650 (87.35)</t>
+          <t>maa://24368 (84.42), maa://46650 (89.52)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (94.74), maa://23504 (93.98), *maa://25141 (78.47), *maa://36663 (79.25), maa://52227 (97.94)</t>
+          <t>maa://29988 (95.63), maa://23504 (94.02), *maa://25141 (79.33), maa://52227 (97.89), *maa://36663 (79.25)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="AB24" s="8" t="inlineStr">
         <is>
-          <t>maa://39349 (96.55)</t>
+          <t>maa://39349 (96.88)</t>
         </is>
       </c>
       <c r="AC24" s="19" t="n"/>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://64165 (98.80), maa://22523 (80.09), maa://29910 (94.20), maa://45831 (93.33)</t>
+          <t>maa://64165 (99.12), maa://22523 (80.09), maa://29910 (94.20), maa://45831 (93.55)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (96.14), maa://63016 (98.66)</t>
+          <t>maa://29753 (96.30), maa://63016 (98.97)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>*maa://29063 (73.45), *maa://25311 (71.01), maa://45047 (84.75)</t>
+          <t>*maa://29063 (74.92), *maa://25311 (70.71), maa://45047 (86.96)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3744,7 +3744,7 @@
       </c>
       <c r="L25" s="8" t="inlineStr">
         <is>
-          <t>maa://24378 (92.86)</t>
+          <t>maa://24378 (93.51)</t>
         </is>
       </c>
       <c r="M25" s="19" t="n"/>
@@ -3760,7 +3760,7 @@
       </c>
       <c r="P25" s="8" t="inlineStr">
         <is>
-          <t>maa://24382 (95.35)</t>
+          <t>maa://24382 (95.65)</t>
         </is>
       </c>
       <c r="Q25" s="19" t="n"/>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="T25" s="8" t="inlineStr">
         <is>
-          <t>maa://20109 (95.53), maa://22545 (100.00)</t>
+          <t>maa://20109 (96.11), maa://22545 (100.00)</t>
         </is>
       </c>
       <c r="U25" s="19" t="n"/>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="X25" s="8" t="inlineStr">
         <is>
-          <t>maa://29890 (89.11)</t>
+          <t>maa://29890 (90.52)</t>
         </is>
       </c>
       <c r="Y25" s="19" t="n"/>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (92.28), *maa://24516 (79.59), maa://26001 (83.33)</t>
+          <t>maa://31215 (92.88), *maa://24516 (79.80), maa://26001 (83.33)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (97.56), maa://36676 (99.76), maa://24621 (96.82), maa://22771 (87.50), maa://37772 (83.33)</t>
+          <t>maa://20108 (97.81), maa://36676 (99.81), maa://24621 (96.84), maa://22771 (88.24), maa://37772 (83.33)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3858,7 +3858,7 @@
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
-          <t>maa://56240 (94.57), maa://24913 (91.89)</t>
+          <t>maa://56240 (95.91), maa://24913 (92.17)</t>
         </is>
       </c>
       <c r="I26" s="19" t="n"/>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="P26" s="8" t="inlineStr">
         <is>
-          <t>maa://39870 (93.55), maa://56625 (100.00)</t>
+          <t>maa://39870 (93.94), maa://56625 (100.00)</t>
         </is>
       </c>
       <c r="Q26" s="19" t="n"/>
@@ -3922,7 +3922,7 @@
       </c>
       <c r="X26" s="8" t="inlineStr">
         <is>
-          <t>maa://24389 (97.87)</t>
+          <t>maa://24389 (98.08)</t>
         </is>
       </c>
       <c r="Y26" s="19" t="n"/>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="AB26" s="8" t="inlineStr">
         <is>
-          <t>maa://42235 (97.95)</t>
+          <t>maa://42235 (98.26)</t>
         </is>
       </c>
       <c r="AC26" s="19" t="n"/>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="AF26" s="8" t="inlineStr">
         <is>
-          <t>*maa://30511 (71.62), **maa://29760 (47.62)</t>
+          <t>*maa://30511 (71.43), **maa://29760 (47.62)</t>
         </is>
       </c>
       <c r="AG26" s="16" t="n"/>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>maa://39601 (88.89), maa://34494 (98.65)</t>
+          <t>maa://39601 (90.48), maa://34494 (97.50)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4004,7 +4004,7 @@
       </c>
       <c r="L27" s="8" t="inlineStr">
         <is>
-          <t>maa://28071 (86.96)</t>
+          <t>maa://28071 (87.76)</t>
         </is>
       </c>
       <c r="M27" s="19" t="n"/>
@@ -4020,7 +4020,7 @@
       </c>
       <c r="P27" s="8" t="inlineStr">
         <is>
-          <t>maa://56400 (88.89)</t>
+          <t>maa://56400 (92.86)</t>
         </is>
       </c>
       <c r="Q27" s="19" t="n"/>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="T27" s="8" t="inlineStr">
         <is>
-          <t>maa://30624 (87.76)</t>
+          <t>maa://30624 (88.96)</t>
         </is>
       </c>
       <c r="U27" s="19" t="n"/>
@@ -4084,7 +4084,7 @@
       </c>
       <c r="AF27" s="8" t="inlineStr">
         <is>
-          <t>maa://24023 (97.25)</t>
+          <t>maa://24023 (97.54)</t>
         </is>
       </c>
       <c r="AG27" s="16" t="n"/>
@@ -4102,7 +4102,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (94.88), maa://25725 (84.43)</t>
+          <t>maa://24465 (95.47), maa://25725 (84.55)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="L28" s="8" t="inlineStr">
         <is>
-          <t>maa://30770 (88.16)</t>
+          <t>maa://30770 (89.29)</t>
         </is>
       </c>
       <c r="M28" s="19" t="n"/>
@@ -4166,7 +4166,7 @@
       </c>
       <c r="T28" s="8" t="inlineStr">
         <is>
-          <t>maa://29765 (90.62), maa://23263 (96.00)</t>
+          <t>maa://29765 (92.31), maa://23263 (96.09)</t>
         </is>
       </c>
       <c r="U28" s="19" t="n"/>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (96.41), maa://41749 (96.96)</t>
+          <t>maa://39929 (96.95), maa://41749 (97.18)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (93.26), maa://65700 (97.94)</t>
+          <t>maa://36660 (93.75), maa://65700 (98.51)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4232,7 +4232,7 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>maa://31694 (99.15)</t>
+          <t>maa://31694 (99.23)</t>
         </is>
       </c>
       <c r="E29" s="19" t="n"/>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (97.07), maa://31400 (98.22), maa://28440 (86.08)</t>
+          <t>maa://28432 (97.57), maa://31400 (98.40), maa://28440 (86.25)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4280,7 +4280,7 @@
       </c>
       <c r="P29" s="8" t="inlineStr">
         <is>
-          <t>maa://54169 (97.44)</t>
+          <t>maa://54169 (96.84)</t>
         </is>
       </c>
       <c r="Q29" s="19" t="n"/>
@@ -4339,12 +4339,12 @@
       </c>
       <c r="AE29" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://42865 (90.00), *maa://24080 (68.86)</t>
+          <t>maa://42865 (91.37)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (94.12), maa://64191 (100.00)</t>
+          <t>maa://45792 (94.55), maa://64191 (100.00)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="L30" s="8" t="inlineStr">
         <is>
-          <t>maa://30442 (97.03)</t>
+          <t>maa://30442 (97.17)</t>
         </is>
       </c>
       <c r="M30" s="19" t="n"/>
@@ -4405,12 +4405,12 @@
       </c>
       <c r="O30" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="P30" s="8" t="inlineStr">
         <is>
-          <t>maa://21442 (99.47), maa://66611 (100.00)</t>
+          <t>maa://21442 (99.55), maa://66611 (100.00), maa://68394 (100.00)</t>
         </is>
       </c>
       <c r="Q30" s="19" t="n"/>
@@ -4426,7 +4426,7 @@
       </c>
       <c r="T30" s="8" t="inlineStr">
         <is>
-          <t>*maa://32940 (77.78), maa://24388 (95.65)</t>
+          <t>*maa://32940 (80.00), maa://24388 (96.00)</t>
         </is>
       </c>
       <c r="U30" s="19" t="n"/>
@@ -4442,7 +4442,7 @@
       </c>
       <c r="X30" s="8" t="inlineStr">
         <is>
-          <t>maa://39477 (95.00)</t>
+          <t>maa://39477 (95.74)</t>
         </is>
       </c>
       <c r="Y30" s="19" t="n"/>
@@ -4458,7 +4458,7 @@
       </c>
       <c r="AB30" s="8" t="inlineStr">
         <is>
-          <t>maa://42979 (99.38), maa://45822 (100.00), maa://45045 (87.50)</t>
+          <t>maa://42979 (99.49), maa://45822 (100.00), maa://45045 (90.91)</t>
         </is>
       </c>
       <c r="AC30" s="19" t="n"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (97.33), maa://36258 (92.20), maa://43904 (86.67)</t>
+          <t>maa://35926 (97.76), maa://36258 (92.62), maa://43904 (88.89)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4556,7 +4556,7 @@
       </c>
       <c r="T31" s="8" t="inlineStr">
         <is>
-          <t>maa://30711 (96.74), maa://30768 (100.00)</t>
+          <t>maa://30711 (97.14), maa://30768 (100.00)</t>
         </is>
       </c>
       <c r="U31" s="19" t="n"/>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://36667 (99.57), maa://21895 (97.91), maa://22760 (100.00)</t>
+          <t>maa://36667 (99.57), maa://21895 (97.92), maa://22760 (100.00)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4654,7 +4654,7 @@
       </c>
       <c r="L32" s="8" t="inlineStr">
         <is>
-          <t>maa://28065 (96.34)</t>
+          <t>maa://28065 (96.84)</t>
         </is>
       </c>
       <c r="M32" s="19" t="n"/>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (99.07), maa://41108 (87.50), maa://41238 (98.07), maa://45523 (100.00)</t>
+          <t>maa://42859 (99.26), maa://41108 (87.50), maa://41238 (98.08), maa://45523 (100.00)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="X32" s="8" t="inlineStr">
         <is>
-          <t>maa://64104 (96.25)</t>
+          <t>maa://64104 (96.84)</t>
         </is>
       </c>
       <c r="Y32" s="19" t="n"/>
@@ -4734,7 +4734,7 @@
       </c>
       <c r="AF32" s="8" t="inlineStr">
         <is>
-          <t>maa://42408 (93.33)</t>
+          <t>maa://42408 (94.12)</t>
         </is>
       </c>
       <c r="AG32" s="16" t="n"/>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (91.95), *maa://22730 (70.59)</t>
+          <t>maa://21956 (93.40), *maa://22730 (70.59)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="T33" s="8" t="inlineStr">
         <is>
-          <t>maa://45558 (91.30)</t>
+          <t>maa://45558 (92.00)</t>
         </is>
       </c>
       <c r="U33" s="19" t="n"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (98.91), maa://56235 (100.00)</t>
+          <t>maa://48817 (99.05), maa://56235 (99.69)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="T34" s="8" t="inlineStr">
         <is>
-          <t>maa://24526 (96.13)</t>
+          <t>maa://24526 (96.70)</t>
         </is>
       </c>
       <c r="U34" s="19" t="n"/>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="AB34" s="8" t="inlineStr">
         <is>
-          <t>maa://64329 (96.43)</t>
+          <t>maa://64329 (96.77)</t>
         </is>
       </c>
       <c r="AC34" s="19" t="n"/>
@@ -4994,7 +4994,7 @@
       </c>
       <c r="AF34" s="8" t="inlineStr">
         <is>
-          <t>maa://32650 (85.37)</t>
+          <t>maa://32650 (87.23)</t>
         </is>
       </c>
       <c r="AG34" s="16" t="n"/>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
-          <t>maa://41296 (99.02)</t>
+          <t>maa://41296 (99.16)</t>
         </is>
       </c>
       <c r="M35" s="19" t="n"/>
@@ -5076,7 +5076,7 @@
       </c>
       <c r="T35" s="8" t="inlineStr">
         <is>
-          <t>maa://24842 (96.25)</t>
+          <t>maa://24842 (96.43)</t>
         </is>
       </c>
       <c r="U35" s="19" t="n"/>
@@ -5124,7 +5124,7 @@
       </c>
       <c r="AF35" s="8" t="inlineStr">
         <is>
-          <t>maa://39479 (95.35)</t>
+          <t>maa://39479 (95.83)</t>
         </is>
       </c>
       <c r="AG35" s="16" t="n"/>
@@ -5158,7 +5158,7 @@
       </c>
       <c r="H36" s="8" t="inlineStr">
         <is>
-          <t>maa://24375 (93.10)</t>
+          <t>maa://24375 (93.75)</t>
         </is>
       </c>
       <c r="I36" s="19" t="n"/>
@@ -5206,7 +5206,7 @@
       </c>
       <c r="T36" s="8" t="inlineStr">
         <is>
-          <t>maa://27613 (99.44)</t>
+          <t>maa://27613 (99.50)</t>
         </is>
       </c>
       <c r="U36" s="19" t="n"/>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="AB36" s="19" t="inlineStr">
         <is>
-          <t>maa://64106 (95.24)</t>
+          <t>maa://64106 (96.15)</t>
         </is>
       </c>
       <c r="AC36" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (99.23), maa://56336 (98.99), maa://47069 (85.71), maa://45789 (100.00)</t>
+          <t>maa://45718 (99.31), maa://56336 (99.22), maa://47069 (86.49), maa://45789 (100.00)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="P37" s="8" t="inlineStr">
         <is>
-          <t>maa://21280 (96.63)</t>
+          <t>maa://21280 (97.21)</t>
         </is>
       </c>
       <c r="Q37" s="19" t="n"/>
@@ -5336,7 +5336,7 @@
       </c>
       <c r="T37" s="8" t="inlineStr">
         <is>
-          <t>**maa://39354 (44.44)</t>
+          <t>**maa://39354 (47.37)</t>
         </is>
       </c>
       <c r="U37" s="19" t="n"/>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="P38" s="8" t="inlineStr">
         <is>
-          <t>*maa://24383 (78.06)</t>
+          <t>*maa://24383 (79.64)</t>
         </is>
       </c>
       <c r="Q38" s="19" t="n"/>
@@ -5450,7 +5450,7 @@
       </c>
       <c r="T38" s="8" t="inlineStr">
         <is>
-          <t>maa://30713 (97.96)</t>
+          <t>maa://30713 (98.18)</t>
         </is>
       </c>
       <c r="U38" s="19" t="n"/>
@@ -5482,7 +5482,7 @@
       </c>
       <c r="AF38" s="8" t="inlineStr">
         <is>
-          <t>maa://36697 (94.88)</t>
+          <t>maa://36697 (95.60)</t>
         </is>
       </c>
       <c r="AG38" s="16" t="n"/>
@@ -5503,7 +5503,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://25199 (84.92), maa://30434 (94.94), maa://45059 (83.12), maa://44165 (83.33)</t>
+          <t>maa://25199 (84.44), maa://30434 (95.11), maa://45059 (89.31), maa://44165 (85.71)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://47093 (97.33), maa://24709 (93.30)</t>
+          <t>maa://47093 (97.85), maa://24709 (93.56)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (94.14), maa://45790 (86.67)</t>
+          <t>maa://47079 (94.76), maa://45790 (87.69)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5583,7 +5583,7 @@
       </c>
       <c r="AF39" s="8" t="inlineStr">
         <is>
-          <t>maa://62953 (96.55)</t>
+          <t>maa://62953 (96.91)</t>
         </is>
       </c>
       <c r="AG39" s="16" t="n"/>
@@ -5636,7 +5636,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (97.61), maa://21386 (95.90), maa://36664 (89.33), *maa://45550 (80.00)</t>
+          <t>maa://23278 (97.86), maa://21386 (95.92), maa://36664 (89.47), *maa://45550 (72.73)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://65283 (96.58), maa://64205 (96.55)</t>
+          <t>maa://65283 (95.97), maa://64205 (93.75)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5705,7 +5705,7 @@
       </c>
       <c r="H41" s="8" t="inlineStr">
         <is>
-          <t>maa://24466 (92.19)</t>
+          <t>maa://24466 (92.54)</t>
         </is>
       </c>
       <c r="I41" s="19" t="n"/>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="P41" s="8" t="inlineStr">
         <is>
-          <t>maa://43177 (94.05)</t>
+          <t>maa://43177 (94.74)</t>
         </is>
       </c>
       <c r="Q41" s="19" t="n"/>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>*maa://22525 (71.62), maa://21284 (96.50)</t>
+          <t>*maa://22525 (71.05), maa://21284 (97.12)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -5939,7 +5939,7 @@
       </c>
       <c r="P43" s="8" t="inlineStr">
         <is>
-          <t>maa://47403 (83.33)</t>
+          <t>maa://47403 (86.21)</t>
         </is>
       </c>
       <c r="Q43" s="19" t="n"/>
@@ -6008,7 +6008,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (98.04), maa://56386 (99.49), maa://27728 (96.33)</t>
+          <t>maa://29768 (98.14), maa://56386 (99.27), maa://27728 (96.36)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6056,7 +6056,7 @@
       </c>
       <c r="T44" s="8" t="inlineStr">
         <is>
-          <t>maa://39366 (92.96)</t>
+          <t>maa://39366 (92.50)</t>
         </is>
       </c>
       <c r="U44" s="19" t="n"/>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://42459 (98.09), maa://21229 (84.93), maa://30807 (94.51)</t>
+          <t>maa://42459 (98.48), maa://21229 (85.33), maa://30807 (94.57)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6109,7 +6109,7 @@
       </c>
       <c r="P45" s="8" t="inlineStr">
         <is>
-          <t>*maa://36237 (80.00)</t>
+          <t>maa://36237 (81.25)</t>
         </is>
       </c>
       <c r="Q45" s="19" t="n"/>
@@ -6125,7 +6125,7 @@
       </c>
       <c r="T45" s="8" t="inlineStr">
         <is>
-          <t>*maa://39364 (61.24)</t>
+          <t>*maa://39364 (64.34)</t>
         </is>
       </c>
       <c r="U45" s="19" t="n"/>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (94.29), maa://43901 (96.23)</t>
+          <t>maa://35931 (95.06), maa://43901 (96.23)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6231,7 +6231,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (97.31), maa://29661 (97.56), maa://56236 (99.65), maa://28038 (84.62)</t>
+          <t>maa://27410 (97.39), maa://29661 (97.61), maa://56236 (99.74), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6258,12 +6258,12 @@
       </c>
       <c r="S47" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="T47" s="8" t="inlineStr">
         <is>
-          <t>maa://67476 (99.40)</t>
+          <t>maa://67476 (99.46), maa://68392 (100.00)</t>
         </is>
       </c>
       <c r="U47" s="19" t="n"/>
@@ -6385,7 +6385,7 @@
       </c>
       <c r="P49" s="8" t="inlineStr">
         <is>
-          <t>*maa://39643 (75.00)</t>
+          <t>*maa://39643 (77.69)</t>
         </is>
       </c>
       <c r="Q49" s="19" t="n"/>
@@ -6401,7 +6401,7 @@
       </c>
       <c r="T49" s="19" t="inlineStr">
         <is>
-          <t>maa://67231 (99.21)</t>
+          <t>maa://67231 (98.88)</t>
         </is>
       </c>
       <c r="U49" s="19" t="n"/>
@@ -6438,7 +6438,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>maa://62852 (91.37)</t>
+          <t>maa://62852 (92.30)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6472,7 +6472,7 @@
       </c>
       <c r="H51" s="8" t="inlineStr">
         <is>
-          <t>maa://30769 (87.50)</t>
+          <t>maa://30769 (88.00)</t>
         </is>
       </c>
       <c r="I51" s="19" t="n"/>
@@ -6522,7 +6522,7 @@
       </c>
       <c r="H52" s="8" t="inlineStr">
         <is>
-          <t>maa://24376 (98.80)</t>
+          <t>maa://24376 (98.88)</t>
         </is>
       </c>
       <c r="I52" s="19" t="n"/>
@@ -6538,7 +6538,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (98.99), maa://59378 (93.75), maa://65511 (100.00)</t>
+          <t>maa://59394 (99.23), maa://59378 (93.83), maa://65511 (100.00)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6572,7 +6572,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (97.19)</t>
+          <t>maa://32534 (97.61)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -6656,7 +6656,7 @@
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>maa://32532 (97.04)</t>
+          <t>maa://32532 (97.54)</t>
         </is>
       </c>
       <c r="I55" s="19" t="n"/>
@@ -6708,7 +6708,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://25176 (98.75), maa://56237 (98.91)</t>
+          <t>maa://56237 (99.16), maa://25176 (98.77)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6726,7 +6726,7 @@
       </c>
       <c r="H58" s="8" t="inlineStr">
         <is>
-          <t>*maa://37964 (64.00)</t>
+          <t>*maa://37964 (65.42)</t>
         </is>
       </c>
       <c r="I58" s="19" t="n"/>
@@ -6744,7 +6744,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (97.92), maa://27746 (88.24)</t>
+          <t>maa://31270 (98.29), maa://27746 (88.89)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -6762,7 +6762,7 @@
       </c>
       <c r="H60" s="8" t="inlineStr">
         <is>
-          <t>maa://40438 (89.06)</t>
+          <t>maa://40438 (90.23)</t>
         </is>
       </c>
       <c r="I60" s="19" t="n"/>
@@ -6798,7 +6798,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (97.30), maa://43903 (100.00), maa://56228 (99.01)</t>
+          <t>maa://42981 (97.53), maa://56228 (99.25), maa://43903 (100.00)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6816,7 +6816,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (99.12), *maa://59693 (73.81), maa://59413 (95.74)</t>
+          <t>maa://59534 (99.29), *maa://59693 (75.00), maa://59413 (96.43)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -6834,7 +6834,7 @@
       </c>
       <c r="H64" s="8" t="inlineStr">
         <is>
-          <t>maa://44405 (89.83)</t>
+          <t>maa://44405 (90.91)</t>
         </is>
       </c>
       <c r="I64" s="19" t="n"/>
@@ -7032,7 +7032,7 @@
       </c>
       <c r="H75" s="19" t="inlineStr">
         <is>
-          <t>maa://67748 (100.00)</t>
+          <t>*maa://67748 (78.57)</t>
         </is>
       </c>
       <c r="I75" s="19" t="n"/>
@@ -7174,7 +7174,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.10 13:19:23</t>
+          <t>更新日期：2025.09.15 13:24:29</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -7336,7 +7336,7 @@
       </c>
       <c r="D4" s="13" t="inlineStr">
         <is>
-          <t>*maa://20996 (60.00)</t>
+          <t>*maa://20996 (66.67)</t>
         </is>
       </c>
       <c r="E4" s="14" t="inlineStr">
@@ -7984,7 +7984,7 @@
       </c>
       <c r="D16" s="13" t="inlineStr">
         <is>
-          <t>maa://20919 (98.00), *maa://31611 (75.00)</t>
+          <t>maa://20919 (98.00), *maa://31611 (76.92)</t>
         </is>
       </c>
       <c r="E16" s="14" t="inlineStr">
@@ -8362,7 +8362,7 @@
       </c>
       <c r="D23" s="13" t="inlineStr">
         <is>
-          <t>maa://20876 (96.15), maa://63498 (100.00)</t>
+          <t>maa://20876 (96.30), maa://63498 (100.00)</t>
         </is>
       </c>
       <c r="E23" s="14" t="inlineStr">
@@ -8578,7 +8578,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (73.21), *maa://28758 (71.11), maa://29036 (96.55), *maa://42172 (71.43), maa://65357 (95.00), maa://30285 (100.00)</t>
+          <t>*maa://20849 (73.21), *maa://28758 (71.11), maa://29036 (96.67), *maa://42172 (71.43), maa://65357 (95.65), maa://30285 (100.00)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8686,7 +8686,7 @@
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>maa://20863 (90.34), maa://20832 (99.20), maa://20727 (100.00)</t>
+          <t>maa://20863 (90.54), maa://20832 (99.21), maa://20727 (100.00)</t>
         </is>
       </c>
       <c r="E29" s="14" t="inlineStr">
@@ -8848,7 +8848,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (89.88), maa://36866 (96.92), maa://62759 (100.00), maa://45572 (88.24), maa://27794 (100.00), maa://20960 (100.00), maa://20843 (100.00), **maa://24483 (50.00), maa://20862 (83.33), *maa://20893 (77.78)</t>
+          <t>maa://36644 (90.12), maa://36866 (96.97), maa://62759 (100.00), maa://45572 (88.24), maa://27794 (100.00), maa://20960 (100.00), maa://20843 (100.00), **maa://24483 (50.00), maa://20862 (83.33), *maa://20893 (77.78)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -8956,7 +8956,7 @@
       </c>
       <c r="D34" s="13" t="inlineStr">
         <is>
-          <t>maa://20916 (82.86), maa://52658 (92.86)</t>
+          <t>maa://20916 (82.86), maa://52658 (93.33)</t>
         </is>
       </c>
       <c r="E34" s="14" t="inlineStr">
@@ -9118,7 +9118,7 @@
       </c>
       <c r="D37" s="13" t="inlineStr">
         <is>
-          <t>maa://27376 (93.33), maa://42635 (94.12), *maa://20838 (55.00)</t>
+          <t>maa://27376 (93.33), maa://42635 (94.23), *maa://20838 (55.00)</t>
         </is>
       </c>
       <c r="E37" s="14" t="inlineStr">
@@ -9388,7 +9388,7 @@
       </c>
       <c r="D42" s="13" t="inlineStr">
         <is>
-          <t>maa://34883 (93.75), maa://20918 (96.00), maa://20824 (100.00)</t>
+          <t>maa://34883 (93.75), maa://20918 (96.15), maa://20824 (100.00)</t>
         </is>
       </c>
       <c r="E42" s="14" t="inlineStr">
@@ -9982,7 +9982,7 @@
       </c>
       <c r="D53" s="13" t="inlineStr">
         <is>
-          <t>maa://20953 (97.14), maa://31173 (94.29)</t>
+          <t>maa://20953 (97.14), maa://31173 (94.59)</t>
         </is>
       </c>
       <c r="E53" s="14" t="inlineStr">
@@ -10090,7 +10090,7 @@
       </c>
       <c r="D55" s="13" t="inlineStr">
         <is>
-          <t>maa://20932 (96.13), maa://42415 (96.15), maa://40838 (100.00)</t>
+          <t>maa://20932 (96.15), maa://42415 (96.15), maa://40838 (100.00)</t>
         </is>
       </c>
       <c r="E55" s="14" t="inlineStr">
@@ -10144,7 +10144,7 @@
       </c>
       <c r="D56" s="13" t="inlineStr">
         <is>
-          <t>maa://44235 (98.38), maa://45604 (100.00), maa://20961 (100.00), maa://44220 (100.00), maa://20910 (100.00)</t>
+          <t>maa://44235 (98.40), maa://45604 (100.00), maa://20961 (100.00), maa://44220 (100.00), maa://20910 (100.00)</t>
         </is>
       </c>
       <c r="E56" s="14" t="inlineStr">
@@ -10198,7 +10198,7 @@
       </c>
       <c r="D57" s="13" t="inlineStr">
         <is>
-          <t>*maa://20965 (71.79)</t>
+          <t>*maa://20965 (72.50)</t>
         </is>
       </c>
       <c r="E57" s="14" t="inlineStr">
@@ -10252,7 +10252,7 @@
       </c>
       <c r="D58" s="13" t="inlineStr">
         <is>
-          <t>maa://28900 (96.97), maa://30126 (100.00)</t>
+          <t>maa://28900 (97.00), maa://30126 (100.00)</t>
         </is>
       </c>
       <c r="E58" s="14" t="inlineStr">
@@ -10306,7 +10306,7 @@
       </c>
       <c r="D59" s="13" t="inlineStr">
         <is>
-          <t>maa://27970 (98.84), maa://41118 (87.50)</t>
+          <t>maa://27970 (98.85), maa://41118 (87.50)</t>
         </is>
       </c>
       <c r="E59" s="14" t="inlineStr">
@@ -10414,7 +10414,7 @@
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (99.18), maa://31559 (93.48), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00)</t>
+          <t>maa://20841 (99.19), maa://31559 (93.62), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -10792,7 +10792,7 @@
       </c>
       <c r="D68" s="13" t="inlineStr">
         <is>
-          <t>maa://20976 (97.71), maa://20815 (100.00)</t>
+          <t>maa://20976 (97.75), maa://20815 (100.00)</t>
         </is>
       </c>
       <c r="E68" s="14" t="inlineStr">
@@ -10846,7 +10846,7 @@
       </c>
       <c r="D69" s="13" t="inlineStr">
         <is>
-          <t>maa://20974 (96.88), maa://29079 (80.95), maa://29096 (95.65), maa://29087 (100.00), *maa://20823 (75.00), maa://20855 (94.12), maa://20904 (100.00), *maa://63722 (75.00)</t>
+          <t>maa://20974 (96.94), maa://29079 (80.95), maa://29096 (95.65), maa://29087 (100.00), *maa://20823 (75.00), maa://20855 (94.12), maa://20904 (100.00), *maa://63722 (80.00)</t>
         </is>
       </c>
       <c r="E69" s="14" t="inlineStr">
@@ -12628,7 +12628,7 @@
       </c>
       <c r="D102" s="13" t="inlineStr">
         <is>
-          <t>maa://40517 (90.00), *maa://39240 (56.25)</t>
+          <t>maa://40517 (90.32), *maa://39240 (56.25)</t>
         </is>
       </c>
       <c r="E102" s="14" t="inlineStr">
@@ -12682,7 +12682,7 @@
       </c>
       <c r="D103" s="13" t="inlineStr">
         <is>
-          <t>*maa://29094 (76.27), maa://28904 (88.37), **maa://20931 (48.57)</t>
+          <t>*maa://29094 (76.27), maa://28904 (88.37), **maa://20931 (47.22)</t>
         </is>
       </c>
       <c r="E103" s="14" t="inlineStr">
@@ -12952,7 +12952,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.83), maa://25018 (96.90), maa://25776 (92.21), maa://28361 (95.35), maa://25772 (94.12), maa://56588 (96.55), maa://45194 (85.71), maa://32653 (81.25), maa://25161 (83.33), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
+          <t>maa://51881 (98.69), maa://25018 (96.91), maa://25776 (92.21), maa://28361 (95.35), maa://25772 (94.12), maa://56588 (96.55), maa://45194 (85.71), maa://32653 (81.25), maa://25161 (83.33), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13006,7 +13006,7 @@
       </c>
       <c r="D109" s="13" t="inlineStr">
         <is>
-          <t>maa://36646 (98.88), maa://25774 (95.89), maa://35996 (97.89), maa://22469 (92.98), maa://30668 (86.67), maa://67286 (100.00)</t>
+          <t>maa://36646 (98.89), maa://25774 (94.59), maa://35996 (97.89), maa://22469 (91.80), maa://30668 (86.67), maa://67286 (100.00)</t>
         </is>
       </c>
       <c r="E109" s="14" t="inlineStr">
@@ -13384,7 +13384,7 @@
       </c>
       <c r="D116" s="13" t="inlineStr">
         <is>
-          <t>maa://20908 (98.17), maa://35723 (96.08), *maa://23346 (77.78), maa://38822 (100.00), maa://58659 (100.00)</t>
+          <t>maa://20908 (98.18), maa://35723 (96.08), *maa://23346 (77.78), maa://38822 (100.00), maa://58659 (100.00)</t>
         </is>
       </c>
       <c r="E116" s="14" t="inlineStr">
@@ -13546,7 +13546,7 @@
       </c>
       <c r="D119" s="13" t="inlineStr">
         <is>
-          <t>maa://20986 (94.12)</t>
+          <t>maa://20986 (94.44)</t>
         </is>
       </c>
       <c r="E119" s="14" t="inlineStr">
@@ -13708,7 +13708,7 @@
       </c>
       <c r="D122" s="13" t="inlineStr">
         <is>
-          <t>maa://20869 (100.00), maa://44690 (95.74)</t>
+          <t>maa://20869 (100.00), maa://44690 (95.83)</t>
         </is>
       </c>
       <c r="E122" s="14" t="inlineStr">
@@ -14842,7 +14842,7 @@
       </c>
       <c r="D143" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (97.75), *maa://23736 (52.44), maa://31185 (91.67), maa://30306 (100.00)</t>
+          <t>maa://28484 (97.77), *maa://23736 (52.44), maa://31185 (91.67), maa://30306 (100.00)</t>
         </is>
       </c>
       <c r="E143" s="14" t="inlineStr">
@@ -14896,7 +14896,7 @@
       </c>
       <c r="D144" s="13" t="inlineStr">
         <is>
-          <t>maa://30670 (96.89), maa://31470 (94.12), *maa://45066 (71.43), maa://61380 (100.00), **maa://30867 (40.00)</t>
+          <t>maa://30670 (96.30), maa://31470 (94.12), maa://61380 (100.00), *maa://45066 (71.43), **maa://30867 (40.00)</t>
         </is>
       </c>
       <c r="E144" s="14" t="inlineStr">
@@ -15220,7 +15220,7 @@
       </c>
       <c r="D150" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.78), maa://36641 (98.48), maa://36865 (95.40), maa://44635 (88.07), maa://44660 (92.68), maa://41128 (84.21), maa://42918 (100.00), maa://46108 (100.00), maa://44119 (97.44), maa://37300 (100.00), maa://64408 (100.00), maa://42917 (100.00)</t>
+          <t>maa://40957 (94.80), maa://36641 (98.24), maa://36865 (95.43), maa://44635 (88.07), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (100.00), maa://42918 (100.00), maa://44119 (97.44), maa://37300 (100.00), maa://64408 (92.31), maa://42917 (100.00)</t>
         </is>
       </c>
       <c r="E150" s="14" t="inlineStr">
@@ -15269,12 +15269,12 @@
       </c>
       <c r="C151" s="12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D151" s="13" t="inlineStr">
         <is>
-          <t>maa://51549 (96.77), maa://51923 (96.30)</t>
+          <t>maa://51549 (96.77), maa://51923 (96.30), maa://67508 (100.00)</t>
         </is>
       </c>
       <c r="E151" s="14" t="inlineStr">
@@ -16192,7 +16192,7 @@
       </c>
       <c r="D168" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (92.18), maa://29627 (92.95), maa://29659 (87.50), maa://49074 (95.59), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
+          <t>maa://29633 (92.18), maa://29627 (92.95), maa://29659 (87.50), maa://49074 (94.20), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
         </is>
       </c>
       <c r="E168" s="14" t="inlineStr">
@@ -16246,7 +16246,7 @@
       </c>
       <c r="D169" s="13" t="inlineStr">
         <is>
-          <t>maa://49867 (94.81), maa://49655 (97.73)</t>
+          <t>maa://49867 (93.59), maa://49655 (97.73)</t>
         </is>
       </c>
       <c r="E169" s="14" t="inlineStr">
@@ -17434,7 +17434,7 @@
       </c>
       <c r="D191" s="13" t="inlineStr">
         <is>
-          <t>maa://34866 (93.75), maa://34714 (96.67)</t>
+          <t>maa://34866 (93.75), maa://34714 (96.77)</t>
         </is>
       </c>
       <c r="E191" s="14" t="inlineStr">
@@ -17812,7 +17812,7 @@
       </c>
       <c r="D198" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.33), maa://35854 (84.75), maa://50388 (98.22), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (93.94)</t>
+          <t>maa://44224 (90.36), maa://35854 (84.75), maa://50388 (98.24), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (94.12)</t>
         </is>
       </c>
       <c r="E198" s="14" t="inlineStr">
@@ -17866,7 +17866,7 @@
       </c>
       <c r="D199" s="13" t="inlineStr">
         <is>
-          <t>maa://39156 (94.19), *maa://39550 (55.00), *maa://53417 (75.00), maa://63806 (87.50)</t>
+          <t>maa://39156 (94.19), *maa://39550 (55.00), *maa://53417 (75.00), *maa://63806 (77.78)</t>
         </is>
       </c>
       <c r="E199" s="14" t="inlineStr">
@@ -18028,7 +18028,7 @@
       </c>
       <c r="D202" s="13" t="inlineStr">
         <is>
-          <t>maa://42223 (99.62), maa://49077 (94.23), maa://42292 (97.22), maa://42402 (100.00)</t>
+          <t>maa://42223 (99.25), maa://49077 (94.44), maa://42292 (97.22), maa://42402 (100.00)</t>
         </is>
       </c>
       <c r="E202" s="14" t="inlineStr">
@@ -18730,7 +18730,7 @@
       </c>
       <c r="D215" s="13" t="inlineStr">
         <is>
-          <t>maa://64044 (94.74)</t>
+          <t>maa://64044 (95.24)</t>
         </is>
       </c>
       <c r="E215" s="14" t="inlineStr">
@@ -19054,7 +19054,7 @@
       </c>
       <c r="D221" s="13" t="inlineStr">
         <is>
-          <t>***maa://26496 (30.00), *maa://20995 (54.55)</t>
+          <t>**maa://26496 (36.36), *maa://20995 (54.55)</t>
         </is>
       </c>
       <c r="E221" s="14" t="inlineStr">
@@ -19378,7 +19378,7 @@
       </c>
       <c r="D227" s="13" t="inlineStr">
         <is>
-          <t>maa://28187 (97.73), maa://43531 (100.00), maa://39520 (100.00)</t>
+          <t>maa://28187 (97.73), maa://39520 (100.00), maa://43531 (100.00)</t>
         </is>
       </c>
       <c r="E227" s="14" t="inlineStr">
@@ -20188,7 +20188,7 @@
       </c>
       <c r="D242" s="13" t="inlineStr">
         <is>
-          <t>*maa://30667 (78.88), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (57.14), maa://39588 (88.14), maa://64079 (84.62), maa://65726 (100.00)</t>
+          <t>*maa://30667 (78.97), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (57.81), maa://39588 (88.14), maa://64079 (81.48), maa://65726 (85.71)</t>
         </is>
       </c>
       <c r="E242" s="14" t="inlineStr">
@@ -20242,7 +20242,7 @@
       </c>
       <c r="D243" s="13" t="inlineStr">
         <is>
-          <t>maa://62759 (100.00), *maa://62764 (75.00)</t>
+          <t>maa://62759 (100.00), *maa://62764 (80.00)</t>
         </is>
       </c>
       <c r="E243" s="14" t="inlineStr">
@@ -20885,12 +20885,12 @@
       </c>
       <c r="C255" s="12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D255" s="13" t="inlineStr">
         <is>
-          <t>maa://31559 (93.48), maa://24093 (100.00), maa://20924 (95.24), **maa://49440 (42.86)</t>
+          <t>maa://31559 (93.62), maa://24093 (100.00), maa://20924 (95.24), **maa://49440 (42.86), maa://63591 (100.00)</t>
         </is>
       </c>
       <c r="E255" s="14" t="inlineStr">
@@ -21484,7 +21484,7 @@
       </c>
       <c r="D266" s="13" t="inlineStr">
         <is>
-          <t>maa://39162 (97.22)</t>
+          <t>maa://39162 (97.30)</t>
         </is>
       </c>
       <c r="E266" s="14" t="inlineStr">
@@ -21911,12 +21911,12 @@
       </c>
       <c r="C274" s="12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D274" s="13" t="inlineStr">
         <is>
-          <t>**maa://62757 (41.18)</t>
+          <t>**maa://62757 (41.18), maa://67819 (100.00)</t>
         </is>
       </c>
       <c r="E274" s="14" t="inlineStr">
@@ -22024,7 +22024,7 @@
       </c>
       <c r="D276" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.83), maa://51630 (96.19), maa://56588 (96.55), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (41.67), *maa://66758 (75.00)</t>
+          <t>maa://51881 (98.69), maa://51630 (96.19), maa://56588 (96.55), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (41.67), *maa://66758 (77.78)</t>
         </is>
       </c>
       <c r="E276" s="14" t="inlineStr">
@@ -22780,7 +22780,7 @@
       </c>
       <c r="D290" s="13" t="inlineStr">
         <is>
-          <t>maa://20899 (90.00), maa://46332 (96.15), ***maa://44744 (25.00)</t>
+          <t>maa://20899 (90.00), maa://46332 (96.30), ***maa://44744 (25.00)</t>
         </is>
       </c>
       <c r="E290" s="14" t="inlineStr">
@@ -22834,7 +22834,7 @@
       </c>
       <c r="D291" s="13" t="inlineStr">
         <is>
-          <t>maa://53353 (83.33)</t>
+          <t>maa://53353 (85.71)</t>
         </is>
       </c>
       <c r="E291" s="14" t="inlineStr">
@@ -23104,7 +23104,7 @@
       </c>
       <c r="D296" s="13" t="inlineStr">
         <is>
-          <t>maa://25774 (95.89), maa://28133 (93.33), maa://22469 (92.98), **maa://39217 (38.89), **maa://31349 (50.00)</t>
+          <t>maa://25774 (94.59), maa://28133 (93.33), maa://22469 (91.80), **maa://39217 (38.89), **maa://31349 (50.00)</t>
         </is>
       </c>
       <c r="E296" s="14" t="inlineStr">
@@ -23698,7 +23698,7 @@
       </c>
       <c r="D307" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (98.46), maa://49642 (97.54), maa://49660 (93.62), maa://50517 (85.71)</t>
+          <t>maa://50280 (98.47), maa://49642 (97.58), maa://49660 (93.62), maa://50517 (85.71)</t>
         </is>
       </c>
       <c r="E307" s="14" t="inlineStr">
@@ -24076,7 +24076,7 @@
       </c>
       <c r="D314" s="13" t="inlineStr">
         <is>
-          <t>maa://53348 (89.29)</t>
+          <t>maa://53348 (86.21)</t>
         </is>
       </c>
       <c r="E314" s="14" t="inlineStr">
@@ -25139,27 +25139,27 @@
       <c r="AF333" s="8" t="n"/>
     </row>
     <row r="334" ht="13.5" customFormat="1" customHeight="1" s="22">
-      <c r="A334" s="25" t="inlineStr">
+      <c r="A334" s="12" t="inlineStr">
         <is>
           <t>折光</t>
         </is>
       </c>
-      <c r="B334" s="24" t="inlineStr">
+      <c r="B334" s="11" t="inlineStr">
         <is>
           <t>6-1</t>
         </is>
       </c>
-      <c r="C334" s="25" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D334" s="32" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E334" s="32" t="inlineStr">
+      <c r="C334" s="12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D334" s="15" t="inlineStr">
+        <is>
+          <t>maa://67818 (100.00)</t>
+        </is>
+      </c>
+      <c r="E334" s="15" t="inlineStr">
         <is>
           <t>&gt; 由非助战折光累计造成80000点伤害&gt; 3星通关主题曲6-1，必须编入非助战折光并上场，且使用折光歼灭至少10名敌人</t>
         </is>
@@ -25679,27 +25679,27 @@
       <c r="AF343" s="8" t="n"/>
     </row>
     <row r="344" ht="13.5" customFormat="1" customHeight="1" s="22">
-      <c r="A344" s="25" t="inlineStr">
+      <c r="A344" s="12" t="inlineStr">
         <is>
           <t>温米</t>
         </is>
       </c>
-      <c r="B344" s="24" t="inlineStr">
+      <c r="B344" s="11" t="inlineStr">
         <is>
           <t>6-11</t>
         </is>
       </c>
-      <c r="C344" s="25" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D344" s="30" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E344" s="30" t="inlineStr">
+      <c r="C344" s="12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D344" s="22" t="inlineStr">
+        <is>
+          <t>maa://67817 (100.00)</t>
+        </is>
+      </c>
+      <c r="E344" s="22" t="inlineStr">
         <is>
           <t>&gt; 由非助战温米累计造成40000点元素伤害&gt; 3星通关主题曲6-11；必须编入非助战温米并上场，其他成员仅可编入7名干员</t>
         </is>
@@ -26020,7 +26020,7 @@
       </c>
       <c r="D350" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (97.72), maa://32415 (86.15), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
+          <t>maa://32647 (97.72), maa://32415 (85.93), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E350" s="22" t="inlineStr">
@@ -26506,7 +26506,7 @@
       </c>
       <c r="D359" s="22" t="inlineStr">
         <is>
-          <t>maa://36868 (99.54), maa://35996 (97.89), **maa://39217 (38.89), maa://47349 (97.37)</t>
+          <t>maa://36868 (99.54), maa://35996 (97.89), maa://47349 (97.40), **maa://39217 (38.89)</t>
         </is>
       </c>
       <c r="E359" s="22" t="inlineStr">
@@ -26560,7 +26560,7 @@
       </c>
       <c r="D360" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.58), maa://49695 (100.00), maa://49758 (98.63), *maa://59402 (58.62), *maa://52357 (73.33), *maa://63091 (62.50)</t>
+          <t>maa://49696 (99.58), maa://49695 (100.00), maa://49758 (98.65), *maa://59402 (58.62), *maa://52357 (73.33), *maa://63091 (62.50)</t>
         </is>
       </c>
       <c r="E360" s="22" t="inlineStr">
@@ -26668,7 +26668,7 @@
       </c>
       <c r="D362" s="22" t="inlineStr">
         <is>
-          <t>maa://42299 (97.73), maa://42224 (84.21)</t>
+          <t>maa://42299 (97.73), maa://42224 (85.00)</t>
         </is>
       </c>
       <c r="E362" s="22" t="inlineStr">
@@ -26776,7 +26776,7 @@
       </c>
       <c r="D364" s="22" t="inlineStr">
         <is>
-          <t>maa://36646 (98.88), maa://36845 (95.86), **maa://39217 (38.89), maa://51007 (98.28)</t>
+          <t>maa://36646 (98.89), maa://36845 (95.86), **maa://39217 (38.89), maa://51007 (98.28)</t>
         </is>
       </c>
       <c r="E364" s="22" t="inlineStr">
@@ -26830,7 +26830,7 @@
       </c>
       <c r="D365" s="22" t="inlineStr">
         <is>
-          <t>maa://36645 (98.42), maa://36841 (92.65), maa://37484 (94.23), maa://37858 (93.55), *maa://56268 (60.00), maa://40489 (100.00)</t>
+          <t>maa://36645 (98.43), maa://36841 (92.65), maa://37484 (94.23), maa://37858 (93.55), *maa://56268 (60.00), maa://40489 (100.00)</t>
         </is>
       </c>
       <c r="E365" s="22" t="inlineStr">
@@ -26884,7 +26884,7 @@
       </c>
       <c r="D366" s="22" t="inlineStr">
         <is>
-          <t>maa://42635 (94.12), maa://50629 (83.33), maa://48859 (100.00)</t>
+          <t>maa://42635 (94.23), maa://50629 (83.33), maa://48859 (100.00)</t>
         </is>
       </c>
       <c r="E366" s="22" t="inlineStr">
@@ -27046,7 +27046,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (94.78), maa://48026 (94.62), maa://44635 (88.07), maa://41035 (93.51), *maa://60251 (76.47), maa://44660 (92.68), maa://41128 (84.21)</t>
+          <t>maa://40957 (94.80), maa://48026 (94.62), maa://44635 (88.07), maa://41035 (93.51), *maa://60251 (76.47), maa://44660 (92.68), maa://41128 (84.21)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -27154,7 +27154,7 @@
       </c>
       <c r="D371" s="22" t="inlineStr">
         <is>
-          <t>maa://63883 (100.00), maa://64045 (100.00), *maa://64041 (75.00)</t>
+          <t>maa://63883 (100.00), maa://64045 (100.00), *maa://64041 (80.00)</t>
         </is>
       </c>
       <c r="E371" s="22" t="inlineStr">
@@ -27802,7 +27802,7 @@
       </c>
       <c r="D383" s="22" t="inlineStr">
         <is>
-          <t>maa://43872 (93.33)</t>
+          <t>maa://43872 (93.75)</t>
         </is>
       </c>
       <c r="E383" s="22" t="inlineStr">
@@ -27856,7 +27856,7 @@
       </c>
       <c r="D384" s="22" t="inlineStr">
         <is>
-          <t>*maa://53307 (68.00)</t>
+          <t>*maa://53307 (69.23)</t>
         </is>
       </c>
       <c r="E384" s="22" t="inlineStr">
@@ -27910,7 +27910,7 @@
       </c>
       <c r="D385" s="22" t="inlineStr">
         <is>
-          <t>maa://43875 (98.31)</t>
+          <t>maa://43875 (98.33)</t>
         </is>
       </c>
       <c r="E385" s="22" t="inlineStr">
@@ -27964,7 +27964,7 @@
       </c>
       <c r="D386" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (81.29), maa://44745 (97.97), **maa://49516 (39.29), *maa://45952 (57.14), ***maa://46851 (12.50), *maa://44896 (77.78)</t>
+          <t>maa://42970 (81.29), maa://44745 (98.01), **maa://49516 (39.29), *maa://45952 (57.14), ***maa://46851 (12.50), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E386" s="22" t="inlineStr">
@@ -28423,7 +28423,7 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>maa://59533 (97.67), maa://59577 (100.00)</t>
+          <t>maa://59533 (97.73), maa://59577 (100.00)</t>
         </is>
       </c>
       <c r="E396" t="inlineStr">
@@ -28558,7 +28558,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>maa://51872 (96.55), maa://51876 (99.04), maa://63228 (87.88), maa://51873 (100.00), maa://62047 (92.00)</t>
+          <t>maa://51872 (96.60), maa://51876 (99.06), maa://63228 (87.88), maa://51873 (100.00), maa://62047 (92.00)</t>
         </is>
       </c>
       <c r="E401" t="inlineStr">
@@ -28568,27 +28568,27 @@
       </c>
     </row>
     <row r="402">
-      <c r="A402" s="28" t="inlineStr">
+      <c r="A402" s="17" t="inlineStr">
         <is>
           <t>Miss.Christine</t>
         </is>
       </c>
-      <c r="B402" s="28" t="inlineStr">
+      <c r="B402" s="17" t="inlineStr">
         <is>
           <t>DM-7</t>
         </is>
       </c>
-      <c r="C402" s="28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D402" s="29" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E402" s="29" t="inlineStr">
+      <c r="C402" s="17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D402" t="inlineStr">
+        <is>
+          <t>**maa://67814 (50.00)</t>
+        </is>
+      </c>
+      <c r="E402" t="inlineStr">
         <is>
           <t>&gt; 战斗中非助战Miss.Christine累计使用“狂饮之宴”10次&gt; 3星通关插曲DM-7，必须编入非助战Miss.Christine并上场，且至少使用2次“狂饮之宴”</t>
         </is>
@@ -28612,7 +28612,7 @@
       </c>
       <c r="D403" t="inlineStr">
         <is>
-          <t>maa://60449 (98.96), maa://59493 (96.83)</t>
+          <t>maa://60449 (98.97), maa://59493 (96.85)</t>
         </is>
       </c>
       <c r="E403" t="inlineStr">
@@ -28622,27 +28622,27 @@
       </c>
     </row>
     <row r="404">
-      <c r="A404" s="28" t="inlineStr">
+      <c r="A404" s="17" t="inlineStr">
         <is>
           <t>录武官</t>
         </is>
       </c>
-      <c r="B404" s="28" t="inlineStr">
+      <c r="B404" s="17" t="inlineStr">
         <is>
           <t>HS-5</t>
         </is>
       </c>
-      <c r="C404" s="28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D404" s="29" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E404" s="29" t="inlineStr">
+      <c r="C404" s="17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D404" t="inlineStr">
+        <is>
+          <t>maa://67815 (100.00)</t>
+        </is>
+      </c>
+      <c r="E404" t="inlineStr">
         <is>
           <t>&gt; 战斗中非助战录武官累计使用“一点关窍”6次&gt; 3星通关插曲HS-5，必须编入非助战录武官并上场，且不编入其他医疗干员</t>
         </is>
@@ -28666,7 +28666,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>maa://62756 (95.59)</t>
+          <t>maa://62756 (95.68)</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">
@@ -28676,27 +28676,27 @@
       </c>
     </row>
     <row r="406">
-      <c r="A406" s="28" t="inlineStr">
+      <c r="A406" s="17" t="inlineStr">
         <is>
           <t>吉星</t>
         </is>
       </c>
-      <c r="B406" s="28" t="inlineStr">
+      <c r="B406" s="17" t="inlineStr">
         <is>
           <t>S5-9</t>
         </is>
       </c>
-      <c r="C406" s="28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D406" s="29" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E406" s="29" t="inlineStr">
+      <c r="C406" s="17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D406" t="inlineStr">
+        <is>
+          <t>maa://67816 (100.00)</t>
+        </is>
+      </c>
+      <c r="E406" t="inlineStr">
         <is>
           <t>&gt; 由非助战吉星累计造成30歼灭数&gt; 3星通关主题曲S5-9，必须编入非助战吉星并上场，且至少使用2次“吉星高照！”</t>
         </is>
@@ -28720,7 +28720,7 @@
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>maa://64040 (98.95), maa://52505 (99.08), maa://66377 (91.67), **maa://66376 (33.33)</t>
+          <t>maa://64040 (98.95), maa://52505 (99.14), maa://66377 (92.31), **maa://66376 (33.33)</t>
         </is>
       </c>
       <c r="E407" t="inlineStr">
@@ -28747,7 +28747,7 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>*maa://67090 (71.43)</t>
+          <t>*maa://67090 (78.95)</t>
         </is>
       </c>
       <c r="E408" t="inlineStr">
@@ -28801,7 +28801,7 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>maa://67089 (100.00), maa://67271 (85.71)</t>
+          <t>maa://67089 (95.45), maa://67271 (87.50)</t>
         </is>
       </c>
       <c r="E410" t="inlineStr">
@@ -28828,7 +28828,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>maa://67088 (92.86)</t>
+          <t>maa://67088 (85.19)</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
@@ -28855,7 +28855,7 @@
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>maa://67087 (92.00), maa://67268 (96.30), maa://67269 (100.00), maa://67648 (100.00)</t>
+          <t>maa://67087 (93.55), maa://67268 (97.83), maa://67269 (90.00), maa://67648 (100.00)</t>
         </is>
       </c>
       <c r="E412" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#237)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -712,7 +712,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (97.92), maa://24702 (95.02), maa://36681 (86.21)</t>
+          <t>maa://25390 (98.04), maa://24702 (95.03), maa://36681 (86.21)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://58660 (98.51), maa://39402 (94.39), *maa://34787 (74.75)</t>
+          <t>maa://58660 (98.61), maa://39402 (94.50), *maa://34787 (74.75)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -776,7 +776,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (96.93), maa://66635 (99.77)</t>
+          <t>maa://22742 (97.00), maa://66635 (99.79)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://36684 (98.01), maa://21246 (91.29)</t>
+          <t>maa://36684 (98.13), maa://21246 (91.29)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://59087 (97.00), maa://25251 (92.25)</t>
+          <t>maa://59087 (96.72), maa://25251 (91.61)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -842,7 +842,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (99.41), maa://36987 (97.06), maa://39849 (90.00)</t>
+          <t>maa://40192 (99.29), maa://36987 (97.10), maa://39849 (90.91)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -858,7 +858,7 @@
       </c>
       <c r="H3" s="8" t="inlineStr">
         <is>
-          <t>maa://21247 (99.24)</t>
+          <t>maa://21247 (99.29)</t>
         </is>
       </c>
       <c r="I3" s="19" t="n"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>maa://22880 (88.76), maa://20276 (93.58), maa://22749 (84.00)</t>
+          <t>maa://22880 (89.38), maa://20276 (93.67), maa://22749 (84.00)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -890,7 +890,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (98.17), maa://26254 (98.08), *maa://22738 (80.00)</t>
+          <t>maa://21249 (98.22), maa://26254 (98.11), *maa://22738 (80.00)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://45854 (85.71), maa://60545 (98.33), maa://24617 (91.18)</t>
+          <t>maa://45854 (85.96), maa://60545 (98.46), maa://24617 (91.18)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (90.75), maa://27484 (99.17), maa://27480 (84.91)</t>
+          <t>maa://27396 (91.13), maa://27484 (99.20), maa://27480 (84.91)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://52241 (99.26), maa://24390 (96.72)</t>
+          <t>maa://52241 (99.30), maa://24390 (96.72)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -954,7 +954,7 @@
       </c>
       <c r="AF3" s="8" t="inlineStr">
         <is>
-          <t>maa://21289 (90.43)</t>
+          <t>maa://21289 (90.62)</t>
         </is>
       </c>
       <c r="AG3" s="16" t="n"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (97.67), maa://22499 (88.89), maa://22746 (100.00)</t>
+          <t>maa://24632 (97.80), maa://22499 (89.47), maa://22746 (100.00)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (98.94), maa://50121 (96.19)</t>
+          <t>maa://49983 (99.00), maa://50121 (96.30)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://27295 (97.31), maa://32509 (95.63), maa://31008 (94.48), maa://22754 (88.00)</t>
+          <t>maa://27295 (97.51), maa://32509 (95.75), maa://31008 (94.67), maa://22754 (88.00)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="AB4" s="8" t="inlineStr">
         <is>
-          <t>maa://32658 (80.43)</t>
+          <t>maa://32658 (80.85)</t>
         </is>
       </c>
       <c r="AC4" s="19" t="n"/>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>*maa://39394 (58.70), *maa://30062 (62.30), ***maa://26209 (13.04)</t>
+          <t>*maa://39394 (58.33), *maa://30062 (61.29), ***maa://26209 (13.04)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (90.53), maa://54105 (98.26), *maa://22744 (80.00)</t>
+          <t>maa://21245 (90.73), maa://54105 (98.38), *maa://22744 (80.00)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="L5" s="8" t="inlineStr">
         <is>
-          <t>maa://22757 (89.90)</t>
+          <t>maa://22757 (90.00)</t>
         </is>
       </c>
       <c r="M5" s="19" t="n"/>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="P5" s="8" t="inlineStr">
         <is>
-          <t>maa://21919 (98.97), maa://21281 (81.25)</t>
+          <t>maa://21919 (98.98), maa://21281 (81.25)</t>
         </is>
       </c>
       <c r="Q5" s="19" t="n"/>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="X5" s="8" t="inlineStr">
         <is>
-          <t>maa://21290 (99.12)</t>
+          <t>maa://21290 (99.15)</t>
         </is>
       </c>
       <c r="Y5" s="19" t="n"/>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="AB5" s="8" t="inlineStr">
         <is>
-          <t>*maa://29863 (62.50), ***maa://22752 (12.50), **maa://26013 (33.33)</t>
+          <t>*maa://29863 (61.22), ***maa://22752 (12.50), **maa://26013 (33.33)</t>
         </is>
       </c>
       <c r="AC5" s="19" t="n"/>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="D6" s="8" t="inlineStr">
         <is>
-          <t>maa://42407 (96.98)</t>
+          <t>maa://42407 (97.03)</t>
         </is>
       </c>
       <c r="E6" s="19" t="n"/>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="H6" s="8" t="inlineStr">
         <is>
-          <t>maa://24370 (97.12)</t>
+          <t>maa://24370 (97.20)</t>
         </is>
       </c>
       <c r="I6" s="19" t="n"/>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="L6" s="8" t="inlineStr">
         <is>
-          <t>maa://24839 (99.31)</t>
+          <t>maa://24839 (99.33)</t>
         </is>
       </c>
       <c r="M6" s="19" t="n"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (98.55), maa://30381 (95.00)</t>
+          <t>maa://31836 (98.60), maa://30381 (95.00)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="X6" s="8" t="inlineStr">
         <is>
-          <t>maa://52754 (95.49)</t>
+          <t>maa://52754 (95.65)</t>
         </is>
       </c>
       <c r="Y6" s="19" t="n"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="AF6" s="8" t="inlineStr">
         <is>
-          <t>*maa://33152 (77.87), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (78.23), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="16" t="n"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>maa://21955 (97.89)</t>
+          <t>maa://21955 (97.93)</t>
         </is>
       </c>
       <c r="E7" s="19" t="n"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>*maa://22763 (73.21), maa://64972 (94.44)</t>
+          <t>*maa://22763 (74.14), maa://64972 (95.00)</t>
         </is>
       </c>
       <c r="I7" s="19" t="n"/>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (98.42), maa://24957 (94.34)</t>
+          <t>maa://28624 (98.49), maa://24957 (94.34)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="P7" s="8" t="inlineStr">
         <is>
-          <t>maa://22750 (96.35)</t>
+          <t>maa://22750 (96.45)</t>
         </is>
       </c>
       <c r="Q7" s="19" t="n"/>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="T7" s="8" t="inlineStr">
         <is>
-          <t>maa://21291 (93.06)</t>
+          <t>maa://21291 (93.29)</t>
         </is>
       </c>
       <c r="U7" s="19" t="n"/>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (96.86), maa://22758 (81.44)</t>
+          <t>maa://22399 (96.98), maa://22758 (81.44)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="AF7" s="8" t="inlineStr">
         <is>
-          <t>maa://45272 (99.25)</t>
+          <t>maa://45272 (99.30)</t>
         </is>
       </c>
       <c r="AG7" s="16" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.15 13:24:29</t>
+          <t>更新日期：2025.09.17 13:21:49</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (89.66), *maa://39431 (58.33), **maa://37551 (50.00)</t>
+          <t>maa://21476 (89.73), *maa://39431 (58.33), **maa://37551 (50.00)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
-          <t>*maa://24371 (76.61)</t>
+          <t>*maa://24371 (76.88)</t>
         </is>
       </c>
       <c r="I8" s="19" t="n"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (91.12), maa://23252 (91.67), maa://37496 (98.25)</t>
+          <t>maa://32931 (91.26), maa://23252 (91.67), maa://37496 (98.25)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (96.12), maa://67587 (97.89)</t>
+          <t>maa://21411 (96.01), maa://67587 (97.31)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="AB8" s="8" t="inlineStr">
         <is>
-          <t>maa://25389 (93.94)</t>
+          <t>maa://25389 (94.23)</t>
         </is>
       </c>
       <c r="AC8" s="19" t="n"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>maa://24479 (83.33), *maa://21990 (51.72)</t>
+          <t>maa://24479 (83.52), *maa://21990 (51.72)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>maa://22765 (94.96), *maa://21915 (78.57)</t>
+          <t>maa://22765 (95.10), *maa://21915 (78.57)</t>
         </is>
       </c>
       <c r="E9" s="19" t="n"/>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="H9" s="8" t="inlineStr">
         <is>
-          <t>*maa://47450 (75.00), maa://56348 (93.75)</t>
+          <t>*maa://47450 (75.00), maa://56348 (94.12)</t>
         </is>
       </c>
       <c r="I9" s="19" t="n"/>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (95.68), maa://39552 (86.36)</t>
+          <t>maa://22762 (95.83), maa://39552 (86.36)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="T9" s="8" t="inlineStr">
         <is>
-          <t>maa://26222 (99.37)</t>
+          <t>maa://26222 (99.38)</t>
         </is>
       </c>
       <c r="U9" s="19" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://52237 (99.69), maa://26223 (98.30)</t>
+          <t>maa://52237 (99.71), maa://26223 (98.31)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (94.35), maa://40166 (94.47)</t>
+          <t>maa://28711 (94.60), maa://40166 (94.66)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (90.94), maa://66916 (97.36)</t>
+          <t>maa://26206 (90.98), maa://66916 (97.51)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>maa://54000 (92.00)</t>
+          <t>maa://54000 (91.14)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1794,7 +1794,7 @@
       </c>
       <c r="L10" s="8" t="inlineStr">
         <is>
-          <t>**maa://24395 (41.30)</t>
+          <t>**maa://24395 (42.55)</t>
         </is>
       </c>
       <c r="M10" s="19" t="n"/>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (91.10), *maa://36669 (73.33)</t>
+          <t>maa://28977 (91.29), *maa://36669 (74.03)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (99.09), maa://22755 (91.18), maa://63521 (93.93)</t>
+          <t>maa://27395 (99.12), maa://22755 (91.23), maa://63521 (94.17)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://45828 (98.96), maa://22301 (97.63), maa://22726 (100.00)</t>
+          <t>maa://45828 (99.02), maa://22301 (97.63), maa://22726 (100.00)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>*maa://25021 (55.10), *maa://22733 (67.21), **maa://22761 (33.33)</t>
+          <t>*maa://25021 (55.41), *maa://22733 (67.21), **maa://22761 (33.33)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="D11" s="8" t="inlineStr">
         <is>
-          <t>maa://36707 (99.69)</t>
+          <t>maa://36707 (99.70)</t>
         </is>
       </c>
       <c r="E11" s="19" t="n"/>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="L11" s="8" t="inlineStr">
         <is>
-          <t>maa://21287 (92.95)</t>
+          <t>maa://21287 (93.04)</t>
         </is>
       </c>
       <c r="M11" s="19" t="n"/>
@@ -1940,7 +1940,7 @@
       </c>
       <c r="P11" s="8" t="inlineStr">
         <is>
-          <t>maa://45557 (95.35)</t>
+          <t>maa://45557 (95.65)</t>
         </is>
       </c>
       <c r="Q11" s="19" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (92.63), maa://22501 (99.45), maa://64808 (100.00), maa://45521 (94.92)</t>
+          <t>maa://22747 (92.90), maa://22501 (99.47), maa://64808 (100.00), maa://45521 (94.92)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="X11" s="8" t="inlineStr">
         <is>
-          <t>maa://36713 (99.13)</t>
+          <t>maa://36713 (99.16)</t>
         </is>
       </c>
       <c r="Y11" s="19" t="n"/>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="AB11" s="8" t="inlineStr">
         <is>
-          <t>maa://29912 (99.65), maa://22516 (86.52)</t>
+          <t>maa://29912 (99.67), maa://22516 (86.52)</t>
         </is>
       </c>
       <c r="AC11" s="19" t="n"/>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="AF11" s="8" t="inlineStr">
         <is>
-          <t>maa://31203 (98.36)</t>
+          <t>maa://31203 (98.46)</t>
         </is>
       </c>
       <c r="AG11" s="16" t="n"/>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>maa://36678 (96.23), maa://30766 (91.18)</t>
+          <t>maa://36678 (96.43), maa://30766 (91.18)</t>
         </is>
       </c>
       <c r="E12" s="19" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (93.17), maa://54294 (95.74)</t>
+          <t>maa://21867 (93.20), maa://54294 (95.95)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (97.69), maa://64046 (98.36)</t>
+          <t>maa://63896 (97.73), maa://64046 (98.43)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="P12" s="8" t="inlineStr">
         <is>
-          <t>maa://57541 (90.32)</t>
+          <t>maa://57541 (90.62)</t>
         </is>
       </c>
       <c r="Q12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://37962 (98.52), maa://21485 (80.80), maa://22753 (92.70)</t>
+          <t>maa://37962 (98.59), maa://21485 (80.97), maa://22753 (92.74)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://36677 (98.94), maa://23669 (95.38), maa://39872 (97.75)</t>
+          <t>maa://36677 (99.00), maa://23669 (95.38), maa://39872 (97.80)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>maa://28932 (93.56)</t>
+          <t>maa://28932 (93.83)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (96.24), maa://36673 (93.60), maa://25001 (88.37)</t>
+          <t>maa://24999 (96.29), maa://36673 (93.80), maa://25001 (88.37)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.09), maa://66545 (98.83)</t>
+          <t>*maa://21248 (73.04), maa://66545 (98.89)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (97.08), maa://22583 (86.43)</t>
+          <t>maa://22676 (97.22), maa://22583 (87.07)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="X13" s="8" t="inlineStr">
         <is>
-          <t>maa://34957 (93.90)</t>
+          <t>maa://34957 (94.06)</t>
         </is>
       </c>
       <c r="Y13" s="19" t="n"/>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (93.09)</t>
+          <t>maa://39883 (93.33)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2282,7 +2282,7 @@
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>maa://30764 (94.62)</t>
+          <t>maa://30764 (94.74)</t>
         </is>
       </c>
       <c r="E14" s="19" t="n"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (98.75), maa://26245 (97.00), maa://36682 (98.14), maa://21288 (96.38)</t>
+          <t>maa://39841 (98.84), maa://26245 (97.00), maa://36682 (98.17), maa://21288 (96.38)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2330,7 +2330,7 @@
       </c>
       <c r="P14" s="8" t="inlineStr">
         <is>
-          <t>maa://23250 (99.56), maa://20107 (87.50), maa://22772 (100.00)</t>
+          <t>maa://23250 (99.58), maa://20107 (87.50), maa://22772 (100.00)</t>
         </is>
       </c>
       <c r="Q14" s="19" t="n"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://42751 (98.68), maa://22521 (95.36)</t>
+          <t>maa://42751 (98.73), maa://22521 (95.41)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="X14" s="8" t="inlineStr">
         <is>
-          <t>maa://37468 (97.59)</t>
+          <t>maa://37468 (97.65)</t>
         </is>
       </c>
       <c r="Y14" s="19" t="n"/>
@@ -2378,7 +2378,7 @@
       </c>
       <c r="AB14" s="8" t="inlineStr">
         <is>
-          <t>maa://22764 (98.73)</t>
+          <t>maa://22764 (98.76)</t>
         </is>
       </c>
       <c r="AC14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (84.85), maa://45058 (98.14), maa://22734 (84.85), *maa://36048 (73.53)</t>
+          <t>maa://22743 (85.06), maa://45058 (98.00), maa://22734 (84.85), *maa://36048 (73.68)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (96.22), maa://21478 (90.48)</t>
+          <t>maa://24304 (96.44), maa://21478 (90.48)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="L15" s="8" t="inlineStr">
         <is>
-          <t>*maa://21334 (66.67)</t>
+          <t>*maa://21334 (67.92)</t>
         </is>
       </c>
       <c r="M15" s="19" t="n"/>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="P15" s="8" t="inlineStr">
         <is>
-          <t>maa://24762 (97.30), *maa://22727 (70.00)</t>
+          <t>maa://24762 (97.41), *maa://22727 (70.00)</t>
         </is>
       </c>
       <c r="Q15" s="19" t="n"/>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="T15" s="8" t="inlineStr">
         <is>
-          <t>maa://23892 (97.37)</t>
+          <t>maa://23892 (97.44)</t>
         </is>
       </c>
       <c r="U15" s="19" t="n"/>
@@ -2519,12 +2519,12 @@
       </c>
       <c r="AE15" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://36666 (95.85), maa://21364 (83.33), *maa://22766 (70.50)</t>
+          <t>maa://36666 (95.93), maa://21364 (83.33), *maa://22766 (70.50), *maa://68306 (80.00)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://37650 (99.69), maa://21441 (96.62), maa://36679 (94.55)</t>
+          <t>maa://37650 (99.70), maa://21441 (96.62), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2590,7 +2590,7 @@
       </c>
       <c r="P16" s="8" t="inlineStr">
         <is>
-          <t>maa://28504 (95.65)</t>
+          <t>maa://28504 (95.69)</t>
         </is>
       </c>
       <c r="Q16" s="19" t="n"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://36674 (97.56), maa://22729 (95.90), *maa://28648 (77.89)</t>
+          <t>maa://36674 (97.69), maa://22729 (95.95), *maa://28648 (77.89)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2622,7 +2622,7 @@
       </c>
       <c r="X16" s="8" t="inlineStr">
         <is>
-          <t>maa://28501 (99.16), maa://28051 (96.88)</t>
+          <t>maa://28501 (99.18), maa://28051 (96.88)</t>
         </is>
       </c>
       <c r="Y16" s="19" t="n"/>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="AB16" s="8" t="inlineStr">
         <is>
-          <t>maa://26228 (97.54)</t>
+          <t>maa://26228 (97.65)</t>
         </is>
       </c>
       <c r="AC16" s="19" t="n"/>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>maa://23911 (89.70), maa://27755 (93.69), maa://67613 (98.94)</t>
+          <t>maa://23911 (89.76), maa://27755 (93.69), maa://67613 (99.09)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2672,7 +2672,7 @@
       </c>
       <c r="D17" s="8" t="inlineStr">
         <is>
-          <t>maa://21624 (87.76), maa://56358 (100.00)</t>
+          <t>maa://21624 (88.00), maa://56358 (100.00)</t>
         </is>
       </c>
       <c r="E17" s="19" t="n"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://39599 (97.79), maa://22430 (90.17)</t>
+          <t>maa://39599 (97.90), maa://22430 (90.17)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="L17" s="8" t="inlineStr">
         <is>
-          <t>maa://21679 (86.96)</t>
+          <t>maa://21679 (87.23)</t>
         </is>
       </c>
       <c r="M17" s="19" t="n"/>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (82.50), maa://56238 (98.02)</t>
+          <t>maa://23890 (82.50), maa://56238 (98.13)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="T17" s="8" t="inlineStr">
         <is>
-          <t>*maa://42324 (67.90)</t>
+          <t>*maa://42324 (68.29)</t>
         </is>
       </c>
       <c r="U17" s="19" t="n"/>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="AF17" s="8" t="inlineStr">
         <is>
-          <t>maa://50136 (98.78)</t>
+          <t>maa://50136 (98.82)</t>
         </is>
       </c>
       <c r="AG17" s="16" t="n"/>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>maa://24570 (98.12)</t>
+          <t>maa://24570 (98.16)</t>
         </is>
       </c>
       <c r="E18" s="19" t="n"/>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="H18" s="8" t="inlineStr">
         <is>
-          <t>maa://24421 (94.59)</t>
+          <t>maa://24421 (94.85)</t>
         </is>
       </c>
       <c r="I18" s="19" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://52226 (99.62), maa://22466 (92.79)</t>
+          <t>maa://52226 (99.64), maa://22466 (92.79)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), maa://54153 (99.57), maa://24380 (100.00)</t>
+          <t>maa://24379 (100.00), maa://54153 (99.59), maa://24380 (100.00)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2866,7 +2866,7 @@
       </c>
       <c r="T18" s="8" t="inlineStr">
         <is>
-          <t>maa://24385 (98.39)</t>
+          <t>maa://24385 (98.41)</t>
         </is>
       </c>
       <c r="U18" s="19" t="n"/>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (98.48), maa://22741 (91.67)</t>
+          <t>maa://21917 (98.56), maa://22741 (91.67)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="AB18" s="8" t="inlineStr">
         <is>
-          <t>maa://24393 (98.83)</t>
+          <t>maa://24393 (98.86)</t>
         </is>
       </c>
       <c r="AC18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://47854 (91.89)</t>
+          <t>maa://47854 (92.37)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -2932,7 +2932,7 @@
       </c>
       <c r="D19" s="8" t="inlineStr">
         <is>
-          <t>maa://62850 (99.28)</t>
+          <t>maa://62850 (99.23)</t>
         </is>
       </c>
       <c r="E19" s="19" t="n"/>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="L19" s="8" t="inlineStr">
         <is>
-          <t>maa://39347 (97.73), maa://56392 (100.00)</t>
+          <t>maa://39347 (97.78), maa://56392 (100.00)</t>
         </is>
       </c>
       <c r="M19" s="19" t="n"/>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="T19" s="8" t="inlineStr">
         <is>
-          <t>maa://24386 (99.60)</t>
+          <t>maa://24386 (99.61)</t>
         </is>
       </c>
       <c r="U19" s="19" t="n"/>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (83.84), *maa://36668 (68.75)</t>
+          <t>maa://30709 (84.24), *maa://36668 (68.75)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3044,7 +3044,7 @@
       </c>
       <c r="AF19" s="8" t="inlineStr">
         <is>
-          <t>*maa://21663 (64.71), maa://52239 (84.62)</t>
+          <t>*maa://21663 (64.71), maa://52239 (85.19)</t>
         </is>
       </c>
       <c r="AG19" s="16" t="n"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://25198 (97.66), maa://36680 (98.83), maa://21432 (91.34)</t>
+          <t>maa://25198 (97.48), maa://36680 (98.90), maa://21432 (91.38)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3078,7 +3078,7 @@
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>maa://22864 (95.29)</t>
+          <t>maa://22864 (95.48)</t>
         </is>
       </c>
       <c r="I20" s="19" t="n"/>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (94.61)</t>
+          <t>maa://41331 (94.78)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="P20" s="8" t="inlineStr">
         <is>
-          <t>maa://37442 (98.26)</t>
+          <t>maa://37442 (98.31)</t>
         </is>
       </c>
       <c r="Q20" s="19" t="n"/>
@@ -3126,7 +3126,7 @@
       </c>
       <c r="T20" s="8" t="inlineStr">
         <is>
-          <t>maa://29113 (92.75)</t>
+          <t>maa://29113 (93.15)</t>
         </is>
       </c>
       <c r="U20" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (95.77), maa://56241 (98.24), maa://49976 (88.35)</t>
+          <t>maa://50085 (96.00), maa://56241 (98.25), maa://49976 (88.35)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>maa://21261 (98.92)</t>
+          <t>maa://21261 (98.96)</t>
         </is>
       </c>
       <c r="E21" s="19" t="n"/>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="H21" s="8" t="inlineStr">
         <is>
-          <t>maa://24372 (98.67)</t>
+          <t>maa://24372 (98.71)</t>
         </is>
       </c>
       <c r="I21" s="19" t="n"/>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="L21" s="8" t="inlineStr">
         <is>
-          <t>maa://31731 (96.08)</t>
+          <t>maa://31731 (96.12)</t>
         </is>
       </c>
       <c r="M21" s="19" t="n"/>
@@ -3240,7 +3240,7 @@
       </c>
       <c r="P21" s="8" t="inlineStr">
         <is>
-          <t>maa://24381 (86.67)</t>
+          <t>maa://24381 (83.87)</t>
         </is>
       </c>
       <c r="Q21" s="19" t="n"/>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (98.01), maa://20110 (87.01)</t>
+          <t>maa://34946 (98.10), maa://20110 (87.01)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="AB21" s="8" t="inlineStr">
         <is>
-          <t>maa://21443 (85.74), *maa://52223 (79.67)</t>
+          <t>maa://21443 (86.18), maa://52223 (80.58)</t>
         </is>
       </c>
       <c r="AC21" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22432 (93.11), maa://22524 (82.69), maa://64221 (97.51)</t>
+          <t>maa://22432 (93.19), maa://22524 (82.75), maa://64221 (97.45)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>maa://25236 (99.00)</t>
+          <t>maa://25236 (99.05)</t>
         </is>
       </c>
       <c r="I22" s="19" t="n"/>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>maa://27127 (81.34), *maa://22751 (70.93), maa://66865 (99.27)</t>
+          <t>maa://27127 (82.11), *maa://22751 (70.93), maa://66865 (99.30)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3386,7 +3386,7 @@
       </c>
       <c r="T22" s="8" t="inlineStr">
         <is>
-          <t>maa://38495 (82.05)</t>
+          <t>maa://38495 (83.33)</t>
         </is>
       </c>
       <c r="U22" s="19" t="n"/>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://37649 (93.23), maa://21282 (98.88)</t>
+          <t>maa://37649 (93.47), maa://21282 (98.89)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="AB22" s="8" t="inlineStr">
         <is>
-          <t>maa://23656 (99.43)</t>
+          <t>maa://23656 (99.44)</t>
         </is>
       </c>
       <c r="AC22" s="19" t="n"/>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="AF22" s="8" t="inlineStr">
         <is>
-          <t>maa://29658 (96.67)</t>
+          <t>maa://29658 (96.81)</t>
         </is>
       </c>
       <c r="AG22" s="16" t="n"/>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>***maa://28036 (29.21), *maa://41753 (61.02)</t>
+          <t>***maa://28036 (29.21), *maa://41753 (62.90)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (98.47), maa://39875 (95.50)</t>
+          <t>maa://39756 (98.47), maa://39875 (95.58)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (96.72), maa://29748 (81.62), maa://37566 (80.33)</t>
+          <t>maa://30587 (96.67), maa://29748 (81.72), maa://37566 (80.33)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="T23" s="8" t="inlineStr">
         <is>
-          <t>maa://31212 (94.85), maa://24387 (84.09), maa://67084 (85.71)</t>
+          <t>maa://31212 (95.00), maa://24387 (84.44), maa://67084 (85.71)</t>
         </is>
       </c>
       <c r="U23" s="19" t="n"/>
@@ -3532,7 +3532,7 @@
       </c>
       <c r="X23" s="8" t="inlineStr">
         <is>
-          <t>*maa://28503 (60.00)</t>
+          <t>*maa://28503 (60.40)</t>
         </is>
       </c>
       <c r="Y23" s="19" t="n"/>
@@ -3548,7 +3548,7 @@
       </c>
       <c r="AB23" s="8" t="inlineStr">
         <is>
-          <t>maa://29652 (96.10)</t>
+          <t>maa://29652 (96.25)</t>
         </is>
       </c>
       <c r="AC23" s="19" t="n"/>
@@ -3564,7 +3564,7 @@
       </c>
       <c r="AF23" s="8" t="inlineStr">
         <is>
-          <t>maa://31489 (97.92)</t>
+          <t>maa://31489 (98.00)</t>
         </is>
       </c>
       <c r="AG23" s="16" t="n"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (84.42), maa://46650 (89.52)</t>
+          <t>maa://24368 (84.62), maa://46650 (89.63)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (95.63), maa://23504 (94.02), *maa://25141 (79.33), maa://52227 (97.89), *maa://36663 (79.25)</t>
+          <t>maa://29988 (95.79), maa://23504 (94.02), *maa://25141 (79.33), maa://52227 (97.95), *maa://36663 (79.25)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="AB24" s="8" t="inlineStr">
         <is>
-          <t>maa://39349 (96.88)</t>
+          <t>maa://39349 (96.97)</t>
         </is>
       </c>
       <c r="AC24" s="19" t="n"/>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://64165 (99.12), maa://22523 (80.09), maa://29910 (94.20), maa://45831 (93.55)</t>
+          <t>maa://64165 (99.16), maa://22523 (80.09), maa://29910 (94.20), maa://45831 (93.55)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (96.30), maa://63016 (98.97)</t>
+          <t>maa://29753 (96.34), maa://63016 (99.01)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>*maa://29063 (74.92), *maa://25311 (70.71), maa://45047 (86.96)</t>
+          <t>*maa://29063 (75.24), *maa://25311 (70.71), maa://45047 (87.14)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3739,12 +3739,12 @@
       </c>
       <c r="K25" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="L25" s="8" t="inlineStr">
         <is>
-          <t>maa://24378 (93.51)</t>
+          <t>maa://24378 (93.59), maa://68415 (100.00)</t>
         </is>
       </c>
       <c r="M25" s="19" t="n"/>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="T25" s="8" t="inlineStr">
         <is>
-          <t>maa://20109 (96.11), maa://22545 (100.00)</t>
+          <t>maa://20109 (96.20), maa://22545 (100.00)</t>
         </is>
       </c>
       <c r="U25" s="19" t="n"/>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="X25" s="8" t="inlineStr">
         <is>
-          <t>maa://29890 (90.52)</t>
+          <t>maa://29890 (90.68)</t>
         </is>
       </c>
       <c r="Y25" s="19" t="n"/>
@@ -3803,12 +3803,12 @@
       </c>
       <c r="AA25" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (92.88), *maa://24516 (79.80), maa://26001 (83.33)</t>
+          <t>maa://31215 (92.89), *maa://24516 (79.80), maa://26001 (83.33), maa://68311 (100.00)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (97.81), maa://36676 (99.81), maa://24621 (96.84), maa://22771 (88.24), maa://37772 (83.33)</t>
+          <t>maa://20108 (97.89), maa://36676 (99.82), maa://24621 (96.84), maa://22771 (88.24), maa://37772 (83.33)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://56374 (100.00), maa://41802 (95.45)</t>
+          <t>maa://56374 (100.00), maa://41802 (95.65)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3858,7 +3858,7 @@
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
-          <t>maa://56240 (95.91), maa://24913 (92.17)</t>
+          <t>maa://56240 (96.07), maa://24913 (92.17)</t>
         </is>
       </c>
       <c r="I26" s="19" t="n"/>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="P26" s="8" t="inlineStr">
         <is>
-          <t>maa://39870 (93.94), maa://56625 (100.00)</t>
+          <t>maa://39870 (94.12), maa://56625 (100.00)</t>
         </is>
       </c>
       <c r="Q26" s="19" t="n"/>
@@ -3922,7 +3922,7 @@
       </c>
       <c r="X26" s="8" t="inlineStr">
         <is>
-          <t>maa://24389 (98.08)</t>
+          <t>maa://24389 (98.11)</t>
         </is>
       </c>
       <c r="Y26" s="19" t="n"/>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="AB26" s="8" t="inlineStr">
         <is>
-          <t>maa://42235 (98.26)</t>
+          <t>maa://42235 (98.31)</t>
         </is>
       </c>
       <c r="AC26" s="19" t="n"/>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="AF26" s="8" t="inlineStr">
         <is>
-          <t>*maa://30511 (71.43), **maa://29760 (47.62)</t>
+          <t>*maa://30511 (72.15), **maa://29760 (47.62)</t>
         </is>
       </c>
       <c r="AG26" s="16" t="n"/>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>maa://39601 (90.48), maa://34494 (97.50)</t>
+          <t>maa://39601 (90.00), maa://34494 (97.50)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4004,7 +4004,7 @@
       </c>
       <c r="L27" s="8" t="inlineStr">
         <is>
-          <t>maa://28071 (87.76)</t>
+          <t>maa://28071 (88.24)</t>
         </is>
       </c>
       <c r="M27" s="19" t="n"/>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="T27" s="8" t="inlineStr">
         <is>
-          <t>maa://30624 (88.96)</t>
+          <t>maa://30624 (89.16)</t>
         </is>
       </c>
       <c r="U27" s="19" t="n"/>
@@ -4102,7 +4102,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (95.47), maa://25725 (84.55)</t>
+          <t>maa://24465 (95.58), maa://25725 (84.80)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="L28" s="8" t="inlineStr">
         <is>
-          <t>maa://30770 (89.29)</t>
+          <t>maa://30770 (89.41)</t>
         </is>
       </c>
       <c r="M28" s="19" t="n"/>
@@ -4166,7 +4166,7 @@
       </c>
       <c r="T28" s="8" t="inlineStr">
         <is>
-          <t>maa://29765 (92.31), maa://23263 (96.09)</t>
+          <t>maa://29765 (92.57), maa://23263 (96.12)</t>
         </is>
       </c>
       <c r="U28" s="19" t="n"/>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (96.95), maa://41749 (97.18)</t>
+          <t>maa://39929 (97.09), maa://41749 (97.03)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (93.75), maa://65700 (98.51)</t>
+          <t>maa://36660 (93.85), maa://65700 (98.59)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4232,7 +4232,7 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>maa://31694 (99.23)</t>
+          <t>maa://31694 (99.26)</t>
         </is>
       </c>
       <c r="E29" s="19" t="n"/>
@@ -4248,7 +4248,7 @@
       </c>
       <c r="H29" s="8" t="inlineStr">
         <is>
-          <t>**maa://25175 (50.00)</t>
+          <t>*maa://25175 (50.46)</t>
         </is>
       </c>
       <c r="I29" s="19" t="n"/>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (97.57), maa://31400 (98.40), maa://28440 (86.25)</t>
+          <t>maa://28432 (97.63), maa://31400 (97.92), maa://28440 (86.25)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4280,7 +4280,7 @@
       </c>
       <c r="P29" s="8" t="inlineStr">
         <is>
-          <t>maa://54169 (96.84)</t>
+          <t>maa://54169 (96.88)</t>
         </is>
       </c>
       <c r="Q29" s="19" t="n"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://42865 (91.37)</t>
+          <t>maa://42865 (91.63)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (94.55), maa://64191 (100.00)</t>
+          <t>maa://45792 (94.74), maa://64191 (100.00)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="L30" s="8" t="inlineStr">
         <is>
-          <t>maa://30442 (97.17)</t>
+          <t>maa://30442 (97.22)</t>
         </is>
       </c>
       <c r="M30" s="19" t="n"/>
@@ -4442,7 +4442,7 @@
       </c>
       <c r="X30" s="8" t="inlineStr">
         <is>
-          <t>maa://39477 (95.74)</t>
+          <t>maa://39477 (95.92)</t>
         </is>
       </c>
       <c r="Y30" s="19" t="n"/>
@@ -4458,7 +4458,7 @@
       </c>
       <c r="AB30" s="8" t="inlineStr">
         <is>
-          <t>maa://42979 (99.49), maa://45822 (100.00), maa://45045 (90.91)</t>
+          <t>maa://42979 (99.51), maa://45822 (100.00), maa://45045 (90.91)</t>
         </is>
       </c>
       <c r="AC30" s="19" t="n"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (97.76), maa://36258 (92.62), maa://43904 (88.89)</t>
+          <t>maa://35926 (97.81), maa://36258 (92.79), maa://43904 (89.47)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4556,7 +4556,7 @@
       </c>
       <c r="T31" s="8" t="inlineStr">
         <is>
-          <t>maa://30711 (97.14), maa://30768 (100.00)</t>
+          <t>maa://30711 (96.36), maa://30768 (100.00)</t>
         </is>
       </c>
       <c r="U31" s="19" t="n"/>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://36667 (99.57), maa://21895 (97.92), maa://22760 (100.00)</t>
+          <t>maa://36667 (99.59), maa://21895 (97.93), maa://22760 (100.00)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4654,7 +4654,7 @@
       </c>
       <c r="L32" s="8" t="inlineStr">
         <is>
-          <t>maa://28065 (96.84)</t>
+          <t>maa://28065 (96.91)</t>
         </is>
       </c>
       <c r="M32" s="19" t="n"/>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (99.26), maa://41108 (87.50), maa://41238 (98.08), maa://45523 (100.00)</t>
+          <t>maa://42859 (99.29), maa://41108 (87.72), maa://41238 (98.08), maa://45523 (100.00)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="X32" s="8" t="inlineStr">
         <is>
-          <t>maa://64104 (96.84)</t>
+          <t>maa://64104 (97.03)</t>
         </is>
       </c>
       <c r="Y32" s="19" t="n"/>
@@ -4734,7 +4734,7 @@
       </c>
       <c r="AF32" s="8" t="inlineStr">
         <is>
-          <t>maa://42408 (94.12)</t>
+          <t>maa://42408 (94.44)</t>
         </is>
       </c>
       <c r="AG32" s="16" t="n"/>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (93.40), *maa://22730 (70.59)</t>
+          <t>maa://21956 (93.76), *maa://22730 (70.59)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="T33" s="8" t="inlineStr">
         <is>
-          <t>maa://45558 (92.00)</t>
+          <t>maa://45558 (92.59)</t>
         </is>
       </c>
       <c r="U33" s="19" t="n"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (99.05), maa://56235 (99.69)</t>
+          <t>maa://48817 (99.09), maa://56235 (99.70)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="T34" s="8" t="inlineStr">
         <is>
-          <t>maa://24526 (96.70)</t>
+          <t>maa://24526 (96.80)</t>
         </is>
       </c>
       <c r="U34" s="19" t="n"/>
@@ -4994,7 +4994,7 @@
       </c>
       <c r="AF34" s="8" t="inlineStr">
         <is>
-          <t>maa://32650 (87.23)</t>
+          <t>maa://32650 (87.50)</t>
         </is>
       </c>
       <c r="AG34" s="16" t="n"/>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
-          <t>maa://41296 (99.16)</t>
+          <t>maa://41296 (99.18)</t>
         </is>
       </c>
       <c r="M35" s="19" t="n"/>
@@ -5076,7 +5076,7 @@
       </c>
       <c r="T35" s="8" t="inlineStr">
         <is>
-          <t>maa://24842 (96.43)</t>
+          <t>maa://24842 (96.47)</t>
         </is>
       </c>
       <c r="U35" s="19" t="n"/>
@@ -5158,7 +5158,7 @@
       </c>
       <c r="H36" s="8" t="inlineStr">
         <is>
-          <t>maa://24375 (93.75)</t>
+          <t>maa://24375 (94.03)</t>
         </is>
       </c>
       <c r="I36" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (99.31), maa://56336 (99.22), maa://47069 (86.49), maa://45789 (100.00)</t>
+          <t>maa://45718 (99.32), maa://56336 (99.26), maa://47069 (87.18), maa://45789 (100.00)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="P37" s="8" t="inlineStr">
         <is>
-          <t>maa://21280 (97.21)</t>
+          <t>maa://21280 (97.31)</t>
         </is>
       </c>
       <c r="Q37" s="19" t="n"/>
@@ -5336,7 +5336,7 @@
       </c>
       <c r="T37" s="8" t="inlineStr">
         <is>
-          <t>**maa://39354 (47.37)</t>
+          <t>**maa://39354 (50.00)</t>
         </is>
       </c>
       <c r="U37" s="19" t="n"/>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="P38" s="8" t="inlineStr">
         <is>
-          <t>*maa://24383 (79.64)</t>
+          <t>maa://24383 (80.35)</t>
         </is>
       </c>
       <c r="Q38" s="19" t="n"/>
@@ -5477,12 +5477,12 @@
       </c>
       <c r="AE38" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF38" s="8" t="inlineStr">
         <is>
-          <t>maa://36697 (95.60)</t>
+          <t>maa://36697 (95.70), maa://68397 (100.00)</t>
         </is>
       </c>
       <c r="AG38" s="16" t="n"/>
@@ -5503,7 +5503,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://25199 (84.44), maa://30434 (95.11), maa://45059 (89.31), maa://44165 (85.71)</t>
+          <t>maa://25199 (84.56), maa://45059 (91.30), maa://30434 (95.11), maa://44165 (85.71)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://47093 (97.85), maa://24709 (93.56)</t>
+          <t>maa://47093 (97.94), maa://24709 (93.56)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (94.76), maa://45790 (87.69)</t>
+          <t>maa://47079 (95.06), maa://45790 (86.96)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5583,7 +5583,7 @@
       </c>
       <c r="AF39" s="8" t="inlineStr">
         <is>
-          <t>maa://62953 (96.91)</t>
+          <t>maa://62953 (96.89)</t>
         </is>
       </c>
       <c r="AG39" s="16" t="n"/>
@@ -5636,7 +5636,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (97.86), maa://21386 (95.92), maa://36664 (89.47), *maa://45550 (72.73)</t>
+          <t>maa://23278 (97.92), maa://21386 (95.92), maa://36664 (89.61), *maa://45550 (72.73)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://65283 (95.97), maa://64205 (93.75)</t>
+          <t>maa://65283 (96.18), maa://64205 (93.75)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="P41" s="8" t="inlineStr">
         <is>
-          <t>maa://43177 (94.74)</t>
+          <t>maa://43177 (94.79)</t>
         </is>
       </c>
       <c r="Q41" s="19" t="n"/>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>*maa://22525 (71.05), maa://21284 (97.12)</t>
+          <t>*maa://22525 (70.74), maa://21284 (97.20)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -5939,7 +5939,7 @@
       </c>
       <c r="P43" s="8" t="inlineStr">
         <is>
-          <t>maa://47403 (86.21)</t>
+          <t>maa://47403 (86.67)</t>
         </is>
       </c>
       <c r="Q43" s="19" t="n"/>
@@ -6008,7 +6008,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (98.14), maa://56386 (99.27), maa://27728 (96.36)</t>
+          <t>maa://29768 (98.17), maa://56386 (99.31), maa://27728 (96.36)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6056,7 +6056,7 @@
       </c>
       <c r="T44" s="8" t="inlineStr">
         <is>
-          <t>maa://39366 (92.50)</t>
+          <t>maa://39366 (92.86)</t>
         </is>
       </c>
       <c r="U44" s="19" t="n"/>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://42459 (98.48), maa://21229 (85.33), maa://30807 (94.57)</t>
+          <t>maa://42459 (98.53), maa://21229 (85.40), maa://30807 (94.57)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6109,7 +6109,7 @@
       </c>
       <c r="P45" s="8" t="inlineStr">
         <is>
-          <t>maa://36237 (81.25)</t>
+          <t>maa://36237 (81.82)</t>
         </is>
       </c>
       <c r="Q45" s="19" t="n"/>
@@ -6125,7 +6125,7 @@
       </c>
       <c r="T45" s="8" t="inlineStr">
         <is>
-          <t>*maa://39364 (64.34)</t>
+          <t>*maa://39364 (66.00)</t>
         </is>
       </c>
       <c r="U45" s="19" t="n"/>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (95.06), maa://43901 (96.23)</t>
+          <t>maa://35931 (95.23), maa://43901 (96.30)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6231,7 +6231,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (97.39), maa://29661 (97.61), maa://56236 (99.74), maa://28038 (84.62)</t>
+          <t>maa://27410 (97.43), maa://29661 (97.62), maa://56236 (99.75), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6263,7 +6263,7 @@
       </c>
       <c r="T47" s="8" t="inlineStr">
         <is>
-          <t>maa://67476 (99.46), maa://68392 (100.00)</t>
+          <t>maa://67476 (99.50), maa://68392 (100.00)</t>
         </is>
       </c>
       <c r="U47" s="19" t="n"/>
@@ -6385,7 +6385,7 @@
       </c>
       <c r="P49" s="8" t="inlineStr">
         <is>
-          <t>*maa://39643 (77.69)</t>
+          <t>*maa://39643 (77.87)</t>
         </is>
       </c>
       <c r="Q49" s="19" t="n"/>
@@ -6401,7 +6401,7 @@
       </c>
       <c r="T49" s="19" t="inlineStr">
         <is>
-          <t>maa://67231 (98.88)</t>
+          <t>maa://67231 (98.94)</t>
         </is>
       </c>
       <c r="U49" s="19" t="n"/>
@@ -6438,7 +6438,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>maa://62852 (92.30)</t>
+          <t>maa://62852 (92.56)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6522,7 +6522,7 @@
       </c>
       <c r="H52" s="8" t="inlineStr">
         <is>
-          <t>maa://24376 (98.88)</t>
+          <t>maa://24376 (98.91)</t>
         </is>
       </c>
       <c r="I52" s="19" t="n"/>
@@ -6538,7 +6538,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (99.23), maa://59378 (93.83), maa://65511 (100.00)</t>
+          <t>maa://59394 (99.27), maa://59378 (93.83), maa://65511 (100.00)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6572,7 +6572,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (97.61)</t>
+          <t>maa://32534 (97.71)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -6656,7 +6656,7 @@
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>maa://32532 (97.54)</t>
+          <t>maa://32532 (97.61)</t>
         </is>
       </c>
       <c r="I55" s="19" t="n"/>
@@ -6708,7 +6708,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://56237 (99.16), maa://25176 (98.77)</t>
+          <t>maa://56237 (99.21), maa://25176 (98.77)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6726,7 +6726,7 @@
       </c>
       <c r="H58" s="8" t="inlineStr">
         <is>
-          <t>*maa://37964 (65.42)</t>
+          <t>*maa://37964 (65.74)</t>
         </is>
       </c>
       <c r="I58" s="19" t="n"/>
@@ -6744,7 +6744,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (98.29), maa://27746 (88.89)</t>
+          <t>maa://31270 (98.33), maa://27746 (88.89)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -6762,7 +6762,7 @@
       </c>
       <c r="H60" s="8" t="inlineStr">
         <is>
-          <t>maa://40438 (90.23)</t>
+          <t>maa://40438 (90.45)</t>
         </is>
       </c>
       <c r="I60" s="19" t="n"/>
@@ -6798,7 +6798,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (97.53), maa://56228 (99.25), maa://43903 (100.00)</t>
+          <t>maa://42981 (97.65), maa://56228 (99.27), maa://43903 (100.00)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6816,7 +6816,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (99.29), *maa://59693 (75.00), maa://59413 (96.43)</t>
+          <t>maa://59534 (99.32), *maa://59693 (75.56), maa://59413 (96.61)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -6834,7 +6834,7 @@
       </c>
       <c r="H64" s="8" t="inlineStr">
         <is>
-          <t>maa://44405 (90.91)</t>
+          <t>maa://44405 (91.18)</t>
         </is>
       </c>
       <c r="I64" s="19" t="n"/>
@@ -7032,7 +7032,7 @@
       </c>
       <c r="H75" s="19" t="inlineStr">
         <is>
-          <t>*maa://67748 (78.57)</t>
+          <t>*maa://67748 (78.95)</t>
         </is>
       </c>
       <c r="I75" s="19" t="n"/>
@@ -7174,7 +7174,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.15 13:24:29</t>
+          <t>更新日期：2025.09.17 13:21:49</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8578,7 +8578,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (73.21), *maa://28758 (71.11), maa://29036 (96.67), *maa://42172 (71.43), maa://65357 (95.65), maa://30285 (100.00)</t>
+          <t>*maa://20849 (73.21), *maa://28758 (71.11), maa://29036 (96.67), *maa://42172 (71.43), maa://65357 (95.83), maa://30285 (100.00)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8686,7 +8686,7 @@
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>maa://20863 (90.54), maa://20832 (99.21), maa://20727 (100.00)</t>
+          <t>maa://20863 (90.57), maa://20832 (99.21), maa://20727 (100.00)</t>
         </is>
       </c>
       <c r="E29" s="14" t="inlineStr">
@@ -8902,7 +8902,7 @@
       </c>
       <c r="D33" s="13" t="inlineStr">
         <is>
-          <t>maa://30500 (98.95), *maa://27290 (72.22), ***maa://42154 (8.33)</t>
+          <t>maa://30500 (98.96), *maa://27290 (72.22), ***maa://42154 (8.33)</t>
         </is>
       </c>
       <c r="E33" s="14" t="inlineStr">
@@ -10414,7 +10414,7 @@
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (99.19), maa://31559 (93.62), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00)</t>
+          <t>maa://20841 (99.20), maa://31559 (93.88), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -10630,7 +10630,7 @@
       </c>
       <c r="D65" s="13" t="inlineStr">
         <is>
-          <t>maa://28567 (97.44), **maa://20947 (45.71), maa://30525 (100.00), maa://38735 (100.00), *maa://28188 (70.00), maa://30524 (100.00)</t>
+          <t>maa://28567 (97.47), **maa://20947 (45.71), maa://30525 (100.00), maa://38735 (100.00), *maa://28188 (70.00), maa://30524 (100.00)</t>
         </is>
       </c>
       <c r="E65" s="14" t="inlineStr">
@@ -10792,7 +10792,7 @@
       </c>
       <c r="D68" s="13" t="inlineStr">
         <is>
-          <t>maa://20976 (97.75), maa://20815 (100.00)</t>
+          <t>maa://20976 (97.78), maa://20815 (100.00)</t>
         </is>
       </c>
       <c r="E68" s="14" t="inlineStr">
@@ -12682,7 +12682,7 @@
       </c>
       <c r="D103" s="13" t="inlineStr">
         <is>
-          <t>*maa://29094 (76.27), maa://28904 (88.37), **maa://20931 (47.22)</t>
+          <t>*maa://29094 (76.27), maa://28904 (88.64), **maa://20931 (47.22)</t>
         </is>
       </c>
       <c r="E103" s="14" t="inlineStr">
@@ -12952,7 +12952,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.69), maa://25018 (96.91), maa://25776 (92.21), maa://28361 (95.35), maa://25772 (94.12), maa://56588 (96.55), maa://45194 (85.71), maa://32653 (81.25), maa://25161 (83.33), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
+          <t>maa://51881 (98.69), maa://25018 (96.92), maa://25776 (92.21), maa://28361 (95.35), maa://25772 (94.12), maa://56588 (96.55), maa://45194 (85.71), maa://32653 (81.25), maa://25161 (83.33), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13006,7 +13006,7 @@
       </c>
       <c r="D109" s="13" t="inlineStr">
         <is>
-          <t>maa://36646 (98.89), maa://25774 (94.59), maa://35996 (97.89), maa://22469 (91.80), maa://30668 (86.67), maa://67286 (100.00)</t>
+          <t>maa://36646 (98.89), maa://25774 (94.59), maa://35996 (97.89), maa://22469 (92.06), maa://30668 (86.67), maa://67286 (100.00)</t>
         </is>
       </c>
       <c r="E109" s="14" t="inlineStr">
@@ -13222,7 +13222,7 @@
       </c>
       <c r="D113" s="13" t="inlineStr">
         <is>
-          <t>maa://20933 (86.52), maa://20822 (100.00)</t>
+          <t>maa://20933 (86.67), maa://20822 (100.00)</t>
         </is>
       </c>
       <c r="E113" s="14" t="inlineStr">
@@ -13276,7 +13276,7 @@
       </c>
       <c r="D114" s="13" t="inlineStr">
         <is>
-          <t>maa://29037 (97.40)</t>
+          <t>maa://29037 (97.44)</t>
         </is>
       </c>
       <c r="E114" s="14" t="inlineStr">
@@ -14842,7 +14842,7 @@
       </c>
       <c r="D143" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (97.77), *maa://23736 (52.44), maa://31185 (91.67), maa://30306 (100.00)</t>
+          <t>maa://28484 (97.78), *maa://23736 (52.44), maa://31185 (91.67), maa://30306 (100.00)</t>
         </is>
       </c>
       <c r="E143" s="14" t="inlineStr">
@@ -15166,7 +15166,7 @@
       </c>
       <c r="D149" s="13" t="inlineStr">
         <is>
-          <t>maa://28828 (88.24), maa://20846 (95.83), *maa://47286 (75.00)</t>
+          <t>maa://28828 (88.24), maa://20846 (96.00), *maa://47286 (75.00)</t>
         </is>
       </c>
       <c r="E149" s="14" t="inlineStr">
@@ -15220,7 +15220,7 @@
       </c>
       <c r="D150" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.80), maa://36641 (98.24), maa://36865 (95.43), maa://44635 (88.07), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (100.00), maa://42918 (100.00), maa://44119 (97.44), maa://37300 (100.00), maa://64408 (92.31), maa://42917 (100.00)</t>
+          <t>maa://40957 (94.80), maa://36641 (98.24), maa://36865 (95.45), maa://44635 (88.07), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (100.00), maa://42918 (100.00), maa://44119 (97.44), maa://37300 (100.00), maa://64408 (92.31), maa://42917 (100.00)</t>
         </is>
       </c>
       <c r="E150" s="14" t="inlineStr">
@@ -16624,7 +16624,7 @@
       </c>
       <c r="D176" s="13" t="inlineStr">
         <is>
-          <t>maa://32418 (99.70), maa://51440 (100.00), maa://63320 (100.00)</t>
+          <t>maa://32418 (99.70), maa://63320 (100.00), maa://51440 (100.00)</t>
         </is>
       </c>
       <c r="E176" s="14" t="inlineStr">
@@ -17812,7 +17812,7 @@
       </c>
       <c r="D198" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.36), maa://35854 (84.75), maa://50388 (98.24), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (94.12)</t>
+          <t>maa://44224 (90.37), maa://35854 (84.75), maa://50388 (98.24), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (94.29)</t>
         </is>
       </c>
       <c r="E198" s="14" t="inlineStr">
@@ -18028,7 +18028,7 @@
       </c>
       <c r="D202" s="13" t="inlineStr">
         <is>
-          <t>maa://42223 (99.25), maa://49077 (94.44), maa://42292 (97.22), maa://42402 (100.00)</t>
+          <t>maa://42223 (99.25), maa://49077 (94.55), maa://42292 (97.22), maa://42402 (100.00)</t>
         </is>
       </c>
       <c r="E202" s="14" t="inlineStr">
@@ -18730,7 +18730,7 @@
       </c>
       <c r="D215" s="13" t="inlineStr">
         <is>
-          <t>maa://64044 (95.24)</t>
+          <t>maa://64044 (95.35)</t>
         </is>
       </c>
       <c r="E215" s="14" t="inlineStr">
@@ -20188,7 +20188,7 @@
       </c>
       <c r="D242" s="13" t="inlineStr">
         <is>
-          <t>*maa://30667 (78.97), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (57.81), maa://39588 (88.14), maa://64079 (81.48), maa://65726 (85.71)</t>
+          <t>*maa://30667 (78.97), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (57.81), maa://39588 (88.14), maa://64079 (81.48), maa://65726 (87.50)</t>
         </is>
       </c>
       <c r="E242" s="14" t="inlineStr">
@@ -20728,7 +20728,7 @@
       </c>
       <c r="D252" s="13" t="inlineStr">
         <is>
-          <t>maa://42287 (91.74), maa://45570 (96.72), maa://60678 (92.86), maa://42225 (100.00)</t>
+          <t>maa://42287 (91.74), maa://45570 (96.72), maa://60678 (93.33), maa://42225 (100.00)</t>
         </is>
       </c>
       <c r="E252" s="14" t="inlineStr">
@@ -20890,7 +20890,7 @@
       </c>
       <c r="D255" s="13" t="inlineStr">
         <is>
-          <t>maa://31559 (93.62), maa://24093 (100.00), maa://20924 (95.24), **maa://49440 (42.86), maa://63591 (100.00)</t>
+          <t>maa://31559 (93.88), maa://24093 (100.00), maa://20924 (95.24), **maa://49440 (42.86), maa://63591 (100.00)</t>
         </is>
       </c>
       <c r="E255" s="14" t="inlineStr">
@@ -21376,7 +21376,7 @@
       </c>
       <c r="D264" s="13" t="inlineStr">
         <is>
-          <t>maa://29027 (98.28)</t>
+          <t>maa://29027 (98.31)</t>
         </is>
       </c>
       <c r="E264" s="14" t="inlineStr">
@@ -23104,7 +23104,7 @@
       </c>
       <c r="D296" s="13" t="inlineStr">
         <is>
-          <t>maa://25774 (94.59), maa://28133 (93.33), maa://22469 (91.80), **maa://39217 (38.89), **maa://31349 (50.00)</t>
+          <t>maa://25774 (94.59), maa://28133 (93.33), maa://22469 (92.06), **maa://39217 (38.89), **maa://31349 (50.00)</t>
         </is>
       </c>
       <c r="E296" s="14" t="inlineStr">
@@ -24724,7 +24724,7 @@
       </c>
       <c r="D326" s="13" t="inlineStr">
         <is>
-          <t>maa://39692 (99.53), maa://39810 (89.66)</t>
+          <t>maa://39692 (99.54), maa://39810 (89.66)</t>
         </is>
       </c>
       <c r="E326" s="14" t="inlineStr">
@@ -24886,7 +24886,7 @@
       </c>
       <c r="D329" s="13" t="inlineStr">
         <is>
-          <t>maa://34867 (96.30), maa://34715 (100.00)</t>
+          <t>maa://34715 (100.00), maa://34867 (96.30)</t>
         </is>
       </c>
       <c r="E329" s="14" t="inlineStr">
@@ -26020,7 +26020,7 @@
       </c>
       <c r="D350" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (97.72), maa://32415 (85.93), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
+          <t>maa://32647 (97.72), maa://32415 (85.21), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E350" s="22" t="inlineStr">
@@ -26560,7 +26560,7 @@
       </c>
       <c r="D360" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.58), maa://49695 (100.00), maa://49758 (98.65), *maa://59402 (58.62), *maa://52357 (73.33), *maa://63091 (62.50)</t>
+          <t>maa://49696 (99.59), maa://49695 (100.00), maa://49758 (98.65), *maa://59402 (56.67), *maa://52357 (73.33), *maa://63091 (66.67)</t>
         </is>
       </c>
       <c r="E360" s="22" t="inlineStr">
@@ -26668,7 +26668,7 @@
       </c>
       <c r="D362" s="22" t="inlineStr">
         <is>
-          <t>maa://42299 (97.73), maa://42224 (85.00)</t>
+          <t>maa://42299 (97.78), maa://42224 (85.00)</t>
         </is>
       </c>
       <c r="E362" s="22" t="inlineStr">
@@ -26722,7 +26722,7 @@
       </c>
       <c r="D363" s="22" t="inlineStr">
         <is>
-          <t>maa://49648 (96.00), maa://49662 (83.33)</t>
+          <t>maa://49648 (96.05), maa://49662 (83.33)</t>
         </is>
       </c>
       <c r="E363" s="22" t="inlineStr">
@@ -28288,7 +28288,7 @@
       </c>
       <c r="D392" s="22" t="inlineStr">
         <is>
-          <t>maa://63890 (97.50), maa://64043 (100.00)</t>
+          <t>maa://63890 (97.56), maa://64043 (100.00)</t>
         </is>
       </c>
       <c r="E392" s="22" t="inlineStr">
@@ -28558,7 +28558,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>maa://51872 (96.60), maa://51876 (99.06), maa://63228 (87.88), maa://51873 (100.00), maa://62047 (92.00)</t>
+          <t>maa://51872 (96.61), maa://51876 (99.06), maa://63228 (87.88), maa://51873 (100.00), maa://62047 (92.00)</t>
         </is>
       </c>
       <c r="E401" t="inlineStr">
@@ -28666,7 +28666,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>maa://62756 (95.68)</t>
+          <t>maa://62756 (95.71)</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">
@@ -28720,7 +28720,7 @@
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>maa://64040 (98.95), maa://52505 (99.14), maa://66377 (92.31), **maa://66376 (33.33)</t>
+          <t>maa://64040 (98.95), maa://52505 (99.15), maa://66377 (92.31), **maa://66376 (33.33)</t>
         </is>
       </c>
       <c r="E407" t="inlineStr">
@@ -28747,7 +28747,7 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>*maa://67090 (78.95)</t>
+          <t>*maa://67090 (80.00)</t>
         </is>
       </c>
       <c r="E408" t="inlineStr">
@@ -28801,7 +28801,7 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>maa://67089 (95.45), maa://67271 (87.50)</t>
+          <t>maa://67089 (96.30), maa://67271 (88.89)</t>
         </is>
       </c>
       <c r="E410" t="inlineStr">
@@ -28828,7 +28828,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>maa://67088 (85.19)</t>
+          <t>maa://67088 (86.21)</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
@@ -28855,7 +28855,7 @@
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>maa://67087 (93.55), maa://67268 (97.83), maa://67269 (90.00), maa://67648 (100.00)</t>
+          <t>maa://67087 (92.65), maa://67268 (96.30), maa://67269 (81.82), maa://67648 (100.00)</t>
         </is>
       </c>
       <c r="E412" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#238)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -712,7 +712,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (98.04), maa://24702 (95.03), maa://36681 (86.21)</t>
+          <t>maa://25390 (98.16), maa://24702 (95.05), maa://36681 (86.21)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://58660 (98.61), maa://39402 (94.50), *maa://34787 (74.75)</t>
+          <t>maa://58660 (98.60), maa://39402 (94.69), *maa://34787 (75.00)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -776,7 +776,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (97.00), maa://66635 (99.79)</t>
+          <t>maa://22742 (97.06), maa://66635 (99.81)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://36684 (98.13), maa://21246 (91.29)</t>
+          <t>maa://36684 (98.24), maa://21246 (91.29)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://59087 (96.72), maa://25251 (91.61)</t>
+          <t>maa://59087 (96.92), maa://25251 (91.61)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -842,7 +842,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (99.29), maa://36987 (97.10), maa://39849 (90.91)</t>
+          <t>maa://40192 (99.26), maa://36987 (97.10), maa://39849 (90.91)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -858,7 +858,7 @@
       </c>
       <c r="H3" s="8" t="inlineStr">
         <is>
-          <t>maa://21247 (99.29)</t>
+          <t>maa://21247 (99.26)</t>
         </is>
       </c>
       <c r="I3" s="19" t="n"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>maa://22880 (89.38), maa://20276 (93.67), maa://22749 (84.00)</t>
+          <t>maa://22880 (89.87), maa://20276 (93.81), maa://22749 (84.00)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -890,7 +890,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (98.22), maa://26254 (98.11), *maa://22738 (80.00)</t>
+          <t>maa://21249 (98.25), maa://26254 (98.11), *maa://22738 (80.00)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://45854 (85.96), maa://60545 (98.46), maa://24617 (91.18)</t>
+          <t>maa://45854 (86.41), maa://60545 (98.56), maa://24617 (91.18)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (91.13), maa://27484 (99.20), maa://27480 (84.91)</t>
+          <t>maa://27396 (91.46), maa://27484 (99.24), maa://27480 (84.91)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://52241 (99.30), maa://24390 (96.72)</t>
+          <t>maa://52241 (99.33), maa://24390 (96.77)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -954,7 +954,7 @@
       </c>
       <c r="AF3" s="8" t="inlineStr">
         <is>
-          <t>maa://21289 (90.62)</t>
+          <t>maa://21289 (91.00)</t>
         </is>
       </c>
       <c r="AG3" s="16" t="n"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (97.80), maa://22499 (89.47), maa://22746 (100.00)</t>
+          <t>maa://24632 (97.89), maa://22499 (90.00), maa://22746 (100.00)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (99.00), maa://50121 (96.30)</t>
+          <t>maa://49983 (99.05), maa://50121 (96.43)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://27295 (97.51), maa://32509 (95.75), maa://31008 (94.67), maa://22754 (88.00)</t>
+          <t>maa://27295 (97.52), maa://32509 (95.98), maa://31008 (94.83), maa://22754 (88.00)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="X4" s="8" t="inlineStr">
         <is>
-          <t>maa://43217 (98.71)</t>
+          <t>maa://43217 (98.79)</t>
         </is>
       </c>
       <c r="Y4" s="19" t="n"/>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>*maa://39394 (58.33), *maa://30062 (61.29), ***maa://26209 (13.04)</t>
+          <t>*maa://39394 (57.14), *maa://30062 (61.29), ***maa://26209 (13.04)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (90.73), maa://54105 (98.38), *maa://22744 (80.00)</t>
+          <t>maa://21245 (90.92), maa://54105 (98.49), *maa://22744 (80.00)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="L5" s="8" t="inlineStr">
         <is>
-          <t>maa://22757 (90.00)</t>
+          <t>maa://22757 (90.29)</t>
         </is>
       </c>
       <c r="M5" s="19" t="n"/>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="P5" s="8" t="inlineStr">
         <is>
-          <t>maa://21919 (98.98), maa://21281 (81.25)</t>
+          <t>maa://21919 (99.00), maa://21281 (81.25)</t>
         </is>
       </c>
       <c r="Q5" s="19" t="n"/>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="X5" s="8" t="inlineStr">
         <is>
-          <t>maa://21290 (99.15)</t>
+          <t>maa://21290 (99.18)</t>
         </is>
       </c>
       <c r="Y5" s="19" t="n"/>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="D6" s="8" t="inlineStr">
         <is>
-          <t>maa://42407 (97.03)</t>
+          <t>maa://42407 (97.10)</t>
         </is>
       </c>
       <c r="E6" s="19" t="n"/>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="H6" s="8" t="inlineStr">
         <is>
-          <t>maa://24370 (97.20)</t>
+          <t>maa://24370 (97.27)</t>
         </is>
       </c>
       <c r="I6" s="19" t="n"/>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="L6" s="8" t="inlineStr">
         <is>
-          <t>maa://24839 (99.33)</t>
+          <t>maa://24839 (99.36)</t>
         </is>
       </c>
       <c r="M6" s="19" t="n"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (98.60), maa://30381 (95.00)</t>
+          <t>maa://31836 (98.68), maa://30381 (95.00)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="X6" s="8" t="inlineStr">
         <is>
-          <t>maa://52754 (95.65)</t>
+          <t>maa://52754 (95.97)</t>
         </is>
       </c>
       <c r="Y6" s="19" t="n"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="AB6" s="8" t="inlineStr">
         <is>
-          <t>maa://22739 (90.59)</t>
+          <t>maa://22739 (90.80)</t>
         </is>
       </c>
       <c r="AC6" s="19" t="n"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="AF6" s="8" t="inlineStr">
         <is>
-          <t>*maa://33152 (78.23), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (78.46), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="16" t="n"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>maa://21955 (97.93)</t>
+          <t>maa://21955 (98.01)</t>
         </is>
       </c>
       <c r="E7" s="19" t="n"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>*maa://22763 (74.14), maa://64972 (95.00)</t>
+          <t>*maa://22763 (74.58), maa://64972 (95.00)</t>
         </is>
       </c>
       <c r="I7" s="19" t="n"/>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (98.49), maa://24957 (94.34)</t>
+          <t>maa://28624 (98.57), maa://24957 (94.44)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="P7" s="8" t="inlineStr">
         <is>
-          <t>maa://22750 (96.45)</t>
+          <t>maa://22750 (96.60)</t>
         </is>
       </c>
       <c r="Q7" s="19" t="n"/>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="T7" s="8" t="inlineStr">
         <is>
-          <t>maa://21291 (93.29)</t>
+          <t>maa://21291 (93.46)</t>
         </is>
       </c>
       <c r="U7" s="19" t="n"/>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (96.98), maa://22758 (81.44)</t>
+          <t>maa://22399 (97.10), maa://22758 (81.63)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="AF7" s="8" t="inlineStr">
         <is>
-          <t>maa://45272 (99.30)</t>
+          <t>maa://45272 (99.35)</t>
         </is>
       </c>
       <c r="AG7" s="16" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.17 13:21:49</t>
+          <t>更新日期：2025.09.20 13:19:46</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (89.73), *maa://39431 (58.33), **maa://37551 (50.00)</t>
+          <t>maa://21476 (89.93), *maa://39431 (58.33), **maa://37551 (50.00)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
-          <t>*maa://24371 (76.88)</t>
+          <t>*maa://24371 (77.78)</t>
         </is>
       </c>
       <c r="I8" s="19" t="n"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (91.26), maa://23252 (91.67), maa://37496 (98.25)</t>
+          <t>maa://32931 (91.25), maa://23252 (91.67), maa://37496 (98.25)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (96.01), maa://67587 (97.31)</t>
+          <t>maa://21411 (96.03), maa://67587 (97.74)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="AB8" s="8" t="inlineStr">
         <is>
-          <t>maa://25389 (94.23)</t>
+          <t>maa://25389 (94.29)</t>
         </is>
       </c>
       <c r="AC8" s="19" t="n"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>maa://24479 (83.52), *maa://21990 (51.72)</t>
+          <t>maa://24479 (83.89), *maa://21990 (51.72)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>maa://22765 (95.10), *maa://21915 (78.57)</t>
+          <t>maa://22765 (95.29), *maa://21915 (78.57)</t>
         </is>
       </c>
       <c r="E9" s="19" t="n"/>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="H9" s="8" t="inlineStr">
         <is>
-          <t>*maa://47450 (75.00), maa://56348 (94.12)</t>
+          <t>*maa://47450 (76.19), maa://56348 (94.44)</t>
         </is>
       </c>
       <c r="I9" s="19" t="n"/>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (95.83), maa://39552 (86.36)</t>
+          <t>maa://22762 (95.96), maa://39552 (86.36)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="T9" s="8" t="inlineStr">
         <is>
-          <t>maa://26222 (99.38)</t>
+          <t>maa://26222 (99.39)</t>
         </is>
       </c>
       <c r="U9" s="19" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://52237 (99.71), maa://26223 (98.31)</t>
+          <t>maa://52237 (99.72), maa://26223 (98.31)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (94.60), maa://40166 (94.66)</t>
+          <t>maa://28711 (94.78), maa://40166 (94.88)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (90.98), maa://66916 (97.51)</t>
+          <t>maa://26206 (91.02), maa://66916 (97.69)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>maa://54000 (91.14)</t>
+          <t>maa://54000 (91.36)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (91.29), *maa://36669 (74.03)</t>
+          <t>maa://28977 (91.60), *maa://36669 (74.03)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (99.12), maa://22755 (91.23), maa://63521 (94.17)</t>
+          <t>maa://27395 (99.17), maa://22755 (91.28), maa://63521 (94.35)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://45828 (99.02), maa://22301 (97.63), maa://22726 (100.00)</t>
+          <t>maa://45828 (99.10), maa://22301 (97.63), maa://22726 (100.00)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>*maa://25021 (55.41), *maa://22733 (67.21), **maa://22761 (33.33)</t>
+          <t>*maa://25021 (56.00), *maa://22733 (65.08), **maa://22761 (33.33)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="D11" s="8" t="inlineStr">
         <is>
-          <t>maa://36707 (99.70)</t>
+          <t>maa://36707 (99.71)</t>
         </is>
       </c>
       <c r="E11" s="19" t="n"/>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="L11" s="8" t="inlineStr">
         <is>
-          <t>maa://21287 (93.04)</t>
+          <t>maa://21287 (93.28)</t>
         </is>
       </c>
       <c r="M11" s="19" t="n"/>
@@ -1940,7 +1940,7 @@
       </c>
       <c r="P11" s="8" t="inlineStr">
         <is>
-          <t>maa://45557 (95.65)</t>
+          <t>maa://45557 (95.74)</t>
         </is>
       </c>
       <c r="Q11" s="19" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (92.90), maa://22501 (99.47), maa://64808 (100.00), maa://45521 (94.92)</t>
+          <t>maa://22747 (93.22), maa://22501 (99.49), maa://64808 (100.00), maa://45521 (94.92)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="X11" s="8" t="inlineStr">
         <is>
-          <t>maa://36713 (99.16)</t>
+          <t>maa://36713 (99.19)</t>
         </is>
       </c>
       <c r="Y11" s="19" t="n"/>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="AB11" s="8" t="inlineStr">
         <is>
-          <t>maa://29912 (99.67), maa://22516 (86.52)</t>
+          <t>maa://29912 (99.68), maa://22516 (86.52)</t>
         </is>
       </c>
       <c r="AC11" s="19" t="n"/>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="AF11" s="8" t="inlineStr">
         <is>
-          <t>maa://31203 (98.46)</t>
+          <t>maa://31203 (98.53)</t>
         </is>
       </c>
       <c r="AG11" s="16" t="n"/>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>maa://36678 (96.43), maa://30766 (91.18)</t>
+          <t>maa://36678 (96.61), maa://30766 (91.18)</t>
         </is>
       </c>
       <c r="E12" s="19" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (93.20), maa://54294 (95.95)</t>
+          <t>maa://21867 (93.23), maa://54294 (96.18)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (97.73), maa://64046 (98.43)</t>
+          <t>maa://63896 (97.84), maa://64046 (98.48)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://37962 (98.59), maa://21485 (80.97), maa://22753 (92.74)</t>
+          <t>maa://37962 (98.67), maa://21485 (81.14), maa://22753 (92.77)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://36677 (99.00), maa://23669 (95.38), maa://39872 (97.80)</t>
+          <t>maa://36677 (99.06), maa://23669 (95.40), maa://39872 (97.85)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>maa://28932 (93.83)</t>
+          <t>maa://28932 (94.10)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (96.29), maa://36673 (93.80), maa://25001 (88.37)</t>
+          <t>maa://24999 (96.38), maa://36673 (93.85), maa://25001 (88.51)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.04), maa://66545 (98.89)</t>
+          <t>*maa://21248 (73.25), maa://66545 (98.92)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (97.22), maa://22583 (87.07)</t>
+          <t>maa://22676 (97.35), maa://22583 (87.07)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="X13" s="8" t="inlineStr">
         <is>
-          <t>maa://34957 (94.06)</t>
+          <t>maa://34957 (94.36)</t>
         </is>
       </c>
       <c r="Y13" s="19" t="n"/>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (93.33)</t>
+          <t>maa://39883 (93.38)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2282,7 +2282,7 @@
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>maa://30764 (94.74)</t>
+          <t>maa://30764 (94.78)</t>
         </is>
       </c>
       <c r="E14" s="19" t="n"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (98.84), maa://26245 (97.00), maa://36682 (98.17), maa://21288 (96.38)</t>
+          <t>maa://39841 (98.92), maa://26245 (97.03), maa://36682 (98.19), maa://21288 (96.40)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2330,7 +2330,7 @@
       </c>
       <c r="P14" s="8" t="inlineStr">
         <is>
-          <t>maa://23250 (99.58), maa://20107 (87.50), maa://22772 (100.00)</t>
+          <t>maa://23250 (99.60), maa://20107 (87.50), maa://22772 (100.00)</t>
         </is>
       </c>
       <c r="Q14" s="19" t="n"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://42751 (98.73), maa://22521 (95.41)</t>
+          <t>maa://42751 (98.80), maa://22521 (95.45)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="X14" s="8" t="inlineStr">
         <is>
-          <t>maa://37468 (97.65)</t>
+          <t>maa://37468 (97.75)</t>
         </is>
       </c>
       <c r="Y14" s="19" t="n"/>
@@ -2378,7 +2378,7 @@
       </c>
       <c r="AB14" s="8" t="inlineStr">
         <is>
-          <t>maa://22764 (98.76)</t>
+          <t>maa://22764 (98.79)</t>
         </is>
       </c>
       <c r="AC14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (85.06), maa://45058 (98.00), maa://22734 (84.85), *maa://36048 (73.68)</t>
+          <t>maa://22743 (85.13), maa://45058 (98.09), maa://22734 (84.85), *maa://36048 (74.29)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (96.44), maa://21478 (90.48)</t>
+          <t>maa://24304 (96.59), maa://21478 (90.48)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="L15" s="8" t="inlineStr">
         <is>
-          <t>*maa://21334 (67.92)</t>
+          <t>*maa://21334 (68.52)</t>
         </is>
       </c>
       <c r="M15" s="19" t="n"/>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="P15" s="8" t="inlineStr">
         <is>
-          <t>maa://24762 (97.41), *maa://22727 (70.00)</t>
+          <t>maa://24762 (97.55), *maa://22727 (70.00)</t>
         </is>
       </c>
       <c r="Q15" s="19" t="n"/>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="T15" s="8" t="inlineStr">
         <is>
-          <t>maa://23892 (97.44)</t>
+          <t>maa://23892 (97.52)</t>
         </is>
       </c>
       <c r="U15" s="19" t="n"/>
@@ -2492,7 +2492,7 @@
       </c>
       <c r="X15" s="8" t="inlineStr">
         <is>
-          <t>maa://38786 (90.91), maa://56102 (100.00)</t>
+          <t>maa://38786 (91.18), maa://56102 (100.00)</t>
         </is>
       </c>
       <c r="Y15" s="19" t="n"/>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://36666 (95.93), maa://21364 (83.33), *maa://22766 (70.50), *maa://68306 (80.00)</t>
+          <t>maa://36666 (96.06), maa://21364 (83.53), *maa://22766 (70.71), maa://68306 (87.50)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://37650 (99.70), maa://21441 (96.62), maa://36679 (94.55)</t>
+          <t>maa://37650 (99.72), maa://21441 (96.62), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2590,7 +2590,7 @@
       </c>
       <c r="P16" s="8" t="inlineStr">
         <is>
-          <t>maa://28504 (95.69)</t>
+          <t>maa://28504 (95.90)</t>
         </is>
       </c>
       <c r="Q16" s="19" t="n"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://36674 (97.69), maa://22729 (95.95), *maa://28648 (77.89)</t>
+          <t>maa://36674 (97.82), maa://22729 (95.99), *maa://28648 (77.89)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2622,7 +2622,7 @@
       </c>
       <c r="X16" s="8" t="inlineStr">
         <is>
-          <t>maa://28501 (99.18), maa://28051 (96.88)</t>
+          <t>maa://28501 (99.22), maa://28051 (96.88)</t>
         </is>
       </c>
       <c r="Y16" s="19" t="n"/>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="AB16" s="8" t="inlineStr">
         <is>
-          <t>maa://26228 (97.65)</t>
+          <t>maa://26228 (97.73)</t>
         </is>
       </c>
       <c r="AC16" s="19" t="n"/>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>maa://23911 (89.76), maa://27755 (93.69), maa://67613 (99.09)</t>
+          <t>maa://23911 (90.00), maa://27755 (93.69), maa://67613 (99.21)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://39599 (97.90), maa://22430 (90.17)</t>
+          <t>maa://39599 (98.02), maa://22430 (90.17)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="L17" s="8" t="inlineStr">
         <is>
-          <t>maa://21679 (87.23)</t>
+          <t>maa://21679 (87.50)</t>
         </is>
       </c>
       <c r="M17" s="19" t="n"/>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (82.50), maa://56238 (98.13)</t>
+          <t>maa://23890 (82.50), maa://56238 (98.23)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="T17" s="8" t="inlineStr">
         <is>
-          <t>*maa://42324 (68.29)</t>
+          <t>*maa://42324 (68.67)</t>
         </is>
       </c>
       <c r="U17" s="19" t="n"/>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="AF17" s="8" t="inlineStr">
         <is>
-          <t>maa://50136 (98.82)</t>
+          <t>maa://50136 (98.86)</t>
         </is>
       </c>
       <c r="AG17" s="16" t="n"/>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>maa://24570 (98.16)</t>
+          <t>maa://24570 (98.21)</t>
         </is>
       </c>
       <c r="E18" s="19" t="n"/>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="H18" s="8" t="inlineStr">
         <is>
-          <t>maa://24421 (94.85)</t>
+          <t>maa://24421 (94.99)</t>
         </is>
       </c>
       <c r="I18" s="19" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://52226 (99.64), maa://22466 (92.79)</t>
+          <t>maa://52226 (99.67), maa://22466 (92.79)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), maa://54153 (99.59), maa://24380 (100.00)</t>
+          <t>maa://24379 (100.00), maa://54153 (99.61), maa://24380 (100.00)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (98.56), maa://22741 (91.67)</t>
+          <t>maa://21917 (98.61), maa://22741 (91.67)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="AB18" s="8" t="inlineStr">
         <is>
-          <t>maa://24393 (98.86)</t>
+          <t>maa://24393 (98.91)</t>
         </is>
       </c>
       <c r="AC18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://47854 (92.37)</t>
+          <t>maa://47854 (92.25)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -2932,7 +2932,7 @@
       </c>
       <c r="D19" s="8" t="inlineStr">
         <is>
-          <t>maa://62850 (99.23)</t>
+          <t>maa://62850 (99.26)</t>
         </is>
       </c>
       <c r="E19" s="19" t="n"/>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="L19" s="8" t="inlineStr">
         <is>
-          <t>maa://39347 (97.78), maa://56392 (100.00)</t>
+          <t>maa://39347 (97.92), maa://56392 (100.00)</t>
         </is>
       </c>
       <c r="M19" s="19" t="n"/>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="T19" s="8" t="inlineStr">
         <is>
-          <t>maa://24386 (99.61)</t>
+          <t>maa://24386 (99.63)</t>
         </is>
       </c>
       <c r="U19" s="19" t="n"/>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (84.24), *maa://36668 (68.75)</t>
+          <t>maa://30709 (84.74), *maa://36668 (68.75)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3044,7 +3044,7 @@
       </c>
       <c r="AF19" s="8" t="inlineStr">
         <is>
-          <t>*maa://21663 (64.71), maa://52239 (85.19)</t>
+          <t>*maa://21663 (65.12), maa://52239 (86.21)</t>
         </is>
       </c>
       <c r="AG19" s="16" t="n"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://25198 (97.48), maa://36680 (98.90), maa://21432 (91.38)</t>
+          <t>maa://25198 (97.52), maa://36680 (98.96), maa://21432 (91.45)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3078,7 +3078,7 @@
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>maa://22864 (95.48)</t>
+          <t>maa://22864 (95.71)</t>
         </is>
       </c>
       <c r="I20" s="19" t="n"/>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (94.78)</t>
+          <t>maa://41331 (94.93)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="P20" s="8" t="inlineStr">
         <is>
-          <t>maa://37442 (98.31)</t>
+          <t>maa://37442 (98.41)</t>
         </is>
       </c>
       <c r="Q20" s="19" t="n"/>
@@ -3126,7 +3126,7 @@
       </c>
       <c r="T20" s="8" t="inlineStr">
         <is>
-          <t>maa://29113 (93.15)</t>
+          <t>maa://29113 (93.24)</t>
         </is>
       </c>
       <c r="U20" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (96.00), maa://56241 (98.25), maa://49976 (88.35)</t>
+          <t>maa://50085 (96.18), maa://56241 (98.33), maa://49976 (88.35)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>maa://21261 (98.96)</t>
+          <t>maa://21261 (98.99)</t>
         </is>
       </c>
       <c r="E21" s="19" t="n"/>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="H21" s="8" t="inlineStr">
         <is>
-          <t>maa://24372 (98.71)</t>
+          <t>maa://24372 (98.76)</t>
         </is>
       </c>
       <c r="I21" s="19" t="n"/>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="L21" s="8" t="inlineStr">
         <is>
-          <t>maa://31731 (96.12)</t>
+          <t>maa://31731 (96.33)</t>
         </is>
       </c>
       <c r="M21" s="19" t="n"/>
@@ -3240,7 +3240,7 @@
       </c>
       <c r="P21" s="8" t="inlineStr">
         <is>
-          <t>maa://24381 (83.87)</t>
+          <t>maa://24381 (84.38)</t>
         </is>
       </c>
       <c r="Q21" s="19" t="n"/>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (98.10), maa://20110 (87.01)</t>
+          <t>maa://34946 (98.16), maa://20110 (87.01)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="AB21" s="8" t="inlineStr">
         <is>
-          <t>maa://21443 (86.18), maa://52223 (80.58)</t>
+          <t>maa://21443 (86.44), maa://52223 (81.50)</t>
         </is>
       </c>
       <c r="AC21" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22432 (93.19), maa://22524 (82.75), maa://64221 (97.45)</t>
+          <t>maa://22432 (93.43), maa://22524 (82.87), maa://64221 (97.62)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>maa://25236 (99.05)</t>
+          <t>maa://25236 (99.12)</t>
         </is>
       </c>
       <c r="I22" s="19" t="n"/>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>maa://27127 (82.11), *maa://22751 (70.93), maa://66865 (99.30)</t>
+          <t>maa://27127 (82.59), *maa://22751 (70.93), maa://66865 (99.34)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3386,7 +3386,7 @@
       </c>
       <c r="T22" s="8" t="inlineStr">
         <is>
-          <t>maa://38495 (83.33)</t>
+          <t>maa://38495 (84.44)</t>
         </is>
       </c>
       <c r="U22" s="19" t="n"/>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://37649 (93.47), maa://21282 (98.89)</t>
+          <t>maa://37649 (93.84), maa://21282 (98.89)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="AB22" s="8" t="inlineStr">
         <is>
-          <t>maa://23656 (99.44)</t>
+          <t>maa://23656 (99.46)</t>
         </is>
       </c>
       <c r="AC22" s="19" t="n"/>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="AF22" s="8" t="inlineStr">
         <is>
-          <t>maa://29658 (96.81)</t>
+          <t>maa://29658 (96.97)</t>
         </is>
       </c>
       <c r="AG22" s="16" t="n"/>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>***maa://28036 (29.21), *maa://41753 (62.90)</t>
+          <t>*maa://41753 (62.90), ***maa://28036 (30.00)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (98.47), maa://39875 (95.58)</t>
+          <t>maa://39756 (98.53), maa://39875 (95.65)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (96.67), maa://29748 (81.72), maa://37566 (80.33)</t>
+          <t>maa://30587 (96.79), maa://29748 (81.82), *maa://37566 (78.12)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="T23" s="8" t="inlineStr">
         <is>
-          <t>maa://31212 (95.00), maa://24387 (84.44), maa://67084 (85.71)</t>
+          <t>maa://31212 (95.19), maa://24387 (84.44), maa://67084 (85.71)</t>
         </is>
       </c>
       <c r="U23" s="19" t="n"/>
@@ -3532,7 +3532,7 @@
       </c>
       <c r="X23" s="8" t="inlineStr">
         <is>
-          <t>*maa://28503 (60.40)</t>
+          <t>*maa://28503 (60.67)</t>
         </is>
       </c>
       <c r="Y23" s="19" t="n"/>
@@ -3548,7 +3548,7 @@
       </c>
       <c r="AB23" s="8" t="inlineStr">
         <is>
-          <t>maa://29652 (96.25)</t>
+          <t>maa://29652 (96.34)</t>
         </is>
       </c>
       <c r="AC23" s="19" t="n"/>
@@ -3564,7 +3564,7 @@
       </c>
       <c r="AF23" s="8" t="inlineStr">
         <is>
-          <t>maa://31489 (98.00)</t>
+          <t>maa://31489 (98.08)</t>
         </is>
       </c>
       <c r="AG23" s="16" t="n"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (84.62), maa://46650 (89.63)</t>
+          <t>maa://24368 (84.76), maa://46650 (89.80)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (95.79), maa://23504 (94.02), *maa://25141 (79.33), maa://52227 (97.95), *maa://36663 (79.25)</t>
+          <t>maa://29988 (95.95), maa://23504 (94.02), *maa://25141 (79.33), maa://52227 (98.01), *maa://36663 (79.25)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="AB24" s="8" t="inlineStr">
         <is>
-          <t>maa://39349 (96.97)</t>
+          <t>maa://39349 (97.06)</t>
         </is>
       </c>
       <c r="AC24" s="19" t="n"/>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://64165 (99.16), maa://22523 (80.09), maa://29910 (94.20), maa://45831 (93.55)</t>
+          <t>maa://64165 (99.21), maa://22523 (80.09), maa://29910 (94.20), maa://45831 (93.55)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (96.34), maa://63016 (99.01)</t>
+          <t>maa://29753 (96.40), maa://63016 (99.04)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>*maa://29063 (75.24), *maa://25311 (70.71), maa://45047 (87.14)</t>
+          <t>*maa://29063 (75.15), *maa://25311 (70.71), maa://45047 (87.50)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3744,7 +3744,7 @@
       </c>
       <c r="L25" s="8" t="inlineStr">
         <is>
-          <t>maa://24378 (93.59), maa://68415 (100.00)</t>
+          <t>maa://24378 (93.75), maa://68415 (100.00)</t>
         </is>
       </c>
       <c r="M25" s="19" t="n"/>
@@ -3760,7 +3760,7 @@
       </c>
       <c r="P25" s="8" t="inlineStr">
         <is>
-          <t>maa://24382 (95.65)</t>
+          <t>maa://24382 (95.92)</t>
         </is>
       </c>
       <c r="Q25" s="19" t="n"/>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="T25" s="8" t="inlineStr">
         <is>
-          <t>maa://20109 (96.20), maa://22545 (100.00)</t>
+          <t>maa://20109 (96.32), maa://22545 (100.00)</t>
         </is>
       </c>
       <c r="U25" s="19" t="n"/>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="X25" s="8" t="inlineStr">
         <is>
-          <t>maa://29890 (90.68)</t>
+          <t>maa://29890 (90.83)</t>
         </is>
       </c>
       <c r="Y25" s="19" t="n"/>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (92.89), *maa://24516 (79.80), maa://26001 (83.33), maa://68311 (100.00)</t>
+          <t>maa://31215 (93.08), *maa://24516 (79.80), maa://26001 (83.33), maa://68311 (100.00)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (97.89), maa://36676 (99.82), maa://24621 (96.84), maa://22771 (88.24), maa://37772 (83.33)</t>
+          <t>maa://20108 (97.93), maa://36676 (99.83), maa://24621 (96.84), maa://22771 (88.24), maa://37772 (83.33)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://56374 (100.00), maa://41802 (95.65)</t>
+          <t>maa://56374 (100.00), maa://41802 (95.74)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3858,7 +3858,7 @@
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
-          <t>maa://56240 (96.07), maa://24913 (92.17)</t>
+          <t>maa://56240 (96.26), maa://24913 (92.17)</t>
         </is>
       </c>
       <c r="I26" s="19" t="n"/>
@@ -3922,7 +3922,7 @@
       </c>
       <c r="X26" s="8" t="inlineStr">
         <is>
-          <t>maa://24389 (98.11)</t>
+          <t>maa://24389 (98.25)</t>
         </is>
       </c>
       <c r="Y26" s="19" t="n"/>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="AB26" s="8" t="inlineStr">
         <is>
-          <t>maa://42235 (98.31)</t>
+          <t>maa://42235 (98.36)</t>
         </is>
       </c>
       <c r="AC26" s="19" t="n"/>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>maa://39601 (90.00), maa://34494 (97.50)</t>
+          <t>maa://39601 (89.47), maa://34494 (96.43)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4020,7 +4020,7 @@
       </c>
       <c r="P27" s="8" t="inlineStr">
         <is>
-          <t>maa://56400 (92.86)</t>
+          <t>maa://56400 (93.33)</t>
         </is>
       </c>
       <c r="Q27" s="19" t="n"/>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="T27" s="8" t="inlineStr">
         <is>
-          <t>maa://30624 (89.16)</t>
+          <t>maa://30624 (89.41)</t>
         </is>
       </c>
       <c r="U27" s="19" t="n"/>
@@ -4084,7 +4084,7 @@
       </c>
       <c r="AF27" s="8" t="inlineStr">
         <is>
-          <t>maa://24023 (97.54)</t>
+          <t>maa://24023 (97.60)</t>
         </is>
       </c>
       <c r="AG27" s="16" t="n"/>
@@ -4102,7 +4102,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (95.58), maa://25725 (84.80)</t>
+          <t>maa://24465 (95.69), maa://25725 (84.92)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="L28" s="8" t="inlineStr">
         <is>
-          <t>maa://30770 (89.41)</t>
+          <t>maa://30770 (89.53)</t>
         </is>
       </c>
       <c r="M28" s="19" t="n"/>
@@ -4166,7 +4166,7 @@
       </c>
       <c r="T28" s="8" t="inlineStr">
         <is>
-          <t>maa://29765 (92.57), maa://23263 (96.12)</t>
+          <t>maa://29765 (92.90), maa://23263 (96.18)</t>
         </is>
       </c>
       <c r="U28" s="19" t="n"/>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (97.09), maa://41749 (97.03)</t>
+          <t>maa://39929 (97.15), maa://41749 (97.11)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (93.85), maa://65700 (98.59)</t>
+          <t>maa://36660 (94.03), maa://65700 (98.68)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4232,7 +4232,7 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>maa://31694 (99.26)</t>
+          <t>maa://31694 (99.28)</t>
         </is>
       </c>
       <c r="E29" s="19" t="n"/>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (97.63), maa://31400 (97.92), maa://28440 (86.25)</t>
+          <t>maa://28432 (97.70), maa://31400 (97.99), maa://28440 (86.25)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4280,7 +4280,7 @@
       </c>
       <c r="P29" s="8" t="inlineStr">
         <is>
-          <t>maa://54169 (96.88)</t>
+          <t>maa://54169 (97.03)</t>
         </is>
       </c>
       <c r="Q29" s="19" t="n"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://42865 (91.63)</t>
+          <t>maa://42865 (91.87)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (94.74), maa://64191 (100.00)</t>
+          <t>maa://45792 (95.00), maa://64191 (100.00)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="L30" s="8" t="inlineStr">
         <is>
-          <t>maa://30442 (97.22)</t>
+          <t>maa://30442 (97.30)</t>
         </is>
       </c>
       <c r="M30" s="19" t="n"/>
@@ -4410,7 +4410,7 @@
       </c>
       <c r="P30" s="8" t="inlineStr">
         <is>
-          <t>maa://21442 (99.55), maa://66611 (100.00), maa://68394 (100.00)</t>
+          <t>maa://21442 (99.56), maa://66611 (100.00), maa://68394 (100.00)</t>
         </is>
       </c>
       <c r="Q30" s="19" t="n"/>
@@ -4442,7 +4442,7 @@
       </c>
       <c r="X30" s="8" t="inlineStr">
         <is>
-          <t>maa://39477 (95.92)</t>
+          <t>maa://39477 (96.23)</t>
         </is>
       </c>
       <c r="Y30" s="19" t="n"/>
@@ -4458,7 +4458,7 @@
       </c>
       <c r="AB30" s="8" t="inlineStr">
         <is>
-          <t>maa://42979 (99.51), maa://45822 (100.00), maa://45045 (90.91)</t>
+          <t>maa://42979 (99.52), maa://45822 (100.00), maa://45045 (90.91)</t>
         </is>
       </c>
       <c r="AC30" s="19" t="n"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (97.81), maa://36258 (92.79), maa://43904 (89.47)</t>
+          <t>maa://35926 (97.87), maa://36258 (92.88), maa://43904 (89.47)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4556,7 +4556,7 @@
       </c>
       <c r="T31" s="8" t="inlineStr">
         <is>
-          <t>maa://30711 (96.36), maa://30768 (100.00)</t>
+          <t>maa://30711 (96.46), maa://30768 (100.00)</t>
         </is>
       </c>
       <c r="U31" s="19" t="n"/>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://36667 (99.59), maa://21895 (97.93), maa://22760 (100.00)</t>
+          <t>maa://36667 (99.61), maa://21895 (97.95), maa://22760 (100.00)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4654,7 +4654,7 @@
       </c>
       <c r="L32" s="8" t="inlineStr">
         <is>
-          <t>maa://28065 (96.91)</t>
+          <t>maa://28065 (97.00)</t>
         </is>
       </c>
       <c r="M32" s="19" t="n"/>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (99.29), maa://41108 (87.72), maa://41238 (98.08), maa://45523 (100.00)</t>
+          <t>maa://42859 (99.32), maa://41108 (87.72), maa://41238 (98.10), maa://45523 (100.00)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="X32" s="8" t="inlineStr">
         <is>
-          <t>maa://64104 (97.03)</t>
+          <t>maa://64104 (97.14)</t>
         </is>
       </c>
       <c r="Y32" s="19" t="n"/>
@@ -4734,7 +4734,7 @@
       </c>
       <c r="AF32" s="8" t="inlineStr">
         <is>
-          <t>maa://42408 (94.44)</t>
+          <t>maa://42408 (94.59)</t>
         </is>
       </c>
       <c r="AG32" s="16" t="n"/>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (93.76), *maa://22730 (70.59)</t>
+          <t>maa://21956 (94.07), *maa://22730 (70.59)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="T33" s="8" t="inlineStr">
         <is>
-          <t>maa://45558 (92.59)</t>
+          <t>maa://45558 (92.86)</t>
         </is>
       </c>
       <c r="U33" s="19" t="n"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (99.09), maa://56235 (99.70)</t>
+          <t>maa://48817 (99.13), maa://56235 (99.71)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="T34" s="8" t="inlineStr">
         <is>
-          <t>maa://24526 (96.80)</t>
+          <t>maa://24526 (96.92)</t>
         </is>
       </c>
       <c r="U34" s="19" t="n"/>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="AB34" s="8" t="inlineStr">
         <is>
-          <t>maa://64329 (96.77)</t>
+          <t>maa://64329 (97.30)</t>
         </is>
       </c>
       <c r="AC34" s="19" t="n"/>
@@ -4994,7 +4994,7 @@
       </c>
       <c r="AF34" s="8" t="inlineStr">
         <is>
-          <t>maa://32650 (87.50)</t>
+          <t>maa://32650 (87.76)</t>
         </is>
       </c>
       <c r="AG34" s="16" t="n"/>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
-          <t>maa://41296 (99.18)</t>
+          <t>maa://41296 (99.21)</t>
         </is>
       </c>
       <c r="M35" s="19" t="n"/>
@@ -5076,7 +5076,7 @@
       </c>
       <c r="T35" s="8" t="inlineStr">
         <is>
-          <t>maa://24842 (96.47)</t>
+          <t>maa://24842 (96.51)</t>
         </is>
       </c>
       <c r="U35" s="19" t="n"/>
@@ -5124,7 +5124,7 @@
       </c>
       <c r="AF35" s="8" t="inlineStr">
         <is>
-          <t>maa://39479 (95.83)</t>
+          <t>maa://39479 (96.00)</t>
         </is>
       </c>
       <c r="AG35" s="16" t="n"/>
@@ -5158,7 +5158,7 @@
       </c>
       <c r="H36" s="8" t="inlineStr">
         <is>
-          <t>maa://24375 (94.03)</t>
+          <t>maa://24375 (94.12)</t>
         </is>
       </c>
       <c r="I36" s="19" t="n"/>
@@ -5206,7 +5206,7 @@
       </c>
       <c r="T36" s="8" t="inlineStr">
         <is>
-          <t>maa://27613 (99.50)</t>
+          <t>maa://27613 (99.52)</t>
         </is>
       </c>
       <c r="U36" s="19" t="n"/>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="AB36" s="19" t="inlineStr">
         <is>
-          <t>maa://64106 (96.15)</t>
+          <t>maa://64106 (96.77)</t>
         </is>
       </c>
       <c r="AC36" s="19" t="n"/>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="H37" s="8" t="inlineStr">
         <is>
-          <t>*maa://24374 (55.93)</t>
+          <t>*maa://24374 (56.67)</t>
         </is>
       </c>
       <c r="I37" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (99.32), maa://56336 (99.26), maa://47069 (87.18), maa://45789 (100.00)</t>
+          <t>maa://45718 (99.17), maa://56336 (99.28), maa://47069 (87.50), maa://45789 (100.00)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="P37" s="8" t="inlineStr">
         <is>
-          <t>maa://21280 (97.31)</t>
+          <t>maa://21280 (97.44)</t>
         </is>
       </c>
       <c r="Q37" s="19" t="n"/>
@@ -5336,7 +5336,7 @@
       </c>
       <c r="T37" s="8" t="inlineStr">
         <is>
-          <t>**maa://39354 (50.00)</t>
+          <t>**maa://39354 (47.62)</t>
         </is>
       </c>
       <c r="U37" s="19" t="n"/>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="P38" s="8" t="inlineStr">
         <is>
-          <t>maa://24383 (80.35)</t>
+          <t>maa://24383 (80.79)</t>
         </is>
       </c>
       <c r="Q38" s="19" t="n"/>
@@ -5450,7 +5450,7 @@
       </c>
       <c r="T38" s="8" t="inlineStr">
         <is>
-          <t>maa://30713 (98.18)</t>
+          <t>maa://30713 (98.25)</t>
         </is>
       </c>
       <c r="U38" s="19" t="n"/>
@@ -5482,7 +5482,7 @@
       </c>
       <c r="AF38" s="8" t="inlineStr">
         <is>
-          <t>maa://36697 (95.70), maa://68397 (100.00)</t>
+          <t>maa://36697 (95.76), maa://68397 (98.39)</t>
         </is>
       </c>
       <c r="AG38" s="16" t="n"/>
@@ -5503,7 +5503,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://25199 (84.56), maa://45059 (91.30), maa://30434 (95.11), maa://44165 (85.71)</t>
+          <t>maa://25199 (84.67), maa://45059 (92.19), maa://30434 (95.19), maa://44165 (85.71)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://47093 (97.94), maa://24709 (93.56)</t>
+          <t>maa://47093 (98.03), maa://24709 (93.70)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (95.06), maa://45790 (86.96)</t>
+          <t>maa://47079 (95.22), maa://45790 (87.14)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5636,7 +5636,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (97.92), maa://21386 (95.92), maa://36664 (89.61), *maa://45550 (72.73)</t>
+          <t>maa://23278 (97.99), maa://21386 (95.92), maa://36664 (89.61), *maa://45550 (72.73)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://65283 (96.18), maa://64205 (93.75)</t>
+          <t>maa://65283 (96.47), maa://64205 (93.75)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5705,7 +5705,7 @@
       </c>
       <c r="H41" s="8" t="inlineStr">
         <is>
-          <t>maa://24466 (92.54)</t>
+          <t>maa://24466 (92.65)</t>
         </is>
       </c>
       <c r="I41" s="19" t="n"/>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="P41" s="8" t="inlineStr">
         <is>
-          <t>maa://43177 (94.79)</t>
+          <t>maa://43177 (95.24)</t>
         </is>
       </c>
       <c r="Q41" s="19" t="n"/>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>*maa://22525 (70.74), maa://21284 (97.20)</t>
+          <t>*maa://22525 (70.87), maa://21284 (97.37)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -5939,7 +5939,7 @@
       </c>
       <c r="P43" s="8" t="inlineStr">
         <is>
-          <t>maa://47403 (86.67)</t>
+          <t>maa://47403 (87.10)</t>
         </is>
       </c>
       <c r="Q43" s="19" t="n"/>
@@ -6008,7 +6008,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (98.17), maa://56386 (99.31), maa://27728 (96.36)</t>
+          <t>maa://29768 (98.19), maa://56386 (99.34), maa://27728 (96.36)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6056,7 +6056,7 @@
       </c>
       <c r="T44" s="8" t="inlineStr">
         <is>
-          <t>maa://39366 (92.86)</t>
+          <t>maa://39366 (93.02)</t>
         </is>
       </c>
       <c r="U44" s="19" t="n"/>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://42459 (98.53), maa://21229 (85.40), maa://30807 (94.57)</t>
+          <t>maa://42459 (98.61), maa://21229 (85.46), maa://30807 (94.62)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6109,7 +6109,7 @@
       </c>
       <c r="P45" s="8" t="inlineStr">
         <is>
-          <t>maa://36237 (81.82)</t>
+          <t>maa://36237 (82.86)</t>
         </is>
       </c>
       <c r="Q45" s="19" t="n"/>
@@ -6125,7 +6125,7 @@
       </c>
       <c r="T45" s="8" t="inlineStr">
         <is>
-          <t>*maa://39364 (66.00)</t>
+          <t>*maa://39364 (66.67)</t>
         </is>
       </c>
       <c r="U45" s="19" t="n"/>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (95.23), maa://43901 (96.30)</t>
+          <t>maa://35931 (95.44), maa://43901 (96.40)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6231,7 +6231,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (97.43), maa://29661 (97.62), maa://56236 (99.75), maa://28038 (84.62)</t>
+          <t>maa://27410 (97.47), maa://29661 (97.17), maa://56236 (99.76), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6263,7 +6263,7 @@
       </c>
       <c r="T47" s="8" t="inlineStr">
         <is>
-          <t>maa://67476 (99.50), maa://68392 (100.00)</t>
+          <t>maa://67476 (99.53), maa://68392 (100.00)</t>
         </is>
       </c>
       <c r="U47" s="19" t="n"/>
@@ -6385,7 +6385,7 @@
       </c>
       <c r="P49" s="8" t="inlineStr">
         <is>
-          <t>*maa://39643 (77.87)</t>
+          <t>*maa://39643 (78.46)</t>
         </is>
       </c>
       <c r="Q49" s="19" t="n"/>
@@ -6401,7 +6401,7 @@
       </c>
       <c r="T49" s="19" t="inlineStr">
         <is>
-          <t>maa://67231 (98.94)</t>
+          <t>maa://67231 (99.01)</t>
         </is>
       </c>
       <c r="U49" s="19" t="n"/>
@@ -6438,7 +6438,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>maa://62852 (92.56)</t>
+          <t>maa://62852 (92.73)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6472,7 +6472,7 @@
       </c>
       <c r="H51" s="8" t="inlineStr">
         <is>
-          <t>maa://30769 (88.00)</t>
+          <t>maa://30769 (88.89)</t>
         </is>
       </c>
       <c r="I51" s="19" t="n"/>
@@ -6522,7 +6522,7 @@
       </c>
       <c r="H52" s="8" t="inlineStr">
         <is>
-          <t>maa://24376 (98.91)</t>
+          <t>maa://24376 (98.95)</t>
         </is>
       </c>
       <c r="I52" s="19" t="n"/>
@@ -6538,7 +6538,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (99.27), maa://59378 (93.83), maa://65511 (100.00)</t>
+          <t>maa://59394 (99.31), maa://59378 (93.83), maa://65511 (100.00)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6572,7 +6572,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (97.71)</t>
+          <t>maa://32534 (97.80)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -6656,7 +6656,7 @@
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>maa://32532 (97.61)</t>
+          <t>maa://32532 (97.68)</t>
         </is>
       </c>
       <c r="I55" s="19" t="n"/>
@@ -6708,7 +6708,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://56237 (99.21), maa://25176 (98.77)</t>
+          <t>maa://56237 (99.26), maa://25176 (98.77)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6726,7 +6726,7 @@
       </c>
       <c r="H58" s="8" t="inlineStr">
         <is>
-          <t>*maa://37964 (65.74)</t>
+          <t>*maa://37964 (66.67)</t>
         </is>
       </c>
       <c r="I58" s="19" t="n"/>
@@ -6744,7 +6744,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (98.33), maa://27746 (88.89)</t>
+          <t>maa://31270 (98.40), maa://27746 (88.95)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -6762,7 +6762,7 @@
       </c>
       <c r="H60" s="8" t="inlineStr">
         <is>
-          <t>maa://40438 (90.45)</t>
+          <t>maa://40438 (90.91)</t>
         </is>
       </c>
       <c r="I60" s="19" t="n"/>
@@ -6798,7 +6798,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (97.65), maa://56228 (99.27), maa://43903 (100.00)</t>
+          <t>maa://42981 (97.73), maa://56228 (99.30), maa://43903 (100.00)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6816,7 +6816,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (99.32), *maa://59693 (75.56), maa://59413 (96.61)</t>
+          <t>maa://59534 (99.35), *maa://59693 (76.09), maa://59413 (96.83)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -6834,7 +6834,7 @@
       </c>
       <c r="H64" s="8" t="inlineStr">
         <is>
-          <t>maa://44405 (91.18)</t>
+          <t>maa://44405 (91.30)</t>
         </is>
       </c>
       <c r="I64" s="19" t="n"/>
@@ -7032,7 +7032,7 @@
       </c>
       <c r="H75" s="19" t="inlineStr">
         <is>
-          <t>*maa://67748 (78.95)</t>
+          <t>maa://67748 (82.61)</t>
         </is>
       </c>
       <c r="I75" s="19" t="n"/>
@@ -7174,7 +7174,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.17 13:21:49</t>
+          <t>更新日期：2025.09.20 13:19:46</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -7552,7 +7552,7 @@
       </c>
       <c r="D8" s="13" t="inlineStr">
         <is>
-          <t>maa://20980 (100.00)</t>
+          <t>maa://20980 (94.12)</t>
         </is>
       </c>
       <c r="E8" s="14" t="inlineStr">
@@ -8362,7 +8362,7 @@
       </c>
       <c r="D23" s="13" t="inlineStr">
         <is>
-          <t>maa://20876 (96.30), maa://63498 (100.00)</t>
+          <t>maa://20876 (96.36), maa://63498 (100.00)</t>
         </is>
       </c>
       <c r="E23" s="14" t="inlineStr">
@@ -8578,7 +8578,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (73.21), *maa://28758 (71.11), maa://29036 (96.67), *maa://42172 (71.43), maa://65357 (95.83), maa://30285 (100.00)</t>
+          <t>*maa://20849 (73.21), *maa://28758 (71.11), maa://29036 (96.67), *maa://42172 (71.43), maa://65357 (96.00), maa://30285 (100.00)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8686,7 +8686,7 @@
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>maa://20863 (90.57), maa://20832 (99.21), maa://20727 (100.00)</t>
+          <t>maa://20863 (90.60), maa://20832 (99.21), maa://20727 (100.00)</t>
         </is>
       </c>
       <c r="E29" s="14" t="inlineStr">
@@ -8848,7 +8848,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (90.12), maa://36866 (96.97), maa://62759 (100.00), maa://45572 (88.24), maa://27794 (100.00), maa://20960 (100.00), maa://20843 (100.00), **maa://24483 (50.00), maa://20862 (83.33), *maa://20893 (77.78)</t>
+          <t>maa://36644 (90.16), maa://36866 (96.97), maa://62759 (100.00), maa://45572 (88.24), maa://27794 (100.00), maa://20960 (100.00), maa://20843 (100.00), **maa://24483 (50.00), maa://20862 (83.33), *maa://20893 (77.78)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -9334,7 +9334,7 @@
       </c>
       <c r="D41" s="13" t="inlineStr">
         <is>
-          <t>maa://20892 (82.18)</t>
+          <t>maa://20892 (82.35)</t>
         </is>
       </c>
       <c r="E41" s="14" t="inlineStr">
@@ -10144,7 +10144,7 @@
       </c>
       <c r="D56" s="13" t="inlineStr">
         <is>
-          <t>maa://44235 (98.40), maa://45604 (100.00), maa://20961 (100.00), maa://44220 (100.00), maa://20910 (100.00)</t>
+          <t>maa://44235 (98.41), maa://45604 (100.00), maa://20961 (100.00), maa://44220 (100.00), maa://20910 (100.00)</t>
         </is>
       </c>
       <c r="E56" s="14" t="inlineStr">
@@ -10414,7 +10414,7 @@
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (99.20), maa://31559 (93.88), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00)</t>
+          <t>maa://20841 (99.21), maa://31559 (93.88), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -10792,7 +10792,7 @@
       </c>
       <c r="D68" s="13" t="inlineStr">
         <is>
-          <t>maa://20976 (97.78), maa://20815 (100.00)</t>
+          <t>maa://20976 (97.79), maa://20815 (100.00)</t>
         </is>
       </c>
       <c r="E68" s="14" t="inlineStr">
@@ -11008,7 +11008,7 @@
       </c>
       <c r="D72" s="13" t="inlineStr">
         <is>
-          <t>maa://36643 (98.43), maa://36864 (98.10), maa://39140 (100.00), maa://66335 (100.00)</t>
+          <t>maa://36643 (98.44), maa://36864 (98.10), maa://39140 (100.00), maa://66335 (100.00)</t>
         </is>
       </c>
       <c r="E72" s="14" t="inlineStr">
@@ -11278,7 +11278,7 @@
       </c>
       <c r="D77" s="13" t="inlineStr">
         <is>
-          <t>maa://20958 (94.87), ***maa://39769 (20.00)</t>
+          <t>maa://20958 (95.00), ***maa://39769 (20.00)</t>
         </is>
       </c>
       <c r="E77" s="14" t="inlineStr">
@@ -12466,7 +12466,7 @@
       </c>
       <c r="D99" s="13" t="inlineStr">
         <is>
-          <t>maa://20929 (92.59)</t>
+          <t>maa://20929 (92.86)</t>
         </is>
       </c>
       <c r="E99" s="14" t="inlineStr">
@@ -12628,7 +12628,7 @@
       </c>
       <c r="D102" s="13" t="inlineStr">
         <is>
-          <t>maa://40517 (90.32), *maa://39240 (56.25)</t>
+          <t>maa://40517 (90.62), *maa://39240 (56.25)</t>
         </is>
       </c>
       <c r="E102" s="14" t="inlineStr">
@@ -12682,7 +12682,7 @@
       </c>
       <c r="D103" s="13" t="inlineStr">
         <is>
-          <t>*maa://29094 (76.27), maa://28904 (88.64), **maa://20931 (47.22)</t>
+          <t>*maa://29094 (76.27), maa://28904 (88.64), **maa://20931 (48.65)</t>
         </is>
       </c>
       <c r="E103" s="14" t="inlineStr">
@@ -12952,7 +12952,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.69), maa://25018 (96.92), maa://25776 (92.21), maa://28361 (95.35), maa://25772 (94.12), maa://56588 (96.55), maa://45194 (85.71), maa://32653 (81.25), maa://25161 (83.33), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
+          <t>maa://51881 (98.70), maa://25018 (96.92), maa://25776 (92.21), maa://28361 (95.35), maa://25772 (94.12), maa://56588 (96.55), maa://45194 (85.71), maa://32653 (81.25), maa://25161 (83.33), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13222,7 +13222,7 @@
       </c>
       <c r="D113" s="13" t="inlineStr">
         <is>
-          <t>maa://20933 (86.67), maa://20822 (100.00)</t>
+          <t>maa://20933 (86.81), maa://20822 (100.00)</t>
         </is>
       </c>
       <c r="E113" s="14" t="inlineStr">
@@ -13492,7 +13492,7 @@
       </c>
       <c r="D118" s="13" t="inlineStr">
         <is>
-          <t>maa://31560 (92.86), maa://20940 (86.67)</t>
+          <t>maa://31560 (92.86), maa://20940 (87.50)</t>
         </is>
       </c>
       <c r="E118" s="14" t="inlineStr">
@@ -14194,7 +14194,7 @@
       </c>
       <c r="D131" s="13" t="inlineStr">
         <is>
-          <t>maa://21422 (99.22)</t>
+          <t>maa://21422 (99.23)</t>
         </is>
       </c>
       <c r="E131" s="14" t="inlineStr">
@@ -14680,7 +14680,7 @@
       </c>
       <c r="D140" s="13" t="inlineStr">
         <is>
-          <t>maa://45258 (90.48), **maa://30679 (50.00)</t>
+          <t>maa://45258 (90.91), **maa://30679 (50.00)</t>
         </is>
       </c>
       <c r="E140" s="14" t="inlineStr">
@@ -14842,7 +14842,7 @@
       </c>
       <c r="D143" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (97.78), *maa://23736 (52.44), maa://31185 (91.67), maa://30306 (100.00)</t>
+          <t>maa://28484 (97.79), *maa://23736 (52.44), maa://31185 (91.67), maa://30306 (100.00)</t>
         </is>
       </c>
       <c r="E143" s="14" t="inlineStr">
@@ -15166,7 +15166,7 @@
       </c>
       <c r="D149" s="13" t="inlineStr">
         <is>
-          <t>maa://28828 (88.24), maa://20846 (96.00), *maa://47286 (75.00)</t>
+          <t>maa://28828 (88.24), maa://20846 (96.15), *maa://47286 (75.00)</t>
         </is>
       </c>
       <c r="E149" s="14" t="inlineStr">
@@ -15220,7 +15220,7 @@
       </c>
       <c r="D150" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.80), maa://36641 (98.24), maa://36865 (95.45), maa://44635 (88.07), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (100.00), maa://42918 (100.00), maa://44119 (97.44), maa://37300 (100.00), maa://64408 (92.31), maa://42917 (100.00)</t>
+          <t>maa://40957 (94.82), maa://36641 (98.24), maa://36865 (95.45), maa://44635 (88.07), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (100.00), maa://42918 (100.00), maa://44119 (97.44), maa://64408 (92.86), maa://37300 (100.00), maa://42917 (100.00)</t>
         </is>
       </c>
       <c r="E150" s="14" t="inlineStr">
@@ -15274,7 +15274,7 @@
       </c>
       <c r="D151" s="13" t="inlineStr">
         <is>
-          <t>maa://51549 (96.77), maa://51923 (96.30), maa://67508 (100.00)</t>
+          <t>maa://51549 (96.83), maa://51923 (96.30), maa://67508 (100.00)</t>
         </is>
       </c>
       <c r="E151" s="14" t="inlineStr">
@@ -15760,7 +15760,7 @@
       </c>
       <c r="D160" s="13" t="inlineStr">
         <is>
-          <t>maa://44232 (98.47), maa://45603 (90.62), *maa://63114 (66.67), *maa://65963 (75.00)</t>
+          <t>maa://44232 (98.47), maa://45603 (90.62), *maa://65963 (75.00), *maa://63114 (66.67)</t>
         </is>
       </c>
       <c r="E160" s="14" t="inlineStr">
@@ -17434,7 +17434,7 @@
       </c>
       <c r="D191" s="13" t="inlineStr">
         <is>
-          <t>maa://34866 (93.75), maa://34714 (96.77)</t>
+          <t>maa://34866 (93.75), maa://34714 (96.88)</t>
         </is>
       </c>
       <c r="E191" s="14" t="inlineStr">
@@ -17812,7 +17812,7 @@
       </c>
       <c r="D198" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.37), maa://35854 (84.75), maa://50388 (98.24), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (94.29)</t>
+          <t>maa://44224 (90.43), maa://35854 (84.75), maa://50388 (98.24), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (94.29)</t>
         </is>
       </c>
       <c r="E198" s="14" t="inlineStr">
@@ -18568,7 +18568,7 @@
       </c>
       <c r="D212" s="13" t="inlineStr">
         <is>
-          <t>maa://20956 (96.14), *maa://20830 (80.00), maa://44703 (92.31)</t>
+          <t>maa://20956 (96.15), *maa://20830 (80.00), maa://44703 (92.31)</t>
         </is>
       </c>
       <c r="E212" s="14" t="inlineStr">
@@ -18676,7 +18676,7 @@
       </c>
       <c r="D214" s="13" t="inlineStr">
         <is>
-          <t>maa://39238 (99.10)</t>
+          <t>maa://39238 (99.11)</t>
         </is>
       </c>
       <c r="E214" s="14" t="inlineStr">
@@ -18730,7 +18730,7 @@
       </c>
       <c r="D215" s="13" t="inlineStr">
         <is>
-          <t>maa://64044 (95.35)</t>
+          <t>maa://64044 (95.83)</t>
         </is>
       </c>
       <c r="E215" s="14" t="inlineStr">
@@ -19756,7 +19756,7 @@
       </c>
       <c r="D234" s="13" t="inlineStr">
         <is>
-          <t>*maa://48263 (76.92)</t>
+          <t>*maa://48263 (75.00)</t>
         </is>
       </c>
       <c r="E234" s="14" t="inlineStr">
@@ -20183,12 +20183,12 @@
       </c>
       <c r="C242" s="12" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D242" s="13" t="inlineStr">
         <is>
-          <t>*maa://30667 (78.97), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (57.81), maa://39588 (88.14), maa://64079 (81.48), maa://65726 (87.50)</t>
+          <t>*maa://30667 (78.85), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (57.81), maa://39588 (86.67), *maa://64079 (78.57), maa://65726 (87.50), maa://68226 (100.00)</t>
         </is>
       </c>
       <c r="E242" s="14" t="inlineStr">
@@ -20242,7 +20242,7 @@
       </c>
       <c r="D243" s="13" t="inlineStr">
         <is>
-          <t>maa://62759 (100.00), *maa://62764 (80.00)</t>
+          <t>maa://62759 (100.00), maa://62764 (83.33)</t>
         </is>
       </c>
       <c r="E243" s="14" t="inlineStr">
@@ -21376,7 +21376,7 @@
       </c>
       <c r="D264" s="13" t="inlineStr">
         <is>
-          <t>maa://29027 (98.31)</t>
+          <t>maa://29027 (98.33)</t>
         </is>
       </c>
       <c r="E264" s="14" t="inlineStr">
@@ -21700,7 +21700,7 @@
       </c>
       <c r="D270" s="13" t="inlineStr">
         <is>
-          <t>maa://49643 (90.48)</t>
+          <t>maa://49643 (91.11)</t>
         </is>
       </c>
       <c r="E270" s="14" t="inlineStr">
@@ -21862,7 +21862,7 @@
       </c>
       <c r="D273" s="13" t="inlineStr">
         <is>
-          <t>maa://25769 (97.52)</t>
+          <t>maa://25769 (96.91)</t>
         </is>
       </c>
       <c r="E273" s="14" t="inlineStr">
@@ -22024,7 +22024,7 @@
       </c>
       <c r="D276" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.69), maa://51630 (96.19), maa://56588 (96.55), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (41.67), *maa://66758 (77.78)</t>
+          <t>maa://51881 (98.70), maa://51630 (96.26), maa://56588 (96.55), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (41.67), *maa://66758 (77.78)</t>
         </is>
       </c>
       <c r="E276" s="14" t="inlineStr">
@@ -22780,7 +22780,7 @@
       </c>
       <c r="D290" s="13" t="inlineStr">
         <is>
-          <t>maa://20899 (90.00), maa://46332 (96.30), ***maa://44744 (25.00)</t>
+          <t>maa://20899 (90.00), maa://46332 (92.86), ***maa://44744 (25.00)</t>
         </is>
       </c>
       <c r="E290" s="14" t="inlineStr">
@@ -23698,7 +23698,7 @@
       </c>
       <c r="D307" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (98.47), maa://49642 (97.58), maa://49660 (93.62), maa://50517 (85.71)</t>
+          <t>maa://50280 (98.47), maa://49642 (97.62), maa://49660 (93.62), maa://50517 (85.71)</t>
         </is>
       </c>
       <c r="E307" s="14" t="inlineStr">
@@ -24076,7 +24076,7 @@
       </c>
       <c r="D314" s="13" t="inlineStr">
         <is>
-          <t>maa://53348 (86.21)</t>
+          <t>maa://53348 (86.67)</t>
         </is>
       </c>
       <c r="E314" s="14" t="inlineStr">
@@ -24400,7 +24400,7 @@
       </c>
       <c r="D320" s="13" t="inlineStr">
         <is>
-          <t>*maa://62755 (68.75), maa://62761 (90.00)</t>
+          <t>*maa://62755 (70.59), maa://62761 (90.91)</t>
         </is>
       </c>
       <c r="E320" s="14" t="inlineStr">
@@ -24724,7 +24724,7 @@
       </c>
       <c r="D326" s="13" t="inlineStr">
         <is>
-          <t>maa://39692 (99.54), maa://39810 (89.66)</t>
+          <t>maa://39692 (99.54), maa://39810 (90.00)</t>
         </is>
       </c>
       <c r="E326" s="14" t="inlineStr">
@@ -24886,7 +24886,7 @@
       </c>
       <c r="D329" s="13" t="inlineStr">
         <is>
-          <t>maa://34715 (100.00), maa://34867 (96.30)</t>
+          <t>maa://34715 (94.74), maa://34867 (96.30)</t>
         </is>
       </c>
       <c r="E329" s="14" t="inlineStr">
@@ -25372,7 +25372,7 @@
       </c>
       <c r="D338" s="22" t="inlineStr">
         <is>
-          <t>maa://44234 (99.17)</t>
+          <t>maa://44234 (99.18)</t>
         </is>
       </c>
       <c r="E338" s="22" t="inlineStr">
@@ -25642,7 +25642,7 @@
       </c>
       <c r="D343" s="22" t="inlineStr">
         <is>
-          <t>maa://30671 (81.41), maa://30669 (99.30), maa://37275 (81.40), *maa://32410 (61.54), maa://41605 (100.00)</t>
+          <t>maa://30671 (81.50), maa://30669 (99.31), maa://37275 (81.40), *maa://32410 (61.54), maa://41605 (100.00)</t>
         </is>
       </c>
       <c r="E343" s="22" t="inlineStr">
@@ -26020,7 +26020,7 @@
       </c>
       <c r="D350" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (97.72), maa://32415 (85.21), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
+          <t>maa://32647 (97.72), maa://32415 (84.80), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E350" s="22" t="inlineStr">
@@ -26506,7 +26506,7 @@
       </c>
       <c r="D359" s="22" t="inlineStr">
         <is>
-          <t>maa://36868 (99.54), maa://35996 (97.89), maa://47349 (97.40), **maa://39217 (38.89)</t>
+          <t>maa://36868 (99.54), maa://35996 (97.89), maa://47349 (97.44), **maa://39217 (38.89)</t>
         </is>
       </c>
       <c r="E359" s="22" t="inlineStr">
@@ -26560,7 +26560,7 @@
       </c>
       <c r="D360" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.59), maa://49695 (100.00), maa://49758 (98.65), *maa://59402 (56.67), *maa://52357 (73.33), *maa://63091 (66.67)</t>
+          <t>maa://49696 (99.59), maa://49695 (100.00), maa://49758 (98.67), *maa://59402 (56.67), *maa://52357 (73.33), *maa://63091 (72.73)</t>
         </is>
       </c>
       <c r="E360" s="22" t="inlineStr">
@@ -26668,7 +26668,7 @@
       </c>
       <c r="D362" s="22" t="inlineStr">
         <is>
-          <t>maa://42299 (97.78), maa://42224 (85.00)</t>
+          <t>maa://42299 (97.83), maa://42224 (85.00)</t>
         </is>
       </c>
       <c r="E362" s="22" t="inlineStr">
@@ -26722,7 +26722,7 @@
       </c>
       <c r="D363" s="22" t="inlineStr">
         <is>
-          <t>maa://49648 (96.05), maa://49662 (83.33)</t>
+          <t>maa://49648 (96.10), maa://49662 (83.87)</t>
         </is>
       </c>
       <c r="E363" s="22" t="inlineStr">
@@ -27046,7 +27046,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (94.80), maa://48026 (94.62), maa://44635 (88.07), maa://41035 (93.51), *maa://60251 (76.47), maa://44660 (92.68), maa://41128 (84.21)</t>
+          <t>maa://40957 (94.82), maa://48026 (94.66), maa://44635 (88.07), maa://41035 (93.51), *maa://60251 (76.47), maa://44660 (92.68), maa://41128 (84.21)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -27532,7 +27532,7 @@
       </c>
       <c r="D378" s="22" t="inlineStr">
         <is>
-          <t>maa://41110 (98.51), maa://45605 (90.00)</t>
+          <t>maa://41110 (98.52), maa://45605 (90.00)</t>
         </is>
       </c>
       <c r="E378" s="22" t="inlineStr">
@@ -27964,7 +27964,7 @@
       </c>
       <c r="D386" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (81.29), maa://44745 (98.01), **maa://49516 (39.29), *maa://45952 (57.14), ***maa://46851 (12.50), *maa://44896 (77.78)</t>
+          <t>maa://42970 (81.00), maa://44745 (98.01), **maa://49516 (39.29), *maa://45952 (57.14), ***maa://46851 (12.50), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E386" s="22" t="inlineStr">
@@ -28288,7 +28288,7 @@
       </c>
       <c r="D392" s="22" t="inlineStr">
         <is>
-          <t>maa://63890 (97.56), maa://64043 (100.00)</t>
+          <t>maa://63890 (97.73), maa://64043 (100.00)</t>
         </is>
       </c>
       <c r="E392" s="22" t="inlineStr">
@@ -28450,7 +28450,7 @@
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>maa://51907 (100.00), maa://51908 (100.00)</t>
+          <t>**maa://51907 (50.00), maa://51908 (100.00)</t>
         </is>
       </c>
       <c r="E397" t="inlineStr">
@@ -28558,7 +28558,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>maa://51872 (96.61), maa://51876 (99.06), maa://63228 (87.88), maa://51873 (100.00), maa://62047 (92.00)</t>
+          <t>maa://51872 (96.62), maa://51876 (99.06), maa://63228 (88.24), maa://51873 (100.00), maa://62047 (92.00)</t>
         </is>
       </c>
       <c r="E401" t="inlineStr">
@@ -28666,7 +28666,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>maa://62756 (95.71)</t>
+          <t>maa://62756 (95.74)</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">
@@ -28720,7 +28720,7 @@
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>maa://64040 (98.95), maa://52505 (99.15), maa://66377 (92.31), **maa://66376 (33.33)</t>
+          <t>maa://64040 (98.97), maa://52505 (98.40), maa://66377 (92.31), ***maa://66376 (25.00)</t>
         </is>
       </c>
       <c r="E407" t="inlineStr">
@@ -28747,7 +28747,7 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>*maa://67090 (80.00)</t>
+          <t>maa://67090 (85.19)</t>
         </is>
       </c>
       <c r="E408" t="inlineStr">
@@ -28774,7 +28774,7 @@
       </c>
       <c r="D409" t="inlineStr">
         <is>
-          <t>maa://67388 (100.00)</t>
+          <t>maa://67388 (90.62)</t>
         </is>
       </c>
       <c r="E409" t="inlineStr">
@@ -28801,7 +28801,7 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>maa://67089 (96.30), maa://67271 (88.89)</t>
+          <t>maa://67089 (97.14), maa://67271 (92.31)</t>
         </is>
       </c>
       <c r="E410" t="inlineStr">
@@ -28828,7 +28828,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>maa://67088 (86.21)</t>
+          <t>maa://67088 (88.64)</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
@@ -28855,7 +28855,7 @@
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>maa://67087 (92.65), maa://67268 (96.30), maa://67269 (81.82), maa://67648 (100.00)</t>
+          <t>maa://67087 (93.67), maa://67268 (95.59), maa://67269 (84.62), maa://67648 (100.00)</t>
         </is>
       </c>
       <c r="E412" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#239)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -712,7 +712,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (98.16), maa://24702 (95.05), maa://36681 (86.21)</t>
+          <t>maa://25390 (98.18), maa://24702 (95.06), maa://36681 (86.21)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://58660 (98.60), maa://39402 (94.69), *maa://34787 (75.00)</t>
+          <t>maa://58660 (98.70), maa://39402 (94.93), *maa://34787 (75.00)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -776,7 +776,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (97.06), maa://66635 (99.81)</t>
+          <t>maa://22742 (97.15), maa://66635 (99.65)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://36684 (98.24), maa://21246 (91.29)</t>
+          <t>maa://36684 (98.18), maa://21246 (91.32)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://59087 (96.92), maa://25251 (91.61)</t>
+          <t>maa://59087 (97.09), maa://25251 (91.61)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -842,7 +842,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (99.26), maa://36987 (97.10), maa://39849 (90.91)</t>
+          <t>maa://40192 (99.30), maa://36987 (97.10), maa://39849 (90.91)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -858,7 +858,7 @@
       </c>
       <c r="H3" s="8" t="inlineStr">
         <is>
-          <t>maa://21247 (99.26)</t>
+          <t>maa://21247 (99.31)</t>
         </is>
       </c>
       <c r="I3" s="19" t="n"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>maa://22880 (89.87), maa://20276 (93.81), maa://22749 (84.00)</t>
+          <t>maa://22880 (90.34), maa://20276 (93.91), maa://22749 (84.00)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -890,7 +890,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (98.25), maa://26254 (98.11), *maa://22738 (80.00)</t>
+          <t>maa://21249 (98.28), maa://26254 (98.11), *maa://22738 (80.00)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://45854 (86.41), maa://60545 (98.56), maa://24617 (91.18)</t>
+          <t>maa://60545 (98.65), maa://45854 (86.98), maa://24617 (91.18)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (91.46), maa://27484 (99.24), maa://27480 (84.91)</t>
+          <t>maa://27396 (91.71), maa://27484 (99.14), maa://27480 (84.91)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://52241 (99.33), maa://24390 (96.77)</t>
+          <t>maa://52241 (99.35), maa://24390 (96.77)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -954,7 +954,7 @@
       </c>
       <c r="AF3" s="8" t="inlineStr">
         <is>
-          <t>maa://21289 (91.00)</t>
+          <t>maa://21289 (91.35)</t>
         </is>
       </c>
       <c r="AG3" s="16" t="n"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (97.89), maa://22499 (90.00), maa://22746 (100.00)</t>
+          <t>maa://24632 (97.99), maa://22499 (90.00), maa://22746 (100.00)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (99.05), maa://50121 (96.43)</t>
+          <t>maa://49983 (99.10), maa://50121 (96.52)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://27295 (97.52), maa://32509 (95.98), maa://31008 (94.83), maa://22754 (88.00)</t>
+          <t>maa://27295 (97.56), maa://32509 (96.14), maa://31008 (94.89), maa://22754 (88.16)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>*maa://39394 (57.14), *maa://30062 (61.29), ***maa://26209 (13.04)</t>
+          <t>*maa://39394 (58.00), *maa://30062 (61.29), ***maa://26209 (13.04)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (90.92), maa://54105 (98.49), *maa://22744 (80.00)</t>
+          <t>maa://21245 (90.91), maa://54105 (98.28), *maa://22744 (80.00)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="L5" s="8" t="inlineStr">
         <is>
-          <t>maa://22757 (90.29)</t>
+          <t>maa://22757 (90.57)</t>
         </is>
       </c>
       <c r="M5" s="19" t="n"/>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="P5" s="8" t="inlineStr">
         <is>
-          <t>maa://21919 (99.00), maa://21281 (81.25)</t>
+          <t>maa://21919 (99.02), maa://21281 (81.25)</t>
         </is>
       </c>
       <c r="Q5" s="19" t="n"/>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="X5" s="8" t="inlineStr">
         <is>
-          <t>maa://21290 (99.18)</t>
+          <t>maa://21290 (99.20)</t>
         </is>
       </c>
       <c r="Y5" s="19" t="n"/>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="D6" s="8" t="inlineStr">
         <is>
-          <t>maa://42407 (97.10)</t>
+          <t>maa://42407 (97.22)</t>
         </is>
       </c>
       <c r="E6" s="19" t="n"/>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="H6" s="8" t="inlineStr">
         <is>
-          <t>maa://24370 (97.27)</t>
+          <t>maa://24370 (97.32)</t>
         </is>
       </c>
       <c r="I6" s="19" t="n"/>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="L6" s="8" t="inlineStr">
         <is>
-          <t>maa://24839 (99.36)</t>
+          <t>maa://24839 (99.38)</t>
         </is>
       </c>
       <c r="M6" s="19" t="n"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (98.68), maa://30381 (95.00)</t>
+          <t>maa://31836 (98.73), maa://30381 (95.00)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="T6" s="8" t="inlineStr">
         <is>
-          <t>*maa://37411 (77.78)</t>
+          <t>*maa://37411 (76.32)</t>
         </is>
       </c>
       <c r="U6" s="19" t="n"/>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="X6" s="8" t="inlineStr">
         <is>
-          <t>maa://52754 (95.97)</t>
+          <t>maa://52754 (96.10)</t>
         </is>
       </c>
       <c r="Y6" s="19" t="n"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="AB6" s="8" t="inlineStr">
         <is>
-          <t>maa://22739 (90.80)</t>
+          <t>maa://22739 (89.13)</t>
         </is>
       </c>
       <c r="AC6" s="19" t="n"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="AF6" s="8" t="inlineStr">
         <is>
-          <t>*maa://33152 (78.46), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (79.56), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="16" t="n"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>maa://21955 (98.01)</t>
+          <t>maa://21955 (98.04)</t>
         </is>
       </c>
       <c r="E7" s="19" t="n"/>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (98.57), maa://24957 (94.44)</t>
+          <t>maa://28624 (98.65), maa://24957 (94.44)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="P7" s="8" t="inlineStr">
         <is>
-          <t>maa://22750 (96.60)</t>
+          <t>maa://22750 (96.73)</t>
         </is>
       </c>
       <c r="Q7" s="19" t="n"/>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="T7" s="8" t="inlineStr">
         <is>
-          <t>maa://21291 (93.46)</t>
+          <t>maa://21291 (93.67)</t>
         </is>
       </c>
       <c r="U7" s="19" t="n"/>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (97.10), maa://22758 (81.63)</t>
+          <t>maa://22399 (96.98), maa://22758 (81.82)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="AF7" s="8" t="inlineStr">
         <is>
-          <t>maa://45272 (99.35)</t>
+          <t>maa://45272 (99.38)</t>
         </is>
       </c>
       <c r="AG7" s="16" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.20 13:19:46</t>
+          <t>更新日期：2025.09.23 13:20:11</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (89.93), *maa://39431 (58.33), **maa://37551 (50.00)</t>
+          <t>maa://21476 (89.68), *maa://39431 (58.33), **maa://37551 (50.00)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
-          <t>*maa://24371 (77.78)</t>
+          <t>*maa://24371 (78.14)</t>
         </is>
       </c>
       <c r="I8" s="19" t="n"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (91.25), maa://23252 (91.67), maa://37496 (98.25)</t>
+          <t>maa://32931 (91.55), maa://23252 (91.67), maa://37496 (98.28)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (96.03), maa://67587 (97.74)</t>
+          <t>maa://21411 (95.98), maa://67587 (98.11)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="AB8" s="8" t="inlineStr">
         <is>
-          <t>maa://25389 (94.29)</t>
+          <t>maa://25389 (94.39)</t>
         </is>
       </c>
       <c r="AC8" s="19" t="n"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>maa://24479 (83.89), *maa://21990 (51.72)</t>
+          <t>maa://24479 (84.07), *maa://21990 (51.72)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>maa://22765 (95.29), *maa://21915 (78.57)</t>
+          <t>maa://22765 (95.47), *maa://21915 (78.57)</t>
         </is>
       </c>
       <c r="E9" s="19" t="n"/>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="H9" s="8" t="inlineStr">
         <is>
-          <t>*maa://47450 (76.19), maa://56348 (94.44)</t>
+          <t>*maa://47450 (77.27), maa://56348 (95.00)</t>
         </is>
       </c>
       <c r="I9" s="19" t="n"/>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (95.96), maa://39552 (86.36)</t>
+          <t>maa://22762 (96.12), maa://39552 (86.67)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="T9" s="8" t="inlineStr">
         <is>
-          <t>maa://26222 (99.39)</t>
+          <t>maa://26222 (99.42)</t>
         </is>
       </c>
       <c r="U9" s="19" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://52237 (99.72), maa://26223 (98.31)</t>
+          <t>maa://52237 (99.74), maa://26223 (98.31)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (94.78), maa://40166 (94.88)</t>
+          <t>maa://28711 (94.96), maa://40166 (94.93)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (91.02), maa://66916 (97.69)</t>
+          <t>maa://26206 (91.09), maa://66916 (97.83)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>maa://54000 (91.36)</t>
+          <t>maa://54000 (91.67)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="H10" s="8" t="inlineStr">
         <is>
-          <t>maa://32651 (95.00)</t>
+          <t>maa://32651 (95.12)</t>
         </is>
       </c>
       <c r="I10" s="19" t="n"/>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (91.60), *maa://36669 (74.03)</t>
+          <t>maa://28977 (91.51), *maa://36669 (74.03)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (99.17), maa://22755 (91.28), maa://63521 (94.35)</t>
+          <t>maa://27395 (99.19), maa://22755 (91.38), maa://63521 (94.49)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://45828 (99.10), maa://22301 (97.63), maa://22726 (100.00)</t>
+          <t>maa://45828 (99.16), maa://22301 (97.64), maa://22726 (100.00)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>*maa://25021 (56.00), *maa://22733 (65.08), **maa://22761 (33.33)</t>
+          <t>*maa://25021 (56.77), *maa://22733 (65.62), **maa://22761 (33.33)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="D11" s="8" t="inlineStr">
         <is>
-          <t>maa://36707 (99.71)</t>
+          <t>maa://36707 (99.72)</t>
         </is>
       </c>
       <c r="E11" s="19" t="n"/>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="L11" s="8" t="inlineStr">
         <is>
-          <t>maa://21287 (93.28)</t>
+          <t>maa://21287 (93.55)</t>
         </is>
       </c>
       <c r="M11" s="19" t="n"/>
@@ -1940,7 +1940,7 @@
       </c>
       <c r="P11" s="8" t="inlineStr">
         <is>
-          <t>maa://45557 (95.74)</t>
+          <t>maa://45557 (95.83)</t>
         </is>
       </c>
       <c r="Q11" s="19" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (93.22), maa://22501 (99.49), maa://64808 (100.00), maa://45521 (94.92)</t>
+          <t>maa://22747 (93.18), maa://22501 (99.51), maa://64808 (100.00), maa://45521 (95.00)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="X11" s="8" t="inlineStr">
         <is>
-          <t>maa://36713 (99.19)</t>
+          <t>maa://36713 (99.22)</t>
         </is>
       </c>
       <c r="Y11" s="19" t="n"/>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="AB11" s="8" t="inlineStr">
         <is>
-          <t>maa://29912 (99.68), maa://22516 (86.52)</t>
+          <t>maa://29912 (99.69), maa://22516 (86.52)</t>
         </is>
       </c>
       <c r="AC11" s="19" t="n"/>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="AF11" s="8" t="inlineStr">
         <is>
-          <t>maa://31203 (98.53)</t>
+          <t>maa://31203 (98.59)</t>
         </is>
       </c>
       <c r="AG11" s="16" t="n"/>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>maa://36678 (96.61), maa://30766 (91.18)</t>
+          <t>maa://36678 (96.83), maa://30766 (91.18)</t>
         </is>
       </c>
       <c r="E12" s="19" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (93.23), maa://54294 (96.18)</t>
+          <t>maa://21867 (93.33), maa://54294 (96.30)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (97.84), maa://64046 (98.48)</t>
+          <t>maa://63896 (97.86), maa://64046 (98.51)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://37962 (98.67), maa://21485 (81.14), maa://22753 (92.77)</t>
+          <t>maa://37962 (98.73), maa://21485 (81.62), maa://22753 (92.80)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://36677 (99.06), maa://23669 (95.40), maa://39872 (97.85)</t>
+          <t>maa://36677 (99.11), maa://23669 (95.40), maa://39872 (98.08)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>maa://28932 (94.10)</t>
+          <t>maa://28932 (94.29)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (96.38), maa://36673 (93.85), maa://25001 (88.51)</t>
+          <t>maa://24999 (96.49), maa://36673 (93.85), maa://25001 (88.76)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.25), maa://66545 (98.92)</t>
+          <t>*maa://21248 (73.33), maa://66545 (98.97)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (97.35), maa://22583 (87.07)</t>
+          <t>maa://22676 (97.44), maa://22583 (87.58)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="X13" s="8" t="inlineStr">
         <is>
-          <t>maa://34957 (94.36)</t>
+          <t>maa://34957 (94.10)</t>
         </is>
       </c>
       <c r="Y13" s="19" t="n"/>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (93.38)</t>
+          <t>maa://39883 (93.59)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2282,7 +2282,7 @@
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>maa://30764 (94.78)</t>
+          <t>maa://30764 (95.04)</t>
         </is>
       </c>
       <c r="E14" s="19" t="n"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (98.92), maa://26245 (97.03), maa://36682 (98.19), maa://21288 (96.40)</t>
+          <t>maa://39841 (98.92), maa://26245 (97.04), maa://36682 (98.22), maa://21288 (96.40)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2325,12 +2325,12 @@
       </c>
       <c r="O14" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="P14" s="8" t="inlineStr">
         <is>
-          <t>maa://23250 (99.60), maa://20107 (87.50), maa://22772 (100.00)</t>
+          <t>maa://23250 (99.62), maa://20107 (87.50), maa://22772 (100.00), maa://68732 (100.00)</t>
         </is>
       </c>
       <c r="Q14" s="19" t="n"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://42751 (98.80), maa://22521 (95.45)</t>
+          <t>maa://42751 (98.86), maa://22521 (95.07)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="X14" s="8" t="inlineStr">
         <is>
-          <t>maa://37468 (97.75)</t>
+          <t>maa://37468 (97.87)</t>
         </is>
       </c>
       <c r="Y14" s="19" t="n"/>
@@ -2378,7 +2378,7 @@
       </c>
       <c r="AB14" s="8" t="inlineStr">
         <is>
-          <t>maa://22764 (98.79)</t>
+          <t>maa://22764 (98.83)</t>
         </is>
       </c>
       <c r="AC14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (85.13), maa://45058 (98.09), maa://22734 (84.85), *maa://36048 (74.29)</t>
+          <t>maa://22743 (85.33), maa://45058 (97.99), maa://22734 (84.85), *maa://36048 (74.58)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (96.59), maa://21478 (90.48)</t>
+          <t>maa://24304 (96.75), maa://21478 (90.48)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="L15" s="8" t="inlineStr">
         <is>
-          <t>*maa://21334 (68.52)</t>
+          <t>*maa://21334 (69.09)</t>
         </is>
       </c>
       <c r="M15" s="19" t="n"/>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="P15" s="8" t="inlineStr">
         <is>
-          <t>maa://24762 (97.55), *maa://22727 (70.00)</t>
+          <t>maa://24762 (97.63), *maa://22727 (70.00)</t>
         </is>
       </c>
       <c r="Q15" s="19" t="n"/>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="T15" s="8" t="inlineStr">
         <is>
-          <t>maa://23892 (97.52)</t>
+          <t>maa://23892 (97.56)</t>
         </is>
       </c>
       <c r="U15" s="19" t="n"/>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://36666 (96.06), maa://21364 (83.53), *maa://22766 (70.71), maa://68306 (87.50)</t>
+          <t>maa://36666 (96.17), maa://21364 (83.61), *maa://22766 (70.71), maa://68306 (85.00)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://37650 (99.72), maa://21441 (96.62), maa://36679 (94.55)</t>
+          <t>maa://37650 (99.73), maa://21441 (96.62), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2590,7 +2590,7 @@
       </c>
       <c r="P16" s="8" t="inlineStr">
         <is>
-          <t>maa://28504 (95.90)</t>
+          <t>maa://28504 (96.00)</t>
         </is>
       </c>
       <c r="Q16" s="19" t="n"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://36674 (97.82), maa://22729 (95.99), *maa://28648 (77.89)</t>
+          <t>maa://36674 (97.91), maa://22729 (96.04), *maa://28648 (77.89)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2622,7 +2622,7 @@
       </c>
       <c r="X16" s="8" t="inlineStr">
         <is>
-          <t>maa://28501 (99.22), maa://28051 (96.88)</t>
+          <t>maa://28501 (99.26), maa://28051 (96.88)</t>
         </is>
       </c>
       <c r="Y16" s="19" t="n"/>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="AB16" s="8" t="inlineStr">
         <is>
-          <t>maa://26228 (97.73)</t>
+          <t>maa://26228 (97.83)</t>
         </is>
       </c>
       <c r="AC16" s="19" t="n"/>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>maa://23911 (90.00), maa://27755 (93.69), maa://67613 (99.21)</t>
+          <t>maa://23911 (90.23), maa://27755 (93.69), maa://67613 (99.29)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://39599 (98.02), maa://22430 (90.17)</t>
+          <t>maa://39599 (98.14), maa://22430 (90.21)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="L17" s="8" t="inlineStr">
         <is>
-          <t>maa://21679 (87.50)</t>
+          <t>maa://21679 (87.76)</t>
         </is>
       </c>
       <c r="M17" s="19" t="n"/>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (82.50), maa://56238 (98.23)</t>
+          <t>maa://23890 (82.64), maa://56238 (98.35)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="T17" s="8" t="inlineStr">
         <is>
-          <t>*maa://42324 (68.67)</t>
+          <t>*maa://42324 (69.05)</t>
         </is>
       </c>
       <c r="U17" s="19" t="n"/>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="AF17" s="8" t="inlineStr">
         <is>
-          <t>maa://50136 (98.86)</t>
+          <t>maa://50136 (98.96)</t>
         </is>
       </c>
       <c r="AG17" s="16" t="n"/>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>maa://24570 (98.21)</t>
+          <t>maa://24570 (98.26)</t>
         </is>
       </c>
       <c r="E18" s="19" t="n"/>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="H18" s="8" t="inlineStr">
         <is>
-          <t>maa://24421 (94.99)</t>
+          <t>maa://24421 (95.04)</t>
         </is>
       </c>
       <c r="I18" s="19" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://52226 (99.67), maa://22466 (92.79)</t>
+          <t>maa://52226 (99.69), maa://22466 (92.83)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), maa://54153 (99.61), maa://24380 (100.00)</t>
+          <t>maa://24379 (100.00), maa://54153 (99.63), maa://24380 (100.00)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (98.61), maa://22741 (91.67)</t>
+          <t>maa://21917 (98.63), maa://22741 (91.67)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="AB18" s="8" t="inlineStr">
         <is>
-          <t>maa://24393 (98.91)</t>
+          <t>maa://24393 (98.94)</t>
         </is>
       </c>
       <c r="AC18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://47854 (92.25)</t>
+          <t>maa://47854 (92.59)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -2932,7 +2932,7 @@
       </c>
       <c r="D19" s="8" t="inlineStr">
         <is>
-          <t>maa://62850 (99.26)</t>
+          <t>maa://62850 (99.28)</t>
         </is>
       </c>
       <c r="E19" s="19" t="n"/>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="L19" s="8" t="inlineStr">
         <is>
-          <t>maa://39347 (97.92), maa://56392 (100.00)</t>
+          <t>maa://39347 (97.96), maa://56392 (100.00)</t>
         </is>
       </c>
       <c r="M19" s="19" t="n"/>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="T19" s="8" t="inlineStr">
         <is>
-          <t>maa://24386 (99.63)</t>
+          <t>maa://24386 (99.65)</t>
         </is>
       </c>
       <c r="U19" s="19" t="n"/>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="X19" s="8" t="inlineStr">
         <is>
-          <t>maa://31386 (100.00), maa://58490 (83.33)</t>
+          <t>maa://31386 (100.00), maa://58490 (85.00)</t>
         </is>
       </c>
       <c r="Y19" s="19" t="n"/>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (84.74), *maa://36668 (68.75)</t>
+          <t>maa://30709 (85.31), *maa://36668 (68.75)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3044,7 +3044,7 @@
       </c>
       <c r="AF19" s="8" t="inlineStr">
         <is>
-          <t>*maa://21663 (65.12), maa://52239 (86.21)</t>
+          <t>*maa://21663 (65.91), maa://52239 (87.10)</t>
         </is>
       </c>
       <c r="AG19" s="16" t="n"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://25198 (97.52), maa://36680 (98.96), maa://21432 (91.45)</t>
+          <t>maa://25198 (97.56), maa://36680 (99.02), maa://21432 (91.49)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3078,7 +3078,7 @@
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>maa://22864 (95.71)</t>
+          <t>maa://22864 (95.96)</t>
         </is>
       </c>
       <c r="I20" s="19" t="n"/>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (94.93)</t>
+          <t>maa://41331 (95.10)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="P20" s="8" t="inlineStr">
         <is>
-          <t>maa://37442 (98.41)</t>
+          <t>maa://37442 (98.44)</t>
         </is>
       </c>
       <c r="Q20" s="19" t="n"/>
@@ -3126,7 +3126,7 @@
       </c>
       <c r="T20" s="8" t="inlineStr">
         <is>
-          <t>maa://29113 (93.24)</t>
+          <t>maa://29113 (93.42)</t>
         </is>
       </c>
       <c r="U20" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (96.18), maa://56241 (98.33), maa://49976 (88.35)</t>
+          <t>maa://50085 (96.32), maa://56241 (98.23), maa://49976 (88.46)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="H21" s="8" t="inlineStr">
         <is>
-          <t>maa://24372 (98.76)</t>
+          <t>maa://24372 (98.83)</t>
         </is>
       </c>
       <c r="I21" s="19" t="n"/>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="L21" s="8" t="inlineStr">
         <is>
-          <t>maa://31731 (96.33)</t>
+          <t>maa://31731 (96.40)</t>
         </is>
       </c>
       <c r="M21" s="19" t="n"/>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (98.16), maa://20110 (87.01)</t>
+          <t>maa://34946 (98.27), maa://20110 (87.01)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="AB21" s="8" t="inlineStr">
         <is>
-          <t>maa://21443 (86.44), maa://52223 (81.50)</t>
+          <t>maa://21443 (86.57), maa://52223 (82.21)</t>
         </is>
       </c>
       <c r="AC21" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22432 (93.43), maa://22524 (82.87), maa://64221 (97.62)</t>
+          <t>maa://22432 (93.74), maa://22524 (83.10), maa://64221 (97.74)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>maa://25236 (99.12)</t>
+          <t>maa://25236 (99.16)</t>
         </is>
       </c>
       <c r="I22" s="19" t="n"/>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>maa://27127 (82.59), *maa://22751 (70.93), maa://66865 (99.34)</t>
+          <t>maa://27127 (83.04), *maa://22751 (70.93), maa://66865 (99.37)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://37649 (93.84), maa://21282 (98.89)</t>
+          <t>maa://37649 (94.21), maa://21282 (98.92)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="AB22" s="8" t="inlineStr">
         <is>
-          <t>maa://23656 (99.46)</t>
+          <t>maa://23656 (99.48)</t>
         </is>
       </c>
       <c r="AC22" s="19" t="n"/>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="AF22" s="8" t="inlineStr">
         <is>
-          <t>maa://29658 (96.97)</t>
+          <t>maa://29658 (97.06)</t>
         </is>
       </c>
       <c r="AG22" s="16" t="n"/>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>*maa://41753 (62.90), ***maa://28036 (30.00)</t>
+          <t>*maa://41753 (65.15), ***maa://28036 (30.00)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (98.53), maa://39875 (95.65)</t>
+          <t>maa://39756 (98.57), maa://39875 (95.73)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (96.79), maa://29748 (81.82), *maa://37566 (78.12)</t>
+          <t>maa://30587 (96.74), maa://29748 (81.82), *maa://37566 (78.12)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="T23" s="8" t="inlineStr">
         <is>
-          <t>maa://31212 (95.19), maa://24387 (84.44), maa://67084 (85.71)</t>
+          <t>maa://31212 (95.28), maa://24387 (84.44), maa://67084 (87.50)</t>
         </is>
       </c>
       <c r="U23" s="19" t="n"/>
@@ -3532,7 +3532,7 @@
       </c>
       <c r="X23" s="8" t="inlineStr">
         <is>
-          <t>*maa://28503 (60.67)</t>
+          <t>*maa://28503 (59.48)</t>
         </is>
       </c>
       <c r="Y23" s="19" t="n"/>
@@ -3548,7 +3548,7 @@
       </c>
       <c r="AB23" s="8" t="inlineStr">
         <is>
-          <t>maa://29652 (96.34)</t>
+          <t>maa://29652 (96.39)</t>
         </is>
       </c>
       <c r="AC23" s="19" t="n"/>
@@ -3564,7 +3564,7 @@
       </c>
       <c r="AF23" s="8" t="inlineStr">
         <is>
-          <t>maa://31489 (98.08)</t>
+          <t>maa://31489 (98.21)</t>
         </is>
       </c>
       <c r="AG23" s="16" t="n"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (84.76), maa://46650 (89.80)</t>
+          <t>maa://24368 (84.97), maa://46650 (89.92)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (95.95), maa://23504 (94.02), *maa://25141 (79.33), maa://52227 (98.01), *maa://36663 (79.25)</t>
+          <t>maa://29988 (96.08), maa://23504 (94.04), *maa://25141 (79.74), maa://52227 (97.67), *maa://36663 (79.25)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="AB24" s="8" t="inlineStr">
         <is>
-          <t>maa://39349 (97.06)</t>
+          <t>maa://39349 (97.22)</t>
         </is>
       </c>
       <c r="AC24" s="19" t="n"/>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://64165 (99.21), maa://22523 (80.09), maa://29910 (94.20), maa://45831 (93.55)</t>
+          <t>maa://64165 (99.24), maa://22523 (80.09), maa://29910 (94.20), maa://45831 (93.55)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (96.40), maa://63016 (99.04)</t>
+          <t>maa://29753 (96.46), maa://63016 (99.07)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>*maa://29063 (75.15), *maa://25311 (70.71), maa://45047 (87.50)</t>
+          <t>*maa://29063 (75.88), *maa://25311 (70.92), maa://45047 (87.67)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3760,7 +3760,7 @@
       </c>
       <c r="P25" s="8" t="inlineStr">
         <is>
-          <t>maa://24382 (95.92)</t>
+          <t>maa://24382 (96.00)</t>
         </is>
       </c>
       <c r="Q25" s="19" t="n"/>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="T25" s="8" t="inlineStr">
         <is>
-          <t>maa://20109 (96.32), maa://22545 (100.00)</t>
+          <t>maa://20109 (96.38), maa://22545 (100.00)</t>
         </is>
       </c>
       <c r="U25" s="19" t="n"/>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="X25" s="8" t="inlineStr">
         <is>
-          <t>maa://29890 (90.83)</t>
+          <t>maa://29890 (91.06)</t>
         </is>
       </c>
       <c r="Y25" s="19" t="n"/>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (93.08), *maa://24516 (79.80), maa://26001 (83.33), maa://68311 (100.00)</t>
+          <t>maa://31215 (93.22), *maa://24516 (79.80), maa://26001 (83.33), maa://68311 (100.00)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (97.93), maa://36676 (99.83), maa://24621 (96.84), maa://22771 (88.24), maa://37772 (83.33)</t>
+          <t>maa://20108 (98.00), maa://36676 (99.83), maa://24621 (96.86), maa://22771 (88.24), maa://37772 (83.33)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://56374 (100.00), maa://41802 (95.74)</t>
+          <t>maa://56374 (100.00), maa://41802 (96.15)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3858,7 +3858,7 @@
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
-          <t>maa://56240 (96.26), maa://24913 (92.17)</t>
+          <t>maa://56240 (96.39), maa://24913 (92.17)</t>
         </is>
       </c>
       <c r="I26" s="19" t="n"/>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="P26" s="8" t="inlineStr">
         <is>
-          <t>maa://39870 (94.12), maa://56625 (100.00)</t>
+          <t>maa://39870 (94.29), maa://56625 (100.00)</t>
         </is>
       </c>
       <c r="Q26" s="19" t="n"/>
@@ -3922,7 +3922,7 @@
       </c>
       <c r="X26" s="8" t="inlineStr">
         <is>
-          <t>maa://24389 (98.25)</t>
+          <t>maa://24389 (98.31)</t>
         </is>
       </c>
       <c r="Y26" s="19" t="n"/>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="AB26" s="8" t="inlineStr">
         <is>
-          <t>maa://42235 (98.36)</t>
+          <t>maa://42235 (98.43)</t>
         </is>
       </c>
       <c r="AC26" s="19" t="n"/>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="AF26" s="8" t="inlineStr">
         <is>
-          <t>*maa://30511 (72.15), **maa://29760 (47.62)</t>
+          <t>*maa://30511 (72.50), **maa://29760 (47.62)</t>
         </is>
       </c>
       <c r="AG26" s="16" t="n"/>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>maa://39601 (89.47), maa://34494 (96.43)</t>
+          <t>maa://39601 (90.48), maa://34494 (96.47)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4004,7 +4004,7 @@
       </c>
       <c r="L27" s="8" t="inlineStr">
         <is>
-          <t>maa://28071 (88.24)</t>
+          <t>maa://28071 (88.89)</t>
         </is>
       </c>
       <c r="M27" s="19" t="n"/>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="T27" s="8" t="inlineStr">
         <is>
-          <t>maa://30624 (89.41)</t>
+          <t>maa://30624 (89.53)</t>
         </is>
       </c>
       <c r="U27" s="19" t="n"/>
@@ -4084,7 +4084,7 @@
       </c>
       <c r="AF27" s="8" t="inlineStr">
         <is>
-          <t>maa://24023 (97.60)</t>
+          <t>maa://24023 (97.69)</t>
         </is>
       </c>
       <c r="AG27" s="16" t="n"/>
@@ -4102,7 +4102,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (95.69), maa://25725 (84.92)</t>
+          <t>maa://24465 (95.79), maa://25725 (85.16)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="L28" s="8" t="inlineStr">
         <is>
-          <t>maa://30770 (89.53)</t>
+          <t>maa://30770 (89.66)</t>
         </is>
       </c>
       <c r="M28" s="19" t="n"/>
@@ -4166,7 +4166,7 @@
       </c>
       <c r="T28" s="8" t="inlineStr">
         <is>
-          <t>maa://29765 (92.90), maa://23263 (96.18)</t>
+          <t>maa://29765 (93.05), maa://23263 (96.18)</t>
         </is>
       </c>
       <c r="U28" s="19" t="n"/>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (97.15), maa://41749 (97.11)</t>
+          <t>maa://39929 (97.28), maa://41749 (97.16)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (94.03), maa://65700 (98.68)</t>
+          <t>maa://36660 (94.14), maa://65700 (98.58)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4232,7 +4232,7 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>maa://31694 (99.28)</t>
+          <t>maa://31694 (99.30)</t>
         </is>
       </c>
       <c r="E29" s="19" t="n"/>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (97.70), maa://31400 (97.99), maa://28440 (86.25)</t>
+          <t>maa://28432 (97.76), maa://31400 (98.02), maa://28440 (86.34)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4280,7 +4280,7 @@
       </c>
       <c r="P29" s="8" t="inlineStr">
         <is>
-          <t>maa://54169 (97.03)</t>
+          <t>maa://54169 (97.14)</t>
         </is>
       </c>
       <c r="Q29" s="19" t="n"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://42865 (91.87)</t>
+          <t>maa://42865 (92.28)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (95.00), maa://64191 (100.00)</t>
+          <t>maa://45792 (95.24), maa://64191 (97.30)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="L30" s="8" t="inlineStr">
         <is>
-          <t>maa://30442 (97.30)</t>
+          <t>maa://30442 (97.39)</t>
         </is>
       </c>
       <c r="M30" s="19" t="n"/>
@@ -4426,7 +4426,7 @@
       </c>
       <c r="T30" s="8" t="inlineStr">
         <is>
-          <t>*maa://32940 (80.00), maa://24388 (96.00)</t>
+          <t>maa://32940 (80.95), maa://24388 (96.00)</t>
         </is>
       </c>
       <c r="U30" s="19" t="n"/>
@@ -4458,7 +4458,7 @@
       </c>
       <c r="AB30" s="8" t="inlineStr">
         <is>
-          <t>maa://42979 (99.52), maa://45822 (100.00), maa://45045 (90.91)</t>
+          <t>maa://42979 (99.54), maa://45822 (100.00), maa://45045 (90.91)</t>
         </is>
       </c>
       <c r="AC30" s="19" t="n"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (97.87), maa://36258 (92.88), maa://43904 (89.47)</t>
+          <t>maa://35926 (97.95), maa://36258 (92.97), maa://43904 (89.47)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4556,7 +4556,7 @@
       </c>
       <c r="T31" s="8" t="inlineStr">
         <is>
-          <t>maa://30711 (96.46), maa://30768 (100.00)</t>
+          <t>maa://30711 (96.52), maa://30768 (100.00)</t>
         </is>
       </c>
       <c r="U31" s="19" t="n"/>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://36667 (99.61), maa://21895 (97.95), maa://22760 (100.00)</t>
+          <t>maa://36667 (99.63), maa://21895 (97.96), maa://22760 (100.00)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (99.32), maa://41108 (87.72), maa://41238 (98.10), maa://45523 (100.00)</t>
+          <t>maa://42859 (99.23), maa://41108 (87.72), maa://41238 (98.12), maa://45523 (100.00)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="X32" s="8" t="inlineStr">
         <is>
-          <t>maa://64104 (97.14)</t>
+          <t>maa://64104 (97.27)</t>
         </is>
       </c>
       <c r="Y32" s="19" t="n"/>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (94.07), *maa://22730 (70.59)</t>
+          <t>maa://21956 (94.41), *maa://22730 (70.59)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="T33" s="8" t="inlineStr">
         <is>
-          <t>maa://45558 (92.86)</t>
+          <t>maa://45558 (93.33)</t>
         </is>
       </c>
       <c r="U33" s="19" t="n"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (99.13), maa://56235 (99.71)</t>
+          <t>maa://48817 (99.17), maa://56235 (99.72)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="T34" s="8" t="inlineStr">
         <is>
-          <t>maa://24526 (96.92)</t>
+          <t>maa://24526 (96.98)</t>
         </is>
       </c>
       <c r="U34" s="19" t="n"/>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="AB34" s="8" t="inlineStr">
         <is>
-          <t>maa://64329 (97.30)</t>
+          <t>maa://64329 (97.56)</t>
         </is>
       </c>
       <c r="AC34" s="19" t="n"/>
@@ -4994,7 +4994,7 @@
       </c>
       <c r="AF34" s="8" t="inlineStr">
         <is>
-          <t>maa://32650 (87.76)</t>
+          <t>maa://32650 (88.00)</t>
         </is>
       </c>
       <c r="AG34" s="16" t="n"/>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
-          <t>maa://41296 (99.21)</t>
+          <t>maa://41296 (99.24)</t>
         </is>
       </c>
       <c r="M35" s="19" t="n"/>
@@ -5076,7 +5076,7 @@
       </c>
       <c r="T35" s="8" t="inlineStr">
         <is>
-          <t>maa://24842 (96.51)</t>
+          <t>maa://24842 (96.55)</t>
         </is>
       </c>
       <c r="U35" s="19" t="n"/>
@@ -5158,7 +5158,7 @@
       </c>
       <c r="H36" s="8" t="inlineStr">
         <is>
-          <t>maa://24375 (94.12)</t>
+          <t>maa://24375 (94.29)</t>
         </is>
       </c>
       <c r="I36" s="19" t="n"/>
@@ -5206,7 +5206,7 @@
       </c>
       <c r="T36" s="8" t="inlineStr">
         <is>
-          <t>maa://27613 (99.52)</t>
+          <t>maa://27613 (99.53)</t>
         </is>
       </c>
       <c r="U36" s="19" t="n"/>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="AB36" s="19" t="inlineStr">
         <is>
-          <t>maa://64106 (96.77)</t>
+          <t>maa://64106 (96.97)</t>
         </is>
       </c>
       <c r="AC36" s="19" t="n"/>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="H37" s="8" t="inlineStr">
         <is>
-          <t>*maa://24374 (56.67)</t>
+          <t>*maa://24374 (57.38)</t>
         </is>
       </c>
       <c r="I37" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (99.17), maa://56336 (99.28), maa://47069 (87.50), maa://45789 (100.00)</t>
+          <t>maa://45718 (99.18), maa://56336 (99.32), maa://47069 (88.10), maa://45789 (100.00)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="P37" s="8" t="inlineStr">
         <is>
-          <t>maa://21280 (97.44)</t>
+          <t>maa://21280 (97.52)</t>
         </is>
       </c>
       <c r="Q37" s="19" t="n"/>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="P38" s="8" t="inlineStr">
         <is>
-          <t>maa://24383 (80.79)</t>
+          <t>maa://24383 (81.32)</t>
         </is>
       </c>
       <c r="Q38" s="19" t="n"/>
@@ -5482,7 +5482,7 @@
       </c>
       <c r="AF38" s="8" t="inlineStr">
         <is>
-          <t>maa://36697 (95.76), maa://68397 (98.39)</t>
+          <t>maa://36697 (95.80), maa://68397 (99.15)</t>
         </is>
       </c>
       <c r="AG38" s="16" t="n"/>
@@ -5503,7 +5503,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://25199 (84.67), maa://45059 (92.19), maa://30434 (95.19), maa://44165 (85.71)</t>
+          <t>maa://25199 (84.67), maa://45059 (93.02), maa://30434 (95.26), maa://44165 (85.71)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://47093 (98.03), maa://24709 (93.70)</t>
+          <t>maa://47093 (98.10), maa://24709 (93.90)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (95.22), maa://45790 (87.14)</t>
+          <t>maa://47079 (95.45), maa://45790 (87.67)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5583,7 +5583,7 @@
       </c>
       <c r="AF39" s="8" t="inlineStr">
         <is>
-          <t>maa://62953 (96.89)</t>
+          <t>maa://62953 (96.77)</t>
         </is>
       </c>
       <c r="AG39" s="16" t="n"/>
@@ -5636,7 +5636,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (97.99), maa://21386 (95.92), maa://36664 (89.61), *maa://45550 (72.73)</t>
+          <t>maa://23278 (98.05), maa://21386 (95.92), maa://36664 (89.61), *maa://45550 (72.73)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://65283 (96.47), maa://64205 (93.75)</t>
+          <t>maa://65283 (96.65), maa://64205 (93.75)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5705,7 +5705,7 @@
       </c>
       <c r="H41" s="8" t="inlineStr">
         <is>
-          <t>maa://24466 (92.65)</t>
+          <t>maa://24466 (92.75)</t>
         </is>
       </c>
       <c r="I41" s="19" t="n"/>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="P41" s="8" t="inlineStr">
         <is>
-          <t>maa://43177 (95.24)</t>
+          <t>maa://43177 (95.33)</t>
         </is>
       </c>
       <c r="Q41" s="19" t="n"/>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>*maa://22525 (70.87), maa://21284 (97.37)</t>
+          <t>*maa://22525 (70.69), maa://21284 (97.53)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -5939,7 +5939,7 @@
       </c>
       <c r="P43" s="8" t="inlineStr">
         <is>
-          <t>maa://47403 (87.10)</t>
+          <t>maa://47403 (87.50)</t>
         </is>
       </c>
       <c r="Q43" s="19" t="n"/>
@@ -6008,7 +6008,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (98.19), maa://56386 (99.34), maa://27728 (96.36)</t>
+          <t>maa://29768 (98.21), maa://56386 (99.37), maa://27728 (96.40)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6056,7 +6056,7 @@
       </c>
       <c r="T44" s="8" t="inlineStr">
         <is>
-          <t>maa://39366 (93.02)</t>
+          <t>maa://39366 (93.26)</t>
         </is>
       </c>
       <c r="U44" s="19" t="n"/>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://42459 (98.61), maa://21229 (85.46), maa://30807 (94.62)</t>
+          <t>maa://42459 (98.66), maa://21229 (85.53), maa://30807 (94.62)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6109,7 +6109,7 @@
       </c>
       <c r="P45" s="8" t="inlineStr">
         <is>
-          <t>maa://36237 (82.86)</t>
+          <t>maa://36237 (83.33)</t>
         </is>
       </c>
       <c r="Q45" s="19" t="n"/>
@@ -6125,7 +6125,7 @@
       </c>
       <c r="T45" s="8" t="inlineStr">
         <is>
-          <t>*maa://39364 (66.67)</t>
+          <t>*maa://39364 (66.45)</t>
         </is>
       </c>
       <c r="U45" s="19" t="n"/>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (95.44), maa://43901 (96.40)</t>
+          <t>maa://35931 (95.53), maa://43901 (96.12)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6231,7 +6231,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (97.47), maa://29661 (97.17), maa://56236 (99.76), maa://28038 (84.62)</t>
+          <t>maa://27410 (97.49), maa://29661 (97.17), maa://56236 (99.77), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6263,7 +6263,7 @@
       </c>
       <c r="T47" s="8" t="inlineStr">
         <is>
-          <t>maa://67476 (99.53), maa://68392 (100.00)</t>
+          <t>maa://67476 (99.55), maa://68392 (100.00)</t>
         </is>
       </c>
       <c r="U47" s="19" t="n"/>
@@ -6385,7 +6385,7 @@
       </c>
       <c r="P49" s="8" t="inlineStr">
         <is>
-          <t>*maa://39643 (78.46)</t>
+          <t>*maa://39643 (79.10)</t>
         </is>
       </c>
       <c r="Q49" s="19" t="n"/>
@@ -6401,7 +6401,7 @@
       </c>
       <c r="T49" s="19" t="inlineStr">
         <is>
-          <t>maa://67231 (99.01)</t>
+          <t>maa://67231 (99.06)</t>
         </is>
       </c>
       <c r="U49" s="19" t="n"/>
@@ -6438,7 +6438,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>maa://62852 (92.73)</t>
+          <t>maa://62852 (93.04)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6522,7 +6522,7 @@
       </c>
       <c r="H52" s="8" t="inlineStr">
         <is>
-          <t>maa://24376 (98.95)</t>
+          <t>maa://24376 (99.00)</t>
         </is>
       </c>
       <c r="I52" s="19" t="n"/>
@@ -6538,7 +6538,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (99.31), maa://59378 (93.83), maa://65511 (100.00)</t>
+          <t>maa://59394 (99.34), maa://59378 (93.83), maa://65511 (100.00)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6572,7 +6572,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (97.80)</t>
+          <t>maa://32534 (97.81)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -6656,7 +6656,7 @@
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>maa://32532 (97.68)</t>
+          <t>maa://32532 (97.77)</t>
         </is>
       </c>
       <c r="I55" s="19" t="n"/>
@@ -6708,7 +6708,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://56237 (99.26), maa://25176 (98.77)</t>
+          <t>maa://56237 (99.30), maa://25176 (98.77)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6726,7 +6726,7 @@
       </c>
       <c r="H58" s="8" t="inlineStr">
         <is>
-          <t>*maa://37964 (66.67)</t>
+          <t>*maa://37964 (65.81)</t>
         </is>
       </c>
       <c r="I58" s="19" t="n"/>
@@ -6744,7 +6744,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (98.40), maa://27746 (88.95)</t>
+          <t>maa://31270 (98.45), maa://27746 (89.01)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -6762,7 +6762,7 @@
       </c>
       <c r="H60" s="8" t="inlineStr">
         <is>
-          <t>maa://40438 (90.91)</t>
+          <t>maa://40438 (91.25)</t>
         </is>
       </c>
       <c r="I60" s="19" t="n"/>
@@ -6798,7 +6798,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (97.73), maa://56228 (99.30), maa://43903 (100.00)</t>
+          <t>maa://42981 (97.73), maa://56228 (99.33), maa://43903 (100.00)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6816,7 +6816,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (99.35), *maa://59693 (76.09), maa://59413 (96.83)</t>
+          <t>maa://59534 (99.38), *maa://59693 (74.47), maa://59413 (97.06)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7032,7 +7032,7 @@
       </c>
       <c r="H75" s="19" t="inlineStr">
         <is>
-          <t>maa://67748 (82.61)</t>
+          <t>*maa://67748 (80.00)</t>
         </is>
       </c>
       <c r="I75" s="19" t="n"/>
@@ -7174,7 +7174,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.20 13:19:46</t>
+          <t>更新日期：2025.09.23 13:20:11</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8578,7 +8578,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (73.21), *maa://28758 (71.11), maa://29036 (96.67), *maa://42172 (71.43), maa://65357 (96.00), maa://30285 (100.00)</t>
+          <t>*maa://20849 (73.21), *maa://28758 (71.11), maa://29036 (96.67), *maa://42172 (71.43), maa://65357 (96.15), maa://30285 (100.00)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8686,7 +8686,7 @@
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>maa://20863 (90.60), maa://20832 (99.21), maa://20727 (100.00)</t>
+          <t>maa://20863 (90.64), maa://20832 (99.21), maa://20727 (100.00)</t>
         </is>
       </c>
       <c r="E29" s="14" t="inlineStr">
@@ -9118,7 +9118,7 @@
       </c>
       <c r="D37" s="13" t="inlineStr">
         <is>
-          <t>maa://27376 (93.33), maa://42635 (94.23), *maa://20838 (55.00)</t>
+          <t>maa://27376 (93.33), maa://42635 (94.34), *maa://20838 (55.00)</t>
         </is>
       </c>
       <c r="E37" s="14" t="inlineStr">
@@ -10085,12 +10085,12 @@
       </c>
       <c r="C55" s="12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D55" s="13" t="inlineStr">
         <is>
-          <t>maa://20932 (96.15), maa://42415 (96.15), maa://40838 (100.00)</t>
+          <t>maa://20932 (96.15), maa://42415 (96.15), maa://40838 (100.00), maa://68386 (100.00)</t>
         </is>
       </c>
       <c r="E55" s="14" t="inlineStr">
@@ -10414,7 +10414,7 @@
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (99.21), maa://31559 (93.88), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00)</t>
+          <t>maa://20841 (99.22), maa://31559 (93.88), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -10792,7 +10792,7 @@
       </c>
       <c r="D68" s="13" t="inlineStr">
         <is>
-          <t>maa://20976 (97.79), maa://20815 (100.00)</t>
+          <t>maa://20976 (97.82), maa://20815 (100.00)</t>
         </is>
       </c>
       <c r="E68" s="14" t="inlineStr">
@@ -10900,7 +10900,7 @@
       </c>
       <c r="D70" s="13" t="inlineStr">
         <is>
-          <t>maa://20944 (96.08), maa://35393 (100.00)</t>
+          <t>maa://20944 (96.15), maa://35393 (100.00)</t>
         </is>
       </c>
       <c r="E70" s="14" t="inlineStr">
@@ -11008,7 +11008,7 @@
       </c>
       <c r="D72" s="13" t="inlineStr">
         <is>
-          <t>maa://36643 (98.44), maa://36864 (98.10), maa://39140 (100.00), maa://66335 (100.00)</t>
+          <t>maa://36643 (98.44), maa://36864 (98.11), maa://39140 (100.00), maa://66335 (100.00)</t>
         </is>
       </c>
       <c r="E72" s="14" t="inlineStr">
@@ -12952,7 +12952,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.70), maa://25018 (96.92), maa://25776 (92.21), maa://28361 (95.35), maa://25772 (94.12), maa://56588 (96.55), maa://45194 (85.71), maa://32653 (81.25), maa://25161 (83.33), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
+          <t>maa://51881 (98.71), maa://25018 (96.93), maa://25776 (92.21), maa://28361 (95.45), maa://25772 (94.12), maa://56588 (93.33), maa://45194 (85.71), maa://32653 (81.25), maa://25161 (83.33), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13870,7 +13870,7 @@
       </c>
       <c r="D125" s="13" t="inlineStr">
         <is>
-          <t>*maa://20909 (71.43)</t>
+          <t>*maa://20909 (68.18)</t>
         </is>
       </c>
       <c r="E125" s="14" t="inlineStr">
@@ -15220,7 +15220,7 @@
       </c>
       <c r="D150" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.82), maa://36641 (98.24), maa://36865 (95.45), maa://44635 (88.07), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (100.00), maa://42918 (100.00), maa://44119 (97.44), maa://64408 (92.86), maa://37300 (100.00), maa://42917 (100.00)</t>
+          <t>maa://40957 (94.83), maa://36641 (98.24), maa://36865 (95.45), maa://44635 (88.18), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (100.00), maa://42918 (100.00), maa://44119 (97.44), maa://64408 (92.86), maa://37300 (100.00), maa://42917 (100.00)</t>
         </is>
       </c>
       <c r="E150" s="14" t="inlineStr">
@@ -16192,7 +16192,7 @@
       </c>
       <c r="D168" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (92.18), maa://29627 (92.95), maa://29659 (87.50), maa://49074 (94.20), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
+          <t>maa://29633 (92.23), maa://29627 (92.95), maa://29659 (87.50), maa://49074 (94.20), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
         </is>
       </c>
       <c r="E168" s="14" t="inlineStr">
@@ -16624,7 +16624,7 @@
       </c>
       <c r="D176" s="13" t="inlineStr">
         <is>
-          <t>maa://32418 (99.70), maa://63320 (100.00), maa://51440 (100.00)</t>
+          <t>maa://32418 (99.70), maa://63320 (97.50), maa://51440 (100.00)</t>
         </is>
       </c>
       <c r="E176" s="14" t="inlineStr">
@@ -17812,7 +17812,7 @@
       </c>
       <c r="D198" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.43), maa://35854 (84.75), maa://50388 (98.24), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (94.29)</t>
+          <t>maa://44224 (90.43), maa://35854 (84.75), maa://50388 (98.24), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (94.44)</t>
         </is>
       </c>
       <c r="E198" s="14" t="inlineStr">
@@ -18568,7 +18568,7 @@
       </c>
       <c r="D212" s="13" t="inlineStr">
         <is>
-          <t>maa://20956 (96.15), *maa://20830 (80.00), maa://44703 (92.31)</t>
+          <t>maa://20956 (96.15), *maa://20830 (80.00), maa://44703 (92.86)</t>
         </is>
       </c>
       <c r="E212" s="14" t="inlineStr">
@@ -18730,7 +18730,7 @@
       </c>
       <c r="D215" s="13" t="inlineStr">
         <is>
-          <t>maa://64044 (95.83)</t>
+          <t>maa://64044 (95.92)</t>
         </is>
       </c>
       <c r="E215" s="14" t="inlineStr">
@@ -20674,7 +20674,7 @@
       </c>
       <c r="D251" s="13" t="inlineStr">
         <is>
-          <t>maa://28923 (91.83), maa://28906 (98.28), ***maa://28825 (11.54), maa://65613 (100.00)</t>
+          <t>maa://28923 (91.87), maa://28906 (98.28), ***maa://28825 (11.54), maa://65613 (100.00)</t>
         </is>
       </c>
       <c r="E251" s="14" t="inlineStr">
@@ -20728,7 +20728,7 @@
       </c>
       <c r="D252" s="13" t="inlineStr">
         <is>
-          <t>maa://42287 (91.74), maa://45570 (96.72), maa://60678 (93.33), maa://42225 (100.00)</t>
+          <t>maa://42287 (91.80), maa://45570 (96.72), maa://60678 (93.33), maa://42225 (100.00)</t>
         </is>
       </c>
       <c r="E252" s="14" t="inlineStr">
@@ -21484,7 +21484,7 @@
       </c>
       <c r="D266" s="13" t="inlineStr">
         <is>
-          <t>maa://39162 (97.30)</t>
+          <t>maa://39162 (97.37)</t>
         </is>
       </c>
       <c r="E266" s="14" t="inlineStr">
@@ -21916,7 +21916,7 @@
       </c>
       <c r="D274" s="13" t="inlineStr">
         <is>
-          <t>**maa://62757 (41.18), maa://67819 (100.00)</t>
+          <t>**maa://62757 (42.86), maa://67819 (100.00)</t>
         </is>
       </c>
       <c r="E274" s="14" t="inlineStr">
@@ -22024,7 +22024,7 @@
       </c>
       <c r="D276" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.70), maa://51630 (96.26), maa://56588 (96.55), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (41.67), *maa://66758 (77.78)</t>
+          <t>maa://51881 (98.71), maa://51630 (96.26), maa://56588 (93.33), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (41.67), *maa://66758 (75.00)</t>
         </is>
       </c>
       <c r="E276" s="14" t="inlineStr">
@@ -22942,7 +22942,7 @@
       </c>
       <c r="D293" s="13" t="inlineStr">
         <is>
-          <t>maa://30710 (97.92), maa://36845 (95.86), maa://31558 (97.14), **maa://39217 (38.89), maa://30668 (86.67)</t>
+          <t>maa://30710 (97.93), maa://36845 (95.86), maa://31558 (97.22), **maa://39217 (38.89), maa://30668 (86.67)</t>
         </is>
       </c>
       <c r="E293" s="14" t="inlineStr">
@@ -23698,7 +23698,7 @@
       </c>
       <c r="D307" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (98.47), maa://49642 (97.62), maa://49660 (93.62), maa://50517 (85.71)</t>
+          <t>maa://50280 (98.48), maa://49642 (97.62), maa://49660 (93.62), maa://50517 (85.71)</t>
         </is>
       </c>
       <c r="E307" s="14" t="inlineStr">
@@ -26020,7 +26020,7 @@
       </c>
       <c r="D350" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (97.72), maa://32415 (84.80), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
+          <t>maa://32647 (97.59), maa://32415 (84.88), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E350" s="22" t="inlineStr">
@@ -26506,7 +26506,7 @@
       </c>
       <c r="D359" s="22" t="inlineStr">
         <is>
-          <t>maa://36868 (99.54), maa://35996 (97.89), maa://47349 (97.44), **maa://39217 (38.89)</t>
+          <t>maa://36868 (99.54), maa://35996 (97.89), maa://47349 (97.47), **maa://39217 (38.89)</t>
         </is>
       </c>
       <c r="E359" s="22" t="inlineStr">
@@ -26560,7 +26560,7 @@
       </c>
       <c r="D360" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.59), maa://49695 (100.00), maa://49758 (98.67), *maa://59402 (56.67), *maa://52357 (73.33), *maa://63091 (72.73)</t>
+          <t>maa://49696 (99.59), maa://49695 (100.00), maa://49758 (98.70), *maa://59402 (56.67), *maa://52357 (75.00), *maa://63091 (72.73)</t>
         </is>
       </c>
       <c r="E360" s="22" t="inlineStr">
@@ -26668,7 +26668,7 @@
       </c>
       <c r="D362" s="22" t="inlineStr">
         <is>
-          <t>maa://42299 (97.83), maa://42224 (85.00)</t>
+          <t>maa://42299 (97.87), maa://42224 (85.00)</t>
         </is>
       </c>
       <c r="E362" s="22" t="inlineStr">
@@ -26830,7 +26830,7 @@
       </c>
       <c r="D365" s="22" t="inlineStr">
         <is>
-          <t>maa://36645 (98.43), maa://36841 (92.65), maa://37484 (94.23), maa://37858 (93.55), *maa://56268 (60.00), maa://40489 (100.00)</t>
+          <t>maa://36645 (98.43), maa://36841 (92.65), maa://37484 (94.23), maa://37858 (93.55), **maa://56268 (50.00), maa://40489 (100.00)</t>
         </is>
       </c>
       <c r="E365" s="22" t="inlineStr">
@@ -26884,7 +26884,7 @@
       </c>
       <c r="D366" s="22" t="inlineStr">
         <is>
-          <t>maa://42635 (94.23), maa://50629 (83.33), maa://48859 (100.00)</t>
+          <t>maa://42635 (94.34), maa://50629 (83.33), maa://48859 (100.00)</t>
         </is>
       </c>
       <c r="E366" s="22" t="inlineStr">
@@ -27046,7 +27046,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (94.82), maa://48026 (94.66), maa://44635 (88.07), maa://41035 (93.51), *maa://60251 (76.47), maa://44660 (92.68), maa://41128 (84.21)</t>
+          <t>maa://40957 (94.83), maa://48026 (94.70), maa://44635 (88.18), maa://41035 (93.51), *maa://60251 (76.47), maa://44660 (92.68), maa://41128 (84.21)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -27316,7 +27316,7 @@
       </c>
       <c r="D374" s="22" t="inlineStr">
         <is>
-          <t>maa://45798 (98.61)</t>
+          <t>maa://45798 (98.63)</t>
         </is>
       </c>
       <c r="E374" s="22" t="inlineStr">
@@ -27964,7 +27964,7 @@
       </c>
       <c r="D386" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (81.00), maa://44745 (98.01), **maa://49516 (39.29), *maa://45952 (57.14), ***maa://46851 (12.50), *maa://44896 (77.78)</t>
+          <t>maa://42970 (81.00), maa://44745 (98.02), **maa://49516 (39.29), *maa://45952 (57.14), ***maa://46851 (12.50), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E386" s="22" t="inlineStr">
@@ -28288,7 +28288,7 @@
       </c>
       <c r="D392" s="22" t="inlineStr">
         <is>
-          <t>maa://63890 (97.73), maa://64043 (100.00)</t>
+          <t>maa://63890 (97.78), maa://64043 (100.00)</t>
         </is>
       </c>
       <c r="E392" s="22" t="inlineStr">
@@ -28423,7 +28423,7 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>maa://59533 (97.73), maa://59577 (100.00)</t>
+          <t>maa://59533 (97.78), maa://59577 (100.00)</t>
         </is>
       </c>
       <c r="E396" t="inlineStr">
@@ -28612,7 +28612,7 @@
       </c>
       <c r="D403" t="inlineStr">
         <is>
-          <t>maa://60449 (98.97), maa://59493 (96.85)</t>
+          <t>maa://60449 (98.98), maa://59493 (96.85)</t>
         </is>
       </c>
       <c r="E403" t="inlineStr">
@@ -28666,7 +28666,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>maa://62756 (95.74)</t>
+          <t>maa://62756 (95.86)</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">
@@ -28720,7 +28720,7 @@
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>maa://64040 (98.97), maa://52505 (98.40), maa://66377 (92.31), ***maa://66376 (25.00)</t>
+          <t>maa://64040 (98.98), maa://52505 (98.47), maa://66377 (92.86), ***maa://66376 (25.00)</t>
         </is>
       </c>
       <c r="E407" t="inlineStr">
@@ -28747,7 +28747,7 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>maa://67090 (85.19)</t>
+          <t>maa://67090 (86.67)</t>
         </is>
       </c>
       <c r="E408" t="inlineStr">
@@ -28774,7 +28774,7 @@
       </c>
       <c r="D409" t="inlineStr">
         <is>
-          <t>maa://67388 (90.62)</t>
+          <t>maa://67388 (91.43)</t>
         </is>
       </c>
       <c r="E409" t="inlineStr">
@@ -28801,7 +28801,7 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>maa://67089 (97.14), maa://67271 (92.31)</t>
+          <t>maa://67089 (97.37), maa://67271 (93.33)</t>
         </is>
       </c>
       <c r="E410" t="inlineStr">
@@ -28828,7 +28828,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>maa://67088 (88.64)</t>
+          <t>maa://67088 (90.38)</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
@@ -28855,7 +28855,7 @@
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>maa://67087 (93.67), maa://67268 (95.59), maa://67269 (84.62), maa://67648 (100.00)</t>
+          <t>maa://67087 (93.33), maa://67268 (95.71), maa://67269 (87.50), maa://67648 (100.00)</t>
         </is>
       </c>
       <c r="E412" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#241)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -712,7 +712,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (98.18), maa://24702 (95.06), maa://36681 (86.21)</t>
+          <t>maa://25390 (98.20), maa://24702 (95.06), maa://36681 (86.21)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://58660 (98.70), maa://39402 (94.93), *maa://34787 (75.00)</t>
+          <t>maa://58660 (98.77), maa://39402 (95.11), *maa://34787 (75.00)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -776,7 +776,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (97.15), maa://66635 (99.65)</t>
+          <t>maa://22742 (97.22), maa://66635 (99.51)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://36684 (98.18), maa://21246 (91.32)</t>
+          <t>maa://36684 (98.26), maa://21246 (91.32)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://59087 (97.09), maa://25251 (91.61)</t>
+          <t>maa://59087 (97.18), maa://25251 (91.61)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -842,7 +842,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (99.30), maa://36987 (97.10), maa://39849 (90.91)</t>
+          <t>maa://40192 (99.34), maa://36987 (97.14), maa://39849 (91.67)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -858,7 +858,7 @@
       </c>
       <c r="H3" s="8" t="inlineStr">
         <is>
-          <t>maa://21247 (99.31)</t>
+          <t>maa://21247 (99.34)</t>
         </is>
       </c>
       <c r="I3" s="19" t="n"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>maa://22880 (90.34), maa://20276 (93.91), maa://22749 (84.00)</t>
+          <t>maa://22880 (90.66), maa://20276 (93.98), maa://22749 (84.62)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -890,7 +890,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (98.28), maa://26254 (98.11), *maa://22738 (80.00)</t>
+          <t>maa://21249 (98.30), maa://26254 (98.11), *maa://22738 (80.00)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://60545 (98.65), maa://45854 (86.98), maa://24617 (91.18)</t>
+          <t>maa://60545 (98.63), maa://45854 (86.73), maa://24617 (91.18)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (91.71), maa://27484 (99.14), maa://27480 (84.91)</t>
+          <t>maa://27396 (91.70), maa://27484 (99.17), maa://27480 (85.45)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://52241 (99.35), maa://24390 (96.77)</t>
+          <t>maa://52241 (99.05), maa://24390 (96.77)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -954,7 +954,7 @@
       </c>
       <c r="AF3" s="8" t="inlineStr">
         <is>
-          <t>maa://21289 (91.35)</t>
+          <t>maa://21289 (91.43)</t>
         </is>
       </c>
       <c r="AG3" s="16" t="n"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (97.99), maa://22499 (90.00), maa://22746 (100.00)</t>
+          <t>maa://24632 (98.05), maa://22499 (90.00), maa://22746 (100.00)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (99.10), maa://50121 (96.52)</t>
+          <t>maa://49983 (99.13), maa://50121 (96.64)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://27295 (97.56), maa://32509 (96.14), maa://31008 (94.89), maa://22754 (88.16)</t>
+          <t>maa://27295 (97.68), maa://32509 (96.19), maa://31008 (95.05), maa://22754 (88.16)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="X4" s="8" t="inlineStr">
         <is>
-          <t>maa://43217 (98.79)</t>
+          <t>maa://43217 (98.78)</t>
         </is>
       </c>
       <c r="Y4" s="19" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (90.91), maa://54105 (98.28), *maa://22744 (80.00)</t>
+          <t>maa://21245 (91.05), maa://54105 (98.38), *maa://22744 (80.00)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="P5" s="8" t="inlineStr">
         <is>
-          <t>maa://21919 (99.02), maa://21281 (81.25)</t>
+          <t>maa://21919 (99.04), maa://21281 (81.25)</t>
         </is>
       </c>
       <c r="Q5" s="19" t="n"/>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="X5" s="8" t="inlineStr">
         <is>
-          <t>maa://21290 (99.20)</t>
+          <t>maa://21290 (99.21)</t>
         </is>
       </c>
       <c r="Y5" s="19" t="n"/>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="D6" s="8" t="inlineStr">
         <is>
-          <t>maa://42407 (97.22)</t>
+          <t>maa://42407 (97.30)</t>
         </is>
       </c>
       <c r="E6" s="19" t="n"/>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="H6" s="8" t="inlineStr">
         <is>
-          <t>maa://24370 (97.32)</t>
+          <t>maa://24370 (97.39)</t>
         </is>
       </c>
       <c r="I6" s="19" t="n"/>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="L6" s="8" t="inlineStr">
         <is>
-          <t>maa://24839 (99.38)</t>
+          <t>maa://24839 (99.39)</t>
         </is>
       </c>
       <c r="M6" s="19" t="n"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (98.73), maa://30381 (95.00)</t>
+          <t>maa://31836 (98.76), maa://30381 (95.00)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="X6" s="8" t="inlineStr">
         <is>
-          <t>maa://52754 (96.10)</t>
+          <t>maa://52754 (96.23)</t>
         </is>
       </c>
       <c r="Y6" s="19" t="n"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="AF6" s="8" t="inlineStr">
         <is>
-          <t>*maa://33152 (79.56), ***maa://22770 (26.09)</t>
+          <t>*maa://33152 (79.71), ***maa://22770 (26.09)</t>
         </is>
       </c>
       <c r="AG6" s="16" t="n"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>maa://21955 (98.04)</t>
+          <t>maa://21955 (98.08)</t>
         </is>
       </c>
       <c r="E7" s="19" t="n"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>*maa://22763 (74.58), maa://64972 (95.00)</t>
+          <t>*maa://22763 (75.00), maa://64972 (95.00)</t>
         </is>
       </c>
       <c r="I7" s="19" t="n"/>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (98.65), maa://24957 (94.44)</t>
+          <t>maa://28624 (98.69), maa://24957 (94.55)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="P7" s="8" t="inlineStr">
         <is>
-          <t>maa://22750 (96.73)</t>
+          <t>maa://22750 (96.77)</t>
         </is>
       </c>
       <c r="Q7" s="19" t="n"/>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="T7" s="8" t="inlineStr">
         <is>
-          <t>maa://21291 (93.67)</t>
+          <t>maa://21291 (93.79)</t>
         </is>
       </c>
       <c r="U7" s="19" t="n"/>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (96.98), maa://22758 (81.82)</t>
+          <t>maa://22399 (97.05), maa://22758 (82.18)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="AF7" s="8" t="inlineStr">
         <is>
-          <t>maa://45272 (99.38)</t>
+          <t>maa://45272 (99.41)</t>
         </is>
       </c>
       <c r="AG7" s="16" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.23 13:20:11</t>
+          <t>更新日期：2025.09.26 13:19:42</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (89.68), *maa://39431 (58.33), **maa://37551 (50.00)</t>
+          <t>maa://21476 (89.94), *maa://39431 (58.33), **maa://37551 (50.00)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
-          <t>*maa://24371 (78.14)</t>
+          <t>*maa://24371 (78.49)</t>
         </is>
       </c>
       <c r="I8" s="19" t="n"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (91.55), maa://23252 (91.67), maa://37496 (98.28)</t>
+          <t>maa://32931 (91.38), maa://23252 (91.67), maa://37496 (98.28)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (95.98), maa://67587 (98.11)</t>
+          <t>maa://21411 (96.00), maa://67587 (98.36)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="AB8" s="8" t="inlineStr">
         <is>
-          <t>maa://25389 (94.39)</t>
+          <t>maa://25389 (94.50)</t>
         </is>
       </c>
       <c r="AC8" s="19" t="n"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>maa://24479 (84.07), *maa://21990 (51.72)</t>
+          <t>maa://24479 (84.24), *maa://21990 (51.72)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>maa://22765 (95.47), *maa://21915 (78.57)</t>
+          <t>maa://22765 (95.56), *maa://21915 (78.57)</t>
         </is>
       </c>
       <c r="E9" s="19" t="n"/>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (96.12), maa://39552 (86.67)</t>
+          <t>maa://22762 (96.23), maa://39552 (86.96)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="T9" s="8" t="inlineStr">
         <is>
-          <t>maa://26222 (99.42)</t>
+          <t>maa://26222 (99.44)</t>
         </is>
       </c>
       <c r="U9" s="19" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://52237 (99.74), maa://26223 (98.31)</t>
+          <t>maa://52237 (99.75), maa://26223 (98.31)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (94.96), maa://40166 (94.93)</t>
+          <t>maa://28711 (95.04), maa://40166 (95.02)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (91.09), maa://66916 (97.83)</t>
+          <t>maa://26206 (91.09), maa://66916 (97.95)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>maa://54000 (91.67)</t>
+          <t>maa://54000 (91.86)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (91.51), *maa://36669 (74.03)</t>
+          <t>maa://28977 (91.70), *maa://36669 (74.03)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (99.19), maa://22755 (91.38), maa://63521 (94.49)</t>
+          <t>maa://27395 (99.22), maa://22755 (91.43), maa://63521 (94.61)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://45828 (99.16), maa://22301 (97.64), maa://22726 (100.00)</t>
+          <t>maa://45828 (99.19), maa://22301 (97.64), maa://22726 (100.00)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>*maa://25021 (56.77), *maa://22733 (65.62), **maa://22761 (33.33)</t>
+          <t>*maa://25021 (56.33), *maa://22733 (64.62), **maa://22761 (33.33)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="D11" s="8" t="inlineStr">
         <is>
-          <t>maa://36707 (99.72)</t>
+          <t>maa://36707 (99.73)</t>
         </is>
       </c>
       <c r="E11" s="19" t="n"/>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="L11" s="8" t="inlineStr">
         <is>
-          <t>maa://21287 (93.55)</t>
+          <t>maa://21287 (93.68)</t>
         </is>
       </c>
       <c r="M11" s="19" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (93.18), maa://22501 (99.51), maa://64808 (100.00), maa://45521 (95.00)</t>
+          <t>maa://22747 (93.28), maa://22501 (99.53), maa://64808 (100.00), maa://45521 (95.16)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="X11" s="8" t="inlineStr">
         <is>
-          <t>maa://36713 (99.22)</t>
+          <t>maa://36713 (99.24)</t>
         </is>
       </c>
       <c r="Y11" s="19" t="n"/>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="AB11" s="8" t="inlineStr">
         <is>
-          <t>maa://29912 (99.69), maa://22516 (86.52)</t>
+          <t>maa://29912 (99.70), maa://22516 (86.52)</t>
         </is>
       </c>
       <c r="AC11" s="19" t="n"/>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="AF11" s="8" t="inlineStr">
         <is>
-          <t>maa://31203 (98.59)</t>
+          <t>maa://31203 (98.61)</t>
         </is>
       </c>
       <c r="AG11" s="16" t="n"/>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>maa://36678 (96.83), maa://30766 (91.18)</t>
+          <t>maa://36678 (97.01), maa://30766 (91.18)</t>
         </is>
       </c>
       <c r="E12" s="19" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (93.33), maa://54294 (96.30)</t>
+          <t>maa://21867 (93.41), maa://54294 (96.41)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (97.86), maa://64046 (98.51)</t>
+          <t>maa://63896 (97.93), maa://64046 (98.55)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="P12" s="8" t="inlineStr">
         <is>
-          <t>maa://57541 (90.62)</t>
+          <t>maa://57541 (91.18)</t>
         </is>
       </c>
       <c r="Q12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://37962 (98.73), maa://21485 (81.62), maa://22753 (92.80)</t>
+          <t>maa://37962 (98.77), maa://21485 (81.62), maa://22753 (92.80)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://36677 (99.11), maa://23669 (95.40), maa://39872 (98.08)</t>
+          <t>maa://36677 (99.00), maa://23669 (95.11), maa://39872 (98.20)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>maa://28932 (94.29)</t>
+          <t>maa://28932 (94.44)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (96.49), maa://36673 (93.85), maa://25001 (88.76)</t>
+          <t>maa://24999 (96.51), maa://36673 (93.94), maa://25001 (88.76)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.33), maa://66545 (98.97)</t>
+          <t>*maa://21248 (72.91), maa://66545 (98.99)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (97.44), maa://22583 (87.58)</t>
+          <t>maa://22676 (97.54), maa://22583 (87.82)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="X13" s="8" t="inlineStr">
         <is>
-          <t>maa://34957 (94.10)</t>
+          <t>maa://34957 (94.47)</t>
         </is>
       </c>
       <c r="Y13" s="19" t="n"/>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (93.59)</t>
+          <t>maa://39883 (93.86)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (98.92), maa://26245 (97.04), maa://36682 (98.22), maa://21288 (96.40)</t>
+          <t>maa://39841 (98.97), maa://26245 (97.06), maa://36682 (98.26), maa://21288 (96.40)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2330,7 +2330,7 @@
       </c>
       <c r="P14" s="8" t="inlineStr">
         <is>
-          <t>maa://23250 (99.62), maa://20107 (87.50), maa://22772 (100.00), maa://68732 (100.00)</t>
+          <t>maa://23250 (99.64), maa://20107 (87.50), maa://22772 (100.00), maa://68732 (100.00)</t>
         </is>
       </c>
       <c r="Q14" s="19" t="n"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://42751 (98.86), maa://22521 (95.07)</t>
+          <t>maa://42751 (98.90), maa://22521 (95.12)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="X14" s="8" t="inlineStr">
         <is>
-          <t>maa://37468 (97.87)</t>
+          <t>maa://37468 (97.96)</t>
         </is>
       </c>
       <c r="Y14" s="19" t="n"/>
@@ -2378,7 +2378,7 @@
       </c>
       <c r="AB14" s="8" t="inlineStr">
         <is>
-          <t>maa://22764 (98.83)</t>
+          <t>maa://22764 (98.85)</t>
         </is>
       </c>
       <c r="AC14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (85.33), maa://45058 (97.99), maa://22734 (84.85), *maa://36048 (74.58)</t>
+          <t>maa://22743 (85.28), maa://45058 (98.07), maa://22734 (84.85), *maa://36048 (74.72)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (96.75), maa://21478 (90.48)</t>
+          <t>maa://24304 (96.86), maa://21478 (90.48)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="L15" s="8" t="inlineStr">
         <is>
-          <t>*maa://21334 (69.09)</t>
+          <t>*maa://21334 (69.64)</t>
         </is>
       </c>
       <c r="M15" s="19" t="n"/>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="P15" s="8" t="inlineStr">
         <is>
-          <t>maa://24762 (97.63), *maa://22727 (70.00)</t>
+          <t>maa://24762 (97.58), *maa://22727 (70.00)</t>
         </is>
       </c>
       <c r="Q15" s="19" t="n"/>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://36666 (96.17), maa://21364 (83.61), *maa://22766 (70.71), maa://68306 (85.00)</t>
+          <t>maa://36666 (96.23), maa://21364 (83.64), *maa://22766 (70.71), maa://68306 (83.33)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://37650 (99.73), maa://21441 (96.62), maa://36679 (94.55)</t>
+          <t>maa://37650 (99.74), maa://21441 (96.62), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2590,7 +2590,7 @@
       </c>
       <c r="P16" s="8" t="inlineStr">
         <is>
-          <t>maa://28504 (96.00)</t>
+          <t>maa://28504 (96.09)</t>
         </is>
       </c>
       <c r="Q16" s="19" t="n"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://36674 (97.91), maa://22729 (96.04), *maa://28648 (77.89)</t>
+          <t>maa://36674 (97.97), maa://22729 (96.08), *maa://28648 (77.89)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2622,7 +2622,7 @@
       </c>
       <c r="X16" s="8" t="inlineStr">
         <is>
-          <t>maa://28501 (99.26), maa://28051 (96.88)</t>
+          <t>maa://28501 (99.28), maa://28051 (96.97)</t>
         </is>
       </c>
       <c r="Y16" s="19" t="n"/>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="AB16" s="8" t="inlineStr">
         <is>
-          <t>maa://26228 (97.83)</t>
+          <t>maa://26228 (97.86)</t>
         </is>
       </c>
       <c r="AC16" s="19" t="n"/>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>maa://23911 (90.23), maa://27755 (93.69), maa://67613 (99.29)</t>
+          <t>maa://23911 (90.38), maa://27755 (93.75), maa://67613 (99.36)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://39599 (98.14), maa://22430 (90.21)</t>
+          <t>maa://39599 (98.13), maa://22430 (90.21)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (82.64), maa://56238 (98.35)</t>
+          <t>maa://23890 (82.64), maa://56238 (98.43)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>maa://24570 (98.26)</t>
+          <t>maa://24570 (98.28)</t>
         </is>
       </c>
       <c r="E18" s="19" t="n"/>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="H18" s="8" t="inlineStr">
         <is>
-          <t>maa://24421 (95.04)</t>
+          <t>maa://24421 (95.21)</t>
         </is>
       </c>
       <c r="I18" s="19" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://52226 (99.69), maa://22466 (92.83)</t>
+          <t>maa://52226 (99.70), maa://22466 (92.83)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2866,7 +2866,7 @@
       </c>
       <c r="T18" s="8" t="inlineStr">
         <is>
-          <t>maa://24385 (98.41)</t>
+          <t>maa://24385 (98.44)</t>
         </is>
       </c>
       <c r="U18" s="19" t="n"/>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (98.63), maa://22741 (91.67)</t>
+          <t>maa://21917 (98.67), maa://22741 (92.31)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="AB18" s="8" t="inlineStr">
         <is>
-          <t>maa://24393 (98.94)</t>
+          <t>maa://24393 (98.96)</t>
         </is>
       </c>
       <c r="AC18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://47854 (92.59)</t>
+          <t>maa://47854 (92.70)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -2932,7 +2932,7 @@
       </c>
       <c r="D19" s="8" t="inlineStr">
         <is>
-          <t>maa://62850 (99.28)</t>
+          <t>maa://62850 (99.31)</t>
         </is>
       </c>
       <c r="E19" s="19" t="n"/>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (85.31), *maa://36668 (68.75)</t>
+          <t>maa://30709 (85.62), *maa://36668 (69.03)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://25198 (97.56), maa://36680 (99.02), maa://21432 (91.49)</t>
+          <t>maa://25198 (97.62), maa://36680 (99.06), maa://21432 (91.49)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3078,7 +3078,7 @@
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>maa://22864 (95.96)</t>
+          <t>maa://22864 (96.07)</t>
         </is>
       </c>
       <c r="I20" s="19" t="n"/>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (95.10)</t>
+          <t>maa://41331 (95.24)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="P20" s="8" t="inlineStr">
         <is>
-          <t>maa://37442 (98.44)</t>
+          <t>maa://37442 (98.48)</t>
         </is>
       </c>
       <c r="Q20" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (96.32), maa://56241 (98.23), maa://49976 (88.46)</t>
+          <t>maa://50085 (96.43), maa://56241 (98.23), maa://49976 (88.46)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>maa://21261 (98.99)</t>
+          <t>maa://21261 (99.03)</t>
         </is>
       </c>
       <c r="E21" s="19" t="n"/>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="H21" s="8" t="inlineStr">
         <is>
-          <t>maa://24372 (98.83)</t>
+          <t>maa://24372 (98.85)</t>
         </is>
       </c>
       <c r="I21" s="19" t="n"/>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="L21" s="8" t="inlineStr">
         <is>
-          <t>maa://31731 (96.40)</t>
+          <t>maa://31731 (96.43)</t>
         </is>
       </c>
       <c r="M21" s="19" t="n"/>
@@ -3240,7 +3240,7 @@
       </c>
       <c r="P21" s="8" t="inlineStr">
         <is>
-          <t>maa://24381 (84.38)</t>
+          <t>maa://24381 (81.82)</t>
         </is>
       </c>
       <c r="Q21" s="19" t="n"/>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (98.27), maa://20110 (87.01)</t>
+          <t>maa://34946 (98.34), maa://20110 (87.01)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="AB21" s="8" t="inlineStr">
         <is>
-          <t>maa://21443 (86.57), maa://52223 (82.21)</t>
+          <t>maa://21443 (86.62), maa://52223 (82.59)</t>
         </is>
       </c>
       <c r="AC21" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22432 (93.74), maa://22524 (83.10), maa://64221 (97.74)</t>
+          <t>maa://22432 (93.93), maa://22524 (83.16), maa://64221 (97.83)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>maa://25236 (99.16)</t>
+          <t>maa://25236 (99.19)</t>
         </is>
       </c>
       <c r="I22" s="19" t="n"/>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>maa://27127 (83.04), *maa://22751 (70.93), maa://66865 (99.37)</t>
+          <t>maa://27127 (83.04), *maa://22751 (70.93), maa://66865 (99.38)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3386,7 +3386,7 @@
       </c>
       <c r="T22" s="8" t="inlineStr">
         <is>
-          <t>maa://38495 (84.44)</t>
+          <t>maa://38495 (84.78)</t>
         </is>
       </c>
       <c r="U22" s="19" t="n"/>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://37649 (94.21), maa://21282 (98.92)</t>
+          <t>maa://37649 (94.44), maa://21282 (98.95)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="AB22" s="8" t="inlineStr">
         <is>
-          <t>maa://23656 (99.48)</t>
+          <t>maa://23656 (99.49)</t>
         </is>
       </c>
       <c r="AC22" s="19" t="n"/>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="AF22" s="8" t="inlineStr">
         <is>
-          <t>maa://29658 (97.06)</t>
+          <t>maa://29658 (97.12)</t>
         </is>
       </c>
       <c r="AG22" s="16" t="n"/>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>*maa://41753 (65.15), ***maa://28036 (30.00)</t>
+          <t>*maa://41753 (66.18), **maa://28036 (30.77)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (98.57), maa://39875 (95.73)</t>
+          <t>maa://39756 (98.57), maa://39875 (95.76)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (96.74), maa://29748 (81.82), *maa://37566 (78.12)</t>
+          <t>maa://30587 (96.65), maa://29748 (81.68), *maa://37566 (78.12)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="T23" s="8" t="inlineStr">
         <is>
-          <t>maa://31212 (95.28), maa://24387 (84.44), maa://67084 (87.50)</t>
+          <t>maa://31212 (94.50), maa://24387 (84.44), maa://67084 (87.50)</t>
         </is>
       </c>
       <c r="U23" s="19" t="n"/>
@@ -3532,7 +3532,7 @@
       </c>
       <c r="X23" s="8" t="inlineStr">
         <is>
-          <t>*maa://28503 (59.48)</t>
+          <t>*maa://28503 (60.00)</t>
         </is>
       </c>
       <c r="Y23" s="19" t="n"/>
@@ -3548,7 +3548,7 @@
       </c>
       <c r="AB23" s="8" t="inlineStr">
         <is>
-          <t>maa://29652 (96.39)</t>
+          <t>maa://29652 (96.47)</t>
         </is>
       </c>
       <c r="AC23" s="19" t="n"/>
@@ -3564,7 +3564,7 @@
       </c>
       <c r="AF23" s="8" t="inlineStr">
         <is>
-          <t>maa://31489 (98.21)</t>
+          <t>maa://31489 (98.31)</t>
         </is>
       </c>
       <c r="AG23" s="16" t="n"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (84.97), maa://46650 (89.92)</t>
+          <t>maa://24368 (85.22), maa://46650 (90.08)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (96.08), maa://23504 (94.04), *maa://25141 (79.74), maa://52227 (97.67), *maa://36663 (79.25)</t>
+          <t>maa://29988 (96.23), maa://23504 (94.05), *maa://25141 (79.74), maa://52227 (97.35), *maa://36663 (79.44)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://64165 (99.24), maa://22523 (80.09), maa://29910 (94.20), maa://45831 (93.55)</t>
+          <t>maa://64165 (99.27), maa://22523 (80.09), maa://29910 (94.20), maa://45831 (93.55)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (96.46), maa://63016 (99.07)</t>
+          <t>maa://29753 (96.53), maa://63016 (99.10)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>*maa://29063 (75.88), *maa://25311 (70.92), maa://45047 (87.67)</t>
+          <t>*maa://29063 (76.02), *maa://25311 (70.42), maa://45047 (88.00)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3744,7 +3744,7 @@
       </c>
       <c r="L25" s="8" t="inlineStr">
         <is>
-          <t>maa://24378 (93.75), maa://68415 (100.00)</t>
+          <t>maa://24378 (93.83), maa://68415 (100.00)</t>
         </is>
       </c>
       <c r="M25" s="19" t="n"/>
@@ -3760,7 +3760,7 @@
       </c>
       <c r="P25" s="8" t="inlineStr">
         <is>
-          <t>maa://24382 (96.00)</t>
+          <t>maa://24382 (96.08)</t>
         </is>
       </c>
       <c r="Q25" s="19" t="n"/>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="T25" s="8" t="inlineStr">
         <is>
-          <t>maa://20109 (96.38), maa://22545 (100.00)</t>
+          <t>maa://20109 (96.21), maa://22545 (100.00)</t>
         </is>
       </c>
       <c r="U25" s="19" t="n"/>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="X25" s="8" t="inlineStr">
         <is>
-          <t>maa://29890 (91.06)</t>
+          <t>maa://29890 (91.20)</t>
         </is>
       </c>
       <c r="Y25" s="19" t="n"/>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (93.22), *maa://24516 (79.80), maa://26001 (83.33), maa://68311 (100.00)</t>
+          <t>maa://31215 (93.32), *maa://24516 (79.80), maa://26001 (83.33), maa://68311 (100.00)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (98.00), maa://36676 (99.83), maa://24621 (96.86), maa://22771 (88.24), maa://37772 (83.33)</t>
+          <t>maa://20108 (98.05), maa://36676 (99.84), maa://24621 (96.86), maa://22771 (88.24), maa://37772 (83.33)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://56374 (100.00), maa://41802 (96.15)</t>
+          <t>maa://56374 (100.00), maa://41802 (96.36)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3858,7 +3858,7 @@
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
-          <t>maa://56240 (96.39), maa://24913 (92.17)</t>
+          <t>maa://56240 (96.02), maa://24913 (92.24)</t>
         </is>
       </c>
       <c r="I26" s="19" t="n"/>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="P26" s="8" t="inlineStr">
         <is>
-          <t>maa://39870 (94.29), maa://56625 (100.00)</t>
+          <t>maa://39870 (94.44), maa://56625 (100.00)</t>
         </is>
       </c>
       <c r="Q26" s="19" t="n"/>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="AB26" s="8" t="inlineStr">
         <is>
-          <t>maa://42235 (98.43)</t>
+          <t>maa://42235 (98.34)</t>
         </is>
       </c>
       <c r="AC26" s="19" t="n"/>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="AF26" s="8" t="inlineStr">
         <is>
-          <t>*maa://30511 (72.50), **maa://29760 (47.62)</t>
+          <t>*maa://30511 (71.60), **maa://29760 (45.45)</t>
         </is>
       </c>
       <c r="AG26" s="16" t="n"/>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>maa://39601 (90.48), maa://34494 (96.47)</t>
+          <t>maa://39601 (90.74), maa://34494 (95.35)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4004,7 +4004,7 @@
       </c>
       <c r="L27" s="8" t="inlineStr">
         <is>
-          <t>maa://28071 (88.89)</t>
+          <t>maa://28071 (89.29)</t>
         </is>
       </c>
       <c r="M27" s="19" t="n"/>
@@ -4020,7 +4020,7 @@
       </c>
       <c r="P27" s="8" t="inlineStr">
         <is>
-          <t>maa://56400 (93.33)</t>
+          <t>maa://56400 (93.75)</t>
         </is>
       </c>
       <c r="Q27" s="19" t="n"/>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="T27" s="8" t="inlineStr">
         <is>
-          <t>maa://30624 (89.53)</t>
+          <t>maa://30624 (89.71)</t>
         </is>
       </c>
       <c r="U27" s="19" t="n"/>
@@ -4084,7 +4084,7 @@
       </c>
       <c r="AF27" s="8" t="inlineStr">
         <is>
-          <t>maa://24023 (97.69)</t>
+          <t>maa://24023 (97.73)</t>
         </is>
       </c>
       <c r="AG27" s="16" t="n"/>
@@ -4102,7 +4102,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (95.79), maa://25725 (85.16)</t>
+          <t>maa://24465 (95.87), maa://25725 (85.27)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="L28" s="8" t="inlineStr">
         <is>
-          <t>maa://30770 (89.66)</t>
+          <t>maa://30770 (90.00)</t>
         </is>
       </c>
       <c r="M28" s="19" t="n"/>
@@ -4166,7 +4166,7 @@
       </c>
       <c r="T28" s="8" t="inlineStr">
         <is>
-          <t>maa://29765 (93.05), maa://23263 (96.18)</t>
+          <t>maa://29765 (93.33), maa://23263 (96.24)</t>
         </is>
       </c>
       <c r="U28" s="19" t="n"/>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (97.28), maa://41749 (97.16)</t>
+          <t>maa://39929 (97.36), maa://41749 (97.19)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (94.14), maa://65700 (98.58)</t>
+          <t>maa://36660 (94.22), maa://65700 (98.64)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4232,7 +4232,7 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>maa://31694 (99.30)</t>
+          <t>maa://31694 (99.31)</t>
         </is>
       </c>
       <c r="E29" s="19" t="n"/>
@@ -4248,7 +4248,7 @@
       </c>
       <c r="H29" s="8" t="inlineStr">
         <is>
-          <t>*maa://25175 (50.46)</t>
+          <t>*maa://25175 (50.91)</t>
         </is>
       </c>
       <c r="I29" s="19" t="n"/>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (97.76), maa://31400 (98.02), maa://28440 (86.34)</t>
+          <t>maa://28432 (97.81), maa://31400 (98.06), maa://28440 (86.42)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4280,7 +4280,7 @@
       </c>
       <c r="P29" s="8" t="inlineStr">
         <is>
-          <t>maa://54169 (97.14)</t>
+          <t>maa://54169 (97.25)</t>
         </is>
       </c>
       <c r="Q29" s="19" t="n"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://42865 (92.28)</t>
+          <t>maa://42865 (92.11)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (95.24), maa://64191 (97.30)</t>
+          <t>maa://45792 (95.38), maa://64191 (97.44)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="L30" s="8" t="inlineStr">
         <is>
-          <t>maa://30442 (97.39)</t>
+          <t>maa://30442 (97.44)</t>
         </is>
       </c>
       <c r="M30" s="19" t="n"/>
@@ -4410,7 +4410,7 @@
       </c>
       <c r="P30" s="8" t="inlineStr">
         <is>
-          <t>maa://21442 (99.56), maa://66611 (100.00), maa://68394 (100.00)</t>
+          <t>maa://21442 (99.57), maa://66611 (100.00), maa://68394 (100.00)</t>
         </is>
       </c>
       <c r="Q30" s="19" t="n"/>
@@ -4426,7 +4426,7 @@
       </c>
       <c r="T30" s="8" t="inlineStr">
         <is>
-          <t>maa://32940 (80.95), maa://24388 (96.00)</t>
+          <t>maa://32940 (80.95), maa://24388 (96.15)</t>
         </is>
       </c>
       <c r="U30" s="19" t="n"/>
@@ -4458,7 +4458,7 @@
       </c>
       <c r="AB30" s="8" t="inlineStr">
         <is>
-          <t>maa://42979 (99.54), maa://45822 (100.00), maa://45045 (90.91)</t>
+          <t>maa://42979 (99.55), maa://45822 (100.00), maa://45045 (90.91)</t>
         </is>
       </c>
       <c r="AC30" s="19" t="n"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (97.95), maa://36258 (92.97), maa://43904 (89.47)</t>
+          <t>maa://35926 (97.98), maa://36258 (93.08), maa://43904 (90.00)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4556,7 +4556,7 @@
       </c>
       <c r="T31" s="8" t="inlineStr">
         <is>
-          <t>maa://30711 (96.52), maa://30768 (100.00)</t>
+          <t>maa://30711 (96.64), maa://30768 (100.00)</t>
         </is>
       </c>
       <c r="U31" s="19" t="n"/>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://36667 (99.63), maa://21895 (97.96), maa://22760 (100.00)</t>
+          <t>maa://36667 (99.64), maa://21895 (97.97), maa://22760 (100.00)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (99.23), maa://41108 (87.72), maa://41238 (98.12), maa://45523 (100.00)</t>
+          <t>maa://42859 (99.26), maa://41108 (87.72), maa://41238 (98.12), maa://45523 (100.00)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="X32" s="8" t="inlineStr">
         <is>
-          <t>maa://64104 (97.27)</t>
+          <t>maa://64104 (97.32)</t>
         </is>
       </c>
       <c r="Y32" s="19" t="n"/>
@@ -4734,7 +4734,7 @@
       </c>
       <c r="AF32" s="8" t="inlineStr">
         <is>
-          <t>maa://42408 (94.59)</t>
+          <t>maa://42408 (94.87)</t>
         </is>
       </c>
       <c r="AG32" s="16" t="n"/>
@@ -4795,12 +4795,12 @@
       </c>
       <c r="O33" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (94.41), *maa://22730 (70.59)</t>
+          <t>maa://21956 (94.61), *maa://22730 (70.59), maa://69135 (100.00)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="T33" s="8" t="inlineStr">
         <is>
-          <t>maa://45558 (93.33)</t>
+          <t>maa://45558 (90.32)</t>
         </is>
       </c>
       <c r="U33" s="19" t="n"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (99.17), maa://56235 (99.72)</t>
+          <t>maa://48817 (99.20), maa://56235 (99.73)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="T34" s="8" t="inlineStr">
         <is>
-          <t>maa://24526 (96.98)</t>
+          <t>maa://24526 (97.06)</t>
         </is>
       </c>
       <c r="U34" s="19" t="n"/>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="AB34" s="8" t="inlineStr">
         <is>
-          <t>maa://64329 (97.56)</t>
+          <t>maa://64329 (97.67)</t>
         </is>
       </c>
       <c r="AC34" s="19" t="n"/>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
-          <t>maa://41296 (99.24)</t>
+          <t>maa://41296 (99.25)</t>
         </is>
       </c>
       <c r="M35" s="19" t="n"/>
@@ -5076,7 +5076,7 @@
       </c>
       <c r="T35" s="8" t="inlineStr">
         <is>
-          <t>maa://24842 (96.55)</t>
+          <t>maa://24842 (96.63)</t>
         </is>
       </c>
       <c r="U35" s="19" t="n"/>
@@ -5158,7 +5158,7 @@
       </c>
       <c r="H36" s="8" t="inlineStr">
         <is>
-          <t>maa://24375 (94.29)</t>
+          <t>maa://24375 (94.44)</t>
         </is>
       </c>
       <c r="I36" s="19" t="n"/>
@@ -5206,7 +5206,7 @@
       </c>
       <c r="T36" s="8" t="inlineStr">
         <is>
-          <t>maa://27613 (99.53)</t>
+          <t>maa://27613 (99.54)</t>
         </is>
       </c>
       <c r="U36" s="19" t="n"/>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="AB36" s="19" t="inlineStr">
         <is>
-          <t>maa://64106 (96.97)</t>
+          <t>maa://64106 (97.06)</t>
         </is>
       </c>
       <c r="AC36" s="19" t="n"/>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="H37" s="8" t="inlineStr">
         <is>
-          <t>*maa://24374 (57.38)</t>
+          <t>*maa://24374 (58.06)</t>
         </is>
       </c>
       <c r="I37" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (99.18), maa://56336 (99.32), maa://47069 (88.10), maa://45789 (100.00)</t>
+          <t>maa://45718 (99.20), maa://56336 (99.34), maa://47069 (86.36), maa://45789 (100.00)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="P37" s="8" t="inlineStr">
         <is>
-          <t>maa://21280 (97.52)</t>
+          <t>maa://21280 (97.57)</t>
         </is>
       </c>
       <c r="Q37" s="19" t="n"/>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="P38" s="8" t="inlineStr">
         <is>
-          <t>maa://24383 (81.32)</t>
+          <t>maa://24383 (81.72)</t>
         </is>
       </c>
       <c r="Q38" s="19" t="n"/>
@@ -5482,7 +5482,7 @@
       </c>
       <c r="AF38" s="8" t="inlineStr">
         <is>
-          <t>maa://36697 (95.80), maa://68397 (99.15)</t>
+          <t>maa://36697 (95.83), maa://68397 (99.35)</t>
         </is>
       </c>
       <c r="AG38" s="16" t="n"/>
@@ -5503,7 +5503,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://25199 (84.67), maa://45059 (93.02), maa://30434 (95.26), maa://44165 (85.71)</t>
+          <t>maa://25199 (84.78), maa://45059 (93.70), maa://30434 (95.26), maa://44165 (85.71)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://47093 (98.10), maa://24709 (93.90)</t>
+          <t>maa://47093 (98.15), maa://24709 (93.93)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (95.45), maa://45790 (87.67)</t>
+          <t>maa://47079 (95.58), maa://45790 (87.67)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5583,7 +5583,7 @@
       </c>
       <c r="AF39" s="8" t="inlineStr">
         <is>
-          <t>maa://62953 (96.77)</t>
+          <t>maa://62953 (96.72)</t>
         </is>
       </c>
       <c r="AG39" s="16" t="n"/>
@@ -5636,7 +5636,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (98.05), maa://21386 (95.92), maa://36664 (89.61), *maa://45550 (72.73)</t>
+          <t>maa://23278 (98.09), maa://21386 (95.94), maa://36664 (89.61), *maa://45550 (72.73)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://65283 (96.65), maa://64205 (93.75)</t>
+          <t>maa://65283 (96.74), maa://64205 (93.75)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="P41" s="8" t="inlineStr">
         <is>
-          <t>maa://43177 (95.33)</t>
+          <t>maa://43177 (95.50)</t>
         </is>
       </c>
       <c r="Q41" s="19" t="n"/>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>*maa://22525 (70.69), maa://21284 (97.53)</t>
+          <t>*maa://22525 (70.39), maa://21284 (97.62)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -6008,7 +6008,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (98.21), maa://56386 (99.37), maa://27728 (96.40)</t>
+          <t>maa://29768 (98.23), maa://56386 (99.39), maa://27728 (96.40)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6056,7 +6056,7 @@
       </c>
       <c r="T44" s="8" t="inlineStr">
         <is>
-          <t>maa://39366 (93.26)</t>
+          <t>maa://39366 (93.41)</t>
         </is>
       </c>
       <c r="U44" s="19" t="n"/>
@@ -6088,12 +6088,12 @@
       </c>
       <c r="G45" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://42459 (98.66), maa://21229 (85.53), maa://30807 (94.62)</t>
+          <t>maa://42459 (98.71), maa://21229 (85.59), maa://30807 (94.62), *maa://22767 (70.59)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6125,7 +6125,7 @@
       </c>
       <c r="T45" s="8" t="inlineStr">
         <is>
-          <t>*maa://39364 (66.45)</t>
+          <t>*maa://39364 (66.46)</t>
         </is>
       </c>
       <c r="U45" s="19" t="n"/>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (95.53), maa://43901 (96.12)</t>
+          <t>maa://35931 (95.66), maa://43901 (96.27)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6231,7 +6231,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (97.49), maa://29661 (97.17), maa://56236 (99.77), maa://28038 (84.62)</t>
+          <t>maa://27410 (97.50), maa://29661 (97.20), maa://56236 (99.78), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6263,7 +6263,7 @@
       </c>
       <c r="T47" s="8" t="inlineStr">
         <is>
-          <t>maa://67476 (99.55), maa://68392 (100.00)</t>
+          <t>maa://67476 (99.56), maa://68392 (100.00)</t>
         </is>
       </c>
       <c r="U47" s="19" t="n"/>
@@ -6385,7 +6385,7 @@
       </c>
       <c r="P49" s="8" t="inlineStr">
         <is>
-          <t>*maa://39643 (79.10)</t>
+          <t>*maa://39643 (78.99)</t>
         </is>
       </c>
       <c r="Q49" s="19" t="n"/>
@@ -6401,7 +6401,7 @@
       </c>
       <c r="T49" s="19" t="inlineStr">
         <is>
-          <t>maa://67231 (99.06)</t>
+          <t>maa://67231 (99.09)</t>
         </is>
       </c>
       <c r="U49" s="19" t="n"/>
@@ -6438,7 +6438,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>maa://62852 (93.04)</t>
+          <t>maa://62852 (93.05)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6472,7 +6472,7 @@
       </c>
       <c r="H51" s="8" t="inlineStr">
         <is>
-          <t>maa://30769 (88.89)</t>
+          <t>maa://30769 (89.66)</t>
         </is>
       </c>
       <c r="I51" s="19" t="n"/>
@@ -6522,7 +6522,7 @@
       </c>
       <c r="H52" s="8" t="inlineStr">
         <is>
-          <t>maa://24376 (99.00)</t>
+          <t>maa://24376 (99.05)</t>
         </is>
       </c>
       <c r="I52" s="19" t="n"/>
@@ -6538,7 +6538,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (99.34), maa://59378 (93.83), maa://65511 (100.00)</t>
+          <t>maa://59394 (99.36), maa://59378 (93.83), maa://65511 (100.00)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6572,7 +6572,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (97.81)</t>
+          <t>maa://32534 (97.87)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -6656,7 +6656,7 @@
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>maa://32532 (97.77)</t>
+          <t>maa://32532 (97.81)</t>
         </is>
       </c>
       <c r="I55" s="19" t="n"/>
@@ -6708,7 +6708,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://56237 (99.30), maa://25176 (98.77)</t>
+          <t>maa://56237 (98.69), maa://25176 (98.77)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6726,7 +6726,7 @@
       </c>
       <c r="H58" s="8" t="inlineStr">
         <is>
-          <t>*maa://37964 (65.81)</t>
+          <t>*maa://37964 (65.25)</t>
         </is>
       </c>
       <c r="I58" s="19" t="n"/>
@@ -6744,7 +6744,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (98.45), maa://27746 (89.01)</t>
+          <t>maa://31270 (98.32), maa://27746 (89.25)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -6762,7 +6762,7 @@
       </c>
       <c r="H60" s="8" t="inlineStr">
         <is>
-          <t>maa://40438 (91.25)</t>
+          <t>maa://40438 (91.53)</t>
         </is>
       </c>
       <c r="I60" s="19" t="n"/>
@@ -6798,7 +6798,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (97.73), maa://56228 (99.33), maa://43903 (100.00)</t>
+          <t>maa://42981 (96.67), maa://56228 (98.68), maa://43903 (100.00)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6816,7 +6816,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (99.38), *maa://59693 (74.47), maa://59413 (97.06)</t>
+          <t>maa://59534 (99.40), *maa://59693 (74.47), maa://59413 (97.30)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7032,7 +7032,7 @@
       </c>
       <c r="H75" s="19" t="inlineStr">
         <is>
-          <t>*maa://67748 (80.00)</t>
+          <t>maa://67748 (82.86)</t>
         </is>
       </c>
       <c r="I75" s="19" t="n"/>
@@ -7174,7 +7174,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.23 13:20:11</t>
+          <t>更新日期：2025.09.26 13:19:42</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8362,7 +8362,7 @@
       </c>
       <c r="D23" s="13" t="inlineStr">
         <is>
-          <t>maa://20876 (96.36), maa://63498 (100.00)</t>
+          <t>maa://20876 (96.43), maa://63498 (100.00)</t>
         </is>
       </c>
       <c r="E23" s="14" t="inlineStr">
@@ -8686,7 +8686,7 @@
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>maa://20863 (90.64), maa://20832 (99.21), maa://20727 (100.00)</t>
+          <t>maa://20863 (90.67), maa://20832 (99.22), maa://20727 (100.00)</t>
         </is>
       </c>
       <c r="E29" s="14" t="inlineStr">
@@ -8848,7 +8848,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (90.16), maa://36866 (96.97), maa://62759 (100.00), maa://45572 (88.24), maa://27794 (100.00), maa://20960 (100.00), maa://20843 (100.00), **maa://24483 (50.00), maa://20862 (83.33), *maa://20893 (77.78)</t>
+          <t>maa://36644 (90.20), maa://36866 (96.97), maa://62759 (100.00), maa://45572 (88.24), maa://27794 (100.00), maa://20960 (100.00), maa://20843 (100.00), **maa://24483 (50.00), maa://20862 (83.33), *maa://20893 (77.78)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -9334,7 +9334,7 @@
       </c>
       <c r="D41" s="13" t="inlineStr">
         <is>
-          <t>maa://20892 (82.35)</t>
+          <t>maa://20892 (82.52)</t>
         </is>
       </c>
       <c r="E41" s="14" t="inlineStr">
@@ -10144,7 +10144,7 @@
       </c>
       <c r="D56" s="13" t="inlineStr">
         <is>
-          <t>maa://44235 (98.41), maa://45604 (100.00), maa://20961 (100.00), maa://44220 (100.00), maa://20910 (100.00)</t>
+          <t>maa://44235 (98.41), maa://45604 (100.00), maa://20961 (100.00), maa://20910 (100.00), maa://44220 (100.00)</t>
         </is>
       </c>
       <c r="E56" s="14" t="inlineStr">
@@ -10360,7 +10360,7 @@
       </c>
       <c r="D60" s="13" t="inlineStr">
         <is>
-          <t>maa://38298 (88.29)</t>
+          <t>maa://38298 (88.39)</t>
         </is>
       </c>
       <c r="E60" s="14" t="inlineStr">
@@ -10409,12 +10409,12 @@
       </c>
       <c r="C61" s="12" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (99.22), maa://31559 (93.88), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00)</t>
+          <t>maa://20841 (99.22), maa://31559 (93.88), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00), maa://66633 (100.00)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -10792,7 +10792,7 @@
       </c>
       <c r="D68" s="13" t="inlineStr">
         <is>
-          <t>maa://20976 (97.82), maa://20815 (100.00)</t>
+          <t>maa://20976 (97.83), maa://20815 (100.00)</t>
         </is>
       </c>
       <c r="E68" s="14" t="inlineStr">
@@ -10954,7 +10954,7 @@
       </c>
       <c r="D71" s="13" t="inlineStr">
         <is>
-          <t>maa://20943 (99.47), maa://30673 (100.00), maa://30672 (100.00), maa://20856 (100.00)</t>
+          <t>maa://20943 (99.48), maa://30673 (100.00), maa://30672 (100.00), maa://20856 (100.00)</t>
         </is>
       </c>
       <c r="E71" s="14" t="inlineStr">
@@ -11008,7 +11008,7 @@
       </c>
       <c r="D72" s="13" t="inlineStr">
         <is>
-          <t>maa://36643 (98.44), maa://36864 (98.11), maa://39140 (100.00), maa://66335 (100.00)</t>
+          <t>maa://36643 (98.45), maa://36864 (98.11), maa://39140 (100.00), maa://66335 (100.00)</t>
         </is>
       </c>
       <c r="E72" s="14" t="inlineStr">
@@ -11872,7 +11872,7 @@
       </c>
       <c r="D88" s="13" t="inlineStr">
         <is>
-          <t>maa://24472 (90.97), *maa://35841 (65.22)</t>
+          <t>maa://24472 (91.01), *maa://35841 (65.22)</t>
         </is>
       </c>
       <c r="E88" s="14" t="inlineStr">
@@ -12358,7 +12358,7 @@
       </c>
       <c r="D97" s="13" t="inlineStr">
         <is>
-          <t>maa://20991 (100.00), maa://51015 (88.10)</t>
+          <t>maa://20991 (100.00), maa://51015 (88.37)</t>
         </is>
       </c>
       <c r="E97" s="14" t="inlineStr">
@@ -12952,7 +12952,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.71), maa://25018 (96.93), maa://25776 (92.21), maa://28361 (95.45), maa://25772 (94.12), maa://56588 (93.33), maa://45194 (85.71), maa://32653 (81.25), maa://25161 (83.33), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
+          <t>maa://51881 (98.72), maa://25018 (96.93), maa://25776 (92.21), maa://28361 (95.45), maa://25772 (94.12), maa://56588 (93.33), maa://45194 (85.71), maa://32653 (81.25), maa://25161 (83.33), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13006,7 +13006,7 @@
       </c>
       <c r="D109" s="13" t="inlineStr">
         <is>
-          <t>maa://36646 (98.89), maa://25774 (94.59), maa://35996 (97.89), maa://22469 (92.06), maa://30668 (86.67), maa://67286 (100.00)</t>
+          <t>maa://36646 (98.90), maa://25774 (94.59), maa://35996 (97.89), maa://22469 (92.06), maa://30668 (86.67), maa://67286 (100.00)</t>
         </is>
       </c>
       <c r="E109" s="14" t="inlineStr">
@@ -14842,7 +14842,7 @@
       </c>
       <c r="D143" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (97.79), *maa://23736 (52.44), maa://31185 (91.67), maa://30306 (100.00)</t>
+          <t>maa://28484 (97.80), *maa://23736 (52.44), maa://31185 (91.67), maa://30306 (100.00)</t>
         </is>
       </c>
       <c r="E143" s="14" t="inlineStr">
@@ -15706,7 +15706,7 @@
       </c>
       <c r="D159" s="13" t="inlineStr">
         <is>
-          <t>maa://20959 (90.91)</t>
+          <t>maa://20959 (91.67)</t>
         </is>
       </c>
       <c r="E159" s="14" t="inlineStr">
@@ -15760,7 +15760,7 @@
       </c>
       <c r="D160" s="13" t="inlineStr">
         <is>
-          <t>maa://44232 (98.47), maa://45603 (90.62), *maa://65963 (75.00), *maa://63114 (66.67)</t>
+          <t>maa://44232 (98.47), maa://45603 (90.62), *maa://65963 (80.00), *maa://63114 (66.67)</t>
         </is>
       </c>
       <c r="E160" s="14" t="inlineStr">
@@ -16192,7 +16192,7 @@
       </c>
       <c r="D168" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (92.23), maa://29627 (92.95), maa://29659 (87.50), maa://49074 (94.20), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
+          <t>maa://29633 (92.26), maa://29627 (92.95), maa://29659 (87.50), maa://49074 (94.20), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
         </is>
       </c>
       <c r="E168" s="14" t="inlineStr">
@@ -17812,7 +17812,7 @@
       </c>
       <c r="D198" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.43), maa://35854 (84.75), maa://50388 (98.24), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (94.44)</t>
+          <t>maa://44224 (90.46), maa://35854 (84.75), maa://50388 (98.25), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (94.59)</t>
         </is>
       </c>
       <c r="E198" s="14" t="inlineStr">
@@ -18730,7 +18730,7 @@
       </c>
       <c r="D215" s="13" t="inlineStr">
         <is>
-          <t>maa://64044 (95.92)</t>
+          <t>maa://64044 (96.00)</t>
         </is>
       </c>
       <c r="E215" s="14" t="inlineStr">
@@ -19054,7 +19054,7 @@
       </c>
       <c r="D221" s="13" t="inlineStr">
         <is>
-          <t>**maa://26496 (36.36), *maa://20995 (54.55)</t>
+          <t>**maa://26496 (41.67), *maa://20995 (54.55)</t>
         </is>
       </c>
       <c r="E221" s="14" t="inlineStr">
@@ -20188,7 +20188,7 @@
       </c>
       <c r="D242" s="13" t="inlineStr">
         <is>
-          <t>*maa://30667 (78.85), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (57.81), maa://39588 (86.67), *maa://64079 (78.57), maa://65726 (87.50), maa://68226 (100.00)</t>
+          <t>*maa://30667 (78.85), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (58.46), maa://39588 (86.67), *maa://64079 (78.57), maa://65726 (87.50), maa://68226 (100.00)</t>
         </is>
       </c>
       <c r="E242" s="14" t="inlineStr">
@@ -22024,7 +22024,7 @@
       </c>
       <c r="D276" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.71), maa://51630 (96.26), maa://56588 (93.33), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (41.67), *maa://66758 (75.00)</t>
+          <t>maa://51881 (98.72), maa://51630 (96.26), maa://56588 (93.33), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (41.67), *maa://66758 (75.00)</t>
         </is>
       </c>
       <c r="E276" s="14" t="inlineStr">
@@ -24346,7 +24346,7 @@
       </c>
       <c r="D319" s="13" t="inlineStr">
         <is>
-          <t>maa://25367 (99.35)</t>
+          <t>maa://25367 (99.36)</t>
         </is>
       </c>
       <c r="E319" s="14" t="inlineStr">
@@ -24400,7 +24400,7 @@
       </c>
       <c r="D320" s="13" t="inlineStr">
         <is>
-          <t>*maa://62755 (70.59), maa://62761 (90.91)</t>
+          <t>*maa://62755 (70.59), maa://62761 (91.67)</t>
         </is>
       </c>
       <c r="E320" s="14" t="inlineStr">
@@ -25102,7 +25102,7 @@
       </c>
       <c r="D333" s="15" t="inlineStr">
         <is>
-          <t>maa://40956 (93.94)</t>
+          <t>maa://40956 (94.00)</t>
         </is>
       </c>
       <c r="E333" s="15" t="inlineStr">
@@ -25750,7 +25750,7 @@
       </c>
       <c r="D345" s="22" t="inlineStr">
         <is>
-          <t>maa://38295 (95.28), maa://49332 (90.91)</t>
+          <t>maa://38295 (95.33), maa://49332 (90.91)</t>
         </is>
       </c>
       <c r="E345" s="22" t="inlineStr">
@@ -26020,7 +26020,7 @@
       </c>
       <c r="D350" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (97.59), maa://32415 (84.88), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
+          <t>maa://32647 (97.59), maa://32415 (84.73), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E350" s="22" t="inlineStr">
@@ -26290,7 +26290,7 @@
       </c>
       <c r="D355" s="22" t="inlineStr">
         <is>
-          <t>maa://34865 (97.88), maa://34717 (94.20), *maa://45066 (71.43)</t>
+          <t>maa://34865 (97.89), maa://34717 (94.20), *maa://45066 (71.43)</t>
         </is>
       </c>
       <c r="E355" s="22" t="inlineStr">
@@ -26506,7 +26506,7 @@
       </c>
       <c r="D359" s="22" t="inlineStr">
         <is>
-          <t>maa://36868 (99.54), maa://35996 (97.89), maa://47349 (97.47), **maa://39217 (38.89)</t>
+          <t>maa://36868 (99.54), maa://35996 (97.89), maa://47349 (97.50), **maa://39217 (38.89)</t>
         </is>
       </c>
       <c r="E359" s="22" t="inlineStr">
@@ -26776,7 +26776,7 @@
       </c>
       <c r="D364" s="22" t="inlineStr">
         <is>
-          <t>maa://36646 (98.89), maa://36845 (95.86), **maa://39217 (38.89), maa://51007 (98.28)</t>
+          <t>maa://36646 (98.90), maa://36845 (95.86), **maa://39217 (38.89), maa://51007 (98.28)</t>
         </is>
       </c>
       <c r="E364" s="22" t="inlineStr">
@@ -27694,7 +27694,7 @@
       </c>
       <c r="D381" s="22" t="inlineStr">
         <is>
-          <t>maa://44233 (91.53), maa://45570 (96.72)</t>
+          <t>maa://44233 (91.67), maa://45570 (96.72)</t>
         </is>
       </c>
       <c r="E381" s="22" t="inlineStr">
@@ -27964,7 +27964,7 @@
       </c>
       <c r="D386" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (81.00), maa://44745 (98.02), **maa://49516 (39.29), *maa://45952 (57.14), ***maa://46851 (12.50), *maa://44896 (77.78)</t>
+          <t>maa://42970 (81.00), maa://44745 (98.04), **maa://49516 (37.93), *maa://45952 (57.14), ***maa://46851 (12.50), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E386" s="22" t="inlineStr">
@@ -28423,7 +28423,7 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>maa://59533 (97.78), maa://59577 (100.00)</t>
+          <t>maa://59533 (97.83), maa://59577 (100.00)</t>
         </is>
       </c>
       <c r="E396" t="inlineStr">
@@ -28558,7 +28558,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>maa://51872 (96.62), maa://51876 (99.06), maa://63228 (88.24), maa://51873 (100.00), maa://62047 (92.00)</t>
+          <t>maa://51872 (96.63), maa://51876 (99.06), maa://63228 (88.24), maa://51873 (100.00), maa://62047 (92.00)</t>
         </is>
       </c>
       <c r="E401" t="inlineStr">
@@ -28612,7 +28612,7 @@
       </c>
       <c r="D403" t="inlineStr">
         <is>
-          <t>maa://60449 (98.98), maa://59493 (96.85)</t>
+          <t>maa://60449 (98.99), maa://59493 (96.88)</t>
         </is>
       </c>
       <c r="E403" t="inlineStr">
@@ -28666,7 +28666,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>maa://62756 (95.86)</t>
+          <t>maa://62756 (95.92)</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">
@@ -28720,7 +28720,7 @@
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>maa://64040 (98.98), maa://52505 (98.47), maa://66377 (92.86), ***maa://66376 (25.00)</t>
+          <t>maa://64040 (98.98), maa://52505 (98.50), maa://66377 (93.33), ***maa://66376 (25.00)</t>
         </is>
       </c>
       <c r="E407" t="inlineStr">
@@ -28747,7 +28747,7 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>maa://67090 (86.67)</t>
+          <t>maa://67090 (87.50)</t>
         </is>
       </c>
       <c r="E408" t="inlineStr">
@@ -28774,7 +28774,7 @@
       </c>
       <c r="D409" t="inlineStr">
         <is>
-          <t>maa://67388 (91.43)</t>
+          <t>maa://67388 (91.89)</t>
         </is>
       </c>
       <c r="E409" t="inlineStr">
@@ -28801,7 +28801,7 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>maa://67089 (97.37), maa://67271 (93.33)</t>
+          <t>maa://67089 (97.50), maa://67271 (93.75)</t>
         </is>
       </c>
       <c r="E410" t="inlineStr">
@@ -28828,7 +28828,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>maa://67088 (90.38)</t>
+          <t>maa://67088 (90.91)</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
@@ -28855,7 +28855,7 @@
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>maa://67087 (93.33), maa://67268 (95.71), maa://67269 (87.50), maa://67648 (100.00)</t>
+          <t>maa://67087 (93.55), maa://67268 (96.05), maa://67269 (88.24), maa://67648 (100.00)</t>
         </is>
       </c>
       <c r="E412" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#242)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -712,7 +712,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (98.20), maa://24702 (95.06), maa://36681 (86.21)</t>
+          <t>maa://25390 (98.31), maa://24702 (95.06), maa://36681 (85.23)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://58660 (98.77), maa://39402 (95.11), *maa://34787 (75.00)</t>
+          <t>maa://58660 (98.85), maa://39402 (94.87), *maa://34787 (75.00)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -776,7 +776,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (97.22), maa://66635 (99.51)</t>
+          <t>maa://22742 (97.29), maa://66635 (99.55)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://36684 (98.26), maa://21246 (91.32)</t>
+          <t>maa://36684 (98.28), maa://21246 (91.32)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://59087 (97.18), maa://25251 (91.61)</t>
+          <t>maa://59087 (97.20), maa://25251 (91.61)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -842,7 +842,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (99.34), maa://36987 (97.14), maa://39849 (91.67)</t>
+          <t>maa://40192 (99.38), maa://36987 (97.18), maa://39849 (91.67)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -858,7 +858,7 @@
       </c>
       <c r="H3" s="8" t="inlineStr">
         <is>
-          <t>maa://21247 (99.34)</t>
+          <t>maa://21247 (99.37)</t>
         </is>
       </c>
       <c r="I3" s="19" t="n"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>maa://22880 (90.66), maa://20276 (93.98), maa://22749 (84.62)</t>
+          <t>maa://22880 (91.07), maa://20276 (94.02), maa://22749 (84.62)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -890,7 +890,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (98.30), maa://26254 (98.11), *maa://22738 (80.00)</t>
+          <t>maa://21249 (98.38), maa://26254 (98.11), *maa://22738 (80.00)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://60545 (98.63), maa://45854 (86.73), maa://24617 (91.18)</t>
+          <t>maa://60545 (98.71), maa://45854 (87.32), maa://24617 (91.18)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (91.70), maa://27484 (99.17), maa://27480 (85.45)</t>
+          <t>maa://27396 (92.11), maa://27484 (99.19), maa://27480 (85.96)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://52241 (99.05), maa://24390 (96.77)</t>
+          <t>maa://52241 (99.10), maa://24390 (96.77)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -954,7 +954,7 @@
       </c>
       <c r="AF3" s="8" t="inlineStr">
         <is>
-          <t>maa://21289 (91.43)</t>
+          <t>maa://21289 (91.82)</t>
         </is>
       </c>
       <c r="AG3" s="16" t="n"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (98.05), maa://22499 (90.00), maa://22746 (100.00)</t>
+          <t>maa://24632 (98.03), maa://22499 (90.00), maa://22746 (100.00)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (99.13), maa://50121 (96.64)</t>
+          <t>maa://49983 (99.09), maa://50121 (96.88)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://27295 (97.68), maa://32509 (96.19), maa://31008 (95.05), maa://22754 (88.16)</t>
+          <t>maa://27295 (97.78), maa://32509 (96.37), maa://31008 (95.16), maa://22754 (88.16)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="X4" s="8" t="inlineStr">
         <is>
-          <t>maa://43217 (98.78)</t>
+          <t>maa://43217 (98.84)</t>
         </is>
       </c>
       <c r="Y4" s="19" t="n"/>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="AB4" s="8" t="inlineStr">
         <is>
-          <t>maa://32658 (80.85)</t>
+          <t>maa://32658 (81.25)</t>
         </is>
       </c>
       <c r="AC4" s="19" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (91.05), maa://54105 (98.38), *maa://22744 (80.00)</t>
+          <t>maa://21245 (91.18), maa://54105 (98.47), *maa://22744 (80.00)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="L5" s="8" t="inlineStr">
         <is>
-          <t>maa://22757 (90.57)</t>
+          <t>maa://22757 (90.83)</t>
         </is>
       </c>
       <c r="M5" s="19" t="n"/>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="P5" s="8" t="inlineStr">
         <is>
-          <t>maa://21919 (99.04), maa://21281 (81.25)</t>
+          <t>maa://21919 (99.08), maa://21281 (81.25)</t>
         </is>
       </c>
       <c r="Q5" s="19" t="n"/>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="X5" s="8" t="inlineStr">
         <is>
-          <t>maa://21290 (99.21)</t>
+          <t>maa://21290 (98.50)</t>
         </is>
       </c>
       <c r="Y5" s="19" t="n"/>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="D6" s="8" t="inlineStr">
         <is>
-          <t>maa://42407 (97.30)</t>
+          <t>maa://42407 (97.41)</t>
         </is>
       </c>
       <c r="E6" s="19" t="n"/>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="H6" s="8" t="inlineStr">
         <is>
-          <t>maa://24370 (97.39)</t>
+          <t>maa://24370 (97.48)</t>
         </is>
       </c>
       <c r="I6" s="19" t="n"/>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="L6" s="8" t="inlineStr">
         <is>
-          <t>maa://24839 (99.39)</t>
+          <t>maa://24839 (99.42)</t>
         </is>
       </c>
       <c r="M6" s="19" t="n"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (98.76), maa://30381 (95.00)</t>
+          <t>maa://31836 (98.83), maa://30381 (95.00)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="X6" s="8" t="inlineStr">
         <is>
-          <t>maa://52754 (96.23)</t>
+          <t>maa://52754 (96.41)</t>
         </is>
       </c>
       <c r="Y6" s="19" t="n"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="AB6" s="8" t="inlineStr">
         <is>
-          <t>maa://22739 (89.13)</t>
+          <t>maa://22739 (89.36)</t>
         </is>
       </c>
       <c r="AC6" s="19" t="n"/>
@@ -1344,12 +1344,12 @@
       </c>
       <c r="AE6" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF6" s="8" t="inlineStr">
         <is>
-          <t>*maa://33152 (79.71), ***maa://22770 (26.09)</t>
+          <t>maa://33152 (80.56)</t>
         </is>
       </c>
       <c r="AG6" s="16" t="n"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>maa://21955 (98.08)</t>
+          <t>maa://21955 (98.16)</t>
         </is>
       </c>
       <c r="E7" s="19" t="n"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>*maa://22763 (75.00), maa://64972 (95.00)</t>
+          <t>*maa://22763 (75.00), maa://64972 (95.45)</t>
         </is>
       </c>
       <c r="I7" s="19" t="n"/>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (98.69), maa://24957 (94.55)</t>
+          <t>maa://28624 (98.58), maa://24957 (94.55)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="P7" s="8" t="inlineStr">
         <is>
-          <t>maa://22750 (96.77)</t>
+          <t>maa://22750 (96.89)</t>
         </is>
       </c>
       <c r="Q7" s="19" t="n"/>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="T7" s="8" t="inlineStr">
         <is>
-          <t>maa://21291 (93.79)</t>
+          <t>maa://21291 (93.98)</t>
         </is>
       </c>
       <c r="U7" s="19" t="n"/>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (97.05), maa://22758 (82.18)</t>
+          <t>maa://22399 (97.18), maa://22758 (82.35)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="AF7" s="8" t="inlineStr">
         <is>
-          <t>maa://45272 (99.41)</t>
+          <t>maa://45272 (99.45)</t>
         </is>
       </c>
       <c r="AG7" s="16" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.26 13:19:42</t>
+          <t>更新日期：2025.10.01 13:20:43</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (89.94), *maa://39431 (58.33), **maa://37551 (50.00)</t>
+          <t>maa://21476 (90.00), *maa://39431 (61.54), **maa://37551 (50.00)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
-          <t>*maa://24371 (78.49)</t>
+          <t>*maa://24371 (79.38)</t>
         </is>
       </c>
       <c r="I8" s="19" t="n"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (91.38), maa://23252 (91.67), maa://37496 (98.28)</t>
+          <t>maa://32931 (91.18), maa://23252 (91.67), maa://37496 (98.33)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (96.00), maa://67587 (98.36)</t>
+          <t>maa://21411 (96.05), maa://67587 (98.55)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>maa://24479 (84.24), *maa://21990 (51.72)</t>
+          <t>maa://24479 (84.29), *maa://21990 (51.72)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>maa://22765 (95.56), *maa://21915 (78.57)</t>
+          <t>maa://22765 (95.68), *maa://21915 (78.57)</t>
         </is>
       </c>
       <c r="E9" s="19" t="n"/>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (96.23), maa://39552 (86.96)</t>
+          <t>maa://22762 (96.31), maa://39552 (87.50)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="T9" s="8" t="inlineStr">
         <is>
-          <t>maa://26222 (99.44)</t>
+          <t>maa://26222 (99.45)</t>
         </is>
       </c>
       <c r="U9" s="19" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://52237 (99.75), maa://26223 (98.31)</t>
+          <t>maa://52237 (99.76), maa://26223 (98.31)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (95.04), maa://40166 (95.02)</t>
+          <t>maa://28711 (95.19), maa://40166 (94.74)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (91.09), maa://66916 (97.95)</t>
+          <t>maa://26206 (91.22), maa://66916 (98.08)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>maa://54000 (91.86)</t>
+          <t>maa://54000 (92.22)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="H10" s="8" t="inlineStr">
         <is>
-          <t>maa://32651 (95.12)</t>
+          <t>maa://32651 (95.24)</t>
         </is>
       </c>
       <c r="I10" s="19" t="n"/>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (91.70), *maa://36669 (74.03)</t>
+          <t>maa://28977 (91.97), *maa://36669 (74.36)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (99.22), maa://22755 (91.43), maa://63521 (94.61)</t>
+          <t>maa://27395 (99.25), maa://22755 (91.53), maa://63521 (94.74)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://45828 (99.19), maa://22301 (97.64), maa://22726 (100.00)</t>
+          <t>maa://45828 (99.24), maa://22301 (97.64), maa://22726 (100.00)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>*maa://25021 (56.33), *maa://22733 (64.62), **maa://22761 (33.33)</t>
+          <t>*maa://25021 (56.79), *maa://22733 (64.62), **maa://22761 (33.33)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="D11" s="8" t="inlineStr">
         <is>
-          <t>maa://36707 (99.73)</t>
+          <t>maa://36707 (99.74)</t>
         </is>
       </c>
       <c r="E11" s="19" t="n"/>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="L11" s="8" t="inlineStr">
         <is>
-          <t>maa://21287 (93.68)</t>
+          <t>maa://21287 (93.54)</t>
         </is>
       </c>
       <c r="M11" s="19" t="n"/>
@@ -1940,7 +1940,7 @@
       </c>
       <c r="P11" s="8" t="inlineStr">
         <is>
-          <t>maa://45557 (95.83)</t>
+          <t>maa://45557 (94.00)</t>
         </is>
       </c>
       <c r="Q11" s="19" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (93.28), maa://22501 (99.53), maa://64808 (100.00), maa://45521 (95.16)</t>
+          <t>maa://22747 (93.26), maa://22501 (99.54), maa://64808 (100.00), maa://45521 (95.24)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="X11" s="8" t="inlineStr">
         <is>
-          <t>maa://36713 (99.24)</t>
+          <t>maa://36713 (99.27)</t>
         </is>
       </c>
       <c r="Y11" s="19" t="n"/>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="AB11" s="8" t="inlineStr">
         <is>
-          <t>maa://29912 (99.70), maa://22516 (86.52)</t>
+          <t>maa://29912 (99.71), maa://22516 (86.52)</t>
         </is>
       </c>
       <c r="AC11" s="19" t="n"/>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="AF11" s="8" t="inlineStr">
         <is>
-          <t>maa://31203 (98.61)</t>
+          <t>maa://31203 (98.65)</t>
         </is>
       </c>
       <c r="AG11" s="16" t="n"/>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>maa://36678 (97.01), maa://30766 (91.18)</t>
+          <t>maa://36678 (97.10), maa://30766 (91.18)</t>
         </is>
       </c>
       <c r="E12" s="19" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (93.41), maa://54294 (96.41)</t>
+          <t>maa://21867 (93.54), maa://54294 (96.63)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (97.93), maa://64046 (98.55)</t>
+          <t>maa://63896 (98.00), maa://64046 (98.58)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="P12" s="8" t="inlineStr">
         <is>
-          <t>maa://57541 (91.18)</t>
+          <t>maa://57541 (91.43)</t>
         </is>
       </c>
       <c r="Q12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://37962 (98.77), maa://21485 (81.62), maa://22753 (92.80)</t>
+          <t>maa://37962 (98.82), maa://21485 (81.70), maa://22753 (92.83)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://36677 (99.00), maa://23669 (95.11), maa://39872 (98.20)</t>
+          <t>maa://36677 (99.04), maa://23669 (95.12), maa://39872 (98.29)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>maa://28932 (94.44)</t>
+          <t>maa://28932 (94.61)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (96.51), maa://36673 (93.94), maa://25001 (88.76)</t>
+          <t>maa://24999 (96.64), maa://36673 (94.07), maa://25001 (88.76)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (72.91), maa://66545 (98.99)</t>
+          <t>*maa://21248 (73.20), maa://66545 (99.03)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (97.54), maa://22583 (87.82)</t>
+          <t>maa://22676 (97.71), maa://22583 (88.12)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="X13" s="8" t="inlineStr">
         <is>
-          <t>maa://34957 (94.47)</t>
+          <t>maa://34957 (94.46)</t>
         </is>
       </c>
       <c r="Y13" s="19" t="n"/>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (93.86)</t>
+          <t>maa://39883 (94.08)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2282,7 +2282,7 @@
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>maa://30764 (95.04)</t>
+          <t>maa://30764 (94.44)</t>
         </is>
       </c>
       <c r="E14" s="19" t="n"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (98.97), maa://26245 (97.06), maa://36682 (98.26), maa://21288 (96.40)</t>
+          <t>maa://39841 (99.03), maa://36682 (98.28), maa://26245 (97.06), maa://21288 (96.40)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2330,7 +2330,7 @@
       </c>
       <c r="P14" s="8" t="inlineStr">
         <is>
-          <t>maa://23250 (99.64), maa://20107 (87.50), maa://22772 (100.00), maa://68732 (100.00)</t>
+          <t>maa://23250 (99.65), maa://20107 (87.50), maa://22772 (100.00), maa://68732 (100.00)</t>
         </is>
       </c>
       <c r="Q14" s="19" t="n"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://42751 (98.90), maa://22521 (95.12)</t>
+          <t>maa://42751 (98.94), maa://22521 (95.26)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="X14" s="8" t="inlineStr">
         <is>
-          <t>maa://37468 (97.96)</t>
+          <t>maa://37468 (98.06)</t>
         </is>
       </c>
       <c r="Y14" s="19" t="n"/>
@@ -2378,7 +2378,7 @@
       </c>
       <c r="AB14" s="8" t="inlineStr">
         <is>
-          <t>maa://22764 (98.85)</t>
+          <t>maa://22764 (98.88)</t>
         </is>
       </c>
       <c r="AC14" s="19" t="n"/>
@@ -2407,12 +2407,12 @@
       </c>
       <c r="C15" s="19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (85.28), maa://45058 (98.07), maa://22734 (84.85), *maa://36048 (74.72)</t>
+          <t>maa://22743 (85.34), maa://45058 (98.17), maa://22734 (84.96), *maa://36048 (74.86), maa://69928 (100.00)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (96.86), maa://21478 (90.48)</t>
+          <t>maa://24304 (96.99), maa://21478 (90.48)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="L15" s="8" t="inlineStr">
         <is>
-          <t>*maa://21334 (69.64)</t>
+          <t>*maa://21334 (70.18)</t>
         </is>
       </c>
       <c r="M15" s="19" t="n"/>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="P15" s="8" t="inlineStr">
         <is>
-          <t>maa://24762 (97.58), *maa://22727 (70.00)</t>
+          <t>maa://24762 (97.65), *maa://22727 (70.00)</t>
         </is>
       </c>
       <c r="Q15" s="19" t="n"/>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="T15" s="8" t="inlineStr">
         <is>
-          <t>maa://23892 (97.56)</t>
+          <t>maa://23892 (97.58)</t>
         </is>
       </c>
       <c r="U15" s="19" t="n"/>
@@ -2492,7 +2492,7 @@
       </c>
       <c r="X15" s="8" t="inlineStr">
         <is>
-          <t>maa://38786 (91.18), maa://56102 (100.00)</t>
+          <t>maa://38786 (91.67), maa://56102 (100.00)</t>
         </is>
       </c>
       <c r="Y15" s="19" t="n"/>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://36666 (96.23), maa://21364 (83.64), *maa://22766 (70.71), maa://68306 (83.33)</t>
+          <t>maa://36666 (96.31), maa://21364 (83.80), *maa://22766 (70.71), maa://68306 (81.08)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://37650 (99.74), maa://21441 (96.62), maa://36679 (94.55)</t>
+          <t>maa://37650 (99.75), maa://21441 (96.62), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2590,7 +2590,7 @@
       </c>
       <c r="P16" s="8" t="inlineStr">
         <is>
-          <t>maa://28504 (96.09)</t>
+          <t>maa://28504 (96.24)</t>
         </is>
       </c>
       <c r="Q16" s="19" t="n"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://36674 (97.97), maa://22729 (96.08), *maa://28648 (77.89)</t>
+          <t>maa://36674 (98.03), maa://22729 (96.17), *maa://28648 (77.89)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2622,7 +2622,7 @@
       </c>
       <c r="X16" s="8" t="inlineStr">
         <is>
-          <t>maa://28501 (99.28), maa://28051 (96.97)</t>
+          <t>maa://28501 (99.33), maa://28051 (97.06)</t>
         </is>
       </c>
       <c r="Y16" s="19" t="n"/>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="AB16" s="8" t="inlineStr">
         <is>
-          <t>maa://26228 (97.86)</t>
+          <t>maa://26228 (97.94)</t>
         </is>
       </c>
       <c r="AC16" s="19" t="n"/>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>maa://23911 (90.38), maa://27755 (93.75), maa://67613 (99.36)</t>
+          <t>maa://23911 (90.57), maa://27755 (93.75), maa://67613 (99.43)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://39599 (98.13), maa://22430 (90.21)</t>
+          <t>maa://39599 (98.22), maa://22430 (90.21)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="L17" s="8" t="inlineStr">
         <is>
-          <t>maa://21679 (87.76)</t>
+          <t>maa://21679 (88.24)</t>
         </is>
       </c>
       <c r="M17" s="19" t="n"/>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (82.64), maa://56238 (98.43)</t>
+          <t>maa://23890 (82.64), maa://56238 (98.48)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="T17" s="8" t="inlineStr">
         <is>
-          <t>*maa://42324 (69.05)</t>
+          <t>*maa://42324 (69.77)</t>
         </is>
       </c>
       <c r="U17" s="19" t="n"/>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="AF17" s="8" t="inlineStr">
         <is>
-          <t>maa://50136 (98.96)</t>
+          <t>maa://50136 (98.98)</t>
         </is>
       </c>
       <c r="AG17" s="16" t="n"/>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>maa://24570 (98.28)</t>
+          <t>maa://24570 (98.34)</t>
         </is>
       </c>
       <c r="E18" s="19" t="n"/>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="H18" s="8" t="inlineStr">
         <is>
-          <t>maa://24421 (95.21)</t>
+          <t>maa://24421 (95.16)</t>
         </is>
       </c>
       <c r="I18" s="19" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://52226 (99.70), maa://22466 (92.83)</t>
+          <t>maa://52226 (99.63), maa://22466 (92.83)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), maa://54153 (99.63), maa://24380 (100.00)</t>
+          <t>maa://24379 (100.00), maa://54153 (99.65), maa://24380 (100.00)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (98.67), maa://22741 (92.31)</t>
+          <t>maa://21917 (98.71), maa://22741 (92.31)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="AB18" s="8" t="inlineStr">
         <is>
-          <t>maa://24393 (98.96)</t>
+          <t>maa://24393 (99.00)</t>
         </is>
       </c>
       <c r="AC18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://47854 (92.70)</t>
+          <t>maa://47854 (92.96)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -2932,7 +2932,7 @@
       </c>
       <c r="D19" s="8" t="inlineStr">
         <is>
-          <t>maa://62850 (99.31)</t>
+          <t>maa://62850 (99.27)</t>
         </is>
       </c>
       <c r="E19" s="19" t="n"/>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="L19" s="8" t="inlineStr">
         <is>
-          <t>maa://39347 (97.96), maa://56392 (100.00)</t>
+          <t>maa://39347 (98.00), maa://56392 (100.00)</t>
         </is>
       </c>
       <c r="M19" s="19" t="n"/>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="T19" s="8" t="inlineStr">
         <is>
-          <t>maa://24386 (99.65)</t>
+          <t>maa://24386 (99.67)</t>
         </is>
       </c>
       <c r="U19" s="19" t="n"/>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="X19" s="8" t="inlineStr">
         <is>
-          <t>maa://31386 (100.00), maa://58490 (85.00)</t>
+          <t>maa://31386 (97.56), maa://58490 (85.00)</t>
         </is>
       </c>
       <c r="Y19" s="19" t="n"/>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (85.62), *maa://36668 (69.03)</t>
+          <t>maa://30709 (86.06), *maa://36668 (69.57)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3044,7 +3044,7 @@
       </c>
       <c r="AF19" s="8" t="inlineStr">
         <is>
-          <t>*maa://21663 (65.91), maa://52239 (87.10)</t>
+          <t>*maa://21663 (65.91), maa://52239 (88.24)</t>
         </is>
       </c>
       <c r="AG19" s="16" t="n"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://25198 (97.62), maa://36680 (99.06), maa://21432 (91.49)</t>
+          <t>maa://25198 (97.66), maa://36680 (99.08), maa://21432 (91.53)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3078,7 +3078,7 @@
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>maa://22864 (96.07)</t>
+          <t>maa://22864 (96.21)</t>
         </is>
       </c>
       <c r="I20" s="19" t="n"/>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (95.24)</t>
+          <t>maa://41331 (95.38)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="P20" s="8" t="inlineStr">
         <is>
-          <t>maa://37442 (98.48)</t>
+          <t>maa://37442 (98.54)</t>
         </is>
       </c>
       <c r="Q20" s="19" t="n"/>
@@ -3126,7 +3126,7 @@
       </c>
       <c r="T20" s="8" t="inlineStr">
         <is>
-          <t>maa://29113 (93.42)</t>
+          <t>maa://29113 (93.59)</t>
         </is>
       </c>
       <c r="U20" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (96.43), maa://56241 (98.23), maa://49976 (88.46)</t>
+          <t>maa://50085 (96.61), maa://56241 (98.24), maa://49976 (88.57)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="H21" s="8" t="inlineStr">
         <is>
-          <t>maa://24372 (98.85)</t>
+          <t>maa://24372 (98.88)</t>
         </is>
       </c>
       <c r="I21" s="19" t="n"/>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="L21" s="8" t="inlineStr">
         <is>
-          <t>maa://31731 (96.43)</t>
+          <t>maa://31731 (96.49)</t>
         </is>
       </c>
       <c r="M21" s="19" t="n"/>
@@ -3240,7 +3240,7 @@
       </c>
       <c r="P21" s="8" t="inlineStr">
         <is>
-          <t>maa://24381 (81.82)</t>
+          <t>maa://24381 (82.35)</t>
         </is>
       </c>
       <c r="Q21" s="19" t="n"/>
@@ -3256,7 +3256,7 @@
       </c>
       <c r="T21" s="8" t="inlineStr">
         <is>
-          <t>maa://21993 (88.89)</t>
+          <t>maa://21993 (90.32)</t>
         </is>
       </c>
       <c r="U21" s="19" t="n"/>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (98.34), maa://20110 (87.01)</t>
+          <t>maa://34946 (98.02), maa://20110 (87.01)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="AB21" s="8" t="inlineStr">
         <is>
-          <t>maa://21443 (86.62), maa://52223 (82.59)</t>
+          <t>maa://21443 (86.96), maa://52223 (83.03)</t>
         </is>
       </c>
       <c r="AC21" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22432 (93.93), maa://22524 (83.16), maa://64221 (97.83)</t>
+          <t>maa://22432 (94.17), maa://22524 (83.16), maa://64221 (97.94)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>maa://25236 (99.19)</t>
+          <t>maa://25236 (99.22)</t>
         </is>
       </c>
       <c r="I22" s="19" t="n"/>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>maa://27127 (83.04), *maa://22751 (70.93), maa://66865 (99.38)</t>
+          <t>maa://27127 (83.40), *maa://22751 (71.26), maa://66865 (99.41)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://37649 (94.44), maa://21282 (98.95)</t>
+          <t>maa://37649 (94.74), maa://21282 (98.95)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="AB22" s="8" t="inlineStr">
         <is>
-          <t>maa://23656 (99.49)</t>
+          <t>maa://23656 (99.50)</t>
         </is>
       </c>
       <c r="AC22" s="19" t="n"/>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="AF22" s="8" t="inlineStr">
         <is>
-          <t>maa://29658 (97.12)</t>
+          <t>maa://29658 (97.14)</t>
         </is>
       </c>
       <c r="AG22" s="16" t="n"/>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>*maa://41753 (66.18), **maa://28036 (30.77)</t>
+          <t>*maa://41753 (66.67), **maa://28036 (30.77)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (98.57), maa://39875 (95.76)</t>
+          <t>maa://39756 (98.62), maa://39875 (95.76)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (96.65), maa://29748 (81.68), *maa://37566 (78.12)</t>
+          <t>maa://30587 (96.74), maa://29748 (81.68), *maa://37566 (78.46)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="T23" s="8" t="inlineStr">
         <is>
-          <t>maa://31212 (94.50), maa://24387 (84.44), maa://67084 (87.50)</t>
+          <t>maa://31212 (94.87), maa://24387 (84.44), maa://67084 (87.50)</t>
         </is>
       </c>
       <c r="U23" s="19" t="n"/>
@@ -3532,7 +3532,7 @@
       </c>
       <c r="X23" s="8" t="inlineStr">
         <is>
-          <t>*maa://28503 (60.00)</t>
+          <t>*maa://28503 (60.26)</t>
         </is>
       </c>
       <c r="Y23" s="19" t="n"/>
@@ -3564,7 +3564,7 @@
       </c>
       <c r="AF23" s="8" t="inlineStr">
         <is>
-          <t>maa://31489 (98.31)</t>
+          <t>maa://31489 (98.33)</t>
         </is>
       </c>
       <c r="AG23" s="16" t="n"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (85.22), maa://46650 (90.08)</t>
+          <t>maa://24368 (85.41), maa://46650 (90.59)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (96.23), maa://23504 (94.05), *maa://25141 (79.74), maa://52227 (97.35), *maa://36663 (79.44)</t>
+          <t>maa://29988 (96.38), maa://23504 (94.06), *maa://25141 (79.74), maa://52227 (97.43), *maa://36663 (79.44)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="AB24" s="8" t="inlineStr">
         <is>
-          <t>maa://39349 (97.22)</t>
+          <t>maa://39349 (97.30)</t>
         </is>
       </c>
       <c r="AC24" s="19" t="n"/>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://64165 (99.27), maa://22523 (80.09), maa://29910 (94.20), maa://45831 (93.55)</t>
+          <t>maa://64165 (99.19), maa://22523 (80.18), maa://29910 (94.20), maa://45831 (93.55)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (96.53), maa://63016 (99.10)</t>
+          <t>maa://29753 (96.60), maa://63016 (99.13)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>*maa://29063 (76.02), *maa://25311 (70.42), maa://45047 (88.00)</t>
+          <t>*maa://29063 (76.01), *maa://25311 (70.63), maa://45047 (88.31)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3760,7 +3760,7 @@
       </c>
       <c r="P25" s="8" t="inlineStr">
         <is>
-          <t>maa://24382 (96.08)</t>
+          <t>maa://24382 (96.23)</t>
         </is>
       </c>
       <c r="Q25" s="19" t="n"/>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="T25" s="8" t="inlineStr">
         <is>
-          <t>maa://20109 (96.21), maa://22545 (100.00)</t>
+          <t>maa://20109 (96.30), maa://22545 (100.00)</t>
         </is>
       </c>
       <c r="U25" s="19" t="n"/>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="X25" s="8" t="inlineStr">
         <is>
-          <t>maa://29890 (91.20)</t>
+          <t>maa://29890 (91.47)</t>
         </is>
       </c>
       <c r="Y25" s="19" t="n"/>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (93.32), *maa://24516 (79.80), maa://26001 (83.33), maa://68311 (100.00)</t>
+          <t>maa://31215 (93.40), *maa://24516 (79.80), maa://26001 (83.33), maa://68311 (100.00)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (98.05), maa://36676 (99.84), maa://24621 (96.86), maa://22771 (88.24), maa://37772 (83.33)</t>
+          <t>maa://20108 (98.15), maa://36676 (99.84), maa://24621 (96.88), maa://22771 (88.24), maa://37772 (85.71)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://56374 (100.00), maa://41802 (96.36)</t>
+          <t>maa://56374 (100.00), maa://41802 (96.61)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3858,7 +3858,7 @@
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
-          <t>maa://56240 (96.02), maa://24913 (92.24)</t>
+          <t>maa://56240 (96.21), maa://24913 (92.24)</t>
         </is>
       </c>
       <c r="I26" s="19" t="n"/>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="P26" s="8" t="inlineStr">
         <is>
-          <t>maa://39870 (94.44), maa://56625 (100.00)</t>
+          <t>maa://39870 (94.59), maa://56625 (100.00)</t>
         </is>
       </c>
       <c r="Q26" s="19" t="n"/>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="AB26" s="8" t="inlineStr">
         <is>
-          <t>maa://42235 (98.34)</t>
+          <t>maa://42235 (98.39)</t>
         </is>
       </c>
       <c r="AC26" s="19" t="n"/>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>maa://39601 (90.74), maa://34494 (95.35)</t>
+          <t>maa://39601 (91.38), maa://34494 (95.45)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4004,7 +4004,7 @@
       </c>
       <c r="L27" s="8" t="inlineStr">
         <is>
-          <t>maa://28071 (89.29)</t>
+          <t>maa://28071 (89.47)</t>
         </is>
       </c>
       <c r="M27" s="19" t="n"/>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="T27" s="8" t="inlineStr">
         <is>
-          <t>maa://30624 (89.71)</t>
+          <t>maa://30624 (89.83)</t>
         </is>
       </c>
       <c r="U27" s="19" t="n"/>
@@ -4084,7 +4084,7 @@
       </c>
       <c r="AF27" s="8" t="inlineStr">
         <is>
-          <t>maa://24023 (97.73)</t>
+          <t>maa://24023 (97.79)</t>
         </is>
       </c>
       <c r="AG27" s="16" t="n"/>
@@ -4102,7 +4102,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (95.87), maa://25725 (85.27)</t>
+          <t>maa://24465 (95.93), maa://25725 (85.38)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="L28" s="8" t="inlineStr">
         <is>
-          <t>maa://30770 (90.00)</t>
+          <t>maa://30770 (90.32)</t>
         </is>
       </c>
       <c r="M28" s="19" t="n"/>
@@ -4166,7 +4166,7 @@
       </c>
       <c r="T28" s="8" t="inlineStr">
         <is>
-          <t>maa://29765 (93.33), maa://23263 (96.24)</t>
+          <t>maa://29765 (93.62), maa://23263 (96.24)</t>
         </is>
       </c>
       <c r="U28" s="19" t="n"/>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (97.36), maa://41749 (97.19)</t>
+          <t>maa://39929 (97.45), maa://41749 (97.22)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (94.22), maa://65700 (98.64)</t>
+          <t>maa://36660 (94.34), maa://65700 (98.68)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4232,7 +4232,7 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>maa://31694 (99.31)</t>
+          <t>maa://31694 (99.33)</t>
         </is>
       </c>
       <c r="E29" s="19" t="n"/>
@@ -4248,7 +4248,7 @@
       </c>
       <c r="H29" s="8" t="inlineStr">
         <is>
-          <t>*maa://25175 (50.91)</t>
+          <t>*maa://25175 (51.35)</t>
         </is>
       </c>
       <c r="I29" s="19" t="n"/>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (97.81), maa://31400 (98.06), maa://28440 (86.42)</t>
+          <t>maa://28432 (97.78), maa://31400 (98.09), maa://28440 (86.50)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4280,7 +4280,7 @@
       </c>
       <c r="P29" s="8" t="inlineStr">
         <is>
-          <t>maa://54169 (97.25)</t>
+          <t>maa://54169 (97.39)</t>
         </is>
       </c>
       <c r="Q29" s="19" t="n"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://42865 (92.11)</t>
+          <t>maa://42865 (92.14)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (95.38), maa://64191 (97.44)</t>
+          <t>maa://45792 (95.59), maa://64191 (97.50)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="L30" s="8" t="inlineStr">
         <is>
-          <t>maa://30442 (97.44)</t>
+          <t>maa://30442 (97.48)</t>
         </is>
       </c>
       <c r="M30" s="19" t="n"/>
@@ -4458,7 +4458,7 @@
       </c>
       <c r="AB30" s="8" t="inlineStr">
         <is>
-          <t>maa://42979 (99.55), maa://45822 (100.00), maa://45045 (90.91)</t>
+          <t>maa://42979 (99.56), maa://45822 (100.00), maa://45045 (90.91)</t>
         </is>
       </c>
       <c r="AC30" s="19" t="n"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (97.98), maa://36258 (93.08), maa://43904 (90.00)</t>
+          <t>maa://35926 (98.05), maa://36258 (93.12), maa://43904 (90.00)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4556,7 +4556,7 @@
       </c>
       <c r="T31" s="8" t="inlineStr">
         <is>
-          <t>maa://30711 (96.64), maa://30768 (100.00)</t>
+          <t>maa://30711 (96.69), maa://30768 (100.00)</t>
         </is>
       </c>
       <c r="U31" s="19" t="n"/>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://36667 (99.64), maa://21895 (97.97), maa://22760 (100.00)</t>
+          <t>maa://36667 (99.65), maa://21895 (97.97), maa://22760 (100.00)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4654,7 +4654,7 @@
       </c>
       <c r="L32" s="8" t="inlineStr">
         <is>
-          <t>maa://28065 (97.00)</t>
+          <t>maa://28065 (97.06)</t>
         </is>
       </c>
       <c r="M32" s="19" t="n"/>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (99.26), maa://41108 (87.72), maa://41238 (98.12), maa://45523 (100.00)</t>
+          <t>maa://42859 (99.29), maa://41108 (87.72), maa://41238 (98.14), maa://45523 (100.00)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="X32" s="8" t="inlineStr">
         <is>
-          <t>maa://64104 (97.32)</t>
+          <t>maa://64104 (97.48)</t>
         </is>
       </c>
       <c r="Y32" s="19" t="n"/>
@@ -4734,7 +4734,7 @@
       </c>
       <c r="AF32" s="8" t="inlineStr">
         <is>
-          <t>maa://42408 (94.87)</t>
+          <t>maa://42408 (95.12)</t>
         </is>
       </c>
       <c r="AG32" s="16" t="n"/>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (94.61), *maa://22730 (70.59), maa://69135 (100.00)</t>
+          <t>maa://21956 (94.59), *maa://22730 (70.59), maa://69135 (93.75)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (99.20), maa://56235 (99.73)</t>
+          <t>maa://48817 (99.24), maa://56235 (99.49)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="T34" s="8" t="inlineStr">
         <is>
-          <t>maa://24526 (97.06)</t>
+          <t>maa://24526 (97.13)</t>
         </is>
       </c>
       <c r="U34" s="19" t="n"/>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="AB34" s="8" t="inlineStr">
         <is>
-          <t>maa://64329 (97.67)</t>
+          <t>maa://64329 (97.96)</t>
         </is>
       </c>
       <c r="AC34" s="19" t="n"/>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
-          <t>maa://41296 (99.25)</t>
+          <t>maa://41296 (99.27)</t>
         </is>
       </c>
       <c r="M35" s="19" t="n"/>
@@ -5124,7 +5124,7 @@
       </c>
       <c r="AF35" s="8" t="inlineStr">
         <is>
-          <t>maa://39479 (96.00)</t>
+          <t>maa://39479 (96.08)</t>
         </is>
       </c>
       <c r="AG35" s="16" t="n"/>
@@ -5206,7 +5206,7 @@
       </c>
       <c r="T36" s="8" t="inlineStr">
         <is>
-          <t>maa://27613 (99.54)</t>
+          <t>maa://27613 (99.56)</t>
         </is>
       </c>
       <c r="U36" s="19" t="n"/>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="AB36" s="19" t="inlineStr">
         <is>
-          <t>maa://64106 (97.06)</t>
+          <t>maa://64106 (97.14)</t>
         </is>
       </c>
       <c r="AC36" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (99.20), maa://56336 (99.34), maa://47069 (86.36), maa://45789 (100.00)</t>
+          <t>maa://45718 (99.20), maa://56336 (99.37), maa://47069 (86.67), maa://45789 (100.00)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="P37" s="8" t="inlineStr">
         <is>
-          <t>maa://21280 (97.57)</t>
+          <t>maa://21280 (97.64)</t>
         </is>
       </c>
       <c r="Q37" s="19" t="n"/>
@@ -5418,7 +5418,7 @@
       </c>
       <c r="L38" s="8" t="inlineStr">
         <is>
-          <t>maa://39384 (100.00), maa://49735 (100.00)</t>
+          <t>maa://39384 (99.28), maa://49735 (92.86)</t>
         </is>
       </c>
       <c r="M38" s="19" t="n"/>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="P38" s="8" t="inlineStr">
         <is>
-          <t>maa://24383 (81.72)</t>
+          <t>maa://24383 (82.01)</t>
         </is>
       </c>
       <c r="Q38" s="19" t="n"/>
@@ -5450,7 +5450,7 @@
       </c>
       <c r="T38" s="8" t="inlineStr">
         <is>
-          <t>maa://30713 (98.25)</t>
+          <t>maa://30713 (98.31)</t>
         </is>
       </c>
       <c r="U38" s="19" t="n"/>
@@ -5482,7 +5482,7 @@
       </c>
       <c r="AF38" s="8" t="inlineStr">
         <is>
-          <t>maa://36697 (95.83), maa://68397 (99.35)</t>
+          <t>maa://36697 (95.72), maa://68397 (99.03)</t>
         </is>
       </c>
       <c r="AG38" s="16" t="n"/>
@@ -5503,7 +5503,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://25199 (84.78), maa://45059 (93.70), maa://30434 (95.26), maa://44165 (85.71)</t>
+          <t>maa://25199 (84.78), maa://45059 (93.94), maa://30434 (95.31), maa://44165 (85.71)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://47093 (98.15), maa://24709 (93.93)</t>
+          <t>maa://47093 (98.25), maa://24709 (94.05)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (95.58), maa://45790 (87.67)</t>
+          <t>maa://47079 (95.75), maa://45790 (88.00)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5583,7 +5583,7 @@
       </c>
       <c r="AF39" s="8" t="inlineStr">
         <is>
-          <t>maa://62953 (96.72)</t>
+          <t>maa://62953 (96.75)</t>
         </is>
       </c>
       <c r="AG39" s="16" t="n"/>
@@ -5636,7 +5636,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (98.09), maa://21386 (95.94), maa://36664 (89.61), *maa://45550 (72.73)</t>
+          <t>maa://23278 (98.13), maa://21386 (95.94), maa://36664 (89.61), *maa://45550 (75.00)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://65283 (96.74), maa://64205 (93.75)</t>
+          <t>maa://65283 (96.95), maa://64205 (93.75)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="P41" s="8" t="inlineStr">
         <is>
-          <t>maa://43177 (95.50)</t>
+          <t>maa://43177 (95.54)</t>
         </is>
       </c>
       <c r="Q41" s="19" t="n"/>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>*maa://22525 (70.39), maa://21284 (97.62)</t>
+          <t>*maa://22525 (70.09), maa://21284 (97.75)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -6008,7 +6008,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (98.23), maa://56386 (99.39), maa://27728 (96.40)</t>
+          <t>maa://29768 (98.28), maa://56386 (99.41), maa://27728 (96.40)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6056,7 +6056,7 @@
       </c>
       <c r="T44" s="8" t="inlineStr">
         <is>
-          <t>maa://39366 (93.41)</t>
+          <t>maa://39366 (93.48)</t>
         </is>
       </c>
       <c r="U44" s="19" t="n"/>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://42459 (98.71), maa://21229 (85.59), maa://30807 (94.62), *maa://22767 (70.59)</t>
+          <t>maa://42459 (98.74), maa://21229 (85.65), maa://30807 (94.62), *maa://22767 (70.83)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6125,7 +6125,7 @@
       </c>
       <c r="T45" s="8" t="inlineStr">
         <is>
-          <t>*maa://39364 (66.46)</t>
+          <t>*maa://39364 (67.48)</t>
         </is>
       </c>
       <c r="U45" s="19" t="n"/>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (95.66), maa://43901 (96.27)</t>
+          <t>maa://35931 (95.81), maa://43901 (96.34)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6231,7 +6231,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (97.50), maa://29661 (97.20), maa://56236 (99.78), maa://28038 (84.62)</t>
+          <t>maa://27410 (97.51), maa://29661 (97.22), maa://56236 (99.79), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6263,7 +6263,7 @@
       </c>
       <c r="T47" s="8" t="inlineStr">
         <is>
-          <t>maa://67476 (99.56), maa://68392 (100.00)</t>
+          <t>maa://67476 (99.57), maa://68392 (99.56)</t>
         </is>
       </c>
       <c r="U47" s="19" t="n"/>
@@ -6314,11 +6314,7 @@
           <t>0</t>
         </is>
       </c>
-      <c r="P48" s="8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
+      <c r="P48" s="8" t="inlineStr"/>
       <c r="Q48" s="19" t="n"/>
       <c r="R48" s="19" t="inlineStr">
         <is>
@@ -6385,7 +6381,7 @@
       </c>
       <c r="P49" s="8" t="inlineStr">
         <is>
-          <t>*maa://39643 (78.99)</t>
+          <t>*maa://39643 (79.14)</t>
         </is>
       </c>
       <c r="Q49" s="19" t="n"/>
@@ -6401,7 +6397,7 @@
       </c>
       <c r="T49" s="19" t="inlineStr">
         <is>
-          <t>maa://67231 (99.09)</t>
+          <t>maa://67231 (99.13)</t>
         </is>
       </c>
       <c r="U49" s="19" t="n"/>
@@ -6438,7 +6434,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>maa://62852 (93.05)</t>
+          <t>maa://62852 (93.12)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6522,7 +6518,7 @@
       </c>
       <c r="H52" s="8" t="inlineStr">
         <is>
-          <t>maa://24376 (99.05)</t>
+          <t>maa://24376 (99.09)</t>
         </is>
       </c>
       <c r="I52" s="19" t="n"/>
@@ -6538,7 +6534,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (99.36), maa://59378 (93.83), maa://65511 (100.00)</t>
+          <t>maa://59394 (99.39), maa://59378 (93.83), maa://65511 (100.00)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6572,7 +6568,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (97.87)</t>
+          <t>maa://32534 (97.93)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -6656,7 +6652,7 @@
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>maa://32532 (97.81)</t>
+          <t>maa://32532 (97.86)</t>
         </is>
       </c>
       <c r="I55" s="19" t="n"/>
@@ -6708,7 +6704,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://56237 (98.69), maa://25176 (98.77)</t>
+          <t>maa://56237 (98.17), maa://25176 (98.77)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6726,7 +6722,7 @@
       </c>
       <c r="H58" s="8" t="inlineStr">
         <is>
-          <t>*maa://37964 (65.25)</t>
+          <t>*maa://37964 (65.57)</t>
         </is>
       </c>
       <c r="I58" s="19" t="n"/>
@@ -6744,7 +6740,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (98.32), maa://27746 (89.25)</t>
+          <t>maa://31270 (98.35), maa://27746 (89.42)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -6762,7 +6758,7 @@
       </c>
       <c r="H60" s="8" t="inlineStr">
         <is>
-          <t>maa://40438 (91.53)</t>
+          <t>maa://40438 (91.63)</t>
         </is>
       </c>
       <c r="I60" s="19" t="n"/>
@@ -6798,7 +6794,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (96.67), maa://56228 (98.68), maa://43903 (100.00)</t>
+          <t>maa://42981 (96.74), maa://56228 (98.10), maa://43903 (100.00)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6816,7 +6812,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (99.40), *maa://59693 (74.47), maa://59413 (97.30)</t>
+          <t>maa://59534 (99.42), *maa://59693 (72.92), maa://59413 (97.44)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7032,7 +7028,7 @@
       </c>
       <c r="H75" s="19" t="inlineStr">
         <is>
-          <t>maa://67748 (82.86)</t>
+          <t>maa://67748 (80.95)</t>
         </is>
       </c>
       <c r="I75" s="19" t="n"/>
@@ -7174,7 +7170,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.09.26 13:19:42</t>
+          <t>更新日期：2025.10.01 13:20:43</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -7498,7 +7494,7 @@
       </c>
       <c r="D7" s="13" t="inlineStr">
         <is>
-          <t>maa://20850 (88.89)</t>
+          <t>maa://20850 (89.47)</t>
         </is>
       </c>
       <c r="E7" s="14" t="inlineStr">
@@ -7984,7 +7980,7 @@
       </c>
       <c r="D16" s="13" t="inlineStr">
         <is>
-          <t>maa://20919 (98.00), *maa://31611 (76.92)</t>
+          <t>maa://20919 (98.04), *maa://31611 (76.92)</t>
         </is>
       </c>
       <c r="E16" s="14" t="inlineStr">
@@ -8200,7 +8196,7 @@
       </c>
       <c r="D20" s="13" t="inlineStr">
         <is>
-          <t>maa://20865 (92.31), maa://20826 (85.71)</t>
+          <t>maa://20865 (92.86), maa://20826 (85.71)</t>
         </is>
       </c>
       <c r="E20" s="14" t="inlineStr">
@@ -8578,7 +8574,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (73.21), *maa://28758 (71.11), maa://29036 (96.67), *maa://42172 (71.43), maa://65357 (96.15), maa://30285 (100.00)</t>
+          <t>*maa://20849 (73.21), *maa://28758 (71.11), maa://29036 (96.67), *maa://42172 (71.43), maa://65357 (96.43), maa://30285 (100.00)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8686,7 +8682,7 @@
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>maa://20863 (90.67), maa://20832 (99.22), maa://20727 (100.00)</t>
+          <t>maa://20863 (90.76), maa://20832 (99.22), maa://20727 (100.00)</t>
         </is>
       </c>
       <c r="E29" s="14" t="inlineStr">
@@ -8848,7 +8844,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (90.20), maa://36866 (96.97), maa://62759 (100.00), maa://45572 (88.24), maa://27794 (100.00), maa://20960 (100.00), maa://20843 (100.00), **maa://24483 (50.00), maa://20862 (83.33), *maa://20893 (77.78)</t>
+          <t>maa://36644 (89.84), maa://36866 (97.01), maa://62759 (100.00), maa://45572 (88.24), maa://27794 (100.00), maa://20960 (100.00), maa://20843 (100.00), **maa://24483 (50.00), *maa://20893 (73.68), maa://20862 (83.33)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -9010,7 +9006,7 @@
       </c>
       <c r="D35" s="13" t="inlineStr">
         <is>
-          <t>maa://20847 (96.77)</t>
+          <t>maa://20847 (96.88)</t>
         </is>
       </c>
       <c r="E35" s="14" t="inlineStr">
@@ -9118,7 +9114,7 @@
       </c>
       <c r="D37" s="13" t="inlineStr">
         <is>
-          <t>maa://27376 (93.33), maa://42635 (94.34), *maa://20838 (55.00)</t>
+          <t>maa://27376 (93.44), maa://42635 (94.34), *maa://20838 (55.00)</t>
         </is>
       </c>
       <c r="E37" s="14" t="inlineStr">
@@ -9766,7 +9762,7 @@
       </c>
       <c r="D49" s="13" t="inlineStr">
         <is>
-          <t>*maa://32845 (80.00), *maa://20982 (75.00)</t>
+          <t>*maa://32845 (76.19), *maa://20982 (75.00)</t>
         </is>
       </c>
       <c r="E49" s="14" t="inlineStr">
@@ -9982,7 +9978,7 @@
       </c>
       <c r="D53" s="13" t="inlineStr">
         <is>
-          <t>maa://20953 (97.14), maa://31173 (94.59)</t>
+          <t>maa://20953 (97.14), maa://31173 (94.74)</t>
         </is>
       </c>
       <c r="E53" s="14" t="inlineStr">
@@ -10144,7 +10140,7 @@
       </c>
       <c r="D56" s="13" t="inlineStr">
         <is>
-          <t>maa://44235 (98.41), maa://45604 (100.00), maa://20961 (100.00), maa://20910 (100.00), maa://44220 (100.00)</t>
+          <t>maa://44235 (98.44), maa://45604 (100.00), maa://20961 (100.00), maa://20910 (100.00), maa://44220 (100.00)</t>
         </is>
       </c>
       <c r="E56" s="14" t="inlineStr">
@@ -10198,7 +10194,7 @@
       </c>
       <c r="D57" s="13" t="inlineStr">
         <is>
-          <t>*maa://20965 (72.50)</t>
+          <t>*maa://20965 (73.17)</t>
         </is>
       </c>
       <c r="E57" s="14" t="inlineStr">
@@ -10414,7 +10410,7 @@
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (99.22), maa://31559 (93.88), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00), maa://66633 (100.00)</t>
+          <t>maa://20841 (99.23), maa://31559 (94.00), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00), maa://66633 (100.00)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -10522,7 +10518,7 @@
       </c>
       <c r="D63" s="13" t="inlineStr">
         <is>
-          <t>*maa://20845 (69.23), maa://38727 (91.67)</t>
+          <t>*maa://20845 (70.37), maa://38727 (91.67)</t>
         </is>
       </c>
       <c r="E63" s="14" t="inlineStr">
@@ -10630,7 +10626,7 @@
       </c>
       <c r="D65" s="13" t="inlineStr">
         <is>
-          <t>maa://28567 (97.47), **maa://20947 (45.71), maa://30525 (100.00), maa://38735 (100.00), *maa://28188 (70.00), maa://30524 (100.00)</t>
+          <t>maa://28567 (97.50), **maa://20947 (45.71), maa://30525 (100.00), maa://38735 (100.00), *maa://28188 (70.00), maa://30524 (100.00)</t>
         </is>
       </c>
       <c r="E65" s="14" t="inlineStr">
@@ -10792,7 +10788,7 @@
       </c>
       <c r="D68" s="13" t="inlineStr">
         <is>
-          <t>maa://20976 (97.83), maa://20815 (100.00)</t>
+          <t>maa://20976 (97.84), maa://20815 (100.00)</t>
         </is>
       </c>
       <c r="E68" s="14" t="inlineStr">
@@ -10846,7 +10842,7 @@
       </c>
       <c r="D69" s="13" t="inlineStr">
         <is>
-          <t>maa://20974 (96.94), maa://29079 (80.95), maa://29096 (95.65), maa://29087 (100.00), *maa://20823 (75.00), maa://20855 (94.12), maa://20904 (100.00), *maa://63722 (80.00)</t>
+          <t>maa://20974 (96.97), maa://29079 (80.95), maa://29096 (95.65), maa://29087 (100.00), *maa://20823 (75.00), maa://20855 (94.12), maa://20904 (100.00), *maa://63722 (80.00)</t>
         </is>
       </c>
       <c r="E69" s="14" t="inlineStr">
@@ -10900,7 +10896,7 @@
       </c>
       <c r="D70" s="13" t="inlineStr">
         <is>
-          <t>maa://20944 (96.15), maa://35393 (100.00)</t>
+          <t>maa://20944 (96.30), maa://35393 (100.00)</t>
         </is>
       </c>
       <c r="E70" s="14" t="inlineStr">
@@ -12358,7 +12354,7 @@
       </c>
       <c r="D97" s="13" t="inlineStr">
         <is>
-          <t>maa://20991 (100.00), maa://51015 (88.37)</t>
+          <t>maa://20991 (100.00), maa://51015 (88.64)</t>
         </is>
       </c>
       <c r="E97" s="14" t="inlineStr">
@@ -12466,7 +12462,7 @@
       </c>
       <c r="D99" s="13" t="inlineStr">
         <is>
-          <t>maa://20929 (92.86)</t>
+          <t>maa://20929 (93.10)</t>
         </is>
       </c>
       <c r="E99" s="14" t="inlineStr">
@@ -12574,7 +12570,7 @@
       </c>
       <c r="D101" s="13" t="inlineStr">
         <is>
-          <t>maa://45572 (88.24), maa://27794 (100.00), *maa://20893 (77.78)</t>
+          <t>maa://45572 (88.24), maa://27794 (100.00), *maa://20893 (73.68)</t>
         </is>
       </c>
       <c r="E101" s="14" t="inlineStr">
@@ -12682,7 +12678,7 @@
       </c>
       <c r="D103" s="13" t="inlineStr">
         <is>
-          <t>*maa://29094 (76.27), maa://28904 (88.64), **maa://20931 (48.65)</t>
+          <t>*maa://29094 (76.27), maa://28904 (88.64), **maa://20931 (47.37)</t>
         </is>
       </c>
       <c r="E103" s="14" t="inlineStr">
@@ -12952,7 +12948,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.72), maa://25018 (96.93), maa://25776 (92.21), maa://28361 (95.45), maa://25772 (94.12), maa://56588 (93.33), maa://45194 (85.71), maa://32653 (81.25), maa://25161 (83.33), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
+          <t>maa://51881 (98.73), maa://25018 (96.96), maa://25776 (92.21), maa://28361 (95.45), maa://25772 (94.12), maa://56588 (93.33), maa://45194 (85.71), maa://32653 (81.25), maa://25161 (83.33), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13006,7 +13002,7 @@
       </c>
       <c r="D109" s="13" t="inlineStr">
         <is>
-          <t>maa://36646 (98.90), maa://25774 (94.59), maa://35996 (97.89), maa://22469 (92.06), maa://30668 (86.67), maa://67286 (100.00)</t>
+          <t>maa://36646 (98.91), maa://25774 (94.59), maa://35996 (97.89), maa://22469 (92.06), maa://30668 (86.67), maa://67286 (100.00)</t>
         </is>
       </c>
       <c r="E109" s="14" t="inlineStr">
@@ -13384,7 +13380,7 @@
       </c>
       <c r="D116" s="13" t="inlineStr">
         <is>
-          <t>maa://20908 (98.18), maa://35723 (96.08), *maa://23346 (77.78), maa://38822 (100.00), maa://58659 (100.00)</t>
+          <t>maa://20908 (98.19), maa://35723 (96.08), *maa://23346 (77.78), maa://38822 (100.00), maa://58659 (100.00)</t>
         </is>
       </c>
       <c r="E116" s="14" t="inlineStr">
@@ -13438,7 +13434,7 @@
       </c>
       <c r="D117" s="13" t="inlineStr">
         <is>
-          <t>maa://29659 (87.50), maa://29031 (89.13)</t>
+          <t>maa://29659 (85.37), maa://29031 (89.36)</t>
         </is>
       </c>
       <c r="E117" s="14" t="inlineStr">
@@ -13708,7 +13704,7 @@
       </c>
       <c r="D122" s="13" t="inlineStr">
         <is>
-          <t>maa://20869 (100.00), maa://44690 (95.83)</t>
+          <t>maa://20869 (100.00), maa://44690 (95.92)</t>
         </is>
       </c>
       <c r="E122" s="14" t="inlineStr">
@@ -13762,7 +13758,7 @@
       </c>
       <c r="D123" s="13" t="inlineStr">
         <is>
-          <t>maa://29650 (98.51), maa://45570 (96.72)</t>
+          <t>maa://29650 (98.53), maa://45570 (96.72)</t>
         </is>
       </c>
       <c r="E123" s="14" t="inlineStr">
@@ -14194,7 +14190,7 @@
       </c>
       <c r="D131" s="13" t="inlineStr">
         <is>
-          <t>maa://21422 (99.23)</t>
+          <t>maa://21422 (99.24)</t>
         </is>
       </c>
       <c r="E131" s="14" t="inlineStr">
@@ -14842,7 +14838,7 @@
       </c>
       <c r="D143" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (97.80), *maa://23736 (52.44), maa://31185 (91.67), maa://30306 (100.00)</t>
+          <t>maa://28484 (97.81), *maa://23736 (52.44), maa://31185 (91.67), maa://30306 (100.00)</t>
         </is>
       </c>
       <c r="E143" s="14" t="inlineStr">
@@ -15220,7 +15216,7 @@
       </c>
       <c r="D150" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.83), maa://36641 (98.24), maa://36865 (95.45), maa://44635 (88.18), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (100.00), maa://42918 (100.00), maa://44119 (97.44), maa://64408 (92.86), maa://37300 (100.00), maa://42917 (100.00)</t>
+          <t>maa://40957 (94.86), maa://36641 (98.24), maa://36865 (95.45), maa://44635 (88.18), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (100.00), maa://42918 (100.00), maa://44119 (97.44), maa://64408 (92.86), maa://37300 (100.00), maa://42917 (100.00)</t>
         </is>
       </c>
       <c r="E150" s="14" t="inlineStr">
@@ -15274,7 +15270,7 @@
       </c>
       <c r="D151" s="13" t="inlineStr">
         <is>
-          <t>maa://51549 (96.83), maa://51923 (96.30), maa://67508 (100.00)</t>
+          <t>maa://51549 (96.97), maa://51923 (96.30), maa://67508 (100.00)</t>
         </is>
       </c>
       <c r="E151" s="14" t="inlineStr">
@@ -15760,7 +15756,7 @@
       </c>
       <c r="D160" s="13" t="inlineStr">
         <is>
-          <t>maa://44232 (98.47), maa://45603 (90.62), *maa://65963 (80.00), *maa://63114 (66.67)</t>
+          <t>maa://44232 (98.48), maa://45603 (90.62), *maa://65963 (80.00), *maa://63114 (66.67)</t>
         </is>
       </c>
       <c r="E160" s="14" t="inlineStr">
@@ -15976,7 +15972,7 @@
       </c>
       <c r="D164" s="13" t="inlineStr">
         <is>
-          <t>*maa://32845 (80.00), maa://29054 (100.00)</t>
+          <t>*maa://32845 (76.19), maa://29054 (100.00)</t>
         </is>
       </c>
       <c r="E164" s="14" t="inlineStr">
@@ -16192,7 +16188,7 @@
       </c>
       <c r="D168" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (92.26), maa://29627 (92.95), maa://29659 (87.50), maa://49074 (94.20), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
+          <t>maa://29633 (92.26), maa://29627 (92.95), maa://29659 (85.37), maa://49074 (94.20), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
         </is>
       </c>
       <c r="E168" s="14" t="inlineStr">
@@ -16246,7 +16242,7 @@
       </c>
       <c r="D169" s="13" t="inlineStr">
         <is>
-          <t>maa://49867 (93.59), maa://49655 (97.73)</t>
+          <t>maa://49867 (93.75), maa://49655 (97.73)</t>
         </is>
       </c>
       <c r="E169" s="14" t="inlineStr">
@@ -17434,7 +17430,7 @@
       </c>
       <c r="D191" s="13" t="inlineStr">
         <is>
-          <t>maa://34866 (93.75), maa://34714 (96.88)</t>
+          <t>maa://34866 (93.75), maa://34714 (96.97)</t>
         </is>
       </c>
       <c r="E191" s="14" t="inlineStr">
@@ -17812,7 +17808,7 @@
       </c>
       <c r="D198" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.46), maa://35854 (84.75), maa://50388 (98.25), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (94.59)</t>
+          <t>maa://44224 (90.48), maa://35854 (84.75), maa://50388 (98.25), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (95.00)</t>
         </is>
       </c>
       <c r="E198" s="14" t="inlineStr">
@@ -17866,7 +17862,7 @@
       </c>
       <c r="D199" s="13" t="inlineStr">
         <is>
-          <t>maa://39156 (94.19), *maa://39550 (55.00), *maa://53417 (75.00), *maa://63806 (77.78)</t>
+          <t>maa://39156 (94.19), *maa://39550 (55.00), *maa://53417 (77.78), *maa://63806 (77.78)</t>
         </is>
       </c>
       <c r="E199" s="14" t="inlineStr">
@@ -17920,7 +17916,7 @@
       </c>
       <c r="D200" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (86.17), *maa://28190 (62.86), maa://22894 (91.67), *maa://20906 (72.22), **maa://20907 (34.38)</t>
+          <t>maa://27823 (86.32), *maa://28190 (62.86), maa://22894 (91.67), *maa://20906 (72.22), **maa://20907 (34.38)</t>
         </is>
       </c>
       <c r="E200" s="14" t="inlineStr">
@@ -17974,7 +17970,7 @@
       </c>
       <c r="D201" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (86.17), *maa://28190 (62.86), maa://22894 (91.67), *maa://20906 (72.22), **maa://20907 (34.38)</t>
+          <t>maa://27823 (86.32), *maa://28190 (62.86), maa://22894 (91.67), *maa://20906 (72.22), **maa://20907 (34.38)</t>
         </is>
       </c>
       <c r="E201" s="14" t="inlineStr">
@@ -18730,7 +18726,7 @@
       </c>
       <c r="D215" s="13" t="inlineStr">
         <is>
-          <t>maa://64044 (96.00)</t>
+          <t>maa://64044 (96.08)</t>
         </is>
       </c>
       <c r="E215" s="14" t="inlineStr">
@@ -19486,7 +19482,7 @@
       </c>
       <c r="D229" s="13" t="inlineStr">
         <is>
-          <t>maa://20987 (94.06), *maa://35801 (77.78)</t>
+          <t>maa://20987 (94.17), *maa://35801 (77.78)</t>
         </is>
       </c>
       <c r="E229" s="14" t="inlineStr">
@@ -19540,7 +19536,7 @@
       </c>
       <c r="D230" s="13" t="inlineStr">
         <is>
-          <t>*maa://29644 (73.08), maa://39159 (96.88), ***maa://30061 (27.27)</t>
+          <t>*maa://29644 (73.08), maa://39159 (93.94), ***maa://30061 (27.27)</t>
         </is>
       </c>
       <c r="E230" s="14" t="inlineStr">
@@ -19756,7 +19752,7 @@
       </c>
       <c r="D234" s="13" t="inlineStr">
         <is>
-          <t>*maa://48263 (75.00)</t>
+          <t>*maa://48263 (75.86)</t>
         </is>
       </c>
       <c r="E234" s="14" t="inlineStr">
@@ -20188,7 +20184,7 @@
       </c>
       <c r="D242" s="13" t="inlineStr">
         <is>
-          <t>*maa://30667 (78.85), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (58.46), maa://39588 (86.67), *maa://64079 (78.57), maa://65726 (87.50), maa://68226 (100.00)</t>
+          <t>*maa://30667 (78.85), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (58.46), maa://39588 (86.67), *maa://64079 (78.57), maa://65726 (88.89), maa://68226 (100.00)</t>
         </is>
       </c>
       <c r="E242" s="14" t="inlineStr">
@@ -20458,7 +20454,7 @@
       </c>
       <c r="D247" s="13" t="inlineStr">
         <is>
-          <t>maa://20867 (93.33), maa://38485 (96.43), *maa://32202 (80.00)</t>
+          <t>maa://20867 (93.33), maa://38485 (96.67), *maa://32202 (80.00)</t>
         </is>
       </c>
       <c r="E247" s="14" t="inlineStr">
@@ -20674,7 +20670,7 @@
       </c>
       <c r="D251" s="13" t="inlineStr">
         <is>
-          <t>maa://28923 (91.87), maa://28906 (98.28), ***maa://28825 (11.54), maa://65613 (100.00)</t>
+          <t>maa://28923 (91.87), maa://28906 (98.31), ***maa://28825 (11.54), maa://65613 (100.00)</t>
         </is>
       </c>
       <c r="E251" s="14" t="inlineStr">
@@ -20728,7 +20724,7 @@
       </c>
       <c r="D252" s="13" t="inlineStr">
         <is>
-          <t>maa://42287 (91.80), maa://45570 (96.72), maa://60678 (93.33), maa://42225 (100.00)</t>
+          <t>maa://42287 (91.87), maa://45570 (96.72), maa://60678 (93.33), maa://42225 (100.00)</t>
         </is>
       </c>
       <c r="E252" s="14" t="inlineStr">
@@ -20890,7 +20886,7 @@
       </c>
       <c r="D255" s="13" t="inlineStr">
         <is>
-          <t>maa://31559 (93.88), maa://24093 (100.00), maa://20924 (95.24), **maa://49440 (42.86), maa://63591 (100.00)</t>
+          <t>maa://31559 (94.00), maa://24093 (100.00), maa://20924 (95.24), **maa://49440 (42.86), maa://63591 (100.00)</t>
         </is>
       </c>
       <c r="E255" s="14" t="inlineStr">
@@ -20944,7 +20940,7 @@
       </c>
       <c r="D256" s="13" t="inlineStr">
         <is>
-          <t>maa://40958 (90.32), *maa://45067 (75.00)</t>
+          <t>maa://40958 (90.62), *maa://45067 (75.00)</t>
         </is>
       </c>
       <c r="E256" s="14" t="inlineStr">
@@ -21052,7 +21048,7 @@
       </c>
       <c r="D258" s="13" t="inlineStr">
         <is>
-          <t>maa://20877 (98.75), *maa://45067 (75.00), maa://20836 (100.00), maa://20632 (100.00)</t>
+          <t>maa://20877 (98.77), *maa://45067 (75.00), maa://20836 (100.00), maa://20632 (100.00)</t>
         </is>
       </c>
       <c r="E258" s="14" t="inlineStr">
@@ -21106,7 +21102,7 @@
       </c>
       <c r="D259" s="13" t="inlineStr">
         <is>
-          <t>maa://20879 (86.14), maa://20834 (92.86)</t>
+          <t>maa://20879 (86.27), maa://20834 (92.86)</t>
         </is>
       </c>
       <c r="E259" s="14" t="inlineStr">
@@ -21862,7 +21858,7 @@
       </c>
       <c r="D273" s="13" t="inlineStr">
         <is>
-          <t>maa://25769 (96.91)</t>
+          <t>maa://25769 (96.93)</t>
         </is>
       </c>
       <c r="E273" s="14" t="inlineStr">
@@ -22024,7 +22020,7 @@
       </c>
       <c r="D276" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.72), maa://51630 (96.26), maa://56588 (93.33), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (41.67), *maa://66758 (75.00)</t>
+          <t>maa://51881 (98.73), maa://51630 (96.26), maa://56588 (93.33), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (41.67), *maa://66758 (75.00)</t>
         </is>
       </c>
       <c r="E276" s="14" t="inlineStr">
@@ -22780,7 +22776,7 @@
       </c>
       <c r="D290" s="13" t="inlineStr">
         <is>
-          <t>maa://20899 (90.00), maa://46332 (92.86), ***maa://44744 (25.00)</t>
+          <t>maa://20899 (90.06), maa://46332 (92.86), ***maa://44744 (25.00)</t>
         </is>
       </c>
       <c r="E290" s="14" t="inlineStr">
@@ -22942,7 +22938,7 @@
       </c>
       <c r="D293" s="13" t="inlineStr">
         <is>
-          <t>maa://30710 (97.93), maa://36845 (95.86), maa://31558 (97.22), **maa://39217 (38.89), maa://30668 (86.67)</t>
+          <t>maa://30710 (97.93), maa://36845 (95.89), maa://31558 (97.22), **maa://39217 (38.89), maa://30668 (86.67)</t>
         </is>
       </c>
       <c r="E293" s="14" t="inlineStr">
@@ -23212,7 +23208,7 @@
       </c>
       <c r="D298" s="13" t="inlineStr">
         <is>
-          <t>maa://32414 (98.81), maa://39155 (97.50), maa://32505 (100.00)</t>
+          <t>maa://32414 (98.82), maa://39155 (97.50), maa://32505 (100.00)</t>
         </is>
       </c>
       <c r="E298" s="14" t="inlineStr">
@@ -23698,7 +23694,7 @@
       </c>
       <c r="D307" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (98.48), maa://49642 (97.62), maa://49660 (93.62), maa://50517 (85.71)</t>
+          <t>maa://50280 (98.49), maa://49642 (97.62), maa://49660 (93.62), maa://50517 (85.71)</t>
         </is>
       </c>
       <c r="E307" s="14" t="inlineStr">
@@ -24076,7 +24072,7 @@
       </c>
       <c r="D314" s="13" t="inlineStr">
         <is>
-          <t>maa://53348 (86.67)</t>
+          <t>maa://53348 (87.10)</t>
         </is>
       </c>
       <c r="E314" s="14" t="inlineStr">
@@ -24346,7 +24342,7 @@
       </c>
       <c r="D319" s="13" t="inlineStr">
         <is>
-          <t>maa://25367 (99.36)</t>
+          <t>maa://25367 (99.37)</t>
         </is>
       </c>
       <c r="E319" s="14" t="inlineStr">
@@ -24400,7 +24396,7 @@
       </c>
       <c r="D320" s="13" t="inlineStr">
         <is>
-          <t>*maa://62755 (70.59), maa://62761 (91.67)</t>
+          <t>*maa://62755 (72.22), maa://62761 (93.33)</t>
         </is>
       </c>
       <c r="E320" s="14" t="inlineStr">
@@ -24724,7 +24720,7 @@
       </c>
       <c r="D326" s="13" t="inlineStr">
         <is>
-          <t>maa://39692 (99.54), maa://39810 (90.00)</t>
+          <t>maa://39692 (99.54), maa://39810 (90.32)</t>
         </is>
       </c>
       <c r="E326" s="14" t="inlineStr">
@@ -25102,7 +25098,7 @@
       </c>
       <c r="D333" s="15" t="inlineStr">
         <is>
-          <t>maa://40956 (94.00)</t>
+          <t>maa://40956 (94.12)</t>
         </is>
       </c>
       <c r="E333" s="15" t="inlineStr">
@@ -25426,7 +25422,7 @@
       </c>
       <c r="D339" s="22" t="inlineStr">
         <is>
-          <t>maa://42968 (99.16), maa://49245 (100.00)</t>
+          <t>maa://42968 (99.17), maa://49245 (100.00)</t>
         </is>
       </c>
       <c r="E339" s="22" t="inlineStr">
@@ -26020,7 +26016,7 @@
       </c>
       <c r="D350" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (97.59), maa://32415 (84.73), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
+          <t>maa://32647 (97.59), maa://32415 (84.53), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E350" s="22" t="inlineStr">
@@ -26506,7 +26502,7 @@
       </c>
       <c r="D359" s="22" t="inlineStr">
         <is>
-          <t>maa://36868 (99.54), maa://35996 (97.89), maa://47349 (97.50), **maa://39217 (38.89)</t>
+          <t>maa://36868 (99.33), maa://35996 (97.89), maa://47349 (97.56), **maa://39217 (38.89)</t>
         </is>
       </c>
       <c r="E359" s="22" t="inlineStr">
@@ -26560,7 +26556,7 @@
       </c>
       <c r="D360" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.59), maa://49695 (100.00), maa://49758 (98.70), *maa://59402 (56.67), *maa://52357 (75.00), *maa://63091 (72.73)</t>
+          <t>maa://49696 (99.60), maa://49695 (100.00), maa://49758 (98.70), *maa://59402 (56.67), *maa://52357 (75.00), *maa://63091 (75.00)</t>
         </is>
       </c>
       <c r="E360" s="22" t="inlineStr">
@@ -26722,7 +26718,7 @@
       </c>
       <c r="D363" s="22" t="inlineStr">
         <is>
-          <t>maa://49648 (96.10), maa://49662 (83.87)</t>
+          <t>maa://49648 (96.10), maa://49662 (81.25)</t>
         </is>
       </c>
       <c r="E363" s="22" t="inlineStr">
@@ -26776,7 +26772,7 @@
       </c>
       <c r="D364" s="22" t="inlineStr">
         <is>
-          <t>maa://36646 (98.90), maa://36845 (95.86), **maa://39217 (38.89), maa://51007 (98.28)</t>
+          <t>maa://36646 (98.91), maa://36845 (95.89), **maa://39217 (38.89), maa://51007 (98.28)</t>
         </is>
       </c>
       <c r="E364" s="22" t="inlineStr">
@@ -27046,7 +27042,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (94.83), maa://48026 (94.70), maa://44635 (88.18), maa://41035 (93.51), *maa://60251 (76.47), maa://44660 (92.68), maa://41128 (84.21)</t>
+          <t>maa://40957 (94.86), maa://48026 (94.70), maa://44635 (88.18), maa://41035 (93.51), *maa://60251 (76.47), maa://44660 (92.68), maa://41128 (84.21)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -27532,7 +27528,7 @@
       </c>
       <c r="D378" s="22" t="inlineStr">
         <is>
-          <t>maa://41110 (98.52), maa://45605 (90.00)</t>
+          <t>maa://41110 (98.54), maa://45605 (90.00)</t>
         </is>
       </c>
       <c r="E378" s="22" t="inlineStr">
@@ -27694,7 +27690,7 @@
       </c>
       <c r="D381" s="22" t="inlineStr">
         <is>
-          <t>maa://44233 (91.67), maa://45570 (96.72)</t>
+          <t>maa://44233 (91.80), maa://45570 (96.72)</t>
         </is>
       </c>
       <c r="E381" s="22" t="inlineStr">
@@ -27856,7 +27852,7 @@
       </c>
       <c r="D384" s="22" t="inlineStr">
         <is>
-          <t>*maa://53307 (69.23)</t>
+          <t>*maa://53307 (68.97)</t>
         </is>
       </c>
       <c r="E384" s="22" t="inlineStr">
@@ -27964,7 +27960,7 @@
       </c>
       <c r="D386" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (81.00), maa://44745 (98.04), **maa://49516 (37.93), *maa://45952 (57.14), ***maa://46851 (12.50), *maa://44896 (77.78)</t>
+          <t>maa://42970 (81.07), maa://44745 (98.05), **maa://49516 (37.93), *maa://45952 (57.14), ***maa://46851 (12.50), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E386" s="22" t="inlineStr">
@@ -28288,7 +28284,7 @@
       </c>
       <c r="D392" s="22" t="inlineStr">
         <is>
-          <t>maa://63890 (97.78), maa://64043 (100.00)</t>
+          <t>maa://63890 (97.92), maa://64043 (100.00)</t>
         </is>
       </c>
       <c r="E392" s="22" t="inlineStr">
@@ -28369,7 +28365,7 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>maa://47023 (87.80)</t>
+          <t>maa://47023 (86.27)</t>
         </is>
       </c>
       <c r="E394" t="inlineStr">
@@ -28423,7 +28419,7 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>maa://59533 (97.83), maa://59577 (100.00)</t>
+          <t>maa://59533 (97.87), maa://59577 (100.00)</t>
         </is>
       </c>
       <c r="E396" t="inlineStr">
@@ -28558,7 +28554,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>maa://51872 (96.63), maa://51876 (99.06), maa://63228 (88.24), maa://51873 (100.00), maa://62047 (92.00)</t>
+          <t>maa://51872 (96.66), maa://51876 (99.07), maa://63228 (88.24), maa://51873 (100.00), maa://62047 (92.00)</t>
         </is>
       </c>
       <c r="E401" t="inlineStr">
@@ -28612,7 +28608,7 @@
       </c>
       <c r="D403" t="inlineStr">
         <is>
-          <t>maa://60449 (98.99), maa://59493 (96.88)</t>
+          <t>maa://60449 (99.00), maa://59493 (96.88)</t>
         </is>
       </c>
       <c r="E403" t="inlineStr">
@@ -28666,7 +28662,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>maa://62756 (95.92)</t>
+          <t>maa://62756 (96.00)</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">
@@ -28720,7 +28716,7 @@
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>maa://64040 (98.98), maa://52505 (98.50), maa://66377 (93.33), ***maa://66376 (25.00)</t>
+          <t>maa://64040 (99.01), maa://52505 (98.18), maa://66377 (93.75), ***maa://66376 (20.00)</t>
         </is>
       </c>
       <c r="E407" t="inlineStr">
@@ -28747,7 +28743,7 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>maa://67090 (87.50)</t>
+          <t>maa://67090 (89.47)</t>
         </is>
       </c>
       <c r="E408" t="inlineStr">
@@ -28774,7 +28770,7 @@
       </c>
       <c r="D409" t="inlineStr">
         <is>
-          <t>maa://67388 (91.89)</t>
+          <t>maa://67388 (93.02)</t>
         </is>
       </c>
       <c r="E409" t="inlineStr">
@@ -28801,7 +28797,7 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>maa://67089 (97.50), maa://67271 (93.75)</t>
+          <t>maa://67089 (97.67), maa://67271 (93.75)</t>
         </is>
       </c>
       <c r="E410" t="inlineStr">
@@ -28828,7 +28824,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>maa://67088 (90.91)</t>
+          <t>maa://67088 (91.94)</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
@@ -28855,7 +28851,7 @@
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>maa://67087 (93.55), maa://67268 (96.05), maa://67269 (88.24), maa://67648 (100.00)</t>
+          <t>maa://67087 (94.12), maa://67268 (96.63), maa://67269 (88.89), maa://67648 (100.00)</t>
         </is>
       </c>
       <c r="E412" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#243)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -712,7 +712,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (98.31), maa://24702 (95.06), maa://36681 (85.23)</t>
+          <t>maa://25390 (98.33), maa://24702 (95.08), maa://36681 (85.39)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://58660 (98.85), maa://39402 (94.87), *maa://34787 (75.00)</t>
+          <t>maa://58660 (98.88), maa://39402 (94.94), *maa://34787 (75.00)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -776,7 +776,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (97.29), maa://66635 (99.55)</t>
+          <t>maa://22742 (97.32), maa://66635 (99.57)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://36684 (98.28), maa://21246 (91.32)</t>
+          <t>maa://36684 (98.25), maa://21246 (91.37)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://59087 (97.20), maa://25251 (91.61)</t>
+          <t>maa://59087 (97.27), maa://25251 (91.61)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -842,7 +842,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (99.38), maa://36987 (97.18), maa://39849 (91.67)</t>
+          <t>maa://40192 (99.40), maa://36987 (97.18), maa://39849 (91.67)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -858,7 +858,7 @@
       </c>
       <c r="H3" s="8" t="inlineStr">
         <is>
-          <t>maa://21247 (99.37)</t>
+          <t>maa://21247 (99.38)</t>
         </is>
       </c>
       <c r="I3" s="19" t="n"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>maa://22880 (91.07), maa://20276 (94.02), maa://22749 (84.62)</t>
+          <t>maa://22880 (91.09), maa://20276 (94.05), maa://22749 (84.62)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -890,7 +890,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (98.38), maa://26254 (98.11), *maa://22738 (80.00)</t>
+          <t>maa://21249 (98.41), maa://26254 (98.15), *maa://22738 (80.00)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://60545 (98.71), maa://45854 (87.32), maa://24617 (91.18)</t>
+          <t>maa://60545 (98.75), maa://45854 (87.44), maa://24617 (91.18)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (92.11), maa://27484 (99.19), maa://27480 (85.96)</t>
+          <t>maa://27396 (92.26), maa://27484 (99.20), maa://27480 (86.21)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://52241 (99.10), maa://24390 (96.77)</t>
+          <t>maa://52241 (99.41), maa://24390 (96.77)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -954,7 +954,7 @@
       </c>
       <c r="AF3" s="8" t="inlineStr">
         <is>
-          <t>maa://21289 (91.82)</t>
+          <t>maa://21289 (92.04)</t>
         </is>
       </c>
       <c r="AG3" s="16" t="n"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (98.03), maa://22499 (90.00), maa://22746 (100.00)</t>
+          <t>maa://24632 (98.07), maa://22499 (90.00), maa://22746 (100.00)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (99.09), maa://50121 (96.88)</t>
+          <t>maa://49983 (99.11), maa://50121 (96.15)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://27295 (97.78), maa://32509 (96.37), maa://31008 (95.16), maa://22754 (88.16)</t>
+          <t>maa://27295 (97.72), maa://32509 (96.43), maa://31008 (95.21), maa://22754 (88.16)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="X4" s="8" t="inlineStr">
         <is>
-          <t>maa://43217 (98.84)</t>
+          <t>maa://43217 (98.86)</t>
         </is>
       </c>
       <c r="Y4" s="19" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (91.18), maa://54105 (98.47), *maa://22744 (80.00)</t>
+          <t>maa://21245 (91.33), maa://54105 (98.50), *maa://22744 (80.00)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="L5" s="8" t="inlineStr">
         <is>
-          <t>maa://22757 (90.83)</t>
+          <t>maa://22757 (90.91)</t>
         </is>
       </c>
       <c r="M5" s="19" t="n"/>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="P5" s="8" t="inlineStr">
         <is>
-          <t>maa://21919 (99.08), maa://21281 (81.25)</t>
+          <t>maa://21919 (98.65), maa://21281 (81.25)</t>
         </is>
       </c>
       <c r="Q5" s="19" t="n"/>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="X5" s="8" t="inlineStr">
         <is>
-          <t>maa://21290 (98.50)</t>
+          <t>maa://21290 (98.51)</t>
         </is>
       </c>
       <c r="Y5" s="19" t="n"/>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="D6" s="8" t="inlineStr">
         <is>
-          <t>maa://42407 (97.41)</t>
+          <t>maa://42407 (97.45)</t>
         </is>
       </c>
       <c r="E6" s="19" t="n"/>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="H6" s="8" t="inlineStr">
         <is>
-          <t>maa://24370 (97.48)</t>
+          <t>maa://24370 (97.54)</t>
         </is>
       </c>
       <c r="I6" s="19" t="n"/>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="L6" s="8" t="inlineStr">
         <is>
-          <t>maa://24839 (99.42)</t>
+          <t>maa://24839 (99.43)</t>
         </is>
       </c>
       <c r="M6" s="19" t="n"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (98.83), maa://30381 (95.00)</t>
+          <t>maa://31836 (98.86), maa://30381 (95.00)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="X6" s="8" t="inlineStr">
         <is>
-          <t>maa://52754 (96.41)</t>
+          <t>maa://52754 (96.49)</t>
         </is>
       </c>
       <c r="Y6" s="19" t="n"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="AF6" s="8" t="inlineStr">
         <is>
-          <t>maa://33152 (80.56)</t>
+          <t>maa://33152 (80.82)</t>
         </is>
       </c>
       <c r="AG6" s="16" t="n"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>maa://21955 (98.16)</t>
+          <t>maa://21955 (98.20)</t>
         </is>
       </c>
       <c r="E7" s="19" t="n"/>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (98.58), maa://24957 (94.55)</t>
+          <t>maa://28624 (98.62), maa://24957 (94.55)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="P7" s="8" t="inlineStr">
         <is>
-          <t>maa://22750 (96.89)</t>
+          <t>maa://22750 (96.95)</t>
         </is>
       </c>
       <c r="Q7" s="19" t="n"/>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="T7" s="8" t="inlineStr">
         <is>
-          <t>maa://21291 (93.98)</t>
+          <t>maa://21291 (94.01)</t>
         </is>
       </c>
       <c r="U7" s="19" t="n"/>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (97.18), maa://22758 (82.35)</t>
+          <t>maa://22399 (97.23), maa://22758 (82.35)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.10.01 13:20:43</t>
+          <t>更新日期：2025.10.03 13:19:12</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1497,12 +1497,12 @@
       </c>
       <c r="C8" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (90.00), *maa://39431 (61.54), **maa://37551 (50.00)</t>
+          <t>maa://21476 (90.06)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
-          <t>*maa://24371 (79.38)</t>
+          <t>*maa://24371 (79.59)</t>
         </is>
       </c>
       <c r="I8" s="19" t="n"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (91.18), maa://23252 (91.67), maa://37496 (98.33)</t>
+          <t>maa://32931 (91.29), maa://23252 (91.67), maa://37496 (98.33)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (96.05), maa://67587 (98.55)</t>
+          <t>maa://21411 (96.07), maa://67587 (98.62)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="AB8" s="8" t="inlineStr">
         <is>
-          <t>maa://25389 (94.50)</t>
+          <t>maa://25389 (94.64)</t>
         </is>
       </c>
       <c r="AC8" s="19" t="n"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>maa://24479 (84.29), *maa://21990 (51.72)</t>
+          <t>maa://24479 (84.38), *maa://21990 (51.72)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>maa://22765 (95.68), *maa://21915 (78.57)</t>
+          <t>maa://22765 (95.73), *maa://21915 (78.57)</t>
         </is>
       </c>
       <c r="E9" s="19" t="n"/>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (96.31), maa://39552 (87.50)</t>
+          <t>maa://22762 (96.33), maa://39552 (88.00)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://52237 (99.76), maa://26223 (98.31)</t>
+          <t>maa://52237 (99.77), maa://26223 (98.31)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (95.19), maa://40166 (94.74)</t>
+          <t>maa://28711 (95.23), maa://40166 (94.81)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (91.22), maa://66916 (98.08)</t>
+          <t>maa://26206 (91.32), maa://66916 (98.12)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>maa://54000 (92.22)</t>
+          <t>maa://54000 (92.31)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (99.25), maa://22755 (91.53), maa://63521 (94.74)</t>
+          <t>maa://27395 (99.26), maa://22755 (91.62), maa://63521 (94.40)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://45828 (99.24), maa://22301 (97.64), maa://22726 (100.00)</t>
+          <t>maa://45828 (99.26), maa://22301 (97.64), maa://22726 (100.00)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>*maa://25021 (56.79), *maa://22733 (64.62), **maa://22761 (33.33)</t>
+          <t>*maa://25021 (57.32), *maa://22733 (64.62), **maa://22761 (33.33)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="L11" s="8" t="inlineStr">
         <is>
-          <t>maa://21287 (93.54)</t>
+          <t>maa://21287 (93.28)</t>
         </is>
       </c>
       <c r="M11" s="19" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (93.26), maa://22501 (99.54), maa://64808 (100.00), maa://45521 (95.24)</t>
+          <t>maa://22747 (93.33), maa://22501 (99.54), maa://64808 (100.00), maa://45521 (95.24)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="AF11" s="8" t="inlineStr">
         <is>
-          <t>maa://31203 (98.65)</t>
+          <t>maa://31203 (98.67)</t>
         </is>
       </c>
       <c r="AG11" s="16" t="n"/>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>maa://36678 (97.10), maa://30766 (91.18)</t>
+          <t>maa://36678 (97.14), maa://30766 (91.18)</t>
         </is>
       </c>
       <c r="E12" s="19" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (93.54), maa://54294 (96.63)</t>
+          <t>maa://21867 (93.56), maa://54294 (96.69)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (98.00), maa://64046 (98.58)</t>
+          <t>maa://63896 (98.01), maa://64046 (98.60)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://37962 (98.82), maa://21485 (81.70), maa://22753 (92.83)</t>
+          <t>maa://37962 (98.83), maa://21485 (81.70), maa://22753 (92.83)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://36677 (99.04), maa://23669 (95.12), maa://39872 (98.29)</t>
+          <t>maa://36677 (99.06), maa://23669 (94.83), maa://39872 (98.32)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>maa://28932 (94.61)</t>
+          <t>maa://28932 (94.67)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (96.64), maa://36673 (94.07), maa://25001 (88.76)</t>
+          <t>maa://24999 (96.69), maa://36673 (94.16), maa://25001 (88.76)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.20), maa://66545 (99.03)</t>
+          <t>*maa://21248 (73.33), maa://66545 (99.04)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (97.71), maa://22583 (88.12)</t>
+          <t>maa://22676 (97.76), maa://22583 (88.12)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="X13" s="8" t="inlineStr">
         <is>
-          <t>maa://34957 (94.46)</t>
+          <t>maa://34957 (94.57)</t>
         </is>
       </c>
       <c r="Y13" s="19" t="n"/>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (94.08)</t>
+          <t>maa://39883 (93.97)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (99.03), maa://36682 (98.28), maa://26245 (97.06), maa://21288 (96.40)</t>
+          <t>maa://39841 (99.05), maa://36682 (98.31), maa://26245 (97.06), maa://21288 (96.40)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2330,7 +2330,7 @@
       </c>
       <c r="P14" s="8" t="inlineStr">
         <is>
-          <t>maa://23250 (99.65), maa://20107 (87.50), maa://22772 (100.00), maa://68732 (100.00)</t>
+          <t>maa://23250 (99.66), maa://20107 (87.50), maa://22772 (100.00), maa://68732 (100.00)</t>
         </is>
       </c>
       <c r="Q14" s="19" t="n"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://42751 (98.94), maa://22521 (95.26)</t>
+          <t>maa://42751 (98.95), maa://22521 (95.26)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2378,7 +2378,7 @@
       </c>
       <c r="AB14" s="8" t="inlineStr">
         <is>
-          <t>maa://22764 (98.88)</t>
+          <t>maa://22764 (98.92)</t>
         </is>
       </c>
       <c r="AC14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (85.34), maa://45058 (98.17), maa://22734 (84.96), *maa://36048 (74.86), maa://69928 (100.00)</t>
+          <t>maa://22743 (85.42), maa://45058 (98.20), maa://22734 (84.96), *maa://36048 (74.86), maa://69928 (100.00)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (96.99), maa://21478 (90.48)</t>
+          <t>maa://24304 (97.05), maa://21478 (90.48)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="P15" s="8" t="inlineStr">
         <is>
-          <t>maa://24762 (97.65), *maa://22727 (70.00)</t>
+          <t>maa://24762 (97.69), *maa://22727 (70.00)</t>
         </is>
       </c>
       <c r="Q15" s="19" t="n"/>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="T15" s="8" t="inlineStr">
         <is>
-          <t>maa://23892 (97.58)</t>
+          <t>maa://23892 (97.63)</t>
         </is>
       </c>
       <c r="U15" s="19" t="n"/>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://36666 (96.31), maa://21364 (83.80), *maa://22766 (70.71), maa://68306 (81.08)</t>
+          <t>maa://36666 (96.34), maa://21364 (83.80), *maa://22766 (70.71), *maa://68306 (78.95)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2590,7 +2590,7 @@
       </c>
       <c r="P16" s="8" t="inlineStr">
         <is>
-          <t>maa://28504 (96.24)</t>
+          <t>maa://28504 (96.30)</t>
         </is>
       </c>
       <c r="Q16" s="19" t="n"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://36674 (98.03), maa://22729 (96.17), *maa://28648 (77.89)</t>
+          <t>maa://36674 (98.06), maa://22729 (96.20), *maa://28648 (77.89)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2622,7 +2622,7 @@
       </c>
       <c r="X16" s="8" t="inlineStr">
         <is>
-          <t>maa://28501 (99.33), maa://28051 (97.06)</t>
+          <t>maa://28501 (99.34), maa://28051 (97.14)</t>
         </is>
       </c>
       <c r="Y16" s="19" t="n"/>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="AB16" s="8" t="inlineStr">
         <is>
-          <t>maa://26228 (97.94)</t>
+          <t>maa://26228 (97.97)</t>
         </is>
       </c>
       <c r="AC16" s="19" t="n"/>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>maa://23911 (90.57), maa://27755 (93.75), maa://67613 (99.43)</t>
+          <t>maa://23911 (90.64), maa://27755 (93.75), maa://67613 (99.46)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://39599 (98.22), maa://22430 (90.21)</t>
+          <t>maa://39599 (98.25), maa://22430 (90.25)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (82.64), maa://56238 (98.48)</t>
+          <t>maa://23890 (82.64), maa://56238 (98.52)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="T17" s="8" t="inlineStr">
         <is>
-          <t>*maa://42324 (69.77)</t>
+          <t>*maa://42324 (70.45)</t>
         </is>
       </c>
       <c r="U17" s="19" t="n"/>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="AF17" s="8" t="inlineStr">
         <is>
-          <t>maa://50136 (98.98)</t>
+          <t>maa://50136 (99.01)</t>
         </is>
       </c>
       <c r="AG17" s="16" t="n"/>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>maa://24570 (98.34)</t>
+          <t>maa://24570 (98.37)</t>
         </is>
       </c>
       <c r="E18" s="19" t="n"/>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="H18" s="8" t="inlineStr">
         <is>
-          <t>maa://24421 (95.16)</t>
+          <t>maa://24421 (95.15)</t>
         </is>
       </c>
       <c r="I18" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), maa://54153 (99.65), maa://24380 (100.00)</t>
+          <t>maa://24379 (100.00), maa://54153 (99.66), maa://24380 (100.00)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (98.71), maa://22741 (92.31)</t>
+          <t>maa://21917 (98.72), maa://22741 (92.31)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="AB18" s="8" t="inlineStr">
         <is>
-          <t>maa://24393 (99.00)</t>
+          <t>maa://24393 (99.01)</t>
         </is>
       </c>
       <c r="AC18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://47854 (92.96)</t>
+          <t>maa://47854 (93.06)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -2932,7 +2932,7 @@
       </c>
       <c r="D19" s="8" t="inlineStr">
         <is>
-          <t>maa://62850 (99.27)</t>
+          <t>maa://62850 (99.28)</t>
         </is>
       </c>
       <c r="E19" s="19" t="n"/>
@@ -2948,7 +2948,7 @@
       </c>
       <c r="H19" s="8" t="inlineStr">
         <is>
-          <t>maa://66740 (91.67)</t>
+          <t>maa://66740 (92.31)</t>
         </is>
       </c>
       <c r="I19" s="19" t="n"/>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="T19" s="8" t="inlineStr">
         <is>
-          <t>maa://24386 (99.67)</t>
+          <t>maa://24386 (99.68)</t>
         </is>
       </c>
       <c r="U19" s="19" t="n"/>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (86.06), *maa://36668 (69.57)</t>
+          <t>maa://30709 (86.18), *maa://36668 (69.83)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3044,7 +3044,7 @@
       </c>
       <c r="AF19" s="8" t="inlineStr">
         <is>
-          <t>*maa://21663 (65.91), maa://52239 (88.24)</t>
+          <t>*maa://21663 (65.91), maa://52239 (86.11)</t>
         </is>
       </c>
       <c r="AG19" s="16" t="n"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://25198 (97.66), maa://36680 (99.08), maa://21432 (91.53)</t>
+          <t>maa://25198 (97.68), maa://36680 (99.09), maa://21432 (91.53)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3078,7 +3078,7 @@
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>maa://22864 (96.21)</t>
+          <t>maa://22864 (96.05)</t>
         </is>
       </c>
       <c r="I20" s="19" t="n"/>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (95.38)</t>
+          <t>maa://41331 (95.42)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="P20" s="8" t="inlineStr">
         <is>
-          <t>maa://37442 (98.54)</t>
+          <t>maa://37442 (98.55)</t>
         </is>
       </c>
       <c r="Q20" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (96.61), maa://56241 (98.24), maa://49976 (88.57)</t>
+          <t>maa://50085 (96.54), maa://56241 (98.27), maa://49976 (88.57)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="L21" s="8" t="inlineStr">
         <is>
-          <t>maa://31731 (96.49)</t>
+          <t>maa://31731 (96.52)</t>
         </is>
       </c>
       <c r="M21" s="19" t="n"/>
@@ -3240,7 +3240,7 @@
       </c>
       <c r="P21" s="8" t="inlineStr">
         <is>
-          <t>maa://24381 (82.35)</t>
+          <t>maa://24381 (82.86)</t>
         </is>
       </c>
       <c r="Q21" s="19" t="n"/>
@@ -3256,7 +3256,7 @@
       </c>
       <c r="T21" s="8" t="inlineStr">
         <is>
-          <t>maa://21993 (90.32)</t>
+          <t>maa://21993 (90.62)</t>
         </is>
       </c>
       <c r="U21" s="19" t="n"/>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (98.02), maa://20110 (87.01)</t>
+          <t>maa://34946 (98.09), maa://20110 (87.01)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="AB21" s="8" t="inlineStr">
         <is>
-          <t>maa://21443 (86.96), maa://52223 (83.03)</t>
+          <t>maa://21443 (87.07), maa://52223 (83.14)</t>
         </is>
       </c>
       <c r="AC21" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22432 (94.17), maa://22524 (83.16), maa://64221 (97.94)</t>
+          <t>maa://22432 (94.24), maa://22524 (83.16), maa://64221 (97.96)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>maa://25236 (99.22)</t>
+          <t>maa://25236 (99.23)</t>
         </is>
       </c>
       <c r="I22" s="19" t="n"/>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>maa://27127 (83.40), *maa://22751 (71.26), maa://66865 (99.41)</t>
+          <t>maa://27127 (83.47), *maa://22751 (71.26), maa://66865 (99.42)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://37649 (94.74), maa://21282 (98.95)</t>
+          <t>maa://37649 (94.80), maa://21282 (98.96)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="AB22" s="8" t="inlineStr">
         <is>
-          <t>maa://23656 (99.50)</t>
+          <t>maa://23656 (99.51)</t>
         </is>
       </c>
       <c r="AC22" s="19" t="n"/>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>*maa://41753 (66.67), **maa://28036 (30.77)</t>
+          <t>*maa://41753 (65.71), **maa://28036 (30.43)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (98.62), maa://39875 (95.76)</t>
+          <t>maa://39756 (98.59), maa://39875 (95.80)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (96.74), maa://29748 (81.68), *maa://37566 (78.46)</t>
+          <t>maa://30587 (96.76), maa://29748 (81.77), *maa://37566 (78.46)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3532,7 +3532,7 @@
       </c>
       <c r="X23" s="8" t="inlineStr">
         <is>
-          <t>*maa://28503 (60.26)</t>
+          <t>*maa://28503 (60.51)</t>
         </is>
       </c>
       <c r="Y23" s="19" t="n"/>
@@ -3548,7 +3548,7 @@
       </c>
       <c r="AB23" s="8" t="inlineStr">
         <is>
-          <t>maa://29652 (96.47)</t>
+          <t>maa://29652 (96.59)</t>
         </is>
       </c>
       <c r="AC23" s="19" t="n"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (85.41), maa://46650 (90.59)</t>
+          <t>maa://24368 (85.50), maa://46650 (90.75)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (96.38), maa://23504 (94.06), *maa://25141 (79.74), maa://52227 (97.43), *maa://36663 (79.44)</t>
+          <t>maa://29988 (96.42), maa://23504 (94.06), *maa://25141 (79.74), maa://52227 (97.45), *maa://36663 (79.44)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (96.60), maa://63016 (99.13)</t>
+          <t>maa://29753 (96.62), maa://63016 (99.14)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>*maa://29063 (76.01), *maa://25311 (70.63), maa://45047 (88.31)</t>
+          <t>*maa://29063 (76.22), *maa://25311 (70.83), maa://45047 (88.46)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3760,7 +3760,7 @@
       </c>
       <c r="P25" s="8" t="inlineStr">
         <is>
-          <t>maa://24382 (96.23)</t>
+          <t>maa://24382 (96.30)</t>
         </is>
       </c>
       <c r="Q25" s="19" t="n"/>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="T25" s="8" t="inlineStr">
         <is>
-          <t>maa://20109 (96.30), maa://22545 (100.00)</t>
+          <t>maa://20109 (96.37), maa://22545 (100.00)</t>
         </is>
       </c>
       <c r="U25" s="19" t="n"/>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="X25" s="8" t="inlineStr">
         <is>
-          <t>maa://29890 (91.47)</t>
+          <t>maa://29890 (91.60)</t>
         </is>
       </c>
       <c r="Y25" s="19" t="n"/>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (93.40), *maa://24516 (79.80), maa://26001 (83.33), maa://68311 (100.00)</t>
+          <t>maa://31215 (93.41), *maa://24516 (79.00), maa://26001 (83.33), maa://68311 (98.57)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (98.15), maa://36676 (99.84), maa://24621 (96.88), maa://22771 (88.24), maa://37772 (85.71)</t>
+          <t>maa://20108 (98.17), maa://36676 (99.84), maa://24621 (96.88), maa://22771 (88.24), maa://37772 (85.71)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3858,7 +3858,7 @@
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
-          <t>maa://56240 (96.21), maa://24913 (92.24)</t>
+          <t>maa://56240 (96.28), maa://24913 (92.24)</t>
         </is>
       </c>
       <c r="I26" s="19" t="n"/>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="AB26" s="8" t="inlineStr">
         <is>
-          <t>maa://42235 (98.39)</t>
+          <t>maa://42235 (98.40)</t>
         </is>
       </c>
       <c r="AC26" s="19" t="n"/>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>maa://39601 (91.38), maa://34494 (95.45)</t>
+          <t>maa://39601 (91.45), maa://34494 (95.45)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="T27" s="8" t="inlineStr">
         <is>
-          <t>maa://30624 (89.83)</t>
+          <t>maa://30624 (89.94)</t>
         </is>
       </c>
       <c r="U27" s="19" t="n"/>
@@ -4102,7 +4102,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (95.93), maa://25725 (85.38)</t>
+          <t>maa://24465 (95.95), maa://25725 (85.38)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="L28" s="8" t="inlineStr">
         <is>
-          <t>maa://30770 (90.32)</t>
+          <t>maa://30770 (90.43)</t>
         </is>
       </c>
       <c r="M28" s="19" t="n"/>
@@ -4166,7 +4166,7 @@
       </c>
       <c r="T28" s="8" t="inlineStr">
         <is>
-          <t>maa://29765 (93.62), maa://23263 (96.24)</t>
+          <t>maa://29765 (93.71), maa://23263 (96.27)</t>
         </is>
       </c>
       <c r="U28" s="19" t="n"/>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (97.45), maa://41749 (97.22)</t>
+          <t>maa://39929 (97.36), maa://41749 (97.23)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (94.34), maa://65700 (98.68)</t>
+          <t>maa://36660 (94.38), maa://65700 (98.69)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4232,7 +4232,7 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>maa://31694 (99.33)</t>
+          <t>maa://31694 (99.34)</t>
         </is>
       </c>
       <c r="E29" s="19" t="n"/>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (97.78), maa://31400 (98.09), maa://28440 (86.50)</t>
+          <t>maa://28432 (97.80), maa://31400 (98.10), maa://28440 (86.50)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4280,7 +4280,7 @@
       </c>
       <c r="P29" s="8" t="inlineStr">
         <is>
-          <t>maa://54169 (97.39)</t>
+          <t>maa://54169 (97.50)</t>
         </is>
       </c>
       <c r="Q29" s="19" t="n"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://42865 (92.14)</t>
+          <t>maa://42865 (92.16)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (95.59), maa://64191 (97.50)</t>
+          <t>maa://45792 (95.65), maa://64191 (97.56)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="L30" s="8" t="inlineStr">
         <is>
-          <t>maa://30442 (97.48)</t>
+          <t>maa://30442 (97.52)</t>
         </is>
       </c>
       <c r="M30" s="19" t="n"/>
@@ -4442,7 +4442,7 @@
       </c>
       <c r="X30" s="8" t="inlineStr">
         <is>
-          <t>maa://39477 (96.23)</t>
+          <t>maa://39477 (96.30)</t>
         </is>
       </c>
       <c r="Y30" s="19" t="n"/>
@@ -4458,7 +4458,7 @@
       </c>
       <c r="AB30" s="8" t="inlineStr">
         <is>
-          <t>maa://42979 (99.56), maa://45822 (100.00), maa://45045 (90.91)</t>
+          <t>maa://42979 (99.57), maa://45822 (100.00), maa://45045 (90.91)</t>
         </is>
       </c>
       <c r="AC30" s="19" t="n"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (98.05), maa://36258 (93.12), maa://43904 (90.00)</t>
+          <t>maa://35926 (98.07), maa://36258 (93.15), maa://43904 (88.10)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://36667 (99.65), maa://21895 (97.97), maa://22760 (100.00)</t>
+          <t>maa://36667 (99.59), maa://21895 (97.97), maa://22760 (100.00)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4654,7 +4654,7 @@
       </c>
       <c r="L32" s="8" t="inlineStr">
         <is>
-          <t>maa://28065 (97.06)</t>
+          <t>maa://28065 (97.09)</t>
         </is>
       </c>
       <c r="M32" s="19" t="n"/>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (99.29), maa://41108 (87.72), maa://41238 (98.14), maa://45523 (100.00)</t>
+          <t>maa://42859 (99.30), maa://41108 (87.72), maa://41238 (98.14), maa://45523 (100.00)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="X32" s="8" t="inlineStr">
         <is>
-          <t>maa://64104 (97.48)</t>
+          <t>maa://64104 (97.54)</t>
         </is>
       </c>
       <c r="Y32" s="19" t="n"/>
@@ -4795,12 +4795,12 @@
       </c>
       <c r="O33" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (94.59), *maa://22730 (70.59), maa://69135 (93.75)</t>
+          <t>maa://21956 (94.59), maa://69135 (95.00)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (99.24), maa://56235 (99.49)</t>
+          <t>maa://48817 (99.24), maa://56235 (99.50)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="T34" s="8" t="inlineStr">
         <is>
-          <t>maa://24526 (97.13)</t>
+          <t>maa://24526 (97.15)</t>
         </is>
       </c>
       <c r="U34" s="19" t="n"/>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="AB34" s="8" t="inlineStr">
         <is>
-          <t>maa://64329 (97.96)</t>
+          <t>maa://64329 (98.00)</t>
         </is>
       </c>
       <c r="AC34" s="19" t="n"/>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
-          <t>maa://41296 (99.27)</t>
+          <t>maa://41296 (99.28)</t>
         </is>
       </c>
       <c r="M35" s="19" t="n"/>
@@ -5206,7 +5206,7 @@
       </c>
       <c r="T36" s="8" t="inlineStr">
         <is>
-          <t>maa://27613 (99.56)</t>
+          <t>maa://27613 (99.57)</t>
         </is>
       </c>
       <c r="U36" s="19" t="n"/>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="AB36" s="19" t="inlineStr">
         <is>
-          <t>maa://64106 (97.14)</t>
+          <t>maa://64106 (97.22)</t>
         </is>
       </c>
       <c r="AC36" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (99.20), maa://56336 (99.37), maa://47069 (86.67), maa://45789 (100.00)</t>
+          <t>maa://45718 (99.05), maa://56336 (99.38), maa://47069 (86.67), maa://45789 (100.00)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="P37" s="8" t="inlineStr">
         <is>
-          <t>maa://21280 (97.64)</t>
+          <t>maa://21280 (97.66)</t>
         </is>
       </c>
       <c r="Q37" s="19" t="n"/>
@@ -5418,7 +5418,7 @@
       </c>
       <c r="L38" s="8" t="inlineStr">
         <is>
-          <t>maa://39384 (99.28), maa://49735 (92.86)</t>
+          <t>maa://39384 (99.29), maa://49735 (92.86)</t>
         </is>
       </c>
       <c r="M38" s="19" t="n"/>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="P38" s="8" t="inlineStr">
         <is>
-          <t>maa://24383 (82.01)</t>
+          <t>maa://24383 (82.20)</t>
         </is>
       </c>
       <c r="Q38" s="19" t="n"/>
@@ -5450,7 +5450,7 @@
       </c>
       <c r="T38" s="8" t="inlineStr">
         <is>
-          <t>maa://30713 (98.31)</t>
+          <t>maa://30713 (98.33)</t>
         </is>
       </c>
       <c r="U38" s="19" t="n"/>
@@ -5482,7 +5482,7 @@
       </c>
       <c r="AF38" s="8" t="inlineStr">
         <is>
-          <t>maa://36697 (95.72), maa://68397 (99.03)</t>
+          <t>maa://36697 (95.75), maa://68397 (99.10)</t>
         </is>
       </c>
       <c r="AG38" s="16" t="n"/>
@@ -5503,7 +5503,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://25199 (84.78), maa://45059 (93.94), maa://30434 (95.31), maa://44165 (85.71)</t>
+          <t>maa://25199 (84.78), maa://45059 (94.12), maa://30434 (95.34), maa://44165 (85.71)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://47093 (98.25), maa://24709 (94.05)</t>
+          <t>maa://47093 (98.28), maa://24709 (94.07)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (95.75), maa://45790 (88.00)</t>
+          <t>maa://47079 (95.70), maa://45790 (88.16)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5583,7 +5583,7 @@
       </c>
       <c r="AF39" s="8" t="inlineStr">
         <is>
-          <t>maa://62953 (96.75)</t>
+          <t>maa://62953 (96.81)</t>
         </is>
       </c>
       <c r="AG39" s="16" t="n"/>
@@ -5636,7 +5636,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (98.13), maa://21386 (95.94), maa://36664 (89.61), *maa://45550 (75.00)</t>
+          <t>maa://23278 (98.14), maa://21386 (95.96), maa://36664 (89.74), *maa://45550 (75.00)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://65283 (96.95), maa://64205 (93.75)</t>
+          <t>maa://65283 (97.03), maa://64205 (93.75)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>*maa://22525 (70.09), maa://21284 (97.75)</t>
+          <t>*maa://22525 (70.09), maa://21284 (97.77)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -6008,7 +6008,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (98.28), maa://56386 (99.41), maa://27728 (96.40)</t>
+          <t>maa://29768 (98.29), maa://56386 (99.42), maa://27728 (96.40)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6056,7 +6056,7 @@
       </c>
       <c r="T44" s="8" t="inlineStr">
         <is>
-          <t>maa://39366 (93.48)</t>
+          <t>maa://39366 (93.62)</t>
         </is>
       </c>
       <c r="U44" s="19" t="n"/>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://42459 (98.74), maa://21229 (85.65), maa://30807 (94.62), *maa://22767 (70.83)</t>
+          <t>maa://42459 (98.75), maa://21229 (85.78), maa://30807 (94.62), *maa://22767 (70.83)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6125,7 +6125,7 @@
       </c>
       <c r="T45" s="8" t="inlineStr">
         <is>
-          <t>*maa://39364 (67.48)</t>
+          <t>*maa://39364 (67.88)</t>
         </is>
       </c>
       <c r="U45" s="19" t="n"/>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (95.81), maa://43901 (96.34)</t>
+          <t>maa://35931 (95.85), maa://43901 (96.34)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6231,7 +6231,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (97.51), maa://29661 (97.22), maa://56236 (99.79), maa://28038 (84.62)</t>
+          <t>maa://27410 (97.52), maa://29661 (97.24), maa://56236 (99.79), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6263,7 +6263,7 @@
       </c>
       <c r="T47" s="8" t="inlineStr">
         <is>
-          <t>maa://67476 (99.57), maa://68392 (99.56)</t>
+          <t>maa://67476 (99.57), maa://68392 (99.61)</t>
         </is>
       </c>
       <c r="U47" s="19" t="n"/>
@@ -6381,7 +6381,7 @@
       </c>
       <c r="P49" s="8" t="inlineStr">
         <is>
-          <t>*maa://39643 (79.14)</t>
+          <t>*maa://39643 (79.58)</t>
         </is>
       </c>
       <c r="Q49" s="19" t="n"/>
@@ -6397,7 +6397,7 @@
       </c>
       <c r="T49" s="19" t="inlineStr">
         <is>
-          <t>maa://67231 (99.13)</t>
+          <t>maa://67231 (99.15)</t>
         </is>
       </c>
       <c r="U49" s="19" t="n"/>
@@ -6434,7 +6434,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>maa://62852 (93.12)</t>
+          <t>maa://62852 (93.25)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6468,7 +6468,7 @@
       </c>
       <c r="H51" s="8" t="inlineStr">
         <is>
-          <t>maa://30769 (89.66)</t>
+          <t>maa://30769 (90.00)</t>
         </is>
       </c>
       <c r="I51" s="19" t="n"/>
@@ -6518,7 +6518,7 @@
       </c>
       <c r="H52" s="8" t="inlineStr">
         <is>
-          <t>maa://24376 (99.09)</t>
+          <t>maa://24376 (99.11)</t>
         </is>
       </c>
       <c r="I52" s="19" t="n"/>
@@ -6534,7 +6534,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (99.39), maa://59378 (93.83), maa://65511 (100.00)</t>
+          <t>maa://59394 (99.40), maa://59378 (93.83), maa://65511 (100.00)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6568,7 +6568,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (97.93)</t>
+          <t>maa://32534 (97.94)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -6652,7 +6652,7 @@
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>maa://32532 (97.86)</t>
+          <t>maa://32532 (97.89)</t>
         </is>
       </c>
       <c r="I55" s="19" t="n"/>
@@ -6704,7 +6704,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://56237 (98.17), maa://25176 (98.77)</t>
+          <t>maa://56237 (98.22), maa://25176 (98.77)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6722,7 +6722,7 @@
       </c>
       <c r="H58" s="8" t="inlineStr">
         <is>
-          <t>*maa://37964 (65.57)</t>
+          <t>*maa://37964 (65.85)</t>
         </is>
       </c>
       <c r="I58" s="19" t="n"/>
@@ -6740,7 +6740,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (98.35), maa://27746 (89.42)</t>
+          <t>maa://31270 (98.36), maa://27746 (89.47)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -6758,7 +6758,7 @@
       </c>
       <c r="H60" s="8" t="inlineStr">
         <is>
-          <t>maa://40438 (91.63)</t>
+          <t>maa://40438 (91.80)</t>
         </is>
       </c>
       <c r="I60" s="19" t="n"/>
@@ -6794,7 +6794,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (96.74), maa://56228 (98.10), maa://43903 (100.00)</t>
+          <t>maa://42981 (96.74), maa://56228 (98.12), maa://43903 (100.00)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6812,7 +6812,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (99.42), *maa://59693 (72.92), maa://59413 (97.44)</t>
+          <t>maa://59534 (99.43), *maa://59693 (73.47), maa://59413 (97.50)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7028,7 +7028,7 @@
       </c>
       <c r="H75" s="19" t="inlineStr">
         <is>
-          <t>maa://67748 (80.95)</t>
+          <t>maa://67748 (81.82)</t>
         </is>
       </c>
       <c r="I75" s="19" t="n"/>
@@ -7170,7 +7170,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.10.01 13:20:43</t>
+          <t>更新日期：2025.10.03 13:19:12</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8574,7 +8574,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (73.21), *maa://28758 (71.11), maa://29036 (96.67), *maa://42172 (71.43), maa://65357 (96.43), maa://30285 (100.00)</t>
+          <t>*maa://20849 (73.21), *maa://28758 (71.74), maa://29036 (96.67), *maa://42172 (71.43), maa://65357 (96.55), maa://30285 (100.00)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8844,7 +8844,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (89.84), maa://36866 (97.01), maa://62759 (100.00), maa://45572 (88.24), maa://27794 (100.00), maa://20960 (100.00), maa://20843 (100.00), **maa://24483 (50.00), *maa://20893 (73.68), maa://20862 (83.33)</t>
+          <t>maa://36644 (89.88), maa://36866 (97.01), maa://62759 (100.00), maa://45572 (88.24), maa://27794 (100.00), maa://20960 (100.00), maa://20843 (100.00), **maa://24483 (50.00), *maa://20893 (73.68), maa://20862 (83.33)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -9114,7 +9114,7 @@
       </c>
       <c r="D37" s="13" t="inlineStr">
         <is>
-          <t>maa://27376 (93.44), maa://42635 (94.34), *maa://20838 (55.00)</t>
+          <t>maa://27376 (93.44), maa://42635 (94.44), *maa://20838 (55.00)</t>
         </is>
       </c>
       <c r="E37" s="14" t="inlineStr">
@@ -9978,7 +9978,7 @@
       </c>
       <c r="D53" s="13" t="inlineStr">
         <is>
-          <t>maa://20953 (97.14), maa://31173 (94.74)</t>
+          <t>maa://20953 (97.14), maa://31173 (94.87)</t>
         </is>
       </c>
       <c r="E53" s="14" t="inlineStr">
@@ -10140,7 +10140,7 @@
       </c>
       <c r="D56" s="13" t="inlineStr">
         <is>
-          <t>maa://44235 (98.44), maa://45604 (100.00), maa://20961 (100.00), maa://20910 (100.00), maa://44220 (100.00)</t>
+          <t>maa://44235 (98.45), maa://45604 (100.00), maa://20961 (100.00), maa://20910 (100.00), maa://44220 (100.00)</t>
         </is>
       </c>
       <c r="E56" s="14" t="inlineStr">
@@ -10248,7 +10248,7 @@
       </c>
       <c r="D58" s="13" t="inlineStr">
         <is>
-          <t>maa://28900 (97.00), maa://30126 (100.00)</t>
+          <t>maa://28900 (97.03), maa://30126 (100.00)</t>
         </is>
       </c>
       <c r="E58" s="14" t="inlineStr">
@@ -10788,7 +10788,7 @@
       </c>
       <c r="D68" s="13" t="inlineStr">
         <is>
-          <t>maa://20976 (97.84), maa://20815 (100.00)</t>
+          <t>maa://20976 (97.85), maa://20815 (100.00)</t>
         </is>
       </c>
       <c r="E68" s="14" t="inlineStr">
@@ -11004,7 +11004,7 @@
       </c>
       <c r="D72" s="13" t="inlineStr">
         <is>
-          <t>maa://36643 (98.45), maa://36864 (98.11), maa://39140 (100.00), maa://66335 (100.00)</t>
+          <t>maa://36643 (98.46), maa://36864 (98.11), maa://39140 (100.00), maa://66335 (100.00)</t>
         </is>
       </c>
       <c r="E72" s="14" t="inlineStr">
@@ -11976,7 +11976,7 @@
       </c>
       <c r="D90" s="13" t="inlineStr">
         <is>
-          <t>*maa://28190 (62.86), maa://20880 (93.10)</t>
+          <t>*maa://28190 (63.89), maa://20880 (93.10)</t>
         </is>
       </c>
       <c r="E90" s="14" t="inlineStr">
@@ -12354,7 +12354,7 @@
       </c>
       <c r="D97" s="13" t="inlineStr">
         <is>
-          <t>maa://20991 (100.00), maa://51015 (88.64)</t>
+          <t>maa://20991 (100.00), maa://51015 (88.89)</t>
         </is>
       </c>
       <c r="E97" s="14" t="inlineStr">
@@ -12948,7 +12948,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.73), maa://25018 (96.96), maa://25776 (92.21), maa://28361 (95.45), maa://25772 (94.12), maa://56588 (93.33), maa://45194 (85.71), maa://32653 (81.25), maa://25161 (83.33), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
+          <t>maa://51881 (98.73), maa://25018 (96.96), maa://25776 (92.31), maa://28361 (95.56), maa://25772 (94.12), maa://56588 (93.33), maa://45194 (86.36), maa://32653 (81.25), maa://25161 (84.21), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13272,7 +13272,7 @@
       </c>
       <c r="D114" s="13" t="inlineStr">
         <is>
-          <t>maa://29037 (97.44)</t>
+          <t>maa://29037 (97.47)</t>
         </is>
       </c>
       <c r="E114" s="14" t="inlineStr">
@@ -14838,7 +14838,7 @@
       </c>
       <c r="D143" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (97.81), *maa://23736 (52.44), maa://31185 (91.67), maa://30306 (100.00)</t>
+          <t>maa://28484 (97.84), *maa://23736 (52.44), maa://31185 (91.67), maa://30306 (100.00)</t>
         </is>
       </c>
       <c r="E143" s="14" t="inlineStr">
@@ -15216,7 +15216,7 @@
       </c>
       <c r="D150" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.86), maa://36641 (98.24), maa://36865 (95.45), maa://44635 (88.18), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (100.00), maa://42918 (100.00), maa://44119 (97.44), maa://64408 (92.86), maa://37300 (100.00), maa://42917 (100.00)</t>
+          <t>maa://40957 (94.86), maa://36641 (98.24), maa://36865 (95.48), maa://44635 (88.18), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (100.00), maa://42918 (100.00), maa://44119 (97.44), maa://64408 (92.86), maa://37300 (100.00), maa://42917 (100.00)</t>
         </is>
       </c>
       <c r="E150" s="14" t="inlineStr">
@@ -16188,7 +16188,7 @@
       </c>
       <c r="D168" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (92.26), maa://29627 (92.95), maa://29659 (85.37), maa://49074 (94.20), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
+          <t>maa://29633 (92.31), maa://29627 (92.95), maa://29659 (85.37), maa://49074 (94.20), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
         </is>
       </c>
       <c r="E168" s="14" t="inlineStr">
@@ -16620,7 +16620,7 @@
       </c>
       <c r="D176" s="13" t="inlineStr">
         <is>
-          <t>maa://32418 (99.70), maa://63320 (97.50), maa://51440 (100.00)</t>
+          <t>maa://32418 (99.70), maa://63320 (97.73), maa://51440 (100.00)</t>
         </is>
       </c>
       <c r="E176" s="14" t="inlineStr">
@@ -17700,7 +17700,7 @@
       </c>
       <c r="D196" s="13" t="inlineStr">
         <is>
-          <t>*maa://28190 (62.86), maa://20994 (100.00)</t>
+          <t>*maa://28190 (63.89), maa://20994 (100.00)</t>
         </is>
       </c>
       <c r="E196" s="14" t="inlineStr">
@@ -17808,7 +17808,7 @@
       </c>
       <c r="D198" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.48), maa://35854 (84.75), maa://50388 (98.25), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (95.00)</t>
+          <t>maa://44224 (90.52), maa://35854 (84.75), maa://50388 (98.25), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (95.35)</t>
         </is>
       </c>
       <c r="E198" s="14" t="inlineStr">
@@ -17862,7 +17862,7 @@
       </c>
       <c r="D199" s="13" t="inlineStr">
         <is>
-          <t>maa://39156 (94.19), *maa://39550 (55.00), *maa://53417 (77.78), *maa://63806 (77.78)</t>
+          <t>maa://39156 (94.25), *maa://39550 (55.00), *maa://53417 (77.78), *maa://63806 (77.78)</t>
         </is>
       </c>
       <c r="E199" s="14" t="inlineStr">
@@ -17916,7 +17916,7 @@
       </c>
       <c r="D200" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (86.32), *maa://28190 (62.86), maa://22894 (91.67), *maa://20906 (72.22), **maa://20907 (34.38)</t>
+          <t>maa://27823 (86.32), *maa://28190 (63.89), maa://22894 (91.67), *maa://20906 (72.22), **maa://20907 (34.38)</t>
         </is>
       </c>
       <c r="E200" s="14" t="inlineStr">
@@ -17970,7 +17970,7 @@
       </c>
       <c r="D201" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (86.32), *maa://28190 (62.86), maa://22894 (91.67), *maa://20906 (72.22), **maa://20907 (34.38)</t>
+          <t>maa://27823 (86.32), *maa://28190 (63.89), maa://22894 (91.67), *maa://20906 (72.22), **maa://20907 (34.38)</t>
         </is>
       </c>
       <c r="E201" s="14" t="inlineStr">
@@ -18672,7 +18672,7 @@
       </c>
       <c r="D214" s="13" t="inlineStr">
         <is>
-          <t>maa://39238 (99.11)</t>
+          <t>maa://39238 (99.12)</t>
         </is>
       </c>
       <c r="E214" s="14" t="inlineStr">
@@ -18726,7 +18726,7 @@
       </c>
       <c r="D215" s="13" t="inlineStr">
         <is>
-          <t>maa://64044 (96.08)</t>
+          <t>maa://64044 (96.23)</t>
         </is>
       </c>
       <c r="E215" s="14" t="inlineStr">
@@ -20076,7 +20076,7 @@
       </c>
       <c r="D240" s="13" t="inlineStr">
         <is>
-          <t>maa://20922 (94.37), *maa://32623 (77.27), maa://34242 (85.71)</t>
+          <t>maa://20922 (94.44), *maa://32623 (77.27), maa://34242 (85.71)</t>
         </is>
       </c>
       <c r="E240" s="14" t="inlineStr">
@@ -21750,7 +21750,7 @@
       </c>
       <c r="D271" s="13" t="inlineStr">
         <is>
-          <t>maa://48265 (84.62)</t>
+          <t>maa://48265 (81.48)</t>
         </is>
       </c>
       <c r="E271" s="14" t="inlineStr">
@@ -22020,7 +22020,7 @@
       </c>
       <c r="D276" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.73), maa://51630 (96.26), maa://56588 (93.33), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (41.67), *maa://66758 (75.00)</t>
+          <t>maa://51881 (98.73), maa://51630 (96.26), maa://56588 (93.33), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (41.67), maa://66758 (83.33)</t>
         </is>
       </c>
       <c r="E276" s="14" t="inlineStr">
@@ -22776,7 +22776,7 @@
       </c>
       <c r="D290" s="13" t="inlineStr">
         <is>
-          <t>maa://20899 (90.06), maa://46332 (92.86), ***maa://44744 (25.00)</t>
+          <t>maa://20899 (90.11), maa://46332 (92.86), ***maa://44744 (25.00)</t>
         </is>
       </c>
       <c r="E290" s="14" t="inlineStr">
@@ -23689,12 +23689,12 @@
       </c>
       <c r="C307" s="12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D307" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (98.49), maa://49642 (97.62), maa://49660 (93.62), maa://50517 (85.71)</t>
+          <t>maa://50280 (98.49), maa://49642 (97.62), maa://49660 (93.62), maa://50517 (85.71), maa://70004 (100.00)</t>
         </is>
       </c>
       <c r="E307" s="14" t="inlineStr">
@@ -24342,7 +24342,7 @@
       </c>
       <c r="D319" s="13" t="inlineStr">
         <is>
-          <t>maa://25367 (99.37)</t>
+          <t>maa://25367 (99.38)</t>
         </is>
       </c>
       <c r="E319" s="14" t="inlineStr">
@@ -24720,7 +24720,7 @@
       </c>
       <c r="D326" s="13" t="inlineStr">
         <is>
-          <t>maa://39692 (99.54), maa://39810 (90.32)</t>
+          <t>maa://39692 (99.55), maa://39810 (90.32)</t>
         </is>
       </c>
       <c r="E326" s="14" t="inlineStr">
@@ -25638,7 +25638,7 @@
       </c>
       <c r="D343" s="22" t="inlineStr">
         <is>
-          <t>maa://30671 (81.50), maa://30669 (99.31), maa://37275 (81.40), *maa://32410 (61.54), maa://41605 (100.00)</t>
+          <t>maa://30671 (81.59), maa://30669 (99.31), maa://37275 (81.40), *maa://32410 (61.54), maa://41605 (100.00)</t>
         </is>
       </c>
       <c r="E343" s="22" t="inlineStr">
@@ -25746,7 +25746,7 @@
       </c>
       <c r="D345" s="22" t="inlineStr">
         <is>
-          <t>maa://38295 (95.33), maa://49332 (90.91)</t>
+          <t>maa://38295 (95.37), maa://49332 (90.91)</t>
         </is>
       </c>
       <c r="E345" s="22" t="inlineStr">
@@ -26016,7 +26016,7 @@
       </c>
       <c r="D350" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (97.59), maa://32415 (84.53), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
+          <t>maa://32647 (97.59), maa://32415 (84.57), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E350" s="22" t="inlineStr">
@@ -26556,7 +26556,7 @@
       </c>
       <c r="D360" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.60), maa://49695 (100.00), maa://49758 (98.70), *maa://59402 (56.67), *maa://52357 (75.00), *maa://63091 (75.00)</t>
+          <t>maa://49696 (99.60), maa://49695 (100.00), maa://49758 (98.72), *maa://59402 (56.67), *maa://52357 (75.00), *maa://63091 (75.00)</t>
         </is>
       </c>
       <c r="E360" s="22" t="inlineStr">
@@ -26772,7 +26772,7 @@
       </c>
       <c r="D364" s="22" t="inlineStr">
         <is>
-          <t>maa://36646 (98.91), maa://36845 (95.89), **maa://39217 (38.89), maa://51007 (98.28)</t>
+          <t>maa://36646 (98.91), maa://36845 (95.89), **maa://39217 (38.89), maa://51007 (98.31)</t>
         </is>
       </c>
       <c r="E364" s="22" t="inlineStr">
@@ -26880,7 +26880,7 @@
       </c>
       <c r="D366" s="22" t="inlineStr">
         <is>
-          <t>maa://42635 (94.34), maa://50629 (83.33), maa://48859 (100.00)</t>
+          <t>maa://42635 (94.44), maa://50629 (83.33), maa://48859 (100.00)</t>
         </is>
       </c>
       <c r="E366" s="22" t="inlineStr">
@@ -27042,7 +27042,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (94.86), maa://48026 (94.70), maa://44635 (88.18), maa://41035 (93.51), *maa://60251 (76.47), maa://44660 (92.68), maa://41128 (84.21)</t>
+          <t>maa://40957 (94.86), maa://48026 (94.70), maa://44635 (88.18), maa://41035 (93.59), *maa://60251 (76.47), maa://44660 (92.68), maa://41128 (84.21)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -27960,7 +27960,7 @@
       </c>
       <c r="D386" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (81.07), maa://44745 (98.05), **maa://49516 (37.93), *maa://45952 (57.14), ***maa://46851 (12.50), *maa://44896 (77.78)</t>
+          <t>maa://42970 (81.07), maa://44745 (98.06), **maa://49516 (37.93), *maa://45952 (57.14), ***maa://46851 (12.50), *maa://44896 (77.78)</t>
         </is>
       </c>
       <c r="E386" s="22" t="inlineStr">
@@ -28365,7 +28365,7 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>maa://47023 (86.27)</t>
+          <t>maa://47023 (87.04)</t>
         </is>
       </c>
       <c r="E394" t="inlineStr">
@@ -28419,7 +28419,7 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>maa://59533 (97.87), maa://59577 (100.00)</t>
+          <t>maa://59533 (97.92), maa://59577 (100.00)</t>
         </is>
       </c>
       <c r="E396" t="inlineStr">
@@ -28554,7 +28554,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>maa://51872 (96.66), maa://51876 (99.07), maa://63228 (88.24), maa://51873 (100.00), maa://62047 (92.00)</t>
+          <t>maa://51872 (96.67), maa://51876 (99.07), maa://63228 (88.24), maa://51873 (100.00), maa://62047 (92.31)</t>
         </is>
       </c>
       <c r="E401" t="inlineStr">
@@ -28608,7 +28608,7 @@
       </c>
       <c r="D403" t="inlineStr">
         <is>
-          <t>maa://60449 (99.00), maa://59493 (96.88)</t>
+          <t>maa://60449 (99.01), maa://59493 (96.88)</t>
         </is>
       </c>
       <c r="E403" t="inlineStr">
@@ -28662,7 +28662,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>maa://62756 (96.00)</t>
+          <t>maa://62756 (96.03)</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">
@@ -28716,7 +28716,7 @@
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>maa://64040 (99.01), maa://52505 (98.18), maa://66377 (93.75), ***maa://66376 (20.00)</t>
+          <t>maa://64040 (99.02), maa://52505 (98.21), maa://66377 (93.75), ***maa://66376 (20.00)</t>
         </is>
       </c>
       <c r="E407" t="inlineStr">
@@ -28743,7 +28743,7 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>maa://67090 (89.47)</t>
+          <t>maa://67090 (90.00)</t>
         </is>
       </c>
       <c r="E408" t="inlineStr">
@@ -28770,7 +28770,7 @@
       </c>
       <c r="D409" t="inlineStr">
         <is>
-          <t>maa://67388 (93.02)</t>
+          <t>maa://67388 (93.75)</t>
         </is>
       </c>
       <c r="E409" t="inlineStr">
@@ -28797,7 +28797,7 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>maa://67089 (97.67), maa://67271 (93.75)</t>
+          <t>maa://67089 (97.83), maa://67271 (94.44)</t>
         </is>
       </c>
       <c r="E410" t="inlineStr">
@@ -28824,7 +28824,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>maa://67088 (91.94)</t>
+          <t>maa://67088 (92.31)</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
@@ -28851,7 +28851,7 @@
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>maa://67087 (94.12), maa://67268 (96.63), maa://67269 (88.89), maa://67648 (100.00)</t>
+          <t>maa://67087 (94.34), maa://67268 (96.70), maa://67269 (88.89), maa://67648 (100.00)</t>
         </is>
       </c>
       <c r="E412" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#244)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -712,7 +712,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (98.33), maa://24702 (95.08), maa://36681 (85.39)</t>
+          <t>maa://25390 (98.36), maa://24702 (95.11), maa://36681 (85.39)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://58660 (98.88), maa://39402 (94.94), *maa://34787 (75.00)</t>
+          <t>maa://58660 (98.90), maa://39402 (95.00), *maa://34787 (75.00)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -776,7 +776,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (97.32), maa://66635 (99.57)</t>
+          <t>maa://22742 (97.35), maa://66635 (99.58)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://36684 (98.25), maa://21246 (91.37)</t>
+          <t>maa://36684 (98.27), maa://21246 (91.37)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://59087 (97.27), maa://25251 (91.61)</t>
+          <t>maa://59087 (97.32), maa://25251 (91.61)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -858,7 +858,7 @@
       </c>
       <c r="H3" s="8" t="inlineStr">
         <is>
-          <t>maa://21247 (99.38)</t>
+          <t>maa://21247 (99.39)</t>
         </is>
       </c>
       <c r="I3" s="19" t="n"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>maa://22880 (91.09), maa://20276 (94.05), maa://22749 (84.62)</t>
+          <t>maa://22880 (91.18), maa://20276 (94.06), maa://22749 (84.62)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -890,7 +890,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (98.41), maa://26254 (98.15), *maa://22738 (80.00)</t>
+          <t>maa://21249 (98.44), maa://26254 (98.15), *maa://22738 (80.00)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://60545 (98.75), maa://45854 (87.44), maa://24617 (91.18)</t>
+          <t>maa://60545 (98.77), maa://45854 (87.56), maa://24617 (91.18)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (92.26), maa://27484 (99.20), maa://27480 (86.21)</t>
+          <t>maa://27396 (92.31), maa://27484 (99.20), maa://27480 (86.21)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://52241 (99.41), maa://24390 (96.77)</t>
+          <t>maa://52241 (99.42), maa://24390 (96.83)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -954,7 +954,7 @@
       </c>
       <c r="AF3" s="8" t="inlineStr">
         <is>
-          <t>maa://21289 (92.04)</t>
+          <t>maa://21289 (92.11)</t>
         </is>
       </c>
       <c r="AG3" s="16" t="n"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (98.07), maa://22499 (90.00), maa://22746 (100.00)</t>
+          <t>maa://24632 (98.09), maa://22499 (90.00), maa://22746 (100.00)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (99.11), maa://50121 (96.15)</t>
+          <t>maa://49983 (99.12), maa://50121 (96.18)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://27295 (97.72), maa://32509 (96.43), maa://31008 (95.21), maa://22754 (88.16)</t>
+          <t>maa://27295 (97.75), maa://32509 (96.46), maa://31008 (95.21), maa://22754 (88.16)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="X4" s="8" t="inlineStr">
         <is>
-          <t>maa://43217 (98.86)</t>
+          <t>maa://43217 (98.88)</t>
         </is>
       </c>
       <c r="Y4" s="19" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (91.33), maa://54105 (98.50), *maa://22744 (80.00)</t>
+          <t>maa://21245 (91.34), maa://54105 (98.40), *maa://22744 (80.00)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="L5" s="8" t="inlineStr">
         <is>
-          <t>maa://22757 (90.91)</t>
+          <t>maa://22757 (91.15)</t>
         </is>
       </c>
       <c r="M5" s="19" t="n"/>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="P5" s="8" t="inlineStr">
         <is>
-          <t>maa://21919 (98.65), maa://21281 (81.25)</t>
+          <t>maa://21919 (98.68), maa://21281 (81.25)</t>
         </is>
       </c>
       <c r="Q5" s="19" t="n"/>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="X5" s="8" t="inlineStr">
         <is>
-          <t>maa://21290 (98.51)</t>
+          <t>maa://21290 (98.52)</t>
         </is>
       </c>
       <c r="Y5" s="19" t="n"/>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="D6" s="8" t="inlineStr">
         <is>
-          <t>maa://42407 (97.45)</t>
+          <t>maa://42407 (97.47)</t>
         </is>
       </c>
       <c r="E6" s="19" t="n"/>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="H6" s="8" t="inlineStr">
         <is>
-          <t>maa://24370 (97.54)</t>
+          <t>maa://24370 (97.62)</t>
         </is>
       </c>
       <c r="I6" s="19" t="n"/>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="L6" s="8" t="inlineStr">
         <is>
-          <t>maa://24839 (99.43)</t>
+          <t>maa://24839 (99.44)</t>
         </is>
       </c>
       <c r="M6" s="19" t="n"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (98.86), maa://30381 (95.00)</t>
+          <t>maa://31836 (98.87), maa://30381 (95.00)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="X6" s="8" t="inlineStr">
         <is>
-          <t>maa://52754 (96.49)</t>
+          <t>maa://52754 (96.55)</t>
         </is>
       </c>
       <c r="Y6" s="19" t="n"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="AB6" s="8" t="inlineStr">
         <is>
-          <t>maa://22739 (89.36)</t>
+          <t>maa://22739 (89.58)</t>
         </is>
       </c>
       <c r="AC6" s="19" t="n"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="AF6" s="8" t="inlineStr">
         <is>
-          <t>maa://33152 (80.82)</t>
+          <t>maa://33152 (80.95)</t>
         </is>
       </c>
       <c r="AG6" s="16" t="n"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>maa://21955 (98.20)</t>
+          <t>maa://21955 (98.22)</t>
         </is>
       </c>
       <c r="E7" s="19" t="n"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>*maa://22763 (75.00), maa://64972 (95.45)</t>
+          <t>*maa://22763 (75.00), maa://64972 (95.83)</t>
         </is>
       </c>
       <c r="I7" s="19" t="n"/>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (98.62), maa://24957 (94.55)</t>
+          <t>maa://28624 (98.65), maa://24957 (94.55)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="P7" s="8" t="inlineStr">
         <is>
-          <t>maa://22750 (96.95)</t>
+          <t>maa://22750 (97.01)</t>
         </is>
       </c>
       <c r="Q7" s="19" t="n"/>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="T7" s="8" t="inlineStr">
         <is>
-          <t>maa://21291 (94.01)</t>
+          <t>maa://21291 (94.08)</t>
         </is>
       </c>
       <c r="U7" s="19" t="n"/>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (97.23), maa://22758 (82.35)</t>
+          <t>maa://22399 (97.25), maa://22758 (82.35)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="AF7" s="8" t="inlineStr">
         <is>
-          <t>maa://45272 (99.45)</t>
+          <t>maa://45272 (99.47)</t>
         </is>
       </c>
       <c r="AG7" s="16" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.10.03 13:19:12</t>
+          <t>更新日期：2025.10.05 13:18:08</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (90.06)</t>
+          <t>maa://21476 (90.30)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
-          <t>*maa://24371 (79.59)</t>
+          <t>*maa://24371 (79.80)</t>
         </is>
       </c>
       <c r="I8" s="19" t="n"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (91.29), maa://23252 (91.67), maa://37496 (98.33)</t>
+          <t>maa://32931 (91.33), maa://23252 (91.67), maa://37496 (98.33)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (96.07), maa://67587 (98.62)</t>
+          <t>maa://21411 (96.09), maa://67587 (98.65)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="AB8" s="8" t="inlineStr">
         <is>
-          <t>maa://25389 (94.64)</t>
+          <t>maa://25389 (94.69)</t>
         </is>
       </c>
       <c r="AC8" s="19" t="n"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>maa://24479 (84.38), *maa://21990 (51.72)</t>
+          <t>maa://24479 (84.54), *maa://21990 (51.72)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>maa://22765 (95.73), *maa://21915 (78.57)</t>
+          <t>maa://22765 (95.74), *maa://21915 (78.57)</t>
         </is>
       </c>
       <c r="E9" s="19" t="n"/>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (96.33), maa://39552 (88.00)</t>
+          <t>maa://22762 (96.35), maa://39552 (88.00)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="T9" s="8" t="inlineStr">
         <is>
-          <t>maa://26222 (99.45)</t>
+          <t>maa://26222 (99.46)</t>
         </is>
       </c>
       <c r="U9" s="19" t="n"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (95.23), maa://40166 (94.81)</t>
+          <t>maa://28711 (95.27), maa://40166 (94.89)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (91.32), maa://66916 (98.12)</t>
+          <t>maa://26206 (91.39), maa://66916 (98.16)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>maa://54000 (92.31)</t>
+          <t>maa://54000 (92.39)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="H10" s="8" t="inlineStr">
         <is>
-          <t>maa://32651 (95.24)</t>
+          <t>maa://32651 (95.35)</t>
         </is>
       </c>
       <c r="I10" s="19" t="n"/>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (91.97), *maa://36669 (74.36)</t>
+          <t>maa://28977 (92.09), *maa://36669 (74.36)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (99.26), maa://22755 (91.62), maa://63521 (94.40)</t>
+          <t>maa://27395 (99.27), maa://22755 (91.67), maa://63521 (94.05)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://45828 (99.26), maa://22301 (97.64), maa://22726 (100.00)</t>
+          <t>maa://45828 (99.26), maa://22301 (97.65), maa://22726 (100.00)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>*maa://25021 (57.32), *maa://22733 (64.62), **maa://22761 (33.33)</t>
+          <t>*maa://25021 (57.32), *maa://22733 (65.15), **maa://22761 (33.33)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="L11" s="8" t="inlineStr">
         <is>
-          <t>maa://21287 (93.28)</t>
+          <t>maa://21287 (93.33)</t>
         </is>
       </c>
       <c r="M11" s="19" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (93.33), maa://22501 (99.54), maa://64808 (100.00), maa://45521 (95.24)</t>
+          <t>maa://22747 (93.18), maa://22501 (99.55), maa://64808 (100.00), maa://45521 (95.24)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="X11" s="8" t="inlineStr">
         <is>
-          <t>maa://36713 (99.27)</t>
+          <t>maa://36713 (99.28)</t>
         </is>
       </c>
       <c r="Y11" s="19" t="n"/>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="AB11" s="8" t="inlineStr">
         <is>
-          <t>maa://29912 (99.71), maa://22516 (86.52)</t>
+          <t>maa://29912 (99.72), maa://22516 (86.52)</t>
         </is>
       </c>
       <c r="AC11" s="19" t="n"/>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="AF11" s="8" t="inlineStr">
         <is>
-          <t>maa://31203 (98.67)</t>
+          <t>maa://31203 (98.68)</t>
         </is>
       </c>
       <c r="AG11" s="16" t="n"/>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>maa://36678 (97.14), maa://30766 (91.18)</t>
+          <t>maa://36678 (97.18), maa://30766 (91.18)</t>
         </is>
       </c>
       <c r="E12" s="19" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (93.56), maa://54294 (96.69)</t>
+          <t>maa://21867 (93.58), maa://54294 (96.74)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (98.01), maa://64046 (98.60)</t>
+          <t>maa://63896 (98.03), maa://64046 (98.61)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://37962 (98.83), maa://21485 (81.70), maa://22753 (92.83)</t>
+          <t>maa://37962 (98.85), maa://21485 (81.86), maa://22753 (92.83)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://36677 (99.06), maa://23669 (94.83), maa://39872 (98.32)</t>
+          <t>maa://36677 (99.08), maa://23669 (94.83), maa://39872 (98.33)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>maa://28932 (94.67)</t>
+          <t>maa://28932 (94.71)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (96.69), maa://36673 (94.16), maa://25001 (88.76)</t>
+          <t>maa://24999 (96.74), maa://36673 (94.16), maa://25001 (88.76)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.33), maa://66545 (99.04)</t>
+          <t>*maa://21248 (73.40), maa://66545 (98.83)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (97.76), maa://22583 (88.12)</t>
+          <t>maa://22676 (97.79), maa://22583 (88.48)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="X13" s="8" t="inlineStr">
         <is>
-          <t>maa://34957 (94.57)</t>
+          <t>maa://34957 (94.58)</t>
         </is>
       </c>
       <c r="Y13" s="19" t="n"/>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (93.97)</t>
+          <t>maa://39883 (94.07)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2282,7 +2282,7 @@
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>maa://30764 (94.44)</t>
+          <t>maa://30764 (94.56)</t>
         </is>
       </c>
       <c r="E14" s="19" t="n"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (99.05), maa://36682 (98.31), maa://26245 (97.06), maa://21288 (96.40)</t>
+          <t>maa://39841 (99.06), maa://36682 (98.32), maa://26245 (97.07), maa://21288 (96.40)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (85.42), maa://45058 (98.20), maa://22734 (84.96), *maa://36048 (74.86), maa://69928 (100.00)</t>
+          <t>maa://22743 (85.50), maa://45058 (98.23), maa://22734 (84.96), *maa://36048 (75.00), maa://69928 (100.00)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (97.05), maa://21478 (90.48)</t>
+          <t>maa://24304 (97.16), maa://21478 (90.48)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="L15" s="8" t="inlineStr">
         <is>
-          <t>*maa://21334 (70.18)</t>
+          <t>*maa://21334 (70.69)</t>
         </is>
       </c>
       <c r="M15" s="19" t="n"/>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="P15" s="8" t="inlineStr">
         <is>
-          <t>maa://24762 (97.69), *maa://22727 (70.00)</t>
+          <t>maa://24762 (97.70), *maa://22727 (70.00)</t>
         </is>
       </c>
       <c r="Q15" s="19" t="n"/>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="T15" s="8" t="inlineStr">
         <is>
-          <t>maa://23892 (97.63)</t>
+          <t>maa://23892 (97.69)</t>
         </is>
       </c>
       <c r="U15" s="19" t="n"/>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://36666 (96.34), maa://21364 (83.80), *maa://22766 (70.71), *maa://68306 (78.95)</t>
+          <t>maa://36666 (96.37), maa://21364 (83.80), *maa://22766 (70.71), maa://68306 (80.49)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2590,7 +2590,7 @@
       </c>
       <c r="P16" s="8" t="inlineStr">
         <is>
-          <t>maa://28504 (96.30)</t>
+          <t>maa://28504 (96.40)</t>
         </is>
       </c>
       <c r="Q16" s="19" t="n"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://36674 (98.06), maa://22729 (96.20), *maa://28648 (77.89)</t>
+          <t>maa://36674 (97.92), maa://22729 (96.22), *maa://28648 (77.89)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2622,7 +2622,7 @@
       </c>
       <c r="X16" s="8" t="inlineStr">
         <is>
-          <t>maa://28501 (99.34), maa://28051 (97.14)</t>
+          <t>maa://28501 (99.35), maa://28051 (97.14)</t>
         </is>
       </c>
       <c r="Y16" s="19" t="n"/>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>maa://23911 (90.64), maa://27755 (93.75), maa://67613 (99.46)</t>
+          <t>maa://23911 (90.64), maa://27755 (93.75), maa://67613 (99.47)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://39599 (98.25), maa://22430 (90.25)</t>
+          <t>maa://39599 (98.27), maa://22430 (90.25)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="L17" s="8" t="inlineStr">
         <is>
-          <t>maa://21679 (88.24)</t>
+          <t>maa://21679 (88.46)</t>
         </is>
       </c>
       <c r="M17" s="19" t="n"/>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (82.64), maa://56238 (98.52)</t>
+          <t>maa://23890 (82.93), maa://56238 (98.54)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="T17" s="8" t="inlineStr">
         <is>
-          <t>*maa://42324 (70.45)</t>
+          <t>*maa://42324 (70.79)</t>
         </is>
       </c>
       <c r="U17" s="19" t="n"/>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>maa://24570 (98.37)</t>
+          <t>maa://24570 (98.26)</t>
         </is>
       </c>
       <c r="E18" s="19" t="n"/>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="H18" s="8" t="inlineStr">
         <is>
-          <t>maa://24421 (95.15)</t>
+          <t>maa://24421 (95.20)</t>
         </is>
       </c>
       <c r="I18" s="19" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://52226 (99.63), maa://22466 (92.83)</t>
+          <t>maa://52226 (99.64), maa://22466 (92.83)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (98.72), maa://22741 (92.31)</t>
+          <t>maa://21917 (98.73), maa://22741 (92.31)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="AB18" s="8" t="inlineStr">
         <is>
-          <t>maa://24393 (99.01)</t>
+          <t>maa://24393 (99.02)</t>
         </is>
       </c>
       <c r="AC18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://47854 (93.06)</t>
+          <t>maa://47854 (93.15)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="T19" s="8" t="inlineStr">
         <is>
-          <t>maa://24386 (99.68)</t>
+          <t>maa://24386 (99.52)</t>
         </is>
       </c>
       <c r="U19" s="19" t="n"/>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="X19" s="8" t="inlineStr">
         <is>
-          <t>maa://31386 (97.56), maa://58490 (85.00)</t>
+          <t>maa://31386 (97.62), maa://58490 (85.71)</t>
         </is>
       </c>
       <c r="Y19" s="19" t="n"/>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (86.18), *maa://36668 (69.83)</t>
+          <t>maa://30709 (86.25), *maa://36668 (69.83)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3044,7 +3044,7 @@
       </c>
       <c r="AF19" s="8" t="inlineStr">
         <is>
-          <t>*maa://21663 (65.91), maa://52239 (86.11)</t>
+          <t>*maa://21663 (65.91), maa://52239 (86.84)</t>
         </is>
       </c>
       <c r="AG19" s="16" t="n"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://25198 (97.68), maa://36680 (99.09), maa://21432 (91.53)</t>
+          <t>maa://25198 (97.70), maa://36680 (99.10), maa://21432 (91.56)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3078,7 +3078,7 @@
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>maa://22864 (96.05)</t>
+          <t>maa://22864 (96.09)</t>
         </is>
       </c>
       <c r="I20" s="19" t="n"/>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (95.42)</t>
+          <t>maa://41331 (95.44)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="P20" s="8" t="inlineStr">
         <is>
-          <t>maa://37442 (98.55)</t>
+          <t>maa://37442 (98.57)</t>
         </is>
       </c>
       <c r="Q20" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (96.54), maa://56241 (98.27), maa://49976 (88.57)</t>
+          <t>maa://50085 (96.59), maa://56241 (98.28), maa://49976 (88.57)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>maa://21261 (99.03)</t>
+          <t>maa://21261 (99.06)</t>
         </is>
       </c>
       <c r="E21" s="19" t="n"/>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="H21" s="8" t="inlineStr">
         <is>
-          <t>maa://24372 (98.88)</t>
+          <t>maa://24372 (98.91)</t>
         </is>
       </c>
       <c r="I21" s="19" t="n"/>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="L21" s="8" t="inlineStr">
         <is>
-          <t>maa://31731 (96.52)</t>
+          <t>maa://31731 (96.61)</t>
         </is>
       </c>
       <c r="M21" s="19" t="n"/>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (98.09), maa://20110 (87.01)</t>
+          <t>maa://34946 (98.12), maa://20110 (87.01)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="AB21" s="8" t="inlineStr">
         <is>
-          <t>maa://21443 (87.07), maa://52223 (83.14)</t>
+          <t>maa://21443 (87.17), maa://52223 (83.45)</t>
         </is>
       </c>
       <c r="AC21" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22432 (94.24), maa://22524 (83.16), maa://64221 (97.96)</t>
+          <t>maa://22432 (94.34), maa://22524 (83.22), maa://64221 (97.99)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>maa://25236 (99.23)</t>
+          <t>maa://25236 (99.24)</t>
         </is>
       </c>
       <c r="I22" s="19" t="n"/>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>maa://27127 (83.47), *maa://22751 (71.26), maa://66865 (99.42)</t>
+          <t>maa://27127 (83.54), *maa://22751 (71.26), maa://66865 (99.44)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://37649 (94.80), maa://21282 (98.96)</t>
+          <t>maa://37649 (94.90), maa://21282 (98.97)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="AB22" s="8" t="inlineStr">
         <is>
-          <t>maa://23656 (99.51)</t>
+          <t>maa://23656 (99.52)</t>
         </is>
       </c>
       <c r="AC22" s="19" t="n"/>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="AF22" s="8" t="inlineStr">
         <is>
-          <t>maa://29658 (97.14)</t>
+          <t>maa://29658 (97.17)</t>
         </is>
       </c>
       <c r="AG22" s="16" t="n"/>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (98.59), maa://39875 (95.80)</t>
+          <t>maa://39756 (98.61), maa://39875 (95.80)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (96.76), maa://29748 (81.77), *maa://37566 (78.46)</t>
+          <t>maa://30587 (96.79), maa://29748 (81.77), *maa://37566 (78.46)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="T23" s="8" t="inlineStr">
         <is>
-          <t>maa://31212 (94.87), maa://24387 (84.44), maa://67084 (87.50)</t>
+          <t>maa://31212 (94.92), maa://24387 (84.44), maa://67084 (87.50)</t>
         </is>
       </c>
       <c r="U23" s="19" t="n"/>
@@ -3532,7 +3532,7 @@
       </c>
       <c r="X23" s="8" t="inlineStr">
         <is>
-          <t>*maa://28503 (60.51)</t>
+          <t>*maa://28503 (61.01)</t>
         </is>
       </c>
       <c r="Y23" s="19" t="n"/>
@@ -3548,7 +3548,7 @@
       </c>
       <c r="AB23" s="8" t="inlineStr">
         <is>
-          <t>maa://29652 (96.59)</t>
+          <t>maa://29652 (96.63)</t>
         </is>
       </c>
       <c r="AC23" s="19" t="n"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (85.50), maa://46650 (90.75)</t>
+          <t>maa://24368 (85.55), maa://46650 (90.82)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (96.42), maa://23504 (94.06), *maa://25141 (79.74), maa://52227 (97.45), *maa://36663 (79.44)</t>
+          <t>maa://29988 (96.39), maa://23504 (94.06), *maa://25141 (79.74), maa://52227 (97.12), *maa://36663 (79.63)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://64165 (99.19), maa://22523 (80.18), maa://29910 (94.20), maa://45831 (93.55)</t>
+          <t>maa://64165 (99.20), maa://22523 (80.18), maa://29910 (94.20), maa://45831 (93.55)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (96.62), maa://63016 (99.14)</t>
+          <t>maa://29753 (96.63), maa://63016 (99.15)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>*maa://29063 (76.22), *maa://25311 (70.83), maa://45047 (88.46)</t>
+          <t>*maa://29063 (76.42), *maa://25311 (70.83), maa://45047 (88.46)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3744,7 +3744,7 @@
       </c>
       <c r="L25" s="8" t="inlineStr">
         <is>
-          <t>maa://24378 (93.83), maa://68415 (100.00)</t>
+          <t>maa://24378 (93.90), maa://68415 (100.00)</t>
         </is>
       </c>
       <c r="M25" s="19" t="n"/>
@@ -3760,7 +3760,7 @@
       </c>
       <c r="P25" s="8" t="inlineStr">
         <is>
-          <t>maa://24382 (96.30)</t>
+          <t>maa://24382 (96.49)</t>
         </is>
       </c>
       <c r="Q25" s="19" t="n"/>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="T25" s="8" t="inlineStr">
         <is>
-          <t>maa://20109 (96.37), maa://22545 (100.00)</t>
+          <t>maa://20109 (96.38), maa://22545 (100.00)</t>
         </is>
       </c>
       <c r="U25" s="19" t="n"/>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="X25" s="8" t="inlineStr">
         <is>
-          <t>maa://29890 (91.60)</t>
+          <t>maa://29890 (91.67)</t>
         </is>
       </c>
       <c r="Y25" s="19" t="n"/>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (93.41), *maa://24516 (79.00), maa://26001 (83.33), maa://68311 (98.57)</t>
+          <t>maa://31215 (93.45), *maa://24516 (79.00), maa://26001 (83.33), maa://68311 (98.68)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (98.17), maa://36676 (99.84), maa://24621 (96.88), maa://22771 (88.24), maa://37772 (85.71)</t>
+          <t>maa://20108 (98.18), maa://36676 (99.85), maa://24621 (96.89), maa://22771 (88.24), maa://37772 (85.71)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3858,7 +3858,7 @@
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
-          <t>maa://56240 (96.28), maa://24913 (92.24)</t>
+          <t>maa://56240 (96.33), maa://24913 (92.31)</t>
         </is>
       </c>
       <c r="I26" s="19" t="n"/>
@@ -3922,7 +3922,7 @@
       </c>
       <c r="X26" s="8" t="inlineStr">
         <is>
-          <t>maa://24389 (98.31)</t>
+          <t>maa://24389 (98.39)</t>
         </is>
       </c>
       <c r="Y26" s="19" t="n"/>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="AB26" s="8" t="inlineStr">
         <is>
-          <t>maa://42235 (98.40)</t>
+          <t>maa://42235 (98.42)</t>
         </is>
       </c>
       <c r="AC26" s="19" t="n"/>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="AF26" s="8" t="inlineStr">
         <is>
-          <t>*maa://30511 (71.60), **maa://29760 (45.45)</t>
+          <t>*maa://30511 (71.95), **maa://29760 (45.45)</t>
         </is>
       </c>
       <c r="AG26" s="16" t="n"/>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>maa://39601 (91.45), maa://34494 (95.45)</t>
+          <t>maa://39601 (91.60), maa://34494 (95.45)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="T27" s="8" t="inlineStr">
         <is>
-          <t>maa://30624 (89.94)</t>
+          <t>maa://30624 (90.06)</t>
         </is>
       </c>
       <c r="U27" s="19" t="n"/>
@@ -4084,7 +4084,7 @@
       </c>
       <c r="AF27" s="8" t="inlineStr">
         <is>
-          <t>maa://24023 (97.79)</t>
+          <t>maa://24023 (97.81)</t>
         </is>
       </c>
       <c r="AG27" s="16" t="n"/>
@@ -4102,7 +4102,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (95.95), maa://25725 (85.38)</t>
+          <t>maa://24465 (95.98), maa://25725 (85.38)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="L28" s="8" t="inlineStr">
         <is>
-          <t>maa://30770 (90.43)</t>
+          <t>maa://30770 (90.53)</t>
         </is>
       </c>
       <c r="M28" s="19" t="n"/>
@@ -4166,7 +4166,7 @@
       </c>
       <c r="T28" s="8" t="inlineStr">
         <is>
-          <t>maa://29765 (93.71), maa://23263 (96.27)</t>
+          <t>maa://29765 (93.77), maa://23263 (96.27)</t>
         </is>
       </c>
       <c r="U28" s="19" t="n"/>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (97.36), maa://41749 (97.23)</t>
+          <t>maa://39929 (97.38), maa://41749 (97.24)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (94.38), maa://65700 (98.69)</t>
+          <t>maa://36660 (94.41), maa://65700 (98.71)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (97.80), maa://31400 (98.10), maa://28440 (86.50)</t>
+          <t>maa://28432 (97.82), maa://31400 (98.10), maa://28440 (86.50)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4280,7 +4280,7 @@
       </c>
       <c r="P29" s="8" t="inlineStr">
         <is>
-          <t>maa://54169 (97.50)</t>
+          <t>maa://54169 (97.58)</t>
         </is>
       </c>
       <c r="Q29" s="19" t="n"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://42865 (92.16)</t>
+          <t>maa://42865 (92.20)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (95.65), maa://64191 (97.56)</t>
+          <t>maa://45792 (95.65), maa://64191 (97.62)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="L30" s="8" t="inlineStr">
         <is>
-          <t>maa://30442 (97.52)</t>
+          <t>maa://30442 (97.56)</t>
         </is>
       </c>
       <c r="M30" s="19" t="n"/>
@@ -4442,7 +4442,7 @@
       </c>
       <c r="X30" s="8" t="inlineStr">
         <is>
-          <t>maa://39477 (96.30)</t>
+          <t>maa://39477 (96.36)</t>
         </is>
       </c>
       <c r="Y30" s="19" t="n"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (98.07), maa://36258 (93.15), maa://43904 (88.10)</t>
+          <t>maa://35926 (98.09), maa://36258 (93.21), maa://43904 (88.10)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4556,7 +4556,7 @@
       </c>
       <c r="T31" s="8" t="inlineStr">
         <is>
-          <t>maa://30711 (96.69), maa://30768 (100.00)</t>
+          <t>maa://30711 (96.72), maa://30768 (100.00)</t>
         </is>
       </c>
       <c r="U31" s="19" t="n"/>
@@ -4588,7 +4588,7 @@
       </c>
       <c r="AB31" s="8" t="inlineStr">
         <is>
-          <t>maa://66997 (100.00)</t>
+          <t>maa://66997 (95.45)</t>
         </is>
       </c>
       <c r="AC31" s="19" t="n"/>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (99.30), maa://41108 (87.72), maa://41238 (98.14), maa://45523 (100.00)</t>
+          <t>maa://42859 (99.31), maa://41108 (87.72), maa://41238 (98.14), maa://45523 (100.00)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="X32" s="8" t="inlineStr">
         <is>
-          <t>maa://64104 (97.54)</t>
+          <t>maa://64104 (97.56)</t>
         </is>
       </c>
       <c r="Y32" s="19" t="n"/>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (94.59), maa://69135 (95.00)</t>
+          <t>maa://21956 (94.63), maa://69135 (91.67)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="T33" s="8" t="inlineStr">
         <is>
-          <t>maa://45558 (90.32)</t>
+          <t>maa://45558 (90.62)</t>
         </is>
       </c>
       <c r="U33" s="19" t="n"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (99.24), maa://56235 (99.50)</t>
+          <t>maa://48817 (99.25), maa://56235 (99.50)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="T34" s="8" t="inlineStr">
         <is>
-          <t>maa://24526 (97.15)</t>
+          <t>maa://24526 (97.17)</t>
         </is>
       </c>
       <c r="U34" s="19" t="n"/>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="AB34" s="8" t="inlineStr">
         <is>
-          <t>maa://64329 (98.00)</t>
+          <t>maa://64329 (98.04)</t>
         </is>
       </c>
       <c r="AC34" s="19" t="n"/>
@@ -5076,7 +5076,7 @@
       </c>
       <c r="T35" s="8" t="inlineStr">
         <is>
-          <t>maa://24842 (96.63)</t>
+          <t>maa://24842 (96.67)</t>
         </is>
       </c>
       <c r="U35" s="19" t="n"/>
@@ -5124,7 +5124,7 @@
       </c>
       <c r="AF35" s="8" t="inlineStr">
         <is>
-          <t>maa://39479 (96.08)</t>
+          <t>maa://39479 (96.15)</t>
         </is>
       </c>
       <c r="AG35" s="16" t="n"/>
@@ -5158,7 +5158,7 @@
       </c>
       <c r="H36" s="8" t="inlineStr">
         <is>
-          <t>maa://24375 (94.44)</t>
+          <t>maa://24375 (94.52)</t>
         </is>
       </c>
       <c r="I36" s="19" t="n"/>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="AB36" s="19" t="inlineStr">
         <is>
-          <t>maa://64106 (97.22)</t>
+          <t>maa://64106 (97.30)</t>
         </is>
       </c>
       <c r="AC36" s="19" t="n"/>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="H37" s="8" t="inlineStr">
         <is>
-          <t>*maa://24374 (58.06)</t>
+          <t>*maa://24374 (58.73)</t>
         </is>
       </c>
       <c r="I37" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (99.05), maa://56336 (99.38), maa://47069 (86.67), maa://45789 (100.00)</t>
+          <t>maa://45718 (99.06), maa://56336 (99.38), maa://47069 (86.67), maa://45789 (100.00)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="P37" s="8" t="inlineStr">
         <is>
-          <t>maa://21280 (97.66)</t>
+          <t>maa://21280 (97.59)</t>
         </is>
       </c>
       <c r="Q37" s="19" t="n"/>
@@ -5418,7 +5418,7 @@
       </c>
       <c r="L38" s="8" t="inlineStr">
         <is>
-          <t>maa://39384 (99.29), maa://49735 (92.86)</t>
+          <t>maa://39384 (99.32), maa://49735 (92.86)</t>
         </is>
       </c>
       <c r="M38" s="19" t="n"/>
@@ -5482,7 +5482,7 @@
       </c>
       <c r="AF38" s="8" t="inlineStr">
         <is>
-          <t>maa://36697 (95.75), maa://68397 (99.10)</t>
+          <t>maa://36697 (95.76), maa://68397 (99.19)</t>
         </is>
       </c>
       <c r="AG38" s="16" t="n"/>
@@ -5503,7 +5503,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://25199 (84.78), maa://45059 (94.12), maa://30434 (95.34), maa://44165 (85.71)</t>
+          <t>maa://25199 (84.78), maa://45059 (94.31), maa://30434 (95.34), maa://44165 (85.71)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://47093 (98.28), maa://24709 (94.07)</t>
+          <t>maa://47093 (98.31), maa://24709 (94.12)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (95.70), maa://45790 (88.16)</t>
+          <t>maa://47079 (95.74), maa://45790 (88.16)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5583,7 +5583,7 @@
       </c>
       <c r="AF39" s="8" t="inlineStr">
         <is>
-          <t>maa://62953 (96.81)</t>
+          <t>maa://62953 (96.85)</t>
         </is>
       </c>
       <c r="AG39" s="16" t="n"/>
@@ -5636,7 +5636,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (98.14), maa://21386 (95.96), maa://36664 (89.74), *maa://45550 (75.00)</t>
+          <t>maa://23278 (98.16), maa://21386 (95.96), maa://36664 (89.74), *maa://45550 (75.00)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://65283 (97.03), maa://64205 (93.75)</t>
+          <t>maa://65283 (97.09), maa://64205 (93.94)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="P41" s="8" t="inlineStr">
         <is>
-          <t>maa://43177 (95.54)</t>
+          <t>maa://43177 (95.61)</t>
         </is>
       </c>
       <c r="Q41" s="19" t="n"/>
@@ -5902,12 +5902,12 @@
       </c>
       <c r="G43" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>*maa://22525 (70.09), maa://21284 (97.77)</t>
+          <t>maa://21284 (97.81)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -6008,7 +6008,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (98.29), maa://56386 (99.42), maa://27728 (96.40)</t>
+          <t>maa://29768 (98.30), maa://56386 (99.43), maa://27728 (96.40)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6056,7 +6056,7 @@
       </c>
       <c r="T44" s="8" t="inlineStr">
         <is>
-          <t>maa://39366 (93.62)</t>
+          <t>maa://39366 (93.68)</t>
         </is>
       </c>
       <c r="U44" s="19" t="n"/>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://42459 (98.75), maa://21229 (85.78), maa://30807 (94.62), *maa://22767 (70.83)</t>
+          <t>maa://42459 (98.76), maa://21229 (85.78), maa://30807 (94.62), *maa://22767 (71.23)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6125,7 +6125,7 @@
       </c>
       <c r="T45" s="8" t="inlineStr">
         <is>
-          <t>*maa://39364 (67.88)</t>
+          <t>*maa://39364 (68.07)</t>
         </is>
       </c>
       <c r="U45" s="19" t="n"/>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (95.85), maa://43901 (96.34)</t>
+          <t>maa://35931 (95.89), maa://43901 (96.38)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6231,7 +6231,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (97.52), maa://29661 (97.24), maa://56236 (99.79), maa://28038 (84.62)</t>
+          <t>maa://27410 (97.53), maa://29661 (97.24), maa://56236 (99.80), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6263,7 +6263,7 @@
       </c>
       <c r="T47" s="8" t="inlineStr">
         <is>
-          <t>maa://67476 (99.57), maa://68392 (99.61)</t>
+          <t>maa://67476 (99.57), maa://68392 (99.64)</t>
         </is>
       </c>
       <c r="U47" s="19" t="n"/>
@@ -6381,7 +6381,7 @@
       </c>
       <c r="P49" s="8" t="inlineStr">
         <is>
-          <t>*maa://39643 (79.58)</t>
+          <t>*maa://39643 (79.86)</t>
         </is>
       </c>
       <c r="Q49" s="19" t="n"/>
@@ -6397,7 +6397,7 @@
       </c>
       <c r="T49" s="19" t="inlineStr">
         <is>
-          <t>maa://67231 (99.15)</t>
+          <t>maa://67231 (99.16)</t>
         </is>
       </c>
       <c r="U49" s="19" t="n"/>
@@ -6434,7 +6434,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>maa://62852 (93.25)</t>
+          <t>maa://62852 (93.32)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6468,7 +6468,7 @@
       </c>
       <c r="H51" s="8" t="inlineStr">
         <is>
-          <t>maa://30769 (90.00)</t>
+          <t>maa://30769 (90.32)</t>
         </is>
       </c>
       <c r="I51" s="19" t="n"/>
@@ -6518,7 +6518,7 @@
       </c>
       <c r="H52" s="8" t="inlineStr">
         <is>
-          <t>maa://24376 (99.11)</t>
+          <t>maa://24376 (99.12)</t>
         </is>
       </c>
       <c r="I52" s="19" t="n"/>
@@ -6534,7 +6534,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (99.40), maa://59378 (93.83), maa://65511 (100.00)</t>
+          <t>maa://59394 (99.41), maa://59378 (93.83), maa://65511 (100.00)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6568,7 +6568,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (97.94)</t>
+          <t>maa://32534 (97.96)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -6652,7 +6652,7 @@
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>maa://32532 (97.89)</t>
+          <t>maa://32532 (97.90)</t>
         </is>
       </c>
       <c r="I55" s="19" t="n"/>
@@ -6704,7 +6704,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://56237 (98.22), maa://25176 (98.77)</t>
+          <t>maa://56237 (98.29), maa://25176 (98.77)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6722,7 +6722,7 @@
       </c>
       <c r="H58" s="8" t="inlineStr">
         <is>
-          <t>*maa://37964 (65.85)</t>
+          <t>*maa://37964 (66.13)</t>
         </is>
       </c>
       <c r="I58" s="19" t="n"/>
@@ -6740,7 +6740,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (98.36), maa://27746 (89.47)</t>
+          <t>maa://31270 (98.37), maa://27746 (89.47)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -6758,7 +6758,7 @@
       </c>
       <c r="H60" s="8" t="inlineStr">
         <is>
-          <t>maa://40438 (91.80)</t>
+          <t>maa://40438 (91.86)</t>
         </is>
       </c>
       <c r="I60" s="19" t="n"/>
@@ -6794,7 +6794,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (96.74), maa://56228 (98.12), maa://43903 (100.00)</t>
+          <t>maa://42981 (96.74), maa://56228 (98.15), maa://43903 (100.00)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6812,7 +6812,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (99.43), *maa://59693 (73.47), maa://59413 (97.50)</t>
+          <t>maa://59534 (99.44), *maa://59693 (73.47), maa://59413 (97.50)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7028,7 +7028,7 @@
       </c>
       <c r="H75" s="19" t="inlineStr">
         <is>
-          <t>maa://67748 (81.82)</t>
+          <t>*maa://67748 (80.00)</t>
         </is>
       </c>
       <c r="I75" s="19" t="n"/>
@@ -7170,7 +7170,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.10.03 13:19:12</t>
+          <t>更新日期：2025.10.05 13:18:08</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8574,7 +8574,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (73.21), *maa://28758 (71.74), maa://29036 (96.67), *maa://42172 (71.43), maa://65357 (96.55), maa://30285 (100.00)</t>
+          <t>*maa://20849 (73.21), *maa://28758 (71.74), maa://29036 (96.67), *maa://42172 (71.43), maa://65357 (96.67), maa://30285 (100.00)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -9114,7 +9114,7 @@
       </c>
       <c r="D37" s="13" t="inlineStr">
         <is>
-          <t>maa://27376 (93.44), maa://42635 (94.44), *maa://20838 (55.00)</t>
+          <t>maa://27376 (91.94), maa://42635 (94.44), *maa://20838 (55.00)</t>
         </is>
       </c>
       <c r="E37" s="14" t="inlineStr">
@@ -9600,7 +9600,7 @@
       </c>
       <c r="D46" s="13" t="inlineStr">
         <is>
-          <t>*maa://39025 (77.78)</t>
+          <t>*maa://39025 (80.00)</t>
         </is>
       </c>
       <c r="E46" s="14" t="inlineStr">
@@ -10140,7 +10140,7 @@
       </c>
       <c r="D56" s="13" t="inlineStr">
         <is>
-          <t>maa://44235 (98.45), maa://45604 (100.00), maa://20961 (100.00), maa://20910 (100.00), maa://44220 (100.00)</t>
+          <t>maa://44235 (98.45), maa://45604 (100.00), maa://20961 (93.75), maa://44220 (100.00), maa://20910 (100.00)</t>
         </is>
       </c>
       <c r="E56" s="14" t="inlineStr">
@@ -10842,7 +10842,7 @@
       </c>
       <c r="D69" s="13" t="inlineStr">
         <is>
-          <t>maa://20974 (96.97), maa://29079 (80.95), maa://29096 (95.65), maa://29087 (100.00), *maa://20823 (75.00), maa://20855 (94.12), maa://20904 (100.00), *maa://63722 (80.00)</t>
+          <t>maa://20974 (97.00), maa://29079 (80.95), maa://29096 (95.65), maa://29087 (100.00), *maa://20823 (75.00), maa://20855 (94.12), maa://20904 (100.00), *maa://63722 (80.00)</t>
         </is>
       </c>
       <c r="E69" s="14" t="inlineStr">
@@ -11274,7 +11274,7 @@
       </c>
       <c r="D77" s="13" t="inlineStr">
         <is>
-          <t>maa://20958 (95.00), ***maa://39769 (20.00)</t>
+          <t>maa://20958 (95.12), ***maa://39769 (20.00)</t>
         </is>
       </c>
       <c r="E77" s="14" t="inlineStr">
@@ -11868,7 +11868,7 @@
       </c>
       <c r="D88" s="13" t="inlineStr">
         <is>
-          <t>maa://24472 (91.01), *maa://35841 (65.22)</t>
+          <t>maa://24472 (91.04), *maa://35841 (65.22)</t>
         </is>
       </c>
       <c r="E88" s="14" t="inlineStr">
@@ -12192,7 +12192,7 @@
       </c>
       <c r="D94" s="13" t="inlineStr">
         <is>
-          <t>maa://40157 (87.50)</t>
+          <t>maa://40157 (88.89)</t>
         </is>
       </c>
       <c r="E94" s="14" t="inlineStr">
@@ -12354,7 +12354,7 @@
       </c>
       <c r="D97" s="13" t="inlineStr">
         <is>
-          <t>maa://20991 (100.00), maa://51015 (88.89)</t>
+          <t>maa://20991 (100.00), maa://51015 (87.23)</t>
         </is>
       </c>
       <c r="E97" s="14" t="inlineStr">
@@ -12624,7 +12624,7 @@
       </c>
       <c r="D102" s="13" t="inlineStr">
         <is>
-          <t>maa://40517 (90.62), *maa://39240 (56.25)</t>
+          <t>maa://40517 (90.91), *maa://39240 (56.25)</t>
         </is>
       </c>
       <c r="E102" s="14" t="inlineStr">
@@ -12678,7 +12678,7 @@
       </c>
       <c r="D103" s="13" t="inlineStr">
         <is>
-          <t>*maa://29094 (76.27), maa://28904 (88.64), **maa://20931 (47.37)</t>
+          <t>*maa://29094 (76.27), maa://28904 (88.89), **maa://20931 (47.37)</t>
         </is>
       </c>
       <c r="E103" s="14" t="inlineStr">
@@ -12948,7 +12948,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.73), maa://25018 (96.96), maa://25776 (92.31), maa://28361 (95.56), maa://25772 (94.12), maa://56588 (93.33), maa://45194 (86.36), maa://32653 (81.25), maa://25161 (84.21), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
+          <t>maa://51881 (98.74), maa://25018 (96.96), maa://25776 (92.41), maa://28361 (95.56), maa://25772 (94.12), maa://56588 (93.33), maa://45194 (86.36), maa://32653 (81.25), maa://25161 (84.21), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13488,7 +13488,7 @@
       </c>
       <c r="D118" s="13" t="inlineStr">
         <is>
-          <t>maa://31560 (92.86), maa://20940 (87.50)</t>
+          <t>maa://31560 (93.33), maa://20940 (87.50)</t>
         </is>
       </c>
       <c r="E118" s="14" t="inlineStr">
@@ -13596,7 +13596,7 @@
       </c>
       <c r="D120" s="13" t="inlineStr">
         <is>
-          <t>maa://31560 (92.86), maa://20851 (100.00)</t>
+          <t>maa://31560 (93.33), maa://20851 (100.00)</t>
         </is>
       </c>
       <c r="E120" s="14" t="inlineStr">
@@ -14838,7 +14838,7 @@
       </c>
       <c r="D143" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (97.84), *maa://23736 (52.44), maa://31185 (91.67), maa://30306 (100.00)</t>
+          <t>maa://28484 (97.86), *maa://23736 (53.01), maa://31185 (91.67), maa://30306 (100.00)</t>
         </is>
       </c>
       <c r="E143" s="14" t="inlineStr">
@@ -15270,7 +15270,7 @@
       </c>
       <c r="D151" s="13" t="inlineStr">
         <is>
-          <t>maa://51549 (96.97), maa://51923 (96.30), maa://67508 (100.00)</t>
+          <t>maa://51549 (96.97), maa://51923 (96.30), *maa://67508 (66.67)</t>
         </is>
       </c>
       <c r="E151" s="14" t="inlineStr">
@@ -15324,7 +15324,7 @@
       </c>
       <c r="D152" s="13" t="inlineStr">
         <is>
-          <t>maa://20961 (100.00)</t>
+          <t>maa://20961 (93.75)</t>
         </is>
       </c>
       <c r="E152" s="14" t="inlineStr">
@@ -15756,7 +15756,7 @@
       </c>
       <c r="D160" s="13" t="inlineStr">
         <is>
-          <t>maa://44232 (98.48), maa://45603 (90.62), *maa://65963 (80.00), *maa://63114 (66.67)</t>
+          <t>maa://44232 (98.48), maa://45603 (90.62), maa://65963 (83.33), *maa://63114 (66.67)</t>
         </is>
       </c>
       <c r="E160" s="14" t="inlineStr">
@@ -16242,7 +16242,7 @@
       </c>
       <c r="D169" s="13" t="inlineStr">
         <is>
-          <t>maa://49867 (93.75), maa://49655 (97.73)</t>
+          <t>maa://49867 (93.75), maa://49655 (97.78)</t>
         </is>
       </c>
       <c r="E169" s="14" t="inlineStr">
@@ -16998,7 +16998,7 @@
       </c>
       <c r="D183" s="13" t="inlineStr">
         <is>
-          <t>maa://31560 (92.86), *maa://20968 (66.67)</t>
+          <t>maa://31560 (93.33), *maa://20968 (66.67)</t>
         </is>
       </c>
       <c r="E183" s="14" t="inlineStr">
@@ -17376,7 +17376,7 @@
       </c>
       <c r="D190" s="13" t="inlineStr">
         <is>
-          <t>maa://39153 (100.00)</t>
+          <t>*maa://39153 (66.67)</t>
         </is>
       </c>
       <c r="E190" s="14" t="inlineStr">
@@ -17803,12 +17803,12 @@
       </c>
       <c r="C198" s="12" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="D198" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.52), maa://35854 (84.75), maa://50388 (98.25), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (95.35)</t>
+          <t>maa://44224 (90.41), maa://35854 (84.75), maa://50388 (98.26), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (95.56), maa://70161 (100.00)</t>
         </is>
       </c>
       <c r="E198" s="14" t="inlineStr">
@@ -17862,7 +17862,7 @@
       </c>
       <c r="D199" s="13" t="inlineStr">
         <is>
-          <t>maa://39156 (94.25), *maa://39550 (55.00), *maa://53417 (77.78), *maa://63806 (77.78)</t>
+          <t>maa://39156 (94.25), *maa://39550 (55.00), *maa://53417 (77.78), *maa://63806 (80.00)</t>
         </is>
       </c>
       <c r="E199" s="14" t="inlineStr">
@@ -18510,7 +18510,7 @@
       </c>
       <c r="D211" s="13" t="inlineStr">
         <is>
-          <t>maa://28133 (93.33), **maa://39217 (38.89), maa://25369 (95.12)</t>
+          <t>maa://28133 (93.33), **maa://39217 (38.89), maa://25369 (95.24)</t>
         </is>
       </c>
       <c r="E211" s="14" t="inlineStr">
@@ -19374,7 +19374,7 @@
       </c>
       <c r="D227" s="13" t="inlineStr">
         <is>
-          <t>maa://28187 (97.73), maa://39520 (100.00), maa://43531 (100.00)</t>
+          <t>maa://28187 (97.73), maa://43531 (100.00), maa://39520 (100.00)</t>
         </is>
       </c>
       <c r="E227" s="14" t="inlineStr">
@@ -19482,7 +19482,7 @@
       </c>
       <c r="D229" s="13" t="inlineStr">
         <is>
-          <t>maa://20987 (94.17), *maa://35801 (77.78)</t>
+          <t>maa://20987 (94.23), *maa://35801 (77.78)</t>
         </is>
       </c>
       <c r="E229" s="14" t="inlineStr">
@@ -19698,7 +19698,7 @@
       </c>
       <c r="D233" s="13" t="inlineStr">
         <is>
-          <t>maa://29058 (96.30), maa://39140 (100.00), maa://38723 (100.00)</t>
+          <t>maa://29058 (96.34), maa://39140 (100.00), maa://38723 (100.00)</t>
         </is>
       </c>
       <c r="E233" s="14" t="inlineStr">
@@ -20454,7 +20454,7 @@
       </c>
       <c r="D247" s="13" t="inlineStr">
         <is>
-          <t>maa://20867 (93.33), maa://38485 (96.67), *maa://32202 (80.00)</t>
+          <t>maa://20867 (93.33), maa://38485 (96.77), *maa://32202 (80.00)</t>
         </is>
       </c>
       <c r="E247" s="14" t="inlineStr">
@@ -21264,7 +21264,7 @@
       </c>
       <c r="D262" s="13" t="inlineStr">
         <is>
-          <t>maa://31560 (92.86), maa://20884 (96.30)</t>
+          <t>maa://31560 (93.33), maa://20884 (96.30)</t>
         </is>
       </c>
       <c r="E262" s="14" t="inlineStr">
@@ -21372,7 +21372,7 @@
       </c>
       <c r="D264" s="13" t="inlineStr">
         <is>
-          <t>maa://29027 (98.33)</t>
+          <t>maa://29027 (98.36)</t>
         </is>
       </c>
       <c r="E264" s="14" t="inlineStr">
@@ -22020,7 +22020,7 @@
       </c>
       <c r="D276" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.73), maa://51630 (96.26), maa://56588 (93.33), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (41.67), maa://66758 (83.33)</t>
+          <t>maa://51881 (98.74), maa://51630 (96.26), maa://56588 (93.33), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (41.67), maa://66758 (83.33)</t>
         </is>
       </c>
       <c r="E276" s="14" t="inlineStr">
@@ -23478,7 +23478,7 @@
       </c>
       <c r="D303" s="13" t="inlineStr">
         <is>
-          <t>maa://29005 (98.78), maa://31560 (92.86)</t>
+          <t>maa://29005 (98.78), maa://31560 (93.33)</t>
         </is>
       </c>
       <c r="E303" s="14" t="inlineStr">
@@ -23694,7 +23694,7 @@
       </c>
       <c r="D307" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (98.49), maa://49642 (97.62), maa://49660 (93.62), maa://50517 (85.71), maa://70004 (100.00)</t>
+          <t>maa://50280 (98.50), maa://49642 (97.66), maa://49660 (93.62), maa://50517 (85.71), maa://70004 (100.00)</t>
         </is>
       </c>
       <c r="E307" s="14" t="inlineStr">
@@ -25368,7 +25368,7 @@
       </c>
       <c r="D338" s="22" t="inlineStr">
         <is>
-          <t>maa://44234 (99.18)</t>
+          <t>maa://44234 (99.19)</t>
         </is>
       </c>
       <c r="E338" s="22" t="inlineStr">
@@ -26178,7 +26178,7 @@
       </c>
       <c r="D353" s="22" t="inlineStr">
         <is>
-          <t>maa://34716 (88.89)</t>
+          <t>maa://34716 (90.00)</t>
         </is>
       </c>
       <c r="E353" s="22" t="inlineStr">
@@ -26556,7 +26556,7 @@
       </c>
       <c r="D360" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.60), maa://49695 (100.00), maa://49758 (98.72), *maa://59402 (56.67), *maa://52357 (75.00), *maa://63091 (75.00)</t>
+          <t>maa://49696 (99.60), maa://49695 (100.00), maa://49758 (98.73), *maa://52357 (75.00), *maa://59402 (56.67), *maa://63091 (75.00)</t>
         </is>
       </c>
       <c r="E360" s="22" t="inlineStr">
@@ -28284,7 +28284,7 @@
       </c>
       <c r="D392" s="22" t="inlineStr">
         <is>
-          <t>maa://63890 (97.92), maa://64043 (100.00)</t>
+          <t>maa://63890 (97.96), maa://64043 (100.00)</t>
         </is>
       </c>
       <c r="E392" s="22" t="inlineStr">
@@ -28365,7 +28365,7 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>maa://47023 (87.04)</t>
+          <t>maa://47023 (87.27)</t>
         </is>
       </c>
       <c r="E394" t="inlineStr">
@@ -28554,7 +28554,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>maa://51872 (96.67), maa://51876 (99.07), maa://63228 (88.24), maa://51873 (100.00), maa://62047 (92.31)</t>
+          <t>maa://51872 (96.68), maa://51876 (99.07), maa://63228 (88.24), maa://51873 (100.00), maa://62047 (92.59)</t>
         </is>
       </c>
       <c r="E401" t="inlineStr">
@@ -28581,7 +28581,7 @@
       </c>
       <c r="D402" t="inlineStr">
         <is>
-          <t>**maa://67814 (50.00)</t>
+          <t>*maa://67814 (66.67)</t>
         </is>
       </c>
       <c r="E402" t="inlineStr">
@@ -28716,7 +28716,7 @@
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>maa://64040 (99.02), maa://52505 (98.21), maa://66377 (93.75), ***maa://66376 (20.00)</t>
+          <t>maa://64040 (99.03), maa://52505 (98.21), maa://66377 (93.75), ***maa://66376 (20.00)</t>
         </is>
       </c>
       <c r="E407" t="inlineStr">
@@ -28770,7 +28770,7 @@
       </c>
       <c r="D409" t="inlineStr">
         <is>
-          <t>maa://67388 (93.75)</t>
+          <t>maa://67388 (93.88)</t>
         </is>
       </c>
       <c r="E409" t="inlineStr">
@@ -28824,7 +28824,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>maa://67088 (92.31)</t>
+          <t>maa://67088 (92.42)</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
@@ -28851,7 +28851,7 @@
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>maa://67087 (94.34), maa://67268 (96.70), maa://67269 (88.89), maa://67648 (100.00)</t>
+          <t>maa://67087 (94.44), maa://67268 (96.81), maa://67269 (88.89), maa://67648 (100.00)</t>
         </is>
       </c>
       <c r="E412" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#247)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -712,7 +712,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (98.50), maa://24702 (95.12), maa://36681 (85.39)</t>
+          <t>maa://25390 (98.49), maa://24702 (95.15), maa://36681 (85.39)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://58660 (98.85), maa://39402 (94.98), *maa://34787 (74.26)</t>
+          <t>maa://58660 (98.88), maa://39402 (95.02), *maa://34787 (74.26)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -776,7 +776,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (97.48), maa://66635 (99.62)</t>
+          <t>maa://22742 (97.51), maa://66635 (99.51)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://36684 (98.41), maa://21246 (91.40)</t>
+          <t>maa://36684 (98.45), maa://21246 (91.40)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -824,7 +824,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://59087 (97.61), maa://25251 (91.61)</t>
+          <t>maa://59087 (97.68), maa://25251 (91.61)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -842,7 +842,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (99.46), maa://36987 (97.22), maa://39849 (92.86)</t>
+          <t>maa://40192 (99.42), maa://36987 (97.22), maa://39849 (92.86)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -858,7 +858,7 @@
       </c>
       <c r="H3" s="8" t="inlineStr">
         <is>
-          <t>maa://21247 (99.44)</t>
+          <t>maa://21247 (99.45)</t>
         </is>
       </c>
       <c r="I3" s="19" t="n"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>maa://22880 (91.73), maa://20276 (94.18), maa://22749 (84.62)</t>
+          <t>maa://22880 (91.88), maa://20276 (94.24), maa://22749 (85.71)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -890,7 +890,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (98.56), maa://26254 (98.25), *maa://22738 (80.00)</t>
+          <t>maa://21249 (98.59), maa://26254 (98.25), *maa://22738 (80.00)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://60545 (98.88), maa://45854 (88.18), maa://24617 (91.18)</t>
+          <t>maa://60545 (98.91), maa://45854 (87.95), maa://24617 (91.18)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (92.91), maa://27484 (99.24), maa://27480 (86.44)</t>
+          <t>maa://27396 (93.03), maa://27484 (99.25), maa://27480 (86.44)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://52241 (99.47), maa://24390 (96.88)</t>
+          <t>maa://52241 (99.48), maa://24390 (96.90)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -954,7 +954,7 @@
       </c>
       <c r="AF3" s="8" t="inlineStr">
         <is>
-          <t>maa://21289 (91.74)</t>
+          <t>maa://21289 (91.94)</t>
         </is>
       </c>
       <c r="AG3" s="16" t="n"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (98.24), maa://22499 (90.00), maa://22746 (100.00)</t>
+          <t>maa://24632 (98.28), maa://22499 (90.00), maa://22746 (100.00)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (99.20), maa://50121 (96.50)</t>
+          <t>maa://49983 (99.22), maa://50121 (96.60)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://27295 (97.89), maa://32509 (96.67), maa://31008 (95.38), maa://22754 (88.16), maa://70489 (100.00)</t>
+          <t>maa://27295 (97.94), maa://32509 (96.73), maa://31008 (95.41), maa://22754 (88.16), maa://70489 (100.00)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="X4" s="8" t="inlineStr">
         <is>
-          <t>maa://43217 (98.98)</t>
+          <t>maa://43217 (98.95)</t>
         </is>
       </c>
       <c r="Y4" s="19" t="n"/>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="AB4" s="8" t="inlineStr">
         <is>
-          <t>maa://32658 (81.25)</t>
+          <t>*maa://32658 (79.59)</t>
         </is>
       </c>
       <c r="AC4" s="19" t="n"/>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>*maa://39394 (56.86), *maa://30062 (61.29), ***maa://26209 (13.04)</t>
+          <t>*maa://39394 (55.77), *maa://30062 (61.29), ***maa://26209 (13.04)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (91.64), maa://54105 (98.45), *maa://22744 (80.00)</t>
+          <t>maa://21245 (91.74), maa://54105 (98.51), *maa://22744 (80.00)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="L5" s="8" t="inlineStr">
         <is>
-          <t>maa://22757 (91.45)</t>
+          <t>maa://22757 (91.53)</t>
         </is>
       </c>
       <c r="M5" s="19" t="n"/>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="P5" s="8" t="inlineStr">
         <is>
-          <t>maa://21919 (98.73), maa://21281 (82.35)</t>
+          <t>maa://21919 (98.77), maa://21281 (83.33)</t>
         </is>
       </c>
       <c r="Q5" s="19" t="n"/>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="X5" s="8" t="inlineStr">
         <is>
-          <t>maa://21290 (98.64)</t>
+          <t>maa://21290 (98.68)</t>
         </is>
       </c>
       <c r="Y5" s="19" t="n"/>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="AB5" s="8" t="inlineStr">
         <is>
-          <t>*maa://29863 (60.00), ***maa://22752 (12.50), **maa://26013 (33.33)</t>
+          <t>*maa://29863 (60.00), ***maa://22752 (12.50), **maa://26013 (38.46)</t>
         </is>
       </c>
       <c r="AC5" s="19" t="n"/>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="D6" s="8" t="inlineStr">
         <is>
-          <t>maa://42407 (97.67)</t>
+          <t>maa://42407 (97.77)</t>
         </is>
       </c>
       <c r="E6" s="19" t="n"/>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="H6" s="8" t="inlineStr">
         <is>
-          <t>maa://24370 (97.81)</t>
+          <t>maa://24370 (97.83)</t>
         </is>
       </c>
       <c r="I6" s="19" t="n"/>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="L6" s="8" t="inlineStr">
         <is>
-          <t>maa://24839 (99.49)</t>
+          <t>maa://24839 (99.50)</t>
         </is>
       </c>
       <c r="M6" s="19" t="n"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (98.94), maa://30381 (95.00)</t>
+          <t>maa://31836 (98.97), maa://30381 (95.24)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="T6" s="8" t="inlineStr">
         <is>
-          <t>*maa://37411 (77.50)</t>
+          <t>*maa://37411 (78.57)</t>
         </is>
       </c>
       <c r="U6" s="19" t="n"/>
@@ -1312,12 +1312,12 @@
       </c>
       <c r="W6" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="X6" s="8" t="inlineStr">
         <is>
-          <t>maa://52754 (96.84)</t>
+          <t>maa://52754 (96.89), maa://71825 (100.00)</t>
         </is>
       </c>
       <c r="Y6" s="19" t="n"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="AF6" s="8" t="inlineStr">
         <is>
-          <t>maa://33152 (81.82)</t>
+          <t>maa://33152 (81.94)</t>
         </is>
       </c>
       <c r="AG6" s="16" t="n"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>maa://21955 (98.32)</t>
+          <t>maa://21955 (98.36)</t>
         </is>
       </c>
       <c r="E7" s="19" t="n"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>*maa://22763 (75.81), maa://64972 (96.00)</t>
+          <t>*maa://22763 (76.19), maa://64972 (96.15)</t>
         </is>
       </c>
       <c r="I7" s="19" t="n"/>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (98.69), maa://24957 (94.55)</t>
+          <t>maa://28624 (98.73), maa://24957 (94.55)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="P7" s="8" t="inlineStr">
         <is>
-          <t>maa://22750 (97.18)</t>
+          <t>maa://22750 (97.22)</t>
         </is>
       </c>
       <c r="Q7" s="19" t="n"/>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="T7" s="8" t="inlineStr">
         <is>
-          <t>maa://21291 (93.85)</t>
+          <t>maa://21291 (93.96)</t>
         </is>
       </c>
       <c r="U7" s="19" t="n"/>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (97.50), maa://22758 (82.52)</t>
+          <t>maa://22399 (97.53), maa://22758 (82.86)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="AF7" s="8" t="inlineStr">
         <is>
-          <t>maa://45272 (99.51)</t>
+          <t>maa://45272 (99.52)</t>
         </is>
       </c>
       <c r="AG7" s="16" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.10.16 13:20:24</t>
+          <t>更新日期：2025.10.20 13:21:27</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (90.91)</t>
+          <t>maa://21476 (90.50)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
-          <t>maa://24371 (80.49)</t>
+          <t>maa://24371 (80.86)</t>
         </is>
       </c>
       <c r="I8" s="19" t="n"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (91.82), maa://23252 (91.67), maa://37496 (98.39)</t>
+          <t>maa://32931 (91.93), maa://23252 (91.67), maa://37496 (98.39)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (96.05), maa://67587 (98.56)</t>
+          <t>maa://21411 (96.06), maa://67587 (98.46)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="AB8" s="8" t="inlineStr">
         <is>
-          <t>maa://25389 (95.12)</t>
+          <t>maa://25389 (95.20)</t>
         </is>
       </c>
       <c r="AC8" s="19" t="n"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>maa://24479 (85.58), **maa://21990 (50.00)</t>
+          <t>maa://24479 (86.18), **maa://21990 (50.00)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>maa://22765 (96.08), *maa://21915 (80.00)</t>
+          <t>maa://22765 (96.15), *maa://21915 (80.00)</t>
         </is>
       </c>
       <c r="E9" s="19" t="n"/>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (96.48), maa://39552 (87.27)</t>
+          <t>maa://22762 (96.49), maa://39552 (87.50)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="T9" s="8" t="inlineStr">
         <is>
-          <t>maa://26222 (99.52)</t>
+          <t>maa://26222 (99.53)</t>
         </is>
       </c>
       <c r="U9" s="19" t="n"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (95.40), maa://40166 (95.10)</t>
+          <t>maa://28711 (95.22), maa://40166 (95.16)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (91.51), maa://66916 (98.36)</t>
+          <t>maa://26206 (91.51), maa://66916 (98.41)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>maa://54000 (91.92)</t>
+          <t>maa://54000 (92.08)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="H10" s="8" t="inlineStr">
         <is>
-          <t>maa://32651 (95.56)</t>
+          <t>maa://32651 (95.65)</t>
         </is>
       </c>
       <c r="I10" s="19" t="n"/>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (92.51), *maa://36669 (75.00)</t>
+          <t>maa://28977 (92.60), *maa://36669 (75.00)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (99.30), maa://22755 (91.76), maa://63521 (94.22)</t>
+          <t>maa://27395 (99.30), maa://22755 (91.80), maa://63521 (94.64)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://45828 (99.32), maa://22301 (97.65), maa://22726 (100.00)</t>
+          <t>maa://45828 (99.34), maa://22301 (97.65), maa://22726 (100.00)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>*maa://25021 (58.58), *maa://22733 (66.18), **maa://22761 (33.33)</t>
+          <t>*maa://25021 (58.82), *maa://22733 (66.67), **maa://22761 (33.33)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="L11" s="8" t="inlineStr">
         <is>
-          <t>maa://21287 (93.94)</t>
+          <t>maa://21287 (94.02)</t>
         </is>
       </c>
       <c r="M11" s="19" t="n"/>
@@ -1940,7 +1940,7 @@
       </c>
       <c r="P11" s="8" t="inlineStr">
         <is>
-          <t>maa://45557 (94.74)</t>
+          <t>maa://45557 (94.92)</t>
         </is>
       </c>
       <c r="Q11" s="19" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (93.69), maa://22501 (99.56), maa://64808 (100.00), maa://45521 (95.31)</t>
+          <t>maa://22747 (93.72), maa://22501 (99.57), maa://64808 (100.00), maa://45521 (95.31)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="X11" s="8" t="inlineStr">
         <is>
-          <t>maa://36713 (99.33)</t>
+          <t>maa://36713 (99.30)</t>
         </is>
       </c>
       <c r="Y11" s="19" t="n"/>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="AF11" s="8" t="inlineStr">
         <is>
-          <t>maa://31203 (98.72)</t>
+          <t>maa://31203 (98.77)</t>
         </is>
       </c>
       <c r="AG11" s="16" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (93.75), maa://54294 (97.09)</t>
+          <t>maa://21867 (93.75), maa://54294 (97.24)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (98.12), maa://64046 (98.64)</t>
+          <t>maa://63896 (98.16), maa://64046 (98.66)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="P12" s="8" t="inlineStr">
         <is>
-          <t>maa://57541 (90.24)</t>
+          <t>maa://57541 (90.48)</t>
         </is>
       </c>
       <c r="Q12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://37962 (98.91), maa://21485 (82.38), maa://22753 (92.92)</t>
+          <t>maa://37962 (98.92), maa://21485 (82.52), maa://22753 (92.95)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://36677 (99.14), maa://23669 (94.85), maa://39872 (98.52)</t>
+          <t>maa://36677 (99.15), maa://23669 (94.86), maa://39872 (98.56)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>maa://28932 (94.85)</t>
+          <t>maa://28932 (94.80)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (96.92), maa://36673 (94.33), maa://25001 (88.89)</t>
+          <t>maa://24999 (96.99), maa://36673 (94.48), maa://25001 (89.01)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.32), maa://66545 (98.66)</t>
+          <t>*maa://21248 (73.27), maa://66545 (98.67)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (97.91), maa://22583 (89.08), *maa://22500 (71.21)</t>
+          <t>maa://22676 (97.94), maa://22583 (89.33), *maa://22500 (71.64)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="X13" s="8" t="inlineStr">
         <is>
-          <t>maa://34957 (94.73)</t>
+          <t>maa://34957 (94.80)</t>
         </is>
       </c>
       <c r="Y13" s="19" t="n"/>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (94.37)</t>
+          <t>maa://39883 (94.08)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2282,7 +2282,7 @@
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>maa://30764 (94.77)</t>
+          <t>maa://30764 (94.81)</t>
         </is>
       </c>
       <c r="E14" s="19" t="n"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (99.05), maa://36682 (98.35), maa://26245 (97.07), maa://21288 (96.40)</t>
+          <t>maa://39841 (99.08), maa://36682 (98.37), maa://26245 (97.07), maa://21288 (96.40)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://42751 (99.00), maa://22521 (95.56)</t>
+          <t>maa://42751 (99.00), maa://22521 (95.59)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="X14" s="8" t="inlineStr">
         <is>
-          <t>maa://37468 (98.18)</t>
+          <t>maa://37468 (98.20)</t>
         </is>
       </c>
       <c r="Y14" s="19" t="n"/>
@@ -2378,7 +2378,7 @@
       </c>
       <c r="AB14" s="8" t="inlineStr">
         <is>
-          <t>maa://22764 (99.00)</t>
+          <t>maa://22764 (99.01)</t>
         </is>
       </c>
       <c r="AC14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (86.06), maa://45058 (98.30), maa://22734 (84.96), *maa://36048 (75.53), maa://69928 (100.00)</t>
+          <t>maa://22743 (86.35), maa://45058 (98.32), maa://22734 (84.96), *maa://36048 (75.66), maa://69928 (100.00)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (97.36), maa://21478 (90.48)</t>
+          <t>maa://24304 (97.42), maa://21478 (90.48)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="L15" s="8" t="inlineStr">
         <is>
-          <t>*maa://21334 (73.02)</t>
+          <t>*maa://21334 (72.73)</t>
         </is>
       </c>
       <c r="M15" s="19" t="n"/>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="T15" s="8" t="inlineStr">
         <is>
-          <t>maa://23892 (97.81)</t>
+          <t>maa://23892 (97.83)</t>
         </is>
       </c>
       <c r="U15" s="19" t="n"/>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://36666 (96.51), maa://21364 (83.94), *maa://22766 (70.71), maa://68306 (85.07)</t>
+          <t>maa://36666 (96.54), maa://21364 (83.94), *maa://22766 (70.71), maa://68306 (85.14)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://37650 (99.77), maa://21441 (96.64), maa://36679 (94.55)</t>
+          <t>maa://37650 (99.78), maa://21441 (96.64), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://36674 (98.00), maa://22729 (96.36), *maa://28648 (77.89)</t>
+          <t>maa://36674 (98.01), maa://22729 (96.40), *maa://28648 (77.89)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2622,7 +2622,7 @@
       </c>
       <c r="X16" s="8" t="inlineStr">
         <is>
-          <t>maa://28501 (99.40), maa://28051 (97.14)</t>
+          <t>maa://28501 (99.41), maa://28051 (97.14)</t>
         </is>
       </c>
       <c r="Y16" s="19" t="n"/>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="AB16" s="8" t="inlineStr">
         <is>
-          <t>maa://26228 (98.07)</t>
+          <t>maa://26228 (98.09)</t>
         </is>
       </c>
       <c r="AC16" s="19" t="n"/>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>maa://23911 (90.87), maa://27755 (93.75), maa://67613 (99.56)</t>
+          <t>maa://23911 (90.95), maa://27755 (93.75), maa://67613 (99.60)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://39599 (98.39), maa://22430 (90.38)</t>
+          <t>maa://39599 (98.43), maa://22430 (90.38)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (83.06), maa://56238 (97.99)</t>
+          <t>maa://23890 (83.06), maa://56238 (98.04)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="T17" s="8" t="inlineStr">
         <is>
-          <t>*maa://42324 (72.63)</t>
+          <t>*maa://42324 (72.92)</t>
         </is>
       </c>
       <c r="U17" s="19" t="n"/>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="AF17" s="8" t="inlineStr">
         <is>
-          <t>maa://50136 (99.07)</t>
+          <t>maa://50136 (99.08)</t>
         </is>
       </c>
       <c r="AG17" s="16" t="n"/>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>maa://24570 (98.33)</t>
+          <t>maa://24570 (98.35)</t>
         </is>
       </c>
       <c r="E18" s="19" t="n"/>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="H18" s="8" t="inlineStr">
         <is>
-          <t>maa://24421 (95.62)</t>
+          <t>maa://24421 (95.63)</t>
         </is>
       </c>
       <c r="I18" s="19" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://52226 (99.67), maa://22466 (92.86)</t>
+          <t>maa://52226 (99.68), maa://22466 (92.86)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), maa://54153 (99.69), maa://24380 (100.00)</t>
+          <t>maa://24379 (100.00), maa://54153 (99.70), maa://24380 (100.00)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2866,7 +2866,7 @@
       </c>
       <c r="T18" s="8" t="inlineStr">
         <is>
-          <t>maa://24385 (98.67)</t>
+          <t>maa://24385 (98.72)</t>
         </is>
       </c>
       <c r="U18" s="19" t="n"/>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (98.81), maa://22741 (92.86)</t>
+          <t>maa://21917 (98.84), maa://22741 (92.86)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="AB18" s="8" t="inlineStr">
         <is>
-          <t>maa://24393 (99.08)</t>
+          <t>maa://24393 (99.10)</t>
         </is>
       </c>
       <c r="AC18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://47854 (94.08), *maa://68715 (75.00)</t>
+          <t>maa://47854 (94.22), *maa://68715 (75.00)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -2932,7 +2932,7 @@
       </c>
       <c r="D19" s="8" t="inlineStr">
         <is>
-          <t>maa://62850 (99.34)</t>
+          <t>maa://62850 (99.35)</t>
         </is>
       </c>
       <c r="E19" s="19" t="n"/>
@@ -2948,7 +2948,7 @@
       </c>
       <c r="H19" s="8" t="inlineStr">
         <is>
-          <t>maa://66740 (93.33)</t>
+          <t>maa://66740 (93.75)</t>
         </is>
       </c>
       <c r="I19" s="19" t="n"/>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="L19" s="8" t="inlineStr">
         <is>
-          <t>maa://39347 (98.04), maa://56392 (100.00)</t>
+          <t>maa://39347 (98.08), maa://56392 (100.00)</t>
         </is>
       </c>
       <c r="M19" s="19" t="n"/>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="T19" s="8" t="inlineStr">
         <is>
-          <t>maa://24386 (99.55)</t>
+          <t>maa://24386 (99.57)</t>
         </is>
       </c>
       <c r="U19" s="19" t="n"/>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="X19" s="8" t="inlineStr">
         <is>
-          <t>maa://31386 (97.73), maa://58490 (86.36)</t>
+          <t>maa://31386 (97.83), maa://58490 (86.36)</t>
         </is>
       </c>
       <c r="Y19" s="19" t="n"/>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (87.07), *maa://36668 (70.34)</t>
+          <t>maa://30709 (87.42), *maa://36668 (70.34)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://25198 (97.81), maa://36680 (99.14), maa://21432 (91.60)</t>
+          <t>maa://25198 (97.64), maa://36680 (99.15), maa://21432 (91.60)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3078,7 +3078,7 @@
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>maa://22864 (96.23)</t>
+          <t>maa://22864 (96.26)</t>
         </is>
       </c>
       <c r="I20" s="19" t="n"/>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (95.59)</t>
+          <t>maa://41331 (95.70)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="P20" s="8" t="inlineStr">
         <is>
-          <t>maa://37442 (98.70)</t>
+          <t>maa://37442 (98.71)</t>
         </is>
       </c>
       <c r="Q20" s="19" t="n"/>
@@ -3126,7 +3126,7 @@
       </c>
       <c r="T20" s="8" t="inlineStr">
         <is>
-          <t>maa://29113 (94.25)</t>
+          <t>maa://29113 (94.32)</t>
         </is>
       </c>
       <c r="U20" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (96.76), maa://56241 (98.29), maa://49976 (88.57)</t>
+          <t>maa://50085 (96.77), maa://56241 (98.34), maa://49976 (88.57)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>maa://21261 (99.10)</t>
+          <t>maa://21261 (99.11)</t>
         </is>
       </c>
       <c r="E21" s="19" t="n"/>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="H21" s="8" t="inlineStr">
         <is>
-          <t>maa://24372 (99.00)</t>
+          <t>maa://24372 (99.02)</t>
         </is>
       </c>
       <c r="I21" s="19" t="n"/>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="L21" s="8" t="inlineStr">
         <is>
-          <t>maa://31731 (96.69)</t>
+          <t>maa://31731 (96.72)</t>
         </is>
       </c>
       <c r="M21" s="19" t="n"/>
@@ -3240,7 +3240,7 @@
       </c>
       <c r="P21" s="8" t="inlineStr">
         <is>
-          <t>maa://24381 (84.62)</t>
+          <t>maa://24381 (85.00)</t>
         </is>
       </c>
       <c r="Q21" s="19" t="n"/>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (98.28), maa://20110 (87.01)</t>
+          <t>maa://34946 (98.33), maa://20110 (87.01)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="AB21" s="8" t="inlineStr">
         <is>
-          <t>maa://21443 (87.41), maa://52223 (84.69)</t>
+          <t>maa://21443 (87.46), maa://52223 (85.21)</t>
         </is>
       </c>
       <c r="AC21" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22432 (94.59), maa://22524 (82.99), maa://64221 (97.93)</t>
+          <t>maa://22432 (94.63), maa://22524 (82.99), maa://64221 (98.01)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>maa://25236 (99.28)</t>
+          <t>maa://25236 (99.29)</t>
         </is>
       </c>
       <c r="I22" s="19" t="n"/>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>maa://27127 (83.95), *maa://22751 (71.26), maa://66865 (99.50)</t>
+          <t>maa://27127 (84.02), *maa://22751 (71.26), maa://66865 (99.52)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://37649 (94.92), maa://21282 (98.98)</t>
+          <t>maa://37649 (94.89), maa://21282 (99.00)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="AF22" s="8" t="inlineStr">
         <is>
-          <t>maa://29658 (97.22)</t>
+          <t>maa://29658 (97.25)</t>
         </is>
       </c>
       <c r="AG22" s="16" t="n"/>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>*maa://41753 (66.67), **maa://28036 (30.43)</t>
+          <t>*maa://41753 (67.12), **maa://28036 (30.43)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (98.70), maa://39875 (95.04)</t>
+          <t>maa://39756 (98.72), maa://39875 (95.08)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (96.90), maa://29748 (82.05), *maa://37566 (78.79)</t>
+          <t>maa://30587 (96.99), maa://29748 (82.23), *maa://37566 (78.79)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="T23" s="8" t="inlineStr">
         <is>
-          <t>maa://31212 (95.12), maa://24387 (84.78), maa://67084 (88.89)</t>
+          <t>maa://31212 (95.24), maa://24387 (84.78), maa://67084 (88.89)</t>
         </is>
       </c>
       <c r="U23" s="19" t="n"/>
@@ -3548,7 +3548,7 @@
       </c>
       <c r="AB23" s="8" t="inlineStr">
         <is>
-          <t>maa://29652 (96.74)</t>
+          <t>maa://29652 (96.81)</t>
         </is>
       </c>
       <c r="AC23" s="19" t="n"/>
@@ -3564,7 +3564,7 @@
       </c>
       <c r="AF23" s="8" t="inlineStr">
         <is>
-          <t>maa://31489 (98.53)</t>
+          <t>maa://31489 (98.59)</t>
         </is>
       </c>
       <c r="AG23" s="16" t="n"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (85.58), maa://46650 (91.15)</t>
+          <t>maa://24368 (85.69), maa://46650 (91.38)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (96.64), maa://23504 (94.08), *maa://25141 (80.00), maa://52227 (97.25), *maa://36663 (79.63)</t>
+          <t>maa://29988 (96.72), maa://23504 (94.08), maa://25141 (80.13), maa://52227 (97.29), *maa://36663 (79.63)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="AB24" s="8" t="inlineStr">
         <is>
-          <t>maa://39349 (97.50)</t>
+          <t>maa://39349 (97.62)</t>
         </is>
       </c>
       <c r="AC24" s="19" t="n"/>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://64165 (99.27), maa://22523 (80.18), maa://29910 (94.20), maa://45831 (93.94)</t>
+          <t>maa://64165 (99.19), *maa://22523 (79.82), maa://29910 (94.20), maa://45831 (93.94)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (96.76), maa://63016 (99.25)</t>
+          <t>maa://29753 (96.78), maa://63016 (99.30)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>*maa://29063 (77.36), *maa://25311 (71.23), maa://45047 (88.61)</t>
+          <t>*maa://29063 (77.84), *maa://25311 (70.75), maa://45047 (88.61)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="T25" s="8" t="inlineStr">
         <is>
-          <t>maa://20109 (96.66), maa://22545 (100.00)</t>
+          <t>maa://20109 (96.76), maa://22545 (100.00)</t>
         </is>
       </c>
       <c r="U25" s="19" t="n"/>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="X25" s="8" t="inlineStr">
         <is>
-          <t>maa://29890 (92.25)</t>
+          <t>maa://29890 (92.31)</t>
         </is>
       </c>
       <c r="Y25" s="19" t="n"/>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (93.41), *maa://24516 (78.43), maa://26001 (81.97), maa://68311 (97.69)</t>
+          <t>maa://31215 (93.46), *maa://24516 (78.43), maa://26001 (81.97), maa://68311 (97.16)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (98.37), maa://36676 (99.85), maa://24621 (96.91), maa://22771 (88.24), maa://37772 (85.71)</t>
+          <t>maa://20108 (98.43), maa://36676 (99.85), maa://24621 (96.91), maa://22771 (88.24), maa://37772 (87.50)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3858,7 +3858,7 @@
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
-          <t>maa://56240 (96.22), maa://24913 (92.44)</t>
+          <t>maa://56240 (96.30), maa://24913 (92.50)</t>
         </is>
       </c>
       <c r="I26" s="19" t="n"/>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="P26" s="8" t="inlineStr">
         <is>
-          <t>maa://39870 (94.74), maa://56625 (98.73)</t>
+          <t>maa://39870 (94.87), maa://56625 (98.73)</t>
         </is>
       </c>
       <c r="Q26" s="19" t="n"/>
@@ -3922,7 +3922,7 @@
       </c>
       <c r="X26" s="8" t="inlineStr">
         <is>
-          <t>maa://24389 (98.51)</t>
+          <t>maa://24389 (98.55)</t>
         </is>
       </c>
       <c r="Y26" s="19" t="n"/>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="AB26" s="8" t="inlineStr">
         <is>
-          <t>maa://42235 (98.55)</t>
+          <t>maa://42235 (98.58)</t>
         </is>
       </c>
       <c r="AC26" s="19" t="n"/>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>maa://39601 (92.09), maa://34494 (95.83)</t>
+          <t>maa://39601 (92.25), maa://34494 (95.83)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4004,7 +4004,7 @@
       </c>
       <c r="L27" s="8" t="inlineStr">
         <is>
-          <t>maa://28071 (90.16)</t>
+          <t>maa://28071 (90.32)</t>
         </is>
       </c>
       <c r="M27" s="19" t="n"/>
@@ -4020,7 +4020,7 @@
       </c>
       <c r="P27" s="8" t="inlineStr">
         <is>
-          <t>maa://56400 (88.89)</t>
+          <t>maa://56400 (90.00)</t>
         </is>
       </c>
       <c r="Q27" s="19" t="n"/>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="T27" s="8" t="inlineStr">
         <is>
-          <t>maa://30624 (90.72)</t>
+          <t>maa://30624 (90.95)</t>
         </is>
       </c>
       <c r="U27" s="19" t="n"/>
@@ -4084,7 +4084,7 @@
       </c>
       <c r="AF27" s="8" t="inlineStr">
         <is>
-          <t>maa://24023 (97.92)</t>
+          <t>maa://24023 (97.93)</t>
         </is>
       </c>
       <c r="AG27" s="16" t="n"/>
@@ -4102,7 +4102,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (96.12), maa://25725 (85.50)</t>
+          <t>maa://24465 (96.15), maa://25725 (85.50)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="L28" s="8" t="inlineStr">
         <is>
-          <t>maa://30770 (91.26)</t>
+          <t>maa://30770 (91.51)</t>
         </is>
       </c>
       <c r="M28" s="19" t="n"/>
@@ -4166,7 +4166,7 @@
       </c>
       <c r="T28" s="8" t="inlineStr">
         <is>
-          <t>maa://29765 (94.19), maa://23263 (96.35)</t>
+          <t>maa://29765 (94.26), maa://23263 (96.35)</t>
         </is>
       </c>
       <c r="U28" s="19" t="n"/>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (97.50), maa://41749 (97.27)</t>
+          <t>maa://39929 (97.54), maa://41749 (97.27)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (94.29), maa://65700 (98.83)</t>
+          <t>maa://36660 (94.19), maa://65700 (98.49)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4232,7 +4232,7 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>maa://31694 (99.38)</t>
+          <t>maa://31694 (99.39)</t>
         </is>
       </c>
       <c r="E29" s="19" t="n"/>
@@ -4248,7 +4248,7 @@
       </c>
       <c r="H29" s="8" t="inlineStr">
         <is>
-          <t>*maa://25175 (52.21)</t>
+          <t>*maa://25175 (51.75)</t>
         </is>
       </c>
       <c r="I29" s="19" t="n"/>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (97.97), maa://31400 (98.13), maa://28440 (86.67)</t>
+          <t>maa://28432 (98.01), maa://31400 (98.13), maa://28440 (86.67)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4280,7 +4280,7 @@
       </c>
       <c r="P29" s="8" t="inlineStr">
         <is>
-          <t>maa://54169 (97.69)</t>
+          <t>maa://54169 (97.74)</t>
         </is>
       </c>
       <c r="Q29" s="19" t="n"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://42865 (92.57)</t>
+          <t>maa://42865 (92.59)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (95.83), maa://64191 (97.78)</t>
+          <t>maa://45792 (95.83), maa://64191 (97.83)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="L30" s="8" t="inlineStr">
         <is>
-          <t>maa://30442 (97.76)</t>
+          <t>maa://30442 (97.78)</t>
         </is>
       </c>
       <c r="M30" s="19" t="n"/>
@@ -4426,7 +4426,7 @@
       </c>
       <c r="T30" s="8" t="inlineStr">
         <is>
-          <t>*maa://32940 (80.00), maa://24388 (96.30)</t>
+          <t>*maa://32940 (76.92), maa://24388 (96.43)</t>
         </is>
       </c>
       <c r="U30" s="19" t="n"/>
@@ -4458,7 +4458,7 @@
       </c>
       <c r="AB30" s="8" t="inlineStr">
         <is>
-          <t>maa://42979 (99.60), maa://45822 (100.00), maa://45045 (93.75)</t>
+          <t>maa://42979 (99.61), maa://45822 (100.00), maa://45045 (93.75)</t>
         </is>
       </c>
       <c r="AC30" s="19" t="n"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (98.22), maa://36258 (93.39), maa://43904 (89.36)</t>
+          <t>maa://35926 (98.26), maa://36258 (93.41), maa://43904 (89.58)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4588,7 +4588,7 @@
       </c>
       <c r="AB31" s="8" t="inlineStr">
         <is>
-          <t>maa://66997 (96.43)</t>
+          <t>maa://66997 (96.55)</t>
         </is>
       </c>
       <c r="AC31" s="19" t="n"/>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://36667 (99.62), maa://21895 (97.99), maa://22760 (100.00)</t>
+          <t>maa://36667 (99.63), maa://21895 (97.99), maa://22760 (100.00)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (99.36), maa://41108 (87.93), maa://41238 (98.17), maa://45523 (100.00)</t>
+          <t>maa://42859 (99.33), maa://41108 (87.93), maa://41238 (98.17), maa://45523 (100.00)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="X32" s="8" t="inlineStr">
         <is>
-          <t>maa://64104 (97.81)</t>
+          <t>maa://64104 (97.84)</t>
         </is>
       </c>
       <c r="Y32" s="19" t="n"/>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (94.79), maa://69135 (97.10)</t>
+          <t>maa://21956 (94.83), maa://69135 (97.78)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="T33" s="8" t="inlineStr">
         <is>
-          <t>maa://45558 (88.57)</t>
+          <t>maa://45558 (88.89)</t>
         </is>
       </c>
       <c r="U33" s="19" t="n"/>
@@ -4898,7 +4898,7 @@
       </c>
       <c r="H34" s="8" t="inlineStr">
         <is>
-          <t>maa://66817 (99.42)</t>
+          <t>maa://66817 (99.44)</t>
         </is>
       </c>
       <c r="I34" s="19" t="n"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (99.29), maa://56235 (99.56)</t>
+          <t>maa://48817 (99.31), maa://56235 (99.58)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="T34" s="8" t="inlineStr">
         <is>
-          <t>maa://24526 (97.34)</t>
+          <t>maa://24526 (97.39)</t>
         </is>
       </c>
       <c r="U34" s="19" t="n"/>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="AB34" s="8" t="inlineStr">
         <is>
-          <t>maa://64329 (98.28)</t>
+          <t>maa://64329 (98.39)</t>
         </is>
       </c>
       <c r="AC34" s="19" t="n"/>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
-          <t>maa://41296 (99.33)</t>
+          <t>maa://41296 (99.34)</t>
         </is>
       </c>
       <c r="M35" s="19" t="n"/>
@@ -5076,7 +5076,7 @@
       </c>
       <c r="T35" s="8" t="inlineStr">
         <is>
-          <t>maa://24842 (96.84)</t>
+          <t>maa://24842 (96.88)</t>
         </is>
       </c>
       <c r="U35" s="19" t="n"/>
@@ -5124,7 +5124,7 @@
       </c>
       <c r="AF35" s="8" t="inlineStr">
         <is>
-          <t>maa://39479 (93.44)</t>
+          <t>maa://39479 (93.55)</t>
         </is>
       </c>
       <c r="AG35" s="16" t="n"/>
@@ -5158,7 +5158,7 @@
       </c>
       <c r="H36" s="8" t="inlineStr">
         <is>
-          <t>maa://24375 (94.74)</t>
+          <t>maa://24375 (94.81)</t>
         </is>
       </c>
       <c r="I36" s="19" t="n"/>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="AB36" s="19" t="inlineStr">
         <is>
-          <t>maa://64106 (97.87)</t>
+          <t>maa://64106 (97.96)</t>
         </is>
       </c>
       <c r="AC36" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (99.08), maa://56336 (99.43), maa://47069 (86.96), maa://45789 (100.00)</t>
+          <t>maa://45718 (99.09), maa://56336 (99.43), maa://47069 (86.96), maa://45789 (100.00)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="P37" s="8" t="inlineStr">
         <is>
-          <t>maa://21280 (97.73)</t>
+          <t>maa://21280 (97.77)</t>
         </is>
       </c>
       <c r="Q37" s="19" t="n"/>
@@ -5418,7 +5418,7 @@
       </c>
       <c r="L38" s="8" t="inlineStr">
         <is>
-          <t>maa://39384 (99.36), maa://49735 (92.86)</t>
+          <t>maa://39384 (99.37), maa://49735 (92.86)</t>
         </is>
       </c>
       <c r="M38" s="19" t="n"/>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="P38" s="8" t="inlineStr">
         <is>
-          <t>maa://24383 (83.17)</t>
+          <t>maa://24383 (83.25)</t>
         </is>
       </c>
       <c r="Q38" s="19" t="n"/>
@@ -5450,7 +5450,7 @@
       </c>
       <c r="T38" s="8" t="inlineStr">
         <is>
-          <t>maa://30713 (98.53)</t>
+          <t>maa://30713 (98.55)</t>
         </is>
       </c>
       <c r="U38" s="19" t="n"/>
@@ -5482,7 +5482,7 @@
       </c>
       <c r="AF38" s="8" t="inlineStr">
         <is>
-          <t>maa://36697 (95.74), maa://68397 (98.29)</t>
+          <t>maa://36697 (95.76), maa://68397 (98.47)</t>
         </is>
       </c>
       <c r="AG38" s="16" t="n"/>
@@ -5516,7 +5516,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://25199 (85.11), maa://45059 (94.53), maa://30434 (95.48), maa://44165 (85.71)</t>
+          <t>maa://25199 (85.11), maa://45059 (94.32), maa://30434 (95.48), maa://44165 (85.71)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5548,7 +5548,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://47093 (98.46), maa://24709 (94.23)</t>
+          <t>maa://47093 (98.50), maa://24709 (94.23)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5564,7 +5564,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (95.83), maa://45790 (88.89)</t>
+          <t>maa://47079 (95.92), maa://45790 (89.02)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5596,7 +5596,7 @@
       </c>
       <c r="AF39" s="8" t="inlineStr">
         <is>
-          <t>maa://62953 (96.98)</t>
+          <t>maa://62953 (97.03)</t>
         </is>
       </c>
       <c r="AG39" s="16" t="n"/>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (98.19), maa://21386 (95.98), maa://36664 (89.74), *maa://45550 (75.00)</t>
+          <t>maa://23278 (98.22), maa://21386 (95.98), maa://36664 (90.00), *maa://45550 (75.00)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5697,7 +5697,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://65283 (96.93), maa://64205 (94.12)</t>
+          <t>maa://65283 (96.98), maa://64205 (94.12)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5718,7 +5718,7 @@
       </c>
       <c r="H41" s="8" t="inlineStr">
         <is>
-          <t>maa://24466 (92.96)</t>
+          <t>maa://24466 (93.06)</t>
         </is>
       </c>
       <c r="I41" s="19" t="n"/>
@@ -5750,7 +5750,7 @@
       </c>
       <c r="P41" s="8" t="inlineStr">
         <is>
-          <t>maa://43177 (95.93)</t>
+          <t>maa://43177 (95.97)</t>
         </is>
       </c>
       <c r="Q41" s="19" t="n"/>
@@ -5920,7 +5920,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>maa://21284 (98.00)</t>
+          <t>maa://21284 (98.04)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -5952,7 +5952,7 @@
       </c>
       <c r="P43" s="8" t="inlineStr">
         <is>
-          <t>maa://47403 (89.47)</t>
+          <t>maa://47403 (89.74)</t>
         </is>
       </c>
       <c r="Q43" s="19" t="n"/>
@@ -6021,7 +6021,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (98.33), maa://56386 (99.48), maa://27728 (96.43)</t>
+          <t>maa://29768 (98.34), maa://56386 (99.49), maa://27728 (96.43)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6069,7 +6069,7 @@
       </c>
       <c r="T44" s="8" t="inlineStr">
         <is>
-          <t>maa://39366 (94.34)</t>
+          <t>maa://39366 (94.44)</t>
         </is>
       </c>
       <c r="U44" s="19" t="n"/>
@@ -6106,7 +6106,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://42459 (98.87), maa://21229 (85.90), maa://30807 (94.62), *maa://22767 (72.00)</t>
+          <t>maa://42459 (98.91), maa://21229 (85.96), maa://30807 (94.62), *maa://22767 (72.37)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6154,7 +6154,7 @@
       </c>
       <c r="T45" s="8" t="inlineStr">
         <is>
-          <t>*maa://39364 (70.00)</t>
+          <t>*maa://39364 (70.65)</t>
         </is>
       </c>
       <c r="U45" s="19" t="n"/>
@@ -6191,7 +6191,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (96.26), maa://43901 (96.60)</t>
+          <t>maa://35931 (96.34), maa://43901 (96.63)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6260,7 +6260,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (97.58), maa://29661 (97.25), maa://56236 (99.81), maa://28038 (84.62)</t>
+          <t>maa://27410 (97.58), maa://56236 (99.82), maa://29661 (97.26), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6292,7 +6292,7 @@
       </c>
       <c r="T47" s="8" t="inlineStr">
         <is>
-          <t>maa://67476 (99.58), maa://68392 (99.54)</t>
+          <t>maa://67476 (99.58), maa://68392 (99.58)</t>
         </is>
       </c>
       <c r="U47" s="19" t="n"/>
@@ -6430,7 +6430,7 @@
       </c>
       <c r="T49" s="19" t="inlineStr">
         <is>
-          <t>maa://67231 (99.23)</t>
+          <t>maa://67231 (99.25)</t>
         </is>
       </c>
       <c r="U49" s="19" t="n"/>
@@ -6467,7 +6467,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>maa://62852 (93.61)</t>
+          <t>maa://62852 (93.71)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6551,7 +6551,7 @@
       </c>
       <c r="H52" s="8" t="inlineStr">
         <is>
-          <t>maa://24376 (99.19)</t>
+          <t>maa://24376 (99.22)</t>
         </is>
       </c>
       <c r="I52" s="19" t="n"/>
@@ -6601,7 +6601,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (98.09)</t>
+          <t>maa://32534 (98.12)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -6701,7 +6701,7 @@
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>maa://32532 (97.96)</t>
+          <t>maa://32532 (97.97)</t>
         </is>
       </c>
       <c r="I55" s="19" t="n"/>
@@ -6753,7 +6753,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://56237 (98.45), maa://25176 (98.78)</t>
+          <t>maa://56237 (98.51), maa://25176 (98.78)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6789,7 +6789,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (98.49), maa://27746 (89.80)</t>
+          <t>maa://31270 (98.51), maa://27746 (89.85)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -6807,7 +6807,7 @@
       </c>
       <c r="H60" s="8" t="inlineStr">
         <is>
-          <t>maa://40438 (92.78)</t>
+          <t>maa://40438 (92.62)</t>
         </is>
       </c>
       <c r="I60" s="19" t="n"/>
@@ -6843,7 +6843,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (96.88), maa://56228 (98.31), maa://43903 (100.00)</t>
+          <t>maa://42981 (96.91), maa://56228 (98.34), maa://43903 (100.00)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6861,7 +6861,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (99.48), *maa://59693 (72.00), maa://59413 (97.73)</t>
+          <t>maa://59534 (99.48), *maa://59693 (72.00), maa://59413 (97.78)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7077,7 +7077,7 @@
       </c>
       <c r="H75" s="19" t="inlineStr">
         <is>
-          <t>maa://67748 (85.48)</t>
+          <t>maa://67748 (85.94)</t>
         </is>
       </c>
       <c r="I75" s="19" t="n"/>
@@ -7219,7 +7219,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.10.16 13:20:24</t>
+          <t>更新日期：2025.10.20 13:21:27</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -7489,7 +7489,7 @@
       </c>
       <c r="D6" s="13" t="inlineStr">
         <is>
-          <t>maa://20925 (81.82)</t>
+          <t>maa://20925 (83.33)</t>
         </is>
       </c>
       <c r="E6" s="14" t="inlineStr">
@@ -8407,7 +8407,7 @@
       </c>
       <c r="D23" s="13" t="inlineStr">
         <is>
-          <t>maa://20876 (96.61), maa://63498 (100.00)</t>
+          <t>maa://20876 (96.72), maa://63498 (100.00)</t>
         </is>
       </c>
       <c r="E23" s="14" t="inlineStr">
@@ -8623,7 +8623,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (73.68), *maa://28758 (72.34), maa://65357 (97.22), maa://29036 (96.77), *maa://42172 (71.43), maa://30285 (100.00)</t>
+          <t>*maa://20849 (73.68), *maa://28758 (72.34), maa://65357 (97.30), maa://29036 (96.77), *maa://42172 (71.43), maa://30285 (100.00)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8731,7 +8731,7 @@
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>maa://20863 (90.61), maa://20832 (99.24), maa://20727 (100.00)</t>
+          <t>maa://20863 (90.65), maa://20832 (99.24), maa://20727 (100.00)</t>
         </is>
       </c>
       <c r="E29" s="14" t="inlineStr">
@@ -8893,7 +8893,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (90.11), maa://36866 (97.06), maa://62759 (100.00), maa://45572 (88.24), maa://27794 (100.00), maa://20960 (100.00), maa://20843 (100.00), **maa://24483 (50.00), *maa://20893 (73.68), maa://20862 (83.33), maa://70680 (100.00)</t>
+          <t>maa://36644 (90.22), maa://36866 (97.10), maa://62759 (100.00), maa://45572 (88.24), maa://27794 (100.00), maa://20960 (100.00), maa://20843 (100.00), **maa://24483 (50.00), *maa://20893 (73.68), maa://20862 (83.33), maa://70680 (100.00)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -9163,7 +9163,7 @@
       </c>
       <c r="D37" s="13" t="inlineStr">
         <is>
-          <t>maa://27376 (90.77), maa://42635 (94.64), *maa://20838 (55.00)</t>
+          <t>maa://27376 (90.77), maa://42635 (94.74), *maa://20838 (55.00)</t>
         </is>
       </c>
       <c r="E37" s="14" t="inlineStr">
@@ -9433,7 +9433,7 @@
       </c>
       <c r="D42" s="13" t="inlineStr">
         <is>
-          <t>maa://34883 (93.75), maa://20918 (96.30), maa://20824 (100.00)</t>
+          <t>maa://34883 (94.12), maa://20918 (96.30), maa://20824 (100.00)</t>
         </is>
       </c>
       <c r="E42" s="14" t="inlineStr">
@@ -10189,7 +10189,7 @@
       </c>
       <c r="D56" s="13" t="inlineStr">
         <is>
-          <t>maa://44235 (98.47), maa://45604 (100.00), maa://20961 (94.44), maa://44220 (100.00), maa://20910 (100.00)</t>
+          <t>maa://44235 (98.47), maa://45604 (100.00), maa://20961 (94.44), maa://20910 (100.00), maa://44220 (100.00)</t>
         </is>
       </c>
       <c r="E56" s="14" t="inlineStr">
@@ -10405,7 +10405,7 @@
       </c>
       <c r="D60" s="13" t="inlineStr">
         <is>
-          <t>maa://38298 (88.39)</t>
+          <t>maa://38298 (88.50)</t>
         </is>
       </c>
       <c r="E60" s="14" t="inlineStr">
@@ -10459,7 +10459,7 @@
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (99.25), maa://31559 (94.00), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00), maa://66633 (100.00)</t>
+          <t>maa://20841 (99.26), maa://31559 (94.00), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00), maa://66633 (100.00)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -10567,7 +10567,7 @@
       </c>
       <c r="D63" s="13" t="inlineStr">
         <is>
-          <t>maa://20844 (97.06)</t>
+          <t>maa://20844 (97.14)</t>
         </is>
       </c>
       <c r="E63" s="14" t="inlineStr">
@@ -10891,7 +10891,7 @@
       </c>
       <c r="D69" s="13" t="inlineStr">
         <is>
-          <t>maa://20976 (98.08), maa://20815 (100.00)</t>
+          <t>maa://20976 (98.31), maa://20815 (100.00)</t>
         </is>
       </c>
       <c r="E69" s="14" t="inlineStr">
@@ -10999,7 +10999,7 @@
       </c>
       <c r="D71" s="13" t="inlineStr">
         <is>
-          <t>maa://20944 (96.36), maa://35393 (100.00)</t>
+          <t>maa://20944 (96.43), maa://35393 (100.00)</t>
         </is>
       </c>
       <c r="E71" s="14" t="inlineStr">
@@ -11107,7 +11107,7 @@
       </c>
       <c r="D73" s="13" t="inlineStr">
         <is>
-          <t>maa://36643 (98.48), maa://36864 (98.11), maa://39140 (100.00), maa://66335 (100.00)</t>
+          <t>maa://36643 (98.49), maa://36864 (98.11), maa://39140 (100.00), maa://66335 (100.00)</t>
         </is>
       </c>
       <c r="E73" s="14" t="inlineStr">
@@ -11377,7 +11377,7 @@
       </c>
       <c r="D78" s="13" t="inlineStr">
         <is>
-          <t>maa://20958 (95.35), ***maa://39769 (20.00)</t>
+          <t>maa://20958 (95.45), ***maa://39769 (20.00)</t>
         </is>
       </c>
       <c r="E78" s="14" t="inlineStr">
@@ -11971,7 +11971,7 @@
       </c>
       <c r="D89" s="13" t="inlineStr">
         <is>
-          <t>maa://24472 (91.17), *maa://35841 (66.67)</t>
+          <t>maa://24472 (91.17), *maa://35841 (68.00)</t>
         </is>
       </c>
       <c r="E89" s="14" t="inlineStr">
@@ -12133,7 +12133,7 @@
       </c>
       <c r="D92" s="13" t="inlineStr">
         <is>
-          <t>maa://24609 (93.33)</t>
+          <t>maa://24609 (93.55)</t>
         </is>
       </c>
       <c r="E92" s="14" t="inlineStr">
@@ -12457,7 +12457,7 @@
       </c>
       <c r="D98" s="13" t="inlineStr">
         <is>
-          <t>maa://20991 (100.00), maa://51015 (88.00)</t>
+          <t>maa://20991 (100.00), maa://51015 (88.24)</t>
         </is>
       </c>
       <c r="E98" s="14" t="inlineStr">
@@ -13051,7 +13051,7 @@
       </c>
       <c r="D109" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.75), maa://25018 (96.96), maa://25776 (92.50), maa://28361 (95.56), maa://25772 (94.12), maa://56588 (93.33), maa://45194 (86.36), maa://32653 (81.25), maa://25161 (84.21), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
+          <t>maa://51881 (98.64), maa://25018 (96.97), maa://25776 (92.50), maa://28361 (95.56), maa://25772 (94.12), maa://56588 (93.55), maa://45194 (86.36), maa://32653 (81.25), maa://25161 (84.21), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E109" s="14" t="inlineStr">
@@ -13105,7 +13105,7 @@
       </c>
       <c r="D110" s="13" t="inlineStr">
         <is>
-          <t>maa://36646 (98.92), maa://25774 (94.59), maa://35996 (98.00), maa://22469 (92.19), maa://30668 (87.10), maa://67286 (100.00)</t>
+          <t>maa://36646 (98.92), maa://25774 (94.67), maa://35996 (98.02), maa://22469 (90.77), maa://30668 (87.10), maa://67286 (100.00)</t>
         </is>
       </c>
       <c r="E110" s="14" t="inlineStr">
@@ -13321,7 +13321,7 @@
       </c>
       <c r="D114" s="13" t="inlineStr">
         <is>
-          <t>maa://20933 (86.96), maa://20822 (100.00)</t>
+          <t>maa://20933 (87.10), maa://20822 (100.00)</t>
         </is>
       </c>
       <c r="E114" s="14" t="inlineStr">
@@ -13483,7 +13483,7 @@
       </c>
       <c r="D117" s="13" t="inlineStr">
         <is>
-          <t>maa://20908 (98.19), maa://35723 (96.08), *maa://23346 (77.78), maa://38822 (100.00), maa://58659 (100.00)</t>
+          <t>maa://20908 (98.21), maa://35723 (96.08), *maa://23346 (77.78), maa://38822 (100.00), maa://58659 (100.00)</t>
         </is>
       </c>
       <c r="E117" s="14" t="inlineStr">
@@ -13807,7 +13807,7 @@
       </c>
       <c r="D123" s="13" t="inlineStr">
         <is>
-          <t>maa://20869 (100.00), maa://44690 (95.92)</t>
+          <t>maa://20869 (100.00), maa://44690 (96.00)</t>
         </is>
       </c>
       <c r="E123" s="14" t="inlineStr">
@@ -13969,7 +13969,7 @@
       </c>
       <c r="D126" s="13" t="inlineStr">
         <is>
-          <t>*maa://20909 (68.18)</t>
+          <t>*maa://20909 (65.22)</t>
         </is>
       </c>
       <c r="E126" s="14" t="inlineStr">
@@ -14941,7 +14941,7 @@
       </c>
       <c r="D144" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (97.94), *maa://23736 (53.49), maa://31185 (92.31), maa://30306 (100.00)</t>
+          <t>maa://28484 (97.96), *maa://23736 (53.49), maa://31185 (92.31), maa://30306 (100.00)</t>
         </is>
       </c>
       <c r="E144" s="14" t="inlineStr">
@@ -15319,7 +15319,7 @@
       </c>
       <c r="D151" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.79), maa://36641 (98.25), maa://36865 (95.48), maa://44635 (88.18), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (100.00), maa://42918 (100.00), maa://44119 (97.44), maa://64408 (93.75), maa://37300 (100.00), maa://42917 (100.00)</t>
+          <t>maa://40957 (94.81), maa://36641 (98.25), maa://36865 (95.48), maa://44635 (88.18), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (100.00), maa://42918 (100.00), maa://44119 (97.44), maa://64408 (94.12), maa://37300 (100.00), maa://42917 (100.00)</t>
         </is>
       </c>
       <c r="E151" s="14" t="inlineStr">
@@ -15373,7 +15373,7 @@
       </c>
       <c r="D152" s="13" t="inlineStr">
         <is>
-          <t>maa://51549 (95.71), maa://51923 (96.43), *maa://67508 (75.00)</t>
+          <t>maa://51549 (95.77), maa://51923 (96.55), *maa://67508 (60.00)</t>
         </is>
       </c>
       <c r="E152" s="14" t="inlineStr">
@@ -15854,12 +15854,12 @@
       </c>
       <c r="C161" s="12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D161" s="13" t="inlineStr">
         <is>
-          <t>maa://44232 (98.49), maa://45603 (90.62), maa://65963 (83.33), *maa://63114 (66.67)</t>
+          <t>maa://44232 (98.50), maa://45603 (90.62), maa://65963 (83.33), *maa://63114 (66.67), maa://71762 (100.00)</t>
         </is>
       </c>
       <c r="E161" s="14" t="inlineStr">
@@ -16237,7 +16237,7 @@
       </c>
       <c r="D168" s="13" t="inlineStr">
         <is>
-          <t>maa://20975 (91.67), maa://47950 (90.00), maa://30806 (100.00)</t>
+          <t>maa://20975 (91.67), maa://47950 (90.91), maa://30806 (100.00)</t>
         </is>
       </c>
       <c r="E168" s="14" t="inlineStr">
@@ -16345,7 +16345,7 @@
       </c>
       <c r="D170" s="13" t="inlineStr">
         <is>
-          <t>maa://49867 (94.12), maa://49655 (97.83)</t>
+          <t>maa://49867 (94.25), maa://49655 (97.83)</t>
         </is>
       </c>
       <c r="E170" s="14" t="inlineStr">
@@ -16777,7 +16777,7 @@
       </c>
       <c r="D178" s="13" t="inlineStr">
         <is>
-          <t>maa://37690 (93.75)</t>
+          <t>maa://37690 (94.12)</t>
         </is>
       </c>
       <c r="E178" s="14" t="inlineStr">
@@ -17533,7 +17533,7 @@
       </c>
       <c r="D192" s="13" t="inlineStr">
         <is>
-          <t>maa://34866 (94.00), maa://34714 (96.97)</t>
+          <t>maa://34866 (94.12), maa://34714 (96.97)</t>
         </is>
       </c>
       <c r="E192" s="14" t="inlineStr">
@@ -17587,7 +17587,7 @@
       </c>
       <c r="D193" s="13" t="inlineStr">
         <is>
-          <t>maa://34883 (93.75), maa://20895 (100.00)</t>
+          <t>maa://34883 (94.12), maa://20895 (100.00)</t>
         </is>
       </c>
       <c r="E193" s="14" t="inlineStr">
@@ -17911,7 +17911,7 @@
       </c>
       <c r="D199" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.50), maa://35854 (84.75), maa://50388 (98.26), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (95.92), maa://70161 (100.00)</t>
+          <t>maa://44224 (90.52), maa://35854 (84.75), maa://50388 (98.26), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (95.92), maa://70161 (100.00)</t>
         </is>
       </c>
       <c r="E199" s="14" t="inlineStr">
@@ -18019,7 +18019,7 @@
       </c>
       <c r="D201" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (86.46), *maa://28190 (64.86), maa://22894 (91.89), *maa://20906 (72.22), **maa://20907 (34.38)</t>
+          <t>maa://27823 (86.60), *maa://28190 (64.86), maa://22894 (91.89), *maa://20906 (72.22), **maa://20907 (34.38)</t>
         </is>
       </c>
       <c r="E201" s="14" t="inlineStr">
@@ -18073,7 +18073,7 @@
       </c>
       <c r="D202" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (86.46), *maa://28190 (64.86), maa://22894 (91.89), *maa://20906 (72.22), **maa://20907 (34.38)</t>
+          <t>maa://27823 (86.60), *maa://28190 (64.86), maa://22894 (91.89), *maa://20906 (72.22), **maa://20907 (34.38)</t>
         </is>
       </c>
       <c r="E202" s="14" t="inlineStr">
@@ -18613,7 +18613,7 @@
       </c>
       <c r="D212" s="13" t="inlineStr">
         <is>
-          <t>maa://28133 (93.55), **maa://39217 (38.89), maa://25369 (95.24)</t>
+          <t>maa://28133 (93.65), **maa://39217 (36.84), maa://25369 (95.24)</t>
         </is>
       </c>
       <c r="E212" s="14" t="inlineStr">
@@ -20125,7 +20125,7 @@
       </c>
       <c r="D240" s="13" t="inlineStr">
         <is>
-          <t>maa://30714 (97.83), maa://30675 (100.00)</t>
+          <t>maa://30714 (97.87), maa://30675 (100.00)</t>
         </is>
       </c>
       <c r="E240" s="14" t="inlineStr">
@@ -20827,7 +20827,7 @@
       </c>
       <c r="D253" s="13" t="inlineStr">
         <is>
-          <t>maa://42287 (93.29), maa://45570 (96.92), maa://60678 (90.91), maa://42225 (100.00)</t>
+          <t>maa://42287 (92.99), maa://45570 (96.92), maa://60678 (91.67), maa://42225 (94.12)</t>
         </is>
       </c>
       <c r="E253" s="14" t="inlineStr">
@@ -21205,7 +21205,7 @@
       </c>
       <c r="D260" s="13" t="inlineStr">
         <is>
-          <t>maa://20879 (85.85), maa://20834 (92.86)</t>
+          <t>maa://20879 (85.98), maa://20834 (92.86)</t>
         </is>
       </c>
       <c r="E260" s="14" t="inlineStr">
@@ -21961,7 +21961,7 @@
       </c>
       <c r="D274" s="13" t="inlineStr">
         <is>
-          <t>maa://25769 (96.97)</t>
+          <t>maa://25769 (96.99)</t>
         </is>
       </c>
       <c r="E274" s="14" t="inlineStr">
@@ -22015,7 +22015,7 @@
       </c>
       <c r="D275" s="13" t="inlineStr">
         <is>
-          <t>**maa://62757 (42.86), maa://67819 (100.00)</t>
+          <t>**maa://62757 (44.44), maa://67819 (100.00)</t>
         </is>
       </c>
       <c r="E275" s="14" t="inlineStr">
@@ -22123,7 +22123,7 @@
       </c>
       <c r="D277" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.75), maa://51630 (96.33), maa://56588 (93.33), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (41.67), maa://66758 (83.33)</t>
+          <t>maa://51881 (98.64), maa://51630 (96.36), maa://56588 (93.55), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (41.67), *maa://66758 (76.92)</t>
         </is>
       </c>
       <c r="E277" s="14" t="inlineStr">
@@ -22393,7 +22393,7 @@
       </c>
       <c r="D282" s="13" t="inlineStr">
         <is>
-          <t>maa://28133 (93.55), maa://33394 (100.00)</t>
+          <t>maa://28133 (93.65), maa://33394 (100.00)</t>
         </is>
       </c>
       <c r="E282" s="14" t="inlineStr">
@@ -22879,7 +22879,7 @@
       </c>
       <c r="D291" s="13" t="inlineStr">
         <is>
-          <t>maa://20899 (90.11), maa://46332 (93.10), ***maa://44744 (25.00)</t>
+          <t>maa://20899 (90.16), maa://46332 (93.10), ***maa://44744 (25.00)</t>
         </is>
       </c>
       <c r="E291" s="14" t="inlineStr">
@@ -23041,7 +23041,7 @@
       </c>
       <c r="D294" s="13" t="inlineStr">
         <is>
-          <t>maa://30710 (97.96), maa://36845 (95.92), maa://31558 (97.22), **maa://39217 (38.89), maa://30668 (87.10)</t>
+          <t>maa://30710 (97.96), maa://36845 (95.92), maa://31558 (97.22), **maa://39217 (36.84), maa://30668 (87.10)</t>
         </is>
       </c>
       <c r="E294" s="14" t="inlineStr">
@@ -23203,7 +23203,7 @@
       </c>
       <c r="D297" s="13" t="inlineStr">
         <is>
-          <t>maa://25774 (94.59), maa://28133 (93.55), maa://22469 (92.19), **maa://39217 (38.89), **maa://31349 (50.00)</t>
+          <t>maa://25774 (94.67), maa://28133 (93.65), maa://22469 (90.77), **maa://39217 (36.84), **maa://31349 (50.00)</t>
         </is>
       </c>
       <c r="E297" s="14" t="inlineStr">
@@ -23797,7 +23797,7 @@
       </c>
       <c r="D308" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (98.52), maa://49642 (97.67), maa://49660 (93.62), maa://50517 (85.71), maa://70004 (100.00)</t>
+          <t>maa://50280 (98.52), maa://49642 (97.67), maa://49660 (93.62), maa://70004 (100.00), maa://50517 (85.71)</t>
         </is>
       </c>
       <c r="E308" s="14" t="inlineStr">
@@ -24499,7 +24499,7 @@
       </c>
       <c r="D321" s="13" t="inlineStr">
         <is>
-          <t>maa://25367 (99.38)</t>
+          <t>maa://25367 (99.39)</t>
         </is>
       </c>
       <c r="E321" s="14" t="inlineStr">
@@ -24553,7 +24553,7 @@
       </c>
       <c r="D322" s="13" t="inlineStr">
         <is>
-          <t>*maa://62755 (78.26), maa://62761 (88.24)</t>
+          <t>*maa://62755 (78.26), maa://62761 (88.89)</t>
         </is>
       </c>
       <c r="E322" s="14" t="inlineStr">
@@ -24877,7 +24877,7 @@
       </c>
       <c r="D328" s="13" t="inlineStr">
         <is>
-          <t>maa://39692 (99.55), maa://39810 (90.91)</t>
+          <t>maa://39692 (99.56), maa://39810 (90.91)</t>
         </is>
       </c>
       <c r="E328" s="14" t="inlineStr">
@@ -24931,7 +24931,7 @@
       </c>
       <c r="D329" s="13" t="inlineStr">
         <is>
-          <t>*maa://39174 (75.00)</t>
+          <t>*maa://39174 (80.00)</t>
         </is>
       </c>
       <c r="E329" s="14" t="inlineStr">
@@ -25255,7 +25255,7 @@
       </c>
       <c r="D335" s="15" t="inlineStr">
         <is>
-          <t>maa://40956 (94.23)</t>
+          <t>maa://40956 (94.29)</t>
         </is>
       </c>
       <c r="E335" s="15" t="inlineStr">
@@ -25579,7 +25579,7 @@
       </c>
       <c r="D341" s="22" t="inlineStr">
         <is>
-          <t>maa://44234 (99.20)</t>
+          <t>maa://44234 (99.21)</t>
         </is>
       </c>
       <c r="E341" s="22" t="inlineStr">
@@ -25687,7 +25687,7 @@
       </c>
       <c r="D343" s="22" t="inlineStr">
         <is>
-          <t>maa://67275 (100.00), *maa://69909 (60.00)</t>
+          <t>maa://67275 (100.00), *maa://69909 (57.14)</t>
         </is>
       </c>
       <c r="E343" s="22" t="inlineStr">
@@ -25849,7 +25849,7 @@
       </c>
       <c r="D346" s="22" t="inlineStr">
         <is>
-          <t>maa://30671 (81.59), maa://30669 (99.32), maa://37275 (81.40), *maa://32410 (61.54), maa://41605 (100.00)</t>
+          <t>maa://30671 (81.59), maa://30669 (99.33), maa://37275 (81.40), *maa://32410 (61.54), maa://41605 (100.00)</t>
         </is>
       </c>
       <c r="E346" s="22" t="inlineStr">
@@ -25957,7 +25957,7 @@
       </c>
       <c r="D348" s="22" t="inlineStr">
         <is>
-          <t>maa://38295 (95.41), maa://49332 (91.67)</t>
+          <t>maa://38295 (95.45), maa://49332 (91.67)</t>
         </is>
       </c>
       <c r="E348" s="22" t="inlineStr">
@@ -26713,7 +26713,7 @@
       </c>
       <c r="D362" s="22" t="inlineStr">
         <is>
-          <t>maa://36868 (99.38), maa://35996 (98.00), maa://47349 (97.70), **maa://39217 (38.89), maa://71203 (100.00)</t>
+          <t>maa://36868 (99.38), maa://35996 (98.02), maa://47349 (97.83), **maa://39217 (36.84), *maa://71203 (75.00)</t>
         </is>
       </c>
       <c r="E362" s="22" t="inlineStr">
@@ -26767,7 +26767,7 @@
       </c>
       <c r="D363" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.60), maa://49695 (100.00), maa://49758 (98.82), *maa://52357 (77.78), *maa://59402 (58.06), *maa://63091 (66.67)</t>
+          <t>maa://49696 (99.60), maa://49695 (100.00), maa://49758 (98.84), *maa://52357 (77.78), *maa://59402 (58.06), *maa://63091 (66.67)</t>
         </is>
       </c>
       <c r="E363" s="22" t="inlineStr">
@@ -26978,12 +26978,12 @@
       </c>
       <c r="C367" s="12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D367" s="22" t="inlineStr">
         <is>
-          <t>maa://36646 (98.92), maa://36845 (95.92), **maa://39217 (38.89), maa://51007 (98.33), maa://70752 (100.00)</t>
+          <t>maa://36646 (98.92), maa://36845 (95.92), **maa://39217 (36.84), maa://51007 (98.33), maa://70752 (100.00), maa://71932 (100.00)</t>
         </is>
       </c>
       <c r="E367" s="22" t="inlineStr">
@@ -27091,7 +27091,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://42635 (94.64), maa://50629 (85.71), maa://48859 (100.00)</t>
+          <t>maa://42635 (94.74), maa://50629 (85.71), maa://48859 (100.00)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -27253,7 +27253,7 @@
       </c>
       <c r="D372" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (94.79), maa://48026 (94.70), maa://44635 (88.18), maa://41035 (93.59), *maa://60251 (76.47), maa://44660 (92.68), maa://41128 (84.21)</t>
+          <t>maa://40957 (94.81), maa://48026 (94.70), maa://44635 (88.18), maa://41035 (93.59), *maa://60251 (76.47), maa://44660 (92.68), maa://41128 (84.21)</t>
         </is>
       </c>
       <c r="E372" s="22" t="inlineStr">
@@ -27361,7 +27361,7 @@
       </c>
       <c r="D374" s="22" t="inlineStr">
         <is>
-          <t>maa://63883 (100.00), maa://64045 (100.00), maa://64041 (83.33)</t>
+          <t>maa://63883 (97.62), maa://64045 (100.00), maa://64041 (83.33)</t>
         </is>
       </c>
       <c r="E374" s="22" t="inlineStr">
@@ -27415,7 +27415,7 @@
       </c>
       <c r="D375" s="22" t="inlineStr">
         <is>
-          <t>maa://48268 (93.33)</t>
+          <t>maa://48268 (93.75)</t>
         </is>
       </c>
       <c r="E375" s="22" t="inlineStr">
@@ -27523,7 +27523,7 @@
       </c>
       <c r="D377" s="22" t="inlineStr">
         <is>
-          <t>maa://70756 (97.37), maa://71182 (91.30), maa://71524 (100.00)</t>
+          <t>maa://71182 (96.36), maa://70756 (97.62), maa://71524 (100.00)</t>
         </is>
       </c>
       <c r="E377" s="22" t="inlineStr">
@@ -28063,7 +28063,7 @@
       </c>
       <c r="D387" s="22" t="inlineStr">
         <is>
-          <t>maa://43872 (93.75)</t>
+          <t>maa://43872 (94.12)</t>
         </is>
       </c>
       <c r="E387" s="22" t="inlineStr">
@@ -28225,7 +28225,7 @@
       </c>
       <c r="D390" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (80.78), maa://44745 (98.12), **maa://49516 (37.93), *maa://45952 (57.14), ***maa://46851 (10.00), *maa://44896 (80.00)</t>
+          <t>maa://42970 (80.85), maa://44745 (98.13), **maa://49516 (37.93), *maa://45952 (57.14), ***maa://46851 (10.00), *maa://44896 (80.00)</t>
         </is>
       </c>
       <c r="E390" s="22" t="inlineStr">
@@ -28468,7 +28468,7 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>maa://63890 (98.15), maa://64043 (100.00)</t>
+          <t>maa://63890 (98.18), maa://64043 (100.00)</t>
         </is>
       </c>
       <c r="E396" t="inlineStr">
@@ -28522,7 +28522,7 @@
       </c>
       <c r="D398" t="inlineStr">
         <is>
-          <t>maa://47023 (87.72)</t>
+          <t>maa://47023 (87.93)</t>
         </is>
       </c>
       <c r="E398" t="inlineStr">
@@ -28603,7 +28603,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>maa://59533 (98.04), maa://59577 (100.00)</t>
+          <t>maa://59533 (96.15), maa://59577 (100.00)</t>
         </is>
       </c>
       <c r="E401" t="inlineStr">
@@ -28711,7 +28711,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>maa://51880 (99.28), maa://56651 (100.00), maa://51878 (100.00)</t>
+          <t>maa://51880 (99.29), maa://56651 (100.00), maa://51878 (100.00)</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">
@@ -28738,7 +28738,7 @@
       </c>
       <c r="D406" t="inlineStr">
         <is>
-          <t>maa://51872 (96.43), maa://51876 (99.09), maa://63228 (88.57), maa://51873 (98.00), maa://62047 (90.32)</t>
+          <t>maa://51872 (96.44), maa://51876 (99.11), maa://63228 (86.11), maa://51873 (98.00), maa://62047 (90.32)</t>
         </is>
       </c>
       <c r="E406" t="inlineStr">
@@ -28792,7 +28792,7 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>maa://60449 (98.47), maa://59493 (96.90)</t>
+          <t>maa://60449 (98.52), maa://59493 (96.90)</t>
         </is>
       </c>
       <c r="E408" t="inlineStr">
@@ -28900,7 +28900,7 @@
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>maa://64040 (99.08), maa://52505 (97.58), maa://66377 (93.75), ***maa://66376 (14.29), ***maa://70187 (11.11)</t>
+          <t>maa://64040 (99.11), maa://52505 (97.77), maa://66377 (94.44), ***maa://66376 (14.29), ***maa://70187 (10.00)</t>
         </is>
       </c>
       <c r="E412" t="inlineStr">
@@ -28927,7 +28927,7 @@
       </c>
       <c r="D413" t="inlineStr">
         <is>
-          <t>maa://67090 (91.30)</t>
+          <t>maa://67090 (91.84)</t>
         </is>
       </c>
       <c r="E413" t="inlineStr">
@@ -28954,7 +28954,7 @@
       </c>
       <c r="D414" t="inlineStr">
         <is>
-          <t>maa://67388 (89.83), *maa://71184 (75.00)</t>
+          <t>maa://67388 (90.00), maa://71184 (85.71)</t>
         </is>
       </c>
       <c r="E414" t="inlineStr">
@@ -28981,7 +28981,7 @@
       </c>
       <c r="D415" t="inlineStr">
         <is>
-          <t>maa://67089 (96.08), maa://67271 (95.24)</t>
+          <t>maa://67089 (96.23), maa://67271 (95.45)</t>
         </is>
       </c>
       <c r="E415" t="inlineStr">
@@ -29008,7 +29008,7 @@
       </c>
       <c r="D416" t="inlineStr">
         <is>
-          <t>maa://67088 (93.15)</t>
+          <t>maa://67088 (93.42)</t>
         </is>
       </c>
       <c r="E416" t="inlineStr">
@@ -29035,7 +29035,7 @@
       </c>
       <c r="D417" t="inlineStr">
         <is>
-          <t>maa://67087 (95.28), maa://67268 (97.25), maa://67269 (85.00), maa://67648 (100.00)</t>
+          <t>maa://67087 (95.83), maa://67268 (97.39), maa://67269 (86.36), maa://67648 (100.00)</t>
         </is>
       </c>
       <c r="E417" t="inlineStr">
@@ -29116,7 +29116,7 @@
       </c>
       <c r="D420" t="inlineStr">
         <is>
-          <t>maa://70877 (96.88)</t>
+          <t>maa://70877 (97.73)</t>
         </is>
       </c>
       <c r="E420" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#248)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -712,7 +712,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (98.49), maa://24702 (95.15), maa://36681 (85.39)</t>
+          <t>maa://25390 (98.60), maa://24702 (95.21), maa://36681 (85.71)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -744,7 +744,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://58660 (98.88), maa://39402 (95.02), *maa://34787 (74.26)</t>
+          <t>maa://58660 (98.98), maa://39402 (95.27), *maa://34787 (74.76)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -776,7 +776,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (97.51), maa://66635 (99.51)</t>
+          <t>maa://22742 (97.64), maa://66635 (99.34)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -808,7 +808,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://36684 (98.45), maa://21246 (91.40)</t>
+          <t>maa://36684 (98.53), maa://21246 (91.11)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -842,7 +842,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (99.42), maa://36987 (97.22), maa://39849 (92.86)</t>
+          <t>maa://40192 (99.42), maa://36987 (97.30), maa://39849 (92.86)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -858,7 +858,7 @@
       </c>
       <c r="H3" s="8" t="inlineStr">
         <is>
-          <t>maa://21247 (99.45)</t>
+          <t>maa://21247 (99.49)</t>
         </is>
       </c>
       <c r="I3" s="19" t="n"/>
@@ -874,7 +874,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>maa://22880 (91.88), maa://20276 (94.24), maa://22749 (85.71)</t>
+          <t>maa://22880 (92.57), maa://20276 (94.30), maa://22749 (85.71)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -890,7 +890,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (98.59), maa://26254 (98.25), *maa://22738 (80.00)</t>
+          <t>maa://21249 (98.70), maa://26254 (96.55), *maa://22738 (80.00)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://60545 (98.91), maa://45854 (87.95), maa://24617 (91.18)</t>
+          <t>maa://60545 (98.94), maa://45854 (88.51), maa://24617 (91.18)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -922,7 +922,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (93.03), maa://27484 (99.25), maa://27480 (86.44)</t>
+          <t>maa://27396 (93.61), maa://27484 (99.29), maa://27480 (86.89)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -938,7 +938,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://52241 (99.48), maa://24390 (96.90)</t>
+          <t>maa://52241 (99.51), maa://24390 (96.99)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -954,7 +954,7 @@
       </c>
       <c r="AF3" s="8" t="inlineStr">
         <is>
-          <t>maa://21289 (91.94)</t>
+          <t>maa://21289 (92.31)</t>
         </is>
       </c>
       <c r="AG3" s="16" t="n"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (98.28), maa://22499 (90.00), maa://22746 (100.00)</t>
+          <t>maa://24632 (98.41), maa://22499 (90.48), maa://22746 (100.00)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (99.22), maa://50121 (96.60)</t>
+          <t>maa://49983 (99.28), maa://50121 (96.67)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://27295 (97.94), maa://32509 (96.73), maa://31008 (95.41), maa://22754 (88.16), maa://70489 (100.00)</t>
+          <t>maa://27295 (98.07), maa://32509 (96.89), maa://31008 (95.02), maa://22754 (88.16), maa://70489 (100.00)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="X4" s="8" t="inlineStr">
         <is>
-          <t>maa://43217 (98.95)</t>
+          <t>maa://43217 (98.89)</t>
         </is>
       </c>
       <c r="Y4" s="19" t="n"/>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="AB4" s="8" t="inlineStr">
         <is>
-          <t>*maa://32658 (79.59)</t>
+          <t>*maa://32658 (76.92)</t>
         </is>
       </c>
       <c r="AC4" s="19" t="n"/>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>*maa://39394 (55.77), *maa://30062 (61.29), ***maa://26209 (13.04)</t>
+          <t>*maa://39394 (54.72), *maa://30062 (60.32), ***maa://26209 (12.50)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (91.74), maa://54105 (98.51), *maa://22744 (80.00)</t>
+          <t>maa://21245 (91.98), maa://54105 (98.67), *maa://22744 (80.00)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="L5" s="8" t="inlineStr">
         <is>
-          <t>maa://22757 (91.53)</t>
+          <t>maa://22757 (92.19)</t>
         </is>
       </c>
       <c r="M5" s="19" t="n"/>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="P5" s="8" t="inlineStr">
         <is>
-          <t>maa://21919 (98.77), maa://21281 (83.33)</t>
+          <t>maa://21919 (98.81), maa://21281 (83.33)</t>
         </is>
       </c>
       <c r="Q5" s="19" t="n"/>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="X5" s="8" t="inlineStr">
         <is>
-          <t>maa://21290 (98.68)</t>
+          <t>maa://21290 (98.72)</t>
         </is>
       </c>
       <c r="Y5" s="19" t="n"/>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="AB5" s="8" t="inlineStr">
         <is>
-          <t>*maa://29863 (60.00), ***maa://22752 (12.50), **maa://26013 (38.46)</t>
+          <t>*maa://29863 (60.78), ***maa://22752 (12.50), **maa://26013 (38.46)</t>
         </is>
       </c>
       <c r="AC5" s="19" t="n"/>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="D6" s="8" t="inlineStr">
         <is>
-          <t>maa://42407 (97.77)</t>
+          <t>maa://42407 (97.91)</t>
         </is>
       </c>
       <c r="E6" s="19" t="n"/>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="H6" s="8" t="inlineStr">
         <is>
-          <t>maa://24370 (97.83)</t>
+          <t>maa://24370 (97.90)</t>
         </is>
       </c>
       <c r="I6" s="19" t="n"/>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="L6" s="8" t="inlineStr">
         <is>
-          <t>maa://24839 (99.50)</t>
+          <t>maa://24839 (99.54)</t>
         </is>
       </c>
       <c r="M6" s="19" t="n"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (98.97), maa://30381 (95.24)</t>
+          <t>maa://31836 (99.03), maa://30381 (95.24)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="T6" s="8" t="inlineStr">
         <is>
-          <t>*maa://37411 (78.57)</t>
+          <t>*maa://37411 (79.07)</t>
         </is>
       </c>
       <c r="U6" s="19" t="n"/>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="X6" s="8" t="inlineStr">
         <is>
-          <t>maa://52754 (96.89), maa://71825 (100.00)</t>
+          <t>maa://52754 (96.45), maa://71825 (100.00)</t>
         </is>
       </c>
       <c r="Y6" s="19" t="n"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="AF6" s="8" t="inlineStr">
         <is>
-          <t>maa://33152 (81.94)</t>
+          <t>maa://33152 (83.03)</t>
         </is>
       </c>
       <c r="AG6" s="16" t="n"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>maa://21955 (98.36)</t>
+          <t>maa://21955 (98.49)</t>
         </is>
       </c>
       <c r="E7" s="19" t="n"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>*maa://22763 (76.19), maa://64972 (96.15)</t>
+          <t>*maa://22763 (76.56), maa://64972 (96.55)</t>
         </is>
       </c>
       <c r="I7" s="19" t="n"/>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (98.73), maa://24957 (94.55)</t>
+          <t>maa://28624 (98.76), maa://24957 (94.55)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="P7" s="8" t="inlineStr">
         <is>
-          <t>maa://22750 (97.22)</t>
+          <t>maa://22750 (97.33)</t>
         </is>
       </c>
       <c r="Q7" s="19" t="n"/>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="T7" s="8" t="inlineStr">
         <is>
-          <t>maa://21291 (93.96)</t>
+          <t>maa://21291 (94.12)</t>
         </is>
       </c>
       <c r="U7" s="19" t="n"/>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (97.53), maa://22758 (82.86)</t>
+          <t>maa://22399 (97.68), maa://22758 (83.64)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1474,12 +1474,12 @@
       </c>
       <c r="AE7" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="AF7" s="8" t="inlineStr">
         <is>
-          <t>maa://45272 (99.52)</t>
+          <t>maa://45272 (99.56), *maa://26191 (70.10)</t>
         </is>
       </c>
       <c r="AG7" s="16" t="n"/>
@@ -1487,7 +1487,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.10.20 13:21:27</t>
+          <t>更新日期：2025.10.31 13:21:33</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (90.50)</t>
+          <t>maa://21476 (91.35)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
-          <t>maa://24371 (80.86)</t>
+          <t>maa://24371 (81.74)</t>
         </is>
       </c>
       <c r="I8" s="19" t="n"/>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (91.93), maa://23252 (91.67), maa://37496 (98.39)</t>
+          <t>maa://32931 (92.01), maa://23252 (91.67), maa://37496 (98.44)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (96.06), maa://67587 (98.46)</t>
+          <t>maa://21411 (96.11), maa://67587 (98.41)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="AB8" s="8" t="inlineStr">
         <is>
-          <t>maa://25389 (95.20)</t>
+          <t>maa://25389 (95.42)</t>
         </is>
       </c>
       <c r="AC8" s="19" t="n"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>maa://24479 (86.18), **maa://21990 (50.00)</t>
+          <t>maa://24479 (86.96), **maa://21990 (50.00)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>maa://22765 (96.15), *maa://21915 (80.00)</t>
+          <t>maa://22765 (96.44), maa://21915 (81.63)</t>
         </is>
       </c>
       <c r="E9" s="19" t="n"/>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="H9" s="8" t="inlineStr">
         <is>
-          <t>*maa://47450 (79.17), maa://56348 (95.24)</t>
+          <t>*maa://47450 (80.00), maa://56348 (95.83)</t>
         </is>
       </c>
       <c r="I9" s="19" t="n"/>
@@ -1664,7 +1664,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (96.49), maa://39552 (87.50)</t>
+          <t>maa://22762 (96.10), maa://39552 (88.89)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="T9" s="8" t="inlineStr">
         <is>
-          <t>maa://26222 (99.53)</t>
+          <t>maa://26222 (99.57)</t>
         </is>
       </c>
       <c r="U9" s="19" t="n"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://52237 (99.80), maa://26223 (98.31)</t>
+          <t>maa://52237 (99.82), maa://26223 (98.31)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (95.22), maa://40166 (95.16)</t>
+          <t>maa://28711 (95.34), maa://40166 (95.31)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (91.51), maa://66916 (98.41)</t>
+          <t>maa://26206 (91.58), maa://66916 (98.55)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>maa://54000 (92.08)</t>
+          <t>maa://54000 (92.59)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="H10" s="8" t="inlineStr">
         <is>
-          <t>maa://32651 (95.65)</t>
+          <t>maa://32651 (95.74)</t>
         </is>
       </c>
       <c r="I10" s="19" t="n"/>
@@ -1794,7 +1794,7 @@
       </c>
       <c r="L10" s="8" t="inlineStr">
         <is>
-          <t>**maa://24395 (41.67)</t>
+          <t>**maa://24395 (44.00)</t>
         </is>
       </c>
       <c r="M10" s="19" t="n"/>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (92.60), *maa://36669 (75.00)</t>
+          <t>maa://28977 (92.90), *maa://36669 (75.00)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (99.30), maa://22755 (91.80), maa://63521 (94.64)</t>
+          <t>maa://27395 (99.32), maa://22755 (91.80), maa://63521 (95.05)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://45828 (99.34), maa://22301 (97.65), maa://22726 (100.00)</t>
+          <t>maa://45828 (99.38), maa://22301 (97.66), maa://22726 (100.00)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>*maa://25021 (58.82), *maa://22733 (66.67), **maa://22761 (33.33)</t>
+          <t>*maa://25021 (59.20), *maa://22733 (68.06), ***maa://22761 (25.00)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="D11" s="8" t="inlineStr">
         <is>
-          <t>maa://36707 (99.66)</t>
+          <t>maa://36707 (99.67)</t>
         </is>
       </c>
       <c r="E11" s="19" t="n"/>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="L11" s="8" t="inlineStr">
         <is>
-          <t>maa://21287 (94.02)</t>
+          <t>maa://21287 (94.08)</t>
         </is>
       </c>
       <c r="M11" s="19" t="n"/>
@@ -1940,7 +1940,7 @@
       </c>
       <c r="P11" s="8" t="inlineStr">
         <is>
-          <t>maa://45557 (94.92)</t>
+          <t>maa://45557 (95.08)</t>
         </is>
       </c>
       <c r="Q11" s="19" t="n"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (93.72), maa://22501 (99.57), maa://64808 (100.00), maa://45521 (95.31)</t>
+          <t>maa://22747 (94.13), maa://22501 (99.58), maa://64808 (100.00), maa://45521 (94.03)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="X11" s="8" t="inlineStr">
         <is>
-          <t>maa://36713 (99.30)</t>
+          <t>maa://36713 (99.34)</t>
         </is>
       </c>
       <c r="Y11" s="19" t="n"/>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="AB11" s="8" t="inlineStr">
         <is>
-          <t>maa://29912 (99.73), maa://22516 (86.52)</t>
+          <t>maa://29912 (99.74), maa://22516 (86.52)</t>
         </is>
       </c>
       <c r="AC11" s="19" t="n"/>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="AF11" s="8" t="inlineStr">
         <is>
-          <t>maa://31203 (98.77)</t>
+          <t>maa://31203 (98.85)</t>
         </is>
       </c>
       <c r="AG11" s="16" t="n"/>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>maa://36678 (97.33), maa://30766 (91.43)</t>
+          <t>maa://36678 (97.47), maa://30766 (91.67)</t>
         </is>
       </c>
       <c r="E12" s="19" t="n"/>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (93.75), maa://54294 (97.24)</t>
+          <t>maa://21867 (93.84), maa://54294 (97.31)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (98.16), maa://64046 (98.66)</t>
+          <t>maa://63896 (98.21), maa://64046 (98.72)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="P12" s="8" t="inlineStr">
         <is>
-          <t>maa://57541 (90.48)</t>
+          <t>maa://57541 (88.89)</t>
         </is>
       </c>
       <c r="Q12" s="19" t="n"/>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://37962 (98.92), maa://21485 (82.52), maa://22753 (92.95)</t>
+          <t>maa://37962 (98.77), maa://21485 (82.73), maa://22753 (93.09)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://36677 (99.15), maa://23669 (94.86), maa://39872 (98.56)</t>
+          <t>maa://36677 (99.21), maa://23669 (94.91), maa://39872 (98.64)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>maa://28932 (94.80)</t>
+          <t>maa://28932 (94.87)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (96.99), maa://36673 (94.48), maa://25001 (89.01)</t>
+          <t>maa://24999 (97.13), maa://36673 (94.67), maa://25001 (89.47)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (73.27), maa://66545 (98.67)</t>
+          <t>*maa://21248 (73.79), maa://66545 (98.73)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (97.94), maa://22583 (89.33), *maa://22500 (71.64)</t>
+          <t>maa://22676 (97.65), maa://22583 (90.26), *maa://22500 (71.64)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="X13" s="8" t="inlineStr">
         <is>
-          <t>maa://34957 (94.80)</t>
+          <t>maa://34957 (94.99)</t>
         </is>
       </c>
       <c r="Y13" s="19" t="n"/>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (94.08)</t>
+          <t>maa://39883 (94.42)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2282,7 +2282,7 @@
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>maa://30764 (94.81)</t>
+          <t>maa://30764 (94.97)</t>
         </is>
       </c>
       <c r="E14" s="19" t="n"/>
@@ -2298,7 +2298,7 @@
       </c>
       <c r="H14" s="8" t="inlineStr">
         <is>
-          <t>*maa://32656 (55.56)</t>
+          <t>**maa://32656 (50.00)</t>
         </is>
       </c>
       <c r="I14" s="19" t="n"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (99.08), maa://36682 (98.37), maa://26245 (97.07), maa://21288 (96.40)</t>
+          <t>maa://39841 (99.17), maa://36682 (98.41), maa://26245 (97.09), maa://21288 (96.40)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2330,7 +2330,7 @@
       </c>
       <c r="P14" s="8" t="inlineStr">
         <is>
-          <t>maa://23250 (99.69), maa://20107 (87.50), maa://22772 (100.00), maa://68732 (100.00)</t>
+          <t>maa://23250 (99.65), maa://20107 (87.50), maa://22772 (100.00), maa://68732 (100.00)</t>
         </is>
       </c>
       <c r="Q14" s="19" t="n"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://42751 (99.00), maa://22521 (95.59)</t>
+          <t>maa://42751 (99.05), maa://22521 (95.83)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="X14" s="8" t="inlineStr">
         <is>
-          <t>maa://37468 (98.20)</t>
+          <t>maa://37468 (98.35)</t>
         </is>
       </c>
       <c r="Y14" s="19" t="n"/>
@@ -2378,7 +2378,7 @@
       </c>
       <c r="AB14" s="8" t="inlineStr">
         <is>
-          <t>maa://22764 (99.01)</t>
+          <t>maa://22764 (99.06)</t>
         </is>
       </c>
       <c r="AC14" s="19" t="n"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (86.35), maa://45058 (98.32), maa://22734 (84.96), *maa://36048 (75.66), maa://69928 (100.00)</t>
+          <t>maa://22743 (87.03), maa://45058 (98.37), maa://22734 (85.07), *maa://36048 (76.41), maa://69928 (98.04)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2428,7 +2428,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (97.42), maa://21478 (90.48)</t>
+          <t>maa://24304 (97.56), maa://21478 (90.70)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="L15" s="8" t="inlineStr">
         <is>
-          <t>*maa://21334 (72.73)</t>
+          <t>*maa://21334 (71.43)</t>
         </is>
       </c>
       <c r="M15" s="19" t="n"/>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="P15" s="8" t="inlineStr">
         <is>
-          <t>maa://24762 (97.80), *maa://22727 (70.00)</t>
+          <t>maa://24762 (97.79), *maa://22727 (70.00)</t>
         </is>
       </c>
       <c r="Q15" s="19" t="n"/>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="T15" s="8" t="inlineStr">
         <is>
-          <t>maa://23892 (97.83)</t>
+          <t>maa://23892 (97.93)</t>
         </is>
       </c>
       <c r="U15" s="19" t="n"/>
@@ -2492,7 +2492,7 @@
       </c>
       <c r="X15" s="8" t="inlineStr">
         <is>
-          <t>maa://38786 (93.02), maa://56102 (100.00)</t>
+          <t>maa://38786 (93.33), maa://56102 (100.00)</t>
         </is>
       </c>
       <c r="Y15" s="19" t="n"/>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://36666 (96.54), maa://21364 (83.94), *maa://22766 (70.71), maa://68306 (85.14)</t>
+          <t>maa://36666 (96.62), maa://21364 (84.13), *maa://22766 (71.13), maa://68306 (86.73)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://37650 (99.78), maa://21441 (96.64), maa://36679 (94.55)</t>
+          <t>maa://37650 (99.79), maa://21441 (96.64), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2590,7 +2590,7 @@
       </c>
       <c r="P16" s="8" t="inlineStr">
         <is>
-          <t>maa://28504 (96.62)</t>
+          <t>maa://28504 (96.84)</t>
         </is>
       </c>
       <c r="Q16" s="19" t="n"/>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://36674 (98.01), maa://22729 (96.40), *maa://28648 (77.89)</t>
+          <t>maa://36674 (97.94), maa://22729 (96.60), *maa://28648 (77.89)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2622,7 +2622,7 @@
       </c>
       <c r="X16" s="8" t="inlineStr">
         <is>
-          <t>maa://28501 (99.41), maa://28051 (97.14)</t>
+          <t>maa://28501 (99.45), maa://28051 (97.22)</t>
         </is>
       </c>
       <c r="Y16" s="19" t="n"/>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="AB16" s="8" t="inlineStr">
         <is>
-          <t>maa://26228 (98.09)</t>
+          <t>maa://26228 (98.16)</t>
         </is>
       </c>
       <c r="AC16" s="19" t="n"/>
@@ -2654,7 +2654,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>maa://23911 (90.95), maa://27755 (93.75), maa://67613 (99.60)</t>
+          <t>maa://23911 (91.08), maa://27755 (93.75), maa://67613 (99.66)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2672,7 +2672,7 @@
       </c>
       <c r="D17" s="8" t="inlineStr">
         <is>
-          <t>maa://21624 (88.24), maa://56358 (100.00)</t>
+          <t>maa://21624 (88.46), maa://56358 (100.00)</t>
         </is>
       </c>
       <c r="E17" s="19" t="n"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://39599 (98.43), maa://22430 (90.38)</t>
+          <t>maa://39599 (98.51), maa://22430 (90.38)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="L17" s="8" t="inlineStr">
         <is>
-          <t>maa://21679 (88.68)</t>
+          <t>maa://21679 (89.29)</t>
         </is>
       </c>
       <c r="M17" s="19" t="n"/>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (83.06), maa://56238 (98.04)</t>
+          <t>maa://23890 (83.33), maa://56238 (98.18)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="T17" s="8" t="inlineStr">
         <is>
-          <t>*maa://42324 (72.92)</t>
+          <t>*maa://42324 (73.47)</t>
         </is>
       </c>
       <c r="U17" s="19" t="n"/>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="AF17" s="8" t="inlineStr">
         <is>
-          <t>maa://50136 (99.08)</t>
+          <t>maa://50136 (99.16)</t>
         </is>
       </c>
       <c r="AG17" s="16" t="n"/>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>maa://24570 (98.35)</t>
+          <t>maa://24570 (98.44)</t>
         </is>
       </c>
       <c r="E18" s="19" t="n"/>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="H18" s="8" t="inlineStr">
         <is>
-          <t>maa://24421 (95.63)</t>
+          <t>maa://24421 (95.75)</t>
         </is>
       </c>
       <c r="I18" s="19" t="n"/>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://52226 (99.68), maa://22466 (92.86)</t>
+          <t>maa://52226 (99.70), maa://22466 (92.92)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://24379 (100.00), maa://54153 (99.70), maa://24380 (100.00)</t>
+          <t>maa://24379 (100.00), maa://54153 (99.72), maa://24380 (100.00)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2866,7 +2866,7 @@
       </c>
       <c r="T18" s="8" t="inlineStr">
         <is>
-          <t>maa://24385 (98.72)</t>
+          <t>maa://24385 (97.50)</t>
         </is>
       </c>
       <c r="U18" s="19" t="n"/>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (98.84), maa://22741 (92.86)</t>
+          <t>maa://21917 (98.95), maa://22741 (93.33)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2898,7 +2898,7 @@
       </c>
       <c r="AB18" s="8" t="inlineStr">
         <is>
-          <t>maa://24393 (99.10)</t>
+          <t>maa://24393 (99.16)</t>
         </is>
       </c>
       <c r="AC18" s="19" t="n"/>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://47854 (94.22), *maa://68715 (75.00)</t>
+          <t>maa://47854 (94.57), *maa://68715 (75.00)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -2932,7 +2932,7 @@
       </c>
       <c r="D19" s="8" t="inlineStr">
         <is>
-          <t>maa://62850 (99.35)</t>
+          <t>maa://62850 (99.38)</t>
         </is>
       </c>
       <c r="E19" s="19" t="n"/>
@@ -2948,7 +2948,7 @@
       </c>
       <c r="H19" s="8" t="inlineStr">
         <is>
-          <t>maa://66740 (93.75)</t>
+          <t>maa://66740 (94.12)</t>
         </is>
       </c>
       <c r="I19" s="19" t="n"/>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="L19" s="8" t="inlineStr">
         <is>
-          <t>maa://39347 (98.08), maa://56392 (100.00)</t>
+          <t>maa://39347 (98.28), maa://56392 (100.00)</t>
         </is>
       </c>
       <c r="M19" s="19" t="n"/>
@@ -2996,7 +2996,7 @@
       </c>
       <c r="T19" s="8" t="inlineStr">
         <is>
-          <t>maa://24386 (99.57)</t>
+          <t>maa://24386 (99.59)</t>
         </is>
       </c>
       <c r="U19" s="19" t="n"/>
@@ -3012,7 +3012,7 @@
       </c>
       <c r="X19" s="8" t="inlineStr">
         <is>
-          <t>maa://31386 (97.83), maa://58490 (86.36)</t>
+          <t>maa://31386 (98.00), maa://58490 (88.46)</t>
         </is>
       </c>
       <c r="Y19" s="19" t="n"/>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (87.42), *maa://36668 (70.34)</t>
+          <t>maa://30709 (88.06), *maa://36668 (70.34)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3044,7 +3044,7 @@
       </c>
       <c r="AF19" s="8" t="inlineStr">
         <is>
-          <t>*maa://21663 (66.67), maa://52239 (89.36)</t>
+          <t>*maa://21663 (67.39), maa://52239 (90.00)</t>
         </is>
       </c>
       <c r="AG19" s="16" t="n"/>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://25198 (97.64), maa://36680 (99.15), maa://21432 (91.60)</t>
+          <t>maa://25198 (97.69), maa://36680 (99.18), maa://21432 (91.67)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3078,7 +3078,7 @@
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>maa://22864 (96.26)</t>
+          <t>maa://22864 (96.36)</t>
         </is>
       </c>
       <c r="I20" s="19" t="n"/>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (95.70)</t>
+          <t>maa://41331 (95.81)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="P20" s="8" t="inlineStr">
         <is>
-          <t>maa://37442 (98.71)</t>
+          <t>maa://37442 (98.79)</t>
         </is>
       </c>
       <c r="Q20" s="19" t="n"/>
@@ -3126,7 +3126,7 @@
       </c>
       <c r="T20" s="8" t="inlineStr">
         <is>
-          <t>maa://29113 (94.32)</t>
+          <t>maa://29113 (94.57)</t>
         </is>
       </c>
       <c r="U20" s="19" t="n"/>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://50085 (96.77), maa://56241 (98.34), maa://49976 (88.57)</t>
+          <t>maa://50085 (96.92), maa://56241 (98.34), maa://49976 (88.57)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>maa://21261 (99.11)</t>
+          <t>maa://21261 (99.13)</t>
         </is>
       </c>
       <c r="E21" s="19" t="n"/>
@@ -3208,7 +3208,7 @@
       </c>
       <c r="H21" s="8" t="inlineStr">
         <is>
-          <t>maa://24372 (99.02)</t>
+          <t>maa://24372 (99.10)</t>
         </is>
       </c>
       <c r="I21" s="19" t="n"/>
@@ -3224,7 +3224,7 @@
       </c>
       <c r="L21" s="8" t="inlineStr">
         <is>
-          <t>maa://31731 (96.72)</t>
+          <t>maa://31731 (96.90)</t>
         </is>
       </c>
       <c r="M21" s="19" t="n"/>
@@ -3240,7 +3240,7 @@
       </c>
       <c r="P21" s="8" t="inlineStr">
         <is>
-          <t>maa://24381 (85.00)</t>
+          <t>maa://24381 (83.33)</t>
         </is>
       </c>
       <c r="Q21" s="19" t="n"/>
@@ -3272,7 +3272,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (98.33), maa://20110 (87.01)</t>
+          <t>maa://34946 (98.43), maa://20110 (87.18)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="AB21" s="8" t="inlineStr">
         <is>
-          <t>maa://21443 (87.46), maa://52223 (85.21)</t>
+          <t>maa://21443 (87.59), maa://52223 (86.18)</t>
         </is>
       </c>
       <c r="AC21" s="19" t="n"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22432 (94.63), maa://22524 (82.99), maa://64221 (98.01)</t>
+          <t>maa://22432 (94.87), maa://22524 (83.22), maa://64221 (98.09)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>maa://25236 (99.29)</t>
+          <t>maa://25236 (99.15)</t>
         </is>
       </c>
       <c r="I22" s="19" t="n"/>
@@ -3354,7 +3354,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>maa://27127 (84.02), *maa://22751 (71.26), maa://66865 (99.52)</t>
+          <t>maa://27127 (84.40), *maa://22751 (71.26), maa://66865 (99.57)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3386,7 +3386,7 @@
       </c>
       <c r="T22" s="8" t="inlineStr">
         <is>
-          <t>maa://38495 (85.11)</t>
+          <t>maa://38495 (85.42)</t>
         </is>
       </c>
       <c r="U22" s="19" t="n"/>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://37649 (94.89), maa://21282 (99.00)</t>
+          <t>maa://37649 (94.92), maa://21282 (99.03)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3418,7 +3418,7 @@
       </c>
       <c r="AB22" s="8" t="inlineStr">
         <is>
-          <t>maa://23656 (99.55)</t>
+          <t>maa://23656 (99.57)</t>
         </is>
       </c>
       <c r="AC22" s="19" t="n"/>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="AF22" s="8" t="inlineStr">
         <is>
-          <t>maa://29658 (97.25)</t>
+          <t>maa://29658 (97.27)</t>
         </is>
       </c>
       <c r="AG22" s="16" t="n"/>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>*maa://41753 (67.12), **maa://28036 (30.43)</t>
+          <t>*maa://41753 (67.53), **maa://28036 (31.18)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (98.72), maa://39875 (95.08)</t>
+          <t>maa://39756 (98.80), maa://39875 (95.08)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (96.99), maa://29748 (82.23), *maa://37566 (78.79)</t>
+          <t>maa://30587 (97.12), maa://29748 (82.32), *maa://37566 (79.10)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="T23" s="8" t="inlineStr">
         <is>
-          <t>maa://31212 (95.24), maa://24387 (84.78), maa://67084 (88.89)</t>
+          <t>maa://31212 (95.56), maa://24387 (84.78), maa://67084 (88.89)</t>
         </is>
       </c>
       <c r="U23" s="19" t="n"/>
@@ -3532,7 +3532,7 @@
       </c>
       <c r="X23" s="8" t="inlineStr">
         <is>
-          <t>*maa://28503 (61.59)</t>
+          <t>*maa://28503 (61.21)</t>
         </is>
       </c>
       <c r="Y23" s="19" t="n"/>
@@ -3548,7 +3548,7 @@
       </c>
       <c r="AB23" s="8" t="inlineStr">
         <is>
-          <t>maa://29652 (96.81)</t>
+          <t>maa://29652 (96.91)</t>
         </is>
       </c>
       <c r="AC23" s="19" t="n"/>
@@ -3564,7 +3564,7 @@
       </c>
       <c r="AF23" s="8" t="inlineStr">
         <is>
-          <t>maa://31489 (98.59)</t>
+          <t>maa://31489 (98.65)</t>
         </is>
       </c>
       <c r="AG23" s="16" t="n"/>
@@ -3582,7 +3582,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (85.69), maa://46650 (91.38)</t>
+          <t>maa://24368 (86.08), maa://46650 (91.43)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (96.72), maa://23504 (94.08), maa://25141 (80.13), maa://52227 (97.29), *maa://36663 (79.63)</t>
+          <t>maa://29988 (96.92), maa://23504 (94.09), maa://25141 (80.50), maa://52227 (97.42), *maa://36663 (80.00)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="AB24" s="8" t="inlineStr">
         <is>
-          <t>maa://39349 (97.62)</t>
+          <t>maa://39349 (97.78)</t>
         </is>
       </c>
       <c r="AC24" s="19" t="n"/>
@@ -3694,7 +3694,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://64165 (99.19), *maa://22523 (79.82), maa://29910 (94.20), maa://45831 (93.94)</t>
+          <t>maa://64165 (99.15), *maa://22523 (79.82), maa://29910 (94.20), maa://45831 (94.12)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3712,7 +3712,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (96.78), maa://63016 (99.30)</t>
+          <t>maa://29753 (96.80), maa://63016 (99.36)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3728,7 +3728,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>*maa://29063 (77.84), *maa://25311 (70.75), maa://45047 (88.61)</t>
+          <t>*maa://29063 (79.05), *maa://25311 (70.95), maa://45047 (89.02)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3744,7 +3744,7 @@
       </c>
       <c r="L25" s="8" t="inlineStr">
         <is>
-          <t>maa://24378 (93.90), maa://68415 (100.00)</t>
+          <t>maa://24378 (94.05), maa://68415 (92.31)</t>
         </is>
       </c>
       <c r="M25" s="19" t="n"/>
@@ -3760,7 +3760,7 @@
       </c>
       <c r="P25" s="8" t="inlineStr">
         <is>
-          <t>maa://24382 (96.72)</t>
+          <t>maa://24382 (96.77)</t>
         </is>
       </c>
       <c r="Q25" s="19" t="n"/>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="T25" s="8" t="inlineStr">
         <is>
-          <t>maa://20109 (96.76), maa://22545 (100.00)</t>
+          <t>maa://20109 (96.92), maa://22545 (100.00)</t>
         </is>
       </c>
       <c r="U25" s="19" t="n"/>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="X25" s="8" t="inlineStr">
         <is>
-          <t>maa://29890 (92.31)</t>
+          <t>maa://29890 (92.62)</t>
         </is>
       </c>
       <c r="Y25" s="19" t="n"/>
@@ -3808,7 +3808,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (93.46), *maa://24516 (78.43), maa://26001 (81.97), maa://68311 (97.16)</t>
+          <t>maa://31215 (93.58), *maa://24516 (78.43), maa://26001 (81.97), maa://68311 (97.22)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (98.43), maa://36676 (99.85), maa://24621 (96.91), maa://22771 (88.24), maa://37772 (87.50)</t>
+          <t>maa://20108 (98.58), maa://36676 (99.86), maa://24621 (96.93), maa://22771 (88.24), maa://37772 (87.50)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://56374 (100.00), maa://41802 (97.33)</t>
+          <t>maa://56374 (100.00), maa://41802 (97.56)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3858,7 +3858,7 @@
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
-          <t>maa://56240 (96.30), maa://24913 (92.50)</t>
+          <t>maa://56240 (95.44), maa://24913 (92.56)</t>
         </is>
       </c>
       <c r="I26" s="19" t="n"/>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="P26" s="8" t="inlineStr">
         <is>
-          <t>maa://39870 (94.87), maa://56625 (98.73)</t>
+          <t>maa://39870 (95.00), maa://56625 (98.78)</t>
         </is>
       </c>
       <c r="Q26" s="19" t="n"/>
@@ -3922,7 +3922,7 @@
       </c>
       <c r="X26" s="8" t="inlineStr">
         <is>
-          <t>maa://24389 (98.55)</t>
+          <t>maa://24389 (98.61)</t>
         </is>
       </c>
       <c r="Y26" s="19" t="n"/>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="AB26" s="8" t="inlineStr">
         <is>
-          <t>maa://42235 (98.58)</t>
+          <t>maa://42235 (98.66)</t>
         </is>
       </c>
       <c r="AC26" s="19" t="n"/>
@@ -3954,7 +3954,7 @@
       </c>
       <c r="AF26" s="8" t="inlineStr">
         <is>
-          <t>*maa://30511 (71.95), **maa://29760 (45.45)</t>
+          <t>*maa://30511 (70.93), **maa://29760 (45.45)</t>
         </is>
       </c>
       <c r="AG26" s="16" t="n"/>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>maa://39601 (92.25), maa://34494 (95.83)</t>
+          <t>maa://39601 (92.86), maa://34494 (95.96)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4004,7 +4004,7 @@
       </c>
       <c r="L27" s="8" t="inlineStr">
         <is>
-          <t>maa://28071 (90.32)</t>
+          <t>maa://28071 (91.04)</t>
         </is>
       </c>
       <c r="M27" s="19" t="n"/>
@@ -4020,7 +4020,7 @@
       </c>
       <c r="P27" s="8" t="inlineStr">
         <is>
-          <t>maa://56400 (90.00)</t>
+          <t>maa://56400 (90.91)</t>
         </is>
       </c>
       <c r="Q27" s="19" t="n"/>
@@ -4036,7 +4036,7 @@
       </c>
       <c r="T27" s="8" t="inlineStr">
         <is>
-          <t>maa://30624 (90.95)</t>
+          <t>maa://30624 (90.87)</t>
         </is>
       </c>
       <c r="U27" s="19" t="n"/>
@@ -4084,7 +4084,7 @@
       </c>
       <c r="AF27" s="8" t="inlineStr">
         <is>
-          <t>maa://24023 (97.93)</t>
+          <t>maa://24023 (98.00)</t>
         </is>
       </c>
       <c r="AG27" s="16" t="n"/>
@@ -4102,7 +4102,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (96.15), maa://25725 (85.50)</t>
+          <t>maa://24465 (96.20), maa://25725 (85.71)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="L28" s="8" t="inlineStr">
         <is>
-          <t>maa://30770 (91.51)</t>
+          <t>maa://30770 (91.67)</t>
         </is>
       </c>
       <c r="M28" s="19" t="n"/>
@@ -4166,7 +4166,7 @@
       </c>
       <c r="T28" s="8" t="inlineStr">
         <is>
-          <t>maa://29765 (94.26), maa://23263 (96.35)</t>
+          <t>maa://29765 (94.51), maa://23263 (96.43)</t>
         </is>
       </c>
       <c r="U28" s="19" t="n"/>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (97.54), maa://41749 (97.27)</t>
+          <t>maa://39929 (97.56), maa://41749 (97.19)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (94.19), maa://65700 (98.49)</t>
+          <t>maa://36660 (94.29), maa://65700 (98.56)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4232,7 +4232,7 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>maa://31694 (99.39)</t>
+          <t>maa://31694 (99.41)</t>
         </is>
       </c>
       <c r="E29" s="19" t="n"/>
@@ -4264,7 +4264,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (98.01), maa://31400 (98.13), maa://28440 (86.67)</t>
+          <t>maa://28432 (98.13), maa://31400 (98.19), maa://28440 (86.67)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4280,7 +4280,7 @@
       </c>
       <c r="P29" s="8" t="inlineStr">
         <is>
-          <t>maa://54169 (97.74)</t>
+          <t>maa://54169 (97.89)</t>
         </is>
       </c>
       <c r="Q29" s="19" t="n"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://42865 (92.59)</t>
+          <t>maa://42865 (93.13)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (95.83), maa://64191 (97.83)</t>
+          <t>maa://45792 (95.95), maa://64191 (97.87)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="L30" s="8" t="inlineStr">
         <is>
-          <t>maa://30442 (97.78)</t>
+          <t>maa://30442 (97.87)</t>
         </is>
       </c>
       <c r="M30" s="19" t="n"/>
@@ -4442,7 +4442,7 @@
       </c>
       <c r="X30" s="8" t="inlineStr">
         <is>
-          <t>maa://39477 (96.61)</t>
+          <t>maa://39477 (96.77)</t>
         </is>
       </c>
       <c r="Y30" s="19" t="n"/>
@@ -4458,7 +4458,7 @@
       </c>
       <c r="AB30" s="8" t="inlineStr">
         <is>
-          <t>maa://42979 (99.61), maa://45822 (100.00), maa://45045 (93.75)</t>
+          <t>maa://42979 (99.62), maa://45822 (100.00), maa://45045 (93.75)</t>
         </is>
       </c>
       <c r="AC30" s="19" t="n"/>
@@ -4524,7 +4524,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (98.26), maa://36258 (93.41), maa://43904 (89.58)</t>
+          <t>maa://35926 (98.34), maa://36258 (93.70), maa://43904 (89.58)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4556,7 +4556,7 @@
       </c>
       <c r="T31" s="8" t="inlineStr">
         <is>
-          <t>maa://30711 (96.83), maa://30768 (100.00)</t>
+          <t>maa://30711 (96.88), maa://30768 (100.00)</t>
         </is>
       </c>
       <c r="U31" s="19" t="n"/>
@@ -4588,7 +4588,7 @@
       </c>
       <c r="AB31" s="8" t="inlineStr">
         <is>
-          <t>maa://66997 (96.55)</t>
+          <t>maa://66997 (96.77)</t>
         </is>
       </c>
       <c r="AC31" s="19" t="n"/>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://36667 (99.63), maa://21895 (97.99), maa://22760 (100.00)</t>
+          <t>maa://36667 (99.66), maa://21895 (98.00), maa://22760 (100.00)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4654,7 +4654,7 @@
       </c>
       <c r="L32" s="8" t="inlineStr">
         <is>
-          <t>maa://28065 (97.17)</t>
+          <t>maa://28065 (97.22)</t>
         </is>
       </c>
       <c r="M32" s="19" t="n"/>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (99.33), maa://41108 (87.93), maa://41238 (98.17), maa://45523 (100.00)</t>
+          <t>maa://42859 (99.28), maa://41108 (88.14), maa://41238 (98.20), maa://45523 (100.00)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="X32" s="8" t="inlineStr">
         <is>
-          <t>maa://64104 (97.84)</t>
+          <t>maa://64104 (97.93)</t>
         </is>
       </c>
       <c r="Y32" s="19" t="n"/>
@@ -4800,7 +4800,7 @@
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (94.83), maa://69135 (97.78)</t>
+          <t>maa://21956 (94.99), maa://69135 (98.53)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4898,7 +4898,7 @@
       </c>
       <c r="H34" s="8" t="inlineStr">
         <is>
-          <t>maa://66817 (99.44)</t>
+          <t>maa://66817 (98.98)</t>
         </is>
       </c>
       <c r="I34" s="19" t="n"/>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://48817 (99.31), maa://56235 (99.58)</t>
+          <t>maa://48817 (99.33), maa://56235 (99.41)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="T34" s="8" t="inlineStr">
         <is>
-          <t>maa://24526 (97.39)</t>
+          <t>maa://24526 (97.46)</t>
         </is>
       </c>
       <c r="U34" s="19" t="n"/>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="AB34" s="8" t="inlineStr">
         <is>
-          <t>maa://64329 (98.39)</t>
+          <t>maa://64329 (98.55)</t>
         </is>
       </c>
       <c r="AC34" s="19" t="n"/>
@@ -4994,7 +4994,7 @@
       </c>
       <c r="AF34" s="8" t="inlineStr">
         <is>
-          <t>maa://32650 (88.89)</t>
+          <t>maa://32650 (89.83)</t>
         </is>
       </c>
       <c r="AG34" s="16" t="n"/>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
-          <t>maa://41296 (99.34)</t>
+          <t>maa://41296 (99.37)</t>
         </is>
       </c>
       <c r="M35" s="19" t="n"/>
@@ -5076,7 +5076,7 @@
       </c>
       <c r="T35" s="8" t="inlineStr">
         <is>
-          <t>maa://24842 (96.88)</t>
+          <t>maa://24842 (96.94)</t>
         </is>
       </c>
       <c r="U35" s="19" t="n"/>
@@ -5124,7 +5124,7 @@
       </c>
       <c r="AF35" s="8" t="inlineStr">
         <is>
-          <t>maa://39479 (93.55)</t>
+          <t>maa://39479 (93.65)</t>
         </is>
       </c>
       <c r="AG35" s="16" t="n"/>
@@ -5158,7 +5158,7 @@
       </c>
       <c r="H36" s="8" t="inlineStr">
         <is>
-          <t>maa://24375 (94.81)</t>
+          <t>maa://24375 (95.06)</t>
         </is>
       </c>
       <c r="I36" s="19" t="n"/>
@@ -5174,7 +5174,7 @@
       </c>
       <c r="L36" s="8" t="inlineStr">
         <is>
-          <t>maa://42240 (100.00)</t>
+          <t>maa://42240 (98.97)</t>
         </is>
       </c>
       <c r="M36" s="19" t="n"/>
@@ -5206,7 +5206,7 @@
       </c>
       <c r="T36" s="8" t="inlineStr">
         <is>
-          <t>maa://27613 (99.60)</t>
+          <t>maa://27613 (99.63)</t>
         </is>
       </c>
       <c r="U36" s="19" t="n"/>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="AB36" s="19" t="inlineStr">
         <is>
-          <t>maa://64106 (97.96)</t>
+          <t>maa://64106 (98.15)</t>
         </is>
       </c>
       <c r="AC36" s="19" t="n"/>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="H37" s="8" t="inlineStr">
         <is>
-          <t>*maa://24374 (60.00)</t>
+          <t>*maa://24374 (60.61)</t>
         </is>
       </c>
       <c r="I37" s="19" t="n"/>
@@ -5304,7 +5304,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (99.09), maa://56336 (99.43), maa://47069 (86.96), maa://45789 (100.00)</t>
+          <t>maa://45718 (99.11), maa://56336 (99.40), maa://47069 (88.00), maa://45789 (100.00)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="P37" s="8" t="inlineStr">
         <is>
-          <t>maa://21280 (97.77)</t>
+          <t>maa://21280 (97.87)</t>
         </is>
       </c>
       <c r="Q37" s="19" t="n"/>
@@ -5418,7 +5418,7 @@
       </c>
       <c r="L38" s="8" t="inlineStr">
         <is>
-          <t>maa://39384 (99.37), maa://49735 (92.86)</t>
+          <t>maa://39384 (99.40), maa://49735 (92.86)</t>
         </is>
       </c>
       <c r="M38" s="19" t="n"/>
@@ -5434,7 +5434,7 @@
       </c>
       <c r="P38" s="8" t="inlineStr">
         <is>
-          <t>maa://24383 (83.25)</t>
+          <t>maa://24383 (83.57)</t>
         </is>
       </c>
       <c r="Q38" s="19" t="n"/>
@@ -5450,7 +5450,7 @@
       </c>
       <c r="T38" s="8" t="inlineStr">
         <is>
-          <t>maa://30713 (98.55)</t>
+          <t>maa://30713 (98.59)</t>
         </is>
       </c>
       <c r="U38" s="19" t="n"/>
@@ -5482,7 +5482,7 @@
       </c>
       <c r="AF38" s="8" t="inlineStr">
         <is>
-          <t>maa://36697 (95.76), maa://68397 (98.47)</t>
+          <t>maa://36697 (95.83), maa://68397 (98.61)</t>
         </is>
       </c>
       <c r="AG38" s="16" t="n"/>
@@ -5516,7 +5516,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://25199 (85.11), maa://45059 (94.32), maa://30434 (95.48), maa://44165 (85.71)</t>
+          <t>maa://45059 (94.74), maa://25199 (84.51), maa://30434 (95.57), maa://44165 (85.71)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5548,7 +5548,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://47093 (98.50), maa://24709 (94.23)</t>
+          <t>maa://47093 (98.60), maa://24709 (94.32)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5564,7 +5564,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (95.92), maa://45790 (89.02)</t>
+          <t>maa://47079 (95.98), maa://45790 (89.29)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5596,7 +5596,7 @@
       </c>
       <c r="AF39" s="8" t="inlineStr">
         <is>
-          <t>maa://62953 (97.03)</t>
+          <t>maa://62953 (97.06)</t>
         </is>
       </c>
       <c r="AG39" s="16" t="n"/>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (98.22), maa://21386 (95.98), maa://36664 (90.00), *maa://45550 (75.00)</t>
+          <t>maa://23278 (98.23), maa://21386 (95.98), maa://36664 (90.12), *maa://45550 (75.00)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5697,7 +5697,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://65283 (96.98), maa://64205 (94.12)</t>
+          <t>maa://65283 (97.15), maa://64205 (94.12)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5718,7 +5718,7 @@
       </c>
       <c r="H41" s="8" t="inlineStr">
         <is>
-          <t>maa://24466 (93.06)</t>
+          <t>maa://24466 (93.42)</t>
         </is>
       </c>
       <c r="I41" s="19" t="n"/>
@@ -5750,7 +5750,7 @@
       </c>
       <c r="P41" s="8" t="inlineStr">
         <is>
-          <t>maa://43177 (95.97)</t>
+          <t>maa://43177 (96.06)</t>
         </is>
       </c>
       <c r="Q41" s="19" t="n"/>
@@ -5920,7 +5920,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>maa://21284 (98.04)</t>
+          <t>maa://21284 (98.17)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -5952,7 +5952,7 @@
       </c>
       <c r="P43" s="8" t="inlineStr">
         <is>
-          <t>maa://47403 (89.74)</t>
+          <t>maa://47403 (90.48)</t>
         </is>
       </c>
       <c r="Q43" s="19" t="n"/>
@@ -6021,7 +6021,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (98.34), maa://56386 (99.49), maa://27728 (96.43)</t>
+          <t>maa://29768 (98.36), maa://56386 (99.52), maa://27728 (96.46)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6069,7 +6069,7 @@
       </c>
       <c r="T44" s="8" t="inlineStr">
         <is>
-          <t>maa://39366 (94.44)</t>
+          <t>maa://39366 (94.74)</t>
         </is>
       </c>
       <c r="U44" s="19" t="n"/>
@@ -6106,7 +6106,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://42459 (98.91), maa://21229 (85.96), maa://30807 (94.62), *maa://22767 (72.37)</t>
+          <t>maa://42459 (99.00), maa://21229 (86.08), maa://30807 (94.62), *maa://22767 (72.73)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6138,7 +6138,7 @@
       </c>
       <c r="P45" s="8" t="inlineStr">
         <is>
-          <t>maa://36237 (85.37)</t>
+          <t>maa://36237 (86.36)</t>
         </is>
       </c>
       <c r="Q45" s="19" t="n"/>
@@ -6154,7 +6154,7 @@
       </c>
       <c r="T45" s="8" t="inlineStr">
         <is>
-          <t>*maa://39364 (70.65)</t>
+          <t>*maa://39364 (70.47)</t>
         </is>
       </c>
       <c r="U45" s="19" t="n"/>
@@ -6191,7 +6191,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (96.34), maa://43901 (96.63)</t>
+          <t>maa://35931 (96.49), maa://43901 (96.75)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6260,7 +6260,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (97.58), maa://56236 (99.82), maa://29661 (97.26), maa://28038 (84.62)</t>
+          <t>maa://27410 (97.61), maa://56236 (99.83), maa://29661 (97.30), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6292,7 +6292,7 @@
       </c>
       <c r="T47" s="8" t="inlineStr">
         <is>
-          <t>maa://67476 (99.58), maa://68392 (99.58)</t>
+          <t>maa://67476 (99.59), maa://68392 (99.67)</t>
         </is>
       </c>
       <c r="U47" s="19" t="n"/>
@@ -6414,7 +6414,7 @@
       </c>
       <c r="P49" s="8" t="inlineStr">
         <is>
-          <t>maa://39643 (80.39)</t>
+          <t>maa://39643 (81.37)</t>
         </is>
       </c>
       <c r="Q49" s="19" t="n"/>
@@ -6430,7 +6430,7 @@
       </c>
       <c r="T49" s="19" t="inlineStr">
         <is>
-          <t>maa://67231 (99.25)</t>
+          <t>maa://67231 (99.29)</t>
         </is>
       </c>
       <c r="U49" s="19" t="n"/>
@@ -6467,7 +6467,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>maa://62852 (93.71)</t>
+          <t>maa://62852 (93.96)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6501,7 +6501,7 @@
       </c>
       <c r="H51" s="8" t="inlineStr">
         <is>
-          <t>maa://30769 (90.62)</t>
+          <t>maa://30769 (90.91)</t>
         </is>
       </c>
       <c r="I51" s="19" t="n"/>
@@ -6551,7 +6551,7 @@
       </c>
       <c r="H52" s="8" t="inlineStr">
         <is>
-          <t>maa://24376 (99.22)</t>
+          <t>maa://24376 (99.26)</t>
         </is>
       </c>
       <c r="I52" s="19" t="n"/>
@@ -6567,7 +6567,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (99.46), maa://59378 (93.90), maa://65511 (100.00)</t>
+          <t>maa://59394 (99.49), maa://65511 (100.00), maa://59378 (93.98)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6601,7 +6601,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (98.12)</t>
+          <t>maa://32534 (98.15)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -6701,7 +6701,7 @@
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>maa://32532 (97.97)</t>
+          <t>maa://32532 (98.05)</t>
         </is>
       </c>
       <c r="I55" s="19" t="n"/>
@@ -6753,7 +6753,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://56237 (98.51), maa://25176 (98.78)</t>
+          <t>maa://56237 (98.65), maa://25176 (98.80)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6771,7 +6771,7 @@
       </c>
       <c r="H58" s="8" t="inlineStr">
         <is>
-          <t>*maa://37964 (67.94)</t>
+          <t>*maa://37964 (69.34)</t>
         </is>
       </c>
       <c r="I58" s="19" t="n"/>
@@ -6789,7 +6789,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (98.51), maa://27746 (89.85)</t>
+          <t>maa://31270 (98.57), maa://27746 (90.00)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -6807,7 +6807,7 @@
       </c>
       <c r="H60" s="8" t="inlineStr">
         <is>
-          <t>maa://40438 (92.62)</t>
+          <t>maa://40438 (93.19)</t>
         </is>
       </c>
       <c r="I60" s="19" t="n"/>
@@ -6843,7 +6843,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (96.91), maa://56228 (98.34), maa://43903 (100.00)</t>
+          <t>maa://42981 (96.04), maa://56228 (98.49), maa://43903 (100.00)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6861,7 +6861,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (99.48), *maa://59693 (72.00), maa://59413 (97.78)</t>
+          <t>maa://59534 (99.51), *maa://59693 (72.55), maa://59413 (97.92)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -6879,7 +6879,7 @@
       </c>
       <c r="H64" s="8" t="inlineStr">
         <is>
-          <t>maa://44405 (92.11)</t>
+          <t>maa://44405 (92.21)</t>
         </is>
       </c>
       <c r="I64" s="19" t="n"/>
@@ -7077,7 +7077,7 @@
       </c>
       <c r="H75" s="19" t="inlineStr">
         <is>
-          <t>maa://67748 (85.94)</t>
+          <t>maa://67748 (87.50)</t>
         </is>
       </c>
       <c r="I75" s="19" t="n"/>
@@ -7219,7 +7219,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.10.20 13:21:27</t>
+          <t>更新日期：2025.10.31 13:21:33</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8245,7 +8245,7 @@
       </c>
       <c r="D20" s="13" t="inlineStr">
         <is>
-          <t>maa://20865 (92.86), maa://20826 (85.71)</t>
+          <t>maa://20865 (93.33), maa://20826 (85.71)</t>
         </is>
       </c>
       <c r="E20" s="14" t="inlineStr">
@@ -8353,7 +8353,7 @@
       </c>
       <c r="D22" s="13" t="inlineStr">
         <is>
-          <t>maa://20948 (88.89), maa://30844 (100.00), maa://63387 (100.00), maa://58691 (100.00)</t>
+          <t>maa://20948 (90.00), maa://30844 (100.00), maa://63387 (100.00), maa://58691 (100.00)</t>
         </is>
       </c>
       <c r="E22" s="14" t="inlineStr">
@@ -8623,7 +8623,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (73.68), *maa://28758 (72.34), maa://65357 (97.30), maa://29036 (96.77), *maa://42172 (71.43), maa://30285 (100.00)</t>
+          <t>*maa://20849 (74.14), *maa://28758 (72.34), maa://65357 (97.62), maa://29036 (96.77), *maa://42172 (71.43), maa://30285 (100.00)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8731,7 +8731,7 @@
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>maa://20863 (90.65), maa://20832 (99.24), maa://20727 (100.00)</t>
+          <t>maa://20863 (90.79), maa://20832 (99.25), maa://20727 (100.00)</t>
         </is>
       </c>
       <c r="E29" s="14" t="inlineStr">
@@ -8839,7 +8839,7 @@
       </c>
       <c r="D31" s="13" t="inlineStr">
         <is>
-          <t>*maa://39024 (60.00)</t>
+          <t>*maa://39024 (66.67)</t>
         </is>
       </c>
       <c r="E31" s="14" t="inlineStr">
@@ -8893,7 +8893,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (90.22), maa://36866 (97.10), maa://62759 (100.00), maa://45572 (88.24), maa://27794 (100.00), maa://20960 (100.00), maa://20843 (100.00), **maa://24483 (50.00), *maa://20893 (73.68), maa://20862 (83.33), maa://70680 (100.00)</t>
+          <t>maa://36644 (90.22), maa://36866 (97.18), maa://62759 (100.00), maa://45572 (88.24), maa://27794 (100.00), maa://20960 (100.00), maa://20843 (100.00), maa://70680 (100.00), **maa://24483 (50.00), *maa://20893 (75.00), maa://20862 (85.71)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -8947,7 +8947,7 @@
       </c>
       <c r="D33" s="13" t="inlineStr">
         <is>
-          <t>maa://30500 (98.96), *maa://27290 (72.22), ***maa://42154 (8.33)</t>
+          <t>maa://30500 (98.99), *maa://27290 (72.22), ***maa://42154 (8.33)</t>
         </is>
       </c>
       <c r="E33" s="14" t="inlineStr">
@@ -9163,7 +9163,7 @@
       </c>
       <c r="D37" s="13" t="inlineStr">
         <is>
-          <t>maa://27376 (90.77), maa://42635 (94.74), *maa://20838 (55.00)</t>
+          <t>maa://27376 (91.30), maa://42635 (94.74), *maa://20838 (55.00)</t>
         </is>
       </c>
       <c r="E37" s="14" t="inlineStr">
@@ -9271,7 +9271,7 @@
       </c>
       <c r="D39" s="13" t="inlineStr">
         <is>
-          <t>maa://29012 (85.71), maa://20928 (100.00)</t>
+          <t>maa://29012 (87.50), maa://20928 (100.00)</t>
         </is>
       </c>
       <c r="E39" s="14" t="inlineStr">
@@ -9433,7 +9433,7 @@
       </c>
       <c r="D42" s="13" t="inlineStr">
         <is>
-          <t>maa://34883 (94.12), maa://20918 (96.30), maa://20824 (100.00)</t>
+          <t>maa://34883 (94.44), maa://20918 (96.30), maa://20824 (100.00)</t>
         </is>
       </c>
       <c r="E42" s="14" t="inlineStr">
@@ -9649,7 +9649,7 @@
       </c>
       <c r="D46" s="13" t="inlineStr">
         <is>
-          <t>*maa://39025 (80.00)</t>
+          <t>maa://39025 (81.82)</t>
         </is>
       </c>
       <c r="E46" s="14" t="inlineStr">
@@ -9811,7 +9811,7 @@
       </c>
       <c r="D49" s="13" t="inlineStr">
         <is>
-          <t>*maa://32845 (77.27), *maa://20982 (75.00)</t>
+          <t>*maa://32845 (78.26), *maa://20982 (75.00)</t>
         </is>
       </c>
       <c r="E49" s="14" t="inlineStr">
@@ -10135,7 +10135,7 @@
       </c>
       <c r="D55" s="13" t="inlineStr">
         <is>
-          <t>maa://20932 (96.15), maa://42415 (96.30), maa://40838 (100.00), maa://68386 (100.00)</t>
+          <t>maa://20932 (96.15), maa://42415 (96.43), maa://40838 (100.00), maa://68386 (100.00)</t>
         </is>
       </c>
       <c r="E55" s="14" t="inlineStr">
@@ -10189,7 +10189,7 @@
       </c>
       <c r="D56" s="13" t="inlineStr">
         <is>
-          <t>maa://44235 (98.47), maa://45604 (100.00), maa://20961 (94.44), maa://20910 (100.00), maa://44220 (100.00)</t>
+          <t>maa://44235 (98.48), maa://45604 (100.00), maa://20961 (94.44), maa://20910 (100.00), maa://44220 (100.00)</t>
         </is>
       </c>
       <c r="E56" s="14" t="inlineStr">
@@ -10243,7 +10243,7 @@
       </c>
       <c r="D57" s="13" t="inlineStr">
         <is>
-          <t>*maa://20965 (73.81)</t>
+          <t>*maa://20965 (74.42)</t>
         </is>
       </c>
       <c r="E57" s="14" t="inlineStr">
@@ -10297,7 +10297,7 @@
       </c>
       <c r="D58" s="13" t="inlineStr">
         <is>
-          <t>maa://28900 (97.09), maa://30126 (100.00)</t>
+          <t>maa://28900 (97.17), maa://30126 (100.00)</t>
         </is>
       </c>
       <c r="E58" s="14" t="inlineStr">
@@ -10351,7 +10351,7 @@
       </c>
       <c r="D59" s="13" t="inlineStr">
         <is>
-          <t>maa://27970 (98.88), maa://41118 (87.50)</t>
+          <t>maa://27970 (98.90), maa://41118 (88.89)</t>
         </is>
       </c>
       <c r="E59" s="14" t="inlineStr">
@@ -10405,7 +10405,7 @@
       </c>
       <c r="D60" s="13" t="inlineStr">
         <is>
-          <t>maa://38298 (88.50)</t>
+          <t>maa://38298 (88.03)</t>
         </is>
       </c>
       <c r="E60" s="14" t="inlineStr">
@@ -10459,7 +10459,7 @@
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (99.26), maa://31559 (94.00), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00), maa://66633 (100.00)</t>
+          <t>maa://20841 (99.29), maa://31559 (94.12), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00), maa://66633 (100.00)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -10508,12 +10508,12 @@
       </c>
       <c r="C62" s="12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D62" s="13" t="inlineStr">
         <is>
-          <t>maa://40590 (99.37)</t>
+          <t>maa://40590 (99.40), **maa://72388 (50.00)</t>
         </is>
       </c>
       <c r="E62" s="14" t="inlineStr">
@@ -10567,7 +10567,7 @@
       </c>
       <c r="D63" s="13" t="inlineStr">
         <is>
-          <t>maa://20844 (97.14)</t>
+          <t>maa://20844 (97.22)</t>
         </is>
       </c>
       <c r="E63" s="14" t="inlineStr">
@@ -10675,7 +10675,7 @@
       </c>
       <c r="D65" s="13" t="inlineStr">
         <is>
-          <t>maa://28187 (97.78), maa://45144 (100.00), maa://33504 (100.00), maa://43531 (100.00)</t>
+          <t>maa://28187 (97.83), maa://45144 (100.00), maa://33504 (100.00), maa://43531 (100.00)</t>
         </is>
       </c>
       <c r="E65" s="14" t="inlineStr">
@@ -10729,7 +10729,7 @@
       </c>
       <c r="D66" s="13" t="inlineStr">
         <is>
-          <t>maa://28567 (97.50), **maa://20947 (45.71), maa://30525 (100.00), maa://38735 (100.00), *maa://28188 (70.00), maa://30524 (100.00), maa://70681 (100.00)</t>
+          <t>maa://28567 (97.56), **maa://20947 (45.71), maa://30525 (100.00), maa://38735 (100.00), *maa://28188 (70.00), maa://70681 (100.00), maa://30524 (100.00)</t>
         </is>
       </c>
       <c r="E66" s="14" t="inlineStr">
@@ -10783,7 +10783,7 @@
       </c>
       <c r="D67" s="13" t="inlineStr">
         <is>
-          <t>maa://20993 (100.00), maa://45606 (100.00), maa://20914 (100.00), maa://20829 (100.00), maa://20900 (100.00), maa://40159 (100.00)</t>
+          <t>maa://20993 (100.00), maa://45606 (100.00), maa://20914 (100.00), maa://20900 (100.00), maa://20829 (100.00), maa://40159 (100.00)</t>
         </is>
       </c>
       <c r="E67" s="14" t="inlineStr">
@@ -10891,7 +10891,7 @@
       </c>
       <c r="D69" s="13" t="inlineStr">
         <is>
-          <t>maa://20976 (98.31), maa://20815 (100.00)</t>
+          <t>maa://20976 (98.45), maa://20815 (100.00)</t>
         </is>
       </c>
       <c r="E69" s="14" t="inlineStr">
@@ -10945,7 +10945,7 @@
       </c>
       <c r="D70" s="13" t="inlineStr">
         <is>
-          <t>maa://20974 (97.03), maa://29079 (80.95), maa://29096 (95.65), maa://29087 (100.00), *maa://20823 (75.00), maa://20855 (94.12), maa://63722 (85.71), maa://20904 (100.00)</t>
+          <t>maa://20974 (97.09), maa://29079 (80.95), maa://29096 (95.65), maa://29087 (100.00), *maa://20823 (75.00), maa://20855 (94.44), maa://63722 (85.71), maa://20904 (100.00)</t>
         </is>
       </c>
       <c r="E70" s="14" t="inlineStr">
@@ -11048,12 +11048,12 @@
       </c>
       <c r="C72" s="12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D72" s="13" t="inlineStr">
         <is>
-          <t>maa://20943 (99.48), maa://30673 (100.00), maa://30672 (100.00), maa://20856 (100.00)</t>
+          <t>maa://20943 (99.49), maa://30673 (100.00), maa://30672 (100.00), maa://20856 (100.00), maa://71555 (100.00)</t>
         </is>
       </c>
       <c r="E72" s="14" t="inlineStr">
@@ -11107,7 +11107,7 @@
       </c>
       <c r="D73" s="13" t="inlineStr">
         <is>
-          <t>maa://36643 (98.49), maa://36864 (98.11), maa://39140 (100.00), maa://66335 (100.00)</t>
+          <t>maa://36643 (98.52), maa://36864 (98.13), maa://39140 (100.00), maa://66335 (100.00)</t>
         </is>
       </c>
       <c r="E73" s="14" t="inlineStr">
@@ -11377,7 +11377,7 @@
       </c>
       <c r="D78" s="13" t="inlineStr">
         <is>
-          <t>maa://20958 (95.45), ***maa://39769 (20.00)</t>
+          <t>maa://20958 (95.65), ***maa://39769 (20.00)</t>
         </is>
       </c>
       <c r="E78" s="14" t="inlineStr">
@@ -11485,7 +11485,7 @@
       </c>
       <c r="D80" s="13" t="inlineStr">
         <is>
-          <t>maa://20875 (92.86)</t>
+          <t>maa://20875 (93.33)</t>
         </is>
       </c>
       <c r="E80" s="14" t="inlineStr">
@@ -11971,7 +11971,7 @@
       </c>
       <c r="D89" s="13" t="inlineStr">
         <is>
-          <t>maa://24472 (91.17), *maa://35841 (68.00)</t>
+          <t>maa://24472 (91.29), *maa://35841 (65.38)</t>
         </is>
       </c>
       <c r="E89" s="14" t="inlineStr">
@@ -12079,7 +12079,7 @@
       </c>
       <c r="D91" s="13" t="inlineStr">
         <is>
-          <t>*maa://28190 (64.86), maa://20880 (93.10)</t>
+          <t>*maa://28190 (67.50), maa://20880 (93.10)</t>
         </is>
       </c>
       <c r="E91" s="14" t="inlineStr">
@@ -12295,7 +12295,7 @@
       </c>
       <c r="D95" s="13" t="inlineStr">
         <is>
-          <t>maa://40157 (88.89)</t>
+          <t>maa://40157 (90.00)</t>
         </is>
       </c>
       <c r="E95" s="14" t="inlineStr">
@@ -12457,7 +12457,7 @@
       </c>
       <c r="D98" s="13" t="inlineStr">
         <is>
-          <t>maa://20991 (100.00), maa://51015 (88.24)</t>
+          <t>maa://20991 (100.00), maa://51015 (88.68)</t>
         </is>
       </c>
       <c r="E98" s="14" t="inlineStr">
@@ -12565,7 +12565,7 @@
       </c>
       <c r="D100" s="13" t="inlineStr">
         <is>
-          <t>maa://20929 (93.10)</t>
+          <t>maa://20929 (93.55)</t>
         </is>
       </c>
       <c r="E100" s="14" t="inlineStr">
@@ -12673,7 +12673,7 @@
       </c>
       <c r="D102" s="13" t="inlineStr">
         <is>
-          <t>maa://45572 (88.24), maa://27794 (100.00), *maa://20893 (73.68)</t>
+          <t>maa://45572 (88.24), maa://27794 (100.00), *maa://20893 (75.00)</t>
         </is>
       </c>
       <c r="E102" s="14" t="inlineStr">
@@ -12727,7 +12727,7 @@
       </c>
       <c r="D103" s="13" t="inlineStr">
         <is>
-          <t>maa://40517 (91.67), *maa://39240 (56.25)</t>
+          <t>maa://40517 (91.89), *maa://39240 (56.25)</t>
         </is>
       </c>
       <c r="E103" s="14" t="inlineStr">
@@ -12835,7 +12835,7 @@
       </c>
       <c r="D105" s="13" t="inlineStr">
         <is>
-          <t>maa://20966 (87.50)</t>
+          <t>maa://20966 (88.89)</t>
         </is>
       </c>
       <c r="E105" s="14" t="inlineStr">
@@ -13051,7 +13051,7 @@
       </c>
       <c r="D109" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.64), maa://25018 (96.97), maa://25776 (92.50), maa://28361 (95.56), maa://25772 (94.12), maa://56588 (93.55), maa://45194 (86.36), maa://32653 (81.25), maa://25161 (84.21), maa://61839 (100.00), **maa://60902 (41.67), maa://61275 (100.00)</t>
+          <t>maa://51881 (98.68), maa://25018 (97.00), maa://25776 (92.68), maa://28361 (95.56), maa://25772 (94.12), maa://56588 (94.29), maa://45194 (86.36), maa://32653 (81.25), maa://25161 (84.21), maa://61839 (100.00), **maa://60902 (38.46), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E109" s="14" t="inlineStr">
@@ -13321,7 +13321,7 @@
       </c>
       <c r="D114" s="13" t="inlineStr">
         <is>
-          <t>maa://20933 (87.10), maa://20822 (100.00)</t>
+          <t>maa://20933 (87.37), maa://20822 (100.00)</t>
         </is>
       </c>
       <c r="E114" s="14" t="inlineStr">
@@ -13375,7 +13375,7 @@
       </c>
       <c r="D115" s="13" t="inlineStr">
         <is>
-          <t>maa://29037 (97.47)</t>
+          <t>maa://29037 (97.50)</t>
         </is>
       </c>
       <c r="E115" s="14" t="inlineStr">
@@ -13483,7 +13483,7 @@
       </c>
       <c r="D117" s="13" t="inlineStr">
         <is>
-          <t>maa://20908 (98.21), maa://35723 (96.08), *maa://23346 (77.78), maa://38822 (100.00), maa://58659 (100.00)</t>
+          <t>maa://20908 (98.23), maa://35723 (96.08), *maa://23346 (77.78), maa://38822 (100.00), maa://58659 (91.67)</t>
         </is>
       </c>
       <c r="E117" s="14" t="inlineStr">
@@ -13537,7 +13537,7 @@
       </c>
       <c r="D118" s="13" t="inlineStr">
         <is>
-          <t>maa://29659 (85.37), maa://29031 (89.36)</t>
+          <t>maa://29659 (83.33), maa://29031 (89.36)</t>
         </is>
       </c>
       <c r="E118" s="14" t="inlineStr">
@@ -13591,7 +13591,7 @@
       </c>
       <c r="D119" s="13" t="inlineStr">
         <is>
-          <t>maa://31560 (93.33), maa://20940 (87.50)</t>
+          <t>maa://31560 (93.75), maa://20940 (89.47)</t>
         </is>
       </c>
       <c r="E119" s="14" t="inlineStr">
@@ -13699,7 +13699,7 @@
       </c>
       <c r="D121" s="13" t="inlineStr">
         <is>
-          <t>maa://31560 (93.33), maa://20851 (100.00)</t>
+          <t>maa://31560 (93.75), maa://20851 (100.00)</t>
         </is>
       </c>
       <c r="E121" s="14" t="inlineStr">
@@ -13753,7 +13753,7 @@
       </c>
       <c r="D122" s="13" t="inlineStr">
         <is>
-          <t>maa://20949 (93.33)</t>
+          <t>maa://20949 (93.75)</t>
         </is>
       </c>
       <c r="E122" s="14" t="inlineStr">
@@ -13807,7 +13807,7 @@
       </c>
       <c r="D123" s="13" t="inlineStr">
         <is>
-          <t>maa://20869 (100.00), maa://44690 (96.00)</t>
+          <t>maa://20869 (100.00), maa://44690 (96.08)</t>
         </is>
       </c>
       <c r="E123" s="14" t="inlineStr">
@@ -13861,7 +13861,7 @@
       </c>
       <c r="D124" s="13" t="inlineStr">
         <is>
-          <t>maa://29650 (98.57), maa://45570 (96.92)</t>
+          <t>maa://29650 (98.59), maa://45570 (96.92)</t>
         </is>
       </c>
       <c r="E124" s="14" t="inlineStr">
@@ -14023,7 +14023,7 @@
       </c>
       <c r="D127" s="13" t="inlineStr">
         <is>
-          <t>maa://44403 (100.00)</t>
+          <t>maa://44403 (93.75)</t>
         </is>
       </c>
       <c r="E127" s="14" t="inlineStr">
@@ -14185,7 +14185,7 @@
       </c>
       <c r="D130" s="13" t="inlineStr">
         <is>
-          <t>maa://37484 (94.23), maa://24611 (91.18)</t>
+          <t>maa://37484 (94.34), maa://24611 (91.18)</t>
         </is>
       </c>
       <c r="E130" s="14" t="inlineStr">
@@ -14293,7 +14293,7 @@
       </c>
       <c r="D132" s="13" t="inlineStr">
         <is>
-          <t>maa://21422 (99.25)</t>
+          <t>maa://21422 (98.91)</t>
         </is>
       </c>
       <c r="E132" s="14" t="inlineStr">
@@ -14401,7 +14401,7 @@
       </c>
       <c r="D134" s="13" t="inlineStr">
         <is>
-          <t>maa://20837 (100.00), maa://37666 (90.91)</t>
+          <t>maa://20837 (100.00), maa://37666 (91.67)</t>
         </is>
       </c>
       <c r="E134" s="14" t="inlineStr">
@@ -14455,7 +14455,7 @@
       </c>
       <c r="D135" s="13" t="inlineStr">
         <is>
-          <t>maa://29023 (100.00), maa://39515 (91.67)</t>
+          <t>maa://29023 (100.00), maa://39515 (92.31)</t>
         </is>
       </c>
       <c r="E135" s="14" t="inlineStr">
@@ -14779,7 +14779,7 @@
       </c>
       <c r="D141" s="13" t="inlineStr">
         <is>
-          <t>maa://45258 (91.30), **maa://30679 (50.00)</t>
+          <t>maa://45258 (91.67), **maa://30679 (50.00)</t>
         </is>
       </c>
       <c r="E141" s="14" t="inlineStr">
@@ -14941,7 +14941,7 @@
       </c>
       <c r="D144" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (97.96), *maa://23736 (53.49), maa://31185 (92.31), maa://30306 (100.00)</t>
+          <t>maa://28484 (97.98), *maa://23736 (53.49), maa://31185 (92.31), maa://30306 (100.00)</t>
         </is>
       </c>
       <c r="E144" s="14" t="inlineStr">
@@ -14995,7 +14995,7 @@
       </c>
       <c r="D145" s="13" t="inlineStr">
         <is>
-          <t>maa://30670 (96.30), maa://31470 (94.12), maa://61380 (100.00), *maa://45066 (71.43), **maa://30867 (40.00)</t>
+          <t>maa://30670 (96.34), maa://31470 (94.29), maa://61380 (100.00), *maa://45066 (71.43), **maa://30867 (40.00)</t>
         </is>
       </c>
       <c r="E145" s="14" t="inlineStr">
@@ -15319,7 +15319,7 @@
       </c>
       <c r="D151" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.81), maa://36641 (98.25), maa://36865 (95.48), maa://44635 (88.18), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (100.00), maa://42918 (100.00), maa://44119 (97.44), maa://64408 (94.12), maa://37300 (100.00), maa://42917 (100.00)</t>
+          <t>maa://40957 (94.85), maa://36641 (98.25), maa://36865 (95.56), maa://44635 (88.18), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (100.00), maa://42918 (100.00), maa://44119 (97.44), maa://64408 (94.12), maa://37300 (100.00), maa://42917 (100.00)</t>
         </is>
       </c>
       <c r="E151" s="14" t="inlineStr">
@@ -15373,7 +15373,7 @@
       </c>
       <c r="D152" s="13" t="inlineStr">
         <is>
-          <t>maa://51549 (95.77), maa://51923 (96.55), *maa://67508 (60.00)</t>
+          <t>maa://51549 (95.77), maa://51923 (96.55), *maa://67508 (66.67)</t>
         </is>
       </c>
       <c r="E152" s="14" t="inlineStr">
@@ -15805,7 +15805,7 @@
       </c>
       <c r="D160" s="13" t="inlineStr">
         <is>
-          <t>maa://20959 (92.31)</t>
+          <t>maa://20959 (92.86)</t>
         </is>
       </c>
       <c r="E160" s="14" t="inlineStr">
@@ -15859,7 +15859,7 @@
       </c>
       <c r="D161" s="13" t="inlineStr">
         <is>
-          <t>maa://44232 (98.50), maa://45603 (90.62), maa://65963 (83.33), *maa://63114 (66.67), maa://71762 (100.00)</t>
+          <t>maa://44232 (98.51), maa://45603 (90.62), *maa://65963 (71.43), *maa://63114 (66.67), maa://71762 (100.00)</t>
         </is>
       </c>
       <c r="E161" s="14" t="inlineStr">
@@ -15913,7 +15913,7 @@
       </c>
       <c r="D162" s="13" t="inlineStr">
         <is>
-          <t>maa://20936 (92.86)</t>
+          <t>maa://20936 (93.33)</t>
         </is>
       </c>
       <c r="E162" s="14" t="inlineStr">
@@ -15967,7 +15967,7 @@
       </c>
       <c r="D163" s="13" t="inlineStr">
         <is>
-          <t>maa://20855 (94.12)</t>
+          <t>maa://20855 (94.44)</t>
         </is>
       </c>
       <c r="E163" s="14" t="inlineStr">
@@ -16075,7 +16075,7 @@
       </c>
       <c r="D165" s="13" t="inlineStr">
         <is>
-          <t>*maa://32845 (77.27), maa://29054 (100.00)</t>
+          <t>*maa://32845 (78.26), maa://29054 (100.00)</t>
         </is>
       </c>
       <c r="E165" s="14" t="inlineStr">
@@ -16237,7 +16237,7 @@
       </c>
       <c r="D168" s="13" t="inlineStr">
         <is>
-          <t>maa://20975 (91.67), maa://47950 (90.91), maa://30806 (100.00)</t>
+          <t>maa://20975 (91.67), maa://47950 (91.67), maa://30806 (100.00)</t>
         </is>
       </c>
       <c r="E168" s="14" t="inlineStr">
@@ -16291,7 +16291,7 @@
       </c>
       <c r="D169" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (92.31), maa://29627 (92.98), maa://29659 (85.37), maa://49074 (94.20), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
+          <t>maa://29633 (92.36), maa://29627 (92.98), maa://29659 (83.33), maa://49074 (94.29), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
         </is>
       </c>
       <c r="E169" s="14" t="inlineStr">
@@ -16345,7 +16345,7 @@
       </c>
       <c r="D170" s="13" t="inlineStr">
         <is>
-          <t>maa://49867 (94.25), maa://49655 (97.83)</t>
+          <t>maa://49867 (94.38), maa://49655 (98.00)</t>
         </is>
       </c>
       <c r="E170" s="14" t="inlineStr">
@@ -16669,7 +16669,7 @@
       </c>
       <c r="D176" s="13" t="inlineStr">
         <is>
-          <t>maa://59681 (100.00), maa://64200 (100.00)</t>
+          <t>maa://64200 (100.00), maa://59681 (100.00)</t>
         </is>
       </c>
       <c r="E176" s="14" t="inlineStr">
@@ -16723,7 +16723,7 @@
       </c>
       <c r="D177" s="13" t="inlineStr">
         <is>
-          <t>maa://32418 (99.71), maa://63320 (97.73), maa://51440 (100.00)</t>
+          <t>maa://32418 (99.71), maa://63320 (97.78), maa://51440 (100.00)</t>
         </is>
       </c>
       <c r="E177" s="14" t="inlineStr">
@@ -16939,7 +16939,7 @@
       </c>
       <c r="D181" s="13" t="inlineStr">
         <is>
-          <t>maa://20911 (96.00), maa://29012 (85.71)</t>
+          <t>maa://20911 (96.30), maa://29012 (87.50)</t>
         </is>
       </c>
       <c r="E181" s="14" t="inlineStr">
@@ -17101,7 +17101,7 @@
       </c>
       <c r="D184" s="13" t="inlineStr">
         <is>
-          <t>maa://31560 (93.33), *maa://20968 (75.00)</t>
+          <t>maa://31560 (93.75), *maa://20968 (75.00)</t>
         </is>
       </c>
       <c r="E184" s="14" t="inlineStr">
@@ -17533,7 +17533,7 @@
       </c>
       <c r="D192" s="13" t="inlineStr">
         <is>
-          <t>maa://34866 (94.12), maa://34714 (96.97)</t>
+          <t>maa://34866 (94.12), maa://34714 (97.22)</t>
         </is>
       </c>
       <c r="E192" s="14" t="inlineStr">
@@ -17587,7 +17587,7 @@
       </c>
       <c r="D193" s="13" t="inlineStr">
         <is>
-          <t>maa://34883 (94.12), maa://20895 (100.00)</t>
+          <t>maa://34883 (94.44), maa://20895 (100.00)</t>
         </is>
       </c>
       <c r="E193" s="14" t="inlineStr">
@@ -17803,7 +17803,7 @@
       </c>
       <c r="D197" s="13" t="inlineStr">
         <is>
-          <t>*maa://28190 (64.86), maa://20994 (100.00)</t>
+          <t>*maa://28190 (67.50), maa://20994 (100.00)</t>
         </is>
       </c>
       <c r="E197" s="14" t="inlineStr">
@@ -17857,7 +17857,7 @@
       </c>
       <c r="D198" s="13" t="inlineStr">
         <is>
-          <t>maa://20860 (100.00)</t>
+          <t>*maa://20860 (66.67)</t>
         </is>
       </c>
       <c r="E198" s="14" t="inlineStr">
@@ -17906,12 +17906,12 @@
       </c>
       <c r="C199" s="12" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D199" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.52), maa://35854 (84.75), maa://50388 (98.26), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (95.92), maa://70161 (100.00)</t>
+          <t>maa://44224 (90.50), maa://35854 (84.75), maa://50388 (98.28), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://51066 (87.50), maa://63024 (96.36), maa://70161 (100.00), maa://72380 (100.00)</t>
         </is>
       </c>
       <c r="E199" s="14" t="inlineStr">
@@ -17965,7 +17965,7 @@
       </c>
       <c r="D200" s="13" t="inlineStr">
         <is>
-          <t>maa://39156 (94.25), *maa://39550 (55.00), *maa://53417 (77.78), maa://63806 (81.82)</t>
+          <t>maa://39156 (94.32), *maa://39550 (55.00), *maa://53417 (77.78), maa://63806 (81.82)</t>
         </is>
       </c>
       <c r="E200" s="14" t="inlineStr">
@@ -18019,7 +18019,7 @@
       </c>
       <c r="D201" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (86.60), *maa://28190 (64.86), maa://22894 (91.89), *maa://20906 (72.22), **maa://20907 (34.38)</t>
+          <t>maa://27823 (85.71), *maa://28190 (67.50), maa://22894 (91.89), *maa://20906 (72.22), **maa://20907 (34.38)</t>
         </is>
       </c>
       <c r="E201" s="14" t="inlineStr">
@@ -18073,7 +18073,7 @@
       </c>
       <c r="D202" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (86.60), *maa://28190 (64.86), maa://22894 (91.89), *maa://20906 (72.22), **maa://20907 (34.38)</t>
+          <t>maa://27823 (85.71), *maa://28190 (67.50), maa://22894 (91.89), *maa://20906 (72.22), **maa://20907 (34.38)</t>
         </is>
       </c>
       <c r="E202" s="14" t="inlineStr">
@@ -18613,7 +18613,7 @@
       </c>
       <c r="D212" s="13" t="inlineStr">
         <is>
-          <t>maa://28133 (93.65), **maa://39217 (36.84), maa://25369 (95.24)</t>
+          <t>maa://28133 (92.42), **maa://39217 (36.84), maa://25369 (95.24)</t>
         </is>
       </c>
       <c r="E212" s="14" t="inlineStr">
@@ -18667,7 +18667,7 @@
       </c>
       <c r="D213" s="13" t="inlineStr">
         <is>
-          <t>maa://20956 (96.17), *maa://20830 (80.00), maa://44703 (92.86)</t>
+          <t>maa://20956 (95.71), *maa://20830 (80.00), maa://44703 (92.86)</t>
         </is>
       </c>
       <c r="E213" s="14" t="inlineStr">
@@ -18721,7 +18721,7 @@
       </c>
       <c r="D214" s="13" t="inlineStr">
         <is>
-          <t>maa://20955 (81.82)</t>
+          <t>maa://20955 (82.22)</t>
         </is>
       </c>
       <c r="E214" s="14" t="inlineStr">
@@ -18775,7 +18775,7 @@
       </c>
       <c r="D215" s="13" t="inlineStr">
         <is>
-          <t>maa://39238 (99.12)</t>
+          <t>maa://39238 (99.13)</t>
         </is>
       </c>
       <c r="E215" s="14" t="inlineStr">
@@ -18829,7 +18829,7 @@
       </c>
       <c r="D216" s="13" t="inlineStr">
         <is>
-          <t>maa://64044 (96.77)</t>
+          <t>maa://64044 (97.10)</t>
         </is>
       </c>
       <c r="E216" s="14" t="inlineStr">
@@ -19099,7 +19099,7 @@
       </c>
       <c r="D221" s="13" t="inlineStr">
         <is>
-          <t>maa://39157 (87.50)</t>
+          <t>maa://39157 (88.89)</t>
         </is>
       </c>
       <c r="E221" s="14" t="inlineStr">
@@ -19369,7 +19369,7 @@
       </c>
       <c r="D226" s="13" t="inlineStr">
         <is>
-          <t>maa://20988 (91.67)</t>
+          <t>maa://20988 (92.31)</t>
         </is>
       </c>
       <c r="E226" s="14" t="inlineStr">
@@ -19477,7 +19477,7 @@
       </c>
       <c r="D228" s="13" t="inlineStr">
         <is>
-          <t>maa://28187 (97.78), maa://39520 (100.00), maa://43531 (100.00)</t>
+          <t>maa://28187 (97.83), maa://39520 (100.00), maa://43531 (100.00)</t>
         </is>
       </c>
       <c r="E228" s="14" t="inlineStr">
@@ -19639,7 +19639,7 @@
       </c>
       <c r="D231" s="13" t="inlineStr">
         <is>
-          <t>*maa://29644 (73.08), maa://39159 (94.12), ***maa://30061 (27.27)</t>
+          <t>*maa://29644 (73.08), maa://39159 (94.29), ***maa://30061 (27.27)</t>
         </is>
       </c>
       <c r="E231" s="14" t="inlineStr">
@@ -19855,7 +19855,7 @@
       </c>
       <c r="D235" s="13" t="inlineStr">
         <is>
-          <t>*maa://48263 (77.42)</t>
+          <t>*maa://48263 (78.79)</t>
         </is>
       </c>
       <c r="E235" s="14" t="inlineStr">
@@ -19963,7 +19963,7 @@
       </c>
       <c r="D237" s="15" t="inlineStr">
         <is>
-          <t>maa://49491 (91.67)</t>
+          <t>maa://49491 (92.31)</t>
         </is>
       </c>
       <c r="E237" s="14" t="inlineStr">
@@ -20125,7 +20125,7 @@
       </c>
       <c r="D240" s="13" t="inlineStr">
         <is>
-          <t>maa://30714 (97.87), maa://30675 (100.00)</t>
+          <t>maa://30714 (97.92), maa://30675 (100.00)</t>
         </is>
       </c>
       <c r="E240" s="14" t="inlineStr">
@@ -20287,7 +20287,7 @@
       </c>
       <c r="D243" s="13" t="inlineStr">
         <is>
-          <t>*maa://30667 (78.89), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (58.46), maa://39588 (86.67), *maa://64079 (78.57), maa://65726 (88.89), maa://68226 (100.00)</t>
+          <t>*maa://30667 (78.89), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (58.46), maa://39588 (86.67), *maa://64079 (78.57), maa://65726 (90.91), maa://68226 (83.33)</t>
         </is>
       </c>
       <c r="E243" s="14" t="inlineStr">
@@ -20557,7 +20557,7 @@
       </c>
       <c r="D248" s="13" t="inlineStr">
         <is>
-          <t>maa://20867 (93.33), maa://38485 (96.77), *maa://32202 (80.00)</t>
+          <t>maa://20867 (93.33), maa://38485 (96.88), *maa://32202 (80.00)</t>
         </is>
       </c>
       <c r="E248" s="14" t="inlineStr">
@@ -20773,7 +20773,7 @@
       </c>
       <c r="D252" s="13" t="inlineStr">
         <is>
-          <t>maa://28923 (91.43), maa://28906 (98.31), ***maa://28825 (11.54), maa://65613 (88.89)</t>
+          <t>maa://28923 (91.51), maa://28906 (98.31), ***maa://28825 (11.54), maa://65613 (88.89)</t>
         </is>
       </c>
       <c r="E252" s="14" t="inlineStr">
@@ -20827,7 +20827,7 @@
       </c>
       <c r="D253" s="13" t="inlineStr">
         <is>
-          <t>maa://42287 (92.99), maa://45570 (96.92), maa://60678 (91.67), maa://42225 (94.12)</t>
+          <t>maa://42287 (93.12), maa://45570 (96.92), maa://60678 (92.00), maa://42225 (94.12)</t>
         </is>
       </c>
       <c r="E253" s="14" t="inlineStr">
@@ -20989,7 +20989,7 @@
       </c>
       <c r="D256" s="13" t="inlineStr">
         <is>
-          <t>maa://31559 (94.00), maa://24093 (100.00), maa://20924 (95.24), **maa://49440 (37.50), maa://63591 (100.00)</t>
+          <t>maa://31559 (94.12), maa://24093 (100.00), maa://20924 (95.24), **maa://49440 (37.50), maa://63591 (100.00)</t>
         </is>
       </c>
       <c r="E256" s="14" t="inlineStr">
@@ -21043,7 +21043,7 @@
       </c>
       <c r="D257" s="13" t="inlineStr">
         <is>
-          <t>maa://40958 (91.18), *maa://45067 (77.78)</t>
+          <t>maa://40958 (91.67), *maa://45067 (77.78)</t>
         </is>
       </c>
       <c r="E257" s="14" t="inlineStr">
@@ -21367,7 +21367,7 @@
       </c>
       <c r="D263" s="13" t="inlineStr">
         <is>
-          <t>maa://31560 (93.33), maa://20884 (96.30)</t>
+          <t>maa://31560 (93.75), maa://20884 (96.30)</t>
         </is>
       </c>
       <c r="E263" s="14" t="inlineStr">
@@ -21691,7 +21691,7 @@
       </c>
       <c r="D269" s="13" t="inlineStr">
         <is>
-          <t>maa://22467 (95.92)</t>
+          <t>maa://22467 (96.00)</t>
         </is>
       </c>
       <c r="E269" s="14" t="inlineStr">
@@ -21799,7 +21799,7 @@
       </c>
       <c r="D271" s="13" t="inlineStr">
         <is>
-          <t>maa://49643 (92.00)</t>
+          <t>maa://49643 (92.59)</t>
         </is>
       </c>
       <c r="E271" s="14" t="inlineStr">
@@ -21853,7 +21853,7 @@
       </c>
       <c r="D272" s="13" t="inlineStr">
         <is>
-          <t>maa://48265 (83.87)</t>
+          <t>maa://48265 (84.38)</t>
         </is>
       </c>
       <c r="E272" s="14" t="inlineStr">
@@ -21907,7 +21907,7 @@
       </c>
       <c r="D273" s="13" t="inlineStr">
         <is>
-          <t>*maa://20825 (73.33), *maa://21445 (72.22), *maa://35726 (61.54), ***maa://20891 (30.00)</t>
+          <t>*maa://20825 (74.19), *maa://21445 (72.22), *maa://35726 (61.54), ***maa://20891 (30.00)</t>
         </is>
       </c>
       <c r="E273" s="14" t="inlineStr">
@@ -21961,7 +21961,7 @@
       </c>
       <c r="D274" s="13" t="inlineStr">
         <is>
-          <t>maa://25769 (96.99)</t>
+          <t>maa://25769 (97.01)</t>
         </is>
       </c>
       <c r="E274" s="14" t="inlineStr">
@@ -22069,7 +22069,7 @@
       </c>
       <c r="D276" s="13" t="inlineStr">
         <is>
-          <t>maa://20862 (83.33)</t>
+          <t>maa://20862 (85.71)</t>
         </is>
       </c>
       <c r="E276" s="14" t="inlineStr">
@@ -22123,7 +22123,7 @@
       </c>
       <c r="D277" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.64), maa://51630 (96.36), maa://56588 (93.55), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (41.67), *maa://66758 (76.92)</t>
+          <t>maa://51881 (98.68), maa://51630 (96.46), maa://56588 (94.29), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (38.46), *maa://66758 (76.92)</t>
         </is>
       </c>
       <c r="E277" s="14" t="inlineStr">
@@ -22393,7 +22393,7 @@
       </c>
       <c r="D282" s="13" t="inlineStr">
         <is>
-          <t>maa://28133 (93.65), maa://33394 (100.00)</t>
+          <t>maa://28133 (92.42), maa://33394 (100.00)</t>
         </is>
       </c>
       <c r="E282" s="14" t="inlineStr">
@@ -22447,7 +22447,7 @@
       </c>
       <c r="D283" s="13" t="inlineStr">
         <is>
-          <t>maa://42311 (91.30)</t>
+          <t>maa://42311 (91.67)</t>
         </is>
       </c>
       <c r="E283" s="14" t="inlineStr">
@@ -22825,7 +22825,7 @@
       </c>
       <c r="D290" s="13" t="inlineStr">
         <is>
-          <t>maa://38296 (91.18)</t>
+          <t>maa://38296 (88.89)</t>
         </is>
       </c>
       <c r="E290" s="14" t="inlineStr">
@@ -22879,7 +22879,7 @@
       </c>
       <c r="D291" s="13" t="inlineStr">
         <is>
-          <t>maa://20899 (90.16), maa://46332 (93.10), ***maa://44744 (25.00)</t>
+          <t>maa://20899 (90.22), maa://46332 (93.33), ***maa://44744 (25.00)</t>
         </is>
       </c>
       <c r="E291" s="14" t="inlineStr">
@@ -22933,7 +22933,7 @@
       </c>
       <c r="D292" s="13" t="inlineStr">
         <is>
-          <t>maa://53353 (85.71)</t>
+          <t>maa://53353 (87.50)</t>
         </is>
       </c>
       <c r="E292" s="14" t="inlineStr">
@@ -23041,7 +23041,7 @@
       </c>
       <c r="D294" s="13" t="inlineStr">
         <is>
-          <t>maa://30710 (97.96), maa://36845 (95.92), maa://31558 (97.22), **maa://39217 (36.84), maa://30668 (87.10)</t>
+          <t>maa://30710 (97.97), maa://36845 (95.92), maa://31558 (97.22), **maa://39217 (36.84), maa://30668 (87.10)</t>
         </is>
       </c>
       <c r="E294" s="14" t="inlineStr">
@@ -23203,7 +23203,7 @@
       </c>
       <c r="D297" s="13" t="inlineStr">
         <is>
-          <t>maa://25774 (94.67), maa://28133 (93.65), maa://22469 (90.77), **maa://39217 (36.84), **maa://31349 (50.00)</t>
+          <t>maa://25774 (94.67), maa://28133 (92.42), maa://22469 (90.77), **maa://39217 (36.84), **maa://31349 (50.00)</t>
         </is>
       </c>
       <c r="E297" s="14" t="inlineStr">
@@ -23311,7 +23311,7 @@
       </c>
       <c r="D299" s="13" t="inlineStr">
         <is>
-          <t>maa://32414 (98.84), maa://39155 (97.50), maa://32505 (100.00)</t>
+          <t>maa://32414 (98.85), maa://39155 (97.73), maa://32505 (100.00)</t>
         </is>
       </c>
       <c r="E299" s="14" t="inlineStr">
@@ -23473,7 +23473,7 @@
       </c>
       <c r="D302" s="13" t="inlineStr">
         <is>
-          <t>maa://36642 (100.00), maa://36867 (97.06), maa://39155 (97.50)</t>
+          <t>maa://36642 (100.00), maa://36867 (97.14), maa://39155 (97.73)</t>
         </is>
       </c>
       <c r="E302" s="14" t="inlineStr">
@@ -23527,7 +23527,7 @@
       </c>
       <c r="D303" s="13" t="inlineStr">
         <is>
-          <t>**maa://39166 (50.00), maa://39167 (100.00)</t>
+          <t>**maa://39166 (33.33), maa://39167 (100.00)</t>
         </is>
       </c>
       <c r="E303" s="14" t="inlineStr">
@@ -23581,7 +23581,7 @@
       </c>
       <c r="D304" s="13" t="inlineStr">
         <is>
-          <t>maa://29005 (98.78), maa://31560 (93.33)</t>
+          <t>maa://29005 (98.78), maa://31560 (93.75)</t>
         </is>
       </c>
       <c r="E304" s="14" t="inlineStr">
@@ -23797,7 +23797,7 @@
       </c>
       <c r="D308" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (98.52), maa://49642 (97.67), maa://49660 (93.62), maa://70004 (100.00), maa://50517 (85.71)</t>
+          <t>maa://50280 (98.53), maa://49642 (97.69), maa://49660 (93.75), maa://70004 (100.00), maa://50517 (85.71)</t>
         </is>
       </c>
       <c r="E308" s="14" t="inlineStr">
@@ -24067,7 +24067,7 @@
       </c>
       <c r="D313" s="13" t="inlineStr">
         <is>
-          <t>maa://36005 (94.44)</t>
+          <t>maa://36005 (95.00)</t>
         </is>
       </c>
       <c r="E313" s="14" t="inlineStr">
@@ -24121,7 +24121,7 @@
       </c>
       <c r="D314" s="13" t="inlineStr">
         <is>
-          <t>maa://35859 (97.85)</t>
+          <t>maa://35859 (97.87)</t>
         </is>
       </c>
       <c r="E314" s="14" t="inlineStr">
@@ -24175,7 +24175,7 @@
       </c>
       <c r="D315" s="13" t="inlineStr">
         <is>
-          <t>maa://53348 (87.88)</t>
+          <t>maa://53348 (88.24)</t>
         </is>
       </c>
       <c r="E315" s="14" t="inlineStr">
@@ -24337,7 +24337,7 @@
       </c>
       <c r="D318" s="13" t="inlineStr">
         <is>
-          <t>maa://25775 (92.39), *maa://25393 (75.00)</t>
+          <t>maa://25775 (92.47), *maa://25393 (75.00)</t>
         </is>
       </c>
       <c r="E318" s="14" t="inlineStr">
@@ -24877,7 +24877,7 @@
       </c>
       <c r="D328" s="13" t="inlineStr">
         <is>
-          <t>maa://39692 (99.56), maa://39810 (90.91)</t>
+          <t>maa://39692 (99.57), maa://39810 (90.91)</t>
         </is>
       </c>
       <c r="E328" s="14" t="inlineStr">
@@ -25039,7 +25039,7 @@
       </c>
       <c r="D331" s="15" t="inlineStr">
         <is>
-          <t>maa://34715 (94.74), maa://34867 (96.30)</t>
+          <t>maa://34715 (94.74), maa://34867 (96.36)</t>
         </is>
       </c>
       <c r="E331" s="15" t="inlineStr">
@@ -25255,7 +25255,7 @@
       </c>
       <c r="D335" s="15" t="inlineStr">
         <is>
-          <t>maa://40956 (94.29)</t>
+          <t>maa://40956 (94.34)</t>
         </is>
       </c>
       <c r="E335" s="15" t="inlineStr">
@@ -25471,7 +25471,7 @@
       </c>
       <c r="D339" s="22" t="inlineStr">
         <is>
-          <t>maa://34205 (90.00), *maa://39541 (75.00)</t>
+          <t>maa://34205 (90.00), *maa://39541 (80.00)</t>
         </is>
       </c>
       <c r="E339" s="22" t="inlineStr">
@@ -25687,7 +25687,7 @@
       </c>
       <c r="D343" s="22" t="inlineStr">
         <is>
-          <t>maa://67275 (100.00), *maa://69909 (57.14)</t>
+          <t>maa://67275 (100.00), *maa://69909 (55.56)</t>
         </is>
       </c>
       <c r="E343" s="22" t="inlineStr">
@@ -25849,7 +25849,7 @@
       </c>
       <c r="D346" s="22" t="inlineStr">
         <is>
-          <t>maa://30671 (81.59), maa://30669 (99.33), maa://37275 (81.40), *maa://32410 (61.54), maa://41605 (100.00)</t>
+          <t>maa://30671 (81.59), maa://30669 (99.34), maa://37275 (81.40), *maa://32410 (61.54), maa://41605 (100.00)</t>
         </is>
       </c>
       <c r="E346" s="22" t="inlineStr">
@@ -26227,7 +26227,7 @@
       </c>
       <c r="D353" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (97.61), maa://32415 (84.38), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
+          <t>maa://32647 (97.61), maa://32415 (84.23), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E353" s="22" t="inlineStr">
@@ -26497,7 +26497,7 @@
       </c>
       <c r="D358" s="22" t="inlineStr">
         <is>
-          <t>maa://34865 (97.90), maa://34717 (94.20), *maa://45066 (71.43)</t>
+          <t>maa://34865 (97.91), maa://34717 (94.20), *maa://45066 (71.43)</t>
         </is>
       </c>
       <c r="E358" s="22" t="inlineStr">
@@ -26600,12 +26600,12 @@
       </c>
       <c r="C360" s="12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D360" s="22" t="inlineStr">
         <is>
-          <t>maa://45834 (100.00), maa://45833 (100.00)</t>
+          <t>maa://50147 (100.00), maa://45834 (100.00), maa://45833 (100.00)</t>
         </is>
       </c>
       <c r="E360" s="22" t="inlineStr">
@@ -26713,7 +26713,7 @@
       </c>
       <c r="D362" s="22" t="inlineStr">
         <is>
-          <t>maa://36868 (99.38), maa://35996 (98.02), maa://47349 (97.83), **maa://39217 (36.84), *maa://71203 (75.00)</t>
+          <t>maa://36868 (99.39), maa://35996 (98.02), maa://47349 (97.96), **maa://39217 (36.84), maa://71203 (85.71)</t>
         </is>
       </c>
       <c r="E362" s="22" t="inlineStr">
@@ -26767,7 +26767,7 @@
       </c>
       <c r="D363" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.60), maa://49695 (100.00), maa://49758 (98.84), *maa://52357 (77.78), *maa://59402 (58.06), *maa://63091 (66.67)</t>
+          <t>maa://49696 (99.61), maa://49695 (100.00), maa://49758 (98.84), *maa://52357 (78.95), *maa://59402 (56.25), *maa://63091 (64.71)</t>
         </is>
       </c>
       <c r="E363" s="22" t="inlineStr">
@@ -26875,7 +26875,7 @@
       </c>
       <c r="D365" s="22" t="inlineStr">
         <is>
-          <t>maa://42299 (97.87), maa://42224 (85.00)</t>
+          <t>maa://42299 (97.96), maa://42224 (85.71)</t>
         </is>
       </c>
       <c r="E365" s="22" t="inlineStr">
@@ -26929,7 +26929,7 @@
       </c>
       <c r="D366" s="22" t="inlineStr">
         <is>
-          <t>maa://49648 (96.25), *maa://49662 (76.47)</t>
+          <t>maa://49648 (96.34), *maa://49662 (76.47)</t>
         </is>
       </c>
       <c r="E366" s="22" t="inlineStr">
@@ -27037,7 +27037,7 @@
       </c>
       <c r="D368" s="22" t="inlineStr">
         <is>
-          <t>maa://36645 (98.44), maa://36841 (92.65), maa://37484 (94.23), maa://37858 (93.55), **maa://56268 (50.00), maa://40489 (100.00)</t>
+          <t>maa://36645 (98.44), maa://36841 (92.65), maa://37484 (94.34), maa://37858 (93.55), **maa://56268 (50.00), maa://40489 (100.00)</t>
         </is>
       </c>
       <c r="E368" s="22" t="inlineStr">
@@ -27091,7 +27091,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://42635 (94.74), maa://50629 (85.71), maa://48859 (100.00)</t>
+          <t>maa://42635 (94.74), maa://50629 (87.50), maa://48859 (100.00)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -27253,7 +27253,7 @@
       </c>
       <c r="D372" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (94.81), maa://48026 (94.70), maa://44635 (88.18), maa://41035 (93.59), *maa://60251 (76.47), maa://44660 (92.68), maa://41128 (84.21)</t>
+          <t>maa://40957 (94.85), maa://48026 (94.70), maa://44635 (88.18), maa://41035 (93.59), *maa://60251 (77.78), maa://44660 (92.68), maa://41128 (84.21)</t>
         </is>
       </c>
       <c r="E372" s="22" t="inlineStr">
@@ -27307,7 +27307,7 @@
       </c>
       <c r="D373" s="22" t="inlineStr">
         <is>
-          <t>maa://40164 (83.33)</t>
+          <t>maa://40164 (85.71)</t>
         </is>
       </c>
       <c r="E373" s="22" t="inlineStr">
@@ -27361,7 +27361,7 @@
       </c>
       <c r="D374" s="22" t="inlineStr">
         <is>
-          <t>maa://63883 (97.62), maa://64045 (100.00), maa://64041 (83.33)</t>
+          <t>maa://63883 (97.78), maa://64045 (100.00), maa://64041 (83.33)</t>
         </is>
       </c>
       <c r="E374" s="22" t="inlineStr">
@@ -27518,12 +27518,12 @@
       </c>
       <c r="C377" s="12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D377" s="22" t="inlineStr">
         <is>
-          <t>maa://71182 (96.36), maa://70756 (97.62), maa://71524 (100.00)</t>
+          <t>maa://71182 (97.06), maa://70756 (97.67), maa://71524 (100.00), maa://72244 (100.00)</t>
         </is>
       </c>
       <c r="E377" s="22" t="inlineStr">
@@ -27577,7 +27577,7 @@
       </c>
       <c r="D378" s="22" t="inlineStr">
         <is>
-          <t>maa://45798 (98.67)</t>
+          <t>maa://45798 (98.68)</t>
         </is>
       </c>
       <c r="E378" s="22" t="inlineStr">
@@ -27793,7 +27793,7 @@
       </c>
       <c r="D382" s="22" t="inlineStr">
         <is>
-          <t>maa://41110 (98.57), maa://45605 (90.00)</t>
+          <t>maa://41110 (98.58), maa://45605 (90.00)</t>
         </is>
       </c>
       <c r="E382" s="22" t="inlineStr">
@@ -28063,7 +28063,7 @@
       </c>
       <c r="D387" s="22" t="inlineStr">
         <is>
-          <t>maa://43872 (94.12)</t>
+          <t>maa://43872 (94.44)</t>
         </is>
       </c>
       <c r="E387" s="22" t="inlineStr">
@@ -28117,7 +28117,7 @@
       </c>
       <c r="D388" s="22" t="inlineStr">
         <is>
-          <t>*maa://53307 (66.67)</t>
+          <t>*maa://53307 (67.74)</t>
         </is>
       </c>
       <c r="E388" s="22" t="inlineStr">
@@ -28171,7 +28171,7 @@
       </c>
       <c r="D389" s="22" t="inlineStr">
         <is>
-          <t>maa://43875 (98.33)</t>
+          <t>maa://43875 (98.36)</t>
         </is>
       </c>
       <c r="E389" s="22" t="inlineStr">
@@ -28225,7 +28225,7 @@
       </c>
       <c r="D390" s="22" t="inlineStr">
         <is>
-          <t>maa://42970 (80.85), maa://44745 (98.13), **maa://49516 (37.93), *maa://45952 (57.14), ***maa://46851 (10.00), *maa://44896 (80.00)</t>
+          <t>maa://42970 (80.85), maa://44745 (98.19), **maa://49516 (40.00), *maa://45952 (57.14), ***maa://46851 (10.00), *maa://44896 (80.00)</t>
         </is>
       </c>
       <c r="E390" s="22" t="inlineStr">
@@ -28468,7 +28468,7 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>maa://63890 (98.18), maa://64043 (100.00)</t>
+          <t>maa://63890 (98.36), maa://64043 (100.00)</t>
         </is>
       </c>
       <c r="E396" t="inlineStr">
@@ -28522,7 +28522,7 @@
       </c>
       <c r="D398" t="inlineStr">
         <is>
-          <t>maa://47023 (87.93)</t>
+          <t>maa://47023 (88.33)</t>
         </is>
       </c>
       <c r="E398" t="inlineStr">
@@ -28603,7 +28603,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>maa://59533 (96.15), maa://59577 (100.00)</t>
+          <t>maa://59533 (96.30), maa://59577 (100.00)</t>
         </is>
       </c>
       <c r="E401" t="inlineStr">
@@ -28657,7 +28657,7 @@
       </c>
       <c r="D403" t="inlineStr">
         <is>
-          <t>**maa://59691 (50.00)</t>
+          <t>*maa://59691 (66.67)</t>
         </is>
       </c>
       <c r="E403" t="inlineStr">
@@ -28711,7 +28711,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>maa://51880 (99.29), maa://56651 (100.00), maa://51878 (100.00)</t>
+          <t>maa://51880 (99.30), maa://56651 (100.00), maa://51878 (100.00)</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">
@@ -28738,7 +28738,7 @@
       </c>
       <c r="D406" t="inlineStr">
         <is>
-          <t>maa://51872 (96.44), maa://51876 (99.11), maa://63228 (86.11), maa://51873 (98.00), maa://62047 (90.32)</t>
+          <t>maa://51872 (96.53), maa://51876 (99.11), maa://63228 (86.11), maa://51873 (98.00), maa://62047 (90.32)</t>
         </is>
       </c>
       <c r="E406" t="inlineStr">
@@ -28765,7 +28765,7 @@
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>**maa://67814 (50.00)</t>
+          <t>*maa://67814 (57.14)</t>
         </is>
       </c>
       <c r="E407" t="inlineStr">
@@ -28792,7 +28792,7 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>maa://60449 (98.52), maa://59493 (96.90)</t>
+          <t>maa://60449 (98.57), maa://59493 (96.92)</t>
         </is>
       </c>
       <c r="E408" t="inlineStr">
@@ -28846,7 +28846,7 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>maa://62756 (96.10)</t>
+          <t>maa://62756 (96.23)</t>
         </is>
       </c>
       <c r="E410" t="inlineStr">
@@ -28900,7 +28900,7 @@
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>maa://64040 (99.11), maa://52505 (97.77), maa://66377 (94.44), ***maa://66376 (14.29), ***maa://70187 (10.00)</t>
+          <t>maa://52505 (97.86), maa://64040 (99.15), maa://66377 (94.44), ***maa://66376 (14.29), ***maa://70187 (9.09)</t>
         </is>
       </c>
       <c r="E412" t="inlineStr">
@@ -28927,7 +28927,7 @@
       </c>
       <c r="D413" t="inlineStr">
         <is>
-          <t>maa://67090 (91.84)</t>
+          <t>maa://67090 (93.55)</t>
         </is>
       </c>
       <c r="E413" t="inlineStr">
@@ -28954,7 +28954,7 @@
       </c>
       <c r="D414" t="inlineStr">
         <is>
-          <t>maa://67388 (90.00), maa://71184 (85.71)</t>
+          <t>maa://67388 (89.06), *maa://71184 (77.78)</t>
         </is>
       </c>
       <c r="E414" t="inlineStr">
@@ -28981,7 +28981,7 @@
       </c>
       <c r="D415" t="inlineStr">
         <is>
-          <t>maa://67089 (96.23), maa://67271 (95.45)</t>
+          <t>maa://67089 (96.49), maa://67271 (92.31)</t>
         </is>
       </c>
       <c r="E415" t="inlineStr">
@@ -29008,7 +29008,7 @@
       </c>
       <c r="D416" t="inlineStr">
         <is>
-          <t>maa://67088 (93.42)</t>
+          <t>maa://67088 (93.10)</t>
         </is>
       </c>
       <c r="E416" t="inlineStr">
@@ -29035,7 +29035,7 @@
       </c>
       <c r="D417" t="inlineStr">
         <is>
-          <t>maa://67087 (95.83), maa://67268 (97.39), maa://67269 (86.36), maa://67648 (100.00)</t>
+          <t>maa://67087 (96.61), maa://67268 (97.66), maa://67269 (88.00), maa://67648 (100.00)</t>
         </is>
       </c>
       <c r="E417" t="inlineStr">
@@ -29116,7 +29116,7 @@
       </c>
       <c r="D420" t="inlineStr">
         <is>
-          <t>maa://70877 (97.73)</t>
+          <t>maa://70877 (98.59)</t>
         </is>
       </c>
       <c r="E420" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#250)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -715,7 +715,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (98.74), maa://24702 (95.24), maa://36681 (85.71)</t>
+          <t>maa://25390 (98.86), maa://24702 (95.25), maa://36681 (85.71)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -747,7 +747,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://58660 (98.96), maa://39402 (95.62), *maa://34787 (74.76), *maa://54304 (70.00)</t>
+          <t>maa://58660 (99.02), maa://39402 (95.90), *maa://34787 (74.76), *maa://54304 (70.00)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -779,7 +779,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (97.76), maa://66635 (99.32)</t>
+          <t>maa://22742 (97.87), maa://66635 (99.40)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -811,7 +811,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://36684 (98.70), maa://21246 (91.11)</t>
+          <t>maa://36684 (98.69), maa://21246 (91.14)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -827,7 +827,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://59087 (97.74), maa://25251 (91.67)</t>
+          <t>maa://59087 (97.92), maa://25251 (91.67)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -845,7 +845,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (99.48), maa://36987 (97.33), maa://39849 (93.33)</t>
+          <t>maa://40192 (99.48), maa://36987 (97.37), maa://39849 (94.12)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -861,7 +861,7 @@
       </c>
       <c r="H3" s="8" t="inlineStr">
         <is>
-          <t>maa://21247 (99.50)</t>
+          <t>maa://21247 (99.49)</t>
         </is>
       </c>
       <c r="I3" s="19" t="n"/>
@@ -877,7 +877,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>maa://22880 (93.16), maa://20276 (94.48), maa://22749 (86.21)</t>
+          <t>maa://22880 (93.67), maa://20276 (94.62), maa://22749 (87.88)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -893,7 +893,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (98.81), maa://26254 (96.55), maa://22738 (83.33)</t>
+          <t>maa://21249 (98.91), maa://26254 (95.31), maa://22738 (85.71)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -909,7 +909,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://60545 (99.04), maa://45854 (89.20), maa://24617 (91.18)</t>
+          <t>maa://60545 (99.13), maa://45854 (89.93), maa://24617 (91.18)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -925,7 +925,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (94.27), maa://27484 (99.33), maa://27480 (86.89)</t>
+          <t>maa://27396 (94.74), maa://27484 (99.27), maa://27480 (87.30)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -941,7 +941,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://52241 (99.37), maa://24390 (97.06)</t>
+          <t>maa://52241 (99.45), maa://24390 (97.26)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -957,7 +957,7 @@
       </c>
       <c r="AF3" s="8" t="inlineStr">
         <is>
-          <t>maa://21289 (92.75)</t>
+          <t>maa://21289 (93.42)</t>
         </is>
       </c>
       <c r="AG3" s="16" t="n"/>
@@ -975,7 +975,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (98.57), maa://22499 (90.48), maa://22746 (100.00)</t>
+          <t>maa://24632 (98.69), maa://22499 (90.48), maa://22746 (88.89)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (99.37), maa://50121 (97.04)</t>
+          <t>maa://49983 (99.43), maa://50121 (97.30)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://27295 (98.24), maa://32509 (97.00), maa://31008 (95.19), maa://22754 (88.16), maa://70489 (99.44)</t>
+          <t>maa://27295 (98.36), maa://32509 (97.10), maa://31008 (95.31), maa://22754 (88.16), maa://70489 (99.22)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="X4" s="8" t="inlineStr">
         <is>
-          <t>maa://43217 (99.01)</t>
+          <t>maa://43217 (99.10)</t>
         </is>
       </c>
       <c r="Y4" s="19" t="n"/>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="AB4" s="8" t="inlineStr">
         <is>
-          <t>*maa://32658 (77.78)</t>
+          <t>*maa://32658 (78.57)</t>
         </is>
       </c>
       <c r="AC4" s="19" t="n"/>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>*maa://39394 (53.70), *maa://30062 (60.94), ***maa://26209 (12.50)</t>
+          <t>*maa://39394 (53.57), *maa://30062 (61.54), ***maa://26209 (12.50)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (92.16), maa://54105 (98.76), *maa://22744 (80.00)</t>
+          <t>maa://21245 (92.42), maa://54105 (98.74), *maa://22744 (80.00)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="L5" s="8" t="inlineStr">
         <is>
-          <t>maa://22757 (92.81)</t>
+          <t>maa://22757 (93.49)</t>
         </is>
       </c>
       <c r="M5" s="19" t="n"/>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="P5" s="8" t="inlineStr">
         <is>
-          <t>maa://21919 (98.95), maa://21281 (83.33)</t>
+          <t>maa://21919 (99.07), maa://21281 (83.33)</t>
         </is>
       </c>
       <c r="Q5" s="19" t="n"/>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="X5" s="8" t="inlineStr">
         <is>
-          <t>maa://21290 (98.83)</t>
+          <t>maa://21290 (98.94)</t>
         </is>
       </c>
       <c r="Y5" s="19" t="n"/>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="AB5" s="8" t="inlineStr">
         <is>
-          <t>*maa://29863 (60.38), ***maa://22752 (12.50), **maa://26013 (38.46)</t>
+          <t>*maa://29863 (60.00), ***maa://22752 (12.50), **maa://26013 (33.33)</t>
         </is>
       </c>
       <c r="AC5" s="19" t="n"/>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="D6" s="8" t="inlineStr">
         <is>
-          <t>maa://42407 (98.20)</t>
+          <t>maa://42407 (98.31)</t>
         </is>
       </c>
       <c r="E6" s="19" t="n"/>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="H6" s="8" t="inlineStr">
         <is>
-          <t>maa://24370 (98.08)</t>
+          <t>maa://24370 (98.27)</t>
         </is>
       </c>
       <c r="I6" s="19" t="n"/>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="L6" s="8" t="inlineStr">
         <is>
-          <t>maa://24839 (99.59)</t>
+          <t>maa://24839 (99.63)</t>
         </is>
       </c>
       <c r="M6" s="19" t="n"/>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (99.12), maa://30381 (95.45)</t>
+          <t>maa://31836 (99.20), maa://30381 (95.45)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1304,7 +1304,7 @@
       </c>
       <c r="T6" s="8" t="inlineStr">
         <is>
-          <t>maa://37411 (80.85)</t>
+          <t>maa://37411 (83.64)</t>
         </is>
       </c>
       <c r="U6" s="19" t="n"/>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="X6" s="8" t="inlineStr">
         <is>
-          <t>maa://52754 (96.55), maa://71825 (100.00)</t>
+          <t>maa://52754 (96.60), maa://71825 (100.00)</t>
         </is>
       </c>
       <c r="Y6" s="19" t="n"/>
@@ -1336,7 +1336,7 @@
       </c>
       <c r="AB6" s="8" t="inlineStr">
         <is>
-          <t>maa://22739 (89.42)</t>
+          <t>maa://22739 (90.09)</t>
         </is>
       </c>
       <c r="AC6" s="19" t="n"/>
@@ -1352,7 +1352,7 @@
       </c>
       <c r="AF6" s="8" t="inlineStr">
         <is>
-          <t>maa://33152 (84.95)</t>
+          <t>maa://33152 (86.00)</t>
         </is>
       </c>
       <c r="AG6" s="16" t="n"/>
@@ -1370,7 +1370,7 @@
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>maa://21955 (98.58)</t>
+          <t>maa://21955 (98.70)</t>
         </is>
       </c>
       <c r="E7" s="19" t="n"/>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>*maa://22763 (77.94), maa://64972 (94.12)</t>
+          <t>*maa://22763 (78.26), maa://64972 (95.24)</t>
         </is>
       </c>
       <c r="I7" s="19" t="n"/>
@@ -1402,7 +1402,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (98.93), maa://24957 (94.55)</t>
+          <t>maa://28624 (98.99), maa://24957 (92.86)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="P7" s="8" t="inlineStr">
         <is>
-          <t>maa://22750 (97.49)</t>
+          <t>maa://22750 (97.75)</t>
         </is>
       </c>
       <c r="Q7" s="19" t="n"/>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="T7" s="8" t="inlineStr">
         <is>
-          <t>maa://21291 (94.47)</t>
+          <t>maa://21291 (94.95)</t>
         </is>
       </c>
       <c r="U7" s="19" t="n"/>
@@ -1450,7 +1450,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (97.86), maa://22758 (84.35)</t>
+          <t>maa://22399 (98.04), maa://22758 (84.68)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1482,7 +1482,7 @@
       </c>
       <c r="AF7" s="8" t="inlineStr">
         <is>
-          <t>maa://45272 (99.63), *maa://26191 (70.71)</t>
+          <t>maa://45272 (99.67), *maa://26191 (70.71)</t>
         </is>
       </c>
       <c r="AG7" s="16" t="n"/>
@@ -1490,7 +1490,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.11.03 13:29:46</t>
+          <t>更新日期：2025.11.06 13:22:37</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1505,7 +1505,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (92.34)</t>
+          <t>maa://21476 (93.01)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
-          <t>maa://24371 (82.98)</t>
+          <t>maa://24371 (83.94)</t>
         </is>
       </c>
       <c r="I8" s="19" t="n"/>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (92.77), maa://23252 (91.67), maa://37496 (98.55)</t>
+          <t>maa://32931 (93.15), maa://23252 (91.67), maa://37496 (98.59)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (96.23), maa://67587 (98.58)</t>
+          <t>maa://21411 (96.31), maa://67587 (98.68)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1601,7 +1601,7 @@
       </c>
       <c r="AB8" s="8" t="inlineStr">
         <is>
-          <t>maa://25389 (95.80)</t>
+          <t>maa://25389 (96.20)</t>
         </is>
       </c>
       <c r="AC8" s="19" t="n"/>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>maa://24479 (88.28), **maa://21990 (50.00)</t>
+          <t>maa://24479 (89.44), **maa://21990 (50.00)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>maa://22765 (96.81), maa://21915 (83.33)</t>
+          <t>maa://22765 (97.15), maa://21915 (83.33)</t>
         </is>
       </c>
       <c r="E9" s="19" t="n"/>
@@ -1651,7 +1651,7 @@
       </c>
       <c r="H9" s="8" t="inlineStr">
         <is>
-          <t>maa://47450 (80.77), maa://56348 (96.30)</t>
+          <t>maa://47450 (83.33), maa://56348 (96.88)</t>
         </is>
       </c>
       <c r="I9" s="19" t="n"/>
@@ -1667,7 +1667,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (96.23), maa://39552 (89.19)</t>
+          <t>maa://22762 (96.53), maa://39552 (89.61)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1699,7 +1699,7 @@
       </c>
       <c r="T9" s="8" t="inlineStr">
         <is>
-          <t>maa://26222 (99.62)</t>
+          <t>maa://26222 (99.65)</t>
         </is>
       </c>
       <c r="U9" s="19" t="n"/>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://52237 (99.85), maa://26223 (98.34)</t>
+          <t>maa://52237 (99.74), maa://26223 (98.38)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (95.65), maa://40166 (95.71)</t>
+          <t>maa://28711 (95.94), maa://40166 (95.39)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (91.87), maa://66916 (98.78)</t>
+          <t>maa://26206 (91.95), maa://66916 (98.62)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1765,7 +1765,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>maa://54000 (93.04)</t>
+          <t>maa://54000 (93.70)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1781,7 +1781,7 @@
       </c>
       <c r="H10" s="8" t="inlineStr">
         <is>
-          <t>maa://32651 (94.34)</t>
+          <t>maa://32651 (94.64)</t>
         </is>
       </c>
       <c r="I10" s="19" t="n"/>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="L10" s="8" t="inlineStr">
         <is>
-          <t>**maa://24395 (48.15)</t>
+          <t>**maa://24395 (47.27)</t>
         </is>
       </c>
       <c r="M10" s="19" t="n"/>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (93.24), *maa://36669 (75.31)</t>
+          <t>maa://28977 (93.51), *maa://36669 (75.61)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1829,7 +1829,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (99.39), maa://22755 (91.98), maa://63521 (95.66), maa://73485 (100.00)</t>
+          <t>maa://27395 (99.43), maa://22755 (92.27), maa://63521 (96.07), maa://73485 (94.74)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1845,7 +1845,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://45828 (99.44), maa://22301 (97.67), maa://22726 (100.00)</t>
+          <t>maa://45828 (99.50), maa://22301 (97.67), maa://22726 (100.00)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1872,12 +1872,12 @@
       </c>
       <c r="AE10" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF10" s="8" t="inlineStr">
         <is>
-          <t>*maa://25021 (60.22), *maa://22733 (67.12), ***maa://22761 (25.00)</t>
+          <t>maa://74007 (100.00)</t>
         </is>
       </c>
       <c r="AG10" s="16" t="n"/>
@@ -1895,7 +1895,7 @@
       </c>
       <c r="D11" s="8" t="inlineStr">
         <is>
-          <t>maa://36707 (99.70)</t>
+          <t>maa://36707 (99.72)</t>
         </is>
       </c>
       <c r="E11" s="19" t="n"/>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="L11" s="8" t="inlineStr">
         <is>
-          <t>maa://21287 (94.54)</t>
+          <t>maa://21287 (94.72)</t>
         </is>
       </c>
       <c r="M11" s="19" t="n"/>
@@ -1943,7 +1943,7 @@
       </c>
       <c r="P11" s="8" t="inlineStr">
         <is>
-          <t>maa://45557 (95.31)</t>
+          <t>maa://45557 (95.71)</t>
         </is>
       </c>
       <c r="Q11" s="19" t="n"/>
@@ -1959,7 +1959,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (94.42), maa://22501 (99.61), maa://64808 (100.00), maa://45521 (94.12)</t>
+          <t>maa://22747 (94.92), maa://22501 (99.63), maa://64808 (99.59), maa://45521 (94.20)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1975,7 +1975,7 @@
       </c>
       <c r="X11" s="8" t="inlineStr">
         <is>
-          <t>maa://36713 (99.42)</t>
+          <t>maa://36713 (99.46)</t>
         </is>
       </c>
       <c r="Y11" s="19" t="n"/>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="AB11" s="8" t="inlineStr">
         <is>
-          <t>maa://29912 (99.77), maa://22516 (86.52)</t>
+          <t>maa://29912 (99.78), maa://22516 (86.52)</t>
         </is>
       </c>
       <c r="AC11" s="19" t="n"/>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="AF11" s="8" t="inlineStr">
         <is>
-          <t>maa://31203 (98.94)</t>
+          <t>maa://31203 (99.02)</t>
         </is>
       </c>
       <c r="AG11" s="16" t="n"/>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>maa://36678 (97.78), maa://30766 (91.67)</t>
+          <t>maa://36678 (97.92), maa://30766 (91.67)</t>
         </is>
       </c>
       <c r="E12" s="19" t="n"/>
@@ -2041,7 +2041,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (94.06), maa://54294 (97.81)</t>
+          <t>maa://21867 (94.31), maa://54294 (98.07)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (98.37), maa://64046 (98.82)</t>
+          <t>maa://63896 (98.51), maa://64046 (98.91)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2073,7 +2073,7 @@
       </c>
       <c r="P12" s="8" t="inlineStr">
         <is>
-          <t>maa://57541 (90.20)</t>
+          <t>maa://57541 (91.23)</t>
         </is>
       </c>
       <c r="Q12" s="19" t="n"/>
@@ -2100,12 +2100,12 @@
       </c>
       <c r="W12" s="19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://37962 (98.78), maa://21485 (83.27), maa://22753 (93.20)</t>
+          <t>maa://37962 (98.84), maa://21485 (83.83), maa://22753 (93.28), maa://73860 (92.45)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://36677 (99.21), maa://23669 (94.96), maa://39872 (98.73)</t>
+          <t>maa://36677 (99.11), maa://23669 (95.00), maa://39872 (98.24)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>maa://28932 (95.36)</t>
+          <t>maa://28932 (95.69)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2155,7 +2155,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (97.33), maa://36673 (95.06), maa://25001 (89.69)</t>
+          <t>maa://24999 (97.54), maa://36673 (95.32), maa://25001 (89.00)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2166,12 +2166,12 @@
       </c>
       <c r="G13" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.38), maa://66545 (98.80)</t>
+          <t>*maa://21248 (74.84), maa://66545 (98.68), *maa://22728 (70.19)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2203,7 +2203,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (97.83), maa://22583 (91.08), *maa://22500 (72.06)</t>
+          <t>maa://22676 (97.86), maa://22583 (92.48), *maa://22500 (72.46)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2235,7 +2235,7 @@
       </c>
       <c r="X13" s="8" t="inlineStr">
         <is>
-          <t>maa://34957 (95.45)</t>
+          <t>maa://34957 (95.57)</t>
         </is>
       </c>
       <c r="Y13" s="19" t="n"/>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (94.98)</t>
+          <t>maa://39883 (95.31)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>maa://30764 (95.35)</t>
+          <t>maa://30764 (95.51)</t>
         </is>
       </c>
       <c r="E14" s="19" t="n"/>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (99.26), maa://36682 (98.43), maa://26245 (97.13), maa://21288 (96.43)</t>
+          <t>maa://39841 (99.29), maa://36682 (98.46), maa://26245 (97.13), maa://21288 (96.43)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="P14" s="8" t="inlineStr">
         <is>
-          <t>maa://23250 (99.68), maa://20107 (87.50), maa://22772 (100.00), maa://68732 (100.00)</t>
+          <t>maa://23250 (99.65), maa://20107 (87.50), maa://22772 (100.00), maa://68732 (100.00)</t>
         </is>
       </c>
       <c r="Q14" s="19" t="n"/>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://42751 (99.20), maa://22521 (96.20)</t>
+          <t>maa://42751 (99.28), maa://22521 (96.59)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="X14" s="8" t="inlineStr">
         <is>
-          <t>maa://37468 (98.51)</t>
+          <t>maa://37468 (98.66)</t>
         </is>
       </c>
       <c r="Y14" s="19" t="n"/>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="AB14" s="8" t="inlineStr">
         <is>
-          <t>maa://22764 (99.16)</t>
+          <t>maa://22764 (99.24)</t>
         </is>
       </c>
       <c r="AC14" s="19" t="n"/>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (87.88), maa://45058 (98.47), maa://22734 (85.19), *maa://36048 (77.23), maa://69928 (97.10)</t>
+          <t>maa://22743 (88.24), maa://45058 (98.55), maa://22734 (85.29), *maa://36048 (77.88), maa://69928 (97.70)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2431,7 +2431,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (97.82), maa://21478 (90.91)</t>
+          <t>maa://24304 (98.03), maa://21478 (90.91)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2447,7 +2447,7 @@
       </c>
       <c r="L15" s="8" t="inlineStr">
         <is>
-          <t>*maa://21334 (72.00), maa://73742 (100.00)</t>
+          <t>*maa://21334 (72.73), maa://73742 (100.00)</t>
         </is>
       </c>
       <c r="M15" s="19" t="n"/>
@@ -2463,7 +2463,7 @@
       </c>
       <c r="P15" s="8" t="inlineStr">
         <is>
-          <t>maa://24762 (97.97), *maa://22727 (70.00)</t>
+          <t>maa://24762 (98.12), *maa://22727 (70.00)</t>
         </is>
       </c>
       <c r="Q15" s="19" t="n"/>
@@ -2479,7 +2479,7 @@
       </c>
       <c r="T15" s="8" t="inlineStr">
         <is>
-          <t>maa://23892 (98.12)</t>
+          <t>maa://23892 (98.25)</t>
         </is>
       </c>
       <c r="U15" s="19" t="n"/>
@@ -2495,7 +2495,7 @@
       </c>
       <c r="X15" s="8" t="inlineStr">
         <is>
-          <t>maa://38786 (93.62), maa://56102 (100.00)</t>
+          <t>maa://38786 (94.00), maa://56102 (100.00)</t>
         </is>
       </c>
       <c r="Y15" s="19" t="n"/>
@@ -2527,7 +2527,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://36666 (96.74), maa://21364 (84.34), *maa://22766 (71.13), maa://68306 (89.51)</t>
+          <t>maa://36666 (96.94), maa://21364 (84.58), *maa://22766 (71.13), maa://68306 (90.16)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2545,7 +2545,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://37650 (99.82), maa://21441 (96.65), maa://36679 (94.55)</t>
+          <t>maa://37650 (99.76), maa://21441 (96.67), maa://36679 (94.55)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2593,7 +2593,7 @@
       </c>
       <c r="P16" s="8" t="inlineStr">
         <is>
-          <t>maa://28504 (97.22)</t>
+          <t>maa://28504 (97.40)</t>
         </is>
       </c>
       <c r="Q16" s="19" t="n"/>
@@ -2609,7 +2609,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://36674 (98.10), maa://22729 (96.82), *maa://28648 (77.89)</t>
+          <t>maa://36674 (98.20), maa://22729 (97.18), *maa://28648 (77.89)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="X16" s="8" t="inlineStr">
         <is>
-          <t>maa://28501 (99.36), maa://28051 (97.37)</t>
+          <t>maa://28501 (99.44), maa://28051 (97.37)</t>
         </is>
       </c>
       <c r="Y16" s="19" t="n"/>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="AB16" s="8" t="inlineStr">
         <is>
-          <t>maa://26228 (98.27)</t>
+          <t>maa://26228 (98.17)</t>
         </is>
       </c>
       <c r="AC16" s="19" t="n"/>
@@ -2657,7 +2657,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>maa://23911 (91.48), maa://67613 (99.73), maa://27755 (93.75)</t>
+          <t>maa://23911 (91.72), maa://67613 (99.32), maa://27755 (93.75)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2675,7 +2675,7 @@
       </c>
       <c r="D17" s="8" t="inlineStr">
         <is>
-          <t>maa://21624 (88.46), maa://56358 (100.00)</t>
+          <t>maa://21624 (88.68), maa://56358 (100.00)</t>
         </is>
       </c>
       <c r="E17" s="19" t="n"/>
@@ -2691,7 +2691,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://39599 (98.69), maa://22430 (90.42)</t>
+          <t>maa://39599 (98.81), maa://22430 (90.50)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2707,7 +2707,7 @@
       </c>
       <c r="L17" s="8" t="inlineStr">
         <is>
-          <t>maa://21679 (89.83)</t>
+          <t>maa://21679 (91.18)</t>
         </is>
       </c>
       <c r="M17" s="19" t="n"/>
@@ -2723,7 +2723,7 @@
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (83.59), maa://56238 (98.40)</t>
+          <t>maa://23890 (83.72), maa://56238 (98.56)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2739,7 +2739,7 @@
       </c>
       <c r="T17" s="8" t="inlineStr">
         <is>
-          <t>*maa://42324 (74.04)</t>
+          <t>*maa://42324 (75.23)</t>
         </is>
       </c>
       <c r="U17" s="19" t="n"/>
@@ -2787,7 +2787,7 @@
       </c>
       <c r="AF17" s="8" t="inlineStr">
         <is>
-          <t>maa://50136 (99.26)</t>
+          <t>maa://50136 (99.31)</t>
         </is>
       </c>
       <c r="AG17" s="16" t="n"/>
@@ -2805,7 +2805,7 @@
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>maa://24570 (98.57)</t>
+          <t>maa://24570 (98.68)</t>
         </is>
       </c>
       <c r="E18" s="19" t="n"/>
@@ -2821,7 +2821,7 @@
       </c>
       <c r="H18" s="8" t="inlineStr">
         <is>
-          <t>maa://24421 (96.04)</t>
+          <t>maa://24421 (96.34)</t>
         </is>
       </c>
       <c r="I18" s="19" t="n"/>
@@ -2837,7 +2837,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://52226 (99.68), maa://22466 (92.95)</t>
+          <t>maa://52226 (99.71), maa://22466 (92.95)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2853,7 +2853,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://54153 (99.76), maa://24379 (100.00), maa://24380 (100.00)</t>
+          <t>maa://54153 (99.79), maa://24379 (100.00), maa://24380 (100.00)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="T18" s="8" t="inlineStr">
         <is>
-          <t>maa://24385 (97.70)</t>
+          <t>maa://24385 (97.78)</t>
         </is>
       </c>
       <c r="U18" s="19" t="n"/>
@@ -2885,7 +2885,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (99.11), maa://22741 (93.75)</t>
+          <t>maa://21917 (99.23), maa://22741 (94.12)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2901,7 +2901,7 @@
       </c>
       <c r="AB18" s="8" t="inlineStr">
         <is>
-          <t>maa://24393 (99.25)</t>
+          <t>maa://24393 (99.31)</t>
         </is>
       </c>
       <c r="AC18" s="19" t="n"/>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://47854 (95.37), *maa://68715 (75.00)</t>
+          <t>maa://47854 (95.32), *maa://68715 (75.00)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -2935,7 +2935,7 @@
       </c>
       <c r="D19" s="8" t="inlineStr">
         <is>
-          <t>maa://62850 (99.41)</t>
+          <t>maa://62850 (99.46)</t>
         </is>
       </c>
       <c r="E19" s="19" t="n"/>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="L19" s="8" t="inlineStr">
         <is>
-          <t>maa://39347 (98.41), maa://56392 (100.00)</t>
+          <t>maa://39347 (98.55), maa://56392 (100.00)</t>
         </is>
       </c>
       <c r="M19" s="19" t="n"/>
@@ -2999,7 +2999,7 @@
       </c>
       <c r="T19" s="8" t="inlineStr">
         <is>
-          <t>maa://24386 (99.63)</t>
+          <t>maa://24386 (99.66)</t>
         </is>
       </c>
       <c r="U19" s="19" t="n"/>
@@ -3015,7 +3015,7 @@
       </c>
       <c r="X19" s="8" t="inlineStr">
         <is>
-          <t>maa://31386 (98.18), maa://58490 (89.29)</t>
+          <t>maa://31386 (98.33), maa://58490 (91.43)</t>
         </is>
       </c>
       <c r="Y19" s="19" t="n"/>
@@ -3031,7 +3031,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (89.33), *maa://36668 (70.83)</t>
+          <t>maa://30709 (90.06), *maa://36668 (71.54)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3042,12 +3042,12 @@
       </c>
       <c r="AE19" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF19" s="8" t="inlineStr">
         <is>
-          <t>*maa://21663 (68.42), maa://52239 (89.23)</t>
+          <t>maa://52239 (91.03)</t>
         </is>
       </c>
       <c r="AG19" s="16" t="n"/>
@@ -3065,7 +3065,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://25198 (97.88), maa://36680 (99.25), maa://21432 (91.67)</t>
+          <t>maa://25198 (98.04), maa://36680 (99.17), maa://21432 (91.74)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3081,7 +3081,7 @@
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>maa://22864 (96.59)</t>
+          <t>maa://22864 (96.77)</t>
         </is>
       </c>
       <c r="I20" s="19" t="n"/>
@@ -3097,7 +3097,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (96.09)</t>
+          <t>maa://41331 (96.36)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3113,7 +3113,7 @@
       </c>
       <c r="P20" s="8" t="inlineStr">
         <is>
-          <t>maa://37442 (98.94)</t>
+          <t>maa://37442 (99.03)</t>
         </is>
       </c>
       <c r="Q20" s="19" t="n"/>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="T20" s="8" t="inlineStr">
         <is>
-          <t>maa://29113 (94.95)</t>
+          <t>maa://29113 (95.37)</t>
         </is>
       </c>
       <c r="U20" s="19" t="n"/>
@@ -3145,7 +3145,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://56241 (98.56), maa://50085 (97.14), maa://49976 (88.57)</t>
+          <t>maa://56241 (98.53), maa://50085 (97.33), maa://49976 (88.57)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3195,7 +3195,7 @@
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>maa://21261 (99.21)</t>
+          <t>maa://21261 (99.28)</t>
         </is>
       </c>
       <c r="E21" s="19" t="n"/>
@@ -3211,7 +3211,7 @@
       </c>
       <c r="H21" s="8" t="inlineStr">
         <is>
-          <t>maa://24372 (99.18)</t>
+          <t>maa://24372 (99.25)</t>
         </is>
       </c>
       <c r="I21" s="19" t="n"/>
@@ -3227,7 +3227,7 @@
       </c>
       <c r="L21" s="8" t="inlineStr">
         <is>
-          <t>maa://31731 (97.28)</t>
+          <t>maa://31731 (97.42)</t>
         </is>
       </c>
       <c r="M21" s="19" t="n"/>
@@ -3243,7 +3243,7 @@
       </c>
       <c r="P21" s="8" t="inlineStr">
         <is>
-          <t>maa://24381 (84.78)</t>
+          <t>maa://24381 (85.42)</t>
         </is>
       </c>
       <c r="Q21" s="19" t="n"/>
@@ -3259,7 +3259,7 @@
       </c>
       <c r="T21" s="8" t="inlineStr">
         <is>
-          <t>maa://21993 (92.11)</t>
+          <t>maa://21993 (92.50)</t>
         </is>
       </c>
       <c r="U21" s="19" t="n"/>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (98.66), maa://20110 (87.18)</t>
+          <t>maa://34946 (98.56), maa://20110 (87.18)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3291,7 +3291,7 @@
       </c>
       <c r="AB21" s="8" t="inlineStr">
         <is>
-          <t>maa://21443 (87.73), maa://52223 (88.42)</t>
+          <t>maa://21443 (87.86), maa://52223 (89.53)</t>
         </is>
       </c>
       <c r="AC21" s="19" t="n"/>
@@ -3307,7 +3307,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22432 (95.32), maa://22524 (83.28), maa://64221 (98.23)</t>
+          <t>maa://22432 (95.62), maa://22524 (83.00), maa://64221 (98.20)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>maa://25236 (99.23)</t>
+          <t>maa://25236 (99.30)</t>
         </is>
       </c>
       <c r="I22" s="19" t="n"/>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>maa://27127 (84.71), maa://66865 (99.64), *maa://22751 (71.26)</t>
+          <t>maa://27127 (85.17), maa://66865 (99.68), *maa://22751 (71.26)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="T22" s="8" t="inlineStr">
         <is>
-          <t>maa://38495 (86.27)</t>
+          <t>maa://38495 (86.79)</t>
         </is>
       </c>
       <c r="U22" s="19" t="n"/>
@@ -3405,7 +3405,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://37649 (95.58), maa://21282 (99.05)</t>
+          <t>maa://37649 (95.95), maa://21282 (99.07)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="AB22" s="8" t="inlineStr">
         <is>
-          <t>maa://23656 (99.61)</t>
+          <t>maa://23656 (99.64)</t>
         </is>
       </c>
       <c r="AC22" s="19" t="n"/>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="AF22" s="8" t="inlineStr">
         <is>
-          <t>maa://29658 (97.48)</t>
+          <t>maa://29658 (97.62)</t>
         </is>
       </c>
       <c r="AG22" s="16" t="n"/>
@@ -3455,7 +3455,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>*maa://41753 (70.24), **maa://28036 (30.85)</t>
+          <t>*maa://41753 (71.59), **maa://28036 (31.58)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3487,7 +3487,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (98.92), maa://39875 (95.28)</t>
+          <t>maa://39756 (99.00), maa://39875 (95.45)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3503,7 +3503,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (97.40), maa://29748 (82.50), *maa://37566 (79.41)</t>
+          <t>maa://30587 (97.64), maa://29748 (83.09), *maa://37566 (79.41)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="T23" s="8" t="inlineStr">
         <is>
-          <t>maa://31212 (96.05), maa://24387 (85.42), maa://67084 (90.00)</t>
+          <t>maa://31212 (96.25), maa://24387 (86.00), maa://67084 (90.91)</t>
         </is>
       </c>
       <c r="U23" s="19" t="n"/>
@@ -3535,7 +3535,7 @@
       </c>
       <c r="X23" s="8" t="inlineStr">
         <is>
-          <t>*maa://28503 (61.24)</t>
+          <t>*maa://28503 (62.23)</t>
         </is>
       </c>
       <c r="Y23" s="19" t="n"/>
@@ -3551,7 +3551,7 @@
       </c>
       <c r="AB23" s="8" t="inlineStr">
         <is>
-          <t>maa://29652 (97.37)</t>
+          <t>maa://29652 (97.52)</t>
         </is>
       </c>
       <c r="AC23" s="19" t="n"/>
@@ -3567,7 +3567,7 @@
       </c>
       <c r="AF23" s="8" t="inlineStr">
         <is>
-          <t>maa://31489 (98.75)</t>
+          <t>maa://31489 (98.84)</t>
         </is>
       </c>
       <c r="AG23" s="16" t="n"/>
@@ -3585,7 +3585,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (86.71), maa://46650 (92.49)</t>
+          <t>maa://24368 (87.35), maa://46650 (93.01)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3649,7 +3649,7 @@
       </c>
       <c r="T24" s="8" t="inlineStr">
         <is>
-          <t>maa://73341 (98.00)</t>
+          <t>maa://73341 (98.25)</t>
         </is>
       </c>
       <c r="U24" s="19" t="n"/>
@@ -3665,7 +3665,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (97.29), maa://23504 (94.12), maa://25141 (80.62), maa://52227 (97.55), maa://36663 (80.36)</t>
+          <t>maa://29988 (97.41), maa://23504 (94.14), maa://25141 (80.98), maa://52227 (97.78), maa://36663 (80.36)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3681,7 +3681,7 @@
       </c>
       <c r="AB24" s="8" t="inlineStr">
         <is>
-          <t>maa://39349 (98.08)</t>
+          <t>maa://39349 (98.21)</t>
         </is>
       </c>
       <c r="AC24" s="19" t="n"/>
@@ -3697,7 +3697,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://64165 (99.25), *maa://22523 (79.82), maa://29910 (94.20), maa://45831 (94.29)</t>
+          <t>maa://64165 (99.33), *maa://22523 (79.82), maa://29910 (94.20), maa://45831 (94.59)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3715,7 +3715,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (96.99), maa://63016 (99.43)</t>
+          <t>maa://29753 (97.19), maa://63016 (99.48)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3731,7 +3731,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>maa://29063 (80.32), *maa://25311 (71.33), maa://45047 (87.50)</t>
+          <t>maa://29063 (80.62), *maa://25311 (71.05), maa://45047 (87.91)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3747,7 +3747,7 @@
       </c>
       <c r="L25" s="8" t="inlineStr">
         <is>
-          <t>maa://24378 (94.12), maa://68415 (94.74)</t>
+          <t>maa://24378 (94.19), maa://68415 (91.67)</t>
         </is>
       </c>
       <c r="M25" s="19" t="n"/>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="P25" s="8" t="inlineStr">
         <is>
-          <t>maa://24382 (97.06)</t>
+          <t>maa://24382 (97.18)</t>
         </is>
       </c>
       <c r="Q25" s="19" t="n"/>
@@ -3779,7 +3779,7 @@
       </c>
       <c r="T25" s="8" t="inlineStr">
         <is>
-          <t>maa://20109 (97.23), maa://22545 (100.00)</t>
+          <t>maa://20109 (97.42), maa://22545 (99.87)</t>
         </is>
       </c>
       <c r="U25" s="19" t="n"/>
@@ -3795,7 +3795,7 @@
       </c>
       <c r="X25" s="8" t="inlineStr">
         <is>
-          <t>maa://29890 (93.33)</t>
+          <t>maa://29890 (93.68)</t>
         </is>
       </c>
       <c r="Y25" s="19" t="n"/>
@@ -3811,7 +3811,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (93.72), *maa://24516 (78.43), maa://68311 (98.05), maa://26001 (81.97)</t>
+          <t>maa://31215 (93.90), maa://68311 (98.49), *maa://24516 (78.43), maa://26001 (81.97)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3827,7 +3827,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (98.65), maa://36676 (99.86), maa://24621 (96.93), maa://22771 (88.89), maa://37772 (87.50)</t>
+          <t>maa://20108 (98.83), maa://36676 (99.87), maa://24621 (96.95), maa://22771 (88.89), maa://37772 (87.50)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3845,7 +3845,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://56374 (100.00), maa://41802 (97.87)</t>
+          <t>maa://56374 (100.00), maa://41802 (98.08)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3861,7 +3861,7 @@
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
-          <t>maa://56240 (95.56), maa://24913 (92.74)</t>
+          <t>maa://56240 (95.67), maa://24913 (92.86)</t>
         </is>
       </c>
       <c r="I26" s="19" t="n"/>
@@ -3893,7 +3893,7 @@
       </c>
       <c r="P26" s="8" t="inlineStr">
         <is>
-          <t>maa://56625 (98.98), maa://39870 (95.35)</t>
+          <t>maa://56625 (99.09), maa://39870 (95.35)</t>
         </is>
       </c>
       <c r="Q26" s="19" t="n"/>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="X26" s="8" t="inlineStr">
         <is>
-          <t>maa://24389 (98.77)</t>
+          <t>maa://24389 (98.85)</t>
         </is>
       </c>
       <c r="Y26" s="19" t="n"/>
@@ -3941,7 +3941,7 @@
       </c>
       <c r="AB26" s="8" t="inlineStr">
         <is>
-          <t>maa://42235 (98.83)</t>
+          <t>maa://42235 (98.93)</t>
         </is>
       </c>
       <c r="AC26" s="19" t="n"/>
@@ -3957,7 +3957,7 @@
       </c>
       <c r="AF26" s="8" t="inlineStr">
         <is>
-          <t>*maa://30511 (72.22), **maa://29760 (45.45)</t>
+          <t>*maa://30511 (73.40), **maa://29760 (45.45)</t>
         </is>
       </c>
       <c r="AG26" s="16" t="n"/>
@@ -3991,7 +3991,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>maa://39601 (93.85), maa://34494 (96.15)</t>
+          <t>maa://39601 (94.58), maa://34494 (96.23)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4007,7 +4007,7 @@
       </c>
       <c r="L27" s="8" t="inlineStr">
         <is>
-          <t>maa://28071 (91.67)</t>
+          <t>maa://28071 (92.21)</t>
         </is>
       </c>
       <c r="M27" s="19" t="n"/>
@@ -4023,7 +4023,7 @@
       </c>
       <c r="P27" s="8" t="inlineStr">
         <is>
-          <t>maa://56400 (91.30)</t>
+          <t>maa://56400 (92.00)</t>
         </is>
       </c>
       <c r="Q27" s="19" t="n"/>
@@ -4039,7 +4039,7 @@
       </c>
       <c r="T27" s="8" t="inlineStr">
         <is>
-          <t>maa://30624 (91.32)</t>
+          <t>maa://30624 (91.95)</t>
         </is>
       </c>
       <c r="U27" s="19" t="n"/>
@@ -4087,7 +4087,7 @@
       </c>
       <c r="AF27" s="8" t="inlineStr">
         <is>
-          <t>maa://24023 (98.22)</t>
+          <t>maa://24023 (98.37)</t>
         </is>
       </c>
       <c r="AG27" s="16" t="n"/>
@@ -4105,7 +4105,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (96.44), maa://25725 (85.71)</t>
+          <t>maa://24465 (96.64), maa://25725 (86.03)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4137,7 +4137,7 @@
       </c>
       <c r="L28" s="8" t="inlineStr">
         <is>
-          <t>maa://30770 (91.15)</t>
+          <t>maa://30770 (90.83)</t>
         </is>
       </c>
       <c r="M28" s="19" t="n"/>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="T28" s="8" t="inlineStr">
         <is>
-          <t>maa://29765 (94.92), maa://23263 (96.91)</t>
+          <t>maa://29765 (95.25), maa://23263 (97.14)</t>
         </is>
       </c>
       <c r="U28" s="19" t="n"/>
@@ -4185,7 +4185,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (97.88), maa://41749 (97.31)</t>
+          <t>maa://39929 (97.98), maa://41749 (97.43)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4217,7 +4217,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (94.64), maa://65700 (98.72)</t>
+          <t>maa://36660 (94.81), maa://65700 (98.73)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4235,7 +4235,7 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>maa://31694 (99.45)</t>
+          <t>maa://31694 (99.48)</t>
         </is>
       </c>
       <c r="E29" s="19" t="n"/>
@@ -4267,7 +4267,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (98.21), maa://31400 (98.25), maa://28440 (86.98)</t>
+          <t>maa://28432 (98.36), maa://31400 (98.30), maa://28440 (87.13)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4283,7 +4283,7 @@
       </c>
       <c r="P29" s="8" t="inlineStr">
         <is>
-          <t>maa://54169 (98.14)</t>
+          <t>maa://54169 (97.83)</t>
         </is>
       </c>
       <c r="Q29" s="19" t="n"/>
@@ -4347,7 +4347,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://42865 (93.99)</t>
+          <t>maa://42865 (94.23)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4365,7 +4365,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (96.25), maa://64191 (96.55)</t>
+          <t>maa://45792 (96.43), maa://64191 (97.06)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4397,7 +4397,7 @@
       </c>
       <c r="L30" s="8" t="inlineStr">
         <is>
-          <t>maa://30442 (98.12)</t>
+          <t>maa://30442 (98.21)</t>
         </is>
       </c>
       <c r="M30" s="19" t="n"/>
@@ -4413,7 +4413,7 @@
       </c>
       <c r="P30" s="8" t="inlineStr">
         <is>
-          <t>maa://21442 (99.59), maa://68394 (100.00), maa://66611 (100.00)</t>
+          <t>maa://21442 (99.60), maa://68394 (100.00), maa://66611 (100.00)</t>
         </is>
       </c>
       <c r="Q30" s="19" t="n"/>
@@ -4445,7 +4445,7 @@
       </c>
       <c r="X30" s="8" t="inlineStr">
         <is>
-          <t>maa://39477 (97.26)</t>
+          <t>maa://39477 (97.44)</t>
         </is>
       </c>
       <c r="Y30" s="19" t="n"/>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="AB30" s="8" t="inlineStr">
         <is>
-          <t>maa://42979 (99.62), maa://45822 (100.00), maa://45045 (94.12)</t>
+          <t>maa://42979 (99.61), maa://45822 (100.00), maa://45045 (94.12)</t>
         </is>
       </c>
       <c r="AC30" s="19" t="n"/>
@@ -4527,7 +4527,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (98.51), maa://36258 (93.97), maa://43904 (90.38)</t>
+          <t>maa://35926 (98.64), maa://36258 (94.09), maa://43904 (91.94)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="T31" s="8" t="inlineStr">
         <is>
-          <t>maa://30711 (97.18), maa://30768 (100.00)</t>
+          <t>maa://30711 (97.37), maa://30768 (100.00)</t>
         </is>
       </c>
       <c r="U31" s="19" t="n"/>
@@ -4591,7 +4591,7 @@
       </c>
       <c r="AB31" s="8" t="inlineStr">
         <is>
-          <t>maa://66997 (96.97)</t>
+          <t>maa://66997 (97.30)</t>
         </is>
       </c>
       <c r="AC31" s="19" t="n"/>
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://36667 (99.69), maa://21895 (98.04), maa://22760 (100.00)</t>
+          <t>maa://36667 (99.71), maa://21895 (98.06), maa://22760 (100.00)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4657,7 +4657,7 @@
       </c>
       <c r="L32" s="8" t="inlineStr">
         <is>
-          <t>maa://28065 (97.44)</t>
+          <t>maa://28065 (97.62)</t>
         </is>
       </c>
       <c r="M32" s="19" t="n"/>
@@ -4689,7 +4689,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (99.39), maa://41108 (88.33), maa://41238 (98.22), maa://45523 (100.00)</t>
+          <t>maa://42859 (99.45), maa://41108 (88.89), maa://41238 (98.26), maa://45523 (100.00)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4705,7 +4705,7 @@
       </c>
       <c r="X32" s="8" t="inlineStr">
         <is>
-          <t>maa://64104 (97.63)</t>
+          <t>maa://64104 (97.33)</t>
         </is>
       </c>
       <c r="Y32" s="19" t="n"/>
@@ -4737,7 +4737,7 @@
       </c>
       <c r="AF32" s="8" t="inlineStr">
         <is>
-          <t>maa://42408 (95.74)</t>
+          <t>maa://42408 (95.92)</t>
         </is>
       </c>
       <c r="AG32" s="16" t="n"/>
@@ -4803,7 +4803,7 @@
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (95.17), maa://69135 (98.91), maa://73357 (100.00)</t>
+          <t>maa://21956 (95.36), maa://69135 (98.96), maa://73357 (100.00)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4819,7 +4819,7 @@
       </c>
       <c r="T33" s="8" t="inlineStr">
         <is>
-          <t>maa://45558 (90.48)</t>
+          <t>maa://45558 (90.91)</t>
         </is>
       </c>
       <c r="U33" s="19" t="n"/>
@@ -4851,7 +4851,7 @@
       </c>
       <c r="AB33" s="8" t="inlineStr">
         <is>
-          <t>maa://73340 (99.56), maa://73523 (100.00)</t>
+          <t>maa://73340 (99.59), maa://73523 (95.65)</t>
         </is>
       </c>
       <c r="AC33" s="19" t="n"/>
@@ -4901,7 +4901,7 @@
       </c>
       <c r="H34" s="8" t="inlineStr">
         <is>
-          <t>maa://66817 (99.15)</t>
+          <t>maa://66817 (99.25)</t>
         </is>
       </c>
       <c r="I34" s="19" t="n"/>
@@ -4933,7 +4933,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://56235 (99.51), maa://48817 (99.38)</t>
+          <t>maa://56235 (99.57), maa://48817 (99.44)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -4949,7 +4949,7 @@
       </c>
       <c r="T34" s="8" t="inlineStr">
         <is>
-          <t>maa://24526 (97.69)</t>
+          <t>maa://24526 (97.82)</t>
         </is>
       </c>
       <c r="U34" s="19" t="n"/>
@@ -4960,12 +4960,12 @@
       </c>
       <c r="W34" s="19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="X34" s="19" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>maa://74001 (100.00)</t>
         </is>
       </c>
       <c r="Y34" s="19" t="n"/>
@@ -4981,7 +4981,7 @@
       </c>
       <c r="AB34" s="8" t="inlineStr">
         <is>
-          <t>maa://64329 (98.78)</t>
+          <t>maa://64329 (98.92)</t>
         </is>
       </c>
       <c r="AC34" s="19" t="n"/>
@@ -4997,7 +4997,7 @@
       </c>
       <c r="AF34" s="8" t="inlineStr">
         <is>
-          <t>maa://32650 (89.55)</t>
+          <t>maa://32650 (90.28)</t>
         </is>
       </c>
       <c r="AG34" s="16" t="n"/>
@@ -5047,7 +5047,7 @@
       </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
-          <t>maa://41296 (99.43)</t>
+          <t>maa://41296 (99.48)</t>
         </is>
       </c>
       <c r="M35" s="19" t="n"/>
@@ -5079,7 +5079,7 @@
       </c>
       <c r="T35" s="8" t="inlineStr">
         <is>
-          <t>maa://24842 (97.35)</t>
+          <t>maa://24842 (97.44)</t>
         </is>
       </c>
       <c r="U35" s="19" t="n"/>
@@ -5127,7 +5127,7 @@
       </c>
       <c r="AF35" s="8" t="inlineStr">
         <is>
-          <t>maa://39479 (94.29)</t>
+          <t>maa://39479 (94.52)</t>
         </is>
       </c>
       <c r="AG35" s="16" t="n"/>
@@ -5161,7 +5161,7 @@
       </c>
       <c r="H36" s="8" t="inlineStr">
         <is>
-          <t>maa://24375 (95.51)</t>
+          <t>maa://24375 (95.74)</t>
         </is>
       </c>
       <c r="I36" s="19" t="n"/>
@@ -5177,7 +5177,7 @@
       </c>
       <c r="L36" s="8" t="inlineStr">
         <is>
-          <t>maa://42240 (99.08)</t>
+          <t>maa://42240 (99.18)</t>
         </is>
       </c>
       <c r="M36" s="19" t="n"/>
@@ -5209,7 +5209,7 @@
       </c>
       <c r="T36" s="8" t="inlineStr">
         <is>
-          <t>maa://27613 (99.65)</t>
+          <t>maa://27613 (99.67)</t>
         </is>
       </c>
       <c r="U36" s="19" t="n"/>
@@ -5291,7 +5291,7 @@
       </c>
       <c r="H37" s="8" t="inlineStr">
         <is>
-          <t>*maa://24374 (62.32)</t>
+          <t>*maa://24374 (62.86)</t>
         </is>
       </c>
       <c r="I37" s="19" t="n"/>
@@ -5307,7 +5307,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (99.00), maa://56336 (99.45), maa://47069 (88.68), maa://45789 (100.00)</t>
+          <t>maa://45718 (99.04), maa://56336 (99.45), maa://47069 (89.66), maa://45789 (100.00)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5323,7 +5323,7 @@
       </c>
       <c r="P37" s="8" t="inlineStr">
         <is>
-          <t>maa://21280 (98.00), *maa://21239 (70.59)</t>
+          <t>maa://21280 (98.12), *maa://21239 (70.59)</t>
         </is>
       </c>
       <c r="Q37" s="19" t="n"/>
@@ -5339,7 +5339,7 @@
       </c>
       <c r="T37" s="8" t="inlineStr">
         <is>
-          <t>*maa://39354 (58.62)</t>
+          <t>*maa://39354 (61.29)</t>
         </is>
       </c>
       <c r="U37" s="19" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="L38" s="8" t="inlineStr">
         <is>
-          <t>maa://39384 (99.46), maa://49735 (88.24)</t>
+          <t>maa://39384 (99.51), maa://49735 (90.00)</t>
         </is>
       </c>
       <c r="M38" s="19" t="n"/>
@@ -5437,7 +5437,7 @@
       </c>
       <c r="P38" s="8" t="inlineStr">
         <is>
-          <t>maa://24383 (84.82)</t>
+          <t>maa://24383 (85.65)</t>
         </is>
       </c>
       <c r="Q38" s="19" t="n"/>
@@ -5453,7 +5453,7 @@
       </c>
       <c r="T38" s="8" t="inlineStr">
         <is>
-          <t>maa://30713 (98.72)</t>
+          <t>maa://30713 (98.81)</t>
         </is>
       </c>
       <c r="U38" s="19" t="n"/>
@@ -5485,7 +5485,7 @@
       </c>
       <c r="AF38" s="8" t="inlineStr">
         <is>
-          <t>maa://36697 (95.93), maa://68397 (98.93)</t>
+          <t>maa://36697 (96.02), maa://68397 (99.07)</t>
         </is>
       </c>
       <c r="AG38" s="16" t="n"/>
@@ -5519,7 +5519,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://45059 (95.26), maa://25199 (85.03), maa://30434 (95.69), maa://44165 (85.71)</t>
+          <t>maa://45059 (95.63), maa://25199 (85.23), maa://30434 (95.69), maa://44165 (85.71)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://47093 (98.79), maa://24709 (94.64)</t>
+          <t>maa://47093 (98.92), maa://24709 (94.83)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5567,7 +5567,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (96.28), maa://45790 (89.25), *maa://56232 (71.56)</t>
+          <t>maa://47079 (96.54), maa://45790 (89.47), *maa://56232 (73.50)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5599,7 +5599,7 @@
       </c>
       <c r="AF39" s="8" t="inlineStr">
         <is>
-          <t>maa://62953 (97.26)</t>
+          <t>maa://62953 (97.47)</t>
         </is>
       </c>
       <c r="AG39" s="16" t="n"/>
@@ -5665,7 +5665,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (98.29), maa://21386 (96.04), maa://36664 (89.16), *maa://45550 (76.92)</t>
+          <t>maa://23278 (98.36), maa://21386 (96.15), maa://36664 (89.29), *maa://45550 (76.92)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5713,7 +5713,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://65283 (97.27), *maa://64107 (71.11), maa://64205 (94.87)</t>
+          <t>maa://65283 (97.57), *maa://64107 (72.34), maa://64205 (95.00)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="H41" s="8" t="inlineStr">
         <is>
-          <t>maa://24466 (93.90)</t>
+          <t>maa://24466 (94.05)</t>
         </is>
       </c>
       <c r="I41" s="19" t="n"/>
@@ -5766,7 +5766,7 @@
       </c>
       <c r="P41" s="8" t="inlineStr">
         <is>
-          <t>maa://43177 (96.69)</t>
+          <t>maa://43177 (96.91)</t>
         </is>
       </c>
       <c r="Q41" s="19" t="n"/>
@@ -5936,7 +5936,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>maa://21284 (98.34)</t>
+          <t>maa://21284 (98.49)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -5968,7 +5968,7 @@
       </c>
       <c r="P43" s="8" t="inlineStr">
         <is>
-          <t>maa://47403 (91.30)</t>
+          <t>maa://47403 (92.31)</t>
         </is>
       </c>
       <c r="Q43" s="19" t="n"/>
@@ -5984,7 +5984,7 @@
       </c>
       <c r="T43" s="8" t="inlineStr">
         <is>
-          <t>maa://43198 (100.00), maa://46286 (93.75)</t>
+          <t>maa://43198 (100.00), maa://46286 (94.12)</t>
         </is>
       </c>
       <c r="U43" s="19" t="n"/>
@@ -6037,7 +6037,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (98.43), maa://56386 (99.61), maa://27728 (96.46)</t>
+          <t>maa://29768 (98.51), maa://56386 (99.65), maa://27728 (96.46)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6085,7 +6085,7 @@
       </c>
       <c r="T44" s="8" t="inlineStr">
         <is>
-          <t>maa://39366 (95.04)</t>
+          <t>maa://39366 (95.28)</t>
         </is>
       </c>
       <c r="U44" s="19" t="n"/>
@@ -6138,7 +6138,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://42459 (98.86), maa://21229 (86.36), maa://30807 (94.62), *maa://22767 (78.00)</t>
+          <t>maa://42459 (98.94), maa://21229 (86.96), maa://30807 (94.68), maa://22767 (81.15)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="P45" s="8" t="inlineStr">
         <is>
-          <t>maa://36237 (87.50)</t>
+          <t>maa://36237 (88.24)</t>
         </is>
       </c>
       <c r="Q45" s="19" t="n"/>
@@ -6181,12 +6181,12 @@
       </c>
       <c r="S45" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="T45" s="8" t="inlineStr">
         <is>
-          <t>*maa://39364 (72.77)</t>
+          <t>*maa://39364 (74.78), maa://73997 (100.00)</t>
         </is>
       </c>
       <c r="U45" s="19" t="n"/>
@@ -6223,7 +6223,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (96.79), maa://43901 (97.31)</t>
+          <t>maa://35931 (96.86), maa://43901 (97.64)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6234,12 +6234,12 @@
       </c>
       <c r="O46" s="19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P46" s="8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>maa://74003 (100.00)</t>
         </is>
       </c>
       <c r="Q46" s="19" t="n"/>
@@ -6292,7 +6292,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (97.67), maa://56236 (99.86), maa://29661 (97.37), maa://28038 (84.62)</t>
+          <t>maa://27410 (97.71), maa://56236 (99.87), maa://29661 (97.42), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6324,7 +6324,7 @@
       </c>
       <c r="T47" s="8" t="inlineStr">
         <is>
-          <t>maa://67476 (99.59), maa://68392 (99.68)</t>
+          <t>maa://68392 (99.75), maa://67476 (99.60)</t>
         </is>
       </c>
       <c r="U47" s="19" t="n"/>
@@ -6446,7 +6446,7 @@
       </c>
       <c r="P49" s="8" t="inlineStr">
         <is>
-          <t>maa://39643 (82.29)</t>
+          <t>maa://39643 (83.94)</t>
         </is>
       </c>
       <c r="Q49" s="19" t="n"/>
@@ -6462,7 +6462,7 @@
       </c>
       <c r="T49" s="19" t="inlineStr">
         <is>
-          <t>maa://67231 (99.39)</t>
+          <t>maa://67231 (99.40)</t>
         </is>
       </c>
       <c r="U49" s="19" t="n"/>
@@ -6499,7 +6499,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>maa://62852 (94.47), maa://73565 (100.00)</t>
+          <t>maa://62852 (94.69), maa://73565 (97.73)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6533,7 +6533,7 @@
       </c>
       <c r="H51" s="8" t="inlineStr">
         <is>
-          <t>maa://30769 (91.89)</t>
+          <t>maa://30769 (89.74)</t>
         </is>
       </c>
       <c r="I51" s="19" t="n"/>
@@ -6583,7 +6583,7 @@
       </c>
       <c r="H52" s="8" t="inlineStr">
         <is>
-          <t>maa://24376 (99.34)</t>
+          <t>maa://24376 (99.40)</t>
         </is>
       </c>
       <c r="I52" s="19" t="n"/>
@@ -6599,7 +6599,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (99.49), maa://65511 (100.00), maa://59378 (94.05)</t>
+          <t>maa://59394 (99.54), maa://65511 (100.00), maa://59378 (94.05)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6633,7 +6633,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (98.34)</t>
+          <t>maa://32534 (98.48)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -6733,7 +6733,7 @@
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>maa://32532 (98.26)</t>
+          <t>maa://32532 (98.40)</t>
         </is>
       </c>
       <c r="I55" s="19" t="n"/>
@@ -6749,7 +6749,7 @@
       </c>
       <c r="P55" s="16" t="inlineStr">
         <is>
-          <t>maa://73349 (100.00)</t>
+          <t>maa://73349 (97.30)</t>
         </is>
       </c>
       <c r="Q55" s="16" t="n"/>
@@ -6828,12 +6828,12 @@
       </c>
       <c r="G57" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://56237 (98.53), maa://25176 (98.85)</t>
+          <t>maa://56237 (98.59), maa://25176 (98.85), maa://73737 (100.00)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6851,7 +6851,7 @@
       </c>
       <c r="H58" s="8" t="inlineStr">
         <is>
-          <t>*maa://37964 (71.52)</t>
+          <t>*maa://37964 (72.56)</t>
         </is>
       </c>
       <c r="I58" s="19" t="n"/>
@@ -6869,7 +6869,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (98.76), maa://27746 (90.10)</t>
+          <t>maa://31270 (98.84), maa://27746 (90.15)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -6882,12 +6882,12 @@
       </c>
       <c r="G60" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H60" s="8" t="inlineStr">
         <is>
-          <t>maa://40438 (93.82)</t>
+          <t>maa://40438 (94.39), *maa://73999 (80.00)</t>
         </is>
       </c>
       <c r="I60" s="19" t="n"/>
@@ -6923,7 +6923,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (96.12), maa://56228 (98.69), maa://43903 (100.00)</t>
+          <t>maa://42981 (96.23), maa://56228 (98.87), maa://43903 (100.00)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6941,7 +6941,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (99.58), *maa://59693 (72.73), maa://59413 (98.10)</t>
+          <t>maa://59534 (99.61), *maa://59693 (71.93), maa://59413 (98.28)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -6977,7 +6977,7 @@
       </c>
       <c r="H65" s="8" t="inlineStr">
         <is>
-          <t>maa://73343 (99.00)</t>
+          <t>maa://73343 (99.08)</t>
         </is>
       </c>
       <c r="I65" s="19" t="n"/>
@@ -7157,7 +7157,7 @@
       </c>
       <c r="H75" s="19" t="inlineStr">
         <is>
-          <t>maa://67748 (88.89)</t>
+          <t>maa://67748 (90.32)</t>
         </is>
       </c>
       <c r="I75" s="19" t="n"/>
@@ -7317,7 +7317,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.11.03 13:29:46</t>
+          <t>更新日期：2025.11.06 13:22:37</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -7695,7 +7695,7 @@
       </c>
       <c r="D8" s="13" t="inlineStr">
         <is>
-          <t>maa://20980 (94.12)</t>
+          <t>maa://20980 (94.44)</t>
         </is>
       </c>
       <c r="E8" s="14" t="inlineStr">
@@ -8721,7 +8721,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (74.14), *maa://28758 (72.34), maa://65357 (97.62), maa://29036 (96.77), *maa://42172 (71.43), maa://30285 (100.00)</t>
+          <t>*maa://20849 (74.14), *maa://28758 (72.34), maa://65357 (97.73), maa://29036 (96.77), *maa://42172 (71.43), maa://30285 (100.00)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8829,7 +8829,7 @@
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>maa://20863 (90.82), maa://20832 (99.25), maa://20727 (100.00)</t>
+          <t>maa://20863 (90.82), maa://20832 (98.51), maa://20727 (100.00)</t>
         </is>
       </c>
       <c r="E29" s="14" t="inlineStr">
@@ -8991,7 +8991,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (90.66), maa://36866 (97.22), maa://62759 (100.00), maa://45572 (88.24), maa://27794 (100.00), maa://70680 (100.00), maa://20960 (100.00), maa://20843 (100.00), **maa://24483 (50.00), *maa://20893 (75.00), maa://20862 (85.71)</t>
+          <t>maa://36644 (90.78), maa://36866 (97.26), maa://62759 (100.00), maa://45572 (88.89), maa://27794 (100.00), maa://70680 (100.00), maa://20960 (100.00), maa://20843 (100.00), *maa://20893 (75.00), **maa://24483 (50.00), maa://20862 (85.71)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -9261,7 +9261,7 @@
       </c>
       <c r="D37" s="13" t="inlineStr">
         <is>
-          <t>maa://27376 (91.30), maa://42635 (94.74), *maa://20838 (55.00)</t>
+          <t>maa://27376 (91.43), maa://42635 (94.83), *maa://20838 (55.00)</t>
         </is>
       </c>
       <c r="E37" s="14" t="inlineStr">
@@ -9531,7 +9531,7 @@
       </c>
       <c r="D42" s="13" t="inlineStr">
         <is>
-          <t>maa://34883 (94.44), maa://20918 (96.30), maa://20824 (100.00)</t>
+          <t>maa://34883 (94.44), maa://20918 (96.55), maa://20824 (100.00)</t>
         </is>
       </c>
       <c r="E42" s="14" t="inlineStr">
@@ -9747,7 +9747,7 @@
       </c>
       <c r="D46" s="13" t="inlineStr">
         <is>
-          <t>maa://39025 (81.82)</t>
+          <t>maa://39025 (83.33)</t>
         </is>
       </c>
       <c r="E46" s="14" t="inlineStr">
@@ -10125,7 +10125,7 @@
       </c>
       <c r="D53" s="13" t="inlineStr">
         <is>
-          <t>maa://20953 (97.14), maa://31173 (95.00)</t>
+          <t>maa://20953 (97.22), maa://31173 (95.00)</t>
         </is>
       </c>
       <c r="E53" s="14" t="inlineStr">
@@ -10449,7 +10449,7 @@
       </c>
       <c r="D59" s="13" t="inlineStr">
         <is>
-          <t>maa://27970 (98.91), maa://41118 (88.89)</t>
+          <t>maa://27970 (98.92), maa://41118 (88.89)</t>
         </is>
       </c>
       <c r="E59" s="14" t="inlineStr">
@@ -10611,7 +10611,7 @@
       </c>
       <c r="D62" s="13" t="inlineStr">
         <is>
-          <t>maa://40590 (99.40), *maa://72388 (57.14)</t>
+          <t>maa://40590 (99.41), *maa://72388 (57.14)</t>
         </is>
       </c>
       <c r="E62" s="14" t="inlineStr">
@@ -11043,7 +11043,7 @@
       </c>
       <c r="D70" s="13" t="inlineStr">
         <is>
-          <t>maa://20974 (97.09), maa://29079 (80.95), maa://29096 (91.67), maa://29087 (100.00), *maa://20823 (75.00), maa://20855 (94.44), maa://63722 (85.71), maa://20904 (100.00), **maa://72704 (50.00)</t>
+          <t>maa://20974 (97.12), maa://29079 (80.95), maa://29096 (91.67), maa://29087 (100.00), *maa://20823 (75.00), maa://20855 (94.44), maa://63722 (85.71), maa://20904 (100.00), **maa://72704 (50.00)</t>
         </is>
       </c>
       <c r="E70" s="14" t="inlineStr">
@@ -11205,7 +11205,7 @@
       </c>
       <c r="D73" s="13" t="inlineStr">
         <is>
-          <t>maa://36643 (98.53), maa://36864 (98.15), maa://39140 (100.00), maa://66335 (100.00)</t>
+          <t>maa://36643 (98.54), maa://36864 (98.17), maa://39140 (100.00), maa://66335 (100.00)</t>
         </is>
       </c>
       <c r="E73" s="14" t="inlineStr">
@@ -11475,7 +11475,7 @@
       </c>
       <c r="D78" s="13" t="inlineStr">
         <is>
-          <t>maa://20958 (95.74), ***maa://39769 (20.00)</t>
+          <t>maa://20958 (95.83), ***maa://39769 (20.00)</t>
         </is>
       </c>
       <c r="E78" s="14" t="inlineStr">
@@ -11799,7 +11799,7 @@
       </c>
       <c r="D84" s="13" t="inlineStr">
         <is>
-          <t>maa://45572 (88.24), maa://27794 (100.00), maa://20960 (100.00)</t>
+          <t>maa://45572 (88.89), maa://27794 (100.00), maa://20960 (100.00)</t>
         </is>
       </c>
       <c r="E84" s="14" t="inlineStr">
@@ -12015,7 +12015,7 @@
       </c>
       <c r="D88" s="13" t="inlineStr">
         <is>
-          <t>maa://20886 (94.59), maa://60772 (100.00)</t>
+          <t>maa://20886 (94.74), maa://60772 (100.00)</t>
         </is>
       </c>
       <c r="E88" s="14" t="inlineStr">
@@ -12069,7 +12069,7 @@
       </c>
       <c r="D89" s="13" t="inlineStr">
         <is>
-          <t>maa://24472 (91.29), *maa://35841 (65.38)</t>
+          <t>maa://24472 (91.32), *maa://35841 (65.38)</t>
         </is>
       </c>
       <c r="E89" s="14" t="inlineStr">
@@ -12825,7 +12825,7 @@
       </c>
       <c r="D103" s="13" t="inlineStr">
         <is>
-          <t>maa://45572 (88.24), maa://27794 (100.00), *maa://20893 (75.00)</t>
+          <t>maa://45572 (88.89), maa://27794 (100.00), *maa://20893 (75.00)</t>
         </is>
       </c>
       <c r="E103" s="14" t="inlineStr">
@@ -12879,7 +12879,7 @@
       </c>
       <c r="D104" s="13" t="inlineStr">
         <is>
-          <t>maa://40517 (91.89), *maa://39240 (56.25)</t>
+          <t>maa://40517 (92.11), *maa://39240 (56.25)</t>
         </is>
       </c>
       <c r="E104" s="14" t="inlineStr">
@@ -13095,7 +13095,7 @@
       </c>
       <c r="D108" s="13" t="inlineStr">
         <is>
-          <t>maa://45572 (88.24), maa://27794 (100.00), maa://20843 (100.00), **maa://24483 (50.00)</t>
+          <t>maa://45572 (88.89), maa://27794 (100.00), maa://20843 (100.00), **maa://24483 (50.00)</t>
         </is>
       </c>
       <c r="E108" s="14" t="inlineStr">
@@ -13203,7 +13203,7 @@
       </c>
       <c r="D110" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.68), maa://25018 (97.00), maa://25776 (92.77), maa://28361 (95.56), maa://25772 (94.12), maa://56588 (94.44), maa://45194 (86.36), maa://32653 (81.25), maa://25161 (84.21), maa://61839 (100.00), **maa://60902 (38.46), maa://61275 (100.00), **maa://73473 (50.00)</t>
+          <t>maa://51881 (98.69), maa://25018 (97.01), maa://25776 (92.77), maa://28361 (95.56), maa://25772 (94.12), maa://56588 (94.59), maa://45194 (86.36), maa://32653 (81.25), maa://25161 (84.21), maa://61839 (100.00), **maa://60902 (38.46), maa://61275 (100.00), *maa://73473 (66.67)</t>
         </is>
       </c>
       <c r="E110" s="14" t="inlineStr">
@@ -13959,7 +13959,7 @@
       </c>
       <c r="D124" s="13" t="inlineStr">
         <is>
-          <t>maa://20869 (100.00), maa://44690 (96.15)</t>
+          <t>maa://20869 (100.00), maa://44690 (96.23)</t>
         </is>
       </c>
       <c r="E124" s="14" t="inlineStr">
@@ -14175,7 +14175,7 @@
       </c>
       <c r="D128" s="13" t="inlineStr">
         <is>
-          <t>maa://44403 (93.75)</t>
+          <t>maa://44403 (94.12)</t>
         </is>
       </c>
       <c r="E128" s="14" t="inlineStr">
@@ -14445,7 +14445,7 @@
       </c>
       <c r="D133" s="13" t="inlineStr">
         <is>
-          <t>maa://21422 (98.93)</t>
+          <t>maa://21422 (98.95)</t>
         </is>
       </c>
       <c r="E133" s="14" t="inlineStr">
@@ -14931,7 +14931,7 @@
       </c>
       <c r="D142" s="13" t="inlineStr">
         <is>
-          <t>maa://29025 (83.87), **maa://21000 (43.75)</t>
+          <t>maa://29025 (84.38), **maa://21000 (45.45)</t>
         </is>
       </c>
       <c r="E142" s="14" t="inlineStr">
@@ -15147,7 +15147,7 @@
       </c>
       <c r="D146" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (97.99), *maa://23736 (53.49), maa://31185 (92.31), maa://30306 (100.00)</t>
+          <t>maa://28484 (98.00), *maa://23736 (53.49), maa://31185 (92.31), maa://30306 (100.00)</t>
         </is>
       </c>
       <c r="E146" s="14" t="inlineStr">
@@ -15525,7 +15525,7 @@
       </c>
       <c r="D153" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.87), maa://36641 (98.25), maa://36865 (95.58), maa://44635 (88.18), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (96.67), maa://42918 (100.00), maa://44119 (97.44), maa://64408 (94.74), maa://37300 (100.00), maa://42917 (100.00)</t>
+          <t>maa://40957 (94.88), maa://36641 (98.26), maa://36865 (95.63), maa://44635 (88.18), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (96.77), maa://42918 (100.00), maa://44119 (97.44), maa://64408 (94.74), maa://37300 (100.00), maa://42917 (100.00)</t>
         </is>
       </c>
       <c r="E153" s="14" t="inlineStr">
@@ -15579,7 +15579,7 @@
       </c>
       <c r="D154" s="13" t="inlineStr">
         <is>
-          <t>maa://51549 (95.77), maa://51923 (96.55), *maa://67508 (71.43)</t>
+          <t>maa://51549 (95.77), maa://51923 (96.67), *maa://67508 (71.43)</t>
         </is>
       </c>
       <c r="E154" s="14" t="inlineStr">
@@ -16065,7 +16065,7 @@
       </c>
       <c r="D163" s="13" t="inlineStr">
         <is>
-          <t>maa://44232 (98.51), maa://45603 (90.62), *maa://65963 (71.43), *maa://63114 (66.67), maa://71762 (100.00)</t>
+          <t>maa://44232 (98.52), maa://45603 (90.62), *maa://65963 (71.43), *maa://63114 (66.67), maa://71762 (100.00)</t>
         </is>
       </c>
       <c r="E163" s="14" t="inlineStr">
@@ -16497,7 +16497,7 @@
       </c>
       <c r="D171" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (92.38), maa://29627 (92.98), maa://29659 (83.33), maa://49074 (94.29), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
+          <t>maa://29633 (92.09), maa://29627 (92.98), maa://29659 (83.33), maa://49074 (94.29), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
         </is>
       </c>
       <c r="E171" s="14" t="inlineStr">
@@ -17145,7 +17145,7 @@
       </c>
       <c r="D183" s="13" t="inlineStr">
         <is>
-          <t>maa://20911 (96.30), maa://29012 (87.50)</t>
+          <t>maa://20911 (96.43), maa://29012 (87.50)</t>
         </is>
       </c>
       <c r="E183" s="14" t="inlineStr">
@@ -17739,7 +17739,7 @@
       </c>
       <c r="D194" s="13" t="inlineStr">
         <is>
-          <t>maa://34866 (94.12), maa://34714 (97.22)</t>
+          <t>maa://34866 (94.23), maa://34714 (97.22)</t>
         </is>
       </c>
       <c r="E194" s="14" t="inlineStr">
@@ -18117,7 +18117,7 @@
       </c>
       <c r="D201" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.52), maa://35854 (84.75), maa://50388 (98.29), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://63024 (96.49), maa://51066 (87.50), maa://70161 (100.00), maa://72380 (100.00)</t>
+          <t>maa://44224 (90.61), maa://35854 (84.75), maa://50388 (98.31), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://63024 (96.49), maa://51066 (87.50), maa://70161 (100.00), maa://72380 (100.00)</t>
         </is>
       </c>
       <c r="E201" s="14" t="inlineStr">
@@ -18333,7 +18333,7 @@
       </c>
       <c r="D205" s="13" t="inlineStr">
         <is>
-          <t>maa://42223 (99.26), maa://49077 (94.64), maa://42292 (97.30), maa://42402 (100.00)</t>
+          <t>maa://42223 (99.27), maa://49077 (94.64), maa://42292 (97.30), maa://42402 (100.00)</t>
         </is>
       </c>
       <c r="E205" s="14" t="inlineStr">
@@ -19305,7 +19305,7 @@
       </c>
       <c r="D223" s="13" t="inlineStr">
         <is>
-          <t>maa://39157 (88.89)</t>
+          <t>maa://39157 (90.00)</t>
         </is>
       </c>
       <c r="E223" s="14" t="inlineStr">
@@ -19359,7 +19359,7 @@
       </c>
       <c r="D224" s="13" t="inlineStr">
         <is>
-          <t>**maa://26496 (41.67), *maa://20995 (54.55)</t>
+          <t>**maa://26496 (46.15), *maa://20995 (54.55)</t>
         </is>
       </c>
       <c r="E224" s="14" t="inlineStr">
@@ -19575,7 +19575,7 @@
       </c>
       <c r="D228" s="13" t="inlineStr">
         <is>
-          <t>maa://20988 (92.31)</t>
+          <t>maa://20988 (92.86)</t>
         </is>
       </c>
       <c r="E228" s="14" t="inlineStr">
@@ -19791,7 +19791,7 @@
       </c>
       <c r="D232" s="13" t="inlineStr">
         <is>
-          <t>maa://20987 (94.50), *maa://35801 (77.78)</t>
+          <t>maa://20987 (94.55), *maa://35801 (77.78)</t>
         </is>
       </c>
       <c r="E232" s="14" t="inlineStr">
@@ -20547,7 +20547,7 @@
       </c>
       <c r="D246" s="13" t="inlineStr">
         <is>
-          <t>*maa://30667 (78.94), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (59.09), maa://39588 (86.67), *maa://64079 (80.00), maa://65726 (90.91), maa://68226 (87.50)</t>
+          <t>*maa://30667 (78.94), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (59.09), maa://39588 (86.67), *maa://64079 (80.00), maa://65726 (90.91), maa://68226 (88.89)</t>
         </is>
       </c>
       <c r="E246" s="14" t="inlineStr">
@@ -21033,7 +21033,7 @@
       </c>
       <c r="D255" s="13" t="inlineStr">
         <is>
-          <t>maa://28923 (91.51), maa://28906 (98.31), ***maa://28825 (11.54), maa://65613 (88.89)</t>
+          <t>maa://28923 (91.51), maa://28906 (98.31), ***maa://28825 (11.54), maa://65613 (90.00)</t>
         </is>
       </c>
       <c r="E255" s="14" t="inlineStr">
@@ -21087,7 +21087,7 @@
       </c>
       <c r="D256" s="13" t="inlineStr">
         <is>
-          <t>maa://42287 (93.45), maa://45570 (96.92), maa://60678 (93.55), maa://42225 (94.44)</t>
+          <t>maa://42287 (93.57), maa://45570 (96.92), maa://60678 (93.75), maa://42225 (94.44)</t>
         </is>
       </c>
       <c r="E256" s="14" t="inlineStr">
@@ -22275,7 +22275,7 @@
       </c>
       <c r="D278" s="13" t="inlineStr">
         <is>
-          <t>maa://25769 (97.01)</t>
+          <t>maa://25769 (97.02)</t>
         </is>
       </c>
       <c r="E278" s="14" t="inlineStr">
@@ -22437,7 +22437,7 @@
       </c>
       <c r="D281" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.68), maa://51630 (96.46), maa://56588 (94.44), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (38.46), *maa://66758 (76.92)</t>
+          <t>maa://51881 (98.69), maa://51630 (96.46), maa://56588 (94.59), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (38.46), *maa://66758 (76.92)</t>
         </is>
       </c>
       <c r="E281" s="14" t="inlineStr">
@@ -23247,7 +23247,7 @@
       </c>
       <c r="D296" s="13" t="inlineStr">
         <is>
-          <t>maa://53353 (87.50)</t>
+          <t>maa://53353 (88.89)</t>
         </is>
       </c>
       <c r="E296" s="14" t="inlineStr">
@@ -24111,7 +24111,7 @@
       </c>
       <c r="D312" s="13" t="inlineStr">
         <is>
-          <t>maa://50280 (98.53), maa://49642 (97.71), maa://49660 (93.75), maa://70004 (100.00), maa://50517 (85.71)</t>
+          <t>maa://50280 (98.53), maa://49642 (97.74), maa://49660 (93.75), maa://70004 (100.00), maa://50517 (85.71)</t>
         </is>
       </c>
       <c r="E312" s="14" t="inlineStr">
@@ -24651,7 +24651,7 @@
       </c>
       <c r="D322" s="13" t="inlineStr">
         <is>
-          <t>maa://25775 (92.47), *maa://25393 (75.00)</t>
+          <t>maa://25775 (92.55), *maa://25393 (75.00)</t>
         </is>
       </c>
       <c r="E322" s="14" t="inlineStr">
@@ -24867,7 +24867,7 @@
       </c>
       <c r="D326" s="13" t="inlineStr">
         <is>
-          <t>*maa://62755 (78.26), maa://62761 (88.89)</t>
+          <t>*maa://62755 (79.17), maa://62761 (88.89)</t>
         </is>
       </c>
       <c r="E326" s="14" t="inlineStr">
@@ -25569,7 +25569,7 @@
       </c>
       <c r="D339" s="22" t="inlineStr">
         <is>
-          <t>maa://40956 (94.39)</t>
+          <t>maa://40956 (94.44)</t>
         </is>
       </c>
       <c r="E339" s="22" t="inlineStr">
@@ -25947,7 +25947,7 @@
       </c>
       <c r="D346" s="22" t="inlineStr">
         <is>
-          <t>maa://42968 (99.17), maa://49245 (100.00)</t>
+          <t>maa://42968 (99.18), maa://49245 (100.00)</t>
         </is>
       </c>
       <c r="E346" s="22" t="inlineStr">
@@ -26163,7 +26163,7 @@
       </c>
       <c r="D350" s="22" t="inlineStr">
         <is>
-          <t>maa://30671 (81.59), maa://30669 (99.35), maa://37275 (81.40), *maa://32410 (61.54), maa://41605 (100.00)</t>
+          <t>maa://30671 (81.28), maa://30669 (99.35), maa://37275 (81.40), *maa://32410 (61.54), maa://41605 (100.00)</t>
         </is>
       </c>
       <c r="E350" s="22" t="inlineStr">
@@ -26271,7 +26271,7 @@
       </c>
       <c r="D352" s="22" t="inlineStr">
         <is>
-          <t>maa://38295 (95.50), maa://49332 (91.67)</t>
+          <t>maa://38295 (95.54), maa://49332 (91.67)</t>
         </is>
       </c>
       <c r="E352" s="22" t="inlineStr">
@@ -26541,7 +26541,7 @@
       </c>
       <c r="D357" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (97.61), maa://32415 (84.08), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
+          <t>maa://32647 (97.61), maa://32415 (83.93), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E357" s="22" t="inlineStr">
@@ -27189,7 +27189,7 @@
       </c>
       <c r="D369" s="22" t="inlineStr">
         <is>
-          <t>maa://42299 (97.96), maa://42224 (85.71)</t>
+          <t>maa://42299 (98.04), maa://42224 (85.71)</t>
         </is>
       </c>
       <c r="E369" s="22" t="inlineStr">
@@ -27243,7 +27243,7 @@
       </c>
       <c r="D370" s="22" t="inlineStr">
         <is>
-          <t>maa://49648 (96.43), *maa://49662 (76.47)</t>
+          <t>maa://49648 (96.47), *maa://49662 (76.47)</t>
         </is>
       </c>
       <c r="E370" s="22" t="inlineStr">
@@ -27351,7 +27351,7 @@
       </c>
       <c r="D372" s="22" t="inlineStr">
         <is>
-          <t>maa://36645 (98.46), maa://36841 (92.86), maa://37484 (94.34), maa://37858 (93.55), **maa://56268 (50.00), maa://40489 (100.00)</t>
+          <t>maa://36645 (98.46), maa://36841 (92.86), maa://37484 (94.34), maa://37858 (93.55), *maa://56268 (57.14), maa://40489 (100.00)</t>
         </is>
       </c>
       <c r="E372" s="22" t="inlineStr">
@@ -27405,7 +27405,7 @@
       </c>
       <c r="D373" s="22" t="inlineStr">
         <is>
-          <t>maa://42635 (94.74), maa://50629 (88.89), maa://48859 (100.00)</t>
+          <t>maa://42635 (94.83), maa://50629 (90.91), maa://48859 (100.00)</t>
         </is>
       </c>
       <c r="E373" s="22" t="inlineStr">
@@ -27567,7 +27567,7 @@
       </c>
       <c r="D376" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (94.87), maa://48026 (94.70), maa://44635 (88.18), maa://41035 (93.59), *maa://60251 (77.78), maa://44660 (92.68), maa://41128 (84.21)</t>
+          <t>maa://40957 (94.88), maa://48026 (94.70), maa://44635 (88.18), maa://41035 (93.59), *maa://60251 (73.68), maa://44660 (92.68), maa://41128 (84.21)</t>
         </is>
       </c>
       <c r="E376" s="22" t="inlineStr">
@@ -27729,7 +27729,7 @@
       </c>
       <c r="D379" s="22" t="inlineStr">
         <is>
-          <t>maa://48268 (93.75)</t>
+          <t>maa://48268 (94.12)</t>
         </is>
       </c>
       <c r="E379" s="22" t="inlineStr">
@@ -27837,7 +27837,7 @@
       </c>
       <c r="D381" s="22" t="inlineStr">
         <is>
-          <t>maa://71182 (96.26), maa://70756 (97.67), maa://71524 (100.00), maa://72244 (100.00)</t>
+          <t>maa://71182 (96.36), maa://70756 (97.67), maa://71524 (100.00), maa://72244 (100.00)</t>
         </is>
       </c>
       <c r="E381" s="22" t="inlineStr">
@@ -28269,7 +28269,7 @@
       </c>
       <c r="D389" s="22" t="inlineStr">
         <is>
-          <t>maa://44233 (91.80), maa://45570 (96.92)</t>
+          <t>maa://44233 (91.94), maa://45570 (96.92)</t>
         </is>
       </c>
       <c r="E389" s="22" t="inlineStr">
@@ -28539,7 +28539,7 @@
       </c>
       <c r="D395" t="inlineStr">
         <is>
-          <t>maa://42970 (80.28), maa://44745 (98.23), **maa://49516 (40.00), *maa://45952 (57.14), ***maa://46851 (10.00), *maa://44896 (80.00)</t>
+          <t>maa://42970 (80.28), maa://44745 (98.26), **maa://49516 (41.94), *maa://45952 (57.14), ***maa://46851 (10.00), *maa://44896 (80.00)</t>
         </is>
       </c>
       <c r="E395" t="inlineStr">
@@ -28809,7 +28809,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>**maa://48618 (50.00)</t>
+          <t>*maa://48618 (66.67)</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">
@@ -28836,7 +28836,7 @@
       </c>
       <c r="D406" t="inlineStr">
         <is>
-          <t>maa://59533 (96.30), maa://59577 (100.00)</t>
+          <t>maa://59533 (96.36), maa://59577 (100.00)</t>
         </is>
       </c>
       <c r="E406" t="inlineStr">
@@ -28971,7 +28971,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>maa://51872 (96.55), maa://51876 (99.12), maa://63228 (86.11), maa://51873 (98.00), maa://62047 (90.32)</t>
+          <t>maa://51872 (96.56), maa://51876 (99.12), maa://63228 (86.11), maa://51873 (98.04), maa://62047 (90.32)</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
@@ -29025,7 +29025,7 @@
       </c>
       <c r="D413" t="inlineStr">
         <is>
-          <t>maa://60449 (98.57), maa://59493 (96.92)</t>
+          <t>maa://60449 (98.58), maa://59493 (96.92)</t>
         </is>
       </c>
       <c r="E413" t="inlineStr">
@@ -29079,7 +29079,7 @@
       </c>
       <c r="D415" t="inlineStr">
         <is>
-          <t>maa://62756 (96.25)</t>
+          <t>maa://62756 (96.27)</t>
         </is>
       </c>
       <c r="E415" t="inlineStr">
@@ -29133,7 +29133,7 @@
       </c>
       <c r="D417" t="inlineStr">
         <is>
-          <t>maa://52505 (97.87), maa://64040 (99.15), maa://66377 (94.44), ***maa://66376 (14.29), ***maa://70187 (9.09)</t>
+          <t>maa://52505 (97.88), maa://64040 (99.15), maa://66377 (94.44), ***maa://66376 (14.29), ***maa://70187 (9.09)</t>
         </is>
       </c>
       <c r="E417" t="inlineStr">
@@ -29165,7 +29165,7 @@
       </c>
       <c r="E418" t="inlineStr">
         <is>
-          <t>&gt; 由非助战维斩业星熊累计造成100000点伤害&gt; 3星通关插曲火蓝之心OF-8；必须编入非助战斩业星熊并上场，且所有干员不被击倒</t>
+          <t>&gt; 由非助战斩业星熊累计造成100000点伤害&gt; 3星通关插曲火蓝之心OF-8；必须编入非助战斩业星熊并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
@@ -29187,7 +29187,7 @@
       </c>
       <c r="D419" t="inlineStr">
         <is>
-          <t>maa://67090 (93.65)</t>
+          <t>maa://67090 (93.75)</t>
         </is>
       </c>
       <c r="E419" t="inlineStr">
@@ -29214,7 +29214,7 @@
       </c>
       <c r="D420" t="inlineStr">
         <is>
-          <t>maa://67388 (89.06), *maa://71184 (78.95)</t>
+          <t>maa://67388 (89.06), maa://71184 (80.95)</t>
         </is>
       </c>
       <c r="E420" t="inlineStr">
@@ -29241,7 +29241,7 @@
       </c>
       <c r="D421" t="inlineStr">
         <is>
-          <t>maa://67089 (96.49), maa://67271 (92.31)</t>
+          <t>maa://67089 (96.61), maa://67271 (92.59)</t>
         </is>
       </c>
       <c r="E421" t="inlineStr">
@@ -29268,7 +29268,7 @@
       </c>
       <c r="D422" t="inlineStr">
         <is>
-          <t>maa://67088 (93.18)</t>
+          <t>maa://67088 (93.26)</t>
         </is>
       </c>
       <c r="E422" t="inlineStr">
@@ -29295,7 +29295,7 @@
       </c>
       <c r="D423" t="inlineStr">
         <is>
-          <t>maa://67087 (97.29), maa://67268 (97.86), maa://67269 (88.89), maa://67648 (100.00)</t>
+          <t>maa://67087 (97.47), maa://67268 (97.90), maa://67269 (89.29), maa://67648 (100.00)</t>
         </is>
       </c>
       <c r="E423" t="inlineStr">
@@ -29440,27 +29440,27 @@
       </c>
     </row>
     <row r="429">
-      <c r="A429" s="28" t="inlineStr">
+      <c r="A429" s="17" t="inlineStr">
         <is>
           <t>溯光星源</t>
         </is>
       </c>
-      <c r="B429" s="28" t="inlineStr">
+      <c r="B429" s="17" t="inlineStr">
         <is>
           <t>BI-6</t>
         </is>
       </c>
-      <c r="C429" s="28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D429" s="29" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E429" s="29" t="inlineStr">
+      <c r="C429" s="17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D429" t="inlineStr">
+        <is>
+          <t>maa://74092 (100.00)</t>
+        </is>
+      </c>
+      <c r="E429" t="inlineStr">
         <is>
           <t>&gt; 战斗中非助战溯光星源累计使用3次并流连锁&gt; 3星通关插曲风雪过境BI-6；必须编入非助战溯光星源并上场，且至少使用1次并流连锁</t>
         </is>
@@ -29479,12 +29479,12 @@
       </c>
       <c r="C430" s="17" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D430" t="inlineStr">
         <is>
-          <t>maa://73227 (95.83), maa://73422 (87.50)</t>
+          <t>maa://73227 (97.59), maa://73422 (90.91), maa://73447 (100.00)</t>
         </is>
       </c>
       <c r="E430" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#251)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -715,7 +715,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (98.86), maa://24702 (95.25), maa://36681 (85.71)</t>
+          <t>maa://25390 (98.87), maa://24702 (95.27), maa://36681 (85.71)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -747,7 +747,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://58660 (99.02), maa://39402 (95.90), *maa://34787 (74.76), *maa://54304 (70.00)</t>
+          <t>maa://58660 (99.05), maa://39402 (96.06), *maa://34787 (75.24), *maa://54304 (70.00)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -779,7 +779,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (97.87), maa://66635 (99.40)</t>
+          <t>maa://22742 (97.95), maa://66635 (99.45)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -811,7 +811,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://36684 (98.69), maa://21246 (91.14)</t>
+          <t>maa://36684 (98.69), maa://21246 (91.19)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -827,7 +827,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://59087 (97.92), maa://25251 (91.67)</t>
+          <t>maa://59087 (98.04), maa://25251 (91.67)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -845,7 +845,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (99.48), maa://36987 (97.37), maa://39849 (94.12)</t>
+          <t>maa://40192 (99.52), maa://36987 (97.40), maa://39849 (94.12)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -861,7 +861,7 @@
       </c>
       <c r="H3" s="8" t="inlineStr">
         <is>
-          <t>maa://21247 (99.49)</t>
+          <t>maa://21247 (99.52)</t>
         </is>
       </c>
       <c r="I3" s="19" t="n"/>
@@ -877,7 +877,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>maa://22880 (93.67), maa://20276 (94.62), maa://22749 (87.88)</t>
+          <t>maa://22880 (93.89), maa://20276 (94.69), maa://22749 (86.49)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -893,7 +893,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (98.91), maa://26254 (95.31), maa://22738 (85.71)</t>
+          <t>maa://21249 (98.94), maa://26254 (95.45), maa://22738 (85.71)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -909,7 +909,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://60545 (99.13), maa://45854 (89.93), maa://24617 (91.18)</t>
+          <t>maa://60545 (99.20), maa://45854 (90.36), maa://24617 (91.30)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -925,7 +925,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (94.74), maa://27484 (99.27), maa://27480 (87.30)</t>
+          <t>maa://27396 (95.12), maa://27484 (99.29), maa://27480 (87.69)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -941,7 +941,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://52241 (99.45), maa://24390 (97.26)</t>
+          <t>maa://52241 (99.33), maa://24390 (97.28)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -957,7 +957,7 @@
       </c>
       <c r="AF3" s="8" t="inlineStr">
         <is>
-          <t>maa://21289 (93.42)</t>
+          <t>maa://21289 (93.67)</t>
         </is>
       </c>
       <c r="AG3" s="16" t="n"/>
@@ -975,7 +975,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (98.69), maa://22499 (90.48), maa://22746 (88.89)</t>
+          <t>maa://24632 (98.77), maa://22499 (90.91), maa://22746 (88.89)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (99.43), maa://50121 (97.30)</t>
+          <t>maa://49983 (99.42), maa://50121 (97.54)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://27295 (98.36), maa://32509 (97.10), maa://31008 (95.31), maa://22754 (88.16), maa://70489 (99.22)</t>
+          <t>maa://27295 (98.42), maa://32509 (96.88), maa://31008 (95.45), maa://70489 (99.40), maa://22754 (88.16)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="X4" s="8" t="inlineStr">
         <is>
-          <t>maa://43217 (99.10)</t>
+          <t>maa://43217 (99.12)</t>
         </is>
       </c>
       <c r="Y4" s="19" t="n"/>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="AB4" s="8" t="inlineStr">
         <is>
-          <t>*maa://32658 (78.57)</t>
+          <t>*maa://32658 (77.19)</t>
         </is>
       </c>
       <c r="AC4" s="19" t="n"/>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>*maa://39394 (53.57), *maa://30062 (61.54), ***maa://26209 (12.50)</t>
+          <t>*maa://39394 (53.57), *maa://30062 (62.12), ***maa://26209 (12.00)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://21245 (92.42), maa://54105 (98.74), *maa://22744 (80.00)</t>
+          <t>maa://54105 (98.77), maa://21245 (92.60), *maa://22744 (80.00)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="L5" s="8" t="inlineStr">
         <is>
-          <t>maa://22757 (93.49)</t>
+          <t>maa://22757 (94.15)</t>
         </is>
       </c>
       <c r="M5" s="19" t="n"/>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="P5" s="8" t="inlineStr">
         <is>
-          <t>maa://21919 (99.07), maa://21281 (83.33)</t>
+          <t>maa://21919 (99.12), maa://21281 (84.21)</t>
         </is>
       </c>
       <c r="Q5" s="19" t="n"/>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="X5" s="8" t="inlineStr">
         <is>
-          <t>maa://21290 (98.94)</t>
+          <t>maa://21290 (99.02)</t>
         </is>
       </c>
       <c r="Y5" s="19" t="n"/>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="AB5" s="8" t="inlineStr">
         <is>
-          <t>*maa://29863 (60.00), ***maa://22752 (12.50), **maa://26013 (33.33)</t>
+          <t>*maa://29863 (60.00), ***maa://22752 (11.76), **maa://26013 (33.33)</t>
         </is>
       </c>
       <c r="AC5" s="19" t="n"/>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="D6" s="8" t="inlineStr">
         <is>
-          <t>maa://42407 (98.31)</t>
+          <t>maa://42407 (98.40)</t>
         </is>
       </c>
       <c r="E6" s="19" t="n"/>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="H6" s="8" t="inlineStr">
         <is>
-          <t>maa://24370 (98.27)</t>
+          <t>maa://24370 (98.41)</t>
         </is>
       </c>
       <c r="I6" s="19" t="n"/>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="L6" s="8" t="inlineStr">
         <is>
-          <t>maa://24839 (99.63)</t>
+          <t>maa://24839 (99.65)</t>
         </is>
       </c>
       <c r="M6" s="19" t="n"/>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (99.20), maa://30381 (95.45)</t>
+          <t>maa://31836 (99.28), maa://30381 (95.45)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1304,7 +1304,7 @@
       </c>
       <c r="T6" s="8" t="inlineStr">
         <is>
-          <t>maa://37411 (83.64)</t>
+          <t>maa://37411 (85.00)</t>
         </is>
       </c>
       <c r="U6" s="19" t="n"/>
@@ -1336,7 +1336,7 @@
       </c>
       <c r="AB6" s="8" t="inlineStr">
         <is>
-          <t>maa://22739 (90.09)</t>
+          <t>maa://22739 (90.43)</t>
         </is>
       </c>
       <c r="AC6" s="19" t="n"/>
@@ -1352,7 +1352,7 @@
       </c>
       <c r="AF6" s="8" t="inlineStr">
         <is>
-          <t>maa://33152 (86.00)</t>
+          <t>maa://33152 (87.04)</t>
         </is>
       </c>
       <c r="AG6" s="16" t="n"/>
@@ -1370,7 +1370,7 @@
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>maa://21955 (98.70)</t>
+          <t>maa://21955 (98.78)</t>
         </is>
       </c>
       <c r="E7" s="19" t="n"/>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>*maa://22763 (78.26), maa://64972 (95.24)</t>
+          <t>*maa://22763 (79.73), maa://64972 (95.74)</t>
         </is>
       </c>
       <c r="I7" s="19" t="n"/>
@@ -1402,7 +1402,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (98.99), maa://24957 (92.86)</t>
+          <t>maa://28624 (99.05), maa://24957 (92.86)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="P7" s="8" t="inlineStr">
         <is>
-          <t>maa://22750 (97.75)</t>
+          <t>maa://22750 (97.94)</t>
         </is>
       </c>
       <c r="Q7" s="19" t="n"/>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="T7" s="8" t="inlineStr">
         <is>
-          <t>maa://21291 (94.95)</t>
+          <t>maa://21291 (94.37)</t>
         </is>
       </c>
       <c r="U7" s="19" t="n"/>
@@ -1450,7 +1450,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (98.04), maa://22758 (84.68)</t>
+          <t>maa://22399 (98.18), maa://22758 (84.92)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1482,7 +1482,7 @@
       </c>
       <c r="AF7" s="8" t="inlineStr">
         <is>
-          <t>maa://45272 (99.67), *maa://26191 (70.71)</t>
+          <t>maa://45272 (99.70), *maa://26191 (70.71)</t>
         </is>
       </c>
       <c r="AG7" s="16" t="n"/>
@@ -1490,7 +1490,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.11.06 13:22:37</t>
+          <t>更新日期：2025.11.10 13:23:00</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1505,7 +1505,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (93.01)</t>
+          <t>maa://21476 (93.50)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
-          <t>maa://24371 (83.94)</t>
+          <t>maa://24371 (85.02)</t>
         </is>
       </c>
       <c r="I8" s="19" t="n"/>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (93.15), maa://23252 (91.67), maa://37496 (98.59)</t>
+          <t>maa://32931 (93.23), maa://23252 (91.67), maa://37496 (98.68)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (96.31), maa://67587 (98.68)</t>
+          <t>maa://21411 (96.37), maa://67587 (98.74)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1601,7 +1601,7 @@
       </c>
       <c r="AB8" s="8" t="inlineStr">
         <is>
-          <t>maa://25389 (96.20)</t>
+          <t>maa://25389 (96.51)</t>
         </is>
       </c>
       <c r="AC8" s="19" t="n"/>
@@ -1612,12 +1612,12 @@
       </c>
       <c r="AE8" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="AF8" s="8" t="inlineStr">
         <is>
-          <t>maa://24479 (89.44), **maa://21990 (50.00)</t>
+          <t>maa://24479 (90.13)</t>
         </is>
       </c>
       <c r="AG8" s="16" t="n"/>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>maa://22765 (97.15), maa://21915 (83.33)</t>
+          <t>maa://22765 (97.31), maa://21915 (84.21)</t>
         </is>
       </c>
       <c r="E9" s="19" t="n"/>
@@ -1651,7 +1651,7 @@
       </c>
       <c r="H9" s="8" t="inlineStr">
         <is>
-          <t>maa://47450 (83.33), maa://56348 (96.88)</t>
+          <t>maa://47450 (86.11), maa://56348 (97.06)</t>
         </is>
       </c>
       <c r="I9" s="19" t="n"/>
@@ -1667,7 +1667,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (96.53), maa://39552 (89.61)</t>
+          <t>maa://22762 (96.80), maa://39552 (89.74)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1699,7 +1699,7 @@
       </c>
       <c r="T9" s="8" t="inlineStr">
         <is>
-          <t>maa://26222 (99.65)</t>
+          <t>maa://26222 (99.68)</t>
         </is>
       </c>
       <c r="U9" s="19" t="n"/>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://52237 (99.74), maa://26223 (98.38)</t>
+          <t>maa://52237 (99.76), maa://26223 (98.38)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (95.94), maa://40166 (95.39)</t>
+          <t>maa://28711 (96.09), maa://40166 (95.57)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (91.95), maa://66916 (98.62)</t>
+          <t>maa://26206 (92.05), maa://66916 (98.76)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1760,12 +1760,12 @@
       </c>
       <c r="C10" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>maa://54000 (93.70)</t>
+          <t>maa://54000 (93.23), *maa://45271 (70.13)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1781,7 +1781,7 @@
       </c>
       <c r="H10" s="8" t="inlineStr">
         <is>
-          <t>maa://32651 (94.64)</t>
+          <t>maa://32651 (94.92)</t>
         </is>
       </c>
       <c r="I10" s="19" t="n"/>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="L10" s="8" t="inlineStr">
         <is>
-          <t>**maa://24395 (47.27)</t>
+          <t>**maa://24395 (49.15)</t>
         </is>
       </c>
       <c r="M10" s="19" t="n"/>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (93.51), *maa://36669 (75.61)</t>
+          <t>maa://28977 (93.35), *maa://36669 (75.00)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1829,7 +1829,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (99.43), maa://22755 (92.27), maa://63521 (96.07), maa://73485 (94.74)</t>
+          <t>maa://27395 (99.46), maa://22755 (92.39), maa://63521 (96.39), maa://73485 (96.77)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1845,7 +1845,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://45828 (99.50), maa://22301 (97.67), maa://22726 (100.00)</t>
+          <t>maa://45828 (99.53), maa://22301 (97.68), maa://22726 (100.00)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1895,7 +1895,7 @@
       </c>
       <c r="D11" s="8" t="inlineStr">
         <is>
-          <t>maa://36707 (99.72)</t>
+          <t>maa://36707 (99.74)</t>
         </is>
       </c>
       <c r="E11" s="19" t="n"/>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="L11" s="8" t="inlineStr">
         <is>
-          <t>maa://21287 (94.72)</t>
+          <t>maa://21287 (95.00)</t>
         </is>
       </c>
       <c r="M11" s="19" t="n"/>
@@ -1943,7 +1943,7 @@
       </c>
       <c r="P11" s="8" t="inlineStr">
         <is>
-          <t>maa://45557 (95.71)</t>
+          <t>maa://45557 (96.05)</t>
         </is>
       </c>
       <c r="Q11" s="19" t="n"/>
@@ -1959,7 +1959,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (94.92), maa://22501 (99.63), maa://64808 (99.59), maa://45521 (94.20)</t>
+          <t>maa://22747 (95.18), maa://22501 (99.64), maa://64808 (99.62), maa://45521 (94.44)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1975,7 +1975,7 @@
       </c>
       <c r="X11" s="8" t="inlineStr">
         <is>
-          <t>maa://36713 (99.46)</t>
+          <t>maa://36713 (99.50)</t>
         </is>
       </c>
       <c r="Y11" s="19" t="n"/>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="AB11" s="8" t="inlineStr">
         <is>
-          <t>maa://29912 (99.78), maa://22516 (86.52)</t>
+          <t>maa://29912 (99.69), maa://22516 (85.56)</t>
         </is>
       </c>
       <c r="AC11" s="19" t="n"/>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="AF11" s="8" t="inlineStr">
         <is>
-          <t>maa://31203 (99.02)</t>
+          <t>maa://31203 (98.13)</t>
         </is>
       </c>
       <c r="AG11" s="16" t="n"/>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>maa://36678 (97.92), maa://30766 (91.67)</t>
+          <t>maa://36678 (98.18), maa://30766 (91.67)</t>
         </is>
       </c>
       <c r="E12" s="19" t="n"/>
@@ -2041,7 +2041,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (94.31), maa://54294 (98.07)</t>
+          <t>maa://21867 (94.46), maa://54294 (98.26)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (98.51), maa://64046 (98.91)</t>
+          <t>maa://63896 (98.57), maa://64046 (98.96)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2073,7 +2073,7 @@
       </c>
       <c r="P12" s="8" t="inlineStr">
         <is>
-          <t>maa://57541 (91.23)</t>
+          <t>maa://57541 (92.19)</t>
         </is>
       </c>
       <c r="Q12" s="19" t="n"/>
@@ -2105,7 +2105,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://37962 (98.84), maa://21485 (83.83), maa://22753 (93.28), maa://73860 (92.45)</t>
+          <t>maa://37962 (98.79), maa://21485 (83.96), maa://22753 (93.31), maa://73860 (95.50)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://36677 (99.11), maa://23669 (95.00), maa://39872 (98.24)</t>
+          <t>maa://36677 (99.18), maa://23669 (95.03), maa://39872 (98.31)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>maa://28932 (95.69)</t>
+          <t>maa://28932 (95.93)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2155,7 +2155,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (97.54), maa://36673 (95.32), maa://25001 (89.00)</t>
+          <t>maa://24999 (97.69), maa://36673 (95.38), maa://25001 (89.22)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.84), maa://66545 (98.68), *maa://22728 (70.19)</t>
+          <t>*maa://21248 (74.84), maa://66545 (98.73), *maa://22728 (73.04)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2203,7 +2203,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (97.86), maa://22583 (92.48), *maa://22500 (72.46)</t>
+          <t>maa://22676 (97.97), maa://22583 (92.96), *maa://22500 (73.61)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2219,7 +2219,7 @@
       </c>
       <c r="T13" s="8" t="inlineStr">
         <is>
-          <t>maa://21484 (100.00)</t>
+          <t>maa://21484 (99.33)</t>
         </is>
       </c>
       <c r="U13" s="19" t="n"/>
@@ -2235,7 +2235,7 @@
       </c>
       <c r="X13" s="8" t="inlineStr">
         <is>
-          <t>maa://34957 (95.57)</t>
+          <t>maa://34957 (95.83)</t>
         </is>
       </c>
       <c r="Y13" s="19" t="n"/>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (95.31)</t>
+          <t>maa://39883 (95.39)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>maa://30764 (95.51)</t>
+          <t>maa://30764 (95.81)</t>
         </is>
       </c>
       <c r="E14" s="19" t="n"/>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (99.29), maa://36682 (98.46), maa://26245 (97.13), maa://21288 (96.43)</t>
+          <t>maa://39841 (99.31), maa://36682 (98.49), maa://26245 (97.16), maa://21288 (96.43)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="P14" s="8" t="inlineStr">
         <is>
-          <t>maa://23250 (99.65), maa://20107 (87.50), maa://22772 (100.00), maa://68732 (100.00)</t>
+          <t>maa://23250 (99.72), maa://20107 (87.50), maa://22772 (100.00), maa://68732 (100.00)</t>
         </is>
       </c>
       <c r="Q14" s="19" t="n"/>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://42751 (99.28), maa://22521 (96.59)</t>
+          <t>maa://42751 (99.32), maa://22521 (96.76)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="X14" s="8" t="inlineStr">
         <is>
-          <t>maa://37468 (98.66)</t>
+          <t>maa://37468 (98.80)</t>
         </is>
       </c>
       <c r="Y14" s="19" t="n"/>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="AB14" s="8" t="inlineStr">
         <is>
-          <t>maa://22764 (99.24)</t>
+          <t>maa://22764 (99.31)</t>
         </is>
       </c>
       <c r="AC14" s="19" t="n"/>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (88.24), maa://45058 (98.55), maa://22734 (85.29), *maa://36048 (77.88), maa://69928 (97.70)</t>
+          <t>maa://22743 (88.58), maa://45058 (98.61), maa://22734 (85.40), *maa://36048 (78.04), maa://69928 (96.91)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2431,7 +2431,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (98.03), maa://21478 (90.91)</t>
+          <t>maa://24304 (98.11), maa://21478 (90.91)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2463,7 +2463,7 @@
       </c>
       <c r="P15" s="8" t="inlineStr">
         <is>
-          <t>maa://24762 (98.12), *maa://22727 (70.00)</t>
+          <t>maa://24762 (98.24), *maa://22727 (70.00)</t>
         </is>
       </c>
       <c r="Q15" s="19" t="n"/>
@@ -2479,7 +2479,7 @@
       </c>
       <c r="T15" s="8" t="inlineStr">
         <is>
-          <t>maa://23892 (98.25)</t>
+          <t>maa://23892 (98.37)</t>
         </is>
       </c>
       <c r="U15" s="19" t="n"/>
@@ -2495,7 +2495,7 @@
       </c>
       <c r="X15" s="8" t="inlineStr">
         <is>
-          <t>maa://38786 (94.00), maa://56102 (100.00)</t>
+          <t>maa://38786 (94.44), maa://56102 (100.00)</t>
         </is>
       </c>
       <c r="Y15" s="19" t="n"/>
@@ -2527,7 +2527,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://36666 (96.94), maa://21364 (84.58), *maa://22766 (71.13), maa://68306 (90.16)</t>
+          <t>maa://36666 (97.02), maa://21364 (84.75), *maa://22766 (71.13), maa://68306 (91.24)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2545,7 +2545,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://37650 (99.76), maa://21441 (96.67), maa://36679 (94.55)</t>
+          <t>maa://37650 (99.78), maa://21441 (96.68), maa://36679 (94.64)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2593,7 +2593,7 @@
       </c>
       <c r="P16" s="8" t="inlineStr">
         <is>
-          <t>maa://28504 (97.40)</t>
+          <t>maa://28504 (97.54)</t>
         </is>
       </c>
       <c r="Q16" s="19" t="n"/>
@@ -2609,7 +2609,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://36674 (98.20), maa://22729 (97.18), *maa://28648 (77.89)</t>
+          <t>maa://36674 (98.28), maa://22729 (97.33), *maa://28648 (77.89)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="X16" s="8" t="inlineStr">
         <is>
-          <t>maa://28501 (99.44), maa://28051 (97.37)</t>
+          <t>maa://28501 (99.47), maa://28051 (97.37)</t>
         </is>
       </c>
       <c r="Y16" s="19" t="n"/>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="AB16" s="8" t="inlineStr">
         <is>
-          <t>maa://26228 (98.17)</t>
+          <t>maa://26228 (98.49)</t>
         </is>
       </c>
       <c r="AC16" s="19" t="n"/>
@@ -2657,7 +2657,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>maa://23911 (91.72), maa://67613 (99.32), maa://27755 (93.75)</t>
+          <t>maa://23911 (91.86), maa://67613 (99.18), maa://27755 (93.75)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2675,7 +2675,7 @@
       </c>
       <c r="D17" s="8" t="inlineStr">
         <is>
-          <t>maa://21624 (88.68), maa://56358 (100.00)</t>
+          <t>maa://21624 (88.89), maa://56358 (100.00)</t>
         </is>
       </c>
       <c r="E17" s="19" t="n"/>
@@ -2691,7 +2691,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://39599 (98.81), maa://22430 (90.50)</t>
+          <t>maa://39599 (98.88), maa://22430 (90.50)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2707,7 +2707,7 @@
       </c>
       <c r="L17" s="8" t="inlineStr">
         <is>
-          <t>maa://21679 (91.18)</t>
+          <t>maa://21679 (91.43)</t>
         </is>
       </c>
       <c r="M17" s="19" t="n"/>
@@ -2723,7 +2723,7 @@
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (83.72), maa://56238 (98.56)</t>
+          <t>maa://23890 (84.09), maa://56238 (98.25)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2739,7 +2739,7 @@
       </c>
       <c r="T17" s="8" t="inlineStr">
         <is>
-          <t>*maa://42324 (75.23)</t>
+          <t>*maa://42324 (75.45)</t>
         </is>
       </c>
       <c r="U17" s="19" t="n"/>
@@ -2787,7 +2787,7 @@
       </c>
       <c r="AF17" s="8" t="inlineStr">
         <is>
-          <t>maa://50136 (99.31)</t>
+          <t>maa://50136 (99.34)</t>
         </is>
       </c>
       <c r="AG17" s="16" t="n"/>
@@ -2805,7 +2805,7 @@
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>maa://24570 (98.68)</t>
+          <t>maa://24570 (98.74)</t>
         </is>
       </c>
       <c r="E18" s="19" t="n"/>
@@ -2821,7 +2821,7 @@
       </c>
       <c r="H18" s="8" t="inlineStr">
         <is>
-          <t>maa://24421 (96.34)</t>
+          <t>maa://24421 (96.51)</t>
         </is>
       </c>
       <c r="I18" s="19" t="n"/>
@@ -2837,7 +2837,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://52226 (99.71), maa://22466 (92.95)</t>
+          <t>maa://52226 (99.68), maa://22466 (93.01)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2853,7 +2853,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://54153 (99.79), maa://24379 (100.00), maa://24380 (100.00)</t>
+          <t>maa://54153 (99.81), maa://24379 (100.00), maa://24380 (100.00)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="T18" s="8" t="inlineStr">
         <is>
-          <t>maa://24385 (97.78)</t>
+          <t>maa://24385 (97.87)</t>
         </is>
       </c>
       <c r="U18" s="19" t="n"/>
@@ -2885,7 +2885,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (99.23), maa://22741 (94.12)</t>
+          <t>maa://21917 (99.28), maa://22741 (94.12)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2901,7 +2901,7 @@
       </c>
       <c r="AB18" s="8" t="inlineStr">
         <is>
-          <t>maa://24393 (99.31)</t>
+          <t>maa://24393 (99.36)</t>
         </is>
       </c>
       <c r="AC18" s="19" t="n"/>
@@ -2912,12 +2912,12 @@
       </c>
       <c r="AE18" s="19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://47854 (95.32), *maa://68715 (75.00)</t>
+          <t>maa://47854 (95.49), *maa://68715 (75.00), maa://74015 (90.91)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -2935,7 +2935,7 @@
       </c>
       <c r="D19" s="8" t="inlineStr">
         <is>
-          <t>maa://62850 (99.46)</t>
+          <t>maa://62850 (99.48)</t>
         </is>
       </c>
       <c r="E19" s="19" t="n"/>
@@ -2951,7 +2951,7 @@
       </c>
       <c r="H19" s="8" t="inlineStr">
         <is>
-          <t>maa://66740 (95.24)</t>
+          <t>maa://66740 (95.45)</t>
         </is>
       </c>
       <c r="I19" s="19" t="n"/>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="L19" s="8" t="inlineStr">
         <is>
-          <t>maa://39347 (98.55), maa://56392 (100.00)</t>
+          <t>maa://39347 (98.65), maa://56392 (100.00)</t>
         </is>
       </c>
       <c r="M19" s="19" t="n"/>
@@ -2999,7 +2999,7 @@
       </c>
       <c r="T19" s="8" t="inlineStr">
         <is>
-          <t>maa://24386 (99.66)</t>
+          <t>maa://24386 (99.68)</t>
         </is>
       </c>
       <c r="U19" s="19" t="n"/>
@@ -3015,7 +3015,7 @@
       </c>
       <c r="X19" s="8" t="inlineStr">
         <is>
-          <t>maa://31386 (98.33), maa://58490 (91.43)</t>
+          <t>maa://31386 (96.83), maa://58490 (92.11)</t>
         </is>
       </c>
       <c r="Y19" s="19" t="n"/>
@@ -3031,7 +3031,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (90.06), *maa://36668 (71.54)</t>
+          <t>maa://30709 (90.51), *maa://36668 (72.00)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="AF19" s="8" t="inlineStr">
         <is>
-          <t>maa://52239 (91.03)</t>
+          <t>maa://52239 (91.95)</t>
         </is>
       </c>
       <c r="AG19" s="16" t="n"/>
@@ -3065,7 +3065,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://25198 (98.04), maa://36680 (99.17), maa://21432 (91.74)</t>
+          <t>maa://25198 (98.14), maa://36680 (99.09), maa://21432 (91.77)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3076,12 +3076,12 @@
       </c>
       <c r="G20" s="19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>maa://22864 (96.77)</t>
+          <t>maa://22864 (96.86), *maa://53361 (71.35)</t>
         </is>
       </c>
       <c r="I20" s="19" t="n"/>
@@ -3097,7 +3097,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (96.36)</t>
+          <t>maa://41331 (96.47)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3113,7 +3113,7 @@
       </c>
       <c r="P20" s="8" t="inlineStr">
         <is>
-          <t>maa://37442 (99.03)</t>
+          <t>maa://37442 (99.10)</t>
         </is>
       </c>
       <c r="Q20" s="19" t="n"/>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="T20" s="8" t="inlineStr">
         <is>
-          <t>maa://29113 (95.37)</t>
+          <t>maa://29113 (95.65)</t>
         </is>
       </c>
       <c r="U20" s="19" t="n"/>
@@ -3145,7 +3145,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://56241 (98.53), maa://50085 (97.33), maa://49976 (88.57)</t>
+          <t>maa://56241 (98.63), maa://50085 (97.35), maa://49976 (88.89)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3195,7 +3195,7 @@
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>maa://21261 (99.28)</t>
+          <t>maa://21261 (99.33)</t>
         </is>
       </c>
       <c r="E21" s="19" t="n"/>
@@ -3211,7 +3211,7 @@
       </c>
       <c r="H21" s="8" t="inlineStr">
         <is>
-          <t>maa://24372 (99.25)</t>
+          <t>maa://24372 (99.31)</t>
         </is>
       </c>
       <c r="I21" s="19" t="n"/>
@@ -3227,7 +3227,7 @@
       </c>
       <c r="L21" s="8" t="inlineStr">
         <is>
-          <t>maa://31731 (97.42)</t>
+          <t>maa://31731 (97.56)</t>
         </is>
       </c>
       <c r="M21" s="19" t="n"/>
@@ -3243,7 +3243,7 @@
       </c>
       <c r="P21" s="8" t="inlineStr">
         <is>
-          <t>maa://24381 (85.42)</t>
+          <t>maa://24381 (86.27)</t>
         </is>
       </c>
       <c r="Q21" s="19" t="n"/>
@@ -3259,7 +3259,7 @@
       </c>
       <c r="T21" s="8" t="inlineStr">
         <is>
-          <t>maa://21993 (92.50)</t>
+          <t>maa://21993 (93.02)</t>
         </is>
       </c>
       <c r="U21" s="19" t="n"/>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (98.56), maa://20110 (87.18)</t>
+          <t>maa://34946 (98.67), maa://20110 (87.18)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3291,7 +3291,7 @@
       </c>
       <c r="AB21" s="8" t="inlineStr">
         <is>
-          <t>maa://21443 (87.86), maa://52223 (89.53)</t>
+          <t>maa://21443 (87.90), maa://52223 (90.18)</t>
         </is>
       </c>
       <c r="AC21" s="19" t="n"/>
@@ -3307,7 +3307,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22432 (95.62), maa://22524 (83.00), maa://64221 (98.20)</t>
+          <t>maa://22432 (95.71), maa://64221 (98.26), maa://22524 (82.72)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>maa://25236 (99.30)</t>
+          <t>maa://25236 (99.33)</t>
         </is>
       </c>
       <c r="I22" s="19" t="n"/>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>maa://27127 (85.17), maa://66865 (99.68), *maa://22751 (71.26)</t>
+          <t>maa://27127 (85.39), maa://66865 (99.71), *maa://22751 (71.26)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="T22" s="8" t="inlineStr">
         <is>
-          <t>maa://38495 (86.79)</t>
+          <t>maa://38495 (87.72)</t>
         </is>
       </c>
       <c r="U22" s="19" t="n"/>
@@ -3405,7 +3405,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://37649 (95.95), maa://21282 (99.07)</t>
+          <t>maa://37649 (96.04), maa://21282 (99.10)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="AB22" s="8" t="inlineStr">
         <is>
-          <t>maa://23656 (99.64)</t>
+          <t>maa://23656 (99.67)</t>
         </is>
       </c>
       <c r="AC22" s="19" t="n"/>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="AF22" s="8" t="inlineStr">
         <is>
-          <t>maa://29658 (97.62)</t>
+          <t>maa://29658 (97.71)</t>
         </is>
       </c>
       <c r="AG22" s="16" t="n"/>
@@ -3455,7 +3455,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>*maa://41753 (71.59), **maa://28036 (31.58)</t>
+          <t>*maa://41753 (73.12), **maa://28036 (31.58)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3487,7 +3487,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (99.00), maa://39875 (95.45)</t>
+          <t>maa://39756 (99.03), maa://39875 (95.52)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3503,7 +3503,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (97.64), maa://29748 (83.09), *maa://37566 (79.41)</t>
+          <t>maa://30587 (97.76), maa://29748 (83.64), *maa://37566 (79.71)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="T23" s="8" t="inlineStr">
         <is>
-          <t>maa://31212 (96.25), maa://24387 (86.00), maa://67084 (90.91)</t>
+          <t>maa://31212 (96.45), maa://24387 (86.00), maa://67084 (90.91)</t>
         </is>
       </c>
       <c r="U23" s="19" t="n"/>
@@ -3535,7 +3535,7 @@
       </c>
       <c r="X23" s="8" t="inlineStr">
         <is>
-          <t>*maa://28503 (62.23)</t>
+          <t>*maa://28503 (61.26)</t>
         </is>
       </c>
       <c r="Y23" s="19" t="n"/>
@@ -3551,7 +3551,7 @@
       </c>
       <c r="AB23" s="8" t="inlineStr">
         <is>
-          <t>maa://29652 (97.52)</t>
+          <t>maa://29652 (97.67)</t>
         </is>
       </c>
       <c r="AC23" s="19" t="n"/>
@@ -3567,7 +3567,7 @@
       </c>
       <c r="AF23" s="8" t="inlineStr">
         <is>
-          <t>maa://31489 (98.84)</t>
+          <t>maa://31489 (98.89)</t>
         </is>
       </c>
       <c r="AG23" s="16" t="n"/>
@@ -3585,7 +3585,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (87.35), maa://46650 (93.01)</t>
+          <t>maa://24368 (87.67), maa://46650 (92.97)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3649,7 +3649,7 @@
       </c>
       <c r="T24" s="8" t="inlineStr">
         <is>
-          <t>maa://73341 (98.25)</t>
+          <t>maa://73341 (98.12)</t>
         </is>
       </c>
       <c r="U24" s="19" t="n"/>
@@ -3665,7 +3665,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (97.41), maa://23504 (94.14), maa://25141 (80.98), maa://52227 (97.78), maa://36663 (80.36)</t>
+          <t>maa://29988 (97.59), maa://23504 (94.16), maa://25141 (81.10), maa://52227 (97.86), maa://36663 (80.53)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3681,7 +3681,7 @@
       </c>
       <c r="AB24" s="8" t="inlineStr">
         <is>
-          <t>maa://39349 (98.21)</t>
+          <t>maa://39349 (98.36)</t>
         </is>
       </c>
       <c r="AC24" s="19" t="n"/>
@@ -3697,7 +3697,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://64165 (99.33), *maa://22523 (79.82), maa://29910 (94.20), maa://45831 (94.59)</t>
+          <t>maa://64165 (99.38), *maa://22523 (79.82), maa://29910 (94.20), maa://45831 (94.59)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3715,7 +3715,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (97.19), maa://63016 (99.48)</t>
+          <t>maa://29753 (97.13), maa://63016 (99.51)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3731,7 +3731,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>maa://29063 (80.62), *maa://25311 (71.05), maa://45047 (87.91)</t>
+          <t>maa://29063 (80.95), *maa://25311 (70.78), maa://45047 (87.91)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3747,7 +3747,7 @@
       </c>
       <c r="L25" s="8" t="inlineStr">
         <is>
-          <t>maa://24378 (94.19), maa://68415 (91.67)</t>
+          <t>maa://24378 (94.25), maa://68415 (93.10)</t>
         </is>
       </c>
       <c r="M25" s="19" t="n"/>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="P25" s="8" t="inlineStr">
         <is>
-          <t>maa://24382 (97.18)</t>
+          <t>maa://24382 (96.05)</t>
         </is>
       </c>
       <c r="Q25" s="19" t="n"/>
@@ -3779,7 +3779,7 @@
       </c>
       <c r="T25" s="8" t="inlineStr">
         <is>
-          <t>maa://20109 (97.42), maa://22545 (99.87)</t>
+          <t>maa://20109 (97.61), maa://22545 (99.87)</t>
         </is>
       </c>
       <c r="U25" s="19" t="n"/>
@@ -3795,7 +3795,7 @@
       </c>
       <c r="X25" s="8" t="inlineStr">
         <is>
-          <t>maa://29890 (93.68)</t>
+          <t>maa://29890 (93.82)</t>
         </is>
       </c>
       <c r="Y25" s="19" t="n"/>
@@ -3811,7 +3811,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (93.90), maa://68311 (98.49), *maa://24516 (78.43), maa://26001 (81.97)</t>
+          <t>maa://31215 (93.98), maa://68311 (98.65), *maa://24516 (78.43), maa://26001 (81.97)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3827,7 +3827,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (98.83), maa://36676 (99.87), maa://24621 (96.95), maa://22771 (88.89), maa://37772 (87.50)</t>
+          <t>maa://20108 (98.92), maa://36676 (99.87), maa://24621 (96.97), maa://22771 (88.89), maa://37772 (87.50)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3845,7 +3845,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://56374 (100.00), maa://41802 (98.08)</t>
+          <t>maa://56374 (100.00), maa://41802 (98.21)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3861,7 +3861,7 @@
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
-          <t>maa://56240 (95.67), maa://24913 (92.86)</t>
+          <t>maa://56240 (95.81), maa://24913 (92.91)</t>
         </is>
       </c>
       <c r="I26" s="19" t="n"/>
@@ -3893,7 +3893,7 @@
       </c>
       <c r="P26" s="8" t="inlineStr">
         <is>
-          <t>maa://56625 (99.09), maa://39870 (95.35)</t>
+          <t>maa://56625 (99.17), maa://39870 (95.35)</t>
         </is>
       </c>
       <c r="Q26" s="19" t="n"/>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="X26" s="8" t="inlineStr">
         <is>
-          <t>maa://24389 (98.85)</t>
+          <t>maa://24389 (98.90)</t>
         </is>
       </c>
       <c r="Y26" s="19" t="n"/>
@@ -3941,7 +3941,7 @@
       </c>
       <c r="AB26" s="8" t="inlineStr">
         <is>
-          <t>maa://42235 (98.93)</t>
+          <t>maa://42235 (98.98)</t>
         </is>
       </c>
       <c r="AC26" s="19" t="n"/>
@@ -3957,7 +3957,7 @@
       </c>
       <c r="AF26" s="8" t="inlineStr">
         <is>
-          <t>*maa://30511 (73.40), **maa://29760 (45.45)</t>
+          <t>*maa://30511 (73.68), **maa://29760 (45.45)</t>
         </is>
       </c>
       <c r="AG26" s="16" t="n"/>
@@ -3991,7 +3991,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>maa://39601 (94.58), maa://34494 (96.23)</t>
+          <t>maa://39601 (94.39), maa://34494 (96.26)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4007,7 +4007,7 @@
       </c>
       <c r="L27" s="8" t="inlineStr">
         <is>
-          <t>maa://28071 (92.21)</t>
+          <t>maa://28071 (92.59)</t>
         </is>
       </c>
       <c r="M27" s="19" t="n"/>
@@ -4023,7 +4023,7 @@
       </c>
       <c r="P27" s="8" t="inlineStr">
         <is>
-          <t>maa://56400 (92.00)</t>
+          <t>maa://56400 (92.86)</t>
         </is>
       </c>
       <c r="Q27" s="19" t="n"/>
@@ -4039,7 +4039,7 @@
       </c>
       <c r="T27" s="8" t="inlineStr">
         <is>
-          <t>maa://30624 (91.95)</t>
+          <t>maa://30624 (91.90)</t>
         </is>
       </c>
       <c r="U27" s="19" t="n"/>
@@ -4087,7 +4087,7 @@
       </c>
       <c r="AF27" s="8" t="inlineStr">
         <is>
-          <t>maa://24023 (98.37)</t>
+          <t>maa://24023 (98.48)</t>
         </is>
       </c>
       <c r="AG27" s="16" t="n"/>
@@ -4105,7 +4105,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (96.64), maa://25725 (86.03)</t>
+          <t>maa://24465 (96.77), maa://25725 (86.52)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4137,7 +4137,7 @@
       </c>
       <c r="L28" s="8" t="inlineStr">
         <is>
-          <t>maa://30770 (90.83)</t>
+          <t>maa://30770 (91.13)</t>
         </is>
       </c>
       <c r="M28" s="19" t="n"/>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="T28" s="8" t="inlineStr">
         <is>
-          <t>maa://29765 (95.25), maa://23263 (97.14)</t>
+          <t>maa://29765 (95.45), maa://23263 (97.27)</t>
         </is>
       </c>
       <c r="U28" s="19" t="n"/>
@@ -4185,7 +4185,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (97.98), maa://41749 (97.43)</t>
+          <t>maa://39929 (98.09), maa://41749 (97.47)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4217,7 +4217,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (94.81), maa://65700 (98.73)</t>
+          <t>maa://36660 (95.12), maa://65700 (98.80)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4235,7 +4235,7 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>maa://31694 (99.48)</t>
+          <t>maa://31694 (99.50)</t>
         </is>
       </c>
       <c r="E29" s="19" t="n"/>
@@ -4251,7 +4251,7 @@
       </c>
       <c r="H29" s="8" t="inlineStr">
         <is>
-          <t>maa://73558 (100.00)</t>
+          <t>maa://73558 (92.31)</t>
         </is>
       </c>
       <c r="I29" s="19" t="n"/>
@@ -4267,7 +4267,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (98.36), maa://31400 (98.30), maa://28440 (87.13)</t>
+          <t>maa://28432 (98.46), maa://31400 (98.33), maa://28440 (87.21)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4283,7 +4283,7 @@
       </c>
       <c r="P29" s="8" t="inlineStr">
         <is>
-          <t>maa://54169 (97.83)</t>
+          <t>maa://54169 (97.52)</t>
         </is>
       </c>
       <c r="Q29" s="19" t="n"/>
@@ -4347,7 +4347,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://42865 (94.23)</t>
+          <t>maa://42865 (94.47)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4365,7 +4365,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (96.43), maa://64191 (97.06)</t>
+          <t>maa://45792 (96.51), maa://64191 (96.15)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4397,7 +4397,7 @@
       </c>
       <c r="L30" s="8" t="inlineStr">
         <is>
-          <t>maa://30442 (98.21)</t>
+          <t>maa://30442 (98.24)</t>
         </is>
       </c>
       <c r="M30" s="19" t="n"/>
@@ -4413,7 +4413,7 @@
       </c>
       <c r="P30" s="8" t="inlineStr">
         <is>
-          <t>maa://21442 (99.60), maa://68394 (100.00), maa://66611 (100.00)</t>
+          <t>maa://21442 (99.47), maa://68394 (100.00), maa://66611 (100.00)</t>
         </is>
       </c>
       <c r="Q30" s="19" t="n"/>
@@ -4429,7 +4429,7 @@
       </c>
       <c r="T30" s="8" t="inlineStr">
         <is>
-          <t>*maa://32940 (80.00), maa://24388 (96.77)</t>
+          <t>maa://32940 (81.25), maa://24388 (96.77)</t>
         </is>
       </c>
       <c r="U30" s="19" t="n"/>
@@ -4445,7 +4445,7 @@
       </c>
       <c r="X30" s="8" t="inlineStr">
         <is>
-          <t>maa://39477 (97.44)</t>
+          <t>maa://39477 (96.30)</t>
         </is>
       </c>
       <c r="Y30" s="19" t="n"/>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="AB30" s="8" t="inlineStr">
         <is>
-          <t>maa://42979 (99.61), maa://45822 (100.00), maa://45045 (94.12)</t>
+          <t>maa://42979 (99.64), maa://45822 (100.00), maa://45045 (94.74)</t>
         </is>
       </c>
       <c r="AC30" s="19" t="n"/>
@@ -4527,7 +4527,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (98.64), maa://36258 (94.09), maa://43904 (91.94)</t>
+          <t>maa://35926 (98.68), maa://36258 (94.18), maa://43904 (92.42)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="T31" s="8" t="inlineStr">
         <is>
-          <t>maa://30711 (97.37), maa://30768 (100.00)</t>
+          <t>maa://30711 (97.52), maa://30768 (100.00)</t>
         </is>
       </c>
       <c r="U31" s="19" t="n"/>
@@ -4591,7 +4591,7 @@
       </c>
       <c r="AB31" s="8" t="inlineStr">
         <is>
-          <t>maa://66997 (97.30)</t>
+          <t>maa://66997 (97.44)</t>
         </is>
       </c>
       <c r="AC31" s="19" t="n"/>
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://36667 (99.71), maa://21895 (98.06), maa://22760 (100.00)</t>
+          <t>maa://36667 (99.72), maa://21895 (98.08), maa://22760 (100.00)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4657,7 +4657,7 @@
       </c>
       <c r="L32" s="8" t="inlineStr">
         <is>
-          <t>maa://28065 (97.62)</t>
+          <t>maa://28065 (97.74)</t>
         </is>
       </c>
       <c r="M32" s="19" t="n"/>
@@ -4689,7 +4689,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (99.45), maa://41108 (88.89), maa://41238 (98.26), maa://45523 (100.00)</t>
+          <t>maa://42859 (99.48), maa://41108 (89.06), maa://41238 (98.30), maa://45523 (100.00)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4705,7 +4705,7 @@
       </c>
       <c r="X32" s="8" t="inlineStr">
         <is>
-          <t>maa://64104 (97.33)</t>
+          <t>maa://64104 (97.46)</t>
         </is>
       </c>
       <c r="Y32" s="19" t="n"/>
@@ -4737,7 +4737,7 @@
       </c>
       <c r="AF32" s="8" t="inlineStr">
         <is>
-          <t>maa://42408 (95.92)</t>
+          <t>maa://42408 (96.15)</t>
         </is>
       </c>
       <c r="AG32" s="16" t="n"/>
@@ -4803,7 +4803,7 @@
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (95.36), maa://69135 (98.96), maa://73357 (100.00)</t>
+          <t>maa://21956 (95.51), maa://69135 (98.99), maa://73357 (100.00)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4819,7 +4819,7 @@
       </c>
       <c r="T33" s="8" t="inlineStr">
         <is>
-          <t>maa://45558 (90.91)</t>
+          <t>maa://45558 (91.84)</t>
         </is>
       </c>
       <c r="U33" s="19" t="n"/>
@@ -4851,7 +4851,7 @@
       </c>
       <c r="AB33" s="8" t="inlineStr">
         <is>
-          <t>maa://73340 (99.59), maa://73523 (95.65)</t>
+          <t>maa://73340 (99.69), maa://73523 (97.44)</t>
         </is>
       </c>
       <c r="AC33" s="19" t="n"/>
@@ -4901,7 +4901,7 @@
       </c>
       <c r="H34" s="8" t="inlineStr">
         <is>
-          <t>maa://66817 (99.25)</t>
+          <t>maa://66817 (99.29)</t>
         </is>
       </c>
       <c r="I34" s="19" t="n"/>
@@ -4933,7 +4933,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://56235 (99.57), maa://48817 (99.44)</t>
+          <t>maa://56235 (99.47), maa://48817 (99.46)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -4949,7 +4949,7 @@
       </c>
       <c r="T34" s="8" t="inlineStr">
         <is>
-          <t>maa://24526 (97.82)</t>
+          <t>maa://24526 (97.92)</t>
         </is>
       </c>
       <c r="U34" s="19" t="n"/>
@@ -4981,7 +4981,7 @@
       </c>
       <c r="AB34" s="8" t="inlineStr">
         <is>
-          <t>maa://64329 (98.92)</t>
+          <t>maa://64329 (99.02)</t>
         </is>
       </c>
       <c r="AC34" s="19" t="n"/>
@@ -4997,7 +4997,7 @@
       </c>
       <c r="AF34" s="8" t="inlineStr">
         <is>
-          <t>maa://32650 (90.28)</t>
+          <t>maa://32650 (90.54)</t>
         </is>
       </c>
       <c r="AG34" s="16" t="n"/>
@@ -5047,7 +5047,7 @@
       </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
-          <t>maa://41296 (99.48)</t>
+          <t>maa://41296 (99.50)</t>
         </is>
       </c>
       <c r="M35" s="19" t="n"/>
@@ -5079,7 +5079,7 @@
       </c>
       <c r="T35" s="8" t="inlineStr">
         <is>
-          <t>maa://24842 (97.44)</t>
+          <t>maa://24842 (97.50)</t>
         </is>
       </c>
       <c r="U35" s="19" t="n"/>
@@ -5127,7 +5127,7 @@
       </c>
       <c r="AF35" s="8" t="inlineStr">
         <is>
-          <t>maa://39479 (94.52)</t>
+          <t>maa://39479 (94.74)</t>
         </is>
       </c>
       <c r="AG35" s="16" t="n"/>
@@ -5161,7 +5161,7 @@
       </c>
       <c r="H36" s="8" t="inlineStr">
         <is>
-          <t>maa://24375 (95.74)</t>
+          <t>maa://24375 (96.04)</t>
         </is>
       </c>
       <c r="I36" s="19" t="n"/>
@@ -5177,7 +5177,7 @@
       </c>
       <c r="L36" s="8" t="inlineStr">
         <is>
-          <t>maa://42240 (99.18)</t>
+          <t>maa://42240 (99.22)</t>
         </is>
       </c>
       <c r="M36" s="19" t="n"/>
@@ -5209,7 +5209,7 @@
       </c>
       <c r="T36" s="8" t="inlineStr">
         <is>
-          <t>maa://27613 (99.67)</t>
+          <t>maa://27613 (99.69)</t>
         </is>
       </c>
       <c r="U36" s="19" t="n"/>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="AB36" s="19" t="inlineStr">
         <is>
-          <t>maa://64106 (96.92)</t>
+          <t>maa://64106 (97.10)</t>
         </is>
       </c>
       <c r="AC36" s="19" t="n"/>
@@ -5291,7 +5291,7 @@
       </c>
       <c r="H37" s="8" t="inlineStr">
         <is>
-          <t>*maa://24374 (62.86)</t>
+          <t>*maa://24374 (62.50)</t>
         </is>
       </c>
       <c r="I37" s="19" t="n"/>
@@ -5307,7 +5307,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (99.04), maa://56336 (99.45), maa://47069 (89.66), maa://45789 (100.00)</t>
+          <t>maa://45718 (99.06), maa://56336 (99.49), maa://47069 (89.66), maa://45789 (100.00)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5323,7 +5323,7 @@
       </c>
       <c r="P37" s="8" t="inlineStr">
         <is>
-          <t>maa://21280 (98.12), *maa://21239 (70.59)</t>
+          <t>maa://21280 (98.19), *maa://21239 (70.59)</t>
         </is>
       </c>
       <c r="Q37" s="19" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="L38" s="8" t="inlineStr">
         <is>
-          <t>maa://39384 (99.51), maa://49735 (90.00)</t>
+          <t>maa://39384 (99.55), maa://49735 (90.00)</t>
         </is>
       </c>
       <c r="M38" s="19" t="n"/>
@@ -5437,7 +5437,7 @@
       </c>
       <c r="P38" s="8" t="inlineStr">
         <is>
-          <t>maa://24383 (85.65)</t>
+          <t>maa://24383 (86.18)</t>
         </is>
       </c>
       <c r="Q38" s="19" t="n"/>
@@ -5453,7 +5453,7 @@
       </c>
       <c r="T38" s="8" t="inlineStr">
         <is>
-          <t>maa://30713 (98.81)</t>
+          <t>maa://30713 (98.82)</t>
         </is>
       </c>
       <c r="U38" s="19" t="n"/>
@@ -5485,7 +5485,7 @@
       </c>
       <c r="AF38" s="8" t="inlineStr">
         <is>
-          <t>maa://36697 (96.02), maa://68397 (99.07)</t>
+          <t>maa://36697 (96.07), maa://68397 (99.10)</t>
         </is>
       </c>
       <c r="AG38" s="16" t="n"/>
@@ -5519,7 +5519,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://45059 (95.63), maa://25199 (85.23), maa://30434 (95.69), maa://44165 (85.71)</t>
+          <t>maa://45059 (95.67), maa://25199 (85.53), maa://30434 (95.71), maa://44165 (85.71)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://47093 (98.92), maa://24709 (94.83)</t>
+          <t>maa://47093 (98.99), maa://24709 (94.93)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5567,7 +5567,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (96.54), maa://45790 (89.47), *maa://56232 (73.50)</t>
+          <t>maa://47079 (96.67), maa://45790 (89.69), *maa://56232 (73.98)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5665,7 +5665,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (98.36), maa://21386 (96.15), maa://36664 (89.29), *maa://45550 (76.92)</t>
+          <t>maa://23278 (98.41), maa://21386 (96.19), maa://36664 (89.41), *maa://45550 (76.92)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5713,7 +5713,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://65283 (97.57), *maa://64107 (72.34), maa://64205 (95.00)</t>
+          <t>maa://65283 (97.71), *maa://64107 (72.92), maa://64205 (95.24)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="H41" s="8" t="inlineStr">
         <is>
-          <t>maa://24466 (94.05)</t>
+          <t>maa://24466 (94.38)</t>
         </is>
       </c>
       <c r="I41" s="19" t="n"/>
@@ -5766,7 +5766,7 @@
       </c>
       <c r="P41" s="8" t="inlineStr">
         <is>
-          <t>maa://43177 (96.91)</t>
+          <t>maa://43177 (97.13)</t>
         </is>
       </c>
       <c r="Q41" s="19" t="n"/>
@@ -5936,7 +5936,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>maa://21284 (98.49)</t>
+          <t>maa://21284 (98.58)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -5968,7 +5968,7 @@
       </c>
       <c r="P43" s="8" t="inlineStr">
         <is>
-          <t>maa://47403 (92.31)</t>
+          <t>maa://47403 (92.59)</t>
         </is>
       </c>
       <c r="Q43" s="19" t="n"/>
@@ -5984,7 +5984,7 @@
       </c>
       <c r="T43" s="8" t="inlineStr">
         <is>
-          <t>maa://43198 (100.00), maa://46286 (94.12)</t>
+          <t>maa://43198 (100.00), maa://46286 (94.74)</t>
         </is>
       </c>
       <c r="U43" s="19" t="n"/>
@@ -6037,7 +6037,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (98.51), maa://56386 (99.65), maa://27728 (96.46)</t>
+          <t>maa://29768 (98.54), maa://56386 (99.68), maa://27728 (96.46)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6085,7 +6085,7 @@
       </c>
       <c r="T44" s="8" t="inlineStr">
         <is>
-          <t>maa://39366 (95.28)</t>
+          <t>maa://39366 (94.70)</t>
         </is>
       </c>
       <c r="U44" s="19" t="n"/>
@@ -6138,7 +6138,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://42459 (98.94), maa://21229 (86.96), maa://30807 (94.68), maa://22767 (81.15)</t>
+          <t>maa://42459 (99.00), maa://21229 (87.26), maa://30807 (94.68), maa://22767 (82.22)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="P45" s="8" t="inlineStr">
         <is>
-          <t>maa://36237 (88.24)</t>
+          <t>maa://36237 (88.46)</t>
         </is>
       </c>
       <c r="Q45" s="19" t="n"/>
@@ -6186,7 +6186,7 @@
       </c>
       <c r="T45" s="8" t="inlineStr">
         <is>
-          <t>*maa://39364 (74.78), maa://73997 (100.00)</t>
+          <t>*maa://39364 (75.00), maa://73997 (100.00)</t>
         </is>
       </c>
       <c r="U45" s="19" t="n"/>
@@ -6223,7 +6223,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (96.86), maa://43901 (97.64)</t>
+          <t>maa://35931 (96.92), maa://43901 (97.81)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6292,7 +6292,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (97.71), maa://56236 (99.87), maa://29661 (97.42), maa://28038 (84.62)</t>
+          <t>maa://27410 (97.74), maa://56236 (99.88), maa://29661 (97.47), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6324,7 +6324,7 @@
       </c>
       <c r="T47" s="8" t="inlineStr">
         <is>
-          <t>maa://68392 (99.75), maa://67476 (99.60)</t>
+          <t>maa://68392 (99.78), maa://67476 (99.60)</t>
         </is>
       </c>
       <c r="U47" s="19" t="n"/>
@@ -6446,7 +6446,7 @@
       </c>
       <c r="P49" s="8" t="inlineStr">
         <is>
-          <t>maa://39643 (83.94)</t>
+          <t>maa://39643 (84.34)</t>
         </is>
       </c>
       <c r="Q49" s="19" t="n"/>
@@ -6462,7 +6462,7 @@
       </c>
       <c r="T49" s="19" t="inlineStr">
         <is>
-          <t>maa://67231 (99.40)</t>
+          <t>maa://67231 (99.44)</t>
         </is>
       </c>
       <c r="U49" s="19" t="n"/>
@@ -6499,7 +6499,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>maa://62852 (94.69), maa://73565 (97.73)</t>
+          <t>maa://62852 (94.75), maa://73565 (97.75)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6533,7 +6533,7 @@
       </c>
       <c r="H51" s="8" t="inlineStr">
         <is>
-          <t>maa://30769 (89.74)</t>
+          <t>maa://30769 (90.24)</t>
         </is>
       </c>
       <c r="I51" s="19" t="n"/>
@@ -6583,7 +6583,7 @@
       </c>
       <c r="H52" s="8" t="inlineStr">
         <is>
-          <t>maa://24376 (99.40)</t>
+          <t>maa://24376 (99.44)</t>
         </is>
       </c>
       <c r="I52" s="19" t="n"/>
@@ -6599,7 +6599,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (99.54), maa://65511 (100.00), maa://59378 (94.05)</t>
+          <t>maa://59394 (99.56), maa://65511 (100.00), maa://59378 (94.05)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6633,7 +6633,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (98.48)</t>
+          <t>maa://32534 (98.57)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -6733,7 +6733,7 @@
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>maa://32532 (98.40)</t>
+          <t>maa://32532 (98.49)</t>
         </is>
       </c>
       <c r="I55" s="19" t="n"/>
@@ -6749,7 +6749,7 @@
       </c>
       <c r="P55" s="16" t="inlineStr">
         <is>
-          <t>maa://73349 (97.30)</t>
+          <t>maa://73349 (97.87)</t>
         </is>
       </c>
       <c r="Q55" s="16" t="n"/>
@@ -6833,7 +6833,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://56237 (98.59), maa://25176 (98.85), maa://73737 (100.00)</t>
+          <t>maa://56237 (98.61), maa://25176 (97.73), maa://73737 (100.00)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6851,7 +6851,7 @@
       </c>
       <c r="H58" s="8" t="inlineStr">
         <is>
-          <t>*maa://37964 (72.56)</t>
+          <t>*maa://37964 (72.51)</t>
         </is>
       </c>
       <c r="I58" s="19" t="n"/>
@@ -6869,7 +6869,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (98.84), maa://27746 (90.15)</t>
+          <t>maa://31270 (98.91), maa://27746 (90.20)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -6887,7 +6887,7 @@
       </c>
       <c r="H60" s="8" t="inlineStr">
         <is>
-          <t>maa://40438 (94.39), *maa://73999 (80.00)</t>
+          <t>maa://40438 (94.66), *maa://73999 (77.78)</t>
         </is>
       </c>
       <c r="I60" s="19" t="n"/>
@@ -6923,7 +6923,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (96.23), maa://56228 (98.87), maa://43903 (100.00)</t>
+          <t>maa://42981 (96.36), maa://56228 (98.93), maa://43903 (100.00)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6941,7 +6941,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (99.61), *maa://59693 (71.93), maa://59413 (98.28)</t>
+          <t>maa://59534 (99.64), *maa://59693 (71.19), maa://59413 (98.40)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -7157,7 +7157,7 @@
       </c>
       <c r="H75" s="19" t="inlineStr">
         <is>
-          <t>maa://67748 (90.32)</t>
+          <t>maa://67748 (90.38)</t>
         </is>
       </c>
       <c r="I75" s="19" t="n"/>
@@ -7317,7 +7317,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.11.06 13:22:37</t>
+          <t>更新日期：2025.11.10 13:23:00</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -7803,7 +7803,7 @@
       </c>
       <c r="D10" s="13" t="inlineStr">
         <is>
-          <t>*maa://20888 (80.00)</t>
+          <t>maa://20888 (81.82)</t>
         </is>
       </c>
       <c r="E10" s="14" t="inlineStr">
@@ -8451,7 +8451,7 @@
       </c>
       <c r="D22" s="13" t="inlineStr">
         <is>
-          <t>maa://20948 (90.00), maa://30844 (100.00), maa://63387 (100.00), maa://58691 (100.00)</t>
+          <t>maa://20948 (90.91), maa://30844 (100.00), maa://63387 (100.00), maa://58691 (100.00)</t>
         </is>
       </c>
       <c r="E22" s="14" t="inlineStr">
@@ -8721,7 +8721,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (74.14), *maa://28758 (72.34), maa://65357 (97.73), maa://29036 (96.77), *maa://42172 (71.43), maa://30285 (100.00)</t>
+          <t>*maa://20849 (74.14), *maa://28758 (72.34), maa://65357 (97.78), maa://29036 (96.77), *maa://42172 (71.43), maa://30285 (100.00)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8829,7 +8829,7 @@
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>maa://20863 (90.82), maa://20832 (98.51), maa://20727 (100.00)</t>
+          <t>maa://20863 (90.85), maa://20832 (98.52), maa://20727 (100.00)</t>
         </is>
       </c>
       <c r="E29" s="14" t="inlineStr">
@@ -8986,12 +8986,12 @@
       </c>
       <c r="C32" s="12" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (90.78), maa://36866 (97.26), maa://62759 (100.00), maa://45572 (88.89), maa://27794 (100.00), maa://70680 (100.00), maa://20960 (100.00), maa://20843 (100.00), *maa://20893 (75.00), **maa://24483 (50.00), maa://20862 (85.71)</t>
+          <t>maa://36644 (90.78), maa://36866 (97.26), maa://62759 (100.00), maa://45572 (88.89), maa://27794 (100.00), maa://70680 (100.00), maa://20960 (100.00), maa://20843 (100.00), *maa://20893 (75.00), **maa://24483 (50.00), maa://20862 (85.71), maa://74314 (100.00)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -9045,7 +9045,7 @@
       </c>
       <c r="D33" s="13" t="inlineStr">
         <is>
-          <t>maa://30500 (98.99), *maa://27290 (72.22), ***maa://42154 (8.33)</t>
+          <t>maa://30500 (99.00), *maa://27290 (72.22), ***maa://42154 (8.33)</t>
         </is>
       </c>
       <c r="E33" s="14" t="inlineStr">
@@ -9261,7 +9261,7 @@
       </c>
       <c r="D37" s="13" t="inlineStr">
         <is>
-          <t>maa://27376 (91.43), maa://42635 (94.83), *maa://20838 (55.00)</t>
+          <t>maa://27376 (91.55), maa://42635 (94.83), *maa://20838 (55.00)</t>
         </is>
       </c>
       <c r="E37" s="14" t="inlineStr">
@@ -9531,7 +9531,7 @@
       </c>
       <c r="D42" s="13" t="inlineStr">
         <is>
-          <t>maa://34883 (94.44), maa://20918 (96.55), maa://20824 (100.00)</t>
+          <t>maa://34883 (94.44), maa://20918 (96.67), maa://20824 (100.00)</t>
         </is>
       </c>
       <c r="E42" s="14" t="inlineStr">
@@ -10449,7 +10449,7 @@
       </c>
       <c r="D59" s="13" t="inlineStr">
         <is>
-          <t>maa://27970 (98.92), maa://41118 (88.89)</t>
+          <t>maa://27970 (98.96), maa://41118 (90.00)</t>
         </is>
       </c>
       <c r="E59" s="14" t="inlineStr">
@@ -10557,7 +10557,7 @@
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (99.31), maa://31559 (94.12), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00), maa://66633 (100.00)</t>
+          <t>maa://20841 (99.32), maa://31559 (94.23), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00), maa://66633 (100.00)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -10611,7 +10611,7 @@
       </c>
       <c r="D62" s="13" t="inlineStr">
         <is>
-          <t>maa://40590 (99.41), *maa://72388 (57.14)</t>
+          <t>maa://40590 (99.42), *maa://72388 (55.56)</t>
         </is>
       </c>
       <c r="E62" s="14" t="inlineStr">
@@ -11043,7 +11043,7 @@
       </c>
       <c r="D70" s="13" t="inlineStr">
         <is>
-          <t>maa://20974 (97.12), maa://29079 (80.95), maa://29096 (91.67), maa://29087 (100.00), *maa://20823 (75.00), maa://20855 (94.44), maa://63722 (85.71), maa://20904 (100.00), **maa://72704 (50.00)</t>
+          <t>maa://20974 (97.12), maa://29079 (80.95), maa://29096 (91.67), maa://29087 (100.00), *maa://20823 (75.00), maa://20855 (94.44), maa://63722 (85.71), maa://20904 (100.00), *maa://72704 (66.67)</t>
         </is>
       </c>
       <c r="E70" s="14" t="inlineStr">
@@ -11151,7 +11151,7 @@
       </c>
       <c r="D72" s="13" t="inlineStr">
         <is>
-          <t>maa://20943 (99.49), maa://30673 (100.00), maa://30672 (100.00), maa://20856 (100.00), maa://71555 (100.00)</t>
+          <t>maa://20943 (99.50), maa://30673 (100.00), maa://30672 (100.00), maa://20856 (100.00), maa://71555 (85.71)</t>
         </is>
       </c>
       <c r="E72" s="14" t="inlineStr">
@@ -11205,7 +11205,7 @@
       </c>
       <c r="D73" s="13" t="inlineStr">
         <is>
-          <t>maa://36643 (98.54), maa://36864 (98.17), maa://39140 (100.00), maa://66335 (100.00)</t>
+          <t>maa://36643 (98.55), maa://36864 (98.17), maa://39140 (100.00), maa://66335 (100.00)</t>
         </is>
       </c>
       <c r="E73" s="14" t="inlineStr">
@@ -11475,7 +11475,7 @@
       </c>
       <c r="D78" s="13" t="inlineStr">
         <is>
-          <t>maa://20958 (95.83), ***maa://39769 (20.00)</t>
+          <t>maa://20958 (95.92), ***maa://39769 (20.00)</t>
         </is>
       </c>
       <c r="E78" s="14" t="inlineStr">
@@ -12609,7 +12609,7 @@
       </c>
       <c r="D99" s="13" t="inlineStr">
         <is>
-          <t>maa://20991 (100.00), maa://51015 (88.68)</t>
+          <t>maa://20991 (100.00), maa://51015 (87.50)</t>
         </is>
       </c>
       <c r="E99" s="14" t="inlineStr">
@@ -12717,7 +12717,7 @@
       </c>
       <c r="D101" s="13" t="inlineStr">
         <is>
-          <t>maa://20929 (93.55)</t>
+          <t>maa://20929 (93.75)</t>
         </is>
       </c>
       <c r="E101" s="14" t="inlineStr">
@@ -12933,7 +12933,7 @@
       </c>
       <c r="D105" s="13" t="inlineStr">
         <is>
-          <t>*maa://29094 (75.81), maa://28904 (89.36), **maa://20931 (47.37)</t>
+          <t>*maa://29094 (76.19), maa://28904 (89.36), **maa://20931 (47.37)</t>
         </is>
       </c>
       <c r="E105" s="14" t="inlineStr">
@@ -13203,7 +13203,7 @@
       </c>
       <c r="D110" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.69), maa://25018 (97.01), maa://25776 (92.77), maa://28361 (95.56), maa://25772 (94.12), maa://56588 (94.59), maa://45194 (86.36), maa://32653 (81.25), maa://25161 (84.21), maa://61839 (100.00), **maa://60902 (38.46), maa://61275 (100.00), *maa://73473 (66.67)</t>
+          <t>maa://51881 (98.70), maa://25018 (97.02), maa://25776 (92.77), maa://28361 (95.56), maa://25772 (94.12), maa://56588 (94.59), maa://45194 (86.36), maa://32653 (81.25), maa://25161 (84.21), maa://61839 (100.00), **maa://60902 (38.46), maa://61275 (100.00), *maa://73473 (75.00)</t>
         </is>
       </c>
       <c r="E110" s="14" t="inlineStr">
@@ -13635,7 +13635,7 @@
       </c>
       <c r="D118" s="13" t="inlineStr">
         <is>
-          <t>maa://20908 (98.24), maa://35723 (96.08), *maa://23346 (77.78), maa://38822 (100.00), maa://58659 (92.31)</t>
+          <t>maa://20908 (98.25), maa://35723 (96.08), *maa://23346 (77.78), maa://38822 (100.00), maa://58659 (92.31)</t>
         </is>
       </c>
       <c r="E118" s="14" t="inlineStr">
@@ -13689,7 +13689,7 @@
       </c>
       <c r="D119" s="13" t="inlineStr">
         <is>
-          <t>maa://29659 (83.33), maa://29031 (89.36)</t>
+          <t>maa://29659 (83.72), maa://29031 (89.36)</t>
         </is>
       </c>
       <c r="E119" s="14" t="inlineStr">
@@ -13959,7 +13959,7 @@
       </c>
       <c r="D124" s="13" t="inlineStr">
         <is>
-          <t>maa://20869 (100.00), maa://44690 (96.23)</t>
+          <t>maa://20869 (100.00), maa://44690 (96.43)</t>
         </is>
       </c>
       <c r="E124" s="14" t="inlineStr">
@@ -14013,7 +14013,7 @@
       </c>
       <c r="D125" s="13" t="inlineStr">
         <is>
-          <t>maa://29650 (98.59), maa://45570 (96.92)</t>
+          <t>maa://29650 (98.59), maa://45570 (95.45)</t>
         </is>
       </c>
       <c r="E125" s="14" t="inlineStr">
@@ -14445,7 +14445,7 @@
       </c>
       <c r="D133" s="13" t="inlineStr">
         <is>
-          <t>maa://21422 (98.95)</t>
+          <t>maa://21422 (98.99)</t>
         </is>
       </c>
       <c r="E133" s="14" t="inlineStr">
@@ -15525,7 +15525,7 @@
       </c>
       <c r="D153" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.88), maa://36641 (98.26), maa://36865 (95.63), maa://44635 (88.18), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (96.77), maa://42918 (100.00), maa://44119 (97.44), maa://64408 (94.74), maa://37300 (100.00), maa://42917 (100.00)</t>
+          <t>maa://40957 (94.75), maa://36641 (98.27), maa://36865 (95.63), maa://44635 (88.18), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (96.88), maa://42918 (100.00), maa://44119 (97.44), maa://64408 (95.24), maa://37300 (100.00), maa://42917 (100.00)</t>
         </is>
       </c>
       <c r="E153" s="14" t="inlineStr">
@@ -15957,7 +15957,7 @@
       </c>
       <c r="D161" s="13" t="inlineStr">
         <is>
-          <t>*maa://39149 (66.67)</t>
+          <t>**maa://39149 (50.00)</t>
         </is>
       </c>
       <c r="E161" s="14" t="inlineStr">
@@ -16443,7 +16443,7 @@
       </c>
       <c r="D170" s="13" t="inlineStr">
         <is>
-          <t>maa://47950 (91.67), maa://20975 (91.67), maa://30806 (100.00)</t>
+          <t>maa://47950 (94.12), maa://20975 (91.67), maa://30806 (100.00)</t>
         </is>
       </c>
       <c r="E170" s="14" t="inlineStr">
@@ -16497,7 +16497,7 @@
       </c>
       <c r="D171" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (92.09), maa://29627 (92.98), maa://29659 (83.33), maa://49074 (94.29), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
+          <t>maa://29633 (92.09), maa://29627 (92.98), maa://29659 (83.72), maa://49074 (94.29), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
         </is>
       </c>
       <c r="E171" s="14" t="inlineStr">
@@ -16551,7 +16551,7 @@
       </c>
       <c r="D172" s="13" t="inlineStr">
         <is>
-          <t>maa://49867 (94.51), maa://49655 (98.00)</t>
+          <t>maa://49867 (94.68), maa://49655 (98.04)</t>
         </is>
       </c>
       <c r="E172" s="14" t="inlineStr">
@@ -16929,7 +16929,7 @@
       </c>
       <c r="D179" s="13" t="inlineStr">
         <is>
-          <t>maa://32418 (99.71), maa://63320 (97.78), maa://51440 (100.00)</t>
+          <t>maa://32418 (99.72), maa://63320 (97.92), maa://51440 (100.00)</t>
         </is>
       </c>
       <c r="E179" s="14" t="inlineStr">
@@ -18112,12 +18112,12 @@
       </c>
       <c r="C201" s="12" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="D201" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.61), maa://35854 (84.75), maa://50388 (98.31), maa://25760 (86.55), ***maa://43911 (11.11), *maa://20872 (52.00), maa://63024 (96.49), maa://51066 (87.50), maa://70161 (100.00), maa://72380 (100.00)</t>
+          <t>maa://44224 (90.52), maa://35854 (84.75), maa://50388 (98.31), maa://25760 (86.55), ***maa://43911 (11.11), maa://63024 (96.55), *maa://20872 (52.00), maa://51066 (87.50), maa://70161 (100.00), *maa://72380 (75.00), maa://74410 (100.00)</t>
         </is>
       </c>
       <c r="E201" s="14" t="inlineStr">
@@ -18225,7 +18225,7 @@
       </c>
       <c r="D203" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (85.71), *maa://28190 (67.50), maa://22894 (91.89), *maa://20906 (72.22), **maa://20907 (34.38)</t>
+          <t>maa://27823 (85.71), *maa://28190 (67.50), maa://22894 (92.11), *maa://20906 (72.22), **maa://20907 (34.38)</t>
         </is>
       </c>
       <c r="E203" s="14" t="inlineStr">
@@ -18279,7 +18279,7 @@
       </c>
       <c r="D204" s="13" t="inlineStr">
         <is>
-          <t>maa://27823 (85.71), *maa://28190 (67.50), maa://22894 (91.89), *maa://20906 (72.22), **maa://20907 (34.38)</t>
+          <t>maa://27823 (85.71), *maa://28190 (67.50), maa://22894 (92.11), *maa://20906 (72.22), **maa://20907 (34.38)</t>
         </is>
       </c>
       <c r="E204" s="14" t="inlineStr">
@@ -18333,7 +18333,7 @@
       </c>
       <c r="D205" s="13" t="inlineStr">
         <is>
-          <t>maa://42223 (99.27), maa://49077 (94.64), maa://42292 (97.30), maa://42402 (100.00)</t>
+          <t>maa://42223 (99.28), maa://49077 (94.64), maa://42292 (97.30), maa://42402 (100.00)</t>
         </is>
       </c>
       <c r="E205" s="14" t="inlineStr">
@@ -18819,7 +18819,7 @@
       </c>
       <c r="D214" s="13" t="inlineStr">
         <is>
-          <t>maa://28133 (92.42), **maa://39217 (36.84), maa://25369 (95.24)</t>
+          <t>maa://28133 (92.42), **maa://39217 (36.84), maa://25369 (95.35)</t>
         </is>
       </c>
       <c r="E214" s="14" t="inlineStr">
@@ -19035,7 +19035,7 @@
       </c>
       <c r="D218" s="13" t="inlineStr">
         <is>
-          <t>maa://64044 (97.10)</t>
+          <t>maa://64044 (97.14)</t>
         </is>
       </c>
       <c r="E218" s="14" t="inlineStr">
@@ -19521,7 +19521,7 @@
       </c>
       <c r="D227" s="13" t="inlineStr">
         <is>
-          <t>maa://39695 (100.00), ***maa://39911 (20.00)</t>
+          <t>maa://39695 (100.00), ***maa://39911 (16.67)</t>
         </is>
       </c>
       <c r="E227" s="14" t="inlineStr">
@@ -20061,7 +20061,7 @@
       </c>
       <c r="D237" s="15" t="inlineStr">
         <is>
-          <t>*maa://48263 (79.41)</t>
+          <t>maa://48263 (80.56)</t>
         </is>
       </c>
       <c r="E237" s="14" t="inlineStr">
@@ -20547,7 +20547,7 @@
       </c>
       <c r="D246" s="13" t="inlineStr">
         <is>
-          <t>*maa://30667 (78.94), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (59.09), maa://39588 (86.67), *maa://64079 (80.00), maa://65726 (90.91), maa://68226 (88.89)</t>
+          <t>*maa://30667 (78.98), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (59.09), maa://39588 (86.67), *maa://64079 (80.00), maa://65726 (84.62), maa://68226 (90.91)</t>
         </is>
       </c>
       <c r="E246" s="14" t="inlineStr">
@@ -21033,7 +21033,7 @@
       </c>
       <c r="D255" s="13" t="inlineStr">
         <is>
-          <t>maa://28923 (91.51), maa://28906 (98.31), ***maa://28825 (11.54), maa://65613 (90.00)</t>
+          <t>maa://28923 (91.55), maa://28906 (98.31), ***maa://28825 (11.54), maa://65613 (90.00)</t>
         </is>
       </c>
       <c r="E255" s="14" t="inlineStr">
@@ -21087,7 +21087,7 @@
       </c>
       <c r="D256" s="13" t="inlineStr">
         <is>
-          <t>maa://42287 (93.57), maa://45570 (96.92), maa://60678 (93.75), maa://42225 (94.44)</t>
+          <t>maa://42287 (93.64), maa://45570 (95.45), maa://60678 (93.75), maa://42225 (94.44)</t>
         </is>
       </c>
       <c r="E256" s="14" t="inlineStr">
@@ -21249,7 +21249,7 @@
       </c>
       <c r="D259" s="13" t="inlineStr">
         <is>
-          <t>maa://31559 (94.12), maa://24093 (100.00), maa://20924 (95.24), **maa://49440 (37.50), maa://63591 (100.00)</t>
+          <t>maa://31559 (94.23), maa://24093 (100.00), maa://20924 (95.24), **maa://49440 (37.50), maa://63591 (100.00)</t>
         </is>
       </c>
       <c r="E259" s="14" t="inlineStr">
@@ -21411,7 +21411,7 @@
       </c>
       <c r="D262" s="13" t="inlineStr">
         <is>
-          <t>maa://20877 (98.78), *maa://45067 (77.78), maa://20836 (100.00), maa://20632 (100.00)</t>
+          <t>maa://20877 (98.80), *maa://45067 (77.78), maa://20836 (100.00), maa://20632 (100.00)</t>
         </is>
       </c>
       <c r="E262" s="14" t="inlineStr">
@@ -21465,7 +21465,7 @@
       </c>
       <c r="D263" s="13" t="inlineStr">
         <is>
-          <t>maa://20879 (85.98), maa://20834 (92.86)</t>
+          <t>maa://20879 (86.11), maa://20834 (92.86)</t>
         </is>
       </c>
       <c r="E263" s="14" t="inlineStr">
@@ -22437,7 +22437,7 @@
       </c>
       <c r="D281" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.69), maa://51630 (96.46), maa://56588 (94.59), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (38.46), *maa://66758 (76.92)</t>
+          <t>maa://51881 (98.70), maa://51630 (96.46), maa://56588 (94.59), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (38.46), *maa://66758 (76.92)</t>
         </is>
       </c>
       <c r="E281" s="14" t="inlineStr">
@@ -23193,7 +23193,7 @@
       </c>
       <c r="D295" s="13" t="inlineStr">
         <is>
-          <t>maa://20899 (90.27), maa://46332 (93.33), ***maa://44744 (25.00)</t>
+          <t>maa://20899 (90.32), maa://46332 (93.33), **maa://44744 (40.00)</t>
         </is>
       </c>
       <c r="E295" s="14" t="inlineStr">
@@ -23895,7 +23895,7 @@
       </c>
       <c r="D308" s="13" t="inlineStr">
         <is>
-          <t>maa://29005 (98.78), maa://31560 (93.75)</t>
+          <t>maa://29005 (98.80), maa://31560 (93.75)</t>
         </is>
       </c>
       <c r="E308" s="14" t="inlineStr">
@@ -24489,7 +24489,7 @@
       </c>
       <c r="D319" s="13" t="inlineStr">
         <is>
-          <t>maa://53348 (88.24)</t>
+          <t>maa://53348 (88.57)</t>
         </is>
       </c>
       <c r="E319" s="14" t="inlineStr">
@@ -24867,7 +24867,7 @@
       </c>
       <c r="D326" s="13" t="inlineStr">
         <is>
-          <t>*maa://62755 (79.17), maa://62761 (88.89)</t>
+          <t>*maa://62755 (80.00), maa://62761 (88.89)</t>
         </is>
       </c>
       <c r="E326" s="14" t="inlineStr">
@@ -26001,7 +26001,7 @@
       </c>
       <c r="D347" s="22" t="inlineStr">
         <is>
-          <t>maa://67275 (100.00), *maa://69909 (55.56)</t>
+          <t>maa://67275 (100.00), *maa://69909 (63.64)</t>
         </is>
       </c>
       <c r="E347" s="22" t="inlineStr">
@@ -26163,7 +26163,7 @@
       </c>
       <c r="D350" s="22" t="inlineStr">
         <is>
-          <t>maa://30671 (81.28), maa://30669 (99.35), maa://37275 (81.40), *maa://32410 (61.54), maa://41605 (100.00)</t>
+          <t>maa://30671 (81.28), maa://30669 (99.36), maa://37275 (81.40), *maa://32410 (61.54), maa://41605 (100.00)</t>
         </is>
       </c>
       <c r="E350" s="22" t="inlineStr">
@@ -26541,7 +26541,7 @@
       </c>
       <c r="D357" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (97.61), maa://32415 (83.93), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
+          <t>maa://32647 (97.61), maa://32415 (83.70), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E357" s="22" t="inlineStr">
@@ -27027,7 +27027,7 @@
       </c>
       <c r="D366" s="22" t="inlineStr">
         <is>
-          <t>maa://36868 (99.39), maa://35996 (98.04), maa://47349 (98.02), **maa://39217 (36.84), maa://71203 (87.50)</t>
+          <t>maa://36868 (99.40), maa://35996 (98.04), maa://47349 (98.04), **maa://39217 (36.84), maa://71203 (90.91)</t>
         </is>
       </c>
       <c r="E366" s="22" t="inlineStr">
@@ -27243,7 +27243,7 @@
       </c>
       <c r="D370" s="22" t="inlineStr">
         <is>
-          <t>maa://49648 (96.47), *maa://49662 (76.47)</t>
+          <t>maa://49648 (96.55), *maa://49662 (76.47)</t>
         </is>
       </c>
       <c r="E370" s="22" t="inlineStr">
@@ -27351,7 +27351,7 @@
       </c>
       <c r="D372" s="22" t="inlineStr">
         <is>
-          <t>maa://36645 (98.46), maa://36841 (92.86), maa://37484 (94.34), maa://37858 (93.55), *maa://56268 (57.14), maa://40489 (100.00)</t>
+          <t>maa://36645 (98.48), maa://36841 (92.86), maa://37484 (94.34), maa://37858 (93.55), *maa://56268 (57.14), maa://40489 (100.00)</t>
         </is>
       </c>
       <c r="E372" s="22" t="inlineStr">
@@ -27405,7 +27405,7 @@
       </c>
       <c r="D373" s="22" t="inlineStr">
         <is>
-          <t>maa://42635 (94.83), maa://50629 (90.91), maa://48859 (100.00)</t>
+          <t>maa://42635 (94.83), maa://50629 (91.67), maa://48859 (100.00)</t>
         </is>
       </c>
       <c r="E373" s="22" t="inlineStr">
@@ -27567,7 +27567,7 @@
       </c>
       <c r="D376" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (94.88), maa://48026 (94.70), maa://44635 (88.18), maa://41035 (93.59), *maa://60251 (73.68), maa://44660 (92.68), maa://41128 (84.21)</t>
+          <t>maa://40957 (94.75), maa://48026 (94.70), maa://44635 (88.18), maa://41035 (93.59), *maa://60251 (73.68), maa://44660 (92.68), maa://41128 (84.21)</t>
         </is>
       </c>
       <c r="E376" s="22" t="inlineStr">
@@ -27729,7 +27729,7 @@
       </c>
       <c r="D379" s="22" t="inlineStr">
         <is>
-          <t>maa://48268 (94.12)</t>
+          <t>maa://48268 (94.44)</t>
         </is>
       </c>
       <c r="E379" s="22" t="inlineStr">
@@ -27837,7 +27837,7 @@
       </c>
       <c r="D381" s="22" t="inlineStr">
         <is>
-          <t>maa://71182 (96.36), maa://70756 (97.67), maa://71524 (100.00), maa://72244 (100.00)</t>
+          <t>maa://71182 (96.61), maa://70756 (97.67), maa://71524 (100.00), maa://72244 (100.00)</t>
         </is>
       </c>
       <c r="E381" s="22" t="inlineStr">
@@ -27891,7 +27891,7 @@
       </c>
       <c r="D382" s="22" t="inlineStr">
         <is>
-          <t>maa://45798 (98.68)</t>
+          <t>maa://45798 (98.70)</t>
         </is>
       </c>
       <c r="E382" s="22" t="inlineStr">
@@ -28269,7 +28269,7 @@
       </c>
       <c r="D389" s="22" t="inlineStr">
         <is>
-          <t>maa://44233 (91.94), maa://45570 (96.92)</t>
+          <t>maa://44233 (91.94), maa://45570 (95.45)</t>
         </is>
       </c>
       <c r="E389" s="22" t="inlineStr">
@@ -28485,7 +28485,7 @@
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>*maa://53307 (67.74)</t>
+          <t>*maa://53307 (68.75)</t>
         </is>
       </c>
       <c r="E393" t="inlineStr">
@@ -28539,7 +28539,7 @@
       </c>
       <c r="D395" t="inlineStr">
         <is>
-          <t>maa://42970 (80.28), maa://44745 (98.26), **maa://49516 (41.94), *maa://45952 (57.14), ***maa://46851 (10.00), *maa://44896 (80.00)</t>
+          <t>maa://42970 (80.35), maa://44745 (98.30), **maa://49516 (45.45), *maa://45952 (57.14), ***maa://46851 (10.00), *maa://44896 (72.73)</t>
         </is>
       </c>
       <c r="E395" t="inlineStr">
@@ -28615,12 +28615,12 @@
       </c>
       <c r="C398" s="17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D398" t="inlineStr">
         <is>
-          <t>maa://48113 (100.00)</t>
+          <t>maa://48113 (100.00), maa://70166 (100.00)</t>
         </is>
       </c>
       <c r="E398" t="inlineStr">
@@ -28701,7 +28701,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>maa://63890 (98.36), maa://64043 (100.00)</t>
+          <t>maa://63890 (98.41), maa://64043 (100.00)</t>
         </is>
       </c>
       <c r="E401" t="inlineStr">
@@ -28755,7 +28755,7 @@
       </c>
       <c r="D403" t="inlineStr">
         <is>
-          <t>maa://47023 (88.52)</t>
+          <t>maa://47023 (88.71)</t>
         </is>
       </c>
       <c r="E403" t="inlineStr">
@@ -28971,7 +28971,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>maa://51872 (96.56), maa://51876 (99.12), maa://63228 (86.11), maa://51873 (98.04), maa://62047 (90.32)</t>
+          <t>maa://51872 (96.58), maa://51876 (99.12), maa://63228 (86.11), maa://51873 (98.04), maa://62047 (90.32)</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
@@ -29025,7 +29025,7 @@
       </c>
       <c r="D413" t="inlineStr">
         <is>
-          <t>maa://60449 (98.58), maa://59493 (96.92)</t>
+          <t>maa://60449 (98.58), maa://59493 (96.95)</t>
         </is>
       </c>
       <c r="E413" t="inlineStr">
@@ -29079,7 +29079,7 @@
       </c>
       <c r="D415" t="inlineStr">
         <is>
-          <t>maa://62756 (96.27)</t>
+          <t>maa://62756 (96.30)</t>
         </is>
       </c>
       <c r="E415" t="inlineStr">
@@ -29133,7 +29133,7 @@
       </c>
       <c r="D417" t="inlineStr">
         <is>
-          <t>maa://52505 (97.88), maa://64040 (99.15), maa://66377 (94.44), ***maa://66376 (14.29), ***maa://70187 (9.09)</t>
+          <t>maa://52505 (97.93), maa://64040 (99.15), maa://66377 (94.44), ***maa://66376 (14.29), ***maa://70187 (9.09)</t>
         </is>
       </c>
       <c r="E417" t="inlineStr">
@@ -29187,7 +29187,7 @@
       </c>
       <c r="D419" t="inlineStr">
         <is>
-          <t>maa://67090 (93.75)</t>
+          <t>maa://67090 (93.85)</t>
         </is>
       </c>
       <c r="E419" t="inlineStr">
@@ -29214,7 +29214,7 @@
       </c>
       <c r="D420" t="inlineStr">
         <is>
-          <t>maa://67388 (89.06), maa://71184 (80.95)</t>
+          <t>maa://67388 (89.06), maa://71184 (84.00)</t>
         </is>
       </c>
       <c r="E420" t="inlineStr">
@@ -29268,7 +29268,7 @@
       </c>
       <c r="D422" t="inlineStr">
         <is>
-          <t>maa://67088 (93.26)</t>
+          <t>maa://67088 (93.33)</t>
         </is>
       </c>
       <c r="E422" t="inlineStr">
@@ -29295,7 +29295,7 @@
       </c>
       <c r="D423" t="inlineStr">
         <is>
-          <t>maa://67087 (97.47), maa://67268 (97.90), maa://67269 (89.29), maa://67648 (100.00)</t>
+          <t>maa://67087 (97.67), maa://67268 (98.05), maa://67269 (89.66), maa://67648 (100.00)</t>
         </is>
       </c>
       <c r="E423" t="inlineStr">
@@ -29376,7 +29376,7 @@
       </c>
       <c r="D426" t="inlineStr">
         <is>
-          <t>maa://70877 (98.59)</t>
+          <t>maa://70877 (98.63)</t>
         </is>
       </c>
       <c r="E426" t="inlineStr">
@@ -29484,7 +29484,7 @@
       </c>
       <c r="D430" t="inlineStr">
         <is>
-          <t>maa://73227 (97.59), maa://73422 (90.91), maa://73447 (100.00)</t>
+          <t>maa://73227 (97.25), maa://73422 (95.24), maa://73447 (100.00)</t>
         </is>
       </c>
       <c r="E430" t="inlineStr">

</xml_diff>

<commit_message>
CI: Auto Update Data (#252)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/悖论&模组作业作者版.xlsx
+++ b/Excel/悖论&模组作业作者版.xlsx
@@ -715,7 +715,7 @@
       </c>
       <c r="D2" s="8" t="inlineStr">
         <is>
-          <t>maa://25390 (98.87), maa://24702 (95.27), maa://36681 (85.71)</t>
+          <t>maa://25390 (98.89), maa://24702 (95.28), maa://36681 (85.71)</t>
         </is>
       </c>
       <c r="E2" s="19" t="n"/>
@@ -747,7 +747,7 @@
       </c>
       <c r="L2" s="8" t="inlineStr">
         <is>
-          <t>maa://58660 (99.05), maa://39402 (96.06), *maa://34787 (75.24), *maa://54304 (70.00)</t>
+          <t>maa://58660 (99.11), maa://39402 (96.26), *maa://34787 (75.24), *maa://54304 (70.00)</t>
         </is>
       </c>
       <c r="M2" s="19" t="n"/>
@@ -779,7 +779,7 @@
       </c>
       <c r="T2" s="8" t="inlineStr">
         <is>
-          <t>maa://22742 (97.95), maa://66635 (99.45)</t>
+          <t>maa://22742 (98.01), maa://66635 (99.49)</t>
         </is>
       </c>
       <c r="U2" s="19" t="n"/>
@@ -811,7 +811,7 @@
       </c>
       <c r="AB2" s="8" t="inlineStr">
         <is>
-          <t>maa://36684 (98.69), maa://21246 (91.19)</t>
+          <t>maa://36684 (98.78), maa://21246 (91.19)</t>
         </is>
       </c>
       <c r="AC2" s="19" t="n"/>
@@ -827,7 +827,7 @@
       </c>
       <c r="AF2" s="8" t="inlineStr">
         <is>
-          <t>maa://59087 (98.04), maa://25251 (91.67)</t>
+          <t>maa://59087 (98.21), maa://25251 (91.67)</t>
         </is>
       </c>
       <c r="AG2" s="16" t="n"/>
@@ -845,7 +845,7 @@
       </c>
       <c r="D3" s="8" t="inlineStr">
         <is>
-          <t>maa://40192 (99.52), maa://36987 (97.40), maa://39849 (94.12)</t>
+          <t>maa://40192 (99.55), maa://36987 (97.40), maa://39849 (94.12)</t>
         </is>
       </c>
       <c r="E3" s="19" t="n"/>
@@ -861,7 +861,7 @@
       </c>
       <c r="H3" s="8" t="inlineStr">
         <is>
-          <t>maa://21247 (99.52)</t>
+          <t>maa://21247 (99.51)</t>
         </is>
       </c>
       <c r="I3" s="19" t="n"/>
@@ -877,7 +877,7 @@
       </c>
       <c r="L3" s="8" t="inlineStr">
         <is>
-          <t>maa://22880 (93.89), maa://20276 (94.69), maa://22749 (86.49)</t>
+          <t>maa://22880 (94.12), maa://20276 (94.79), maa://22749 (86.84)</t>
         </is>
       </c>
       <c r="M3" s="19" t="n"/>
@@ -893,7 +893,7 @@
       </c>
       <c r="P3" s="8" t="inlineStr">
         <is>
-          <t>maa://21249 (98.94), maa://26254 (95.45), maa://22738 (85.71)</t>
+          <t>maa://21249 (98.95), maa://26254 (95.83), maa://22738 (85.71)</t>
         </is>
       </c>
       <c r="Q3" s="19" t="n"/>
@@ -909,7 +909,7 @@
       </c>
       <c r="T3" s="8" t="inlineStr">
         <is>
-          <t>maa://60545 (99.20), maa://45854 (90.36), maa://24617 (91.30)</t>
+          <t>maa://60545 (99.25), maa://45854 (90.75), maa://24617 (91.30)</t>
         </is>
       </c>
       <c r="U3" s="19" t="n"/>
@@ -925,7 +925,7 @@
       </c>
       <c r="X3" s="8" t="inlineStr">
         <is>
-          <t>maa://27396 (95.12), maa://27484 (99.29), maa://27480 (87.69)</t>
+          <t>maa://27396 (95.44), maa://27484 (99.31), maa://27480 (87.88)</t>
         </is>
       </c>
       <c r="Y3" s="19" t="n"/>
@@ -941,7 +941,7 @@
       </c>
       <c r="AB3" s="8" t="inlineStr">
         <is>
-          <t>maa://52241 (99.33), maa://24390 (97.28)</t>
+          <t>maa://52241 (99.37), maa://24390 (97.30)</t>
         </is>
       </c>
       <c r="AC3" s="19" t="n"/>
@@ -957,7 +957,7 @@
       </c>
       <c r="AF3" s="8" t="inlineStr">
         <is>
-          <t>maa://21289 (93.67)</t>
+          <t>maa://21289 (93.79)</t>
         </is>
       </c>
       <c r="AG3" s="16" t="n"/>
@@ -975,7 +975,7 @@
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>maa://24632 (98.77), maa://22499 (90.91), maa://22746 (88.89)</t>
+          <t>maa://24632 (98.84), maa://22499 (90.91), maa://22746 (88.89)</t>
         </is>
       </c>
       <c r="E4" s="19" t="n"/>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="P4" s="8" t="inlineStr">
         <is>
-          <t>maa://49983 (99.42), maa://50121 (97.54)</t>
+          <t>maa://49983 (99.46), maa://50121 (97.66)</t>
         </is>
       </c>
       <c r="Q4" s="19" t="n"/>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="T4" s="8" t="inlineStr">
         <is>
-          <t>maa://27295 (98.42), maa://32509 (96.88), maa://31008 (95.45), maa://70489 (99.40), maa://22754 (88.16)</t>
+          <t>maa://27295 (98.48), maa://32509 (97.01), maa://31008 (95.54), maa://70489 (99.49), maa://22754 (88.16)</t>
         </is>
       </c>
       <c r="U4" s="19" t="n"/>
@@ -1055,7 +1055,7 @@
       </c>
       <c r="X4" s="8" t="inlineStr">
         <is>
-          <t>maa://43217 (99.12)</t>
+          <t>maa://43217 (99.17)</t>
         </is>
       </c>
       <c r="Y4" s="19" t="n"/>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="AB4" s="8" t="inlineStr">
         <is>
-          <t>*maa://32658 (77.19)</t>
+          <t>*maa://32658 (75.86)</t>
         </is>
       </c>
       <c r="AC4" s="19" t="n"/>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="AF4" s="8" t="inlineStr">
         <is>
-          <t>*maa://39394 (53.57), *maa://30062 (62.12), ***maa://26209 (12.00)</t>
+          <t>*maa://39394 (53.57), *maa://30062 (62.69), ***maa://26209 (12.00)</t>
         </is>
       </c>
       <c r="AG4" s="16" t="n"/>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>maa://54105 (98.77), maa://21245 (92.60), *maa://22744 (80.00)</t>
+          <t>maa://54105 (98.84), maa://21245 (92.71), *maa://22744 (80.00)</t>
         </is>
       </c>
       <c r="E5" s="19" t="n"/>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="L5" s="8" t="inlineStr">
         <is>
-          <t>maa://22757 (94.15)</t>
+          <t>maa://22757 (94.12)</t>
         </is>
       </c>
       <c r="M5" s="19" t="n"/>
@@ -1158,7 +1158,7 @@
       </c>
       <c r="P5" s="8" t="inlineStr">
         <is>
-          <t>maa://21919 (99.12), maa://21281 (84.21)</t>
+          <t>maa://21919 (99.15), maa://21281 (84.21)</t>
         </is>
       </c>
       <c r="Q5" s="19" t="n"/>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="X5" s="8" t="inlineStr">
         <is>
-          <t>maa://21290 (99.02)</t>
+          <t>maa://21290 (99.05)</t>
         </is>
       </c>
       <c r="Y5" s="19" t="n"/>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="AB5" s="8" t="inlineStr">
         <is>
-          <t>*maa://29863 (60.00), ***maa://22752 (11.76), **maa://26013 (33.33)</t>
+          <t>*maa://29863 (58.93), ***maa://22752 (11.76), **maa://26013 (33.33)</t>
         </is>
       </c>
       <c r="AC5" s="19" t="n"/>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="D6" s="8" t="inlineStr">
         <is>
-          <t>maa://42407 (98.40)</t>
+          <t>maa://42407 (98.47)</t>
         </is>
       </c>
       <c r="E6" s="19" t="n"/>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="H6" s="8" t="inlineStr">
         <is>
-          <t>maa://24370 (98.41)</t>
+          <t>maa://24370 (98.45)</t>
         </is>
       </c>
       <c r="I6" s="19" t="n"/>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="L6" s="8" t="inlineStr">
         <is>
-          <t>maa://24839 (99.65)</t>
+          <t>maa://24839 (99.60)</t>
         </is>
       </c>
       <c r="M6" s="19" t="n"/>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="P6" s="8" t="inlineStr">
         <is>
-          <t>maa://31836 (99.28), maa://30381 (95.45)</t>
+          <t>maa://31836 (99.31), maa://30381 (95.45)</t>
         </is>
       </c>
       <c r="Q6" s="19" t="n"/>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="X6" s="8" t="inlineStr">
         <is>
-          <t>maa://52754 (96.60), maa://71825 (100.00)</t>
+          <t>maa://52754 (96.63), maa://71825 (98.43)</t>
         </is>
       </c>
       <c r="Y6" s="19" t="n"/>
@@ -1336,7 +1336,7 @@
       </c>
       <c r="AB6" s="8" t="inlineStr">
         <is>
-          <t>maa://22739 (90.43)</t>
+          <t>maa://22739 (90.76)</t>
         </is>
       </c>
       <c r="AC6" s="19" t="n"/>
@@ -1352,7 +1352,7 @@
       </c>
       <c r="AF6" s="8" t="inlineStr">
         <is>
-          <t>maa://33152 (87.04)</t>
+          <t>maa://33152 (87.17)</t>
         </is>
       </c>
       <c r="AG6" s="16" t="n"/>
@@ -1370,7 +1370,7 @@
       </c>
       <c r="D7" s="8" t="inlineStr">
         <is>
-          <t>maa://21955 (98.78)</t>
+          <t>maa://21955 (98.81)</t>
         </is>
       </c>
       <c r="E7" s="19" t="n"/>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
-          <t>*maa://22763 (79.73), maa://64972 (95.74)</t>
+          <t>maa://22763 (81.01), maa://64972 (95.83)</t>
         </is>
       </c>
       <c r="I7" s="19" t="n"/>
@@ -1402,7 +1402,7 @@
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>maa://28624 (99.05), maa://24957 (92.86)</t>
+          <t>maa://28624 (99.10), maa://24957 (92.86)</t>
         </is>
       </c>
       <c r="M7" s="19" t="n"/>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="P7" s="8" t="inlineStr">
         <is>
-          <t>maa://22750 (97.94)</t>
+          <t>maa://22750 (97.99)</t>
         </is>
       </c>
       <c r="Q7" s="19" t="n"/>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="T7" s="8" t="inlineStr">
         <is>
-          <t>maa://21291 (94.37)</t>
+          <t>maa://21291 (94.58)</t>
         </is>
       </c>
       <c r="U7" s="19" t="n"/>
@@ -1450,7 +1450,7 @@
       </c>
       <c r="X7" s="8" t="inlineStr">
         <is>
-          <t>maa://22399 (98.18), maa://22758 (84.92)</t>
+          <t>maa://22399 (98.25), maa://22758 (85.04)</t>
         </is>
       </c>
       <c r="Y7" s="19" t="n"/>
@@ -1482,7 +1482,7 @@
       </c>
       <c r="AF7" s="8" t="inlineStr">
         <is>
-          <t>maa://45272 (99.70), *maa://26191 (70.71)</t>
+          <t>maa://45272 (99.72), *maa://26191 (71.00)</t>
         </is>
       </c>
       <c r="AG7" s="16" t="n"/>
@@ -1490,7 +1490,7 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="18" t="inlineStr">
         <is>
-          <t>更新日期：2025.11.10 13:23:00</t>
+          <t>更新日期：2025.11.13 13:22:25</t>
         </is>
       </c>
       <c r="B8" s="19" t="inlineStr">
@@ -1505,7 +1505,7 @@
       </c>
       <c r="D8" s="8" t="inlineStr">
         <is>
-          <t>maa://21476 (93.50)</t>
+          <t>maa://21476 (93.75)</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
-          <t>maa://24371 (85.02)</t>
+          <t>maa://24371 (85.51)</t>
         </is>
       </c>
       <c r="I8" s="19" t="n"/>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="P8" s="8" t="inlineStr">
         <is>
-          <t>maa://32931 (93.23), maa://23252 (91.67), maa://37496 (98.68)</t>
+          <t>maa://32931 (93.56), maa://23252 (91.67), maa://37496 (98.73)</t>
         </is>
       </c>
       <c r="Q8" s="19" t="n"/>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="X8" s="8" t="inlineStr">
         <is>
-          <t>maa://21411 (96.37), maa://67587 (98.74)</t>
+          <t>maa://21411 (96.41), maa://67587 (98.85)</t>
         </is>
       </c>
       <c r="Y8" s="19" t="n"/>
@@ -1601,7 +1601,7 @@
       </c>
       <c r="AB8" s="8" t="inlineStr">
         <is>
-          <t>maa://25389 (96.51)</t>
+          <t>maa://25389 (96.67)</t>
         </is>
       </c>
       <c r="AC8" s="19" t="n"/>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="D9" s="8" t="inlineStr">
         <is>
-          <t>maa://22765 (97.31), maa://21915 (84.21)</t>
+          <t>maa://22765 (97.52), maa://21915 (85.00)</t>
         </is>
       </c>
       <c r="E9" s="19" t="n"/>
@@ -1651,7 +1651,7 @@
       </c>
       <c r="H9" s="8" t="inlineStr">
         <is>
-          <t>maa://47450 (86.11), maa://56348 (97.06)</t>
+          <t>maa://47450 (86.49), maa://56348 (97.14)</t>
         </is>
       </c>
       <c r="I9" s="19" t="n"/>
@@ -1667,7 +1667,7 @@
       </c>
       <c r="L9" s="8" t="inlineStr">
         <is>
-          <t>maa://22762 (96.80), maa://39552 (89.74)</t>
+          <t>maa://22762 (96.91), maa://39552 (90.24)</t>
         </is>
       </c>
       <c r="M9" s="19" t="n"/>
@@ -1699,7 +1699,7 @@
       </c>
       <c r="T9" s="8" t="inlineStr">
         <is>
-          <t>maa://26222 (99.68)</t>
+          <t>maa://26222 (99.70)</t>
         </is>
       </c>
       <c r="U9" s="19" t="n"/>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="X9" s="8" t="inlineStr">
         <is>
-          <t>maa://52237 (99.76), maa://26223 (98.38)</t>
+          <t>maa://52237 (99.78), maa://26223 (98.38)</t>
         </is>
       </c>
       <c r="Y9" s="19" t="n"/>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="AB9" s="8" t="inlineStr">
         <is>
-          <t>maa://28711 (96.09), maa://40166 (95.57)</t>
+          <t>maa://28711 (96.03), maa://40166 (95.25)</t>
         </is>
       </c>
       <c r="AC9" s="19" t="n"/>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="AF9" s="8" t="inlineStr">
         <is>
-          <t>maa://26206 (92.05), maa://66916 (98.76)</t>
+          <t>maa://26206 (92.13), maa://66916 (98.86)</t>
         </is>
       </c>
       <c r="AG9" s="16" t="n"/>
@@ -1765,7 +1765,7 @@
       </c>
       <c r="D10" s="8" t="inlineStr">
         <is>
-          <t>maa://54000 (93.23), *maa://45271 (70.13)</t>
+          <t>maa://54000 (93.57), *maa://45271 (70.51)</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -1781,7 +1781,7 @@
       </c>
       <c r="H10" s="8" t="inlineStr">
         <is>
-          <t>maa://32651 (94.92)</t>
+          <t>maa://32651 (95.08)</t>
         </is>
       </c>
       <c r="I10" s="19" t="n"/>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="L10" s="8" t="inlineStr">
         <is>
-          <t>**maa://24395 (49.15)</t>
+          <t>**maa://24395 (50.00)</t>
         </is>
       </c>
       <c r="M10" s="19" t="n"/>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="P10" s="8" t="inlineStr">
         <is>
-          <t>maa://28977 (93.35), *maa://36669 (75.00)</t>
+          <t>maa://28977 (93.69), *maa://36669 (75.29)</t>
         </is>
       </c>
       <c r="Q10" s="19" t="n"/>
@@ -1829,7 +1829,7 @@
       </c>
       <c r="T10" s="8" t="inlineStr">
         <is>
-          <t>maa://27395 (99.46), maa://22755 (92.39), maa://63521 (96.39), maa://73485 (96.77)</t>
+          <t>maa://27395 (99.48), maa://22755 (92.61), maa://63521 (96.49), maa://73485 (98.04)</t>
         </is>
       </c>
       <c r="U10" s="19" t="n"/>
@@ -1845,7 +1845,7 @@
       </c>
       <c r="X10" s="8" t="inlineStr">
         <is>
-          <t>maa://45828 (99.53), maa://22301 (97.68), maa://22726 (100.00)</t>
+          <t>maa://45828 (99.57), maa://22301 (97.68), maa://22726 (100.00)</t>
         </is>
       </c>
       <c r="Y10" s="19" t="n"/>
@@ -1895,7 +1895,7 @@
       </c>
       <c r="D11" s="8" t="inlineStr">
         <is>
-          <t>maa://36707 (99.74)</t>
+          <t>maa://36707 (99.75)</t>
         </is>
       </c>
       <c r="E11" s="19" t="n"/>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="L11" s="8" t="inlineStr">
         <is>
-          <t>maa://21287 (95.00)</t>
+          <t>maa://21287 (95.20)</t>
         </is>
       </c>
       <c r="M11" s="19" t="n"/>
@@ -1943,7 +1943,7 @@
       </c>
       <c r="P11" s="8" t="inlineStr">
         <is>
-          <t>maa://45557 (96.05)</t>
+          <t>maa://45557 (96.25)</t>
         </is>
       </c>
       <c r="Q11" s="19" t="n"/>
@@ -1959,7 +1959,7 @@
       </c>
       <c r="T11" s="8" t="inlineStr">
         <is>
-          <t>maa://22747 (95.18), maa://22501 (99.64), maa://64808 (99.62), maa://45521 (94.44)</t>
+          <t>maa://22747 (95.39), maa://22501 (99.65), maa://64808 (99.63), maa://45521 (94.44)</t>
         </is>
       </c>
       <c r="U11" s="19" t="n"/>
@@ -1975,7 +1975,7 @@
       </c>
       <c r="X11" s="8" t="inlineStr">
         <is>
-          <t>maa://36713 (99.50)</t>
+          <t>maa://36713 (99.53)</t>
         </is>
       </c>
       <c r="Y11" s="19" t="n"/>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="AB11" s="8" t="inlineStr">
         <is>
-          <t>maa://29912 (99.69), maa://22516 (85.56)</t>
+          <t>maa://29912 (99.71), maa://22516 (85.56)</t>
         </is>
       </c>
       <c r="AC11" s="19" t="n"/>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="AF11" s="8" t="inlineStr">
         <is>
-          <t>maa://31203 (98.13)</t>
+          <t>maa://31203 (98.25)</t>
         </is>
       </c>
       <c r="AG11" s="16" t="n"/>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="D12" s="8" t="inlineStr">
         <is>
-          <t>maa://36678 (98.18), maa://30766 (91.67)</t>
+          <t>maa://36678 (98.26), maa://30766 (91.89)</t>
         </is>
       </c>
       <c r="E12" s="19" t="n"/>
@@ -2041,7 +2041,7 @@
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>maa://21867 (94.46), maa://54294 (98.26)</t>
+          <t>maa://21867 (94.55), maa://54294 (98.38)</t>
         </is>
       </c>
       <c r="I12" s="19" t="n"/>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="L12" s="8" t="inlineStr">
         <is>
-          <t>maa://63896 (98.57), maa://64046 (98.96)</t>
+          <t>maa://63896 (98.62), maa://64046 (98.99)</t>
         </is>
       </c>
       <c r="M12" s="19" t="n"/>
@@ -2073,7 +2073,7 @@
       </c>
       <c r="P12" s="8" t="inlineStr">
         <is>
-          <t>maa://57541 (92.19)</t>
+          <t>maa://57541 (91.55)</t>
         </is>
       </c>
       <c r="Q12" s="19" t="n"/>
@@ -2105,7 +2105,7 @@
       </c>
       <c r="X12" s="8" t="inlineStr">
         <is>
-          <t>maa://37962 (98.79), maa://21485 (83.96), maa://22753 (93.31), maa://73860 (95.50)</t>
+          <t>maa://37962 (98.80), maa://21485 (84.13), maa://22753 (93.41), maa://73860 (96.43)</t>
         </is>
       </c>
       <c r="Y12" s="19" t="n"/>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="AB12" s="8" t="inlineStr">
         <is>
-          <t>maa://36677 (99.18), maa://23669 (95.03), maa://39872 (98.31)</t>
+          <t>maa://36677 (99.23), maa://23669 (95.06), maa://39872 (98.38)</t>
         </is>
       </c>
       <c r="AC12" s="19" t="n"/>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="AF12" s="8" t="inlineStr">
         <is>
-          <t>maa://28932 (95.93)</t>
+          <t>maa://28932 (95.99)</t>
         </is>
       </c>
       <c r="AG12" s="16" t="n"/>
@@ -2155,7 +2155,7 @@
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
-          <t>maa://24999 (97.69), maa://36673 (95.38), maa://25001 (89.22)</t>
+          <t>maa://24999 (97.79), maa://36673 (95.38), maa://25001 (89.42)</t>
         </is>
       </c>
       <c r="E13" s="19" t="n"/>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
-          <t>*maa://21248 (74.84), maa://66545 (98.73), *maa://22728 (73.04)</t>
+          <t>*maa://21248 (74.95), maa://66545 (98.76), *maa://22728 (74.19)</t>
         </is>
       </c>
       <c r="I13" s="19" t="n"/>
@@ -2203,7 +2203,7 @@
       </c>
       <c r="P13" s="8" t="inlineStr">
         <is>
-          <t>maa://22676 (97.97), maa://22583 (92.96), *maa://22500 (73.61)</t>
+          <t>maa://22676 (98.09), maa://22583 (93.51), *maa://22500 (73.97)</t>
         </is>
       </c>
       <c r="Q13" s="19" t="n"/>
@@ -2219,7 +2219,7 @@
       </c>
       <c r="T13" s="8" t="inlineStr">
         <is>
-          <t>maa://21484 (99.33)</t>
+          <t>maa://21484 (99.34)</t>
         </is>
       </c>
       <c r="U13" s="19" t="n"/>
@@ -2235,7 +2235,7 @@
       </c>
       <c r="X13" s="8" t="inlineStr">
         <is>
-          <t>maa://34957 (95.83)</t>
+          <t>maa://34957 (95.98)</t>
         </is>
       </c>
       <c r="Y13" s="19" t="n"/>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="AF13" s="8" t="inlineStr">
         <is>
-          <t>maa://39883 (95.39)</t>
+          <t>maa://39883 (95.63)</t>
         </is>
       </c>
       <c r="AG13" s="16" t="n"/>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="D14" s="8" t="inlineStr">
         <is>
-          <t>maa://30764 (95.81)</t>
+          <t>maa://30764 (95.98)</t>
         </is>
       </c>
       <c r="E14" s="19" t="n"/>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="L14" s="8" t="inlineStr">
         <is>
-          <t>maa://39841 (99.31), maa://36682 (98.49), maa://26245 (97.16), maa://21288 (96.43)</t>
+          <t>maa://39841 (99.35), maa://36682 (98.53), maa://26245 (97.17), maa://21288 (96.43)</t>
         </is>
       </c>
       <c r="M14" s="19" t="n"/>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="P14" s="8" t="inlineStr">
         <is>
-          <t>maa://23250 (99.72), maa://20107 (87.50), maa://22772 (100.00), maa://68732 (100.00)</t>
+          <t>maa://23250 (99.74), maa://20107 (87.50), maa://22772 (100.00), maa://68732 (100.00)</t>
         </is>
       </c>
       <c r="Q14" s="19" t="n"/>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="T14" s="8" t="inlineStr">
         <is>
-          <t>maa://42751 (99.32), maa://22521 (96.76)</t>
+          <t>maa://42751 (99.35), maa://22521 (96.91)</t>
         </is>
       </c>
       <c r="U14" s="19" t="n"/>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="X14" s="8" t="inlineStr">
         <is>
-          <t>maa://37468 (98.80)</t>
+          <t>maa://37468 (98.87)</t>
         </is>
       </c>
       <c r="Y14" s="19" t="n"/>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="AB14" s="8" t="inlineStr">
         <is>
-          <t>maa://22764 (99.31)</t>
+          <t>maa://22764 (99.34)</t>
         </is>
       </c>
       <c r="AC14" s="19" t="n"/>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="D15" s="8" t="inlineStr">
         <is>
-          <t>maa://22743 (88.58), maa://45058 (98.61), maa://22734 (85.40), *maa://36048 (78.04), maa://69928 (96.91)</t>
+          <t>maa://22743 (88.90), maa://45058 (98.67), maa://22734 (85.40), *maa://36048 (78.54), maa://69928 (97.12)</t>
         </is>
       </c>
       <c r="E15" s="19" t="n"/>
@@ -2431,7 +2431,7 @@
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
-          <t>maa://24304 (98.11), maa://21478 (90.91)</t>
+          <t>maa://24304 (98.20), maa://21478 (90.91)</t>
         </is>
       </c>
       <c r="I15" s="19" t="n"/>
@@ -2447,7 +2447,7 @@
       </c>
       <c r="L15" s="8" t="inlineStr">
         <is>
-          <t>*maa://21334 (72.73), maa://73742 (100.00)</t>
+          <t>*maa://21334 (73.08), maa://73742 (100.00)</t>
         </is>
       </c>
       <c r="M15" s="19" t="n"/>
@@ -2463,7 +2463,7 @@
       </c>
       <c r="P15" s="8" t="inlineStr">
         <is>
-          <t>maa://24762 (98.24), *maa://22727 (70.00)</t>
+          <t>maa://24762 (98.31), *maa://22727 (70.00)</t>
         </is>
       </c>
       <c r="Q15" s="19" t="n"/>
@@ -2479,7 +2479,7 @@
       </c>
       <c r="T15" s="8" t="inlineStr">
         <is>
-          <t>maa://23892 (98.37)</t>
+          <t>maa://23892 (98.41)</t>
         </is>
       </c>
       <c r="U15" s="19" t="n"/>
@@ -2495,7 +2495,7 @@
       </c>
       <c r="X15" s="8" t="inlineStr">
         <is>
-          <t>maa://38786 (94.44), maa://56102 (100.00)</t>
+          <t>maa://38786 (94.83), maa://56102 (100.00)</t>
         </is>
       </c>
       <c r="Y15" s="19" t="n"/>
@@ -2527,7 +2527,7 @@
       </c>
       <c r="AF15" s="8" t="inlineStr">
         <is>
-          <t>maa://36666 (97.02), maa://21364 (84.75), *maa://22766 (71.13), maa://68306 (91.24)</t>
+          <t>maa://36666 (97.11), maa://21364 (84.91), *maa://22766 (71.13), maa://68306 (91.98)</t>
         </is>
       </c>
       <c r="AG15" s="16" t="n"/>
@@ -2545,7 +2545,7 @@
       </c>
       <c r="D16" s="8" t="inlineStr">
         <is>
-          <t>maa://37650 (99.78), maa://21441 (96.68), maa://36679 (94.64)</t>
+          <t>maa://37650 (99.79), maa://21441 (96.68), maa://36679 (94.64)</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2593,7 +2593,7 @@
       </c>
       <c r="P16" s="8" t="inlineStr">
         <is>
-          <t>maa://28504 (97.54)</t>
+          <t>maa://28504 (97.64)</t>
         </is>
       </c>
       <c r="Q16" s="19" t="n"/>
@@ -2609,7 +2609,7 @@
       </c>
       <c r="T16" s="8" t="inlineStr">
         <is>
-          <t>maa://36674 (98.28), maa://22729 (97.33), *maa://28648 (77.89)</t>
+          <t>maa://36674 (98.36), maa://22729 (97.10), *maa://28648 (77.89)</t>
         </is>
       </c>
       <c r="U16" s="19" t="n"/>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="X16" s="8" t="inlineStr">
         <is>
-          <t>maa://28501 (99.47), maa://28051 (97.37)</t>
+          <t>maa://28501 (99.50), maa://28051 (97.50)</t>
         </is>
       </c>
       <c r="Y16" s="19" t="n"/>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="AB16" s="8" t="inlineStr">
         <is>
-          <t>maa://26228 (98.49)</t>
+          <t>maa://26228 (98.55)</t>
         </is>
       </c>
       <c r="AC16" s="19" t="n"/>
@@ -2657,7 +2657,7 @@
       </c>
       <c r="AF16" s="8" t="inlineStr">
         <is>
-          <t>maa://23911 (91.86), maa://67613 (99.18), maa://27755 (93.75)</t>
+          <t>maa://23911 (92.05), maa://67613 (99.28), maa://27755 (93.75)</t>
         </is>
       </c>
       <c r="AG16" s="16" t="n"/>
@@ -2675,7 +2675,7 @@
       </c>
       <c r="D17" s="8" t="inlineStr">
         <is>
-          <t>maa://21624 (88.89), maa://56358 (100.00)</t>
+          <t>maa://21624 (89.29), maa://56358 (100.00)</t>
         </is>
       </c>
       <c r="E17" s="19" t="n"/>
@@ -2691,7 +2691,7 @@
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
-          <t>maa://39599 (98.88), maa://22430 (90.50)</t>
+          <t>maa://39599 (98.94), maa://22430 (90.57)</t>
         </is>
       </c>
       <c r="I17" s="19" t="n"/>
@@ -2707,7 +2707,7 @@
       </c>
       <c r="L17" s="8" t="inlineStr">
         <is>
-          <t>maa://21679 (91.43)</t>
+          <t>maa://21679 (91.89)</t>
         </is>
       </c>
       <c r="M17" s="19" t="n"/>
@@ -2723,7 +2723,7 @@
       </c>
       <c r="P17" s="8" t="inlineStr">
         <is>
-          <t>maa://23890 (84.09), maa://56238 (98.25)</t>
+          <t>maa://23890 (84.09), maa://56238 (98.33)</t>
         </is>
       </c>
       <c r="Q17" s="19" t="n"/>
@@ -2739,7 +2739,7 @@
       </c>
       <c r="T17" s="8" t="inlineStr">
         <is>
-          <t>*maa://42324 (75.45)</t>
+          <t>*maa://42324 (75.00)</t>
         </is>
       </c>
       <c r="U17" s="19" t="n"/>
@@ -2787,7 +2787,7 @@
       </c>
       <c r="AF17" s="8" t="inlineStr">
         <is>
-          <t>maa://50136 (99.34)</t>
+          <t>maa://50136 (99.35)</t>
         </is>
       </c>
       <c r="AG17" s="16" t="n"/>
@@ -2805,7 +2805,7 @@
       </c>
       <c r="D18" s="8" t="inlineStr">
         <is>
-          <t>maa://24570 (98.74)</t>
+          <t>maa://24570 (98.78)</t>
         </is>
       </c>
       <c r="E18" s="19" t="n"/>
@@ -2821,7 +2821,7 @@
       </c>
       <c r="H18" s="8" t="inlineStr">
         <is>
-          <t>maa://24421 (96.51)</t>
+          <t>maa://24421 (96.62)</t>
         </is>
       </c>
       <c r="I18" s="19" t="n"/>
@@ -2837,7 +2837,7 @@
       </c>
       <c r="L18" s="8" t="inlineStr">
         <is>
-          <t>maa://52226 (99.68), maa://22466 (93.01)</t>
+          <t>maa://52226 (99.69), maa://22466 (93.04)</t>
         </is>
       </c>
       <c r="M18" s="19" t="n"/>
@@ -2853,7 +2853,7 @@
       </c>
       <c r="P18" s="8" t="inlineStr">
         <is>
-          <t>maa://54153 (99.81), maa://24379 (100.00), maa://24380 (100.00)</t>
+          <t>maa://54153 (99.83), maa://24379 (100.00), maa://24380 (100.00)</t>
         </is>
       </c>
       <c r="Q18" s="19" t="n"/>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="T18" s="8" t="inlineStr">
         <is>
-          <t>maa://24385 (97.87)</t>
+          <t>maa://24385 (97.89)</t>
         </is>
       </c>
       <c r="U18" s="19" t="n"/>
@@ -2885,7 +2885,7 @@
       </c>
       <c r="X18" s="8" t="inlineStr">
         <is>
-          <t>maa://21917 (99.28), maa://22741 (94.12)</t>
+          <t>maa://21917 (99.31), maa://22741 (94.74)</t>
         </is>
       </c>
       <c r="Y18" s="19" t="n"/>
@@ -2901,7 +2901,7 @@
       </c>
       <c r="AB18" s="8" t="inlineStr">
         <is>
-          <t>maa://24393 (99.36)</t>
+          <t>maa://24393 (99.38)</t>
         </is>
       </c>
       <c r="AC18" s="19" t="n"/>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="AF18" s="8" t="inlineStr">
         <is>
-          <t>maa://47854 (95.49), *maa://68715 (75.00), maa://74015 (90.91)</t>
+          <t>maa://47854 (95.62), *maa://68715 (75.00), maa://74015 (92.86)</t>
         </is>
       </c>
       <c r="AG18" s="16" t="n"/>
@@ -2935,7 +2935,7 @@
       </c>
       <c r="D19" s="8" t="inlineStr">
         <is>
-          <t>maa://62850 (99.48)</t>
+          <t>maa://62850 (99.50)</t>
         </is>
       </c>
       <c r="E19" s="19" t="n"/>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="L19" s="8" t="inlineStr">
         <is>
-          <t>maa://39347 (98.65), maa://56392 (100.00)</t>
+          <t>maa://39347 (98.72), maa://56392 (100.00)</t>
         </is>
       </c>
       <c r="M19" s="19" t="n"/>
@@ -2999,7 +2999,7 @@
       </c>
       <c r="T19" s="8" t="inlineStr">
         <is>
-          <t>maa://24386 (99.68)</t>
+          <t>maa://24386 (99.69)</t>
         </is>
       </c>
       <c r="U19" s="19" t="n"/>
@@ -3015,7 +3015,7 @@
       </c>
       <c r="X19" s="8" t="inlineStr">
         <is>
-          <t>maa://31386 (96.83), maa://58490 (92.11)</t>
+          <t>maa://31386 (96.97), maa://58490 (92.31)</t>
         </is>
       </c>
       <c r="Y19" s="19" t="n"/>
@@ -3031,7 +3031,7 @@
       </c>
       <c r="AB19" s="8" t="inlineStr">
         <is>
-          <t>maa://30709 (90.51), *maa://36668 (72.00)</t>
+          <t>maa://30709 (90.95), *maa://36668 (72.22)</t>
         </is>
       </c>
       <c r="AC19" s="19" t="n"/>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="AF19" s="8" t="inlineStr">
         <is>
-          <t>maa://52239 (91.95)</t>
+          <t>maa://52239 (92.22)</t>
         </is>
       </c>
       <c r="AG19" s="16" t="n"/>
@@ -3065,7 +3065,7 @@
       </c>
       <c r="D20" s="8" t="inlineStr">
         <is>
-          <t>maa://25198 (98.14), maa://36680 (99.09), maa://21432 (91.77)</t>
+          <t>maa://25198 (98.19), maa://36680 (99.11), maa://21432 (91.87)</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -3081,7 +3081,7 @@
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>maa://22864 (96.86), *maa://53361 (71.35)</t>
+          <t>maa://22864 (96.95), *maa://53361 (72.16)</t>
         </is>
       </c>
       <c r="I20" s="19" t="n"/>
@@ -3097,7 +3097,7 @@
       </c>
       <c r="L20" s="8" t="inlineStr">
         <is>
-          <t>maa://41331 (96.47)</t>
+          <t>maa://41331 (96.61)</t>
         </is>
       </c>
       <c r="M20" s="19" t="n"/>
@@ -3113,7 +3113,7 @@
       </c>
       <c r="P20" s="8" t="inlineStr">
         <is>
-          <t>maa://37442 (99.10)</t>
+          <t>maa://37442 (99.16)</t>
         </is>
       </c>
       <c r="Q20" s="19" t="n"/>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="T20" s="8" t="inlineStr">
         <is>
-          <t>maa://29113 (95.65)</t>
+          <t>maa://29113 (95.87)</t>
         </is>
       </c>
       <c r="U20" s="19" t="n"/>
@@ -3145,7 +3145,7 @@
       </c>
       <c r="X20" s="8" t="inlineStr">
         <is>
-          <t>maa://56241 (98.63), maa://50085 (97.35), maa://49976 (88.89)</t>
+          <t>maa://56241 (98.68), maa://50085 (97.43), maa://49976 (88.99)</t>
         </is>
       </c>
       <c r="Y20" s="19" t="n"/>
@@ -3195,7 +3195,7 @@
       </c>
       <c r="D21" s="8" t="inlineStr">
         <is>
-          <t>maa://21261 (99.33)</t>
+          <t>maa://21261 (99.35)</t>
         </is>
       </c>
       <c r="E21" s="19" t="n"/>
@@ -3211,7 +3211,7 @@
       </c>
       <c r="H21" s="8" t="inlineStr">
         <is>
-          <t>maa://24372 (99.31)</t>
+          <t>maa://24372 (99.35)</t>
         </is>
       </c>
       <c r="I21" s="19" t="n"/>
@@ -3227,7 +3227,7 @@
       </c>
       <c r="L21" s="8" t="inlineStr">
         <is>
-          <t>maa://31731 (97.56)</t>
+          <t>maa://31731 (97.60)</t>
         </is>
       </c>
       <c r="M21" s="19" t="n"/>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="X21" s="8" t="inlineStr">
         <is>
-          <t>maa://34946 (98.67), maa://20110 (87.18)</t>
+          <t>maa://34946 (98.55), maa://20110 (87.18)</t>
         </is>
       </c>
       <c r="Y21" s="19" t="n"/>
@@ -3291,7 +3291,7 @@
       </c>
       <c r="AB21" s="8" t="inlineStr">
         <is>
-          <t>maa://21443 (87.90), maa://52223 (90.18)</t>
+          <t>maa://21443 (88.04), maa://52223 (90.72)</t>
         </is>
       </c>
       <c r="AC21" s="19" t="n"/>
@@ -3307,7 +3307,7 @@
       </c>
       <c r="AF21" s="8" t="inlineStr">
         <is>
-          <t>maa://22432 (95.71), maa://64221 (98.26), maa://22524 (82.72)</t>
+          <t>maa://22432 (95.90), maa://64221 (98.29), maa://22524 (82.84)</t>
         </is>
       </c>
       <c r="AG21" s="16" t="n"/>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>maa://25236 (99.33)</t>
+          <t>maa://25236 (99.36)</t>
         </is>
       </c>
       <c r="I22" s="19" t="n"/>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="L22" s="8" t="inlineStr">
         <is>
-          <t>maa://27127 (85.39), maa://66865 (99.71), *maa://22751 (71.26)</t>
+          <t>maa://27127 (85.45), maa://66865 (99.72), *maa://22751 (71.26)</t>
         </is>
       </c>
       <c r="M22" s="19" t="n"/>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="T22" s="8" t="inlineStr">
         <is>
-          <t>maa://38495 (87.72)</t>
+          <t>maa://38495 (86.67)</t>
         </is>
       </c>
       <c r="U22" s="19" t="n"/>
@@ -3405,7 +3405,7 @@
       </c>
       <c r="X22" s="8" t="inlineStr">
         <is>
-          <t>maa://37649 (96.04), maa://21282 (99.10)</t>
+          <t>maa://37649 (95.90), maa://21282 (99.11)</t>
         </is>
       </c>
       <c r="Y22" s="19" t="n"/>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="AB22" s="8" t="inlineStr">
         <is>
-          <t>maa://23656 (99.67)</t>
+          <t>maa://23656 (99.68)</t>
         </is>
       </c>
       <c r="AC22" s="19" t="n"/>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="AF22" s="8" t="inlineStr">
         <is>
-          <t>maa://29658 (97.71)</t>
+          <t>maa://29658 (97.74)</t>
         </is>
       </c>
       <c r="AG22" s="16" t="n"/>
@@ -3455,7 +3455,7 @@
       </c>
       <c r="D23" s="8" t="inlineStr">
         <is>
-          <t>*maa://41753 (73.12), **maa://28036 (31.58)</t>
+          <t>*maa://41753 (74.51), **maa://28036 (31.58)</t>
         </is>
       </c>
       <c r="E23" s="19" t="n"/>
@@ -3487,7 +3487,7 @@
       </c>
       <c r="L23" s="8" t="inlineStr">
         <is>
-          <t>maa://39756 (99.03), maa://39875 (95.52)</t>
+          <t>maa://39756 (99.07), maa://39875 (95.59)</t>
         </is>
       </c>
       <c r="M23" s="19" t="n"/>
@@ -3503,7 +3503,7 @@
       </c>
       <c r="P23" s="8" t="inlineStr">
         <is>
-          <t>maa://30587 (97.76), maa://29748 (83.64), *maa://37566 (79.71)</t>
+          <t>maa://30587 (97.84), maa://29748 (83.87), *maa://37566 (79.71)</t>
         </is>
       </c>
       <c r="Q23" s="19" t="n"/>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="T23" s="8" t="inlineStr">
         <is>
-          <t>maa://31212 (96.45), maa://24387 (86.00), maa://67084 (90.91)</t>
+          <t>maa://31212 (96.59), maa://24387 (86.00), maa://67084 (90.91)</t>
         </is>
       </c>
       <c r="U23" s="19" t="n"/>
@@ -3535,7 +3535,7 @@
       </c>
       <c r="X23" s="8" t="inlineStr">
         <is>
-          <t>*maa://28503 (61.26)</t>
+          <t>*maa://28503 (61.66)</t>
         </is>
       </c>
       <c r="Y23" s="19" t="n"/>
@@ -3551,7 +3551,7 @@
       </c>
       <c r="AB23" s="8" t="inlineStr">
         <is>
-          <t>maa://29652 (97.67)</t>
+          <t>maa://29652 (97.74)</t>
         </is>
       </c>
       <c r="AC23" s="19" t="n"/>
@@ -3567,7 +3567,7 @@
       </c>
       <c r="AF23" s="8" t="inlineStr">
         <is>
-          <t>maa://31489 (98.89)</t>
+          <t>maa://31489 (98.92)</t>
         </is>
       </c>
       <c r="AG23" s="16" t="n"/>
@@ -3585,7 +3585,7 @@
       </c>
       <c r="D24" s="8" t="inlineStr">
         <is>
-          <t>maa://24368 (87.67), maa://46650 (92.97)</t>
+          <t>maa://24368 (87.97), maa://46650 (93.46)</t>
         </is>
       </c>
       <c r="E24" s="19" t="n"/>
@@ -3649,7 +3649,7 @@
       </c>
       <c r="T24" s="8" t="inlineStr">
         <is>
-          <t>maa://73341 (98.12)</t>
+          <t>maa://73341 (98.39)</t>
         </is>
       </c>
       <c r="U24" s="19" t="n"/>
@@ -3665,7 +3665,7 @@
       </c>
       <c r="X24" s="8" t="inlineStr">
         <is>
-          <t>maa://29988 (97.59), maa://23504 (94.16), maa://25141 (81.10), maa://52227 (97.86), maa://36663 (80.53)</t>
+          <t>maa://29988 (97.69), maa://23504 (94.19), maa://25141 (81.33), maa://52227 (97.95), maa://36663 (80.53)</t>
         </is>
       </c>
       <c r="Y24" s="19" t="n"/>
@@ -3681,7 +3681,7 @@
       </c>
       <c r="AB24" s="8" t="inlineStr">
         <is>
-          <t>maa://39349 (98.36)</t>
+          <t>maa://39349 (98.44)</t>
         </is>
       </c>
       <c r="AC24" s="19" t="n"/>
@@ -3697,7 +3697,7 @@
       </c>
       <c r="AF24" s="8" t="inlineStr">
         <is>
-          <t>maa://64165 (99.38), *maa://22523 (79.82), maa://29910 (94.20), maa://45831 (94.59)</t>
+          <t>maa://64165 (99.35), *maa://22523 (79.82), maa://29910 (94.20), maa://45831 (95.00)</t>
         </is>
       </c>
       <c r="AG24" s="16" t="n"/>
@@ -3715,7 +3715,7 @@
       </c>
       <c r="D25" s="8" t="inlineStr">
         <is>
-          <t>maa://29753 (97.13), maa://63016 (99.51)</t>
+          <t>maa://29753 (97.20), maa://63016 (99.53)</t>
         </is>
       </c>
       <c r="E25" s="19" t="n"/>
@@ -3731,7 +3731,7 @@
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
-          <t>maa://29063 (80.95), *maa://25311 (70.78), maa://45047 (87.91)</t>
+          <t>maa://29063 (80.88), *maa://25311 (71.15), maa://45047 (87.10)</t>
         </is>
       </c>
       <c r="I25" s="19" t="n"/>
@@ -3747,7 +3747,7 @@
       </c>
       <c r="L25" s="8" t="inlineStr">
         <is>
-          <t>maa://24378 (94.25), maa://68415 (93.10)</t>
+          <t>maa://24378 (94.38), maa://68415 (92.11)</t>
         </is>
       </c>
       <c r="M25" s="19" t="n"/>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="P25" s="8" t="inlineStr">
         <is>
-          <t>maa://24382 (96.05)</t>
+          <t>maa://24382 (96.15)</t>
         </is>
       </c>
       <c r="Q25" s="19" t="n"/>
@@ -3779,7 +3779,7 @@
       </c>
       <c r="T25" s="8" t="inlineStr">
         <is>
-          <t>maa://20109 (97.61), maa://22545 (99.87)</t>
+          <t>maa://20109 (97.59), maa://22545 (99.87)</t>
         </is>
       </c>
       <c r="U25" s="19" t="n"/>
@@ -3795,7 +3795,7 @@
       </c>
       <c r="X25" s="8" t="inlineStr">
         <is>
-          <t>maa://29890 (93.82)</t>
+          <t>maa://29890 (94.18)</t>
         </is>
       </c>
       <c r="Y25" s="19" t="n"/>
@@ -3811,7 +3811,7 @@
       </c>
       <c r="AB25" s="8" t="inlineStr">
         <is>
-          <t>maa://31215 (93.98), maa://68311 (98.65), *maa://24516 (78.43), maa://26001 (81.97)</t>
+          <t>maa://31215 (94.15), maa://68311 (98.49), *maa://24516 (78.43), maa://26001 (81.97)</t>
         </is>
       </c>
       <c r="AC25" s="19" t="n"/>
@@ -3827,7 +3827,7 @@
       </c>
       <c r="AF25" s="8" t="inlineStr">
         <is>
-          <t>maa://20108 (98.92), maa://36676 (99.87), maa://24621 (96.97), maa://22771 (88.89), maa://37772 (87.50)</t>
+          <t>maa://20108 (98.99), maa://36676 (99.88), maa://24621 (96.99), maa://22771 (88.89), maa://37772 (87.50)</t>
         </is>
       </c>
       <c r="AG25" s="16" t="n"/>
@@ -3845,7 +3845,7 @@
       </c>
       <c r="D26" s="8" t="inlineStr">
         <is>
-          <t>maa://56374 (100.00), maa://41802 (98.21)</t>
+          <t>maa://56374 (100.00), maa://41802 (98.26)</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -3861,7 +3861,7 @@
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
-          <t>maa://56240 (95.81), maa://24913 (92.91)</t>
+          <t>maa://56240 (96.08), maa://24913 (93.02)</t>
         </is>
       </c>
       <c r="I26" s="19" t="n"/>
@@ -3893,7 +3893,7 @@
       </c>
       <c r="P26" s="8" t="inlineStr">
         <is>
-          <t>maa://56625 (99.17), maa://39870 (95.35)</t>
+          <t>maa://56625 (99.21), maa://39870 (95.45)</t>
         </is>
       </c>
       <c r="Q26" s="19" t="n"/>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="X26" s="8" t="inlineStr">
         <is>
-          <t>maa://24389 (98.90)</t>
+          <t>maa://24389 (98.91)</t>
         </is>
       </c>
       <c r="Y26" s="19" t="n"/>
@@ -3941,7 +3941,7 @@
       </c>
       <c r="AB26" s="8" t="inlineStr">
         <is>
-          <t>maa://42235 (98.98)</t>
+          <t>maa://42235 (99.03)</t>
         </is>
       </c>
       <c r="AC26" s="19" t="n"/>
@@ -3957,7 +3957,7 @@
       </c>
       <c r="AF26" s="8" t="inlineStr">
         <is>
-          <t>*maa://30511 (73.68), **maa://29760 (45.45)</t>
+          <t>*maa://30511 (73.96), **maa://29760 (45.45)</t>
         </is>
       </c>
       <c r="AG26" s="16" t="n"/>
@@ -3991,7 +3991,7 @@
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
-          <t>maa://39601 (94.39), maa://34494 (96.26)</t>
+          <t>maa://39601 (94.87), maa://34494 (96.30)</t>
         </is>
       </c>
       <c r="I27" s="19" t="n"/>
@@ -4007,7 +4007,7 @@
       </c>
       <c r="L27" s="8" t="inlineStr">
         <is>
-          <t>maa://28071 (92.59)</t>
+          <t>maa://28071 (93.55)</t>
         </is>
       </c>
       <c r="M27" s="19" t="n"/>
@@ -4039,7 +4039,7 @@
       </c>
       <c r="T27" s="8" t="inlineStr">
         <is>
-          <t>maa://30624 (91.90)</t>
+          <t>maa://30624 (92.25)</t>
         </is>
       </c>
       <c r="U27" s="19" t="n"/>
@@ -4087,7 +4087,7 @@
       </c>
       <c r="AF27" s="8" t="inlineStr">
         <is>
-          <t>maa://24023 (98.48)</t>
+          <t>maa://24023 (98.55)</t>
         </is>
       </c>
       <c r="AG27" s="16" t="n"/>
@@ -4105,7 +4105,7 @@
       </c>
       <c r="D28" s="8" t="inlineStr">
         <is>
-          <t>maa://24465 (96.77), maa://25725 (86.52)</t>
+          <t>maa://24465 (96.85), maa://25725 (87.16)</t>
         </is>
       </c>
       <c r="E28" s="19" t="n"/>
@@ -4137,7 +4137,7 @@
       </c>
       <c r="L28" s="8" t="inlineStr">
         <is>
-          <t>maa://30770 (91.13)</t>
+          <t>maa://30770 (91.54)</t>
         </is>
       </c>
       <c r="M28" s="19" t="n"/>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="T28" s="8" t="inlineStr">
         <is>
-          <t>maa://29765 (95.45), maa://23263 (97.27)</t>
+          <t>maa://29765 (95.62), maa://23263 (97.38)</t>
         </is>
       </c>
       <c r="U28" s="19" t="n"/>
@@ -4185,7 +4185,7 @@
       </c>
       <c r="X28" s="8" t="inlineStr">
         <is>
-          <t>maa://39929 (98.09), maa://41749 (97.47)</t>
+          <t>maa://39929 (98.13), maa://41749 (97.51)</t>
         </is>
       </c>
       <c r="Y28" s="19" t="n"/>
@@ -4217,7 +4217,7 @@
       </c>
       <c r="AF28" s="8" t="inlineStr">
         <is>
-          <t>maa://36660 (95.12), maa://65700 (98.80)</t>
+          <t>maa://36660 (95.23), maa://65700 (98.87)</t>
         </is>
       </c>
       <c r="AG28" s="16" t="n"/>
@@ -4235,7 +4235,7 @@
       </c>
       <c r="D29" s="8" t="inlineStr">
         <is>
-          <t>maa://31694 (99.50)</t>
+          <t>maa://31694 (99.52)</t>
         </is>
       </c>
       <c r="E29" s="19" t="n"/>
@@ -4251,7 +4251,7 @@
       </c>
       <c r="H29" s="8" t="inlineStr">
         <is>
-          <t>maa://73558 (92.31)</t>
+          <t>maa://73558 (94.44)</t>
         </is>
       </c>
       <c r="I29" s="19" t="n"/>
@@ -4267,7 +4267,7 @@
       </c>
       <c r="L29" s="8" t="inlineStr">
         <is>
-          <t>maa://28432 (98.46), maa://31400 (98.33), maa://28440 (87.21)</t>
+          <t>maa://28432 (98.53), maa://31400 (98.37), maa://28440 (87.36)</t>
         </is>
       </c>
       <c r="M29" s="19" t="n"/>
@@ -4283,7 +4283,7 @@
       </c>
       <c r="P29" s="8" t="inlineStr">
         <is>
-          <t>maa://54169 (97.52)</t>
+          <t>maa://54169 (97.13)</t>
         </is>
       </c>
       <c r="Q29" s="19" t="n"/>
@@ -4347,7 +4347,7 @@
       </c>
       <c r="AF29" s="8" t="inlineStr">
         <is>
-          <t>maa://42865 (94.47)</t>
+          <t>maa://42865 (94.62)</t>
         </is>
       </c>
       <c r="AG29" s="16" t="n"/>
@@ -4365,7 +4365,7 @@
       </c>
       <c r="D30" s="8" t="inlineStr">
         <is>
-          <t>maa://45792 (96.51), maa://64191 (96.15)</t>
+          <t>maa://45792 (96.55), maa://64191 (96.47)</t>
         </is>
       </c>
       <c r="E30" s="19" t="n"/>
@@ -4397,7 +4397,7 @@
       </c>
       <c r="L30" s="8" t="inlineStr">
         <is>
-          <t>maa://30442 (98.24)</t>
+          <t>maa://30442 (98.27)</t>
         </is>
       </c>
       <c r="M30" s="19" t="n"/>
@@ -4413,7 +4413,7 @@
       </c>
       <c r="P30" s="8" t="inlineStr">
         <is>
-          <t>maa://21442 (99.47), maa://68394 (100.00), maa://66611 (100.00)</t>
+          <t>maa://21442 (99.48), maa://68394 (100.00), maa://66611 (100.00)</t>
         </is>
       </c>
       <c r="Q30" s="19" t="n"/>
@@ -4445,7 +4445,7 @@
       </c>
       <c r="X30" s="8" t="inlineStr">
         <is>
-          <t>maa://39477 (96.30)</t>
+          <t>maa://39477 (96.34)</t>
         </is>
       </c>
       <c r="Y30" s="19" t="n"/>
@@ -4461,7 +4461,7 @@
       </c>
       <c r="AB30" s="8" t="inlineStr">
         <is>
-          <t>maa://42979 (99.64), maa://45822 (100.00), maa://45045 (94.74)</t>
+          <t>maa://42979 (99.65), maa://45822 (100.00), maa://45045 (94.74)</t>
         </is>
       </c>
       <c r="AC30" s="19" t="n"/>
@@ -4527,7 +4527,7 @@
       </c>
       <c r="L31" s="8" t="inlineStr">
         <is>
-          <t>maa://35926 (98.68), maa://36258 (94.18), maa://43904 (92.42)</t>
+          <t>maa://35926 (98.73), maa://36258 (94.32), maa://43904 (92.96)</t>
         </is>
       </c>
       <c r="M31" s="19" t="n"/>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="T31" s="8" t="inlineStr">
         <is>
-          <t>maa://30711 (97.52), maa://30768 (100.00)</t>
+          <t>maa://30711 (97.58), maa://30768 (100.00)</t>
         </is>
       </c>
       <c r="U31" s="19" t="n"/>
@@ -4591,7 +4591,7 @@
       </c>
       <c r="AB31" s="8" t="inlineStr">
         <is>
-          <t>maa://66997 (97.44)</t>
+          <t>maa://66997 (97.56)</t>
         </is>
       </c>
       <c r="AC31" s="19" t="n"/>
@@ -4641,7 +4641,7 @@
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>maa://36667 (99.72), maa://21895 (98.08), maa://22760 (100.00)</t>
+          <t>maa://36667 (99.69), maa://21895 (98.10), maa://22760 (100.00)</t>
         </is>
       </c>
       <c r="I32" s="19" t="n"/>
@@ -4657,7 +4657,7 @@
       </c>
       <c r="L32" s="8" t="inlineStr">
         <is>
-          <t>maa://28065 (97.74)</t>
+          <t>maa://28065 (97.83)</t>
         </is>
       </c>
       <c r="M32" s="19" t="n"/>
@@ -4689,7 +4689,7 @@
       </c>
       <c r="T32" s="8" t="inlineStr">
         <is>
-          <t>maa://42859 (99.48), maa://41108 (89.06), maa://41238 (98.30), maa://45523 (100.00)</t>
+          <t>maa://42859 (99.50), maa://41108 (89.23), maa://41238 (98.31), maa://45523 (100.00)</t>
         </is>
       </c>
       <c r="U32" s="19" t="n"/>
@@ -4705,7 +4705,7 @@
       </c>
       <c r="X32" s="8" t="inlineStr">
         <is>
-          <t>maa://64104 (97.46)</t>
+          <t>maa://64104 (97.54)</t>
         </is>
       </c>
       <c r="Y32" s="19" t="n"/>
@@ -4737,7 +4737,7 @@
       </c>
       <c r="AF32" s="8" t="inlineStr">
         <is>
-          <t>maa://42408 (96.15)</t>
+          <t>maa://42408 (96.36)</t>
         </is>
       </c>
       <c r="AG32" s="16" t="n"/>
@@ -4803,7 +4803,7 @@
       </c>
       <c r="P33" s="8" t="inlineStr">
         <is>
-          <t>maa://21956 (95.51), maa://69135 (98.99), maa://73357 (100.00)</t>
+          <t>maa://21956 (95.77), maa://69135 (99.04), maa://73357 (100.00)</t>
         </is>
       </c>
       <c r="Q33" s="19" t="n"/>
@@ -4819,7 +4819,7 @@
       </c>
       <c r="T33" s="8" t="inlineStr">
         <is>
-          <t>maa://45558 (91.84)</t>
+          <t>maa://45558 (92.31)</t>
         </is>
       </c>
       <c r="U33" s="19" t="n"/>
@@ -4851,7 +4851,7 @@
       </c>
       <c r="AB33" s="8" t="inlineStr">
         <is>
-          <t>maa://73340 (99.69), maa://73523 (97.44)</t>
+          <t>maa://73340 (99.74), maa://73523 (97.96)</t>
         </is>
       </c>
       <c r="AC33" s="19" t="n"/>
@@ -4901,7 +4901,7 @@
       </c>
       <c r="H34" s="8" t="inlineStr">
         <is>
-          <t>maa://66817 (99.29)</t>
+          <t>maa://66817 (99.31)</t>
         </is>
       </c>
       <c r="I34" s="19" t="n"/>
@@ -4933,7 +4933,7 @@
       </c>
       <c r="P34" s="8" t="inlineStr">
         <is>
-          <t>maa://56235 (99.47), maa://48817 (99.46)</t>
+          <t>maa://56235 (99.49), maa://48817 (99.48)</t>
         </is>
       </c>
       <c r="Q34" s="19" t="n"/>
@@ -4949,7 +4949,7 @@
       </c>
       <c r="T34" s="8" t="inlineStr">
         <is>
-          <t>maa://24526 (97.92)</t>
+          <t>maa://24526 (97.99)</t>
         </is>
       </c>
       <c r="U34" s="19" t="n"/>
@@ -4981,7 +4981,7 @@
       </c>
       <c r="AB34" s="8" t="inlineStr">
         <is>
-          <t>maa://64329 (99.02)</t>
+          <t>maa://64329 (99.06)</t>
         </is>
       </c>
       <c r="AC34" s="19" t="n"/>
@@ -4997,7 +4997,7 @@
       </c>
       <c r="AF34" s="8" t="inlineStr">
         <is>
-          <t>maa://32650 (90.54)</t>
+          <t>maa://32650 (90.67)</t>
         </is>
       </c>
       <c r="AG34" s="16" t="n"/>
@@ -5047,7 +5047,7 @@
       </c>
       <c r="L35" s="8" t="inlineStr">
         <is>
-          <t>maa://41296 (99.50)</t>
+          <t>maa://41296 (99.52)</t>
         </is>
       </c>
       <c r="M35" s="19" t="n"/>
@@ -5079,7 +5079,7 @@
       </c>
       <c r="T35" s="8" t="inlineStr">
         <is>
-          <t>maa://24842 (97.50)</t>
+          <t>maa://24842 (97.54)</t>
         </is>
       </c>
       <c r="U35" s="19" t="n"/>
@@ -5127,7 +5127,7 @@
       </c>
       <c r="AF35" s="8" t="inlineStr">
         <is>
-          <t>maa://39479 (94.74)</t>
+          <t>maa://39479 (93.67)</t>
         </is>
       </c>
       <c r="AG35" s="16" t="n"/>
@@ -5161,7 +5161,7 @@
       </c>
       <c r="H36" s="8" t="inlineStr">
         <is>
-          <t>maa://24375 (96.04)</t>
+          <t>maa://24375 (96.08)</t>
         </is>
       </c>
       <c r="I36" s="19" t="n"/>
@@ -5177,7 +5177,7 @@
       </c>
       <c r="L36" s="8" t="inlineStr">
         <is>
-          <t>maa://42240 (99.22)</t>
+          <t>maa://42240 (99.24)</t>
         </is>
       </c>
       <c r="M36" s="19" t="n"/>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="AB36" s="19" t="inlineStr">
         <is>
-          <t>maa://64106 (97.10)</t>
+          <t>maa://64106 (97.14)</t>
         </is>
       </c>
       <c r="AC36" s="19" t="n"/>
@@ -5307,7 +5307,7 @@
       </c>
       <c r="L37" s="8" t="inlineStr">
         <is>
-          <t>maa://45718 (99.06), maa://56336 (99.49), maa://47069 (89.66), maa://45789 (100.00)</t>
+          <t>maa://45718 (99.08), maa://56336 (99.51), maa://47069 (90.00), maa://45789 (100.00)</t>
         </is>
       </c>
       <c r="M37" s="19" t="n"/>
@@ -5323,7 +5323,7 @@
       </c>
       <c r="P37" s="8" t="inlineStr">
         <is>
-          <t>maa://21280 (98.19), *maa://21239 (70.59)</t>
+          <t>maa://21280 (98.26), *maa://21239 (72.22)</t>
         </is>
       </c>
       <c r="Q37" s="19" t="n"/>
@@ -5339,7 +5339,7 @@
       </c>
       <c r="T37" s="8" t="inlineStr">
         <is>
-          <t>*maa://39354 (61.29)</t>
+          <t>*maa://39354 (62.50)</t>
         </is>
       </c>
       <c r="U37" s="19" t="n"/>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="L38" s="8" t="inlineStr">
         <is>
-          <t>maa://39384 (99.55), maa://49735 (90.00)</t>
+          <t>maa://39384 (99.14), maa://49735 (90.00)</t>
         </is>
       </c>
       <c r="M38" s="19" t="n"/>
@@ -5437,7 +5437,7 @@
       </c>
       <c r="P38" s="8" t="inlineStr">
         <is>
-          <t>maa://24383 (86.18)</t>
+          <t>maa://24383 (86.67)</t>
         </is>
       </c>
       <c r="Q38" s="19" t="n"/>
@@ -5453,7 +5453,7 @@
       </c>
       <c r="T38" s="8" t="inlineStr">
         <is>
-          <t>maa://30713 (98.82)</t>
+          <t>maa://30713 (98.84)</t>
         </is>
       </c>
       <c r="U38" s="19" t="n"/>
@@ -5485,7 +5485,7 @@
       </c>
       <c r="AF38" s="8" t="inlineStr">
         <is>
-          <t>maa://36697 (96.07), maa://68397 (99.10)</t>
+          <t>maa://36697 (96.12), maa://68397 (99.16)</t>
         </is>
       </c>
       <c r="AG38" s="16" t="n"/>
@@ -5519,7 +5519,7 @@
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>maa://45059 (95.67), maa://25199 (85.53), maa://30434 (95.71), maa://44165 (85.71)</t>
+          <t>maa://45059 (95.81), maa://25199 (85.71), maa://30434 (95.75), maa://44165 (85.71)</t>
         </is>
       </c>
       <c r="I39" s="19" t="n"/>
@@ -5551,7 +5551,7 @@
       </c>
       <c r="P39" s="8" t="inlineStr">
         <is>
-          <t>maa://47093 (98.99), maa://24709 (94.93)</t>
+          <t>maa://47093 (98.90), maa://24709 (94.70)</t>
         </is>
       </c>
       <c r="Q39" s="19" t="n"/>
@@ -5567,7 +5567,7 @@
       </c>
       <c r="T39" s="8" t="inlineStr">
         <is>
-          <t>maa://47079 (96.67), maa://45790 (89.69), *maa://56232 (73.98)</t>
+          <t>maa://47079 (96.68), maa://45790 (89.32), *maa://56232 (75.00)</t>
         </is>
       </c>
       <c r="U39" s="19" t="n"/>
@@ -5599,7 +5599,7 @@
       </c>
       <c r="AF39" s="8" t="inlineStr">
         <is>
-          <t>maa://62953 (97.47)</t>
+          <t>maa://62953 (97.44)</t>
         </is>
       </c>
       <c r="AG39" s="16" t="n"/>
@@ -5665,7 +5665,7 @@
       </c>
       <c r="P40" s="8" t="inlineStr">
         <is>
-          <t>maa://23278 (98.41), maa://21386 (96.19), maa://36664 (89.41), *maa://45550 (76.92)</t>
+          <t>maa://23278 (98.44), maa://21386 (95.73), maa://36664 (88.37), *maa://45550 (71.43)</t>
         </is>
       </c>
       <c r="Q40" s="19" t="n"/>
@@ -5713,7 +5713,7 @@
       </c>
       <c r="AF40" s="19" t="inlineStr">
         <is>
-          <t>maa://65283 (97.71), *maa://64107 (72.92), maa://64205 (95.24)</t>
+          <t>maa://65283 (97.81), *maa://64107 (74.00), maa://64205 (95.24)</t>
         </is>
       </c>
       <c r="AG40" s="16" t="n"/>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="H41" s="8" t="inlineStr">
         <is>
-          <t>maa://24466 (94.38)</t>
+          <t>maa://24466 (94.44)</t>
         </is>
       </c>
       <c r="I41" s="19" t="n"/>
@@ -5766,7 +5766,7 @@
       </c>
       <c r="P41" s="8" t="inlineStr">
         <is>
-          <t>maa://43177 (97.13)</t>
+          <t>maa://43177 (97.27)</t>
         </is>
       </c>
       <c r="Q41" s="19" t="n"/>
@@ -5936,7 +5936,7 @@
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
-          <t>maa://21284 (98.58)</t>
+          <t>maa://21284 (98.65)</t>
         </is>
       </c>
       <c r="I43" s="19" t="n"/>
@@ -5984,7 +5984,7 @@
       </c>
       <c r="T43" s="8" t="inlineStr">
         <is>
-          <t>maa://43198 (100.00), maa://46286 (94.74)</t>
+          <t>maa://43198 (100.00), maa://46286 (95.00)</t>
         </is>
       </c>
       <c r="U43" s="19" t="n"/>
@@ -6037,7 +6037,7 @@
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
-          <t>maa://29768 (98.54), maa://56386 (99.68), maa://27728 (96.46)</t>
+          <t>maa://29768 (98.57), maa://56386 (99.70), maa://27728 (96.49)</t>
         </is>
       </c>
       <c r="I44" s="19" t="n"/>
@@ -6085,7 +6085,7 @@
       </c>
       <c r="T44" s="8" t="inlineStr">
         <is>
-          <t>maa://39366 (94.70)</t>
+          <t>maa://39366 (94.74)</t>
         </is>
       </c>
       <c r="U44" s="19" t="n"/>
@@ -6138,7 +6138,7 @@
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
-          <t>maa://42459 (99.00), maa://21229 (87.26), maa://30807 (94.68), maa://22767 (82.22)</t>
+          <t>maa://42459 (99.06), maa://21229 (87.55), maa://30807 (94.68), maa://22767 (83.10)</t>
         </is>
       </c>
       <c r="I45" s="19" t="n"/>
@@ -6170,7 +6170,7 @@
       </c>
       <c r="P45" s="8" t="inlineStr">
         <is>
-          <t>maa://36237 (88.46)</t>
+          <t>maa://36237 (89.09)</t>
         </is>
       </c>
       <c r="Q45" s="19" t="n"/>
@@ -6186,7 +6186,7 @@
       </c>
       <c r="T45" s="8" t="inlineStr">
         <is>
-          <t>*maa://39364 (75.00), maa://73997 (100.00)</t>
+          <t>*maa://39364 (75.21), maa://73997 (100.00)</t>
         </is>
       </c>
       <c r="U45" s="19" t="n"/>
@@ -6223,7 +6223,7 @@
       </c>
       <c r="H46" s="8" t="inlineStr">
         <is>
-          <t>maa://35931 (96.92), maa://43901 (97.81)</t>
+          <t>maa://35931 (97.01), maa://43901 (97.91)</t>
         </is>
       </c>
       <c r="I46" s="19" t="n"/>
@@ -6292,7 +6292,7 @@
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>maa://27410 (97.74), maa://56236 (99.88), maa://29661 (97.47), maa://28038 (84.62)</t>
+          <t>maa://27410 (97.76), maa://56236 (99.89), maa://29661 (97.47), maa://28038 (84.62)</t>
         </is>
       </c>
       <c r="I47" s="19" t="n"/>
@@ -6324,7 +6324,7 @@
       </c>
       <c r="T47" s="8" t="inlineStr">
         <is>
-          <t>maa://68392 (99.78), maa://67476 (99.60)</t>
+          <t>maa://68392 (99.79), maa://67476 (99.61)</t>
         </is>
       </c>
       <c r="U47" s="19" t="n"/>
@@ -6446,7 +6446,7 @@
       </c>
       <c r="P49" s="8" t="inlineStr">
         <is>
-          <t>maa://39643 (84.34)</t>
+          <t>maa://39643 (84.58)</t>
         </is>
       </c>
       <c r="Q49" s="19" t="n"/>
@@ -6462,7 +6462,7 @@
       </c>
       <c r="T49" s="19" t="inlineStr">
         <is>
-          <t>maa://67231 (99.44)</t>
+          <t>maa://67231 (99.43)</t>
         </is>
       </c>
       <c r="U49" s="19" t="n"/>
@@ -6499,7 +6499,7 @@
       </c>
       <c r="P50" s="8" t="inlineStr">
         <is>
-          <t>maa://62852 (94.75), maa://73565 (97.75)</t>
+          <t>maa://62852 (94.72), maa://73565 (97.66)</t>
         </is>
       </c>
       <c r="Q50" s="19" t="n"/>
@@ -6583,7 +6583,7 @@
       </c>
       <c r="H52" s="8" t="inlineStr">
         <is>
-          <t>maa://24376 (99.44)</t>
+          <t>maa://24376 (99.46)</t>
         </is>
       </c>
       <c r="I52" s="19" t="n"/>
@@ -6599,7 +6599,7 @@
       </c>
       <c r="P52" s="8" t="inlineStr">
         <is>
-          <t>maa://59394 (99.56), maa://65511 (100.00), maa://59378 (94.05)</t>
+          <t>maa://59394 (99.54), maa://65511 (100.00), maa://59378 (94.05)</t>
         </is>
       </c>
       <c r="Q52" s="19" t="n"/>
@@ -6633,7 +6633,7 @@
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
-          <t>maa://32534 (98.57)</t>
+          <t>maa://32534 (98.63)</t>
         </is>
       </c>
       <c r="I53" s="19" t="n"/>
@@ -6733,7 +6733,7 @@
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
-          <t>maa://32532 (98.49)</t>
+          <t>maa://32532 (98.54)</t>
         </is>
       </c>
       <c r="I55" s="19" t="n"/>
@@ -6749,7 +6749,7 @@
       </c>
       <c r="P55" s="16" t="inlineStr">
         <is>
-          <t>maa://73349 (97.87)</t>
+          <t>maa://73349 (98.15)</t>
         </is>
       </c>
       <c r="Q55" s="16" t="n"/>
@@ -6833,7 +6833,7 @@
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>maa://56237 (98.61), maa://25176 (97.73), maa://73737 (100.00)</t>
+          <t>maa://56237 (98.62), maa://25176 (97.73), maa://73737 (100.00)</t>
         </is>
       </c>
       <c r="I57" s="19" t="n"/>
@@ -6851,7 +6851,7 @@
       </c>
       <c r="H58" s="8" t="inlineStr">
         <is>
-          <t>*maa://37964 (72.51)</t>
+          <t>*maa://37964 (73.60)</t>
         </is>
       </c>
       <c r="I58" s="19" t="n"/>
@@ -6869,7 +6869,7 @@
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
-          <t>maa://31270 (98.91), maa://27746 (90.20)</t>
+          <t>maa://31270 (98.94), maa://27746 (90.24)</t>
         </is>
       </c>
       <c r="I59" s="19" t="n"/>
@@ -6887,7 +6887,7 @@
       </c>
       <c r="H60" s="8" t="inlineStr">
         <is>
-          <t>maa://40438 (94.66), *maa://73999 (77.78)</t>
+          <t>maa://40438 (94.79), maa://73999 (84.62)</t>
         </is>
       </c>
       <c r="I60" s="19" t="n"/>
@@ -6923,7 +6923,7 @@
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
-          <t>maa://42981 (96.36), maa://56228 (98.93), maa://43903 (100.00)</t>
+          <t>maa://42981 (96.36), maa://56228 (98.98), maa://43903 (100.00)</t>
         </is>
       </c>
       <c r="I62" s="19" t="n"/>
@@ -6941,7 +6941,7 @@
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>maa://59534 (99.64), *maa://59693 (71.19), maa://59413 (98.40)</t>
+          <t>maa://59534 (99.66), *maa://59693 (72.58), maa://59413 (98.44)</t>
         </is>
       </c>
       <c r="I63" s="19" t="n"/>
@@ -6977,7 +6977,7 @@
       </c>
       <c r="H65" s="8" t="inlineStr">
         <is>
-          <t>maa://73343 (99.08)</t>
+          <t>maa://73343 (99.22)</t>
         </is>
       </c>
       <c r="I65" s="19" t="n"/>
@@ -7157,7 +7157,7 @@
       </c>
       <c r="H75" s="19" t="inlineStr">
         <is>
-          <t>maa://67748 (90.38)</t>
+          <t>maa://67748 (90.83)</t>
         </is>
       </c>
       <c r="I75" s="19" t="n"/>
@@ -7317,7 +7317,7 @@
     <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22">
       <c r="A1" s="21" t="inlineStr">
         <is>
-          <t>更新日期：2025.11.10 13:23:00</t>
+          <t>更新日期：2025.11.13 13:22:25</t>
         </is>
       </c>
       <c r="E1" s="9" t="inlineStr">
@@ -8721,7 +8721,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>*maa://20849 (74.14), *maa://28758 (72.34), maa://65357 (97.78), maa://29036 (96.77), *maa://42172 (71.43), maa://30285 (100.00)</t>
+          <t>*maa://20849 (74.14), *maa://28758 (72.34), maa://65357 (97.87), maa://29036 (96.88), *maa://42172 (71.43), maa://30285 (100.00)</t>
         </is>
       </c>
       <c r="E27" s="14" t="inlineStr">
@@ -8829,7 +8829,7 @@
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>maa://20863 (90.85), maa://20832 (98.52), maa://20727 (100.00)</t>
+          <t>maa://20863 (90.88), maa://20832 (98.53), maa://20727 (100.00)</t>
         </is>
       </c>
       <c r="E29" s="14" t="inlineStr">
@@ -8991,7 +8991,7 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>maa://36644 (90.78), maa://36866 (97.26), maa://62759 (100.00), maa://45572 (88.89), maa://27794 (100.00), maa://70680 (100.00), maa://20960 (100.00), maa://20843 (100.00), *maa://20893 (75.00), **maa://24483 (50.00), maa://20862 (85.71), maa://74314 (100.00)</t>
+          <t>maa://36644 (90.82), maa://36866 (97.26), maa://62759 (100.00), maa://45572 (88.89), maa://27794 (100.00), maa://70680 (100.00), maa://20960 (100.00), maa://20843 (100.00), *maa://20893 (75.00), **maa://24483 (50.00), maa://20862 (85.71), maa://74314 (100.00)</t>
         </is>
       </c>
       <c r="E32" s="14" t="inlineStr">
@@ -10125,7 +10125,7 @@
       </c>
       <c r="D53" s="13" t="inlineStr">
         <is>
-          <t>maa://20953 (97.22), maa://31173 (95.00)</t>
+          <t>maa://20953 (97.37), maa://31173 (95.12)</t>
         </is>
       </c>
       <c r="E53" s="14" t="inlineStr">
@@ -10233,7 +10233,7 @@
       </c>
       <c r="D55" s="13" t="inlineStr">
         <is>
-          <t>maa://20932 (96.15), maa://42415 (96.55), maa://40838 (100.00), maa://68386 (100.00)</t>
+          <t>maa://20932 (96.17), maa://42415 (96.55), maa://40838 (100.00), maa://68386 (100.00)</t>
         </is>
       </c>
       <c r="E55" s="14" t="inlineStr">
@@ -10287,7 +10287,7 @@
       </c>
       <c r="D56" s="13" t="inlineStr">
         <is>
-          <t>maa://44235 (98.48), maa://45604 (100.00), maa://20961 (94.44), maa://20910 (100.00), maa://44220 (100.00)</t>
+          <t>maa://44235 (98.50), maa://45604 (100.00), maa://20961 (94.44), maa://20910 (100.00), maa://44220 (100.00)</t>
         </is>
       </c>
       <c r="E56" s="14" t="inlineStr">
@@ -10557,7 +10557,7 @@
       </c>
       <c r="D61" s="13" t="inlineStr">
         <is>
-          <t>maa://20841 (99.32), maa://31559 (94.23), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00), maa://66633 (100.00)</t>
+          <t>maa://20841 (99.32), maa://31559 (94.34), maa://24093 (100.00), maa://20924 (95.24), maa://25777 (100.00), maa://20631 (100.00), maa://28241 (100.00), maa://66633 (100.00)</t>
         </is>
       </c>
       <c r="E61" s="14" t="inlineStr">
@@ -10827,7 +10827,7 @@
       </c>
       <c r="D66" s="13" t="inlineStr">
         <is>
-          <t>maa://28567 (97.56), **maa://20947 (45.71), maa://30525 (100.00), maa://38735 (100.00), *maa://28188 (70.00), maa://70681 (100.00), maa://30524 (100.00)</t>
+          <t>maa://28567 (97.62), **maa://20947 (45.71), maa://30525 (100.00), maa://38735 (100.00), *maa://28188 (70.00), maa://70681 (100.00), maa://30524 (100.00)</t>
         </is>
       </c>
       <c r="E66" s="14" t="inlineStr">
@@ -10989,7 +10989,7 @@
       </c>
       <c r="D69" s="13" t="inlineStr">
         <is>
-          <t>maa://20976 (98.46), maa://20815 (100.00)</t>
+          <t>maa://20976 (98.47), maa://20815 (100.00)</t>
         </is>
       </c>
       <c r="E69" s="14" t="inlineStr">
@@ -11043,7 +11043,7 @@
       </c>
       <c r="D70" s="13" t="inlineStr">
         <is>
-          <t>maa://20974 (97.12), maa://29079 (80.95), maa://29096 (91.67), maa://29087 (100.00), *maa://20823 (75.00), maa://20855 (94.44), maa://63722 (85.71), maa://20904 (100.00), *maa://72704 (66.67)</t>
+          <t>maa://20974 (97.12), maa://29079 (80.95), maa://29096 (91.67), maa://29087 (100.00), *maa://20823 (75.00), maa://20855 (94.44), maa://63722 (85.71), maa://20904 (100.00), **maa://72704 (50.00)</t>
         </is>
       </c>
       <c r="E70" s="14" t="inlineStr">
@@ -11097,7 +11097,7 @@
       </c>
       <c r="D71" s="13" t="inlineStr">
         <is>
-          <t>maa://20944 (96.43), maa://35393 (100.00)</t>
+          <t>maa://20944 (96.49), maa://35393 (100.00)</t>
         </is>
       </c>
       <c r="E71" s="14" t="inlineStr">
@@ -11151,7 +11151,7 @@
       </c>
       <c r="D72" s="13" t="inlineStr">
         <is>
-          <t>maa://20943 (99.50), maa://30673 (100.00), maa://30672 (100.00), maa://20856 (100.00), maa://71555 (85.71)</t>
+          <t>maa://20943 (99.50), maa://30673 (100.00), maa://30672 (100.00), maa://20856 (100.00), maa://71555 (90.00)</t>
         </is>
       </c>
       <c r="E72" s="14" t="inlineStr">
@@ -11205,7 +11205,7 @@
       </c>
       <c r="D73" s="13" t="inlineStr">
         <is>
-          <t>maa://36643 (98.55), maa://36864 (98.17), maa://39140 (100.00), maa://66335 (100.00)</t>
+          <t>maa://36643 (98.56), maa://36864 (98.17), maa://39140 (100.00), maa://66335 (100.00)</t>
         </is>
       </c>
       <c r="E73" s="14" t="inlineStr">
@@ -12609,7 +12609,7 @@
       </c>
       <c r="D99" s="13" t="inlineStr">
         <is>
-          <t>maa://20991 (100.00), maa://51015 (87.50)</t>
+          <t>maa://20991 (100.00), maa://51015 (87.72)</t>
         </is>
       </c>
       <c r="E99" s="14" t="inlineStr">
@@ -12717,7 +12717,7 @@
       </c>
       <c r="D101" s="13" t="inlineStr">
         <is>
-          <t>maa://20929 (93.75)</t>
+          <t>maa://20929 (93.94)</t>
         </is>
       </c>
       <c r="E101" s="14" t="inlineStr">
@@ -13203,7 +13203,7 @@
       </c>
       <c r="D110" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.70), maa://25018 (97.02), maa://25776 (92.77), maa://28361 (95.56), maa://25772 (94.12), maa://56588 (94.59), maa://45194 (86.36), maa://32653 (81.25), maa://25161 (84.21), maa://61839 (100.00), **maa://60902 (38.46), maa://61275 (100.00), *maa://73473 (75.00)</t>
+          <t>maa://51881 (98.71), maa://25018 (97.03), maa://25776 (92.77), maa://28361 (95.56), maa://25772 (94.12), maa://56588 (94.59), maa://45194 (86.36), maa://32653 (81.25), maa://25161 (84.21), maa://61839 (100.00), **maa://60902 (38.46), maa://61275 (100.00), *maa://73473 (75.00)</t>
         </is>
       </c>
       <c r="E110" s="14" t="inlineStr">
@@ -13797,7 +13797,7 @@
       </c>
       <c r="D121" s="13" t="inlineStr">
         <is>
-          <t>maa://20986 (94.44)</t>
+          <t>maa://20986 (89.47)</t>
         </is>
       </c>
       <c r="E121" s="14" t="inlineStr">
@@ -13959,7 +13959,7 @@
       </c>
       <c r="D124" s="13" t="inlineStr">
         <is>
-          <t>maa://20869 (100.00), maa://44690 (96.43)</t>
+          <t>maa://20869 (100.00), maa://44690 (96.55)</t>
         </is>
       </c>
       <c r="E124" s="14" t="inlineStr">
@@ -14445,7 +14445,7 @@
       </c>
       <c r="D133" s="13" t="inlineStr">
         <is>
-          <t>maa://21422 (98.99)</t>
+          <t>maa://21422 (99.01)</t>
         </is>
       </c>
       <c r="E133" s="14" t="inlineStr">
@@ -14985,7 +14985,7 @@
       </c>
       <c r="D143" s="13" t="inlineStr">
         <is>
-          <t>maa://45258 (91.67), **maa://30679 (50.00)</t>
+          <t>maa://45258 (88.00), **maa://30679 (50.00)</t>
         </is>
       </c>
       <c r="E143" s="14" t="inlineStr">
@@ -15147,7 +15147,7 @@
       </c>
       <c r="D146" s="13" t="inlineStr">
         <is>
-          <t>maa://28484 (98.00), *maa://23736 (53.49), maa://31185 (92.31), maa://30306 (100.00)</t>
+          <t>maa://28484 (98.02), *maa://23736 (53.49), maa://31185 (92.31), maa://30306 (100.00)</t>
         </is>
       </c>
       <c r="E146" s="14" t="inlineStr">
@@ -15525,7 +15525,7 @@
       </c>
       <c r="D153" s="13" t="inlineStr">
         <is>
-          <t>maa://40957 (94.75), maa://36641 (98.27), maa://36865 (95.63), maa://44635 (88.18), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (96.88), maa://42918 (100.00), maa://44119 (97.44), maa://64408 (95.24), maa://37300 (100.00), maa://42917 (100.00)</t>
+          <t>maa://40957 (94.78), maa://36641 (98.28), maa://36865 (95.65), maa://44635 (88.18), maa://44660 (92.68), maa://41128 (84.21), maa://46108 (96.88), maa://42918 (100.00), maa://44119 (97.44), maa://64408 (91.67), maa://37300 (100.00), maa://42917 (100.00)</t>
         </is>
       </c>
       <c r="E153" s="14" t="inlineStr">
@@ -16443,7 +16443,7 @@
       </c>
       <c r="D170" s="13" t="inlineStr">
         <is>
-          <t>maa://47950 (94.12), maa://20975 (91.67), maa://30806 (100.00)</t>
+          <t>maa://47950 (96.00), maa://20975 (91.67), maa://30806 (100.00)</t>
         </is>
       </c>
       <c r="E170" s="14" t="inlineStr">
@@ -16497,7 +16497,7 @@
       </c>
       <c r="D171" s="13" t="inlineStr">
         <is>
-          <t>maa://29633 (92.09), maa://29627 (92.98), maa://29659 (83.72), maa://49074 (94.29), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
+          <t>maa://29633 (91.80), maa://29627 (93.01), maa://29659 (83.72), maa://49074 (94.29), **maa://30679 (50.00), maa://29861 (100.00), maa://42343 (100.00)</t>
         </is>
       </c>
       <c r="E171" s="14" t="inlineStr">
@@ -16551,7 +16551,7 @@
       </c>
       <c r="D172" s="13" t="inlineStr">
         <is>
-          <t>maa://49867 (94.68), maa://49655 (98.04)</t>
+          <t>maa://49867 (94.85), maa://49655 (98.08)</t>
         </is>
       </c>
       <c r="E172" s="14" t="inlineStr">
@@ -18117,7 +18117,7 @@
       </c>
       <c r="D201" s="13" t="inlineStr">
         <is>
-          <t>maa://44224 (90.52), maa://35854 (84.75), maa://50388 (98.31), maa://25760 (86.55), ***maa://43911 (11.11), maa://63024 (96.55), *maa://20872 (52.00), maa://51066 (87.50), maa://70161 (100.00), *maa://72380 (75.00), maa://74410 (100.00)</t>
+          <t>maa://44224 (90.61), maa://35854 (84.75), maa://50388 (98.31), maa://25760 (86.55), ***maa://43911 (11.11), maa://63024 (96.67), *maa://20872 (52.00), maa://51066 (87.50), maa://70161 (100.00), *maa://72380 (75.00), maa://74410 (100.00)</t>
         </is>
       </c>
       <c r="E201" s="14" t="inlineStr">
@@ -19035,7 +19035,7 @@
       </c>
       <c r="D218" s="13" t="inlineStr">
         <is>
-          <t>maa://64044 (97.14)</t>
+          <t>maa://64044 (97.18)</t>
         </is>
       </c>
       <c r="E218" s="14" t="inlineStr">
@@ -19791,7 +19791,7 @@
       </c>
       <c r="D232" s="13" t="inlineStr">
         <is>
-          <t>maa://20987 (94.55), *maa://35801 (77.78)</t>
+          <t>maa://20987 (94.59), *maa://35801 (77.78)</t>
         </is>
       </c>
       <c r="E232" s="14" t="inlineStr">
@@ -20439,7 +20439,7 @@
       </c>
       <c r="D244" s="13" t="inlineStr">
         <is>
-          <t>maa://20922 (94.44), *maa://32623 (77.27), maa://34242 (85.71)</t>
+          <t>maa://20922 (94.52), *maa://32623 (77.27), maa://34242 (85.71)</t>
         </is>
       </c>
       <c r="E244" s="14" t="inlineStr">
@@ -20547,7 +20547,7 @@
       </c>
       <c r="D246" s="13" t="inlineStr">
         <is>
-          <t>*maa://30667 (78.98), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (59.09), maa://39588 (86.67), *maa://64079 (80.00), maa://65726 (84.62), maa://68226 (90.91)</t>
+          <t>*maa://30667 (79.02), maa://30666 (83.90), **maa://30739 (42.11), *maa://30723 (59.70), maa://39588 (86.67), *maa://64079 (80.00), maa://65726 (84.62), maa://68226 (92.31)</t>
         </is>
       </c>
       <c r="E246" s="14" t="inlineStr">
@@ -20601,7 +20601,7 @@
       </c>
       <c r="D247" s="13" t="inlineStr">
         <is>
-          <t>maa://62759 (100.00), maa://62764 (83.33), maa://70680 (100.00)</t>
+          <t>maa://62759 (100.00), maa://70680 (100.00), maa://62764 (83.33)</t>
         </is>
       </c>
       <c r="E247" s="14" t="inlineStr">
@@ -21033,7 +21033,7 @@
       </c>
       <c r="D255" s="13" t="inlineStr">
         <is>
-          <t>maa://28923 (91.55), maa://28906 (98.31), ***maa://28825 (11.54), maa://65613 (90.00)</t>
+          <t>maa://28923 (91.59), maa://28906 (98.31), ***maa://28825 (11.54), maa://65613 (90.00)</t>
         </is>
       </c>
       <c r="E255" s="14" t="inlineStr">
@@ -21087,7 +21087,7 @@
       </c>
       <c r="D256" s="13" t="inlineStr">
         <is>
-          <t>maa://42287 (93.64), maa://45570 (95.45), maa://60678 (93.75), maa://42225 (94.44)</t>
+          <t>maa://42287 (93.75), maa://45570 (95.45), maa://60678 (93.75), maa://42225 (94.44)</t>
         </is>
       </c>
       <c r="E256" s="14" t="inlineStr">
@@ -21249,7 +21249,7 @@
       </c>
       <c r="D259" s="13" t="inlineStr">
         <is>
-          <t>maa://31559 (94.23), maa://24093 (100.00), maa://20924 (95.24), **maa://49440 (37.50), maa://63591 (100.00)</t>
+          <t>maa://31559 (94.34), maa://24093 (100.00), maa://20924 (95.24), **maa://49440 (44.44), maa://63591 (100.00)</t>
         </is>
       </c>
       <c r="E259" s="14" t="inlineStr">
@@ -22437,7 +22437,7 @@
       </c>
       <c r="D281" s="13" t="inlineStr">
         <is>
-          <t>maa://51881 (98.70), maa://51630 (96.46), maa://56588 (94.59), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (38.46), *maa://66758 (76.92)</t>
+          <t>maa://51881 (98.71), maa://51630 (96.46), maa://56588 (94.59), *maa://55171 (60.87), maa://51893 (90.00), **maa://60902 (38.46), *maa://66758 (76.92)</t>
         </is>
       </c>
       <c r="E281" s="14" t="inlineStr">
@@ -22491,7 +22491,7 @@
       </c>
       <c r="D282" s="13" t="inlineStr">
         <is>
-          <t>maa://39163 (100.00)</t>
+          <t>maa://39163 (94.44)</t>
         </is>
       </c>
       <c r="E282" s="14" t="inlineStr">
@@ -23355,7 +23355,7 @@
       </c>
       <c r="D298" s="13" t="inlineStr">
         <is>
-          <t>maa://30710 (97.97), maa://36845 (95.95), maa://31558 (97.22), **maa://39217 (36.84), maa://30668 (87.10)</t>
+          <t>maa://30710 (97.99), maa://36845 (95.95), maa://31558 (97.22), **maa://39217 (36.84), maa://30668 (87.10)</t>
         </is>
       </c>
       <c r="E298" s="14" t="inlineStr">
@@ -24435,7 +24435,7 @@
       </c>
       <c r="D318" s="13" t="inlineStr">
         <is>
-          <t>maa://35859 (97.87)</t>
+          <t>maa://35859 (97.89)</t>
         </is>
       </c>
       <c r="E318" s="14" t="inlineStr">
@@ -25186,12 +25186,12 @@
       </c>
       <c r="C332" s="12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D332" s="15" t="inlineStr">
         <is>
-          <t>maa://39692 (99.57), maa://39810 (90.91)</t>
+          <t>maa://39692 (99.57), maa://39810 (90.91), maa://74041 (100.00)</t>
         </is>
       </c>
       <c r="E332" s="15" t="inlineStr">
@@ -26163,7 +26163,7 @@
       </c>
       <c r="D350" s="22" t="inlineStr">
         <is>
-          <t>maa://30671 (81.28), maa://30669 (99.36), maa://37275 (81.40), *maa://32410 (61.54), maa://41605 (100.00)</t>
+          <t>maa://30671 (81.28), maa://30669 (99.37), maa://37275 (81.40), *maa://32410 (61.54), maa://41605 (100.00)</t>
         </is>
       </c>
       <c r="E350" s="22" t="inlineStr">
@@ -26541,7 +26541,7 @@
       </c>
       <c r="D357" s="22" t="inlineStr">
         <is>
-          <t>maa://32647 (97.61), maa://32415 (83.70), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
+          <t>maa://32647 (97.61), maa://32415 (83.47), maa://34677 (100.00), maa://32892 (100.00), maa://32653 (81.25), maa://61839 (100.00), maa://61275 (100.00)</t>
         </is>
       </c>
       <c r="E357" s="22" t="inlineStr">
@@ -27027,7 +27027,7 @@
       </c>
       <c r="D366" s="22" t="inlineStr">
         <is>
-          <t>maa://36868 (99.40), maa://35996 (98.04), maa://47349 (98.04), **maa://39217 (36.84), maa://71203 (90.91)</t>
+          <t>maa://36868 (99.41), maa://35996 (98.04), maa://47349 (98.04), **maa://39217 (36.84), maa://71203 (92.31)</t>
         </is>
       </c>
       <c r="E366" s="22" t="inlineStr">
@@ -27081,7 +27081,7 @@
       </c>
       <c r="D367" s="22" t="inlineStr">
         <is>
-          <t>maa://49696 (99.62), maa://49695 (100.00), maa://49758 (98.85), *maa://52357 (78.95), *maa://59402 (56.25), *maa://63091 (64.71)</t>
+          <t>maa://49696 (99.62), maa://49695 (100.00), maa://49758 (98.85), *maa://52357 (78.95), *maa://59402 (56.25), *maa://63091 (66.67)</t>
         </is>
       </c>
       <c r="E367" s="22" t="inlineStr">
@@ -27351,7 +27351,7 @@
       </c>
       <c r="D372" s="22" t="inlineStr">
         <is>
-          <t>maa://36645 (98.48), maa://36841 (92.86), maa://37484 (94.34), maa://37858 (93.55), *maa://56268 (57.14), maa://40489 (100.00)</t>
+          <t>maa://36645 (98.49), maa://36841 (92.86), maa://37484 (94.34), maa://37858 (93.55), *maa://56268 (55.56), maa://40489 (100.00)</t>
         </is>
       </c>
       <c r="E372" s="22" t="inlineStr">
@@ -27405,7 +27405,7 @@
       </c>
       <c r="D373" s="22" t="inlineStr">
         <is>
-          <t>maa://42635 (94.83), maa://50629 (91.67), maa://48859 (100.00)</t>
+          <t>maa://42635 (94.83), maa://50629 (84.62), maa://48859 (100.00)</t>
         </is>
       </c>
       <c r="E373" s="22" t="inlineStr">
@@ -27567,7 +27567,7 @@
       </c>
       <c r="D376" s="22" t="inlineStr">
         <is>
-          <t>maa://40957 (94.75), maa://48026 (94.70), maa://44635 (88.18), maa://41035 (93.59), *maa://60251 (73.68), maa://44660 (92.68), maa://41128 (84.21)</t>
+          <t>maa://40957 (94.78), maa://48026 (94.74), maa://44635 (88.18), maa://41035 (93.59), *maa://60251 (73.68), maa://44660 (92.68), maa://41128 (84.21)</t>
         </is>
       </c>
       <c r="E376" s="22" t="inlineStr">
@@ -27837,7 +27837,7 @@
       </c>
       <c r="D381" s="22" t="inlineStr">
         <is>
-          <t>maa://71182 (96.61), maa://70756 (97.67), maa://71524 (100.00), maa://72244 (100.00)</t>
+          <t>maa://71182 (96.21), maa://70756 (97.67), maa://71524 (100.00), maa://72244 (100.00)</t>
         </is>
       </c>
       <c r="E381" s="22" t="inlineStr">
@@ -28539,7 +28539,7 @@
       </c>
       <c r="D395" t="inlineStr">
         <is>
-          <t>maa://42970 (80.35), maa://44745 (98.30), **maa://49516 (45.45), *maa://45952 (57.14), ***maa://46851 (10.00), *maa://44896 (72.73)</t>
+          <t>maa://42970 (80.49), maa://44745 (98.38), **maa://49516 (47.06), *maa://45952 (57.14), ***maa://46851 (10.00), *maa://44896 (72.73)</t>
         </is>
       </c>
       <c r="E395" t="inlineStr">
@@ -28836,7 +28836,7 @@
       </c>
       <c r="D406" t="inlineStr">
         <is>
-          <t>maa://59533 (96.36), maa://59577 (100.00)</t>
+          <t>maa://59533 (96.43), maa://59577 (100.00)</t>
         </is>
       </c>
       <c r="E406" t="inlineStr">
@@ -28971,7 +28971,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>maa://51872 (96.58), maa://51876 (99.12), maa://63228 (86.11), maa://51873 (98.04), maa://62047 (90.32)</t>
+          <t>maa://51872 (96.60), maa://51876 (99.12), maa://63228 (86.11), maa://51873 (98.04), maa://62047 (90.32)</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
@@ -29025,7 +29025,7 @@
       </c>
       <c r="D413" t="inlineStr">
         <is>
-          <t>maa://60449 (98.58), maa://59493 (96.95)</t>
+          <t>maa://60449 (98.60), maa://59493 (96.95)</t>
         </is>
       </c>
       <c r="E413" t="inlineStr">
@@ -29079,7 +29079,7 @@
       </c>
       <c r="D415" t="inlineStr">
         <is>
-          <t>maa://62756 (96.30)</t>
+          <t>maa://62756 (96.34)</t>
         </is>
       </c>
       <c r="E415" t="inlineStr">
@@ -29133,7 +29133,7 @@
       </c>
       <c r="D417" t="inlineStr">
         <is>
-          <t>maa://52505 (97.93), maa://64040 (99.15), maa://66377 (94.44), ***maa://66376 (14.29), ***maa://70187 (9.09)</t>
+          <t>maa://52505 (97.97), maa://64040 (99.16), maa://66377 (94.44), ***maa://66376 (14.29), ***maa://70187 (9.09)</t>
         </is>
       </c>
       <c r="E417" t="inlineStr">
@@ -29155,12 +29155,12 @@
       </c>
       <c r="C418" s="17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D418" t="inlineStr">
         <is>
-          <t>maa://73193 (100.00)</t>
+          <t>maa://73193 (100.00), maa://74820 (83.33)</t>
         </is>
       </c>
       <c r="E418" t="inlineStr">
@@ -29214,7 +29214,7 @@
       </c>
       <c r="D420" t="inlineStr">
         <is>
-          <t>maa://67388 (89.06), maa://71184 (84.00)</t>
+          <t>maa://67388 (89.06), maa://71184 (85.71)</t>
         </is>
       </c>
       <c r="E420" t="inlineStr">
@@ -29241,7 +29241,7 @@
       </c>
       <c r="D421" t="inlineStr">
         <is>
-          <t>maa://67089 (96.61), maa://67271 (92.59)</t>
+          <t>maa://67089 (96.67), maa://67271 (92.59)</t>
         </is>
       </c>
       <c r="E421" t="inlineStr">
@@ -29268,7 +29268,7 @@
       </c>
       <c r="D422" t="inlineStr">
         <is>
-          <t>maa://67088 (93.33)</t>
+          <t>maa://67088 (93.41)</t>
         </is>
       </c>
       <c r="E422" t="inlineStr">
@@ -29295,7 +29295,7 @@
       </c>
       <c r="D423" t="inlineStr">
         <is>
-          <t>maa://67087 (97.67),